<commit_message>
PDB construct selection script now apportions replicates for a given number of constructs.
</commit_message>
<xml_diff>
--- a/analysis/PDB_construct_selection/PDB_constructs.xlsx
+++ b/analysis/PDB_construct_selection/PDB_constructs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="229">
   <si>
     <t>ATGGAAAGCGACCTGCACCAGATCATCCACTCCTCACAGCCCCTCACACTGGAACACGTGCGCTACTTCCTGTACCAACTGCTGCGGGGCCTGAAGTACATGCACTCGGCTCAGGTCATCCACCGTGACCTGAAGCCCTCCAACCTATTGGTGAATGAGAACTGTGAGCTCAAGATTGGTGACTTTGGTATGGCTCGTGGCCTGTGCACCTCGCCCGCTGAACATCAGTACTTCATGACTGAGTATGTGGCCACGCGCTGGTACCGTGCGCCCGAGCTCATGCTCTCTTTGCATGAGTATACACAGGCTATTGACCTCTGGTCTGTGGGCTGCATCTTTGGTGAGATGCTGGCCCGGCGCCAGCTCTTCCCAGGCAAAAACTATGTACACCAGCTACAGCTCATCATGATGGTGCTGGGTACCCCATCACCAGCCGTGATTCAGGCTGTGGGGGCTGAGAGGGTGCGGGCCTATATCCAGAGCTTGCCACCACGCCAGCCTGTGCCCTGGGAGACAGTGTACCCAGGTGCCGACCGCCAGGCCCTATCACTGCTGGGTCGCATGCTGCGTTTTGAGCCCAGCGCTCGCATCTCAGCAGCTGCTGCCCTTCGCCACCCTTTCCTGGCCAAGTACCATGATCCTGATGATGAGCCTGACTGTGCCCCGCCCTTTGACTTTGCCTTTGACCGCGAAGCCCTCACTCGGGAGCGCATTAAGGAGGCCATTGTGGCTGAAATTGAGGACTTCCATGCAAGGCGTGAGGGCATCCGCCAACAGATCCGCTTCCAGCCTTCTCTACAGCCTGTGGCTAGTGAGCCTGGCTGTCCAGATGTTGAAATGCCCAGTCCCTGGGCTCCCAGTGGGGACTGTGCCATG</t>
   </si>
@@ -32,868 +32,676 @@
     <t>CDK6_HUMAN_D0_4EZ5_A</t>
   </si>
   <si>
+    <t>SPQREPQRVSHEQFRAALQLVVDPGDPRSYLDNFIKIGEGSTGIVCIATVRSSGKLVAVKKMDLRKQQRRELLFNEVVIMRDYQHENVVEMYNSYLVGDELWVVMEFLEGGALTDIVTHTRMNEEQIAAVCLAVLQALSVLHAQGVIHRDIKSDSILLTHDGRVKLSDFGFCAQVSKEVPRRKSLVGTPYWMAPELISRLPYGPEVDIWSLGIMVIEMVDGEPPYFNEPPLKAMKMIRDNLPPRLKNLHKVSPSLKGFLDRLLVRDPAQRATAAELLKHPFLAKAGPPASIVPLMRQNRTR</t>
+  </si>
+  <si>
+    <t>ELKDDDFEKISELGAGNGGVVFKVSHKPSGLVMARKLIHLEIKPAIRNQIIRELQVLHECNSPYIVGFYGAFYSDGEISICMEHMDGGSLDQVLKKAGRIPEQILGKVSIAVIKGLTYLREKHKIMHRAYGMDSRPPMAIFELLDYIVNEPPPKLPSGVFSLEFQDFVNKCLIKNPAERADLKQLMVHAFIKRSDAEEVDFAGWLCSTIGLN</t>
+  </si>
+  <si>
+    <t>PMYT1_HUMAN_D0_3P1A_A</t>
+  </si>
+  <si>
+    <t>GPEDELPDWAAAKEFYQKYDPKDVIGRGVSSVVRRCVHRATGHEFAVKIMEVTAERLSPEQLEEVREATRRETHILRQVAGHPHIITLIDSYESSSFMFLVFDLMRKGELFDYLTEKVALSEKETRSIMRSLLEAVSFLHANNIVHRDLKPENILLDDNMQIRLSDFGFSCHLEPGEKLRELCGTPGYLAPEILKCSMDETHPGYGKEVDLWACGVILFTLLAGSPPFWHRRQILMLRMIMEGQYQFSSPEWDDRSSTVKDLISRLLQVDPEARLTAEQALQHPFFER</t>
+  </si>
+  <si>
+    <t>GTGGAGGACCATTATGAGATGGGGGAGGAGCTGGGCAGCGGCCAGTTTGCGATCGTGCGGAAGTGCCGGCAGAAGGGCACGGGCAAGGAGTACGCAGCCAAGTTCATCAAGAAGCGCCGCCTGTCATCCAGCCGGCGTGGGGTGAGCCGGGAGGAGATCGAGCGGGAGGTGAACATCCTGCGGGAGATCCGGCACCCCAACATCATCACCCTGCACGACATCTTCGAGAACAAGACGGACGTGGTCCTCATCCTGGAGCTGGTCTCTGGCGGGGAGCTCTTTGACTTCCTGGCGGAGAAGGAGTCGCTGACGGAGGACGAGGCCACCCAGTTCCTCAAGCAGATCCTGGACGGCGTTCACTACCTGCACTCTAAGCGCATCGCACACTTTGACCTGAAGCCGGAAAACATCATGCTGCTGGACAAGAACGTGCCCAACCCACGAATCAAGCTCATCGACTTCGGCATCGCGCACAAGATCGAGGCGGGGAACGAGTTCAAGAACATCTTCGGCACCCCGGAGTTTGTGGCCCCAGAGATTGTGAACTATGAGCCGCTGGGCCTGGAGGCGGACATGTGGAGCATCGGTGTCATCACCTATATCCTCCTGAGCGGTGCATCCCCGTTCCTGGGCGAGACCAAGCAGGAGACGCTCACCAACATCTCAGCCGTGAACTACGACTTCGACGAGGAGTACTTCAGCAACACCAGCGAGCTGGCCAAGGACTTCATTCGCCGGCTGCTCGTCAAAGATCCCAAGCGGAGAATGACCATTGCCCAGAGCCTGGAACATTCCTGGATTAAGGCGATCCGGCGGCGGAACGTGCGTGGTGAGGACAGCGGC</t>
+  </si>
+  <si>
+    <t>TCAGTTTATCCTAAGGCATTAAGAGATGAATACATCATGTCAAAAACTCTTGGAAGTGGTGCCTGTGGAGAGGTAAAGCTGGCTTTCGAGAGGAAAACATGTAAGAAAGTAGCCATAAAGATCATCAGCAAAAGGAAGTTTGCTATTGGTTCAGCAAGAGAGGCAGACCCAGCTCTCAATGTTGAAACAGAAATAGAAATTTTGAAAAAGCTAAATCATCCTTGCATCATCAAGATTAAAAACTTTTTTGATGCAGAAGATTATTATATTGTTTTGGAATTGATGGAAGGGGGAGAGCTGTTTGACAAAGTGGTGGGGAATAAACGCCTGAAAGAAGCTACCTGCAAGCTCTATTTTTACCAGATGCTCTTGGCTGTGCAGTACCTTCATGAAAACGGTATTATACACCGTGACTTAAAGCCAGAGAATGTTTTACTGTCATCTCAAGAAGAGGACTGTCTTATAAAGATTACTGATTTTGGGCACTCCAAGATTTGGGGAGAGACCTCTCTCATGAGAACCTTATGTGGAACCCCCACCTACTTGGCGCCTGAAGTTCTTGTTTCTGTTGGGACTGCTGGGTATAACCGTGCTGTGGACTGCTGGAGTTTAGGAGTTATTCTTTTTATCTGCCTTAGTGGGTATCCACCTTTCTCTGAGCATAGGACTCAAGTGTCACTGAAGGATCAGATCACCAGTGGAAAATACAACTTCATTCCTGAAGTCTGGGCAGAAGTCTCAGAGAAAGCTCTGGACCTTGTCAAGAAGTTGTTGGTAGTGGATCCAAAGGCACGTTTTACGACAGAAGAAGCCTTAAGACACCCGTGGCTTCAGGATGAAGACATGAAGAGAAAGTTTCAAGATCTTCTGTCTGAGGAAAATGAATCCACAGCTCTACCCCAGGTTCTAGCCCAGCCTTCTACTAGTCGAAAGCGGCCCCGTGAAGGGGAAGCCGAGGGTGCCGAG</t>
+  </si>
+  <si>
+    <t>MSGPRAGFYRQELNKTVWEVPQRLQGLRPVGSGAYGSVCSAYDARLRQKVAVKKLSRPFQSLIHARRTYRELRLLKHLKHENVIGLLDVFTPATSIEDFSEVYLVTTLMGADLNNIVKCQALSDEHVQFLVYQLLRGLKYIHSAGIIHRDLKPSNVAVNEDCELRILDFGLARQADEEMTGYVATRWYRAPEIMLNWMHYNQTVDIWSVGCIMAELLQGKALFPGSDYIDQLKRIMEVVGTPSPEVLAKISSEHARTYIQSLPPMPQKDLSSIFRGANPLAIDLLGRMLVLDSDQRVSAAEALAHAYFSQYHDPEDEPEAEPYDESVEAKERTLEEWKELTYQEVLSFKPPEPPKPPGSLEIEQ</t>
+  </si>
+  <si>
+    <t>CSKP_HUMAN_D0_3TAC_A</t>
+  </si>
+  <si>
+    <t>MST4_HUMAN_D0_4FZD_B</t>
+  </si>
+  <si>
+    <t>MARK2_HUMAN_D0_3IEC_D</t>
+  </si>
+  <si>
+    <t>ACCGTGTTCAGGCAGGAAAACGTGGATGATTACTACGACACCGGCGAGGAACTTGGCAGTGGACAGTTTGCGGTTGTGAAGAAATGCCGTGAGAAAAGCACCGGCCTCCAGTATGCCGCCAAATTCATCAAGAAAAGGAGGACTAAGTCCAGCCGGCGGGGTGTGAGCCGCGAGGACATCGAGCGGGAGGTCAGCATCCTGAAGGAGATCCAGCACCCCAATGTCATCACCCTGCACGAGGTCTATGAGAACAAGACGGACGTCATCCTGATCTTGGAACTCGTTGCAGGTGGCGAGCTGTTTGACTTCTTAGCTGAAAAGGAATCTTTAACTGAAGAGGAAGCAACTGAATTTCTCAAACAAACTCTTAATGGTGTTTACTACCTGCACTCCCTTCAAATCGCCCACTTTGATCTTAAGCCTGAGAACATAATGCTTTTGGATAGAAATGTCCCCAAACCTCGGATCAAGATCATTGACTTTGGGTTGGCCCATAAAATTGACTTTGGAAATGAATTTAAAAACATATTTGGGACTCCAGAGTTTGTCGCTCCTGAGATAGTCAACTATGAACCTCTTGGTCTTGAGGCAGATATGTGGAGTATCGGGGTAATAACCTATATCCTCCTAAGTGGGGCCTCCCCATTTCTTGGAGACACTAAGCAAGAAACGTTAGCAAATGTATCCGCTGTCAACTACGAATTTGAGGATGAATACTTCAGTAATACCAGTGCCCTAGCCAAAGATTTCATAAGAAGACTTCTGGTCAAGGATCCAAAGAAGAGAATGACAATTCAAGATAGTTTGCAGCATCCCTGGATCAAGCCTAAAGATACACAACAGGCACTTAGT</t>
+  </si>
+  <si>
+    <t>CCATTTCCAGAAGGCAAGGTTCTGGATGATATGGAAGGCAATCAGTGGGTACTGGGCAAGAAGATTGGCTCTGGAGGATTTGGATTGATATATTTAGCTTTCCCCACAAATAAACCAGAGAAAGATGCAAGACATGTAGTAAAAGTGGAATATCAAGAAAATGGCCCGTTATTTTCAGAACTTAAATTTTATCAGAGAGTTGCAAAAAAAGACTGTATCAAAAAGTGGATAGAACGCAAACAACTTGATTATTTAGGAATTCCTCTGTTTTATGGATCTGGTCTGACTGAATTCAAGGGAAGAAGTTACAGATTTATGGTAATGGAAAGACTAGGAATAGATTTACAGAAGATCTCAGGCCAGAATGGTACCTTTAAAAAGTCAACTGTCCTGCAATTAGGTATCCGAATGTTGGATGTACTGGAATATATACATGAAAATGAATATGTTCATGGTGATATAAAAGCAGCAAATCTACTTTTGGGTTACAAAAATCCAGACCAGGTTTATCTTGCAGATTATGGACTTTCCTACAGATATTGTCCCAATGGGAACCACAAACAGTATCAGGAAAATCCTAGAAAAGGCCATAATGGGACAATAGAGTTTACCAGCTTGGATGCCCACAAGGGAGTAGCCTTGTCCAGACGAAGTGACGTTGAGATCCTCGGCTACTGCATGCTGCGGTGGTTGTGTGGGAAACTTCCCTGGGAACAGAACCTGAAGGACCCTGTGGCTGTGCAGACTGCTAAAACAAATCTGTTGGACGAGCTCCCCCAGTCAGTGCTTAAATGGGCTCCTTCTGGAAGCAGTTGCTGTGAAATAGCCCAATTTTTGGTATGTGCTCATAGTTTAGCATATGATGAAAAGCCAAACTATCAAGCCCTCAAGAAAATTTTGAACCCTCATGGAATACCTTTAGGACCACTGGACTTTTCCACAAAAGGACAGAGTATAAATGTCCAT</t>
+  </si>
+  <si>
+    <t>GGGGACTCTGATATATCCAGTCCATTACTGCAAAATACTGTCCACATTGACCTCAGTGCTCTAAATCCAGAGCTGGTCCAGGCAGTGCAGCATGTAGTGATTGGGCCCAGTAGCCTGATTGTGCATTTCAATGAAGTCATAGGAAGAGGGCATTTTGGTTGTGTATATCATGGGACTTTGTTGGACAATGATGGCAAGAAAATTCACTGTGCTGTGAAATCCTTGAACAGAATCACTGACATAGGAGAAGTTTCCCAATTTCTGACCGAGGGAATCATCATGAAAGATTTTAGTCATCCCAATGTCCTCTCGCTCCTGGGAATCTGCCTGCGAAGTGAAGGGTCTCCGCTGGTGGTCCTACCATACATGAAACATGGAGATCTTCGAAATTTCATTCGAAATGAGACTCATAATCCAACTGTAAAAGATCTTATTGGCTTTGGTCTTCAAGTAGCCAAAGGCATGAAATATCTTGCAAGCAAAAAGTTTGTCCACAGAGACTTGGCTGCAAGAAACTGTATGCTGGATGAAAAATTCACAGTCAAGGTTGCTGATTTTGGTCTTGCCAGAGACATGTATGATAAAGAATACTATAGTGTACACAACAAAACAGGTGCAAAGCTGCCAGTGAAGTGGATGGCTTTGGAAAGTCTGCAAACTCAAAAGTTTACCACCAAGTCAGATGTGTGGTCCTTTGGCGTGCTCCTCTGGGAGCTGATGACAAGAGGAGCCCCACCTTATCCTGACGTAAACACCTTTGATATAACTGTTTACTTGTTGCAAGGGAGAAGACTCCTACAACCCGAATACTGCCCAGACCCCTTATATGAAGTAATGCTAAAATGCTGGCACCCTAAAGCCGAAATGCGCCCATCCTTTTCTGAACTGGTGTCCCGGATATCAGCGATCTTCTCTACTTTCATTGGG</t>
+  </si>
+  <si>
+    <t>YQLFEELGKGAFSVVRRCVKVLAGQEYAAKIINTKKLSARDHQKLEREARICRLLKHPNIVRLHDSISEEGHHYLIFDLVTGGELFEDIVAREYYSEADASHCIQQILEAVLHCHQMGVVHRDLKPENLLLASKLKGAAVKLADFGLAIEVEGEQQAWFGFAGTPGYLSPEVLRKDPYGKPVDLWACGVILYILLVGYPPFWDEDQHRLYLQIKAGAYDFPSPEWDTVTPEAKDLINKMLTINPSKRITAAEALKHPWISHRSTVASCMHRQETVDCLKKFNARRKLKGA</t>
+  </si>
+  <si>
+    <t>ENFQKVEKIGEGTYGVVYKARNKLTGEVVALKKIRLDTETEGVPSTAIREISLLKELNHPNIVKLLDVIHTENKLYLVFEFLHQDLKKFMDASALTGIPLPLIKSYLFQLLQGLAFCHSHRVLHRDLKPQNLLINTEGAIKLADFGLARAFGVPVRTYTHEVVTLWYRAPEILLGCKYYSTAVDIWSLGCIFAEMVTRRALFPGDSEIDQLFRIFRTLGTPDEVVWPGVTSMPDYKPSFPKWARQDFSKVVPPLDEDGRSLLSQMLHYDPNKRISAKAALAHPFFQDVTKPVPHL</t>
+  </si>
+  <si>
+    <t>TTK_HUMAN_D0_3H9F_A</t>
+  </si>
+  <si>
+    <t>SVKGRIYSILKQIGSGGSSKVFQVLNEKKQIYAIKYVNLEEADNQTLDSYRNEIAYLNKLQQHSDKIIRLYDYEITDQYIYMVMECGNIDLNSWLKKKKSIDPWERKSYWKNMLEAVHTIHQHGIVHSDLKPANFLIVDGMLKLIDFGIANQMQPDTTSVVKDSQVGTVNYMPPEAIKDMSSSRENGKSKSKISPKSDVWSLGCILYYMTYGKTPFQQIINQISKLHAIIDPNHEIEFPDIPEKDLQDVLKCCLKRDPKQRISIPELLAHPYVQIQTHPVNQMAKGTTEE</t>
+  </si>
+  <si>
+    <t>GTGAAAGAATTCTTAGCCAAAGCCAAAGAAGATTTTCTTAAAAAATGGGAAAGTCCCGCTCAGAACACAGCCCACTTGGATCAGTTTGAACGAATCAAGACCCTCGGCACGGGCTCCTTCGGGCGGGTGATGCTGGTGAAACACAAGGAGACCGGGAACCACTATGCCATGAAGATCCTCGACAAACAGAAGGTGGTGAAACTGAAACAGATCGAACACACCCTGAATGAAAAGCGCATCCTGCAAGCTGTCAACTTTCCGTTCCTCGTCAAACTCGAGTTCTCCTTCAAGGACAACTCAAACTTATACATGGTCATGGAGTACGTGCCCGGCGGGGAGATGTTCTCACACCTACGGCGGATCGGAAGGTTCAGTGAGCCCCATGCCCGTTTCTACGCGGCCCAGATCGTCCTGACCTTTGAGTATCTGCACTCGCTGGATCTCATCTACAGGGACCTGAAGCCGGAGAATCTGCTCATTGACCAGCAGGGCTACATTCAGGTGACAGACTTCGGTTTCGCCAAGCGCGTGAAGGGCCGCACTTGGACCTTGTGCGGCACCCCTGAGTACCTGGCCCCTGAGATTATCCTGAGCAAAGGCTACAACAAGGCCGTGGACTGGTGGGCCCTGGGGGTTCTTATCTATGAAATGGCCGCTGGCTACCCGCCCTTCTTCGCAGACCAGCCCATCCAGATCTATGAGAAGATCGTCTCTGGGAAGGTGCGCTTCCCTTCCCACTTCAGCTCTGACTTGAAGGACCTGCTGCGGAACCTCCTGCAGGTAGATCTCACCAAGCGCTTTGGGAACCTCAAGAATGGGGTCAACGATATCAAGAACCACAAGTGGTTTGCCACAACTGACTGGATTGCCATCTACCAGAGGAAGGTGGAAGCTCCCTTCATACCAAAGTTTAAAGGCCCTGGGGATACGAGTAACTTTGACGACTATGAGGAAGAAGAAATCCGGGTCTCCATCAATGAGAAGTGTGGCAAGGAGTTTTCTGAGTTT</t>
+  </si>
+  <si>
+    <t>TCCCCCAACTACGACAAGTGGGAGATGGAACGCACGGACATCACCATGAAGCACAAGCTGGGCGGGGGCCAGTACGGGGAGGTGTACGAGGGCGTGTGGAAGAAATACAGCCTGACGGTGGCCGTGAAGACCTTGAAGGAGGACACCATGGAGGTGGAAGAGTTCTTGAAAGAAGCTGCAGTCATGAAAGAGATCAAACACCCTAACCTGGTGCAGCTCCTTGGGGTCTGCACCCGGGAGCCCCCGTTCTATATCATCACTGAGTTCATGACCTACGGGAACCTCCTGGACTACCTGAGGGAGTGCAACCGGCAGGAGGTGAACGCCGTGGTGCTGCTGTACATGGCCACTCAGATCTCGTCAGCCATGGAGTACCTGGAGAAGAAAAACTTCATCCACAGAGATCTTGCTGCCCGAAACTGCCTGGTAGGGGAGAACCACTTGGTGAAGGTAGCTGATTTTGGCCTGAGCAGGTTGATGACAGGGGACACCTACACAGCCCATGCTGGAGCCAAGTTCCCCATCAAATGGACTGCACCCGAGAGCCTGGCCTACAACAAGTTCTCCATCAAGTCCGACGTCTGGGCATTTGGAGTATTGCTTTGGGAAATTGCTACCTATGGCATGTCCCCTTACCCGGGAATTGACCTGTCCCAGGTGTATGAGCTGCTAGAGAAGGACTACCGCATGGAGCGCCCAGAAGGCTGCCCAGAGAAGGTCTATGAACTCATGCGAGCATGTTGGCAGTGGAATCCCTCTGACCGGCCCTCCTTTGCTGAAATCCACCAAGCCTTTGAAACAATGTTCCAGGAATCCAGTATCTCAGACGAAGTGGAAAAGGAGCTGGGGAAA</t>
+  </si>
+  <si>
+    <t>MK01_HUMAN_D0_4FMQ_A</t>
+  </si>
+  <si>
+    <t>KS6A1_HUMAN_D1_3RNY_B</t>
+  </si>
+  <si>
+    <t>ACCGACAGCTTCTCGGGCAGGTTTGAAGACGTCTACCAGCTGCAGGAAGATGTGCTGGGGGAGGGCGCTCATGCCCGAGTGCAGACCTGCATCAACCTGATCACCAGCCAGGAGTACGCCGTCAAGATCATTGAGAAGCAGCCAGGCCACATTCGGAGCAGGGTTTTCAGGGAGGTGGAGATGCTGTACCAGTGCCAGGGACACAGGAACGTCCTAGAGCTGATTGAGTTCTTCGAGGAGGAGGACCGCTTCTACCTGGTGTTTGAGAAGATGCGGGGAGGCTCCATCCTGAGCCACATCCACAAGCGCCGGCACTTCAACGAGCTGGAGGCCAGCGTGGTGGTGCAGGACGTGGCCAGCGCCTTGGACTTTCTGCATAACAAAGGCATCGCCCACAGGGACCTAAAGCCGGAAAACATCCTCTGTGAGCACCCCAACCAGGTCTCCCCCGTGAAGATCTGTGACTTCGACCTGGGCAGCGGCATCAAACTCAACGGGGACTGCTCCCCTATCTCCACCCCGGAGCTGCTCACTCCGTGCGGCTCGGCGGAGTACATGGCCCCGGAGGTAGTGGAGGCCTTCAGCGAGGAGGCTAGCATCTACGACAAGCGCTGCGACCTGTGGAGCCTGGGCGTCATCTTGTATATCCTACTCAGCGGCTACCCGCCCTTCGTGGGCCGCTGTGGCAGCGACTGCGGCTGGGACCGCGGCGAGGCCTGCCCTGCCTGCCAGAACATGCTGTTTGAGAGCATCCAGGAGGGCAAGTACGAGTTCCCCGACAAGGACTGGGCCCACATCTCCTGCGCTGCCAAAGACCTCATCTCCAAGCTGCTGGTCCGTGACGCCAAGCAGAGGCTGAGTGCCGCCCAAGTCCTGCAGCACCCCTGGGTTCAGGGGTGCGCCCCGGAGAACACCTTGCCCACTCCCATGGTCCTGCAGAGG</t>
+  </si>
+  <si>
+    <t>MSRSKRDNNFYSVEIGDSTFTVLKRYQNLKPIGSGAQGIVCAAYDAILERNVAIKKLSRPFQNQTHAKRAYRELVLMKCVNHKNIIGLLNVFTPQKSLEEFQDVYIVMELMDANLCQVIQMELDHERMSYLLYQMLCGIKHLHSAGIIHRDLKPSNIVVKSDCTLKILDFGLARTAGTSFMMTPYVVTRYYRAPEVILGMGYKENVDLWSVGCIMGEMVCHKILFPGRDYIDQWNKVIEQLGTPCPEFMKKLQPTVRTYVENRPKYAGYSFEKLFPDVLFPADSEHNKLKASQARDLLSKMLVIDASKRISVDEALQHPYINVWYDPSEAEAPPPKIPDKQLDEREHTIEEWKELIYKEVMDLE</t>
+  </si>
+  <si>
+    <t>STRAA_HUMAN_D0_3GNI_B</t>
+  </si>
+  <si>
+    <t>MP2K2_HUMAN_D0_1S9I_A</t>
+  </si>
+  <si>
+    <t>PIM1_HUMAN_D0_4A7C_A</t>
+  </si>
+  <si>
+    <t>EAFLTQKAKVGELKDDDFERISELGAGNGGVVTKVQHRPSGLIMARKLIHLEIKPAIRNQIIRELQVLHECNSPYIVGFYGAFYSDGEISICMEHMDGGSLDQVLKEAKRIPEEILGKVSIAVLRGLAYLREKHQIMHRDVKPSNILVNSRGEIKLCDFGVSGQLIDSMANSFVGTRSYMAPERLQGTHYSVQSDIWSMGLSLVELAVGRYPIPPPDAKELEAIFGRPVVDGEEGEPHSISPRPRPPGRPVSGHGMDSRPAMAIFELLDYIVNEPPPKLPNGVFTPDFQEFVNKCLIKNPAERADLKMLTNHTFIKRSEVEEVDFAGWLCKTLRLNQPGTPTRTAV</t>
+  </si>
+  <si>
+    <t>GGGCCGGAGGATGAGCTGCCCGACTGGGCCGCCGCCAAAGAGTTTTACCAGAAGTACGACCCTAAGGACGTCATCGGCAGAGGAGTGAGCTCTGTGGTCCGCCGTTGTGTTCATCGAGCTACTGGCCACGAGTTTGCGGTGAAGATTATGGAAGTGACAGCTGAGCGGCTGAGTCCTGAGCAGCTGGAGGAGGTGCGGGAAGCCACACGGCGAGAGACACACATCCTTCGCCAGGTCGCCGGCCACCCCCACATCATCACCCTCATCGATTCCTACGAGTCTTCTAGCTTCATGTTCCTGGTGTTTGACCTGATGCGGAAGGGAGAGCTGTTTGACTATCTCACAGAGAAGGTGGCCCTCTCTGAAAAGGAAACCAGGTCCATCATGCGGTCTCTGCTGGAAGCAGTGAGCTTTCTCCATGCCAACAACATTGTGCATCGAGATCTGAAGCCCGAGAATATTCTCCTAGATGACAATATGCAGATCCGACTTTCAGATTTCGGGTTCTCCTGCCACTTGGAACCTGGCGAGAAGCTTCGAGAGTTGTGTGGGACCCCAGGGTATCTAGCGCCAGAGATCCTTAAATGCTCCATGGATGAAACCCACCCAGGCTATGGCAAGGAGGTCGACCTCTGGGCCTGTGGGGTGATCTTGTTCACACTCCTGGCTGGCTCGCCACCCTTCTGGCACCGGCGGCAGATCCTGATGTTACGCATGATCATGGAGGGCCAGTACCAGTTCAGTTCCCCCGAGTGGGATGACCGTTCCAGCACTGTCAAAGACCTGATCTCCAGGCTGCTGCAGGTGGATCCTGAGGCACGCCTGACAGCTGAGCAGGCCCTACAGCACCCCTTCTTTGAGCGT</t>
+  </si>
+  <si>
+    <t>KC1E_HUMAN_D0_4HNI_A</t>
+  </si>
+  <si>
+    <t>VRK2_HUMAN_D0_2V62_B</t>
+  </si>
+  <si>
+    <t>ETYIKLDKLGEGTYATVYKGKSKLTDNLVALKEIRLEHEEGAPCTAIREVSLLKDLKHANIVTLHDIIHTEKSLTLVFEYLDKDLKQYLDDCGNIINMHNVKLFLFQLLRGLAYCHRQKVLHRDLKPQNLLINERGELKLADFGLARAKSIPTKTYSNEVVTLWYRPPDILLGSTDYSTQIDMWGVGCIFYEMATGRPLFPGSTVEEQLHFIFRILGTPTEETWPGILSNEEFKTYNYPKYRAEALLSHAPRLDSDGADLLTKLLQFEGRNRISAEDAMKHPFFLSLGERIHKLPDTTSIFALKEIQLQKEASLRS</t>
+  </si>
+  <si>
+    <t>HQLQPRRVSFRGEASETLQSPGYDPSRPESFFQQSFQRLSRLGHGSYGEVFKVRSKEDGRLYAVKRSMSPFRGPKDRARKLAEVGSHEKVGQHPCCVRLEQAWEEGGILYLQTELCGPSLQQHCEAWGASLPEAQVWGYLRDTLLALAHLHSQGLVHLDVKPANIFLGPRGRCKLGDFGLLVELGTAGAGEVQEGDPRYMAPELLQGSYGTAADVFSLGLTILEVACNMELPHGGEGWQQLRQGYLPPEFTAGLSSELRSVLVMMLEPDPKLRATAEALLALPVLRQP</t>
+  </si>
+  <si>
+    <t>aa_end</t>
+  </si>
+  <si>
+    <t>TACCAGCTCTTCGAGGAATTGGGCAAGGGAGCCTTCTCGGTGGTGCGAAGGTGTGTGAAGGTGCTGGCTGGCCAGGAGTATGCTGCCAAGATCATCAACACAAAGAAGCTGTCAGCCAGAGACCATCAGAAGCTGGAGCGTGAAGCCCGCATCTGCCGCCTGCTGAAGCACCCCAACATCGTCCGACTACATGACAGCATCTCAGAGGAGGGACACCACTACCTGATCTTCGACCTGGTCACTGGTGGGGAACTGTTTGAAGATATCGTGGCCCGGGAGTATTACAGTGAGGCGGATGCCAGTCACTGTATCCAGCAGATCCTGGAGGCTGTGCTGCACTGCCACCAGATGGGGGTGGTGCACCGGGACCTGAAGCCTGAGAATCTGTTGCTGGCCTCCAAGCTCAAGGGTGCCGCAGTGAAGCTGGCAGACTTTGGCCTGGCCATAGAGGTGGAGGGGGAGCAGCAGGCATGGTTTGGGTTTGCAGGGACTCCTGGATATCTCTCCCCAGAAGTGCTGCGGAAGGACCCGTACGGGAAGCCTGTGGACCTGTGGGCTTGTGGGGTCATCCTGTACATCCTGCTGGTTGGGTACCCCCCGTTCTGGGATGAGGACCAGCACCGCCTGTACCTGCAGATCAAAGCCGGCGCCTATGATTTCCCATCGCCGGAATGGGACACTGTCACCCCGGAAGCCAAGGATCTGATCAATAAGATGCTGACCATTAACCCATCCAAACGCATCACAGCTGCCGAAGCCCTTAAGCACCCCTGGATCTCGCACCGCTCCACCGTGGCATCCTGCATGCACAGACAGGAGACCGTGGACTGCCTGAAGAAGTTCAATGCCAGGAGGAAACTGAAGGGAGCC</t>
+  </si>
+  <si>
+    <t>MK08_HUMAN_D0_2NO3_A</t>
+  </si>
+  <si>
+    <t>TCGGTTAAAGGAAGAATTTATTCCATATTAAAGCAGATAGGAAGTGGAGGTTCAAGCAAGGTATTTCAGGTGTTAAATGAAAAGAAACAGATATATGCTATAAAATATGTGAACTTAGAAGAAGCAGATAACCAAACTCTTGATAGTTACCGGAACGAAATAGCTTATTTGAATAAACTACAACAACACAGTGATAAGATCATCCGACTTTATGATTATGAAATCACGGACCAGTACATCTACATGGTAATGGAGTGTGGAAATATTGATCTTAATAGTTGGCTTAAAAAGAAAAAATCCATTGATCCATGGGAACGCAAGAGTTACTGGAAAAATATGTTAGAGGCAGTTCACACAATCCATCAACATGGCATTGTTCACAGTGATCTTAAACCAGCTAACTTTCTGATAGTTGATGGAATGCTAAAGCTAATTGATTTTGGGATTGCAAACCAAATGCAACCAGATACAACAAGTGTTGTTAAAGATTCTCAGGTTGGCACAGTTAATTATATGCCACCAGAAGCAATCAAAGATATGTCTTCCTCCAGAGAGAATGGGAAATCTAAGTCAAAGATAAGCCCCAAAAGTGATGTTTGGTCCTTAGGATGTATTTTGTACTATATGACTTACGGGAAAACACCATTTCAGCAGATAATTAATCAGATTTCTAAATTACATGCCATAATTGATCCTAATCATGAAATTGAATTTCCCGATATTCCAGAGAAAGATCTTCAAGATGTGTTAAAGTGTTGTTTAAAAAGGGACCCAAAACAGAGGATATCCATTCCTGAGCTCCTGGCTCATCCATATGTTCAAATTCAAACTCATCCAGTTAACCAAATGGCCAAGGGAACCACTGAAGAA</t>
+  </si>
+  <si>
+    <t>PAK1_HUMAN_D0_3Q52_A</t>
+  </si>
+  <si>
+    <t>CDK9_HUMAN_D0_4IMY_A</t>
+  </si>
+  <si>
+    <t>GAAACAAAGTATACTGTGGACAAGAGGTTTGGCATGGATTTTAAAGAAATAGAATTAATTGGCTCAGGTGGATTTGGCCAAGTTTTCAAAGCAAAACACAGAATTGACGGAAAGACTTACGTTATTAAACGTGTTAAATATAATAACGAGAAGGCGGAGCGTGAAGTAAAAGCATTGGCAAAACTTGATCATGTAAATATTGTTCACTACAATGGCTGTTGGGATGGATTTGATTATGATCCTGAGACCAGTGATGATTCTCTTGAGAGCAGTGATTATGATCCTGAGAACAGCAAAAATAGTTCAAGGTCAAAGACTAAGTGCCTTTTCATCCAAATGGAATTCTGTGATAAAGGGACCTTGGAACAATGGATTGAAAAAAGAAGAGGCGAGAAACTAGACAAAGTTTTGGCTTTGGAACTCTTTGAACAAATAACAAAAGGGGTGGATTATATACATTCAAAAAAATTAATTCATAGAGATCTTAAGCCAAGTAATATATTCTTAGTAGATACAAAACAAGTAAAGATTGGAGACTTTGGACTTGTAACATCTCTGAAAAATGATGGAAAGCGAACAAGGAGTAAGGGAACTTTGCGATACATGAGCCCAGAACAGATTTCTTCGCAAGACTATGGAAAGGAAGTGGACCTCTACGCTTTGGGGCTAATTCTTGCTGAACTTCTTCATGTATGTGACACTGCTTTTGAAACATCAAAGTTTTTCACAGACCTACGGGATGGCATCATCTCAGATATATTTGATAAAAAAGAAAAAACTCTTCTACAGAAATTACTCTCAAAGAAACCTGAGGATCGACCTAACACATCTGAAATACTAAGGACCTTGACTGTGTGGAAGAAAAGCCCAGAGAAAAATGAACGACACACATGT</t>
+  </si>
+  <si>
+    <t>PAK7_HUMAN_D0_2F57_B</t>
+  </si>
+  <si>
+    <t>RDSSDDWEIPDGQITVGQRIGSGSFGTVYKGKWHGDVAVKMLNVTAPTPQQLQAFKNEVGVLRKTRHVNILLFMGYSTKPQLAIVTQWCEGSSLYHHLHIIETKFEMIKLIDIARQTAQGMDYLHAKSIIHRDLKSNNIFLHEDLTVKIGDFGLATVKSRWSGSHQFEQLSGSILWMAPEVIRMQDKNPYSFQSDVYAFGIVLYELMTGQLPYSNINNRDQIIFMVGRGYLSPDLSKVRSNCPKAMKRLMAECLKKKRDERPLFPQILASIELLAR</t>
+  </si>
+  <si>
+    <t>GAGAACTTCCAAAAGGTGGAAAAGATCGGAGAGGGCACGTACGGAGTTGTGTACAAAGCCAGAAACAAGTTGACGGGAGAGGTGGTGGCGCTTAAGAAAATCCGCCTGGACACTGAGACTGAGGGTGTGCCCAGTACTGCCATCCGAGAGATCTCTCTGCTTAAGGAGCTTAACCATCCTAATATTGTCAAGCTGCTGGATGTCATTCACACAGAAAATAAACTCTACCTGGTTTTTGAATTTCTGCACCAAGATCTCAAGAAATTCATGGATGCCTCTGCTCTCACTGGCATTCCTCTTCCCCTCATCAAGAGCTATCTGTTCCAGCTGCTCCAGGGCCTAGCTTTCTGCCATTCTCATCGGGTCCTCCACCGAGACCTTAAACCTCAGAATCTGCTTATTAACACAGAGGGGGCCATCAAGCTAGCAGACTTTGGACTAGCCAGAGCTTTTGGAGTCCCTGTTCGTACTTACACCCATGAGGTGGTGACCCTGTGGTACCGAGCTCCTGAAATCCTCCTGGGCTGCAAATATTATTCCACAGCTGTGGACATCTGGAGCCTGGGCTGCATCTTTGCTGAGATGGTGACTCGCCGGGCCCTATTCCCTGGAGATTCTGAGATTGACCAGCTCTTCCGGATCTTTCGGACTCTGGGGACCCCAGATGAGGTGGTGTGGCCAGGAGTTACTTCTATGCCTGATTACAAGCCAAGTTTCCCCAAGTGGGCCCGGCAAGATTTTAGTAAAGTTGTACCTCCCCTGGATGAAGATGGACGGAGCTTGTTATCGCAAATGCTGCACTACGACCCTAACAAGCGGATTTCGGCCAAGGCAGCCCTGGCTCACCCTTTCTTCCAGGATGTGACCAAGCCAGTACCCCATCTT</t>
+  </si>
+  <si>
+    <t>GGGGAATGCAGTCAGAAGGGTCCTGTCCCCTTTAGCCATTGCCTTCCCACAGAAAAACTGCAACGCTGTGAGAAGATTGGGGAAGGGGTGTTTGGCGAAGTGTTTCAAACAATTGCTGATCACACACCCGTAGCCATAAAAATCATTGCTATTGAAGGACCAGATTTAGTCAATGGATCCCATCAGAAAACCTTTGAGGAAATCCTGCCAGAGATCATCATCTCCAAAGAGTTGAGCCTCTTATCCGGTGAAGTGTGCAACCGCACAGAAGGCTTTATCGGGCTGAACTCAGTGCACTGTGTCCAGGGATCTTACCCTCCCTTGCTCCTCAAAGCCTGGGATCACTATAATTCAACCAAAGGCTCTGCAAATGACCGGCCTGATTTTTTTAAAGACGACCAGCTCTTCATTGTGCTGGAATTTGAGTTTGGAGGGATTGACTTAGAGCAAATGCGAACCAAGTTGTCTTCCTTGGCTACTGCAAAGAGCATTCTACACCAGCTCACAGCCTCCCTCGCAGTGGCAGAGGCATCACTGCGCTTTGAGCACCGAGACTTACACTGGGGGAACGTGCTCTTAAAGAAAACCAGCCTCAAAAAACTCCACTACACCCTCAATGGGAAGAGCAGCACTATCCCCAGCTGTGGGTTGCAAGTGAGCATCATTGACTACACCCTGTCGCGCTTGGAACGGGATGGGATTGTGGTTTTCTGTGACGTTTCCATGGATGAGGACCTGTTTACCGGTGACGGTGACTACCAGTTTGACATCTACAGGCTCATGAAGAAGGAGAATAACAACCGCTGGGGTGAATATCACCCTTATAGTAATGTGCTCTGGTTACATTACCTGACAGACAAGATGCTGAAACAAATGACCTTCAAGACTAAATGTAACACTCCTGCCATGAAGCAAATTAAGAGAAAAATCCAGGAGTTCCACAGGACAATGCTGAACTTCAGCTCTGCCACTGACTTGCTCTGCCAGCACAGACTGTTTAAG</t>
+  </si>
+  <si>
+    <t>TDSLPGKFEDMYKLTSELLGEGAYAKVQGAVSLQNGKEYAVKIIEKQAGHSRSRVFREVETLYQCQGNKNILELIEFFEDDTRFYLVFEKLQGGSILAHIQKQKHFNEREASRVVRDVAAALDFLHTKDKVSLCHLGGSARAPSGLTAAPTSLGSSDPPTSASQVAGTTGIDHRDLKPENILCESPEKVSPVKICDFDLGSGMKLNNSCTPITTPELTTPCGSAEYMAPEVGEVFTDQATFYDKRCDLWSLGVVLYIMLSGYPPFVGHCGADCGWDRGEVCRVCQNKLFESIQEGKYEFPDKDWAHISSEAKDLISKLLVRDAKQRLSAAQVLQHPWVQGQAPEKG</t>
+  </si>
+  <si>
+    <t>VRK3_HUMAN_D0_2JII_A</t>
+  </si>
+  <si>
+    <t>ATGAGCCTCATCCGGAAAAAGGGCTTCTACAAGCAGGACGTCAACAAGACCGCCTGGGAGCTGCCCAAGACCTACGTGTCCCCGACGCACGTCGGCAGCGGGGCCTATGGCTCCGTGTGCTCGGCCATCGACAAGCGGTCAGGGGAGAAGGTGGCCATCAAGAAGCTGAGCCGACCCTTTCAGTCCGAGATCTTCGCCAAGCGCGCCTACCGGGAGCTGCTGCTGCTGAAGCACATGCAGCATGAGAACGTCATTGGGCTCCTGGATGTCTTCACCCCAGCCTCCTCCCTGCGCAACTTCTATGACTTCTACCTGGTGATGCCCTTCATGCAGACGGATCTGCAGAAGATCATGGGGATGGAGTTCAGTGAGGAGAAGATCCAGTACCTGGTGTATCAGATGCTCAAAGGCCTTAAGTACATCCACTCTGCTGGGGTCGTGCACAGGGACCTGAAGCCAGGCAACCTGGCTGTGAATGAGGACTGTGAACTGAAGATTCTGGATTTTGGGCTGGCGCGACATGCAGACGCCGAGATGACTGGCTACGTGGTGACCCGCTGGTACCGAGCCCCCGAGGTGATCCTCAGCTGGATGCACTACAACCAGACAGTGGACATCTGGTCTGTGGTCTGTATCATGGCAGAGATGCTGACAGGGAAAACTCTGTTCAAGGGGAAAGATTACCTGGACCAGCTGACCCAGATCCTGAAAGTGACCGGGGTGCCTGGCACGGAGTTTGTGCAGAAGCTGAACGACAAAGCGGCCAAATCCTACATCCAGTCCCTGCCACAGACCCCCAGGAAGGATTTCACTCAGCTGTTCCCACGGGCCAGCCCCCAGGCTGCGGACCTGCTGGAGAAGATGCTGGAGCTAGACGTGGACAAGCGCCTGACGGCCGCGCAGGCCCTCACCCATCCCTTCTTTGAACCCTTCCGGGACCCTGAGGAAGAGACGGAGGCCCAGCAGCCGTTTGATGATTCCTTAGAACACGAGAAACTCACAGTGGATGAATGGAAGCAGCACATCTACAAGGAGATTGTGAACTTCAGCCCCATT</t>
+  </si>
+  <si>
+    <t>ACTGACTCCTTGCCAGGAAAGTTTGAAGATATGTACAAGCTGACCTCTGAATTGCTGGGAGAGGGAGCCTATGCCAAAGTTCAAGGTGCCGTGAGCCTACAGAATGGCAAAGAGTATGCCGTCAAAATCATCGAGAAACAAGCAGGGCACAGTCGGAGTAGGGTGTTTCGAGAGGTGGAGACGCTGTATCAGTGTCAGGGAAACAAGAACATTTTGGAGCTGATTGAGTTCTTTGAAGATGACACAAGGTTTTACTTGGTCTTTGAGAAATTGCAAGGAGGTTCCATCTTAGCCCACATCCAGAAGCAAAAGCACTTCAATGAGCGAGAAGCCAGCCGAGTGGTGCGGGACGTTGCTGCTGCCCTTGACTTCCTGCATACCAAAGACAAAGTCTCTCTCTGTCACCTAGGCGGGAGTGCTAGGGCGCCATCAGGGCTCACTGCAGCCCCAACCTCCCTGGGCTCCAGTGATCCTCCCACCTCAGCCTCCCAAGTAGCTGGGACTACAGGCATTGATCATCGTGATCTGAAACCAGAAAATATATTGTGTGAATCTCCAGAAAAGGTGTCTCCAGTGAAAATCTGTGACTTTGACTTGGGCAGTGGGATGAAACTGAACAACTCCTGTACCCCCATAACCACACCAGAGCTGACCACCCCATGTGGCTCTGCAGAATACATGGCCCCTGAGGTAGGGGAGGTCTTCACGGACCAGGCCACATTCTACGACAAGCGCTGTGACCTGTGGAGCCTGGGCGTGGTCCTCTACATCATGCTGAGTGGCTACCCACCCTTCGTGGGTCACTGCGGGGCCGACTGTGGCTGGGACCGGGGCGAGGTCTGCAGGGTGTGCCAGAACAAGCTGTTTGAAAGCATCCAGGAAGGCAAGTATGAGTTTCCTGACAAGGACTGGGCACACATCTCCAGTGAAGCCAAAGACCTCATCTCCAAGCTCCTGGTGCGAGATGCAAAGCAGAGACTTAGCGCCGCCCAAGTTCTGCAGCACCCATGGGTGCAGGGGCAAGCTCCAGAAAAGGGA</t>
+  </si>
+  <si>
+    <t>PAK4_HUMAN_D0_2J0I_A</t>
+  </si>
+  <si>
+    <t>AGVSEYELPEDPRWELPRDRLVLGKPLGEGCFGQVVLAEAIGLDKDKPNRVTKVAVKMLKSDATEKDLSDLISEMEMMKMIGKHKNIINLLGACTQDGPLYVIVEYASKGNLREYLQARRPPGLEYCYNPSHNPEEQLSSKDLVSCAYQVARGMEYLASKKCIHRDLAARNVLVTEDNVMKIADFGLARDIHHIDYYKKTTNGRLPVKWMAPEALFDRIYTHQSDVWSFGVLLWEIFTLGGSPYPGVPVEELFKLLKEGHRMDKPSNCTNELYMMMRDCWHAVPSQRPTFKQLVEDLDRIVALTSNQEYLDLSMPLD</t>
+  </si>
+  <si>
+    <t>MAAAAAQGGGGGEPRRTEGVGPGVPGEVEMVKGQPFDVGPRYTQLQYIGEGAYGMVSSAYDHVRKTRVAIKKISPFEHQTYCQRTLREIQILLRFRHENVIGIRDILRASTLEAMRDVYIVQDLMETDLYKLLKSQQLSNDHICYFLYQILRGLKYIHSANVLHRDLKPSNLLINTTCDLKICDFGLARIADPEHDHTGFLTEYVATRWYRAPEIMLNSKGYTKSIDIWSVGCILAEMLSNRPIFPGKHYLDQLNHILGILGSPSQEDLNCIINMKARNYLQSLPSKTKVAWAKLFPKSDSKALDLLDRMLTFNPNKRITVEEALAHPYLEQYYDPTDEPVAEEPFTFAMELDDLPKERLKELIFQETARFQPGVLEAP</t>
+  </si>
+  <si>
+    <t>GAGCCCAAGAAGTACGCAGTGACCGACGACTACCAGTTGTCCAAGCAGGTGCTGGGCCTGGGTGTGAACGGCAAAGTGCTGGAGTGCTTCCATCGGCGCACTGGACAGAAGTGTGCCCTGAAGCTCCTGTATGACAGCCCCAAGGCCCGGCAGGAGGTAGACCATCACTGGCAGGCTTCTGGCGGCCCCCATATTGTCTGCATCCTGGATGTGTATGAGAACATGCACCATGGCAAGCGCTGTCTCCTCATCATCATGGAATGCATGGAAGGTGGTGAGTTGTTCAGCAGGATTCAGGAGCGTGGCGACCAGGCTTTCACTGAGAGAGAAGCTGCAGAGATAATGCGGGATATTGGCACTGCCATCCAGTTTCTGCACAGCCATAACATTGCCCACCGAGATGTCAAGCCTGAAAACCTACTCTACACATCTAAGGAGAAAGACGCAGTGCTTAAGCTCACCGATTTTGGCTTTGCTAAGGAGACCACCCAAAATGCCCTGCAGACACCCTGCTATACTCCCTATTATGTGGCCCCTGAGGTCCTGGGTCCAGAGAAGTATGACAAGTCATGTGACATGTGGTCCCTGGGTGTCATCATGTACATCCTCCTTTGTGGCTTCCCACCCTTCTACTCCAACACGGGCCAGGCCATCTCCCCGGGGATGAAGAGGAGGATTCGCCTGGGCCAGTACGGCTTCCCCAATCCTGAGTGGTCAGAAGTCTCTGAGGATGCCAAGCAGCTGATCCGCCTCCTGTTGAAGACAGACCCCACAGAGAGGCTGACCATCACTCAGTTCATGAACCACCCCTGGATCAACCAATCGATGGTAGTGCCACAGACCCCACTCCACACGGCCCGAGTGCTGCAGGAGGACAAAGACCACTGGGACGAAGTCAAGGAGGAGATGACCAGTGCCTTGGCCACTATGCGGGTAGACTACGACCAGGTG</t>
+  </si>
+  <si>
+    <t>ATGTCTCAGGAGAGGCCCACGTTCTACCGGCAGGAGCTGAACAAGACAATCTGGGAGGTGCCCGAGCGTTACCAGAACCTGTCTCCAGTGGGCTCTGGCGCCTATGGCTCTGTGTGTGCTGCTTTTGACACAAAAACGGGGTTACGTGTGGCAGTGAAGAAGCTCTCCAGACCATTTCAGTCCATCATTCATGCGAAAAGAACCTACAGAGAACTGCGGTTACTTAAACATATGAAACATGAAAATGTGATTGGTCTGTTGGACGTTTTTACACCTGCAAGGTCTCTGGAGGAATTCAATGATGTGTATCTGGTGACCCATCTCATGGGGGCAGATCTGAACAACATTGTGAAATGTCAGAAGCTTACAGATGACCATGTTCAGTTCCTTATCTACCAAATTCTCCGAGGTCTAAAGTATATACATTCAGCTGACATAATTCACAGGGACCTAAAACCTAGTAATCTAGCTGTGAATGAAGACTGTGAGCTGAAGATTCTGGATTTTGGACTGGCTCGGCACACAGATGATGAAATGACAGGCTACGTGGCCACTAGGTGGTACAGGGCTCCTGAGATCATGCTGAACTGGATGCATTACAACCAGACAGTTGATATTTGGTCAGTGGGATGCATAATGGCCGAGCTGTTGACTGGAAGAACATTGTTTCCTGGTACAGACCATATTGATCAGTTGAAGCTCATTTTAAGACTCGTTGGAACCCCAGGGGCTGAGCTTTTGAAGAAAATCTCCTCAGAGTCTGCAAGAAACTATATTCAGTCTTTGACTCAGATGCCGAAGATGAACTTTGCGAATGTATTTATTGGTGCCAATCCCCTGGCTGTCGACTTGCTGGAGAAGATGCTTGTATTGGACTCAGATAAGAGAATTACAGCGGCCCAAGCCCTTGCACATGCCTACTTTGCTCAGTACCACGATCCTGATGATGAACCAGTGGCCGATCCTTATGATCAGTCCTTTGAAAGCAGGGACCTCCTTATAGATGAGTGGAAAAGCCTGACCTATGATGAAGTCATCAGCTTTGTGCCACCACCCCTTGACCAAGAAGAGATGGAGTCC</t>
+  </si>
+  <si>
+    <t>MK11_HUMAN_D0_3GC8_A</t>
+  </si>
+  <si>
+    <t>MK14_HUMAN_D0_3K3J_A</t>
+  </si>
+  <si>
+    <t>CDK16_HUMAN_D0_3MTL_A</t>
+  </si>
+  <si>
+    <t>PLK1_HUMAN_D0_2V5Q_A</t>
+  </si>
+  <si>
+    <t>NEK7_HUMAN_D0_2WQN_A</t>
+  </si>
+  <si>
+    <t>PAK6_HUMAN_D0_2C30_A</t>
+  </si>
+  <si>
+    <t>FGFR1_HUMAN_D0_3GQL_B</t>
+  </si>
+  <si>
+    <t>TCTTCGGTCACCGCCAGTGCGGCCCCGGGGACCGCGAGCCTCGTCCCGGATTACTGGATCGACGGCTCCAACAGGGATGCGCTGAGCGATTTCTTCGAGGTGGAGTCGGAGCTGGGACGGGGTGCTACATCCATTGTGTACAGATGCAAACAGAAGGGGACCCAGAAGCCTTATGCTCTCAAAGTGTTAAAGAAAACAGTGGACAAAAAAATCGTAAGAACTGAGATAGGAGTTCTTCTTCGCCTCTCACATCCAAACATTATAAAACTTAAAGAGATATTTGAAACCCCTACAGAAATCAGTCTGGTCCTAGAACTCGTCACAGGAGGAGAACTGTTTGATAGGATTGTGGAAAAGGGATATTACAGTGAGCGAGATGCTGCAGATGCCGTTAAACAAATCCTGGAGGCAGTTGCTTATCTACATGAAAATGGGATTGTCCATCGTGATCTCAAACCAGAGAATCTTCTTTATGCAACTCCAGCCCCAGATGCACCACTCAAAATCGCTGATTTTGGACTCTCTAAAATTGTGGAACATCAAGTGCTCATGAAGACAGTATGTGGAACCCCAGGGTACTGCGCACCTGAAATTCTTAGAGGTTGTGCCTATGGACCTGAGGTGGACATGTGGTCTGTAGGAATAATCACCTACATCTTACTTTGTGGATTTGAACCATTCTATGATGAAAGAGGCGATCAGTTCATGTTCAGGAGAATTCTGAATTGTGAATATTACTTTATCTCCCCCTGGTGGGATGAAGTATCTCTAAATGCCAAGGACTTGGTCAGAAAATTAATTGTTTTGGATCCAAAGAAACGGCTGACTACATTTCAAGCTCTCCAGCATCCGTGGGTCACAGGTAAAGCAGCCAATTTTGTACACATGGATACCGCTCAAAAGAAGCTCCAAGAATTCAATGCCCGGCGTAAGCTTAAGGCAGCGGTGAAGGCTGTGGTGGCCTCTTCCCGCCTGGGA</t>
+  </si>
+  <si>
+    <t>MEAAASEPSLDLDNLKLLELIGRGRYGAVYKGSLDERPVAVKVFSFANRQNFINEKNIYRVPLMEHDNIARFIVGDERVTADGRMEYLLVMEYYPNGSLCKYLSLHTSDWVSSCRLAHSVTRGLAYLHTELPRGDHYKPAISHRDLNSRNVLVKNDGTCVISDFGLSMRLTGNRLVRPGEEDNAAISEVGTIRYMAPEVLEGAVNLRDCESALKQVDMYALGLIYWEIFMRCTDLFPGESVPEYQMAFQTEVGNHPTFEDMQVLVSREKQRPKFPEAWKENSLAVRSLKETIEDCWDQDAEARLTAQCAEERMAELMMIWERNKSVSPT</t>
+  </si>
+  <si>
+    <t>GTCATCATTGACAATAAGCGCTACCTCTTCATCCAGAAACTGGGGGAGGGTGGGTTCAGCTATGTGGACCTAGTGGAAGGGTTACATGATGGACACTTCTACGCCCTGAAGCGAATCCTGTGTCACGAGCAGCAGGACCGGGAGGAGGCCCAGCGAGAAGCCGACATGCATCGCCTCTTCAATCACCCCAACATCCTTCGCCTCGTGGCTTACTGTCTGAGGGAACGGGGTGCTAAGCATGAGGCCTGGCTGCTGCTACCATTCTTCAAGAGAGGTACGCTGTGGAATGAGATAGAAAGGCTGAAGGACAAAGGCAACTTCCTGACCGAGGATCAAATCCTTTGGCTGCTGCTGGGGATCTGCAGAGGCCTTGAGGCCATTCATGCCAAGGGTTATGCCCACAGAGACTTGAAGCCCACCAATATATTGCTTGGAGATGAGGGGCAGCCAGTTTTAATGGACTTGGGTTCCATGAATCAAGCATGCATCCATGTGGAGGGCTCCCGCCAGGCTCTGACCCTGCAGGACTGGGCAGCCCAGCGGTGCACCATCTCCTACCGAGCCCCAGAGCTCTTCTCTGTGCAGAGTCACTGTGTCATCGATGAGCGGACTGATGTCTGGTCCCTAGGCTGCGTGCTATATGCCATGATGTTTGGGGAAGGCCCTTATGACATGGTGTTCCAAAAGGGTGACAGTGTGGCCCTTGCTGTGCAGAACCAACTCAGCATCCCACAAAGCCCCAGGCATTCTTCAGCATTGTGGCAGCTCCTGAACTCGATGATGACCGTGGACCCGCATCAGCGTCCTCACATTCCTCTCCTCCTCAGTCAGCTGGAGGCGCTGCAG</t>
+  </si>
+  <si>
+    <t>BMPR2_HUMAN_D0_3G2F_A</t>
+  </si>
+  <si>
+    <t>dna_start</t>
+  </si>
+  <si>
+    <t>PHKG2_HUMAN_D0_2Y7J_D</t>
+  </si>
+  <si>
+    <t>MAPK2_HUMAN_D0_2JBO_A</t>
+  </si>
+  <si>
+    <t>ATGGAGAAGGACGGCCTGTGCCGCGCTGACCAGCAGTACGAATGCGTGGCGGAGATCGGGGAGGGCGCCTATGGGAAGGTGTTCAAGGCCCGCGACTTGAAGAACGGAGGCCGTTTCGTGGCGTTGAAGCGCGTGCGGGTGCAGACCGGCGAGGAGGGCATGCCGCTCTCCACCATCCGCGAGGTGGCGGTGCTGAGGCACCTGGAGACCTTCGAGCACCCCAACGTGGTCAGGTTGTTTGATGTGTGCACAGTGTCACGAACAGACAGAGAAACCAAACTAACTTTAGTGTTTGAACATGTCGATCAAGACTTGACCACTTACTTGGATAAAGTTCCAGAGCCTGGAGTGCCCACTGAAACCATAAAGGATATGATGTTTCAGCTTCTCCGAGGTCTGGACTTTCTTCATTCACACCGAGTAGTGCATCGCGATCTAAAACCACAGAACATTCTGGTGACCAGCAGCGGACAAATAAAACTCGCTGACTTCGGCCTTGCCCGCATCTATAGTTTCCAGATGGCTCTAACCTCAGTGGTCGTCACGCTGTGGTACAGAGCACCCGAAGTCTTGCTCCAGTCCAGCTACGCCACCCCCGTGGATCTCTGGAGTGTTGGCTGCATATTTGCAGAAATGTTTCGTAGAAAGCCTCTTTTTCGTGGAAGTTCAGATGTTGATCAACTAGGAAAAATCTTGGACGTGATTGGACTCCCAGGAGAAGAAGACTGGCCTAGAGATGTTGCCCTTCCCAGGCAGGCTTTTCATTCAAAATCTGCCCAACCAATTGAGAAGTTTGTAACAGATATCGATGAACTAGGCAAAGACCTACTTCTGAAGTGTTTGACATTTAACCCAGCCAAAAGAATATCTGCCTACAGTGCCCTGTCTCACCCATACTTCCAG</t>
+  </si>
+  <si>
+    <t>ATGTCGGGCCCTCGCGCCGGCTTCTACCGGCAGGAGCTGAACAAGACCGTGTGGGAGGTGCCGCAGCGGCTGCAGGGGCTGCGCCCGGTGGGCTCCGGCGCCTACGGCTCCGTCTGTTCGGCCTACGACGCCCGGCTGCGCCAGAAGGTGGCGGTGAAGAAGCTGTCGCGCCCCTTCCAGTCGCTGATCCACGCGCGCAGAACGTACCGGGAGCTGCGGCTGCTCAAGCACCTGAAGCACGAGAACGTCATCGGGCTTCTGGACGTCTTCACGCCGGCCACGTCCATCGAGGACTTCAGCGAAGTGTACTTGGTGACCACCCTGATGGGCGCCGACCTGAACAACATCGTCAAGTGCCAGGCGCTGAGCGACGAGCACGTTCAATTCCTGGTTTACCAGCTGCTGCGCGGGCTGAAGTACATCCACTCGGCCGGGATCATCCACCGGGACCTGAAGCCCAGCAACGTGGCTGTGAACGAGGACTGTGAGCTCAGGATCCTGGATTTCGGGCTGGCGCGCCAGGCGGACGAGGAGATGACCGGCTATGTGGCCACGCGCTGGTACCGGGCACCTGAGATCATGCTCAACTGGATGCATTACAACCAAACAGTGGATATCTGGTCCGTGGGCTGCATCATGGCTGAGCTGCTCCAGGGCAAGGCCCTCTTCCCGGGAAGCGACTACATTGACCAGCTGAAGCGCATCATGGAAGTGGTGGGCACACCCAGCCCTGAGGTTCTGGCAAAAATCTCCTCGGAACACGCCCGGACATATATCCAGTCCCTGCCCCCCATGCCCCAGAAGGACCTGAGCAGCATCTTCCGTGGAGCCAACCCCCTGGCCATAGACCTCCTTGGAAGGATGCTGGTGCTGGACAGTGACCAGAGGGTCAGTGCAGCTGAGGCACTGGCCCACGCCTACTTCAGCCAGTACCACGACCCCGAGGATGAGCCAGAGGCCGAGCCATATGATGAGAGCGTTGAGGCCAAGGAGCGCACGCTGGAGGAGTGGAAGGAGCTCACTTACCAGGAAGTCCTCAGCTTCAAGCCCCCAGAGCCACCGAAGCCACCTGGCAGCCTGGAGATTGAGCAG</t>
+  </si>
+  <si>
+    <t>E2AK2_HUMAN_D0_3UIU_A</t>
+  </si>
+  <si>
+    <t>MEKYEKIGKIGEGSYGVVFKCRNRDTGQIVAIKKFLESEDDPVIKKIALREIRMLKQLKHPNLVNLLEVFRRKRRLHLVFEYCDHTVLHELDRYQRGVPEHLVKSITWQTLQAVNFCHKHNCIHRDVKPENILITKHSVIKLCDFGFARLLTGPSDYYTDYVATRWYRSPELLVGDTQYGPPVDVWAIGCVFAELLSGVPLWPGKSDVDQLYLIRKTLGDLIPRHQQVFSTNQYFSGVKIPDPEDMEPLELKFPNISYPALGLL</t>
+  </si>
+  <si>
+    <t>GeneID</t>
+  </si>
+  <si>
+    <t>BRAF_HUMAN_D0_4FK3_B</t>
+  </si>
+  <si>
+    <t>ATGGATGAGCAATCACAAGGAATGCAAGGGCCACCTGTTCCTCAGTTCCAACCACAGAAGGCCTTACGACCGGATATGGGCTATAATACATTAGCCAACTTTCGAATAGAAAAGAAAATTGGTCGCGGACAATTTAGTGAAGTTTATAGAGCAGCCTGTCTCTTGGATGGAGTACCAGTAGCTTTAAAAAAAGTGCAGATATTTGATTTAATGGATGCCAAAGCACGTGCTGATTGCATCAAAGAAATAGATCTTCTTAAGCAACTCAACCATCCAAATGTAATAAAATATTATGCATCATTCATTGAAGATAATGAACTAAACATAGTTTTGGAACTAGCAGATGCTGGCGACCTATCCAGAATGATCAAGCATTTTAAGAAGCAAAAGAGGCTAATTCCTGAAAGAACTGTTTGGAAGTATTTTGTTCAGCTTTGCAGTGCATTGGAACACATGCATTCTCGAAGAGTCATGCATAGAGATATAAAACCAGCTAATGTGTTCATTACAGCCACTGGGGTGGTAAAACTTGGAGATCTTGGGCTTGGCCGGTTTTTCAGCTCAAAAACCACAGCTGCACATTCTTTAGTTGGTACGCCTTATTACATGTCTCCAGAGAGAATACATGAAAATGGATACAACTTCAAATCTGACATCTGGTCTCTTGGCTGTCTACTATATGAGATGGCTGCATTACAAAGTCCTTTCTATGGTGACAAAATGAATTTATACTCACTGTGTAAGAAGATAGAACAGTGTGACTACCCACCTCTTCCTTCAGATCACTATTCAGAAGAACTCCGACAGTTAGTTAATATGTGCATCAACCCAGATCCAGAGAAGCGACCAGACGTCACCTATGTTTATGACGTAGCAAAGAGGATGCATGCATGCACTGCAAGCAGC</t>
+  </si>
+  <si>
+    <t>DAPK3_HUMAN_D0_2J90_A</t>
+  </si>
+  <si>
+    <t>VKEFLAKAKEDFLKKWESPAQNTAHLDQFERIKTLGTGSFGRVMLVKHKETGNHYAMKILDKQKVVKLKQIEHTLNEKRILQAVNFPFLVKLEFSFKDNSNLYMVMEYVPGGEMFSHLRRIGRFSEPHARFYAAQIVLTFEYLHSLDLIYRDLKPENLLIDQQGYIQVTDFGFAKRVKGRTWTLCGTPEYLAPEIILSKGYNKAVDWWALGVLIYEMAAGYPPFFADQPIQIYEKIVSGKVRFPSHFSSDLKDLLRNLLQVDLTKRFGNLKNGVNDIKNHKWFATTDWIAIYQRKVEAPFIPKFKGPGDTSNFDDYEEEEIRVSINEKCGKEFSEF</t>
+  </si>
+  <si>
+    <t>TCCAGGGTGTCCCATGAACAGTTTCGGGCGGCCCTGCAGCTGGTGGTCAGCCCAGGAGACCCCAGGGAATACTTGGCCAACTTTATCAAAATCGGGGAAGGCTCAACCGGCATCGTATGCATCGCCACCGAGAAACACACAGGGAAACAAGTTGCAGTGAAGAAAATGGACCTCCGGAAGCAACAGAGACGAGAACTGCTTTTCAATGAGGTCGTGATCATGCGGGATTACCACCATGACAATGTGGTTGACATGTACAGCAGCTACCTTGTCGGCGATGAGCTCTGGGTGGTCATGGAGTTTCTAGAAGGTGGTGCCTTGACAGACATTGTGACTCACACCAGAATGAATGAAGAACAGATAGCTACTGTCTGCCTGTCAGTTCTGAGAGCTCTCTCCTACCTTCATAACCAAGGAGTGATTCACAGGGACATAAAAAGTGACTCCATCCTCCTGACAAGCGATGGCCGGATAAAGTTGTCTGATTTTGGTTTCTGTGCTCAAGTTTCCAAAGAGGTGCCGAAGAGGAAATCATTGGTTGGCACTCCCTACTGGATGGCCCCTGAGGTGATTTCTAGGCTACCTTATGGGACAGAGGTGGACATCTGGTCCCTCGGGATCATGGTGATAGAAATGATTGATGGCGAGCCCCCCTACTTCAATGAGCCTCCCCTCCAGGCGATGCGGAGGATCCGGGACAGTTTACCTCCAAGAGTGAAGGACCTACACAAGGTTTCTTCAGTGCTCCGGGGATTCCTAGACTTGATGTTGGTGAGGGAGCCCTCTCAGAGAGCAACAGCCCAGGAACTCCTCGGACATCCATTCTTAAAACTAGCAGGTCCACCGTCTTGCATTGTCCCCCTCATGAGACAATACAGGCATCAC</t>
+  </si>
+  <si>
+    <t>KRQWALEDFEIGRPLGKGKFGNVYLAREKQSKFILALKVLFKAQLEKAGVEHQLRREVEIQSHLRHPNILRLYGYFHDATRVYLILEYAPLGTVYRELQKLSKFDEQRTATYITELANALSYCHSKRVIHRDIKPENLLLGSAGELKIADFGWSVHAPSSRRTTLCGTLDYLPPEMIEGRMHDEKVDLWSLGVLCYEFLVGKPPFEANTYQETYKRISRVEFTFPDFVTEGARDLISRLLKHNPSQRPMLREVLEHPWITANSSKPS</t>
+  </si>
+  <si>
+    <t>EGFR_HUMAN_D0_2RF9_A</t>
+  </si>
+  <si>
+    <t>SLK_HUMAN_D0_2JFL_A</t>
+  </si>
+  <si>
+    <t>SRVSHEQFRAALQLVVSPGDPREYLANFIKIGEGSTGIVCIATEKHTGKQVAVKKMDLRKQQRRELLFNEVVIMRDYHHDNVVDMYSSYLVGDELWVVMEFLEGGALTDIVTHTRMNEEQIATVCLSVLRALSYLHNQGVIHRDIKSDSILLTSDGRIKLSDFGFCAQVSKEVPKRKSLVGTPYWMAPEVISRLPYGTEVDIWSLGIMVIEMIDGEPPYFNEPPLQAMRRIRDSLPPRVKDLHKVSSVLRGFLDLMLVREPSQRATAQELLGHPFLKLAGPPSCIVPLMRQYRHH</t>
+  </si>
+  <si>
+    <t>TQTVHEFAKELDATNISIDKVVGAGEFGEVCSGRLKLPSKKEISVAIKTLKVGYTEKQRRDFLGEASIMGQFDHPNIIRLEGVVTKSKPVMIVTEYMENGSLDSFLRKHDAQFTVIQLVGMLRGIASGMKYLSDMGYVHRDLAARNILINSNLVCKVSDFGLSRVLEDDPEAAYTTRGGKIPIRWTSPEAIAYRKFTSASDVWSYGIVLWEVMSYGERPYWEMSNQDVIKAVDEGYRLPPPMDCPAALYQLMLDCWQKDRNNRPKFEQIVSILDKLIRNPGSLKIITSAAARPSNLLLDQSNVDITTFRTTGDWLNGVWTAHCKEIFTGVEYSSCDTIAKIS</t>
+  </si>
+  <si>
+    <t>QQFPQFHVKSGLQIKKNAIIDDYKVTSQVLGLGINGKVLQIFNKRTQEKFALKMLQDCPKARREVELHWRASQCPHIVRIVDVYENLYAGRKCLLIVMECLDGGELFSRIQDRGDQAFTEREASEIMKSIGEAIQYLHSINIAHRDVKPENLLYTSKRPNAILKLTDFGFAKETTSHNSLTTPCYTPYYVAPEVLGPEKYDKSCDMWSLGVIMYILLCGYPPFYSNHGLAISPGMKTRIRMGQYEFPNPEWSEVSEEVKMLIRNLLKTEPTQRMTITEFMNHPWIMQSTKVPQTPLHTSRVLKEDKERWEDVKGCLHDKNSDQA</t>
+  </si>
+  <si>
+    <t>CSK21_HUMAN_D0_3AXW_A</t>
+  </si>
+  <si>
+    <t>ATCTRFTDDYQLFEELGKGAFSVVRRCVKKTPTQEYAAKIINTKKLSARDHQKLEREARICRLLKHPNIVRLHDSISEEGFHYLVFDLVTGGELFEDIVAREYYSEADASHCIHQILESVNHIHQHDIVHRDLKPENLLLASKCKGAAVKLADFGLAIEVQGEQQAWFGFAGTPGYLSPEVLRKDPYGKPVDIWACGVILYILLVGYPPFWDEDQHKLYQQIKAGAYDFPSPEWDTVTPEAKNLINQMLTINPAKRITADQALKHPWVCQRSTVASMMHRQETVECLRKFNARRKLKGAILTTMLVSRNFS</t>
+  </si>
+  <si>
+    <t>VIDPSELTFVQEIGSGQFGLVHLGYWLNKDKVAIKTIREGAMSEEDFIEEAEVMMKLSHPKLVQLYGVCLEQAPICLVFEFMEHGCLSDYLRTQRGLFAAETLLGMCLDVCEGMAYLEEACVIHRDLAARNCLVGENQVIKVSDFGMTRFVLDDQYTSSTGTKFPVKWASPEVFSFSRYSSKSDVWSFGVLMWEVFSEGKIPYENRSNSEVVEDISTGFRLYKPRLASTHVYQIMNHCWKERPEDRPAFSRLLRQLAEIAESGL</t>
+  </si>
+  <si>
+    <t>CGTGTAAAAGCAGCTCAAGCTGGAAGACAGAGCTCTGCAAAGAGACATCTTGCAGAACAATTTGCAGTTGGAGAGATAATAACTGACATGGCAAAAAAGGAATGGAAAGTAGGATTACCCATTGGCCAAGGAGGCTTTGGCTGTATATATCTTGCTGATATGAATTCTTCAGAGTCAGTTGGCAGTGATGCACCTTGTGTTGTAAAAGTGGAACCCAGTGACAATGGACCTCTTTTTACTGAATTAAAGTTCTACCAACGAGCTGCAAAACCAGAGCAAATTCAGAAATGGATTCGTACCCGTAAGCTGAAGTACCTGGGTGTTCCTAAGTATTGGGGGTCTGGTCTACATGACAAAAATGGAAAAAGTTACAGGTTTATGATAATGGATCGCTTTGGGAGTGACCTTCAGAAAATATATGAAGCAAATGCCAAAAGGTTTTCTCGGAAAACTGTCTTGCAGCTAAGCTTAAGAATTCTGGATATTCTGGAATATATTCACGAGCATGAGTATGTGCATGGAGATATCAAGGCCTCAAATCTTCTTCTGAACTACAAGAATCCTGACCAGGTGTACTTGGTAGATTATGGCCTTGCTTATCGGTACTGCCCAGAAGGAGTTCATAAAGAATACAAAGAAGACCCCAAAAGATGTCACGATGGCACTATTGAATTCACGAGCATCGATGCACACAATGGCGTGGCCCCATCAAGACGTGGTGATTTGGAAATACTTGGTTATTGCATGATCCAATGGCTTACTGGCCATCTTCCTTGGGAGGATAATTTGAAAGATCCTAAATATGTTAGAGATTCCAAAATTAGATACAGAGAAAATATTGCAAGTTTGATGGACAAATGTTTTCCTGAGAAAAACAAACCAGGTGAAATTGCCAAATACATGGAAACAGTGAAATTACTAGACTACACTGAAAAACCTCTTTATGAAAATTTACGTGACATTCTTTTGCAAGGACTAAAAGCTATAGGAAGTAAGGATGATGGCAAATTGGACCTCAGTGTTGTGGAGAATGGAGGTTTGAAAGCAAAAACAATAACAAAGAAGCGAAAGAAAGAAATTGAAGAA</t>
+  </si>
+  <si>
+    <t>KS6A1_HUMAN_D0_3RNY_B</t>
+  </si>
+  <si>
+    <t>MP2K6_HUMAN_D0_3VN9_A</t>
+  </si>
+  <si>
+    <t>RVKAAQAGRQSSAKRHLAEQFAVGEIITDMAKKEWKVGLPIGQGGFGCIYLADMNSSESVGSDAPCVVKVEPSDNGPLFTELKFYQRAAKPEQIQKWIRTRKLKYLGVPKYWGSGLHDKNGKSYRFMIMDRFGSDLQKIYEANAKRFSRKTVLQLSLRILDILEYIHEHEYVHGDIKASNLLLNYKNPDQVYLVDYGLAYRYCPEGVHKEYKEDPKRCHDGTIEFTSIDAHNGVAPSRRGDLEILGYCMIQWLTGHLPWEDNLKDPKYVRDSKIRYRENIASLMDKCFPEKNKPGEIAKYMETVKLLDYTEKPLYENLRDILLQGLKAIGSKDDGKLDLSVVENGGLKAKTITKKRKKEIEE</t>
+  </si>
+  <si>
+    <t>MKNK1_HUMAN_D0_2HW6_B</t>
+  </si>
+  <si>
+    <t>MSLIRKKGFYKQDVNKTAWELPKTYVSPTHVGSGAYGSVCSAIDKRSGEKVAIKKLSRPFQSEIFAKRAYRELLLLKHMQHENVIGLLDVFTPASSLRNFYDFYLVMPFMQTDLQKIMGMEFSEEKIQYLVYQMLKGLKYIHSAGVVHRDLKPGNLAVNEDCELKILDFGLARHADAEMTGYVVTRWYRAPEVILSWMHYNQTVDIWSVVCIMAEMLTGKTLFKGKDYLDQLTQILKVTGVPGTEFVQKLNDKAAKSYIQSLPQTPRKDFTQLFPRASPQAADLLEKMLELDVDKRLTAAQALTHPFFEPFRDPEEETEAQQPFDDSLEHEKLTVDEWKQHIYKEIVNFSPI</t>
+  </si>
+  <si>
+    <t>AAPPAKEIPEVLVDPRSRRRYVRGRFLGKGGFAKCFEISDADTKEVFAGKIVPKSLLLKPHQREKMSMEISIHRSLAHQHVVGFHGFFEDNDFVFVVLELCRRRSLLELHKRRKALTEPEARYYLRQIVLGCQYLHRNRVIHRDLKLGNLFLNEDLEVKIGDFGLATKVEYDGERKKTLCGTPNYIAPEVLSKKGHSFEVDVWSIGCIMYTLLVGKPPFETSCLKETYLRIKKNEYSIPKHINPVAASLIQKMLQTDPTARPTINELLNDEFFTSGYIPARLPITCLTIPPRFSIAPSSLDPSNRKPLTVLNK</t>
+  </si>
+  <si>
+    <t>ITK_HUMAN_D0_3QGW_B</t>
+  </si>
+  <si>
+    <t>KS6A3_HUMAN_D1_4JG7_A</t>
+  </si>
+  <si>
+    <t>KCC4_HUMAN_D0_2W4O_A</t>
+  </si>
+  <si>
+    <t>CSK_HUMAN_D0_3D7T_A</t>
+  </si>
+  <si>
+    <t>KCC2A_HUMAN_D0_2VZ6_B</t>
+  </si>
+  <si>
+    <t>ATGTCTGATGAGGAGATCTTGGAGAAATTACGAAGCATAGTGAGTGTGGGCGATCCTAAGAAGAAATATACACGGTTTGAGAAGATTGGACAAGGTGCTTCAGGCACCGTGTACACAGCAATGGATGTGGCCACAGGACAGGAGGTGGCCATTAAGCAGATGAATCTTCAGCAGCAGCCCAAGAAAGAGCTGATTATTAATGAGATCCTGGTCATGAGGGAAAACAAGAACCCAAACATTGTGAATTACTTGGACAGTTACCTCGTGGGAGATGAGCTGTGGGTTGTTATGGAATACTTGGCTGGAGGCTCCTTGACAGATGTGGTGACAGAAACTTGCATGGATGAAGGCCAAATTGCAGCTGTGTGCCGTGAGTGTCTGCAGGCTCTGGAGTTCTTGCATTCGAACCAGGTCATTCACAGAGACATCAAGAGTGACAATATTCTGTTGGGAATGGATGGCTCTGTCAAGCTAACTGACTTTGGATTCTGTGCACAGATAACCCCAGAGCAGAGCAAACGGAGCACCATGGTAGGAACCCCATACTGGATGGCACCAGAGGTTGTGACACGAAAGGCCTATGGGCCCAAGGTTGACATCTGGTCCCTGGGCATCAAGGCCATCGAAATGATTGAAGGGGAGCCTCCATACCTCAATGAAAACCCTCTGAGAGCCTTGTACCTCATTGCCACCAATGGGACCCCAGAACTTCAGAACCCAGAGAAGCTGTCAGCTATCTTCCGGGACTTTCTGAACCGCTGTCTCGAGATGGATGTGGAGAAGAGAGGTTCAGCTAAAGAGCTGCTACAGCATCAATTCCTGAAGATTGCCAAGCCCCTCTCCAGCCTCACTCCACTTATTGCTGCAGCTAAGGAGGCAACAAAGAACAATCAC</t>
+  </si>
+  <si>
+    <t>expression tag location</t>
+  </si>
+  <si>
+    <t>ATGGAGGCAGCAGCATCCGAACCCTCTCTTGATCTAGATAATCTGAAACTGTTGGAGCTGATTGGCCGAGGTCGATATGGAGCAGTATATAAAGGCTCCTTGGATGAGCGTCCAGTTGCTGTAAAAGTGTTTTCCTTTGCAAACCGTCAGAATTTTATCAACGAAAAGAACATTTACAGAGTGCCTTTGATGGAACATGACAACATTGCCCGCTTTATAGTTGGAGATGAGAGAGTCACTGCAGATGGACGCATGGAATATTTGCTTGTGATGGAGTACTATCCCAATGGATCTTTATGCAAGTATTTAAGTCTCCACACAAGTGACTGGGTAAGCTCTTGCCGTCTTGCTCATTCTGTTACTAGAGGACTGGCTTATCTTCACACAGAATTACCACGAGGAGATCATTATAAACCTGCAATTTCCCATCGAGATTTAAACAGCAGAAATGTCCTAGTGAAAAATGATGGAACCTGTGTTATTAGTGACTTTGGACTGTCCATGAGGCTGACTGGAAATAGACTGGTGCGCCCAGGGGAGGAAGATAATGCAGCCATAAGCGAGGTTGGCACTATCAGATATATGGCACCAGAAGTGCTAGAAGGAGCTGTGAACTTGAGGGACTGTGAATCAGCTTTGAAACAAGTAGACATGTATGCTCTTGGACTAATCTATTGGGAGATATTTATGAGATGTACAGACCTCTTCCCAGGGGAATCCGTACCAGAGTACCAGATGGCTTTTCAGACAGAGGTTGGAAACCATCCCACTTTTGAGGATATGCAGGTTCTCGTGTCTAGGGAAAAACAGAGACCCAAGTTCCCAGAAGCCTGGAAAGAAAATAGCCTGGCAGTGAGGTCACTCAAGGAGACAATCGAAGACTGTTGGGACCAGGATGCAGAGGCTCGGCTTACTGCACAGTGTGCTGAGGAAAGGATGGCTGAACTTATGATGATTTGGGAAAGAAACAAATCTGTGAGCCCAACA</t>
+  </si>
+  <si>
+    <t>GGAGAAGCTCCCAACCAAGCTCTCTTGAGGATCTTGAAGGAAACTGAATTCAAAAAGATCAAAGTGCTGGGCTCCGGTGCGTTCGGCACGGTGTATAAGGGACTCTGGATCCCAGAAGGTGAGAAAGTTAAAATTCCCGTCGCTATCAAGGAATTAAGAGAAGCAACATCTCCGAAAGCCAACAAGGAAATCCTCGATGAAGCCTACGTGATGGCCAGCGTGGACAACCCCCACGTGTGCCGCCTGCTGGGCATCTGCCTCACCTCCACCGTGCAaCTCATCACGCAGCTCATGCCCTTCGGCTGCCTCCTGGACTATGTCCGGGAACACAAAGACAATATTGGCTCCCAGTACCTGCTCAACTGGTGTGTGCAGATCGCAAAGGGCATGAACTACTTGGAGGACCGTCGCTTGGTGCACCGCGACCTGGCAGCCAGGAACGTACTGGTGAAAACACCGCAGCATGTCAAGATCACAGATTTTGGGCgGGCCAAACTGCTGGGTGCGGAAGAGAAAGAATACCATGCAGAAGGAGGCAAAGTGCCTATCAAGTGGATGGCATTGGAATCAATTTTACACAGAATCTATACCCACCAGAGTGATGTCTGGAGCTACGGGGTGACCGTTTGGGAGTTGATGACCTTTGGATCCAAGCCATATGACGGAATCCCTGCCAGCGAGATCTCCTCCATCCTGGAGAAAGGAGAACGCCTCCCTCAGCCACCCATATGTACCATCGATGTCTACATGATCATGGTCAAGTGCTGGATGATAGACGCAGATAGTCGCCCAAAGTTCCGTGAGTTGATCATCGAATTCTCCAAAATGGCCCGAGACCCCCAGCGCTACCTTGTCATTCAGGGGGATGAAAGAATGCATTTGCCAAGTCCTACAGACTCCAACTTCTACCGTGCCCTGATGGATGAAGAAGACATGGACGACGTGGTGGATGCCGACGAGTACCTCATCCCACAGCAGGGC</t>
+  </si>
+  <si>
+    <t>GCCACCTGCACACGTTTCACCGACGACTACCAGCTCTTCGAGGAGCTTGGCAAGGGTGCTTTCTCTGTGGTCCGCAGGTGTGTGAAGAAAACCCCCACGCAGGAGTACGCAGCAAAAATCATCAATACCAAGAAATTGTCTGCCCGGGATCACCAGAAACTAGAACGTGAGGCTCGGATATGTCGACTTCTGAAACATCCAAACATCGTGCGCCTCCATGACAGTATTTCTGAAGAAGGGTTTCACTACCTCGTGTTTGACCTTGTTACCGGCGGGGAGCTGTTTGAAGACATTGTGGCCAGAGAGTACTACAGTGAAGCAGATGCCAGCCACTGTATACATCAGATTCTGGAGAGTGTTAACCACATCCACCAGCATGACATCGTCCACAGGGACCTGAAGCCTGAGAACCTGCTGCTGGCGAGTAAATGCAAGGGTGCCGCCGTCAAGCTGGCTGATTTTGGCCTAGCCATCGAAGTACAGGGAGAGCAGCAGGCTTGGTTTGGTTTTGCTGGCACCCCAGGTTACTTGTCCCCTGAGGTCTTGAGGAAAGATCCCTATGGAAAACCTGTGGATATCTGGGCCTGCGGGGTCATCCTGTATATCCTCCTGGTGGGCTATCCTCCCTTCTGGGATGAGGATCAGCACAAGCTGTATCAGCAGATCAAGGCTGGAGCCTATGATTTCCCATCACCAGAATGGGACACGGTAACTCCTGAAGCCAAGAACTTGATCAACCAGATGCTGACCATAAACCCAGCAAAGCGCATCACGGCTGACCAGGCTCTCAAGCACCCGTGGGTCTGTCAACGATCCACGGTGGCATCCATGATGCATCGTCAGGAGACTGTGGAGTGTTTGCGCAAGTTCAATGCCCGGAGAAAACTGAAGGGTGCCATCCTCACGACCATGCTTGTCTCCAGGAACTTCTCA</t>
+  </si>
+  <si>
+    <t>GAGACCTACATTAAGCTGGACAAACTGGGCGAGGGTACCTATGCCACCGTCTACAAAGGCAAAAGCAAGCTCACAGACAACCTTGTGGCACTCAAGGAGATCAGACTGGAACATGAAGAGGGGGCACCCTGCACCGCCATCCGGGAAGTGTCCCTACTCAAGGACCTCAAACACGCCAACATCGTTACGCTACATGACATTATCCACACGGAGAAGTCCCTCACCCTTGTCTTTGAGTACCTGGACAAGGACCTGAAGCAGTACCTGGATGACTGTGGGAACATCATCAACATGCACAACGTGAAACTGTTCCTGTTCCAGCTGCTCCGTGGCCTGGCCTACTGCCACCGGCAGAAGGTGCTACACCGAGACCTCAAGCCCCAGAACCTGCTCATCAACGAGAGGGGAGAGCTCAAGCTGGCTGACTTTGGCCTGGCCCGAGCCAAGTCAATCCCAACAAAGACATACTCCAATGAGGTGGTGACACTGTGGTACCGGCCCCCTGACATCCTGCTTGGGTCCACGGACTACTCCACTCAGATTGACATGTGGGGTGTGGGCTGCATCTTCTATGAGATGGCCACAGGCCGTCCCCTCTTTCCGGGCTCCACGGTGGAGGAACAGCTACACTTCATCTTCCGTATCTTAGGAACCCCAACTGAGGAGACGTGGCCAGGCATCCTGTCCAACGAGGAGTTCAAGACATACAACTACCCCAAGTACCGAGCCGAGGCCCTTTTGAGCCACGCACCCCGACTTGATAGCGACGGGGCCGACCTCCTCACCAAGCTGTTGCAGTTTGAGGGTCGAAATCGGATCTCCGCAGAGGATGCCATGAAACATCCATTCTTCCTCAGTCTGGGGGAGCGGATCCACAAACTTCCTGACACTACTTCCATATTTGCACTAAAGGAGATTCAGCTACAAAAGGAGGCCAGCCTTCGGTCT</t>
+  </si>
+  <si>
+    <t>MK13_HUMAN_D0_4EYJ_A</t>
+  </si>
+  <si>
+    <t>STK16_HUMAN_D0_2BUJ_B</t>
+  </si>
+  <si>
+    <t>AAGCACGACGGGCGGGTGAAGATCGGACACTACGTGCTGGGCGACACGCTGGGCGTCGGCACCTTCGGCAAAGTGAAGATTGGAGAACATCAATTAACAGGCCATAAAGTGGCAGTTAAAATCTTAAATAGACAGAAGATTCGCAGTTTAGATGTTGTTGGAAAAATAAAACGAGAAATTCAAAATCTAAAACTCTTTCGTCATCCTCATATTATCAAACTATACCAGGTGATCAGCACTCCAACAGATTTTTTTATGGTAATGGAATATGTGTCTGGAGGTGAATTATTTGACTACATCTGTAAGCATGGACGGGTTGAAGAGATGGAAGCCAGGCGRCTCTTTCAGCAGATTCTGTCTGCTGTGGATTACTGTCATAGGCATATGGTTGTTCATCGAGACCTGAAACCAGAGAATGTCCTGTTGGATGCACACATGAATGCCAAGATAGCCGATTTCGGATTATCTAATATGATGTCAGATGGTGAATTTCTGAGAACTAGTTGCGGATCTCCAAATTATGCAGCACCTGAAGTCATCTCAGGCAGATTGTATGCAGGTCCTGAAGTTGATATCTGGAGCTGTGGTGTTATCTTGTATGCTCTTCTTTGTGGCACCCTCCCATTTGATGATGAGCATGTACCTACGTTATTTAAGAAGATCCGAGGGGGTGTCTTTTATATCCCAGAATATCTCAATCGTTCTGTCGCCACTCTCCTGATGCATATGCTGCAGGTTGACCCACTGAAACGAGCAACTATCAAAGACATAAGAGAGCATGAATGGTTTAAACAAGATTTGCCCAGTTACTTATTTCCTGAA</t>
+  </si>
+  <si>
+    <t>CAGAGCAGTAAGCGCAGCAGCCGGAGTGTGGAAGATGACAAGGAGGGTCACCTGGTGTGCCGGATCGGCGATTGGCTCCAAGAGCGATATGAGATTGTGGGGAACCTGGGTGAAGGCACCTTTGGCAAGGTGGTGGAGTGCTTGGACCATGCCAGAGGGAAGTCTCAGGTTGCCCTGAAGATCATCCGCAACGTGGGCAAGTACCGGGAGGCTGCCCGGCTAGAAATCAACGTGCTCAAAAAAATCAAGGAGAAGGACAAAGAAAACAAGTTCCTGTGTGTCTTGATGTCTGACTGGTTCAACTTCCACGGTCACATGTGCATCGCCTTTGAGCTCCTGGGCAAGAACACCTTTGAGTTCCTGAAGGAGAATAACTTCCAGCCTTACCCCCTACCACATGTCCGGCACATGGCCTACCAGCTCTGCCACGCCCTTAGATTTCTGCATGAGAATCAGCTGACCCATACAGACTTGAAACCAGAGAACATCCTGTTTGTGAATTCTGAGTTTGAAACCCTCTACAATGAGCACAAGAGCTGTGAGGAGAAGTCAGTGAAGAACACCAGCATCCGAGTGGCTGACTTTGGCAGTGCCACATTTGACCATGAGCACCACACCACCATTGTGGCCACCCGTCACTATCGCCCGCCTGAGGTGATCCTTGAGCTGGGCTGGGCACAGCCCTGTGACGTCTGGAGCATTGGCTGCATTCTCTTTGAGTACTACCGGGGCTTCACACTCTTCCAGACCCACGAAAACCGAGAGCACCTGGTGATGATGGAGAAGATCCTAGGGCCCATCCCATCACACATGATCCACCGTACCAGGAAGCAGAAATATTTCTACAAAGGGGGCCTAGTTTGGGATGAGAACAGCTCTGACGGCCGGTATGTGAAGGAGAACTGCAAACCTCTGAAGAGTTACATGCTCCAAGACTCCCTGGAGCACGTGCAGCTGTTTGACCTGATGAGGAGGATGTTAGAATTTGACCCTGCCCAGCGCATCACACTGGCCGAGGCCCTGCTGCACCCCTTCTTTGCTGGCCTGACCCCTGAGGAGCGGTCCTTCCACACC</t>
+  </si>
+  <si>
+    <t>GAACTGAAGGATGACGACTTTGAGAAGATCAGTGAGCTGGGGGCTGGCAATGGCGGTGTGGTGTTCAAGGTCTCCCACAAGCCTTCTGGCCTGGTCATGGCCAGAAAGCTAATTCATCTGGAGATCAAACCCGCAATCCGGAACCAGATCATAAGGGAGCTGCAGGTTCTGCATGAGTGCAACTCTCCGTACATCGTGGGCTTCTATGGTGCGTTCTACAGCGATGGCGAGATCAGTATCTGCATGGAGCACATGGATGGAGGTTCTCTGGATCAAGTCCTGAAGAAAGCTGGAAGAATTCCTGAACAAATTTTAGGAAAAGTTAGCATTGCTGTAATAAAAGGCCTGACATATCTGAGGGAGAAGCACAAGATCATGCACAGAGCATACGGAATGGACAGCCGACCTCCCATGGCAATTTTTGAGTTGTTGGATTACATAGTCAACGAGCCTCCTCCAAAACTGCCCAGTGGAGTGTTCAGTCTGGAATTTCAAGATTTTGTGAATAAATGCTTAATAAAAAACCCCGCAGAGAGAGCAGATTTGAAGCAACTCATGGTTCATGCTTTTATCAAGAGATCTGATGCTGAGGAAGTGGATTTTGCAGGTTGGCTCTGCTCCACCATCGGCCTTAAC</t>
+  </si>
+  <si>
+    <t>MQTVGVHSIVQQLHRNSIQFTDGYEVKEDIGVGSYSVCKRCIHKATNMEFAVKIIDKSKRDPTEEIEILLRYGQHPNIITLKDVYDDGKYVYVVTELMKGGELLDKILRQKFFSEREASAVLFTITKTVEYLHAQGVVHRDLKPSNILYVDESGNPESIRICDFGFAKQLRAENGLLMTPCYTANFVAPEVLKRQGYDAACDIWSLGVLLYTMLTGYTPFANGPDDTPEEILARIGSGKFSLSGGYWNSVSDTAKDLVSKMLHVDPHQRLTAALVLRHPWIVHWDQLPQYQLNRQDAPHLVKGAMAATYSALNRNQSPVLEPVGRSTLAQRRGIKKITSTAL</t>
+  </si>
+  <si>
+    <t>KAPCA_HUMAN_D0_4AE9_A</t>
+  </si>
+  <si>
+    <t>KCC2G_HUMAN_D0_2V7O_A</t>
+  </si>
+  <si>
+    <t>KQYEHVKRDLNPEDFWEIIGELGDGAFGKVYKAQNKETSVLAAAKVIDTKSEEELEDYMVEIDILASCDHPNIVKLLDAFYYENNLWILIEFCAGGAVDAVMLELERPLTESQIQVVCKQTLDALNYLHDNKIIHRDLKAGNILFTLDGDIKLADFGVSAKNMRTIQRRDSFIGTPYWMAPEVVMCETSKDRPYDYKADVWSLGITLIEMAEIEPPHHELNPMRVLLKIAKSEPPTLAQPSRWSSNFKDFLKKCLEKNVDARWTTSQLLQHPFVTVDSNKPIRELIAEAKAEVTEEVEDGKE</t>
+  </si>
+  <si>
+    <t>ACCCAAACTGTTCATGAGTTTGCCAAGGAATTGGATGCCACCAACATATCCATTGATAAAGTTGTTGGAGCAGGTGAATTTGGAGAGGTGTGCAGTGGTCGCTTAAAACTTCCTTCAAAAAAAGAGATTTCAGTGGCCATTAAGACCCTGAAAGTTGGCTACACAGAAAAGCAGAGGAGAGACTTCCTGGGAGAAGCAAGCATTATGGGACAGTTTGACCACCCCAATATCATTCGACTGGAAGGAGTTGTTACCAAAAGTAAGCCAGTTATGATTGTCACAGAATACATGGAGAATGGTTCCTTGGATAGTTTCCTACGTAAACACGATGCCCAGTTTACTGTCATTCAGCTAGTGGGGATGCTTCGAGGGATAGCATCTGGCATGAAGTACCTGTCAGACATGGGCTATGTTCACCGAGACCTCGCTGCTCGGAACATCTTGATCAACAGTAACTTGGTGTGTAAGGTTTCTGATTTCGGACTTTCGCGTGTCCTGGAGGATGACCCAGAAGCTGCTTATACAACAAGAGGAGGGAAGATCCCAATCAGGTGGACATCACCAGAAGCTATAGCCTACCGCAAGTTCACGTCAGCCAGCGATGTATGGAGTTATGGGATTGTTCTCTGGGAGGTGATGTCTTATGGAGAGAGACCATACTGGGAGATGTCCAATCAGGATGTAATTAAAGCTGTAGATGAGGGCTATCGACTGCCACCCCCCATGGACTGCCCAGCTGCCTTGTATCAGCTGATGCTGGACTGCTGGCAGAAAGACAGGAACAACAGACCCAAGTTTGAGCAGATTGTTAGTATTCTGGACAAGCTTATCCGGAATCCCGGCAGCCTGAAGATCATCACCAGTGCAGCCGCAAGGCCATCAAACCTTCTTCTGGACCAAAGCAATGTGGATATCACTACCTTCCGCACAACAGGTGACTGGCTTAATGGTGTCTGGACAGCACACTGCAAGGAAATCTTCACGGGTGTGGAGTACAGTTCTTGTGACACAATAGCCAAGATTTCC</t>
+  </si>
+  <si>
+    <t>MEKDGLCRADQQYECVAEIGEGAYGKVFKARDLKNGGRFVALKRVRVQTGEEGMPLSTIREVAVLRHLETFEHPNVVRLFDVCTVSRTDRETKLTLVFEHVDQDLTTYLDKVPEPGVPTETIKDMMFQLLRGLDFLHSHRVVHRDLKPQNILVTSSGQIKLADFGLARIYSFQMALTSVVVTLWYRAPEVLLQSSYATPVDLWSVGCIFAEMFRRKPLFRGSSDVDQLGKILDVIGLPGEEDWPRDVALPRQAFHSKSAQPIEKFVTDIDELGKDLLLKCLTFNPAKRISAYSALSHPYFQ</t>
+  </si>
+  <si>
+    <t>EPHA3_HUMAN_D0_4GK2_A</t>
+  </si>
+  <si>
+    <t>ATGCCCGGCCCGGCCGCGGGCAGCAGGGCCCGGGTCTACGCCGAGGTGAACAGTCTGAGGAGCCGCGAGTACTGGGACTACGAGGCTCACGTCCCGAGCTGGGGTAATCAAGATGATTACCAACTGGTTCGAAAACTTGGTCGGGGAAAATATAGTGAAGTATTTGAGGCCATTAATATCACCAACAATGAGAGAGTGGTTGTAAAAATCCTGAAGCCAGTGAAGAAAAAGAAGATAAAACGAGAGGTTAAGATTCTGGAGAACCTTCGTGGTGGAACAAATATCATTAAGCTGATTGACACTGTAAAGGACCCCGTGTCAAAGACACCAGCTTTGGTATTTGAATATATCAATAATACAGATTTTAAGCAACTCTACCAGATCCTGACAGACTTTGATATCCGGTTTTATATGTATGAACTACTTAAAGCTCTGGATTACTGCCACAGCAAGGGAATCATGCACAGGGATGTGAAACCTCACAATGTCATGATAGATCACCAACAGAAAAAGCTGCGACTGATAGATTGGGGTCTGGCAGAATTCTATCATCCTGCTCAGGAGTACAATGTTCGTGTAGCCTCAAGGTACTTCAAGGGACCAGAGCTCCTCGTGGACTATCAGATGTATGATTATAGCTTGGACATGTGGAGTTTGGGCTGTATGTTAGCAAGCATGATCTTTCGAAGGGAACCATTCTTCCATGGACAGGACAACTATGACCAGCTTGTTCGCATTGCCAAGGTTCTGGGTACAGAAGAACTGTATGGGTATCTGAAGAAGTATCACATAGACCTAGATCCACACTTCAACGATATCCTGGGACAACATTCACGGAAACGCTGGGAAAACTTTATCCATAGTGAGAACAGACACCTTGTCAGCCCTGAGGCCCTAGATCTTCTGGACAAACTTCTGCGATACGACCATCAACAGAGACTGACTGCCAAAGAGGCCATGGAGCACCCATACTTCTACCCTGTGGTGAAGGAGCAGTCCCAG</t>
+  </si>
+  <si>
+    <t>ETKYTVDKRFGMDFKEIELIGSGGFGQVFKAKHRIDGKTYVIKRVKYNNEKAEREVKALAKLDHVNIVHYNGCWDGFDYDPETSDDSLESSDYDPENSKNSSRSKTKCLFIQMEFCDKGTLEQWIEKRRGEKLDKVLALELFEQITKGVDYIHSKKLIHRDLKPSNIFLVDTKQVKIGDFGLVTSLKNDGKRTRSKGTLRYMSPEQISSQDYGKEVDLYALGLILAELLHVCDTAFETSKFFTDLRDGIISDIFDKKEKTLLQKLLSKKPEDRPNTSEILRTLTVWKKSPEKNERHTC</t>
+  </si>
+  <si>
+    <t>NEK2_HUMAN_D0_2XKE_A</t>
+  </si>
+  <si>
+    <t>ATGGAGCTGAGAGTCGGGAACAGGTACCGGCTGGGCCGGAAGATCGGCAGCGGCTCCTTCGGAGACATCTATCTCGGTACGGACATTGCTGCAGGAGAAGAGGTTGCCATCAAGCTTGAATGTGTCAAAACCAAACACCCTCAGCTCCACATTGAGAGCAAAATCTACAAGATGATGCAGGGAGGAGTGGGCATCCCCACCATCAGATGGTGCGGGGCAGAGGGGGACTACAACGTCATGGTGATGGAGCTGCTGGGGCCAAGCCTGGAGGACCTCTTCAACTTCTGCTCCAGGAAATTCAGCCTCAAAACCGTCCTGCTGCTTGCTGACCAAATGATCAGTCGCATCGAATACATTCATTCAAAGAACTTCATCCACCGGGATGTGAAGCCAGACAACTTCCTCATGGGCCTGGGGAAGAAGGGCAACCTGGTGTACATCATCGACTTCGGGCTGGCCAAGAAGTACCGGGATGCACGCACCCACCAGCACATCCCCTATCGTGAGAACAAGAACCTCACGGGGACGGCGCGGTACGCCTCCATCAACACGCACCTTGGAATTGAACAATCCCGAAGAGATGACTTGGAGTCTCTGGGCTACGTGCTAATGTACTTCAACCTGGGCTCTCTCCCCTGGCAGGGGCTGAAGGCTGCCACCAAGAGACAGAAATACGAAAGGATTAGCGAGAAGAAAATGTCCACCCCCATCGAAGTGTTGTGTAAAGGCTACCCTTCCGAATTTGCCACATACCTGAATTTCTGCCGTTCCTTGCGTTTTGACGACAAGCCTGACTACTCGTACCTGCGGCAGCTTTTCCGGAATCTGTTCCATCGCCAGGGCTTCTCCTATGACTACGTGTTCGACTGGAACATGCTCAAA</t>
+  </si>
+  <si>
+    <t>ATGGCGGCGGCGGCGGCGGCGGGCGCGGGCCCGGAGATGGTCCGCGGGCAGGTGTTCGACGTGGGGCCGCGCTACACCAACCTCTCGTACATCGGCGAGGGCGCCTACGGCATGGTGTGCTCTGCTTATGATAATGTCAACAAAGTTCGAGTAGCTATCAAGAAAATCAGCCCCTTTGAGCACCAGACCTACTGCCAGAGAACCCTGAGGGAGATAAAAATCTTACTGCGCTTCAGACATGAGAACATCATTGGAATCAATGACATTATTCGAGCACCAACCATCGAGCAAATGAAAGATGTATATATAGTACAGGACCTCATGGAAACAGATCTTTACAAGCTCTTGAAGACACAACACCTCAGCAATGACCATATCTGCTATTTTCTCTACCAGATCCTCAGAGGGTTAAAATATATCCATTCAGCTAACGTTCTGCACCGTGACCTCAAGCCTTCCAACCTGCTGCTCAACACCACCTGTGATCTCAAGATCTGTGACTTTGGCCTGGCCCGTGTTGCAGATCCAGACCATGATCACACAGGGTTCCTGACAGAATATGTGGCCACACGTTGGTACAGGGCTCCAGAAATTATGTTGAATTCCAAGGGCTACACCAAGTCCATTGATATTTGGTCTGTAGGCTGCATTCTGGCAGAAATGCTTTCTAACAGGCCCATCTTTCCAGGGAAGCATTATCTTGACCAGCTGAACCACATTTTGGGTATTCTTGGATCCCCATCACAAGAAGACCTGAATTGTATAATAAATTTAAAAGCTAGGAACTATTTGCTTTCTCTTCCACACAAAAATAAGGTGCCATGGAACAGGCTGTTCCCAAATGCTGACTCCAAAGCTCTGGACTTATTGGACAAAATGTTGACATTCAACCCACACAAGAGGATTGAAGTAGAACAGGCTCTGGCCCACCCATATCTGGAGCAGTATTACGACCCGAGTGACGAGCCCATCGCCGAAGCACCATTCAAGTTCGACATGGAATTGGATGACTTGCCTAAGGAAAAGCTCAAAGAACTAATTTTTGAAGAGACTGCTAGATTCCAGCCAGGATACAGATCT</t>
+  </si>
+  <si>
+    <t>MDEQSQGMQGPPVPQFQPQKALRPDMGYNTLANFRIEKKIGRGQFSEVYRAACLLDGVPVALKKVQIFDLMDAKARADCIKEIDLLKQLNHPNVIKYYASFIEDNELNIVLELADAGDLSRMIKHFKKQKRLIPERTVWKYFVQLCSALEHMHSRRVMHRDIKPANVFITATGVVKLGDLGLGRFFSSKTTAAHSLVGTPYYMSPERIHENGYNFKSDIWSLGCLLYEMAALQSPFYGDKMNLYSLCKKIEQCDYPPLPSDHYSEELRQLVNMCINPDPEKRPDVTYVYDVAKRMHACTASS</t>
+  </si>
+  <si>
+    <t>GECSQKGPVPFSHCLPTEKLQRCEKIGEGVFGEVFQTIADHTPVAIKIIAIEGPDLVNGSHQKTFEEILPEIIISKELSLLSGEVCNRTEGFIGLNSVHCVQGSYPPLLLKAWDHYNSTKGSANDRPDFFKDDQLFIVLEFEFGGIDLEQMRTKLSSLATAKSILHQLTASLAVAEASLRFEHRDLHWGNVLLKKTSLKKLHYTLNGKSSTIPSCGLQVSIIDYTLSRLERDGIVVFCDVSMDEDLFTGDGDYQFDIYRLMKKENNNRWGEYHPYSNVLWLHYLTDKMLKQMTFKTKCNTPAMKQIKRKIQEFHRTMLNFSSATDLLCQHRLFK</t>
+  </si>
+  <si>
+    <t>MENFNNFYILTSKELGRGKFAVVRQCISKSTGQEYAAKFLKKRRRGQDCRAEILHEIAVLELAKSCPRVINLHEVYENTSEIILILEYAAGGEIFSLCLPELAEMVSENDVIRLIKQILEGVYYLHQNNIVHLDLKPQNILLSSIYPLGDIKIVDFGMSRKIGHACELREIMGTPEYLAPEILNYDPITTATDMWNIGIIAYMLLTHTSPFVGEDNQETYLNISQVNVDYSEETFSSVSQLATDFIQSLLVKNPEKRPTAEICLSHSWLQQWDFENLFHPEETSSSSQTQDHSVRSSEDKTSKSS</t>
+  </si>
+  <si>
+    <t>GCTGATCCAGAAGAACTGTTCACAAAATTAGAGCGCATTGGGAAAGGCTCATTTGGGGAAGTTTTCAAAGGAATTGATAACCGTACCCAGCAAGTCGTTGCTATTAAAATCATAGACCTTGAGGAAGCCGAAGATGAAATAGAAGACATTCAGCAAGAAATAACTGTCTTGAGTCAATGTGACAGCTCATATGTAACAAAATACTATGGGTCATATTTAAAGGGGTCTAAATTATGGATAATAATGGAATACCTGGGCGGTGGTTCAGCACTGGATCTTCTTCGAGCTGGTCCATTTGATGAGTTCCAGATTGCTACCATGCTAAAGGAAATTTTAAAAGGTCTGGACTATCTGCATTCAGAAAAGAAAATTCACCGAGACATAAAAGCTGCCAATGTCTTGCTCTCAGAACAAGGAGATGTTAAACTTGCTGATTTTGGAGTTGCTGGTCAGCTGACAGATACACAGATTAAAAGAAATACCTTTGTGGGAACTCCATTTTGGATGGCTCCTGAAGTTATTCAACAGTCAGCTTATGACTCAAAAGCTGACATTTGGTCATTGGGAATTACTGCTATTGAACTAGCCAAGGGAGAGCCACCTAACTCCGATATGCATCCAATGAGAGTTCTGTTTCTTATTCCCAAAAACAATCCTCCAACTCTTGTTGGAGACTTTACTAAGTCTTTTAAGGAGTTTATTGATGCTTGCCTGAACAAAGATCCATCATTTCGTCCTACAGCAAAAGAACTTCTGAAACACAAATTCATTGTAAAAAATTCAAAGAAGACTTCTTATCTGACTGAACTGATAGATCGTTTTAAGAGATGGAAGGCAGAA</t>
+  </si>
+  <si>
+    <t>MELRVGNKYRLGRKIGSGSFGDIYLGANIASGEEVAIKLECVKTKHPQLHIESKFYKMMQGGVGIPSIKWCGAEGDYNVMVMELLGPSLEDLFNFCSRKFSLKTVLLLADQMISRIEYIHSKNFIHRDVKPDNFLMGLGKKGNLVYIIDFGLAKKYRDARTHQHIPYRENKNLTGTARYASINTHLGIEQSRRDDLESLGYVLMYFNLGSLPWQGLKAATKRQKYERISEKKMSTPIEVLCKGYPSEFSTYLNFCRSLRFDDKPDYSYLRQLFRNLFHRQGFSYDYVFDWNMLK</t>
+  </si>
+  <si>
+    <t>SSVTASAAPGTASLVPDYWIDGSNRDALSDFFEVESELGRGATSIVYRCKQKGTQKPYALKVLKKTVDKKIVRTEIGVLLRLSHPNIIKLKEIFETPTEISLVLELVTGGELFDRIVEKGYYSERDAADAVKQILEAVAYLHENGIVHRDLKPENLLYATPAPDAPLKIADFGLSKIVEHQVLMKTVCGTPGYCAPEILRGCAYGPEVDMWSVGIITYILLCGFEPFYDERGDQFMFRRILNCEYYFISPWWDEVSLNAKDLVRKLIVLDPKKRLTTFQALQHPWVTGKAANFVHMDTAQKKLQEFNARRKLKAAVKAVVASSRLG</t>
+  </si>
+  <si>
+    <t>dna_end</t>
+  </si>
+  <si>
+    <t>MADDDVLFEDVYELCEVIGKGPFSVVRRCINRETGQQFAVKIVDVAKFTSSPGLSTEDLKREASICHMLKHPHIVELLETYSSDGMLYMVFEFMDGADLCFEIVKRADAGFVYSEAVASHYMRQILEALRYCHDNNIIHRDVKPHCVLLASKENSAPVKLGGFGVAIQLGESGLVAGGRVGTPHFMAPEVVKREPYGKPVDVWGCGVILFILLSGCLPFYGTKERLFEGIIKGKYKMNPRQWSHISESAKDLVRRMLMLDPAERITVYEALNHPWLKERDRYAYKIHLPETVEQLRKFNARRKLKGAVLAAVSSHKFNSFYGDPPEELPDFSEDPTSSGA</t>
+  </si>
+  <si>
+    <t>FAK1_HUMAN_D0_2IJM_B</t>
+  </si>
+  <si>
+    <t>DAPK1_HUMAN_D0_3F5G_A</t>
+  </si>
+  <si>
+    <t>CHK2_HUMAN_D0_2CN5_A</t>
+  </si>
+  <si>
+    <t>GTGATCGACCCCTCAGAGCTCACTTTTGTCCAAGAGATTGGCAGTGGGCAATTTGGGTTGGTGCATCTGGGCTACTGGCTCAACAAGGACAAGGTGGCTATCAAAACCATTCGGGAAGGGGCTATGTCAGAAGAGGACTTCATAGAGGAGGCTGAAGTAATGATGAAACTCTCTCATCCCAAACTGGTGCAGCTGTATGGGGTGTGCCTGGAGCAGGCCCCCATCTGCCTGGTGTTTGAGTTCATGGAGCACGGCTGCCTGTCAGATTATCTACGCACCCAGCGGGGACTTTTTGCTGCAGAGACCCTGCTGGGCATGTGTCTGGATGTGTGTGAGGGCATGGCCTACCTGGAAGAGGCATGTGTCATCCACAGAGACTTGGCTGCCAGAAATTGTTTGGTGGGAGAAAACCAAGTCATCAAGGTGTCTGACTTTGGGATGACAAGGTTCGTTCTGGATGATCAGTACACCAGTTCCACAGGCACCAAATTCCCGGTGAAGTGGGCATCCCCAGAGGTTTTCTCTTTCAGTCGCTATAGCAGCAAGTCCGATGTGTGGTCATTTGGTGTGCTGATGTGGGAAGTTTTCAGTGAAGGCAAAATCCCGTATGAAAACCGAAGCAACTCAGAGGTGGTGGAAGACATCAGTACCGGATTTCGGTTGTACAAGCCCCGGCTGGCCTCCACACACGTCTACCAGATTATGAATCACTGCTGGAAAGAGAGACCAGAAGATCGGCCAGCCTTCTCCAGACTGCTGCGTCAACTGGCTGAAATTGCAGAATCAGGACTT</t>
+  </si>
+  <si>
+    <t>MSDEEILEKLRSIVSVGDPKKKYTRFEKIGQGASGTVYTAMDVATGQEVAIKQMNLQQQPKKELIINEILVMRENKNPNIVNYLDSYLVGDELWVVMEYLAGGSLTDVVTETCMDEGQIAAVCRECLQALEFLHSNQVIHRDIKSDNILLGMDGSVKLTDFGFCAQITPEQSKRSTMVGTPYWMAPEVVTRKAYGPKVDIWSLGIKAIEMIEGEPPYLNENPLRALYLIATNGTPELQNPEKLSAIFRDFLNRCLEMDVEKRGSAKELLQHQFLKIAKPLSSLTPLIAAAKEATKNNH</t>
+  </si>
+  <si>
+    <t>MSQSKGKKRNPGLKIPKEAFEQPQTSSTPPRDLDSKACISIGNQNFEVKADDLEPIMELGRGAYGVVEKMRHVPSGQIMAVKRIRATVNSQEQKRLLMDLDISMRTVDCPFTVTFYGALFREGDVWICMELMDTSLDKFYKQVIDKGQTIPEDILGKIAVSIVKALEHLHSKLSVIHRDVKPSNVLINALGQVKMCDFGISGYLVDSVAKTIDAGCKPYMAPERINPELNQKGYSVKSDIWSLGITMIELAILRFPYDSWGTPFQQLKQVVEEPSPQLPADKFSAEFVDFTSQCLKKNSKERPTYPELMQHPFFTLHESKGTDVASFVKLILGD</t>
+  </si>
+  <si>
+    <t>DYRK2_HUMAN_D0_3KVW_A</t>
+  </si>
+  <si>
+    <t>GCGGCTCCACCGGCGAAAGAGATCCCGGAGGTCCTAGTGGACCCACGCAGCCGGCGGCGCTATGTGCGGGGCCGCTTTTTGGGCAAGGGCGGCTTTGCCAAGTGCTTCGAGATCTCGGACGCGGACACCAAGGAGGTGTTCGCGGGCAAGATTGTGCCTAAGTCTCTGCTGCTCAAGCCGCACCAGAGGGAGAAGATGTCCATGGAAATATCCATTCACCGCAGCCTCGCCCACCAGCACGTCGTAGGATTCCACGGCTTTTTCGAGGACAACGACTTCGTGTTCGTGGTGTTGGAGCTCTGCCGCCGGAGGTCTCTCCTGGAGCTGCACAAGAGGAGGAAAGCCCTGACTGAGCCTGAGGCCCGATACTACCTACGGCAAATTGTGCTTGGCTGCCAGTACCTGCACCGAAACCGAGTTATTCATCGAGACCTCAAGCTGGGCAACCTTTTCCTGAATGAAGATCTGGAGGTGAAAATAGGGGATTTTGGACTGGCAACCAAAGTCGAATATGACGGGGAGAGGAAGAAGACCCTGTGTGGGACTCCTAATTACATAGCTCCCGAGGTGCTGAGCAAGAAAGGGCACAGTTTCGAGGTGGATGTGTGGTCCATTGGGTGTATCATGTATACCTTGTTAGTGGGCAAACCACCTTTTGAGACTTCTTGCCTAAAAGAGACCTACCTCCGGATCAAGAAGAATGAATACAGTATTCCCAAGCACATCAACCCCGTGGCCGCCTCCCTCATCCAGAAGATGCTTCAGACAGATCCCACTGCCCGCCCAACCATTAACGAGCTGCTTAATGACGAGTTCTTTACTTCTGGCTATATCCCTGCCCGTCTCCCCATCACCTGCCTGACCATTCCACCAAGGTTTTCGATTGCTCCCAGCAGCCTGGACCCCAGCAACCGGAAGCCCCTCACAGTCCTCAATAAA</t>
+  </si>
+  <si>
+    <t>QSSKRSSRSVEDDKEGHLVCRIGDWLQERYEIVGNLGEGTFGKVVECLDHARGKSQVALKIIRNVGKYREAARLEINVLKKIKEKDKENKFLCVLMSDWFNFHGHMCIAFELLGKNTFEFLKENNFQPYPLPHVRHMAYQLCHALRFLHENQLTHTDLKPENILFVNSEFETLYNEHKSCEEKSVKNTSIRVADFGSATFDHEHHTTIVATRHYRPPEVILELGWAQPCDVWSIGCILFEYYRGFTLFQTHENREHLVMMEKILGPIPSHMIHRTRKQKYFYKGGLVWDENSSDGRYVKENCKPLKSYMLQDSLEHVQLFDLMRRMLEFDPAQRITLAEALLHPFFAGLTPEERSFHT</t>
+  </si>
+  <si>
+    <t>MK07_HUMAN_D0_4IC7_D</t>
+  </si>
+  <si>
+    <t>ATGCAGACAGTTGGTGTACATTCAATTGTTCAGCAGTTACACAGGAACAGTATTCAGTTTACTGATGGATATGAAGTAAAAGAAGATATTGGAGTTGGCTCCTACTCTGTTTGCAAGAGATGTATACATAAAGCTACAAACATGGAGTTTGCAGTGAAGATTATTGATAAAAGCAAGAGAGACCCAACAGAAGAAATTGAAATTCTTCTTCGTTATGGACAGCATCCAAACATTATCACTCTAAAGGATGTATATGATGATGGAAAGTATGTGTATGTAGTAACAGAACTTATGAAAGGAGGTGAATTGCTGGATAAAATTCTTAGACAAAAATTTTTCTCTGAACGAGAGGCCAGTGCTGTCCTGTTCACTATAACTAAAACCGTTGAATATCTTCACGCACAAGGGGTGGTTCATAGAGACTTGAAACCTAGCAACATTCTTTATGTGGATGAATCTGGTAATCCGGAATCTATTCGAATTTGTGATTTTGGCTTTGCAAAACAGCTGAGAGCGGAAAATGGTCTTCTCATGACTCCTTGTTACACTGCAAATTTTGTTGCACCAGAGGTTTTAAAAAGACAAGGCTATGATGCTGCTTGTGATATATGGAGTCTTGGTGTCCTACTCTATACAATGCTTACCGGTTACACTCCATTTGCAAATGGTCCTGATGATACACCAGAGGAAATATTGGCACGAATAGGTAGCGGAAAATTCTCACTCAGTGGTGGTTACTGGAATTCTGTTTCAGACACAGCAAAGGACCTGGTGTCAAAGATGCTTCATGTAGACCCTCATCAGAGACTGACTGCTGCTCTTGTGCTCAGACATCCTTGGATCGTCCACTGGGACCAACTGCCACAATACCAACTAAACAGACAGGATGCACCACATCTAGTAAAGGGTGCCATGGCAGCTACATATTCTGCTTTGAACCGTAATCAGTCACCAGTTTTGGAACCAGTAGGCCGCTCTACTCTTGCTCAGCGGAGAGGTATTAAAAAAATCACCTCAACAGCCCTG</t>
+  </si>
+  <si>
+    <t>KS6A3_HUMAN_D0_4JG7_A</t>
+  </si>
+  <si>
+    <t>MGKVKATPMTPEQAMKQYMQKLTAFEHHEIFSYPEIYFLGLNAKKRQGMTGGPNNGGYDDDQGSYVQVPHDHVAYRYEVLKVIGKGSFGQVVKAYDHKVHQHVALKMVRNEKRFHRQAAEEIRILEHLRKQDKDNTMNVIHMLENFTFRNHICMTFELLSMNLYELIKKNKFQGFSLPLVRKFAHSILQCLDALHKNRIIHCDLKPENILLKQQGRSGIKVIDFGSSCYEHQRVYTYIQSRFYRAPEVILGARYGMPIDMWSLGCILAELLTGYPLLPGEDEGDQLACMIELLGMPSQKLLDASKRAKNFVSSKGYPRYCTVTTLSDGSVVLNGGRSRRGKLRGPPESREWGNALKGCDDPLFLDFLKQCLEWDPAVRMTPGQALRHPWLRRRLPKPPTGEKTSVKR</t>
+  </si>
+  <si>
+    <t>CAGCAGTTCCCGCAGTTCCACGTCAAGTCCGGCCTGCAGATCAAGAAGAACGCCATCATCGATGACTACAAGGTCACCAGCCAGGTCCTGGGGCTGGGCATCAACGGCAAAGTTTTGCAGATCTTCAACAAGAGGACCCAGGAGAAATTCGCCCTCAAAATGCTTCAGGACTGCCCCAAGGCCCGCAGGGAGGTGGAGCTGCACTGGCGGGCCTCCCAGTGCCCGCACATCGTACGGATCGTGGATGTGTACGAGAATCTGTACGCAGGGAGGAAGTGCCTGCTGATTGTCATGGAATGTTTGGACGGTGGAGAACTCTTTAGCCGAATCCAGGATCGAGGAGACCAGGCATTCACAGAAAGAGAAGCATCCGAAATCATGAAGAGCATCGGTGAGGCCATCCAGTATCTGCATTCAATCAACATTGCCCATCGGGATGTCAAGCCTGAGAATCTCTTATACACCTCCAAAAGGCCCAACGCCATCCTGAAACTCACTGACTTTGGCTTTGCCAAGGAAACCACCAGCCACAACTCTTTGACCACTCCTTGTTATACACCGTACTATGTGGCTCCAGAAGTGCTGGGTCCAGAGAAGTATGACAAGTCCTGTGACATGTGGTCCCTGGGTGTCATCATGTACATCCTGCTGTGTGGGTATCCCCCCTTCTACTCCAACCACGGCCTTGCCATCTCTCCGGGCATGAAGACTCGCATCCGAATGGGCCAGTATGAATTTCCCAACCCAGAATGGTCAGAAGTATCAGAGGAAGTGAAGATGCTCATTCGGAATCTGCTGAAAACAGAGCCCACCCAGAGAATGACCATCACCGAGTTTATGAACCACCCTTGGATCATGCAATCAACAAAGGTCCCTCAAACCCCACTGCACACCAGCCGGGTCCTGAAGGAGGACAAGGAGCGGTGGGAGGATGTCAAGGGGTGTCTTCATGACAAGAACAGCGACCAGGCC</t>
+  </si>
+  <si>
+    <t>CDK2_HUMAN_D0_4BCP_A</t>
+  </si>
+  <si>
+    <t>MP2K4_HUMAN_D0_3ALN_C</t>
+  </si>
+  <si>
+    <t>CGGGACTCGAGTGATGATTGGGAGATTCCTGATGGGCAGATTACAGTGGGACAAAGAATTGGATCTGGATCATTTGGAACAGTCTACAAGGGAAAGTGGCATGGTGATGTGGCAGTGAAAATGTTGAATGTGACAGCACCTACACCTCAGCAGTTACAAGCCTTCAAAAATGAAGTAGGAGTACTCAGGAAAACACGACATGTGAATATCCTACTCTTCATGGGCTATTCCACAAAGCCACAACTGGCTATTGTTACCCAGTGGTGTGAGGGCTCCAGCTTGTATCACCATCTCCATATCATTGAGACCAAATTTGAGATGATCAAgCTTATAGATATTGCACGACAGACTGCACAGGGCATGGATTACTTACACGCCAAGTCAATCATCCACAGAGACCTCAAGAGTAATAATATATTTCTTCATGAAGACCTCACAGTAAAAATAGGTGATTTTGGTCTAGCTACAGTGAAATCTCGATGGAGTGGGTCCCATCAGTTTGAACAGTTGTCTGGgTCCATTTTGTGGATGGCACCAGAAGTCATCAGAATGCAAGATAAAAATCCATACAGCTTTCAGTCAGATGTATATGCATTTGGgATTGTTCTGTATGAATTGATGACTGGACAGTTACCTTATTCAAACATCAACAACAGGGACCAGATAATTTTTATGGTGGGACGAGGATACCTGTCTCCAGATCTCAGTAAGGTACGGAGTAACTGTCCAAAAGCCATGAAGAGATTAATGGCAGAGTGCCTCAAAAAGAAAAGAGATGAGAGACCACTCTTTCCCCAAATTCTCGCCTCTATTGAGCTGCTGGCCCGC</t>
+  </si>
+  <si>
+    <t>ACCACCTCACTTGAAGCTTTGCCCACAGGGACAGTGCTGACAGACAAGAGTGGGCGACAGTGGAAGCTGAAGTCCTTCCAGACCAGGGACAACCAGGGCATTCTCTATGAAGCTGCACCCACCTCCACCCTCACCTGTGACTCAGGACCACAGAAGCAAAAGTTCTCACTCAAACTGGATGCCAAGGATGGGCGCTTGTTCAATGAGCAGAACTTCTTCCAGCGGGCCGCCAAGCCTCTGCAAGTCAACAAGTGGAAGAAGCTGTACTCGACCCCACTGCTGGCCATCCCTACCTGCATGGGTTTCGGTGTTCACCAGGACAAATACAGGTTCTTGGTGTTACCCAGCCTGGGGAGGAGCCTTCAGTCGGCCCTGGATGTCAGCCCAAAGCATGTGCTGTCAGAGAGGTCTGTGCTGCAGGTGGCCTGCCGGCTGCTGGATGCCCTGGAGTTCCTCCATGAGAATGAGTATGTTCATGGAAATGTGACAGCTGAAAATATCTTTGTGGATCCAGAGGACCAGAGTCAGGTGACTTTGGCAGGCTATGGCTTCGCCTTCCGCTATTGCCCAAGTGGCAAACACGTGGCCTACGTGGAAGGCAGCAGGAGCCCTCACGAGGGGGACCTTGAGTTCATTAGCATGGACCTGCACAAGGGATGCGGGCCCTCCCGCCGCAGCGACCTCCAGAGCCTGGGCTACTGCATGCTGAAGTGGCTCTACGGGTTTCTGCCATGGACAAATTGCCTTCCCAACACTGAGGACATCATGAAGCAAAAACAGAAGTTTGTTGATAAGCCGGGGCCCTTCGTGGGACCCTGCGGTCACTGGATCAGGCCCTCAGAGACCCTGCAGAAGTACCTGAAGGTGGTGATGGCCCTCACGTATGAGGAGAAGCCGCCCTACGCCATGCTGAGGAACAACCTAGAAGCTTTGCTGCAGGATCTGCGTGTGTCTCCATATGACCCCATTGGCCTCCCGATGGTGCCC</t>
+  </si>
+  <si>
+    <t>TCACCACAGCGGGAGCCACAGCGAGTATCCCATGAGCAGTTCCGGGCTGCCCTGCAGCTGGTGGTGGACCCAGGCGACCCCCGCTCCTACCTGGACAACTTCATCAAGATTGGCGAGGGCTCCACGGGCATCGTGTGCATCGCCACCGTGCGCAGCTCGGGCAAGCTGGTGGCCGTCAAGAAGATGGACCTGCGCAAGCAGCAGAGGCGCGAGCTGCTCTTCAACGAGGTGGTAATCATGAGGGACTACCAGCACGAGAATGTGGTGGAGATGTACAACAGCTACCTGGTGGGGGACGAGCTCTGGGTGGTCATGGAGTTCCTGGAAGGAGGCGCCCTCACCGACATCGTCACCCACACCAGGATGAACGAGGAGCAGATCGCGGCCGTGTGCCTTGCAGTGCTGCAGGCCCTGTCGGTGCTCCACGCCCAGGGCGTCATCCACCGGGACATCAAGAGCGACTCGATCCTGCTGACCCATGATGGCAGGGTGAAGCTGTCAGACTTTGGGTTCTGCGCCCAGGTGAGCAAGGAAGTGCCCCGAAGGAAGTCGCTGGTCGGCACGCCCTACTGGATGGCCCCAGAGCTCATCTCCCGCCTTCCCTACGGGCCAGAGGTAGACATCTGGTCGCTGGGGATAATGGTGATTGAGATGGTGGACGGAGAGCCCCCCTACTTCAACGAGCCACCCCTCAAAGCCATGAAGATGATTCGGGACAACCTGCCACCCCGACTGAAGAACCTGCACAAGGTGTCGCCATCCCTGAAGGGCTTCCTGGACCGCCTGCTGGTGCGAGACCCTGCCCAGCGGGCCACGGCAGCCGAGCTGCTGAAGCACCCATTCCTGGCCAAGGCAGGGCCGCCTGCCAGCATCGTGCCCCTCATGCGCCAGAACCGCACCAGA</t>
+  </si>
+  <si>
+    <t>SIESSGKLKISPEQHWDFTAEDLKDLGEIGRGAYGSVNKMVHKPSGQIMAVKRIRSTVDEKEQKQLLMDLDVVMRSSDCPYIVQFYGALFREGDCWICMELMSTSFDKFYKYVYSVLDDVIPEEILGKITLATVKALNHLKENLKIIHRDIKPSNILLDRSGNIKLCDFGISGQLVDSIAKTRDAGCRPYMAPERIDPSASRQGYDVRSDVWSLGITLYELATGRFPYPKWNSVFDQLTQVVKGDPPQLSNSEEREFSPSFINFVNLCLTKDESKRPKYKELLKHPFILMYEERAVEVACYVCKILDQMPATPSSPMYVD</t>
+  </si>
+  <si>
+    <t>TDSFSGRFEDVYQLQEDVLGEGAHARVQTCINLITSQEYAVKIIEKQPGHIRSRVFREVEMLYQCQGHRNVLELIEFFEEEDRFYLVFEKMRGGSILSHIHKRRHFNELEASVVVQDVASALDFLHNKGIAHRDLKPENILCEHPNQVSPVKICDFDLGSGIKLNGDCSPISTPELLTPCGSAEYMAPEVVEAFSEEASIYDKRCDLWSLGVILYILLSGYPPFVGRCGSDCGWDRGEACPACQNMLFESIQEGKYEFPDKDWAHISCAAKDLISKLLVRDAKQRLSAAQVLQHPWVQGCAPENTLPTPMVLQR</t>
+  </si>
+  <si>
+    <t>WALNMKELKLLQTIGKGEFGDVMLGDYRGNKVAVKCIKNDATAQAFLAEASVMTQLRHSNLVQLLGVIVEEKGGLYIVTEYMAKGSLVDYLRSRGRSVLGGDCLLKFSLDVCEAMEYLEGNNFVHRDLAARNVLVSEDNVAKVSDFGLTKEASSTQDTGKLPVKWTAPEALREKKFSTKSDVWSFGILLWEIYSFGRVPYPRIPLKDVVPRVEKGYKMDAPDGCPPAVYEVMKNCWHLDAAMRPSFLQLREQLEHIKTHELHL</t>
+  </si>
+  <si>
+    <t>MPGPAAGSRARVYAEVNSLRSREYWDYEAHVPSWGNQDDYQLVRKLGRGKYSEVFEAINITNNERVVVKILKPVKKKKIKREVKILENLRGGTNIIKLIDTVKDPVSKTPALVFEYINNTDFKQLYQILTDFDIRFYMYELLKALDYCHSKGIMHRDVKPHNVMIDHQQKKLRLIDWGLAEFYHPAQEYNVRVASRYFKGPELLVDYQMYDYSLDMWSLGCMLASMIFRREPFFHGQDNYDQLVRIAKVLGTEELYGYLKKYHIDLDPHFNDILGQHSRKRWENFIHSENRHLVSPEALDLLDKLLRYDHQQRLTAKEAMEHPYFYPVVKEQSQ</t>
+  </si>
+  <si>
+    <t>AAGAGGCAGTGGGCTTTGGAAGACTTTGAAATTGGTCGCCCTCTGGGTAAAGGAAAGTTTGGTAATGTTTATTTGGCAAGAGAAAAGCAAAGCAAGTTTATTCTGGCTCTTAAAGTGTTATTTAAAGCTCAGCTGGAGAAAGCCGGAGTGGAGCATCAGCTCAGAAGAGAAGTAGAAATACAGTCCCACCTTCGGCATCCTAATATTCTTAGACTGTATGGTTATTTCCATGATGCTACCAGAGTCTACCTAATTCTGGAATATGCACCACTTGGAACAGTTTATAGAGAACTTCAGAAACTTTCAAAGTTTGATGAGCAGAGAACTGCTACTTATATAACAGAATTGGCAAATGCCCTGTCTTACTGTCATTCGAAGAGAGTTATTCATAGAGACATTAAGCCAGAGAACTTACTTCTTGGATCAGCTGGAGAGCTTAAAATTGCAGATTTTGGGTGGTCAGTACATGCTCCATCTTCCAGGAGGACCACTCTCTGTGGCACCCTGGACTACCTGCCCCCTGAAATGATTGAAGGTCGGATGCATGATGAGAAGGTGGATCTCTGGAGCCTTGGAGTTCTTTGCTATGAATTTTTAGTTGGGAAGCCTCCTTTTGAGGCAAACACATACCAAGAGACCTACAAAAGAATATCACGGGTTGAATTCACATTCCCTGACTTTGTAACAGAGGGAGCCAGGGACCTCATTTCAAGACTGTTGAAGCATAATCCCAGCCAGAGGCCAATGCTCAGAGAAGTACTTGAACACCCCTGGATCACAGCAAATTCATCAAAACCATCA</t>
+  </si>
+  <si>
+    <t>ATGGAGCTACGTGTGGGGAACAAGTACCGCCTGGGACGGAAGATCGGGAGCGGGTCCTTCGGAGATATCTACCTGGGTGCCAACATCGCCTCTGGTGAGGAAGTCGCCATCAAGCTGGAGTGTGTGAAGACAAAGCACCCCCAGCTGCACATCGAGAGCAAGTTCTACAAGATGATGCAGGGTGGCGTGGGGATCCCGTCCATCAAGTGGTGCGGAGCTGAGGGCGACTACAACGTGATGGTCATGGAGCTGCTGGGGCCTAGCCTCGAGGACCTGTTCAACTTCTGTTCCCGCAAATTCAGCCTCAAGACGGTGCTGCTCTTGGCCGACCAGATGATCAGCCGCATCGAGTATATCCACTCCAAGAACTTCATCCACCGGGACGTCAAGCCCGACAACTTCCTCATGGGGCTGGGGAAGAAGGGCAACCTGGTCTACATCATCGACTTCGGCCTGGCCAAGAAGTACCGGGACGCCCGCACCCACCAGCACATTCCCTACCGGGAAAACAAGAACCTGACCGGCACGGCCCGCTACGCTTCCATCAACACGCACCTGGGCATTGAGCAAAGCCGTCGAGATGACCTGGAGAGCCTGGGCTACGTGCTCATGTACTTCAACCTGGGCTCCCTGCCCTGGCAGGGGCTCAAAGCAGCCACCAAGCGCCAGAAGTATGAACGGATCAGCGAGAAGAAGATGTCAACGCCCATCGAGGTCCTCTGCAAAGGCTATCCCTCCGAATTCTCAACATACCTCAACTTCTGCCGCTCCCTGCGGTTTGACGACAAGCCCGACTACTCTTACCTACGTCAGCTCTTCCGCAACCTCTTCCACCGGCAGGGCTTCTCCTATGACTACGTCTTTGACTGGAACATGCTGAAA</t>
+  </si>
+  <si>
+    <t>MK03_HUMAN_D0_2ZOQ_B</t>
+  </si>
+  <si>
+    <t>ATGTCTCAGTCGAAAGGCAAGAAGCGAAACCCTGGCCTTAAAATTCCAAAAGAAGCATTTGAACAACCTCAGACCAGTTCCACACCACCTCGAGATTTAGACTCCAAGGCTTGCATTTCTATTGGAAATCAGAACTTTGAGGTGAAGGCAGATGACCTGGAGCCTATAATGGAACTGGGACGAGGTGCGTACGGGGTGGTGGAGAAGATGCGGCACGTGCCCAGCGGGCAGATCATGGCAGTGAAGCGGATCCGAGCCACAGTAAATAGCCAGGAACAGAAACGGCTACTGATGGATTTGGATATTTCCATGAGGACGGTGGACTGTCCATTCACTGTCACCTTTTATGGCGCACTGTTTCGGGAGGGTGATGTGTGGATCTGCATGGAGCTCATGGATACATCACTAGATAAATTCTACAAACAAGTTATTGATAAAGGCCAGACAATTCCAGAGGACATCTTAGGGAAAATAGCAGTTTCTATTGTAAAAGCATTAGAACATTTACATAGTAAGCTGTCTGTCATTCACAGAGACGTCAAGCCTTCTAATGTACTCATCAATGCTCTCGGTCAAGTGAAGATGTGCGATTTTGGAATCAGTGGCTACTTGGTGGACTCTGTTGCTAAAACAATTGATGCAGGTTGCAAACCATACATGGCCCCTGAAAGAATAAACCCAGAGCTCAACCAGAAGGGATACAGTGTGAAGTCTGACATTTGGAGTCTGGGCATCACGATGATTGAGTTGGCCATCCTTCGATTTCCCTATGATTCATGGGGAACTCCATTTCAGCAGCTCAAACAGGTGGTAGAGGAGCCATCGCCACAACTCCCAGCAGACAAGTTCTCTGCAGAGTTTGTTGACTTTACCTCACAGTGCTTAAAGAAGAATTCCAAAGAACGGCCTACATACCCAGAGCTAATGCAACATCCATTTTTCACCCTACATGAATCCAAAGGAACAGATGTGGCATCTTTTGTAAAACTGATTCTTGGAGAC</t>
+  </si>
+  <si>
+    <t>TCAACCAGGGATTATGAGATTCAAAGAGAAAGAATAGAACTTGGACGATGTATTGGAGAAGGCCAATTTGGAGATGTACATCAAGGCATTTATATGAGTCCAGAGAATCCAGCTTTGGCGGTTGCAATTAAAACATGTAAAAACTGTACTTCGGACAGCGTGAGAGAGAAATTTCTTCAAGAAGCCTTAACAATGCGTCAGTTTGACCATCCTCATATTGTGAAGCTGATTGGAGTCATCACAGAGAATCCTGTCTGGATAATCATGGAGCTGTGCACACTTGGAGAGCTGAGGTCATTTTTGCAAGTAAGGAAATACAGTTTGGATCTAGCATCTTTGATCCTGTATGCCTATCAGCTTAGTACAGCTCTTGCATATCTAGAGAGCAAAAGATTTGTACACAGGGACATTGCTGCTCGGAATGTTCTGGTGTCCTCAAATGATTGTGTAAAATTAGGAGACTTTGGATTATCCCGATATATGGAAGATAGTACTTACTACAAAGCTTCCAAAGGAAAATTGCCTATTAAATGGATGGCTCCAGAGTCAATCAATTTTCGACGTTTTACCTCAGCTAGTGACGTATGGATGTTTGGTGTGTGTATGTGGGAGATACTGATGCATGGTGTGAAGCCTTTTCAAGGAGTGAAGAACAATGATGTAATCGGTCGAATTGAAAATGGGGAAAGATTACCAATGCCTCCAAATTGTCCTCCTACCCTCTACAGCCTTATGACGAAATGCTGGGCCTATGACCCCAGCAGGCGGCCCAGGTTTACTGAACTTAAAGCTCAGCTCAGCACAATCCTGGAGGAAGAGAAGGCTCAGCAAGAAGAG</t>
+  </si>
+  <si>
+    <t>DPEELFTKLEKIGKGSFGEVFKGIDNRTQKVVAIKIIDLEEAEDEIEDIQQEITVLSQCDSPYVTKYYGSYLKDTKLWIIMEYLGGGSALDLLEPGPLDETQIATILREILKGLDYLHSEKKIHRDIKAANVLLSEHGEVKLADFGVAGQLTDTQIKRNTFVGTPFWMAPEVIKQSAYDSKADIWSLGITAIELARGEPPHSELHPMKVLFLIPKNNPPTLEGNYSKPLKEFVEACLNKEPSFRPTAKELLKHKFILRNAKKTSYLTELID</t>
+  </si>
+  <si>
+    <t>MAPK3_HUMAN_D0_3FXW_A</t>
+  </si>
+  <si>
+    <t>AAGCAGTACGAACACGTGAAGAGGGACCTGAACCCCGAAGACTTTTGGGAGATTATAGGAGAACTGGGCGACGGAGCCTTTGGGAAAGTGTACAAGGCCCAGAATAAAGAGACCAGTGTTTTAGCTGCTGCAAAAGTGATTGACACTAAATCTGAAGAAGAACTTGAAGATTACATGGTAGAGATTGACATATTAGCATCTTGTGATCACCCAAATATAGTCAAGCTTCTAGATGCCTTCTATTATGAGAACAATCTTTGGATCCTCATTGAATTTTGTGCAGGTGGAGCAGTAGATGCTGTGATGCTTGAACTTGAGAGACCATTAACTGAGTCCCAAATACAAGTAGTTTGCAAGCAGACTTTAGATGCATTGAACTACTTACATGATAATAAGATCATCCACAGAGATCTGAAGGCTGGCAACATTCTCTTTACCTTAGATGGAGATATCAAATTGGCGGATTTTGGAGTATCAGCTAAAAACATGAGGACAATTCAAAGAAGAGATTCCTTTATTGGTACACCATATTGGATGGCTCCTGAAGTAGTCATGTGTGAAACATCTAAGGACAGACCCTATGACTACAAAGCTGATGTTTGGTCCCTGGGTATCACTTTAATAGAAATGGCTGAGATAGAACCACCTCATCATGAATTAAATCCAATGCGAGTGCTGCTAAAAATAGCAAAATCTGAGCCACCTACATTAGCACAGCCATCCAGATGGTCTTCAAATTTTAAGGACTTTCTAAAGAAATGCTTAGAAAAGAATGTGGATGCCAGGTGGACTACATCTCAGCTGCTGCAGCATCCCTTTGTTACTGTTGATTCCAACAAACCCATCCGAGAATTGATTGCAGAGGCGAAGGCTGAAGTAACAGAAGAAGTTGAAGATGGCAAAGAG</t>
+  </si>
+  <si>
+    <t>ATGCCTTCCCGGGCTGAGGACTATGAAGTGTTGTACACCATTGGCACAGGCTCCTACGGCCGCTGCCAGAAGATCCGGAGGAAGAGTGATGGCAAGATATTAGTTTGGAAAGAACTTGACTATGGCTCCATGACAGAAGCTGAGAAACAGATGCTTGTTTCTGAAGTGAATTTGCTTCGTGAACTGAAACATCCAAACATCGTTCGTTACTATGATCGGATTATTGACCGGACCAATACAACACTGTACATTGTAATGGAATATTGTGAAGGAGGGGATCTGGCTAGTGTAATTACAAAGGGAACCAAGGAAAGGCAATACTTAGATGAAGAGTTTGTTCTTCGAGTGATGACTCAGTTGACTCTGGCCCTGAAGGAATGCCACAGACGAAGTGATGGTGGTCATACCGTATTGCATCGGGATCTGAAACCAGCCAATGTTTTCCTGGATGGCAAGCAAAACGTCAAGCTTGGAGACTTTGGGCTAGCTAGAATATTAAACCATGACACGAGTTTTGCAAAAACATTTGTTGGCACACCTTATTACATGTCTCCTGAACAAATGAATCGCATGTCCTACAATGAGAAATCAGATATCTGGTCATTGGGCTGCTTGCTGTATGAGTTATGTGCATTAATGCCTCCATTTACAGCTTTTAGCCAGAAAGAACTCGCTGGGAAAATCAGAGAAGGCAAATTCAGGCGAATTCCATACCGTTACTCTGATGAATTGAATGAAATTATTACGAGGATGTTAAACTTAAAGGATTACCATCGACCTTCTGTTGAAGAAATTCTTGAGAACCCTTTAATA</t>
+  </si>
+  <si>
+    <t>TVFRQENVDDYYDTGEELGSGQFAVVKKCREKSTGLQYAAKFIKKRRTKSSRRGVSREDIEREVSILKEIQHPNVITLHEVYENKTDVILILELVAGGELFDFLAEKESLTEEEATEFLKQTLNGVYYLHSLQIAHFDLKPENIMLLDRNVPKPRIKIIDFGLAHKIDFGNEFKNIFGTPEFVAPEIVNYEPLGLEADMWSIGVITYILLSGASPFLGDTKQETLANVSAVNYEFEDEYFSNTSALAKDFIRRLLVKDPKKRMTIQDSLQHPWIKPKDTQQALS</t>
+  </si>
+  <si>
+    <t>GATGAACAACCTCACATCGGAAACTACAGACTGTTGAAAACAATCGGCAAGGGGAATTTTGCAAAAGTAAAATTGGCAAGACATATCCTTACAGGCAGAGAGGTTGCAATAAAAATAATTGACAAAACTCAGTTGAATCCAACAAGTCTACAAAAGCTCTTCAGAGAAGTAAGAATAATGAAGATTTTAAATCATCCCAATATAGTGAAGTTATTCGAAGTCATTGAAACTGAAAAAACACTCTACCTAATCATGGAATATGCAAGTGGAGGTGAAGTATTTGACTATTTGGTTGCACATGGCAGGATGAAGGAAAAAGAAGCAAGATCTAAATTTAGACAGATTGTGTCTGCAGTTCAATACTGCCATCAGAAACGGATCGTACATCGAGACCTCAAGGCTGAAAATCTATTGTTAGATGCCGATATGAACATTAAAATAGCAGATTTCGGTTTTAGCAATGAATTTACTGTTGGCGGTAAACTCGACACGTTTTGTGGCAGTCCTCCATACGCAGCACCTGAGCTCTTCCAGGGCAAGAAATATGACGGGCCAGAAGTGGATGTGTGGAGTCTGGGGGTCATTTTATACACACTAGTCAGTGGCTCACTTCCCTTTGATGGGCAAAACCTAAAGGAACTGAGAGAGAGAGTATTAAGAGGGAAATACAGAATTCCCTTCTACATGTCTACAGACTGTGAAAACCTTCTCAAACGTTTCCTGGTGCTAAATCCAATTAAACGCGGCACTCTAGAGCAAATCATGAAGGACAGGTGGATCAATGCAGGGCATGAAGAAGATGAACTCAAACCATTTGTTGAACCAGAGCTAGACATCTCAGACCAAAAAAGAATAGATATTATGGTGGGAATGGGATATTCACAAGAAGAAATTCAAGAATCTCTTAGTAAGATGAAATACGATGAAATCACAGCTACATATTTGTTATTGGGGAGAAAATCTTCAGAG</t>
+  </si>
+  <si>
+    <t>CACCAGCTGCAGCCCCGGCGGGTGTCATTCCGGGGCGAGGCCTCAGAGACTCTGCAGAGCCCTGGGTATGACCCAAGCCGGCCAGAGTCCTTCTTCCAGCAGAGCTTCCAGAGGCTCAGCCGCCTGGGCCATGGCTCCTACGGAGAGGTCTTCAAGGTGCGCTCCAAGGAGGACGGCCGGCTCTATGCGGTAAAGCGTTCCATGTCACCATTCCGGGGCCCCAAGGACCGGGCCCGCAAGTTGGCCGAGGTGGGCAGCCACGAGAAGGTGGGGCAGCACCCATGCTGCGTGCGGCTGGAGCAGGCCTGGGAGGAGGGCGGCATCCTGTACCTGCAGACGGAGCTGTGCGGGCCCAGCCTGCAGCAACACTGTGAGGCCTGGGGTGCCAGCCTGCCTGAGGCCCAGGTCTGGGGCTACCTGCGGGACACGCTGCTTGCCCTGGCCCATCTGCACAGCCAGGGCCTGGTGCACCTTGATGTCAAGCCTGCCAACATCTTCCTGGGGCCCCGGGGCCGCTGCAAGCTGGGTGACTTCGGACTGCTGGTGGAGCTGGGTACAGCAGGAGCTGGTGAGGTCCAGGAGGGAGACCCCCGCTACATGGCCCCCGAGCTGCTGCAGGGCTCCTATGGGACAGCAGCGGATGTGTTCAGTCTGGGCCTCACCATCCTGGAAGTGGCATGCAACATGGAGCTGCCCCACGGTGGGGAGGGCTGGCAGCAGCTGCGCCAGGGCTACCTGCCCCCTGAGTTCACTGCCGGTCTGTCTTCCGAGCTGCGTTCTGTCCTTGTCATGATGCTGGAGCCAGACCCCAAGCTGCGGGCCACGGCCGAGGCCCTGCTGGCACTGCCTGTGTTGAGGCAGCCG</t>
+  </si>
+  <si>
+    <t>KEKEPLESQYQVGPLLGSGGFGSVYSGIRVSDNLPVAIKHVEKDRISDWGELPNGTRVPMEVVLLKKVSSGFSGVIRLLDWFERPDSFVLILERPEPVQDLFDFITERGALQEELARSFFWQVLEAVRHCHNCGVLHRDIKDENILIDLNRGELKLIDFGSGALLKDTVYTDFDGTRVYSPPEWIRYHRYHGRSAAVWSLGILLYDMVCGDIPFEHDEEIIGGQVFFRQRVSSECQHLIRWCLALRPSDRPTFEEIQNHPWMQDVLLPQETAEIHLHSLSPGPSK</t>
+  </si>
+  <si>
+    <t>VEDHYEMGEELGSGQFAIVRKCRQKGTGKEYAAKFIKKRRLSSSRRGVSREEIEREVNILREIRHPNIITLHDIFENKTDVVLILELVSGGELFDFLAEKESLTEDEATQFLKQILDGVHYLHSKRIAHFDLKPENIMLLDKNVPNPRIKLIDFGIAHKIEAGNEFKNIFGTPEFVAPEIVNYEPLGLEADMWSIGVITYILLSGASPFLGETKQETLTNISAVNYDFDEEYFSNTSELAKDFIRRLLVKDPKRRMTIAQSLEHSWIKAIRRRNVRGEDSG</t>
+  </si>
+  <si>
+    <t>MET_HUMAN_D0_4EEV_A</t>
+  </si>
+  <si>
+    <t>MSSFLPEGGCYELLTVIGKGFEDLMTVNLARYKPTGEYVTVRRINLEACSNEMVTFLQGELHVSKLFNHPNIVPYRATFIADNELWVVTSFMAYGSAKDLICTHFMDGMNELAIAYILQGVLKALDYIHHMGYVHRSVKASHILISVDGKVYLSGLRSNLSMISHGQRQRVVHDFPKYSVKVLPWLSPEVLQQNLQGYDAKSDIYSVGITACELANGHVPFKDMPATQMLLEKLNGTVPCLLDTSTIPAEELTMSPSRSVANSGLSDSLTTSTPRPSNGDSPSHPYHRTFSPHFHHFVEQCLQRNPDARPSASTLLNHSFFKQIKRRASEVLPELLRPVTPITNFEGSQSQDHSGIFGLVTNLEELEVDDWEF</t>
+  </si>
+  <si>
+    <t>MP2K1_HUMAN_D0_3MBL_A</t>
+  </si>
+  <si>
+    <t>ATGTCGGGACCCGTGCCAAGCAGGGCCAGAGTTTACACAGATGTTAATACACACAGACCTCGAGAATACTGGGATTACGAGTCACATGTGGTGGAATGGGGAAATCAAGATGACTACCAGCTGGTTCGAAAATTAGGCCGAGGTAAATACAGTGAAGTATTTGAAGCCATCAACATCACAAATAATGAAAAAGTTGTTGTTAAAATTCTCAAGCCAGTAAAAAAGAAGAAAATTAAGCGTGAAATAAAGATTTTGGAGAATTTGAGAGGAGGTCCCAACATCATCACACTGGCAGACATTGTAAAAGACCCTGTGTCACGAACCCCCGCCTTGGTTTTTGAACACGTAAACAACACAGACTTCAAGCAATTGTACCAGACGTTAACAGACTATGATATTCGATTTTACATGTATGAGATTCTGAAGGCCCTGGATTATTGTCACAGCATGGGAATTATGCACAGAGATGTCAAGCCCCATAATGTCATGATTGATCATGAGCACAGAAAGCTACGACTAATAGACTGGGGTTTGGCTGAGTTTTATCATCCTGGCCAAGAATATAATGTCCGAGTTGCTTCCCGATACTTCAAAGGTCCTGAGCTACTTGTAGACTATCAGATGTACGATTATAGTTTGGATATGTGGAGTTTGGGTTGTATGCTGGCAAGTATGATCTTTCGGAAGGAGCCATTTTTCCATGGACATGACAATTATGATCAGTTGGTGAGGATAGCCAAGGTTCTGGGGACAGAAGATTTATATGACTATATTGACAAATACAACATTGAATTAGATCCACGTTTCAATGATATCTTGGGCAGACACTCTCGAAAGCGATGGGAACGCTTTGTCCACAGTGAAAATCAGCACCTTGTCAGCCCTGAGGCCTTGGATTTCCTGGACAAACTGCTGCGATATGACCACCAGTCACGGCTTACTGCAAGAGAGGCAATGGAGCACCCCTATTTCTACACTGTTGTGAAGGACCAGGCTCGAATGGGT</t>
+  </si>
+  <si>
+    <t>CDKL1_HUMAN_D0_4AGU_C</t>
+  </si>
+  <si>
+    <t>MARK3_HUMAN_D0_2QNJ_A</t>
+  </si>
+  <si>
+    <t>NLVFSDGYVVKETIGVGSYSECKRCVHKATNMEYAVKVIDKSKRDPSEEIEILLRYGQHPNIITLKDVYDDGKHVYLVTELMRGGELLDKILRQKFFSEREASFVLHTIGKTVEYLHSQGVVHRDLKPSNILYVDESGNPECLRICDFGFAKQLRAENGLLMTPCYTANFVAPEVLKRQGYDEGCDIWSLGILLYTMLAGYTPFANGPSDTPEEILTRIGSGKFTLSGGNWNTVSETAKDLVSKMLHVDPHQRLTAKQVLQHPWVTQKDKLPQSQLSHQDLQLVKGAMAATYSALNSSKPTPQLKPIESSILAQRRVRKLPSTTL</t>
+  </si>
+  <si>
+    <t>GGTGTTGTGACACATGAGCAGTTCAAGGCTGCGCTCAGGATGGTGGTGGACCAGGGTGACCCCCGGCTGCTGCTGGACAGCTACGTGAAGATTGGCGAGGGCTCCACCGGCATCGTCTGCTTGGCCCGGGAGAAGCACTCGGGCCGCCAGGTGGCCGTCAAGATGATGGACCTCAGGAAGCAGCAGCGCAGGGAGCTGCTCTTCAACGAGGTGGTGATCATGCGGGACTACCAGCACTTCAACGTGGTGGAGATGTACAAGAGCTACCTGGTGGGCGAGGAGCTGTGGGTGCTCATGGAGTTCCTGCAGGGAGGAGCCCTCACAGACATCGTCTCCCAAGTCAGGCTGAATGAGGAGCAGATTGCCACTGTGTGTGAGGCTGTGCTGCAGGCCCTGGCCTACCTGCATGCTCAGGGTGTCATCCACCGGGACATCAAGAGTGACTCCATCCTGCTGACCCTCGATGGCAGGGTGAAGCTCTCGGACTTCGGATTCTGTGCTCAGATCAGCAAAGACGTCCCTAAGAGGAAGTCCCTGGTGGGAACCCCCTACTGGATGGCTCCTGAAGTGATCTCCAGGTCTTTGTATGCCACTGAGGTGGATATCTGGTCTCTGGGCATCATGGTGATTGAGATGGTAGATGGGGAGCCACCGTACTTCAGTGACTCCCCAGTGCAAGCCATGAAGAGGCTCCGGGACAGCCCCCCACCCAAGCTGAAAAACTCTCACAAGGTCTCCCCAGTGCTGCGAGACTTCCTGGAGCGGATGCTGGTGCGGGACCCCCAAGAGAGAGCCACAGCCCAGGAGCTCCTAGACCACCCCTTCCTGCTGCAGACAGGGCTACCTGAGTGCCTGGTGCCCCTGATCCAGCTCTACCGAAAGCAGACCTCCACCTGC</t>
+  </si>
+  <si>
+    <t>CACATTGGAAACTACCGGCTCCTCAAGACCATTGGCAAGGGTAATTTTGCCAAGGTGAAGTTGGCCCGACACATCCTGACTGGGAAAGAGGTAGCTGTGAAGATCATTGACAAGACTCAACTGAACTCCTCCAGCCTCCAGAAACTATTCCGCGAAGTAAGAATAATGAAGGTTTTGAATCATCCCAACATAGTTAAATTATTTGAAGTGATTGAGACTGAGAAAACGCTCTACCTTGTCATGGAGTACGCTAGTGGCGGAGAGGTATTTGATTACCTAGTGGCTCATGGCAGGATGAAAGAAAAAGAGGCTCGAGCCAAATTCCGCCAGATAGTGTCTGCTGTGCAGTACTGTCACCAGAAGTTTATTGTCCATAGAGACTTAAAGGCAGAAAACCTGCTCTTGGATGCTGATATGAACATCAAGATTGCAGACTTTGGCTTCAGCAATGAATTCACCTTTGGGAACAAGCTGGACACCTTCTGTGGCAGTCCCCCTTATGCTGCCCCAGAACTCTTCCAGGGCAAAAAATATGATGGACCCGAGGTGGATGTGTGGAGCCTAGGAGTTATCCTCTATACACTGGTCAGCGGATCCCTGCCTTTTGATGGACAGAACCTCAAGGAGCTGCGGGAACGGGTACTGAGGGGAAAATACCGTATTCCATTCTACATGTCCACGGACTGTGAAAACCTGCTTAAGAAATTTCTCATTCTTAATCCCAGCAAGAGAGGCACTTTAGAGCAAATCATGAAAGATCGATGGATGAATGTGGGTCACGAAGATGATGAACTAAAGCCTTACGTGGAGCCACTCCCTGACTACAAGGACCCCCGGCGGACAGAGCTGATGGTGTCCATGGGTTATACACGGGAAGAGATCCAGGACTCGCTGGTGGGCCAGAGATACAACGAGGTGATGGCCACCTATCTGCTCCTGGGCTAC</t>
+  </si>
+  <si>
+    <t>ST17B_HUMAN_D0_3LM0_A</t>
+  </si>
+  <si>
+    <t>GDSDISSPLLQNTVHIDLSALNPELVQAVQHVVIGPSSLIVHFNEVIGRGHFGCVYHGTLLDNDGKKIHCAVKSLNRITDIGEVSQFLTEGIIMKDFSHPNVLSLLGICLRSEGSPLVVLPYMKHGDLRNFIRNETHNPTVKDLIGFGLQVAKGMKYLASKKFVHRDLAARNCMLDEKFTVKVADFGLARDMYDKEYYSVHNKTGAKLPVKWMALESLQTQKFTTKSDVWSFGVLLWELMTRGAPPYPDVNTFDITVYLLQGRRLLQPEYCPDPLYEVMLKCWHPKAEMRPSFSELVSRISAIFSTFIG</t>
+  </si>
+  <si>
+    <t>ATGAGTAGCTTTCTGCCAGAGGGAGGGTGTTACGAGCTGCTCACTGTGATAGGCAAAGGATTTGAGGACCTGATGACTGTGAATCTAGCAAGGTACAAACCAACAGGAGAGTACGTGACTGTACGGAGGATTAACCTAGAAGCTTGTTCCAATGAGATGGTAACATTCTTGCAGGGCGAGCTGCATGTCTCCAAACTCTTCAACCATCCCAATATCGTGCCATATCGAGCCACTTTTATTGCAGACAATGAGCTGTGGGTTGTCACATCATTCATGGCATACGGTTCTGCAAAAGATCTCATCTGTACACACTTCATGGATGGCATGAATGAGCTGGCGATTGCTTACATCCTGCAGGGGGTGCTGAAGGCCCTCGACTACATCCACCACATGGGATATGTACACAGGAGTGTCAAAGCCAGCCACATCCTGATCTCTGTGGATGGGAAGGTCTACCTGTCTGGTTTGCGCAGCAACCTCAGCATGATAAGCCATGGGCAGCGGCAGCGAGTGGTCCACGATTTTCCCAAGTACAGTGTCAAGGTTCTGCCGTGGCTCAGCCCCGAGGTCCTCCAGCAGAATCTCCAGGGTTATGATGCCAAGTCTGACATCTACAGTGTGGGAATCACAGCCTGTGAACTGGCCAACGGCCATGTCCCCTTTAAGGATATGCCTGCCACCCAGATGCTGCTAGAGAAACTGAACGGCACAGTGCCCTGCCTGTTGGATACCAGCACCATCCCCGCTGAGGAGCTGACCATGAGCCCTTCGCGCTCAGTGGCCAACTCTGGCCTGAGTGACAGCCTGACCACCAGCACCCCCCGGCCCTCCAACGGTGACTCGCCCTCCCACCCCTACCACCGAACCTTCTCCCCCCACTTCCACCACTTTGTGGAGCAGTGCCTTCAGCGCAACCCGGATGCCAGGCCCAGTGCCAGCACCCTCCTGAACCACTCTTTCTTCAAGCAGATCAAGCGACGTGCCTCAGAGGTTTTGCCCGAATTGCTTCGTCCTGTCACCCCCATCACCAATTTTGAGGGCAGCCAGTCTCAGGACCACAGTGGAATCTTTGGCCTGGTAACAAACCTGGAAGAGCTGGAGGTGGACGATTGGGAGTTC</t>
+  </si>
+  <si>
+    <t>ADPEELFTKLERIGKGSFGEVFKGIDNRTQQVVAIKIIDLEEAEDEIEDIQQEITVLSQCDSSYVTKYYGSYLKGSKLWIIMEYLGGGSALDLLRAGPFDEFQIATMLKEILKGLDYLHSEKKIHRDIKAANVLLSEQGDVKLADFGVAGQLTDTQIKRNTFVGTPFWMAPEVIQQSAYDSKADIWSLGITAIELAKGEPPNSDMHPMRVLFLIPKNNPPTLVGDFTKSFKEFIDACLNKDPSFRPTAKELLKHKFIVKNSKKTSYLTELIDRFKRWKAE</t>
+  </si>
+  <si>
+    <t>AURKA_HUMAN_D0_2NP8_A</t>
+  </si>
+  <si>
+    <t>HIGNYRLLKTIGKGNFAKVKLARHILTGKEVAVKIIDKTQLNSSSLQKLFREVRIMKVLNHPNIVKLFEVIETEKTLYLVMEYASGGEVFDYLVAHGRMKEKEARAKFRQIVSAVQYCHQKFIVHRDLKAENLLLDADMNIKIADFGFSNEFTFGNKLDTFCGSPPYAAPELFQGKKYDGPEVDVWSLGVILYTLVSGSLPFDGQNLKELRERVLRGKYRIPFYMSTDCENLLKKFLILNPSKRGTLEQIMKDRWMNVGHEDDELKPYVEPLPDYKDPRRTELMVSMGYTREEIQDSLVGQRYNEVMATYLLLGY</t>
+  </si>
+  <si>
+    <t>GVVTHEQFKAALRMVVDQGDPRLLLDSYVKIGEGSTGIVCLAREKHSGRQVAVKMMDLRKQQRRELLFNEVVIMRDYQHFNVVEMYKSYLVGEELWVLMEFLQGGALTDIVSQVRLNEEQIATVCEAVLQALAYLHAQGVIHRDIKSDSILLTLDGRVKLSDFGFCAQISKDVPKRKSLVGTPYWMAPEVISRSLYATEVDIWSLGIMVIEMVDGEPPYFSDSPVQAMKRLRDSPPPKLKNSHKVSPVLRDFLERMLVRDPQERATAQELLDHPFLLQTGLPECLVPLIQLYRKQTSTC</t>
+  </si>
+  <si>
+    <t>ATGGCAAAGCAGTACGACTCGGTGGAGTGCCCTTTTTGTGATGAAGTTTCCAAATACGAGAAGCTCGCCAAGATCGGCCAAGGCACCTTCGGGGAGGTGTTCAAGGCCAGGCACCGCAAGACCGGCCAGAAGGTGGCTCTGAAGAAGGTGCTGATGGAAAACGAGAAGGAGGGGTTCCCCATTACAGCCTTGCGGGAGATCAAGATCCTTCAGCTTCTAAAACACGAGAATGTGGTCAACTTGATTGAGATTTGTCGAACCAAAGCTTCCCCCTATAACCGCTGCAAGGGTAGTATATACCTGGTGTTCGACTTCTGCGAGCATGACCTTGCTGGGCTGTTGAGCAATGTTTTGGTCAAGTTCACGCTGTCTGAGATCAAGAGGGTGATGCAGATGCTGCTTAACGGCCTCTACTACATCCACAGAAACAAGATCCTGCATAGGGACATGAAGGCTGCTAATGTGCTTATCACTCGTGATGGGGTCCCGAAGCTGGCAGACTTTGGGCTGGCCCGGGCCTTCAGCCTGGCCAAGAACAGCCAGCCCAACCGCTACACCAACCGTGTGGTGACACTCTGGTACCGGCCCCCGGAGCTGTTGCTCGGGGAGCGGGACTACGGCCCCCCCATTGACCTGTGGGGTGCTGGGTGCATCATGGCAGAGATGTGGACCCGCAGCCCCATCATGCAGGGCAACACGGAGCAGCACCAACTCGCCCTCATCAGTCAGCTCTGCGGCTCCATCACCCCTGAGGTGTGGCCAAACGTGGACAACTATGAGCTGTACGAAAAGCTGGAGCTGGTCAAGGGCCAGAAGCGGAAGGTGAAGGACAGGCTGAAGGCCTATGTGCGTGACCCATACGCACTGGACCTCATCGACAAGCTGCTGGTGCTGGACCCTGCCCAGCGCATCGACAGCGATGACGCCCTCAACCACGACTTCTTCTGGTCCGACCCCATGCCCTCCGACCTCAAGGGCATGCTCTCCACC</t>
+  </si>
+  <si>
+    <t>MSQERPTFYRQELNKTIWEVPERYQNLSPVGSGAYGSVCAAFDTKTGLRVAVKKLSRPFQSIIHAKRTYRELRLLKHMKHENVIGLLDVFTPARSLEEFNDVYLVTHLMGADLNNIVKCQKLTDDHVQFLIYQILRGLKYIHSADIIHRDLKPSNLAVNEDCELKILDFGLARHTDDEMTGYVATRWYRAPEIMLNWMHYNQTVDIWSVGCIMAELLTGRTLFPGTDHIDQLKLILRLVGTPGAELLKKISSESARNYIQSLTQMPKMNFANVFIGANPLAVDLLEKMLVLDSDKRITAAQALAHAYFAQYHDPDDEPVADPYDQSFESRDLLIDEWKSLTYDEVISFVPPPLDQEEMES</t>
+  </si>
+  <si>
+    <t>MELRVGNRYRLGRKIGSGSFGDIYLGTDIAAGEEVAIKLECVKTKHPQLHIESKIYKMMQGGVGIPTIRWCGAEGDYNVMVMELLGPSLEDLFNFCSRKFSLKTVLLLADQMISRIEYIHSKNFIHRDVKPDNFLMGLGKKGNLVYIIDFGLAKKYRDARTHQHIPYRENKNLTGTARYASINTHLGIEQSRRDDLESLGYVLMYFNLGSLPWQGLKAATKRQKYERISEKKMSTPIEVLCKGYPSEFATYLNFCRSLRFDDKPDYSYLRQLFRNLFHRQGFSYDYVFDWNMLK</t>
+  </si>
+  <si>
+    <t>MAKQYDSVECPFCDEVSKYEKLAKIGQGTFGEVFKARHRKTGQKVALKKVLMENEKEGFPITALREIKILQLLKHENVVNLIEICRTKASPYNRCKGSIYLVFDFCEHDLAGLLSNVLVKFTLSEIKRVMQMLLNGLYYIHRNKILHRDMKAANVLITRDGVPKLADFGLARAFSLAKNSQPNRYTNRVVTLWYRPPELLLGERDYGPPIDLWGAGCIMAEMWTRSPIMQGNTEQHQLALISQLCGSITPEVWPNVDNYELYEKLELVKGQKRKVKDRLKAYVRDPYALDLIDKLLVLDPAQRIDSDDALNHDFFWSDPMPSDLKGMLST</t>
+  </si>
+  <si>
     <t>targetID</t>
   </si>
   <si>
-    <t>SPQREPQRVSHEQFRAALQLVVDPGDPRSYLDNFIKIGEGSTGIVCIATVRSSGKLVAVKKMDLRKQQRRELLFNEVVIMRDYQHENVVEMYNSYLVGDELWVVMEFLEGGALTDIVTHTRMNEEQIAAVCLAVLQALSVLHAQGVIHRDIKSDSILLTHDGRVKLSDFGFCAQVSKEVPRRKSLVGTPYWMAPELISRLPYGPEVDIWSLGIMVIEMVDGEPPYFNEPPLKAMKMIRDNLPPRLKNLHKVSPSLKGFLDRLLVRDPAQRATAAELLKHPFLAKAGPPASIVPLMRQNRTR</t>
-  </si>
-  <si>
-    <t>ELKDDDFEKISELGAGNGGVVFKVSHKPSGLVMARKLIHLEIKPAIRNQIIRELQVLHECNSPYIVGFYGAFYSDGEISICMEHMDGGSLDQVLKKAGRIPEQILGKVSIAVIKGLTYLREKHKIMHRAYGMDSRPPMAIFELLDYIVNEPPPKLPSGVFSLEFQDFVNKCLIKNPAERADLKQLMVHAFIKRSDAEEVDFAGWLCSTIGLN</t>
-  </si>
-  <si>
-    <t>PMYT1_HUMAN_D0_3P1A_A</t>
-  </si>
-  <si>
-    <t>GPEDELPDWAAAKEFYQKYDPKDVIGRGVSSVVRRCVHRATGHEFAVKIMEVTAERLSPEQLEEVREATRRETHILRQVAGHPHIITLIDSYESSSFMFLVFDLMRKGELFDYLTEKVALSEKETRSIMRSLLEAVSFLHANNIVHRDLKPENILLDDNMQIRLSDFGFSCHLEPGEKLRELCGTPGYLAPEILKCSMDETHPGYGKEVDLWACGVILFTLLAGSPPFWHRRQILMLRMIMEGQYQFSSPEWDDRSSTVKDLISRLLQVDPEARLTAEQALQHPFFER</t>
-  </si>
-  <si>
-    <t>QKVMENSSGTPDILTRHFTIDDFEIGRPLGKGKFGNVYLAREKKSHFIVALKVLFKSQIEKEGVEHQLRREIEIQAHLHHPNILRLYNYFYDRRRIYLILEYAPRGELYKELQKSCTFDEQRTATIMEELADALMYCHGKKVIHRDIKPENLLLGLKGELKIADFGWSVHAPSLRRKTMCGTLDYLPPEMIEGRMHNEKVDLWCIGVLCYELLVGNPPFESASHNETYRRIVKVDLKFPASVPTGAQDLISKLLRHNPSERLPLAQVSAHPWVRANSRRVLPPSALQSVA</t>
-  </si>
-  <si>
-    <t>GTGGAGGACCATTATGAGATGGGGGAGGAGCTGGGCAGCGGCCAGTTTGCGATCGTGCGGAAGTGCCGGCAGAAGGGCACGGGCAAGGAGTACGCAGCCAAGTTCATCAAGAAGCGCCGCCTGTCATCCAGCCGGCGTGGGGTGAGCCGGGAGGAGATCGAGCGGGAGGTGAACATCCTGCGGGAGATCCGGCACCCCAACATCATCACCCTGCACGACATCTTCGAGAACAAGACGGACGTGGTCCTCATCCTGGAGCTGGTCTCTGGCGGGGAGCTCTTTGACTTCCTGGCGGAGAAGGAGTCGCTGACGGAGGACGAGGCCACCCAGTTCCTCAAGCAGATCCTGGACGGCGTTCACTACCTGCACTCTAAGCGCATCGCACACTTTGACCTGAAGCCGGAAAACATCATGCTGCTGGACAAGAACGTGCCCAACCCACGAATCAAGCTCATCGACTTCGGCATCGCGCACAAGATCGAGGCGGGGAACGAGTTCAAGAACATCTTCGGCACCCCGGAGTTTGTGGCCCCAGAGATTGTGAACTATGAGCCGCTGGGCCTGGAGGCGGACATGTGGAGCATCGGTGTCATCACCTATATCCTCCTGAGCGGTGCATCCCCGTTCCTGGGCGAGACCAAGCAGGAGACGCTCACCAACATCTCAGCCGTGAACTACGACTTCGACGAGGAGTACTTCAGCAACACCAGCGAGCTGGCCAAGGACTTCATTCGCCGGCTGCTCGTCAAAGATCCCAAGCGGAGAATGACCATTGCCCAGAGCCTGGAACATTCCTGGATTAAGGCGATCCGGCGGCGGAACGTGCGTGGTGAGGACAGCGGC</t>
-  </si>
-  <si>
-    <t>CTGGAGTATGACTATGAATATGATGAAAATGGTGACAGAGTCGTTTTAGGAAAAGGCACTTATGGGATAGTCTACGCAGGTCGGGACTTGAGCAACCAAGTCAGAATTGCTATTAAGGAAATCCCAGAGAGAGACAGCAGATACTCTCAGCCCCTGCATGAAGAAATAGCATTGCATAAACACCTGAAGCACAAAAATATTGTCCAGTATCTGGGCTCTTTCAGTGAGAATGGTTTCATTAAAATCTTCATGGAGCAGGTCCCTGGAGGAAGTCTTTCTGCTCTCCTTCGTTCCAAATGGGGTCCATTAAAAGACAATGAGCAAACAATTGGCTTTTATACAAAGCAAATACTGGAAGGATTAAAATATCTCCATGACAATCAGATAGTTCACCGGGACATAAAGGGTGACAATGTGTTGATTAATACCTACAGTGGTGTTCTCAAGATCTCTGACTTCGGAACATCAAAGAGGCTTGCTGGCATAAACCCCTGTACTGAAACTTTTACTGGTACCCTCCAGTATATGGCACCAGAAATAATAGATAAAGGACCAAGAGGCTACGGAAAAGCAGCAGACATCTGGTCTCTGGGCTGTACAATCATTGAAATGGCCACAGGAAAACCCCCATTTTATGAACTGGGAGAACCACAAGCAGCTATGTTCAAGGTGGGAATGTTTAAAGTCCACCCTGAGATCCCAGAGTCCATGTCTGCAGAGGCCAAGGCATTCATACTGAAATGTTTTGAACCAGATCCTGACAAGAGAGCCTGTGCTAACGACTTGCTTGTTGATGAGTTTTTAAAA</t>
-  </si>
-  <si>
-    <t>BMR1B_HUMAN_D0_3MDY_C</t>
-  </si>
-  <si>
-    <t>MSGPRAGFYRQELNKTVWEVPQRLQGLRPVGSGAYGSVCSAYDARLRQKVAVKKLSRPFQSLIHARRTYRELRLLKHLKHENVIGLLDVFTPATSIEDFSEVYLVTTLMGADLNNIVKCQALSDEHVQFLVYQLLRGLKYIHSAGIIHRDLKPSNVAVNEDCELRILDFGLARQADEEMTGYVATRWYRAPEIMLNWMHYNQTVDIWSVGCIMAELLQGKALFPGSDYIDQLKRIMEVVGTPSPEVLAKISSEHARTYIQSLPPMPQKDLSSIFRGANPLAIDLLGRMLVLDSDQRVSAAEALAHAYFSQYHDPEDEPEAEPYDESVEAKERTLEEWKELTYQEVLSFKPPEPPKPPGSLEIEQ</t>
-  </si>
-  <si>
-    <t>CSKP_HUMAN_D0_3TAC_A</t>
-  </si>
-  <si>
-    <t>EGFR_HUMAN_D0_2RF9_A</t>
-  </si>
-  <si>
-    <t>MARK2_HUMAN_D0_3IEC_D</t>
-  </si>
-  <si>
-    <t>MK10_HUMAN_D0_2B1P_A</t>
-  </si>
-  <si>
-    <t>CCATTTCCAGAAGGCAAGGTTCTGGATGATATGGAAGGCAATCAGTGGGTACTGGGCAAGAAGATTGGCTCTGGAGGATTTGGATTGATATATTTAGCTTTCCCCACAAATAAACCAGAGAAAGATGCAAGACATGTAGTAAAAGTGGAATATCAAGAAAATGGCCCGTTATTTTCAGAACTTAAATTTTATCAGAGAGTTGCAAAAAAAGACTGTATCAAAAAGTGGATAGAACGCAAACAACTTGATTATTTAGGAATTCCTCTGTTTTATGGATCTGGTCTGACTGAATTCAAGGGAAGAAGTTACAGATTTATGGTAATGGAAAGACTAGGAATAGATTTACAGAAGATCTCAGGCCAGAATGGTACCTTTAAAAAGTCAACTGTCCTGCAATTAGGTATCCGAATGTTGGATGTACTGGAATATATACATGAAAATGAATATGTTCATGGTGATATAAAAGCAGCAAATCTACTTTTGGGTTACAAAAATCCAGACCAGGTTTATCTTGCAGATTATGGACTTTCCTACAGATATTGTCCCAATGGGAACCACAAACAGTATCAGGAAAATCCTAGAAAAGGCCATAATGGGACAATAGAGTTTACCAGCTTGGATGCCCACAAGGGAGTAGCCTTGTCCAGACGAAGTGACGTTGAGATCCTCGGCTACTGCATGCTGCGGTGGTTGTGTGGGAAACTTCCCTGGGAACAGAACCTGAAGGACCCTGTGGCTGTGCAGACTGCTAAAACAAATCTGTTGGACGAGCTCCCCCAGTCAGTGCTTAAATGGGCTCCTTCTGGAAGCAGTTGCTGTGAAATAGCCCAATTTTTGGTATGTGCTCATAGTTTAGCATATGATGAAAAGCCAAACTATCAAGCCCTCAAGAAAATTTTGAACCCTCATGGAATACCTTTAGGACCACTGGACTTTTCCACAAAAGGACAGAGTATAAATGTCCAT</t>
-  </si>
-  <si>
-    <t>GGGGACTCTGATATATCCAGTCCATTACTGCAAAATACTGTCCACATTGACCTCAGTGCTCTAAATCCAGAGCTGGTCCAGGCAGTGCAGCATGTAGTGATTGGGCCCAGTAGCCTGATTGTGCATTTCAATGAAGTCATAGGAAGAGGGCATTTTGGTTGTGTATATCATGGGACTTTGTTGGACAATGATGGCAAGAAAATTCACTGTGCTGTGAAATCCTTGAACAGAATCACTGACATAGGAGAAGTTTCCCAATTTCTGACCGAGGGAATCATCATGAAAGATTTTAGTCATCCCAATGTCCTCTCGCTCCTGGGAATCTGCCTGCGAAGTGAAGGGTCTCCGCTGGTGGTCCTACCATACATGAAACATGGAGATCTTCGAAATTTCATTCGAAATGAGACTCATAATCCAACTGTAAAAGATCTTATTGGCTTTGGTCTTCAAGTAGCCAAAGGCATGAAATATCTTGCAAGCAAAAAGTTTGTCCACAGAGACTTGGCTGCAAGAAACTGTATGCTGGATGAAAAATTCACAGTCAAGGTTGCTGATTTTGGTCTTGCCAGAGACATGTATGATAAAGAATACTATAGTGTACACAACAAAACAGGTGCAAAGCTGCCAGTGAAGTGGATGGCTTTGGAAAGTCTGCAAACTCAAAAGTTTACCACCAAGTCAGATGTGTGGTCCTTTGGCGTGCTCCTCTGGGAGCTGATGACAAGAGGAGCCCCACCTTATCCTGACGTAAACACCTTTGATATAACTGTTTACTTGTTGCAAGGGAGAAGACTCCTACAACCCGAATACTGCCCAGACCCCTTATATGAAGTAATGCTAAAATGCTGGCACCCTAAAGCCGAAATGCGCCCATCCTTTTCTGAACTGGTGTCCCGGATATCAGCGATCTTCTCTACTTTCATTGGG</t>
-  </si>
-  <si>
-    <t>OXSR1_HUMAN_D0_3DAK_B</t>
-  </si>
-  <si>
-    <t>YQLFEELGKGAFSVVRRCVKVLAGQEYAAKIINTKKLSARDHQKLEREARICRLLKHPNIVRLHDSISEEGHHYLIFDLVTGGELFEDIVAREYYSEADASHCIQQILEAVLHCHQMGVVHRDLKPENLLLASKLKGAAVKLADFGLAIEVEGEQQAWFGFAGTPGYLSPEVLRKDPYGKPVDLWACGVILYILLVGYPPFWDEDQHRLYLQIKAGAYDFPSPEWDTVTPEAKDLINKMLTINPSKRITAAEALKHPWISHRSTVASCMHRQETVDCLKKFNARRKLKGA</t>
-  </si>
-  <si>
-    <t>ENFQKVEKIGEGTYGVVYKARNKLTGEVVALKKIRLDTETEGVPSTAIREISLLKELNHPNIVKLLDVIHTENKLYLVFEFLHQDLKKFMDASALTGIPLPLIKSYLFQLLQGLAFCHSHRVLHRDLKPQNLLINTEGAIKLADFGLARAFGVPVRTYTHEVVTLWYRAPEILLGCKYYSTAVDIWSLGCIFAEMVTRRALFPGDSEIDQLFRIFRTLGTPDEVVWPGVTSMPDYKPSFPKWARQDFSKVVPPLDEDGRSLLSQMLHYDPNKRISAKAALAHPFFQDVTKPVPHL</t>
-  </si>
-  <si>
-    <t>TTK_HUMAN_D0_3H9F_A</t>
-  </si>
-  <si>
-    <t>MK03_HUMAN_D0_2ZOQ_B</t>
-  </si>
-  <si>
-    <t>ATGTCTCAGGAGAGGCCCACGTTCTACCGGCAGGAGCTGAACAAGACAATCTGGGAGGTGCCCGAGCGTTACCAGAACCTGTCTCCAGTGGGCTCTGGCGCCTATGGCTCTGTGTGTGCTGCTTTTGACACAAAAACGGGGTTACGTGTGGCAGTGAAGAAGCTCTCCAGACCATTTCAGTCCATCATTCATGCGAAAAGAACCTACAGAGAACTGCGGTTACTTAAACATATGAAACATGAAAATGTGATTGGTCTGTTGGACGTTTTTACACCTGCAAGGTCTCTGGAGGAATTCAATGATGTGTATCTGGTGACCCATCTCATGGGGGCAGATCTGAACAACATTGTGAAATGTCAGAAGCTTACAGATGACCATGTTCAGTTCCTTATCTACCAAATTCTCCGAGGTCTAAAGTATATACATTCAGCTGACATAATTCACAGGGACCTAAAACCTAGTAATCTAGCTGTGAATGAAGACTGTGAGCTGAAGATTCTGGATTTTGGACTGGCTCGGCACACAGATGATGAAATGACAGGCTACGTGGCCACTAGGTGGTACAGGGCTCCTGAGATCATGCTGAACTGGATGCATTACAACCAGACAGTTGATATTTGGTCAGTGGGATGCATAATGGCCGAGCTGTTGACTGGAAGAACATTGTTTCCTGGTACAGACCATATTGATCAGTTGAAGCTCATTTTAAGACTCGTTGGAACCCCAGGGGCTGAGCTTTTGAAGAAAATCTCCTCAGAGTCTGCAAGAAACTATATTCAGTCTTTGACTCAGATGCCGAAGATGAACTTTGCGAATGTATTTATTGGTGCCAATCCCCTGGCTGTCGACTTGCTGGAGAAGATGCTTGTATTGGACTCAGATAAGAGAATTACAGCGGCCCAAGCCCTTGCACATGCCTACTTTGCTCAGTACCACGATCCTGATGATGAACCAGTGGCCGATCCTTATGATCAGTCCTTTGAAAGCAGGGACCTCCTTATAGATGAGTGGAAAAGCCTGACCTATGATGAAGTCATCAGCTTTGTGCCACCACCCCTTGACCAAGAAGAGATGGAGTCC</t>
-  </si>
-  <si>
-    <t>TCCCCCAACTACGACAAGTGGGAGATGGAACGCACGGACATCACCATGAAGCACAAGCTGGGCGGGGGCCAGTACGGGGAGGTGTACGAGGGCGTGTGGAAGAAATACAGCCTGACGGTGGCCGTGAAGACCTTGAAGGAGGACACCATGGAGGTGGAAGAGTTCTTGAAAGAAGCTGCAGTCATGAAAGAGATCAAACACCCTAACCTGGTGCAGCTCCTTGGGGTCTGCACCCGGGAGCCCCCGTTCTATATCATCACTGAGTTCATGACCTACGGGAACCTCCTGGACTACCTGAGGGAGTGCAACCGGCAGGAGGTGAACGCCGTGGTGCTGCTGTACATGGCCACTCAGATCTCGTCAGCCATGGAGTACCTGGAGAAGAAAAACTTCATCCACAGAGATCTTGCTGCCCGAAACTGCCTGGTAGGGGAGAACCACTTGGTGAAGGTAGCTGATTTTGGCCTGAGCAGGTTGATGACAGGGGACACCTACACAGCCCATGCTGGAGCCAAGTTCCCCATCAAATGGACTGCACCCGAGAGCCTGGCCTACAACAAGTTCTCCATCAAGTCCGACGTCTGGGCATTTGGAGTATTGCTTTGGGAAATTGCTACCTATGGCATGTCCCCTTACCCGGGAATTGACCTGTCCCAGGTGTATGAGCTGCTAGAGAAGGACTACCGCATGGAGCGCCCAGAAGGCTGCCCAGAGAAGGTCTATGAACTCATGCGAGCATGTTGGCAGTGGAATCCCTCTGACCGGCCCTCCTTTGCTGAAATCCACCAAGCCTTTGAAACAATGTTCCAGGAATCCAGTATCTCAGACGAAGTGGAAAAGGAGCTGGGGAAA</t>
-  </si>
-  <si>
-    <t>MK01_HUMAN_D0_4FMQ_A</t>
-  </si>
-  <si>
-    <t>ATGTCTCAGTCGAAAGGCAAGAAGCGAAACCCTGGCCTTAAAATTCCAAAAGAAGCATTTGAACAACCTCAGACCAGTTCCACACCACCTCGAGATTTAGACTCCAAGGCTTGCATTTCTATTGGAAATCAGAACTTTGAGGTGAAGGCAGATGACCTGGAGCCTATAATGGAACTGGGACGAGGTGCGTACGGGGTGGTGGAGAAGATGCGGCACGTGCCCAGCGGGCAGATCATGGCAGTGAAGCGGATCCGAGCCACAGTAAATAGCCAGGAACAGAAACGGCTACTGATGGATTTGGATATTTCCATGAGGACGGTGGACTGTCCATTCACTGTCACCTTTTATGGCGCACTGTTTCGGGAGGGTGATGTGTGGATCTGCATGGAGCTCATGGATACATCACTAGATAAATTCTACAAACAAGTTATTGATAAAGGCCAGACAATTCCAGAGGACATCTTAGGGAAAATAGCAGTTTCTATTGTAAAAGCATTAGAACATTTACATAGTAAGCTGTCTGTCATTCACAGAGACGTCAAGCCTTCTAATGTACTCATCAATGCTCTCGGTCAAGTGAAGATGTGCGATTTTGGAATCAGTGGCTACTTGGTGGACTCTGTTGCTAAAACAATTGATGCAGGTTGCAAACCATACATGGCCCCTGAAAGAATAAACCCAGAGCTCAACCAGAAGGGATACAGTGTGAAGTCTGACATTTGGAGTCTGGGCATCACGATGATTGAGTTGGCCATCCTTCGATTTCCCTATGATTCATGGGGAACTCCATTTCAGCAGCTCAAACAGGTGGTAGAGGAGCCATCGCCACAACTCCCAGCAGACAAGTTCTCTGCAGAGTTTGTTGACTTTACCTCACAGTGCTTAAAGAAGAATTCCAAAGAACGGCCTACATACCCAGAGCTAATGCAACATCCATTTTTCACCCTACATGAATCCAAAGGAACAGATGTGGCATCTTTTGTAAAACTGATTCTTGGAGAC</t>
-  </si>
-  <si>
-    <t>AACAAACACTCTGGCATTGACTTCAAACAGCTTAACTTCCTGACGAAGCTCAACGAGAATCACTCTGGAGAGCTATGGAAGGGCCGCTGGCAGGGCAATGACATTGTCGTGAAGGTGCTGAAGGTTCGAGACTGGAGTACAAGGAAGAGCAGGGACTTCAATGAAGAGTGTCCCCGGCTCAGGATTTTCTCGCATCCAAATGTGCTCCCAGTGCTAGGTGCCTGCCAGTCTCCACCTGCTCCTCATCCTACTCTCATCACACACTGGATGCCATATGGATCCCTCTACAATGTACTACATGAAGGCACCAATTTCGTCGTGGACCAGAGCCAGGCTGTGAAGTTTGCTTTGGACATGGCAAGGGGCATGGCCTTCCTACACACACTAGAGCCCCTCATCCCACGACATGCACTCAATAGCCGTAGTGTAATGATTGATGAGGACATGACTGCCCGAATTAGCATGGCTGATGTCAAGTTCTCTTTCCAATGTCCTGGTCGCATGTATGCACCTGCCTGGGTAGCCCCCGAAGCTCTGCAGAAGAAGCCTGAAGACACAAACAGACGCTCAGCAGACATGTGGAGTTTTGCAGTGCTTCTGTGGGAACTGGTGACACGGGAGGTACCCTTTGCTGACCTCTCCAATATGGAGATTGGAATGAAGGTGGCATTGGAAGGCCTTCGGCCTACCATCCCACCAGGTATTTCCCCTCATGTGTGTAAGCTCATGAAGATCTGCATGAATGAAGACCCTGCAAAGCGACCCAAATTTGACATGATTGTGCCTATCCTTGAGAAGATGCAGGACAAG</t>
-  </si>
-  <si>
-    <t>KS6A1_HUMAN_D1_3RNY_B</t>
-  </si>
-  <si>
-    <t>ACCGACAGCTTCTCGGGCAGGTTTGAAGACGTCTACCAGCTGCAGGAAGATGTGCTGGGGGAGGGCGCTCATGCCCGAGTGCAGACCTGCATCAACCTGATCACCAGCCAGGAGTACGCCGTCAAGATCATTGAGAAGCAGCCAGGCCACATTCGGAGCAGGGTTTTCAGGGAGGTGGAGATGCTGTACCAGTGCCAGGGACACAGGAACGTCCTAGAGCTGATTGAGTTCTTCGAGGAGGAGGACCGCTTCTACCTGGTGTTTGAGAAGATGCGGGGAGGCTCCATCCTGAGCCACATCCACAAGCGCCGGCACTTCAACGAGCTGGAGGCCAGCGTGGTGGTGCAGGACGTGGCCAGCGCCTTGGACTTTCTGCATAACAAAGGCATCGCCCACAGGGACCTAAAGCCGGAAAACATCCTCTGTGAGCACCCCAACCAGGTCTCCCCCGTGAAGATCTGTGACTTCGACCTGGGCAGCGGCATCAAACTCAACGGGGACTGCTCCCCTATCTCCACCCCGGAGCTGCTCACTCCGTGCGGCTCGGCGGAGTACATGGCCCCGGAGGTAGTGGAGGCCTTCAGCGAGGAGGCTAGCATCTACGACAAGCGCTGCGACCTGTGGAGCCTGGGCGTCATCTTGTATATCCTACTCAGCGGCTACCCGCCCTTCGTGGGCCGCTGTGGCAGCGACTGCGGCTGGGACCGCGGCGAGGCCTGCCCTGCCTGCCAGAACATGCTGTTTGAGAGCATCCAGGAGGGCAAGTACGAGTTCCCCGACAAGGACTGGGCCCACATCTCCTGCGCTGCCAAAGACCTCATCTCCAAGCTGCTGGTCCGTGACGCCAAGCAGAGGCTGAGTGCCGCCCAAGTCCTGCAGCACCCCTGGGTTCAGGGGTGCGCCCCGGAGAACACCTTGCCCACTCCCATGGTCCTGCAGAGG</t>
-  </si>
-  <si>
-    <t>MSRSKRDNNFYSVEIGDSTFTVLKRYQNLKPIGSGAQGIVCAAYDAILERNVAIKKLSRPFQNQTHAKRAYRELVLMKCVNHKNIIGLLNVFTPQKSLEEFQDVYIVMELMDANLCQVIQMELDHERMSYLLYQMLCGIKHLHSAGIIHRDLKPSNIVVKSDCTLKILDFGLARTAGTSFMMTPYVVTRYYRAPEVILGMGYKENVDLWSVGCIMGEMVCHKILFPGRDYIDQWNKVIEQLGTPCPEFMKKLQPTVRTYVENRPKYAGYSFEKLFPDVLFPADSEHNKLKASQARDLLSKMLVIDASKRISVDEALQHPYINVWYDPSEAEAPPPKIPDKQLDEREHTIEEWKELIYKEVMDLE</t>
-  </si>
-  <si>
-    <t>STRAA_HUMAN_D0_3GNI_B</t>
-  </si>
-  <si>
-    <t>MP2K2_HUMAN_D0_1S9I_A</t>
-  </si>
-  <si>
-    <t>LDRKLLTLEDKELGSGNFGTVKKGYYQMKKVVKTVAVKILKNEANDPALKDELLAEANVMQQLDNPYIVRMIGICEAESWMLVMEMAELGPLNKYLQQNRHVKDKNIIELVHQVSMGMKYLEESNFVHRDLAARNVLLVTQHYAKISDFGLSKALRADENYYKAQTHGKWPVKWYAPECINYYKFSSKSDVWSFGVLMWEAFSYGQKPYRGMKGSEVTAMLEKGERMGCPAGCPREMYDLMNLCWTYDVENRPGFAAVELRLRNYYYDVVN</t>
-  </si>
-  <si>
-    <t>AURKB_HUMAN_D0_4AF3_A</t>
-  </si>
-  <si>
-    <t>PIM1_HUMAN_D0_4A7C_A</t>
-  </si>
-  <si>
-    <t>CACCTGATCTGTCAGAGTGGAGACGTACTAAGTGCAAGATATGAAATTGTTGATACTTTAGGTGAAGGAGCTTTTGGAAAAGTTGTGGAGTGCATCGATCATAAAGCGGGAGGTAGACATGTAGCAGTAAAAATAGTTAAAAATGTGGATAGATACTGTGAAGCTGCTCGCTCAGAAATACAAGTTCTGGAACATCTGAATACAACAGACCCCAACAGTACTTTCCGCTGTGTCCAGATGTTGGAATGGTTTGAGCATCATGGTCACATTTGCATTGTTTTTGAACTATTGGGACTTAGTACTTACGACTTCATTAAAGAAAATGGTTTTCTACCATTTCGACTGGATCATATCAGAAAGATGGCATATCAGATATGCAAGTCTGTGAATTTTTTGCACAGTAATAAGTTGACTCACACAGACTTAAAGCCTGAAAACATCTTATTTGTGCAGTCTGACTACACAGAGGCGTATAATCCCAAAATAAAACGTGATGAACGCACCTTAATAAATCCAGATATTAAAGTTGTAGACTTTGGTAGTGCAACATATGATGACGAACATCACAGTACATTGGTATCTACAAGACATTATAGAGCACCTGAAGTTATTTTAGCCCTAGGGTGGTCCCAACCATGTGATGTCTGGAGCATAGGATGCATTCTTATTGAATACTATCTTGGGTTTACCGTATTTCCAACACACGATAGTAAGGAGCATTTAGCAATGATGGAAAGGATTCTTGGACCTCTACCAAAACATATGATACAGAAAACCAGGAAACGTAAATATTTTCACCACGATCGATTAGACTGGGATGAACACAGTTCTGCCGGCAGATATGTTTCAAGACGCTGTAAACCTCTGAAGGAATTTATGCTTTCTCAAGATGTTGAACATGAGCGTCTCTTTGACCTCATTCAGAAAATGTTGGAGTATGATCCAGCCAAAAGAATTACTCTCAGAGAAGCCTTAAAGCATCCTTTCTTTGACCTTCTGAAGAAAAGTATA</t>
-  </si>
-  <si>
-    <t>EAFLTQKAKVGELKDDDFERISELGAGNGGVVTKVQHRPSGLIMARKLIHLEIKPAIRNQIIRELQVLHECNSPYIVGFYGAFYSDGEISICMEHMDGGSLDQVLKEAKRIPEEILGKVSIAVLRGLAYLREKHQIMHRDVKPSNILVNSRGEIKLCDFGVSGQLIDSMANSFVGTRSYMAPERLQGTHYSVQSDIWSMGLSLVELAVGRYPIPPPDAKELEAIFGRPVVDGEEGEPHSISPRPRPPGRPVSGHGMDSRPAMAIFELLDYIVNEPPPKLPNGVFTPDFQEFVNKCLIKNPAERADLKMLTNHTFIKRSEVEEVDFAGWLCKTLRLNQPGTPTRTAV</t>
-  </si>
-  <si>
-    <t>STK10_HUMAN_D0_4BC6_A</t>
-  </si>
-  <si>
-    <t>GGGCCGGAGGATGAGCTGCCCGACTGGGCCGCCGCCAAAGAGTTTTACCAGAAGTACGACCCTAAGGACGTCATCGGCAGAGGAGTGAGCTCTGTGGTCCGCCGTTGTGTTCATCGAGCTACTGGCCACGAGTTTGCGGTGAAGATTATGGAAGTGACAGCTGAGCGGCTGAGTCCTGAGCAGCTGGAGGAGGTGCGGGAAGCCACACGGCGAGAGACACACATCCTTCGCCAGGTCGCCGGCCACCCCCACATCATCACCCTCATCGATTCCTACGAGTCTTCTAGCTTCATGTTCCTGGTGTTTGACCTGATGCGGAAGGGAGAGCTGTTTGACTATCTCACAGAGAAGGTGGCCCTCTCTGAAAAGGAAACCAGGTCCATCATGCGGTCTCTGCTGGAAGCAGTGAGCTTTCTCCATGCCAACAACATTGTGCATCGAGATCTGAAGCCCGAGAATATTCTCCTAGATGACAATATGCAGATCCGACTTTCAGATTTCGGGTTCTCCTGCCACTTGGAACCTGGCGAGAAGCTTCGAGAGTTGTGTGGGACCCCAGGGTATCTAGCGCCAGAGATCCTTAAATGCTCCATGGATGAAACCCACCCAGGCTATGGCAAGGAGGTCGACCTCTGGGCCTGTGGGGTGATCTTGTTCACACTCCTGGCTGGCTCGCCACCCTTCTGGCACCGGCGGCAGATCCTGATGTTACGCATGATCATGGAGGGCCAGTACCAGTTCAGTTCCCCCGAGTGGGATGACCGTTCCAGCACTGTCAAAGACCTGATCTCCAGGCTGCTGCAGGTGGATCCTGAGGCACGCCTGACAGCTGAGCAGGCCCTACAGCACCCCTTCTTTGAGCGT</t>
-  </si>
-  <si>
-    <t>KC1E_HUMAN_D0_4HNI_A</t>
-  </si>
-  <si>
-    <t>VRK2_HUMAN_D0_2V62_B</t>
-  </si>
-  <si>
-    <t>ETYIKLDKLGEGTYATVYKGKSKLTDNLVALKEIRLEHEEGAPCTAIREVSLLKDLKHANIVTLHDIIHTEKSLTLVFEYLDKDLKQYLDDCGNIINMHNVKLFLFQLLRGLAYCHRQKVLHRDLKPQNLLINERGELKLADFGLARAKSIPTKTYSNEVVTLWYRPPDILLGSTDYSTQIDMWGVGCIFYEMATGRPLFPGSTVEEQLHFIFRILGTPTEETWPGILSNEEFKTYNYPKYRAEALLSHAPRLDSDGADLLTKLLQFEGRNRISAEDAMKHPFFLSLGERIHKLPDTTSIFALKEIQLQKEASLRS</t>
-  </si>
-  <si>
-    <t>HQLQPRRVSFRGEASETLQSPGYDPSRPESFFQQSFQRLSRLGHGSYGEVFKVRSKEDGRLYAVKRSMSPFRGPKDRARKLAEVGSHEKVGQHPCCVRLEQAWEEGGILYLQTELCGPSLQQHCEAWGASLPEAQVWGYLRDTLLALAHLHSQGLVHLDVKPANIFLGPRGRCKLGDFGLLVELGTAGAGEVQEGDPRYMAPELLQGSYGTAADVFSLGLTILEVACNMELPHGGEGWQQLRQGYLPPEFTAGLSSELRSVLVMMLEPDPKLRATAEALLALPVLRQP</t>
-  </si>
-  <si>
-    <t>aa_end</t>
-  </si>
-  <si>
-    <t>TACCAGCTCTTCGAGGAATTGGGCAAGGGAGCCTTCTCGGTGGTGCGAAGGTGTGTGAAGGTGCTGGCTGGCCAGGAGTATGCTGCCAAGATCATCAACACAAAGAAGCTGTCAGCCAGAGACCATCAGAAGCTGGAGCGTGAAGCCCGCATCTGCCGCCTGCTGAAGCACCCCAACATCGTCCGACTACATGACAGCATCTCAGAGGAGGGACACCACTACCTGATCTTCGACCTGGTCACTGGTGGGGAACTGTTTGAAGATATCGTGGCCCGGGAGTATTACAGTGAGGCGGATGCCAGTCACTGTATCCAGCAGATCCTGGAGGCTGTGCTGCACTGCCACCAGATGGGGGTGGTGCACCGGGACCTGAAGCCTGAGAATCTGTTGCTGGCCTCCAAGCTCAAGGGTGCCGCAGTGAAGCTGGCAGACTTTGGCCTGGCCATAGAGGTGGAGGGGGAGCAGCAGGCATGGTTTGGGTTTGCAGGGACTCCTGGATATCTCTCCCCAGAAGTGCTGCGGAAGGACCCGTACGGGAAGCCTGTGGACCTGTGGGCTTGTGGGGTCATCCTGTACATCCTGCTGGTTGGGTACCCCCCGTTCTGGGATGAGGACCAGCACCGCCTGTACCTGCAGATCAAAGCCGGCGCCTATGATTTCCCATCGCCGGAATGGGACACTGTCACCCCGGAAGCCAAGGATCTGATCAATAAGATGCTGACCATTAACCCATCCAAACGCATCACAGCTGCCGAAGCCCTTAAGCACCCCTGGATCTCGCACCGCTCCACCGTGGCATCCTGCATGCACAGACAGGAGACCGTGGACTGCCTGAAGAAGTTCAATGCCAGGAGGAAACTGAAGGGAGCC</t>
-  </si>
-  <si>
-    <t>MK08_HUMAN_D0_2NO3_A</t>
-  </si>
-  <si>
-    <t>TCGGTTAAAGGAAGAATTTATTCCATATTAAAGCAGATAGGAAGTGGAGGTTCAAGCAAGGTATTTCAGGTGTTAAATGAAAAGAAACAGATATATGCTATAAAATATGTGAACTTAGAAGAAGCAGATAACCAAACTCTTGATAGTTACCGGAACGAAATAGCTTATTTGAATAAACTACAACAACACAGTGATAAGATCATCCGACTTTATGATTATGAAATCACGGACCAGTACATCTACATGGTAATGGAGTGTGGAAATATTGATCTTAATAGTTGGCTTAAAAAGAAAAAATCCATTGATCCATGGGAACGCAAGAGTTACTGGAAAAATATGTTAGAGGCAGTTCACACAATCCATCAACATGGCATTGTTCACAGTGATCTTAAACCAGCTAACTTTCTGATAGTTGATGGAATGCTAAAGCTAATTGATTTTGGGATTGCAAACCAAATGCAACCAGATACAACAAGTGTTGTTAAAGATTCTCAGGTTGGCACAGTTAATTATATGCCACCAGAAGCAATCAAAGATATGTCTTCCTCCAGAGAGAATGGGAAATCTAAGTCAAAGATAAGCCCCAAAAGTGATGTTTGGTCCTTAGGATGTATTTTGTACTATATGACTTACGGGAAAACACCATTTCAGCAGATAATTAATCAGATTTCTAAATTACATGCCATAATTGATCCTAATCATGAAATTGAATTTCCCGATATTCCAGAGAAAGATCTTCAAGATGTGTTAAAGTGTTGTTTAAAAAGGGACCCAAAACAGAGGATATCCATTCCTGAGCTCCTGGCTCATCCATATGTTCAAATTCAAACTCATCCAGTTAACCAAATGGCCAAGGGAACCACTGAAGAA</t>
-  </si>
-  <si>
-    <t>PAK1_HUMAN_D0_3Q52_A</t>
+    <t>TGGGCCCTGAACATGAAGGAGCTGAAGCTGCTGCAGACCATCGGGAAGGGGGAGTTCGGAGACGTGATGCTGGGCGATTACCGAGGGAACAAAGTCGCCGTCAAGTGCATTAAGAACGACGCCACTGCCCAGGCCTTCCTGGCTGAAGCCTCAGTCATGACGCAACTGCGGCATAGCAACCTGGTGCAGCTCCTGGGCGTGATCGTGGAGGAGAAGGGCGGGCTCTACATCGTCACTGAGTACATGGCCAAGGGGAGCCTTGTGGACTACCTGCGGTCTAGGGGTCGGTCAGTGCTGGGCGGAGACTGTCTCCTCAAGTTCTCGCTAGATGTCTGCGAGGCCATGGAATACCTGGAGGGCAACAATTTCGTGCATCGAGACCTGGCTGCCCGCAATGTGCTGGTGTCTGAGGACAACGTGGCCAAGGTCAGCGACTTTGGTCTCACCAAGGAGGCGTCCAGCACCCAGGACACGGGCAAGCTGCCAGTCAAGTGGACAGCCCCTGAGGCCCTGAGAGAGAAGAAATTCTCCACTAAGTCTGACGTGTGGAGTTTCGGAATCCTTCTCTGGGAAATCTACTCCTTTGGGCGAGTGCCTTATCCAAGAATTCCCCTGAAGGACGTCGTCCCTCGGGTGGAGAAGGGCTACAAGATGGATGCCCCCGACGGCTGCCCGCCCGCAGTCTATGAAGTCATGAAGAACTGCTGGCACCTGGACGCCGCCATGCGGCCCTCCTTCCTACAGCTCCGAGAGCAGCTTGAGCACATCAAAACCCACGAGCTGCACCTG</t>
+  </si>
+  <si>
+    <t>dna_seq</t>
+  </si>
+  <si>
+    <t>AACCTGGTTTTTAGTGACGGCTACGTGGTAAAGGAGACAATTGGTGTGGGCTCCTACTCTGAGTGCAAGCGCTGTGTCCACAAGGCCACCAACATGGAGTATGCTGTCAAGGTCATTGATAAGAGCAAGCGGGATCCTTCAGAAGAGATTGAGATTCTTCTGCGGTATGGCCAGCACCCCAACATCATCACTCTGAAAGATGTGTATGATGATGGCAAACACGTGTACCTGGTGACAGAGCTGATGCGGGGTGGGGAGCTGCTGGACAAGATCCTGCGGCAGAAGTTCTTCTCAGAGCGGGAGGCCAGCTTTGTCCTGCACACCATTGGCAAAACTGTGGAGTATCTGCACTCACAGGGGGTTGTGCACAGGGACCTGAAGCCCAGCAACATCCTGTATGTGGACGAGTCCGGGAATCCCGAGTGCCTGCGCATCTGTGACTTTGGTTTTGCCAAACAGCTGCGGGCTGAGAATGGGCTCCTCATGACACCTTGCTACACAGCCAACTTTGTGGCGCCTGAGGTGCTGAAGCGCCAGGGCTACGATGAAGGCTGCGACATCTGGAGCCTGGGCATTCTGCTGTACACCATGCTGGCAGGATATACTCCATTTGCCAACGGTCCCAGTGACACACCAGAGGAAATCCTAACCCGGATCGGCAGTGGGAAGTTTACCCTCAGTGGGGGAAATTGGAACACAGTTTCAGAGACAGCCAAGGACCTGGTGTCCAAGATGCTACACGTGGATCCCCACCAGCGCCTCACAGCTAAGCAGGTTCTGCAGCATCCATGGGTCACCCAGAAAGACAAGCTTCCCCAAAGCCAGCTGTCCCACCAGGACCTACAGCTTGTGAAGGGAGCCATGGCTGCCACGTACTCCGCACTCAACAGCTCCAAGCCCACCCCCCAGCTGAAGCCCATCGAGTCATCCATCCTGGCCCAGCGGCGAGTGAGGAAGTTGCCATCCACCACCCTG</t>
+  </si>
+  <si>
+    <t>ATGGCCGACGACGACGTGCTGTTCGAGGATGTGTACGAGCTGTGCGAGGTGATCGGAAAGGGTCCCTTCAGTGTTGTACGACGATGTATCAACAGAGAAACTGGGCAACAATTTGCTGTAAAAATTGTTGATGTAGCCAAGTTCACATCAAGTCCAGGGTTAAGTACAGAAGATCTAAAGCGGGAAGCCAGTATCTGTCATATGCTGAAACATCCACACATTGTAGAGTTATTGGAGACATATAGCTCAGATGGAATGCTTTACATGGTTTTCGAATTTATGGATGGAGCAGATCTGTGTTTTGAAATCGTAAAGCGAGCTGACGCTGGTTTTGTGTACAGTGAAGCTGTAGCCAGCCATTATATGAGACAGATACTGGAAGCTCTACGCTACTGCCATGATAATAACATAATTCACAGGGATGTGAAGCCCCACTGTGTTCTCCTTGCCTCAAAAGAAAACTCGGCACCTGTTAAACTTGGAGGCTTTGGGGTAGCTATTCAATTAGGGGAGTCTGGACTTGTAGCTGGAGGACGTGTTGGAACACCTCATTTTATGGCACCAGAAGTGGTCAAAAGAGAGCCTTACGGAAAGCCTGTAGACGTCTGGGGGTGCGGTGTGATCCTTTTTATCCTGCTCAGTGGTTGTTTGCCTTTTTACGGAACCAAGGAAAGATTGTTTGAAGGCATTATTAAAGGAAAATATAAGATGAATCCAAGGCAGTGGAGCCATATCTCTGAAAGTGCCAAAGACCTAGTACGTCGCATGCTGATGCTGGATCCAGCTGAAAGGATCACTGTTTATGAAGCACTGAATCACCCATGGCTTAAGGAGCGGGATCGTTACGCCTACAAGATTCATCTTCCAGAAACAGTAGAGCAGCTGAGGAAATTCAATGCAAGGAGGAAACTAAAGGGTGCAGTACTAGCCGCTGTGTCAAGTCACAAATTCAACTCATTCTATGGGGATCCCCCTGAAGAGTTACCAGATTTCTCCGAAGACCCTACCTCCTCAGGAGCA</t>
+  </si>
+  <si>
+    <t>VRK1_HUMAN_D0_3OP5_D</t>
+  </si>
+  <si>
+    <t>ATGGGGAAGGTGAAAGCCACCCCCATGACACCTGAACAAGCAATGAAGCAATACATGCAAAAACTCACAGCCTTCGAACACCATGAGATTTTCAGCTACCCTGAAATATATTTCTTGGGTCTAAATGCTAAGAAGCGCCAGGGCATGACAGGTGGGCCCAACAATGGTGGCTATGATGATGACCAGGGATCATATGTGCAGGTGCCCCACGATCACGTGGCTTACAGGTATGAGGTCCTCAAGGTCATTGGGAAGGGGAGCTTTGGGCAGGTGGTCAAGGCCTACGATCACAAAGTCCACCAGCACGTGGCCCTAAAGATGGTGCGGAATGAGAAGCGCTTCCACCGGCAAGCAGCGGAGGAGATCCGAATCCTGGAACACCTGCGGAAGCAGGACAAGGATAACACAATGAATGTCATCCATATGCTGGAGAATTTCACCTTCCGCAACCACATCTGCATGACGTTTGAGCTGCTGAGCATGAACCTCTATGAGCTCATCAAGAAGAATAAATTCCAGGGCTTCAGTCTGCCTTTGGTTCGCAAGTTTGCCCACTCGATTCTGCAGTGCTTGGATGCTTTGCACAAAAACAGAATAATTCACTGTGACCTTAAGCCCGAGAACATTTTGTTAAAGCAGCAGGGTAGAAGCGGTATTAAAGTAATTGATTTTGGCTCCAGTTGTTACGAGCATCAGCGTGTCTACACGTACATCCAGTCGCGTTTTTACCGGGCTCCAGAAGTGATCCTTGGGGCCAGGTATGGCATGCCCATTGATATGTGGAGCCTGGGCTGCATTTTAGCAGAGCTCCTGACGGGTTACCCCCTCTTGCCTGGGGAAGATGAAGGGGACCAGCTGGCCTGTATGATTGAACTGTTGGGCATGCCCTCACAGAAACTGCTGGATGCATCCAAACGAGCCAAAAATTTTGTGAGCTCCAAGGGTTATCCCCGTTACTGCACTGTCACGACTCTCTCAGATGGCTCTGTGGTCCTAAACGGAGGCCGTTCCCGGAGGGGGAAACTGAGGGGCCCACCGGAGAGCAGAGAGTGGGGGAACGCGCTGAAGGGGTGTGATGATCCCCTTTTCCTTGACTTCTTAAAACAGTGTTTAGAGTGGGATCCTGCAGTGCGCATGACCCCAGGCCAGGCTTTGCGGCACCCCTGGCTGAGGAGGCGGTTGCCAAAGCCTCCCACCGGGGAGAAAACGTCAGTGAAAAGG</t>
+  </si>
+  <si>
+    <t>SVYPKALRDEYIMSKTLGSGACGEVKLAFERKTCKKVAIKIISKRKFAIGSAREADPALNVETEIEILKKLNHPCIIKIKNFFDAEDYYIVLELMEGGELFDKVVGNKRLKEATCKLYFYQMLLAVQYLHENGIIHRDLKPENVLLSSQEEDCLIKITDFGHSKIWGETSLMRTLCGTPTYLAPEVLVSVGTAGYNRAVDCWSLGVILFICLSGYPPFSEHRTQVSLKDQITSGKYNFIPEVWAEVSEKALDLVKKLLVVDPKARFTTEEALRHPWLQDEDMKRKFQDLLSEENESTALPQVLAQPSTSRKRPREGEAEGAE</t>
+  </si>
+  <si>
+    <t>ATGGAGAAGTATGAAAAAATTGGGAAAATTGGAGAAGGATCCTATGGAGTTGTTTTCAAATGTAGAAACAGGGACACGGGTCAGATTGTGGCCATCAAGAAGTTTCTGGAATCAGAAGATGACCCTGTCATAAAGAAAATTGCCCTTCGGGAAATCCGAATGCTCAAGCAACTCAAGCATCCCAACCTTGTTAACCTCCTGGAAGTCTTCAGGAGGAAACGGAGGCTTCACCTGGTGTTTGAATATTGTGACCACACAGTTCTCCATGAGTTGGACAGATACCAAAGAGGGGTACCAGAACATCTCGTGAAGAGCATAACTTGGCAGACACTGCAAGCTGTAAATTTTTGCCATAAACACAATTGCATACATAGAGACGTGAAGCCAGAAAATATCCTCATCACGAAACATTCCGTGATTAAGCTTTGTGACTTTGGATTTGCTCGGCTTTTGACTGGACCGAGTGACTACTATACAGACTACGTGGCTACCAGGTGGTACCGCTCCCCTGAGCTGCTGGTGGGGGACACGCAGTACGGCCCCCCGGTGGATGTTTGGGCAATTGGCTGTGTCTTTGCTGAGCTGCTGTCAGGAGTGCCTCTGTGGCCAGGAAAATCGGATGTGGATCAGCTGTATCTGATTAGGAAGACCTTGGGGGATCTCATTCCTAGGCACCAGCAAGTGTTTAGCACGAATCAGTACTTCAGTGGAGTGAAAATTCCAGACCCTGAAGATATGGAACCACTTGAATTAAAATTCCCAAACATCTCTTATCCTGCCCTGGGGCTCCTA</t>
+  </si>
+  <si>
+    <t>KHDGRVKIGHYVLGDTLGVGTFGKVKIGEHQLTGHKVAVKILNRQKIRSLDVVGKIKREIQNLKLFRHPHIIKLYQVISTPTDFFMVMEYVSGGELFDYICKHGRVEEMEARRLFQQILSAVDYCHRHMVVHRDLKPENVLLDAHMNAKIADFGLSNMMSDGEFLRTSCGSPNYAAPEVISGRLYAGPEVDIWSCGVILYALLCGTLPFDDEHVPTLFKKIRGGVFYIPEYLNRSVATLLMHMLQVDPLKRATIKDIREHEWFKQDLPSYLFPE</t>
+  </si>
+  <si>
+    <t>ATGGAAAACTTTAATAATTTCTATATACTTACATCTAAAGAGCTAGGGAGAGGAAAATTTGCTGTGGTTAGACAATGTATATCAAAATCTACTGGCCAAGAATATGCTGCAAAATTTCTAAAAAAGAGAAGAAGAGGACAGGATTGTCGAGCAGAAATTTTACACGAGATTGCTGTGCTTGAATTGGCAAAGTCTTGTCCCCGTGTTATTAATCTTCATGAGGTCTATGAAAATACAAGTGAAATCATTTTGATATTGGAATATGCTGCAGGTGGAGAAATTTTCAGCCTGTGTTTACCTGAGTTGGCTGAAATGGTTTCTGAAAATGATGTTATCAGACTCATTAAACAAATACTTGAAGGAGTTTATTATCTACATCAGAATAACATTGTACACCTTGATTTAAAGCCACAGAATATATTACTGAGCAGCATATACCCTCTCGGGGACATTAAAATAGTAGATTTTGGAATGTCTCGAAAAATAGGGCATGCGTGTGAACTTCGGGAAATCATGGGAACACCAGAATATTTAGCTCCAGAAATCCTGAACTATGATCCCATTACCACAGCAACAGATATGTGGAATATTGGTATAATAGCATATATGTTGTTAACTCACACATCACCATTTGTGGGAGAAGATAATCAAGAAACATACCTCAATATTTCTCAAGTTAATGTAGATTATTCGGAAGAAACTTTTTCATCAGTTTCACAGCTGGCCACAGACTTTATTCAGAGCCTTTTAGTAAAAAATCCAGAGAAAAGACCAACAGCAGAGATATGCCTTTCTCATTCTTGGCTACAGCAGTGGGACTTTGAAAACTTGTTTCACCCTGAAGAAACTTCCAGTTCCTCTCAAACTCAGGATCATTCTGTAAGGTCCTCTGAAGACAAGACTTCTAAATCCTCC</t>
+  </si>
+  <si>
+    <t>MPSRAEDYEVLYTIGTGSYGRCQKIRRKSDGKILVWKELDYGSMTEAEKQMLVSEVNLLRELKHPNIVRYYDRIIDRTNTTLYIVMEYCEGGDLASVITKGTKERQYLDEEFVLRVMTQLTLALKECHRRSDGGHTVLHRDLKPANVFLDGKQNVKLGDFGLARILNHDTSFAKTFVGTPYYMSPEQMNRMSYNEKSDIWSLGCLLYELCALMPPFTAFSQKELAGKIREGKFRRIPYRYSDELNEIITRMLNLKDYHRPSVEEILENPLI</t>
+  </si>
+  <si>
+    <t>GACCCAGAAGAGCTTTTTACAAAACTAGAGAAAATTGGGAAGGGCTCCTTTGGAGAGGTGTTCAAAGGCATTGACAATCGGACTCAGAAAGTGGTTGCCATAAAGATCATTGATCTGGAAGAAGCTGAAGATGAGATAGAGGACATTCAACAAGAAATCACAGTGCTGAGTCAGTGTGACAGTCCATATGTAACCAAATATTATGGATCCTATCTGAAGGATACAAAATTATGGATAATAATGGAATATCTTGGTGGAGGCTCCGCACTAGATCTATTAGAACCTGGCCCATTAGATGAAACCCAGATCGCTACTATATTAAGAGAAATACTGAAAGGACTCGATTATCTCCATTCGGAGAAGAAAATCCACAGAGACATTAAAGCGGCCAACGTCCTGCTGTCTGAGCATGGCGAGGTGAAGCTGGCGGACTTTGGCGTGGCTGGCCAGCTGACAGACACCCAGATCAAAAGGAACACCTTCGTGGGCACCCCATTCTGGATGGCACCCGAGGTCATCAAACAGTCGGCCTATGACTCGAAGGCAGACATCTGGTCCCTGGGCATAACAGCTATTGAACTTGCAAGAGGGGAACCACCTCATTCCGAGCTGCACCCCATGAAAGTTTTATTCCTCATTCCAAAGAACAACCCACCGACGTTGGAAGGAAACTACAGTAAACCCCTCAAGGAGTTTGTGGAGGCCTGTTTGAATAAGGAGCCGAGCTTTAGACCCACTGCTAAGGAGTTATTGAAGCACAAGTTTATACTACGCAATGCAAAGAAAACTTCCTACTTGACCGAGCTCATCGAC</t>
+  </si>
+  <si>
+    <t>VIIDNKRYLFIQKLGEGGFSYVDLVEGLHDGHFYALKRILCHEQQDREEAQREADMHRLFNHPNILRLVAYCLRERGAKHEAWLLLPFFKRGTLWNEIERLKDKGNFLTEDQILWLLLGICRGLEAIHAKGYAHRDLKPTNILLGDEGQPVLMDLGSMNQACIHVEGSRQALTLQDWAAQRCTISYRAPELFSVQSHCVIDERTDVWSLGCVLYAMMFGEGPYDMVFQKGDSVALAVQNQLSIPQSPRHSSALWQLLNSMMTVDPHQRPHIPLLLSQLEALQ</t>
+  </si>
+  <si>
+    <t>DEQPHIGNYRLLKTIGKGNFAKVKLARHILTGREVAIKIIDKTQLNPTSLQKLFREVRIMKILNHPNIVKLFEVIETEKTLYLIMEYASGGEVFDYLVAHGRMKEKEARSKFRQIVSAVQYCHQKRIVHRDLKAENLLLDADMNIKIADFGFSNEFTVGGKLDTFCGSPPYAAPELFQGKKYDGPEVDVWSLGVILYTLVSGSLPFDGQNLKELRERVLRGKYRIPFYMSTDCENLLKRFLVLNPIKRGTLEQIMKDRWINAGHEEDELKPFVEPELDISDQKRIDIMVGMGYSQEEIQESLSKMKYDEITATYLLLGRKSSE</t>
+  </si>
+  <si>
+    <t>AAGGAGAAGGAGCCCCTGGAGTCGCAGTACCAGGTGGGCCCGCTACTGGGCAGCGGCGGCTTCGGCTCGGTCTACTCAGGCATCCGCGTCTCCGACAACTTGCCGGTGGCCATCAAACACGTGGAGAAGGACCGGATTTCCGACTGGGGAGAGCTGCCTAATGGCACTCGAGTGCCCATGGAAGTGGTCCTGCTGAAGAAGGTGAGCTCGGGTTTCTCCGGCGTCATTAGGCTCCTGGACTGGTTCGAGAGGCCCGACAGTTTCGTCCTGATCCTGGAGAGGCCCGAGCCGGTGCAAGATCTCTTCGACTTCATCACGGAAAGGGGAGCCCTGCAAGAGGAGCTGGCCCGCAGCTTCTTCTGGCAGGTGCTGGAGGCCGTGCGGCACTGCCACAACTGCGGGGTGCTCCACCGCGACATCAAGGACGAAAACATCCTTATCGACCTCAATCGCGGCGAGCTCAAGCTCATCGACTTCGGGTCGGGGGCGCTGCTCAAGGACACCGTCTACACGGACTTCGATGGGACCCGAGTGTATAGCCCTCCAGAGTGGATCCGCTACCATCGCTACCATGGCAGGTCGGCGGCAGTCTGGTCCCTGGGGATCCTGCTGTATGATATGGTGTGTGGAGATATTCCTTTCGAGCATGACGAAGAGATCATCGGGGGCCAGGTTTTCTTCAGGCAGAGGGTCTCTTCAGAATGTCAGCATCTCATTAGATGGTGCTTGGCCCTGAGACCATCAGATAGGCCAACCTTCGAAGAAATCCAGAACCATCCATGGATGCAAGATGTTCTCCTGCCCCAGGAAACTGCTGAGATCCACCTCCACAGCCTGTCGCCGGGGCCCAGCAAA</t>
+  </si>
+  <si>
+    <t>PFPEGKVLDDMEGNQWVLGKKIGSGGFGLIYLAFPTNKPEKDARHVVKVEYQENGPLFSELKFYQRVAKKDCIKKWIERKQLDYLGIPLFYGSGLTEFKGRSYRFMVMERLGIDLQKISGQNGTFKKSTVLQLGIRMLDVLEYIHENEYVHGDIKAANLLLGYKNPDQVYLADYGLSYRYCPNGNHKQYQENPRKGHNGTIEFTSLDAHKGVALSRRSDVEILGYCMLRWLCGKLPWEQNLKDPVAVQTAKTNLLDELPQSVLKWAPSGSSCCEIAQFLVCAHSLAYDEKPNYQALKKILNPHGIPLGPLDFSTKGQSINVH</t>
+  </si>
+  <si>
+    <t>MESDLHQIIHSSQPLTLEHVRYFLYQLLRGLKYMHSAQVIHRDLKPSNLLVNENCELKIGDFGMARGLCTSPAEHQYFMTEYVATRWYRAPELMLSLHEYTQAIDLWSVGCIFGEMLARRQLFPGKNYVHQLQLIMMVLGTPSPAVIQAVGAERVRAYIQSLPPRQPVPWETVYPGADRQALSLLGRMLRFEPSARISAAAALRHPFLAKYHDPDDEPDCAPPFDFAFDREALTRERIKEAIVAEIEDFHARREGIRQQIRFQPSLQPVASEPGCPDVEMPSPWAPSGDCAM</t>
+  </si>
+  <si>
+    <t>EPKKYAVTDDYQLSKQVLGLGVNGKVLECFHRRTGQKCALKLLYDSPKARQEVDHHWQASGGPHIVCILDVYENMHHGKRCLLIIMECMEGGELFSRIQERGDQAFTEREAAEIMRDIGTAIQFLHSHNIAHRDVKPENLLYTSKEKDAVLKLTDFGFAKETTQNALQTPCYTPYYVAPEVLGPEKYDKSCDMWSLGVIMYILLCGFPPFYSNTGQAISPGMKRRIRLGQYGFPNPEWSEVSEDAKQLIRLLLKTDPTERLTITQFMNHPWINQSMVVPQTPLHTARVLQEDKDHWDEVKEEMTSALATMRVDYDQV</t>
+  </si>
+  <si>
+    <t>STK24_HUMAN_D0_3ZHP_C</t>
+  </si>
+  <si>
+    <t>aa_seq</t>
+  </si>
+  <si>
+    <t>KC1D_HUMAN_D0_4HNF_B</t>
+  </si>
+  <si>
+    <t>AGCATTGAGTCATCAGGAAAACTGAAGATCTCCCCTGAACAACACTGGGATTTCACTGCAGAGGACTTGAAAGACCTTGGAGAAATTGGACGAGGAGCTTATGGTTCTGTCAACAAAATGGTCCACAAACCAAGTGGGCAAATAATGGCAGTTAAAAGAATTCGGTCAACAGTGGATGAAAAAGAACAAAAACAACTTCTTATGGATTTGGATGTAGTAATGCGGAGTAGTGATTGCCCATACATTGTTCAGTTTTATGGTGCACTCTTCAGAGAGGGTGACTGTTGGATCTGTATGGAACTCATGTCTACCTCGTTTGATAAGTTTTACAAATATGTATATAGTGTATTAGATGATGTTATTCCAGAAGAAATTTTAGGCAAAATCACTTTAGCAACTGTGAAAGCACTAAACCACTTAAAAGAAAACTTGAAAATTATTCACAGAGATATCAAACCTTCCAATATTCTTCTGGACAGAAGTGGAAATATTAAGCTCTGTGACTTCGGCATCAGTGGACAGCTTGTGGACTCTATTGCCAAGACAAGAGATGCTGGCTGTAGGCCATACATGGCACCTGAAAGAATAGACCCAAGCGCATCACGACAAGGATATGATGTCCGCTCTGATGTCTGGAGTTTGGGGATCACATTGTATGAGTTGGCCACAGGCCGATTTCCTTATCCAAAGTGGAATAGTGTATTTGATCAACTAACACAAGTCGTGAAAGGAGATCCTCCGCAGCTGAGTAATTCTGAGGAAAGGGAATTCTCCCCGAGTTTCATCAACTTTGTCAACTTGTGCCTTACGAAGGATGAATCCAAAAGGCCAAAGTATAAAGAGCTTCTGAAACATCCCTTTATTTTGATGTATGAAGAACGTGCCGTTGAGGTCGCATGCTATGTTTGTAAAATCCTGGATCAAATGCCAGCTACTCCCAGCTCTCCCATGTATGTCGAT</t>
+  </si>
+  <si>
+    <t>AAPK2_HUMAN_D0_2H6D_A</t>
+  </si>
+  <si>
+    <t>CLK3_HUMAN_D0_2WU7_A</t>
+  </si>
+  <si>
+    <t>GAAGCCTTTCTCACCCAGAAAGCCAAGGTCGGCGAACTCAAAGACGATGACTTCGAAAGGATCTCAGAGCTGGGCGCGGGCAACGGCGGGGTGGTCACCAAAGTCCAGCACAGACCCTCGGGCCTCATCATGGCCAGGAAGCTGATCCACCTTGAGATCAAGCCGGCCATCCGGAACCAGATCATCCGCGAGCTGCAGGTCCTGCACGAATGCAACTCGCCGTACATCGTGGGCTTCTACGGGGCCTTCTACAGTGACGGGGAGATCAGCATTTGCATGGAACACATGGACGGCGGCTCCCTGGACCAGGTGCTGAAAGAGGCCAAGAGGATTCCCGAGGAGATCCTGGGGAAAGTCAGCATCGCGGTTCTCCGGGGCTTGGCGTACCTCCGAGAGAAGCACCAGATCATGCACCGAGATGTGAAGCCCTCCAACATCCTCGTGAACTCTAGAGGGGAGATCAAGCTGTGTGACTTCGGGGTGAGCGGCCAGCTCATAGACTCCATGGCCAACTCCTTCGTGGGCACGCGCTCCTACATGGCTCCGGAGCGGTTGCAGGGCACACATTACTCGGTGCAGTCGGACATCTGGAGCATGGGCCTGTCCCTGGTGGAGCTGGCCGTCGGAAGGTACCCCATCCCCCCGCCCGACGCCAAAGAGCTGGAGGCCATCTTTGGCCGGCCCGTGGTCGACGGGGAAGAAGGAGAGCCTCACAGCATCTCGCCTCGGCCGAGGCCCCCCGGGCGCCCCGTCAGCGGTCACGGGATGGATAGCCGGCCTGCCATGGCCATCTTTGAACTCCTGGACTATATTGTGAACGAGCCACCTCCTAAGCTGCCCAACGGTGTGTTCACCCCCGACTTCCAGGAGTTTGTCAATAAATGCCTCATCAAGAACCCAGCGGAGCGGGCGGACCTGAAGATGCTCACAAACCACACCTTCATCAAGCGGTCCGAGGTGGAAGAAGTGGATTTTGCCGGCTGGTTGTGTAAAACCCTGCGGCTGAACCAGCCCGGCACACCCACGCGCACCGCCGTG</t>
+  </si>
+  <si>
+    <t>MKNK2_HUMAN_D0_2AC3_A</t>
+  </si>
+  <si>
+    <t>STRDYEIQRERIELGRCIGEGQFGDVHQGIYMSPENPALAVAIKTCKNCTSDSVREKFLQEALTMRQFDHPHIVKLIGVITENPVWIIMELCTLGELRSFLQVRKYSLDLASLILYAYQLSTALAYLESKRFVHRDIAARNVLVSSNDCVKLGDFGLSRYMEDSTYYKASKGKLPIKWMAPESINFRRFTSASDVWMFGVCMWEILMHGVKPFQGVKNNDVIGRIENGERLPMPPNCPPTLYSLMTKCWAYDPSRRPRFTELKAQLSTILEEEKAQQEE</t>
+  </si>
+  <si>
+    <t>CSK22_HUMAN_D0_3E3B_X</t>
+  </si>
+  <si>
+    <t>Cterm</t>
+  </si>
+  <si>
+    <t>ATGAGCAGAAGCAAGCGTGACAACAATTTTTATAGTGTAGAGATTGGAGATTCTACATTCACAGTCCTGAAACGATATCAGAATTTAAAACCTATAGGCTCAGGAGCTCAAGGAATAGTATGCGCAGCTTATGATGCCATTCTTGAAAGAAATGTTGCAATCAAGAAGCTAAGCCGACCATTTCAGAATCAGACTCATGCCAAGCGGGCCTACAGAGAGCTAGTTCTTATGAAATGTGTTAATCACAAAAATATAATTGGCCTTTTGAATGTTTTCACACCACAGAAATCCCTAGAAGAATTTCAAGATGTTTACATAGTCATGGAGCTCATGGATGCAAATCTTTGCCAAGTGATTCAGATGGAGCTAGATCATGAAAGAATGTCCTACCTTCTCTATCAGATGCTGTGTGGAATCAAGCACCTTCATTCTGCTGGAATTATTCATCGGGACTTAAAGCCCAGTAATATAGTAGTAAAATCTGATTGCACTTTGAAGATTCTTGACTTCGGTCTGGCCAGGACTGCAGGAACGAGTTTTATGATGACGCCTTATGTAGTGACTCGCTACTACAGAGCACCCGAGGTCATCCTTGGCATGGGCTACAAGGAAAACGTGGATTTATGGTCTGTGGGGTGCATTATGGGAGAAATGGTTTGCCACAAAATCCTCTTTCCAGGAAGGGACTATATTGATCAGTGGAATAAAGTTATTGAACAGCTTGGAACACCATGTCCTGAATTCATGAAGAAACTGCAACCAACAGTAAGGACTTACGTTGAAAACAGACCTAAATATGCTGGATATAGCTTTGAGAAACTCTTCCCTGATGTCCTTTTCCCAGCTGACTCAGAACACAACAAACTTAAAGCCAGTCAGGCAAGGGATTTGTTATCCAAAATGCTGGTAATAGATGCATCTAAAAGGATCTCTGTAGATGAAGCTCTCCAACACCCGTACATCAATGTCTGGTATGATCCTTCTGAAGCAGAAGCTCCACCACCAAAGATCCCTGACAAGCAGTTAGATGAAAGGGAACACACAATAGAAGAGTGGAAAGAATTGATATATAAGGAAGTTATGGACTTGGAG</t>
+  </si>
+  <si>
+    <t>TTSLEALPTGTVLTDKSGRQWKLKSFQTRDNQGILYEAAPTSTLTCDSGPQKQKFSLKLDAKDGRLFNEQNFFQRAAKPLQVNKWKKLYSTPLLAIPTCMGFGVHQDKYRFLVLPSLGRSLQSALDVSPKHVLSERSVLQVACRLLDALEFLHENEYVHGNVTAENIFVDPEDQSQVTLAGYGFAFRYCPSGKHVAYVEGSRSPHEGDLEFISMDLHKGCGPSRRSDLQSLGYCMLKWLYGFLPWTNCLPNTEDIMKQKQKFVDKPGPFVGPCGHWIRPSETLQKYLKVVMALTYEEKPPYAMLRNNLEALLQDLRVSPYDPIGLPMVP</t>
+  </si>
+  <si>
+    <t>SPNYDKWEMERTDITMKHKLGGGQYGEVYEGVWKKYSLTVAVKTLKEDTMEVEEFLKEAAVMKEIKHPNLVQLLGVCTREPPFYIITEFMTYGNLLDYLRECNRQEVNAVVLLYMATQISSAMEYLEKKNFIHRDLAARNCLVGENHLVKVADFGLSRLMTGDTYTAHAGAKFPIKWTAPESLAYNKFSIKSDVWAFGVLLWEIATYGMSPYPGIDLSQVYELLEKDYRMERPEGCPEKVYELMRACWQWNPSDRPSFAEIHQAFETMFQESSISDEVEKELGK</t>
+  </si>
+  <si>
+    <t>ATGGCGGCGGCGGCGGCTCAGGGGGGCGGGGGCGGGGAGCCCCGTAGAACCGAGGGGGTCGGCCCGGGGGTCCCGGGGGAGGTGGAGATGGTGAAGGGGCAGCCGTTCGACGTGGGCCCGCGCTACACGCAGTTGCAGTACATCGGCGAGGGCGCGTACGGCATGGTCAGCTCGGCCTATGACCACGTGCGCAAGACTCGCGTGGCCATCAAGAAGATCAGCCCCTTCGAACATCAGACCTACTGCCAGCGCACGCTCCGGGAGATCCAGATCCTGCTGCGCTTCCGCCATGAGAATGTCATCGGCATCCGAGACATTCTGCGGGCGTCCACCCTGGAAGCCATGAGAGATGTCTACATTGTGCAGGACCTGATGGAGACTGACCTGTACAAGTTGCTGAAAAGCCAGCAGCTGAGCAATGACCATATCTGCTACTTCCTCTACCAGATCCTGCGGGGCCTCAAGTACATCCACTCCGCCAACGTGCTCCACCGAGATCTAAAGCCCTCCAACCTGCTCATCAACACCACCTGCGACCTTAAGATTTGTGATTTCGGCCTGGCCCGGATTGCCGATCCTGAGCATGACCACACCGGCTTCCTGACGGAGTATGTGGCTACGCGCTGGTACCGGGCCCCAGAGATCATGCTGAACTCCAAGGGCTATACCAAGTCCATCGACATCTGGTCTGTGGGCTGCATTCTGGCTGAGATGCTCTCTAACCGGCCCATCTTCCCTGGCAAGCACTACCTGGATCAGCTCAACCACATTCTGGGCATCCTGGGCTCCCCATCCCAGGAGGACCTGAATTGTATCATCAACATGAAGGCCCGAAACTACCTACAGTCTCTGCCCTCCAAGACCAAGGTGGCTTGGGCCAAGCTTTTCCCCAAGTCAGACTCCAAAGCCCTTGACCTGCTGGACCGGATGTTAACCTTTAACCCCAATAAACGGATCACAGTGGAGGAAGCGCTGGCTCACCCCTACCTGGAGCAGTACTATGACCCGACGGATGAGCCAGTGGCCGAGGAGCCCTTCACCTTCGCCATGGAGCTGGATGACCTACCTAAGGAGCGGCTGAAGGAGCTCATCTTCCAGGAGACAGCACGCTTCCAGCCCGGAGTGCTGGAGGCCCCC</t>
+  </si>
+  <si>
+    <t>GEAPNQALLRILKETEFKKIKVLGSGAFGTVYKGLWIPEGEKVKIPVAIKELREATSPKANKEILDEAYVMASVDNPHVCRLLGICLTSTVQLITQLMPFGCLLDYVREHKDNIGSQYLLNWCVQIAKGMNYLEDRRLVHRDLAARNVLVKTPQHVKITDFGRAKLLGAEEKEYHAEGGKVPIKWMALESILHRIYTHQSDVWSYGVTVWELMTFGSKPYDGIPASEISSILEKGERLPQPPICTIDVYMIMVKCWMIDADSRPKFRELIIEFSKMARDPQRYLVIQGDERMHLPSPTDSNFYRALMDEEDMDDVVDADEYLIPQQG</t>
+  </si>
+  <si>
+    <t>aa_start</t>
+  </si>
+  <si>
+    <t>MSGPVPSRARVYTDVNTHRPREYWDYESHVVEWGNQDDYQLVRKLGRGKYSEVFEAINITNNEKVVVKILKPVKKKKIKREIKILENLRGGPNIITLADIVKDPVSRTPALVFEHVNNTDFKQLYQTLTDYDIRFYMYEILKALDYCHSMGIMHRDVKPHNVMIDHEHRKLRLIDWGLAEFYHPGQEYNVRVASRYFKGPELLVDYQMYDYSLDMWSLGCMLASMIFRKEPFFHGHDNYDQLVRIAKVLGTEDLYDYIDKYNIELDPRFNDILGRHSRKRWERFVHSENQHLVSPEALDFLDKLLRYDHQSRLTAREAMEHPYFYTVVKDQARMG</t>
+  </si>
+  <si>
+    <t>MAAAAAAGAGPEMVRGQVFDVGPRYTNLSYIGEGAYGMVCSAYDNVNKVRVAIKKISPFEHQTYCQRTLREIKILLRFRHENIIGINDIIRAPTIEQMKDVYIVQDLMETDLYKLLKTQHLSNDHICYFLYQILRGLKYIHSANVLHRDLKPSNLLLNTTCDLKICDFGLARVADPDHDHTGFLTEYVATRWYRAPEIMLNSKGYTKSIDIWSVGCILAEMLSNRPIFPGKHYLDQLNHILGILGSPSQEDLNCIINLKARNYLLSLPHKNKVPWNRLFPNADSKALDLLDKMLTFNPHKRIEVEQALAHPYLEQYYDPSDEPIAEAPFKFDMELDDLPKEKLKELIFEETARFQPGYRS</t>
   </si>
   <si>
     <t>GCAGGGGTCTCTGAGTATGAGCTTCCCGAAGACCCTCGCTGGGAGCTGCCTCGGGACAGACTGGTCTTAGGCAAACCCCTGGGAGAGGGCTGCTTTGGGCAGGTGGTGTTGGCAGAGGCTATCGGGCTGGACAAGGACAAACCCAACCGTGTGACCAAAGTGGCTGTGAAGATGTTGAAGTCGGACGCAACAGAGAAAGACTTGTCAGACCTGATCTCAGAAATGGAGATGATGAAGATGATCGGGAAGCATAAGAATATCATCAACCTGCTGGGGGCCTGCACGCAGGATGGTCCCTTGTATGTCATCGTGGAGTATGCCTCCAAGGGCAACCTGCGGGAGTACCTGCAGGCCCGGAGGCCCCCAGGGCTGGAATACTGCTACAACCCCAGCCACAACCCAGAGGAGCAGCTCTCCTCCAAGGACCTGGTGTCCTGCGCCTACCAGGTGGCCCGAGGCATGGAGTATCTGGCCTCCAAGAAGTGCATACACCGAGACCTGGCAGCCAGGAATGTCCTGGTGACAGAGGACAATGTGATGAAGATAGCAGACTTTGGCCTCGCACGGGACATTCACCACATCGACTACTATAAAAAGACAACCAACGGCCGACTGCCTGTGAAGTGGATGGCACCCGAGGCATTATTTGACCGGATCTACACCCACCAGAGTGATGTGTGGTCTTTCGGGGTGCTCCTGTGGGAGATCTTCACTCTGGGCGGCTCCCCATACCCCGGTGTGCCTGTGGAGGAACTTTTCAAGCTGCTGAAGGAGGGTCACCGCATGGACAAGCCCAGTAACTGCACCAACGAGCTGTACATGATGATGCGGGACTGCTGGCATGCAGTGCCCTCACAGAGACCCACCTTCAAGCAGCTGGTGGAAGACCTGGACCGCATCGTGGCCTTGACCTCCAACCAGGAGTACCTGGACCTGTCCATGCCCCTGGAC</t>
-  </si>
-  <si>
-    <t>GAAACAAAGTATACTGTGGACAAGAGGTTTGGCATGGATTTTAAAGAAATAGAATTAATTGGCTCAGGTGGATTTGGCCAAGTTTTCAAAGCAAAACACAGAATTGACGGAAAGACTTACGTTATTAAACGTGTTAAATATAATAACGAGAAGGCGGAGCGTGAAGTAAAAGCATTGGCAAAACTTGATCATGTAAATATTGTTCACTACAATGGCTGTTGGGATGGATTTGATTATGATCCTGAGACCAGTGATGATTCTCTTGAGAGCAGTGATTATGATCCTGAGAACAGCAAAAATAGTTCAAGGTCAAAGACTAAGTGCCTTTTCATCCAAATGGAATTCTGTGATAAAGGGACCTTGGAACAATGGATTGAAAAAAGAAGAGGCGAGAAACTAGACAAAGTTTTGGCTTTGGAACTCTTTGAACAAATAACAAAAGGGGTGGATTATATACATTCAAAAAAATTAATTCATAGAGATCTTAAGCCAAGTAATATATTCTTAGTAGATACAAAACAAGTAAAGATTGGAGACTTTGGACTTGTAACATCTCTGAAAAATGATGGAAAGCGAACAAGGAGTAAGGGAACTTTGCGATACATGAGCCCAGAACAGATTTCTTCGCAAGACTATGGAAAGGAAGTGGACCTCTACGCTTTGGGGCTAATTCTTGCTGAACTTCTTCATGTATGTGACACTGCTTTTGAAACATCAAAGTTTTTCACAGACCTACGGGATGGCATCATCTCAGATATATTTGATAAAAAAGAAAAAACTCTTCTACAGAAATTACTCTCAAAGAAACCTGAGGATCGACCTAACACATCTGAAATACTAAGGACCTTGACTGTGTGGAAGAAAAGCCCAGAGAAAAATGAACGACACACATGT</t>
-  </si>
-  <si>
-    <t>PAK7_HUMAN_D0_2F57_B</t>
-  </si>
-  <si>
-    <t>RDSSDDWEIPDGQITVGQRIGSGSFGTVYKGKWHGDVAVKMLNVTAPTPQQLQAFKNEVGVLRKTRHVNILLFMGYSTKPQLAIVTQWCEGSSLYHHLHIIETKFEMIKLIDIARQTAQGMDYLHAKSIIHRDLKSNNIFLHEDLTVKIGDFGLATVKSRWSGSHQFEQLSGSILWMAPEVIRMQDKNPYSFQSDVYAFGIVLYELMTGQLPYSNINNRDQIIFMVGRGYLSPDLSKVRSNCPKAMKRLMAECLKKKRDERPLFPQILASIELLAR</t>
-  </si>
-  <si>
-    <t>TYIPPGESLRDLIEQSQSSGSGSGLPLLVQRTIAKQIQMVKQIGKGRYGEVWMGKWRGEKVAVKVFFTTEEASWFRETEIYQTVLMRHENILGFIAADIKGTGSWTQLYLITDYHENGSLYDYLKSTTLDAKSMLKLAYSSVSGLCHLHTEIFSTQGKPAIAHRDLKSKNILVKKNGTCCIADLGLAVKFISDTNEVDIPPNTRVGTKRYMPPEVLDESLNRNHFQSYIMADMYSFGLILWEVARRCVSGGIVEEYQLPYHDLVPSDPSYEDMREIVCIKKLRPSFPNRWSSDECLRQMGKLMTECWAHNPASRLTALRVKKTLAKMSESQDIKL</t>
-  </si>
-  <si>
-    <t>GAGAACTTCCAAAAGGTGGAAAAGATCGGAGAGGGCACGTACGGAGTTGTGTACAAAGCCAGAAACAAGTTGACGGGAGAGGTGGTGGCGCTTAAGAAAATCCGCCTGGACACTGAGACTGAGGGTGTGCCCAGTACTGCCATCCGAGAGATCTCTCTGCTTAAGGAGCTTAACCATCCTAATATTGTCAAGCTGCTGGATGTCATTCACACAGAAAATAAACTCTACCTGGTTTTTGAATTTCTGCACCAAGATCTCAAGAAATTCATGGATGCCTCTGCTCTCACTGGCATTCCTCTTCCCCTCATCAAGAGCTATCTGTTCCAGCTGCTCCAGGGCCTAGCTTTCTGCCATTCTCATCGGGTCCTCCACCGAGACCTTAAACCTCAGAATCTGCTTATTAACACAGAGGGGGCCATCAAGCTAGCAGACTTTGGACTAGCCAGAGCTTTTGGAGTCCCTGTTCGTACTTACACCCATGAGGTGGTGACCCTGTGGTACCGAGCTCCTGAAATCCTCCTGGGCTGCAAATATTATTCCACAGCTGTGGACATCTGGAGCCTGGGCTGCATCTTTGCTGAGATGGTGACTCGCCGGGCCCTATTCCCTGGAGATTCTGAGATTGACCAGCTCTTCCGGATCTTTCGGACTCTGGGGACCCCAGATGAGGTGGTGTGGCCAGGAGTTACTTCTATGCCTGATTACAAGCCAAGTTTCCCCAAGTGGGCCCGGCAAGATTTTAGTAAAGTTGTACCTCCCCTGGATGAAGATGGACGGAGCTTGTTATCGCAAATGCTGCACTACGACCCTAACAAGCGGATTTCGGCCAAGGCAGCCCTGGCTCACCCTTTCTTCCAGGATGTGACCAAGCCAGTACCCCATCTT</t>
-  </si>
-  <si>
-    <t>GGGGAATGCAGTCAGAAGGGTCCTGTCCCCTTTAGCCATTGCCTTCCCACAGAAAAACTGCAACGCTGTGAGAAGATTGGGGAAGGGGTGTTTGGCGAAGTGTTTCAAACAATTGCTGATCACACACCCGTAGCCATAAAAATCATTGCTATTGAAGGACCAGATTTAGTCAATGGATCCCATCAGAAAACCTTTGAGGAAATCCTGCCAGAGATCATCATCTCCAAAGAGTTGAGCCTCTTATCCGGTGAAGTGTGCAACCGCACAGAAGGCTTTATCGGGCTGAACTCAGTGCACTGTGTCCAGGGATCTTACCCTCCCTTGCTCCTCAAAGCCTGGGATCACTATAATTCAACCAAAGGCTCTGCAAATGACCGGCCTGATTTTTTTAAAGACGACCAGCTCTTCATTGTGCTGGAATTTGAGTTTGGAGGGATTGACTTAGAGCAAATGCGAACCAAGTTGTCTTCCTTGGCTACTGCAAAGAGCATTCTACACCAGCTCACAGCCTCCCTCGCAGTGGCAGAGGCATCACTGCGCTTTGAGCACCGAGACTTACACTGGGGGAACGTGCTCTTAAAGAAAACCAGCCTCAAAAAACTCCACTACACCCTCAATGGGAAGAGCAGCACTATCCCCAGCTGTGGGTTGCAAGTGAGCATCATTGACTACACCCTGTCGCGCTTGGAACGGGATGGGATTGTGGTTTTCTGTGACGTTTCCATGGATGAGGACCTGTTTACCGGTGACGGTGACTACCAGTTTGACATCTACAGGCTCATGAAGAAGGAGAATAACAACCGCTGGGGTGAATATCACCCTTATAGTAATGTGCTCTGGTTACATTACCTGACAGACAAGATGCTGAAACAAATGACCTTCAAGACTAAATGTAACACTCCTGCCATGAAGCAAATTAAGAGAAAAATCCAGGAGTTCCACAGGACAATGCTGAACTTCAGCTCTGCCACTGACTTGCTCTGCCAGCACAGACTGTTTAAG</t>
-  </si>
-  <si>
-    <t>INSR_HUMAN_D0_1RQQ_A</t>
-  </si>
-  <si>
-    <t>TDSLPGKFEDMYKLTSELLGEGAYAKVQGAVSLQNGKEYAVKIIEKQAGHSRSRVFREVETLYQCQGNKNILELIEFFEDDTRFYLVFEKLQGGSILAHIQKQKHFNEREASRVVRDVAAALDFLHTKDKVSLCHLGGSARAPSGLTAAPTSLGSSDPPTSASQVAGTTGIDHRDLKPENILCESPEKVSPVKICDFDLGSGMKLNNSCTPITTPELTTPCGSAEYMAPEVGEVFTDQATFYDKRCDLWSLGVVLYIMLSGYPPFVGHCGADCGWDRGEVCRVCQNKLFESIQEGKYEFPDKDWAHISSEAKDLISKLLVRDAKQRLSAAQVLQHPWVQGQAPEKG</t>
-  </si>
-  <si>
-    <t>VRK3_HUMAN_D0_2JII_A</t>
-  </si>
-  <si>
-    <t>ATGAGCCTCATCCGGAAAAAGGGCTTCTACAAGCAGGACGTCAACAAGACCGCCTGGGAGCTGCCCAAGACCTACGTGTCCCCGACGCACGTCGGCAGCGGGGCCTATGGCTCCGTGTGCTCGGCCATCGACAAGCGGTCAGGGGAGAAGGTGGCCATCAAGAAGCTGAGCCGACCCTTTCAGTCCGAGATCTTCGCCAAGCGCGCCTACCGGGAGCTGCTGCTGCTGAAGCACATGCAGCATGAGAACGTCATTGGGCTCCTGGATGTCTTCACCCCAGCCTCCTCCCTGCGCAACTTCTATGACTTCTACCTGGTGATGCCCTTCATGCAGACGGATCTGCAGAAGATCATGGGGATGGAGTTCAGTGAGGAGAAGATCCAGTACCTGGTGTATCAGATGCTCAAAGGCCTTAAGTACATCCACTCTGCTGGGGTCGTGCACAGGGACCTGAAGCCAGGCAACCTGGCTGTGAATGAGGACTGTGAACTGAAGATTCTGGATTTTGGGCTGGCGCGACATGCAGACGCCGAGATGACTGGCTACGTGGTGACCCGCTGGTACCGAGCCCCCGAGGTGATCCTCAGCTGGATGCACTACAACCAGACAGTGGACATCTGGTCTGTGGTCTGTATCATGGCAGAGATGCTGACAGGGAAAACTCTGTTCAAGGGGAAAGATTACCTGGACCAGCTGACCCAGATCCTGAAAGTGACCGGGGTGCCTGGCACGGAGTTTGTGCAGAAGCTGAACGACAAAGCGGCCAAATCCTACATCCAGTCCCTGCCACAGACCCCCAGGAAGGATTTCACTCAGCTGTTCCCACGGGCCAGCCCCCAGGCTGCGGACCTGCTGGAGAAGATGCTGGAGCTAGACGTGGACAAGCGCCTGACGGCCGCGCAGGCCCTCACCCATCCCTTCTTTGAACCCTTCCGGGACCCTGAGGAAGAGACGGAGGCCCAGCAGCCGTTTGATGATTCCTTAGAACACGAGAAACTCACAGTGGATGAATGGAAGCAGCACATCTACAAGGAGATTGTGAACTTCAGCCCCATT</t>
-  </si>
-  <si>
-    <t>ACTGACTCCTTGCCAGGAAAGTTTGAAGATATGTACAAGCTGACCTCTGAATTGCTGGGAGAGGGAGCCTATGCCAAAGTTCAAGGTGCCGTGAGCCTACAGAATGGCAAAGAGTATGCCGTCAAAATCATCGAGAAACAAGCAGGGCACAGTCGGAGTAGGGTGTTTCGAGAGGTGGAGACGCTGTATCAGTGTCAGGGAAACAAGAACATTTTGGAGCTGATTGAGTTCTTTGAAGATGACACAAGGTTTTACTTGGTCTTTGAGAAATTGCAAGGAGGTTCCATCTTAGCCCACATCCAGAAGCAAAAGCACTTCAATGAGCGAGAAGCCAGCCGAGTGGTGCGGGACGTTGCTGCTGCCCTTGACTTCCTGCATACCAAAGACAAAGTCTCTCTCTGTCACCTAGGCGGGAGTGCTAGGGCGCCATCAGGGCTCACTGCAGCCCCAACCTCCCTGGGCTCCAGTGATCCTCCCACCTCAGCCTCCCAAGTAGCTGGGACTACAGGCATTGATCATCGTGATCTGAAACCAGAAAATATATTGTGTGAATCTCCAGAAAAGGTGTCTCCAGTGAAAATCTGTGACTTTGACTTGGGCAGTGGGATGAAACTGAACAACTCCTGTACCCCCATAACCACACCAGAGCTGACCACCCCATGTGGCTCTGCAGAATACATGGCCCCTGAGGTAGGGGAGGTCTTCACGGACCAGGCCACATTCTACGACAAGCGCTGTGACCTGTGGAGCCTGGGCGTGGTCCTCTACATCATGCTGAGTGGCTACCCACCCTTCGTGGGTCACTGCGGGGCCGACTGTGGCTGGGACCGGGGCGAGGTCTGCAGGGTGTGCCAGAACAAGCTGTTTGAAAGCATCCAGGAAGGCAAGTATGAGTTTCCTGACAAGGACTGGGCACACATCTCCAGTGAAGCCAAAGACCTCATCTCCAAGCTCCTGGTGCGAGATGCAAAGCAGAGACTTAGCGCCGCCCAAGTTCTGCAGCACCCATGGGTGCAGGGGCAAGCTCCAGAAAAGGGA</t>
-  </si>
-  <si>
-    <t>PAK4_HUMAN_D0_2J0I_A</t>
-  </si>
-  <si>
-    <t>ACTTACATTCCTCCTGGAGAATCCCTGAGAGACTTAATTGAGCAGTCTCAGAGCTCAGGAAGTGGATCAGGCCTCCCTCTGCTGGTCCAAAGGACTATAGCTAAGCAGATTCAGATGGTGAAACAGATTGGAAAAGGTCGCTATGGGGAAGTTTGGATGGGAAAGTGGCGTGGCGAAAAGGTAGCTGTGAAAGTGTTCTTCACCACAGAGGAAGCCAGCTGGTTCAGAGAGACAGAAATATATCAGACAGTGTTGATGAGGCATGAAAACATTTTGGGTTTCATTGCTGCAGATATCAAAGGGACAGGGTCCTGGACCCAGTTGTACCTAATCACAGACTATCATGAAAATGGTTCCCTTTATGATTATCTGAAGTCCACCACCCTAGACGCTAAATCAATGCTGAAGTTAGCCTACTCTTCTGTCAGTGGCTTATGTCATTTACACACAGAAATCTTTAGTACTCAAGGCAAACCAGCAATTGCCCATCGAGATCTGAAAAGTAAAAACATTCTGGTGAAGAAAAATGGAACTTGCTGTATTGCTGACCTGGGCCTGGCTGTTAAATTTATTAGTGATACAAATGAAGTTGACATACCACCTAACACTCGAGTTGGCACCAAACGCTATATGCCTCCAGAAGTGTTGGACGAGAGCTTGAACAGAAATCACTTCCAGTCTTACATCATGGCTGACATGTATAGTTTTGGCCTCATCCTTTGGGAGGTTGCTAGGAGATGTGTATCAGGAGGTATAGTGGAAGAATACCAGCTTCCTTATCATGACCTAGTGCCCAGTGACCCCTCTTATGAGGACATGAGGGAGATTGTGTGCATCAAGAAGTTACGCCCCTCATTCCCAAACCGGTGGAGCAGTGATGAGTGTCTAAGGCAGATGGGAAAACTCATGACAGAATGCTGGGCTCACAATCCTGCATCAAGGCTGACAGCCCTGCGGGTTAAGAAAACACTTGCCAAAATGTCAGAGTCCCAGGACATTAAACTC</t>
-  </si>
-  <si>
-    <t>AGVSEYELPEDPRWELPRDRLVLGKPLGEGCFGQVVLAEAIGLDKDKPNRVTKVAVKMLKSDATEKDLSDLISEMEMMKMIGKHKNIINLLGACTQDGPLYVIVEYASKGNLREYLQARRPPGLEYCYNPSHNPEEQLSSKDLVSCAYQVARGMEYLASKKCIHRDLAARNVLVTEDNVMKIADFGLARDIHHIDYYKKTTNGRLPVKWMAPEALFDRIYTHQSDVWSFGVLLWEIFTLGGSPYPGVPVEELFKLLKEGHRMDKPSNCTNELYMMMRDCWHAVPSQRPTFKQLVEDLDRIVALTSNQEYLDLSMPLD</t>
-  </si>
-  <si>
-    <t>MEPFKQQKVEDFYDIGEELGSGQFAIVKKCREKSTGLEYAAKFIKKRQSRASRRGVSREEIEREVSILRQVLHHNVITLHDVYENRTDVVLILELVSGGELFDFLAQKESLSEEEATSFIKQILDGVNYLHTKKIAHFDLKPENIMLLDKNIPIPHIKLIDFGLAHEIEDGVEFKNIFGTPEFVAPEIVNYEPLGLEADMWSIGVITYILLSGASPFLGDTKQETLANITAVSYDFDEEFFSQTSELAKDFIRKLLVKETRKRLTIQEALRHPWITPVDNQQAMVRRESVVNLENFRKQYVRRRWKLSFSIVSLCNHLTR</t>
-  </si>
-  <si>
-    <t>KCC1A_HUMAN_D0_4FG7_A</t>
-  </si>
-  <si>
-    <t>MAAAAAQGGGGGEPRRTEGVGPGVPGEVEMVKGQPFDVGPRYTQLQYIGEGAYGMVSSAYDHVRKTRVAIKKISPFEHQTYCQRTLREIQILLRFRHENVIGIRDILRASTLEAMRDVYIVQDLMETDLYKLLKSQQLSNDHICYFLYQILRGLKYIHSANVLHRDLKPSNLLINTTCDLKICDFGLARIADPEHDHTGFLTEYVATRWYRAPEIMLNSKGYTKSIDIWSVGCILAEMLSNRPIFPGKHYLDQLNHILGILGSPSQEDLNCIINMKARNYLQSLPSKTKVAWAKLFPKSDSKALDLLDRMLTFNPNKRITVEEALAHPYLEQYYDPTDEPVAEEPFTFAMELDDLPKERLKELIFQETARFQPGVLEAP</t>
-  </si>
-  <si>
-    <t>GAGCCCAAGAAGTACGCAGTGACCGACGACTACCAGTTGTCCAAGCAGGTGCTGGGCCTGGGTGTGAACGGCAAAGTGCTGGAGTGCTTCCATCGGCGCACTGGACAGAAGTGTGCCCTGAAGCTCCTGTATGACAGCCCCAAGGCCCGGCAGGAGGTAGACCATCACTGGCAGGCTTCTGGCGGCCCCCATATTGTCTGCATCCTGGATGTGTATGAGAACATGCACCATGGCAAGCGCTGTCTCCTCATCATCATGGAATGCATGGAAGGTGGTGAGTTGTTCAGCAGGATTCAGGAGCGTGGCGACCAGGCTTTCACTGAGAGAGAAGCTGCAGAGATAATGCGGGATATTGGCACTGCCATCCAGTTTCTGCACAGCCATAACATTGCCCACCGAGATGTCAAGCCTGAAAACCTACTCTACACATCTAAGGAGAAAGACGCAGTGCTTAAGCTCACCGATTTTGGCTTTGCTAAGGAGACCACCCAAAATGCCCTGCAGACACCCTGCTATACTCCCTATTATGTGGCCCCTGAGGTCCTGGGTCCAGAGAAGTATGACAAGTCATGTGACATGTGGTCCCTGGGTGTCATCATGTACATCCTCCTTTGTGGCTTCCCACCCTTCTACTCCAACACGGGCCAGGCCATCTCCCCGGGGATGAAGAGGAGGATTCGCCTGGGCCAGTACGGCTTCCCCAATCCTGAGTGGTCAGAAGTCTCTGAGGATGCCAAGCAGCTGATCCGCCTCCTGTTGAAGACAGACCCCACAGAGAGGCTGACCATCACTCAGTTCATGAACCACCCCTGGATCAACCAATCGATGGTAGTGCCACAGACCCCACTCCACACGGCCCGAGTGCTGCAGGAGGACAAAGACCACTGGGACGAAGTCAAGGAGGAGATGACCAGTGCCTTGGCCACTATGCGGGTAGACTACGACCAGGTG</t>
-  </si>
-  <si>
-    <t>IGF1R_HUMAN_D0_3O23_A</t>
-  </si>
-  <si>
-    <t>MK11_HUMAN_D0_3GC8_A</t>
-  </si>
-  <si>
-    <t>FAK2_HUMAN_D0_3ET7_A</t>
-  </si>
-  <si>
-    <t>CTGGACCGAAAGCTGCTGACGCTGGAAGACAAAGAACTGGGCTCTGGTAATTTTGGAACTGTGAAAAAGGGCTACTACCAAATGAAAAAAGTTGTGAAAACCGTGGCTGTGAAAATACTGAAAAACGAGGCCAATGACCCCGCTCTTAAAGATGAGTTATTAGCAGAAGCAAATGTCATGCAGCAGCTGGACAACCCGTACATCGTGCGCATGATCGGGATATGCGAGGCCGAGTCCTGGATGCTAGTTATGGAGATGGCAGAACTTGGTCCCCTCAATAAGTATTTGCAGCAGAACAGACATGTCAAGGATAAGAACATCATAGAACTGGTTCATCAGGTTTCCATGGGCATGAAGTACTTGGAGGAGAGCAATTTTGTGCACAGAGATCTGGCTGCAAGAAATGTGTTGCTAGTTACCCAACATTATGCCAAGATCAGTGATTTCGGACTCTCCAAAGCACTGCGTGCTGATGAAAACTACTACAAGGCCCAGACCCATGGAAAGTGGCCTGTCAAGTGGTACGCTCCGGAATGCATCAACTACTACAAGTTCTCCAGCAAAAGCGATGTCTGGAGCTTTGGAGTGTTGATGTGGGAAGCATTCTCCTATGGGCAGAAGCCATATCGAGGGATGAAAGGAAGTGAAGTCACCGCTATGTTAGAGAAAGGAGAGCGGATGGGGTGCCCTGCAGGGTGTCCAAGAGAGATGTACGATCTCATGAATCTGTGCTGGACATACGATGTGGAAAACAGGCCCGGATTCGCAGCAGTGGAACTGCGGCTGCGCAATTACTACTATGACGTGGTGAAC</t>
-  </si>
-  <si>
-    <t>CDK16_HUMAN_D0_3MTL_A</t>
-  </si>
-  <si>
-    <t>KS6A1_HUMAN_D0_3RNY_B</t>
-  </si>
-  <si>
-    <t>PLK1_HUMAN_D0_2V5Q_A</t>
-  </si>
-  <si>
-    <t>LEYDYEYDENGDRVVLGKGTYGIVYAGRDLSNQVRIAIKEIPERDSRYSQPLHEEIALHKHLKHKNIVQYLGSFSENGFIKIFMEQVPGGSLSALLRSKWGPLKDNEQTIGFYTKQILEGLKYLHDNQIVHRDIKGDNVLINTYSGVLKISDFGTSKRLAGINPCTETFTGTLQYMAPEIIDKGPRGYGKAADIWSLGCTIIEMATGKPPFYELGEPQAAMFKVGMFKVHPEIPESMSAEAKAFILKCFEPDPDKRACANDLLVDEFLK</t>
-  </si>
-  <si>
-    <t>KAPCA_HUMAN_D0_4AE9_A</t>
-  </si>
-  <si>
-    <t>PAK6_HUMAN_D0_2C30_A</t>
-  </si>
-  <si>
-    <t>MP2K6_HUMAN_D0_3VN9_A</t>
-  </si>
-  <si>
-    <t>KS6A5_HUMAN_D1_3KN6_A</t>
-  </si>
-  <si>
-    <t>FGFR1_HUMAN_D0_3GQL_B</t>
-  </si>
-  <si>
-    <t>TCTTCGGTCACCGCCAGTGCGGCCCCGGGGACCGCGAGCCTCGTCCCGGATTACTGGATCGACGGCTCCAACAGGGATGCGCTGAGCGATTTCTTCGAGGTGGAGTCGGAGCTGGGACGGGGTGCTACATCCATTGTGTACAGATGCAAACAGAAGGGGACCCAGAAGCCTTATGCTCTCAAAGTGTTAAAGAAAACAGTGGACAAAAAAATCGTAAGAACTGAGATAGGAGTTCTTCTTCGCCTCTCACATCCAAACATTATAAAACTTAAAGAGATATTTGAAACCCCTACAGAAATCAGTCTGGTCCTAGAACTCGTCACAGGAGGAGAACTGTTTGATAGGATTGTGGAAAAGGGATATTACAGTGAGCGAGATGCTGCAGATGCCGTTAAACAAATCCTGGAGGCAGTTGCTTATCTACATGAAAATGGGATTGTCCATCGTGATCTCAAACCAGAGAATCTTCTTTATGCAACTCCAGCCCCAGATGCACCACTCAAAATCGCTGATTTTGGACTCTCTAAAATTGTGGAACATCAAGTGCTCATGAAGACAGTATGTGGAACCCCAGGGTACTGCGCACCTGAAATTCTTAGAGGTTGTGCCTATGGACCTGAGGTGGACATGTGGTCTGTAGGAATAATCACCTACATCTTACTTTGTGGATTTGAACCATTCTATGATGAAAGAGGCGATCAGTTCATGTTCAGGAGAATTCTGAATTGTGAATATTACTTTATCTCCCCCTGGTGGGATGAAGTATCTCTAAATGCCAAGGACTTGGTCAGAAAATTAATTGTTTTGGATCCAAAGAAACGGCTGACTACATTTCAAGCTCTCCAGCATCCGTGGGTCACAGGTAAAGCAGCCAATTTTGTACACATGGATACCGCTCAAAAGAAGCTCCAAGAATTCAATGCCCGGCGTAAGCTTAAGGCAGCGGTGAAGGCTGTGGTGGCCTCTTCCCGCCTGGGA</t>
-  </si>
-  <si>
-    <t>MEAAASEPSLDLDNLKLLELIGRGRYGAVYKGSLDERPVAVKVFSFANRQNFINEKNIYRVPLMEHDNIARFIVGDERVTADGRMEYLLVMEYYPNGSLCKYLSLHTSDWVSSCRLAHSVTRGLAYLHTELPRGDHYKPAISHRDLNSRNVLVKNDGTCVISDFGLSMRLTGNRLVRPGEEDNAAISEVGTIRYMAPEVLEGAVNLRDCESALKQVDMYALGLIYWEIFMRCTDLFPGESVPEYQMAFQTEVGNHPTFEDMQVLVSREKQRPKFPEAWKENSLAVRSLKETIEDCWDQDAEARLTAQCAEERMAELMMIWERNKSVSPT</t>
-  </si>
-  <si>
-    <t>GTCATCATTGACAATAAGCGCTACCTCTTCATCCAGAAACTGGGGGAGGGTGGGTTCAGCTATGTGGACCTAGTGGAAGGGTTACATGATGGACACTTCTACGCCCTGAAGCGAATCCTGTGTCACGAGCAGCAGGACCGGGAGGAGGCCCAGCGAGAAGCCGACATGCATCGCCTCTTCAATCACCCCAACATCCTTCGCCTCGTGGCTTACTGTCTGAGGGAACGGGGTGCTAAGCATGAGGCCTGGCTGCTGCTACCATTCTTCAAGAGAGGTACGCTGTGGAATGAGATAGAAAGGCTGAAGGACAAAGGCAACTTCCTGACCGAGGATCAAATCCTTTGGCTGCTGCTGGGGATCTGCAGAGGCCTTGAGGCCATTCATGCCAAGGGTTATGCCCACAGAGACTTGAAGCCCACCAATATATTGCTTGGAGATGAGGGGCAGCCAGTTTTAATGGACTTGGGTTCCATGAATCAAGCATGCATCCATGTGGAGGGCTCCCGCCAGGCTCTGACCCTGCAGGACTGGGCAGCCCAGCGGTGCACCATCTCCTACCGAGCCCCAGAGCTCTTCTCTGTGCAGAGTCACTGTGTCATCGATGAGCGGACTGATGTCTGGTCCCTAGGCTGCGTGCTATATGCCATGATGTTTGGGGAAGGCCCTTATGACATGGTGTTCCAAAAGGGTGACAGTGTGGCCCTTGCTGTGCAGAACCAACTCAGCATCCCACAAAGCCCCAGGCATTCTTCAGCATTGTGGCAGCTCCTGAACTCGATGATGACCGTGGACCCGCATCAGCGTCCTCACATTCCTCTCCTCCTCAGTCAGCTGGAGGCGCTGCAG</t>
-  </si>
-  <si>
-    <t>BMPR2_HUMAN_D0_3G2F_A</t>
-  </si>
-  <si>
-    <t>dna_start</t>
-  </si>
-  <si>
-    <t>PHKG2_HUMAN_D0_2Y7J_D</t>
-  </si>
-  <si>
-    <t>MAPK2_HUMAN_D0_2JBO_A</t>
-  </si>
-  <si>
-    <t>ATGGAGAAGGACGGCCTGTGCCGCGCTGACCAGCAGTACGAATGCGTGGCGGAGATCGGGGAGGGCGCCTATGGGAAGGTGTTCAAGGCCCGCGACTTGAAGAACGGAGGCCGTTTCGTGGCGTTGAAGCGCGTGCGGGTGCAGACCGGCGAGGAGGGCATGCCGCTCTCCACCATCCGCGAGGTGGCGGTGCTGAGGCACCTGGAGACCTTCGAGCACCCCAACGTGGTCAGGTTGTTTGATGTGTGCACAGTGTCACGAACAGACAGAGAAACCAAACTAACTTTAGTGTTTGAACATGTCGATCAAGACTTGACCACTTACTTGGATAAAGTTCCAGAGCCTGGAGTGCCCACTGAAACCATAAAGGATATGATGTTTCAGCTTCTCCGAGGTCTGGACTTTCTTCATTCACACCGAGTAGTGCATCGCGATCTAAAACCACAGAACATTCTGGTGACCAGCAGCGGACAAATAAAACTCGCTGACTTCGGCCTTGCCCGCATCTATAGTTTCCAGATGGCTCTAACCTCAGTGGTCGTCACGCTGTGGTACAGAGCACCCGAAGTCTTGCTCCAGTCCAGCTACGCCACCCCCGTGGATCTCTGGAGTGTTGGCTGCATATTTGCAGAAATGTTTCGTAGAAAGCCTCTTTTTCGTGGAAGTTCAGATGTTGATCAACTAGGAAAAATCTTGGACGTGATTGGACTCCCAGGAGAAGAAGACTGGCCTAGAGATGTTGCCCTTCCCAGGCAGGCTTTTCATTCAAAATCTGCCCAACCAATTGAGAAGTTTGTAACAGATATCGATGAACTAGGCAAAGACCTACTTCTGAAGTGTTTGACATTTAACCCAGCCAAAAGAATATCTGCCTACAGTGCCCTGTCTCACCCATACTTCCAG</t>
-  </si>
-  <si>
-    <t>ATTCCGGAGGTGCAGAAGCCCCTGCATGAGCAGCTGTGGTACCACGGGGCCATCCCGAGGGCAGAGGTGGCTGAGCTGCTGGTGCACTCTGGGGACTTCCTGGTGCGGGAGAGCCAGGGCAAGCAGGAGTACGTGCTGTCGGTGCTGTGGGATGGTCTGCCCCGGCACTTCATCATCCAGTCCTTGGATAACCTGTACCGACTGGAAGGGGAAGGCTTTCCTAGCATTCCTTTGCTCATCGACCACCTACTGAGCACCCAGCAGCCCCTCACCAAGAAGAGTGGTGTTGTCCTGCACAGGGCTGTGCCCAAGGACAAGTGGGTGCTGAACCATGAGGACCTGGTGTTGGGTGAGCAGATTGGACGGGGGAACTTTGGCGAAGTGTTCAGCGGACGCCTGCGAGCCGACAACACCCTGGTGGCGGTGAAGTCTTGTCGAGAGACGCTCCCACCTGACCTCAAGGCCAAGTTTCTACAGGAAGCGAGGATCCTGAAGCAGTACAGCCACCCCAACATCGTGCGTCTCATTGGTGTCTGCACCCAGAAGCAGCCCATCTACATCGTCATGGAGCTTGTGCAGGGGGGCGACTTCCTGACCTTCCTCCGCACGGAGGGGGCCCGCCTGCGGGTGAAGACTCTGCTGCAGATGGTGGGGGATGCAGCTGCTGGCATGGAGTACCTGGAGAGCAAGTGCTGCATCCACCGGGACCTGGCTGCTCGGAACTGCCTGGTGACAGAGAAGAATGTCCTGAAGATCAGTGACTTTGGGATGTCCCGAGAGGAAGCCGATGGGGTCTATGCAGCCTCAGGGGGCCTCAGACAAGTCCCCGTGAAGTGGACCGCACCTGAGGCCCTTAACTACGGCCGCTACTCCTCCGAAAGCGACGTGTGGAGCTTTGGCATCTTGCTCTGGGAGACCTTCAGCCTGGGGGCCTCCCCCTATCCCAACCTCAGCAATCAGCAGACACGGGAGTTTGTGGAGAAGGGGGGCCGTCTGCCCTGCCCAGAGCTGTGTCCTGATGCCGTGTTCAGGCTCATGGAGCAGTGCTGGGCCTATGAGCCTGGGCAGCGGCCCAGCTTCAGCACCATCTACCAGGAGCTGCAGAGCATCCGAAAGCGGCATCGG</t>
-  </si>
-  <si>
-    <t>ATGTCGGGCCCTCGCGCCGGCTTCTACCGGCAGGAGCTGAACAAGACCGTGTGGGAGGTGCCGCAGCGGCTGCAGGGGCTGCGCCCGGTGGGCTCCGGCGCCTACGGCTCCGTCTGTTCGGCCTACGACGCCCGGCTGCGCCAGAAGGTGGCGGTGAAGAAGCTGTCGCGCCCCTTCCAGTCGCTGATCCACGCGCGCAGAACGTACCGGGAGCTGCGGCTGCTCAAGCACCTGAAGCACGAGAACGTCATCGGGCTTCTGGACGTCTTCACGCCGGCCACGTCCATCGAGGACTTCAGCGAAGTGTACTTGGTGACCACCCTGATGGGCGCCGACCTGAACAACATCGTCAAGTGCCAGGCGCTGAGCGACGAGCACGTTCAATTCCTGGTTTACCAGCTGCTGCGCGGGCTGAAGTACATCCACTCGGCCGGGATCATCCACCGGGACCTGAAGCCCAGCAACGTGGCTGTGAACGAGGACTGTGAGCTCAGGATCCTGGATTTCGGGCTGGCGCGCCAGGCGGACGAGGAGATGACCGGCTATGTGGCCACGCGCTGGTACCGGGCACCTGAGATCATGCTCAACTGGATGCATTACAACCAAACAGTGGATATCTGGTCCGTGGGCTGCATCATGGCTGAGCTGCTCCAGGGCAAGGCCCTCTTCCCGGGAAGCGACTACATTGACCAGCTGAAGCGCATCATGGAAGTGGTGGGCACACCCAGCCCTGAGGTTCTGGCAAAAATCTCCTCGGAACACGCCCGGACATATATCCAGTCCCTGCCCCCCATGCCCCAGAAGGACCTGAGCAGCATCTTCCGTGGAGCCAACCCCCTGGCCATAGACCTCCTTGGAAGGATGCTGGTGCTGGACAGTGACCAGAGGGTCAGTGCAGCTGAGGCACTGGCCCACGCCTACTTCAGCCAGTACCACGACCCCGAGGATGAGCCAGAGGCCGAGCCATATGATGAGAGCGTTGAGGCCAAGGAGCGCACGCTGGAGGAGTGGAAGGAGCTCACTTACCAGGAAGTCCTCAGCTTCAAGCCCCCAGAGCCACCGAAGCCACCTGGCAGCCTGGAGATTGAGCAG</t>
-  </si>
-  <si>
-    <t>E2AK2_HUMAN_D0_3UIU_A</t>
-  </si>
-  <si>
-    <t>FES_HUMAN_D0_3CBL_A</t>
-  </si>
-  <si>
-    <t>GeneID</t>
-  </si>
-  <si>
-    <t>BRAF_HUMAN_D0_4FK3_B</t>
-  </si>
-  <si>
-    <t>AVPFVEDWDLVQTLGEGAYGEVQLAVNRVTEEAVAVKIVDMKRAVDCPENIKKEICINKMLNHENVVKFYGHRREGNIQYLFLEYCSGGELFDRIEPDIGMPEPDAQRFFHQLMAGVVYLHGIGITHRDIKPENLLLDERDNLKISDFGLATVFRYNNRERLLNKMCGTLPYVAPELLKRREFHAEPVDVWSCGIVLTAMLAGELPWDQPSDSCQEYSDWKEKKTYLNPWKKIDSAPLALLHKILVENPSARITIPDIKKDRWYNKPL</t>
-  </si>
-  <si>
-    <t>ATGGATGAGCAATCACAAGGAATGCAAGGGCCACCTGTTCCTCAGTTCCAACCACAGAAGGCCTTACGACCGGATATGGGCTATAATACATTAGCCAACTTTCGAATAGAAAAGAAAATTGGTCGCGGACAATTTAGTGAAGTTTATAGAGCAGCCTGTCTCTTGGATGGAGTACCAGTAGCTTTAAAAAAAGTGCAGATATTTGATTTAATGGATGCCAAAGCACGTGCTGATTGCATCAAAGAAATAGATCTTCTTAAGCAACTCAACCATCCAAATGTAATAAAATATTATGCATCATTCATTGAAGATAATGAACTAAACATAGTTTTGGAACTAGCAGATGCTGGCGACCTATCCAGAATGATCAAGCATTTTAAGAAGCAAAAGAGGCTAATTCCTGAAAGAACTGTTTGGAAGTATTTTGTTCAGCTTTGCAGTGCATTGGAACACATGCATTCTCGAAGAGTCATGCATAGAGATATAAAACCAGCTAATGTGTTCATTACAGCCACTGGGGTGGTAAAACTTGGAGATCTTGGGCTTGGCCGGTTTTTCAGCTCAAAAACCACAGCTGCACATTCTTTAGTTGGTACGCCTTATTACATGTCTCCAGAGAGAATACATGAAAATGGATACAACTTCAAATCTGACATCTGGTCTCTTGGCTGTCTACTATATGAGATGGCTGCATTACAAAGTCCTTTCTATGGTGACAAAATGAATTTATACTCACTGTGTAAGAAGATAGAACAGTGTGACTACCCACCTCTTCCTTCAGATCACTATTCAGAAGAACTCCGACAGTTAGTTAATATGTGCATCAACCCAGATCCAGAGAAGCGACCAGACGTCACCTATGTTTATGACGTAGCAAAGAGGATGCATGCATGCACTGCAAGCAGC</t>
-  </si>
-  <si>
-    <t>DAPK3_HUMAN_D0_2J90_A</t>
-  </si>
-  <si>
-    <t>VKEFLAKAKEDFLKKWESPAQNTAHLDQFERIKTLGTGSFGRVMLVKHKETGNHYAMKILDKQKVVKLKQIEHTLNEKRILQAVNFPFLVKLEFSFKDNSNLYMVMEYVPGGEMFSHLRRIGRFSEPHARFYAAQIVLTFEYLHSLDLIYRDLKPENLLIDQQGYIQVTDFGFAKRVKGRTWTLCGTPEYLAPEIILSKGYNKAVDWWALGVLIYEMAAGYPPFFADQPIQIYEKIVSGKVRFPSHFSSDLKDLLRNLLQVDLTKRFGNLKNGVNDIKNHKWFATTDWIAIYQRKVEAPFIPKFKGPGDTSNFDDYEEEEIRVSINEKCGKEFSEF</t>
-  </si>
-  <si>
-    <t>TCCAGGGTGTCCCATGAACAGTTTCGGGCGGCCCTGCAGCTGGTGGTCAGCCCAGGAGACCCCAGGGAATACTTGGCCAACTTTATCAAAATCGGGGAAGGCTCAACCGGCATCGTATGCATCGCCACCGAGAAACACACAGGGAAACAAGTTGCAGTGAAGAAAATGGACCTCCGGAAGCAACAGAGACGAGAACTGCTTTTCAATGAGGTCGTGATCATGCGGGATTACCACCATGACAATGTGGTTGACATGTACAGCAGCTACCTTGTCGGCGATGAGCTCTGGGTGGTCATGGAGTTTCTAGAAGGTGGTGCCTTGACAGACATTGTGACTCACACCAGAATGAATGAAGAACAGATAGCTACTGTCTGCCTGTCAGTTCTGAGAGCTCTCTCCTACCTTCATAACCAAGGAGTGATTCACAGGGACATAAAAAGTGACTCCATCCTCCTGACAAGCGATGGCCGGATAAAGTTGTCTGATTTTGGTTTCTGTGCTCAAGTTTCCAAAGAGGTGCCGAAGAGGAAATCATTGGTTGGCACTCCCTACTGGATGGCCCCTGAGGTGATTTCTAGGCTACCTTATGGGACAGAGGTGGACATCTGGTCCCTCGGGATCATGGTGATAGAAATGATTGATGGCGAGCCCCCCTACTTCAATGAGCCTCCCCTCCAGGCGATGCGGAGGATCCGGGACAGTTTACCTCCAAGAGTGAAGGACCTACACAAGGTTTCTTCAGTGCTCCGGGGATTCCTAGACTTGATGTTGGTGAGGGAGCCCTCTCAGAGAGCAACAGCCCAGGAACTCCTCGGACATCCATTCTTAAAACTAGCAGGTCCACCGTCTTGCATTGTCCCCCTCATGAGACAATACAGGCATCAC</t>
-  </si>
-  <si>
-    <t>KSYK_HUMAN_D0_4F4P_A</t>
-  </si>
-  <si>
-    <t>KRQWALEDFEIGRPLGKGKFGNVYLAREKQSKFILALKVLFKAQLEKAGVEHQLRREVEIQSHLRHPNILRLYGYFHDATRVYLILEYAPLGTVYRELQKLSKFDEQRTATYITELANALSYCHSKRVIHRDIKPENLLLGSAGELKIADFGWSVHAPSSRRTTLCGTLDYLPPEMIEGRMHDEKVDLWSLGVLCYEFLVGKPPFEANTYQETYKRISRVEFTFPDFVTEGARDLISRLLKHNPSQRPMLREVLEHPWITANSSKPS</t>
-  </si>
-  <si>
-    <t>TTNVGDSTLADLLDHSCTSGSGSGLPFLVQRTVARQITLLECVGKGRYGEVWRGSWQGENVAVKIFSSRDEKSWFRETELYNTVMLRHENILGFIASDMTSRHSSTQLWLITHYHEMGSLYDYLQLTTLDTVSCLRIVLSIASGLAHLHIEIFGTQGKPAIAHRDLKSKNILVKKNGQCCIADLGLAVMHSQSTNQLDVGNNPRVGTKRYMAPEVLDETIQVDCFDSYKRVDIWAFGLVLWEVARRMVSNGIVEDYKPPFYDVVPNDPSFEDMRKVVCVDQQRPNIPNRWFSDPTLTSLAKLMKECWYQNPSARLTALRIKKTLTKID</t>
-  </si>
-  <si>
-    <t>SLK_HUMAN_D0_2JFL_A</t>
-  </si>
-  <si>
-    <t>SRVSHEQFRAALQLVVSPGDPREYLANFIKIGEGSTGIVCIATEKHTGKQVAVKKMDLRKQQRRELLFNEVVIMRDYHHDNVVDMYSSYLVGDELWVVMEFLEGGALTDIVTHTRMNEEQIATVCLSVLRALSYLHNQGVIHRDIKSDSILLTSDGRIKLSDFGFCAQVSKEVPKRKSLVGTPYWMAPEVISRLPYGTEVDIWSLGIMVIEMIDGEPPYFNEPPLQAMRRIRDSLPPRVKDLHKVSSVLRGFLDLMLVREPSQRATAQELLGHPFLKLAGPPSCIVPLMRQYRHH</t>
-  </si>
-  <si>
-    <t>TQTVHEFAKELDATNISIDKVVGAGEFGEVCSGRLKLPSKKEISVAIKTLKVGYTEKQRRDFLGEASIMGQFDHPNIIRLEGVVTKSKPVMIVTEYMENGSLDSFLRKHDAQFTVIQLVGMLRGIASGMKYLSDMGYVHRDLAARNILINSNLVCKVSDFGLSRVLEDDPEAAYTTRGGKIPIRWTSPEAIAYRKFTSASDVWSYGIVLWEVMSYGERPYWEMSNQDVIKAVDEGYRLPPPMDCPAALYQLMLDCWQKDRNNRPKFEQIVSILDKLIRNPGSLKIITSAAARPSNLLLDQSNVDITTFRTTGDWLNGVWTAHCKEIFTGVEYSSCDTIAKIS</t>
-  </si>
-  <si>
-    <t>NQFYSVEVGDSTFTVLKRYQNLKPIGSGAQGIVCAAYDAVLDRNVAIKKLSRPFQNQTHAKRAYRELVLMKCVNHKNIISLLNVFTPQKTLEEFQDVYLVMELMDANLCQVIQMELDHERMSYLLYQMLCGIKHLHSAGIIHRDLKPSNIVVKSDCTLKILDFGLARTAGTSFMMTPYVVTRYYRAPEVILGMGYKENVDIWSVGCIMGEMVRHKILFPGRDYIDQWNKVIEQLGTPCPEFMKKLQPTVRNYVENRPKYAGLTFPKLFPDSLFPADSEHNKLKASQARDLLSKMLVIDPAKRISVDDALQHPYINVWYDPAEVEAPPPQIYDKQLDEREHTIEEWKELIYKEVMN</t>
-  </si>
-  <si>
-    <t>QQFPQFHVKSGLQIKKNAIIDDYKVTSQVLGLGINGKVLQIFNKRTQEKFALKMLQDCPKARREVELHWRASQCPHIVRIVDVYENLYAGRKCLLIVMECLDGGELFSRIQDRGDQAFTEREASEIMKSIGEAIQYLHSINIAHRDVKPENLLYTSKRPNAILKLTDFGFAKETTSHNSLTTPCYTPYYVAPEVLGPEKYDKSCDMWSLGVIMYILLCGYPPFYSNHGLAISPGMKTRIRMGQYEFPNPEWSEVSEEVKMLIRNLLKTEPTQRMTITEFMNHPWIMQSTKVPQTPLHTSRVLKEDKERWEDVKGCLHDKNSDQA</t>
-  </si>
-  <si>
-    <t>CSK21_HUMAN_D0_3AXW_A</t>
-  </si>
-  <si>
-    <t>ATCTRFTDDYQLFEELGKGAFSVVRRCVKKTPTQEYAAKIINTKKLSARDHQKLEREARICRLLKHPNIVRLHDSISEEGFHYLVFDLVTGGELFEDIVAREYYSEADASHCIHQILESVNHIHQHDIVHRDLKPENLLLASKCKGAAVKLADFGLAIEVQGEQQAWFGFAGTPGYLSPEVLRKDPYGKPVDIWACGVILYILLVGYPPFWDEDQHKLYQQIKAGAYDFPSPEWDTVTPEAKNLINQMLTINPAKRITADQALKHPWVCQRSTVASMMHRQETVECLRKFNARRKLKGAILTTMLVSRNFS</t>
-  </si>
-  <si>
-    <t>VIDPSELTFVQEIGSGQFGLVHLGYWLNKDKVAIKTIREGAMSEEDFIEEAEVMMKLSHPKLVQLYGVCLEQAPICLVFEFMEHGCLSDYLRTQRGLFAAETLLGMCLDVCEGMAYLEEACVIHRDLAARNCLVGENQVIKVSDFGMTRFVLDDQYTSSTGTKFPVKWASPEVFSFSRYSSKSDVWSFGVLMWEVFSEGKIPYENRSNSEVVEDISTGFRLYKPRLASTHVYQIMNHCWKERPEDRPAFSRLLRQLAEIAESGL</t>
-  </si>
-  <si>
-    <t>CGTGTAAAAGCAGCTCAAGCTGGAAGACAGAGCTCTGCAAAGAGACATCTTGCAGAACAATTTGCAGTTGGAGAGATAATAACTGACATGGCAAAAAAGGAATGGAAAGTAGGATTACCCATTGGCCAAGGAGGCTTTGGCTGTATATATCTTGCTGATATGAATTCTTCAGAGTCAGTTGGCAGTGATGCACCTTGTGTTGTAAAAGTGGAACCCAGTGACAATGGACCTCTTTTTACTGAATTAAAGTTCTACCAACGAGCTGCAAAACCAGAGCAAATTCAGAAATGGATTCGTACCCGTAAGCTGAAGTACCTGGGTGTTCCTAAGTATTGGGGGTCTGGTCTACATGACAAAAATGGAAAAAGTTACAGGTTTATGATAATGGATCGCTTTGGGAGTGACCTTCAGAAAATATATGAAGCAAATGCCAAAAGGTTTTCTCGGAAAACTGTCTTGCAGCTAAGCTTAAGAATTCTGGATATTCTGGAATATATTCACGAGCATGAGTATGTGCATGGAGATATCAAGGCCTCAAATCTTCTTCTGAACTACAAGAATCCTGACCAGGTGTACTTGGTAGATTATGGCCTTGCTTATCGGTACTGCCCAGAAGGAGTTCATAAAGAATACAAAGAAGACCCCAAAAGATGTCACGATGGCACTATTGAATTCACGAGCATCGATGCACACAATGGCGTGGCCCCATCAAGACGTGGTGATTTGGAAATACTTGGTTATTGCATGATCCAATGGCTTACTGGCCATCTTCCTTGGGAGGATAATTTGAAAGATCCTAAATATGTTAGAGATTCCAAAATTAGATACAGAGAAAATATTGCAAGTTTGATGGACAAATGTTTTCCTGAGAAAAACAAACCAGGTGAAATTGCCAAATACATGGAAACAGTGAAATTACTAGACTACACTGAAAAACCTCTTTATGAAAATTTACGTGACATTCTTTTGCAAGGACTAAAAGCTATAGGAAGTAAGGATGATGGCAAATTGGACCTCAGTGTTGTGGAGAATGGAGGTTTGAAAGCAAAAACAATAACAAAGAAGCGAAAGAAAGAAATTGAAGAA</t>
-  </si>
-  <si>
-    <t>EHVRRDLDPNEVWEIVGELGDGAFGKVYKAKNKETGALAAAKVIETKSEEELEDYIVEIEILATCDHPYIVKLLGAYYHDGKLWIMIEFCPGGAVDAIMLELDRGLTEPQIQVVCRQMLEALNFLHSKRIIHRDLKAGNVLMTLEGDIRLADFGVSAKNLKTLQKRDSFIGTPYWMAPEVVMCETMKDTPYDYKADIWSLGITLIEMAQIEPPHHELNPMRVLLKIAKSDPPTLLTPSKWSVEFRDFLKIALDKNPETRPSAAQLLEHPFVSSITSNKALRELVAEAKAEVME</t>
-  </si>
-  <si>
-    <t>ACCGTGTTCAGGCAGGAAAACGTGGATGATTACTACGACACCGGCGAGGAACTTGGCAGTGGACAGTTTGCGGTTGTGAAGAAATGCCGTGAGAAAAGCACCGGCCTCCAGTATGCCGCCAAATTCATCAAGAAAAGGAGGACTAAGTCCAGCCGGCGGGGTGTGAGCCGCGAGGACATCGAGCGGGAGGTCAGCATCCTGAAGGAGATCCAGCACCCCAATGTCATCACCCTGCACGAGGTCTATGAGAACAAGACGGACGTCATCCTGATCTTGGAACTCGTTGCAGGTGGCGAGCTGTTTGACTTCTTAGCTGAAAAGGAATCTTTAACTGAAGAGGAAGCAACTGAATTTCTCAAACAAACTCTTAATGGTGTTTACTACCTGCACTCCCTTCAAATCGCCCACTTTGATCTTAAGCCTGAGAACATAATGCTTTTGGATAGAAATGTCCCCAAACCTCGGATCAAGATCATTGACTTTGGGTTGGCCCATAAAATTGACTTTGGAAATGAATTTAAAAACATATTTGGGACTCCAGAGTTTGTCGCTCCTGAGATAGTCAACTATGAACCTCTTGGTCTTGAGGCAGATATGTGGAGTATCGGGGTAATAACCTATATCCTCCTAAGTGGGGCCTCCCCATTTCTTGGAGACACTAAGCAAGAAACGTTAGCAAATGTATCCGCTGTCAACTACGAATTTGAGGATGAATACTTCAGTAATACCAGTGCCCTAGCCAAAGATTTCATAAGAAGACTTCTGGTCAAGGATCCAAAGAAGAGAATGACAATTCAAGATAGTTTGCAGCATCCCTGGATCAAGCCTAAAGATACACAACAGGCACTTAGT</t>
-  </si>
-  <si>
-    <t>CDK9_HUMAN_D0_4IMY_A</t>
-  </si>
-  <si>
-    <t>MK07_HUMAN_D0_4IC7_D</t>
-  </si>
-  <si>
-    <t>AGCGCTGCTGATGTGTACGTTCCTGATGAGTGGGAGGTGGCTCGGGAGAAGATCACCATGAGCCGGGAACTTGGGCAGGGGTCGTTTGGGATGGTCTATGAAGGAGTTGCCAAGGGTGTGGTGAAAGATGAACCTGAAACCAGAGTGGCCATTAAAACAGTGAACGAGGCCGCAAGCATGCGTGAGAGGATTGAGTTTCTCAACGAAGCTTCTGTGATGAAGGAGTTCAATTGTCACCATGTGGTGCGATTGCTGGGTGTGGTGTCCCAAGGCCAGCCAACACTGGTCATCATGGAACTGATGACACGGGGCGATCTCAAAAGTTATCTCCGGTCTCTGAGGCCAGAAATGGAGAATAATCCAGTCCTAGCACCTCCAAGCCTGAGCAAGATGATTCAGATGGCCGGAGAGATTGCAGACGGCATGGCATACCTCAACGCCAATAAGTTCGTCCACAGAGACCTTGCTGCCCGGAATTGCATGGTAGCCGAAGATTTCACAGTCAAAATCGGAGATTTTGGTATGACGCGAGATATCTATGAGACAGACTATTACCGGAAAGGAGGGAAAGGGCTGCTGCCCGTGCGCTGGATGTCTCCTGAGTCCCTCAAGGATGGAGTCTTCACCACTTACTCGGACGTCTGGTCCTTCGGGGTCGTCCTCTGGGAGATCGCCACACTGGCCGAGCAGCCCTACCAGGGCTTGTCCAACGAGCAAGTCCTTCGCTTCGTCATGGAGGGCGGCCTTCTGGACAAGCCAGACAACTGTCCTGACATGCTGTTTGAACTGATGCGCATGTGCTGGCAGTATAACCCCAAGATGAGGCCTTCCTTCCTGGAGATCATCAGCAGCATCAAAGAGGAGATGGAGCCTGGCTTCCGGGAGGTCTCCTTCTACTACAGCGAGGAGAACAAG</t>
-  </si>
-  <si>
-    <t>RVKAAQAGRQSSAKRHLAEQFAVGEIITDMAKKEWKVGLPIGQGGFGCIYLADMNSSESVGSDAPCVVKVEPSDNGPLFTELKFYQRAAKPEQIQKWIRTRKLKYLGVPKYWGSGLHDKNGKSYRFMIMDRFGSDLQKIYEANAKRFSRKTVLQLSLRILDILEYIHEHEYVHGDIKASNLLLNYKNPDQVYLVDYGLAYRYCPEGVHKEYKEDPKRCHDGTIEFTSIDAHNGVAPSRRGDLEILGYCMIQWLTGHLPWEDNLKDPKYVRDSKIRYRENIASLMDKCFPEKNKPGEIAKYMETVKLLDYTEKPLYENLRDILLQGLKAIGSKDDGKLDLSVVENGGLKAKTITKKRKKEIEE</t>
-  </si>
-  <si>
-    <t>VFPCSVYVPDEWEVSREKITLLRELGQGSFGMVYEGNARDIIKGEAETRVAVKTVNESASLRERIEFLNEASVMKGFTCHHVVRLLGVVSKGQPTLVVMELMAHGDLKSYLRSLRPEAENNPGRPPPTLQEMIQMAAEIADGMAYLNAKKFVHRDLAARNCMVAHDFTVKIGDFGMTRDIYETDYYRKGGKGLLPVRWMAPESLKDGVFTTSSDMWSFGVVLWEITSLAEQPYQGLSNEQVLKFVMDGGYLDQPDNCPERVTDLMRMCWQFNPKMRPTFLEIVNLLKDDLHPSFPEVSFFHSEENK</t>
-  </si>
-  <si>
-    <t>MKNK1_HUMAN_D0_2HW6_B</t>
-  </si>
-  <si>
-    <t>AAAAACAACCCAGATCCTACAATTTATCCAGTGCTTGACTGGAATGACATCAAATTTCAAGATGTGATTGGGGAGGGCAATTTTGGCCAAGTTCTTAAGGCGCGCATCAAGAAGGATGGGTTACGGATGGATGCTGCCATCAAAAGAATGAAAGAATATGCCTCCAAAGATGATCACAGGGACTTTGCAGGAGAACTGGAAGTTCTTTGTAAACTTGGACACCATCCAAACATCATCAATCTCTTAGGAGCATGTGAACATCGAGGCTACTTGTACCTGGCCATTGAGTACGCGCCCCATGGAAACCTTCTGGACTTCCTTCGCAAGAGCCGTGTGCTGGAGACGGACCCAGCATTTGCCATTGCCAATAGCACCGCGTCCACACTGTCCTCCCATCATCTCCTTCACTTCGCTGCCGACGTGGCCCGGGGCATGGACTACTTGAGCCAAAAACAGTTTATCCACAGGGATCTGGCTGCCAGAAACATTTTAGTTGGTGAAAACTATGTGGCAAAAATAGCAGATTTTGGATTGTCCCGAGGTCAAGAGGTGTATGTGAAAAAGACAATGGGAAGGCTCCCAGTGCGCTGGATGGCCATCGAGTCACTGAATTACAGTGTGTACACAACCAACAGTGATGTATGGTCCTATGGTGTGTTACTATGGGAGATTGTTAGCTTAGGAGGCACACCCTACTGCGGGATGACTTGTGCAGAACTCTACGAGAAGCTGCCCCAGGGCTACAGACTGGAGAAGCCCCTGAACTGTGATGATGAGGTGTATGATCTAATGAGACAATGCTGGCGGGAGAAGCCTTATGAGAGGCCATCATTTGCCCAGATATTGGTGTCCTTAAACAGAATGTTAGAGGAGCGAAAGACCTACGTGAATACCACGCTTTATGAGAAGTTTACTTATGCAGGAATTGACTGTTCTGCTGAAGAAGCGGCC</t>
-  </si>
-  <si>
-    <t>MSLIRKKGFYKQDVNKTAWELPKTYVSPTHVGSGAYGSVCSAIDKRSGEKVAIKKLSRPFQSEIFAKRAYRELLLLKHMQHENVIGLLDVFTPASSLRNFYDFYLVMPFMQTDLQKIMGMEFSEEKIQYLVYQMLKGLKYIHSAGVVHRDLKPGNLAVNEDCELKILDFGLARHADAEMTGYVVTRWYRAPEVILSWMHYNQTVDIWSVVCIMAEMLTGKTLFKGKDYLDQLTQILKVTGVPGTEFVQKLNDKAAKSYIQSLPQTPRKDFTQLFPRASPQAADLLEKMLELDVDKRLTAAQALTHPFFEPFRDPEEETEAQQPFDDSLEHEKLTVDEWKQHIYKEIVNFSPI</t>
-  </si>
-  <si>
-    <t>KNNPDPTIYPVLDWNDIKFQDVIGEGNFGQVLKARIKKDGLRMDAAIKRMKEYASKDDHRDFAGELEVLCKLGHHPNIINLLGACEHRGYLYLAIEYAPHGNLLDFLRKSRVLETDPAFAIANSTASTLSSHHLLHFAADVARGMDYLSQKQFIHRDLAARNILVGENYVAKIADFGLSRGQEVYVKKTMGRLPVRWMAIESLNYSVYTTNSDVWSYGVLLWEIVSLGGTPYCGMTCAELYEKLPQGYRLEKPLNCDDEVYDLMRQCWREKPYERPSFAQILVSLNRMLEERKTYVNTTLYEKFTYAGIDCSAEEAA</t>
-  </si>
-  <si>
-    <t>AAPPAKEIPEVLVDPRSRRRYVRGRFLGKGGFAKCFEISDADTKEVFAGKIVPKSLLLKPHQREKMSMEISIHRSLAHQHVVGFHGFFEDNDFVFVVLELCRRRSLLELHKRRKALTEPEARYYLRQIVLGCQYLHRNRVIHRDLKLGNLFLNEDLEVKIGDFGLATKVEYDGERKKTLCGTPNYIAPEVLSKKGHSFEVDVWSIGCIMYTLLVGKPPFETSCLKETYLRIKKNEYSIPKHINPVAASLIQKMLQTDPTARPTINELLNDEFFTSGYIPARLPITCLTIPPRFSIAPSSLDPSNRKPLTVLNK</t>
-  </si>
-  <si>
-    <t>ITK_HUMAN_D0_3QGW_B</t>
-  </si>
-  <si>
-    <t>STK24_HUMAN_D0_3ZHP_C</t>
-  </si>
-  <si>
-    <t>KS6A3_HUMAN_D1_4JG7_A</t>
-  </si>
-  <si>
-    <t>KCC4_HUMAN_D0_2W4O_A</t>
-  </si>
-  <si>
-    <t>CSK_HUMAN_D0_3D7T_A</t>
-  </si>
-  <si>
-    <t>KCC2A_HUMAN_D0_2VZ6_B</t>
-  </si>
-  <si>
-    <t>CAGAGCAGTAAGCGCAGCAGCCGGAGTGTGGAAGATGACAAGGAGGGTCACCTGGTGTGCCGGATCGGCGATTGGCTCCAAGAGCGATATGAGATTGTGGGGAACCTGGGTGAAGGCACCTTTGGCAAGGTGGTGGAGTGCTTGGACCATGCCAGAGGGAAGTCTCAGGTTGCCCTGAAGATCATCCGCAACGTGGGCAAGTACCGGGAGGCTGCCCGGCTAGAAATCAACGTGCTCAAAAAAATCAAGGAGAAGGACAAAGAAAACAAGTTCCTGTGTGTCTTGATGTCTGACTGGTTCAACTTCCACGGTCACATGTGCATCGCCTTTGAGCTCCTGGGCAAGAACACCTTTGAGTTCCTGAAGGAGAATAACTTCCAGCCTTACCCCCTACCACATGTCCGGCACATGGCCTACCAGCTCTGCCACGCCCTTAGATTTCTGCATGAGAATCAGCTGACCCATACAGACTTGAAACCAGAGAACATCCTGTTTGTGAATTCTGAGTTTGAAACCCTCTACAATGAGCACAAGAGCTGTGAGGAGAAGTCAGTGAAGAACACCAGCATCCGAGTGGCTGACTTTGGCAGTGCCACATTTGACCATGAGCACCACACCACCATTGTGGCCACCCGTCACTATCGCCCGCCTGAGGTGATCCTTGAGCTGGGCTGGGCACAGCCCTGTGACGTCTGGAGCATTGGCTGCATTCTCTTTGAGTACTACCGGGGCTTCACACTCTTCCAGACCCACGAAAACCGAGAGCACCTGGTGATGATGGAGAAGATCCTAGGGCCCATCCCATCACACATGATCCACCGTACCAGGAAGCAGAAATATTTCTACAAAGGGGGCCTAGTTTGGGATGAGAACAGCTCTGACGGCCGGTATGTGAAGGAGAACTGCAAACCTCTGAAGAGTTACATGCTCCAAGACTCCCTGGAGCACGTGCAGCTGTTTGACCTGATGAGGAGGATGTTAGAATTTGACCCTGCCCAGCGCATCACACTGGCCGAGGCCCTGCTGCACCCCTTCTTTGCTGGCCTGACCCCTGAGGAGCGGTCCTTCCACACC</t>
-  </si>
-  <si>
-    <t>ATGTCTGATGAGGAGATCTTGGAGAAATTACGAAGCATAGTGAGTGTGGGCGATCCTAAGAAGAAATATACACGGTTTGAGAAGATTGGACAAGGTGCTTCAGGCACCGTGTACACAGCAATGGATGTGGCCACAGGACAGGAGGTGGCCATTAAGCAGATGAATCTTCAGCAGCAGCCCAAGAAAGAGCTGATTATTAATGAGATCCTGGTCATGAGGGAAAACAAGAACCCAAACATTGTGAATTACTTGGACAGTTACCTCGTGGGAGATGAGCTGTGGGTTGTTATGGAATACTTGGCTGGAGGCTCCTTGACAGATGTGGTGACAGAAACTTGCATGGATGAAGGCCAAATTGCAGCTGTGTGCCGTGAGTGTCTGCAGGCTCTGGAGTTCTTGCATTCGAACCAGGTCATTCACAGAGACATCAAGAGTGACAATATTCTGTTGGGAATGGATGGCTCTGTCAAGCTAACTGACTTTGGATTCTGTGCACAGATAACCCCAGAGCAGAGCAAACGGAGCACCATGGTAGGAACCCCATACTGGATGGCACCAGAGGTTGTGACACGAAAGGCCTATGGGCCCAAGGTTGACATCTGGTCCCTGGGCATCAAGGCCATCGAAATGATTGAAGGGGAGCCTCCATACCTCAATGAAAACCCTCTGAGAGCCTTGTACCTCATTGCCACCAATGGGACCCCAGAACTTCAGAACCCAGAGAAGCTGTCAGCTATCTTCCGGGACTTTCTGAACCGCTGTCTCGAGATGGATGTGGAGAAGAGAGGTTCAGCTAAAGAGCTGCTACAGCATCAATTCCTGAAGATTGCCAAGCCCCTCTCCAGCCTCACTCCACTTATTGCTGCAGCTAAGGAGGCAACAAAGAACAATCAC</t>
-  </si>
-  <si>
-    <t>expression tag location</t>
-  </si>
-  <si>
-    <t>ATGGAGGCAGCAGCATCCGAACCCTCTCTTGATCTAGATAATCTGAAACTGTTGGAGCTGATTGGCCGAGGTCGATATGGAGCAGTATATAAAGGCTCCTTGGATGAGCGTCCAGTTGCTGTAAAAGTGTTTTCCTTTGCAAACCGTCAGAATTTTATCAACGAAAAGAACATTTACAGAGTGCCTTTGATGGAACATGACAACATTGCCCGCTTTATAGTTGGAGATGAGAGAGTCACTGCAGATGGACGCATGGAATATTTGCTTGTGATGGAGTACTATCCCAATGGATCTTTATGCAAGTATTTAAGTCTCCACACAAGTGACTGGGTAAGCTCTTGCCGTCTTGCTCATTCTGTTACTAGAGGACTGGCTTATCTTCACACAGAATTACCACGAGGAGATCATTATAAACCTGCAATTTCCCATCGAGATTTAAACAGCAGAAATGTCCTAGTGAAAAATGATGGAACCTGTGTTATTAGTGACTTTGGACTGTCCATGAGGCTGACTGGAAATAGACTGGTGCGCCCAGGGGAGGAAGATAATGCAGCCATAAGCGAGGTTGGCACTATCAGATATATGGCACCAGAAGTGCTAGAAGGAGCTGTGAACTTGAGGGACTGTGAATCAGCTTTGAAACAAGTAGACATGTATGCTCTTGGACTAATCTATTGGGAGATATTTATGAGATGTACAGACCTCTTCCCAGGGGAATCCGTACCAGAGTACCAGATGGCTTTTCAGACAGAGGTTGGAAACCATCCCACTTTTGAGGATATGCAGGTTCTCGTGTCTAGGGAAAAACAGAGACCCAAGTTCCCAGAAGCCTGGAAAGAAAATAGCCTGGCAGTGAGGTCACTCAAGGAGACAATCGAAGACTGTTGGGACCAGGATGCAGAGGCTCGGCTTACTGCACAGTGTGCTGAGGAAAGGATGGCTGAACTTATGATGATTTGGGAAAGAAACAAATCTGTGAGCCCAACA</t>
-  </si>
-  <si>
-    <t>GGAGAAGCTCCCAACCAAGCTCTCTTGAGGATCTTGAAGGAAACTGAATTCAAAAAGATCAAAGTGCTGGGCTCCGGTGCGTTCGGCACGGTGTATAAGGGACTCTGGATCCCAGAAGGTGAGAAAGTTAAAATTCCCGTCGCTATCAAGGAATTAAGAGAAGCAACATCTCCGAAAGCCAACAAGGAAATCCTCGATGAAGCCTACGTGATGGCCAGCGTGGACAACCCCCACGTGTGCCGCCTGCTGGGCATCTGCCTCACCTCCACCGTGCAaCTCATCACGCAGCTCATGCCCTTCGGCTGCCTCCTGGACTATGTCCGGGAACACAAAGACAATATTGGCTCCCAGTACCTGCTCAACTGGTGTGTGCAGATCGCAAAGGGCATGAACTACTTGGAGGACCGTCGCTTGGTGCACCGCGACCTGGCAGCCAGGAACGTACTGGTGAAAACACCGCAGCATGTCAAGATCACAGATTTTGGGCgGGCCAAACTGCTGGGTGCGGAAGAGAAAGAATACCATGCAGAAGGAGGCAAAGTGCCTATCAAGTGGATGGCATTGGAATCAATTTTACACAGAATCTATACCCACCAGAGTGATGTCTGGAGCTACGGGGTGACCGTTTGGGAGTTGATGACCTTTGGATCCAAGCCATATGACGGAATCCCTGCCAGCGAGATCTCCTCCATCCTGGAGAAAGGAGAACGCCTCCCTCAGCCACCCATATGTACCATCGATGTCTACATGATCATGGTCAAGTGCTGGATGATAGACGCAGATAGTCGCCCAAAGTTCCGTGAGTTGATCATCGAATTCTCCAAAATGGCCCGAGACCCCCAGCGCTACCTTGTCATTCAGGGGGATGAAAGAATGCATTTGCCAAGTCCTACAGACTCCAACTTCTACCGTGCCCTGATGGATGAAGAAGACATGGACGACGTGGTGGATGCCGACGAGTACCTCATCCCACAGCAGGGC</t>
-  </si>
-  <si>
-    <t>KS6A5_HUMAN_D0_3KN6_A</t>
-  </si>
-  <si>
-    <t>GAGACCTACATTAAGCTGGACAAACTGGGCGAGGGTACCTATGCCACCGTCTACAAAGGCAAAAGCAAGCTCACAGACAACCTTGTGGCACTCAAGGAGATCAGACTGGAACATGAAGAGGGGGCACCCTGCACCGCCATCCGGGAAGTGTCCCTACTCAAGGACCTCAAACACGCCAACATCGTTACGCTACATGACATTATCCACACGGAGAAGTCCCTCACCCTTGTCTTTGAGTACCTGGACAAGGACCTGAAGCAGTACCTGGATGACTGTGGGAACATCATCAACATGCACAACGTGAAACTGTTCCTGTTCCAGCTGCTCCGTGGCCTGGCCTACTGCCACCGGCAGAAGGTGCTACACCGAGACCTCAAGCCCCAGAACCTGCTCATCAACGAGAGGGGAGAGCTCAAGCTGGCTGACTTTGGCCTGGCCCGAGCCAAGTCAATCCCAACAAAGACATACTCCAATGAGGTGGTGACACTGTGGTACCGGCCCCCTGACATCCTGCTTGGGTCCACGGACTACTCCACTCAGATTGACATGTGGGGTGTGGGCTGCATCTTCTATGAGATGGCCACAGGCCGTCCCCTCTTTCCGGGCTCCACGGTGGAGGAACAGCTACACTTCATCTTCCGTATCTTAGGAACCCCAACTGAGGAGACGTGGCCAGGCATCCTGTCCAACGAGGAGTTCAAGACATACAACTACCCCAAGTACCGAGCCGAGGCCCTTTTGAGCCACGCACCCCGACTTGATAGCGACGGGGCCGACCTCCTCACCAAGCTGTTGCAGTTTGAGGGTCGAAATCGGATCTCCGCAGAGGATGCCATGAAACATCCATTCTTCCTCAGTCTGGGGGAGCGGATCCACAAACTTCCTGACACTACTTCCATATTTGCACTAAAGGAGATTCAGCTACAAAAGGAGGCCAGCCTTCGGTCT</t>
-  </si>
-  <si>
-    <t>MK13_HUMAN_D0_4EYJ_A</t>
-  </si>
-  <si>
-    <t>STK16_HUMAN_D0_2BUJ_B</t>
-  </si>
-  <si>
-    <t>AAGCACGACGGGCGGGTGAAGATCGGACACTACGTGCTGGGCGACACGCTGGGCGTCGGCACCTTCGGCAAAGTGAAGATTGGAGAACATCAATTAACAGGCCATAAAGTGGCAGTTAAAATCTTAAATAGACAGAAGATTCGCAGTTTAGATGTTGTTGGAAAAATAAAACGAGAAATTCAAAATCTAAAACTCTTTCGTCATCCTCATATTATCAAACTATACCAGGTGATCAGCACTCCAACAGATTTTTTTATGGTAATGGAATATGTGTCTGGAGGTGAATTATTTGACTACATCTGTAAGCATGGACGGGTTGAAGAGATGGAAGCCAGGCGRCTCTTTCAGCAGATTCTGTCTGCTGTGGATTACTGTCATAGGCATATGGTTGTTCATCGAGACCTGAAACCAGAGAATGTCCTGTTGGATGCACACATGAATGCCAAGATAGCCGATTTCGGATTATCTAATATGATGTCAGATGGTGAATTTCTGAGAACTAGTTGCGGATCTCCAAATTATGCAGCACCTGAAGTCATCTCAGGCAGATTGTATGCAGGTCCTGAAGTTGATATCTGGAGCTGTGGTGTTATCTTGTATGCTCTTCTTTGTGGCACCCTCCCATTTGATGATGAGCATGTACCTACGTTATTTAAGAAGATCCGAGGGGGTGTCTTTTATATCCCAGAATATCTCAATCGTTCTGTCGCCACTCTCCTGATGCATATGCTGCAGGTTGACCCACTGAAACGAGCAACTATCAAAGACATAAGAGAGCATGAATGGTTTAAACAAGATTTGCCCAGTTACTTATTTCCTGAA</t>
-  </si>
-  <si>
-    <t>NEK7_HUMAN_D0_2WQN_A</t>
-  </si>
-  <si>
-    <t>ATGCTGGGGGCAGTGGAAGGCCCCAGGTGGAAGCAGGCGGAGGACATTAGAGACATCTACGACTTCCGAGATGTTCTGGGCACGGGGGCCTTCTCGGAGGTGATCCTGGCAGAAGATAAGAGGACGCAGAAGCTGGTGGCCATCAAATGCATTGCCAAGGAGGCCCTGGAGGGCAAGGAAGGCAGCATGGAGAATGAGATTGCTGTCCTGCACAAGATCAAGCACCCCAACATTGTAGCCCTGGATGACATCTATGAGAGTGGGGGCCACCTCTACCTCATCATGCAGCTGGTGTCGGGTGGGGAGCTCTTTGACCGTATTGTGGAAAAAGGCTTCTACACGGAGCGGGACGCCAGCCGCCTCATCTTCCAGGTGCTGGATGCTGTGAAATACCTGCATGACCTGGGCATTGTACACCGGGATCTCAAGCCAGAGAATCTGCTGTACTACAGCCTGGATGAAGACTCCAAAATCATGATCTCCGACTTTGGCCTCTCCAAGATGGAGGACCCGGGCAGTGTGCTCTCCACCGCCTGTGGAACTCCGGGATACGTGGCCCCTGAAGTCCTGGCCCAGAAGCCCTACAGCAAGGCTGTGGATTGCTGGTCCATAGGTGTCATCGCCTACATCTTGCTCTGCGGTTACCCTCCCTTCTATGACGAGAATGATGCCAAACTCTTTGAACAGATTTTGAAGGCCGAGTACGAGTTTGACTCTCCTTACTGGGACGACATCTCTGACTCTGCCAAAGATTTCATCCGGCACTTGATGGAGAAGGACCCAGAGAAAAGATTCACCTGTGAGCAGGCCTTGCAGCACCCATGGATTGCAGGAGATACAGCTCTAGATAAGAATATCCACCAGTCGGTGAGTGAGCAG</t>
-  </si>
-  <si>
-    <t>CAGAAGGTGATGGAGAATAGCAGTGGGACACCCGACATCTTAACGCGGCACTTCACAATTGATGACTTTGAGATTGGGCGTCCTCTGGGCAAAGGCAAGTTTGGAAACGTGTACTTGGCTCGGGAGAAGAAAAGCCATTTCATCGTGGCGCTCAAGGTCCTCTTCAAGTCCCAGATAGAGAAGGAGGGCGTGGAGCATCAGCTGCGCAGAGAGATCGAAATCCAGGCCCACCTGCACCATCCCAACATCCTGCGTCTCTACAACTATTTTTATGACCGGAGGAGGATCTACTTGATTCTAGAGTATGCCCCCCGCGGGGAGCTCTACAAGGAGCTGCAGAAGAGCTGCACATTTGACGAGCAGCGAACAGCCACGATCATGGAGGAGTTGGCAGATGCTCTAATGTACTGCCATGGGAAGAAGGTGATTCACAGAGACATAAAGCCAGAAAATCTGCTCTTAGGGCTCAAGGGAGAGCTGAAGATTGCTGACTTCGGCTGGTCTGTGCATGCGCCCTCCCTGAGGAGGAAGACAATGTGTGGCACCCTGGACTACCTGCCCCCAGAGATGATTGAGGGGCGCATGCACAATGAGAAGGTGGATCTGTGGTGCATTGGAGTGCTTTGCTATGAGCTGCTGGTGGGGAACCCACCCTTTGAGAGTGCATCACACAACGAGACCTATCGCCGCATCGTCAAGGTGGACCTAAAGTTCCCCGCTTCTGTGCCCACGGGAGCCCAGGACCTCATCTCCAAACTGCTCAGGCATAACCCCTCGGAACGGCTGCCCCTGGCCCAGGTCTCAGCCCACCCTTGGGTCCGGGCCAACTCTCGGAGGGTGCTGCCTCCCTCTGCCCTTCAATCTGTCGCC</t>
-  </si>
-  <si>
-    <t>GAACTGAAGGATGACGACTTTGAGAAGATCAGTGAGCTGGGGGCTGGCAATGGCGGTGTGGTGTTCAAGGTCTCCCACAAGCCTTCTGGCCTGGTCATGGCCAGAAAGCTAATTCATCTGGAGATCAAACCCGCAATCCGGAACCAGATCATAAGGGAGCTGCAGGTTCTGCATGAGTGCAACTCTCCGTACATCGTGGGCTTCTATGGTGCGTTCTACAGCGATGGCGAGATCAGTATCTGCATGGAGCACATGGATGGAGGTTCTCTGGATCAAGTCCTGAAGAAAGCTGGAAGAATTCCTGAACAAATTTTAGGAAAAGTTAGCATTGCTGTAATAAAAGGCCTGACATATCTGAGGGAGAAGCACAAGATCATGCACAGAGCATACGGAATGGACAGCCGACCTCCCATGGCAATTTTTGAGTTGTTGGATTACATAGTCAACGAGCCTCCTCCAAAACTGCCCAGTGGAGTGTTCAGTCTGGAATTTCAAGATTTTGTGAATAAATGCTTAATAAAAAACCCCGCAGAGAGAGCAGATTTGAAGCAACTCATGGTTCATGCTTTTATCAAGAGATCTGATGCTGAGGAAGTGGATTTTGCAGGTTGGCTCTGCTCCACCATCGGCCTTAAC</t>
-  </si>
-  <si>
-    <t>MEKYEKIGKIGEGSYGVVFKCRNRDTGQIVAIKKFLESEDDPVIKKIALREIRMLKQLKHPNLVNLLEVFRRKRRLHLVFEYCDHTVLHELDRYQRGVPEHLVKSITWQTLQAVNFCHKHNCIHRDVKPENILITKHSVIKLCDFGFARLLTGPSDYYTDYVATRWYRSPELLVGDTQYGPPVDVWAIGCVFAELLSGVPLWPGKSDVDQLYLIRKTLGDLIPRHQQVFSTNQYFSGVKIPDPEDMEPLELKFPNISYPALGLL</t>
-  </si>
-  <si>
-    <t>CLK1_HUMAN_D0_2VAG_A</t>
-  </si>
-  <si>
-    <t>MQTVGVHSIVQQLHRNSIQFTDGYEVKEDIGVGSYSVCKRCIHKATNMEFAVKIIDKSKRDPTEEIEILLRYGQHPNIITLKDVYDDGKYVYVVTELMKGGELLDKILRQKFFSEREASAVLFTITKTVEYLHAQGVVHRDLKPSNILYVDESGNPESIRICDFGFAKQLRAENGLLMTPCYTANFVAPEVLKRQGYDAACDIWSLGVLLYTMLTGYTPFANGPDDTPEEILARIGSGKFSLSGGYWNSVSDTAKDLVSKMLHVDPHQRLTAALVLRHPWIVHWDQLPQYQLNRQDAPHLVKGAMAATYSALNRNQSPVLEPVGRSTLAQRRGIKKITSTAL</t>
-  </si>
-  <si>
-    <t>GTGAAAGAATTCTTAGCCAAAGCCAAAGAAGATTTTCTTAAAAAATGGGAAAGTCCCGCTCAGAACACAGCCCACTTGGATCAGTTTGAACGAATCAAGACCCTCGGCACGGGCTCCTTCGGGCGGGTGATGCTGGTGAAACACAAGGAGACCGGGAACCACTATGCCATGAAGATCCTCGACAAACAGAAGGTGGTGAAACTGAAACAGATCGAACACACCCTGAATGAAAAGCGCATCCTGCAAGCTGTCAACTTTCCGTTCCTCGTCAAACTCGAGTTCTCCTTCAAGGACAACTCAAACTTATACATGGTCATGGAGTACGTGCCCGGCGGGGAGATGTTCTCACACCTACGGCGGATCGGAAGGTTCAGTGAGCCCCATGCCCGTTTCTACGCGGCCCAGATCGTCCTGACCTTTGAGTATCTGCACTCGCTGGATCTCATCTACAGGGACCTGAAGCCGGAGAATCTGCTCATTGACCAGCAGGGCTACATTCAGGTGACAGACTTCGGTTTCGCCAAGCGCGTGAAGGGCCGCACTTGGACCTTGTGCGGCACCCCTGAGTACCTGGCCCCTGAGATTATCCTGAGCAAAGGCTACAACAAGGCCGTGGACTGGTGGGCCCTGGGGGTTCTTATCTATGAAATGGCCGCTGGCTACCCGCCCTTCTTCGCAGACCAGCCCATCCAGATCTATGAGAAGATCGTCTCTGGGAAGGTGCGCTTCCCTTCCCACTTCAGCTCTGACTTGAAGGACCTGCTGCGGAACCTCCTGCAGGTAGATCTCACCAAGCGCTTTGGGAACCTCAAGAATGGGGTCAACGATATCAAGAACCACAAGTGGTTTGCCACAACTGACTGGATTGCCATCTACCAGAGGAAGGTGGAAGCTCCCTTCATACCAAAGTTTAAAGGCCCTGGGGATACGAGTAACTTTGACGACTATGAGGAAGAAGAAATCCGGGTCTCCATCAATGAGAAGTGTGGCAAGGAGTTTTCTGAGTTT</t>
-  </si>
-  <si>
-    <t>SALPWSINRDDYELQEVIGSGATAVVQAAYCAPKKEKVAIKRINLEKCQTSMDELLKEIQAMSQCHHPNIVSYYTSFVVKDELWLVMKLLSGGSVLDIIKHIVAKGEHKSGVLDESTIATILREVLEGLEYLHKNGQIHRDVKAGNILLGEDGSVQIADFGVSAFLATGGDITRNKVRKTFVGTPCWMAPEVMEQVRGYDFKADIWSFGITAIELATGAAPYHKYPPMKVLMLTLQNDPPSLETGVQDKEMLKKYGKSFRKMISLCLQKDPEKRPTAAELLRHKFFQKAK</t>
-  </si>
-  <si>
-    <t>MSDSKCDSQFYSVQVADSTFTVLKRYQQLKPIGSGAQGIVCAAFDTVLGINVAVKKLSRPFQNQTHAKRAYRELVLLKCVNHKNIISLLNVFTPQKTLEEFQDVYLVMELMDANLCQVIHMELDHERMSYLLYQMLCGIKHLHSAGIIHRDLKPSNIVVKSDCTLKILDFGLARTACTNFMMTPYVVTRYYRAPEVILGMGYKENVDIWSVGCIMAEMVLHKVLFPGRDYIDQWNKVIEQLGTPSAEFMKKLQPTVRNYVENRPKYPGIKFEELFPDWIFPSESERDKIKTSQARDLLSKMLVIDPDKRISVDEALRHPYITVWYDPAEAEAPPPQIYDAQLEEREHAIEEWKELIYKEVMDWE</t>
-  </si>
-  <si>
-    <t>KCC2G_HUMAN_D0_2V7O_A</t>
-  </si>
-  <si>
-    <t>KQYEHVKRDLNPEDFWEIIGELGDGAFGKVYKAQNKETSVLAAAKVIDTKSEEELEDYMVEIDILASCDHPNIVKLLDAFYYENNLWILIEFCAGGAVDAVMLELERPLTESQIQVVCKQTLDALNYLHDNKIIHRDLKAGNILFTLDGDIKLADFGVSAKNMRTIQRRDSFIGTPYWMAPEVVMCETSKDRPYDYKADVWSLGITLIEMAEIEPPHHELNPMRVLLKIAKSEPPTLAQPSRWSSNFKDFLKKCLEKNVDARWTTSQLLQHPFVTVDSNKPIRELIAEAKAEVTEEVEDGKE</t>
-  </si>
-  <si>
-    <t>ACCACCAATGTTGGAGACAGCACTTTAGCAGATTTATTGGATCATTCGTGTACATCAGGAAGTGGCTCTGGTCTTCCTTTTCTGGTACAAAGAACAGTGGCTCGCCAGATTACACTGTTGGAGTGTGTCGGGAAAGGCAGGTATGGTGAGGTGTGGAGGGGCAGCTGGCAAGGGGAAAATGTTGCCGTGAAGATCTTCTCCTCCCGTGATGAGAAGTCATGGTTCAGGGAAACGGAATTGTACAACACTGTGATGCTGAGGCATGAAAATATCTTAGGTTTCATTGCTTCAGACATGACATCAAGACACTCCAGTACCCAGCTGTGGTTAATTACACATTATCATGAAATGGGATCGTTGTACGACTATCTTCAGCTTACTACTCTGGATACAGTTAGCTGCCTTCGAATAGTGCTGTCCATAGCTAGTGGTCTTGCACATTTGCACATAGAGATATTTGGGACCCAAGGGAAACCAGCCATTGCCCATCGAGATTTAAAGAGCAAAAATATTCTGGTTAAGAAGAATGGACAGTGTTGCATAGCAGATTTGGGCCTGGCAGTCATGCATTCCCAGAGCACCAATCAGCTTGATGTGGGGAACAATCCCCGTGTGGGCACCAAGCGCTACATGGCCCCCGAAGTTCTAGATGAAACCATCCAGGTGGATTGTTTCGATTCTTATAAAAGGGTCGATATTTGGGCCTTTGGACTTGTTTTGTGGGAAGTGGCCAGGCGGATGGTGAGCAATGGTATAGTGGAGGATTACAAGCCACCGTTCTACGATGTGGTTCCCAATGACCCAAGTTTTGAAGATATGAGGAAGGTAGTCTGTGTGGATCAACAAAGGCCAAACATACCCAACAGATGGTTCTCAGACCCGACATTAACCTCTCTGGCCAAGCTAATGAAAGAATGCTGGTATCAAAATCCATCCGCAAGACTCACAGCACTGCGTATCAAAAAGACTTTGACCAAAATTGAT</t>
-  </si>
-  <si>
-    <t>ACCCAAACTGTTCATGAGTTTGCCAAGGAATTGGATGCCACCAACATATCCATTGATAAAGTTGTTGGAGCAGGTGAATTTGGAGAGGTGTGCAGTGGTCGCTTAAAACTTCCTTCAAAAAAAGAGATTTCAGTGGCCATTAAGACCCTGAAAGTTGGCTACACAGAAAAGCAGAGGAGAGACTTCCTGGGAGAAGCAAGCATTATGGGACAGTTTGACCACCCCAATATCATTCGACTGGAAGGAGTTGTTACCAAAAGTAAGCCAGTTATGATTGTCACAGAATACATGGAGAATGGTTCCTTGGATAGTTTCCTACGTAAACACGATGCCCAGTTTACTGTCATTCAGCTAGTGGGGATGCTTCGAGGGATAGCATCTGGCATGAAGTACCTGTCAGACATGGGCTATGTTCACCGAGACCTCGCTGCTCGGAACATCTTGATCAACAGTAACTTGGTGTGTAAGGTTTCTGATTTCGGACTTTCGCGTGTCCTGGAGGATGACCCAGAAGCTGCTTATACAACAAGAGGAGGGAAGATCCCAATCAGGTGGACATCACCAGAAGCTATAGCCTACCGCAAGTTCACGTCAGCCAGCGATGTATGGAGTTATGGGATTGTTCTCTGGGAGGTGATGTCTTATGGAGAGAGACCATACTGGGAGATGTCCAATCAGGATGTAATTAAAGCTGTAGATGAGGGCTATCGACTGCCACCCCCCATGGACTGCCCAGCTGCCTTGTATCAGCTGATGCTGGACTGCTGGCAGAAAGACAGGAACAACAGACCCAAGTTTGAGCAGATTGTTAGTATTCTGGACAAGCTTATCCGGAATCCCGGCAGCCTGAAGATCATCACCAGTGCAGCCGCAAGGCCATCAAACCTTCTTCTGGACCAAAGCAATGTGGATATCACTACCTTCCGCACAACAGGTGACTGGCTTAATGGTGTCTGGACAGCACACTGCAAGGAAATCTTCACGGGTGTGGAGTACAGTTCTTGTGACACAATAGCCAAGATTTCC</t>
-  </si>
-  <si>
-    <t>MEKDGLCRADQQYECVAEIGEGAYGKVFKARDLKNGGRFVALKRVRVQTGEEGMPLSTIREVAVLRHLETFEHPNVVRLFDVCTVSRTDRETKLTLVFEHVDQDLTTYLDKVPEPGVPTETIKDMMFQLLRGLDFLHSHRVVHRDLKPQNILVTSSGQIKLADFGLARIYSFQMALTSVVVTLWYRAPEVLLQSSYATPVDLWSVGCIFAEMFRRKPLFRGSSDVDQLGKILDVIGLPGEEDWPRDVALPRQAFHSKSAQPIEKFVTDIDELGKDLLLKCLTFNPAKRISAYSALSHPYFQ</t>
-  </si>
-  <si>
-    <t>EPHA3_HUMAN_D0_4GK2_A</t>
-  </si>
-  <si>
-    <t>ATGCCCGGCCCGGCCGCGGGCAGCAGGGCCCGGGTCTACGCCGAGGTGAACAGTCTGAGGAGCCGCGAGTACTGGGACTACGAGGCTCACGTCCCGAGCTGGGGTAATCAAGATGATTACCAACTGGTTCGAAAACTTGGTCGGGGAAAATATAGTGAAGTATTTGAGGCCATTAATATCACCAACAATGAGAGAGTGGTTGTAAAAATCCTGAAGCCAGTGAAGAAAAAGAAGATAAAACGAGAGGTTAAGATTCTGGAGAACCTTCGTGGTGGAACAAATATCATTAAGCTGATTGACACTGTAAAGGACCCCGTGTCAAAGACACCAGCTTTGGTATTTGAATATATCAATAATACAGATTTTAAGCAACTCTACCAGATCCTGACAGACTTTGATATCCGGTTTTATATGTATGAACTACTTAAAGCTCTGGATTACTGCCACAGCAAGGGAATCATGCACAGGGATGTGAAACCTCACAATGTCATGATAGATCACCAACAGAAAAAGCTGCGACTGATAGATTGGGGTCTGGCAGAATTCTATCATCCTGCTCAGGAGTACAATGTTCGTGTAGCCTCAAGGTACTTCAAGGGACCAGAGCTCCTCGTGGACTATCAGATGTATGATTATAGCTTGGACATGTGGAGTTTGGGCTGTATGTTAGCAAGCATGATCTTTCGAAGGGAACCATTCTTCCATGGACAGGACAACTATGACCAGCTTGTTCGCATTGCCAAGGTTCTGGGTACAGAAGAACTGTATGGGTATCTGAAGAAGTATCACATAGACCTAGATCCACACTTCAACGATATCCTGGGACAACATTCACGGAAACGCTGGGAAAACTTTATCCATAGTGAGAACAGACACCTTGTCAGCCCTGAGGCCCTAGATCTTCTGGACAAACTTCTGCGATACGACCATCAACAGAGACTGACTGCCAAAGAGGCCATGGAGCACCCATACTTCTACCCTGTGGTGAAGGAGCAGTCCCAG</t>
-  </si>
-  <si>
-    <t>ETKYTVDKRFGMDFKEIELIGSGGFGQVFKAKHRIDGKTYVIKRVKYNNEKAEREVKALAKLDHVNIVHYNGCWDGFDYDPETSDDSLESSDYDPENSKNSSRSKTKCLFIQMEFCDKGTLEQWIEKRRGEKLDKVLALELFEQITKGVDYIHSKKLIHRDLKPSNIFLVDTKQVKIGDFGLVTSLKNDGKRTRSKGTLRYMSPEQISSQDYGKEVDLYALGLILAELLHVCDTAFETSKFFTDLRDGIISDIFDKKEKTLLQKLLSKKPEDRPNTSEILRTLTVWKKSPEKNERHTC</t>
-  </si>
-  <si>
-    <t>NEK2_HUMAN_D0_2XKE_A</t>
-  </si>
-  <si>
-    <t>TCAGTTTATCCTAAGGCATTAAGAGATGAATACATCATGTCAAAAACTCTTGGAAGTGGTGCCTGTGGAGAGGTAAAGCTGGCTTTCGAGAGGAAAACATGTAAGAAAGTAGCCATAAAGATCATCAGCAAAAGGAAGTTTGCTATTGGTTCAGCAAGAGAGGCAGACCCAGCTCTCAATGTTGAAACAGAAATAGAAATTTTGAAAAAGCTAAATCATCCTTGCATCATCAAGATTAAAAACTTTTTTGATGCAGAAGATTATTATATTGTTTTGGAATTGATGGAAGGGGGAGAGCTGTTTGACAAAGTGGTGGGGAATAAACGCCTGAAAGAAGCTACCTGCAAGCTCTATTTTTACCAGATGCTCTTGGCTGTGCAGTACCTTCATGAAAACGGTATTATACACCGTGACTTAAAGCCAGAGAATGTTTTACTGTCATCTCAAGAAGAGGACTGTCTTATAAAGATTACTGATTTTGGGCACTCCAAGATTTGGGGAGAGACCTCTCTCATGAGAACCTTATGTGGAACCCCCACCTACTTGGCGCCTGAAGTTCTTGTTTCTGTTGGGACTGCTGGGTATAACCGTGCTGTGGACTGCTGGAGTTTAGGAGTTATTCTTTTTATCTGCCTTAGTGGGTATCCACCTTTCTCTGAGCATAGGACTCAAGTGTCACTGAAGGATCAGATCACCAGTGGAAAATACAACTTCATTCCTGAAGTCTGGGCAGAAGTCTCAGAGAAAGCTCTGGACCTTGTCAAGAAGTTGTTGGTAGTGGATCCAAAGGCACGTTTTACGACAGAAGAAGCCTTAAGACACCCGTGGCTTCAGGATGAAGACATGAAGAGAAAGTTTCAAGATCTTCTGTCTGAGGAAAATGAATCCACAGCTCTACCCCAGGTTCTAGCCCAGCCTTCTACTAGTCGAAAGCGGCCCCGTGAAGGGGAAGCCGAGGGTGCCGAG</t>
-  </si>
-  <si>
-    <t>ATGGAGCTGAGAGTCGGGAACAGGTACCGGCTGGGCCGGAAGATCGGCAGCGGCTCCTTCGGAGACATCTATCTCGGTACGGACATTGCTGCAGGAGAAGAGGTTGCCATCAAGCTTGAATGTGTCAAAACCAAACACCCTCAGCTCCACATTGAGAGCAAAATCTACAAGATGATGCAGGGAGGAGTGGGCATCCCCACCATCAGATGGTGCGGGGCAGAGGGGGACTACAACGTCATGGTGATGGAGCTGCTGGGGCCAAGCCTGGAGGACCTCTTCAACTTCTGCTCCAGGAAATTCAGCCTCAAAACCGTCCTGCTGCTTGCTGACCAAATGATCAGTCGCATCGAATACATTCATTCAAAGAACTTCATCCACCGGGATGTGAAGCCAGACAACTTCCTCATGGGCCTGGGGAAGAAGGGCAACCTGGTGTACATCATCGACTTCGGGCTGGCCAAGAAGTACCGGGATGCACGCACCCACCAGCACATCCCCTATCGTGAGAACAAGAACCTCACGGGGACGGCGCGGTACGCCTCCATCAACACGCACCTTGGAATTGAACAATCCCGAAGAGATGACTTGGAGTCTCTGGGCTACGTGCTAATGTACTTCAACCTGGGCTCTCTCCCCTGGCAGGGGCTGAAGGCTGCCACCAAGAGACAGAAATACGAAAGGATTAGCGAGAAGAAAATGTCCACCCCCATCGAAGTGTTGTGTAAAGGCTACCCTTCCGAATTTGCCACATACCTGAATTTCTGCCGTTCCTTGCGTTTTGACGACAAGCCTGACTACTCGTACCTGCGGCAGCTTTTCCGGAATCTGTTCCATCGCCAGGGCTTCTCCTATGACTACGTGTTCGACTGGAACATGCTCAAA</t>
-  </si>
-  <si>
-    <t>ATGGCGGCGGCGGCGGCGGCGGGCGCGGGCCCGGAGATGGTCCGCGGGCAGGTGTTCGACGTGGGGCCGCGCTACACCAACCTCTCGTACATCGGCGAGGGCGCCTACGGCATGGTGTGCTCTGCTTATGATAATGTCAACAAAGTTCGAGTAGCTATCAAGAAAATCAGCCCCTTTGAGCACCAGACCTACTGCCAGAGAACCCTGAGGGAGATAAAAATCTTACTGCGCTTCAGACATGAGAACATCATTGGAATCAATGACATTATTCGAGCACCAACCATCGAGCAAATGAAAGATGTATATATAGTACAGGACCTCATGGAAACAGATCTTTACAAGCTCTTGAAGACACAACACCTCAGCAATGACCATATCTGCTATTTTCTCTACCAGATCCTCAGAGGGTTAAAATATATCCATTCAGCTAACGTTCTGCACCGTGACCTCAAGCCTTCCAACCTGCTGCTCAACACCACCTGTGATCTCAAGATCTGTGACTTTGGCCTGGCCCGTGTTGCAGATCCAGACCATGATCACACAGGGTTCCTGACAGAATATGTGGCCACACGTTGGTACAGGGCTCCAGAAATTATGTTGAATTCCAAGGGCTACACCAAGTCCATTGATATTTGGTCTGTAGGCTGCATTCTGGCAGAAATGCTTTCTAACAGGCCCATCTTTCCAGGGAAGCATTATCTTGACCAGCTGAACCACATTTTGGGTATTCTTGGATCCCCATCACAAGAAGACCTGAATTGTATAATAAATTTAAAAGCTAGGAACTATTTGCTTTCTCTTCCACACAAAAATAAGGTGCCATGGAACAGGCTGTTCCCAAATGCTGACTCCAAAGCTCTGGACTTATTGGACAAAATGTTGACATTCAACCCACACAAGAGGATTGAAGTAGAACAGGCTCTGGCCCACCCATATCTGGAGCAGTATTACGACCCGAGTGACGAGCCCATCGCCGAAGCACCATTCAAGTTCGACATGGAATTGGATGACTTGCCTAAGGAAAAGCTCAAAGAACTAATTTTTGAAGAGACTGCTAGATTCCAGCCAGGATACAGATCT</t>
-  </si>
-  <si>
-    <t>MDEQSQGMQGPPVPQFQPQKALRPDMGYNTLANFRIEKKIGRGQFSEVYRAACLLDGVPVALKKVQIFDLMDAKARADCIKEIDLLKQLNHPNVIKYYASFIEDNELNIVLELADAGDLSRMIKHFKKQKRLIPERTVWKYFVQLCSALEHMHSRRVMHRDIKPANVFITATGVVKLGDLGLGRFFSSKTTAAHSLVGTPYYMSPERIHENGYNFKSDIWSLGCLLYEMAALQSPFYGDKMNLYSLCKKIEQCDYPPLPSDHYSEELRQLVNMCINPDPEKRPDVTYVYDVAKRMHACTASS</t>
-  </si>
-  <si>
-    <t>GECSQKGPVPFSHCLPTEKLQRCEKIGEGVFGEVFQTIADHTPVAIKIIAIEGPDLVNGSHQKTFEEILPEIIISKELSLLSGEVCNRTEGFIGLNSVHCVQGSYPPLLLKAWDHYNSTKGSANDRPDFFKDDQLFIVLEFEFGGIDLEQMRTKLSSLATAKSILHQLTASLAVAEASLRFEHRDLHWGNVLLKKTSLKKLHYTLNGKSSTIPSCGLQVSIIDYTLSRLERDGIVVFCDVSMDEDLFTGDGDYQFDIYRLMKKENNNRWGEYHPYSNVLWLHYLTDKMLKQMTFKTKCNTPAMKQIKRKIQEFHRTMLNFSSATDLLCQHRLFK</t>
-  </si>
-  <si>
-    <t>MENFNNFYILTSKELGRGKFAVVRQCISKSTGQEYAAKFLKKRRRGQDCRAEILHEIAVLELAKSCPRVINLHEVYENTSEIILILEYAAGGEIFSLCLPELAEMVSENDVIRLIKQILEGVYYLHQNNIVHLDLKPQNILLSSIYPLGDIKIVDFGMSRKIGHACELREIMGTPEYLAPEILNYDPITTATDMWNIGIIAYMLLTHTSPFVGEDNQETYLNISQVNVDYSEETFSSVSQLATDFIQSLLVKNPEKRPTAEICLSHSWLQQWDFENLFHPEETSSSSQTQDHSVRSSEDKTSKSS</t>
-  </si>
-  <si>
-    <t>MSQSKGKKRNPGLKIPKEAFEQPQTSSTPPRDLDSKACISIGNQNFEVKADDLEPIMELGRGAYGVVEKMRHVPSGQIMAVKRIRATVNSQEQKRLLMDLDISMRTVDCPFTVTFYGALFREGDVWICMELMDTSLDKFYKQVIDKGQTIPEDILGKIAVSIVKALEHLHSKLSVIHRDVKPSNVLINALGQVKMCDFGISGYLVDSVAKTIDAGCKPYMAPERINPELNQKGYSVKSDIWSLGITMIELAILRFPYDSWGTPFQQLKQVVEEPSPQLPADKFSAEFVDFTSQCLKKNSKERPTYPELMQHPFFTLHESKGTDVASFVKLILGD</t>
-  </si>
-  <si>
-    <t>MELRVGNKYRLGRKIGSGSFGDIYLGANIASGEEVAIKLECVKTKHPQLHIESKFYKMMQGGVGIPSIKWCGAEGDYNVMVMELLGPSLEDLFNFCSRKFSLKTVLLLADQMISRIEYIHSKNFIHRDVKPDNFLMGLGKKGNLVYIIDFGLAKKYRDARTHQHIPYRENKNLTGTARYASINTHLGIEQSRRDDLESLGYVLMYFNLGSLPWQGLKAATKRQKYERISEKKMSTPIEVLCKGYPSEFSTYLNFCRSLRFDDKPDYSYLRQLFRNLFHRQGFSYDYVFDWNMLK</t>
-  </si>
-  <si>
-    <t>KCC2D_HUMAN_D0_2VN9_A</t>
-  </si>
-  <si>
-    <t>dna_end</t>
-  </si>
-  <si>
-    <t>MST4_HUMAN_D0_4FZD_B</t>
-  </si>
-  <si>
-    <t>MADDDVLFEDVYELCEVIGKGPFSVVRRCINRETGQQFAVKIVDVAKFTSSPGLSTEDLKREASICHMLKHPHIVELLETYSSDGMLYMVFEFMDGADLCFEIVKRADAGFVYSEAVASHYMRQILEALRYCHDNNIIHRDVKPHCVLLASKENSAPVKLGGFGVAIQLGESGLVAGGRVGTPHFMAPEVVKREPYGKPVDVWGCGVILFILLSGCLPFYGTKERLFEGIIKGKYKMNPRQWSHISESAKDLVRRMLMLDPAERITVYEALNHPWLKERDRYAYKIHLPETVEQLRKFNARRKLKGAVLAAVSSHKFNSFYGDPPEELPDFSEDPTSSGA</t>
-  </si>
-  <si>
-    <t>FAK1_HUMAN_D0_2IJM_B</t>
-  </si>
-  <si>
-    <t>DAPK1_HUMAN_D0_3F5G_A</t>
-  </si>
-  <si>
-    <t>CHK2_HUMAN_D0_2CN5_A</t>
-  </si>
-  <si>
-    <t>GTGATCGACCCCTCAGAGCTCACTTTTGTCCAAGAGATTGGCAGTGGGCAATTTGGGTTGGTGCATCTGGGCTACTGGCTCAACAAGGACAAGGTGGCTATCAAAACCATTCGGGAAGGGGCTATGTCAGAAGAGGACTTCATAGAGGAGGCTGAAGTAATGATGAAACTCTCTCATCCCAAACTGGTGCAGCTGTATGGGGTGTGCCTGGAGCAGGCCCCCATCTGCCTGGTGTTTGAGTTCATGGAGCACGGCTGCCTGTCAGATTATCTACGCACCCAGCGGGGACTTTTTGCTGCAGAGACCCTGCTGGGCATGTGTCTGGATGTGTGTGAGGGCATGGCCTACCTGGAAGAGGCATGTGTCATCCACAGAGACTTGGCTGCCAGAAATTGTTTGGTGGGAGAAAACCAAGTCATCAAGGTGTCTGACTTTGGGATGACAAGGTTCGTTCTGGATGATCAGTACACCAGTTCCACAGGCACCAAATTCCCGGTGAAGTGGGCATCCCCAGAGGTTTTCTCTTTCAGTCGCTATAGCAGCAAGTCCGATGTGTGGTCATTTGGTGTGCTGATGTGGGAAGTTTTCAGTGAAGGCAAAATCCCGTATGAAAACCGAAGCAACTCAGAGGTGGTGGAAGACATCAGTACCGGATTTCGGTTGTACAAGCCCCGGCTGGCCTCCACACACGTCTACCAGATTATGAATCACTGCTGGAAAGAGAGACCAGAAGATCGGCCAGCCTTCTCCAGACTGCTGCGTCAACTGGCTGAAATTGCAGAATCAGGACTT</t>
-  </si>
-  <si>
-    <t>MSDEEILEKLRSIVSVGDPKKKYTRFEKIGQGASGTVYTAMDVATGQEVAIKQMNLQQQPKKELIINEILVMRENKNPNIVNYLDSYLVGDELWVVMEYLAGGSLTDVVTETCMDEGQIAAVCRECLQALEFLHSNQVIHRDIKSDNILLGMDGSVKLTDFGFCAQITPEQSKRSTMVGTPYWMAPEVVTRKAYGPKVDIWSLGIKAIEMIEGEPPYLNENPLRALYLIATNGTPELQNPEKLSAIFRDFLNRCLEMDVEKRGSAKELLQHQFLKIAKPLSSLTPLIAAAKEATKNNH</t>
-  </si>
-  <si>
-    <t>CHK1_HUMAN_D0_2E9V_A</t>
-  </si>
-  <si>
-    <t>DYRK2_HUMAN_D0_3KVW_A</t>
-  </si>
-  <si>
-    <t>ATGGAGCCATTCAAGCAGCAGAAGGTGGAGGACTTTTATGACATCGGAGAGGAGCTGGGGAGTGGCCAGTTTGCCATCGTGAAGAAGTGCCGGGAGAAGAGCACGGGGCTTGAGTATGCAGCCAAGTTCATCAAGAAGCGGCAGAGCCGGGCGAGCCGGCGCGGTGTGAGCCGGGAGGAGATCGAGCGGGAGGTGAGCATCCTGCGGCAGGTGCTGCACCACAATGTCATCACGCTGCACGACGTCTATGAGAACCGCACCGACGTGGTGCTCATCCTTGAGCTAGTGTCTGGAGGAGAGCTCTTCGATTTCCTGGCCCAGAAGGAGTCACTGAGTGAGGAGGAGGCCACCAGCTTCATTAAGCAGATCCTGGATGGGGTGAACTACCTTCACACAAAGAAAATTGCTCACTTTGATCTCAAGCCAGAAAACATTATGTTGTTAGACAAGAATATTCCCATTCCACACATCAAGCTGATTGACTTTGGTCTGGCTCACGAAATAGAAGATGGAGTTGAATTTAAGAATATTTTTGGGACGCCGGAATTTGTTGCTCCAGAAATTGTGAACTACGAGCCCCTGGGTCTGGAGGCTGACATGTGGAGCATAGGCGTCATCACCTACATCCTCTTAAGTGGAGCATCCCCTTTCCTGGGAGACACGAAGCAGGAAACACTGGCAAATATCACAGCAGTGAGTTACGACTTTGATGAGGAATTCTTCAGCCAGACGAGCGAGCTGGCCAAGGACTTTATTCGGAAGCTTCTGGTTAAAGAGACCCGGAAACGGCTCACAATCCAAGAGGCTCTCAGACACCCCTGGATCACGCCGGTGGACAACCAGCAAGCCATGGTGCGCAGGGAGTCTGTGGTCAATCTGGAGAACTTCAGGAAGCAGTATGTCCGCAGGCGGTGGAAGCTTTCCTTCAGCATCGTGTCCCTGTGCAACCACCTCACCCGC</t>
-  </si>
-  <si>
-    <t>GCGGCTCCACCGGCGAAAGAGATCCCGGAGGTCCTAGTGGACCCACGCAGCCGGCGGCGCTATGTGCGGGGCCGCTTTTTGGGCAAGGGCGGCTTTGCCAAGTGCTTCGAGATCTCGGACGCGGACACCAAGGAGGTGTTCGCGGGCAAGATTGTGCCTAAGTCTCTGCTGCTCAAGCCGCACCAGAGGGAGAAGATGTCCATGGAAATATCCATTCACCGCAGCCTCGCCCACCAGCACGTCGTAGGATTCCACGGCTTTTTCGAGGACAACGACTTCGTGTTCGTGGTGTTGGAGCTCTGCCGCCGGAGGTCTCTCCTGGAGCTGCACAAGAGGAGGAAAGCCCTGACTGAGCCTGAGGCCCGATACTACCTACGGCAAATTGTGCTTGGCTGCCAGTACCTGCACCGAAACCGAGTTATTCATCGAGACCTCAAGCTGGGCAACCTTTTCCTGAATGAAGATCTGGAGGTGAAAATAGGGGATTTTGGACTGGCAACCAAAGTCGAATATGACGGGGAGAGGAAGAAGACCCTGTGTGGGACTCCTAATTACATAGCTCCCGAGGTGCTGAGCAAGAAAGGGCACAGTTTCGAGGTGGATGTGTGGTCCATTGGGTGTATCATGTATACCTTGTTAGTGGGCAAACCACCTTTTGAGACTTCTTGCCTAAAAGAGACCTACCTCCGGATCAAGAAGAATGAATACAGTATTCCCAAGCACATCAACCCCGTGGCCGCCTCCCTCATCCAGAAGATGCTTCAGACAGATCCCACTGCCCGCCCAACCATTAACGAGCTGCTTAATGACGAGTTCTTTACTTCTGGCTATATCCCTGCCCGTCTCCCCATCACCTGCCTGACCATTCCACCAAGGTTTTCGATTGCTCCCAGCAGCCTGGACCCCAGCAACCGGAAGCCCCTCACAGTCCTCAATAAA</t>
-  </si>
-  <si>
-    <t>QSSKRSSRSVEDDKEGHLVCRIGDWLQERYEIVGNLGEGTFGKVVECLDHARGKSQVALKIIRNVGKYREAARLEINVLKKIKEKDKENKFLCVLMSDWFNFHGHMCIAFELLGKNTFEFLKENNFQPYPLPHVRHMAYQLCHALRFLHENQLTHTDLKPENILFVNSEFETLYNEHKSCEEKSVKNTSIRVADFGSATFDHEHHTTIVATRHYRPPEVILELGWAQPCDVWSIGCILFEYYRGFTLFQTHENREHLVMMEKILGPIPSHMIHRTRKQKYFYKGGLVWDENSSDGRYVKENCKPLKSYMLQDSLEHVQLFDLMRRMLEFDPAQRITLAEALLHPFFAGLTPEERSFHT</t>
-  </si>
-  <si>
-    <t>GTGTTTCCATGCTCTGTGTACGTGCCGGACGAGTGGGAGGTGTCTCGAGAGAAGATCACCCTCCTTCGAGAGCTGGGGCAGGGCTCCTTCGGCATGGTGTATGAGGGCAATGCCAGGGACATCATCAAGGGTGAGGCAGAGACCCGCGTGGCGGTGAAGACGGTCAACGAGTCAGCCAGTCTCCGAGAGCGGATTGAGTTCCTCAATGAGGCCTCGGTCATGAAGGGCTTCACCTGCCATCACGTGGTGCGCCTCCTGGGAGTGGTGTCCAAGGGCCAGCCCACGCTGGTGGTGATGGAGCTGATGGCTCACGGAGACCTGAAGAGCTACCTCCGTTCTCTGCGGCCAGAGGCTGAGAATAATCCTGGCCGCCCTCCCCCTACCCTTCAAGAGATGATTCAGATGGCGGCAGAGATTGCTGACGGGATGGCCTACCTGAACGCCAAGAAGTTTGTGCATCGGGACCTGGCAGCGAGAAACTGCATGGTCGCCCATGATTTTACTGTCAAAATTGGAGACTTTGGAATGACCAGAGACATCTATGAAACGGATTACTACCGGAAAGGGGGCAAGGGTCTGCTCCCTGTACGGTGGATGGCACCGGAGTCCCTGAAGGATGGGGTCTTCACCACTTCTTCTGACATGTGGTCCTTTGGCGTGGTCCTTTGGGAAATCACCAGCTTGGCAGAACAGCCTTACCAAGGCCTGTCTAATGAACAGGTGTTGAAATTTGTCATGGATGGAGGGTATCTGGATCAACCCGACAACTGTCCAGAGAGAGTCACTGACCTCATGCGCATGTGCTGGCAATTCAACCCCAAGATGAGGCCAACCTTCCTGGAGATTGTCAACCTGCTCAAGGACGACCTGCACCCCAGCTTTCCAGAGGTGTCGTTCTTCCACAGCGAGGAGAACAAG</t>
-  </si>
-  <si>
-    <t>ATGCAGACAGTTGGTGTACATTCAATTGTTCAGCAGTTACACAGGAACAGTATTCAGTTTACTGATGGATATGAAGTAAAAGAAGATATTGGAGTTGGCTCCTACTCTGTTTGCAAGAGATGTATACATAAAGCTACAAACATGGAGTTTGCAGTGAAGATTATTGATAAAAGCAAGAGAGACCCAACAGAAGAAATTGAAATTCTTCTTCGTTATGGACAGCATCCAAACATTATCACTCTAAAGGATGTATATGATGATGGAAAGTATGTGTATGTAGTAACAGAACTTATGAAAGGAGGTGAATTGCTGGATAAAATTCTTAGACAAAAATTTTTCTCTGAACGAGAGGCCAGTGCTGTCCTGTTCACTATAACTAAAACCGTTGAATATCTTCACGCACAAGGGGTGGTTCATAGAGACTTGAAACCTAGCAACATTCTTTATGTGGATGAATCTGGTAATCCGGAATCTATTCGAATTTGTGATTTTGGCTTTGCAAAACAGCTGAGAGCGGAAAATGGTCTTCTCATGACTCCTTGTTACACTGCAAATTTTGTTGCACCAGAGGTTTTAAAAAGACAAGGCTATGATGCTGCTTGTGATATATGGAGTCTTGGTGTCCTACTCTATACAATGCTTACCGGTTACACTCCATTTGCAAATGGTCCTGATGATACACCAGAGGAAATATTGGCACGAATAGGTAGCGGAAAATTCTCACTCAGTGGTGGTTACTGGAATTCTGTTTCAGACACAGCAAAGGACCTGGTGTCAAAGATGCTTCATGTAGACCCTCATCAGAGACTGACTGCTGCTCTTGTGCTCAGACATCCTTGGATCGTCCACTGGGACCAACTGCCACAATACCAACTAAACAGACAGGATGCACCACATCTAGTAAAGGGTGCCATGGCAGCTACATATTCTGCTTTGAACCGTAATCAGTCACCAGTTTTGGAACCAGTAGGCCGCTCTACTCTTGCTCAGCGGAGAGGTATTAAAAAAATCACCTCAACAGCCCTG</t>
-  </si>
-  <si>
-    <t>KS6A3_HUMAN_D0_4JG7_A</t>
-  </si>
-  <si>
-    <t>MGKVKATPMTPEQAMKQYMQKLTAFEHHEIFSYPEIYFLGLNAKKRQGMTGGPNNGGYDDDQGSYVQVPHDHVAYRYEVLKVIGKGSFGQVVKAYDHKVHQHVALKMVRNEKRFHRQAAEEIRILEHLRKQDKDNTMNVIHMLENFTFRNHICMTFELLSMNLYELIKKNKFQGFSLPLVRKFAHSILQCLDALHKNRIIHCDLKPENILLKQQGRSGIKVIDFGSSCYEHQRVYTYIQSRFYRAPEVILGARYGMPIDMWSLGCILAELLTGYPLLPGEDEGDQLACMIELLGMPSQKLLDASKRAKNFVSSKGYPRYCTVTTLSDGSVVLNGGRSRRGKLRGPPESREWGNALKGCDDPLFLDFLKQCLEWDPAVRMTPGQALRHPWLRRRLPKPPTGEKTSVKR</t>
-  </si>
-  <si>
-    <t>CDK2_HUMAN_D0_4BCP_A</t>
-  </si>
-  <si>
-    <t>CAGCAGTTCCCGCAGTTCCACGTCAAGTCCGGCCTGCAGATCAAGAAGAACGCCATCATCGATGACTACAAGGTCACCAGCCAGGTCCTGGGGCTGGGCATCAACGGCAAAGTTTTGCAGATCTTCAACAAGAGGACCCAGGAGAAATTCGCCCTCAAAATGCTTCAGGACTGCCCCAAGGCCCGCAGGGAGGTGGAGCTGCACTGGCGGGCCTCCCAGTGCCCGCACATCGTACGGATCGTGGATGTGTACGAGAATCTGTACGCAGGGAGGAAGTGCCTGCTGATTGTCATGGAATGTTTGGACGGTGGAGAACTCTTTAGCCGAATCCAGGATCGAGGAGACCAGGCATTCACAGAAAGAGAAGCATCCGAAATCATGAAGAGCATCGGTGAGGCCATCCAGTATCTGCATTCAATCAACATTGCCCATCGGGATGTCAAGCCTGAGAATCTCTTATACACCTCCAAAAGGCCCAACGCCATCCTGAAACTCACTGACTTTGGCTTTGCCAAGGAAACCACCAGCCACAACTCTTTGACCACTCCTTGTTATACACCGTACTATGTGGCTCCAGAAGTGCTGGGTCCAGAGAAGTATGACAAGTCCTGTGACATGTGGTCCCTGGGTGTCATCATGTACATCCTGCTGTGTGGGTATCCCCCCTTCTACTCCAACCACGGCCTTGCCATCTCTCCGGGCATGAAGACTCGCATCCGAATGGGCCAGTATGAATTTCCCAACCCAGAATGGTCAGAAGTATCAGAGGAAGTGAAGATGCTCATTCGGAATCTGCTGAAAACAGAGCCCACCCAGAGAATGACCATCACCGAGTTTATGAACCACCCTTGGATCATGCAATCAACAAAGGTCCCTCAAACCCCACTGCACACCAGCCGGGTCCTGAAGGAGGACAAGGAGCGGTGGGAGGATGTCAAGGGGTGTCTTCATGACAAGAACAGCGACCAGGCC</t>
-  </si>
-  <si>
-    <t>DEQPHIGNYRLLKTIGKGNFAKVKLARHILTGREVAIKIIDKTQLNPTSLQKLFREVRIMKILNHPNIVKLFEVIETEKTLYLIMEYASGGEVFDYLVAHGRMKEKEARSKFRQIVSAVQYCHQKRIVHRDLKAENLLLDADMNIKIADFGFSNEFTVGGKLDTFCGSPPYAAPELFQGKKYDGPEVDVWSLGVILYTLVSGSLPFDGQNLKELRERVLRGKYRIPFYMSTDCENLLKRFLVLNPIKRGTLEQIMKDRWINAGHEEDELKPFVEPELDISDQKRIDIMVGMGYSQEEIQESLSKMKYDEITATYLLLGRKSSE</t>
-  </si>
-  <si>
-    <t>MP2K4_HUMAN_D0_3ALN_C</t>
-  </si>
-  <si>
-    <t>CGGGACTCGAGTGATGATTGGGAGATTCCTGATGGGCAGATTACAGTGGGACAAAGAATTGGATCTGGATCATTTGGAACAGTCTACAAGGGAAAGTGGCATGGTGATGTGGCAGTGAAAATGTTGAATGTGACAGCACCTACACCTCAGCAGTTACAAGCCTTCAAAAATGAAGTAGGAGTACTCAGGAAAACACGACATGTGAATATCCTACTCTTCATGGGCTATTCCACAAAGCCACAACTGGCTATTGTTACCCAGTGGTGTGAGGGCTCCAGCTTGTATCACCATCTCCATATCATTGAGACCAAATTTGAGATGATCAAgCTTATAGATATTGCACGACAGACTGCACAGGGCATGGATTACTTACACGCCAAGTCAATCATCCACAGAGACCTCAAGAGTAATAATATATTTCTTCATGAAGACCTCACAGTAAAAATAGGTGATTTTGGTCTAGCTACAGTGAAATCTCGATGGAGTGGGTCCCATCAGTTTGAACAGTTGTCTGGgTCCATTTTGTGGATGGCACCAGAAGTCATCAGAATGCAAGATAAAAATCCATACAGCTTTCAGTCAGATGTATATGCATTTGGgATTGTTCTGTATGAATTGATGACTGGACAGTTACCTTATTCAAACATCAACAACAGGGACCAGATAATTTTTATGGTGGGACGAGGATACCTGTCTCCAGATCTCAGTAAGGTACGGAGTAACTGTCCAAAAGCCATGAAGAGATTAATGGCAGAGTGCCTCAAAAAGAAAAGAGATGAGAGACCACTCTTTCCCCAAATTCTCGCCTCTATTGAGCTGCTGGCCCGC</t>
-  </si>
-  <si>
-    <t>ACCACCTCACTTGAAGCTTTGCCCACAGGGACAGTGCTGACAGACAAGAGTGGGCGACAGTGGAAGCTGAAGTCCTTCCAGACCAGGGACAACCAGGGCATTCTCTATGAAGCTGCACCCACCTCCACCCTCACCTGTGACTCAGGACCACAGAAGCAAAAGTTCTCACTCAAACTGGATGCCAAGGATGGGCGCTTGTTCAATGAGCAGAACTTCTTCCAGCGGGCCGCCAAGCCTCTGCAAGTCAACAAGTGGAAGAAGCTGTACTCGACCCCACTGCTGGCCATCCCTACCTGCATGGGTTTCGGTGTTCACCAGGACAAATACAGGTTCTTGGTGTTACCCAGCCTGGGGAGGAGCCTTCAGTCGGCCCTGGATGTCAGCCCAAAGCATGTGCTGTCAGAGAGGTCTGTGCTGCAGGTGGCCTGCCGGCTGCTGGATGCCCTGGAGTTCCTCCATGAGAATGAGTATGTTCATGGAAATGTGACAGCTGAAAATATCTTTGTGGATCCAGAGGACCAGAGTCAGGTGACTTTGGCAGGCTATGGCTTCGCCTTCCGCTATTGCCCAAGTGGCAAACACGTGGCCTACGTGGAAGGCAGCAGGAGCCCTCACGAGGGGGACCTTGAGTTCATTAGCATGGACCTGCACAAGGGATGCGGGCCCTCCCGCCGCAGCGACCTCCAGAGCCTGGGCTACTGCATGCTGAAGTGGCTCTACGGGTTTCTGCCATGGACAAATTGCCTTCCCAACACTGAGGACATCATGAAGCAAAAACAGAAGTTTGTTGATAAGCCGGGGCCCTTCGTGGGACCCTGCGGTCACTGGATCAGGCCCTCAGAGACCCTGCAGAAGTACCTGAAGGTGGTGATGGCCCTCACGTATGAGGAGAAGCCGCCCTACGCCATGCTGAGGAACAACCTAGAAGCTTTGCTGCAGGATCTGCGTGTGTCTCCATATGACCCCATTGGCCTCCCGATGGTGCCC</t>
-  </si>
-  <si>
-    <t>TCACCACAGCGGGAGCCACAGCGAGTATCCCATGAGCAGTTCCGGGCTGCCCTGCAGCTGGTGGTGGACCCAGGCGACCCCCGCTCCTACCTGGACAACTTCATCAAGATTGGCGAGGGCTCCACGGGCATCGTGTGCATCGCCACCGTGCGCAGCTCGGGCAAGCTGGTGGCCGTCAAGAAGATGGACCTGCGCAAGCAGCAGAGGCGCGAGCTGCTCTTCAACGAGGTGGTAATCATGAGGGACTACCAGCACGAGAATGTGGTGGAGATGTACAACAGCTACCTGGTGGGGGACGAGCTCTGGGTGGTCATGGAGTTCCTGGAAGGAGGCGCCCTCACCGACATCGTCACCCACACCAGGATGAACGAGGAGCAGATCGCGGCCGTGTGCCTTGCAGTGCTGCAGGCCCTGTCGGTGCTCCACGCCCAGGGCGTCATCCACCGGGACATCAAGAGCGACTCGATCCTGCTGACCCATGATGGCAGGGTGAAGCTGTCAGACTTTGGGTTCTGCGCCCAGGTGAGCAAGGAAGTGCCCCGAAGGAAGTCGCTGGTCGGCACGCCCTACTGGATGGCCCCAGAGCTCATCTCCCGCCTTCCCTACGGGCCAGAGGTAGACATCTGGTCGCTGGGGATAATGGTGATTGAGATGGTGGACGGAGAGCCCCCCTACTTCAACGAGCCACCCCTCAAAGCCATGAAGATGATTCGGGACAACCTGCCACCCCGACTGAAGAACCTGCACAAGGTGTCGCCATCCCTGAAGGGCTTCCTGGACCGCCTGCTGGTGCGAGACCCTGCCCAGCGGGCCACGGCAGCCGAGCTGCTGAAGCACCCATTCCTGGCCAAGGCAGGGCCGCCTGCCAGCATCGTGCCCCTCATGCGCCAGAACCGCACCAGA</t>
-  </si>
-  <si>
-    <t>TIE2_HUMAN_D0_3L8P_A</t>
-  </si>
-  <si>
-    <t>SIESSGKLKISPEQHWDFTAEDLKDLGEIGRGAYGSVNKMVHKPSGQIMAVKRIRSTVDEKEQKQLLMDLDVVMRSSDCPYIVQFYGALFREGDCWICMELMSTSFDKFYKYVYSVLDDVIPEEILGKITLATVKALNHLKENLKIIHRDIKPSNILLDRSGNIKLCDFGISGQLVDSIAKTRDAGCRPYMAPERIDPSASRQGYDVRSDVWSLGITLYELATGRFPYPKWNSVFDQLTQVVKGDPPQLSNSEEREFSPSFINFVNLCLTKDESKRPKYKELLKHPFILMYEERAVEVACYVCKILDQMPATPSSPMYVD</t>
-  </si>
-  <si>
-    <t>HLICQSGDVLSARYEIVDTLGEGAFGKVVECIDHKAGGRHVAVKIVKNVDRYCEAARSEIQVLEHLNTTDPNSTFRCVQMLEWFEHHGHICIVFELLGLSTYDFIKENGFLPFRLDHIRKMAYQICKSVNFLHSNKLTHTDLKPENILFVQSDYTEAYNPKIKRDERTLINPDIKVVDFGSATYDDEHHSTLVSTRHYRAPEVILALGWSQPCDVWSIGCILIEYYLGFTVFPTHDSKEHLAMMERILGPLPKHMIQKTRKRKYFHHDRLDWDEHSSAGRYVSRRCKPLKEFMLSQDVEHERLFDLIQKMLEYDPAKRITLREALKHPFFDLLKKSI</t>
-  </si>
-  <si>
-    <t>TDSFSGRFEDVYQLQEDVLGEGAHARVQTCINLITSQEYAVKIIEKQPGHIRSRVFREVEMLYQCQGHRNVLELIEFFEEEDRFYLVFEKMRGGSILSHIHKRRHFNELEASVVVQDVASALDFLHNKGIAHRDLKPENILCEHPNQVSPVKICDFDLGSGIKLNGDCSPISTPELLTPCGSAEYMAPEVVEAFSEEASIYDKRCDLWSLGVILYILLSGYPPFVGRCGSDCGWDRGEACPACQNMLFESIQEGKYEFPDKDWAHISCAAKDLISKLLVRDAKQRLSAAQVLQHPWVQGCAPENTLPTPMVLQR</t>
-  </si>
-  <si>
-    <t>ACGGACGAGTATCAGCTTTTCGAGGAGCTTGGAAAGGGGGCATTCTCAGTGGTGAGAAGATGTATGAAAATTCCTACTGGACAAGAATATGCTGCCAAAATTATCAACACCAAAAAGCTTTCTGCTAGGGATCATCAGAAACTAGAAAGAGAAGCTAGAATCTGCCGTCTTTTGAAGCACCCTAATATTGTGCGACTTCATGATAGCATATCAGAAGAGGGCTTTCACTACTTGGTGTTTGATTTAGTTACTGGAGGTGAACTGTTTGAAGACATAGTGGCAAGAGAATACTACAGTGAAGCTGATGCCAGTCATTGTATACAGCAGATTCTAGAAAGTGTTAATCATTGTCACCTAAATGGCATAGTTCACAGGGACCTGAAGCCTGAGAATTTGCTTTTAGCTAGCAAATCCAAGGGAGCAGCTGTGAAATTGGCAGACTTTGGCTTAGCCATAGAAGTTCAAGGGGACCAGCAGGCGTGGTTTGGTTTTGCTGGCACACCTGGATATCTTTCTCCAGAAGTTTTACGTAAAGATCCTTATGGAAAGCCAGTGGATATGTGGGCATGTGGTGTCATTCTCTATATTCTACTTGTGGGGTATCCACCCTTCTGGGATGAAGACCAACACAGACTCTATCAGCAGATCAAGGCTGGAGCTTATGATTTTCCATCACCAGAATGGGACACGGTGACTCCTGAAGCCAAAGACCTCATCAATAAAATGCTTACTATCAACCCTGCCAAACGCATCACAGCCTCAGAGGCACTGAAGCACCCATGGATCTGTCAACGTTCTACTGTTGCTTCCATGATGCACAGACAGGAGACTGTAGACTGCTTGAAGAAATTTAATGCTAGAAGAAAACTAAAGGGTGCCATCTTGACAACTATGCTG</t>
-  </si>
-  <si>
-    <t>WALNMKELKLLQTIGKGEFGDVMLGDYRGNKVAVKCIKNDATAQAFLAEASVMTQLRHSNLVQLLGVIVEEKGGLYIVTEYMAKGSLVDYLRSRGRSVLGGDCLLKFSLDVCEAMEYLEGNNFVHRDLAARNVLVSEDNVAKVSDFGLTKEASSTQDTGKLPVKWTAPEALREKKFSTKSDVWSFGILLWEIYSFGRVPYPRIPLKDVVPRVEKGYKMDAPDGCPPAVYEVMKNCWHLDAAMRPSFLQLREQLEHIKTHELHL</t>
-  </si>
-  <si>
-    <t>MPGPAAGSRARVYAEVNSLRSREYWDYEAHVPSWGNQDDYQLVRKLGRGKYSEVFEAINITNNERVVVKILKPVKKKKIKREVKILENLRGGTNIIKLIDTVKDPVSKTPALVFEYINNTDFKQLYQILTDFDIRFYMYELLKALDYCHSKGIMHRDVKPHNVMIDHQQKKLRLIDWGLAEFYHPAQEYNVRVASRYFKGPELLVDYQMYDYSLDMWSLGCMLASMIFRREPFFHGQDNYDQLVRIAKVLGTEELYGYLKKYHIDLDPHFNDILGQHSRKRWENFIHSENRHLVSPEALDLLDKLLRYDHQQRLTAKEAMEHPYFYPVVKEQSQ</t>
-  </si>
-  <si>
-    <t>AAGAGGCAGTGGGCTTTGGAAGACTTTGAAATTGGTCGCCCTCTGGGTAAAGGAAAGTTTGGTAATGTTTATTTGGCAAGAGAAAAGCAAAGCAAGTTTATTCTGGCTCTTAAAGTGTTATTTAAAGCTCAGCTGGAGAAAGCCGGAGTGGAGCATCAGCTCAGAAGAGAAGTAGAAATACAGTCCCACCTTCGGCATCCTAATATTCTTAGACTGTATGGTTATTTCCATGATGCTACCAGAGTCTACCTAATTCTGGAATATGCACCACTTGGAACAGTTTATAGAGAACTTCAGAAACTTTCAAAGTTTGATGAGCAGAGAACTGCTACTTATATAACAGAATTGGCAAATGCCCTGTCTTACTGTCATTCGAAGAGAGTTATTCATAGAGACATTAAGCCAGAGAACTTACTTCTTGGATCAGCTGGAGAGCTTAAAATTGCAGATTTTGGGTGGTCAGTACATGCTCCATCTTCCAGGAGGACCACTCTCTGTGGCACCCTGGACTACCTGCCCCCTGAAATGATTGAAGGTCGGATGCATGATGAGAAGGTGGATCTCTGGAGCCTTGGAGTTCTTTGCTATGAATTTTTAGTTGGGAAGCCTCCTTTTGAGGCAAACACATACCAAGAGACCTACAAAAGAATATCACGGGTTGAATTCACATTCCCTGACTTTGTAACAGAGGGAGCCAGGGACCTCATTTCAAGACTGTTGAAGCATAATCCCAGCCAGAGGCCAATGCTCAGAGAAGTACTTGAACACCCCTGGATCACAGCAAATTCATCAAAACCATCA</t>
-  </si>
-  <si>
-    <t>ATGGAGCTACGTGTGGGGAACAAGTACCGCCTGGGACGGAAGATCGGGAGCGGGTCCTTCGGAGATATCTACCTGGGTGCCAACATCGCCTCTGGTGAGGAAGTCGCCATCAAGCTGGAGTGTGTGAAGACAAAGCACCCCCAGCTGCACATCGAGAGCAAGTTCTACAAGATGATGCAGGGTGGCGTGGGGATCCCGTCCATCAAGTGGTGCGGAGCTGAGGGCGACTACAACGTGATGGTCATGGAGCTGCTGGGGCCTAGCCTCGAGGACCTGTTCAACTTCTGTTCCCGCAAATTCAGCCTCAAGACGGTGCTGCTCTTGGCCGACCAGATGATCAGCCGCATCGAGTATATCCACTCCAAGAACTTCATCCACCGGGACGTCAAGCCCGACAACTTCCTCATGGGGCTGGGGAAGAAGGGCAACCTGGTCTACATCATCGACTTCGGCCTGGCCAAGAAGTACCGGGACGCCCGCACCCACCAGCACATTCCCTACCGGGAAAACAAGAACCTGACCGGCACGGCCCGCTACGCTTCCATCAACACGCACCTGGGCATTGAGCAAAGCCGTCGAGATGACCTGGAGAGCCTGGGCTACGTGCTCATGTACTTCAACCTGGGCTCCCTGCCCTGGCAGGGGCTCAAAGCAGCCACCAAGCGCCAGAAGTATGAACGGATCAGCGAGAAGAAGATGTCAACGCCCATCGAGGTCCTCTGCAAAGGCTATCCCTCCGAATTCTCAACATACCTCAACTTCTGCCGCTCCCTGCGGTTTGACGACAAGCCCGACTACTCTTACCTACGTCAGCTCTTCCGCAACCTCTTCCACCGGCAGGGCTTCTCCTATGACTACGTCTTTGACTGGAACATGCTGAAA</t>
-  </si>
-  <si>
-    <t>SVKGRIYSILKQIGSGGSSKVFQVLNEKKQIYAIKYVNLEEADNQTLDSYRNEIAYLNKLQQHSDKIIRLYDYEITDQYIYMVMECGNIDLNSWLKKKKSIDPWERKSYWKNMLEAVHTIHQHGIVHSDLKPANFLIVDGMLKLIDFGIANQMQPDTTSVVKDSQVGTVNYMPPEAIKDMSSSRENGKSKSKISPKSDVWSLGCILYYMTYGKTPFQQIINQISKLHAIIDPNHEIEFPDIPEKDLQDVLKCCLKRDPKQRISIPELLAHPYVQIQTHPVNQMAKGTTEE</t>
-  </si>
-  <si>
-    <t>SAADVYVPDEWEVAREKITMSRELGQGSFGMVYEGVAKGVVKDEPETRVAIKTVNEAASMRERIEFLNEASVMKEFNCHHVVRLLGVVSQGQPTLVIMELMTRGDLKSYLRSLRPEMENNPVLAPPSLSKMIQMAGEIADGMAYLNANKFVHRDLAARNCMVAEDFTVKIGDFGMTRDIYETDYYRKGGKGLLPVRWMSPESLKDGVFTTYSDVWSFGVVLWEIATLAEQPYQGLSNEQVLRFVMEGGLLDKPDNCPDMLFELMRMCWQYNPKMRPSFLEIISSIKEEMEPGFREVSFYYSEENK</t>
-  </si>
-  <si>
-    <t>TCAACCAGGGATTATGAGATTCAAAGAGAAAGAATAGAACTTGGACGATGTATTGGAGAAGGCCAATTTGGAGATGTACATCAAGGCATTTATATGAGTCCAGAGAATCCAGCTTTGGCGGTTGCAATTAAAACATGTAAAAACTGTACTTCGGACAGCGTGAGAGAGAAATTTCTTCAAGAAGCCTTAACAATGCGTCAGTTTGACCATCCTCATATTGTGAAGCTGATTGGAGTCATCACAGAGAATCCTGTCTGGATAATCATGGAGCTGTGCACACTTGGAGAGCTGAGGTCATTTTTGCAAGTAAGGAAATACAGTTTGGATCTAGCATCTTTGATCCTGTATGCCTATCAGCTTAGTACAGCTCTTGCATATCTAGAGAGCAAAAGATTTGTACACAGGGACATTGCTGCTCGGAATGTTCTGGTGTCCTCAAATGATTGTGTAAAATTAGGAGACTTTGGATTATCCCGATATATGGAAGATAGTACTTACTACAAAGCTTCCAAAGGAAAATTGCCTATTAAATGGATGGCTCCAGAGTCAATCAATTTTCGACGTTTTACCTCAGCTAGTGACGTATGGATGTTTGGTGTGTGTATGTGGGAGATACTGATGCATGGTGTGAAGCCTTTTCAAGGAGTGAAGAACAATGATGTAATCGGTCGAATTGAAAATGGGGAAAGATTACCAATGCCTCCAAATTGTCCTCCTACCCTCTACAGCCTTATGACGAAATGCTGGGCCTATGACCCCAGCAGGCGGCCCAGGTTTACTGAACTTAAAGCTCAGCTCAGCACAATCCTGGAGGAAGAGAAGGCTCAGCAAGAAGAG</t>
-  </si>
-  <si>
-    <t>GAGCACGTCCGCCGCGACCTGGACCCCAACGAGGTGTGGGAGATCGTGGGCGAGCTGGGCGACGGCGCCTTCGGCAAGGTTTACAAGGCCAAGAATAAGGAGACGGGTGCTTTGGCTGCGGCCAAAGTCATTGAAACCAAGAGTGAGGAGGAGCTGGAGGACTACATCGTGGAGATTGAGATCCTGGCCACCTGCGACCACCCCTACATTGTGAAGCTCCTGGGAGCCTACTATCACGACGGGAAGCTGTGGATCATGATTGAGTTCTGTCCAGGGGGAGCCGTGGACGCCATCATGCTGGAGCTGGACAGAGGCCTCACGGAGCCCCAGATACAGGTGGTTTGCCGCCAGATGCTAGAAGCCCTCAACTTCCTGCACAGCAAGAGGATCATCCACCGAGATCTGAAAGCTGGCAACGTGCTGATGACCCTCGAGGGAGACATCAGGCTGGCTGACTTTGGTGTGTCTGCCAAGAATCTGAAGACTCTACAGAAACGAGATTCCTTCATCGGCACGCCTTACTGGATGGCCCCCGAGGTGGTCATGTGTGAGACCATGAAAGACACGCCCTACGACTACAAAGCCGACATCTGGTCCCTGGGCATCACGCTGATTGAGATGGCCCAGATCGAGCCGCCACACCACGAGCTCAACCCCATGCGGGTCCTGCTAAAGATCGCCAAGTCAGACCCTCCCACGCTGCTCACGCCCTCCAAGTGGTCTGTAGAGTTCCGTGACTTCCTGAAGATAGCCCTGGATAAGAACCCAGAAACCCGACCCAGTGCCGCGCAGCTGCTGGAGCATCCCTTCGTCAGCAGCATCACCAGTAACAAGGCTCTGCGGGAGCTGGTGGCTGAGGCCAAGGCCGAGGTGATGGAA</t>
-  </si>
-  <si>
-    <t>DPEELFTKLEKIGKGSFGEVFKGIDNRTQKVVAIKIIDLEEAEDEIEDIQQEITVLSQCDSPYVTKYYGSYLKDTKLWIIMEYLGGGSALDLLEPGPLDETQIATILREILKGLDYLHSEKKIHRDIKAANVLLSEHGEVKLADFGVAGQLTDTQIKRNTFVGTPFWMAPEVIKQSAYDSKADIWSLGITAIELARGEPPHSELHPMKVLFLIPKNNPPTLEGNYSKPLKEFVEACLNKEPSFRPTAKELLKHKFILRNAKKTSYLTELID</t>
-  </si>
-  <si>
-    <t>MAPK3_HUMAN_D0_3FXW_A</t>
-  </si>
-  <si>
-    <t>AAGCAGTACGAACACGTGAAGAGGGACCTGAACCCCGAAGACTTTTGGGAGATTATAGGAGAACTGGGCGACGGAGCCTTTGGGAAAGTGTACAAGGCCCAGAATAAAGAGACCAGTGTTTTAGCTGCTGCAAAAGTGATTGACACTAAATCTGAAGAAGAACTTGAAGATTACATGGTAGAGATTGACATATTAGCATCTTGTGATCACCCAAATATAGTCAAGCTTCTAGATGCCTTCTATTATGAGAACAATCTTTGGATCCTCATTGAATTTTGTGCAGGTGGAGCAGTAGATGCTGTGATGCTTGAACTTGAGAGACCATTAACTGAGTCCCAAATACAAGTAGTTTGCAAGCAGACTTTAGATGCATTGAACTACTTACATGATAATAAGATCATCCACAGAGATCTGAAGGCTGGCAACATTCTCTTTACCTTAGATGGAGATATCAAATTGGCGGATTTTGGAGTATCAGCTAAAAACATGAGGACAATTCAAAGAAGAGATTCCTTTATTGGTACACCATATTGGATGGCTCCTGAAGTAGTCATGTGTGAAACATCTAAGGACAGACCCTATGACTACAAAGCTGATGTTTGGTCCCTGGGTATCACTTTAATAGAAATGGCTGAGATAGAACCACCTCATCATGAATTAAATCCAATGCGAGTGCTGCTAAAAATAGCAAAATCTGAGCCACCTACATTAGCACAGCCATCCAGATGGTCTTCAAATTTTAAGGACTTTCTAAAGAAATGCTTAGAAAAGAATGTGGATGCCAGGTGGACTACATCTCAGCTGCTGCAGCATCCCTTTGTTACTGTTGATTCCAACAAACCCATCCGAGAATTGATTGCAGAGGCGAAGGCTGAAGTAACAGAAGAAGTTGAAGATGGCAAAGAG</t>
-  </si>
-  <si>
-    <t>ATGCCTTCCCGGGCTGAGGACTATGAAGTGTTGTACACCATTGGCACAGGCTCCTACGGCCGCTGCCAGAAGATCCGGAGGAAGAGTGATGGCAAGATATTAGTTTGGAAAGAACTTGACTATGGCTCCATGACAGAAGCTGAGAAACAGATGCTTGTTTCTGAAGTGAATTTGCTTCGTGAACTGAAACATCCAAACATCGTTCGTTACTATGATCGGATTATTGACCGGACCAATACAACACTGTACATTGTAATGGAATATTGTGAAGGAGGGGATCTGGCTAGTGTAATTACAAAGGGAACCAAGGAAAGGCAATACTTAGATGAAGAGTTTGTTCTTCGAGTGATGACTCAGTTGACTCTGGCCCTGAAGGAATGCCACAGACGAAGTGATGGTGGTCATACCGTATTGCATCGGGATCTGAAACCAGCCAATGTTTTCCTGGATGGCAAGCAAAACGTCAAGCTTGGAGACTTTGGGCTAGCTAGAATATTAAACCATGACACGAGTTTTGCAAAAACATTTGTTGGCACACCTTATTACATGTCTCCTGAACAAATGAATCGCATGTCCTACAATGAGAAATCAGATATCTGGTCATTGGGCTGCTTGCTGTATGAGTTATGTGCATTAATGCCTCCATTTACAGCTTTTAGCCAGAAAGAACTCGCTGGGAAAATCAGAGAAGGCAAATTCAGGCGAATTCCATACCGTTACTCTGATGAATTGAATGAAATTATTACGAGGATGTTAAACTTAAAGGATTACCATCGACCTTCTGTTGAAGAAATTCTTGAGAACCCTTTAATA</t>
-  </si>
-  <si>
-    <t>AAGGAGAAGGAGCCCCTGGAGTCGCAGTACCAGGTGGGCCCGCTACTGGGCAGCGGCGGCTTCGGCTCGGTCTACTCAGGCATCCGCGTCTCCGACAACTTGCCGGTGGCCATCAAACACGTGGAGAAGGACCGGATTTCCGACTGGGGAGAGCTGCCTAATGGCACTCGAGTGCCCATGGAAGTGGTCCTGCTGAAGAAGGTGAGCTCGGGTTTCTCCGGCGTCATTAGGCTCCTGGACTGGTTCGAGAGGCCCGACAGTTTCGTCCTGATCCTGGAGAGGCCCGAGCCGGTGCAAGATCTCTTCGACTTCATCACGGAAAGGGGAGCCCTGCAAGAGGAGCTGGCCCGCAGCTTCTTCTGGCAGGTGCTGGAGGCCGTGCGGCACTGCCACAACTGCGGGGTGCTCCACCGCGACATCAAGGACGAAAACATCCTTATCGACCTCAATCGCGGCGAGCTCAAGCTCATCGACTTCGGGTCGGGGGCGCTGCTCAAGGACACCGTCTACACGGACTTCGATGGGACCCGAGTGTATAGCCCTCCAGAGTGGATCCGCTACCATCGCTACCATGGCAGGTCGGCGGCAGTCTGGTCCCTGGGGATCCTGCTGTATGATATGGTGTGTGGAGATATTCCTTTCGAGCATGACGAAGAGATCATCGGGGGCCAGGTTTTCTTCAGGCAGAGGGTCTCTTCAGAATGTCAGCATCTCATTAGATGGTGCTTGGCCCTGAGACCATCAGATAGGCCAACCTTCGAAGAAATCCAGAACCATCCATGGATGCAAGATGTTCTCCTGCCCCAGGAAACTGCTGAGATCCACCTCCACAGCCTGTCGCCGGGGCCCAGCAAA</t>
-  </si>
-  <si>
-    <t>GCCACCTGCACACGTTTCACCGACGACTACCAGCTCTTCGAGGAGCTTGGCAAGGGTGCTTTCTCTGTGGTCCGCAGGTGTGTGAAGAAAACCCCCACGCAGGAGTACGCAGCAAAAATCATCAATACCAAGAAATTGTCTGCCCGGGATCACCAGAAACTAGAACGTGAGGCTCGGATATGTCGACTTCTGAAACATCCAAACATCGTGCGCCTCCATGACAGTATTTCTGAAGAAGGGTTTCACTACCTCGTGTTTGACCTTGTTACCGGCGGGGAGCTGTTTGAAGACATTGTGGCCAGAGAGTACTACAGTGAAGCAGATGCCAGCCACTGTATACATCAGATTCTGGAGAGTGTTAACCACATCCACCAGCATGACATCGTCCACAGGGACCTGAAGCCTGAGAACCTGCTGCTGGCGAGTAAATGCAAGGGTGCCGCCGTCAAGCTGGCTGATTTTGGCCTAGCCATCGAAGTACAGGGAGAGCAGCAGGCTTGGTTTGGTTTTGCTGGCACCCCAGGTTACTTGTCCCCTGAGGTCTTGAGGAAAGATCCCTATGGAAAACCTGTGGATATCTGGGCCTGCGGGGTCATCCTGTATATCCTCCTGGTGGGCTATCCTCCCTTCTGGGATGAGGATCAGCACAAGCTGTATCAGCAGATCAAGGCTGGAGCCTATGATTTCCCATCACCAGAATGGGACACGGTAACTCCTGAAGCCAAGAACTTGATCAACCAGATGCTGACCATAAACCCAGCAAAGCGCATCACGGCTGACCAGGCTCTCAAGCACCCGTGGGTCTGTCAACGATCCACGGTGGCATCCATGATGCATCGTCAGGAGACTGTGGAGTGTTTGCGCAAGTTCAATGCCCGGAGAAAACTGAAGGGTGCCATCCTCACGACCATGCTTGTCTCCAGGAACTTCTCA</t>
-  </si>
-  <si>
-    <t>TVFRQENVDDYYDTGEELGSGQFAVVKKCREKSTGLQYAAKFIKKRRTKSSRRGVSREDIEREVSILKEIQHPNVITLHEVYENKTDVILILELVAGGELFDFLAEKESLTEEEATEFLKQTLNGVYYLHSLQIAHFDLKPENIMLLDRNVPKPRIKIIDFGLAHKIDFGNEFKNIFGTPEFVAPEIVNYEPLGLEADMWSIGVITYILLSGASPFLGDTKQETLANVSAVNYEFEDEYFSNTSALAKDFIRRLLVKDPKKRMTIQDSLQHPWIKPKDTQQALS</t>
-  </si>
-  <si>
-    <t>MK14_HUMAN_D0_3K3J_A</t>
-  </si>
-  <si>
-    <t>GATGAACAACCTCACATCGGAAACTACAGACTGTTGAAAACAATCGGCAAGGGGAATTTTGCAAAAGTAAAATTGGCAAGACATATCCTTACAGGCAGAGAGGTTGCAATAAAAATAATTGACAAAACTCAGTTGAATCCAACAAGTCTACAAAAGCTCTTCAGAGAAGTAAGAATAATGAAGATTTTAAATCATCCCAATATAGTGAAGTTATTCGAAGTCATTGAAACTGAAAAAACACTCTACCTAATCATGGAATATGCAAGTGGAGGTGAAGTATTTGACTATTTGGTTGCACATGGCAGGATGAAGGAAAAAGAAGCAAGATCTAAATTTAGACAGATTGTGTCTGCAGTTCAATACTGCCATCAGAAACGGATCGTACATCGAGACCTCAAGGCTGAAAATCTATTGTTAGATGCCGATATGAACATTAAAATAGCAGATTTCGGTTTTAGCAATGAATTTACTGTTGGCGGTAAACTCGACACGTTTTGTGGCAGTCCTCCATACGCAGCACCTGAGCTCTTCCAGGGCAAGAAATATGACGGGCCAGAAGTGGATGTGTGGAGTCTGGGGGTCATTTTATACACACTAGTCAGTGGCTCACTTCCCTTTGATGGGCAAAACCTAAAGGAACTGAGAGAGAGAGTATTAAGAGGGAAATACAGAATTCCCTTCTACATGTCTACAGACTGTGAAAACCTTCTCAAACGTTTCCTGGTGCTAAATCCAATTAAACGCGGCACTCTAGAGCAAATCATGAAGGACAGGTGGATCAATGCAGGGCATGAAGAAGATGAACTCAAACCATTTGTTGAACCAGAGCTAGACATCTCAGACCAAAAAAGAATAGATATTATGGTGGGAATGGGATATTCACAAGAAGAAATTCAAGAATCTCTTAGTAAGATGAAATACGATGAAATCACAGCTACATATTTGTTATTGGGGAGAAAATCTTCAGAG</t>
-  </si>
-  <si>
-    <t>CACCAGCTGCAGCCCCGGCGGGTGTCATTCCGGGGCGAGGCCTCAGAGACTCTGCAGAGCCCTGGGTATGACCCAAGCCGGCCAGAGTCCTTCTTCCAGCAGAGCTTCCAGAGGCTCAGCCGCCTGGGCCATGGCTCCTACGGAGAGGTCTTCAAGGTGCGCTCCAAGGAGGACGGCCGGCTCTATGCGGTAAAGCGTTCCATGTCACCATTCCGGGGCCCCAAGGACCGGGCCCGCAAGTTGGCCGAGGTGGGCAGCCACGAGAAGGTGGGGCAGCACCCATGCTGCGTGCGGCTGGAGCAGGCCTGGGAGGAGGGCGGCATCCTGTACCTGCAGACGGAGCTGTGCGGGCCCAGCCTGCAGCAACACTGTGAGGCCTGGGGTGCCAGCCTGCCTGAGGCCCAGGTCTGGGGCTACCTGCGGGACACGCTGCTTGCCCTGGCCCATCTGCACAGCCAGGGCCTGGTGCACCTTGATGTCAAGCCTGCCAACATCTTCCTGGGGCCCCGGGGCCGCTGCAAGCTGGGTGACTTCGGACTGCTGGTGGAGCTGGGTACAGCAGGAGCTGGTGAGGTCCAGGAGGGAGACCCCCGCTACATGGCCCCCGAGCTGCTGCAGGGCTCCTATGGGACAGCAGCGGATGTGTTCAGTCTGGGCCTCACCATCCTGGAAGTGGCATGCAACATGGAGCTGCCCCACGGTGGGGAGGGCTGGCAGCAGCTGCGCCAGGGCTACCTGCCCCCTGAGTTCACTGCCGGTCTGTCTTCCGAGCTGCGTTCTGTCCTTGTCATGATGCTGGAGCCAGACCCCAAGCTGCGGGCCACGGCCGAGGCCCTGCTGGCACTGCCTGTGTTGAGGCAGCCG</t>
-  </si>
-  <si>
-    <t>SSVTASAAPGTASLVPDYWIDGSNRDALSDFFEVESELGRGATSIVYRCKQKGTQKPYALKVLKKTVDKKIVRTEIGVLLRLSHPNIIKLKEIFETPTEISLVLELVTGGELFDRIVEKGYYSERDAADAVKQILEAVAYLHENGIVHRDLKPENLLYATPAPDAPLKIADFGLSKIVEHQVLMKTVCGTPGYCAPEILRGCAYGPEVDMWSVGIITYILLCGFEPFYDERGDQFMFRRILNCEYYFISPWWDEVSLNAKDLVRKLIVLDPKKRLTTFQALQHPWVTGKAANFVHMDTAQKKLQEFNARRKLKAAVKAVVASSRLG</t>
-  </si>
-  <si>
-    <t>KEKEPLESQYQVGPLLGSGGFGSVYSGIRVSDNLPVAIKHVEKDRISDWGELPNGTRVPMEVVLLKKVSSGFSGVIRLLDWFERPDSFVLILERPEPVQDLFDFITERGALQEELARSFFWQVLEAVRHCHNCGVLHRDIKDENILIDLNRGELKLIDFGSGALLKDTVYTDFDGTRVYSPPEWIRYHRYHGRSAAVWSLGILLYDMVCGDIPFEHDEEIIGGQVFFRQRVSSECQHLIRWCLALRPSDRPTFEEIQNHPWMQDVLLPQETAEIHLHSLSPGPSK</t>
-  </si>
-  <si>
-    <t>VEDHYEMGEELGSGQFAIVRKCRQKGTGKEYAAKFIKKRRLSSSRRGVSREEIEREVNILREIRHPNIITLHDIFENKTDVVLILELVSGGELFDFLAEKESLTEDEATQFLKQILDGVHYLHSKRIAHFDLKPENIMLLDKNVPNPRIKLIDFGIAHKIEAGNEFKNIFGTPEFVAPEIVNYEPLGLEADMWSIGVITYILLSGASPFLGETKQETLTNISAVNYDFDEEYFSNTSELAKDFIRRLLVKDPKRRMTIAQSLEHSWIKAIRRRNVRGEDSG</t>
-  </si>
-  <si>
-    <t>TDEYQLFEELGKGAFSVVRRCMKIPTGQEYAAKIINTKKLSARDHQKLEREARICRLLKHPNIVRLHDSISEEGFHYLVFDLVTGGELFEDIVAREYYSEADASHCIQQILESVNHCHLNGIVHRDLKPENLLLASKSKGAAVKLADFGLAIEVQGDQQAWFGFAGTPGYLSPEVLRKDPYGKPVDMWACGVILYILLVGYPPFWDEDQHRLYQQIKAGAYDFPSPEWDTVTPEAKDLINKMLTINPAKRITASEALKHPWICQRSTVASMMHRQETVDCLKKFNARRKLKGAILTTML</t>
-  </si>
-  <si>
-    <t>GCTGATCCAGAAGAACTGTTCACAAAATTAGAGCGCATTGGGAAAGGCTCATTTGGGGAAGTTTTCAAAGGAATTGATAACCGTACCCAGCAAGTCGTTGCTATTAAAATCATAGACCTTGAGGAAGCCGAAGATGAAATAGAAGACATTCAGCAAGAAATAACTGTCTTGAGTCAATGTGACAGCTCATATGTAACAAAATACTATGGGTCATATTTAAAGGGGTCTAAATTATGGATAATAATGGAATACCTGGGCGGTGGTTCAGCACTGGATCTTCTTCGAGCTGGTCCATTTGATGAGTTCCAGATTGCTACCATGCTAAAGGAAATTTTAAAAGGTCTGGACTATCTGCATTCAGAAAAGAAAATTCACCGAGACATAAAAGCTGCCAATGTCTTGCTCTCAGAACAAGGAGATGTTAAACTTGCTGATTTTGGAGTTGCTGGTCAGCTGACAGATACACAGATTAAAAGAAATACCTTTGTGGGAACTCCATTTTGGATGGCTCCTGAAGTTATTCAACAGTCAGCTTATGACTCAAAAGCTGACATTTGGTCATTGGGAATTACTGCTATTGAACTAGCCAAGGGAGAGCCACCTAACTCCGATATGCATCCAATGAGAGTTCTGTTTCTTATTCCCAAAAACAATCCTCCAACTCTTGTTGGAGACTTTACTAAGTCTTTTAAGGAGTTTATTGATGCTTGCCTGAACAAAGATCCATCATTTCGTCCTACAGCAAAAGAACTTCTGAAACACAAATTCATTGTAAAAAATTCAAAGAAGACTTCTTATCTGACTGAACTGATAGATCGTTTTAAGAGATGGAAGGCAGAA</t>
-  </si>
-  <si>
-    <t>MET_HUMAN_D0_4EEV_A</t>
-  </si>
-  <si>
-    <t>MSSFLPEGGCYELLTVIGKGFEDLMTVNLARYKPTGEYVTVRRINLEACSNEMVTFLQGELHVSKLFNHPNIVPYRATFIADNELWVVTSFMAYGSAKDLICTHFMDGMNELAIAYILQGVLKALDYIHHMGYVHRSVKASHILISVDGKVYLSGLRSNLSMISHGQRQRVVHDFPKYSVKVLPWLSPEVLQQNLQGYDAKSDIYSVGITACELANGHVPFKDMPATQMLLEKLNGTVPCLLDTSTIPAEELTMSPSRSVANSGLSDSLTTSTPRPSNGDSPSHPYHRTFSPHFHHFVEQCLQRNPDARPSASTLLNHSFFKQIKRRASEVLPELLRPVTPITNFEGSQSQDHSGIFGLVTNLEELEVDDWEF</t>
-  </si>
-  <si>
-    <t>MP2K1_HUMAN_D0_3MBL_A</t>
-  </si>
-  <si>
-    <t>ATGTCGGGACCCGTGCCAAGCAGGGCCAGAGTTTACACAGATGTTAATACACACAGACCTCGAGAATACTGGGATTACGAGTCACATGTGGTGGAATGGGGAAATCAAGATGACTACCAGCTGGTTCGAAAATTAGGCCGAGGTAAATACAGTGAAGTATTTGAAGCCATCAACATCACAAATAATGAAAAAGTTGTTGTTAAAATTCTCAAGCCAGTAAAAAAGAAGAAAATTAAGCGTGAAATAAAGATTTTGGAGAATTTGAGAGGAGGTCCCAACATCATCACACTGGCAGACATTGTAAAAGACCCTGTGTCACGAACCCCCGCCTTGGTTTTTGAACACGTAAACAACACAGACTTCAAGCAATTGTACCAGACGTTAACAGACTATGATATTCGATTTTACATGTATGAGATTCTGAAGGCCCTGGATTATTGTCACAGCATGGGAATTATGCACAGAGATGTCAAGCCCCATAATGTCATGATTGATCATGAGCACAGAAAGCTACGACTAATAGACTGGGGTTTGGCTGAGTTTTATCATCCTGGCCAAGAATATAATGTCCGAGTTGCTTCCCGATACTTCAAAGGTCCTGAGCTACTTGTAGACTATCAGATGTACGATTATAGTTTGGATATGTGGAGTTTGGGTTGTATGCTGGCAAGTATGATCTTTCGGAAGGAGCCATTTTTCCATGGACATGACAATTATGATCAGTTGGTGAGGATAGCCAAGGTTCTGGGGACAGAAGATTTATATGACTATATTGACAAATACAACATTGAATTAGATCCACGTTTCAATGATATCTTGGGCAGACACTCTCGAAAGCGATGGGAACGCTTTGTCCACAGTGAAAATCAGCACCTTGTCAGCCCTGAGGCCTTGGATTTCCTGGACAAACTGCTGCGATATGACCACCAGTCACGGCTTACTGCAAGAGAGGCAATGGAGCACCCCTATTTCTACACTGTTGTGAAGGACCAGGCTCGAATGGGT</t>
-  </si>
-  <si>
-    <t>CDKL1_HUMAN_D0_4AGU_C</t>
-  </si>
-  <si>
-    <t>MARK3_HUMAN_D0_2QNJ_A</t>
-  </si>
-  <si>
-    <t>NLVFSDGYVVKETIGVGSYSECKRCVHKATNMEYAVKVIDKSKRDPSEEIEILLRYGQHPNIITLKDVYDDGKHVYLVTELMRGGELLDKILRQKFFSEREASFVLHTIGKTVEYLHSQGVVHRDLKPSNILYVDESGNPECLRICDFGFAKQLRAENGLLMTPCYTANFVAPEVLKRQGYDEGCDIWSLGILLYTMLAGYTPFANGPSDTPEEILTRIGSGKFTLSGGNWNTVSETAKDLVSKMLHVDPHQRLTAKQVLQHPWVTQKDKLPQSQLSHQDLQLVKGAMAATYSALNSSKPTPQLKPIESSILAQRRVRKLPSTTL</t>
-  </si>
-  <si>
-    <t>CCACAGTATGGCATTGCCCGTGAAGATGTGGTCCTGAATCGTATTCTTGGGGAAGGCTTTTTTGGGGAGGTCTATGAAGGTGTCTACACAAATCATAAAGGGGAGAAAATCAATGTAGCTGTCAAGACCTGCAAGAAAGACTGCACTCTGGACAACAAGGAGAAGTTCATGAGCGAGGCAGTGATCATGAAGAACCTCGACCACCCGCACATCGTGAAGCTGATCGGCATCATTGAAGAGGAGCCCACCTGGATCATCATGGAATTGTATCCCTATGGGGAGCTGGGCCACTACCTGGAGCGGAACAAGAACTCCCTGAAGGTGCTCACCCTCGTGCTGTACTCACTGCAGATATGCAAAGCCATGGCCTACCTGGAGAGCATCAACTGCGTGCACAGGGACATTGCTGTCCGGAACATCCTGGTGGCCTCCCCTGAGTGTGTGAAGCTGGGGGACTTTGGTCTTTCCCGGTACATTGAGGACGAGGACTATTACAAAGCCTCTGTGACTCGTCTCCCCATCAAATGGATGTCCCCAGAGTCCATTAACTTCCGACGCTTCACGACAGCCAGTGACGTCTGGATGTTCGCCGTGTGCATGTGGGAGATCCTGAGCTTTGGGAAGCAGCCCTTCTTCTGGCTGGAGAACAAGGATGTCATCGGGGTGCTGGAGAAAGGAGACCGGCTGCCCAAGCCTGATCTCTGTCCACCGGTCCTTTATACCCTCATGACCCGCTGCTGGGACTACGACCCCAGTGACCGGCCCCGCTTCACCGAGCTGGTGTGCAGCCTCAGTGACGTTTATCAGATGGAGAAGGACATTGCCATGGAG</t>
-  </si>
-  <si>
-    <t>GVVTHEQFKAALRMVVDQGDPRLLLDSYVKIGEGSTGIVCLAREKHSGRQVAVKMMDLRKQQRRELLFNEVVIMRDYQHFNVVEMYKSYLVGEELWVLMEFLQGGALTDIVSQVRLNEEQIATVCEAVLQALAYLHAQGVIHRDIKSDSILLTLDGRVKLSDFGFCAQISKDVPKRKSLVGTPYWMAPEVISRSLYATEVDIWSLGIMVIEMVDGEPPYFSDSPVQAMKRLRDSPPPKLKNSHKVSPVLRDFLERMLVRDPQERATAQELLDHPFLLQTGLPECLVPLIQLYRKQTSTC</t>
-  </si>
-  <si>
-    <t>GGTGTTGTGACACATGAGCAGTTCAAGGCTGCGCTCAGGATGGTGGTGGACCAGGGTGACCCCCGGCTGCTGCTGGACAGCTACGTGAAGATTGGCGAGGGCTCCACCGGCATCGTCTGCTTGGCCCGGGAGAAGCACTCGGGCCGCCAGGTGGCCGTCAAGATGATGGACCTCAGGAAGCAGCAGCGCAGGGAGCTGCTCTTCAACGAGGTGGTGATCATGCGGGACTACCAGCACTTCAACGTGGTGGAGATGTACAAGAGCTACCTGGTGGGCGAGGAGCTGTGGGTGCTCATGGAGTTCCTGCAGGGAGGAGCCCTCACAGACATCGTCTCCCAAGTCAGGCTGAATGAGGAGCAGATTGCCACTGTGTGTGAGGCTGTGCTGCAGGCCCTGGCCTACCTGCATGCTCAGGGTGTCATCCACCGGGACATCAAGAGTGACTCCATCCTGCTGACCCTCGATGGCAGGGTGAAGCTCTCGGACTTCGGATTCTGTGCTCAGATCAGCAAAGACGTCCCTAAGAGGAAGTCCCTGGTGGGAACCCCCTACTGGATGGCTCCTGAAGTGATCTCCAGGTCTTTGTATGCCACTGAGGTGGATATCTGGTCTCTGGGCATCATGGTGATTGAGATGGTAGATGGGGAGCCACCGTACTTCAGTGACTCCCCAGTGCAAGCCATGAAGAGGCTCCGGGACAGCCCCCCACCCAAGCTGAAAAACTCTCACAAGGTCTCCCCAGTGCTGCGAGACTTCCTGGAGCGGATGCTGGTGCGGGACCCCCAAGAGAGAGCCACAGCCCAGGAGCTCCTAGACCACCCCTTCCTGCTGCAGACAGGGCTACCTGAGTGCCTGGTGCCCCTGATCCAGCTCTACCGAAAGCAGACCTCCACCTGC</t>
-  </si>
-  <si>
-    <t>CACATTGGAAACTACCGGCTCCTCAAGACCATTGGCAAGGGTAATTTTGCCAAGGTGAAGTTGGCCCGACACATCCTGACTGGGAAAGAGGTAGCTGTGAAGATCATTGACAAGACTCAACTGAACTCCTCCAGCCTCCAGAAACTATTCCGCGAAGTAAGAATAATGAAGGTTTTGAATCATCCCAACATAGTTAAATTATTTGAAGTGATTGAGACTGAGAAAACGCTCTACCTTGTCATGGAGTACGCTAGTGGCGGAGAGGTATTTGATTACCTAGTGGCTCATGGCAGGATGAAAGAAAAAGAGGCTCGAGCCAAATTCCGCCAGATAGTGTCTGCTGTGCAGTACTGTCACCAGAAGTTTATTGTCCATAGAGACTTAAAGGCAGAAAACCTGCTCTTGGATGCTGATATGAACATCAAGATTGCAGACTTTGGCTTCAGCAATGAATTCACCTTTGGGAACAAGCTGGACACCTTCTGTGGCAGTCCCCCTTATGCTGCCCCAGAACTCTTCCAGGGCAAAAAATATGATGGACCCGAGGTGGATGTGTGGAGCCTAGGAGTTATCCTCTATACACTGGTCAGCGGATCCCTGCCTTTTGATGGACAGAACCTCAAGGAGCTGCGGGAACGGGTACTGAGGGGAAAATACCGTATTCCATTCTACATGTCCACGGACTGTGAAAACCTGCTTAAGAAATTTCTCATTCTTAATCCCAGCAAGAGAGGCACTTTAGAGCAAATCATGAAAGATCGATGGATGAATGTGGGTCACGAAGATGATGAACTAAAGCCTTACGTGGAGCCACTCCCTGACTACAAGGACCCCCGGCGGACAGAGCTGATGGTGTCCATGGGTTATACACGGGAAGAGATCCAGGACTCGCTGGTGGGCCAGAGATACAACGAGGTGATGGCCACCTATCTGCTCCTGGGCTAC</t>
-  </si>
-  <si>
-    <t>ST17B_HUMAN_D0_3LM0_A</t>
-  </si>
-  <si>
-    <t>GDSDISSPLLQNTVHIDLSALNPELVQAVQHVVIGPSSLIVHFNEVIGRGHFGCVYHGTLLDNDGKKIHCAVKSLNRITDIGEVSQFLTEGIIMKDFSHPNVLSLLGICLRSEGSPLVVLPYMKHGDLRNFIRNETHNPTVKDLIGFGLQVAKGMKYLASKKFVHRDLAARNCMLDEKFTVKVADFGLARDMYDKEYYSVHNKTGAKLPVKWMALESLQTQKFTTKSDVWSFGVLLWELMTRGAPPYPDVNTFDITVYLLQGRRLLQPEYCPDPLYEVMLKCWHPKAEMRPSFSELVSRISAIFSTFIG</t>
-  </si>
-  <si>
-    <t>ATGAGCGACAGTAAATGTGACAGTCAGTTTTATAGTGTGCAAGTGGCAGACTCAACCTTCACTGTCCTAAAACGTTACCAGCAGCTGAAACCAATTGGCTCTGGGGCCCAAGGGATTGTTTGTGCTGCATTTGATACAGTTCTTGGGATAAATGTTGCAGTCAAGAAACTAAGCCGTCCTTTTCAGAACCAAACTCATGCAAAGAGAGCTTATCGTGAACTTGTCCTCTTAAAATGTGTCAATCATAAAAATATAATTAGTTTGTTAAATGTGTTTACACCACAAAAAACTCTAGAAGAATTTCAAGATGTGTATTTGGTTATGGAATTAATGGATGCTAACTTATGTCAGGTTATTCACATGGAGCTGGATCATGAAAGAATGTCCTACCTTCTTTACCAGATGCTTTGTGGTATTAAACATCTGCATTCAGCTGGTATAATTCATAGAGATTTGAAGCCTAGCAACATTGTTGTGAAATCAGACTGCACCCTGAAGATCCTTGACTTTGGCCTGGCCCGGACAGCGTGCACTAACTTCATGATGACCCCTTACGTGGTGACACGGTACTACCGGGCGCCCGAAGTCATCCTGGGTATGGGCTACAAAGAGAACGTGGACATCTGGTCTGTCGGGTGCATCATGGCAGAAATGGTCCTCCATAAAGTCCTGTTCCCGGGAAGAGACTATATTGATCAGTGGAATAAAGTTATTGAGCAGCTGGGAACACCATCAGCAGAGTTCATGAAGAAACTTCAGCCAACTGTGAGGAATTATGTCGAAAACAGACCAAAGTATCCTGGAATCAAATTTGAAGAACTCTTTCCAGATTGGATATTCCCATCAGAATCTGAGCGAGACAAAATAAAAACAAGTCAAGCCAGAGATCTGTTATCAAAAATGTTAGTGATTGATCCTGACAAGCGGATCTCTGTAGACGAAGCTCTGCGTCACCCATACATCACTGTTTGGTATGACCCCGCCGAAGCAGAAGCCCCACCACCTCAAATTTATGATGCCCAGTTGGAAGAAAGAGAACATGCAATTGAAGAATGGAAAGAGCTAATTTACAAAGAAGTCATGGATTGGGAA</t>
-  </si>
-  <si>
-    <t>ATGAGTAGCTTTCTGCCAGAGGGAGGGTGTTACGAGCTGCTCACTGTGATAGGCAAAGGATTTGAGGACCTGATGACTGTGAATCTAGCAAGGTACAAACCAACAGGAGAGTACGTGACTGTACGGAGGATTAACCTAGAAGCTTGTTCCAATGAGATGGTAACATTCTTGCAGGGCGAGCTGCATGTCTCCAAACTCTTCAACCATCCCAATATCGTGCCATATCGAGCCACTTTTATTGCAGACAATGAGCTGTGGGTTGTCACATCATTCATGGCATACGGTTCTGCAAAAGATCTCATCTGTACACACTTCATGGATGGCATGAATGAGCTGGCGATTGCTTACATCCTGCAGGGGGTGCTGAAGGCCCTCGACTACATCCACCACATGGGATATGTACACAGGAGTGTCAAAGCCAGCCACATCCTGATCTCTGTGGATGGGAAGGTCTACCTGTCTGGTTTGCGCAGCAACCTCAGCATGATAAGCCATGGGCAGCGGCAGCGAGTGGTCCACGATTTTCCCAAGTACAGTGTCAAGGTTCTGCCGTGGCTCAGCCCCGAGGTCCTCCAGCAGAATCTCCAGGGTTATGATGCCAAGTCTGACATCTACAGTGTGGGAATCACAGCCTGTGAACTGGCCAACGGCCATGTCCCCTTTAAGGATATGCCTGCCACCCAGATGCTGCTAGAGAAACTGAACGGCACAGTGCCCTGCCTGTTGGATACCAGCACCATCCCCGCTGAGGAGCTGACCATGAGCCCTTCGCGCTCAGTGGCCAACTCTGGCCTGAGTGACAGCCTGACCACCAGCACCCCCCGGCCCTCCAACGGTGACTCGCCCTCCCACCCCTACCACCGAACCTTCTCCCCCCACTTCCACCACTTTGTGGAGCAGTGCCTTCAGCGCAACCCGGATGCCAGGCCCAGTGCCAGCACCCTCCTGAACCACTCTTTCTTCAAGCAGATCAAGCGACGTGCCTCAGAGGTTTTGCCCGAATTGCTTCGTCCTGTCACCCCCATCACCAATTTTGAGGGCAGCCAGTCTCAGGACCACAGTGGAATCTTTGGCCTGGTAACAAACCTGGAAGAGCTGGAGGTGGACGATTGGGAGTTC</t>
-  </si>
-  <si>
-    <t>ADPEELFTKLERIGKGSFGEVFKGIDNRTQQVVAIKIIDLEEAEDEIEDIQQEITVLSQCDSSYVTKYYGSYLKGSKLWIIMEYLGGGSALDLLRAGPFDEFQIATMLKEILKGLDYLHSEKKIHRDIKAANVLLSEQGDVKLADFGVAGQLTDTQIKRNTFVGTPFWMAPEVIQQSAYDSKADIWSLGITAIELAKGEPPNSDMHPMRVLFLIPKNNPPTLVGDFTKSFKEFIDACLNKDPSFRPTAKELLKHKFIVKNSKKTSYLTELIDRFKRWKAE</t>
-  </si>
-  <si>
-    <t>AACCAGTTCTACAGTGTGGAAGTGGGAGACTCAACCTTCACAGTTCTCAAGCGCTACCAGAATCTAAAGCCTATTGGCTCTGGGGCTCAGGGCATAGTTTGTGCCGCGTATGATGCTGTCCTTGACAGAAATGTGGCCATTAAGAAGCTCAGCAGACCCTTTCAGAACCAAACACATGCCAAGAGAGCGTACCGGGAGCTGGTCCTCATGAAGTGTGTGAACCATAAAAACATTATTAGTTTATTAAATGTCTTCACACCCCAGAAAACGCTGGAGGAGTTCCAAGATGTTTACTTAGTAATGGAACTGATGGATGCCAACTTATGTCAAGTGATTCAGATGGAATTAGACCATGAGCGAATGTCTTACCTGCTGTACCAAATGTTGTGTGGCATTAAGCACCTCCATTCTGCTGGAATTATTCACAGGGATTTAAAACCAAGTAACATTGTAGTCAAGTCTGATTGCACATTGAAAATCCTGGACTTTGGACTGGCCAGGACAGCAGGCACAAGCTTCATGATGACTCCATATGTGGTGACACGTTATTACAGAGCCCCTGAGGTCATCCTGGGGATGGGCTACAAGGAGAACGTGGATATATGGTCTGTGGGATGCATTATGGGAGAAATGGTTCGCCACAAAATCCTCTTTCCAGGAAGGGACTATATTGACCAGTGGAATAAGGTAATTGAACAACTAGGAACACCATGTCCAGAATTCATGAAGAAATTGCAACCCACAGTAAGAAACTATGTGGAGAATCGGCCCAAGTATGCGGGACTCACCTTCCCCAAACTCTTCCCAGATTCCCTCTTCCCAGCGGACTCCGAGCACAATAAACTCAAAGCCAGCCAAGCCAGGGACTTGTTGTCAAAGATGCTAGTGATTGACCCAGCAAAAAGAATATCAGTGGACGACGCCTTACAGCATCCCTACATCAACGTCTGGTATGACCCAGCCGAAGTGGAGGCGCCTCCACCTCAGATATATGACAAGCAGTTGGATGAAAGAGAACACACAATTGAAGAATGGAAAGAACTTATCTACAAGGAAGTAATGAAT</t>
-  </si>
-  <si>
-    <t>HIGNYRLLKTIGKGNFAKVKLARHILTGKEVAVKIIDKTQLNSSSLQKLFREVRIMKVLNHPNIVKLFEVIETEKTLYLVMEYASGGEVFDYLVAHGRMKEKEARAKFRQIVSAVQYCHQKFIVHRDLKAENLLLDADMNIKIADFGFSNEFTFGNKLDTFCGSPPYAAPELFQGKKYDGPEVDVWSLGVILYTLVSGSLPFDGQNLKELRERVLRGKYRIPFYMSTDCENLLKKFLILNPSKRGTLEQIMKDRWMNVGHEDDELKPYVEPLPDYKDPRRTELMVSMGYTREEIQDSLVGQRYNEVMATYLLLGY</t>
-  </si>
-  <si>
-    <t>ILK_HUMAN_D0_3KMW_A</t>
-  </si>
-  <si>
-    <t>DAPK2_HUMAN_D0_1WMK_C</t>
-  </si>
-  <si>
-    <t>ATGGCAAAGCAGTACGACTCGGTGGAGTGCCCTTTTTGTGATGAAGTTTCCAAATACGAGAAGCTCGCCAAGATCGGCCAAGGCACCTTCGGGGAGGTGTTCAAGGCCAGGCACCGCAAGACCGGCCAGAAGGTGGCTCTGAAGAAGGTGCTGATGGAAAACGAGAAGGAGGGGTTCCCCATTACAGCCTTGCGGGAGATCAAGATCCTTCAGCTTCTAAAACACGAGAATGTGGTCAACTTGATTGAGATTTGTCGAACCAAAGCTTCCCCCTATAACCGCTGCAAGGGTAGTATATACCTGGTGTTCGACTTCTGCGAGCATGACCTTGCTGGGCTGTTGAGCAATGTTTTGGTCAAGTTCACGCTGTCTGAGATCAAGAGGGTGATGCAGATGCTGCTTAACGGCCTCTACTACATCCACAGAAACAAGATCCTGCATAGGGACATGAAGGCTGCTAATGTGCTTATCACTCGTGATGGGGTCCCGAAGCTGGCAGACTTTGGGCTGGCCCGGGCCTTCAGCCTGGCCAAGAACAGCCAGCCCAACCGCTACACCAACCGTGTGGTGACACTCTGGTACCGGCCCCCGGAGCTGTTGCTCGGGGAGCGGGACTACGGCCCCCCCATTGACCTGTGGGGTGCTGGGTGCATCATGGCAGAGATGTGGACCCGCAGCCCCATCATGCAGGGCAACACGGAGCAGCACCAACTCGCCCTCATCAGTCAGCTCTGCGGCTCCATCACCCCTGAGGTGTGGCCAAACGTGGACAACTATGAGCTGTACGAAAAGCTGGAGCTGGTCAAGGGCCAGAAGCGGAAGGTGAAGGACAGGCTGAAGGCCTATGTGCGTGACCCATACGCACTGGACCTCATCGACAAGCTGCTGGTGCTGGACCCTGCCCAGCGCATCGACAGCGATGACGCCCTCAACCACGACTTCTTCTGGTCCGACCCCATGCCCTCCGACCTCAAGGGCATGCTCTCCACC</t>
-  </si>
-  <si>
-    <t>PQYGIAREDVVLNRILGEGFFGEVYEGVYTNHKGEKINVAVKTCKKDCTLDNKEKFMSEAVIMKNLDHPHIVKLIGIIEEEPTWIIMELYPYGELGHYLERNKNSLKVLTLVLYSLQICKAMAYLESINCVHRDIAVRNILVASPECVKLGDFGLSRYIEDEDYYKASVTRLPIKWMSPESINFRRFTTASDVWMFAVCMWEILSFGKQPFFWLENKDVIGVLEKGDRLPKPDLCPPVLYTLMTRCWDYDPSDRPRFTELVCSLSDVYQMEKDIAME</t>
-  </si>
-  <si>
-    <t>M3K5_HUMAN_D0_3VW6_A</t>
-  </si>
-  <si>
-    <t>MSQERPTFYRQELNKTIWEVPERYQNLSPVGSGAYGSVCAAFDTKTGLRVAVKKLSRPFQSIIHAKRTYRELRLLKHMKHENVIGLLDVFTPARSLEEFNDVYLVTHLMGADLNNIVKCQKLTDDHVQFLIYQILRGLKYIHSADIIHRDLKPSNLAVNEDCELKILDFGLARHTDDEMTGYVATRWYRAPEIMLNWMHYNQTVDIWSVGCIMAELLTGRTLFPGTDHIDQLKLILRLVGTPGAELLKKISSESARNYIQSLTQMPKMNFANVFIGANPLAVDLLEKMLVLDSDKRITAAQALAHAYFAQYHDPDDEPVADPYDQSFESRDLLIDEWKSLTYDEVISFVPPPLDQEEMES</t>
-  </si>
-  <si>
-    <t>MELRVGNRYRLGRKIGSGSFGDIYLGTDIAAGEEVAIKLECVKTKHPQLHIESKIYKMMQGGVGIPTIRWCGAEGDYNVMVMELLGPSLEDLFNFCSRKFSLKTVLLLADQMISRIEYIHSKNFIHRDVKPDNFLMGLGKKGNLVYIIDFGLAKKYRDARTHQHIPYRENKNLTGTARYASINTHLGIEQSRRDDLESLGYVLMYFNLGSLPWQGLKAATKRQKYERISEKKMSTPIEVLCKGYPSEFATYLNFCRSLRFDDKPDYSYLRQLFRNLFHRQGFSYDYVFDWNMLK</t>
-  </si>
-  <si>
-    <t>MAKQYDSVECPFCDEVSKYEKLAKIGQGTFGEVFKARHRKTGQKVALKKVLMENEKEGFPITALREIKILQLLKHENVVNLIEICRTKASPYNRCKGSIYLVFDFCEHDLAGLLSNVLVKFTLSEIKRVMQMLLNGLYYIHRNKILHRDMKAANVLITRDGVPKLADFGLARAFSLAKNSQPNRYTNRVVTLWYRPPELLLGERDYGPPIDLWGAGCIMAEMWTRSPIMQGNTEQHQLALISQLCGSITPEVWPNVDNYELYEKLELVKGQKRKVKDRLKAYVRDPYALDLIDKLLVLDPAQRIDSDDALNHDFFWSDPMPSDLKGMLST</t>
-  </si>
-  <si>
-    <t>AGCGCCCTGCCCTGGTCCATCAACAGGGACGATTACGAGCTGCAGGAGGTGATCGGGAGTGGAGCAACTGCTGTAGTCCAAGCAGCTTATTGTGCCCCTAAAAAGGAGAAAGTGGCAATCAAACGGATAAACCTTGAGAAATGTCAAACTAGCATGGATGAACTCCTGAAAGAAATTCAAGCCATGAGTCAATGCCATCATCCTAATATTGTATCTTACTACACATCTTTTGTGGTAAAAGATGAGCTGTGGCTTGTCATGAAGCTGCTAAGTGGAGGTTCTGTTCTGGATATTATTAAGCACATTGTGGCAAAAGGGGAACACAAAAGTGGAGTCCTAGATGAATCTACCATTGCTACGATACTCCGAGAAGTACTGGAAGGGCTGGAATATCTGCATAAAAATGGACAGATCCACAGAGATGTGAAAGCTGGAAACATTCTTCTTGGAGAAGATGGCTCAGTACAGATTGCAGACTTTGGGGTTAGTGCTTTTTTAGCAACTGGTGGTGATATTACCCGAAATAAAGTGAGAAAGACCTTTGTTGGCACCCCTTGTTGGATGGCACCTGAAGTTATGGAACAGGTCCGTGGTTATGATTTCAAAGCTGATATTTGGAGTTTTGGAATTACAGCAATTGAATTGGCTACAGGGGCGGCTCCTTATCATAAATATCCACCAATGAAGGTTTTAATGCTGACACTGCAGAACGATCCTCCTTCTTTGGAAACTGGTGTTCAAGATAAAGAAATGCTGAAAAAATATGGAAAATCATTTAGAAAAATGATTTCATTGTGCCTTCAAAAAGATCCAGAAAAAAGACCAACAGCAGCAGAACTATTAAGGCACAAATTTTTCCAGAAAGCAAAG</t>
-  </si>
-  <si>
-    <t>NKHSGIDFKQLNFLTKLNENHSGELWKGRWQGNDIVVKVLKVRDWSTRKSRDFNEECPRLRIFSHPNVLPVLGACQSPPAPHPTLITHWMPYGSLYNVLHEGTNFVVDQSQAVKFALDMARGMAFLHTLEPLIPRHALNSRSVMIDEDMTARISMADVKFSFQCPGRMYAPAWVAPEALQKKPEDTNRRSADMWSFAVLLWELVTREVPFADLSNMEIGMKVALEGLRPTIPPGISPHVCKLMKICMNEDPAKRPKFDMIVPILEKMQDK</t>
-  </si>
-  <si>
-    <t>ACVR1_HUMAN_D0_3H9R_A</t>
-  </si>
-  <si>
-    <t>TGGGCCCTGAACATGAAGGAGCTGAAGCTGCTGCAGACCATCGGGAAGGGGGAGTTCGGAGACGTGATGCTGGGCGATTACCGAGGGAACAAAGTCGCCGTCAAGTGCATTAAGAACGACGCCACTGCCCAGGCCTTCCTGGCTGAAGCCTCAGTCATGACGCAACTGCGGCATAGCAACCTGGTGCAGCTCCTGGGCGTGATCGTGGAGGAGAAGGGCGGGCTCTACATCGTCACTGAGTACATGGCCAAGGGGAGCCTTGTGGACTACCTGCGGTCTAGGGGTCGGTCAGTGCTGGGCGGAGACTGTCTCCTCAAGTTCTCGCTAGATGTCTGCGAGGCCATGGAATACCTGGAGGGCAACAATTTCGTGCATCGAGACCTGGCTGCCCGCAATGTGCTGGTGTCTGAGGACAACGTGGCCAAGGTCAGCGACTTTGGTCTCACCAAGGAGGCGTCCAGCACCCAGGACACGGGCAAGCTGCCAGTCAAGTGGACAGCCCCTGAGGCCCTGAGAGAGAAGAAATTCTCCACTAAGTCTGACGTGTGGAGTTTCGGAATCCTTCTCTGGGAAATCTACTCCTTTGGGCGAGTGCCTTATCCAAGAATTCCCCTGAAGGACGTCGTCCCTCGGGTGGAGAAGGGCTACAAGATGGATGCCCCCGACGGCTGCCCGCCCGCAGTCTATGAAGTCATGAAGAACTGCTGGCACCTGGACGCCGCCATGCGGCCCTCCTTCCTACAGCTCCGAGAGCAGCTTGAGCACATCAAAACCCACGAGCTGCACCTG</t>
-  </si>
-  <si>
-    <t>dna_seq</t>
-  </si>
-  <si>
-    <t>AACCTGGTTTTTAGTGACGGCTACGTGGTAAAGGAGACAATTGGTGTGGGCTCCTACTCTGAGTGCAAGCGCTGTGTCCACAAGGCCACCAACATGGAGTATGCTGTCAAGGTCATTGATAAGAGCAAGCGGGATCCTTCAGAAGAGATTGAGATTCTTCTGCGGTATGGCCAGCACCCCAACATCATCACTCTGAAAGATGTGTATGATGATGGCAAACACGTGTACCTGGTGACAGAGCTGATGCGGGGTGGGGAGCTGCTGGACAAGATCCTGCGGCAGAAGTTCTTCTCAGAGCGGGAGGCCAGCTTTGTCCTGCACACCATTGGCAAAACTGTGGAGTATCTGCACTCACAGGGGGTTGTGCACAGGGACCTGAAGCCCAGCAACATCCTGTATGTGGACGAGTCCGGGAATCCCGAGTGCCTGCGCATCTGTGACTTTGGTTTTGCCAAACAGCTGCGGGCTGAGAATGGGCTCCTCATGACACCTTGCTACACAGCCAACTTTGTGGCGCCTGAGGTGCTGAAGCGCCAGGGCTACGATGAAGGCTGCGACATCTGGAGCCTGGGCATTCTGCTGTACACCATGCTGGCAGGATATACTCCATTTGCCAACGGTCCCAGTGACACACCAGAGGAAATCCTAACCCGGATCGGCAGTGGGAAGTTTACCCTCAGTGGGGGAAATTGGAACACAGTTTCAGAGACAGCCAAGGACCTGGTGTCCAAGATGCTACACGTGGATCCCCACCAGCGCCTCACAGCTAAGCAGGTTCTGCAGCATCCATGGGTCACCCAGAAAGACAAGCTTCCCCAAAGCCAGCTGTCCCACCAGGACCTACAGCTTGTGAAGGGAGCCATGGCTGCCACGTACTCCGCACTCAACAGCTCCAAGCCCACCCCCCAGCTGAAGCCCATCGAGTCATCCATCCTGGCCCAGCGGCGAGTGAGGAAGTTGCCATCCACCACCCTG</t>
-  </si>
-  <si>
-    <t>ATGGCCGACGACGACGTGCTGTTCGAGGATGTGTACGAGCTGTGCGAGGTGATCGGAAAGGGTCCCTTCAGTGTTGTACGACGATGTATCAACAGAGAAACTGGGCAACAATTTGCTGTAAAAATTGTTGATGTAGCCAAGTTCACATCAAGTCCAGGGTTAAGTACAGAAGATCTAAAGCGGGAAGCCAGTATCTGTCATATGCTGAAACATCCACACATTGTAGAGTTATTGGAGACATATAGCTCAGATGGAATGCTTTACATGGTTTTCGAATTTATGGATGGAGCAGATCTGTGTTTTGAAATCGTAAAGCGAGCTGACGCTGGTTTTGTGTACAGTGAAGCTGTAGCCAGCCATTATATGAGACAGATACTGGAAGCTCTACGCTACTGCCATGATAATAACATAATTCACAGGGATGTGAAGCCCCACTGTGTTCTCCTTGCCTCAAAAGAAAACTCGGCACCTGTTAAACTTGGAGGCTTTGGGGTAGCTATTCAATTAGGGGAGTCTGGACTTGTAGCTGGAGGACGTGTTGGAACACCTCATTTTATGGCACCAGAAGTGGTCAAAAGAGAGCCTTACGGAAAGCCTGTAGACGTCTGGGGGTGCGGTGTGATCCTTTTTATCCTGCTCAGTGGTTGTTTGCCTTTTTACGGAACCAAGGAAAGATTGTTTGAAGGCATTATTAAAGGAAAATATAAGATGAATCCAAGGCAGTGGAGCCATATCTCTGAAAGTGCCAAAGACCTAGTACGTCGCATGCTGATGCTGGATCCAGCTGAAAGGATCACTGTTTATGAAGCACTGAATCACCCATGGCTTAAGGAGCGGGATCGTTACGCCTACAAGATTCATCTTCCAGAAACAGTAGAGCAGCTGAGGAAATTCAATGCAAGGAGGAAACTAAAGGGTGCAGTACTAGCCGCTGTGTCAAGTCACAAATTCAACTCATTCTATGGGGATCCCCCTGAAGAGTTACCAGATTTCTCCGAAGACCCTACCTCCTCAGGAGCA</t>
-  </si>
-  <si>
-    <t>VRK1_HUMAN_D0_3OP5_D</t>
-  </si>
-  <si>
-    <t>ATGGGGAAGGTGAAAGCCACCCCCATGACACCTGAACAAGCAATGAAGCAATACATGCAAAAACTCACAGCCTTCGAACACCATGAGATTTTCAGCTACCCTGAAATATATTTCTTGGGTCTAAATGCTAAGAAGCGCCAGGGCATGACAGGTGGGCCCAACAATGGTGGCTATGATGATGACCAGGGATCATATGTGCAGGTGCCCCACGATCACGTGGCTTACAGGTATGAGGTCCTCAAGGTCATTGGGAAGGGGAGCTTTGGGCAGGTGGTCAAGGCCTACGATCACAAAGTCCACCAGCACGTGGCCCTAAAGATGGTGCGGAATGAGAAGCGCTTCCACCGGCAAGCAGCGGAGGAGATCCGAATCCTGGAACACCTGCGGAAGCAGGACAAGGATAACACAATGAATGTCATCCATATGCTGGAGAATTTCACCTTCCGCAACCACATCTGCATGACGTTTGAGCTGCTGAGCATGAACCTCTATGAGCTCATCAAGAAGAATAAATTCCAGGGCTTCAGTCTGCCTTTGGTTCGCAAGTTTGCCCACTCGATTCTGCAGTGCTTGGATGCTTTGCACAAAAACAGAATAATTCACTGTGACCTTAAGCCCGAGAACATTTTGTTAAAGCAGCAGGGTAGAAGCGGTATTAAAGTAATTGATTTTGGCTCCAGTTGTTACGAGCATCAGCGTGTCTACACGTACATCCAGTCGCGTTTTTACCGGGCTCCAGAAGTGATCCTTGGGGCCAGGTATGGCATGCCCATTGATATGTGGAGCCTGGGCTGCATTTTAGCAGAGCTCCTGACGGGTTACCCCCTCTTGCCTGGGGAAGATGAAGGGGACCAGCTGGCCTGTATGATTGAACTGTTGGGCATGCCCTCACAGAAACTGCTGGATGCATCCAAACGAGCCAAAAATTTTGTGAGCTCCAAGGGTTATCCCCGTTACTGCACTGTCACGACTCTCTCAGATGGCTCTGTGGTCCTAAACGGAGGCCGTTCCCGGAGGGGGAAACTGAGGGGCCCACCGGAGAGCAGAGAGTGGGGGAACGCGCTGAAGGGGTGTGATGATCCCCTTTTCCTTGACTTCTTAAAACAGTGTTTAGAGTGGGATCCTGCAGTGCGCATGACCCCAGGCCAGGCTTTGCGGCACCCCTGGCTGAGGAGGCGGTTGCCAAAGCCTCCCACCGGGGAGAAAACGTCAGTGAAAAGG</t>
-  </si>
-  <si>
-    <t>SVYPKALRDEYIMSKTLGSGACGEVKLAFERKTCKKVAIKIISKRKFAIGSAREADPALNVETEIEILKKLNHPCIIKIKNFFDAEDYYIVLELMEGGELFDKVVGNKRLKEATCKLYFYQMLLAVQYLHENGIIHRDLKPENVLLSSQEEDCLIKITDFGHSKIWGETSLMRTLCGTPTYLAPEVLVSVGTAGYNRAVDCWSLGVILFICLSGYPPFSEHRTQVSLKDQITSGKYNFIPEVWAEVSEKALDLVKKLLVVDPKARFTTEEALRHPWLQDEDMKRKFQDLLSEENESTALPQVLAQPSTSRKRPREGEAEGAE</t>
-  </si>
-  <si>
-    <t>ATGGAGAAGTATGAAAAAATTGGGAAAATTGGAGAAGGATCCTATGGAGTTGTTTTCAAATGTAGAAACAGGGACACGGGTCAGATTGTGGCCATCAAGAAGTTTCTGGAATCAGAAGATGACCCTGTCATAAAGAAAATTGCCCTTCGGGAAATCCGAATGCTCAAGCAACTCAAGCATCCCAACCTTGTTAACCTCCTGGAAGTCTTCAGGAGGAAACGGAGGCTTCACCTGGTGTTTGAATATTGTGACCACACAGTTCTCCATGAGTTGGACAGATACCAAAGAGGGGTACCAGAACATCTCGTGAAGAGCATAACTTGGCAGACACTGCAAGCTGTAAATTTTTGCCATAAACACAATTGCATACATAGAGACGTGAAGCCAGAAAATATCCTCATCACGAAACATTCCGTGATTAAGCTTTGTGACTTTGGATTTGCTCGGCTTTTGACTGGACCGAGTGACTACTATACAGACTACGTGGCTACCAGGTGGTACCGCTCCCCTGAGCTGCTGGTGGGGGACACGCAGTACGGCCCCCCGGTGGATGTTTGGGCAATTGGCTGTGTCTTTGCTGAGCTGCTGTCAGGAGTGCCTCTGTGGCCAGGAAAATCGGATGTGGATCAGCTGTATCTGATTAGGAAGACCTTGGGGGATCTCATTCCTAGGCACCAGCAAGTGTTTAGCACGAATCAGTACTTCAGTGGAGTGAAAATTCCAGACCCTGAAGATATGGAACCACTTGAATTAAAATTCCCAAACATCTCTTATCCTGCCCTGGGGCTCCTA</t>
-  </si>
-  <si>
-    <t>KHDGRVKIGHYVLGDTLGVGTFGKVKIGEHQLTGHKVAVKILNRQKIRSLDVVGKIKREIQNLKLFRHPHIIKLYQVISTPTDFFMVMEYVSGGELFDYICKHGRVEEMEARRLFQQILSAVDYCHRHMVVHRDLKPENVLLDAHMNAKIADFGLSNMMSDGEFLRTSCGSPNYAAPEVISGRLYAGPEVDIWSCGVILYALLCGTLPFDDEHVPTLFKKIRGGVFYIPEYLNRSVATLLMHMLQVDPLKRATIKDIREHEWFKQDLPSYLFPE</t>
-  </si>
-  <si>
-    <t>ATGGAAAACTTTAATAATTTCTATATACTTACATCTAAAGAGCTAGGGAGAGGAAAATTTGCTGTGGTTAGACAATGTATATCAAAATCTACTGGCCAAGAATATGCTGCAAAATTTCTAAAAAAGAGAAGAAGAGGACAGGATTGTCGAGCAGAAATTTTACACGAGATTGCTGTGCTTGAATTGGCAAAGTCTTGTCCCCGTGTTATTAATCTTCATGAGGTCTATGAAAATACAAGTGAAATCATTTTGATATTGGAATATGCTGCAGGTGGAGAAATTTTCAGCCTGTGTTTACCTGAGTTGGCTGAAATGGTTTCTGAAAATGATGTTATCAGACTCATTAAACAAATACTTGAAGGAGTTTATTATCTACATCAGAATAACATTGTACACCTTGATTTAAAGCCACAGAATATATTACTGAGCAGCATATACCCTCTCGGGGACATTAAAATAGTAGATTTTGGAATGTCTCGAAAAATAGGGCATGCGTGTGAACTTCGGGAAATCATGGGAACACCAGAATATTTAGCTCCAGAAATCCTGAACTATGATCCCATTACCACAGCAACAGATATGTGGAATATTGGTATAATAGCATATATGTTGTTAACTCACACATCACCATTTGTGGGAGAAGATAATCAAGAAACATACCTCAATATTTCTCAAGTTAATGTAGATTATTCGGAAGAAACTTTTTCATCAGTTTCACAGCTGGCCACAGACTTTATTCAGAGCCTTTTAGTAAAAAATCCAGAGAAAAGACCAACAGCAGAGATATGCCTTTCTCATTCTTGGCTACAGCAGTGGGACTTTGAAAACTTGTTTCACCCTGAAGAAACTTCCAGTTCCTCTCAAACTCAGGATCATTCTGTAAGGTCCTCTGAAGACAAGACTTCTAAATCCTCC</t>
-  </si>
-  <si>
-    <t>MPSRAEDYEVLYTIGTGSYGRCQKIRRKSDGKILVWKELDYGSMTEAEKQMLVSEVNLLRELKHPNIVRYYDRIIDRTNTTLYIVMEYCEGGDLASVITKGTKERQYLDEEFVLRVMTQLTLALKECHRRSDGGHTVLHRDLKPANVFLDGKQNVKLGDFGLARILNHDTSFAKTFVGTPYYMSPEQMNRMSYNEKSDIWSLGCLLYELCALMPPFTAFSQKELAGKIREGKFRRIPYRYSDELNEIITRMLNLKDYHRPSVEEILENPLI</t>
-  </si>
-  <si>
-    <t>GACCCAGAAGAGCTTTTTACAAAACTAGAGAAAATTGGGAAGGGCTCCTTTGGAGAGGTGTTCAAAGGCATTGACAATCGGACTCAGAAAGTGGTTGCCATAAAGATCATTGATCTGGAAGAAGCTGAAGATGAGATAGAGGACATTCAACAAGAAATCACAGTGCTGAGTCAGTGTGACAGTCCATATGTAACCAAATATTATGGATCCTATCTGAAGGATACAAAATTATGGATAATAATGGAATATCTTGGTGGAGGCTCCGCACTAGATCTATTAGAACCTGGCCCATTAGATGAAACCCAGATCGCTACTATATTAAGAGAAATACTGAAAGGACTCGATTATCTCCATTCGGAGAAGAAAATCCACAGAGACATTAAAGCGGCCAACGTCCTGCTGTCTGAGCATGGCGAGGTGAAGCTGGCGGACTTTGGCGTGGCTGGCCAGCTGACAGACACCCAGATCAAAAGGAACACCTTCGTGGGCACCCCATTCTGGATGGCACCCGAGGTCATCAAACAGTCGGCCTATGACTCGAAGGCAGACATCTGGTCCCTGGGCATAACAGCTATTGAACTTGCAAGAGGGGAACCACCTCATTCCGAGCTGCACCCCATGAAAGTTTTATTCCTCATTCCAAAGAACAACCCACCGACGTTGGAAGGAAACTACAGTAAACCCCTCAAGGAGTTTGTGGAGGCCTGTTTGAATAAGGAGCCGAGCTTTAGACCCACTGCTAAGGAGTTATTGAAGCACAAGTTTATACTACGCAATGCAAAGAAAACTTCCTACTTGACCGAGCTCATCGAC</t>
-  </si>
-  <si>
-    <t>VIIDNKRYLFIQKLGEGGFSYVDLVEGLHDGHFYALKRILCHEQQDREEAQREADMHRLFNHPNILRLVAYCLRERGAKHEAWLLLPFFKRGTLWNEIERLKDKGNFLTEDQILWLLLGICRGLEAIHAKGYAHRDLKPTNILLGDEGQPVLMDLGSMNQACIHVEGSRQALTLQDWAAQRCTISYRAPELFSVQSHCVIDERTDVWSLGCVLYAMMFGEGPYDMVFQKGDSVALAVQNQLSIPQSPRHSSALWQLLNSMMTVDPHQRPHIPLLLSQLEALQ</t>
-  </si>
-  <si>
-    <t>GEAPNQALLRILKETEFKKIKVLGSGAFGTVYKGLWIPEGEKVKIPVAIKELREATSPKANKEILDEAYVMASVDNPHVCRLLGICLTSTVQLITQLMPFGCLLDYVREHKDNIGSQYLLNWCVQIAKGMNYLEDRRLVHRDLAARNVLVKTPQHVKITDFGRAKLLGAEEKEYHAEGGKVPIKWMALESILHRIYTHQSDVWSYGVTVWELMTFGSKPYDGIPASEISSILEKGERLPQPPICTIDVYMIMVKCWMIDADSRPKFRELIIEFSKMARDPQRYLVIQGDERMHLPSPTDSNFYRALMDEEDMDDVVDADEYLIPQQG</t>
-  </si>
-  <si>
-    <t>MK09_HUMAN_D0_3NPC_B</t>
-  </si>
-  <si>
-    <t>PFPEGKVLDDMEGNQWVLGKKIGSGGFGLIYLAFPTNKPEKDARHVVKVEYQENGPLFSELKFYQRVAKKDCIKKWIERKQLDYLGIPLFYGSGLTEFKGRSYRFMVMERLGIDLQKISGQNGTFKKSTVLQLGIRMLDVLEYIHENEYVHGDIKAANLLLGYKNPDQVYLADYGLSYRYCPNGNHKQYQENPRKGHNGTIEFTSLDAHKGVALSRRSDVEILGYCMLRWLCGKLPWEQNLKDPVAVQTAKTNLLDELPQSVLKWAPSGSSCCEIAQFLVCAHSLAYDEKPNYQALKKILNPHGIPLGPLDFSTKGQSINVH</t>
-  </si>
-  <si>
-    <t>MESDLHQIIHSSQPLTLEHVRYFLYQLLRGLKYMHSAQVIHRDLKPSNLLVNENCELKIGDFGMARGLCTSPAEHQYFMTEYVATRWYRAPELMLSLHEYTQAIDLWSVGCIFGEMLARRQLFPGKNYVHQLQLIMMVLGTPSPAVIQAVGAERVRAYIQSLPPRQPVPWETVYPGADRQALSLLGRMLRFEPSARISAAAALRHPFLAKYHDPDDEPDCAPPFDFAFDREALTRERIKEAIVAEIEDFHARREGIRQQIRFQPSLQPVASEPGCPDVEMPSPWAPSGDCAM</t>
-  </si>
-  <si>
-    <t>EPKKYAVTDDYQLSKQVLGLGVNGKVLECFHRRTGQKCALKLLYDSPKARQEVDHHWQASGGPHIVCILDVYENMHHGKRCLLIIMECMEGGELFSRIQERGDQAFTEREAAEIMRDIGTAIQFLHSHNIAHRDVKPENLLYTSKEKDAVLKLTDFGFAKETTQNALQTPCYTPYYVAPEVLGPEKYDKSCDMWSLGVIMYILLCGFPPFYSNTGQAISPGMKRRIRLGQYGFPNPEWSEVSEDAKQLIRLLLKTDPTERLTITQFMNHPWINQSMVVPQTPLHTARVLQEDKDHWDEVKEEMTSALATMRVDYDQV</t>
-  </si>
-  <si>
-    <t>ATGAAGGACTCTCCATTCTATCAACACTATGACCTAGATTTGAAGGACAAACCCCTGGGAGAAGGTAGTTTTTCAATTTGTCGAAAGTGTGTGCATAAAAAAAGTAACCAAGCTTTTGCAGTCAAAATAATCAGCAAAAGGATGGAAGCCAATACTCAAAAGGAAATAACAGCTCTGAAACTCTGTGAAGGACACCCCAATATTGTGAAGTTGCATGAAGTTTTTCATGATCAGCTTCACACGTTTCTAGTGATGGAACTTCTGAATGGAGGAGAACTGTTTGAGCGCATTAAGAAAAAGAAGCACTTCAGTGAGACGGAAGCCAGCTACATCATGAGGAAGCTTGTTTCAGCTGTAAGCCACATGCATGATGTTGGAGTGGTGCACAGGGATCTGAAACCTGAGAATTTATTGTTCACCGATGAAAATGACAATTTGGAAATTAAAATAATTGATTTTGGATTTGCACGGCTAAAGCCACCGGATAATCAGCCCCTGAAGACTCCATGCTTCACCCTTCATTATGCCGCCCCAGAGCTCTTGAATCAGAACGGCTACGATGAGTCCTGTGACCTGTGGAGCTTGGGCGTCATTTTGTACACAATGTTGTCAGGACAGGTTCCCTTCCAATCTCATGACCGAAGTTTGACGTGTACCAGCGCGGTGGAAATCATGAAGAAAATTAAAAAGGGAGATTTCTCCTTTGAAGGAGAAGCCTGGAAGAATGTATCCCAAGAGGCTAAAGATTTGATCCAAGGACTTCTCACAGTAGATCCAAACAAAAGGCTTAAAATGTCTGGCTTGAGGTACAATGAATGGCTACAAGATGGAAGTCAGCTGTCCTCCAATCCTCTGATGACTCCGGATATTCTAGGATCTTCCGGAGCTGCCGTGCATACCTGTGTGAAAGCAACCTTCCACGCCTTTAACAAATACAAGAGAGAGGGGTTTTGCCTTCAGAATGTTGATAAGGCC</t>
-  </si>
-  <si>
-    <t>aa_seq</t>
-  </si>
-  <si>
-    <t>KC1D_HUMAN_D0_4HNF_B</t>
-  </si>
-  <si>
-    <t>AGCATTGAGTCATCAGGAAAACTGAAGATCTCCCCTGAACAACACTGGGATTTCACTGCAGAGGACTTGAAAGACCTTGGAGAAATTGGACGAGGAGCTTATGGTTCTGTCAACAAAATGGTCCACAAACCAAGTGGGCAAATAATGGCAGTTAAAAGAATTCGGTCAACAGTGGATGAAAAAGAACAAAAACAACTTCTTATGGATTTGGATGTAGTAATGCGGAGTAGTGATTGCCCATACATTGTTCAGTTTTATGGTGCACTCTTCAGAGAGGGTGACTGTTGGATCTGTATGGAACTCATGTCTACCTCGTTTGATAAGTTTTACAAATATGTATATAGTGTATTAGATGATGTTATTCCAGAAGAAATTTTAGGCAAAATCACTTTAGCAACTGTGAAAGCACTAAACCACTTAAAAGAAAACTTGAAAATTATTCACAGAGATATCAAACCTTCCAATATTCTTCTGGACAGAAGTGGAAATATTAAGCTCTGTGACTTCGGCATCAGTGGACAGCTTGTGGACTCTATTGCCAAGACAAGAGATGCTGGCTGTAGGCCATACATGGCACCTGAAAGAATAGACCCAAGCGCATCACGACAAGGATATGATGTCCGCTCTGATGTCTGGAGTTTGGGGATCACATTGTATGAGTTGGCCACAGGCCGATTTCCTTATCCAAAGTGGAATAGTGTATTTGATCAACTAACACAAGTCGTGAAAGGAGATCCTCCGCAGCTGAGTAATTCTGAGGAAAGGGAATTCTCCCCGAGTTTCATCAACTTTGTCAACTTGTGCCTTACGAAGGATGAATCCAAAAGGCCAAAGTATAAAGAGCTTCTGAAACATCCCTTTATTTTGATGTATGAAGAACGTGCCGTTGAGGTCGCATGCTATGTTTGTAAAATCCTGGATCAAATGCCAGCTACTCCCAGCTCTCCCATGTATGTCGAT</t>
-  </si>
-  <si>
-    <t>AAPK2_HUMAN_D0_2H6D_A</t>
-  </si>
-  <si>
-    <t>CLK3_HUMAN_D0_2WU7_A</t>
-  </si>
-  <si>
-    <t>IPEVQKPLHEQLWYHGAIPRAEVAELLVHSGDFLVRESQGKQEYVLSVLWDGLPRHFIIQSLDNLYRLEGEGFPSIPLLIDHLLSTQQPLTKKSGVVLHRAVPKDKWVLNHEDLVLGEQIGRGNFGEVFSGRLRADNTLVAVKSCRETLPPDLKAKFLQEARILKQYSHPNIVRLIGVCTQKQPIYIVMELVQGGDFLTFLRTEGARLRVKTLLQMVGDAAAGMEYLESKCCIHRDLAARNCLVTEKNVLKISDFGMSREEADGVYAASGGLRQVPVKWTAPEALNYGRYSSESDVWSFGILLWETFSLGASPYPNLSNQQTREFVEKGGRLPCPELCPDAVFRLMEQCWAYEPGQRPSFSTIYQELQSIRKRHR</t>
-  </si>
-  <si>
-    <t>GAAGCCTTTCTCACCCAGAAAGCCAAGGTCGGCGAACTCAAAGACGATGACTTCGAAAGGATCTCAGAGCTGGGCGCGGGCAACGGCGGGGTGGTCACCAAAGTCCAGCACAGACCCTCGGGCCTCATCATGGCCAGGAAGCTGATCCACCTTGAGATCAAGCCGGCCATCCGGAACCAGATCATCCGCGAGCTGCAGGTCCTGCACGAATGCAACTCGCCGTACATCGTGGGCTTCTACGGGGCCTTCTACAGTGACGGGGAGATCAGCATTTGCATGGAACACATGGACGGCGGCTCCCTGGACCAGGTGCTGAAAGAGGCCAAGAGGATTCCCGAGGAGATCCTGGGGAAAGTCAGCATCGCGGTTCTCCGGGGCTTGGCGTACCTCCGAGAGAAGCACCAGATCATGCACCGAGATGTGAAGCCCTCCAACATCCTCGTGAACTCTAGAGGGGAGATCAAGCTGTGTGACTTCGGGGTGAGCGGCCAGCTCATAGACTCCATGGCCAACTCCTTCGTGGGCACGCGCTCCTACATGGCTCCGGAGCGGTTGCAGGGCACACATTACTCGGTGCAGTCGGACATCTGGAGCATGGGCCTGTCCCTGGTGGAGCTGGCCGTCGGAAGGTACCCCATCCCCCCGCCCGACGCCAAAGAGCTGGAGGCCATCTTTGGCCGGCCCGTGGTCGACGGGGAAGAAGGAGAGCCTCACAGCATCTCGCCTCGGCCGAGGCCCCCCGGGCGCCCCGTCAGCGGTCACGGGATGGATAGCCGGCCTGCCATGGCCATCTTTGAACTCCTGGACTATATTGTGAACGAGCCACCTCCTAAGCTGCCCAACGGTGTGTTCACCCCCGACTTCCAGGAGTTTGTCAATAAATGCCTCATCAAGAACCCAGCGGAGCGGGCGGACCTGAAGATGCTCACAAACCACACCTTCATCAAGCGGTCCGAGGTGGAAGAAGTGGATTTTGCCGGCTGGTTGTGTAAAACCCTGCGGCTGAACCAGCCCGGCACACCCACGCGCACCGCCGTG</t>
-  </si>
-  <si>
-    <t>MKDSPFYQHYDLDLKDKPLGEGSFSICRKCVHKKSNQAFAVKIISKRMEANTQKEITALKLCEGHPNIVKLHEVFHDQLHTFLVMELLNGGELFERIKKKKHFSETEASYIMRKLVSAVSHMHDVGVVHRDLKPENLLFTDENDNLEIKIIDFGFARLKPPDNQPLKTPCFTLHYAAPELLNQNGYDESCDLWSLGVILYTMLSGQVPFQSHDRSLTCTSAVEIMKKIKKGDFSFEGEAWKNVSQEAKDLIQGLLTVDPNKRLKMSGLRYNEWLQDGSQLSSNPLMTPDILGSSGAAVHTCVKATFHAFNKYKREGFCLQNVDKA</t>
-  </si>
-  <si>
-    <t>MKNK2_HUMAN_D0_2AC3_A</t>
-  </si>
-  <si>
-    <t>STRDYEIQRERIELGRCIGEGQFGDVHQGIYMSPENPALAVAIKTCKNCTSDSVREKFLQEALTMRQFDHPHIVKLIGVITENPVWIIMELCTLGELRSFLQVRKYSLDLASLILYAYQLSTALAYLESKRFVHRDIAARNVLVSSNDCVKLGDFGLSRYMEDSTYYKASKGKLPIKWMAPESINFRRFTSASDVWMFGVCMWEILMHGVKPFQGVKNNDVIGRIENGERLPMPPNCPPTLYSLMTKCWAYDPSRRPRFTELKAQLSTILEEEKAQQEE</t>
-  </si>
-  <si>
-    <t>CSK22_HUMAN_D0_3E3B_X</t>
-  </si>
-  <si>
-    <t>Cterm</t>
-  </si>
-  <si>
-    <t>ATGAGCAGAAGCAAGCGTGACAACAATTTTTATAGTGTAGAGATTGGAGATTCTACATTCACAGTCCTGAAACGATATCAGAATTTAAAACCTATAGGCTCAGGAGCTCAAGGAATAGTATGCGCAGCTTATGATGCCATTCTTGAAAGAAATGTTGCAATCAAGAAGCTAAGCCGACCATTTCAGAATCAGACTCATGCCAAGCGGGCCTACAGAGAGCTAGTTCTTATGAAATGTGTTAATCACAAAAATATAATTGGCCTTTTGAATGTTTTCACACCACAGAAATCCCTAGAAGAATTTCAAGATGTTTACATAGTCATGGAGCTCATGGATGCAAATCTTTGCCAAGTGATTCAGATGGAGCTAGATCATGAAAGAATGTCCTACCTTCTCTATCAGATGCTGTGTGGAATCAAGCACCTTCATTCTGCTGGAATTATTCATCGGGACTTAAAGCCCAGTAATATAGTAGTAAAATCTGATTGCACTTTGAAGATTCTTGACTTCGGTCTGGCCAGGACTGCAGGAACGAGTTTTATGATGACGCCTTATGTAGTGACTCGCTACTACAGAGCACCCGAGGTCATCCTTGGCATGGGCTACAAGGAAAACGTGGATTTATGGTCTGTGGGGTGCATTATGGGAGAAATGGTTTGCCACAAAATCCTCTTTCCAGGAAGGGACTATATTGATCAGTGGAATAAAGTTATTGAACAGCTTGGAACACCATGTCCTGAATTCATGAAGAAACTGCAACCAACAGTAAGGACTTACGTTGAAAACAGACCTAAATATGCTGGATATAGCTTTGAGAAACTCTTCCCTGATGTCCTTTTCCCAGCTGACTCAGAACACAACAAACTTAAAGCCAGTCAGGCAAGGGATTTGTTATCCAAAATGCTGGTAATAGATGCATCTAAAAGGATCTCTGTAGATGAAGCTCTCCAACACCCGTACATCAATGTCTGGTATGATCCTTCTGAAGCAGAAGCTCCACCACCAAAGATCCCTGACAAGCAGTTAGATGAAAGGGAACACACAATAGAAGAGTGGAAAGAATTGATATATAAGGAAGTTATGGACTTGGAG</t>
-  </si>
-  <si>
-    <t>TTSLEALPTGTVLTDKSGRQWKLKSFQTRDNQGILYEAAPTSTLTCDSGPQKQKFSLKLDAKDGRLFNEQNFFQRAAKPLQVNKWKKLYSTPLLAIPTCMGFGVHQDKYRFLVLPSLGRSLQSALDVSPKHVLSERSVLQVACRLLDALEFLHENEYVHGNVTAENIFVDPEDQSQVTLAGYGFAFRYCPSGKHVAYVEGSRSPHEGDLEFISMDLHKGCGPSRRSDLQSLGYCMLKWLYGFLPWTNCLPNTEDIMKQKQKFVDKPGPFVGPCGHWIRPSETLQKYLKVVMALTYEEKPPYAMLRNNLEALLQDLRVSPYDPIGLPMVP</t>
-  </si>
-  <si>
-    <t>SPNYDKWEMERTDITMKHKLGGGQYGEVYEGVWKKYSLTVAVKTLKEDTMEVEEFLKEAAVMKEIKHPNLVQLLGVCTREPPFYIITEFMTYGNLLDYLRECNRQEVNAVVLLYMATQISSAMEYLEKKNFIHRDLAARNCLVGENHLVKVADFGLSRLMTGDTYTAHAGAKFPIKWTAPESLAYNKFSIKSDVWAFGVLLWEIATYGMSPYPGIDLSQVYELLEKDYRMERPEGCPEKVYELMRACWQWNPSDRPSFAEIHQAFETMFQESSISDEVEKELGK</t>
-  </si>
-  <si>
-    <t>ATGGCGGCGGCGGCGGCTCAGGGGGGCGGGGGCGGGGAGCCCCGTAGAACCGAGGGGGTCGGCCCGGGGGTCCCGGGGGAGGTGGAGATGGTGAAGGGGCAGCCGTTCGACGTGGGCCCGCGCTACACGCAGTTGCAGTACATCGGCGAGGGCGCGTACGGCATGGTCAGCTCGGCCTATGACCACGTGCGCAAGACTCGCGTGGCCATCAAGAAGATCAGCCCCTTCGAACATCAGACCTACTGCCAGCGCACGCTCCGGGAGATCCAGATCCTGCTGCGCTTCCGCCATGAGAATGTCATCGGCATCCGAGACATTCTGCGGGCGTCCACCCTGGAAGCCATGAGAGATGTCTACATTGTGCAGGACCTGATGGAGACTGACCTGTACAAGTTGCTGAAAAGCCAGCAGCTGAGCAATGACCATATCTGCTACTTCCTCTACCAGATCCTGCGGGGCCTCAAGTACATCCACTCCGCCAACGTGCTCCACCGAGATCTAAAGCCCTCCAACCTGCTCATCAACACCACCTGCGACCTTAAGATTTGTGATTTCGGCCTGGCCCGGATTGCCGATCCTGAGCATGACCACACCGGCTTCCTGACGGAGTATGTGGCTACGCGCTGGTACCGGGCCCCAGAGATCATGCTGAACTCCAAGGGCTATACCAAGTCCATCGACATCTGGTCTGTGGGCTGCATTCTGGCTGAGATGCTCTCTAACCGGCCCATCTTCCCTGGCAAGCACTACCTGGATCAGCTCAACCACATTCTGGGCATCCTGGGCTCCCCATCCCAGGAGGACCTGAATTGTATCATCAACATGAAGGCCCGAAACTACCTACAGTCTCTGCCCTCCAAGACCAAGGTGGCTTGGGCCAAGCTTTTCCCCAAGTCAGACTCCAAAGCCCTTGACCTGCTGGACCGGATGTTAACCTTTAACCCCAATAAACGGATCACAGTGGAGGAAGCGCTGGCTCACCCCTACCTGGAGCAGTACTATGACCCGACGGATGAGCCAGTGGCCGAGGAGCCCTTCACCTTCGCCATGGAGCTGGATGACCTACCTAAGGAGCGGCTGAAGGAGCTCATCTTCCAGGAGACAGCACGCTTCCAGCCCGGAGTGCTGGAGGCCCCC</t>
-  </si>
-  <si>
-    <t>MLGAVEGPRWKQAEDIRDIYDFRDVLGTGAFSEVILAEDKRTQKLVAIKCIAKEALEGKEGSMENEIAVLHKIKHPNIVALDDIYESGGHLYLIMQLVSGGELFDRIVEKGFYTERDASRLIFQVLDAVKYLHDLGIVHRDLKPENLLYYSLDEDSKIMISDFGLSKMEDPGSVLSTACGTPGYVAPEVLAQKPYSKAVDCWSIGVIAYILLCGYPPFYDENDAKLFEQILKAEYEFDSPYWDDISDSAKDFIRHLMEKDPEKRFTCEQALQHPWIAGDTALDKNIHQSVSEQ</t>
-  </si>
-  <si>
-    <t>AURKA_HUMAN_D0_2NP8_A</t>
-  </si>
-  <si>
-    <t>aa_start</t>
-  </si>
-  <si>
-    <t>GCAGTGCCCTTTGTGGAAGACTGGGACTTGGTGCAAACCCTGGGAGAAGGTGCCTATGGAGAAGTTCAACTTGCTGTGAATAGAGTAACTGAAGAAGCAGTCGCAGTGAAGATTGTAGATATGAAGCGTGCCGTAGACTGTCCAGAAAATATTAAGAAAGAGATCTGTATCAATAAAATGCTAAATCATGAAAATGTAGTAAAATTCTATGGTCACAGGAGAGAAGGCAATATCCAATATTTATTTCTGGAGTACTGTAGTGGAGGAGAGCTTTTTGACAGAATAGAGCCAGACATAGGCATGCCTGAACCAGATGCTCAGAGATTCTTCCATCAACTCATGGCAGGGGTGGTTTATCTGCATGGTATTGGAATAACTCACAGGGATATTAAACCAGAAAATCTTCTGTTGGATGAAAGGGATAACCTCAAAATCTCAGACTTTGGCTTGGCAACAGTATTTCGGTATAATAATCGTGAGCGTTTGTTGAACAAGATGTGTGGTACTTTACCATATGTTGCTCCAGAACTTCTGAAGAGAAGAGAATTTCATGCAGAACCAGTTGATGTTTGGTCCTGTGGAATAGTACTTACTGCAATGCTCGCTGGAGAATTGCCATGGGACCAACCCAGTGACAGCTGTCAGGAGTATTCTGACTGGAAAGAAAAAAAAACATACCTCAACCCTTGGAAAAAAATCGATTCTGCTCCTCTAGCTCTGCTGCATAAAATCTTAGTTGAGAATCCATCAGCAAGAATTACCATTCCAGACATCAAAAAAGATAGATGGTACAACAAACCCCTC</t>
-  </si>
-  <si>
-    <t>MSGPVPSRARVYTDVNTHRPREYWDYESHVVEWGNQDDYQLVRKLGRGKYSEVFEAINITNNEKVVVKILKPVKKKKIKREIKILENLRGGPNIITLADIVKDPVSRTPALVFEHVNNTDFKQLYQTLTDYDIRFYMYEILKALDYCHSMGIMHRDVKPHNVMIDHEHRKLRLIDWGLAEFYHPGQEYNVRVASRYFKGPELLVDYQMYDYSLDMWSLGCMLASMIFRKEPFFHGHDNYDQLVRIAKVLGTEDLYDYIDKYNIELDPRFNDILGRHSRKRWERFVHSENQHLVSPEALDFLDKLLRYDHQSRLTAREAMEHPYFYTVVKDQARMG</t>
-  </si>
-  <si>
-    <t>MAAAAAAGAGPEMVRGQVFDVGPRYTNLSYIGEGAYGMVCSAYDNVNKVRVAIKKISPFEHQTYCQRTLREIKILLRFRHENIIGINDIIRAPTIEQMKDVYIVQDLMETDLYKLLKTQHLSNDHICYFLYQILRGLKYIHSANVLHRDLKPSNLLLNTTCDLKICDFGLARVADPDHDHTGFLTEYVATRWYRAPEIMLNSKGYTKSIDIWSVGCILAEMLSNRPIFPGKHYLDQLNHILGILGSPSQEDLNCIINLKARNYLLSLPHKNKVPWNRLFPNADSKALDLLDKMLTFNPHKRIEVEQALAHPYLEQYYDPSDEPIAEAPFKFDMELDDLPKEKLKELIFEETARFQPGYRS</t>
   </si>
 </sst>
 </file>
@@ -1250,36 +1058,36 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>190</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
-        <v>135</v>
+        <v>103</v>
       </c>
       <c r="D1" t="s">
-        <v>289</v>
+        <v>225</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
-        <v>271</v>
+        <v>210</v>
       </c>
       <c r="G1" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="H1" t="s">
-        <v>171</v>
+        <v>131</v>
       </c>
       <c r="I1" t="s">
-        <v>253</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>188</v>
+        <v>147</v>
       </c>
       <c r="B2" t="n">
         <v>1017</v>
@@ -1294,7 +1102,7 @@
         <v>296</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G2" t="n">
         <v>4</v>
@@ -1303,12 +1111,12 @@
         <v>888</v>
       </c>
       <c r="I2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>215</v>
+        <v>58</v>
       </c>
       <c r="B3" t="n">
         <v>1432</v>
@@ -1323,7 +1131,7 @@
         <v>360</v>
       </c>
       <c r="F3" t="s">
-        <v>246</v>
+        <v>187</v>
       </c>
       <c r="G3" t="n">
         <v>1</v>
@@ -1332,12 +1140,12 @@
         <v>1080</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>288</v>
+        <v>183</v>
       </c>
       <c r="B4" t="n">
         <v>6790</v>
@@ -1352,7 +1160,7 @@
         <v>391</v>
       </c>
       <c r="F4" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="G4" t="n">
         <v>373</v>
@@ -1361,12 +1169,12 @@
         <v>1173</v>
       </c>
       <c r="I4" t="s">
-        <v>202</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B5" t="n">
         <v>5594</v>
@@ -1381,7 +1189,7 @@
         <v>360</v>
       </c>
       <c r="F5" t="s">
-        <v>292</v>
+        <v>227</v>
       </c>
       <c r="G5" t="n">
         <v>1</v>
@@ -1390,12 +1198,12 @@
         <v>1080</v>
       </c>
       <c r="I5" t="s">
-        <v>164</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="B6" t="n">
         <v>9261</v>
@@ -1410,7 +1218,7 @@
         <v>348</v>
       </c>
       <c r="F6" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="G6" t="n">
         <v>73</v>
@@ -1419,12 +1227,12 @@
         <v>1044</v>
       </c>
       <c r="I6" t="s">
-        <v>189</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B7" t="n">
         <v>10298</v>
@@ -1439,7 +1247,7 @@
         <v>591</v>
       </c>
       <c r="F7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G7" t="n">
         <v>871</v>
@@ -1448,7 +1256,7 @@
         <v>1773</v>
       </c>
       <c r="I7" t="s">
-        <v>194</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1468,7 +1276,7 @@
         <v>512</v>
       </c>
       <c r="F8" t="s">
-        <v>285</v>
+        <v>222</v>
       </c>
       <c r="G8" t="n">
         <v>685</v>
@@ -1477,12 +1285,12 @@
         <v>1536</v>
       </c>
       <c r="I8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>172</v>
+        <v>13</v>
       </c>
       <c r="B9" t="n">
         <v>51765</v>
@@ -1497,7 +1305,7 @@
         <v>297</v>
       </c>
       <c r="F9" t="s">
-        <v>238</v>
+        <v>182</v>
       </c>
       <c r="G9" t="n">
         <v>52</v>
@@ -1506,12 +1314,12 @@
         <v>891</v>
       </c>
       <c r="I9" t="s">
-        <v>222</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>279</v>
+        <v>216</v>
       </c>
       <c r="B10" t="n">
         <v>2872</v>
@@ -1526,7 +1334,7 @@
         <v>385</v>
       </c>
       <c r="F10" t="s">
-        <v>198</v>
+        <v>153</v>
       </c>
       <c r="G10" t="n">
         <v>214</v>
@@ -1535,12 +1343,12 @@
         <v>1155</v>
       </c>
       <c r="I10" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="B11" t="n">
         <v>1956</v>
@@ -1555,7 +1363,7 @@
         <v>1022</v>
       </c>
       <c r="F11" t="s">
-        <v>265</v>
+        <v>224</v>
       </c>
       <c r="G11" t="n">
         <v>2086</v>
@@ -1564,12 +1372,12 @@
         <v>3066</v>
       </c>
       <c r="I11" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>272</v>
+        <v>211</v>
       </c>
       <c r="B12" t="n">
         <v>1453</v>
@@ -1584,7 +1392,7 @@
         <v>294</v>
       </c>
       <c r="F12" t="s">
-        <v>247</v>
+        <v>188</v>
       </c>
       <c r="G12" t="n">
         <v>1</v>
@@ -1593,12 +1401,12 @@
         <v>882</v>
       </c>
       <c r="I12" t="s">
-        <v>163</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B13" t="n">
         <v>1454</v>
@@ -1613,7 +1421,7 @@
         <v>294</v>
       </c>
       <c r="F13" t="s">
-        <v>169</v>
+        <v>129</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
@@ -1622,12 +1430,12 @@
         <v>882</v>
       </c>
       <c r="I13" t="s">
-        <v>203</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="B14" t="n">
         <v>5598</v>
@@ -1642,7 +1450,7 @@
         <v>292</v>
       </c>
       <c r="F14" t="s">
-        <v>268</v>
+        <v>207</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
@@ -1656,7 +1464,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B15" t="n">
         <v>5347</v>
@@ -1671,7 +1479,7 @@
         <v>345</v>
       </c>
       <c r="F15" t="s">
-        <v>126</v>
+        <v>96</v>
       </c>
       <c r="G15" t="n">
         <v>97</v>
@@ -1680,12 +1488,12 @@
         <v>1035</v>
       </c>
       <c r="I15" t="s">
-        <v>182</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>274</v>
+        <v>213</v>
       </c>
       <c r="B16" t="n">
         <v>5563</v>
@@ -1700,7 +1508,7 @@
         <v>279</v>
       </c>
       <c r="F16" t="s">
-        <v>260</v>
+        <v>199</v>
       </c>
       <c r="G16" t="n">
         <v>16</v>
@@ -1709,12 +1517,12 @@
         <v>837</v>
       </c>
       <c r="I16" t="s">
-        <v>142</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>117</v>
+        <v>42</v>
       </c>
       <c r="B17" t="n">
         <v>1025</v>
@@ -1729,7 +1537,7 @@
         <v>330</v>
       </c>
       <c r="F17" t="s">
-        <v>248</v>
+        <v>189</v>
       </c>
       <c r="G17" t="n">
         <v>1</v>
@@ -1738,12 +1546,12 @@
         <v>990</v>
       </c>
       <c r="I17" t="s">
-        <v>243</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>174</v>
+        <v>133</v>
       </c>
       <c r="B18" t="n">
         <v>5747</v>
@@ -1758,7 +1566,7 @@
         <v>689</v>
       </c>
       <c r="F18" t="s">
-        <v>280</v>
+        <v>217</v>
       </c>
       <c r="G18" t="n">
         <v>1231</v>
@@ -1767,12 +1575,12 @@
         <v>2067</v>
       </c>
       <c r="I18" t="s">
-        <v>206</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="B19" t="n">
         <v>8569</v>
@@ -1787,7 +1595,7 @@
         <v>382</v>
       </c>
       <c r="F19" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="G19" t="n">
         <v>109</v>
@@ -1796,12 +1604,12 @@
         <v>1146</v>
       </c>
       <c r="I19" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B20" t="n">
         <v>5292</v>
@@ -1816,7 +1624,7 @@
         <v>313</v>
       </c>
       <c r="F20" t="s">
-        <v>219</v>
+        <v>168</v>
       </c>
       <c r="G20" t="n">
         <v>85</v>
@@ -1825,12 +1633,12 @@
         <v>939</v>
       </c>
       <c r="I20" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B21" t="n">
         <v>7272</v>
@@ -1845,7 +1653,7 @@
         <v>808</v>
       </c>
       <c r="F21" t="s">
-        <v>204</v>
+        <v>21</v>
       </c>
       <c r="G21" t="n">
         <v>1555</v>
@@ -1854,12 +1662,12 @@
         <v>2424</v>
       </c>
       <c r="I21" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>128</v>
+        <v>209</v>
       </c>
       <c r="B22" t="n">
         <v>8428</v>
@@ -1874,7 +1682,7 @@
         <v>289</v>
       </c>
       <c r="F22" t="s">
-        <v>208</v>
+        <v>161</v>
       </c>
       <c r="G22" t="n">
         <v>55</v>
@@ -1883,7 +1691,7 @@
         <v>867</v>
       </c>
       <c r="I22" t="s">
-        <v>263</v>
+        <v>202</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1903,7 +1711,7 @@
         <v>798</v>
       </c>
       <c r="F23" t="s">
-        <v>166</v>
+        <v>126</v>
       </c>
       <c r="G23" t="n">
         <v>1393</v>
@@ -1912,12 +1720,12 @@
         <v>2394</v>
       </c>
       <c r="I23" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>275</v>
+        <v>214</v>
       </c>
       <c r="B24" t="n">
         <v>1198</v>
@@ -1932,7 +1740,7 @@
         <v>484</v>
       </c>
       <c r="F24" t="s">
-        <v>183</v>
+        <v>141</v>
       </c>
       <c r="G24" t="n">
         <v>379</v>
@@ -1941,12 +1749,12 @@
         <v>1452</v>
       </c>
       <c r="I24" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="B25" t="n">
         <v>1613</v>
@@ -1961,7 +1769,7 @@
         <v>289</v>
       </c>
       <c r="F25" t="s">
-        <v>220</v>
+        <v>169</v>
       </c>
       <c r="G25" t="n">
         <v>25</v>
@@ -1970,12 +1778,12 @@
         <v>867</v>
       </c>
       <c r="I25" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>209</v>
+        <v>162</v>
       </c>
       <c r="B26" t="n">
         <v>7867</v>
@@ -1990,7 +1798,7 @@
         <v>349</v>
       </c>
       <c r="F26" t="s">
-        <v>269</v>
+        <v>208</v>
       </c>
       <c r="G26" t="n">
         <v>97</v>
@@ -1999,12 +1807,12 @@
         <v>1047</v>
       </c>
       <c r="I26" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="B27" t="n">
         <v>9748</v>
@@ -2019,7 +1827,7 @@
         <v>320</v>
       </c>
       <c r="F27" t="s">
-        <v>154</v>
+        <v>116</v>
       </c>
       <c r="G27" t="n">
         <v>55</v>
@@ -2028,12 +1836,12 @@
         <v>960</v>
       </c>
       <c r="I27" t="s">
-        <v>210</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>180</v>
+        <v>139</v>
       </c>
       <c r="B28" t="n">
         <v>8445</v>
@@ -2048,7 +1856,7 @@
         <v>552</v>
       </c>
       <c r="F28" t="s">
-        <v>187</v>
+        <v>145</v>
       </c>
       <c r="G28" t="n">
         <v>436</v>
@@ -2057,12 +1865,12 @@
         <v>1656</v>
       </c>
       <c r="I28" t="s">
-        <v>257</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>132</v>
+        <v>101</v>
       </c>
       <c r="B29" t="n">
         <v>815</v>
@@ -2077,7 +1885,7 @@
         <v>302</v>
       </c>
       <c r="F29" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G29" t="n">
         <v>37</v>
@@ -2086,12 +1894,12 @@
         <v>906</v>
       </c>
       <c r="I29" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>234</v>
+        <v>179</v>
       </c>
       <c r="B30" t="n">
         <v>9262</v>
@@ -2106,7 +1914,7 @@
         <v>329</v>
       </c>
       <c r="F30" t="s">
-        <v>167</v>
+        <v>127</v>
       </c>
       <c r="G30" t="n">
         <v>73</v>
@@ -2115,12 +1923,12 @@
         <v>987</v>
       </c>
       <c r="I30" t="s">
-        <v>261</v>
+        <v>200</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>130</v>
+        <v>99</v>
       </c>
       <c r="B31" t="n">
         <v>814</v>
@@ -2135,7 +1943,7 @@
         <v>340</v>
       </c>
       <c r="F31" t="s">
-        <v>218</v>
+        <v>130</v>
       </c>
       <c r="G31" t="n">
         <v>43</v>
@@ -2144,12 +1952,12 @@
         <v>1020</v>
       </c>
       <c r="I31" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>227</v>
+        <v>174</v>
       </c>
       <c r="B32" t="n">
         <v>8814</v>
@@ -2164,7 +1972,7 @@
         <v>265</v>
       </c>
       <c r="F32" t="s">
-        <v>147</v>
+        <v>74</v>
       </c>
       <c r="G32" t="n">
         <v>4</v>
@@ -2173,12 +1981,12 @@
         <v>795</v>
       </c>
       <c r="I32" t="s">
-        <v>259</v>
+        <v>198</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>153</v>
+        <v>115</v>
       </c>
       <c r="B33" t="n">
         <v>818</v>
@@ -2193,7 +2001,7 @@
         <v>315</v>
       </c>
       <c r="F33" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="G33" t="n">
         <v>13</v>
@@ -2202,12 +2010,12 @@
         <v>945</v>
       </c>
       <c r="I33" t="s">
-        <v>213</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="B34" t="n">
         <v>56924</v>
@@ -2222,7 +2030,7 @@
         <v>681</v>
       </c>
       <c r="F34" t="s">
-        <v>231</v>
+        <v>185</v>
       </c>
       <c r="G34" t="n">
         <v>1147</v>
@@ -2231,12 +2039,12 @@
         <v>2043</v>
       </c>
       <c r="I34" t="s">
-        <v>232</v>
+        <v>177</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B35" t="n">
         <v>57144</v>
@@ -2251,7 +2059,7 @@
         <v>719</v>
       </c>
       <c r="F35" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="G35" t="n">
         <v>1273</v>
@@ -2260,12 +2068,12 @@
         <v>2157</v>
       </c>
       <c r="I35" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="B36" t="n">
         <v>5261</v>
@@ -2280,7 +2088,7 @@
         <v>293</v>
       </c>
       <c r="F36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G36" t="n">
         <v>16</v>
@@ -2289,12 +2097,12 @@
         <v>879</v>
       </c>
       <c r="I36" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B37" t="n">
         <v>9088</v>
@@ -2309,7 +2117,7 @@
         <v>360</v>
       </c>
       <c r="F37" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G37" t="n">
         <v>217</v>
@@ -2318,12 +2126,12 @@
         <v>1080</v>
       </c>
       <c r="I37" t="s">
-        <v>217</v>
+        <v>167</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
       <c r="B38" t="n">
         <v>8576</v>
@@ -2338,7 +2146,7 @@
         <v>294</v>
       </c>
       <c r="F38" t="s">
-        <v>264</v>
+        <v>203</v>
       </c>
       <c r="G38" t="n">
         <v>37</v>
@@ -2347,12 +2155,12 @@
         <v>882</v>
       </c>
       <c r="I38" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B39" t="n">
         <v>92335</v>
@@ -2367,7 +2175,7 @@
         <v>402</v>
       </c>
       <c r="F39" t="s">
-        <v>224</v>
+        <v>171</v>
       </c>
       <c r="G39" t="n">
         <v>88</v>
@@ -2376,12 +2184,12 @@
         <v>1206</v>
       </c>
       <c r="I39" t="s">
-        <v>237</v>
+        <v>181</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B40" t="n">
         <v>7444</v>
@@ -2396,7 +2204,7 @@
         <v>335</v>
       </c>
       <c r="F40" t="s">
-        <v>267</v>
+        <v>206</v>
       </c>
       <c r="G40" t="n">
         <v>40</v>
@@ -2405,12 +2213,12 @@
         <v>1005</v>
       </c>
       <c r="I40" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B41" t="n">
         <v>51231</v>
@@ -2425,7 +2233,7 @@
         <v>474</v>
       </c>
       <c r="F41" t="s">
-        <v>284</v>
+        <v>221</v>
       </c>
       <c r="G41" t="n">
         <v>436</v>
@@ -2434,12 +2242,12 @@
         <v>1422</v>
       </c>
       <c r="I41" t="s">
-        <v>193</v>
+        <v>150</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>158</v>
+        <v>119</v>
       </c>
       <c r="B42" t="n">
         <v>2042</v>
@@ -2454,7 +2262,7 @@
         <v>947</v>
       </c>
       <c r="F42" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="G42" t="n">
         <v>1816</v>
@@ -2463,12 +2271,12 @@
         <v>2841</v>
       </c>
       <c r="I42" t="s">
-        <v>156</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="B43" t="n">
         <v>2260</v>
@@ -2483,7 +2291,7 @@
         <v>772</v>
       </c>
       <c r="F43" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="G43" t="n">
         <v>1366</v>
@@ -2492,12 +2300,12 @@
         <v>2316</v>
       </c>
       <c r="I43" t="s">
-        <v>52</v>
+        <v>228</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B44" t="n">
         <v>8573</v>
@@ -2512,7 +2320,7 @@
         <v>340</v>
       </c>
       <c r="F44" t="s">
-        <v>173</v>
+        <v>132</v>
       </c>
       <c r="G44" t="n">
         <v>1</v>
@@ -2521,12 +2329,12 @@
         <v>1020</v>
       </c>
       <c r="I44" t="s">
-        <v>255</v>
+        <v>194</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>127</v>
+        <v>97</v>
       </c>
       <c r="B45" t="n">
         <v>3702</v>
@@ -2541,7 +2349,7 @@
         <v>620</v>
       </c>
       <c r="F45" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="G45" t="n">
         <v>1069</v>
@@ -2550,12 +2358,12 @@
         <v>1860</v>
       </c>
       <c r="I45" t="s">
-        <v>177</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>186</v>
+        <v>144</v>
       </c>
       <c r="B46" t="n">
         <v>6197</v>
@@ -2570,7 +2378,7 @@
         <v>740</v>
       </c>
       <c r="F46" t="s">
-        <v>149</v>
+        <v>113</v>
       </c>
       <c r="G46" t="n">
         <v>1195</v>
@@ -2579,12 +2387,12 @@
         <v>2220</v>
       </c>
       <c r="I46" t="s">
-        <v>185</v>
+        <v>143</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="B47" t="n">
         <v>6197</v>
@@ -2599,7 +2407,7 @@
         <v>740</v>
       </c>
       <c r="F47" t="s">
-        <v>149</v>
+        <v>113</v>
       </c>
       <c r="G47" t="n">
         <v>1195</v>
@@ -2608,12 +2416,12 @@
         <v>2220</v>
       </c>
       <c r="I47" t="s">
-        <v>185</v>
+        <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>223</v>
+        <v>170</v>
       </c>
       <c r="B48" t="n">
         <v>4233</v>
@@ -2628,7 +2436,7 @@
         <v>1346</v>
       </c>
       <c r="F48" t="s">
-        <v>235</v>
+        <v>180</v>
       </c>
       <c r="G48" t="n">
         <v>3112</v>
@@ -2637,12 +2445,12 @@
         <v>4038</v>
       </c>
       <c r="I48" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="B49" t="n">
         <v>673</v>
@@ -2657,7 +2465,7 @@
         <v>719</v>
       </c>
       <c r="F49" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G49" t="n">
         <v>1330</v>
@@ -2666,12 +2474,12 @@
         <v>2157</v>
       </c>
       <c r="I49" t="s">
-        <v>192</v>
+        <v>149</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
       <c r="B50" t="n">
         <v>5603</v>
@@ -2686,7 +2494,7 @@
         <v>352</v>
       </c>
       <c r="F50" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
       <c r="G50" t="n">
         <v>1</v>
@@ -2695,12 +2503,12 @@
         <v>1056</v>
       </c>
       <c r="I50" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" t="s">
-        <v>191</v>
+        <v>148</v>
       </c>
       <c r="B51" t="n">
         <v>6416</v>
@@ -2715,7 +2523,7 @@
         <v>399</v>
       </c>
       <c r="F51" t="s">
-        <v>196</v>
+        <v>152</v>
       </c>
       <c r="G51" t="n">
         <v>238</v>
@@ -2724,12 +2532,12 @@
         <v>1197</v>
       </c>
       <c r="I51" t="s">
-        <v>273</v>
+        <v>212</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="B52" t="n">
         <v>6195</v>
@@ -2744,7 +2552,7 @@
         <v>735</v>
       </c>
       <c r="F52" t="s">
-        <v>229</v>
+        <v>176</v>
       </c>
       <c r="G52" t="n">
         <v>1231</v>
@@ -2753,12 +2561,12 @@
         <v>2205</v>
       </c>
       <c r="I52" t="s">
-        <v>254</v>
+        <v>193</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B53" t="n">
         <v>6195</v>
@@ -2773,7 +2581,7 @@
         <v>735</v>
       </c>
       <c r="F53" t="s">
-        <v>229</v>
+        <v>176</v>
       </c>
       <c r="G53" t="n">
         <v>1231</v>
@@ -2782,18 +2590,18 @@
         <v>2205</v>
       </c>
       <c r="I53" t="s">
-        <v>254</v>
+        <v>193</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B54" t="n">
         <v>5599</v>
       </c>
       <c r="C54" t="s">
-        <v>282</v>
+        <v>219</v>
       </c>
       <c r="D54" t="n">
         <v>1</v>
@@ -2802,7 +2610,7 @@
         <v>364</v>
       </c>
       <c r="F54" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G54" t="n">
         <v>1</v>
@@ -2811,18 +2619,18 @@
         <v>1092</v>
       </c>
       <c r="I54" t="s">
-        <v>283</v>
+        <v>220</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>161</v>
+        <v>122</v>
       </c>
       <c r="B55" t="n">
         <v>4751</v>
       </c>
       <c r="C55" t="s">
-        <v>282</v>
+        <v>219</v>
       </c>
       <c r="D55" t="n">
         <v>1</v>
@@ -2831,7 +2639,7 @@
         <v>271</v>
       </c>
       <c r="F55" t="s">
-        <v>262</v>
+        <v>201</v>
       </c>
       <c r="G55" t="n">
         <v>1</v>
@@ -2840,18 +2648,18 @@
         <v>813</v>
       </c>
       <c r="I55" t="s">
-        <v>211</v>
+        <v>164</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>225</v>
+        <v>172</v>
       </c>
       <c r="B56" t="n">
         <v>5604</v>
       </c>
       <c r="C56" t="s">
-        <v>282</v>
+        <v>219</v>
       </c>
       <c r="D56" t="n">
         <v>62</v>
@@ -2860,7 +2668,7 @@
         <v>273</v>
       </c>
       <c r="F56" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G56" t="n">
         <v>184</v>
@@ -2869,18 +2677,18 @@
         <v>819</v>
       </c>
       <c r="I56" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B57" t="n">
         <v>5058</v>
       </c>
       <c r="C57" t="s">
-        <v>282</v>
+        <v>219</v>
       </c>
       <c r="D57" t="n">
         <v>248</v>
@@ -2889,7 +2697,7 @@
         <v>545</v>
       </c>
       <c r="F57" t="s">
-        <v>178</v>
+        <v>137</v>
       </c>
       <c r="G57" t="n">
         <v>742</v>
@@ -2898,7 +2706,7 @@
         <v>1635</v>
       </c>
       <c r="I57" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -2909,7 +2717,7 @@
         <v>1021</v>
       </c>
       <c r="C58" t="s">
-        <v>282</v>
+        <v>219</v>
       </c>
       <c r="D58" t="n">
         <v>1</v>
@@ -2918,7 +2726,7 @@
         <v>301</v>
       </c>
       <c r="F58" t="s">
-        <v>157</v>
+        <v>118</v>
       </c>
       <c r="G58" t="n">
         <v>1</v>
@@ -2927,18 +2735,18 @@
         <v>903</v>
       </c>
       <c r="I58" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="B59" t="n">
         <v>5610</v>
       </c>
       <c r="C59" t="s">
-        <v>282</v>
+        <v>219</v>
       </c>
       <c r="D59" t="n">
         <v>254</v>
@@ -2947,7 +2755,7 @@
         <v>551</v>
       </c>
       <c r="F59" t="s">
-        <v>160</v>
+        <v>121</v>
       </c>
       <c r="G59" t="n">
         <v>760</v>
@@ -2956,18 +2764,18 @@
         <v>1653</v>
       </c>
       <c r="I59" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="B60" t="n">
         <v>5608</v>
       </c>
       <c r="C60" t="s">
-        <v>282</v>
+        <v>219</v>
       </c>
       <c r="D60" t="n">
         <v>1</v>
@@ -2976,7 +2784,7 @@
         <v>334</v>
       </c>
       <c r="F60" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="G60" t="n">
         <v>1</v>
@@ -2985,18 +2793,18 @@
         <v>1002</v>
       </c>
       <c r="I60" t="s">
-        <v>29</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>143</v>
+        <v>61</v>
       </c>
       <c r="B61" t="n">
         <v>140609</v>
       </c>
       <c r="C61" t="s">
-        <v>282</v>
+        <v>219</v>
       </c>
       <c r="D61" t="n">
         <v>1</v>
@@ -3005,7 +2813,7 @@
         <v>302</v>
       </c>
       <c r="F61" t="s">
-        <v>165</v>
+        <v>125</v>
       </c>
       <c r="G61" t="n">
         <v>1</v>
@@ -3014,18 +2822,18 @@
         <v>906</v>
       </c>
       <c r="I61" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="B62" t="n">
         <v>659</v>
       </c>
       <c r="C62" t="s">
-        <v>282</v>
+        <v>219</v>
       </c>
       <c r="D62" t="n">
         <v>189</v>
@@ -3034,7 +2842,7 @@
         <v>517</v>
       </c>
       <c r="F62" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="G62" t="n">
         <v>565</v>
@@ -3043,18 +2851,18 @@
         <v>1551</v>
       </c>
       <c r="I62" t="s">
-        <v>136</v>
+        <v>104</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B63" t="n">
         <v>5127</v>
       </c>
       <c r="C63" t="s">
-        <v>282</v>
+        <v>219</v>
       </c>
       <c r="D63" t="n">
         <v>163</v>
@@ -3063,7 +2871,7 @@
         <v>478</v>
       </c>
       <c r="F63" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G63" t="n">
         <v>487</v>
@@ -3072,18 +2880,18 @@
         <v>1434</v>
       </c>
       <c r="I63" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B64" t="n">
         <v>5605</v>
       </c>
       <c r="C64" t="s">
-        <v>282</v>
+        <v>219</v>
       </c>
       <c r="D64" t="n">
         <v>55</v>
@@ -3092,7 +2900,7 @@
         <v>400</v>
       </c>
       <c r="F64" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="G64" t="n">
         <v>163</v>
@@ -3101,12 +2909,12 @@
         <v>1200</v>
       </c>
       <c r="I64" t="s">
-        <v>277</v>
+        <v>215</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="B65" t="n">
         <v>1457</v>
@@ -3121,7 +2929,7 @@
         <v>335</v>
       </c>
       <c r="F65" t="s">
-        <v>291</v>
+        <v>226</v>
       </c>
       <c r="G65" t="n">
         <v>1</v>
@@ -3130,12 +2938,12 @@
         <v>1005</v>
       </c>
       <c r="I65" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
       <c r="B66" t="n">
         <v>11200</v>
@@ -3150,7 +2958,7 @@
         <v>531</v>
       </c>
       <c r="F66" t="s">
-        <v>258</v>
+        <v>197</v>
       </c>
       <c r="G66" t="n">
         <v>628</v>
@@ -3159,12 +2967,12 @@
         <v>1593</v>
       </c>
       <c r="I66" t="s">
-        <v>162</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="B67" t="n">
         <v>5566</v>
@@ -3179,7 +2987,7 @@
         <v>351</v>
       </c>
       <c r="F67" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="G67" t="n">
         <v>46</v>
@@ -3188,12 +2996,12 @@
         <v>1053</v>
       </c>
       <c r="I67" t="s">
-        <v>150</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>131</v>
+        <v>100</v>
       </c>
       <c r="B68" t="n">
         <v>1445</v>
@@ -3208,7 +3016,7 @@
         <v>450</v>
       </c>
       <c r="F68" t="s">
-        <v>200</v>
+        <v>154</v>
       </c>
       <c r="G68" t="n">
         <v>562</v>
@@ -3217,12 +3025,12 @@
         <v>1350</v>
       </c>
       <c r="I68" t="s">
-        <v>252</v>
+        <v>191</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B69" t="n">
         <v>5600</v>
@@ -3237,7 +3045,7 @@
         <v>364</v>
       </c>
       <c r="F69" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G69" t="n">
         <v>1</v>
@@ -3246,12 +3054,12 @@
         <v>1092</v>
       </c>
       <c r="I69" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>281</v>
+        <v>218</v>
       </c>
       <c r="B70" t="n">
         <v>1459</v>
@@ -3266,7 +3074,7 @@
         <v>334</v>
       </c>
       <c r="F70" t="s">
-        <v>201</v>
+        <v>155</v>
       </c>
       <c r="G70" t="n">
         <v>1</v>
@@ -3275,12 +3083,12 @@
         <v>1002</v>
       </c>
       <c r="I70" t="s">
-        <v>159</v>
+        <v>120</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>228</v>
+        <v>175</v>
       </c>
       <c r="B71" t="n">
         <v>4140</v>
@@ -3295,7 +3103,7 @@
         <v>370</v>
       </c>
       <c r="F71" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="G71" t="n">
         <v>142</v>
@@ -3304,12 +3112,12 @@
         <v>1110</v>
       </c>
       <c r="I71" t="s">
-        <v>216</v>
+        <v>166</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B72" t="n">
         <v>2011</v>
@@ -3324,7 +3132,7 @@
         <v>330</v>
       </c>
       <c r="F72" t="s">
-        <v>240</v>
+        <v>184</v>
       </c>
       <c r="G72" t="n">
         <v>46</v>
@@ -3333,12 +3141,12 @@
         <v>990</v>
       </c>
       <c r="I72" t="s">
-        <v>233</v>
+        <v>178</v>
       </c>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>25</v>
+        <v>158</v>
       </c>
       <c r="B73" t="n">
         <v>5595</v>
@@ -3353,7 +3161,7 @@
         <v>379</v>
       </c>
       <c r="F73" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="G73" t="n">
         <v>1</v>
@@ -3362,12 +3170,12 @@
         <v>1137</v>
       </c>
       <c r="I73" t="s">
-        <v>286</v>
+        <v>223</v>
       </c>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>256</v>
+        <v>195</v>
       </c>
       <c r="B74" t="n">
         <v>7443</v>
@@ -3382,7 +3190,7 @@
         <v>364</v>
       </c>
       <c r="F74" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="G74" t="n">
         <v>7</v>
@@ -3391,18 +3199,18 @@
         <v>1092</v>
       </c>
       <c r="I74" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
       <c r="B75" t="n">
         <v>1612</v>
       </c>
       <c r="C75" t="s">
-        <v>282</v>
+        <v>219</v>
       </c>
       <c r="D75" t="n">
         <v>2</v>
@@ -3411,7 +3219,7 @@
         <v>285</v>
       </c>
       <c r="F75" t="s">
-        <v>214</v>
+        <v>165</v>
       </c>
       <c r="G75" t="n">
         <v>4</v>
@@ -3420,579 +3228,645 @@
         <v>855</v>
       </c>
       <c r="I75" t="s">
-        <v>116</v>
+        <v>15</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="B76" t="n">
-        <v>5602</v>
+        <v>1956</v>
+      </c>
+      <c r="C76" t="s">
+        <v>2</v>
       </c>
       <c r="D76" t="n">
-        <v>46</v>
+        <v>696</v>
       </c>
       <c r="E76" t="n">
-        <v>400</v>
+        <v>1022</v>
       </c>
       <c r="F76" t="s">
-        <v>109</v>
+        <v>224</v>
       </c>
       <c r="G76" t="n">
-        <v>136</v>
+        <v>2086</v>
       </c>
       <c r="H76" t="n">
-        <v>1200</v>
+        <v>3066</v>
       </c>
       <c r="I76" t="s">
-        <v>239</v>
+        <v>105</v>
       </c>
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>179</v>
+        <v>76</v>
       </c>
       <c r="B77" t="n">
-        <v>1111</v>
+        <v>673</v>
+      </c>
+      <c r="C77" t="s">
+        <v>2</v>
       </c>
       <c r="D77" t="n">
-        <v>2</v>
+        <v>444</v>
       </c>
       <c r="E77" t="n">
-        <v>269</v>
+        <v>719</v>
       </c>
       <c r="F77" t="s">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="G77" t="n">
-        <v>4</v>
+        <v>1330</v>
       </c>
       <c r="H77" t="n">
-        <v>807</v>
+        <v>2157</v>
       </c>
       <c r="I77" t="s">
-        <v>290</v>
+        <v>149</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>242</v>
+        <v>170</v>
       </c>
       <c r="B78" t="n">
-        <v>23604</v>
+        <v>4233</v>
+      </c>
+      <c r="C78" t="s">
+        <v>2</v>
       </c>
       <c r="D78" t="n">
-        <v>11</v>
+        <v>1038</v>
       </c>
       <c r="E78" t="n">
-        <v>330</v>
+        <v>1346</v>
       </c>
       <c r="F78" t="s">
-        <v>67</v>
+        <v>180</v>
       </c>
       <c r="G78" t="n">
-        <v>31</v>
+        <v>3112</v>
       </c>
       <c r="H78" t="n">
-        <v>990</v>
+        <v>4038</v>
       </c>
       <c r="I78" t="s">
-        <v>181</v>
+        <v>17</v>
       </c>
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="B79" t="n">
-        <v>2242</v>
+        <v>2260</v>
+      </c>
+      <c r="C79" t="s">
+        <v>2</v>
       </c>
       <c r="D79" t="n">
-        <v>448</v>
+        <v>456</v>
       </c>
       <c r="E79" t="n">
-        <v>822</v>
+        <v>772</v>
       </c>
       <c r="F79" t="s">
-        <v>276</v>
+        <v>53</v>
       </c>
       <c r="G79" t="n">
-        <v>1342</v>
+        <v>1366</v>
       </c>
       <c r="H79" t="n">
-        <v>2466</v>
+        <v>2316</v>
       </c>
       <c r="I79" t="s">
-        <v>92</v>
+        <v>228</v>
       </c>
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>68</v>
+        <v>1</v>
       </c>
       <c r="B80" t="n">
-        <v>8536</v>
+        <v>25</v>
+      </c>
+      <c r="C80" t="s">
+        <v>2</v>
       </c>
       <c r="D80" t="n">
-        <v>1</v>
+        <v>229</v>
       </c>
       <c r="E80" t="n">
-        <v>293</v>
+        <v>512</v>
       </c>
       <c r="F80" t="s">
-        <v>287</v>
+        <v>222</v>
       </c>
       <c r="G80" t="n">
-        <v>1</v>
+        <v>685</v>
       </c>
       <c r="H80" t="n">
-        <v>879</v>
+        <v>1536</v>
       </c>
       <c r="I80" t="s">
-        <v>144</v>
+        <v>23</v>
       </c>
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B81" t="n">
-        <v>6793</v>
+        <v>1432</v>
+      </c>
+      <c r="C81" t="s">
+        <v>2</v>
       </c>
       <c r="D81" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="E81" t="n">
-        <v>316</v>
+        <v>360</v>
       </c>
       <c r="F81" t="s">
-        <v>115</v>
+        <v>187</v>
       </c>
       <c r="G81" t="n">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="H81" t="n">
-        <v>948</v>
+        <v>1080</v>
       </c>
       <c r="I81" t="s">
-        <v>207</v>
+        <v>56</v>
       </c>
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>241</v>
+        <v>24</v>
       </c>
       <c r="B82" t="n">
-        <v>3611</v>
+        <v>5594</v>
+      </c>
+      <c r="C82" t="s">
+        <v>2</v>
       </c>
       <c r="D82" t="n">
-        <v>183</v>
+        <v>1</v>
       </c>
       <c r="E82" t="n">
-        <v>452</v>
+        <v>360</v>
       </c>
       <c r="F82" t="s">
-        <v>250</v>
+        <v>227</v>
       </c>
       <c r="G82" t="n">
-        <v>547</v>
+        <v>1</v>
       </c>
       <c r="H82" t="n">
-        <v>1356</v>
+        <v>1080</v>
       </c>
       <c r="I82" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="B83" t="n">
-        <v>6850</v>
+        <v>11200</v>
+      </c>
+      <c r="C83" t="s">
+        <v>2</v>
       </c>
       <c r="D83" t="n">
-        <v>365</v>
+        <v>210</v>
       </c>
       <c r="E83" t="n">
-        <v>635</v>
+        <v>531</v>
       </c>
       <c r="F83" t="s">
-        <v>36</v>
+        <v>197</v>
       </c>
       <c r="G83" t="n">
-        <v>1093</v>
+        <v>628</v>
       </c>
       <c r="H83" t="n">
-        <v>1905</v>
+        <v>1593</v>
       </c>
       <c r="I83" t="s">
-        <v>74</v>
+        <v>10</v>
       </c>
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>195</v>
+        <v>147</v>
       </c>
       <c r="B84" t="n">
-        <v>7010</v>
+        <v>1017</v>
+      </c>
+      <c r="C84" t="s">
+        <v>2</v>
       </c>
       <c r="D84" t="n">
-        <v>785</v>
+        <v>2</v>
       </c>
       <c r="E84" t="n">
-        <v>1101</v>
+        <v>296</v>
       </c>
       <c r="F84" t="s">
-        <v>125</v>
+        <v>19</v>
       </c>
       <c r="G84" t="n">
-        <v>2353</v>
+        <v>4</v>
       </c>
       <c r="H84" t="n">
-        <v>3303</v>
+        <v>888</v>
       </c>
       <c r="I84" t="s">
-        <v>123</v>
+        <v>46</v>
       </c>
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>245</v>
+        <v>60</v>
       </c>
       <c r="B85" t="n">
-        <v>4217</v>
+        <v>5347</v>
+      </c>
+      <c r="C85" t="s">
+        <v>2</v>
       </c>
       <c r="D85" t="n">
-        <v>671</v>
+        <v>33</v>
       </c>
       <c r="E85" t="n">
-        <v>939</v>
+        <v>345</v>
       </c>
       <c r="F85" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="G85" t="n">
-        <v>2011</v>
+        <v>97</v>
       </c>
       <c r="H85" t="n">
-        <v>2817</v>
+        <v>1035</v>
       </c>
       <c r="I85" t="s">
-        <v>12</v>
+        <v>140</v>
       </c>
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B86" t="n">
-        <v>1195</v>
+        <v>5747</v>
+      </c>
+      <c r="C86" t="s">
+        <v>2</v>
       </c>
       <c r="D86" t="n">
-        <v>148</v>
+        <v>411</v>
       </c>
       <c r="E86" t="n">
-        <v>484</v>
+        <v>689</v>
       </c>
       <c r="F86" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
       <c r="G86" t="n">
-        <v>442</v>
+        <v>1231</v>
       </c>
       <c r="H86" t="n">
-        <v>1452</v>
+        <v>2067</v>
       </c>
       <c r="I86" t="s">
-        <v>39</v>
+        <v>160</v>
       </c>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="B87" t="n">
-        <v>2185</v>
+        <v>5599</v>
+      </c>
+      <c r="C87" t="s">
+        <v>219</v>
       </c>
       <c r="D87" t="n">
-        <v>416</v>
+        <v>1</v>
       </c>
       <c r="E87" t="n">
-        <v>692</v>
+        <v>364</v>
       </c>
       <c r="F87" t="s">
-        <v>244</v>
+        <v>27</v>
       </c>
       <c r="G87" t="n">
-        <v>1246</v>
+        <v>1</v>
       </c>
       <c r="H87" t="n">
-        <v>2076</v>
+        <v>1092</v>
       </c>
       <c r="I87" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>71</v>
+        <v>172</v>
       </c>
       <c r="B88" t="n">
-        <v>3480</v>
+        <v>5604</v>
+      </c>
+      <c r="C88" t="s">
+        <v>219</v>
       </c>
       <c r="D88" t="n">
-        <v>982</v>
+        <v>62</v>
       </c>
       <c r="E88" t="n">
-        <v>1286</v>
+        <v>273</v>
       </c>
       <c r="F88" t="s">
-        <v>205</v>
+        <v>6</v>
       </c>
       <c r="G88" t="n">
-        <v>2944</v>
+        <v>184</v>
       </c>
       <c r="H88" t="n">
-        <v>3858</v>
+        <v>819</v>
       </c>
       <c r="I88" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>59</v>
+        <v>183</v>
       </c>
       <c r="B89" t="n">
-        <v>3643</v>
+        <v>6790</v>
+      </c>
+      <c r="C89" t="s">
+        <v>2</v>
       </c>
       <c r="D89" t="n">
-        <v>1005</v>
+        <v>125</v>
       </c>
       <c r="E89" t="n">
-        <v>1310</v>
+        <v>391</v>
       </c>
       <c r="F89" t="s">
-        <v>121</v>
+        <v>81</v>
       </c>
       <c r="G89" t="n">
-        <v>3013</v>
+        <v>373</v>
       </c>
       <c r="H89" t="n">
-        <v>3930</v>
+        <v>1173</v>
       </c>
       <c r="I89" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="B90" t="n">
-        <v>817</v>
+        <v>5595</v>
+      </c>
+      <c r="C90" t="s">
+        <v>2</v>
       </c>
       <c r="D90" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="E90" t="n">
-        <v>309</v>
+        <v>379</v>
       </c>
       <c r="F90" t="s">
-        <v>221</v>
+        <v>54</v>
       </c>
       <c r="G90" t="n">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="H90" t="n">
-        <v>927</v>
+        <v>1137</v>
       </c>
       <c r="I90" t="s">
-        <v>199</v>
+        <v>223</v>
       </c>
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B91" t="n">
-        <v>9252</v>
+        <v>6197</v>
+      </c>
+      <c r="C91" t="s">
+        <v>2</v>
       </c>
       <c r="D91" t="n">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="E91" t="n">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="F91" t="s">
-        <v>278</v>
+        <v>113</v>
       </c>
       <c r="G91" t="n">
-        <v>1240</v>
+        <v>1195</v>
       </c>
       <c r="H91" t="n">
-        <v>2214</v>
+        <v>2220</v>
       </c>
       <c r="I91" t="s">
-        <v>270</v>
+        <v>143</v>
       </c>
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="B92" t="n">
-        <v>9252</v>
+        <v>6197</v>
+      </c>
+      <c r="C92" t="s">
+        <v>2</v>
       </c>
       <c r="D92" t="n">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="E92" t="n">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="F92" t="s">
-        <v>278</v>
+        <v>113</v>
       </c>
       <c r="G92" t="n">
-        <v>1240</v>
+        <v>1195</v>
       </c>
       <c r="H92" t="n">
-        <v>2214</v>
+        <v>2220</v>
       </c>
       <c r="I92" t="s">
-        <v>270</v>
+        <v>143</v>
       </c>
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>266</v>
+        <v>97</v>
       </c>
       <c r="B93" t="n">
-        <v>5601</v>
+        <v>3702</v>
+      </c>
+      <c r="C93" t="s">
+        <v>2</v>
       </c>
       <c r="D93" t="n">
-        <v>1</v>
+        <v>357</v>
       </c>
       <c r="E93" t="n">
-        <v>364</v>
+        <v>620</v>
       </c>
       <c r="F93" t="s">
-        <v>152</v>
+        <v>89</v>
       </c>
       <c r="G93" t="n">
-        <v>1</v>
+        <v>1069</v>
       </c>
       <c r="H93" t="n">
-        <v>1092</v>
+        <v>1860</v>
       </c>
       <c r="I93" t="s">
-        <v>236</v>
+        <v>136</v>
       </c>
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="B94" t="n">
-        <v>9943</v>
+        <v>5566</v>
+      </c>
+      <c r="C94" t="s">
+        <v>2</v>
       </c>
       <c r="D94" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E94" t="n">
-        <v>295</v>
+        <v>351</v>
       </c>
       <c r="F94" t="s">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="G94" t="n">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="H94" t="n">
-        <v>885</v>
+        <v>1053</v>
       </c>
       <c r="I94" t="s">
-        <v>249</v>
+        <v>22</v>
       </c>
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="B95" t="n">
-        <v>9212</v>
+        <v>1457</v>
+      </c>
+      <c r="C95" t="s">
+        <v>2</v>
       </c>
       <c r="D95" t="n">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="E95" t="n">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="F95" t="s">
-        <v>10</v>
+        <v>226</v>
       </c>
       <c r="G95" t="n">
-        <v>163</v>
+        <v>1</v>
       </c>
       <c r="H95" t="n">
-        <v>1032</v>
+        <v>1005</v>
       </c>
       <c r="I95" t="s">
-        <v>145</v>
+        <v>173</v>
       </c>
     </row>
     <row r="96" spans="1:9">
       <c r="A96" t="s">
-        <v>251</v>
+        <v>42</v>
       </c>
       <c r="B96" t="n">
-        <v>90</v>
+        <v>1025</v>
+      </c>
+      <c r="C96" t="s">
+        <v>2</v>
       </c>
       <c r="D96" t="n">
-        <v>172</v>
+        <v>1</v>
       </c>
       <c r="E96" t="n">
-        <v>499</v>
+        <v>330</v>
       </c>
       <c r="F96" t="s">
-        <v>105</v>
+        <v>189</v>
       </c>
       <c r="G96" t="n">
-        <v>514</v>
+        <v>1</v>
       </c>
       <c r="H96" t="n">
-        <v>1497</v>
+        <v>990</v>
       </c>
       <c r="I96" t="s">
-        <v>155</v>
+        <v>186</v>
       </c>
     </row>
     <row r="97" spans="1:9">
       <c r="A97" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="B97" t="n">
-        <v>658</v>
+        <v>9261</v>
+      </c>
+      <c r="C97" t="s">
+        <v>2</v>
       </c>
       <c r="D97" t="n">
-        <v>168</v>
+        <v>25</v>
       </c>
       <c r="E97" t="n">
-        <v>502</v>
+        <v>348</v>
       </c>
       <c r="F97" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="G97" t="n">
-        <v>502</v>
+        <v>73</v>
       </c>
       <c r="H97" t="n">
-        <v>1506</v>
+        <v>1044</v>
       </c>
       <c r="I97" t="s">
-        <v>65</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix to PDB construct selection script.
</commit_message>
<xml_diff>
--- a/analysis/PDB_construct_selection/PDB_constructs.xlsx
+++ b/analysis/PDB_construct_selection/PDB_constructs.xlsx
@@ -17,594 +17,591 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="229">
   <si>
+    <t>TCAGTTTATCCTAAGGCATTAAGAGATGAATACATCATGTCAAAAACTCTTGGAAGTGGTGCCTGTGGAGAGGTAAAGCTGGCTTTCGAGAGGAAAACATGTAAGAAAGTAGCCATAAAGATCATCAGCAAAAGGAAGTTTGCTATTGGTTCAGCAAGAGAGGCAGACCCAGCTCTCAATGTTGAAACAGAAATAGAAATTTTGAAAAAGCTAAATCATCCTTGCATCATCAAGATTAAAAACTTTTTTGATGCAGAAGATTATTATATTGTTTTGGAATTGATGGAAGGGGGAGAGCTGTTTGACAAAGTGGTGGGGAATAAACGCCTGAAAGAAGCTACCTGCAAGCTCTATTTTTACCAGATGCTCTTGGCTGTGCAGTACCTTCATGAAAACGGTATTATACACCGTGACTTAAAGCCAGAGAATGTTTTACTGTCATCTCAAGAAGAGGACTGTCTTATAAAGATTACTGATTTTGGGCACTCCAAGATTTGGGGAGAGACCTCTCTCATGAGAACCTTATGTGGAACCCCCACCTACTTGGCGCCTGAAGTTCTTGTTTCTGTTGGGACTGCTGGGTATAACCGTGCTGTGGACTGCTGGAGTTTAGGAGTTATTCTTTTTATCTGCCTTAGTGGGTATCCACCTTTCTCTGAGCATAGGACTCAAGTGTCACTGAAGGATCAGATCACCAGTGGAAAATACAACTTCATTCCTGAAGTCTGGGCAGAAGTCTCAGAGAAAGCTCTGGACCTTGTCAAGAAGTTGTTGGTAGTGGATCCAAAGGCACGTTTTACGACAGAAGAAGCCTTAAGACACCCGTGGCTTCAGGATGAAGACATGAAGAGAAAGTTTCAAGATCTTCTGTCTGAGGAAAATGAATCCACAGCTCTACCCCAGGTTCTAGCCCAGCCTTCTACTAGTCGAAAGCGGCCCCGTGAAGGGGAAGCCGAGGGTGCCGAG</t>
+  </si>
+  <si>
+    <t>ABL1_HUMAN_D0_3UE4_A</t>
+  </si>
+  <si>
+    <t>Nterm</t>
+  </si>
+  <si>
+    <t>HASP_HUMAN_D0_3E7V_A</t>
+  </si>
+  <si>
+    <t>CDK6_HUMAN_D0_4EZ5_A</t>
+  </si>
+  <si>
+    <t>SPQREPQRVSHEQFRAALQLVVDPGDPRSYLDNFIKIGEGSTGIVCIATVRSSGKLVAVKKMDLRKQQRRELLFNEVVIMRDYQHENVVEMYNSYLVGDELWVVMEFLEGGALTDIVTHTRMNEEQIAAVCLAVLQALSVLHAQGVIHRDIKSDSILLTHDGRVKLSDFGFCAQVSKEVPRRKSLVGTPYWMAPELISRLPYGPEVDIWSLGIMVIEMVDGEPPYFNEPPLKAMKMIRDNLPPRLKNLHKVSPSLKGFLDRLLVRDPAQRATAAELLKHPFLAKAGPPASIVPLMRQNRTR</t>
+  </si>
+  <si>
+    <t>ELKDDDFEKISELGAGNGGVVFKVSHKPSGLVMARKLIHLEIKPAIRNQIIRELQVLHECNSPYIVGFYGAFYSDGEISICMEHMDGGSLDQVLKKAGRIPEQILGKVSIAVIKGLTYLREKHKIMHRAYGMDSRPPMAIFELLDYIVNEPPPKLPSGVFSLEFQDFVNKCLIKNPAERADLKQLMVHAFIKRSDAEEVDFAGWLCSTIGLN</t>
+  </si>
+  <si>
+    <t>TACCAGCTCTTCGAGGAATTGGGCAAGGGAGCCTTCTCGGTGGTGCGAAGGTGTGTGAAGGTGCTGGCTGGCCAGGAGTATGCTGCCAAGATCATCAACACAAAGAAGCTGTCAGCCAGAGACCATCAGAAGCTGGAGCGTGAAGCCCGCATCTGCCGCCTGCTGAAGCACCCCAACATCGTCCGACTACATGACAGCATCTCAGAGGAGGGACACCACTACCTGATCTTCGACCTGGTCACTGGTGGGGAACTGTTTGAAGATATCGTGGCCCGGGAGTATTACAGTGAGGCGGATGCCAGTCACTGTATCCAGCAGATCCTGGAGGCTGTGCTGCACTGCCACCAGATGGGGGTGGTGCACCGGGACCTGAAGCCTGAGAATCTGTTGCTGGCCTCCAAGCTCAAGGGTGCCGCAGTGAAGCTGGCAGACTTTGGCCTGGCCATAGAGGTGGAGGGGGAGCAGCAGGCATGGTTTGGGTTTGCAGGGACTCCTGGATATCTCTCCCCAGAAGTGCTGCGGAAGGACCCGTACGGGAAGCCTGTGGACCTGTGGGCTTGTGGGGTCATCCTGTACATCCTGCTGGTTGGGTACCCCCCGTTCTGGGATGAGGACCAGCACCGCCTGTACCTGCAGATCAAAGCCGGCGCCTATGATTTCCCATCGCCGGAATGGGACACTGTCACCCCGGAAGCCAAGGATCTGATCAATAAGATGCTGACCATTAACCCATCCAAACGCATCACAGCTGCCGAAGCCCTTAAGCACCCCTGGATCTCGCACCGCTCCACCGTGGCATCCTGCATGCACAGACAGGAGACCGTGGACTGCCTGAAGAAGTTCAATGCCAGGAGGAAACTGAAGGGAGCC</t>
+  </si>
+  <si>
+    <t>GPEDELPDWAAAKEFYQKYDPKDVIGRGVSSVVRRCVHRATGHEFAVKIMEVTAERLSPEQLEEVREATRRETHILRQVAGHPHIITLIDSYESSSFMFLVFDLMRKGELFDYLTEKVALSEKETRSIMRSLLEAVSFLHANNIVHRDLKPENILLDDNMQIRLSDFGFSCHLEPGEKLRELCGTPGYLAPEILKCSMDETHPGYGKEVDLWACGVILFTLLAGSPPFWHRRQILMLRMIMEGQYQFSSPEWDDRSSTVKDLISRLLQVDPEARLTAEQALQHPFFER</t>
+  </si>
+  <si>
+    <t>GTGGAGGACCATTATGAGATGGGGGAGGAGCTGGGCAGCGGCCAGTTTGCGATCGTGCGGAAGTGCCGGCAGAAGGGCACGGGCAAGGAGTACGCAGCCAAGTTCATCAAGAAGCGCCGCCTGTCATCCAGCCGGCGTGGGGTGAGCCGGGAGGAGATCGAGCGGGAGGTGAACATCCTGCGGGAGATCCGGCACCCCAACATCATCACCCTGCACGACATCTTCGAGAACAAGACGGACGTGGTCCTCATCCTGGAGCTGGTCTCTGGCGGGGAGCTCTTTGACTTCCTGGCGGAGAAGGAGTCGCTGACGGAGGACGAGGCCACCCAGTTCCTCAAGCAGATCCTGGACGGCGTTCACTACCTGCACTCTAAGCGCATCGCACACTTTGACCTGAAGCCGGAAAACATCATGCTGCTGGACAAGAACGTGCCCAACCCACGAATCAAGCTCATCGACTTCGGCATCGCGCACAAGATCGAGGCGGGGAACGAGTTCAAGAACATCTTCGGCACCCCGGAGTTTGTGGCCCCAGAGATTGTGAACTATGAGCCGCTGGGCCTGGAGGCGGACATGTGGAGCATCGGTGTCATCACCTATATCCTCCTGAGCGGTGCATCCCCGTTCCTGGGCGAGACCAAGCAGGAGACGCTCACCAACATCTCAGCCGTGAACTACGACTTCGACGAGGAGTACTTCAGCAACACCAGCGAGCTGGCCAAGGACTTCATTCGCCGGCTGCTCGTCAAAGATCCCAAGCGGAGAATGACCATTGCCCAGAGCCTGGAACATTCCTGGATTAAGGCGATCCGGCGGCGGAACGTGCGTGGTGAGGACAGCGGC</t>
+  </si>
+  <si>
+    <t>CACCACCATCACCACCATTCGCACTCGGGGCCGGAGATCTCGCGGATTATCGTCGACCCCACGACTGGGAAGCGCTACTGCCGGGGCAAAGTGCTGGGAAAGGGTGGCTTTGCAAAATGTTACGAGATGACAGATTTGACAAATAACAAAGTCTACGCCGCAAAAATTATTCCTCACAGCAGAGTAGCTAAACCTCATCAAAGGGAAAAGATTGACAAAGAAATAGAGCTTCACAGAATTCTTCATCATAAGCATGTAGTGCAGTTTTACCACTACTTCGAGGACAAAGAAAACATTTACATTCTCTTGGAATACTGCAGTAGAAGGTCAATGGCTCATATTTTGAAAGCAAGAAAGGTGTTGACAGAGCCAGAAGTTCGATACTACCTCAGGCAGATTGTGTCTGGACTGAAATACCTTCATGAACAAGAAATCTTGCACAGAGATCTCAAACTAGGGAACTTTTTTATTAATGAAGCCATGGAACTAAAAGTTGGGGACTTCGGTCTGGCAGCCAGGCTAGAACCCTTGGAACACAGAAGGAGAACGATATGTGGTACCCCAAATTATCTCTCTCCTGAAGTCCTCAACAAACAAGGACATGGCTGTGAATCAGACATTTGGGCCCTGGGCTGTGTAATGTATACAATGTTACTAGGGAGGCCCCCATTTGAAACTACAAATCTCAAAGAAACTTATAGGTGCATAAGGGAAGCAAGGTATACAATGCCGTCCTCATTGCTGGCTCCTGCCAAGCACTTAATTGCTAGTATGTTGTCCAAAAACCCAGAGGATCGTCCCAGTTTGGATGACATCATTCGACATGACTTTTTTTTGCAGGGCTTCACTCCGGACAGACTGTCTTCTAGCTGTTGTCATACAGTTCCAGATTTCCACTTATCAAGCCCAGCT</t>
+  </si>
+  <si>
+    <t>AAGCACGACGGGCGGGTGAAGATCGGACACTACGTGCTGGGCGACACGCTGGGCGTCGGCACCTTCGGCAAAGTGAAGATTGGAGAACATCAATTAACAGGCCATAAAGTGGCAGTTAAAATCTTAAATAGACAGAAGATTCGCAGTTTAGATGTTGTTGGAAAAATAAAACGAGAAATTCAAAATCTAAAACTCTTTCGTCATCCTCATATTATCAAACTATACCAGGTGATCAGCACTCCAACAGATTTTTTTATGGTAATGGAATATGTGTCTGGAGGTGAATTATTTGACTACATCTGTAAGCATGGACGGGTTGAAGAGATGGAAGCCAGGCGRCTCTTTCAGCAGATTCTGTCTGCTGTGGATTACTGTCATAGGCATATGGTTGTTCATCGAGACCTGAAACCAGAGAATGTCCTGTTGGATGCACACATGAATGCCAAGATAGCCGATTTCGGATTATCTAATATGATGTCAGATGGTGAATTTCTGAGAACTAGTTGCGGATCTCCAAATTATGCAGCACCTGAAGTCATCTCAGGCAGATTGTATGCAGGTCCTGAAGTTGATATCTGGAGCTGTGGTGTTATCTTGTATGCTCTTCTTTGTGGCACCCTCCCATTTGATGATGAGCATGTACCTACGTTATTTAAGAAGATCCGAGGGGGTGTCTTTTATATCCCAGAATATCTCAATCGTTCTGTCGCCACTCTCCTGATGCATATGCTGCAGGTTGACCCACTGAAACGAGCAACTATCAAAGACATAAGAGAGCATGAATGGTTTAAACAAGATTTGCCCAGTTACTTATTTCCTGAA</t>
+  </si>
+  <si>
+    <t>CSKP_HUMAN_D0_3TAC_A</t>
+  </si>
+  <si>
+    <t>MST4_HUMAN_D0_4FZD_B</t>
+  </si>
+  <si>
+    <t>CGGGACTCGAGTGATGATTGGGAGATTCCTGATGGGCAGATTACAGTGGGACAAAGAATTGGATCTGGATCATTTGGAACAGTCTACAAGGGAAAGTGGCATGGTGATGTGGCAGTGAAAATGTTGAATGTGACAGCACCTACACCTCAGCAGTTACAAGCCTTCAAAAATGAAGTAGGAGTACTCAGGAAAACACGACATGTGAATATCCTACTCTTCATGGGCTATTCCACAAAGCCACAACTGGCTATTGTTACCCAGTGGTGTGAGGGCTCCAGCTTGTATCACCATCTCCATATCATTGAGACCAAATTTGAGATGATCAAgCTTATAGATATTGCACGACAGACTGCACAGGGCATGGATTACTTACACGCCAAGTCAATCATCCACAGAGACCTCAAGAGTAATAATATATTTCTTCATGAAGACCTCACAGTAAAAATAGGTGATTTTGGTCTAGCTACAGTGAAATCTCGATGGAGTGGGTCCCATCAGTTTGAACAGTTGTCTGGgTCCATTTTGTGGATGGCACCAGAAGTCATCAGAATGCAAGATAAAAATCCATACAGCTTTCAGTCAGATGTATATGCATTTGGgATTGTTCTGTATGAATTGATGACTGGACAGTTACCTTATTCAAACATCAACAACAGGGACCAGATAATTTTTATGGTGGGACGAGGATACCTGTCTCCAGATCTCAGTAAGGTACGGAGTAACTGTCCAAAAGCCATGAAGAGATTAATGGCAGAGTGCCTCAAAAAGAAAAGAGATGAGAGACCACTCTTTCCCCAAATTCTCGCC</t>
+  </si>
+  <si>
+    <t>MARK2_HUMAN_D0_3IEC_D</t>
+  </si>
+  <si>
+    <t>CCATTTCCAGAAGGCAAGGTTCTGGATGATATGGAAGGCAATCAGTGGGTACTGGGCAAGAAGATTGGCTCTGGAGGATTTGGATTGATATATTTAGCTTTCCCCACAAATAAACCAGAGAAAGATGCAAGACATGTAGTAAAAGTGGAATATCAAGAAAATGGCCCGTTATTTTCAGAACTTAAATTTTATCAGAGAGTTGCAAAAAAAGACTGTATCAAAAAGTGGATAGAACGCAAACAACTTGATTATTTAGGAATTCCTCTGTTTTATGGATCTGGTCTGACTGAATTCAAGGGAAGAAGTTACAGATTTATGGTAATGGAAAGACTAGGAATAGATTTACAGAAGATCTCAGGCCAGAATGGTACCTTTAAAAAGTCAACTGTCCTGCAATTAGGTATCCGAATGTTGGATGTACTGGAATATATACATGAAAATGAATATGTTCATGGTGATATAAAAGCAGCAAATCTACTTTTGGGTTACAAAAATCCAGACCAGGTTTATCTTGCAGATTATGGACTTTCCTACAGATATTGTCCCAATGGGAACCACAAACAGTATCAGGAAAATCCTAGAAAAGGCCATAATGGGACAATAGAGTTTACCAGCTTGGATGCCCACAAGGGAGTAGCCTTGTCCAGACGAAGTGACGTTGAGATCCTCGGCTACTGCATGCTGCGGTGGTTGTGTGGGAAACTTCCCTGGGAACAGAACCTGAAGGACCCTGTGGCTGTGCAGACTGCTAAAACAAATCTGTTGGACGAGCTCCCCCAGTCAGTGCTTAAATGGGCTCCTTCTGGAAGCAGTTGCTGTGAAATAGCCCAATTTTTGGTATGTGCTCATAGTTTAGCATATGATGAAAAGCCAAACTATCAAGCCCTCAAGAAAATTTTGAACCCTCATGGAATACCTTTAGGACCACTGGACTTTTCCACAAAAGGACAGAGTATAAATGTCCAT</t>
+  </si>
+  <si>
+    <t>GGGGACTCTGATATATCCAGTCCATTACTGCAAAATACTGTCCACATTGACCTCAGTGCTCTAAATCCAGAGCTGGTCCAGGCAGTGCAGCATGTAGTGATTGGGCCCAGTAGCCTGATTGTGCATTTCAATGAAGTCATAGGAAGAGGGCATTTTGGTTGTGTATATCATGGGACTTTGTTGGACAATGATGGCAAGAAAATTCACTGTGCTGTGAAATCCTTGAACAGAATCACTGACATAGGAGAAGTTTCCCAATTTCTGACCGAGGGAATCATCATGAAAGATTTTAGTCATCCCAATGTCCTCTCGCTCCTGGGAATCTGCCTGCGAAGTGAAGGGTCTCCGCTGGTGGTCCTACCATACATGAAACATGGAGATCTTCGAAATTTCATTCGAAATGAGACTCATAATCCAACTGTAAAAGATCTTATTGGCTTTGGTCTTCAAGTAGCCAAAGGCATGAAATATCTTGCAAGCAAAAAGTTTGTCCACAGAGACTTGGCTGCAAGAAACTGTATGCTGGATGAAAAATTCACAGTCAAGGTTGCTGATTTTGGTCTTGCCAGAGACATGTATGATAAAGAATACTATAGTGTACACAACAAAACAGGTGCAAAGCTGCCAGTGAAGTGGATGGCTTTGGAAAGTCTGCAAACTCAAAAGTTTACCACCAAGTCAGATGTGTGGTCCTTTGGCGTGCTCCTCTGGGAGCTGATGACAAGAGGAGCCCCACCTTATCCTGACGTAAACACCTTTGATATAACTGTTTACTTGTTGCAAGGGAGAAGACTCCTACAACCCGAATACTGCCCAGACCCCTTATATGAAGTAATGCTAAAATGCTGGCACCCTAAAGCCGAAATGCGCCCATCCTTTTCTGAACTGGTGTCCCGGATATCAGCGATCTTCTCTACTTTCATTGGG</t>
+  </si>
+  <si>
+    <t>YQLFEELGKGAFSVVRRCVKVLAGQEYAAKIINTKKLSARDHQKLEREARICRLLKHPNIVRLHDSISEEGHHYLIFDLVTGGELFEDIVAREYYSEADASHCIQQILEAVLHCHQMGVVHRDLKPENLLLASKLKGAAVKLADFGLAIEVEGEQQAWFGFAGTPGYLSPEVLRKDPYGKPVDLWACGVILYILLVGYPPFWDEDQHRLYLQIKAGAYDFPSPEWDTVTPEAKDLINKMLTINPSKRITAAEALKHPWISHRSTVASCMHRQETVDCLKKFNARRKLKGA</t>
+  </si>
+  <si>
+    <t>ENFQKVEKIGEGTYGVVYKARNKLTGEVVALKKIRLDTETEGVPSTAIREISLLKELNHPNIVKLLDVIHTENKLYLVFEFLHQDLKKFMDASALTGIPLPLIKSYLFQLLQGLAFCHSHRVLHRDLKPQNLLINTEGAIKLADFGLARAFGVPVRTYTHEVVTLWYRAPEILLGCKYYSTAVDIWSLGCIFAEMVTRRALFPGDSEIDQLFRIFRTLGTPDEVVWPGVTSMPDYKPSFPKWARQDFSKVVPPLDEDGRSLLSQMLHYDPNKRISAKAALAHPFFQDVTKPVPHL</t>
+  </si>
+  <si>
+    <t>TTK_HUMAN_D0_3H9F_A</t>
+  </si>
+  <si>
+    <t>SVKGRIYSILKQIGSGGSSKVFQVLNEKKQIYAIKYVNLEEADNQTLDSYRNEIAYLNKLQQHSDKIIRLYDYEITDQYIYMVMECGNIDLNSWLKKKKSIDPWERKSYWKNMLEAVHTIHQHGIVHSDLKPANFLIVDGMLKLIDFGIANQMQPDTTSVVKDSQVGTVNYMPPEAIKDMSSSRENGKSKSKISPKSDVWSLGCILYYMTYGKTPFQQIINQISKLHAIIDPNHEIEFPDIPEKDLQDVLKCCLKRDPKQRISIPELLAHPYVQIQTHPVNQMAKGTTEE</t>
+  </si>
+  <si>
+    <t>GTGAAAGAATTCTTAGCCAAAGCCAAAGAAGATTTTCTTAAAAAATGGGAAAGTCCCGCTCAGAACACAGCCCACTTGGATCAGTTTGAACGAATCAAGACCCTCGGCACGGGCTCCTTCGGGCGGGTGATGCTGGTGAAACACAAGGAGACCGGGAACCACTATGCCATGAAGATCCTCGACAAACAGAAGGTGGTGAAACTGAAACAGATCGAACACACCCTGAATGAAAAGCGCATCCTGCAAGCTGTCAACTTTCCGTTCCTCGTCAAACTCGAGTTCTCCTTCAAGGACAACTCAAACTTATACATGGTCATGGAGTACGTGCCCGGCGGGGAGATGTTCTCACACCTACGGCGGATCGGAAGGTTCAGTGAGCCCCATGCCCGTTTCTACGCGGCCCAGATCGTCCTGACCTTTGAGTATCTGCACTCGCTGGATCTCATCTACAGGGACCTGAAGCCGGAGAATCTGCTCATTGACCAGCAGGGCTACATTCAGGTGACAGACTTCGGTTTCGCCAAGCGCGTGAAGGGCCGCACTTGGACCTTGTGCGGCACCCCTGAGTACCTGGCCCCTGAGATTATCCTGAGCAAAGGCTACAACAAGGCCGTGGACTGGTGGGCCCTGGGGGTTCTTATCTATGAAATGGCCGCTGGCTACCCGCCCTTCTTCGCAGACCAGCCCATCCAGATCTATGAGAAGATCGTCTCTGGGAAGGTGCGCTTCCCTTCCCACTTCAGCTCTGACTTGAAGGACCTGCTGCGGAACCTCCTGCAGGTAGATCTCACCAAGCGCTTTGGGAACCTCAAGAATGGGGTCAACGATATCAAGAACCACAAGTGGTTTGCCACAACTGACTGGATTGCCATCTACCAGAGGAAGGTGGAAGCTCCCTTCATACCAAAGTTTAAAGGCCCTGGGGATACGAGTAACTTTGACGACTATGAGGAAGAAGAAATCCGGGTCTCCATCAATGAGAAGTGTGGCAAGGAGTTTTCTGAGTTT</t>
+  </si>
+  <si>
+    <t>TCCCCCAACTACGACAAGTGGGAGATGGAACGCACGGACATCACCATGAAGCACAAGCTGGGCGGGGGCCAGTACGGGGAGGTGTACGAGGGCGTGTGGAAGAAATACAGCCTGACGGTGGCCGTGAAGACCTTGAAGGAGGACACCATGGAGGTGGAAGAGTTCTTGAAAGAAGCTGCAGTCATGAAAGAGATCAAACACCCTAACCTGGTGCAGCTCCTTGGGGTCTGCACCCGGGAGCCCCCGTTCTATATCATCACTGAGTTCATGACCTACGGGAACCTCCTGGACTACCTGAGGGAGTGCAACCGGCAGGAGGTGAACGCCGTGGTGCTGCTGTACATGGCCACTCAGATCTCGTCAGCCATGGAGTACCTGGAGAAGAAAAACTTCATCCACAGAGATCTTGCTGCCCGAAACTGCCTGGTAGGGGAGAACCACTTGGTGAAGGTAGCTGATTTTGGCCTGAGCAGGTTGATGACAGGGGACACCTACACAGCCCATGCTGGAGCCAAGTTCCCCATCAAATGGACTGCACCCGAGAGCCTGGCCTACAACAAGTTCTCCATCAAGTCCGACGTCTGGGCATTTGGAGTATTGCTTTGGGAAATTGCTACCTATGGCATGTCCCCTTACCCGGGAATTGACCTGTCCCAGGTGTATGAGCTGCTAGAGAAGGACTACCGCATGGAGCGCCCAGAAGGCTGCCCAGAGAAGGTCTATGAACTCATGCGAGCATGTTGGCAGTGGAATCCCTCTGACCGGCCCTCCTTTGCTGAAATCCACCAAGCCTTTGAAACAATGTTCCAGGAATCCAGTATCTCAGACGAAGTGGAAAAGGAGCTGGGGAAA</t>
+  </si>
+  <si>
+    <t>RDSSDDWEIPDGQITVGQRIGSGSFGTVYKGKWHGDVAVKMLNVTAPTPQQLQAFKNEVGVLRKTRHVNILLFMGYSTKPQLAIVTQWCEGSSLYHHLHIIETKFEMIKLIDIARQTAQGMDYLHAKSIIHRDLKSNNIFLHEDLTVKIGDFGLATVKSRWSGSHQFEQLSGSILWMAPEVIRMQDKNPYSFQSDVYAFGIVLYELMTGQLPYSNINNRDQIIFMVGRGYLSPDLSKVRSNCPKAMKRLMAECLKKKRDERPLFPQILA</t>
+  </si>
+  <si>
+    <t>KS6A1_HUMAN_D1_3RNY_B</t>
+  </si>
+  <si>
+    <t>ACCGACAGCTTCTCGGGCAGGTTTGAAGACGTCTACCAGCTGCAGGAAGATGTGCTGGGGGAGGGCGCTCATGCCCGAGTGCAGACCTGCATCAACCTGATCACCAGCCAGGAGTACGCCGTCAAGATCATTGAGAAGCAGCCAGGCCACATTCGGAGCAGGGTTTTCAGGGAGGTGGAGATGCTGTACCAGTGCCAGGGACACAGGAACGTCCTAGAGCTGATTGAGTTCTTCGAGGAGGAGGACCGCTTCTACCTGGTGTTTGAGAAGATGCGGGGAGGCTCCATCCTGAGCCACATCCACAAGCGCCGGCACTTCAACGAGCTGGAGGCCAGCGTGGTGGTGCAGGACGTGGCCAGCGCCTTGGACTTTCTGCATAACAAAGGCATCGCCCACAGGGACCTAAAGCCGGAAAACATCCTCTGTGAGCACCCCAACCAGGTCTCCCCCGTGAAGATCTGTGACTTCGACCTGGGCAGCGGCATCAAACTCAACGGGGACTGCTCCCCTATCTCCACCCCGGAGCTGCTCACTCCGTGCGGCTCGGCGGAGTACATGGCCCCGGAGGTAGTGGAGGCCTTCAGCGAGGAGGCTAGCATCTACGACAAGCGCTGCGACCTGTGGAGCCTGGGCGTCATCTTGTATATCCTACTCAGCGGCTACCCGCCCTTCGTGGGCCGCTGTGGCAGCGACTGCGGCTGGGACCGCGGCGAGGCCTGCCCTGCCTGCCAGAACATGCTGTTTGAGAGCATCCAGGAGGGCAAGTACGAGTTCCCCGACAAGGACTGGGCCCACATCTCCTGCGCTGCCAAAGACCTCATCTCCAAGCTGCTGGTCCGTGACGCCAAGCAGAGGCTGAGTGCCGCCCAAGTCCTGCAGCACCCCTGGGTTCAGGGGTGCGCCCCGGAGAACACCTTGCCCACTCCCATGGTCCTGCAGAGG</t>
+  </si>
+  <si>
+    <t>MSRSKRDNNFYSVEIGDSTFTVLKRYQNLKPIGSGAQGIVCAAYDAILERNVAIKKLSRPFQNQTHAKRAYRELVLMKCVNHKNIIGLLNVFTPQKSLEEFQDVYIVMELMDANLCQVIQMELDHERMSYLLYQMLCGIKHLHSAGIIHRDLKPSNIVVKSDCTLKILDFGLARTAGTSFMMTPYVVTRYYRAPEVILGMGYKENVDLWSVGCIMGEMVCHKILFPGRDYIDQWNKVIEQLGTPCPEFMKKLQPTVRTYVENRPKYAGYSFEKLFPDVLFPADSEHNKLKASQARDLLSKMLVIDASKRISVDEALQHPYINVWYDPSEAEAPPPKIPDKQLDEREHTIEEWKELIYKEVMDLE</t>
+  </si>
+  <si>
+    <t>STRAA_HUMAN_D0_3GNI_B</t>
+  </si>
+  <si>
+    <t>MP2K2_HUMAN_D0_1S9I_A</t>
+  </si>
+  <si>
+    <t>PIM1_HUMAN_D0_4A7C_A</t>
+  </si>
+  <si>
+    <t>EAFLTQKAKVGELKDDDFERISELGAGNGGVVTKVQHRPSGLIMARKLIHLEIKPAIRNQIIRELQVLHECNSPYIVGFYGAFYSDGEISICMEHMDGGSLDQVLKEAKRIPEEILGKVSIAVLRGLAYLREKHQIMHRDVKPSNILVNSRGEIKLCDFGVSGQLIDSMANSFVGTRSYMAPERLQGTHYSVQSDIWSMGLSLVELAVGRYPIPPPDAKELEAIFGRPVVDGEEGEPHSISPRPRPPGRPVSGHGMDSRPAMAIFELLDYIVNEPPPKLPNGVFTPDFQEFVNKCLIKNPAERADLKMLTNHTFIKRSEVEEVDFAGWLCKTLRLNQPGTPTRTAV</t>
+  </si>
+  <si>
+    <t>GGGCCGGAGGATGAGCTGCCCGACTGGGCCGCCGCCAAAGAGTTTTACCAGAAGTACGACCCTAAGGACGTCATCGGCAGAGGAGTGAGCTCTGTGGTCCGCCGTTGTGTTCATCGAGCTACTGGCCACGAGTTTGCGGTGAAGATTATGGAAGTGACAGCTGAGCGGCTGAGTCCTGAGCAGCTGGAGGAGGTGCGGGAAGCCACACGGCGAGAGACACACATCCTTCGCCAGGTCGCCGGCCACCCCCACATCATCACCCTCATCGATTCCTACGAGTCTTCTAGCTTCATGTTCCTGGTGTTTGACCTGATGCGGAAGGGAGAGCTGTTTGACTATCTCACAGAGAAGGTGGCCCTCTCTGAAAAGGAAACCAGGTCCATCATGCGGTCTCTGCTGGAAGCAGTGAGCTTTCTCCATGCCAACAACATTGTGCATCGAGATCTGAAGCCCGAGAATATTCTCCTAGATGACAATATGCAGATCCGACTTTCAGATTTCGGGTTCTCCTGCCACTTGGAACCTGGCGAGAAGCTTCGAGAGTTGTGTGGGACCCCAGGGTATCTAGCGCCAGAGATCCTTAAATGCTCCATGGATGAAACCCACCCAGGCTATGGCAAGGAGGTCGACCTCTGGGCCTGTGGGGTGATCTTGTTCACACTCCTGGCTGGCTCGCCACCCTTCTGGCACCGGCGGCAGATCCTGATGTTACGCATGATCATGGAGGGCCAGTACCAGTTCAGTTCCCCCGAGTGGGATGACCGTTCCAGCACTGTCAAAGACCTGATCTCCAGGCTGCTGCAGGTGGATCCTGAGGCACGCCTGACAGCTGAGCAGGCCCTACAGCACCCCTTCTTTGAGCGT</t>
+  </si>
+  <si>
+    <t>KC1E_HUMAN_D0_4HNI_A</t>
+  </si>
+  <si>
+    <t>VRK2_HUMAN_D0_2V62_B</t>
+  </si>
+  <si>
+    <t>ETYIKLDKLGEGTYATVYKGKSKLTDNLVALKEIRLEHEEGAPCTAIREVSLLKDLKHANIVTLHDIIHTEKSLTLVFEYLDKDLKQYLDDCGNIINMHNVKLFLFQLLRGLAYCHRQKVLHRDLKPQNLLINERGELKLADFGLARAKSIPTKTYSNEVVTLWYRPPDILLGSTDYSTQIDMWGVGCIFYEMATGRPLFPGSTVEEQLHFIFRILGTPTEETWPGILSNEEFKTYNYPKYRAEALLSHAPRLDSDGADLLTKLLQFEGRNRISAEDAMKHPFFLSLGERIHKLPDTTSIFALKEIQLQKEASLRS</t>
+  </si>
+  <si>
+    <t>HQLQPRRVSFRGEASETLQSPGYDPSRPESFFQQSFQRLSRLGHGSYGEVFKVRSKEDGRLYAVKRSMSPFRGPKDRARKLAEVGSHEKVGQHPCCVRLEQAWEEGGILYLQTELCGPSLQQHCEAWGASLPEAQVWGYLRDTLLALAHLHSQGLVHLDVKPANIFLGPRGRCKLGDFGLLVELGTAGAGEVQEGDPRYMAPELLQGSYGTAADVFSLGLTILEVACNMELPHGGEGWQQLRQGYLPPEFTAGLSSELRSVLVMMLEPDPKLRATAEALLALPVLRQP</t>
+  </si>
+  <si>
+    <t>aa_end</t>
+  </si>
+  <si>
+    <t>PMYT1_HUMAN_D0_3P1A_A</t>
+  </si>
+  <si>
+    <t>MK08_HUMAN_D0_2NO3_A</t>
+  </si>
+  <si>
+    <t>TCGGTTAAAGGAAGAATTTATTCCATATTAAAGCAGATAGGAAGTGGAGGTTCAAGCAAGGTATTTCAGGTGTTAAATGAAAAGAAACAGATATATGCTATAAAATATGTGAACTTAGAAGAAGCAGATAACCAAACTCTTGATAGTTACCGGAACGAAATAGCTTATTTGAATAAACTACAACAACACAGTGATAAGATCATCCGACTTTATGATTATGAAATCACGGACCAGTACATCTACATGGTAATGGAGTGTGGAAATATTGATCTTAATAGTTGGCTTAAAAAGAAAAAATCCATTGATCCATGGGAACGCAAGAGTTACTGGAAAAATATGTTAGAGGCAGTTCACACAATCCATCAACATGGCATTGTTCACAGTGATCTTAAACCAGCTAACTTTCTGATAGTTGATGGAATGCTAAAGCTAATTGATTTTGGGATTGCAAACCAAATGCAACCAGATACAACAAGTGTTGTTAAAGATTCTCAGGTTGGCACAGTTAATTATATGCCACCAGAAGCAATCAAAGATATGTCTTCCTCCAGAGAGAATGGGAAATCTAAGTCAAAGATAAGCCCCAAAAGTGATGTTTGGTCCTTAGGATGTATTTTGTACTATATGACTTACGGGAAAACACCATTTCAGCAGATAATTAATCAGATTTCTAAATTACATGCCATAATTGATCCTAATCATGAAATTGAATTTCCCGATATTCCAGAGAAAGATCTTCAAGATGTGTTAAAGTGTTGTTTAAAAAGGGACCCAAAACAGAGGATATCCATTCCTGAGCTCCTGGCTCATCCATATGTTCAAATTCAAACTCATCCAGTTAACCAAATGGCCAAGGGAACCACTGAAGAA</t>
+  </si>
+  <si>
+    <t>PAK1_HUMAN_D0_3Q52_A</t>
+  </si>
+  <si>
+    <t>CDK9_HUMAN_D0_4IMY_A</t>
+  </si>
+  <si>
+    <t>GAAACAAAGTATACTGTGGACAAGAGGTTTGGCATGGATTTTAAAGAAATAGAATTAATTGGCTCAGGTGGATTTGGCCAAGTTTTCAAAGCAAAACACAGAATTGACGGAAAGACTTACGTTATTAAACGTGTTAAATATAATAACGAGAAGGCGGAGCGTGAAGTAAAAGCATTGGCAAAACTTGATCATGTAAATATTGTTCACTACAATGGCTGTTGGGATGGATTTGATTATGATCCTGAGACCAGTGATGATTCTCTTGAGAGCAGTGATTATGATCCTGAGAACAGCAAAAATAGTTCAAGGTCAAAGACTAAGTGCCTTTTCATCCAAATGGAATTCTGTGATAAAGGGACCTTGGAACAATGGATTGAAAAAAGAAGAGGCGAGAAACTAGACAAAGTTTTGGCTTTGGAACTCTTTGAACAAATAACAAAAGGGGTGGATTATATACATTCAAAAAAATTAATTCATAGAGATCTTAAGCCAAGTAATATATTCTTAGTAGATACAAAACAAGTAAAGATTGGAGACTTTGGACTTGTAACATCTCTGAAAAATGATGGAAAGCGAACAAGGAGTAAGGGAACTTTGCGATACATGAGCCCAGAACAGATTTCTTCGCAAGACTATGGAAAGGAAGTGGACCTCTACGCTTTGGGGCTAATTCTTGCTGAACTTCTTCATGTATGTGACACTGCTTTTGAAACATCAAAGTTTTTCACAGACCTACGGGATGGCATCATCTCAGATATATTTGATAAAAAAGAAAAAACTCTTCTACAGAAATTACTCTCAAAGAAACCTGAGGATCGACCTAACACATCTGAAATACTAAGGACCTTGACTGTGTGGAAGAAAAGCCCAGAGAAAAATGAACGACACACATGT</t>
+  </si>
+  <si>
+    <t>PAK7_HUMAN_D0_2F57_B</t>
+  </si>
+  <si>
+    <t>expression tag location</t>
+  </si>
+  <si>
+    <t>GAGAACTTCCAAAAGGTGGAAAAGATCGGAGAGGGCACGTACGGAGTTGTGTACAAAGCCAGAAACAAGTTGACGGGAGAGGTGGTGGCGCTTAAGAAAATCCGCCTGGACACTGAGACTGAGGGTGTGCCCAGTACTGCCATCCGAGAGATCTCTCTGCTTAAGGAGCTTAACCATCCTAATATTGTCAAGCTGCTGGATGTCATTCACACAGAAAATAAACTCTACCTGGTTTTTGAATTTCTGCACCAAGATCTCAAGAAATTCATGGATGCCTCTGCTCTCACTGGCATTCCTCTTCCCCTCATCAAGAGCTATCTGTTCCAGCTGCTCCAGGGCCTAGCTTTCTGCCATTCTCATCGGGTCCTCCACCGAGACCTTAAACCTCAGAATCTGCTTATTAACACAGAGGGGGCCATCAAGCTAGCAGACTTTGGACTAGCCAGAGCTTTTGGAGTCCCTGTTCGTACTTACACCCATGAGGTGGTGACCCTGTGGTACCGAGCTCCTGAAATCCTCCTGGGCTGCAAATATTATTCCACAGCTGTGGACATCTGGAGCCTGGGCTGCATCTTTGCTGAGATGGTGACTCGCCGGGCCCTATTCCCTGGAGATTCTGAGATTGACCAGCTCTTCCGGATCTTTCGGACTCTGGGGACCCCAGATGAGGTGGTGTGGCCAGGAGTTACTTCTATGCCTGATTACAAGCCAAGTTTCCCCAAGTGGGCCCGGCAAGATTTTAGTAAAGTTGTACCTCCCCTGGATGAAGATGGACGGAGCTTGTTATCGCAAATGCTGCACTACGACCCTAACAAGCGGATTTCGGCCAAGGCAGCCCTGGCTCACCCTTTCTTCCAGGATGTGACCAAGCCAGTACCCCATCTT</t>
+  </si>
+  <si>
+    <t>GGGGAATGCAGTCAGAAGGGTCCTGTCCCCTTTAGCCATTGCCTTCCCACAGAAAAACTGCAACGCTGTGAGAAGATTGGGGAAGGGGTGTTTGGCGAAGTGTTTCAAACAATTGCTGATCACACACCCGTAGCCATAAAAATCATTGCTATTGAAGGACCAGATTTAGTCAATGGATCCCATCAGAAAACCTTTGAGGAAATCCTGCCAGAGATCATCATCTCCAAAGAGTTGAGCCTCTTATCCGGTGAAGTGTGCAACCGCACAGAAGGCTTTATCGGGCTGAACTCAGTGCACTGTGTCCAGGGATCTTACCCTCCCTTGCTCCTCAAAGCCTGGGATCACTATAATTCAACCAAAGGCTCTGCAAATGACCGGCCTGATTTTTTTAAAGACGACCAGCTCTTCATTGTGCTGGAATTTGAGTTTGGAGGGATTGACTTAGAGCAAATGCGAACCAAGTTGTCTTCCTTGGCTACTGCAAAGAGCATTCTACACCAGCTCACAGCCTCCCTCGCAGTGGCAGAGGCATCACTGCGCTTTGAGCACCGAGACTTACACTGGGGGAACGTGCTCTTAAAGAAAACCAGCCTCAAAAAACTCCACTACACCCTCAATGGGAAGAGCAGCACTATCCCCAGCTGTGGGTTGCAAGTGAGCATCATTGACTACACCCTGTCGCGCTTGGAACGGGATGGGATTGTGGTTTTCTGTGACGTTTCCATGGATGAGGACCTGTTTACCGGTGACGGTGACTACCAGTTTGACATCTACAGGCTCATGAAGAAGGAGAATAACAACCGCTGGGGTGAATATCACCCTTATAGTAATGTGCTCTGGTTACATTACCTGACAGACAAGATGCTGAAACAAATGACCTTCAAGACTAAATGTAACACTCCTGCCATGAAGCAAATTAAGAGAAAAATCCAGGAGTTCCACAGGACAATGCTGAACTTCAGCTCTGCCACTGACTTGCTCTGCCAGCACAGACTGTTTAAG</t>
+  </si>
+  <si>
+    <t>TDSLPGKFEDMYKLTSELLGEGAYAKVQGAVSLQNGKEYAVKIIEKQAGHSRSRVFREVETLYQCQGNKNILELIEFFEDDTRFYLVFEKLQGGSILAHIQKQKHFNEREASRVVRDVAAALDFLHTKDKVSLCHLGGSARAPSGLTAAPTSLGSSDPPTSASQVAGTTGIDHRDLKPENILCESPEKVSPVKICDFDLGSGMKLNNSCTPITTPELTTPCGSAEYMAPEVGEVFTDQATFYDKRCDLWSLGVVLYIMLSGYPPFVGHCGADCGWDRGEVCRVCQNKLFESIQEGKYEFPDKDWAHISSEAKDLISKLLVRDAKQRLSAAQVLQHPWVQGQAPEKG</t>
+  </si>
+  <si>
+    <t>VRK3_HUMAN_D0_2JII_A</t>
+  </si>
+  <si>
+    <t>ATGAGCCTCATCCGGAAAAAGGGCTTCTACAAGCAGGACGTCAACAAGACCGCCTGGGAGCTGCCCAAGACCTACGTGTCCCCGACGCACGTCGGCAGCGGGGCCTATGGCTCCGTGTGCTCGGCCATCGACAAGCGGTCAGGGGAGAAGGTGGCCATCAAGAAGCTGAGCCGACCCTTTCAGTCCGAGATCTTCGCCAAGCGCGCCTACCGGGAGCTGCTGCTGCTGAAGCACATGCAGCATGAGAACGTCATTGGGCTCCTGGATGTCTTCACCCCAGCCTCCTCCCTGCGCAACTTCTATGACTTCTACCTGGTGATGCCCTTCATGCAGACGGATCTGCAGAAGATCATGGGGATGGAGTTCAGTGAGGAGAAGATCCAGTACCTGGTGTATCAGATGCTCAAAGGCCTTAAGTACATCCACTCTGCTGGGGTCGTGCACAGGGACCTGAAGCCAGGCAACCTGGCTGTGAATGAGGACTGTGAACTGAAGATTCTGGATTTTGGGCTGGCGCGACATGCAGACGCCGAGATGACTGGCTACGTGGTGACCCGCTGGTACCGAGCCCCCGAGGTGATCCTCAGCTGGATGCACTACAACCAGACAGTGGACATCTGGTCTGTGGTCTGTATCATGGCAGAGATGCTGACAGGGAAAACTCTGTTCAAGGGGAAAGATTACCTGGACCAGCTGACCCAGATCCTGAAAGTGACCGGGGTGCCTGGCACGGAGTTTGTGCAGAAGCTGAACGACAAAGCGGCCAAATCCTACATCCAGTCCCTGCCACAGACCCCCAGGAAGGATTTCACTCAGCTGTTCCCACGGGCCAGCCCCCAGGCTGCGGACCTGCTGGAGAAGATGCTGGAGCTAGACGTGGACAAGCGCCTGACGGCCGCGCAGGCCCTCACCCATCCCTTCTTTGAACCCTTCCGGGACCCTGAGGAAGAGACGGAGGCCCAGCAGCCGTTTGATGATTCCTTAGAACACGAGAAACTCACAGTGGATGAATGGAAGCAGCACATCTACAAGGAGATTGTGAACTTCAGCCCCATT</t>
+  </si>
+  <si>
+    <t>ACTGACTCCTTGCCAGGAAAGTTTGAAGATATGTACAAGCTGACCTCTGAATTGCTGGGAGAGGGAGCCTATGCCAAAGTTCAAGGTGCCGTGAGCCTACAGAATGGCAAAGAGTATGCCGTCAAAATCATCGAGAAACAAGCAGGGCACAGTCGGAGTAGGGTGTTTCGAGAGGTGGAGACGCTGTATCAGTGTCAGGGAAACAAGAACATTTTGGAGCTGATTGAGTTCTTTGAAGATGACACAAGGTTTTACTTGGTCTTTGAGAAATTGCAAGGAGGTTCCATCTTAGCCCACATCCAGAAGCAAAAGCACTTCAATGAGCGAGAAGCCAGCCGAGTGGTGCGGGACGTTGCTGCTGCCCTTGACTTCCTGCATACCAAAGACAAAGTCTCTCTCTGTCACCTAGGCGGGAGTGCTAGGGCGCCATCAGGGCTCACTGCAGCCCCAACCTCCCTGGGCTCCAGTGATCCTCCCACCTCAGCCTCCCAAGTAGCTGGGACTACAGGCATTGATCATCGTGATCTGAAACCAGAAAATATATTGTGTGAATCTCCAGAAAAGGTGTCTCCAGTGAAAATCTGTGACTTTGACTTGGGCAGTGGGATGAAACTGAACAACTCCTGTACCCCCATAACCACACCAGAGCTGACCACCCCATGTGGCTCTGCAGAATACATGGCCCCTGAGGTAGGGGAGGTCTTCACGGACCAGGCCACATTCTACGACAAGCGCTGTGACCTGTGGAGCCTGGGCGTGGTCCTCTACATCATGCTGAGTGGCTACCCACCCTTCGTGGGTCACTGCGGGGCCGACTGTGGCTGGGACCGGGGCGAGGTCTGCAGGGTGTGCCAGAACAAGCTGTTTGAAAGCATCCAGGAAGGCAAGTATGAGTTTCCTGACAAGGACTGGGCACACATCTCCAGTGAAGCCAAAGACCTCATCTCCAAGCTCCTGGTGCGAGATGCAAAGCAGAGACTTAGCGCCGCCCAAGTTCTGCAGCACCCATGGGTGCAGGGGCAAGCTCCAGAAAAGGGA</t>
+  </si>
+  <si>
+    <t>PAK4_HUMAN_D0_2J0I_A</t>
+  </si>
+  <si>
+    <t>AGVSEYELPEDPRWELPRDRLVLGKPLGEGCFGQVVLAEAIGLDKDKPNRVTKVAVKMLKSDATEKDLSDLISEMEMMKMIGKHKNIINLLGACTQDGPLYVIVEYASKGNLREYLQARRPPGLEYCYNPSHNPEEQLSSKDLVSCAYQVARGMEYLASKKCIHRDLAARNVLVTEDNVMKIADFGLARDIHHIDYYKKTTNGRLPVKWMAPEALFDRIYTHQSDVWSFGVLLWEIFTLGGSPYPGVPVEELFKLLKEGHRMDKPSNCTNELYMMMRDCWHAVPSQRPTFKQLVEDLDRIVALTSNQEYLDLSMPLD</t>
+  </si>
+  <si>
+    <t>MAAAAAQGGGGGEPRRTEGVGPGVPGEVEMVKGQPFDVGPRYTQLQYIGEGAYGMVSSAYDHVRKTRVAIKKISPFEHQTYCQRTLREIQILLRFRHENVIGIRDILRASTLEAMRDVYIVQDLMETDLYKLLKSQQLSNDHICYFLYQILRGLKYIHSANVLHRDLKPSNLLINTTCDLKICDFGLARIADPEHDHTGFLTEYVATRWYRAPEIMLNSKGYTKSIDIWSVGCILAEMLSNRPIFPGKHYLDQLNHILGILGSPSQEDLNCIINMKARNYLQSLPSKTKVAWAKLFPKSDSKALDLLDRMLTFNPNKRITVEEALAHPYLEQYYDPTDEPVAEEPFTFAMELDDLPKERLKELIFQETARFQPGVLEAP</t>
+  </si>
+  <si>
+    <t>GAGCCCAAGAAGTACGCAGTGACCGACGACTACCAGTTGTCCAAGCAGGTGCTGGGCCTGGGTGTGAACGGCAAAGTGCTGGAGTGCTTCCATCGGCGCACTGGACAGAAGTGTGCCCTGAAGCTCCTGTATGACAGCCCCAAGGCCCGGCAGGAGGTAGACCATCACTGGCAGGCTTCTGGCGGCCCCCATATTGTCTGCATCCTGGATGTGTATGAGAACATGCACCATGGCAAGCGCTGTCTCCTCATCATCATGGAATGCATGGAAGGTGGTGAGTTGTTCAGCAGGATTCAGGAGCGTGGCGACCAGGCTTTCACTGAGAGAGAAGCTGCAGAGATAATGCGGGATATTGGCACTGCCATCCAGTTTCTGCACAGCCATAACATTGCCCACCGAGATGTCAAGCCTGAAAACCTACTCTACACATCTAAGGAGAAAGACGCAGTGCTTAAGCTCACCGATTTTGGCTTTGCTAAGGAGACCACCCAAAATGCCCTGCAGACACCCTGCTATACTCCCTATTATGTGGCCCCTGAGGTCCTGGGTCCAGAGAAGTATGACAAGTCATGTGACATGTGGTCCCTGGGTGTCATCATGTACATCCTCCTTTGTGGCTTCCCACCCTTCTACTCCAACACGGGCCAGGCCATCTCCCCGGGGATGAAGAGGAGGATTCGCCTGGGCCAGTACGGCTTCCCCAATCCTGAGTGGTCAGAAGTCTCTGAGGATGCCAAGCAGCTGATCCGCCTCCTGTTGAAGACAGACCCCACAGAGAGGCTGACCATCACTCAGTTCATGAACCACCCCTGGATCAACCAATCGATGGTAGTGCCACAGACCCCACTCCACACGGCCCGAGTGCTGCAGGAGGACAAAGACCACTGGGACGAAGTCAAGGAGGAGATGACCAGTGCCTTGGCCACTATGCGGGTAGACTACGACCAGGTG</t>
+  </si>
+  <si>
+    <t>ATGTCTCAGGAGAGGCCCACGTTCTACCGGCAGGAGCTGAACAAGACAATCTGGGAGGTGCCCGAGCGTTACCAGAACCTGTCTCCAGTGGGCTCTGGCGCCTATGGCTCTGTGTGTGCTGCTTTTGACACAAAAACGGGGTTACGTGTGGCAGTGAAGAAGCTCTCCAGACCATTTCAGTCCATCATTCATGCGAAAAGAACCTACAGAGAACTGCGGTTACTTAAACATATGAAACATGAAAATGTGATTGGTCTGTTGGACGTTTTTACACCTGCAAGGTCTCTGGAGGAATTCAATGATGTGTATCTGGTGACCCATCTCATGGGGGCAGATCTGAACAACATTGTGAAATGTCAGAAGCTTACAGATGACCATGTTCAGTTCCTTATCTACCAAATTCTCCGAGGTCTAAAGTATATACATTCAGCTGACATAATTCACAGGGACCTAAAACCTAGTAATCTAGCTGTGAATGAAGACTGTGAGCTGAAGATTCTGGATTTTGGACTGGCTCGGCACACAGATGATGAAATGACAGGCTACGTGGCCACTAGGTGGTACAGGGCTCCTGAGATCATGCTGAACTGGATGCATTACAACCAGACAGTTGATATTTGGTCAGTGGGATGCATAATGGCCGAGCTGTTGACTGGAAGAACATTGTTTCCTGGTACAGACCATATTGATCAGTTGAAGCTCATTTTAAGACTCGTTGGAACCCCAGGGGCTGAGCTTTTGAAGAAAATCTCCTCAGAGTCTGCAAGAAACTATATTCAGTCTTTGACTCAGATGCCGAAGATGAACTTTGCGAATGTATTTATTGGTGCCAATCCCCTGGCTGTCGACTTGCTGGAGAAGATGCTTGTATTGGACTCAGATAAGAGAATTACAGCGGCCCAAGCCCTTGCACATGCCTACTTTGCTCAGTACCACGATCCTGATGATGAACCAGTGGCCGATCCTTATGATCAGTCCTTTGAAAGCAGGGACCTCCTTATAGATGAGTGGAAAAGCCTGACCTATGATGAAGTCATCAGCTTTGTGCCACCACCCCTTGACCAAGAAGAGATGGAGTCC</t>
+  </si>
+  <si>
+    <t>MK11_HUMAN_D0_3GC8_A</t>
+  </si>
+  <si>
+    <t>MK14_HUMAN_D0_3K3J_A</t>
+  </si>
+  <si>
+    <t>CDK16_HUMAN_D0_3MTL_A</t>
+  </si>
+  <si>
+    <t>PLK1_HUMAN_D0_2V5Q_A</t>
+  </si>
+  <si>
+    <t>BRAF_HUMAN_D0_4JVG_D</t>
+  </si>
+  <si>
+    <t>NEK7_HUMAN_D0_2WQN_A</t>
+  </si>
+  <si>
+    <t>PAK6_HUMAN_D0_2C30_A</t>
+  </si>
+  <si>
+    <t>FGFR1_HUMAN_D0_3GQL_B</t>
+  </si>
+  <si>
+    <t>TCTTCGGTCACCGCCAGTGCGGCCCCGGGGACCGCGAGCCTCGTCCCGGATTACTGGATCGACGGCTCCAACAGGGATGCGCTGAGCGATTTCTTCGAGGTGGAGTCGGAGCTGGGACGGGGTGCTACATCCATTGTGTACAGATGCAAACAGAAGGGGACCCAGAAGCCTTATGCTCTCAAAGTGTTAAAGAAAACAGTGGACAAAAAAATCGTAAGAACTGAGATAGGAGTTCTTCTTCGCCTCTCACATCCAAACATTATAAAACTTAAAGAGATATTTGAAACCCCTACAGAAATCAGTCTGGTCCTAGAACTCGTCACAGGAGGAGAACTGTTTGATAGGATTGTGGAAAAGGGATATTACAGTGAGCGAGATGCTGCAGATGCCGTTAAACAAATCCTGGAGGCAGTTGCTTATCTACATGAAAATGGGATTGTCCATCGTGATCTCAAACCAGAGAATCTTCTTTATGCAACTCCAGCCCCAGATGCACCACTCAAAATCGCTGATTTTGGACTCTCTAAAATTGTGGAACATCAAGTGCTCATGAAGACAGTATGTGGAACCCCAGGGTACTGCGCACCTGAAATTCTTAGAGGTTGTGCCTATGGACCTGAGGTGGACATGTGGTCTGTAGGAATAATCACCTACATCTTACTTTGTGGATTTGAACCATTCTATGATGAAAGAGGCGATCAGTTCATGTTCAGGAGAATTCTGAATTGTGAATATTACTTTATCTCCCCCTGGTGGGATGAAGTATCTCTAAATGCCAAGGACTTGGTCAGAAAATTAATTGTTTTGGATCCAAAGAAACGGCTGACTACATTTCAAGCTCTCCAGCATCCGTGGGTCACAGGTAAAGCAGCCAATTTTGTACACATGGATACCGCTCAAAAGAAGCTCCAAGAATTCAATGCCCGGCGTAAGCTTAAGGCAGCGGTGAAGGCTGTGGTGGCCTCTTCCCGCCTGGGA</t>
+  </si>
+  <si>
+    <t>MEAAASEPSLDLDNLKLLELIGRGRYGAVYKGSLDERPVAVKVFSFANRQNFINEKNIYRVPLMEHDNIARFIVGDERVTADGRMEYLLVMEYYPNGSLCKYLSLHTSDWVSSCRLAHSVTRGLAYLHTELPRGDHYKPAISHRDLNSRNVLVKNDGTCVISDFGLSMRLTGNRLVRPGEEDNAAISEVGTIRYMAPEVLEGAVNLRDCESALKQVDMYALGLIYWEIFMRCTDLFPGESVPEYQMAFQTEVGNHPTFEDMQVLVSREKQRPKFPEAWKENSLAVRSLKETIEDCWDQDAEARLTAQCAEERMAELMMIWERNKSVSPT</t>
+  </si>
+  <si>
+    <t>GTCATCATTGACAATAAGCGCTACCTCTTCATCCAGAAACTGGGGGAGGGTGGGTTCAGCTATGTGGACCTAGTGGAAGGGTTACATGATGGACACTTCTACGCCCTGAAGCGAATCCTGTGTCACGAGCAGCAGGACCGGGAGGAGGCCCAGCGAGAAGCCGACATGCATCGCCTCTTCAATCACCCCAACATCCTTCGCCTCGTGGCTTACTGTCTGAGGGAACGGGGTGCTAAGCATGAGGCCTGGCTGCTGCTACCATTCTTCAAGAGAGGTACGCTGTGGAATGAGATAGAAAGGCTGAAGGACAAAGGCAACTTCCTGACCGAGGATCAAATCCTTTGGCTGCTGCTGGGGATCTGCAGAGGCCTTGAGGCCATTCATGCCAAGGGTTATGCCCACAGAGACTTGAAGCCCACCAATATATTGCTTGGAGATGAGGGGCAGCCAGTTTTAATGGACTTGGGTTCCATGAATCAAGCATGCATCCATGTGGAGGGCTCCCGCCAGGCTCTGACCCTGCAGGACTGGGCAGCCCAGCGGTGCACCATCTCCTACCGAGCCCCAGAGCTCTTCTCTGTGCAGAGTCACTGTGTCATCGATGAGCGGACTGATGTCTGGTCCCTAGGCTGCGTGCTATATGCCATGATGTTTGGGGAAGGCCCTTATGACATGGTGTTCCAAAAGGGTGACAGTGTGGCCCTTGCTGTGCAGAACCAACTCAGCATCCCACAAAGCCCCAGGCATTCTTCAGCATTGTGGCAGCTCCTGAACTCGATGATGACCGTGGACCCGCATCAGCGTCCTCACATTCCTCTCCTCCTCAGTCAGCTGGAGGCGCTGCAG</t>
+  </si>
+  <si>
+    <t>BMPR2_HUMAN_D0_3G2F_A</t>
+  </si>
+  <si>
+    <t>dna_start</t>
+  </si>
+  <si>
+    <t>PHKG2_HUMAN_D0_2Y7J_D</t>
+  </si>
+  <si>
+    <t>MAPK2_HUMAN_D0_2JBO_A</t>
+  </si>
+  <si>
+    <t>HHHHHHSHSGPEISRIIVDPTTGKRYCRGKVLGKGGFAKCYEMTDLTNNKVYAAKIIPHSRVAKPHQREKIDKEIELHRILHHKHVVQFYHYFEDKENIYILLEYCSRRSMAHILKARKVLTEPEVRYYLRQIVSGLKYLHEQEILHRDLKLGNFFINEAMELKVGDFGLAARLEPLEHRRRTICGTPNYLSPEVLNKQGHGCESDIWALGCVMYTMLLGRPPFETTNLKETYRCIREARYTMPSSLLAPAKHLIASMLSKNPEDRPSLDDIIRHDFFLQGFTPDRLSSSCCHTVPDFHLSSPA</t>
+  </si>
+  <si>
+    <t>ATGGAGAAGGACGGCCTGTGCCGCGCTGACCAGCAGTACGAATGCGTGGCGGAGATCGGGGAGGGCGCCTATGGGAAGGTGTTCAAGGCCCGCGACTTGAAGAACGGAGGCCGTTTCGTGGCGTTGAAGCGCGTGCGGGTGCAGACCGGCGAGGAGGGCATGCCGCTCTCCACCATCCGCGAGGTGGCGGTGCTGAGGCACCTGGAGACCTTCGAGCACCCCAACGTGGTCAGGTTGTTTGATGTGTGCACAGTGTCACGAACAGACAGAGAAACCAAACTAACTTTAGTGTTTGAACATGTCGATCAAGACTTGACCACTTACTTGGATAAAGTTCCAGAGCCTGGAGTGCCCACTGAAACCATAAAGGATATGATGTTTCAGCTTCTCCGAGGTCTGGACTTTCTTCATTCACACCGAGTAGTGCATCGCGATCTAAAACCACAGAACATTCTGGTGACCAGCAGCGGACAAATAAAACTCGCTGACTTCGGCCTTGCCCGCATCTATAGTTTCCAGATGGCTCTAACCTCAGTGGTCGTCACGCTGTGGTACAGAGCACCCGAAGTCTTGCTCCAGTCCAGCTACGCCACCCCCGTGGATCTCTGGAGTGTTGGCTGCATATTTGCAGAAATGTTTCGTAGAAAGCCTCTTTTTCGTGGAAGTTCAGATGTTGATCAACTAGGAAAAATCTTGGACGTGATTGGACTCCCAGGAGAAGAAGACTGGCCTAGAGATGTTGCCCTTCCCAGGCAGGCTTTTCATTCAAAATCTGCCCAACCAATTGAGAAGTTTGTAACAGATATCGATGAACTAGGCAAAGACCTACTTCTGAAGTGTTTGACATTTAACCCAGCCAAAAGAATATCTGCCTACAGTGCCCTGTCTCACCCATACTTCCAG</t>
+  </si>
+  <si>
+    <t>ATGTCGGGCCCTCGCGCCGGCTTCTACCGGCAGGAGCTGAACAAGACCGTGTGGGAGGTGCCGCAGCGGCTGCAGGGGCTGCGCCCGGTGGGCTCCGGCGCCTACGGCTCCGTCTGTTCGGCCTACGACGCCCGGCTGCGCCAGAAGGTGGCGGTGAAGAAGCTGTCGCGCCCCTTCCAGTCGCTGATCCACGCGCGCAGAACGTACCGGGAGCTGCGGCTGCTCAAGCACCTGAAGCACGAGAACGTCATCGGGCTTCTGGACGTCTTCACGCCGGCCACGTCCATCGAGGACTTCAGCGAAGTGTACTTGGTGACCACCCTGATGGGCGCCGACCTGAACAACATCGTCAAGTGCCAGGCGCTGAGCGACGAGCACGTTCAATTCCTGGTTTACCAGCTGCTGCGCGGGCTGAAGTACATCCACTCGGCCGGGATCATCCACCGGGACCTGAAGCCCAGCAACGTGGCTGTGAACGAGGACTGTGAGCTCAGGATCCTGGATTTCGGGCTGGCGCGCCAGGCGGACGAGGAGATGACCGGCTATGTGGCCACGCGCTGGTACCGGGCACCTGAGATCATGCTCAACTGGATGCATTACAACCAAACAGTGGATATCTGGTCCGTGGGCTGCATCATGGCTGAGCTGCTCCAGGGCAAGGCCCTCTTCCCGGGAAGCGACTACATTGACCAGCTGAAGCGCATCATGGAAGTGGTGGGCACACCCAGCCCTGAGGTTCTGGCAAAAATCTCCTCGGAACACGCCCGGACATATATCCAGTCCCTGCCCCCCATGCCCCAGAAGGACCTGAGCAGCATCTTCCGTGGAGCCAACCCCCTGGCCATAGACCTCCTTGGAAGGATGCTGGTGCTGGACAGTGACCAGAGGGTCAGTGCAGCTGAGGCACTGGCCCACGCCTACTTCAGCCAGTACCACGACCCCGAGGATGAGCCAGAGGCCGAGCCATATGATGAGAGCGTTGAGGCCAAGGAGCGCACGCTGGAGGAGTGGAAGGAGCTCACTTACCAGGAAGTCCTCAGCTTCAAGCCCCCAGAGCCACCGAAGCCACCTGGCAGCCTGGAGATTGAGCAG</t>
+  </si>
+  <si>
+    <t>VRK1_HUMAN_D0_3OP5_D</t>
+  </si>
+  <si>
+    <t>MEKYEKIGKIGEGSYGVVFKCRNRDTGQIVAIKKFLESEDDPVIKKIALREIRMLKQLKHPNLVNLLEVFRRKRRLHLVFEYCDHTVLHELDRYQRGVPEHLVKSITWQTLQAVNFCHKHNCIHRDVKPENILITKHSVIKLCDFGFARLLTGPSDYYTDYVATRWYRSPELLVGDTQYGPPVDVWAIGCVFAELLSGVPLWPGKSDVDQLYLIRKTLGDLIPRHQQVFSTNQYFSGVKIPDPEDMEPLELKFPNISYPALGLL</t>
+  </si>
+  <si>
+    <t>GeneID</t>
+  </si>
+  <si>
+    <t>ATGGATGAGCAATCACAAGGAATGCAAGGGCCACCTGTTCCTCAGTTCCAACCACAGAAGGCCTTACGACCGGATATGGGCTATAATACATTAGCCAACTTTCGAATAGAAAAGAAAATTGGTCGCGGACAATTTAGTGAAGTTTATAGAGCAGCCTGTCTCTTGGATGGAGTACCAGTAGCTTTAAAAAAAGTGCAGATATTTGATTTAATGGATGCCAAAGCACGTGCTGATTGCATCAAAGAAATAGATCTTCTTAAGCAACTCAACCATCCAAATGTAATAAAATATTATGCATCATTCATTGAAGATAATGAACTAAACATAGTTTTGGAACTAGCAGATGCTGGCGACCTATCCAGAATGATCAAGCATTTTAAGAAGCAAAAGAGGCTAATTCCTGAAAGAACTGTTTGGAAGTATTTTGTTCAGCTTTGCAGTGCATTGGAACACATGCATTCTCGAAGAGTCATGCATAGAGATATAAAACCAGCTAATGTGTTCATTACAGCCACTGGGGTGGTAAAACTTGGAGATCTTGGGCTTGGCCGGTTTTTCAGCTCAAAAACCACAGCTGCACATTCTTTAGTTGGTACGCCTTATTACATGTCTCCAGAGAGAATACATGAAAATGGATACAACTTCAAATCTGACATCTGGTCTCTTGGCTGTCTACTATATGAGATGGCTGCATTACAAAGTCCTTTCTATGGTGACAAAATGAATTTATACTCACTGTGTAAGAAGATAGAACAGTGTGACTACCCACCTCTTCCTTCAGATCACTATTCAGAAGAACTCCGACAGTTAGTTAATATGTGCATCAACCCAGATCCAGAGAAGCGACCAGACGTCACCTATGTTTATGACGTAGCAAAGAGGATGCATGCATGCACTGCAAGCAGC</t>
+  </si>
+  <si>
+    <t>DAPK3_HUMAN_D0_2J90_A</t>
+  </si>
+  <si>
+    <t>VKEFLAKAKEDFLKKWESPAQNTAHLDQFERIKTLGTGSFGRVMLVKHKETGNHYAMKILDKQKVVKLKQIEHTLNEKRILQAVNFPFLVKLEFSFKDNSNLYMVMEYVPGGEMFSHLRRIGRFSEPHARFYAAQIVLTFEYLHSLDLIYRDLKPENLLIDQQGYIQVTDFGFAKRVKGRTWTLCGTPEYLAPEIILSKGYNKAVDWWALGVLIYEMAAGYPPFFADQPIQIYEKIVSGKVRFPSHFSSDLKDLLRNLLQVDLTKRFGNLKNGVNDIKNHKWFATTDWIAIYQRKVEAPFIPKFKGPGDTSNFDDYEEEEIRVSINEKCGKEFSEF</t>
+  </si>
+  <si>
+    <t>TCCAGGGTGTCCCATGAACAGTTTCGGGCGGCCCTGCAGCTGGTGGTCAGCCCAGGAGACCCCAGGGAATACTTGGCCAACTTTATCAAAATCGGGGAAGGCTCAACCGGCATCGTATGCATCGCCACCGAGAAACACACAGGGAAACAAGTTGCAGTGAAGAAAATGGACCTCCGGAAGCAACAGAGACGAGAACTGCTTTTCAATGAGGTCGTGATCATGCGGGATTACCACCATGACAATGTGGTTGACATGTACAGCAGCTACCTTGTCGGCGATGAGCTCTGGGTGGTCATGGAGTTTCTAGAAGGTGGTGCCTTGACAGACATTGTGACTCACACCAGAATGAATGAAGAACAGATAGCTACTGTCTGCCTGTCAGTTCTGAGAGCTCTCTCCTACCTTCATAACCAAGGAGTGATTCACAGGGACATAAAAAGTGACTCCATCCTCCTGACAAGCGATGGCCGGATAAAGTTGTCTGATTTTGGTTTCTGTGCTCAAGTTTCCAAAGAGGTGCCGAAGAGGAAATCATTGGTTGGCACTCCCTACTGGATGGCCCCTGAGGTGATTTCTAGGCTACCTTATGGGACAGAGGTGGACATCTGGTCCCTCGGGATCATGGTGATAGAAATGATTGATGGCGAGCCCCCCTACTTCAATGAGCCTCCCCTCCAGGCGATGCGGAGGATCCGGGACAGTTTACCTCCAAGAGTGAAGGACCTACACAAGGTTTCTTCAGTGCTCCGGGGATTCCTAGACTTGATGTTGGTGAGGGAGCCCTCTCAGAGAGCAACAGCCCAGGAACTCCTCGGACATCCATTCTTAAAACTAGCAGGTCCACCGTCTTGCATTGTCCCCCTCATGAGACAATACAGGCATCAC</t>
+  </si>
+  <si>
+    <t>KRQWALEDFEIGRPLGKGKFGNVYLAREKQSKFILALKVLFKAQLEKAGVEHQLRREVEIQSHLRHPNILRLYGYFHDATRVYLILEYAPLGTVYRELQKLSKFDEQRTATYITELANALSYCHSKRVIHRDIKPENLLLGSAGELKIADFGWSVHAPSSRRTTLCGTLDYLPPEMIEGRMHDEKVDLWSLGVLCYEFLVGKPPFEANTYQETYKRISRVEFTFPDFVTEGARDLISRLLKHNPSQRPMLREVLEHPWITANSSKPS</t>
+  </si>
+  <si>
+    <t>EGFR_HUMAN_D0_2RF9_A</t>
+  </si>
+  <si>
+    <t>SLK_HUMAN_D0_2JFL_A</t>
+  </si>
+  <si>
+    <t>SRVSHEQFRAALQLVVSPGDPREYLANFIKIGEGSTGIVCIATEKHTGKQVAVKKMDLRKQQRRELLFNEVVIMRDYHHDNVVDMYSSYLVGDELWVVMEFLEGGALTDIVTHTRMNEEQIATVCLSVLRALSYLHNQGVIHRDIKSDSILLTSDGRIKLSDFGFCAQVSKEVPKRKSLVGTPYWMAPEVISRLPYGTEVDIWSLGIMVIEMIDGEPPYFNEPPLQAMRRIRDSLPPRVKDLHKVSSVLRGFLDLMLVREPSQRATAQELLGHPFLKLAGPPSCIVPLMRQYRHH</t>
+  </si>
+  <si>
+    <t>TQTVHEFAKELDATNISIDKVVGAGEFGEVCSGRLKLPSKKEISVAIKTLKVGYTEKQRRDFLGEASIMGQFDHPNIIRLEGVVTKSKPVMIVTEYMENGSLDSFLRKHDAQFTVIQLVGMLRGIASGMKYLSDMGYVHRDLAARNILINSNLVCKVSDFGLSRVLEDDPEAAYTTRGGKIPIRWTSPEAIAYRKFTSASDVWSYGIVLWEVMSYGERPYWEMSNQDVIKAVDEGYRLPPPMDCPAALYQLMLDCWQKDRNNRPKFEQIVSILDKLIRNPGSLKIITSAAARPSNLLLDQSNVDITTFRTTGDWLNGVWTAHCKEIFTGVEYSSCDTIAKIS</t>
+  </si>
+  <si>
+    <t>QQFPQFHVKSGLQIKKNAIIDDYKVTSQVLGLGINGKVLQIFNKRTQEKFALKMLQDCPKARREVELHWRASQCPHIVRIVDVYENLYAGRKCLLIVMECLDGGELFSRIQDRGDQAFTEREASEIMKSIGEAIQYLHSINIAHRDVKPENLLYTSKRPNAILKLTDFGFAKETTSHNSLTTPCYTPYYVAPEVLGPEKYDKSCDMWSLGVIMYILLCGYPPFYSNHGLAISPGMKTRIRMGQYEFPNPEWSEVSEEVKMLIRNLLKTEPTQRMTITEFMNHPWIMQSTKVPQTPLHTSRVLKEDKERWEDVKGCLHDKNSDQA</t>
+  </si>
+  <si>
+    <t>CSK21_HUMAN_D0_3AXW_A</t>
+  </si>
+  <si>
+    <t>ATCTRFTDDYQLFEELGKGAFSVVRRCVKKTPTQEYAAKIINTKKLSARDHQKLEREARICRLLKHPNIVRLHDSISEEGFHYLVFDLVTGGELFEDIVAREYYSEADASHCIHQILESVNHIHQHDIVHRDLKPENLLLASKCKGAAVKLADFGLAIEVQGEQQAWFGFAGTPGYLSPEVLRKDPYGKPVDIWACGVILYILLVGYPPFWDEDQHKLYQQIKAGAYDFPSPEWDTVTPEAKNLINQMLTINPAKRITADQALKHPWVCQRSTVASMMHRQETVECLRKFNARRKLKGAILTTMLVSRNFS</t>
+  </si>
+  <si>
+    <t>VIDPSELTFVQEIGSGQFGLVHLGYWLNKDKVAIKTIREGAMSEEDFIEEAEVMMKLSHPKLVQLYGVCLEQAPICLVFEFMEHGCLSDYLRTQRGLFAAETLLGMCLDVCEGMAYLEEACVIHRDLAARNCLVGENQVIKVSDFGMTRFVLDDQYTSSTGTKFPVKWASPEVFSFSRYSSKSDVWSFGVLMWEVFSEGKIPYENRSNSEVVEDISTGFRLYKPRLASTHVYQIMNHCWKERPEDRPAFSRLLRQLAEIAESGL</t>
+  </si>
+  <si>
+    <t>CGTGTAAAAGCAGCTCAAGCTGGAAGACAGAGCTCTGCAAAGAGACATCTTGCAGAACAATTTGCAGTTGGAGAGATAATAACTGACATGGCAAAAAAGGAATGGAAAGTAGGATTACCCATTGGCCAAGGAGGCTTTGGCTGTATATATCTTGCTGATATGAATTCTTCAGAGTCAGTTGGCAGTGATGCACCTTGTGTTGTAAAAGTGGAACCCAGTGACAATGGACCTCTTTTTACTGAATTAAAGTTCTACCAACGAGCTGCAAAACCAGAGCAAATTCAGAAATGGATTCGTACCCGTAAGCTGAAGTACCTGGGTGTTCCTAAGTATTGGGGGTCTGGTCTACATGACAAAAATGGAAAAAGTTACAGGTTTATGATAATGGATCGCTTTGGGAGTGACCTTCAGAAAATATATGAAGCAAATGCCAAAAGGTTTTCTCGGAAAACTGTCTTGCAGCTAAGCTTAAGAATTCTGGATATTCTGGAATATATTCACGAGCATGAGTATGTGCATGGAGATATCAAGGCCTCAAATCTTCTTCTGAACTACAAGAATCCTGACCAGGTGTACTTGGTAGATTATGGCCTTGCTTATCGGTACTGCCCAGAAGGAGTTCATAAAGAATACAAAGAAGACCCCAAAAGATGTCACGATGGCACTATTGAATTCACGAGCATCGATGCACACAATGGCGTGGCCCCATCAAGACGTGGTGATTTGGAAATACTTGGTTATTGCATGATCCAATGGCTTACTGGCCATCTTCCTTGGGAGGATAATTTGAAAGATCCTAAATATGTTAGAGATTCCAAAATTAGATACAGAGAAAATATTGCAAGTTTGATGGACAAATGTTTTCCTGAGAAAAACAAACCAGGTGAAATTGCCAAATACATGGAAACAGTGAAATTACTAGACTACACTGAAAAACCTCTTTATGAAAATTTACGTGACATTCTTTTGCAAGGACTAAAAGCTATAGGAAGTAAGGATGATGGCAAATTGGACCTCAGTGTTGTGGAGAATGGAGGTTTGAAAGCAAAAACAATAACAAAGAAGCGAAAGAAAGAAATTGAAGAA</t>
+  </si>
+  <si>
+    <t>KS6A1_HUMAN_D0_3RNY_B</t>
+  </si>
+  <si>
+    <t>MP2K6_HUMAN_D0_3VN9_A</t>
+  </si>
+  <si>
+    <t>RVKAAQAGRQSSAKRHLAEQFAVGEIITDMAKKEWKVGLPIGQGGFGCIYLADMNSSESVGSDAPCVVKVEPSDNGPLFTELKFYQRAAKPEQIQKWIRTRKLKYLGVPKYWGSGLHDKNGKSYRFMIMDRFGSDLQKIYEANAKRFSRKTVLQLSLRILDILEYIHEHEYVHGDIKASNLLLNYKNPDQVYLVDYGLAYRYCPEGVHKEYKEDPKRCHDGTIEFTSIDAHNGVAPSRRGDLEILGYCMIQWLTGHLPWEDNLKDPKYVRDSKIRYRENIASLMDKCFPEKNKPGEIAKYMETVKLLDYTEKPLYENLRDILLQGLKAIGSKDDGKLDLSVVENGGLKAKTITKKRKKEIEE</t>
+  </si>
+  <si>
+    <t>MKNK1_HUMAN_D0_2HW6_B</t>
+  </si>
+  <si>
+    <t>MSLIRKKGFYKQDVNKTAWELPKTYVSPTHVGSGAYGSVCSAIDKRSGEKVAIKKLSRPFQSEIFAKRAYRELLLLKHMQHENVIGLLDVFTPASSLRNFYDFYLVMPFMQTDLQKIMGMEFSEEKIQYLVYQMLKGLKYIHSAGVVHRDLKPGNLAVNEDCELKILDFGLARHADAEMTGYVVTRWYRAPEVILSWMHYNQTVDIWSVVCIMAEMLTGKTLFKGKDYLDQLTQILKVTGVPGTEFVQKLNDKAAKSYIQSLPQTPRKDFTQLFPRASPQAADLLEKMLELDVDKRLTAAQALTHPFFEPFRDPEEETEAQQPFDDSLEHEKLTVDEWKQHIYKEIVNFSPI</t>
+  </si>
+  <si>
+    <t>AAPPAKEIPEVLVDPRSRRRYVRGRFLGKGGFAKCFEISDADTKEVFAGKIVPKSLLLKPHQREKMSMEISIHRSLAHQHVVGFHGFFEDNDFVFVVLELCRRRSLLELHKRRKALTEPEARYYLRQIVLGCQYLHRNRVIHRDLKLGNLFLNEDLEVKIGDFGLATKVEYDGERKKTLCGTPNYIAPEVLSKKGHSFEVDVWSIGCIMYTLLVGKPPFETSCLKETYLRIKKNEYSIPKHINPVAASLIQKMLQTDPTARPTINELLNDEFFTSGYIPARLPITCLTIPPRFSIAPSSLDPSNRKPLTVLNK</t>
+  </si>
+  <si>
+    <t>ITK_HUMAN_D0_3QGW_B</t>
+  </si>
+  <si>
+    <t>KS6A3_HUMAN_D1_4JG7_A</t>
+  </si>
+  <si>
+    <t>KCC4_HUMAN_D0_2W4O_A</t>
+  </si>
+  <si>
+    <t>CSK_HUMAN_D0_3D7T_A</t>
+  </si>
+  <si>
+    <t>KCC2A_HUMAN_D0_2VZ6_B</t>
+  </si>
+  <si>
+    <t>ATGTCTGATGAGGAGATCTTGGAGAAATTACGAAGCATAGTGAGTGTGGGCGATCCTAAGAAGAAATATACACGGTTTGAGAAGATTGGACAAGGTGCTTCAGGCACCGTGTACACAGCAATGGATGTGGCCACAGGACAGGAGGTGGCCATTAAGCAGATGAATCTTCAGCAGCAGCCCAAGAAAGAGCTGATTATTAATGAGATCCTGGTCATGAGGGAAAACAAGAACCCAAACATTGTGAATTACTTGGACAGTTACCTCGTGGGAGATGAGCTGTGGGTTGTTATGGAATACTTGGCTGGAGGCTCCTTGACAGATGTGGTGACAGAAACTTGCATGGATGAAGGCCAAATTGCAGCTGTGTGCCGTGAGTGTCTGCAGGCTCTGGAGTTCTTGCATTCGAACCAGGTCATTCACAGAGACATCAAGAGTGACAATATTCTGTTGGGAATGGATGGCTCTGTCAAGCTAACTGACTTTGGATTCTGTGCACAGATAACCCCAGAGCAGAGCAAACGGAGCACCATGGTAGGAACCCCATACTGGATGGCACCAGAGGTTGTGACACGAAAGGCCTATGGGCCCAAGGTTGACATCTGGTCCCTGGGCATCAAGGCCATCGAAATGATTGAAGGGGAGCCTCCATACCTCAATGAAAACCCTCTGAGAGCCTTGTACCTCATTGCCACCAATGGGACCCCAGAACTTCAGAACCCAGAGAAGCTGTCAGCTATCTTCCGGGACTTTCTGAACCGCTGTCTCGAGATGGATGTGGAGAAGAGAGGTTCAGCTAAAGAGCTGCTACAGCATCAATTCCTGAAGATTGCCAAGCCCCTCTCCAGCCTCACTCCACTTATTGCTGCAGCTAAGGAGGCAACAAAGAACAATCAC</t>
+  </si>
+  <si>
+    <t>ATGGAGGCAGCAGCATCCGAACCCTCTCTTGATCTAGATAATCTGAAACTGTTGGAGCTGATTGGCCGAGGTCGATATGGAGCAGTATATAAAGGCTCCTTGGATGAGCGTCCAGTTGCTGTAAAAGTGTTTTCCTTTGCAAACCGTCAGAATTTTATCAACGAAAAGAACATTTACAGAGTGCCTTTGATGGAACATGACAACATTGCCCGCTTTATAGTTGGAGATGAGAGAGTCACTGCAGATGGACGCATGGAATATTTGCTTGTGATGGAGTACTATCCCAATGGATCTTTATGCAAGTATTTAAGTCTCCACACAAGTGACTGGGTAAGCTCTTGCCGTCTTGCTCATTCTGTTACTAGAGGACTGGCTTATCTTCACACAGAATTACCACGAGGAGATCATTATAAACCTGCAATTTCCCATCGAGATTTAAACAGCAGAAATGTCCTAGTGAAAAATGATGGAACCTGTGTTATTAGTGACTTTGGACTGTCCATGAGGCTGACTGGAAATAGACTGGTGCGCCCAGGGGAGGAAGATAATGCAGCCATAAGCGAGGTTGGCACTATCAGATATATGGCACCAGAAGTGCTAGAAGGAGCTGTGAACTTGAGGGACTGTGAATCAGCTTTGAAACAAGTAGACATGTATGCTCTTGGACTAATCTATTGGGAGATATTTATGAGATGTACAGACCTCTTCCCAGGGGAATCCGTACCAGAGTACCAGATGGCTTTTCAGACAGAGGTTGGAAACCATCCCACTTTTGAGGATATGCAGGTTCTCGTGTCTAGGGAAAAACAGAGACCCAAGTTCCCAGAAGCCTGGAAAGAAAATAGCCTGGCAGTGAGGTCACTCAAGGAGACAATCGAAGACTGTTGGGACCAGGATGCAGAGGCTCGGCTTACTGCACAGTGTGCTGAGGAAAGGATGGCTGAACTTATGATGATTTGGGAAAGAAACAAATCTGTGAGCCCAACA</t>
+  </si>
+  <si>
+    <t>GGAGAAGCTCCCAACCAAGCTCTCTTGAGGATCTTGAAGGAAACTGAATTCAAAAAGATCAAAGTGCTGGGCTCCGGTGCGTTCGGCACGGTGTATAAGGGACTCTGGATCCCAGAAGGTGAGAAAGTTAAAATTCCCGTCGCTATCAAGGAATTAAGAGAAGCAACATCTCCGAAAGCCAACAAGGAAATCCTCGATGAAGCCTACGTGATGGCCAGCGTGGACAACCCCCACGTGTGCCGCCTGCTGGGCATCTGCCTCACCTCCACCGTGCAaCTCATCACGCAGCTCATGCCCTTCGGCTGCCTCCTGGACTATGTCCGGGAACACAAAGACAATATTGGCTCCCAGTACCTGCTCAACTGGTGTGTGCAGATCGCAAAGGGCATGAACTACTTGGAGGACCGTCGCTTGGTGCACCGCGACCTGGCAGCCAGGAACGTACTGGTGAAAACACCGCAGCATGTCAAGATCACAGATTTTGGGCgGGCCAAACTGCTGGGTGCGGAAGAGAAAGAATACCATGCAGAAGGAGGCAAAGTGCCTATCAAGTGGATGGCATTGGAATCAATTTTACACAGAATCTATACCCACCAGAGTGATGTCTGGAGCTACGGGGTGACCGTTTGGGAGTTGATGACCTTTGGATCCAAGCCATATGACGGAATCCCTGCCAGCGAGATCTCCTCCATCCTGGAGAAAGGAGAACGCCTCCCTCAGCCACCCATATGTACCATCGATGTCTACATGATCATGGTCAAGTGCTGGATGATAGACGCAGATAGTCGCCCAAAGTTCCGTGAGTTGATCATCGAATTCTCCAAAATGGCCCGAGACCCCCAGCGCTACCTTGTCATTCAGGGGGATGAAAGAATGCATTTGCCAAGTCCTACAGACTCCAACTTCTACCGTGCCCTGATGGATGAAGAAGACATGGACGACGTGGTGGATGCCGACGAGTACCTCATCCCACAGCAGGGC</t>
+  </si>
+  <si>
+    <t>GCCACCTGCACACGTTTCACCGACGACTACCAGCTCTTCGAGGAGCTTGGCAAGGGTGCTTTCTCTGTGGTCCGCAGGTGTGTGAAGAAAACCCCCACGCAGGAGTACGCAGCAAAAATCATCAATACCAAGAAATTGTCTGCCCGGGATCACCAGAAACTAGAACGTGAGGCTCGGATATGTCGACTTCTGAAACATCCAAACATCGTGCGCCTCCATGACAGTATTTCTGAAGAAGGGTTTCACTACCTCGTGTTTGACCTTGTTACCGGCGGGGAGCTGTTTGAAGACATTGTGGCCAGAGAGTACTACAGTGAAGCAGATGCCAGCCACTGTATACATCAGATTCTGGAGAGTGTTAACCACATCCACCAGCATGACATCGTCCACAGGGACCTGAAGCCTGAGAACCTGCTGCTGGCGAGTAAATGCAAGGGTGCCGCCGTCAAGCTGGCTGATTTTGGCCTAGCCATCGAAGTACAGGGAGAGCAGCAGGCTTGGTTTGGTTTTGCTGGCACCCCAGGTTACTTGTCCCCTGAGGTCTTGAGGAAAGATCCCTATGGAAAACCTGTGGATATCTGGGCCTGCGGGGTCATCCTGTATATCCTCCTGGTGGGCTATCCTCCCTTCTGGGATGAGGATCAGCACAAGCTGTATCAGCAGATCAAGGCTGGAGCCTATGATTTCCCATCACCAGAATGGGACACGGTAACTCCTGAAGCCAAGAACTTGATCAACCAGATGCTGACCATAAACCCAGCAAAGCGCATCACGGCTGACCAGGCTCTCAAGCACCCGTGGGTCTGTCAACGATCCACGGTGGCATCCATGATGCATCGTCAGGAGACTGTGGAGTGTTTGCGCAAGTTCAATGCCCGGAGAAAACTGAAGGGTGCCATCCTCACGACCATGCTTGTCTCCAGGAACTTCTCA</t>
+  </si>
+  <si>
+    <t>GAGACCTACATTAAGCTGGACAAACTGGGCGAGGGTACCTATGCCACCGTCTACAAAGGCAAAAGCAAGCTCACAGACAACCTTGTGGCACTCAAGGAGATCAGACTGGAACATGAAGAGGGGGCACCCTGCACCGCCATCCGGGAAGTGTCCCTACTCAAGGACCTCAAACACGCCAACATCGTTACGCTACATGACATTATCCACACGGAGAAGTCCCTCACCCTTGTCTTTGAGTACCTGGACAAGGACCTGAAGCAGTACCTGGATGACTGTGGGAACATCATCAACATGCACAACGTGAAACTGTTCCTGTTCCAGCTGCTCCGTGGCCTGGCCTACTGCCACCGGCAGAAGGTGCTACACCGAGACCTCAAGCCCCAGAACCTGCTCATCAACGAGAGGGGAGAGCTCAAGCTGGCTGACTTTGGCCTGGCCCGAGCCAAGTCAATCCCAACAAAGACATACTCCAATGAGGTGGTGACACTGTGGTACCGGCCCCCTGACATCCTGCTTGGGTCCACGGACTACTCCACTCAGATTGACATGTGGGGTGTGGGCTGCATCTTCTATGAGATGGCCACAGGCCGTCCCCTCTTTCCGGGCTCCACGGTGGAGGAACAGCTACACTTCATCTTCCGTATCTTAGGAACCCCAACTGAGGAGACGTGGCCAGGCATCCTGTCCAACGAGGAGTTCAAGACATACAACTACCCCAAGTACCGAGCCGAGGCCCTTTTGAGCCACGCACCCCGACTTGATAGCGACGGGGCCGACCTCCTCACCAAGCTGTTGCAGTTTGAGGGTCGAAATCGGATCTCCGCAGAGGATGCCATGAAACATCCATTCTTCCTCAGTCTGGGGGAGCGGATCCACAAACTTCCTGACACTACTTCCATATTTGCACTAAAGGAGATTCAGCTACAAAAGGAGGCCAGCCTTCGGTCT</t>
+  </si>
+  <si>
+    <t>MK13_HUMAN_D0_4EYJ_A</t>
+  </si>
+  <si>
+    <t>STK16_HUMAN_D0_2BUJ_B</t>
+  </si>
+  <si>
     <t>ATGGAAAGCGACCTGCACCAGATCATCCACTCCTCACAGCCCCTCACACTGGAACACGTGCGCTACTTCCTGTACCAACTGCTGCGGGGCCTGAAGTACATGCACTCGGCTCAGGTCATCCACCGTGACCTGAAGCCCTCCAACCTATTGGTGAATGAGAACTGTGAGCTCAAGATTGGTGACTTTGGTATGGCTCGTGGCCTGTGCACCTCGCCCGCTGAACATCAGTACTTCATGACTGAGTATGTGGCCACGCGCTGGTACCGTGCGCCCGAGCTCATGCTCTCTTTGCATGAGTATACACAGGCTATTGACCTCTGGTCTGTGGGCTGCATCTTTGGTGAGATGCTGGCCCGGCGCCAGCTCTTCCCAGGCAAAAACTATGTACACCAGCTACAGCTCATCATGATGGTGCTGGGTACCCCATCACCAGCCGTGATTCAGGCTGTGGGGGCTGAGAGGGTGCGGGCCTATATCCAGAGCTTGCCACCACGCCAGCCTGTGCCCTGGGAGACAGTGTACCCAGGTGCCGACCGCCAGGCCCTATCACTGCTGGGTCGCATGCTGCGTTTTGAGCCCAGCGCTCGCATCTCAGCAGCTGCTGCCCTTCGCCACCCTTTCCTGGCCAAGTACCATGATCCTGATGATGAGCCTGACTGTGCCCCGCCCTTTGACTTTGCCTTTGACCGCGAAGCCCTCACTCGGGAGCGCATTAAGGAGGCCATTGTGGCTGAAATTGAGGACTTCCATGCAAGGCGTGAGGGCATCCGCCAACAGATCCGCTTCCAGCCTTCTCTACAGCCTGTGGCTAGTGAGCCTGGCTGTCCAGATGTTGAAATGCCCAGTCCCTGGGCTCCCAGTGGGGACTGTGCCATG</t>
   </si>
   <si>
-    <t>ABL1_HUMAN_D0_3UE4_A</t>
-  </si>
-  <si>
-    <t>Nterm</t>
-  </si>
-  <si>
-    <t>HASP_HUMAN_D0_3E7V_A</t>
-  </si>
-  <si>
-    <t>CDK6_HUMAN_D0_4EZ5_A</t>
-  </si>
-  <si>
-    <t>SPQREPQRVSHEQFRAALQLVVDPGDPRSYLDNFIKIGEGSTGIVCIATVRSSGKLVAVKKMDLRKQQRRELLFNEVVIMRDYQHENVVEMYNSYLVGDELWVVMEFLEGGALTDIVTHTRMNEEQIAAVCLAVLQALSVLHAQGVIHRDIKSDSILLTHDGRVKLSDFGFCAQVSKEVPRRKSLVGTPYWMAPELISRLPYGPEVDIWSLGIMVIEMVDGEPPYFNEPPLKAMKMIRDNLPPRLKNLHKVSPSLKGFLDRLLVRDPAQRATAAELLKHPFLAKAGPPASIVPLMRQNRTR</t>
-  </si>
-  <si>
-    <t>ELKDDDFEKISELGAGNGGVVFKVSHKPSGLVMARKLIHLEIKPAIRNQIIRELQVLHECNSPYIVGFYGAFYSDGEISICMEHMDGGSLDQVLKKAGRIPEQILGKVSIAVIKGLTYLREKHKIMHRAYGMDSRPPMAIFELLDYIVNEPPPKLPSGVFSLEFQDFVNKCLIKNPAERADLKQLMVHAFIKRSDAEEVDFAGWLCSTIGLN</t>
-  </si>
-  <si>
-    <t>PMYT1_HUMAN_D0_3P1A_A</t>
-  </si>
-  <si>
-    <t>GPEDELPDWAAAKEFYQKYDPKDVIGRGVSSVVRRCVHRATGHEFAVKIMEVTAERLSPEQLEEVREATRRETHILRQVAGHPHIITLIDSYESSSFMFLVFDLMRKGELFDYLTEKVALSEKETRSIMRSLLEAVSFLHANNIVHRDLKPENILLDDNMQIRLSDFGFSCHLEPGEKLRELCGTPGYLAPEILKCSMDETHPGYGKEVDLWACGVILFTLLAGSPPFWHRRQILMLRMIMEGQYQFSSPEWDDRSSTVKDLISRLLQVDPEARLTAEQALQHPFFER</t>
-  </si>
-  <si>
-    <t>GTGGAGGACCATTATGAGATGGGGGAGGAGCTGGGCAGCGGCCAGTTTGCGATCGTGCGGAAGTGCCGGCAGAAGGGCACGGGCAAGGAGTACGCAGCCAAGTTCATCAAGAAGCGCCGCCTGTCATCCAGCCGGCGTGGGGTGAGCCGGGAGGAGATCGAGCGGGAGGTGAACATCCTGCGGGAGATCCGGCACCCCAACATCATCACCCTGCACGACATCTTCGAGAACAAGACGGACGTGGTCCTCATCCTGGAGCTGGTCTCTGGCGGGGAGCTCTTTGACTTCCTGGCGGAGAAGGAGTCGCTGACGGAGGACGAGGCCACCCAGTTCCTCAAGCAGATCCTGGACGGCGTTCACTACCTGCACTCTAAGCGCATCGCACACTTTGACCTGAAGCCGGAAAACATCATGCTGCTGGACAAGAACGTGCCCAACCCACGAATCAAGCTCATCGACTTCGGCATCGCGCACAAGATCGAGGCGGGGAACGAGTTCAAGAACATCTTCGGCACCCCGGAGTTTGTGGCCCCAGAGATTGTGAACTATGAGCCGCTGGGCCTGGAGGCGGACATGTGGAGCATCGGTGTCATCACCTATATCCTCCTGAGCGGTGCATCCCCGTTCCTGGGCGAGACCAAGCAGGAGACGCTCACCAACATCTCAGCCGTGAACTACGACTTCGACGAGGAGTACTTCAGCAACACCAGCGAGCTGGCCAAGGACTTCATTCGCCGGCTGCTCGTCAAAGATCCCAAGCGGAGAATGACCATTGCCCAGAGCCTGGAACATTCCTGGATTAAGGCGATCCGGCGGCGGAACGTGCGTGGTGAGGACAGCGGC</t>
-  </si>
-  <si>
-    <t>TCAGTTTATCCTAAGGCATTAAGAGATGAATACATCATGTCAAAAACTCTTGGAAGTGGTGCCTGTGGAGAGGTAAAGCTGGCTTTCGAGAGGAAAACATGTAAGAAAGTAGCCATAAAGATCATCAGCAAAAGGAAGTTTGCTATTGGTTCAGCAAGAGAGGCAGACCCAGCTCTCAATGTTGAAACAGAAATAGAAATTTTGAAAAAGCTAAATCATCCTTGCATCATCAAGATTAAAAACTTTTTTGATGCAGAAGATTATTATATTGTTTTGGAATTGATGGAAGGGGGAGAGCTGTTTGACAAAGTGGTGGGGAATAAACGCCTGAAAGAAGCTACCTGCAAGCTCTATTTTTACCAGATGCTCTTGGCTGTGCAGTACCTTCATGAAAACGGTATTATACACCGTGACTTAAAGCCAGAGAATGTTTTACTGTCATCTCAAGAAGAGGACTGTCTTATAAAGATTACTGATTTTGGGCACTCCAAGATTTGGGGAGAGACCTCTCTCATGAGAACCTTATGTGGAACCCCCACCTACTTGGCGCCTGAAGTTCTTGTTTCTGTTGGGACTGCTGGGTATAACCGTGCTGTGGACTGCTGGAGTTTAGGAGTTATTCTTTTTATCTGCCTTAGTGGGTATCCACCTTTCTCTGAGCATAGGACTCAAGTGTCACTGAAGGATCAGATCACCAGTGGAAAATACAACTTCATTCCTGAAGTCTGGGCAGAAGTCTCAGAGAAAGCTCTGGACCTTGTCAAGAAGTTGTTGGTAGTGGATCCAAAGGCACGTTTTACGACAGAAGAAGCCTTAAGACACCCGTGGCTTCAGGATGAAGACATGAAGAGAAAGTTTCAAGATCTTCTGTCTGAGGAAAATGAATCCACAGCTCTACCCCAGGTTCTAGCCCAGCCTTCTACTAGTCGAAAGCGGCCCCGTGAAGGGGAAGCCGAGGGTGCCGAG</t>
+    <t>CAGAGCAGTAAGCGCAGCAGCCGGAGTGTGGAAGATGACAAGGAGGGTCACCTGGTGTGCCGGATCGGCGATTGGCTCCAAGAGCGATATGAGATTGTGGGGAACCTGGGTGAAGGCACCTTTGGCAAGGTGGTGGAGTGCTTGGACCATGCCAGAGGGAAGTCTCAGGTTGCCCTGAAGATCATCCGCAACGTGGGCAAGTACCGGGAGGCTGCCCGGCTAGAAATCAACGTGCTCAAAAAAATCAAGGAGAAGGACAAAGAAAACAAGTTCCTGTGTGTCTTGATGTCTGACTGGTTCAACTTCCACGGTCACATGTGCATCGCCTTTGAGCTCCTGGGCAAGAACACCTTTGAGTTCCTGAAGGAGAATAACTTCCAGCCTTACCCCCTACCACATGTCCGGCACATGGCCTACCAGCTCTGCCACGCCCTTAGATTTCTGCATGAGAATCAGCTGACCCATACAGACTTGAAACCAGAGAACATCCTGTTTGTGAATTCTGAGTTTGAAACCCTCTACAATGAGCACAAGAGCTGTGAGGAGAAGTCAGTGAAGAACACCAGCATCCGAGTGGCTGACTTTGGCAGTGCCACATTTGACCATGAGCACCACACCACCATTGTGGCCACCCGTCACTATCGCCCGCCTGAGGTGATCCTTGAGCTGGGCTGGGCACAGCCCTGTGACGTCTGGAGCATTGGCTGCATTCTCTTTGAGTACTACCGGGGCTTCACACTCTTCCAGACCCACGAAAACCGAGAGCACCTGGTGATGATGGAGAAGATCCTAGGGCCCATCCCATCACACATGATCCACCGTACCAGGAAGCAGAAATATTTCTACAAAGGGGGCCTAGTTTGGGATGAGAACAGCTCTGACGGCCGGTATGTGAAGGAGAACTGCAAACCTCTGAAGAGTTACATGCTCCAAGACTCCCTGGAGCACGTGCAGCTGTTTGACCTGATGAGGAGGATGTTAGAATTTGACCCTGCCCAGCGCATCACACTGGCCGAGGCCCTGCTGCACCCCTTCTTTGCTGGCCTGACCCCTGAGGAGCGGTCCTTCCACACC</t>
+  </si>
+  <si>
+    <t>GAACTGAAGGATGACGACTTTGAGAAGATCAGTGAGCTGGGGGCTGGCAATGGCGGTGTGGTGTTCAAGGTCTCCCACAAGCCTTCTGGCCTGGTCATGGCCAGAAAGCTAATTCATCTGGAGATCAAACCCGCAATCCGGAACCAGATCATAAGGGAGCTGCAGGTTCTGCATGAGTGCAACTCTCCGTACATCGTGGGCTTCTATGGTGCGTTCTACAGCGATGGCGAGATCAGTATCTGCATGGAGCACATGGATGGAGGTTCTCTGGATCAAGTCCTGAAGAAAGCTGGAAGAATTCCTGAACAAATTTTAGGAAAAGTTAGCATTGCTGTAATAAAAGGCCTGACATATCTGAGGGAGAAGCACAAGATCATGCACAGAGCATACGGAATGGACAGCCGACCTCCCATGGCAATTTTTGAGTTGTTGGATTACATAGTCAACGAGCCTCCTCCAAAACTGCCCAGTGGAGTGTTCAGTCTGGAATTTCAAGATTTTGTGAATAAATGCTTAATAAAAAACCCCGCAGAGAGAGCAGATTTGAAGCAACTCATGGTTCATGCTTTTATCAAGAGATCTGATGCTGAGGAAGTGGATTTTGCAGGTTGGCTCTGCTCCACCATCGGCCTTAAC</t>
+  </si>
+  <si>
+    <t>MQTVGVHSIVQQLHRNSIQFTDGYEVKEDIGVGSYSVCKRCIHKATNMEFAVKIIDKSKRDPTEEIEILLRYGQHPNIITLKDVYDDGKYVYVVTELMKGGELLDKILRQKFFSEREASAVLFTITKTVEYLHAQGVVHRDLKPSNILYVDESGNPESIRICDFGFAKQLRAENGLLMTPCYTANFVAPEVLKRQGYDAACDIWSLGVLLYTMLTGYTPFANGPDDTPEEILARIGSGKFSLSGGYWNSVSDTAKDLVSKMLHVDPHQRLTAALVLRHPWIVHWDQLPQYQLNRQDAPHLVKGAMAATYSALNRNQSPVLEPVGRSTLAQRRGIKKITSTAL</t>
+  </si>
+  <si>
+    <t>KAPCA_HUMAN_D0_4AE9_A</t>
+  </si>
+  <si>
+    <t>KCC2G_HUMAN_D0_2V7O_A</t>
+  </si>
+  <si>
+    <t>KQYEHVKRDLNPEDFWEIIGELGDGAFGKVYKAQNKETSVLAAAKVIDTKSEEELEDYMVEIDILASCDHPNIVKLLDAFYYENNLWILIEFCAGGAVDAVMLELERPLTESQIQVVCKQTLDALNYLHDNKIIHRDLKAGNILFTLDGDIKLADFGVSAKNMRTIQRRDSFIGTPYWMAPEVVMCETSKDRPYDYKADVWSLGITLIEMAEIEPPHHELNPMRVLLKIAKSEPPTLAQPSRWSSNFKDFLKKCLEKNVDARWTTSQLLQHPFVTVDSNKPIRELIAEAKAEVTEEVEDGKE</t>
+  </si>
+  <si>
+    <t>ACCCAAACTGTTCATGAGTTTGCCAAGGAATTGGATGCCACCAACATATCCATTGATAAAGTTGTTGGAGCAGGTGAATTTGGAGAGGTGTGCAGTGGTCGCTTAAAACTTCCTTCAAAAAAAGAGATTTCAGTGGCCATTAAGACCCTGAAAGTTGGCTACACAGAAAAGCAGAGGAGAGACTTCCTGGGAGAAGCAAGCATTATGGGACAGTTTGACCACCCCAATATCATTCGACTGGAAGGAGTTGTTACCAAAAGTAAGCCAGTTATGATTGTCACAGAATACATGGAGAATGGTTCCTTGGATAGTTTCCTACGTAAACACGATGCCCAGTTTACTGTCATTCAGCTAGTGGGGATGCTTCGAGGGATAGCATCTGGCATGAAGTACCTGTCAGACATGGGCTATGTTCACCGAGACCTCGCTGCTCGGAACATCTTGATCAACAGTAACTTGGTGTGTAAGGTTTCTGATTTCGGACTTTCGCGTGTCCTGGAGGATGACCCAGAAGCTGCTTATACAACAAGAGGAGGGAAGATCCCAATCAGGTGGACATCACCAGAAGCTATAGCCTACCGCAAGTTCACGTCAGCCAGCGATGTATGGAGTTATGGGATTGTTCTCTGGGAGGTGATGTCTTATGGAGAGAGACCATACTGGGAGATGTCCAATCAGGATGTAATTAAAGCTGTAGATGAGGGCTATCGACTGCCACCCCCCATGGACTGCCCAGCTGCCTTGTATCAGCTGATGCTGGACTGCTGGCAGAAAGACAGGAACAACAGACCCAAGTTTGAGCAGATTGTTAGTATTCTGGACAAGCTTATCCGGAATCCCGGCAGCCTGAAGATCATCACCAGTGCAGCCGCAAGGCCATCAAACCTTCTTCTGGACCAAAGCAATGTGGATATCACTACCTTCCGCACAACAGGTGACTGGCTTAATGGTGTCTGGACAGCACACTGCAAGGAAATCTTCACGGGTGTGGAGTACAGTTCTTGTGACACAATAGCCAAGATTTCC</t>
+  </si>
+  <si>
+    <t>MEKDGLCRADQQYECVAEIGEGAYGKVFKARDLKNGGRFVALKRVRVQTGEEGMPLSTIREVAVLRHLETFEHPNVVRLFDVCTVSRTDRETKLTLVFEHVDQDLTTYLDKVPEPGVPTETIKDMMFQLLRGLDFLHSHRVVHRDLKPQNILVTSSGQIKLADFGLARIYSFQMALTSVVVTLWYRAPEVLLQSSYATPVDLWSVGCIFAEMFRRKPLFRGSSDVDQLGKILDVIGLPGEEDWPRDVALPRQAFHSKSAQPIEKFVTDIDELGKDLLLKCLTFNPAKRISAYSALSHPYFQ</t>
+  </si>
+  <si>
+    <t>EPHA3_HUMAN_D0_4GK2_A</t>
+  </si>
+  <si>
+    <t>ATGCCCGGCCCGGCCGCGGGCAGCAGGGCCCGGGTCTACGCCGAGGTGAACAGTCTGAGGAGCCGCGAGTACTGGGACTACGAGGCTCACGTCCCGAGCTGGGGTAATCAAGATGATTACCAACTGGTTCGAAAACTTGGTCGGGGAAAATATAGTGAAGTATTTGAGGCCATTAATATCACCAACAATGAGAGAGTGGTTGTAAAAATCCTGAAGCCAGTGAAGAAAAAGAAGATAAAACGAGAGGTTAAGATTCTGGAGAACCTTCGTGGTGGAACAAATATCATTAAGCTGATTGACACTGTAAAGGACCCCGTGTCAAAGACACCAGCTTTGGTATTTGAATATATCAATAATACAGATTTTAAGCAACTCTACCAGATCCTGACAGACTTTGATATCCGGTTTTATATGTATGAACTACTTAAAGCTCTGGATTACTGCCACAGCAAGGGAATCATGCACAGGGATGTGAAACCTCACAATGTCATGATAGATCACCAACAGAAAAAGCTGCGACTGATAGATTGGGGTCTGGCAGAATTCTATCATCCTGCTCAGGAGTACAATGTTCGTGTAGCCTCAAGGTACTTCAAGGGACCAGAGCTCCTCGTGGACTATCAGATGTATGATTATAGCTTGGACATGTGGAGTTTGGGCTGTATGTTAGCAAGCATGATCTTTCGAAGGGAACCATTCTTCCATGGACAGGACAACTATGACCAGCTTGTTCGCATTGCCAAGGTTCTGGGTACAGAAGAACTGTATGGGTATCTGAAGAAGTATCACATAGACCTAGATCCACACTTCAACGATATCCTGGGACAACATTCACGGAAACGCTGGGAAAACTTTATCCATAGTGAGAACAGACACCTTGTCAGCCCTGAGGCCCTAGATCTTCTGGACAAACTTCTGCGATACGACCATCAACAGAGACTGACTGCCAAAGAGGCCATGGAGCACCCATACTTCTACCCTGTGGTGAAGGAGCAGTCCCAG</t>
+  </si>
+  <si>
+    <t>ATGTCGGGACCCGTGCCAAGCAGGGCCAGAGTTTACACAGATGTTAATACACACAGACCTCGAGAATACTGGGATTACGAGTCACATGTGGTGGAATGGGGAAATCAAGATGACTACCAGCTGGTTCGAAAATTAGGCCGAGGTAAATACAGTGAAGTATTTGAAGCCATCAACATCACAAATAATGAAAAAGTTGTTGTTAAAATTCTCAAGCCAGTAAAAAAGAAGAAAATTAAGCGTGAAATAAAGATTTTGGAGAATTTGAGAGGAGGTCCCAACATCATCACACTGGCAGACATTGTAAAAGACCCTGTGTCACGAACCCCCGCCTTGGTTTTTGAACACGTAAACAACACAGACTTCAAGCAATTGTACCAGACGTTAACAGACTATGATATTCGATTTTACATGTATGAGATTCTGAAGGCCCTGGATTATTGTCACAGCATGGGAATTATGCACAGAGATGTCAAGCCCCATAATGTCATGATTGATCATGAGCACAGAAAGCTACGACTAATAGACTGGGGTTTGGCTGAGTTTTATCATCCTGGCCAAGAATATAATGTCCGAGTTGCTTCCCGATACTTCAAAGGTCCTGAGCTACTTGTAGACTATCAGATGTACGATTATAGTTTGGATATGTGGAGTTTGGGTTGTATGCTGGCAAGTATGATCTTTCGGAAGGAGCCATTTTTCCATGGACATGACAATTATGATCAGTTGGTGAGGATAGCCAAGGTTCTGGGGACAGAAGATTTATATGACTATATTGACAAATACAACATTGAATTAGATCCACGTTTCAATGATATCTTGGGCAGACACTCTCGAAAGCGATGGGAACGCTTTGTCCACAGTGAAAATCAGCACCTTGTCAGCCCTGAGGCCTTGGATTTCCTGGACAAACTGCTGCGATATGACCACCAGTCACGGCTTACTGCAAGAGAGGCAATGGAGCACCCCTATTTCTACACTGTTGTGAAGGACCAGGCTCGAATGGGT</t>
+  </si>
+  <si>
+    <t>NEK2_HUMAN_D0_2XKE_A</t>
+  </si>
+  <si>
+    <t>MK01_HUMAN_D0_4FMQ_A</t>
+  </si>
+  <si>
+    <t>ATGGAGCTGAGAGTCGGGAACAGGTACCGGCTGGGCCGGAAGATCGGCAGCGGCTCCTTCGGAGACATCTATCTCGGTACGGACATTGCTGCAGGAGAAGAGGTTGCCATCAAGCTTGAATGTGTCAAAACCAAACACCCTCAGCTCCACATTGAGAGCAAAATCTACAAGATGATGCAGGGAGGAGTGGGCATCCCCACCATCAGATGGTGCGGGGCAGAGGGGGACTACAACGTCATGGTGATGGAGCTGCTGGGGCCAAGCCTGGAGGACCTCTTCAACTTCTGCTCCAGGAAATTCAGCCTCAAAACCGTCCTGCTGCTTGCTGACCAAATGATCAGTCGCATCGAATACATTCATTCAAAGAACTTCATCCACCGGGATGTGAAGCCAGACAACTTCCTCATGGGCCTGGGGAAGAAGGGCAACCTGGTGTACATCATCGACTTCGGGCTGGCCAAGAAGTACCGGGATGCACGCACCCACCAGCACATCCCCTATCGTGAGAACAAGAACCTCACGGGGACGGCGCGGTACGCCTCCATCAACACGCACCTTGGAATTGAACAATCCCGAAGAGATGACTTGGAGTCTCTGGGCTACGTGCTAATGTACTTCAACCTGGGCTCTCTCCCCTGGCAGGGGCTGAAGGCTGCCACCAAGAGACAGAAATACGAAAGGATTAGCGAGAAGAAAATGTCCACCCCCATCGAAGTGTTGTGTAAAGGCTACCCTTCCGAATTTGCCACATACCTGAATTTCTGCCGTTCCTTGCGTTTTGACGACAAGCCTGACTACTCGTACCTGCGGCAGCTTTTCCGGAATCTGTTCCATCGCCAGGGCTTCTCCTATGACTACGTGTTCGACTGGAACATGCTCAAA</t>
+  </si>
+  <si>
+    <t>ATGGCGGCGGCGGCGGCGGCGGGCGCGGGCCCGGAGATGGTCCGCGGGCAGGTGTTCGACGTGGGGCCGCGCTACACCAACCTCTCGTACATCGGCGAGGGCGCCTACGGCATGGTGTGCTCTGCTTATGATAATGTCAACAAAGTTCGAGTAGCTATCAAGAAAATCAGCCCCTTTGAGCACCAGACCTACTGCCAGAGAACCCTGAGGGAGATAAAAATCTTACTGCGCTTCAGACATGAGAACATCATTGGAATCAATGACATTATTCGAGCACCAACCATCGAGCAAATGAAAGATGTATATATAGTACAGGACCTCATGGAAACAGATCTTTACAAGCTCTTGAAGACACAACACCTCAGCAATGACCATATCTGCTATTTTCTCTACCAGATCCTCAGAGGGTTAAAATATATCCATTCAGCTAACGTTCTGCACCGTGACCTCAAGCCTTCCAACCTGCTGCTCAACACCACCTGTGATCTCAAGATCTGTGACTTTGGCCTGGCCCGTGTTGCAGATCCAGACCATGATCACACAGGGTTCCTGACAGAATATGTGGCCACACGTTGGTACAGGGCTCCAGAAATTATGTTGAATTCCAAGGGCTACACCAAGTCCATTGATATTTGGTCTGTAGGCTGCATTCTGGCAGAAATGCTTTCTAACAGGCCCATCTTTCCAGGGAAGCATTATCTTGACCAGCTGAACCACATTTTGGGTATTCTTGGATCCCCATCACAAGAAGACCTGAATTGTATAATAAATTTAAAAGCTAGGAACTATTTGCTTTCTCTTCCACACAAAAATAAGGTGCCATGGAACAGGCTGTTCCCAAATGCTGACTCCAAAGCTCTGGACTTATTGGACAAAATGTTGACATTCAACCCACACAAGAGGATTGAAGTAGAACAGGCTCTGGCCCACCCATATCTGGAGCAGTATTACGACCCGAGTGACGAGCCCATCGCCGAAGCACCATTCAAGTTCGACATGGAATTGGATGACTTGCCTAAGGAAAAGCTCAAAGAACTAATTTTTGAAGAGACTGCTAGATTCCAGCCAGGATACAGATCT</t>
+  </si>
+  <si>
+    <t>MDEQSQGMQGPPVPQFQPQKALRPDMGYNTLANFRIEKKIGRGQFSEVYRAACLLDGVPVALKKVQIFDLMDAKARADCIKEIDLLKQLNHPNVIKYYASFIEDNELNIVLELADAGDLSRMIKHFKKQKRLIPERTVWKYFVQLCSALEHMHSRRVMHRDIKPANVFITATGVVKLGDLGLGRFFSSKTTAAHSLVGTPYYMSPERIHENGYNFKSDIWSLGCLLYEMAALQSPFYGDKMNLYSLCKKIEQCDYPPLPSDHYSEELRQLVNMCINPDPEKRPDVTYVYDVAKRMHACTASS</t>
+  </si>
+  <si>
+    <t>GECSQKGPVPFSHCLPTEKLQRCEKIGEGVFGEVFQTIADHTPVAIKIIAIEGPDLVNGSHQKTFEEILPEIIISKELSLLSGEVCNRTEGFIGLNSVHCVQGSYPPLLLKAWDHYNSTKGSANDRPDFFKDDQLFIVLEFEFGGIDLEQMRTKLSSLATAKSILHQLTASLAVAEASLRFEHRDLHWGNVLLKKTSLKKLHYTLNGKSSTIPSCGLQVSIIDYTLSRLERDGIVVFCDVSMDEDLFTGDGDYQFDIYRLMKKENNNRWGEYHPYSNVLWLHYLTDKMLKQMTFKTKCNTPAMKQIKRKIQEFHRTMLNFSSATDLLCQHRLFK</t>
+  </si>
+  <si>
+    <t>MENFNNFYILTSKELGRGKFAVVRQCISKSTGQEYAAKFLKKRRRGQDCRAEILHEIAVLELAKSCPRVINLHEVYENTSEIILILEYAAGGEIFSLCLPELAEMVSENDVIRLIKQILEGVYYLHQNNIVHLDLKPQNILLSSIYPLGDIKIVDFGMSRKIGHACELREIMGTPEYLAPEILNYDPITTATDMWNIGIIAYMLLTHTSPFVGEDNQETYLNISQVNVDYSEETFSSVSQLATDFIQSLLVKNPEKRPTAEICLSHSWLQQWDFENLFHPEETSSSSQTQDHSVRSSEDKTSKSS</t>
+  </si>
+  <si>
+    <t>GCTGATCCAGAAGAACTGTTCACAAAATTAGAGCGCATTGGGAAAGGCTCATTTGGGGAAGTTTTCAAAGGAATTGATAACCGTACCCAGCAAGTCGTTGCTATTAAAATCATAGACCTTGAGGAAGCCGAAGATGAAATAGAAGACATTCAGCAAGAAATAACTGTCTTGAGTCAATGTGACAGCTCATATGTAACAAAATACTATGGGTCATATTTAAAGGGGTCTAAATTATGGATAATAATGGAATACCTGGGCGGTGGTTCAGCACTGGATCTTCTTCGAGCTGGTCCATTTGATGAGTTCCAGATTGCTACCATGCTAAAGGAAATTTTAAAAGGTCTGGACTATCTGCATTCAGAAAAGAAAATTCACCGAGACATAAAAGCTGCCAATGTCTTGCTCTCAGAACAAGGAGATGTTAAACTTGCTGATTTTGGAGTTGCTGGTCAGCTGACAGATACACAGATTAAAAGAAATACCTTTGTGGGAACTCCATTTTGGATGGCTCCTGAAGTTATTCAACAGTCAGCTTATGACTCAAAAGCTGACATTTGGTCATTGGGAATTACTGCTATTGAACTAGCCAAGGGAGAGCCACCTAACTCCGATATGCATCCAATGAGAGTTCTGTTTCTTATTCCCAAAAACAATCCTCCAACTCTTGTTGGAGACTTTACTAAGTCTTTTAAGGAGTTTATTGATGCTTGCCTGAACAAAGATCCATCATTTCGTCCTACAGCAAAAGAACTTCTGAAACACAAATTCATTGTAAAAAATTCAAAGAAGACTTCTTATCTGACTGAACTGATAGATCGTTTTAAGAGATGGAAGGCAGAA</t>
+  </si>
+  <si>
+    <t>MELRVGNKYRLGRKIGSGSFGDIYLGANIASGEEVAIKLECVKTKHPQLHIESKFYKMMQGGVGIPSIKWCGAEGDYNVMVMELLGPSLEDLFNFCSRKFSLKTVLLLADQMISRIEYIHSKNFIHRDVKPDNFLMGLGKKGNLVYIIDFGLAKKYRDARTHQHIPYRENKNLTGTARYASINTHLGIEQSRRDDLESLGYVLMYFNLGSLPWQGLKAATKRQKYERISEKKMSTPIEVLCKGYPSEFSTYLNFCRSLRFDDKPDYSYLRQLFRNLFHRQGFSYDYVFDWNMLK</t>
+  </si>
+  <si>
+    <t>SSVTASAAPGTASLVPDYWIDGSNRDALSDFFEVESELGRGATSIVYRCKQKGTQKPYALKVLKKTVDKKIVRTEIGVLLRLSHPNIIKLKEIFETPTEISLVLELVTGGELFDRIVEKGYYSERDAADAVKQILEAVAYLHENGIVHRDLKPENLLYATPAPDAPLKIADFGLSKIVEHQVLMKTVCGTPGYCAPEILRGCAYGPEVDMWSVGIITYILLCGFEPFYDERGDQFMFRRILNCEYYFISPWWDEVSLNAKDLVRKLIVLDPKKRLTTFQALQHPWVTGKAANFVHMDTAQKKLQEFNARRKLKAAVKAVVASSRLG</t>
+  </si>
+  <si>
+    <t>dna_end</t>
+  </si>
+  <si>
+    <t>MADDDVLFEDVYELCEVIGKGPFSVVRRCINRETGQQFAVKIVDVAKFTSSPGLSTEDLKREASICHMLKHPHIVELLETYSSDGMLYMVFEFMDGADLCFEIVKRADAGFVYSEAVASHYMRQILEALRYCHDNNIIHRDVKPHCVLLASKENSAPVKLGGFGVAIQLGESGLVAGGRVGTPHFMAPEVVKREPYGKPVDVWGCGVILFILLSGCLPFYGTKERLFEGIIKGKYKMNPRQWSHISESAKDLVRRMLMLDPAERITVYEALNHPWLKERDRYAYKIHLPETVEQLRKFNARRKLKGAVLAAVSSHKFNSFYGDPPEELPDFSEDPTSSGA</t>
+  </si>
+  <si>
+    <t>FAK1_HUMAN_D0_2IJM_B</t>
+  </si>
+  <si>
+    <t>CHK2_HUMAN_D0_2CN5_A</t>
+  </si>
+  <si>
+    <t>GTGATCGACCCCTCAGAGCTCACTTTTGTCCAAGAGATTGGCAGTGGGCAATTTGGGTTGGTGCATCTGGGCTACTGGCTCAACAAGGACAAGGTGGCTATCAAAACCATTCGGGAAGGGGCTATGTCAGAAGAGGACTTCATAGAGGAGGCTGAAGTAATGATGAAACTCTCTCATCCCAAACTGGTGCAGCTGTATGGGGTGTGCCTGGAGCAGGCCCCCATCTGCCTGGTGTTTGAGTTCATGGAGCACGGCTGCCTGTCAGATTATCTACGCACCCAGCGGGGACTTTTTGCTGCAGAGACCCTGCTGGGCATGTGTCTGGATGTGTGTGAGGGCATGGCCTACCTGGAAGAGGCATGTGTCATCCACAGAGACTTGGCTGCCAGAAATTGTTTGGTGGGAGAAAACCAAGTCATCAAGGTGTCTGACTTTGGGATGACAAGGTTCGTTCTGGATGATCAGTACACCAGTTCCACAGGCACCAAATTCCCGGTGAAGTGGGCATCCCCAGAGGTTTTCTCTTTCAGTCGCTATAGCAGCAAGTCCGATGTGTGGTCATTTGGTGTGCTGATGTGGGAAGTTTTCAGTGAAGGCAAAATCCCGTATGAAAACCGAAGCAACTCAGAGGTGGTGGAAGACATCAGTACCGGATTTCGGTTGTACAAGCCCCGGCTGGCCTCCACACACGTCTACCAGATTATGAATCACTGCTGGAAAGAGAGACCAGAAGATCGGCCAGCCTTCTCCAGACTGCTGCGTCAACTGGCTGAAATTGCAGAATCAGGACTT</t>
+  </si>
+  <si>
+    <t>MSDEEILEKLRSIVSVGDPKKKYTRFEKIGQGASGTVYTAMDVATGQEVAIKQMNLQQQPKKELIINEILVMRENKNPNIVNYLDSYLVGDELWVVMEYLAGGSLTDVVTETCMDEGQIAAVCRECLQALEFLHSNQVIHRDIKSDNILLGMDGSVKLTDFGFCAQITPEQSKRSTMVGTPYWMAPEVVTRKAYGPKVDIWSLGIKAIEMIEGEPPYLNENPLRALYLIATNGTPELQNPEKLSAIFRDFLNRCLEMDVEKRGSAKELLQHQFLKIAKPLSSLTPLIAAAKEATKNNH</t>
+  </si>
+  <si>
+    <t>MSQSKGKKRNPGLKIPKEAFEQPQTSSTPPRDLDSKACISIGNQNFEVKADDLEPIMELGRGAYGVVEKMRHVPSGQIMAVKRIRATVNSQEQKRLLMDLDISMRTVDCPFTVTFYGALFREGDVWICMELMDTSLDKFYKQVIDKGQTIPEDILGKIAVSIVKALEHLHSKLSVIHRDVKPSNVLINALGQVKMCDFGISGYLVDSVAKTIDAGCKPYMAPERINPELNQKGYSVKSDIWSLGITMIELAILRFPYDSWGTPFQQLKQVVEEPSPQLPADKFSAEFVDFTSQCLKKNSKERPTYPELMQHPFFTLHESKGTDVASFVKLILGD</t>
+  </si>
+  <si>
+    <t>DYRK2_HUMAN_D0_3KVW_A</t>
+  </si>
+  <si>
+    <t>GCGGCTCCACCGGCGAAAGAGATCCCGGAGGTCCTAGTGGACCCACGCAGCCGGCGGCGCTATGTGCGGGGCCGCTTTTTGGGCAAGGGCGGCTTTGCCAAGTGCTTCGAGATCTCGGACGCGGACACCAAGGAGGTGTTCGCGGGCAAGATTGTGCCTAAGTCTCTGCTGCTCAAGCCGCACCAGAGGGAGAAGATGTCCATGGAAATATCCATTCACCGCAGCCTCGCCCACCAGCACGTCGTAGGATTCCACGGCTTTTTCGAGGACAACGACTTCGTGTTCGTGGTGTTGGAGCTCTGCCGCCGGAGGTCTCTCCTGGAGCTGCACAAGAGGAGGAAAGCCCTGACTGAGCCTGAGGCCCGATACTACCTACGGCAAATTGTGCTTGGCTGCCAGTACCTGCACCGAAACCGAGTTATTCATCGAGACCTCAAGCTGGGCAACCTTTTCCTGAATGAAGATCTGGAGGTGAAAATAGGGGATTTTGGACTGGCAACCAAAGTCGAATATGACGGGGAGAGGAAGAAGACCCTGTGTGGGACTCCTAATTACATAGCTCCCGAGGTGCTGAGCAAGAAAGGGCACAGTTTCGAGGTGGATGTGTGGTCCATTGGGTGTATCATGTATACCTTGTTAGTGGGCAAACCACCTTTTGAGACTTCTTGCCTAAAAGAGACCTACCTCCGGATCAAGAAGAATGAATACAGTATTCCCAAGCACATCAACCCCGTGGCCGCCTCCCTCATCCAGAAGATGCTTCAGACAGATCCCACTGCCCGCCCAACCATTAACGAGCTGCTTAATGACGAGTTCTTTACTTCTGGCTATATCCCTGCCCGTCTCCCCATCACCTGCCTGACCATTCCACCAAGGTTTTCGATTGCTCCCAGCAGCCTGGACCCCAGCAACCGGAAGCCCCTCACAGTCCTCAATAAA</t>
+  </si>
+  <si>
+    <t>QSSKRSSRSVEDDKEGHLVCRIGDWLQERYEIVGNLGEGTFGKVVECLDHARGKSQVALKIIRNVGKYREAARLEINVLKKIKEKDKENKFLCVLMSDWFNFHGHMCIAFELLGKNTFEFLKENNFQPYPLPHVRHMAYQLCHALRFLHENQLTHTDLKPENILFVNSEFETLYNEHKSCEEKSVKNTSIRVADFGSATFDHEHHTTIVATRHYRPPEVILELGWAQPCDVWSIGCILFEYYRGFTLFQTHENREHLVMMEKILGPIPSHMIHRTRKQKYFYKGGLVWDENSSDGRYVKENCKPLKSYMLQDSLEHVQLFDLMRRMLEFDPAQRITLAEALLHPFFAGLTPEERSFHT</t>
+  </si>
+  <si>
+    <t>MK07_HUMAN_D0_4IC7_D</t>
+  </si>
+  <si>
+    <t>ATGCAGACAGTTGGTGTACATTCAATTGTTCAGCAGTTACACAGGAACAGTATTCAGTTTACTGATGGATATGAAGTAAAAGAAGATATTGGAGTTGGCTCCTACTCTGTTTGCAAGAGATGTATACATAAAGCTACAAACATGGAGTTTGCAGTGAAGATTATTGATAAAAGCAAGAGAGACCCAACAGAAGAAATTGAAATTCTTCTTCGTTATGGACAGCATCCAAACATTATCACTCTAAAGGATGTATATGATGATGGAAAGTATGTGTATGTAGTAACAGAACTTATGAAAGGAGGTGAATTGCTGGATAAAATTCTTAGACAAAAATTTTTCTCTGAACGAGAGGCCAGTGCTGTCCTGTTCACTATAACTAAAACCGTTGAATATCTTCACGCACAAGGGGTGGTTCATAGAGACTTGAAACCTAGCAACATTCTTTATGTGGATGAATCTGGTAATCCGGAATCTATTCGAATTTGTGATTTTGGCTTTGCAAAACAGCTGAGAGCGGAAAATGGTCTTCTCATGACTCCTTGTTACACTGCAAATTTTGTTGCACCAGAGGTTTTAAAAAGACAAGGCTATGATGCTGCTTGTGATATATGGAGTCTTGGTGTCCTACTCTATACAATGCTTACCGGTTACACTCCATTTGCAAATGGTCCTGATGATACACCAGAGGAAATATTGGCACGAATAGGTAGCGGAAAATTCTCACTCAGTGGTGGTTACTGGAATTCTGTTTCAGACACAGCAAAGGACCTGGTGTCAAAGATGCTTCATGTAGACCCTCATCAGAGACTGACTGCTGCTCTTGTGCTCAGACATCCTTGGATCGTCCACTGGGACCAACTGCCACAATACCAACTAAACAGACAGGATGCACCACATCTAGTAAAGGGTGCCATGGCAGCTACATATTCTGCTTTGAACCGTAATCAGTCACCAGTTTTGGAACCAGTAGGCCGCTCTACTCTTGCTCAGCGGAGAGGTATTAAAAAAATCACCTCAACAGCCCTG</t>
+  </si>
+  <si>
+    <t>KS6A3_HUMAN_D0_4JG7_A</t>
+  </si>
+  <si>
+    <t>MGKVKATPMTPEQAMKQYMQKLTAFEHHEIFSYPEIYFLGLNAKKRQGMTGGPNNGGYDDDQGSYVQVPHDHVAYRYEVLKVIGKGSFGQVVKAYDHKVHQHVALKMVRNEKRFHRQAAEEIRILEHLRKQDKDNTMNVIHMLENFTFRNHICMTFELLSMNLYELIKKNKFQGFSLPLVRKFAHSILQCLDALHKNRIIHCDLKPENILLKQQGRSGIKVIDFGSSCYEHQRVYTYIQSRFYRAPEVILGARYGMPIDMWSLGCILAELLTGYPLLPGEDEGDQLACMIELLGMPSQKLLDASKRAKNFVSSKGYPRYCTVTTLSDGSVVLNGGRSRRGKLRGPPESREWGNALKGCDDPLFLDFLKQCLEWDPAVRMTPGQALRHPWLRRRLPKPPTGEKTSVKR</t>
+  </si>
+  <si>
+    <t>CAGCAGTTCCCGCAGTTCCACGTCAAGTCCGGCCTGCAGATCAAGAAGAACGCCATCATCGATGACTACAAGGTCACCAGCCAGGTCCTGGGGCTGGGCATCAACGGCAAAGTTTTGCAGATCTTCAACAAGAGGACCCAGGAGAAATTCGCCCTCAAAATGCTTCAGGACTGCCCCAAGGCCCGCAGGGAGGTGGAGCTGCACTGGCGGGCCTCCCAGTGCCCGCACATCGTACGGATCGTGGATGTGTACGAGAATCTGTACGCAGGGAGGAAGTGCCTGCTGATTGTCATGGAATGTTTGGACGGTGGAGAACTCTTTAGCCGAATCCAGGATCGAGGAGACCAGGCATTCACAGAAAGAGAAGCATCCGAAATCATGAAGAGCATCGGTGAGGCCATCCAGTATCTGCATTCAATCAACATTGCCCATCGGGATGTCAAGCCTGAGAATCTCTTATACACCTCCAAAAGGCCCAACGCCATCCTGAAACTCACTGACTTTGGCTTTGCCAAGGAAACCACCAGCCACAACTCTTTGACCACTCCTTGTTATACACCGTACTATGTGGCTCCAGAAGTGCTGGGTCCAGAGAAGTATGACAAGTCCTGTGACATGTGGTCCCTGGGTGTCATCATGTACATCCTGCTGTGTGGGTATCCCCCCTTCTACTCCAACCACGGCCTTGCCATCTCTCCGGGCATGAAGACTCGCATCCGAATGGGCCAGTATGAATTTCCCAACCCAGAATGGTCAGAAGTATCAGAGGAAGTGAAGATGCTCATTCGGAATCTGCTGAAAACAGAGCCCACCCAGAGAATGACCATCACCGAGTTTATGAACCACCCTTGGATCATGCAATCAACAAAGGTCCCTCAAACCCCACTGCACACCAGCCGGGTCCTGAAGGAGGACAAGGAGCGGTGGGAGGATGTCAAGGGGTGTCTTCATGACAAGAACAGCGACCAGGCC</t>
+  </si>
+  <si>
+    <t>CDK2_HUMAN_D0_4BCP_A</t>
+  </si>
+  <si>
+    <t>MP2K4_HUMAN_D0_3ALN_C</t>
+  </si>
+  <si>
+    <t>ACCACCTCACTTGAAGCTTTGCCCACAGGGACAGTGCTGACAGACAAGAGTGGGCGACAGTGGAAGCTGAAGTCCTTCCAGACCAGGGACAACCAGGGCATTCTCTATGAAGCTGCACCCACCTCCACCCTCACCTGTGACTCAGGACCACAGAAGCAAAAGTTCTCACTCAAACTGGATGCCAAGGATGGGCGCTTGTTCAATGAGCAGAACTTCTTCCAGCGGGCCGCCAAGCCTCTGCAAGTCAACAAGTGGAAGAAGCTGTACTCGACCCCACTGCTGGCCATCCCTACCTGCATGGGTTTCGGTGTTCACCAGGACAAATACAGGTTCTTGGTGTTACCCAGCCTGGGGAGGAGCCTTCAGTCGGCCCTGGATGTCAGCCCAAAGCATGTGCTGTCAGAGAGGTCTGTGCTGCAGGTGGCCTGCCGGCTGCTGGATGCCCTGGAGTTCCTCCATGAGAATGAGTATGTTCATGGAAATGTGACAGCTGAAAATATCTTTGTGGATCCAGAGGACCAGAGTCAGGTGACTTTGGCAGGCTATGGCTTCGCCTTCCGCTATTGCCCAAGTGGCAAACACGTGGCCTACGTGGAAGGCAGCAGGAGCCCTCACGAGGGGGACCTTGAGTTCATTAGCATGGACCTGCACAAGGGATGCGGGCCCTCCCGCCGCAGCGACCTCCAGAGCCTGGGCTACTGCATGCTGAAGTGGCTCTACGGGTTTCTGCCATGGACAAATTGCCTTCCCAACACTGAGGACATCATGAAGCAAAAACAGAAGTTTGTTGATAAGCCGGGGCCCTTCGTGGGACCCTGCGGTCACTGGATCAGGCCCTCAGAGACCCTGCAGAAGTACCTGAAGGTGGTGATGGCCCTCACGTATGAGGAGAAGCCGCCCTACGCCATGCTGAGGAACAACCTAGAAGCTTTGCTGCAGGATCTGCGTGTGTCTCCATATGACCCCATTGGCCTCCCGATGGTGCCC</t>
+  </si>
+  <si>
+    <t>TCACCACAGCGGGAGCCACAGCGAGTATCCCATGAGCAGTTCCGGGCTGCCCTGCAGCTGGTGGTGGACCCAGGCGACCCCCGCTCCTACCTGGACAACTTCATCAAGATTGGCGAGGGCTCCACGGGCATCGTGTGCATCGCCACCGTGCGCAGCTCGGGCAAGCTGGTGGCCGTCAAGAAGATGGACCTGCGCAAGCAGCAGAGGCGCGAGCTGCTCTTCAACGAGGTGGTAATCATGAGGGACTACCAGCACGAGAATGTGGTGGAGATGTACAACAGCTACCTGGTGGGGGACGAGCTCTGGGTGGTCATGGAGTTCCTGGAAGGAGGCGCCCTCACCGACATCGTCACCCACACCAGGATGAACGAGGAGCAGATCGCGGCCGTGTGCCTTGCAGTGCTGCAGGCCCTGTCGGTGCTCCACGCCCAGGGCGTCATCCACCGGGACATCAAGAGCGACTCGATCCTGCTGACCCATGATGGCAGGGTGAAGCTGTCAGACTTTGGGTTCTGCGCCCAGGTGAGCAAGGAAGTGCCCCGAAGGAAGTCGCTGGTCGGCACGCCCTACTGGATGGCCCCAGAGCTCATCTCCCGCCTTCCCTACGGGCCAGAGGTAGACATCTGGTCGCTGGGGATAATGGTGATTGAGATGGTGGACGGAGAGCCCCCCTACTTCAACGAGCCACCCCTCAAAGCCATGAAGATGATTCGGGACAACCTGCCACCCCGACTGAAGAACCTGCACAAGGTGTCGCCATCCCTGAAGGGCTTCCTGGACCGCCTGCTGGTGCGAGACCCTGCCCAGCGGGCCACGGCAGCCGAGCTGCTGAAGCACCCATTCCTGGCCAAGGCAGGGCCGCCTGCCAGCATCGTGCCCCTCATGCGCCAGAACCGCACCAGA</t>
+  </si>
+  <si>
+    <t>SIESSGKLKISPEQHWDFTAEDLKDLGEIGRGAYGSVNKMVHKPSGQIMAVKRIRSTVDEKEQKQLLMDLDVVMRSSDCPYIVQFYGALFREGDCWICMELMSTSFDKFYKYVYSVLDDVIPEEILGKITLATVKALNHLKENLKIIHRDIKPSNILLDRSGNIKLCDFGISGQLVDSIAKTRDAGCRPYMAPERIDPSASRQGYDVRSDVWSLGITLYELATGRFPYPKWNSVFDQLTQVVKGDPPQLSNSEEREFSPSFINFVNLCLTKDESKRPKYKELLKHPFILMYEERAVEVACYVCKILDQMPATPSSPMYVD</t>
+  </si>
+  <si>
+    <t>TDSFSGRFEDVYQLQEDVLGEGAHARVQTCINLITSQEYAVKIIEKQPGHIRSRVFREVEMLYQCQGHRNVLELIEFFEEEDRFYLVFEKMRGGSILSHIHKRRHFNELEASVVVQDVASALDFLHNKGIAHRDLKPENILCEHPNQVSPVKICDFDLGSGIKLNGDCSPISTPELLTPCGSAEYMAPEVVEAFSEEASIYDKRCDLWSLGVILYILLSGYPPFVGRCGSDCGWDRGEACPACQNMLFESIQEGKYEFPDKDWAHISCAAKDLISKLLVRDAKQRLSAAQVLQHPWVQGCAPENTLPTPMVLQR</t>
+  </si>
+  <si>
+    <t>WALNMKELKLLQTIGKGEFGDVMLGDYRGNKVAVKCIKNDATAQAFLAEASVMTQLRHSNLVQLLGVIVEEKGGLYIVTEYMAKGSLVDYLRSRGRSVLGGDCLLKFSLDVCEAMEYLEGNNFVHRDLAARNVLVSEDNVAKVSDFGLTKEASSTQDTGKLPVKWTAPEALREKKFSTKSDVWSFGILLWEIYSFGRVPYPRIPLKDVVPRVEKGYKMDAPDGCPPAVYEVMKNCWHLDAAMRPSFLQLREQLEHIKTHELHL</t>
+  </si>
+  <si>
+    <t>MPGPAAGSRARVYAEVNSLRSREYWDYEAHVPSWGNQDDYQLVRKLGRGKYSEVFEAINITNNERVVVKILKPVKKKKIKREVKILENLRGGTNIIKLIDTVKDPVSKTPALVFEYINNTDFKQLYQILTDFDIRFYMYELLKALDYCHSKGIMHRDVKPHNVMIDHQQKKLRLIDWGLAEFYHPAQEYNVRVASRYFKGPELLVDYQMYDYSLDMWSLGCMLASMIFRREPFFHGQDNYDQLVRIAKVLGTEELYGYLKKYHIDLDPHFNDILGQHSRKRWENFIHSENRHLVSPEALDLLDKLLRYDHQQRLTAKEAMEHPYFYPVVKEQSQ</t>
+  </si>
+  <si>
+    <t>AAGAGGCAGTGGGCTTTGGAAGACTTTGAAATTGGTCGCCCTCTGGGTAAAGGAAAGTTTGGTAATGTTTATTTGGCAAGAGAAAAGCAAAGCAAGTTTATTCTGGCTCTTAAAGTGTTATTTAAAGCTCAGCTGGAGAAAGCCGGAGTGGAGCATCAGCTCAGAAGAGAAGTAGAAATACAGTCCCACCTTCGGCATCCTAATATTCTTAGACTGTATGGTTATTTCCATGATGCTACCAGAGTCTACCTAATTCTGGAATATGCACCACTTGGAACAGTTTATAGAGAACTTCAGAAACTTTCAAAGTTTGATGAGCAGAGAACTGCTACTTATATAACAGAATTGGCAAATGCCCTGTCTTACTGTCATTCGAAGAGAGTTATTCATAGAGACATTAAGCCAGAGAACTTACTTCTTGGATCAGCTGGAGAGCTTAAAATTGCAGATTTTGGGTGGTCAGTACATGCTCCATCTTCCAGGAGGACCACTCTCTGTGGCACCCTGGACTACCTGCCCCCTGAAATGATTGAAGGTCGGATGCATGATGAGAAGGTGGATCTCTGGAGCCTTGGAGTTCTTTGCTATGAATTTTTAGTTGGGAAGCCTCCTTTTGAGGCAAACACATACCAAGAGACCTACAAAAGAATATCACGGGTTGAATTCACATTCCCTGACTTTGTAACAGAGGGAGCCAGGGACCTCATTTCAAGACTGTTGAAGCATAATCCCAGCCAGAGGCCAATGCTCAGAGAAGTACTTGAACACCCCTGGATCACAGCAAATTCATCAAAACCATCA</t>
+  </si>
+  <si>
+    <t>ATGGAGCTACGTGTGGGGAACAAGTACCGCCTGGGACGGAAGATCGGGAGCGGGTCCTTCGGAGATATCTACCTGGGTGCCAACATCGCCTCTGGTGAGGAAGTCGCCATCAAGCTGGAGTGTGTGAAGACAAAGCACCCCCAGCTGCACATCGAGAGCAAGTTCTACAAGATGATGCAGGGTGGCGTGGGGATCCCGTCCATCAAGTGGTGCGGAGCTGAGGGCGACTACAACGTGATGGTCATGGAGCTGCTGGGGCCTAGCCTCGAGGACCTGTTCAACTTCTGTTCCCGCAAATTCAGCCTCAAGACGGTGCTGCTCTTGGCCGACCAGATGATCAGCCGCATCGAGTATATCCACTCCAAGAACTTCATCCACCGGGACGTCAAGCCCGACAACTTCCTCATGGGGCTGGGGAAGAAGGGCAACCTGGTCTACATCATCGACTTCGGCCTGGCCAAGAAGTACCGGGACGCCCGCACCCACCAGCACATTCCCTACCGGGAAAACAAGAACCTGACCGGCACGGCCCGCTACGCTTCCATCAACACGCACCTGGGCATTGAGCAAAGCCGTCGAGATGACCTGGAGAGCCTGGGCTACGTGCTCATGTACTTCAACCTGGGCTCCCTGCCCTGGCAGGGGCTCAAAGCAGCCACCAAGCGCCAGAAGTATGAACGGATCAGCGAGAAGAAGATGTCAACGCCCATCGAGGTCCTCTGCAAAGGCTATCCCTCCGAATTCTCAACATACCTCAACTTCTGCCGCTCCCTGCGGTTTGACGACAAGCCCGACTACTCTTACCTACGTCAGCTCTTCCGCAACCTCTTCCACCGGCAGGGCTTCTCCTATGACTACGTCTTTGACTGGAACATGCTGAAA</t>
+  </si>
+  <si>
+    <t>MK03_HUMAN_D0_2ZOQ_B</t>
+  </si>
+  <si>
+    <t>ATGTCTCAGTCGAAAGGCAAGAAGCGAAACCCTGGCCTTAAAATTCCAAAAGAAGCATTTGAACAACCTCAGACCAGTTCCACACCACCTCGAGATTTAGACTCCAAGGCTTGCATTTCTATTGGAAATCAGAACTTTGAGGTGAAGGCAGATGACCTGGAGCCTATAATGGAACTGGGACGAGGTGCGTACGGGGTGGTGGAGAAGATGCGGCACGTGCCCAGCGGGCAGATCATGGCAGTGAAGCGGATCCGAGCCACAGTAAATAGCCAGGAACAGAAACGGCTACTGATGGATTTGGATATTTCCATGAGGACGGTGGACTGTCCATTCACTGTCACCTTTTATGGCGCACTGTTTCGGGAGGGTGATGTGTGGATCTGCATGGAGCTCATGGATACATCACTAGATAAATTCTACAAACAAGTTATTGATAAAGGCCAGACAATTCCAGAGGACATCTTAGGGAAAATAGCAGTTTCTATTGTAAAAGCATTAGAACATTTACATAGTAAGCTGTCTGTCATTCACAGAGACGTCAAGCCTTCTAATGTACTCATCAATGCTCTCGGTCAAGTGAAGATGTGCGATTTTGGAATCAGTGGCTACTTGGTGGACTCTGTTGCTAAAACAATTGATGCAGGTTGCAAACCATACATGGCCCCTGAAAGAATAAACCCAGAGCTCAACCAGAAGGGATACAGTGTGAAGTCTGACATTTGGAGTCTGGGCATCACGATGATTGAGTTGGCCATCCTTCGATTTCCCTATGATTCATGGGGAACTCCATTTCAGCAGCTCAAACAGGTGGTAGAGGAGCCATCGCCACAACTCCCAGCAGACAAGTTCTCTGCAGAGTTTGTTGACTTTACCTCACAGTGCTTAAAGAAGAATTCCAAAGAACGGCCTACATACCCAGAGCTAATGCAACATCCATTTTTCACCCTACATGAATCCAAAGGAACAGATGTGGCATCTTTTGTAAAACTGATTCTTGGAGAC</t>
+  </si>
+  <si>
+    <t>TCAACCAGGGATTATGAGATTCAAAGAGAAAGAATAGAACTTGGACGATGTATTGGAGAAGGCCAATTTGGAGATGTACATCAAGGCATTTATATGAGTCCAGAGAATCCAGCTTTGGCGGTTGCAATTAAAACATGTAAAAACTGTACTTCGGACAGCGTGAGAGAGAAATTTCTTCAAGAAGCCTTAACAATGCGTCAGTTTGACCATCCTCATATTGTGAAGCTGATTGGAGTCATCACAGAGAATCCTGTCTGGATAATCATGGAGCTGTGCACACTTGGAGAGCTGAGGTCATTTTTGCAAGTAAGGAAATACAGTTTGGATCTAGCATCTTTGATCCTGTATGCCTATCAGCTTAGTACAGCTCTTGCATATCTAGAGAGCAAAAGATTTGTACACAGGGACATTGCTGCTCGGAATGTTCTGGTGTCCTCAAATGATTGTGTAAAATTAGGAGACTTTGGATTATCCCGATATATGGAAGATAGTACTTACTACAAAGCTTCCAAAGGAAAATTGCCTATTAAATGGATGGCTCCAGAGTCAATCAATTTTCGACGTTTTACCTCAGCTAGTGACGTATGGATGTTTGGTGTGTGTATGTGGGAGATACTGATGCATGGTGTGAAGCCTTTTCAAGGAGTGAAGAACAATGATGTAATCGGTCGAATTGAAAATGGGGAAAGATTACCAATGCCTCCAAATTGTCCTCCTACCCTCTACAGCCTTATGACGAAATGCTGGGCCTATGACCCCAGCAGGCGGCCCAGGTTTACTGAACTTAAAGCTCAGCTCAGCACAATCCTGGAGGAAGAGAAGGCTCAGCAAGAAGAG</t>
+  </si>
+  <si>
+    <t>DPEELFTKLEKIGKGSFGEVFKGIDNRTQKVVAIKIIDLEEAEDEIEDIQQEITVLSQCDSPYVTKYYGSYLKDTKLWIIMEYLGGGSALDLLEPGPLDETQIATILREILKGLDYLHSEKKIHRDIKAANVLLSEHGEVKLADFGVAGQLTDTQIKRNTFVGTPFWMAPEVIKQSAYDSKADIWSLGITAIELARGEPPHSELHPMKVLFLIPKNNPPTLEGNYSKPLKEFVEACLNKEPSFRPTAKELLKHKFILRNAKKTSYLTELID</t>
+  </si>
+  <si>
+    <t>MAPK3_HUMAN_D0_3FXW_A</t>
+  </si>
+  <si>
+    <t>AAGCAGTACGAACACGTGAAGAGGGACCTGAACCCCGAAGACTTTTGGGAGATTATAGGAGAACTGGGCGACGGAGCCTTTGGGAAAGTGTACAAGGCCCAGAATAAAGAGACCAGTGTTTTAGCTGCTGCAAAAGTGATTGACACTAAATCTGAAGAAGAACTTGAAGATTACATGGTAGAGATTGACATATTAGCATCTTGTGATCACCCAAATATAGTCAAGCTTCTAGATGCCTTCTATTATGAGAACAATCTTTGGATCCTCATTGAATTTTGTGCAGGTGGAGCAGTAGATGCTGTGATGCTTGAACTTGAGAGACCATTAACTGAGTCCCAAATACAAGTAGTTTGCAAGCAGACTTTAGATGCATTGAACTACTTACATGATAATAAGATCATCCACAGAGATCTGAAGGCTGGCAACATTCTCTTTACCTTAGATGGAGATATCAAATTGGCGGATTTTGGAGTATCAGCTAAAAACATGAGGACAATTCAAAGAAGAGATTCCTTTATTGGTACACCATATTGGATGGCTCCTGAAGTAGTCATGTGTGAAACATCTAAGGACAGACCCTATGACTACAAAGCTGATGTTTGGTCCCTGGGTATCACTTTAATAGAAATGGCTGAGATAGAACCACCTCATCATGAATTAAATCCAATGCGAGTGCTGCTAAAAATAGCAAAATCTGAGCCACCTACATTAGCACAGCCATCCAGATGGTCTTCAAATTTTAAGGACTTTCTAAAGAAATGCTTAGAAAAGAATGTGGATGCCAGGTGGACTACATCTCAGCTGCTGCAGCATCCCTTTGTTACTGTTGATTCCAACAAACCCATCCGAGAATTGATTGCAGAGGCGAAGGCTGAAGTAACAGAAGAAGTTGAAGATGGCAAAGAG</t>
+  </si>
+  <si>
+    <t>ATGCCTTCCCGGGCTGAGGACTATGAAGTGTTGTACACCATTGGCACAGGCTCCTACGGCCGCTGCCAGAAGATCCGGAGGAAGAGTGATGGCAAGATATTAGTTTGGAAAGAACTTGACTATGGCTCCATGACAGAAGCTGAGAAACAGATGCTTGTTTCTGAAGTGAATTTGCTTCGTGAACTGAAACATCCAAACATCGTTCGTTACTATGATCGGATTATTGACCGGACCAATACAACACTGTACATTGTAATGGAATATTGTGAAGGAGGGGATCTGGCTAGTGTAATTACAAAGGGAACCAAGGAAAGGCAATACTTAGATGAAGAGTTTGTTCTTCGAGTGATGACTCAGTTGACTCTGGCCCTGAAGGAATGCCACAGACGAAGTGATGGTGGTCATACCGTATTGCATCGGGATCTGAAACCAGCCAATGTTTTCCTGGATGGCAAGCAAAACGTCAAGCTTGGAGACTTTGGGCTAGCTAGAATATTAAACCATGACACGAGTTTTGCAAAAACATTTGTTGGCACACCTTATTACATGTCTCCTGAACAAATGAATCGCATGTCCTACAATGAGAAATCAGATATCTGGTCATTGGGCTGCTTGCTGTATGAGTTATGTGCATTAATGCCTCCATTTACAGCTTTTAGCCAGAAAGAACTCGCTGGGAAAATCAGAGAAGGCAAATTCAGGCGAATTCCATACCGTTACTCTGATGAATTGAATGAAATTATTACGAGGATGTTAAACTTAAAGGATTACCATCGACCTTCTGTTGAAGAAATTCTTGAGAACCCTTTAATA</t>
+  </si>
+  <si>
+    <t>GATGAACAACCTCACATCGGAAACTACAGACTGTTGAAAACAATCGGCAAGGGGAATTTTGCAAAAGTAAAATTGGCAAGACATATCCTTACAGGCAGAGAGGTTGCAATAAAAATAATTGACAAAACTCAGTTGAATCCAACAAGTCTACAAAAGCTCTTCAGAGAAGTAAGAATAATGAAGATTTTAAATCATCCCAATATAGTGAAGTTATTCGAAGTCATTGAAACTGAAAAAACACTCTACCTAATCATGGAATATGCAAGTGGAGGTGAAGTATTTGACTATTTGGTTGCACATGGCAGGATGAAGGAAAAAGAAGCAAGATCTAAATTTAGACAGATTGTGTCTGCAGTTCAATACTGCCATCAGAAACGGATCGTACATCGAGACCTCAAGGCTGAAAATCTATTGTTAGATGCCGATATGAACATTAAAATAGCAGATTTCGGTTTTAGCAATGAATTTACTGTTGGCGGTAAACTCGACACGTTTTGTGGCAGTCCTCCATACGCAGCACCTGAGCTCTTCCAGGGCAAGAAATATGACGGGCCAGAAGTGGATGTGTGGAGTCTGGGGGTCATTTTATACACACTAGTCAGTGGCTCACTTCCCTTTGATGGGCAAAACCTAAAGGAACTGAGAGAGAGAGTATTAAGAGGGAAATACAGAATTCCCTTCTACATGTCTACAGACTGTGAAAACCTTCTCAAACGTTTCCTGGTGCTAAATCCAATTAAACGCGGCACTCTAGAGCAAATCATGAAGGACAGGTGGATCAATGCAGGGCATGAAGAAGATGAACTCAAACCATTTGTTGAACCAGAGCTAGACATCTCAGACCAAAAAAGAATAGATATTATGGTGGGAATGGGATATTCACAAGAAGAAATTCAAGAATCTCTTAGTAAGATGAAATACGATGAAATCACAGCTACATATTTGTTATTGGGGAGAAAATCTTCAGAG</t>
+  </si>
+  <si>
+    <t>CACCAGCTGCAGCCCCGGCGGGTGTCATTCCGGGGCGAGGCCTCAGAGACTCTGCAGAGCCCTGGGTATGACCCAAGCCGGCCAGAGTCCTTCTTCCAGCAGAGCTTCCAGAGGCTCAGCCGCCTGGGCCATGGCTCCTACGGAGAGGTCTTCAAGGTGCGCTCCAAGGAGGACGGCCGGCTCTATGCGGTAAAGCGTTCCATGTCACCATTCCGGGGCCCCAAGGACCGGGCCCGCAAGTTGGCCGAGGTGGGCAGCCACGAGAAGGTGGGGCAGCACCCATGCTGCGTGCGGCTGGAGCAGGCCTGGGAGGAGGGCGGCATCCTGTACCTGCAGACGGAGCTGTGCGGGCCCAGCCTGCAGCAACACTGTGAGGCCTGGGGTGCCAGCCTGCCTGAGGCCCAGGTCTGGGGCTACCTGCGGGACACGCTGCTTGCCCTGGCCCATCTGCACAGCCAGGGCCTGGTGCACCTTGATGTCAAGCCTGCCAACATCTTCCTGGGGCCCCGGGGCCGCTGCAAGCTGGGTGACTTCGGACTGCTGGTGGAGCTGGGTACAGCAGGAGCTGGTGAGGTCCAGGAGGGAGACCCCCGCTACATGGCCCCCGAGCTGCTGCAGGGCTCCTATGGGACAGCAGCGGATGTGTTCAGTCTGGGCCTCACCATCCTGGAAGTGGCATGCAACATGGAGCTGCCCCACGGTGGGGAGGGCTGGCAGCAGCTGCGCCAGGGCTACCTGCCCCCTGAGTTCACTGCCGGTCTGTCTTCCGAGCTGCGTTCTGTCCTTGTCATGATGCTGGAGCCAGACCCCAAGCTGCGGGCCACGGCCGAGGCCCTGCTGGCACTGCCTGTGTTGAGGCAGCCG</t>
+  </si>
+  <si>
+    <t>KEKEPLESQYQVGPLLGSGGFGSVYSGIRVSDNLPVAIKHVEKDRISDWGELPNGTRVPMEVVLLKKVSSGFSGVIRLLDWFERPDSFVLILERPEPVQDLFDFITERGALQEELARSFFWQVLEAVRHCHNCGVLHRDIKDENILIDLNRGELKLIDFGSGALLKDTVYTDFDGTRVYSPPEWIRYHRYHGRSAAVWSLGILLYDMVCGDIPFEHDEEIIGGQVFFRQRVSSECQHLIRWCLALRPSDRPTFEEIQNHPWMQDVLLPQETAEIHLHSLSPGPSK</t>
+  </si>
+  <si>
+    <t>VEDHYEMGEELGSGQFAIVRKCRQKGTGKEYAAKFIKKRRLSSSRRGVSREEIEREVNILREIRHPNIITLHDIFENKTDVVLILELVSGGELFDFLAEKESLTEDEATQFLKQILDGVHYLHSKRIAHFDLKPENIMLLDKNVPNPRIKLIDFGIAHKIEAGNEFKNIFGTPEFVAPEIVNYEPLGLEADMWSIGVITYILLSGASPFLGETKQETLTNISAVNYDFDEEYFSNTSELAKDFIRRLLVKDPKRRMTIAQSLEHSWIKAIRRRNVRGEDSG</t>
+  </si>
+  <si>
+    <t>MET_HUMAN_D0_4EEV_A</t>
+  </si>
+  <si>
+    <t>MSSFLPEGGCYELLTVIGKGFEDLMTVNLARYKPTGEYVTVRRINLEACSNEMVTFLQGELHVSKLFNHPNIVPYRATFIADNELWVVTSFMAYGSAKDLICTHFMDGMNELAIAYILQGVLKALDYIHHMGYVHRSVKASHILISVDGKVYLSGLRSNLSMISHGQRQRVVHDFPKYSVKVLPWLSPEVLQQNLQGYDAKSDIYSVGITACELANGHVPFKDMPATQMLLEKLNGTVPCLLDTSTIPAEELTMSPSRSVANSGLSDSLTTSTPRPSNGDSPSHPYHRTFSPHFHHFVEQCLQRNPDARPSASTLLNHSFFKQIKRRASEVLPELLRPVTPITNFEGSQSQDHSGIFGLVTNLEELEVDDWEF</t>
+  </si>
+  <si>
+    <t>MP2K1_HUMAN_D0_3MBL_A</t>
+  </si>
+  <si>
+    <t>ETKYTVDKRFGMDFKEIELIGSGGFGQVFKAKHRIDGKTYVIKRVKYNNEKAEREVKALAKLDHVNIVHYNGCWDGFDYDPETSDDSLESSDYDPENSKNSSRSKTKCLFIQMEFCDKGTLEQWIEKRRGEKLDKVLALELFEQITKGVDYIHSKKLIHRDLKPSNIFLVDTKQVKIGDFGLVTSLKNDGKRTRSKGTLRYMSPEQISSQDYGKEVDLYALGLILAELLHVCDTAFETSKFFTDLRDGIISDIFDKKEKTLLQKLLSKKPEDRPNTSEILRTLTVWKKSPEKNERHTC</t>
+  </si>
+  <si>
+    <t>CDKL1_HUMAN_D0_4AGU_C</t>
+  </si>
+  <si>
+    <t>MARK3_HUMAN_D0_2QNJ_A</t>
   </si>
   <si>
     <t>MSGPRAGFYRQELNKTVWEVPQRLQGLRPVGSGAYGSVCSAYDARLRQKVAVKKLSRPFQSLIHARRTYRELRLLKHLKHENVIGLLDVFTPATSIEDFSEVYLVTTLMGADLNNIVKCQALSDEHVQFLVYQLLRGLKYIHSAGIIHRDLKPSNVAVNEDCELRILDFGLARQADEEMTGYVATRWYRAPEIMLNWMHYNQTVDIWSVGCIMAELLQGKALFPGSDYIDQLKRIMEVVGTPSPEVLAKISSEHARTYIQSLPPMPQKDLSSIFRGANPLAIDLLGRMLVLDSDQRVSAAEALAHAYFSQYHDPEDEPEAEPYDESVEAKERTLEEWKELTYQEVLSFKPPEPPKPPGSLEIEQ</t>
   </si>
   <si>
-    <t>CSKP_HUMAN_D0_3TAC_A</t>
-  </si>
-  <si>
-    <t>MST4_HUMAN_D0_4FZD_B</t>
-  </si>
-  <si>
-    <t>MARK2_HUMAN_D0_3IEC_D</t>
-  </si>
-  <si>
-    <t>ACCGTGTTCAGGCAGGAAAACGTGGATGATTACTACGACACCGGCGAGGAACTTGGCAGTGGACAGTTTGCGGTTGTGAAGAAATGCCGTGAGAAAAGCACCGGCCTCCAGTATGCCGCCAAATTCATCAAGAAAAGGAGGACTAAGTCCAGCCGGCGGGGTGTGAGCCGCGAGGACATCGAGCGGGAGGTCAGCATCCTGAAGGAGATCCAGCACCCCAATGTCATCACCCTGCACGAGGTCTATGAGAACAAGACGGACGTCATCCTGATCTTGGAACTCGTTGCAGGTGGCGAGCTGTTTGACTTCTTAGCTGAAAAGGAATCTTTAACTGAAGAGGAAGCAACTGAATTTCTCAAACAAACTCTTAATGGTGTTTACTACCTGCACTCCCTTCAAATCGCCCACTTTGATCTTAAGCCTGAGAACATAATGCTTTTGGATAGAAATGTCCCCAAACCTCGGATCAAGATCATTGACTTTGGGTTGGCCCATAAAATTGACTTTGGAAATGAATTTAAAAACATATTTGGGACTCCAGAGTTTGTCGCTCCTGAGATAGTCAACTATGAACCTCTTGGTCTTGAGGCAGATATGTGGAGTATCGGGGTAATAACCTATATCCTCCTAAGTGGGGCCTCCCCATTTCTTGGAGACACTAAGCAAGAAACGTTAGCAAATGTATCCGCTGTCAACTACGAATTTGAGGATGAATACTTCAGTAATACCAGTGCCCTAGCCAAAGATTTCATAAGAAGACTTCTGGTCAAGGATCCAAAGAAGAGAATGACAATTCAAGATAGTTTGCAGCATCCCTGGATCAAGCCTAAAGATACACAACAGGCACTTAGT</t>
-  </si>
-  <si>
-    <t>CCATTTCCAGAAGGCAAGGTTCTGGATGATATGGAAGGCAATCAGTGGGTACTGGGCAAGAAGATTGGCTCTGGAGGATTTGGATTGATATATTTAGCTTTCCCCACAAATAAACCAGAGAAAGATGCAAGACATGTAGTAAAAGTGGAATATCAAGAAAATGGCCCGTTATTTTCAGAACTTAAATTTTATCAGAGAGTTGCAAAAAAAGACTGTATCAAAAAGTGGATAGAACGCAAACAACTTGATTATTTAGGAATTCCTCTGTTTTATGGATCTGGTCTGACTGAATTCAAGGGAAGAAGTTACAGATTTATGGTAATGGAAAGACTAGGAATAGATTTACAGAAGATCTCAGGCCAGAATGGTACCTTTAAAAAGTCAACTGTCCTGCAATTAGGTATCCGAATGTTGGATGTACTGGAATATATACATGAAAATGAATATGTTCATGGTGATATAAAAGCAGCAAATCTACTTTTGGGTTACAAAAATCCAGACCAGGTTTATCTTGCAGATTATGGACTTTCCTACAGATATTGTCCCAATGGGAACCACAAACAGTATCAGGAAAATCCTAGAAAAGGCCATAATGGGACAATAGAGTTTACCAGCTTGGATGCCCACAAGGGAGTAGCCTTGTCCAGACGAAGTGACGTTGAGATCCTCGGCTACTGCATGCTGCGGTGGTTGTGTGGGAAACTTCCCTGGGAACAGAACCTGAAGGACCCTGTGGCTGTGCAGACTGCTAAAACAAATCTGTTGGACGAGCTCCCCCAGTCAGTGCTTAAATGGGCTCCTTCTGGAAGCAGTTGCTGTGAAATAGCCCAATTTTTGGTATGTGCTCATAGTTTAGCATATGATGAAAAGCCAAACTATCAAGCCCTCAAGAAAATTTTGAACCCTCATGGAATACCTTTAGGACCACTGGACTTTTCCACAAAAGGACAGAGTATAAATGTCCAT</t>
-  </si>
-  <si>
-    <t>GGGGACTCTGATATATCCAGTCCATTACTGCAAAATACTGTCCACATTGACCTCAGTGCTCTAAATCCAGAGCTGGTCCAGGCAGTGCAGCATGTAGTGATTGGGCCCAGTAGCCTGATTGTGCATTTCAATGAAGTCATAGGAAGAGGGCATTTTGGTTGTGTATATCATGGGACTTTGTTGGACAATGATGGCAAGAAAATTCACTGTGCTGTGAAATCCTTGAACAGAATCACTGACATAGGAGAAGTTTCCCAATTTCTGACCGAGGGAATCATCATGAAAGATTTTAGTCATCCCAATGTCCTCTCGCTCCTGGGAATCTGCCTGCGAAGTGAAGGGTCTCCGCTGGTGGTCCTACCATACATGAAACATGGAGATCTTCGAAATTTCATTCGAAATGAGACTCATAATCCAACTGTAAAAGATCTTATTGGCTTTGGTCTTCAAGTAGCCAAAGGCATGAAATATCTTGCAAGCAAAAAGTTTGTCCACAGAGACTTGGCTGCAAGAAACTGTATGCTGGATGAAAAATTCACAGTCAAGGTTGCTGATTTTGGTCTTGCCAGAGACATGTATGATAAAGAATACTATAGTGTACACAACAAAACAGGTGCAAAGCTGCCAGTGAAGTGGATGGCTTTGGAAAGTCTGCAAACTCAAAAGTTTACCACCAAGTCAGATGTGTGGTCCTTTGGCGTGCTCCTCTGGGAGCTGATGACAAGAGGAGCCCCACCTTATCCTGACGTAAACACCTTTGATATAACTGTTTACTTGTTGCAAGGGAGAAGACTCCTACAACCCGAATACTGCCCAGACCCCTTATATGAAGTAATGCTAAAATGCTGGCACCCTAAAGCCGAAATGCGCCCATCCTTTTCTGAACTGGTGTCCCGGATATCAGCGATCTTCTCTACTTTCATTGGG</t>
-  </si>
-  <si>
-    <t>YQLFEELGKGAFSVVRRCVKVLAGQEYAAKIINTKKLSARDHQKLEREARICRLLKHPNIVRLHDSISEEGHHYLIFDLVTGGELFEDIVAREYYSEADASHCIQQILEAVLHCHQMGVVHRDLKPENLLLASKLKGAAVKLADFGLAIEVEGEQQAWFGFAGTPGYLSPEVLRKDPYGKPVDLWACGVILYILLVGYPPFWDEDQHRLYLQIKAGAYDFPSPEWDTVTPEAKDLINKMLTINPSKRITAAEALKHPWISHRSTVASCMHRQETVDCLKKFNARRKLKGA</t>
-  </si>
-  <si>
-    <t>ENFQKVEKIGEGTYGVVYKARNKLTGEVVALKKIRLDTETEGVPSTAIREISLLKELNHPNIVKLLDVIHTENKLYLVFEFLHQDLKKFMDASALTGIPLPLIKSYLFQLLQGLAFCHSHRVLHRDLKPQNLLINTEGAIKLADFGLARAFGVPVRTYTHEVVTLWYRAPEILLGCKYYSTAVDIWSLGCIFAEMVTRRALFPGDSEIDQLFRIFRTLGTPDEVVWPGVTSMPDYKPSFPKWARQDFSKVVPPLDEDGRSLLSQMLHYDPNKRISAKAALAHPFFQDVTKPVPHL</t>
-  </si>
-  <si>
-    <t>TTK_HUMAN_D0_3H9F_A</t>
-  </si>
-  <si>
-    <t>SVKGRIYSILKQIGSGGSSKVFQVLNEKKQIYAIKYVNLEEADNQTLDSYRNEIAYLNKLQQHSDKIIRLYDYEITDQYIYMVMECGNIDLNSWLKKKKSIDPWERKSYWKNMLEAVHTIHQHGIVHSDLKPANFLIVDGMLKLIDFGIANQMQPDTTSVVKDSQVGTVNYMPPEAIKDMSSSRENGKSKSKISPKSDVWSLGCILYYMTYGKTPFQQIINQISKLHAIIDPNHEIEFPDIPEKDLQDVLKCCLKRDPKQRISIPELLAHPYVQIQTHPVNQMAKGTTEE</t>
-  </si>
-  <si>
-    <t>GTGAAAGAATTCTTAGCCAAAGCCAAAGAAGATTTTCTTAAAAAATGGGAAAGTCCCGCTCAGAACACAGCCCACTTGGATCAGTTTGAACGAATCAAGACCCTCGGCACGGGCTCCTTCGGGCGGGTGATGCTGGTGAAACACAAGGAGACCGGGAACCACTATGCCATGAAGATCCTCGACAAACAGAAGGTGGTGAAACTGAAACAGATCGAACACACCCTGAATGAAAAGCGCATCCTGCAAGCTGTCAACTTTCCGTTCCTCGTCAAACTCGAGTTCTCCTTCAAGGACAACTCAAACTTATACATGGTCATGGAGTACGTGCCCGGCGGGGAGATGTTCTCACACCTACGGCGGATCGGAAGGTTCAGTGAGCCCCATGCCCGTTTCTACGCGGCCCAGATCGTCCTGACCTTTGAGTATCTGCACTCGCTGGATCTCATCTACAGGGACCTGAAGCCGGAGAATCTGCTCATTGACCAGCAGGGCTACATTCAGGTGACAGACTTCGGTTTCGCCAAGCGCGTGAAGGGCCGCACTTGGACCTTGTGCGGCACCCCTGAGTACCTGGCCCCTGAGATTATCCTGAGCAAAGGCTACAACAAGGCCGTGGACTGGTGGGCCCTGGGGGTTCTTATCTATGAAATGGCCGCTGGCTACCCGCCCTTCTTCGCAGACCAGCCCATCCAGATCTATGAGAAGATCGTCTCTGGGAAGGTGCGCTTCCCTTCCCACTTCAGCTCTGACTTGAAGGACCTGCTGCGGAACCTCCTGCAGGTAGATCTCACCAAGCGCTTTGGGAACCTCAAGAATGGGGTCAACGATATCAAGAACCACAAGTGGTTTGCCACAACTGACTGGATTGCCATCTACCAGAGGAAGGTGGAAGCTCCCTTCATACCAAAGTTTAAAGGCCCTGGGGATACGAGTAACTTTGACGACTATGAGGAAGAAGAAATCCGGGTCTCCATCAATGAGAAGTGTGGCAAGGAGTTTTCTGAGTTT</t>
-  </si>
-  <si>
-    <t>TCCCCCAACTACGACAAGTGGGAGATGGAACGCACGGACATCACCATGAAGCACAAGCTGGGCGGGGGCCAGTACGGGGAGGTGTACGAGGGCGTGTGGAAGAAATACAGCCTGACGGTGGCCGTGAAGACCTTGAAGGAGGACACCATGGAGGTGGAAGAGTTCTTGAAAGAAGCTGCAGTCATGAAAGAGATCAAACACCCTAACCTGGTGCAGCTCCTTGGGGTCTGCACCCGGGAGCCCCCGTTCTATATCATCACTGAGTTCATGACCTACGGGAACCTCCTGGACTACCTGAGGGAGTGCAACCGGCAGGAGGTGAACGCCGTGGTGCTGCTGTACATGGCCACTCAGATCTCGTCAGCCATGGAGTACCTGGAGAAGAAAAACTTCATCCACAGAGATCTTGCTGCCCGAAACTGCCTGGTAGGGGAGAACCACTTGGTGAAGGTAGCTGATTTTGGCCTGAGCAGGTTGATGACAGGGGACACCTACACAGCCCATGCTGGAGCCAAGTTCCCCATCAAATGGACTGCACCCGAGAGCCTGGCCTACAACAAGTTCTCCATCAAGTCCGACGTCTGGGCATTTGGAGTATTGCTTTGGGAAATTGCTACCTATGGCATGTCCCCTTACCCGGGAATTGACCTGTCCCAGGTGTATGAGCTGCTAGAGAAGGACTACCGCATGGAGCGCCCAGAAGGCTGCCCAGAGAAGGTCTATGAACTCATGCGAGCATGTTGGCAGTGGAATCCCTCTGACCGGCCCTCCTTTGCTGAAATCCACCAAGCCTTTGAAACAATGTTCCAGGAATCCAGTATCTCAGACGAAGTGGAAAAGGAGCTGGGGAAA</t>
-  </si>
-  <si>
-    <t>MK01_HUMAN_D0_4FMQ_A</t>
-  </si>
-  <si>
-    <t>KS6A1_HUMAN_D1_3RNY_B</t>
-  </si>
-  <si>
-    <t>ACCGACAGCTTCTCGGGCAGGTTTGAAGACGTCTACCAGCTGCAGGAAGATGTGCTGGGGGAGGGCGCTCATGCCCGAGTGCAGACCTGCATCAACCTGATCACCAGCCAGGAGTACGCCGTCAAGATCATTGAGAAGCAGCCAGGCCACATTCGGAGCAGGGTTTTCAGGGAGGTGGAGATGCTGTACCAGTGCCAGGGACACAGGAACGTCCTAGAGCTGATTGAGTTCTTCGAGGAGGAGGACCGCTTCTACCTGGTGTTTGAGAAGATGCGGGGAGGCTCCATCCTGAGCCACATCCACAAGCGCCGGCACTTCAACGAGCTGGAGGCCAGCGTGGTGGTGCAGGACGTGGCCAGCGCCTTGGACTTTCTGCATAACAAAGGCATCGCCCACAGGGACCTAAAGCCGGAAAACATCCTCTGTGAGCACCCCAACCAGGTCTCCCCCGTGAAGATCTGTGACTTCGACCTGGGCAGCGGCATCAAACTCAACGGGGACTGCTCCCCTATCTCCACCCCGGAGCTGCTCACTCCGTGCGGCTCGGCGGAGTACATGGCCCCGGAGGTAGTGGAGGCCTTCAGCGAGGAGGCTAGCATCTACGACAAGCGCTGCGACCTGTGGAGCCTGGGCGTCATCTTGTATATCCTACTCAGCGGCTACCCGCCCTTCGTGGGCCGCTGTGGCAGCGACTGCGGCTGGGACCGCGGCGAGGCCTGCCCTGCCTGCCAGAACATGCTGTTTGAGAGCATCCAGGAGGGCAAGTACGAGTTCCCCGACAAGGACTGGGCCCACATCTCCTGCGCTGCCAAAGACCTCATCTCCAAGCTGCTGGTCCGTGACGCCAAGCAGAGGCTGAGTGCCGCCCAAGTCCTGCAGCACCCCTGGGTTCAGGGGTGCGCCCCGGAGAACACCTTGCCCACTCCCATGGTCCTGCAGAGG</t>
-  </si>
-  <si>
-    <t>MSRSKRDNNFYSVEIGDSTFTVLKRYQNLKPIGSGAQGIVCAAYDAILERNVAIKKLSRPFQNQTHAKRAYRELVLMKCVNHKNIIGLLNVFTPQKSLEEFQDVYIVMELMDANLCQVIQMELDHERMSYLLYQMLCGIKHLHSAGIIHRDLKPSNIVVKSDCTLKILDFGLARTAGTSFMMTPYVVTRYYRAPEVILGMGYKENVDLWSVGCIMGEMVCHKILFPGRDYIDQWNKVIEQLGTPCPEFMKKLQPTVRTYVENRPKYAGYSFEKLFPDVLFPADSEHNKLKASQARDLLSKMLVIDASKRISVDEALQHPYINVWYDPSEAEAPPPKIPDKQLDEREHTIEEWKELIYKEVMDLE</t>
-  </si>
-  <si>
-    <t>STRAA_HUMAN_D0_3GNI_B</t>
-  </si>
-  <si>
-    <t>MP2K2_HUMAN_D0_1S9I_A</t>
-  </si>
-  <si>
-    <t>PIM1_HUMAN_D0_4A7C_A</t>
-  </si>
-  <si>
-    <t>EAFLTQKAKVGELKDDDFERISELGAGNGGVVTKVQHRPSGLIMARKLIHLEIKPAIRNQIIRELQVLHECNSPYIVGFYGAFYSDGEISICMEHMDGGSLDQVLKEAKRIPEEILGKVSIAVLRGLAYLREKHQIMHRDVKPSNILVNSRGEIKLCDFGVSGQLIDSMANSFVGTRSYMAPERLQGTHYSVQSDIWSMGLSLVELAVGRYPIPPPDAKELEAIFGRPVVDGEEGEPHSISPRPRPPGRPVSGHGMDSRPAMAIFELLDYIVNEPPPKLPNGVFTPDFQEFVNKCLIKNPAERADLKMLTNHTFIKRSEVEEVDFAGWLCKTLRLNQPGTPTRTAV</t>
-  </si>
-  <si>
-    <t>GGGCCGGAGGATGAGCTGCCCGACTGGGCCGCCGCCAAAGAGTTTTACCAGAAGTACGACCCTAAGGACGTCATCGGCAGAGGAGTGAGCTCTGTGGTCCGCCGTTGTGTTCATCGAGCTACTGGCCACGAGTTTGCGGTGAAGATTATGGAAGTGACAGCTGAGCGGCTGAGTCCTGAGCAGCTGGAGGAGGTGCGGGAAGCCACACGGCGAGAGACACACATCCTTCGCCAGGTCGCCGGCCACCCCCACATCATCACCCTCATCGATTCCTACGAGTCTTCTAGCTTCATGTTCCTGGTGTTTGACCTGATGCGGAAGGGAGAGCTGTTTGACTATCTCACAGAGAAGGTGGCCCTCTCTGAAAAGGAAACCAGGTCCATCATGCGGTCTCTGCTGGAAGCAGTGAGCTTTCTCCATGCCAACAACATTGTGCATCGAGATCTGAAGCCCGAGAATATTCTCCTAGATGACAATATGCAGATCCGACTTTCAGATTTCGGGTTCTCCTGCCACTTGGAACCTGGCGAGAAGCTTCGAGAGTTGTGTGGGACCCCAGGGTATCTAGCGCCAGAGATCCTTAAATGCTCCATGGATGAAACCCACCCAGGCTATGGCAAGGAGGTCGACCTCTGGGCCTGTGGGGTGATCTTGTTCACACTCCTGGCTGGCTCGCCACCCTTCTGGCACCGGCGGCAGATCCTGATGTTACGCATGATCATGGAGGGCCAGTACCAGTTCAGTTCCCCCGAGTGGGATGACCGTTCCAGCACTGTCAAAGACCTGATCTCCAGGCTGCTGCAGGTGGATCCTGAGGCACGCCTGACAGCTGAGCAGGCCCTACAGCACCCCTTCTTTGAGCGT</t>
-  </si>
-  <si>
-    <t>KC1E_HUMAN_D0_4HNI_A</t>
-  </si>
-  <si>
-    <t>VRK2_HUMAN_D0_2V62_B</t>
-  </si>
-  <si>
-    <t>ETYIKLDKLGEGTYATVYKGKSKLTDNLVALKEIRLEHEEGAPCTAIREVSLLKDLKHANIVTLHDIIHTEKSLTLVFEYLDKDLKQYLDDCGNIINMHNVKLFLFQLLRGLAYCHRQKVLHRDLKPQNLLINERGELKLADFGLARAKSIPTKTYSNEVVTLWYRPPDILLGSTDYSTQIDMWGVGCIFYEMATGRPLFPGSTVEEQLHFIFRILGTPTEETWPGILSNEEFKTYNYPKYRAEALLSHAPRLDSDGADLLTKLLQFEGRNRISAEDAMKHPFFLSLGERIHKLPDTTSIFALKEIQLQKEASLRS</t>
-  </si>
-  <si>
-    <t>HQLQPRRVSFRGEASETLQSPGYDPSRPESFFQQSFQRLSRLGHGSYGEVFKVRSKEDGRLYAVKRSMSPFRGPKDRARKLAEVGSHEKVGQHPCCVRLEQAWEEGGILYLQTELCGPSLQQHCEAWGASLPEAQVWGYLRDTLLALAHLHSQGLVHLDVKPANIFLGPRGRCKLGDFGLLVELGTAGAGEVQEGDPRYMAPELLQGSYGTAADVFSLGLTILEVACNMELPHGGEGWQQLRQGYLPPEFTAGLSSELRSVLVMMLEPDPKLRATAEALLALPVLRQP</t>
-  </si>
-  <si>
-    <t>aa_end</t>
-  </si>
-  <si>
-    <t>TACCAGCTCTTCGAGGAATTGGGCAAGGGAGCCTTCTCGGTGGTGCGAAGGTGTGTGAAGGTGCTGGCTGGCCAGGAGTATGCTGCCAAGATCATCAACACAAAGAAGCTGTCAGCCAGAGACCATCAGAAGCTGGAGCGTGAAGCCCGCATCTGCCGCCTGCTGAAGCACCCCAACATCGTCCGACTACATGACAGCATCTCAGAGGAGGGACACCACTACCTGATCTTCGACCTGGTCACTGGTGGGGAACTGTTTGAAGATATCGTGGCCCGGGAGTATTACAGTGAGGCGGATGCCAGTCACTGTATCCAGCAGATCCTGGAGGCTGTGCTGCACTGCCACCAGATGGGGGTGGTGCACCGGGACCTGAAGCCTGAGAATCTGTTGCTGGCCTCCAAGCTCAAGGGTGCCGCAGTGAAGCTGGCAGACTTTGGCCTGGCCATAGAGGTGGAGGGGGAGCAGCAGGCATGGTTTGGGTTTGCAGGGACTCCTGGATATCTCTCCCCAGAAGTGCTGCGGAAGGACCCGTACGGGAAGCCTGTGGACCTGTGGGCTTGTGGGGTCATCCTGTACATCCTGCTGGTTGGGTACCCCCCGTTCTGGGATGAGGACCAGCACCGCCTGTACCTGCAGATCAAAGCCGGCGCCTATGATTTCCCATCGCCGGAATGGGACACTGTCACCCCGGAAGCCAAGGATCTGATCAATAAGATGCTGACCATTAACCCATCCAAACGCATCACAGCTGCCGAAGCCCTTAAGCACCCCTGGATCTCGCACCGCTCCACCGTGGCATCCTGCATGCACAGACAGGAGACCGTGGACTGCCTGAAGAAGTTCAATGCCAGGAGGAAACTGAAGGGAGCC</t>
-  </si>
-  <si>
-    <t>MK08_HUMAN_D0_2NO3_A</t>
-  </si>
-  <si>
-    <t>TCGGTTAAAGGAAGAATTTATTCCATATTAAAGCAGATAGGAAGTGGAGGTTCAAGCAAGGTATTTCAGGTGTTAAATGAAAAGAAACAGATATATGCTATAAAATATGTGAACTTAGAAGAAGCAGATAACCAAACTCTTGATAGTTACCGGAACGAAATAGCTTATTTGAATAAACTACAACAACACAGTGATAAGATCATCCGACTTTATGATTATGAAATCACGGACCAGTACATCTACATGGTAATGGAGTGTGGAAATATTGATCTTAATAGTTGGCTTAAAAAGAAAAAATCCATTGATCCATGGGAACGCAAGAGTTACTGGAAAAATATGTTAGAGGCAGTTCACACAATCCATCAACATGGCATTGTTCACAGTGATCTTAAACCAGCTAACTTTCTGATAGTTGATGGAATGCTAAAGCTAATTGATTTTGGGATTGCAAACCAAATGCAACCAGATACAACAAGTGTTGTTAAAGATTCTCAGGTTGGCACAGTTAATTATATGCCACCAGAAGCAATCAAAGATATGTCTTCCTCCAGAGAGAATGGGAAATCTAAGTCAAAGATAAGCCCCAAAAGTGATGTTTGGTCCTTAGGATGTATTTTGTACTATATGACTTACGGGAAAACACCATTTCAGCAGATAATTAATCAGATTTCTAAATTACATGCCATAATTGATCCTAATCATGAAATTGAATTTCCCGATATTCCAGAGAAAGATCTTCAAGATGTGTTAAAGTGTTGTTTAAAAAGGGACCCAAAACAGAGGATATCCATTCCTGAGCTCCTGGCTCATCCATATGTTCAAATTCAAACTCATCCAGTTAACCAAATGGCCAAGGGAACCACTGAAGAA</t>
-  </si>
-  <si>
-    <t>PAK1_HUMAN_D0_3Q52_A</t>
-  </si>
-  <si>
-    <t>CDK9_HUMAN_D0_4IMY_A</t>
-  </si>
-  <si>
-    <t>GAAACAAAGTATACTGTGGACAAGAGGTTTGGCATGGATTTTAAAGAAATAGAATTAATTGGCTCAGGTGGATTTGGCCAAGTTTTCAAAGCAAAACACAGAATTGACGGAAAGACTTACGTTATTAAACGTGTTAAATATAATAACGAGAAGGCGGAGCGTGAAGTAAAAGCATTGGCAAAACTTGATCATGTAAATATTGTTCACTACAATGGCTGTTGGGATGGATTTGATTATGATCCTGAGACCAGTGATGATTCTCTTGAGAGCAGTGATTATGATCCTGAGAACAGCAAAAATAGTTCAAGGTCAAAGACTAAGTGCCTTTTCATCCAAATGGAATTCTGTGATAAAGGGACCTTGGAACAATGGATTGAAAAAAGAAGAGGCGAGAAACTAGACAAAGTTTTGGCTTTGGAACTCTTTGAACAAATAACAAAAGGGGTGGATTATATACATTCAAAAAAATTAATTCATAGAGATCTTAAGCCAAGTAATATATTCTTAGTAGATACAAAACAAGTAAAGATTGGAGACTTTGGACTTGTAACATCTCTGAAAAATGATGGAAAGCGAACAAGGAGTAAGGGAACTTTGCGATACATGAGCCCAGAACAGATTTCTTCGCAAGACTATGGAAAGGAAGTGGACCTCTACGCTTTGGGGCTAATTCTTGCTGAACTTCTTCATGTATGTGACACTGCTTTTGAAACATCAAAGTTTTTCACAGACCTACGGGATGGCATCATCTCAGATATATTTGATAAAAAAGAAAAAACTCTTCTACAGAAATTACTCTCAAAGAAACCTGAGGATCGACCTAACACATCTGAAATACTAAGGACCTTGACTGTGTGGAAGAAAAGCCCAGAGAAAAATGAACGACACACATGT</t>
-  </si>
-  <si>
-    <t>PAK7_HUMAN_D0_2F57_B</t>
-  </si>
-  <si>
-    <t>RDSSDDWEIPDGQITVGQRIGSGSFGTVYKGKWHGDVAVKMLNVTAPTPQQLQAFKNEVGVLRKTRHVNILLFMGYSTKPQLAIVTQWCEGSSLYHHLHIIETKFEMIKLIDIARQTAQGMDYLHAKSIIHRDLKSNNIFLHEDLTVKIGDFGLATVKSRWSGSHQFEQLSGSILWMAPEVIRMQDKNPYSFQSDVYAFGIVLYELMTGQLPYSNINNRDQIIFMVGRGYLSPDLSKVRSNCPKAMKRLMAECLKKKRDERPLFPQILASIELLAR</t>
-  </si>
-  <si>
-    <t>GAGAACTTCCAAAAGGTGGAAAAGATCGGAGAGGGCACGTACGGAGTTGTGTACAAAGCCAGAAACAAGTTGACGGGAGAGGTGGTGGCGCTTAAGAAAATCCGCCTGGACACTGAGACTGAGGGTGTGCCCAGTACTGCCATCCGAGAGATCTCTCTGCTTAAGGAGCTTAACCATCCTAATATTGTCAAGCTGCTGGATGTCATTCACACAGAAAATAAACTCTACCTGGTTTTTGAATTTCTGCACCAAGATCTCAAGAAATTCATGGATGCCTCTGCTCTCACTGGCATTCCTCTTCCCCTCATCAAGAGCTATCTGTTCCAGCTGCTCCAGGGCCTAGCTTTCTGCCATTCTCATCGGGTCCTCCACCGAGACCTTAAACCTCAGAATCTGCTTATTAACACAGAGGGGGCCATCAAGCTAGCAGACTTTGGACTAGCCAGAGCTTTTGGAGTCCCTGTTCGTACTTACACCCATGAGGTGGTGACCCTGTGGTACCGAGCTCCTGAAATCCTCCTGGGCTGCAAATATTATTCCACAGCTGTGGACATCTGGAGCCTGGGCTGCATCTTTGCTGAGATGGTGACTCGCCGGGCCCTATTCCCTGGAGATTCTGAGATTGACCAGCTCTTCCGGATCTTTCGGACTCTGGGGACCCCAGATGAGGTGGTGTGGCCAGGAGTTACTTCTATGCCTGATTACAAGCCAAGTTTCCCCAAGTGGGCCCGGCAAGATTTTAGTAAAGTTGTACCTCCCCTGGATGAAGATGGACGGAGCTTGTTATCGCAAATGCTGCACTACGACCCTAACAAGCGGATTTCGGCCAAGGCAGCCCTGGCTCACCCTTTCTTCCAGGATGTGACCAAGCCAGTACCCCATCTT</t>
-  </si>
-  <si>
-    <t>GGGGAATGCAGTCAGAAGGGTCCTGTCCCCTTTAGCCATTGCCTTCCCACAGAAAAACTGCAACGCTGTGAGAAGATTGGGGAAGGGGTGTTTGGCGAAGTGTTTCAAACAATTGCTGATCACACACCCGTAGCCATAAAAATCATTGCTATTGAAGGACCAGATTTAGTCAATGGATCCCATCAGAAAACCTTTGAGGAAATCCTGCCAGAGATCATCATCTCCAAAGAGTTGAGCCTCTTATCCGGTGAAGTGTGCAACCGCACAGAAGGCTTTATCGGGCTGAACTCAGTGCACTGTGTCCAGGGATCTTACCCTCCCTTGCTCCTCAAAGCCTGGGATCACTATAATTCAACCAAAGGCTCTGCAAATGACCGGCCTGATTTTTTTAAAGACGACCAGCTCTTCATTGTGCTGGAATTTGAGTTTGGAGGGATTGACTTAGAGCAAATGCGAACCAAGTTGTCTTCCTTGGCTACTGCAAAGAGCATTCTACACCAGCTCACAGCCTCCCTCGCAGTGGCAGAGGCATCACTGCGCTTTGAGCACCGAGACTTACACTGGGGGAACGTGCTCTTAAAGAAAACCAGCCTCAAAAAACTCCACTACACCCTCAATGGGAAGAGCAGCACTATCCCCAGCTGTGGGTTGCAAGTGAGCATCATTGACTACACCCTGTCGCGCTTGGAACGGGATGGGATTGTGGTTTTCTGTGACGTTTCCATGGATGAGGACCTGTTTACCGGTGACGGTGACTACCAGTTTGACATCTACAGGCTCATGAAGAAGGAGAATAACAACCGCTGGGGTGAATATCACCCTTATAGTAATGTGCTCTGGTTACATTACCTGACAGACAAGATGCTGAAACAAATGACCTTCAAGACTAAATGTAACACTCCTGCCATGAAGCAAATTAAGAGAAAAATCCAGGAGTTCCACAGGACAATGCTGAACTTCAGCTCTGCCACTGACTTGCTCTGCCAGCACAGACTGTTTAAG</t>
-  </si>
-  <si>
-    <t>TDSLPGKFEDMYKLTSELLGEGAYAKVQGAVSLQNGKEYAVKIIEKQAGHSRSRVFREVETLYQCQGNKNILELIEFFEDDTRFYLVFEKLQGGSILAHIQKQKHFNEREASRVVRDVAAALDFLHTKDKVSLCHLGGSARAPSGLTAAPTSLGSSDPPTSASQVAGTTGIDHRDLKPENILCESPEKVSPVKICDFDLGSGMKLNNSCTPITTPELTTPCGSAEYMAPEVGEVFTDQATFYDKRCDLWSLGVVLYIMLSGYPPFVGHCGADCGWDRGEVCRVCQNKLFESIQEGKYEFPDKDWAHISSEAKDLISKLLVRDAKQRLSAAQVLQHPWVQGQAPEKG</t>
-  </si>
-  <si>
-    <t>VRK3_HUMAN_D0_2JII_A</t>
-  </si>
-  <si>
-    <t>ATGAGCCTCATCCGGAAAAAGGGCTTCTACAAGCAGGACGTCAACAAGACCGCCTGGGAGCTGCCCAAGACCTACGTGTCCCCGACGCACGTCGGCAGCGGGGCCTATGGCTCCGTGTGCTCGGCCATCGACAAGCGGTCAGGGGAGAAGGTGGCCATCAAGAAGCTGAGCCGACCCTTTCAGTCCGAGATCTTCGCCAAGCGCGCCTACCGGGAGCTGCTGCTGCTGAAGCACATGCAGCATGAGAACGTCATTGGGCTCCTGGATGTCTTCACCCCAGCCTCCTCCCTGCGCAACTTCTATGACTTCTACCTGGTGATGCCCTTCATGCAGACGGATCTGCAGAAGATCATGGGGATGGAGTTCAGTGAGGAGAAGATCCAGTACCTGGTGTATCAGATGCTCAAAGGCCTTAAGTACATCCACTCTGCTGGGGTCGTGCACAGGGACCTGAAGCCAGGCAACCTGGCTGTGAATGAGGACTGTGAACTGAAGATTCTGGATTTTGGGCTGGCGCGACATGCAGACGCCGAGATGACTGGCTACGTGGTGACCCGCTGGTACCGAGCCCCCGAGGTGATCCTCAGCTGGATGCACTACAACCAGACAGTGGACATCTGGTCTGTGGTCTGTATCATGGCAGAGATGCTGACAGGGAAAACTCTGTTCAAGGGGAAAGATTACCTGGACCAGCTGACCCAGATCCTGAAAGTGACCGGGGTGCCTGGCACGGAGTTTGTGCAGAAGCTGAACGACAAAGCGGCCAAATCCTACATCCAGTCCCTGCCACAGACCCCCAGGAAGGATTTCACTCAGCTGTTCCCACGGGCCAGCCCCCAGGCTGCGGACCTGCTGGAGAAGATGCTGGAGCTAGACGTGGACAAGCGCCTGACGGCCGCGCAGGCCCTCACCCATCCCTTCTTTGAACCCTTCCGGGACCCTGAGGAAGAGACGGAGGCCCAGCAGCCGTTTGATGATTCCTTAGAACACGAGAAACTCACAGTGGATGAATGGAAGCAGCACATCTACAAGGAGATTGTGAACTTCAGCCCCATT</t>
-  </si>
-  <si>
-    <t>ACTGACTCCTTGCCAGGAAAGTTTGAAGATATGTACAAGCTGACCTCTGAATTGCTGGGAGAGGGAGCCTATGCCAAAGTTCAAGGTGCCGTGAGCCTACAGAATGGCAAAGAGTATGCCGTCAAAATCATCGAGAAACAAGCAGGGCACAGTCGGAGTAGGGTGTTTCGAGAGGTGGAGACGCTGTATCAGTGTCAGGGAAACAAGAACATTTTGGAGCTGATTGAGTTCTTTGAAGATGACACAAGGTTTTACTTGGTCTTTGAGAAATTGCAAGGAGGTTCCATCTTAGCCCACATCCAGAAGCAAAAGCACTTCAATGAGCGAGAAGCCAGCCGAGTGGTGCGGGACGTTGCTGCTGCCCTTGACTTCCTGCATACCAAAGACAAAGTCTCTCTCTGTCACCTAGGCGGGAGTGCTAGGGCGCCATCAGGGCTCACTGCAGCCCCAACCTCCCTGGGCTCCAGTGATCCTCCCACCTCAGCCTCCCAAGTAGCTGGGACTACAGGCATTGATCATCGTGATCTGAAACCAGAAAATATATTGTGTGAATCTCCAGAAAAGGTGTCTCCAGTGAAAATCTGTGACTTTGACTTGGGCAGTGGGATGAAACTGAACAACTCCTGTACCCCCATAACCACACCAGAGCTGACCACCCCATGTGGCTCTGCAGAATACATGGCCCCTGAGGTAGGGGAGGTCTTCACGGACCAGGCCACATTCTACGACAAGCGCTGTGACCTGTGGAGCCTGGGCGTGGTCCTCTACATCATGCTGAGTGGCTACCCACCCTTCGTGGGTCACTGCGGGGCCGACTGTGGCTGGGACCGGGGCGAGGTCTGCAGGGTGTGCCAGAACAAGCTGTTTGAAAGCATCCAGGAAGGCAAGTATGAGTTTCCTGACAAGGACTGGGCACACATCTCCAGTGAAGCCAAAGACCTCATCTCCAAGCTCCTGGTGCGAGATGCAAAGCAGAGACTTAGCGCCGCCCAAGTTCTGCAGCACCCATGGGTGCAGGGGCAAGCTCCAGAAAAGGGA</t>
-  </si>
-  <si>
-    <t>PAK4_HUMAN_D0_2J0I_A</t>
-  </si>
-  <si>
-    <t>AGVSEYELPEDPRWELPRDRLVLGKPLGEGCFGQVVLAEAIGLDKDKPNRVTKVAVKMLKSDATEKDLSDLISEMEMMKMIGKHKNIINLLGACTQDGPLYVIVEYASKGNLREYLQARRPPGLEYCYNPSHNPEEQLSSKDLVSCAYQVARGMEYLASKKCIHRDLAARNVLVTEDNVMKIADFGLARDIHHIDYYKKTTNGRLPVKWMAPEALFDRIYTHQSDVWSFGVLLWEIFTLGGSPYPGVPVEELFKLLKEGHRMDKPSNCTNELYMMMRDCWHAVPSQRPTFKQLVEDLDRIVALTSNQEYLDLSMPLD</t>
-  </si>
-  <si>
-    <t>MAAAAAQGGGGGEPRRTEGVGPGVPGEVEMVKGQPFDVGPRYTQLQYIGEGAYGMVSSAYDHVRKTRVAIKKISPFEHQTYCQRTLREIQILLRFRHENVIGIRDILRASTLEAMRDVYIVQDLMETDLYKLLKSQQLSNDHICYFLYQILRGLKYIHSANVLHRDLKPSNLLINTTCDLKICDFGLARIADPEHDHTGFLTEYVATRWYRAPEIMLNSKGYTKSIDIWSVGCILAEMLSNRPIFPGKHYLDQLNHILGILGSPSQEDLNCIINMKARNYLQSLPSKTKVAWAKLFPKSDSKALDLLDRMLTFNPNKRITVEEALAHPYLEQYYDPTDEPVAEEPFTFAMELDDLPKERLKELIFQETARFQPGVLEAP</t>
-  </si>
-  <si>
-    <t>GAGCCCAAGAAGTACGCAGTGACCGACGACTACCAGTTGTCCAAGCAGGTGCTGGGCCTGGGTGTGAACGGCAAAGTGCTGGAGTGCTTCCATCGGCGCACTGGACAGAAGTGTGCCCTGAAGCTCCTGTATGACAGCCCCAAGGCCCGGCAGGAGGTAGACCATCACTGGCAGGCTTCTGGCGGCCCCCATATTGTCTGCATCCTGGATGTGTATGAGAACATGCACCATGGCAAGCGCTGTCTCCTCATCATCATGGAATGCATGGAAGGTGGTGAGTTGTTCAGCAGGATTCAGGAGCGTGGCGACCAGGCTTTCACTGAGAGAGAAGCTGCAGAGATAATGCGGGATATTGGCACTGCCATCCAGTTTCTGCACAGCCATAACATTGCCCACCGAGATGTCAAGCCTGAAAACCTACTCTACACATCTAAGGAGAAAGACGCAGTGCTTAAGCTCACCGATTTTGGCTTTGCTAAGGAGACCACCCAAAATGCCCTGCAGACACCCTGCTATACTCCCTATTATGTGGCCCCTGAGGTCCTGGGTCCAGAGAAGTATGACAAGTCATGTGACATGTGGTCCCTGGGTGTCATCATGTACATCCTCCTTTGTGGCTTCCCACCCTTCTACTCCAACACGGGCCAGGCCATCTCCCCGGGGATGAAGAGGAGGATTCGCCTGGGCCAGTACGGCTTCCCCAATCCTGAGTGGTCAGAAGTCTCTGAGGATGCCAAGCAGCTGATCCGCCTCCTGTTGAAGACAGACCCCACAGAGAGGCTGACCATCACTCAGTTCATGAACCACCCCTGGATCAACCAATCGATGGTAGTGCCACAGACCCCACTCCACACGGCCCGAGTGCTGCAGGAGGACAAAGACCACTGGGACGAAGTCAAGGAGGAGATGACCAGTGCCTTGGCCACTATGCGGGTAGACTACGACCAGGTG</t>
-  </si>
-  <si>
-    <t>ATGTCTCAGGAGAGGCCCACGTTCTACCGGCAGGAGCTGAACAAGACAATCTGGGAGGTGCCCGAGCGTTACCAGAACCTGTCTCCAGTGGGCTCTGGCGCCTATGGCTCTGTGTGTGCTGCTTTTGACACAAAAACGGGGTTACGTGTGGCAGTGAAGAAGCTCTCCAGACCATTTCAGTCCATCATTCATGCGAAAAGAACCTACAGAGAACTGCGGTTACTTAAACATATGAAACATGAAAATGTGATTGGTCTGTTGGACGTTTTTACACCTGCAAGGTCTCTGGAGGAATTCAATGATGTGTATCTGGTGACCCATCTCATGGGGGCAGATCTGAACAACATTGTGAAATGTCAGAAGCTTACAGATGACCATGTTCAGTTCCTTATCTACCAAATTCTCCGAGGTCTAAAGTATATACATTCAGCTGACATAATTCACAGGGACCTAAAACCTAGTAATCTAGCTGTGAATGAAGACTGTGAGCTGAAGATTCTGGATTTTGGACTGGCTCGGCACACAGATGATGAAATGACAGGCTACGTGGCCACTAGGTGGTACAGGGCTCCTGAGATCATGCTGAACTGGATGCATTACAACCAGACAGTTGATATTTGGTCAGTGGGATGCATAATGGCCGAGCTGTTGACTGGAAGAACATTGTTTCCTGGTACAGACCATATTGATCAGTTGAAGCTCATTTTAAGACTCGTTGGAACCCCAGGGGCTGAGCTTTTGAAGAAAATCTCCTCAGAGTCTGCAAGAAACTATATTCAGTCTTTGACTCAGATGCCGAAGATGAACTTTGCGAATGTATTTATTGGTGCCAATCCCCTGGCTGTCGACTTGCTGGAGAAGATGCTTGTATTGGACTCAGATAAGAGAATTACAGCGGCCCAAGCCCTTGCACATGCCTACTTTGCTCAGTACCACGATCCTGATGATGAACCAGTGGCCGATCCTTATGATCAGTCCTTTGAAAGCAGGGACCTCCTTATAGATGAGTGGAAAAGCCTGACCTATGATGAAGTCATCAGCTTTGTGCCACCACCCCTTGACCAAGAAGAGATGGAGTCC</t>
-  </si>
-  <si>
-    <t>MK11_HUMAN_D0_3GC8_A</t>
-  </si>
-  <si>
-    <t>MK14_HUMAN_D0_3K3J_A</t>
-  </si>
-  <si>
-    <t>CDK16_HUMAN_D0_3MTL_A</t>
-  </si>
-  <si>
-    <t>PLK1_HUMAN_D0_2V5Q_A</t>
-  </si>
-  <si>
-    <t>NEK7_HUMAN_D0_2WQN_A</t>
-  </si>
-  <si>
-    <t>PAK6_HUMAN_D0_2C30_A</t>
-  </si>
-  <si>
-    <t>FGFR1_HUMAN_D0_3GQL_B</t>
-  </si>
-  <si>
-    <t>TCTTCGGTCACCGCCAGTGCGGCCCCGGGGACCGCGAGCCTCGTCCCGGATTACTGGATCGACGGCTCCAACAGGGATGCGCTGAGCGATTTCTTCGAGGTGGAGTCGGAGCTGGGACGGGGTGCTACATCCATTGTGTACAGATGCAAACAGAAGGGGACCCAGAAGCCTTATGCTCTCAAAGTGTTAAAGAAAACAGTGGACAAAAAAATCGTAAGAACTGAGATAGGAGTTCTTCTTCGCCTCTCACATCCAAACATTATAAAACTTAAAGAGATATTTGAAACCCCTACAGAAATCAGTCTGGTCCTAGAACTCGTCACAGGAGGAGAACTGTTTGATAGGATTGTGGAAAAGGGATATTACAGTGAGCGAGATGCTGCAGATGCCGTTAAACAAATCCTGGAGGCAGTTGCTTATCTACATGAAAATGGGATTGTCCATCGTGATCTCAAACCAGAGAATCTTCTTTATGCAACTCCAGCCCCAGATGCACCACTCAAAATCGCTGATTTTGGACTCTCTAAAATTGTGGAACATCAAGTGCTCATGAAGACAGTATGTGGAACCCCAGGGTACTGCGCACCTGAAATTCTTAGAGGTTGTGCCTATGGACCTGAGGTGGACATGTGGTCTGTAGGAATAATCACCTACATCTTACTTTGTGGATTTGAACCATTCTATGATGAAAGAGGCGATCAGTTCATGTTCAGGAGAATTCTGAATTGTGAATATTACTTTATCTCCCCCTGGTGGGATGAAGTATCTCTAAATGCCAAGGACTTGGTCAGAAAATTAATTGTTTTGGATCCAAAGAAACGGCTGACTACATTTCAAGCTCTCCAGCATCCGTGGGTCACAGGTAAAGCAGCCAATTTTGTACACATGGATACCGCTCAAAAGAAGCTCCAAGAATTCAATGCCCGGCGTAAGCTTAAGGCAGCGGTGAAGGCTGTGGTGGCCTCTTCCCGCCTGGGA</t>
-  </si>
-  <si>
-    <t>MEAAASEPSLDLDNLKLLELIGRGRYGAVYKGSLDERPVAVKVFSFANRQNFINEKNIYRVPLMEHDNIARFIVGDERVTADGRMEYLLVMEYYPNGSLCKYLSLHTSDWVSSCRLAHSVTRGLAYLHTELPRGDHYKPAISHRDLNSRNVLVKNDGTCVISDFGLSMRLTGNRLVRPGEEDNAAISEVGTIRYMAPEVLEGAVNLRDCESALKQVDMYALGLIYWEIFMRCTDLFPGESVPEYQMAFQTEVGNHPTFEDMQVLVSREKQRPKFPEAWKENSLAVRSLKETIEDCWDQDAEARLTAQCAEERMAELMMIWERNKSVSPT</t>
-  </si>
-  <si>
-    <t>GTCATCATTGACAATAAGCGCTACCTCTTCATCCAGAAACTGGGGGAGGGTGGGTTCAGCTATGTGGACCTAGTGGAAGGGTTACATGATGGACACTTCTACGCCCTGAAGCGAATCCTGTGTCACGAGCAGCAGGACCGGGAGGAGGCCCAGCGAGAAGCCGACATGCATCGCCTCTTCAATCACCCCAACATCCTTCGCCTCGTGGCTTACTGTCTGAGGGAACGGGGTGCTAAGCATGAGGCCTGGCTGCTGCTACCATTCTTCAAGAGAGGTACGCTGTGGAATGAGATAGAAAGGCTGAAGGACAAAGGCAACTTCCTGACCGAGGATCAAATCCTTTGGCTGCTGCTGGGGATCTGCAGAGGCCTTGAGGCCATTCATGCCAAGGGTTATGCCCACAGAGACTTGAAGCCCACCAATATATTGCTTGGAGATGAGGGGCAGCCAGTTTTAATGGACTTGGGTTCCATGAATCAAGCATGCATCCATGTGGAGGGCTCCCGCCAGGCTCTGACCCTGCAGGACTGGGCAGCCCAGCGGTGCACCATCTCCTACCGAGCCCCAGAGCTCTTCTCTGTGCAGAGTCACTGTGTCATCGATGAGCGGACTGATGTCTGGTCCCTAGGCTGCGTGCTATATGCCATGATGTTTGGGGAAGGCCCTTATGACATGGTGTTCCAAAAGGGTGACAGTGTGGCCCTTGCTGTGCAGAACCAACTCAGCATCCCACAAAGCCCCAGGCATTCTTCAGCATTGTGGCAGCTCCTGAACTCGATGATGACCGTGGACCCGCATCAGCGTCCTCACATTCCTCTCCTCCTCAGTCAGCTGGAGGCGCTGCAG</t>
-  </si>
-  <si>
-    <t>BMPR2_HUMAN_D0_3G2F_A</t>
-  </si>
-  <si>
-    <t>dna_start</t>
-  </si>
-  <si>
-    <t>PHKG2_HUMAN_D0_2Y7J_D</t>
-  </si>
-  <si>
-    <t>MAPK2_HUMAN_D0_2JBO_A</t>
-  </si>
-  <si>
-    <t>ATGGAGAAGGACGGCCTGTGCCGCGCTGACCAGCAGTACGAATGCGTGGCGGAGATCGGGGAGGGCGCCTATGGGAAGGTGTTCAAGGCCCGCGACTTGAAGAACGGAGGCCGTTTCGTGGCGTTGAAGCGCGTGCGGGTGCAGACCGGCGAGGAGGGCATGCCGCTCTCCACCATCCGCGAGGTGGCGGTGCTGAGGCACCTGGAGACCTTCGAGCACCCCAACGTGGTCAGGTTGTTTGATGTGTGCACAGTGTCACGAACAGACAGAGAAACCAAACTAACTTTAGTGTTTGAACATGTCGATCAAGACTTGACCACTTACTTGGATAAAGTTCCAGAGCCTGGAGTGCCCACTGAAACCATAAAGGATATGATGTTTCAGCTTCTCCGAGGTCTGGACTTTCTTCATTCACACCGAGTAGTGCATCGCGATCTAAAACCACAGAACATTCTGGTGACCAGCAGCGGACAAATAAAACTCGCTGACTTCGGCCTTGCCCGCATCTATAGTTTCCAGATGGCTCTAACCTCAGTGGTCGTCACGCTGTGGTACAGAGCACCCGAAGTCTTGCTCCAGTCCAGCTACGCCACCCCCGTGGATCTCTGGAGTGTTGGCTGCATATTTGCAGAAATGTTTCGTAGAAAGCCTCTTTTTCGTGGAAGTTCAGATGTTGATCAACTAGGAAAAATCTTGGACGTGATTGGACTCCCAGGAGAAGAAGACTGGCCTAGAGATGTTGCCCTTCCCAGGCAGGCTTTTCATTCAAAATCTGCCCAACCAATTGAGAAGTTTGTAACAGATATCGATGAACTAGGCAAAGACCTACTTCTGAAGTGTTTGACATTTAACCCAGCCAAAAGAATATCTGCCTACAGTGCCCTGTCTCACCCATACTTCCAG</t>
-  </si>
-  <si>
-    <t>ATGTCGGGCCCTCGCGCCGGCTTCTACCGGCAGGAGCTGAACAAGACCGTGTGGGAGGTGCCGCAGCGGCTGCAGGGGCTGCGCCCGGTGGGCTCCGGCGCCTACGGCTCCGTCTGTTCGGCCTACGACGCCCGGCTGCGCCAGAAGGTGGCGGTGAAGAAGCTGTCGCGCCCCTTCCAGTCGCTGATCCACGCGCGCAGAACGTACCGGGAGCTGCGGCTGCTCAAGCACCTGAAGCACGAGAACGTCATCGGGCTTCTGGACGTCTTCACGCCGGCCACGTCCATCGAGGACTTCAGCGAAGTGTACTTGGTGACCACCCTGATGGGCGCCGACCTGAACAACATCGTCAAGTGCCAGGCGCTGAGCGACGAGCACGTTCAATTCCTGGTTTACCAGCTGCTGCGCGGGCTGAAGTACATCCACTCGGCCGGGATCATCCACCGGGACCTGAAGCCCAGCAACGTGGCTGTGAACGAGGACTGTGAGCTCAGGATCCTGGATTTCGGGCTGGCGCGCCAGGCGGACGAGGAGATGACCGGCTATGTGGCCACGCGCTGGTACCGGGCACCTGAGATCATGCTCAACTGGATGCATTACAACCAAACAGTGGATATCTGGTCCGTGGGCTGCATCATGGCTGAGCTGCTCCAGGGCAAGGCCCTCTTCCCGGGAAGCGACTACATTGACCAGCTGAAGCGCATCATGGAAGTGGTGGGCACACCCAGCCCTGAGGTTCTGGCAAAAATCTCCTCGGAACACGCCCGGACATATATCCAGTCCCTGCCCCCCATGCCCCAGAAGGACCTGAGCAGCATCTTCCGTGGAGCCAACCCCCTGGCCATAGACCTCCTTGGAAGGATGCTGGTGCTGGACAGTGACCAGAGGGTCAGTGCAGCTGAGGCACTGGCCCACGCCTACTTCAGCCAGTACCACGACCCCGAGGATGAGCCAGAGGCCGAGCCATATGATGAGAGCGTTGAGGCCAAGGAGCGCACGCTGGAGGAGTGGAAGGAGCTCACTTACCAGGAAGTCCTCAGCTTCAAGCCCCCAGAGCCACCGAAGCCACCTGGCAGCCTGGAGATTGAGCAG</t>
+    <t>NLVFSDGYVVKETIGVGSYSECKRCVHKATNMEYAVKVIDKSKRDPSEEIEILLRYGQHPNIITLKDVYDDGKHVYLVTELMRGGELLDKILRQKFFSEREASFVLHTIGKTVEYLHSQGVVHRDLKPSNILYVDESGNPECLRICDFGFAKQLRAENGLLMTPCYTANFVAPEVLKRQGYDEGCDIWSLGILLYTMLAGYTPFANGPSDTPEEILTRIGSGKFTLSGGNWNTVSETAKDLVSKMLHVDPHQRLTAKQVLQHPWVTQKDKLPQSQLSHQDLQLVKGAMAATYSALNSSKPTPQLKPIESSILAQRRVRKLPSTTL</t>
+  </si>
+  <si>
+    <t>GGTGTTGTGACACATGAGCAGTTCAAGGCTGCGCTCAGGATGGTGGTGGACCAGGGTGACCCCCGGCTGCTGCTGGACAGCTACGTGAAGATTGGCGAGGGCTCCACCGGCATCGTCTGCTTGGCCCGGGAGAAGCACTCGGGCCGCCAGGTGGCCGTCAAGATGATGGACCTCAGGAAGCAGCAGCGCAGGGAGCTGCTCTTCAACGAGGTGGTGATCATGCGGGACTACCAGCACTTCAACGTGGTGGAGATGTACAAGAGCTACCTGGTGGGCGAGGAGCTGTGGGTGCTCATGGAGTTCCTGCAGGGAGGAGCCCTCACAGACATCGTCTCCCAAGTCAGGCTGAATGAGGAGCAGATTGCCACTGTGTGTGAGGCTGTGCTGCAGGCCCTGGCCTACCTGCATGCTCAGGGTGTCATCCACCGGGACATCAAGAGTGACTCCATCCTGCTGACCCTCGATGGCAGGGTGAAGCTCTCGGACTTCGGATTCTGTGCTCAGATCAGCAAAGACGTCCCTAAGAGGAAGTCCCTGGTGGGAACCCCCTACTGGATGGCTCCTGAAGTGATCTCCAGGTCTTTGTATGCCACTGAGGTGGATATCTGGTCTCTGGGCATCATGGTGATTGAGATGGTAGATGGGGAGCCACCGTACTTCAGTGACTCCCCAGTGCAAGCCATGAAGAGGCTCCGGGACAGCCCCCCACCCAAGCTGAAAAACTCTCACAAGGTCTCCCCAGTGCTGCGAGACTTCCTGGAGCGGATGCTGGTGCGGGACCCCCAAGAGAGAGCCACAGCCCAGGAGCTCCTAGACCACCCCTTCCTGCTGCAGACAGGGCTACCTGAGTGCCTGGTGCCCCTGATCCAGCTCTACCGAAAGCAGACCTCCACCTGC</t>
+  </si>
+  <si>
+    <t>CACATTGGAAACTACCGGCTCCTCAAGACCATTGGCAAGGGTAATTTTGCCAAGGTGAAGTTGGCCCGACACATCCTGACTGGGAAAGAGGTAGCTGTGAAGATCATTGACAAGACTCAACTGAACTCCTCCAGCCTCCAGAAACTATTCCGCGAAGTAAGAATAATGAAGGTTTTGAATCATCCCAACATAGTTAAATTATTTGAAGTGATTGAGACTGAGAAAACGCTCTACCTTGTCATGGAGTACGCTAGTGGCGGAGAGGTATTTGATTACCTAGTGGCTCATGGCAGGATGAAAGAAAAAGAGGCTCGAGCCAAATTCCGCCAGATAGTGTCTGCTGTGCAGTACTGTCACCAGAAGTTTATTGTCCATAGAGACTTAAAGGCAGAAAACCTGCTCTTGGATGCTGATATGAACATCAAGATTGCAGACTTTGGCTTCAGCAATGAATTCACCTTTGGGAACAAGCTGGACACCTTCTGTGGCAGTCCCCCTTATGCTGCCCCAGAACTCTTCCAGGGCAAAAAATATGATGGACCCGAGGTGGATGTGTGGAGCCTAGGAGTTATCCTCTATACACTGGTCAGCGGATCCCTGCCTTTTGATGGACAGAACCTCAAGGAGCTGCGGGAACGGGTACTGAGGGGAAAATACCGTATTCCATTCTACATGTCCACGGACTGTGAAAACCTGCTTAAGAAATTTCTCATTCTTAATCCCAGCAAGAGAGGCACTTTAGAGCAAATCATGAAAGATCGATGGATGAATGTGGGTCACGAAGATGATGAACTAAAGCCTTACGTGGAGCCACTCCCTGACTACAAGGACCCCCGGCGGACAGAGCTGATGGTGTCCATGGGTTATACACGGGAAGAGATCCAGGACTCGCTGGTGGGCCAGAGATACAACGAGGTGATGGCCACCTATCTGCTCCTGGGCTAC</t>
+  </si>
+  <si>
+    <t>ST17B_HUMAN_D0_3LM0_A</t>
+  </si>
+  <si>
+    <t>GDSDISSPLLQNTVHIDLSALNPELVQAVQHVVIGPSSLIVHFNEVIGRGHFGCVYHGTLLDNDGKKIHCAVKSLNRITDIGEVSQFLTEGIIMKDFSHPNVLSLLGICLRSEGSPLVVLPYMKHGDLRNFIRNETHNPTVKDLIGFGLQVAKGMKYLASKKFVHRDLAARNCMLDEKFTVKVADFGLARDMYDKEYYSVHNKTGAKLPVKWMALESLQTQKFTTKSDVWSFGVLLWELMTRGAPPYPDVNTFDITVYLLQGRRLLQPEYCPDPLYEVMLKCWHPKAEMRPSFSELVSRISAIFSTFIG</t>
+  </si>
+  <si>
+    <t>ATGAGTAGCTTTCTGCCAGAGGGAGGGTGTTACGAGCTGCTCACTGTGATAGGCAAAGGATTTGAGGACCTGATGACTGTGAATCTAGCAAGGTACAAACCAACAGGAGAGTACGTGACTGTACGGAGGATTAACCTAGAAGCTTGTTCCAATGAGATGGTAACATTCTTGCAGGGCGAGCTGCATGTCTCCAAACTCTTCAACCATCCCAATATCGTGCCATATCGAGCCACTTTTATTGCAGACAATGAGCTGTGGGTTGTCACATCATTCATGGCATACGGTTCTGCAAAAGATCTCATCTGTACACACTTCATGGATGGCATGAATGAGCTGGCGATTGCTTACATCCTGCAGGGGGTGCTGAAGGCCCTCGACTACATCCACCACATGGGATATGTACACAGGAGTGTCAAAGCCAGCCACATCCTGATCTCTGTGGATGGGAAGGTCTACCTGTCTGGTTTGCGCAGCAACCTCAGCATGATAAGCCATGGGCAGCGGCAGCGAGTGGTCCACGATTTTCCCAAGTACAGTGTCAAGGTTCTGCCGTGGCTCAGCCCCGAGGTCCTCCAGCAGAATCTCCAGGGTTATGATGCCAAGTCTGACATCTACAGTGTGGGAATCACAGCCTGTGAACTGGCCAACGGCCATGTCCCCTTTAAGGATATGCCTGCCACCCAGATGCTGCTAGAGAAACTGAACGGCACAGTGCCCTGCCTGTTGGATACCAGCACCATCCCCGCTGAGGAGCTGACCATGAGCCCTTCGCGCTCAGTGGCCAACTCTGGCCTGAGTGACAGCCTGACCACCAGCACCCCCCGGCCCTCCAACGGTGACTCGCCCTCCCACCCCTACCACCGAACCTTCTCCCCCCACTTCCACCACTTTGTGGAGCAGTGCCTTCAGCGCAACCCGGATGCCAGGCCCAGTGCCAGCACCCTCCTGAACCACTCTTTCTTCAAGCAGATCAAGCGACGTGCCTCAGAGGTTTTGCCCGAATTGCTTCGTCCTGTCACCCCCATCACCAATTTTGAGGGCAGCCAGTCTCAGGACCACAGTGGAATCTTTGGCCTGGTAACAAACCTGGAAGAGCTGGAGGTGGACGATTGGGAGTTC</t>
+  </si>
+  <si>
+    <t>ADPEELFTKLERIGKGSFGEVFKGIDNRTQQVVAIKIIDLEEAEDEIEDIQQEITVLSQCDSSYVTKYYGSYLKGSKLWIIMEYLGGGSALDLLRAGPFDEFQIATMLKEILKGLDYLHSEKKIHRDIKAANVLLSEQGDVKLADFGVAGQLTDTQIKRNTFVGTPFWMAPEVIQQSAYDSKADIWSLGITAIELAKGEPPNSDMHPMRVLFLIPKNNPPTLVGDFTKSFKEFIDACLNKDPSFRPTAKELLKHKFIVKNSKKTSYLTELIDRFKRWKAE</t>
+  </si>
+  <si>
+    <t>AURKA_HUMAN_D0_2NP8_A</t>
+  </si>
+  <si>
+    <t>HIGNYRLLKTIGKGNFAKVKLARHILTGKEVAVKIIDKTQLNSSSLQKLFREVRIMKVLNHPNIVKLFEVIETEKTLYLVMEYASGGEVFDYLVAHGRMKEKEARAKFRQIVSAVQYCHQKFIVHRDLKAENLLLDADMNIKIADFGFSNEFTFGNKLDTFCGSPPYAAPELFQGKKYDGPEVDVWSLGVILYTLVSGSLPFDGQNLKELRERVLRGKYRIPFYMSTDCENLLKKFLILNPSKRGTLEQIMKDRWMNVGHEDDELKPYVEPLPDYKDPRRTELMVSMGYTREEIQDSLVGQRYNEVMATYLLLGY</t>
+  </si>
+  <si>
+    <t>GVVTHEQFKAALRMVVDQGDPRLLLDSYVKIGEGSTGIVCLAREKHSGRQVAVKMMDLRKQQRRELLFNEVVIMRDYQHFNVVEMYKSYLVGEELWVLMEFLQGGALTDIVSQVRLNEEQIATVCEAVLQALAYLHAQGVIHRDIKSDSILLTLDGRVKLSDFGFCAQISKDVPKRKSLVGTPYWMAPEVISRSLYATEVDIWSLGIMVIEMVDGEPPYFSDSPVQAMKRLRDSPPPKLKNSHKVSPVLRDFLERMLVRDPQERATAQELLDHPFLLQTGLPECLVPLIQLYRKQTSTC</t>
+  </si>
+  <si>
+    <t>ATGGCAAAGCAGTACGACTCGGTGGAGTGCCCTTTTTGTGATGAAGTTTCCAAATACGAGAAGCTCGCCAAGATCGGCCAAGGCACCTTCGGGGAGGTGTTCAAGGCCAGGCACCGCAAGACCGGCCAGAAGGTGGCTCTGAAGAAGGTGCTGATGGAAAACGAGAAGGAGGGGTTCCCCATTACAGCCTTGCGGGAGATCAAGATCCTTCAGCTTCTAAAACACGAGAATGTGGTCAACTTGATTGAGATTTGTCGAACCAAAGCTTCCCCCTATAACCGCTGCAAGGGTAGTATATACCTGGTGTTCGACTTCTGCGAGCATGACCTTGCTGGGCTGTTGAGCAATGTTTTGGTCAAGTTCACGCTGTCTGAGATCAAGAGGGTGATGCAGATGCTGCTTAACGGCCTCTACTACATCCACAGAAACAAGATCCTGCATAGGGACATGAAGGCTGCTAATGTGCTTATCACTCGTGATGGGGTCCCGAAGCTGGCAGACTTTGGGCTGGCCCGGGCCTTCAGCCTGGCCAAGAACAGCCAGCCCAACCGCTACACCAACCGTGTGGTGACACTCTGGTACCGGCCCCCGGAGCTGTTGCTCGGGGAGCGGGACTACGGCCCCCCCATTGACCTGTGGGGTGCTGGGTGCATCATGGCAGAGATGTGGACCCGCAGCCCCATCATGCAGGGCAACACGGAGCAGCACCAACTCGCCCTCATCAGTCAGCTCTGCGGCTCCATCACCCCTGAGGTGTGGCCAAACGTGGACAACTATGAGCTGTACGAAAAGCTGGAGCTGGTCAAGGGCCAGAAGCGGAAGGTGAAGGACAGGCTGAAGGCCTATGTGCGTGACCCATACGCACTGGACCTCATCGACAAGCTGCTGGTGCTGGACCCTGCCCAGCGCATCGACAGCGATGACGCCCTCAACCACGACTTCTTCTGGTCCGACCCCATGCCCTCCGACCTCAAGGGCATGCTCTCCACC</t>
+  </si>
+  <si>
+    <t>MSQERPTFYRQELNKTIWEVPERYQNLSPVGSGAYGSVCAAFDTKTGLRVAVKKLSRPFQSIIHAKRTYRELRLLKHMKHENVIGLLDVFTPARSLEEFNDVYLVTHLMGADLNNIVKCQKLTDDHVQFLIYQILRGLKYIHSADIIHRDLKPSNLAVNEDCELKILDFGLARHTDDEMTGYVATRWYRAPEIMLNWMHYNQTVDIWSVGCIMAELLTGRTLFPGTDHIDQLKLILRLVGTPGAELLKKISSESARNYIQSLTQMPKMNFANVFIGANPLAVDLLEKMLVLDSDKRITAAQALAHAYFAQYHDPDDEPVADPYDQSFESRDLLIDEWKSLTYDEVISFVPPPLDQEEMES</t>
+  </si>
+  <si>
+    <t>MELRVGNRYRLGRKIGSGSFGDIYLGTDIAAGEEVAIKLECVKTKHPQLHIESKIYKMMQGGVGIPTIRWCGAEGDYNVMVMELLGPSLEDLFNFCSRKFSLKTVLLLADQMISRIEYIHSKNFIHRDVKPDNFLMGLGKKGNLVYIIDFGLAKKYRDARTHQHIPYRENKNLTGTARYASINTHLGIEQSRRDDLESLGYVLMYFNLGSLPWQGLKAATKRQKYERISEKKMSTPIEVLCKGYPSEFATYLNFCRSLRFDDKPDYSYLRQLFRNLFHRQGFSYDYVFDWNMLK</t>
+  </si>
+  <si>
+    <t>MAKQYDSVECPFCDEVSKYEKLAKIGQGTFGEVFKARHRKTGQKVALKKVLMENEKEGFPITALREIKILQLLKHENVVNLIEICRTKASPYNRCKGSIYLVFDFCEHDLAGLLSNVLVKFTLSEIKRVMQMLLNGLYYIHRNKILHRDMKAANVLITRDGVPKLADFGLARAFSLAKNSQPNRYTNRVVTLWYRPPELLLGERDYGPPIDLWGAGCIMAEMWTRSPIMQGNTEQHQLALISQLCGSITPEVWPNVDNYELYEKLELVKGQKRKVKDRLKAYVRDPYALDLIDKLLVLDPAQRIDSDDALNHDFFWSDPMPSDLKGMLST</t>
+  </si>
+  <si>
+    <t>targetID</t>
+  </si>
+  <si>
+    <t>TGGGCCCTGAACATGAAGGAGCTGAAGCTGCTGCAGACCATCGGGAAGGGGGAGTTCGGAGACGTGATGCTGGGCGATTACCGAGGGAACAAAGTCGCCGTCAAGTGCATTAAGAACGACGCCACTGCCCAGGCCTTCCTGGCTGAAGCCTCAGTCATGACGCAACTGCGGCATAGCAACCTGGTGCAGCTCCTGGGCGTGATCGTGGAGGAGAAGGGCGGGCTCTACATCGTCACTGAGTACATGGCCAAGGGGAGCCTTGTGGACTACCTGCGGTCTAGGGGTCGGTCAGTGCTGGGCGGAGACTGTCTCCTCAAGTTCTCGCTAGATGTCTGCGAGGCCATGGAATACCTGGAGGGCAACAATTTCGTGCATCGAGACCTGGCTGCCCGCAATGTGCTGGTGTCTGAGGACAACGTGGCCAAGGTCAGCGACTTTGGTCTCACCAAGGAGGCGTCCAGCACCCAGGACACGGGCAAGCTGCCAGTCAAGTGGACAGCCCCTGAGGCCCTGAGAGAGAAGAAATTCTCCACTAAGTCTGACGTGTGGAGTTTCGGAATCCTTCTCTGGGAAATCTACTCCTTTGGGCGAGTGCCTTATCCAAGAATTCCCCTGAAGGACGTCGTCCCTCGGGTGGAGAAGGGCTACAAGATGGATGCCCCCGACGGCTGCCCGCCCGCAGTCTATGAAGTCATGAAGAACTGCTGGCACCTGGACGCCGCCATGCGGCCCTCCTTCCTACAGCTCCGAGAGCAGCTTGAGCACATCAAAACCCACGAGCTGCACCTG</t>
+  </si>
+  <si>
+    <t>dna_seq</t>
+  </si>
+  <si>
+    <t>AACCTGGTTTTTAGTGACGGCTACGTGGTAAAGGAGACAATTGGTGTGGGCTCCTACTCTGAGTGCAAGCGCTGTGTCCACAAGGCCACCAACATGGAGTATGCTGTCAAGGTCATTGATAAGAGCAAGCGGGATCCTTCAGAAGAGATTGAGATTCTTCTGCGGTATGGCCAGCACCCCAACATCATCACTCTGAAAGATGTGTATGATGATGGCAAACACGTGTACCTGGTGACAGAGCTGATGCGGGGTGGGGAGCTGCTGGACAAGATCCTGCGGCAGAAGTTCTTCTCAGAGCGGGAGGCCAGCTTTGTCCTGCACACCATTGGCAAAACTGTGGAGTATCTGCACTCACAGGGGGTTGTGCACAGGGACCTGAAGCCCAGCAACATCCTGTATGTGGACGAGTCCGGGAATCCCGAGTGCCTGCGCATCTGTGACTTTGGTTTTGCCAAACAGCTGCGGGCTGAGAATGGGCTCCTCATGACACCTTGCTACACAGCCAACTTTGTGGCGCCTGAGGTGCTGAAGCGCCAGGGCTACGATGAAGGCTGCGACATCTGGAGCCTGGGCATTCTGCTGTACACCATGCTGGCAGGATATACTCCATTTGCCAACGGTCCCAGTGACACACCAGAGGAAATCCTAACCCGGATCGGCAGTGGGAAGTTTACCCTCAGTGGGGGAAATTGGAACACAGTTTCAGAGACAGCCAAGGACCTGGTGTCCAAGATGCTACACGTGGATCCCCACCAGCGCCTCACAGCTAAGCAGGTTCTGCAGCATCCATGGGTCACCCAGAAAGACAAGCTTCCCCAAAGCCAGCTGTCCCACCAGGACCTACAGCTTGTGAAGGGAGCCATGGCTGCCACGTACTCCGCACTCAACAGCTCCAAGCCCACCCCCCAGCTGAAGCCCATCGAGTCATCCATCCTGGCCCAGCGGCGAGTGAGGAAGTTGCCATCCACCACCCTG</t>
+  </si>
+  <si>
+    <t>ATGGCCGACGACGACGTGCTGTTCGAGGATGTGTACGAGCTGTGCGAGGTGATCGGAAAGGGTCCCTTCAGTGTTGTACGACGATGTATCAACAGAGAAACTGGGCAACAATTTGCTGTAAAAATTGTTGATGTAGCCAAGTTCACATCAAGTCCAGGGTTAAGTACAGAAGATCTAAAGCGGGAAGCCAGTATCTGTCATATGCTGAAACATCCACACATTGTAGAGTTATTGGAGACATATAGCTCAGATGGAATGCTTTACATGGTTTTCGAATTTATGGATGGAGCAGATCTGTGTTTTGAAATCGTAAAGCGAGCTGACGCTGGTTTTGTGTACAGTGAAGCTGTAGCCAGCCATTATATGAGACAGATACTGGAAGCTCTACGCTACTGCCATGATAATAACATAATTCACAGGGATGTGAAGCCCCACTGTGTTCTCCTTGCCTCAAAAGAAAACTCGGCACCTGTTAAACTTGGAGGCTTTGGGGTAGCTATTCAATTAGGGGAGTCTGGACTTGTAGCTGGAGGACGTGTTGGAACACCTCATTTTATGGCACCAGAAGTGGTCAAAAGAGAGCCTTACGGAAAGCCTGTAGACGTCTGGGGGTGCGGTGTGATCCTTTTTATCCTGCTCAGTGGTTGTTTGCCTTTTTACGGAACCAAGGAAAGATTGTTTGAAGGCATTATTAAAGGAAAATATAAGATGAATCCAAGGCAGTGGAGCCATATCTCTGAAAGTGCCAAAGACCTAGTACGTCGCATGCTGATGCTGGATCCAGCTGAAAGGATCACTGTTTATGAAGCACTGAATCACCCATGGCTTAAGGAGCGGGATCGTTACGCCTACAAGATTCATCTTCCAGAAACAGTAGAGCAGCTGAGGAAATTCAATGCAAGGAGGAAACTAAAGGGTGCAGTACTAGCCGCTGTGTCAAGTCACAAATTCAACTCATTCTATGGGGATCCCCCTGAAGAGTTACCAGATTTCTCCGAAGACCCTACCTCCTCAGGAGCA</t>
   </si>
   <si>
     <t>E2AK2_HUMAN_D0_3UIU_A</t>
   </si>
   <si>
-    <t>MEKYEKIGKIGEGSYGVVFKCRNRDTGQIVAIKKFLESEDDPVIKKIALREIRMLKQLKHPNLVNLLEVFRRKRRLHLVFEYCDHTVLHELDRYQRGVPEHLVKSITWQTLQAVNFCHKHNCIHRDVKPENILITKHSVIKLCDFGFARLLTGPSDYYTDYVATRWYRSPELLVGDTQYGPPVDVWAIGCVFAELLSGVPLWPGKSDVDQLYLIRKTLGDLIPRHQQVFSTNQYFSGVKIPDPEDMEPLELKFPNISYPALGLL</t>
-  </si>
-  <si>
-    <t>GeneID</t>
-  </si>
-  <si>
-    <t>BRAF_HUMAN_D0_4FK3_B</t>
-  </si>
-  <si>
-    <t>ATGGATGAGCAATCACAAGGAATGCAAGGGCCACCTGTTCCTCAGTTCCAACCACAGAAGGCCTTACGACCGGATATGGGCTATAATACATTAGCCAACTTTCGAATAGAAAAGAAAATTGGTCGCGGACAATTTAGTGAAGTTTATAGAGCAGCCTGTCTCTTGGATGGAGTACCAGTAGCTTTAAAAAAAGTGCAGATATTTGATTTAATGGATGCCAAAGCACGTGCTGATTGCATCAAAGAAATAGATCTTCTTAAGCAACTCAACCATCCAAATGTAATAAAATATTATGCATCATTCATTGAAGATAATGAACTAAACATAGTTTTGGAACTAGCAGATGCTGGCGACCTATCCAGAATGATCAAGCATTTTAAGAAGCAAAAGAGGCTAATTCCTGAAAGAACTGTTTGGAAGTATTTTGTTCAGCTTTGCAGTGCATTGGAACACATGCATTCTCGAAGAGTCATGCATAGAGATATAAAACCAGCTAATGTGTTCATTACAGCCACTGGGGTGGTAAAACTTGGAGATCTTGGGCTTGGCCGGTTTTTCAGCTCAAAAACCACAGCTGCACATTCTTTAGTTGGTACGCCTTATTACATGTCTCCAGAGAGAATACATGAAAATGGATACAACTTCAAATCTGACATCTGGTCTCTTGGCTGTCTACTATATGAGATGGCTGCATTACAAAGTCCTTTCTATGGTGACAAAATGAATTTATACTCACTGTGTAAGAAGATAGAACAGTGTGACTACCCACCTCTTCCTTCAGATCACTATTCAGAAGAACTCCGACAGTTAGTTAATATGTGCATCAACCCAGATCCAGAGAAGCGACCAGACGTCACCTATGTTTATGACGTAGCAAAGAGGATGCATGCATGCACTGCAAGCAGC</t>
-  </si>
-  <si>
-    <t>DAPK3_HUMAN_D0_2J90_A</t>
-  </si>
-  <si>
-    <t>VKEFLAKAKEDFLKKWESPAQNTAHLDQFERIKTLGTGSFGRVMLVKHKETGNHYAMKILDKQKVVKLKQIEHTLNEKRILQAVNFPFLVKLEFSFKDNSNLYMVMEYVPGGEMFSHLRRIGRFSEPHARFYAAQIVLTFEYLHSLDLIYRDLKPENLLIDQQGYIQVTDFGFAKRVKGRTWTLCGTPEYLAPEIILSKGYNKAVDWWALGVLIYEMAAGYPPFFADQPIQIYEKIVSGKVRFPSHFSSDLKDLLRNLLQVDLTKRFGNLKNGVNDIKNHKWFATTDWIAIYQRKVEAPFIPKFKGPGDTSNFDDYEEEEIRVSINEKCGKEFSEF</t>
-  </si>
-  <si>
-    <t>TCCAGGGTGTCCCATGAACAGTTTCGGGCGGCCCTGCAGCTGGTGGTCAGCCCAGGAGACCCCAGGGAATACTTGGCCAACTTTATCAAAATCGGGGAAGGCTCAACCGGCATCGTATGCATCGCCACCGAGAAACACACAGGGAAACAAGTTGCAGTGAAGAAAATGGACCTCCGGAAGCAACAGAGACGAGAACTGCTTTTCAATGAGGTCGTGATCATGCGGGATTACCACCATGACAATGTGGTTGACATGTACAGCAGCTACCTTGTCGGCGATGAGCTCTGGGTGGTCATGGAGTTTCTAGAAGGTGGTGCCTTGACAGACATTGTGACTCACACCAGAATGAATGAAGAACAGATAGCTACTGTCTGCCTGTCAGTTCTGAGAGCTCTCTCCTACCTTCATAACCAAGGAGTGATTCACAGGGACATAAAAAGTGACTCCATCCTCCTGACAAGCGATGGCCGGATAAAGTTGTCTGATTTTGGTTTCTGTGCTCAAGTTTCCAAAGAGGTGCCGAAGAGGAAATCATTGGTTGGCACTCCCTACTGGATGGCCCCTGAGGTGATTTCTAGGCTACCTTATGGGACAGAGGTGGACATCTGGTCCCTCGGGATCATGGTGATAGAAATGATTGATGGCGAGCCCCCCTACTTCAATGAGCCTCCCCTCCAGGCGATGCGGAGGATCCGGGACAGTTTACCTCCAAGAGTGAAGGACCTACACAAGGTTTCTTCAGTGCTCCGGGGATTCCTAGACTTGATGTTGGTGAGGGAGCCCTCTCAGAGAGCAACAGCCCAGGAACTCCTCGGACATCCATTCTTAAAACTAGCAGGTCCACCGTCTTGCATTGTCCCCCTCATGAGACAATACAGGCATCAC</t>
-  </si>
-  <si>
-    <t>KRQWALEDFEIGRPLGKGKFGNVYLAREKQSKFILALKVLFKAQLEKAGVEHQLRREVEIQSHLRHPNILRLYGYFHDATRVYLILEYAPLGTVYRELQKLSKFDEQRTATYITELANALSYCHSKRVIHRDIKPENLLLGSAGELKIADFGWSVHAPSSRRTTLCGTLDYLPPEMIEGRMHDEKVDLWSLGVLCYEFLVGKPPFEANTYQETYKRISRVEFTFPDFVTEGARDLISRLLKHNPSQRPMLREVLEHPWITANSSKPS</t>
-  </si>
-  <si>
-    <t>EGFR_HUMAN_D0_2RF9_A</t>
-  </si>
-  <si>
-    <t>SLK_HUMAN_D0_2JFL_A</t>
-  </si>
-  <si>
-    <t>SRVSHEQFRAALQLVVSPGDPREYLANFIKIGEGSTGIVCIATEKHTGKQVAVKKMDLRKQQRRELLFNEVVIMRDYHHDNVVDMYSSYLVGDELWVVMEFLEGGALTDIVTHTRMNEEQIATVCLSVLRALSYLHNQGVIHRDIKSDSILLTSDGRIKLSDFGFCAQVSKEVPKRKSLVGTPYWMAPEVISRLPYGTEVDIWSLGIMVIEMIDGEPPYFNEPPLQAMRRIRDSLPPRVKDLHKVSSVLRGFLDLMLVREPSQRATAQELLGHPFLKLAGPPSCIVPLMRQYRHH</t>
-  </si>
-  <si>
-    <t>TQTVHEFAKELDATNISIDKVVGAGEFGEVCSGRLKLPSKKEISVAIKTLKVGYTEKQRRDFLGEASIMGQFDHPNIIRLEGVVTKSKPVMIVTEYMENGSLDSFLRKHDAQFTVIQLVGMLRGIASGMKYLSDMGYVHRDLAARNILINSNLVCKVSDFGLSRVLEDDPEAAYTTRGGKIPIRWTSPEAIAYRKFTSASDVWSYGIVLWEVMSYGERPYWEMSNQDVIKAVDEGYRLPPPMDCPAALYQLMLDCWQKDRNNRPKFEQIVSILDKLIRNPGSLKIITSAAARPSNLLLDQSNVDITTFRTTGDWLNGVWTAHCKEIFTGVEYSSCDTIAKIS</t>
-  </si>
-  <si>
-    <t>QQFPQFHVKSGLQIKKNAIIDDYKVTSQVLGLGINGKVLQIFNKRTQEKFALKMLQDCPKARREVELHWRASQCPHIVRIVDVYENLYAGRKCLLIVMECLDGGELFSRIQDRGDQAFTEREASEIMKSIGEAIQYLHSINIAHRDVKPENLLYTSKRPNAILKLTDFGFAKETTSHNSLTTPCYTPYYVAPEVLGPEKYDKSCDMWSLGVIMYILLCGYPPFYSNHGLAISPGMKTRIRMGQYEFPNPEWSEVSEEVKMLIRNLLKTEPTQRMTITEFMNHPWIMQSTKVPQTPLHTSRVLKEDKERWEDVKGCLHDKNSDQA</t>
-  </si>
-  <si>
-    <t>CSK21_HUMAN_D0_3AXW_A</t>
-  </si>
-  <si>
-    <t>ATCTRFTDDYQLFEELGKGAFSVVRRCVKKTPTQEYAAKIINTKKLSARDHQKLEREARICRLLKHPNIVRLHDSISEEGFHYLVFDLVTGGELFEDIVAREYYSEADASHCIHQILESVNHIHQHDIVHRDLKPENLLLASKCKGAAVKLADFGLAIEVQGEQQAWFGFAGTPGYLSPEVLRKDPYGKPVDIWACGVILYILLVGYPPFWDEDQHKLYQQIKAGAYDFPSPEWDTVTPEAKNLINQMLTINPAKRITADQALKHPWVCQRSTVASMMHRQETVECLRKFNARRKLKGAILTTMLVSRNFS</t>
-  </si>
-  <si>
-    <t>VIDPSELTFVQEIGSGQFGLVHLGYWLNKDKVAIKTIREGAMSEEDFIEEAEVMMKLSHPKLVQLYGVCLEQAPICLVFEFMEHGCLSDYLRTQRGLFAAETLLGMCLDVCEGMAYLEEACVIHRDLAARNCLVGENQVIKVSDFGMTRFVLDDQYTSSTGTKFPVKWASPEVFSFSRYSSKSDVWSFGVLMWEVFSEGKIPYENRSNSEVVEDISTGFRLYKPRLASTHVYQIMNHCWKERPEDRPAFSRLLRQLAEIAESGL</t>
-  </si>
-  <si>
-    <t>CGTGTAAAAGCAGCTCAAGCTGGAAGACAGAGCTCTGCAAAGAGACATCTTGCAGAACAATTTGCAGTTGGAGAGATAATAACTGACATGGCAAAAAAGGAATGGAAAGTAGGATTACCCATTGGCCAAGGAGGCTTTGGCTGTATATATCTTGCTGATATGAATTCTTCAGAGTCAGTTGGCAGTGATGCACCTTGTGTTGTAAAAGTGGAACCCAGTGACAATGGACCTCTTTTTACTGAATTAAAGTTCTACCAACGAGCTGCAAAACCAGAGCAAATTCAGAAATGGATTCGTACCCGTAAGCTGAAGTACCTGGGTGTTCCTAAGTATTGGGGGTCTGGTCTACATGACAAAAATGGAAAAAGTTACAGGTTTATGATAATGGATCGCTTTGGGAGTGACCTTCAGAAAATATATGAAGCAAATGCCAAAAGGTTTTCTCGGAAAACTGTCTTGCAGCTAAGCTTAAGAATTCTGGATATTCTGGAATATATTCACGAGCATGAGTATGTGCATGGAGATATCAAGGCCTCAAATCTTCTTCTGAACTACAAGAATCCTGACCAGGTGTACTTGGTAGATTATGGCCTTGCTTATCGGTACTGCCCAGAAGGAGTTCATAAAGAATACAAAGAAGACCCCAAAAGATGTCACGATGGCACTATTGAATTCACGAGCATCGATGCACACAATGGCGTGGCCCCATCAAGACGTGGTGATTTGGAAATACTTGGTTATTGCATGATCCAATGGCTTACTGGCCATCTTCCTTGGGAGGATAATTTGAAAGATCCTAAATATGTTAGAGATTCCAAAATTAGATACAGAGAAAATATTGCAAGTTTGATGGACAAATGTTTTCCTGAGAAAAACAAACCAGGTGAAATTGCCAAATACATGGAAACAGTGAAATTACTAGACTACACTGAAAAACCTCTTTATGAAAATTTACGTGACATTCTTTTGCAAGGACTAAAAGCTATAGGAAGTAAGGATGATGGCAAATTGGACCTCAGTGTTGTGGAGAATGGAGGTTTGAAAGCAAAAACAATAACAAAGAAGCGAAAGAAAGAAATTGAAGAA</t>
-  </si>
-  <si>
-    <t>KS6A1_HUMAN_D0_3RNY_B</t>
-  </si>
-  <si>
-    <t>MP2K6_HUMAN_D0_3VN9_A</t>
-  </si>
-  <si>
-    <t>RVKAAQAGRQSSAKRHLAEQFAVGEIITDMAKKEWKVGLPIGQGGFGCIYLADMNSSESVGSDAPCVVKVEPSDNGPLFTELKFYQRAAKPEQIQKWIRTRKLKYLGVPKYWGSGLHDKNGKSYRFMIMDRFGSDLQKIYEANAKRFSRKTVLQLSLRILDILEYIHEHEYVHGDIKASNLLLNYKNPDQVYLVDYGLAYRYCPEGVHKEYKEDPKRCHDGTIEFTSIDAHNGVAPSRRGDLEILGYCMIQWLTGHLPWEDNLKDPKYVRDSKIRYRENIASLMDKCFPEKNKPGEIAKYMETVKLLDYTEKPLYENLRDILLQGLKAIGSKDDGKLDLSVVENGGLKAKTITKKRKKEIEE</t>
-  </si>
-  <si>
-    <t>MKNK1_HUMAN_D0_2HW6_B</t>
-  </si>
-  <si>
-    <t>MSLIRKKGFYKQDVNKTAWELPKTYVSPTHVGSGAYGSVCSAIDKRSGEKVAIKKLSRPFQSEIFAKRAYRELLLLKHMQHENVIGLLDVFTPASSLRNFYDFYLVMPFMQTDLQKIMGMEFSEEKIQYLVYQMLKGLKYIHSAGVVHRDLKPGNLAVNEDCELKILDFGLARHADAEMTGYVVTRWYRAPEVILSWMHYNQTVDIWSVVCIMAEMLTGKTLFKGKDYLDQLTQILKVTGVPGTEFVQKLNDKAAKSYIQSLPQTPRKDFTQLFPRASPQAADLLEKMLELDVDKRLTAAQALTHPFFEPFRDPEEETEAQQPFDDSLEHEKLTVDEWKQHIYKEIVNFSPI</t>
-  </si>
-  <si>
-    <t>AAPPAKEIPEVLVDPRSRRRYVRGRFLGKGGFAKCFEISDADTKEVFAGKIVPKSLLLKPHQREKMSMEISIHRSLAHQHVVGFHGFFEDNDFVFVVLELCRRRSLLELHKRRKALTEPEARYYLRQIVLGCQYLHRNRVIHRDLKLGNLFLNEDLEVKIGDFGLATKVEYDGERKKTLCGTPNYIAPEVLSKKGHSFEVDVWSIGCIMYTLLVGKPPFETSCLKETYLRIKKNEYSIPKHINPVAASLIQKMLQTDPTARPTINELLNDEFFTSGYIPARLPITCLTIPPRFSIAPSSLDPSNRKPLTVLNK</t>
-  </si>
-  <si>
-    <t>ITK_HUMAN_D0_3QGW_B</t>
-  </si>
-  <si>
-    <t>KS6A3_HUMAN_D1_4JG7_A</t>
-  </si>
-  <si>
-    <t>KCC4_HUMAN_D0_2W4O_A</t>
-  </si>
-  <si>
-    <t>CSK_HUMAN_D0_3D7T_A</t>
-  </si>
-  <si>
-    <t>KCC2A_HUMAN_D0_2VZ6_B</t>
-  </si>
-  <si>
-    <t>ATGTCTGATGAGGAGATCTTGGAGAAATTACGAAGCATAGTGAGTGTGGGCGATCCTAAGAAGAAATATACACGGTTTGAGAAGATTGGACAAGGTGCTTCAGGCACCGTGTACACAGCAATGGATGTGGCCACAGGACAGGAGGTGGCCATTAAGCAGATGAATCTTCAGCAGCAGCCCAAGAAAGAGCTGATTATTAATGAGATCCTGGTCATGAGGGAAAACAAGAACCCAAACATTGTGAATTACTTGGACAGTTACCTCGTGGGAGATGAGCTGTGGGTTGTTATGGAATACTTGGCTGGAGGCTCCTTGACAGATGTGGTGACAGAAACTTGCATGGATGAAGGCCAAATTGCAGCTGTGTGCCGTGAGTGTCTGCAGGCTCTGGAGTTCTTGCATTCGAACCAGGTCATTCACAGAGACATCAAGAGTGACAATATTCTGTTGGGAATGGATGGCTCTGTCAAGCTAACTGACTTTGGATTCTGTGCACAGATAACCCCAGAGCAGAGCAAACGGAGCACCATGGTAGGAACCCCATACTGGATGGCACCAGAGGTTGTGACACGAAAGGCCTATGGGCCCAAGGTTGACATCTGGTCCCTGGGCATCAAGGCCATCGAAATGATTGAAGGGGAGCCTCCATACCTCAATGAAAACCCTCTGAGAGCCTTGTACCTCATTGCCACCAATGGGACCCCAGAACTTCAGAACCCAGAGAAGCTGTCAGCTATCTTCCGGGACTTTCTGAACCGCTGTCTCGAGATGGATGTGGAGAAGAGAGGTTCAGCTAAAGAGCTGCTACAGCATCAATTCCTGAAGATTGCCAAGCCCCTCTCCAGCCTCACTCCACTTATTGCTGCAGCTAAGGAGGCAACAAAGAACAATCAC</t>
-  </si>
-  <si>
-    <t>expression tag location</t>
-  </si>
-  <si>
-    <t>ATGGAGGCAGCAGCATCCGAACCCTCTCTTGATCTAGATAATCTGAAACTGTTGGAGCTGATTGGCCGAGGTCGATATGGAGCAGTATATAAAGGCTCCTTGGATGAGCGTCCAGTTGCTGTAAAAGTGTTTTCCTTTGCAAACCGTCAGAATTTTATCAACGAAAAGAACATTTACAGAGTGCCTTTGATGGAACATGACAACATTGCCCGCTTTATAGTTGGAGATGAGAGAGTCACTGCAGATGGACGCATGGAATATTTGCTTGTGATGGAGTACTATCCCAATGGATCTTTATGCAAGTATTTAAGTCTCCACACAAGTGACTGGGTAAGCTCTTGCCGTCTTGCTCATTCTGTTACTAGAGGACTGGCTTATCTTCACACAGAATTACCACGAGGAGATCATTATAAACCTGCAATTTCCCATCGAGATTTAAACAGCAGAAATGTCCTAGTGAAAAATGATGGAACCTGTGTTATTAGTGACTTTGGACTGTCCATGAGGCTGACTGGAAATAGACTGGTGCGCCCAGGGGAGGAAGATAATGCAGCCATAAGCGAGGTTGGCACTATCAGATATATGGCACCAGAAGTGCTAGAAGGAGCTGTGAACTTGAGGGACTGTGAATCAGCTTTGAAACAAGTAGACATGTATGCTCTTGGACTAATCTATTGGGAGATATTTATGAGATGTACAGACCTCTTCCCAGGGGAATCCGTACCAGAGTACCAGATGGCTTTTCAGACAGAGGTTGGAAACCATCCCACTTTTGAGGATATGCAGGTTCTCGTGTCTAGGGAAAAACAGAGACCCAAGTTCCCAGAAGCCTGGAAAGAAAATAGCCTGGCAGTGAGGTCACTCAAGGAGACAATCGAAGACTGTTGGGACCAGGATGCAGAGGCTCGGCTTACTGCACAGTGTGCTGAGGAAAGGATGGCTGAACTTATGATGATTTGGGAAAGAAACAAATCTGTGAGCCCAACA</t>
-  </si>
-  <si>
-    <t>GGAGAAGCTCCCAACCAAGCTCTCTTGAGGATCTTGAAGGAAACTGAATTCAAAAAGATCAAAGTGCTGGGCTCCGGTGCGTTCGGCACGGTGTATAAGGGACTCTGGATCCCAGAAGGTGAGAAAGTTAAAATTCCCGTCGCTATCAAGGAATTAAGAGAAGCAACATCTCCGAAAGCCAACAAGGAAATCCTCGATGAAGCCTACGTGATGGCCAGCGTGGACAACCCCCACGTGTGCCGCCTGCTGGGCATCTGCCTCACCTCCACCGTGCAaCTCATCACGCAGCTCATGCCCTTCGGCTGCCTCCTGGACTATGTCCGGGAACACAAAGACAATATTGGCTCCCAGTACCTGCTCAACTGGTGTGTGCAGATCGCAAAGGGCATGAACTACTTGGAGGACCGTCGCTTGGTGCACCGCGACCTGGCAGCCAGGAACGTACTGGTGAAAACACCGCAGCATGTCAAGATCACAGATTTTGGGCgGGCCAAACTGCTGGGTGCGGAAGAGAAAGAATACCATGCAGAAGGAGGCAAAGTGCCTATCAAGTGGATGGCATTGGAATCAATTTTACACAGAATCTATACCCACCAGAGTGATGTCTGGAGCTACGGGGTGACCGTTTGGGAGTTGATGACCTTTGGATCCAAGCCATATGACGGAATCCCTGCCAGCGAGATCTCCTCCATCCTGGAGAAAGGAGAACGCCTCCCTCAGCCACCCATATGTACCATCGATGTCTACATGATCATGGTCAAGTGCTGGATGATAGACGCAGATAGTCGCCCAAAGTTCCGTGAGTTGATCATCGAATTCTCCAAAATGGCCCGAGACCCCCAGCGCTACCTTGTCATTCAGGGGGATGAAAGAATGCATTTGCCAAGTCCTACAGACTCCAACTTCTACCGTGCCCTGATGGATGAAGAAGACATGGACGACGTGGTGGATGCCGACGAGTACCTCATCCCACAGCAGGGC</t>
-  </si>
-  <si>
-    <t>GCCACCTGCACACGTTTCACCGACGACTACCAGCTCTTCGAGGAGCTTGGCAAGGGTGCTTTCTCTGTGGTCCGCAGGTGTGTGAAGAAAACCCCCACGCAGGAGTACGCAGCAAAAATCATCAATACCAAGAAATTGTCTGCCCGGGATCACCAGAAACTAGAACGTGAGGCTCGGATATGTCGACTTCTGAAACATCCAAACATCGTGCGCCTCCATGACAGTATTTCTGAAGAAGGGTTTCACTACCTCGTGTTTGACCTTGTTACCGGCGGGGAGCTGTTTGAAGACATTGTGGCCAGAGAGTACTACAGTGAAGCAGATGCCAGCCACTGTATACATCAGATTCTGGAGAGTGTTAACCACATCCACCAGCATGACATCGTCCACAGGGACCTGAAGCCTGAGAACCTGCTGCTGGCGAGTAAATGCAAGGGTGCCGCCGTCAAGCTGGCTGATTTTGGCCTAGCCATCGAAGTACAGGGAGAGCAGCAGGCTTGGTTTGGTTTTGCTGGCACCCCAGGTTACTTGTCCCCTGAGGTCTTGAGGAAAGATCCCTATGGAAAACCTGTGGATATCTGGGCCTGCGGGGTCATCCTGTATATCCTCCTGGTGGGCTATCCTCCCTTCTGGGATGAGGATCAGCACAAGCTGTATCAGCAGATCAAGGCTGGAGCCTATGATTTCCCATCACCAGAATGGGACACGGTAACTCCTGAAGCCAAGAACTTGATCAACCAGATGCTGACCATAAACCCAGCAAAGCGCATCACGGCTGACCAGGCTCTCAAGCACCCGTGGGTCTGTCAACGATCCACGGTGGCATCCATGATGCATCGTCAGGAGACTGTGGAGTGTTTGCGCAAGTTCAATGCCCGGAGAAAACTGAAGGGTGCCATCCTCACGACCATGCTTGTCTCCAGGAACTTCTCA</t>
-  </si>
-  <si>
-    <t>GAGACCTACATTAAGCTGGACAAACTGGGCGAGGGTACCTATGCCACCGTCTACAAAGGCAAAAGCAAGCTCACAGACAACCTTGTGGCACTCAAGGAGATCAGACTGGAACATGAAGAGGGGGCACCCTGCACCGCCATCCGGGAAGTGTCCCTACTCAAGGACCTCAAACACGCCAACATCGTTACGCTACATGACATTATCCACACGGAGAAGTCCCTCACCCTTGTCTTTGAGTACCTGGACAAGGACCTGAAGCAGTACCTGGATGACTGTGGGAACATCATCAACATGCACAACGTGAAACTGTTCCTGTTCCAGCTGCTCCGTGGCCTGGCCTACTGCCACCGGCAGAAGGTGCTACACCGAGACCTCAAGCCCCAGAACCTGCTCATCAACGAGAGGGGAGAGCTCAAGCTGGCTGACTTTGGCCTGGCCCGAGCCAAGTCAATCCCAACAAAGACATACTCCAATGAGGTGGTGACACTGTGGTACCGGCCCCCTGACATCCTGCTTGGGTCCACGGACTACTCCACTCAGATTGACATGTGGGGTGTGGGCTGCATCTTCTATGAGATGGCCACAGGCCGTCCCCTCTTTCCGGGCTCCACGGTGGAGGAACAGCTACACTTCATCTTCCGTATCTTAGGAACCCCAACTGAGGAGACGTGGCCAGGCATCCTGTCCAACGAGGAGTTCAAGACATACAACTACCCCAAGTACCGAGCCGAGGCCCTTTTGAGCCACGCACCCCGACTTGATAGCGACGGGGCCGACCTCCTCACCAAGCTGTTGCAGTTTGAGGGTCGAAATCGGATCTCCGCAGAGGATGCCATGAAACATCCATTCTTCCTCAGTCTGGGGGAGCGGATCCACAAACTTCCTGACACTACTTCCATATTTGCACTAAAGGAGATTCAGCTACAAAAGGAGGCCAGCCTTCGGTCT</t>
-  </si>
-  <si>
-    <t>MK13_HUMAN_D0_4EYJ_A</t>
-  </si>
-  <si>
-    <t>STK16_HUMAN_D0_2BUJ_B</t>
-  </si>
-  <si>
-    <t>AAGCACGACGGGCGGGTGAAGATCGGACACTACGTGCTGGGCGACACGCTGGGCGTCGGCACCTTCGGCAAAGTGAAGATTGGAGAACATCAATTAACAGGCCATAAAGTGGCAGTTAAAATCTTAAATAGACAGAAGATTCGCAGTTTAGATGTTGTTGGAAAAATAAAACGAGAAATTCAAAATCTAAAACTCTTTCGTCATCCTCATATTATCAAACTATACCAGGTGATCAGCACTCCAACAGATTTTTTTATGGTAATGGAATATGTGTCTGGAGGTGAATTATTTGACTACATCTGTAAGCATGGACGGGTTGAAGAGATGGAAGCCAGGCGRCTCTTTCAGCAGATTCTGTCTGCTGTGGATTACTGTCATAGGCATATGGTTGTTCATCGAGACCTGAAACCAGAGAATGTCCTGTTGGATGCACACATGAATGCCAAGATAGCCGATTTCGGATTATCTAATATGATGTCAGATGGTGAATTTCTGAGAACTAGTTGCGGATCTCCAAATTATGCAGCACCTGAAGTCATCTCAGGCAGATTGTATGCAGGTCCTGAAGTTGATATCTGGAGCTGTGGTGTTATCTTGTATGCTCTTCTTTGTGGCACCCTCCCATTTGATGATGAGCATGTACCTACGTTATTTAAGAAGATCCGAGGGGGTGTCTTTTATATCCCAGAATATCTCAATCGTTCTGTCGCCACTCTCCTGATGCATATGCTGCAGGTTGACCCACTGAAACGAGCAACTATCAAAGACATAAGAGAGCATGAATGGTTTAAACAAGATTTGCCCAGTTACTTATTTCCTGAA</t>
-  </si>
-  <si>
-    <t>CAGAGCAGTAAGCGCAGCAGCCGGAGTGTGGAAGATGACAAGGAGGGTCACCTGGTGTGCCGGATCGGCGATTGGCTCCAAGAGCGATATGAGATTGTGGGGAACCTGGGTGAAGGCACCTTTGGCAAGGTGGTGGAGTGCTTGGACCATGCCAGAGGGAAGTCTCAGGTTGCCCTGAAGATCATCCGCAACGTGGGCAAGTACCGGGAGGCTGCCCGGCTAGAAATCAACGTGCTCAAAAAAATCAAGGAGAAGGACAAAGAAAACAAGTTCCTGTGTGTCTTGATGTCTGACTGGTTCAACTTCCACGGTCACATGTGCATCGCCTTTGAGCTCCTGGGCAAGAACACCTTTGAGTTCCTGAAGGAGAATAACTTCCAGCCTTACCCCCTACCACATGTCCGGCACATGGCCTACCAGCTCTGCCACGCCCTTAGATTTCTGCATGAGAATCAGCTGACCCATACAGACTTGAAACCAGAGAACATCCTGTTTGTGAATTCTGAGTTTGAAACCCTCTACAATGAGCACAAGAGCTGTGAGGAGAAGTCAGTGAAGAACACCAGCATCCGAGTGGCTGACTTTGGCAGTGCCACATTTGACCATGAGCACCACACCACCATTGTGGCCACCCGTCACTATCGCCCGCCTGAGGTGATCCTTGAGCTGGGCTGGGCACAGCCCTGTGACGTCTGGAGCATTGGCTGCATTCTCTTTGAGTACTACCGGGGCTTCACACTCTTCCAGACCCACGAAAACCGAGAGCACCTGGTGATGATGGAGAAGATCCTAGGGCCCATCCCATCACACATGATCCACCGTACCAGGAAGCAGAAATATTTCTACAAAGGGGGCCTAGTTTGGGATGAGAACAGCTCTGACGGCCGGTATGTGAAGGAGAACTGCAAACCTCTGAAGAGTTACATGCTCCAAGACTCCCTGGAGCACGTGCAGCTGTTTGACCTGATGAGGAGGATGTTAGAATTTGACCCTGCCCAGCGCATCACACTGGCCGAGGCCCTGCTGCACCCCTTCTTTGCTGGCCTGACCCCTGAGGAGCGGTCCTTCCACACC</t>
-  </si>
-  <si>
-    <t>GAACTGAAGGATGACGACTTTGAGAAGATCAGTGAGCTGGGGGCTGGCAATGGCGGTGTGGTGTTCAAGGTCTCCCACAAGCCTTCTGGCCTGGTCATGGCCAGAAAGCTAATTCATCTGGAGATCAAACCCGCAATCCGGAACCAGATCATAAGGGAGCTGCAGGTTCTGCATGAGTGCAACTCTCCGTACATCGTGGGCTTCTATGGTGCGTTCTACAGCGATGGCGAGATCAGTATCTGCATGGAGCACATGGATGGAGGTTCTCTGGATCAAGTCCTGAAGAAAGCTGGAAGAATTCCTGAACAAATTTTAGGAAAAGTTAGCATTGCTGTAATAAAAGGCCTGACATATCTGAGGGAGAAGCACAAGATCATGCACAGAGCATACGGAATGGACAGCCGACCTCCCATGGCAATTTTTGAGTTGTTGGATTACATAGTCAACGAGCCTCCTCCAAAACTGCCCAGTGGAGTGTTCAGTCTGGAATTTCAAGATTTTGTGAATAAATGCTTAATAAAAAACCCCGCAGAGAGAGCAGATTTGAAGCAACTCATGGTTCATGCTTTTATCAAGAGATCTGATGCTGAGGAAGTGGATTTTGCAGGTTGGCTCTGCTCCACCATCGGCCTTAAC</t>
-  </si>
-  <si>
-    <t>MQTVGVHSIVQQLHRNSIQFTDGYEVKEDIGVGSYSVCKRCIHKATNMEFAVKIIDKSKRDPTEEIEILLRYGQHPNIITLKDVYDDGKYVYVVTELMKGGELLDKILRQKFFSEREASAVLFTITKTVEYLHAQGVVHRDLKPSNILYVDESGNPESIRICDFGFAKQLRAENGLLMTPCYTANFVAPEVLKRQGYDAACDIWSLGVLLYTMLTGYTPFANGPDDTPEEILARIGSGKFSLSGGYWNSVSDTAKDLVSKMLHVDPHQRLTAALVLRHPWIVHWDQLPQYQLNRQDAPHLVKGAMAATYSALNRNQSPVLEPVGRSTLAQRRGIKKITSTAL</t>
-  </si>
-  <si>
-    <t>KAPCA_HUMAN_D0_4AE9_A</t>
-  </si>
-  <si>
-    <t>KCC2G_HUMAN_D0_2V7O_A</t>
-  </si>
-  <si>
-    <t>KQYEHVKRDLNPEDFWEIIGELGDGAFGKVYKAQNKETSVLAAAKVIDTKSEEELEDYMVEIDILASCDHPNIVKLLDAFYYENNLWILIEFCAGGAVDAVMLELERPLTESQIQVVCKQTLDALNYLHDNKIIHRDLKAGNILFTLDGDIKLADFGVSAKNMRTIQRRDSFIGTPYWMAPEVVMCETSKDRPYDYKADVWSLGITLIEMAEIEPPHHELNPMRVLLKIAKSEPPTLAQPSRWSSNFKDFLKKCLEKNVDARWTTSQLLQHPFVTVDSNKPIRELIAEAKAEVTEEVEDGKE</t>
-  </si>
-  <si>
-    <t>ACCCAAACTGTTCATGAGTTTGCCAAGGAATTGGATGCCACCAACATATCCATTGATAAAGTTGTTGGAGCAGGTGAATTTGGAGAGGTGTGCAGTGGTCGCTTAAAACTTCCTTCAAAAAAAGAGATTTCAGTGGCCATTAAGACCCTGAAAGTTGGCTACACAGAAAAGCAGAGGAGAGACTTCCTGGGAGAAGCAAGCATTATGGGACAGTTTGACCACCCCAATATCATTCGACTGGAAGGAGTTGTTACCAAAAGTAAGCCAGTTATGATTGTCACAGAATACATGGAGAATGGTTCCTTGGATAGTTTCCTACGTAAACACGATGCCCAGTTTACTGTCATTCAGCTAGTGGGGATGCTTCGAGGGATAGCATCTGGCATGAAGTACCTGTCAGACATGGGCTATGTTCACCGAGACCTCGCTGCTCGGAACATCTTGATCAACAGTAACTTGGTGTGTAAGGTTTCTGATTTCGGACTTTCGCGTGTCCTGGAGGATGACCCAGAAGCTGCTTATACAACAAGAGGAGGGAAGATCCCAATCAGGTGGACATCACCAGAAGCTATAGCCTACCGCAAGTTCACGTCAGCCAGCGATGTATGGAGTTATGGGATTGTTCTCTGGGAGGTGATGTCTTATGGAGAGAGACCATACTGGGAGATGTCCAATCAGGATGTAATTAAAGCTGTAGATGAGGGCTATCGACTGCCACCCCCCATGGACTGCCCAGCTGCCTTGTATCAGCTGATGCTGGACTGCTGGCAGAAAGACAGGAACAACAGACCCAAGTTTGAGCAGATTGTTAGTATTCTGGACAAGCTTATCCGGAATCCCGGCAGCCTGAAGATCATCACCAGTGCAGCCGCAAGGCCATCAAACCTTCTTCTGGACCAAAGCAATGTGGATATCACTACCTTCCGCACAACAGGTGACTGGCTTAATGGTGTCTGGACAGCACACTGCAAGGAAATCTTCACGGGTGTGGAGTACAGTTCTTGTGACACAATAGCCAAGATTTCC</t>
-  </si>
-  <si>
-    <t>MEKDGLCRADQQYECVAEIGEGAYGKVFKARDLKNGGRFVALKRVRVQTGEEGMPLSTIREVAVLRHLETFEHPNVVRLFDVCTVSRTDRETKLTLVFEHVDQDLTTYLDKVPEPGVPTETIKDMMFQLLRGLDFLHSHRVVHRDLKPQNILVTSSGQIKLADFGLARIYSFQMALTSVVVTLWYRAPEVLLQSSYATPVDLWSVGCIFAEMFRRKPLFRGSSDVDQLGKILDVIGLPGEEDWPRDVALPRQAFHSKSAQPIEKFVTDIDELGKDLLLKCLTFNPAKRISAYSALSHPYFQ</t>
-  </si>
-  <si>
-    <t>EPHA3_HUMAN_D0_4GK2_A</t>
-  </si>
-  <si>
-    <t>ATGCCCGGCCCGGCCGCGGGCAGCAGGGCCCGGGTCTACGCCGAGGTGAACAGTCTGAGGAGCCGCGAGTACTGGGACTACGAGGCTCACGTCCCGAGCTGGGGTAATCAAGATGATTACCAACTGGTTCGAAAACTTGGTCGGGGAAAATATAGTGAAGTATTTGAGGCCATTAATATCACCAACAATGAGAGAGTGGTTGTAAAAATCCTGAAGCCAGTGAAGAAAAAGAAGATAAAACGAGAGGTTAAGATTCTGGAGAACCTTCGTGGTGGAACAAATATCATTAAGCTGATTGACACTGTAAAGGACCCCGTGTCAAAGACACCAGCTTTGGTATTTGAATATATCAATAATACAGATTTTAAGCAACTCTACCAGATCCTGACAGACTTTGATATCCGGTTTTATATGTATGAACTACTTAAAGCTCTGGATTACTGCCACAGCAAGGGAATCATGCACAGGGATGTGAAACCTCACAATGTCATGATAGATCACCAACAGAAAAAGCTGCGACTGATAGATTGGGGTCTGGCAGAATTCTATCATCCTGCTCAGGAGTACAATGTTCGTGTAGCCTCAAGGTACTTCAAGGGACCAGAGCTCCTCGTGGACTATCAGATGTATGATTATAGCTTGGACATGTGGAGTTTGGGCTGTATGTTAGCAAGCATGATCTTTCGAAGGGAACCATTCTTCCATGGACAGGACAACTATGACCAGCTTGTTCGCATTGCCAAGGTTCTGGGTACAGAAGAACTGTATGGGTATCTGAAGAAGTATCACATAGACCTAGATCCACACTTCAACGATATCCTGGGACAACATTCACGGAAACGCTGGGAAAACTTTATCCATAGTGAGAACAGACACCTTGTCAGCCCTGAGGCCCTAGATCTTCTGGACAAACTTCTGCGATACGACCATCAACAGAGACTGACTGCCAAAGAGGCCATGGAGCACCCATACTTCTACCCTGTGGTGAAGGAGCAGTCCCAG</t>
-  </si>
-  <si>
-    <t>ETKYTVDKRFGMDFKEIELIGSGGFGQVFKAKHRIDGKTYVIKRVKYNNEKAEREVKALAKLDHVNIVHYNGCWDGFDYDPETSDDSLESSDYDPENSKNSSRSKTKCLFIQMEFCDKGTLEQWIEKRRGEKLDKVLALELFEQITKGVDYIHSKKLIHRDLKPSNIFLVDTKQVKIGDFGLVTSLKNDGKRTRSKGTLRYMSPEQISSQDYGKEVDLYALGLILAELLHVCDTAFETSKFFTDLRDGIISDIFDKKEKTLLQKLLSKKPEDRPNTSEILRTLTVWKKSPEKNERHTC</t>
-  </si>
-  <si>
-    <t>NEK2_HUMAN_D0_2XKE_A</t>
-  </si>
-  <si>
-    <t>ATGGAGCTGAGAGTCGGGAACAGGTACCGGCTGGGCCGGAAGATCGGCAGCGGCTCCTTCGGAGACATCTATCTCGGTACGGACATTGCTGCAGGAGAAGAGGTTGCCATCAAGCTTGAATGTGTCAAAACCAAACACCCTCAGCTCCACATTGAGAGCAAAATCTACAAGATGATGCAGGGAGGAGTGGGCATCCCCACCATCAGATGGTGCGGGGCAGAGGGGGACTACAACGTCATGGTGATGGAGCTGCTGGGGCCAAGCCTGGAGGACCTCTTCAACTTCTGCTCCAGGAAATTCAGCCTCAAAACCGTCCTGCTGCTTGCTGACCAAATGATCAGTCGCATCGAATACATTCATTCAAAGAACTTCATCCACCGGGATGTGAAGCCAGACAACTTCCTCATGGGCCTGGGGAAGAAGGGCAACCTGGTGTACATCATCGACTTCGGGCTGGCCAAGAAGTACCGGGATGCACGCACCCACCAGCACATCCCCTATCGTGAGAACAAGAACCTCACGGGGACGGCGCGGTACGCCTCCATCAACACGCACCTTGGAATTGAACAATCCCGAAGAGATGACTTGGAGTCTCTGGGCTACGTGCTAATGTACTTCAACCTGGGCTCTCTCCCCTGGCAGGGGCTGAAGGCTGCCACCAAGAGACAGAAATACGAAAGGATTAGCGAGAAGAAAATGTCCACCCCCATCGAAGTGTTGTGTAAAGGCTACCCTTCCGAATTTGCCACATACCTGAATTTCTGCCGTTCCTTGCGTTTTGACGACAAGCCTGACTACTCGTACCTGCGGCAGCTTTTCCGGAATCTGTTCCATCGCCAGGGCTTCTCCTATGACTACGTGTTCGACTGGAACATGCTCAAA</t>
-  </si>
-  <si>
-    <t>ATGGCGGCGGCGGCGGCGGCGGGCGCGGGCCCGGAGATGGTCCGCGGGCAGGTGTTCGACGTGGGGCCGCGCTACACCAACCTCTCGTACATCGGCGAGGGCGCCTACGGCATGGTGTGCTCTGCTTATGATAATGTCAACAAAGTTCGAGTAGCTATCAAGAAAATCAGCCCCTTTGAGCACCAGACCTACTGCCAGAGAACCCTGAGGGAGATAAAAATCTTACTGCGCTTCAGACATGAGAACATCATTGGAATCAATGACATTATTCGAGCACCAACCATCGAGCAAATGAAAGATGTATATATAGTACAGGACCTCATGGAAACAGATCTTTACAAGCTCTTGAAGACACAACACCTCAGCAATGACCATATCTGCTATTTTCTCTACCAGATCCTCAGAGGGTTAAAATATATCCATTCAGCTAACGTTCTGCACCGTGACCTCAAGCCTTCCAACCTGCTGCTCAACACCACCTGTGATCTCAAGATCTGTGACTTTGGCCTGGCCCGTGTTGCAGATCCAGACCATGATCACACAGGGTTCCTGACAGAATATGTGGCCACACGTTGGTACAGGGCTCCAGAAATTATGTTGAATTCCAAGGGCTACACCAAGTCCATTGATATTTGGTCTGTAGGCTGCATTCTGGCAGAAATGCTTTCTAACAGGCCCATCTTTCCAGGGAAGCATTATCTTGACCAGCTGAACCACATTTTGGGTATTCTTGGATCCCCATCACAAGAAGACCTGAATTGTATAATAAATTTAAAAGCTAGGAACTATTTGCTTTCTCTTCCACACAAAAATAAGGTGCCATGGAACAGGCTGTTCCCAAATGCTGACTCCAAAGCTCTGGACTTATTGGACAAAATGTTGACATTCAACCCACACAAGAGGATTGAAGTAGAACAGGCTCTGGCCCACCCATATCTGGAGCAGTATTACGACCCGAGTGACGAGCCCATCGCCGAAGCACCATTCAAGTTCGACATGGAATTGGATGACTTGCCTAAGGAAAAGCTCAAAGAACTAATTTTTGAAGAGACTGCTAGATTCCAGCCAGGATACAGATCT</t>
-  </si>
-  <si>
-    <t>MDEQSQGMQGPPVPQFQPQKALRPDMGYNTLANFRIEKKIGRGQFSEVYRAACLLDGVPVALKKVQIFDLMDAKARADCIKEIDLLKQLNHPNVIKYYASFIEDNELNIVLELADAGDLSRMIKHFKKQKRLIPERTVWKYFVQLCSALEHMHSRRVMHRDIKPANVFITATGVVKLGDLGLGRFFSSKTTAAHSLVGTPYYMSPERIHENGYNFKSDIWSLGCLLYEMAALQSPFYGDKMNLYSLCKKIEQCDYPPLPSDHYSEELRQLVNMCINPDPEKRPDVTYVYDVAKRMHACTASS</t>
-  </si>
-  <si>
-    <t>GECSQKGPVPFSHCLPTEKLQRCEKIGEGVFGEVFQTIADHTPVAIKIIAIEGPDLVNGSHQKTFEEILPEIIISKELSLLSGEVCNRTEGFIGLNSVHCVQGSYPPLLLKAWDHYNSTKGSANDRPDFFKDDQLFIVLEFEFGGIDLEQMRTKLSSLATAKSILHQLTASLAVAEASLRFEHRDLHWGNVLLKKTSLKKLHYTLNGKSSTIPSCGLQVSIIDYTLSRLERDGIVVFCDVSMDEDLFTGDGDYQFDIYRLMKKENNNRWGEYHPYSNVLWLHYLTDKMLKQMTFKTKCNTPAMKQIKRKIQEFHRTMLNFSSATDLLCQHRLFK</t>
-  </si>
-  <si>
-    <t>MENFNNFYILTSKELGRGKFAVVRQCISKSTGQEYAAKFLKKRRRGQDCRAEILHEIAVLELAKSCPRVINLHEVYENTSEIILILEYAAGGEIFSLCLPELAEMVSENDVIRLIKQILEGVYYLHQNNIVHLDLKPQNILLSSIYPLGDIKIVDFGMSRKIGHACELREIMGTPEYLAPEILNYDPITTATDMWNIGIIAYMLLTHTSPFVGEDNQETYLNISQVNVDYSEETFSSVSQLATDFIQSLLVKNPEKRPTAEICLSHSWLQQWDFENLFHPEETSSSSQTQDHSVRSSEDKTSKSS</t>
-  </si>
-  <si>
-    <t>GCTGATCCAGAAGAACTGTTCACAAAATTAGAGCGCATTGGGAAAGGCTCATTTGGGGAAGTTTTCAAAGGAATTGATAACCGTACCCAGCAAGTCGTTGCTATTAAAATCATAGACCTTGAGGAAGCCGAAGATGAAATAGAAGACATTCAGCAAGAAATAACTGTCTTGAGTCAATGTGACAGCTCATATGTAACAAAATACTATGGGTCATATTTAAAGGGGTCTAAATTATGGATAATAATGGAATACCTGGGCGGTGGTTCAGCACTGGATCTTCTTCGAGCTGGTCCATTTGATGAGTTCCAGATTGCTACCATGCTAAAGGAAATTTTAAAAGGTCTGGACTATCTGCATTCAGAAAAGAAAATTCACCGAGACATAAAAGCTGCCAATGTCTTGCTCTCAGAACAAGGAGATGTTAAACTTGCTGATTTTGGAGTTGCTGGTCAGCTGACAGATACACAGATTAAAAGAAATACCTTTGTGGGAACTCCATTTTGGATGGCTCCTGAAGTTATTCAACAGTCAGCTTATGACTCAAAAGCTGACATTTGGTCATTGGGAATTACTGCTATTGAACTAGCCAAGGGAGAGCCACCTAACTCCGATATGCATCCAATGAGAGTTCTGTTTCTTATTCCCAAAAACAATCCTCCAACTCTTGTTGGAGACTTTACTAAGTCTTTTAAGGAGTTTATTGATGCTTGCCTGAACAAAGATCCATCATTTCGTCCTACAGCAAAAGAACTTCTGAAACACAAATTCATTGTAAAAAATTCAAAGAAGACTTCTTATCTGACTGAACTGATAGATCGTTTTAAGAGATGGAAGGCAGAA</t>
-  </si>
-  <si>
-    <t>MELRVGNKYRLGRKIGSGSFGDIYLGANIASGEEVAIKLECVKTKHPQLHIESKFYKMMQGGVGIPSIKWCGAEGDYNVMVMELLGPSLEDLFNFCSRKFSLKTVLLLADQMISRIEYIHSKNFIHRDVKPDNFLMGLGKKGNLVYIIDFGLAKKYRDARTHQHIPYRENKNLTGTARYASINTHLGIEQSRRDDLESLGYVLMYFNLGSLPWQGLKAATKRQKYERISEKKMSTPIEVLCKGYPSEFSTYLNFCRSLRFDDKPDYSYLRQLFRNLFHRQGFSYDYVFDWNMLK</t>
-  </si>
-  <si>
-    <t>SSVTASAAPGTASLVPDYWIDGSNRDALSDFFEVESELGRGATSIVYRCKQKGTQKPYALKVLKKTVDKKIVRTEIGVLLRLSHPNIIKLKEIFETPTEISLVLELVTGGELFDRIVEKGYYSERDAADAVKQILEAVAYLHENGIVHRDLKPENLLYATPAPDAPLKIADFGLSKIVEHQVLMKTVCGTPGYCAPEILRGCAYGPEVDMWSVGIITYILLCGFEPFYDERGDQFMFRRILNCEYYFISPWWDEVSLNAKDLVRKLIVLDPKKRLTTFQALQHPWVTGKAANFVHMDTAQKKLQEFNARRKLKAAVKAVVASSRLG</t>
-  </si>
-  <si>
-    <t>dna_end</t>
-  </si>
-  <si>
-    <t>MADDDVLFEDVYELCEVIGKGPFSVVRRCINRETGQQFAVKIVDVAKFTSSPGLSTEDLKREASICHMLKHPHIVELLETYSSDGMLYMVFEFMDGADLCFEIVKRADAGFVYSEAVASHYMRQILEALRYCHDNNIIHRDVKPHCVLLASKENSAPVKLGGFGVAIQLGESGLVAGGRVGTPHFMAPEVVKREPYGKPVDVWGCGVILFILLSGCLPFYGTKERLFEGIIKGKYKMNPRQWSHISESAKDLVRRMLMLDPAERITVYEALNHPWLKERDRYAYKIHLPETVEQLRKFNARRKLKGAVLAAVSSHKFNSFYGDPPEELPDFSEDPTSSGA</t>
-  </si>
-  <si>
-    <t>FAK1_HUMAN_D0_2IJM_B</t>
-  </si>
-  <si>
-    <t>DAPK1_HUMAN_D0_3F5G_A</t>
-  </si>
-  <si>
-    <t>CHK2_HUMAN_D0_2CN5_A</t>
-  </si>
-  <si>
-    <t>GTGATCGACCCCTCAGAGCTCACTTTTGTCCAAGAGATTGGCAGTGGGCAATTTGGGTTGGTGCATCTGGGCTACTGGCTCAACAAGGACAAGGTGGCTATCAAAACCATTCGGGAAGGGGCTATGTCAGAAGAGGACTTCATAGAGGAGGCTGAAGTAATGATGAAACTCTCTCATCCCAAACTGGTGCAGCTGTATGGGGTGTGCCTGGAGCAGGCCCCCATCTGCCTGGTGTTTGAGTTCATGGAGCACGGCTGCCTGTCAGATTATCTACGCACCCAGCGGGGACTTTTTGCTGCAGAGACCCTGCTGGGCATGTGTCTGGATGTGTGTGAGGGCATGGCCTACCTGGAAGAGGCATGTGTCATCCACAGAGACTTGGCTGCCAGAAATTGTTTGGTGGGAGAAAACCAAGTCATCAAGGTGTCTGACTTTGGGATGACAAGGTTCGTTCTGGATGATCAGTACACCAGTTCCACAGGCACCAAATTCCCGGTGAAGTGGGCATCCCCAGAGGTTTTCTCTTTCAGTCGCTATAGCAGCAAGTCCGATGTGTGGTCATTTGGTGTGCTGATGTGGGAAGTTTTCAGTGAAGGCAAAATCCCGTATGAAAACCGAAGCAACTCAGAGGTGGTGGAAGACATCAGTACCGGATTTCGGTTGTACAAGCCCCGGCTGGCCTCCACACACGTCTACCAGATTATGAATCACTGCTGGAAAGAGAGACCAGAAGATCGGCCAGCCTTCTCCAGACTGCTGCGTCAACTGGCTGAAATTGCAGAATCAGGACTT</t>
-  </si>
-  <si>
-    <t>MSDEEILEKLRSIVSVGDPKKKYTRFEKIGQGASGTVYTAMDVATGQEVAIKQMNLQQQPKKELIINEILVMRENKNPNIVNYLDSYLVGDELWVVMEYLAGGSLTDVVTETCMDEGQIAAVCRECLQALEFLHSNQVIHRDIKSDNILLGMDGSVKLTDFGFCAQITPEQSKRSTMVGTPYWMAPEVVTRKAYGPKVDIWSLGIKAIEMIEGEPPYLNENPLRALYLIATNGTPELQNPEKLSAIFRDFLNRCLEMDVEKRGSAKELLQHQFLKIAKPLSSLTPLIAAAKEATKNNH</t>
-  </si>
-  <si>
-    <t>MSQSKGKKRNPGLKIPKEAFEQPQTSSTPPRDLDSKACISIGNQNFEVKADDLEPIMELGRGAYGVVEKMRHVPSGQIMAVKRIRATVNSQEQKRLLMDLDISMRTVDCPFTVTFYGALFREGDVWICMELMDTSLDKFYKQVIDKGQTIPEDILGKIAVSIVKALEHLHSKLSVIHRDVKPSNVLINALGQVKMCDFGISGYLVDSVAKTIDAGCKPYMAPERINPELNQKGYSVKSDIWSLGITMIELAILRFPYDSWGTPFQQLKQVVEEPSPQLPADKFSAEFVDFTSQCLKKNSKERPTYPELMQHPFFTLHESKGTDVASFVKLILGD</t>
-  </si>
-  <si>
-    <t>DYRK2_HUMAN_D0_3KVW_A</t>
-  </si>
-  <si>
-    <t>GCGGCTCCACCGGCGAAAGAGATCCCGGAGGTCCTAGTGGACCCACGCAGCCGGCGGCGCTATGTGCGGGGCCGCTTTTTGGGCAAGGGCGGCTTTGCCAAGTGCTTCGAGATCTCGGACGCGGACACCAAGGAGGTGTTCGCGGGCAAGATTGTGCCTAAGTCTCTGCTGCTCAAGCCGCACCAGAGGGAGAAGATGTCCATGGAAATATCCATTCACCGCAGCCTCGCCCACCAGCACGTCGTAGGATTCCACGGCTTTTTCGAGGACAACGACTTCGTGTTCGTGGTGTTGGAGCTCTGCCGCCGGAGGTCTCTCCTGGAGCTGCACAAGAGGAGGAAAGCCCTGACTGAGCCTGAGGCCCGATACTACCTACGGCAAATTGTGCTTGGCTGCCAGTACCTGCACCGAAACCGAGTTATTCATCGAGACCTCAAGCTGGGCAACCTTTTCCTGAATGAAGATCTGGAGGTGAAAATAGGGGATTTTGGACTGGCAACCAAAGTCGAATATGACGGGGAGAGGAAGAAGACCCTGTGTGGGACTCCTAATTACATAGCTCCCGAGGTGCTGAGCAAGAAAGGGCACAGTTTCGAGGTGGATGTGTGGTCCATTGGGTGTATCATGTATACCTTGTTAGTGGGCAAACCACCTTTTGAGACTTCTTGCCTAAAAGAGACCTACCTCCGGATCAAGAAGAATGAATACAGTATTCCCAAGCACATCAACCCCGTGGCCGCCTCCCTCATCCAGAAGATGCTTCAGACAGATCCCACTGCCCGCCCAACCATTAACGAGCTGCTTAATGACGAGTTCTTTACTTCTGGCTATATCCCTGCCCGTCTCCCCATCACCTGCCTGACCATTCCACCAAGGTTTTCGATTGCTCCCAGCAGCCTGGACCCCAGCAACCGGAAGCCCCTCACAGTCCTCAATAAA</t>
-  </si>
-  <si>
-    <t>QSSKRSSRSVEDDKEGHLVCRIGDWLQERYEIVGNLGEGTFGKVVECLDHARGKSQVALKIIRNVGKYREAARLEINVLKKIKEKDKENKFLCVLMSDWFNFHGHMCIAFELLGKNTFEFLKENNFQPYPLPHVRHMAYQLCHALRFLHENQLTHTDLKPENILFVNSEFETLYNEHKSCEEKSVKNTSIRVADFGSATFDHEHHTTIVATRHYRPPEVILELGWAQPCDVWSIGCILFEYYRGFTLFQTHENREHLVMMEKILGPIPSHMIHRTRKQKYFYKGGLVWDENSSDGRYVKENCKPLKSYMLQDSLEHVQLFDLMRRMLEFDPAQRITLAEALLHPFFAGLTPEERSFHT</t>
-  </si>
-  <si>
-    <t>MK07_HUMAN_D0_4IC7_D</t>
-  </si>
-  <si>
-    <t>ATGCAGACAGTTGGTGTACATTCAATTGTTCAGCAGTTACACAGGAACAGTATTCAGTTTACTGATGGATATGAAGTAAAAGAAGATATTGGAGTTGGCTCCTACTCTGTTTGCAAGAGATGTATACATAAAGCTACAAACATGGAGTTTGCAGTGAAGATTATTGATAAAAGCAAGAGAGACCCAACAGAAGAAATTGAAATTCTTCTTCGTTATGGACAGCATCCAAACATTATCACTCTAAAGGATGTATATGATGATGGAAAGTATGTGTATGTAGTAACAGAACTTATGAAAGGAGGTGAATTGCTGGATAAAATTCTTAGACAAAAATTTTTCTCTGAACGAGAGGCCAGTGCTGTCCTGTTCACTATAACTAAAACCGTTGAATATCTTCACGCACAAGGGGTGGTTCATAGAGACTTGAAACCTAGCAACATTCTTTATGTGGATGAATCTGGTAATCCGGAATCTATTCGAATTTGTGATTTTGGCTTTGCAAAACAGCTGAGAGCGGAAAATGGTCTTCTCATGACTCCTTGTTACACTGCAAATTTTGTTGCACCAGAGGTTTTAAAAAGACAAGGCTATGATGCTGCTTGTGATATATGGAGTCTTGGTGTCCTACTCTATACAATGCTTACCGGTTACACTCCATTTGCAAATGGTCCTGATGATACACCAGAGGAAATATTGGCACGAATAGGTAGCGGAAAATTCTCACTCAGTGGTGGTTACTGGAATTCTGTTTCAGACACAGCAAAGGACCTGGTGTCAAAGATGCTTCATGTAGACCCTCATCAGAGACTGACTGCTGCTCTTGTGCTCAGACATCCTTGGATCGTCCACTGGGACCAACTGCCACAATACCAACTAAACAGACAGGATGCACCACATCTAGTAAAGGGTGCCATGGCAGCTACATATTCTGCTTTGAACCGTAATCAGTCACCAGTTTTGGAACCAGTAGGCCGCTCTACTCTTGCTCAGCGGAGAGGTATTAAAAAAATCACCTCAACAGCCCTG</t>
-  </si>
-  <si>
-    <t>KS6A3_HUMAN_D0_4JG7_A</t>
-  </si>
-  <si>
-    <t>MGKVKATPMTPEQAMKQYMQKLTAFEHHEIFSYPEIYFLGLNAKKRQGMTGGPNNGGYDDDQGSYVQVPHDHVAYRYEVLKVIGKGSFGQVVKAYDHKVHQHVALKMVRNEKRFHRQAAEEIRILEHLRKQDKDNTMNVIHMLENFTFRNHICMTFELLSMNLYELIKKNKFQGFSLPLVRKFAHSILQCLDALHKNRIIHCDLKPENILLKQQGRSGIKVIDFGSSCYEHQRVYTYIQSRFYRAPEVILGARYGMPIDMWSLGCILAELLTGYPLLPGEDEGDQLACMIELLGMPSQKLLDASKRAKNFVSSKGYPRYCTVTTLSDGSVVLNGGRSRRGKLRGPPESREWGNALKGCDDPLFLDFLKQCLEWDPAVRMTPGQALRHPWLRRRLPKPPTGEKTSVKR</t>
-  </si>
-  <si>
-    <t>CAGCAGTTCCCGCAGTTCCACGTCAAGTCCGGCCTGCAGATCAAGAAGAACGCCATCATCGATGACTACAAGGTCACCAGCCAGGTCCTGGGGCTGGGCATCAACGGCAAAGTTTTGCAGATCTTCAACAAGAGGACCCAGGAGAAATTCGCCCTCAAAATGCTTCAGGACTGCCCCAAGGCCCGCAGGGAGGTGGAGCTGCACTGGCGGGCCTCCCAGTGCCCGCACATCGTACGGATCGTGGATGTGTACGAGAATCTGTACGCAGGGAGGAAGTGCCTGCTGATTGTCATGGAATGTTTGGACGGTGGAGAACTCTTTAGCCGAATCCAGGATCGAGGAGACCAGGCATTCACAGAAAGAGAAGCATCCGAAATCATGAAGAGCATCGGTGAGGCCATCCAGTATCTGCATTCAATCAACATTGCCCATCGGGATGTCAAGCCTGAGAATCTCTTATACACCTCCAAAAGGCCCAACGCCATCCTGAAACTCACTGACTTTGGCTTTGCCAAGGAAACCACCAGCCACAACTCTTTGACCACTCCTTGTTATACACCGTACTATGTGGCTCCAGAAGTGCTGGGTCCAGAGAAGTATGACAAGTCCTGTGACATGTGGTCCCTGGGTGTCATCATGTACATCCTGCTGTGTGGGTATCCCCCCTTCTACTCCAACCACGGCCTTGCCATCTCTCCGGGCATGAAGACTCGCATCCGAATGGGCCAGTATGAATTTCCCAACCCAGAATGGTCAGAAGTATCAGAGGAAGTGAAGATGCTCATTCGGAATCTGCTGAAAACAGAGCCCACCCAGAGAATGACCATCACCGAGTTTATGAACCACCCTTGGATCATGCAATCAACAAAGGTCCCTCAAACCCCACTGCACACCAGCCGGGTCCTGAAGGAGGACAAGGAGCGGTGGGAGGATGTCAAGGGGTGTCTTCATGACAAGAACAGCGACCAGGCC</t>
-  </si>
-  <si>
-    <t>CDK2_HUMAN_D0_4BCP_A</t>
-  </si>
-  <si>
-    <t>MP2K4_HUMAN_D0_3ALN_C</t>
-  </si>
-  <si>
-    <t>CGGGACTCGAGTGATGATTGGGAGATTCCTGATGGGCAGATTACAGTGGGACAAAGAATTGGATCTGGATCATTTGGAACAGTCTACAAGGGAAAGTGGCATGGTGATGTGGCAGTGAAAATGTTGAATGTGACAGCACCTACACCTCAGCAGTTACAAGCCTTCAAAAATGAAGTAGGAGTACTCAGGAAAACACGACATGTGAATATCCTACTCTTCATGGGCTATTCCACAAAGCCACAACTGGCTATTGTTACCCAGTGGTGTGAGGGCTCCAGCTTGTATCACCATCTCCATATCATTGAGACCAAATTTGAGATGATCAAgCTTATAGATATTGCACGACAGACTGCACAGGGCATGGATTACTTACACGCCAAGTCAATCATCCACAGAGACCTCAAGAGTAATAATATATTTCTTCATGAAGACCTCACAGTAAAAATAGGTGATTTTGGTCTAGCTACAGTGAAATCTCGATGGAGTGGGTCCCATCAGTTTGAACAGTTGTCTGGgTCCATTTTGTGGATGGCACCAGAAGTCATCAGAATGCAAGATAAAAATCCATACAGCTTTCAGTCAGATGTATATGCATTTGGgATTGTTCTGTATGAATTGATGACTGGACAGTTACCTTATTCAAACATCAACAACAGGGACCAGATAATTTTTATGGTGGGACGAGGATACCTGTCTCCAGATCTCAGTAAGGTACGGAGTAACTGTCCAAAAGCCATGAAGAGATTAATGGCAGAGTGCCTCAAAAAGAAAAGAGATGAGAGACCACTCTTTCCCCAAATTCTCGCCTCTATTGAGCTGCTGGCCCGC</t>
-  </si>
-  <si>
-    <t>ACCACCTCACTTGAAGCTTTGCCCACAGGGACAGTGCTGACAGACAAGAGTGGGCGACAGTGGAAGCTGAAGTCCTTCCAGACCAGGGACAACCAGGGCATTCTCTATGAAGCTGCACCCACCTCCACCCTCACCTGTGACTCAGGACCACAGAAGCAAAAGTTCTCACTCAAACTGGATGCCAAGGATGGGCGCTTGTTCAATGAGCAGAACTTCTTCCAGCGGGCCGCCAAGCCTCTGCAAGTCAACAAGTGGAAGAAGCTGTACTCGACCCCACTGCTGGCCATCCCTACCTGCATGGGTTTCGGTGTTCACCAGGACAAATACAGGTTCTTGGTGTTACCCAGCCTGGGGAGGAGCCTTCAGTCGGCCCTGGATGTCAGCCCAAAGCATGTGCTGTCAGAGAGGTCTGTGCTGCAGGTGGCCTGCCGGCTGCTGGATGCCCTGGAGTTCCTCCATGAGAATGAGTATGTTCATGGAAATGTGACAGCTGAAAATATCTTTGTGGATCCAGAGGACCAGAGTCAGGTGACTTTGGCAGGCTATGGCTTCGCCTTCCGCTATTGCCCAAGTGGCAAACACGTGGCCTACGTGGAAGGCAGCAGGAGCCCTCACGAGGGGGACCTTGAGTTCATTAGCATGGACCTGCACAAGGGATGCGGGCCCTCCCGCCGCAGCGACCTCCAGAGCCTGGGCTACTGCATGCTGAAGTGGCTCTACGGGTTTCTGCCATGGACAAATTGCCTTCCCAACACTGAGGACATCATGAAGCAAAAACAGAAGTTTGTTGATAAGCCGGGGCCCTTCGTGGGACCCTGCGGTCACTGGATCAGGCCCTCAGAGACCCTGCAGAAGTACCTGAAGGTGGTGATGGCCCTCACGTATGAGGAGAAGCCGCCCTACGCCATGCTGAGGAACAACCTAGAAGCTTTGCTGCAGGATCTGCGTGTGTCTCCATATGACCCCATTGGCCTCCCGATGGTGCCC</t>
-  </si>
-  <si>
-    <t>TCACCACAGCGGGAGCCACAGCGAGTATCCCATGAGCAGTTCCGGGCTGCCCTGCAGCTGGTGGTGGACCCAGGCGACCCCCGCTCCTACCTGGACAACTTCATCAAGATTGGCGAGGGCTCCACGGGCATCGTGTGCATCGCCACCGTGCGCAGCTCGGGCAAGCTGGTGGCCGTCAAGAAGATGGACCTGCGCAAGCAGCAGAGGCGCGAGCTGCTCTTCAACGAGGTGGTAATCATGAGGGACTACCAGCACGAGAATGTGGTGGAGATGTACAACAGCTACCTGGTGGGGGACGAGCTCTGGGTGGTCATGGAGTTCCTGGAAGGAGGCGCCCTCACCGACATCGTCACCCACACCAGGATGAACGAGGAGCAGATCGCGGCCGTGTGCCTTGCAGTGCTGCAGGCCCTGTCGGTGCTCCACGCCCAGGGCGTCATCCACCGGGACATCAAGAGCGACTCGATCCTGCTGACCCATGATGGCAGGGTGAAGCTGTCAGACTTTGGGTTCTGCGCCCAGGTGAGCAAGGAAGTGCCCCGAAGGAAGTCGCTGGTCGGCACGCCCTACTGGATGGCCCCAGAGCTCATCTCCCGCCTTCCCTACGGGCCAGAGGTAGACATCTGGTCGCTGGGGATAATGGTGATTGAGATGGTGGACGGAGAGCCCCCCTACTTCAACGAGCCACCCCTCAAAGCCATGAAGATGATTCGGGACAACCTGCCACCCCGACTGAAGAACCTGCACAAGGTGTCGCCATCCCTGAAGGGCTTCCTGGACCGCCTGCTGGTGCGAGACCCTGCCCAGCGGGCCACGGCAGCCGAGCTGCTGAAGCACCCATTCCTGGCCAAGGCAGGGCCGCCTGCCAGCATCGTGCCCCTCATGCGCCAGAACCGCACCAGA</t>
-  </si>
-  <si>
-    <t>SIESSGKLKISPEQHWDFTAEDLKDLGEIGRGAYGSVNKMVHKPSGQIMAVKRIRSTVDEKEQKQLLMDLDVVMRSSDCPYIVQFYGALFREGDCWICMELMSTSFDKFYKYVYSVLDDVIPEEILGKITLATVKALNHLKENLKIIHRDIKPSNILLDRSGNIKLCDFGISGQLVDSIAKTRDAGCRPYMAPERIDPSASRQGYDVRSDVWSLGITLYELATGRFPYPKWNSVFDQLTQVVKGDPPQLSNSEEREFSPSFINFVNLCLTKDESKRPKYKELLKHPFILMYEERAVEVACYVCKILDQMPATPSSPMYVD</t>
-  </si>
-  <si>
-    <t>TDSFSGRFEDVYQLQEDVLGEGAHARVQTCINLITSQEYAVKIIEKQPGHIRSRVFREVEMLYQCQGHRNVLELIEFFEEEDRFYLVFEKMRGGSILSHIHKRRHFNELEASVVVQDVASALDFLHNKGIAHRDLKPENILCEHPNQVSPVKICDFDLGSGIKLNGDCSPISTPELLTPCGSAEYMAPEVVEAFSEEASIYDKRCDLWSLGVILYILLSGYPPFVGRCGSDCGWDRGEACPACQNMLFESIQEGKYEFPDKDWAHISCAAKDLISKLLVRDAKQRLSAAQVLQHPWVQGCAPENTLPTPMVLQR</t>
-  </si>
-  <si>
-    <t>WALNMKELKLLQTIGKGEFGDVMLGDYRGNKVAVKCIKNDATAQAFLAEASVMTQLRHSNLVQLLGVIVEEKGGLYIVTEYMAKGSLVDYLRSRGRSVLGGDCLLKFSLDVCEAMEYLEGNNFVHRDLAARNVLVSEDNVAKVSDFGLTKEASSTQDTGKLPVKWTAPEALREKKFSTKSDVWSFGILLWEIYSFGRVPYPRIPLKDVVPRVEKGYKMDAPDGCPPAVYEVMKNCWHLDAAMRPSFLQLREQLEHIKTHELHL</t>
-  </si>
-  <si>
-    <t>MPGPAAGSRARVYAEVNSLRSREYWDYEAHVPSWGNQDDYQLVRKLGRGKYSEVFEAINITNNERVVVKILKPVKKKKIKREVKILENLRGGTNIIKLIDTVKDPVSKTPALVFEYINNTDFKQLYQILTDFDIRFYMYELLKALDYCHSKGIMHRDVKPHNVMIDHQQKKLRLIDWGLAEFYHPAQEYNVRVASRYFKGPELLVDYQMYDYSLDMWSLGCMLASMIFRREPFFHGQDNYDQLVRIAKVLGTEELYGYLKKYHIDLDPHFNDILGQHSRKRWENFIHSENRHLVSPEALDLLDKLLRYDHQQRLTAKEAMEHPYFYPVVKEQSQ</t>
-  </si>
-  <si>
-    <t>AAGAGGCAGTGGGCTTTGGAAGACTTTGAAATTGGTCGCCCTCTGGGTAAAGGAAAGTTTGGTAATGTTTATTTGGCAAGAGAAAAGCAAAGCAAGTTTATTCTGGCTCTTAAAGTGTTATTTAAAGCTCAGCTGGAGAAAGCCGGAGTGGAGCATCAGCTCAGAAGAGAAGTAGAAATACAGTCCCACCTTCGGCATCCTAATATTCTTAGACTGTATGGTTATTTCCATGATGCTACCAGAGTCTACCTAATTCTGGAATATGCACCACTTGGAACAGTTTATAGAGAACTTCAGAAACTTTCAAAGTTTGATGAGCAGAGAACTGCTACTTATATAACAGAATTGGCAAATGCCCTGTCTTACTGTCATTCGAAGAGAGTTATTCATAGAGACATTAAGCCAGAGAACTTACTTCTTGGATCAGCTGGAGAGCTTAAAATTGCAGATTTTGGGTGGTCAGTACATGCTCCATCTTCCAGGAGGACCACTCTCTGTGGCACCCTGGACTACCTGCCCCCTGAAATGATTGAAGGTCGGATGCATGATGAGAAGGTGGATCTCTGGAGCCTTGGAGTTCTTTGCTATGAATTTTTAGTTGGGAAGCCTCCTTTTGAGGCAAACACATACCAAGAGACCTACAAAAGAATATCACGGGTTGAATTCACATTCCCTGACTTTGTAACAGAGGGAGCCAGGGACCTCATTTCAAGACTGTTGAAGCATAATCCCAGCCAGAGGCCAATGCTCAGAGAAGTACTTGAACACCCCTGGATCACAGCAAATTCATCAAAACCATCA</t>
-  </si>
-  <si>
-    <t>ATGGAGCTACGTGTGGGGAACAAGTACCGCCTGGGACGGAAGATCGGGAGCGGGTCCTTCGGAGATATCTACCTGGGTGCCAACATCGCCTCTGGTGAGGAAGTCGCCATCAAGCTGGAGTGTGTGAAGACAAAGCACCCCCAGCTGCACATCGAGAGCAAGTTCTACAAGATGATGCAGGGTGGCGTGGGGATCCCGTCCATCAAGTGGTGCGGAGCTGAGGGCGACTACAACGTGATGGTCATGGAGCTGCTGGGGCCTAGCCTCGAGGACCTGTTCAACTTCTGTTCCCGCAAATTCAGCCTCAAGACGGTGCTGCTCTTGGCCGACCAGATGATCAGCCGCATCGAGTATATCCACTCCAAGAACTTCATCCACCGGGACGTCAAGCCCGACAACTTCCTCATGGGGCTGGGGAAGAAGGGCAACCTGGTCTACATCATCGACTTCGGCCTGGCCAAGAAGTACCGGGACGCCCGCACCCACCAGCACATTCCCTACCGGGAAAACAAGAACCTGACCGGCACGGCCCGCTACGCTTCCATCAACACGCACCTGGGCATTGAGCAAAGCCGTCGAGATGACCTGGAGAGCCTGGGCTACGTGCTCATGTACTTCAACCTGGGCTCCCTGCCCTGGCAGGGGCTCAAAGCAGCCACCAAGCGCCAGAAGTATGAACGGATCAGCGAGAAGAAGATGTCAACGCCCATCGAGGTCCTCTGCAAAGGCTATCCCTCCGAATTCTCAACATACCTCAACTTCTGCCGCTCCCTGCGGTTTGACGACAAGCCCGACTACTCTTACCTACGTCAGCTCTTCCGCAACCTCTTCCACCGGCAGGGCTTCTCCTATGACTACGTCTTTGACTGGAACATGCTGAAA</t>
-  </si>
-  <si>
-    <t>MK03_HUMAN_D0_2ZOQ_B</t>
-  </si>
-  <si>
-    <t>ATGTCTCAGTCGAAAGGCAAGAAGCGAAACCCTGGCCTTAAAATTCCAAAAGAAGCATTTGAACAACCTCAGACCAGTTCCACACCACCTCGAGATTTAGACTCCAAGGCTTGCATTTCTATTGGAAATCAGAACTTTGAGGTGAAGGCAGATGACCTGGAGCCTATAATGGAACTGGGACGAGGTGCGTACGGGGTGGTGGAGAAGATGCGGCACGTGCCCAGCGGGCAGATCATGGCAGTGAAGCGGATCCGAGCCACAGTAAATAGCCAGGAACAGAAACGGCTACTGATGGATTTGGATATTTCCATGAGGACGGTGGACTGTCCATTCACTGTCACCTTTTATGGCGCACTGTTTCGGGAGGGTGATGTGTGGATCTGCATGGAGCTCATGGATACATCACTAGATAAATTCTACAAACAAGTTATTGATAAAGGCCAGACAATTCCAGAGGACATCTTAGGGAAAATAGCAGTTTCTATTGTAAAAGCATTAGAACATTTACATAGTAAGCTGTCTGTCATTCACAGAGACGTCAAGCCTTCTAATGTACTCATCAATGCTCTCGGTCAAGTGAAGATGTGCGATTTTGGAATCAGTGGCTACTTGGTGGACTCTGTTGCTAAAACAATTGATGCAGGTTGCAAACCATACATGGCCCCTGAAAGAATAAACCCAGAGCTCAACCAGAAGGGATACAGTGTGAAGTCTGACATTTGGAGTCTGGGCATCACGATGATTGAGTTGGCCATCCTTCGATTTCCCTATGATTCATGGGGAACTCCATTTCAGCAGCTCAAACAGGTGGTAGAGGAGCCATCGCCACAACTCCCAGCAGACAAGTTCTCTGCAGAGTTTGTTGACTTTACCTCACAGTGCTTAAAGAAGAATTCCAAAGAACGGCCTACATACCCAGAGCTAATGCAACATCCATTTTTCACCCTACATGAATCCAAAGGAACAGATGTGGCATCTTTTGTAAAACTGATTCTTGGAGAC</t>
-  </si>
-  <si>
-    <t>TCAACCAGGGATTATGAGATTCAAAGAGAAAGAATAGAACTTGGACGATGTATTGGAGAAGGCCAATTTGGAGATGTACATCAAGGCATTTATATGAGTCCAGAGAATCCAGCTTTGGCGGTTGCAATTAAAACATGTAAAAACTGTACTTCGGACAGCGTGAGAGAGAAATTTCTTCAAGAAGCCTTAACAATGCGTCAGTTTGACCATCCTCATATTGTGAAGCTGATTGGAGTCATCACAGAGAATCCTGTCTGGATAATCATGGAGCTGTGCACACTTGGAGAGCTGAGGTCATTTTTGCAAGTAAGGAAATACAGTTTGGATCTAGCATCTTTGATCCTGTATGCCTATCAGCTTAGTACAGCTCTTGCATATCTAGAGAGCAAAAGATTTGTACACAGGGACATTGCTGCTCGGAATGTTCTGGTGTCCTCAAATGATTGTGTAAAATTAGGAGACTTTGGATTATCCCGATATATGGAAGATAGTACTTACTACAAAGCTTCCAAAGGAAAATTGCCTATTAAATGGATGGCTCCAGAGTCAATCAATTTTCGACGTTTTACCTCAGCTAGTGACGTATGGATGTTTGGTGTGTGTATGTGGGAGATACTGATGCATGGTGTGAAGCCTTTTCAAGGAGTGAAGAACAATGATGTAATCGGTCGAATTGAAAATGGGGAAAGATTACCAATGCCTCCAAATTGTCCTCCTACCCTCTACAGCCTTATGACGAAATGCTGGGCCTATGACCCCAGCAGGCGGCCCAGGTTTACTGAACTTAAAGCTCAGCTCAGCACAATCCTGGAGGAAGAGAAGGCTCAGCAAGAAGAG</t>
-  </si>
-  <si>
-    <t>DPEELFTKLEKIGKGSFGEVFKGIDNRTQKVVAIKIIDLEEAEDEIEDIQQEITVLSQCDSPYVTKYYGSYLKDTKLWIIMEYLGGGSALDLLEPGPLDETQIATILREILKGLDYLHSEKKIHRDIKAANVLLSEHGEVKLADFGVAGQLTDTQIKRNTFVGTPFWMAPEVIKQSAYDSKADIWSLGITAIELARGEPPHSELHPMKVLFLIPKNNPPTLEGNYSKPLKEFVEACLNKEPSFRPTAKELLKHKFILRNAKKTSYLTELID</t>
-  </si>
-  <si>
-    <t>MAPK3_HUMAN_D0_3FXW_A</t>
-  </si>
-  <si>
-    <t>AAGCAGTACGAACACGTGAAGAGGGACCTGAACCCCGAAGACTTTTGGGAGATTATAGGAGAACTGGGCGACGGAGCCTTTGGGAAAGTGTACAAGGCCCAGAATAAAGAGACCAGTGTTTTAGCTGCTGCAAAAGTGATTGACACTAAATCTGAAGAAGAACTTGAAGATTACATGGTAGAGATTGACATATTAGCATCTTGTGATCACCCAAATATAGTCAAGCTTCTAGATGCCTTCTATTATGAGAACAATCTTTGGATCCTCATTGAATTTTGTGCAGGTGGAGCAGTAGATGCTGTGATGCTTGAACTTGAGAGACCATTAACTGAGTCCCAAATACAAGTAGTTTGCAAGCAGACTTTAGATGCATTGAACTACTTACATGATAATAAGATCATCCACAGAGATCTGAAGGCTGGCAACATTCTCTTTACCTTAGATGGAGATATCAAATTGGCGGATTTTGGAGTATCAGCTAAAAACATGAGGACAATTCAAAGAAGAGATTCCTTTATTGGTACACCATATTGGATGGCTCCTGAAGTAGTCATGTGTGAAACATCTAAGGACAGACCCTATGACTACAAAGCTGATGTTTGGTCCCTGGGTATCACTTTAATAGAAATGGCTGAGATAGAACCACCTCATCATGAATTAAATCCAATGCGAGTGCTGCTAAAAATAGCAAAATCTGAGCCACCTACATTAGCACAGCCATCCAGATGGTCTTCAAATTTTAAGGACTTTCTAAAGAAATGCTTAGAAAAGAATGTGGATGCCAGGTGGACTACATCTCAGCTGCTGCAGCATCCCTTTGTTACTGTTGATTCCAACAAACCCATCCGAGAATTGATTGCAGAGGCGAAGGCTGAAGTAACAGAAGAAGTTGAAGATGGCAAAGAG</t>
-  </si>
-  <si>
-    <t>ATGCCTTCCCGGGCTGAGGACTATGAAGTGTTGTACACCATTGGCACAGGCTCCTACGGCCGCTGCCAGAAGATCCGGAGGAAGAGTGATGGCAAGATATTAGTTTGGAAAGAACTTGACTATGGCTCCATGACAGAAGCTGAGAAACAGATGCTTGTTTCTGAAGTGAATTTGCTTCGTGAACTGAAACATCCAAACATCGTTCGTTACTATGATCGGATTATTGACCGGACCAATACAACACTGTACATTGTAATGGAATATTGTGAAGGAGGGGATCTGGCTAGTGTAATTACAAAGGGAACCAAGGAAAGGCAATACTTAGATGAAGAGTTTGTTCTTCGAGTGATGACTCAGTTGACTCTGGCCCTGAAGGAATGCCACAGACGAAGTGATGGTGGTCATACCGTATTGCATCGGGATCTGAAACCAGCCAATGTTTTCCTGGATGGCAAGCAAAACGTCAAGCTTGGAGACTTTGGGCTAGCTAGAATATTAAACCATGACACGAGTTTTGCAAAAACATTTGTTGGCACACCTTATTACATGTCTCCTGAACAAATGAATCGCATGTCCTACAATGAGAAATCAGATATCTGGTCATTGGGCTGCTTGCTGTATGAGTTATGTGCATTAATGCCTCCATTTACAGCTTTTAGCCAGAAAGAACTCGCTGGGAAAATCAGAGAAGGCAAATTCAGGCGAATTCCATACCGTTACTCTGATGAATTGAATGAAATTATTACGAGGATGTTAAACTTAAAGGATTACCATCGACCTTCTGTTGAAGAAATTCTTGAGAACCCTTTAATA</t>
-  </si>
-  <si>
-    <t>TVFRQENVDDYYDTGEELGSGQFAVVKKCREKSTGLQYAAKFIKKRRTKSSRRGVSREDIEREVSILKEIQHPNVITLHEVYENKTDVILILELVAGGELFDFLAEKESLTEEEATEFLKQTLNGVYYLHSLQIAHFDLKPENIMLLDRNVPKPRIKIIDFGLAHKIDFGNEFKNIFGTPEFVAPEIVNYEPLGLEADMWSIGVITYILLSGASPFLGDTKQETLANVSAVNYEFEDEYFSNTSALAKDFIRRLLVKDPKKRMTIQDSLQHPWIKPKDTQQALS</t>
-  </si>
-  <si>
-    <t>GATGAACAACCTCACATCGGAAACTACAGACTGTTGAAAACAATCGGCAAGGGGAATTTTGCAAAAGTAAAATTGGCAAGACATATCCTTACAGGCAGAGAGGTTGCAATAAAAATAATTGACAAAACTCAGTTGAATCCAACAAGTCTACAAAAGCTCTTCAGAGAAGTAAGAATAATGAAGATTTTAAATCATCCCAATATAGTGAAGTTATTCGAAGTCATTGAAACTGAAAAAACACTCTACCTAATCATGGAATATGCAAGTGGAGGTGAAGTATTTGACTATTTGGTTGCACATGGCAGGATGAAGGAAAAAGAAGCAAGATCTAAATTTAGACAGATTGTGTCTGCAGTTCAATACTGCCATCAGAAACGGATCGTACATCGAGACCTCAAGGCTGAAAATCTATTGTTAGATGCCGATATGAACATTAAAATAGCAGATTTCGGTTTTAGCAATGAATTTACTGTTGGCGGTAAACTCGACACGTTTTGTGGCAGTCCTCCATACGCAGCACCTGAGCTCTTCCAGGGCAAGAAATATGACGGGCCAGAAGTGGATGTGTGGAGTCTGGGGGTCATTTTATACACACTAGTCAGTGGCTCACTTCCCTTTGATGGGCAAAACCTAAAGGAACTGAGAGAGAGAGTATTAAGAGGGAAATACAGAATTCCCTTCTACATGTCTACAGACTGTGAAAACCTTCTCAAACGTTTCCTGGTGCTAAATCCAATTAAACGCGGCACTCTAGAGCAAATCATGAAGGACAGGTGGATCAATGCAGGGCATGAAGAAGATGAACTCAAACCATTTGTTGAACCAGAGCTAGACATCTCAGACCAAAAAAGAATAGATATTATGGTGGGAATGGGATATTCACAAGAAGAAATTCAAGAATCTCTTAGTAAGATGAAATACGATGAAATCACAGCTACATATTTGTTATTGGGGAGAAAATCTTCAGAG</t>
-  </si>
-  <si>
-    <t>CACCAGCTGCAGCCCCGGCGGGTGTCATTCCGGGGCGAGGCCTCAGAGACTCTGCAGAGCCCTGGGTATGACCCAAGCCGGCCAGAGTCCTTCTTCCAGCAGAGCTTCCAGAGGCTCAGCCGCCTGGGCCATGGCTCCTACGGAGAGGTCTTCAAGGTGCGCTCCAAGGAGGACGGCCGGCTCTATGCGGTAAAGCGTTCCATGTCACCATTCCGGGGCCCCAAGGACCGGGCCCGCAAGTTGGCCGAGGTGGGCAGCCACGAGAAGGTGGGGCAGCACCCATGCTGCGTGCGGCTGGAGCAGGCCTGGGAGGAGGGCGGCATCCTGTACCTGCAGACGGAGCTGTGCGGGCCCAGCCTGCAGCAACACTGTGAGGCCTGGGGTGCCAGCCTGCCTGAGGCCCAGGTCTGGGGCTACCTGCGGGACACGCTGCTTGCCCTGGCCCATCTGCACAGCCAGGGCCTGGTGCACCTTGATGTCAAGCCTGCCAACATCTTCCTGGGGCCCCGGGGCCGCTGCAAGCTGGGTGACTTCGGACTGCTGGTGGAGCTGGGTACAGCAGGAGCTGGTGAGGTCCAGGAGGGAGACCCCCGCTACATGGCCCCCGAGCTGCTGCAGGGCTCCTATGGGACAGCAGCGGATGTGTTCAGTCTGGGCCTCACCATCCTGGAAGTGGCATGCAACATGGAGCTGCCCCACGGTGGGGAGGGCTGGCAGCAGCTGCGCCAGGGCTACCTGCCCCCTGAGTTCACTGCCGGTCTGTCTTCCGAGCTGCGTTCTGTCCTTGTCATGATGCTGGAGCCAGACCCCAAGCTGCGGGCCACGGCCGAGGCCCTGCTGGCACTGCCTGTGTTGAGGCAGCCG</t>
-  </si>
-  <si>
-    <t>KEKEPLESQYQVGPLLGSGGFGSVYSGIRVSDNLPVAIKHVEKDRISDWGELPNGTRVPMEVVLLKKVSSGFSGVIRLLDWFERPDSFVLILERPEPVQDLFDFITERGALQEELARSFFWQVLEAVRHCHNCGVLHRDIKDENILIDLNRGELKLIDFGSGALLKDTVYTDFDGTRVYSPPEWIRYHRYHGRSAAVWSLGILLYDMVCGDIPFEHDEEIIGGQVFFRQRVSSECQHLIRWCLALRPSDRPTFEEIQNHPWMQDVLLPQETAEIHLHSLSPGPSK</t>
-  </si>
-  <si>
-    <t>VEDHYEMGEELGSGQFAIVRKCRQKGTGKEYAAKFIKKRRLSSSRRGVSREEIEREVNILREIRHPNIITLHDIFENKTDVVLILELVSGGELFDFLAEKESLTEDEATQFLKQILDGVHYLHSKRIAHFDLKPENIMLLDKNVPNPRIKLIDFGIAHKIEAGNEFKNIFGTPEFVAPEIVNYEPLGLEADMWSIGVITYILLSGASPFLGETKQETLTNISAVNYDFDEEYFSNTSELAKDFIRRLLVKDPKRRMTIAQSLEHSWIKAIRRRNVRGEDSG</t>
-  </si>
-  <si>
-    <t>MET_HUMAN_D0_4EEV_A</t>
-  </si>
-  <si>
-    <t>MSSFLPEGGCYELLTVIGKGFEDLMTVNLARYKPTGEYVTVRRINLEACSNEMVTFLQGELHVSKLFNHPNIVPYRATFIADNELWVVTSFMAYGSAKDLICTHFMDGMNELAIAYILQGVLKALDYIHHMGYVHRSVKASHILISVDGKVYLSGLRSNLSMISHGQRQRVVHDFPKYSVKVLPWLSPEVLQQNLQGYDAKSDIYSVGITACELANGHVPFKDMPATQMLLEKLNGTVPCLLDTSTIPAEELTMSPSRSVANSGLSDSLTTSTPRPSNGDSPSHPYHRTFSPHFHHFVEQCLQRNPDARPSASTLLNHSFFKQIKRRASEVLPELLRPVTPITNFEGSQSQDHSGIFGLVTNLEELEVDDWEF</t>
-  </si>
-  <si>
-    <t>MP2K1_HUMAN_D0_3MBL_A</t>
-  </si>
-  <si>
-    <t>ATGTCGGGACCCGTGCCAAGCAGGGCCAGAGTTTACACAGATGTTAATACACACAGACCTCGAGAATACTGGGATTACGAGTCACATGTGGTGGAATGGGGAAATCAAGATGACTACCAGCTGGTTCGAAAATTAGGCCGAGGTAAATACAGTGAAGTATTTGAAGCCATCAACATCACAAATAATGAAAAAGTTGTTGTTAAAATTCTCAAGCCAGTAAAAAAGAAGAAAATTAAGCGTGAAATAAAGATTTTGGAGAATTTGAGAGGAGGTCCCAACATCATCACACTGGCAGACATTGTAAAAGACCCTGTGTCACGAACCCCCGCCTTGGTTTTTGAACACGTAAACAACACAGACTTCAAGCAATTGTACCAGACGTTAACAGACTATGATATTCGATTTTACATGTATGAGATTCTGAAGGCCCTGGATTATTGTCACAGCATGGGAATTATGCACAGAGATGTCAAGCCCCATAATGTCATGATTGATCATGAGCACAGAAAGCTACGACTAATAGACTGGGGTTTGGCTGAGTTTTATCATCCTGGCCAAGAATATAATGTCCGAGTTGCTTCCCGATACTTCAAAGGTCCTGAGCTACTTGTAGACTATCAGATGTACGATTATAGTTTGGATATGTGGAGTTTGGGTTGTATGCTGGCAAGTATGATCTTTCGGAAGGAGCCATTTTTCCATGGACATGACAATTATGATCAGTTGGTGAGGATAGCCAAGGTTCTGGGGACAGAAGATTTATATGACTATATTGACAAATACAACATTGAATTAGATCCACGTTTCAATGATATCTTGGGCAGACACTCTCGAAAGCGATGGGAACGCTTTGTCCACAGTGAAAATCAGCACCTTGTCAGCCCTGAGGCCTTGGATTTCCTGGACAAACTGCTGCGATATGACCACCAGTCACGGCTTACTGCAAGAGAGGCAATGGAGCACCCCTATTTCTACACTGTTGTGAAGGACCAGGCTCGAATGGGT</t>
-  </si>
-  <si>
-    <t>CDKL1_HUMAN_D0_4AGU_C</t>
-  </si>
-  <si>
-    <t>MARK3_HUMAN_D0_2QNJ_A</t>
-  </si>
-  <si>
-    <t>NLVFSDGYVVKETIGVGSYSECKRCVHKATNMEYAVKVIDKSKRDPSEEIEILLRYGQHPNIITLKDVYDDGKHVYLVTELMRGGELLDKILRQKFFSEREASFVLHTIGKTVEYLHSQGVVHRDLKPSNILYVDESGNPECLRICDFGFAKQLRAENGLLMTPCYTANFVAPEVLKRQGYDEGCDIWSLGILLYTMLAGYTPFANGPSDTPEEILTRIGSGKFTLSGGNWNTVSETAKDLVSKMLHVDPHQRLTAKQVLQHPWVTQKDKLPQSQLSHQDLQLVKGAMAATYSALNSSKPTPQLKPIESSILAQRRVRKLPSTTL</t>
-  </si>
-  <si>
-    <t>GGTGTTGTGACACATGAGCAGTTCAAGGCTGCGCTCAGGATGGTGGTGGACCAGGGTGACCCCCGGCTGCTGCTGGACAGCTACGTGAAGATTGGCGAGGGCTCCACCGGCATCGTCTGCTTGGCCCGGGAGAAGCACTCGGGCCGCCAGGTGGCCGTCAAGATGATGGACCTCAGGAAGCAGCAGCGCAGGGAGCTGCTCTTCAACGAGGTGGTGATCATGCGGGACTACCAGCACTTCAACGTGGTGGAGATGTACAAGAGCTACCTGGTGGGCGAGGAGCTGTGGGTGCTCATGGAGTTCCTGCAGGGAGGAGCCCTCACAGACATCGTCTCCCAAGTCAGGCTGAATGAGGAGCAGATTGCCACTGTGTGTGAGGCTGTGCTGCAGGCCCTGGCCTACCTGCATGCTCAGGGTGTCATCCACCGGGACATCAAGAGTGACTCCATCCTGCTGACCCTCGATGGCAGGGTGAAGCTCTCGGACTTCGGATTCTGTGCTCAGATCAGCAAAGACGTCCCTAAGAGGAAGTCCCTGGTGGGAACCCCCTACTGGATGGCTCCTGAAGTGATCTCCAGGTCTTTGTATGCCACTGAGGTGGATATCTGGTCTCTGGGCATCATGGTGATTGAGATGGTAGATGGGGAGCCACCGTACTTCAGTGACTCCCCAGTGCAAGCCATGAAGAGGCTCCGGGACAGCCCCCCACCCAAGCTGAAAAACTCTCACAAGGTCTCCCCAGTGCTGCGAGACTTCCTGGAGCGGATGCTGGTGCGGGACCCCCAAGAGAGAGCCACAGCCCAGGAGCTCCTAGACCACCCCTTCCTGCTGCAGACAGGGCTACCTGAGTGCCTGGTGCCCCTGATCCAGCTCTACCGAAAGCAGACCTCCACCTGC</t>
-  </si>
-  <si>
-    <t>CACATTGGAAACTACCGGCTCCTCAAGACCATTGGCAAGGGTAATTTTGCCAAGGTGAAGTTGGCCCGACACATCCTGACTGGGAAAGAGGTAGCTGTGAAGATCATTGACAAGACTCAACTGAACTCCTCCAGCCTCCAGAAACTATTCCGCGAAGTAAGAATAATGAAGGTTTTGAATCATCCCAACATAGTTAAATTATTTGAAGTGATTGAGACTGAGAAAACGCTCTACCTTGTCATGGAGTACGCTAGTGGCGGAGAGGTATTTGATTACCTAGTGGCTCATGGCAGGATGAAAGAAAAAGAGGCTCGAGCCAAATTCCGCCAGATAGTGTCTGCTGTGCAGTACTGTCACCAGAAGTTTATTGTCCATAGAGACTTAAAGGCAGAAAACCTGCTCTTGGATGCTGATATGAACATCAAGATTGCAGACTTTGGCTTCAGCAATGAATTCACCTTTGGGAACAAGCTGGACACCTTCTGTGGCAGTCCCCCTTATGCTGCCCCAGAACTCTTCCAGGGCAAAAAATATGATGGACCCGAGGTGGATGTGTGGAGCCTAGGAGTTATCCTCTATACACTGGTCAGCGGATCCCTGCCTTTTGATGGACAGAACCTCAAGGAGCTGCGGGAACGGGTACTGAGGGGAAAATACCGTATTCCATTCTACATGTCCACGGACTGTGAAAACCTGCTTAAGAAATTTCTCATTCTTAATCCCAGCAAGAGAGGCACTTTAGAGCAAATCATGAAAGATCGATGGATGAATGTGGGTCACGAAGATGATGAACTAAAGCCTTACGTGGAGCCACTCCCTGACTACAAGGACCCCCGGCGGACAGAGCTGATGGTGTCCATGGGTTATACACGGGAAGAGATCCAGGACTCGCTGGTGGGCCAGAGATACAACGAGGTGATGGCCACCTATCTGCTCCTGGGCTAC</t>
-  </si>
-  <si>
-    <t>ST17B_HUMAN_D0_3LM0_A</t>
-  </si>
-  <si>
-    <t>GDSDISSPLLQNTVHIDLSALNPELVQAVQHVVIGPSSLIVHFNEVIGRGHFGCVYHGTLLDNDGKKIHCAVKSLNRITDIGEVSQFLTEGIIMKDFSHPNVLSLLGICLRSEGSPLVVLPYMKHGDLRNFIRNETHNPTVKDLIGFGLQVAKGMKYLASKKFVHRDLAARNCMLDEKFTVKVADFGLARDMYDKEYYSVHNKTGAKLPVKWMALESLQTQKFTTKSDVWSFGVLLWELMTRGAPPYPDVNTFDITVYLLQGRRLLQPEYCPDPLYEVMLKCWHPKAEMRPSFSELVSRISAIFSTFIG</t>
-  </si>
-  <si>
-    <t>ATGAGTAGCTTTCTGCCAGAGGGAGGGTGTTACGAGCTGCTCACTGTGATAGGCAAAGGATTTGAGGACCTGATGACTGTGAATCTAGCAAGGTACAAACCAACAGGAGAGTACGTGACTGTACGGAGGATTAACCTAGAAGCTTGTTCCAATGAGATGGTAACATTCTTGCAGGGCGAGCTGCATGTCTCCAAACTCTTCAACCATCCCAATATCGTGCCATATCGAGCCACTTTTATTGCAGACAATGAGCTGTGGGTTGTCACATCATTCATGGCATACGGTTCTGCAAAAGATCTCATCTGTACACACTTCATGGATGGCATGAATGAGCTGGCGATTGCTTACATCCTGCAGGGGGTGCTGAAGGCCCTCGACTACATCCACCACATGGGATATGTACACAGGAGTGTCAAAGCCAGCCACATCCTGATCTCTGTGGATGGGAAGGTCTACCTGTCTGGTTTGCGCAGCAACCTCAGCATGATAAGCCATGGGCAGCGGCAGCGAGTGGTCCACGATTTTCCCAAGTACAGTGTCAAGGTTCTGCCGTGGCTCAGCCCCGAGGTCCTCCAGCAGAATCTCCAGGGTTATGATGCCAAGTCTGACATCTACAGTGTGGGAATCACAGCCTGTGAACTGGCCAACGGCCATGTCCCCTTTAAGGATATGCCTGCCACCCAGATGCTGCTAGAGAAACTGAACGGCACAGTGCCCTGCCTGTTGGATACCAGCACCATCCCCGCTGAGGAGCTGACCATGAGCCCTTCGCGCTCAGTGGCCAACTCTGGCCTGAGTGACAGCCTGACCACCAGCACCCCCCGGCCCTCCAACGGTGACTCGCCCTCCCACCCCTACCACCGAACCTTCTCCCCCCACTTCCACCACTTTGTGGAGCAGTGCCTTCAGCGCAACCCGGATGCCAGGCCCAGTGCCAGCACCCTCCTGAACCACTCTTTCTTCAAGCAGATCAAGCGACGTGCCTCAGAGGTTTTGCCCGAATTGCTTCGTCCTGTCACCCCCATCACCAATTTTGAGGGCAGCCAGTCTCAGGACCACAGTGGAATCTTTGGCCTGGTAACAAACCTGGAAGAGCTGGAGGTGGACGATTGGGAGTTC</t>
-  </si>
-  <si>
-    <t>ADPEELFTKLERIGKGSFGEVFKGIDNRTQQVVAIKIIDLEEAEDEIEDIQQEITVLSQCDSSYVTKYYGSYLKGSKLWIIMEYLGGGSALDLLRAGPFDEFQIATMLKEILKGLDYLHSEKKIHRDIKAANVLLSEQGDVKLADFGVAGQLTDTQIKRNTFVGTPFWMAPEVIQQSAYDSKADIWSLGITAIELAKGEPPNSDMHPMRVLFLIPKNNPPTLVGDFTKSFKEFIDACLNKDPSFRPTAKELLKHKFIVKNSKKTSYLTELIDRFKRWKAE</t>
-  </si>
-  <si>
-    <t>AURKA_HUMAN_D0_2NP8_A</t>
-  </si>
-  <si>
-    <t>HIGNYRLLKTIGKGNFAKVKLARHILTGKEVAVKIIDKTQLNSSSLQKLFREVRIMKVLNHPNIVKLFEVIETEKTLYLVMEYASGGEVFDYLVAHGRMKEKEARAKFRQIVSAVQYCHQKFIVHRDLKAENLLLDADMNIKIADFGFSNEFTFGNKLDTFCGSPPYAAPELFQGKKYDGPEVDVWSLGVILYTLVSGSLPFDGQNLKELRERVLRGKYRIPFYMSTDCENLLKKFLILNPSKRGTLEQIMKDRWMNVGHEDDELKPYVEPLPDYKDPRRTELMVSMGYTREEIQDSLVGQRYNEVMATYLLLGY</t>
-  </si>
-  <si>
-    <t>GVVTHEQFKAALRMVVDQGDPRLLLDSYVKIGEGSTGIVCLAREKHSGRQVAVKMMDLRKQQRRELLFNEVVIMRDYQHFNVVEMYKSYLVGEELWVLMEFLQGGALTDIVSQVRLNEEQIATVCEAVLQALAYLHAQGVIHRDIKSDSILLTLDGRVKLSDFGFCAQISKDVPKRKSLVGTPYWMAPEVISRSLYATEVDIWSLGIMVIEMVDGEPPYFSDSPVQAMKRLRDSPPPKLKNSHKVSPVLRDFLERMLVRDPQERATAQELLDHPFLLQTGLPECLVPLIQLYRKQTSTC</t>
-  </si>
-  <si>
-    <t>ATGGCAAAGCAGTACGACTCGGTGGAGTGCCCTTTTTGTGATGAAGTTTCCAAATACGAGAAGCTCGCCAAGATCGGCCAAGGCACCTTCGGGGAGGTGTTCAAGGCCAGGCACCGCAAGACCGGCCAGAAGGTGGCTCTGAAGAAGGTGCTGATGGAAAACGAGAAGGAGGGGTTCCCCATTACAGCCTTGCGGGAGATCAAGATCCTTCAGCTTCTAAAACACGAGAATGTGGTCAACTTGATTGAGATTTGTCGAACCAAAGCTTCCCCCTATAACCGCTGCAAGGGTAGTATATACCTGGTGTTCGACTTCTGCGAGCATGACCTTGCTGGGCTGTTGAGCAATGTTTTGGTCAAGTTCACGCTGTCTGAGATCAAGAGGGTGATGCAGATGCTGCTTAACGGCCTCTACTACATCCACAGAAACAAGATCCTGCATAGGGACATGAAGGCTGCTAATGTGCTTATCACTCGTGATGGGGTCCCGAAGCTGGCAGACTTTGGGCTGGCCCGGGCCTTCAGCCTGGCCAAGAACAGCCAGCCCAACCGCTACACCAACCGTGTGGTGACACTCTGGTACCGGCCCCCGGAGCTGTTGCTCGGGGAGCGGGACTACGGCCCCCCCATTGACCTGTGGGGTGCTGGGTGCATCATGGCAGAGATGTGGACCCGCAGCCCCATCATGCAGGGCAACACGGAGCAGCACCAACTCGCCCTCATCAGTCAGCTCTGCGGCTCCATCACCCCTGAGGTGTGGCCAAACGTGGACAACTATGAGCTGTACGAAAAGCTGGAGCTGGTCAAGGGCCAGAAGCGGAAGGTGAAGGACAGGCTGAAGGCCTATGTGCGTGACCCATACGCACTGGACCTCATCGACAAGCTGCTGGTGCTGGACCCTGCCCAGCGCATCGACAGCGATGACGCCCTCAACCACGACTTCTTCTGGTCCGACCCCATGCCCTCCGACCTCAAGGGCATGCTCTCCACC</t>
-  </si>
-  <si>
-    <t>MSQERPTFYRQELNKTIWEVPERYQNLSPVGSGAYGSVCAAFDTKTGLRVAVKKLSRPFQSIIHAKRTYRELRLLKHMKHENVIGLLDVFTPARSLEEFNDVYLVTHLMGADLNNIVKCQKLTDDHVQFLIYQILRGLKYIHSADIIHRDLKPSNLAVNEDCELKILDFGLARHTDDEMTGYVATRWYRAPEIMLNWMHYNQTVDIWSVGCIMAELLTGRTLFPGTDHIDQLKLILRLVGTPGAELLKKISSESARNYIQSLTQMPKMNFANVFIGANPLAVDLLEKMLVLDSDKRITAAQALAHAYFAQYHDPDDEPVADPYDQSFESRDLLIDEWKSLTYDEVISFVPPPLDQEEMES</t>
-  </si>
-  <si>
-    <t>MELRVGNRYRLGRKIGSGSFGDIYLGTDIAAGEEVAIKLECVKTKHPQLHIESKIYKMMQGGVGIPTIRWCGAEGDYNVMVMELLGPSLEDLFNFCSRKFSLKTVLLLADQMISRIEYIHSKNFIHRDVKPDNFLMGLGKKGNLVYIIDFGLAKKYRDARTHQHIPYRENKNLTGTARYASINTHLGIEQSRRDDLESLGYVLMYFNLGSLPWQGLKAATKRQKYERISEKKMSTPIEVLCKGYPSEFATYLNFCRSLRFDDKPDYSYLRQLFRNLFHRQGFSYDYVFDWNMLK</t>
-  </si>
-  <si>
-    <t>MAKQYDSVECPFCDEVSKYEKLAKIGQGTFGEVFKARHRKTGQKVALKKVLMENEKEGFPITALREIKILQLLKHENVVNLIEICRTKASPYNRCKGSIYLVFDFCEHDLAGLLSNVLVKFTLSEIKRVMQMLLNGLYYIHRNKILHRDMKAANVLITRDGVPKLADFGLARAFSLAKNSQPNRYTNRVVTLWYRPPELLLGERDYGPPIDLWGAGCIMAEMWTRSPIMQGNTEQHQLALISQLCGSITPEVWPNVDNYELYEKLELVKGQKRKVKDRLKAYVRDPYALDLIDKLLVLDPAQRIDSDDALNHDFFWSDPMPSDLKGMLST</t>
-  </si>
-  <si>
-    <t>targetID</t>
-  </si>
-  <si>
-    <t>TGGGCCCTGAACATGAAGGAGCTGAAGCTGCTGCAGACCATCGGGAAGGGGGAGTTCGGAGACGTGATGCTGGGCGATTACCGAGGGAACAAAGTCGCCGTCAAGTGCATTAAGAACGACGCCACTGCCCAGGCCTTCCTGGCTGAAGCCTCAGTCATGACGCAACTGCGGCATAGCAACCTGGTGCAGCTCCTGGGCGTGATCGTGGAGGAGAAGGGCGGGCTCTACATCGTCACTGAGTACATGGCCAAGGGGAGCCTTGTGGACTACCTGCGGTCTAGGGGTCGGTCAGTGCTGGGCGGAGACTGTCTCCTCAAGTTCTCGCTAGATGTCTGCGAGGCCATGGAATACCTGGAGGGCAACAATTTCGTGCATCGAGACCTGGCTGCCCGCAATGTGCTGGTGTCTGAGGACAACGTGGCCAAGGTCAGCGACTTTGGTCTCACCAAGGAGGCGTCCAGCACCCAGGACACGGGCAAGCTGCCAGTCAAGTGGACAGCCCCTGAGGCCCTGAGAGAGAAGAAATTCTCCACTAAGTCTGACGTGTGGAGTTTCGGAATCCTTCTCTGGGAAATCTACTCCTTTGGGCGAGTGCCTTATCCAAGAATTCCCCTGAAGGACGTCGTCCCTCGGGTGGAGAAGGGCTACAAGATGGATGCCCCCGACGGCTGCCCGCCCGCAGTCTATGAAGTCATGAAGAACTGCTGGCACCTGGACGCCGCCATGCGGCCCTCCTTCCTACAGCTCCGAGAGCAGCTTGAGCACATCAAAACCCACGAGCTGCACCTG</t>
-  </si>
-  <si>
-    <t>dna_seq</t>
-  </si>
-  <si>
-    <t>AACCTGGTTTTTAGTGACGGCTACGTGGTAAAGGAGACAATTGGTGTGGGCTCCTACTCTGAGTGCAAGCGCTGTGTCCACAAGGCCACCAACATGGAGTATGCTGTCAAGGTCATTGATAAGAGCAAGCGGGATCCTTCAGAAGAGATTGAGATTCTTCTGCGGTATGGCCAGCACCCCAACATCATCACTCTGAAAGATGTGTATGATGATGGCAAACACGTGTACCTGGTGACAGAGCTGATGCGGGGTGGGGAGCTGCTGGACAAGATCCTGCGGCAGAAGTTCTTCTCAGAGCGGGAGGCCAGCTTTGTCCTGCACACCATTGGCAAAACTGTGGAGTATCTGCACTCACAGGGGGTTGTGCACAGGGACCTGAAGCCCAGCAACATCCTGTATGTGGACGAGTCCGGGAATCCCGAGTGCCTGCGCATCTGTGACTTTGGTTTTGCCAAACAGCTGCGGGCTGAGAATGGGCTCCTCATGACACCTTGCTACACAGCCAACTTTGTGGCGCCTGAGGTGCTGAAGCGCCAGGGCTACGATGAAGGCTGCGACATCTGGAGCCTGGGCATTCTGCTGTACACCATGCTGGCAGGATATACTCCATTTGCCAACGGTCCCAGTGACACACCAGAGGAAATCCTAACCCGGATCGGCAGTGGGAAGTTTACCCTCAGTGGGGGAAATTGGAACACAGTTTCAGAGACAGCCAAGGACCTGGTGTCCAAGATGCTACACGTGGATCCCCACCAGCGCCTCACAGCTAAGCAGGTTCTGCAGCATCCATGGGTCACCCAGAAAGACAAGCTTCCCCAAAGCCAGCTGTCCCACCAGGACCTACAGCTTGTGAAGGGAGCCATGGCTGCCACGTACTCCGCACTCAACAGCTCCAAGCCCACCCCCCAGCTGAAGCCCATCGAGTCATCCATCCTGGCCCAGCGGCGAGTGAGGAAGTTGCCATCCACCACCCTG</t>
-  </si>
-  <si>
-    <t>ATGGCCGACGACGACGTGCTGTTCGAGGATGTGTACGAGCTGTGCGAGGTGATCGGAAAGGGTCCCTTCAGTGTTGTACGACGATGTATCAACAGAGAAACTGGGCAACAATTTGCTGTAAAAATTGTTGATGTAGCCAAGTTCACATCAAGTCCAGGGTTAAGTACAGAAGATCTAAAGCGGGAAGCCAGTATCTGTCATATGCTGAAACATCCACACATTGTAGAGTTATTGGAGACATATAGCTCAGATGGAATGCTTTACATGGTTTTCGAATTTATGGATGGAGCAGATCTGTGTTTTGAAATCGTAAAGCGAGCTGACGCTGGTTTTGTGTACAGTGAAGCTGTAGCCAGCCATTATATGAGACAGATACTGGAAGCTCTACGCTACTGCCATGATAATAACATAATTCACAGGGATGTGAAGCCCCACTGTGTTCTCCTTGCCTCAAAAGAAAACTCGGCACCTGTTAAACTTGGAGGCTTTGGGGTAGCTATTCAATTAGGGGAGTCTGGACTTGTAGCTGGAGGACGTGTTGGAACACCTCATTTTATGGCACCAGAAGTGGTCAAAAGAGAGCCTTACGGAAAGCCTGTAGACGTCTGGGGGTGCGGTGTGATCCTTTTTATCCTGCTCAGTGGTTGTTTGCCTTTTTACGGAACCAAGGAAAGATTGTTTGAAGGCATTATTAAAGGAAAATATAAGATGAATCCAAGGCAGTGGAGCCATATCTCTGAAAGTGCCAAAGACCTAGTACGTCGCATGCTGATGCTGGATCCAGCTGAAAGGATCACTGTTTATGAAGCACTGAATCACCCATGGCTTAAGGAGCGGGATCGTTACGCCTACAAGATTCATCTTCCAGAAACAGTAGAGCAGCTGAGGAAATTCAATGCAAGGAGGAAACTAAAGGGTGCAGTACTAGCCGCTGTGTCAAGTCACAAATTCAACTCATTCTATGGGGATCCCCCTGAAGAGTTACCAGATTTCTCCGAAGACCCTACCTCCTCAGGAGCA</t>
-  </si>
-  <si>
-    <t>VRK1_HUMAN_D0_3OP5_D</t>
-  </si>
-  <si>
     <t>ATGGGGAAGGTGAAAGCCACCCCCATGACACCTGAACAAGCAATGAAGCAATACATGCAAAAACTCACAGCCTTCGAACACCATGAGATTTTCAGCTACCCTGAAATATATTTCTTGGGTCTAAATGCTAAGAAGCGCCAGGGCATGACAGGTGGGCCCAACAATGGTGGCTATGATGATGACCAGGGATCATATGTGCAGGTGCCCCACGATCACGTGGCTTACAGGTATGAGGTCCTCAAGGTCATTGGGAAGGGGAGCTTTGGGCAGGTGGTCAAGGCCTACGATCACAAAGTCCACCAGCACGTGGCCCTAAAGATGGTGCGGAATGAGAAGCGCTTCCACCGGCAAGCAGCGGAGGAGATCCGAATCCTGGAACACCTGCGGAAGCAGGACAAGGATAACACAATGAATGTCATCCATATGCTGGAGAATTTCACCTTCCGCAACCACATCTGCATGACGTTTGAGCTGCTGAGCATGAACCTCTATGAGCTCATCAAGAAGAATAAATTCCAGGGCTTCAGTCTGCCTTTGGTTCGCAAGTTTGCCCACTCGATTCTGCAGTGCTTGGATGCTTTGCACAAAAACAGAATAATTCACTGTGACCTTAAGCCCGAGAACATTTTGTTAAAGCAGCAGGGTAGAAGCGGTATTAAAGTAATTGATTTTGGCTCCAGTTGTTACGAGCATCAGCGTGTCTACACGTACATCCAGTCGCGTTTTTACCGGGCTCCAGAAGTGATCCTTGGGGCCAGGTATGGCATGCCCATTGATATGTGGAGCCTGGGCTGCATTTTAGCAGAGCTCCTGACGGGTTACCCCCTCTTGCCTGGGGAAGATGAAGGGGACCAGCTGGCCTGTATGATTGAACTGTTGGGCATGCCCTCACAGAAACTGCTGGATGCATCCAAACGAGCCAAAAATTTTGTGAGCTCCAAGGGTTATCCCCGTTACTGCACTGTCACGACTCTCTCAGATGGCTCTGTGGTCCTAAACGGAGGCCGTTCCCGGAGGGGGAAACTGAGGGGCCCACCGGAGAGCAGAGAGTGGGGGAACGCGCTGAAGGGGTGTGATGATCCCCTTTTCCTTGACTTCTTAAAACAGTGTTTAGAGTGGGATCCTGCAGTGCGCATGACCCCAGGCCAGGCTTTGCGGCACCCCTGGCTGAGGAGGCGGTTGCCAAAGCCTCCCACCGGGGAGAAAACGTCAGTGAAAAGG</t>
   </si>
   <si>
@@ -684,6 +681,9 @@
   </si>
   <si>
     <t>SPNYDKWEMERTDITMKHKLGGGQYGEVYEGVWKKYSLTVAVKTLKEDTMEVEEFLKEAAVMKEIKHPNLVQLLGVCTREPPFYIITEFMTYGNLLDYLRECNRQEVNAVVLLYMATQISSAMEYLEKKNFIHRDLAARNCLVGENHLVKVADFGLSRLMTGDTYTAHAGAKFPIKWTAPESLAYNKFSIKSDVWAFGVLLWEIATYGMSPYPGIDLSQVYELLEKDYRMERPEGCPEKVYELMRACWQWNPSDRPSFAEIHQAFETMFQESSISDEVEKELGK</t>
+  </si>
+  <si>
+    <t>PLK2_HUMAN_D0_4I6B_A</t>
   </si>
   <si>
     <t>ATGGCGGCGGCGGCGGCTCAGGGGGGCGGGGGCGGGGAGCCCCGTAGAACCGAGGGGGTCGGCCCGGGGGTCCCGGGGGAGGTGGAGATGGTGAAGGGGCAGCCGTTCGACGTGGGCCCGCGCTACACGCAGTTGCAGTACATCGGCGAGGGCGCGTACGGCATGGTCAGCTCGGCCTATGACCACGTGCGCAAGACTCGCGTGGCCATCAAGAAGATCAGCCCCTTCGAACATCAGACCTACTGCCAGCGCACGCTCCGGGAGATCCAGATCCTGCTGCGCTTCCGCCATGAGAATGTCATCGGCATCCGAGACATTCTGCGGGCGTCCACCCTGGAAGCCATGAGAGATGTCTACATTGTGCAGGACCTGATGGAGACTGACCTGTACAAGTTGCTGAAAAGCCAGCAGCTGAGCAATGACCATATCTGCTACTTCCTCTACCAGATCCTGCGGGGCCTCAAGTACATCCACTCCGCCAACGTGCTCCACCGAGATCTAAAGCCCTCCAACCTGCTCATCAACACCACCTGCGACCTTAAGATTTGTGATTTCGGCCTGGCCCGGATTGCCGATCCTGAGCATGACCACACCGGCTTCCTGACGGAGTATGTGGCTACGCGCTGGTACCGGGCCCCAGAGATCATGCTGAACTCCAAGGGCTATACCAAGTCCATCGACATCTGGTCTGTGGGCTGCATTCTGGCTGAGATGCTCTCTAACCGGCCCATCTTCCCTGGCAAGCACTACCTGGATCAGCTCAACCACATTCTGGGCATCCTGGGCTCCCCATCCCAGGAGGACCTGAATTGTATCATCAACATGAAGGCCCGAAACTACCTACAGTCTCTGCCCTCCAAGACCAAGGTGGCTTGGGCCAAGCTTTTCCCCAAGTCAGACTCCAAAGCCCTTGACCTGCTGGACCGGATGTTAACCTTTAACCCCAATAAACGGATCACAGTGGAGGAAGCGCTGGCTCACCCCTACCTGGAGCAGTACTATGACCCGACGGATGAGCCAGTGGCCGAGGAGCCCTTCACCTTCGCCATGGAGCTGGATGACCTACCTAAGGAGCGGCTGAAGGAGCTCATCTTCCAGGAGACAGCACGCTTCCAGCCCGGAGTGCTGGAGGCCCCC</t>
@@ -1058,13 +1058,13 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
-        <v>103</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
         <v>225</v>
@@ -1073,16 +1073,16 @@
         <v>37</v>
       </c>
       <c r="F1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1131,7 +1131,7 @@
         <v>360</v>
       </c>
       <c r="F3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G3" t="n">
         <v>1</v>
@@ -1145,7 +1145,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B4" t="n">
         <v>6790</v>
@@ -1160,7 +1160,7 @@
         <v>391</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G4" t="n">
         <v>373</v>
@@ -1169,12 +1169,12 @@
         <v>1173</v>
       </c>
       <c r="I4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>123</v>
       </c>
       <c r="B5" t="n">
         <v>5594</v>
@@ -1198,12 +1198,12 @@
         <v>1080</v>
       </c>
       <c r="I5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B6" t="n">
         <v>9261</v>
@@ -1218,7 +1218,7 @@
         <v>348</v>
       </c>
       <c r="F6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G6" t="n">
         <v>73</v>
@@ -1256,7 +1256,7 @@
         <v>1773</v>
       </c>
       <c r="I7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1276,7 +1276,7 @@
         <v>512</v>
       </c>
       <c r="F8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G8" t="n">
         <v>685</v>
@@ -1290,126 +1290,126 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="B9" t="n">
-        <v>51765</v>
+        <v>673</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>18</v>
+        <v>444</v>
       </c>
       <c r="E9" t="n">
-        <v>297</v>
+        <v>712</v>
       </c>
       <c r="F9" t="s">
-        <v>182</v>
+        <v>24</v>
       </c>
       <c r="G9" t="n">
-        <v>52</v>
+        <v>1330</v>
       </c>
       <c r="H9" t="n">
-        <v>891</v>
+        <v>2136</v>
       </c>
       <c r="I9" t="s">
-        <v>128</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>216</v>
+        <v>13</v>
       </c>
       <c r="B10" t="n">
-        <v>2872</v>
+        <v>51765</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>72</v>
+        <v>18</v>
       </c>
       <c r="E10" t="n">
-        <v>385</v>
+        <v>297</v>
       </c>
       <c r="F10" t="s">
-        <v>153</v>
+        <v>181</v>
       </c>
       <c r="G10" t="n">
-        <v>214</v>
+        <v>52</v>
       </c>
       <c r="H10" t="n">
-        <v>1155</v>
+        <v>891</v>
       </c>
       <c r="I10" t="s">
-        <v>26</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>82</v>
+        <v>215</v>
       </c>
       <c r="B11" t="n">
-        <v>1956</v>
+        <v>2872</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
       </c>
       <c r="D11" t="n">
-        <v>696</v>
+        <v>72</v>
       </c>
       <c r="E11" t="n">
-        <v>1022</v>
+        <v>385</v>
       </c>
       <c r="F11" t="s">
-        <v>224</v>
+        <v>152</v>
       </c>
       <c r="G11" t="n">
-        <v>2086</v>
+        <v>214</v>
       </c>
       <c r="H11" t="n">
-        <v>3066</v>
+        <v>1155</v>
       </c>
       <c r="I11" t="s">
-        <v>105</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>211</v>
+        <v>83</v>
       </c>
       <c r="B12" t="n">
-        <v>1453</v>
+        <v>1956</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>696</v>
       </c>
       <c r="E12" t="n">
-        <v>294</v>
+        <v>1022</v>
       </c>
       <c r="F12" t="s">
-        <v>188</v>
+        <v>224</v>
       </c>
       <c r="G12" t="n">
-        <v>1</v>
+        <v>2086</v>
       </c>
       <c r="H12" t="n">
-        <v>882</v>
+        <v>3066</v>
       </c>
       <c r="I12" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>210</v>
       </c>
       <c r="B13" t="n">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
@@ -1421,7 +1421,7 @@
         <v>294</v>
       </c>
       <c r="F13" t="s">
-        <v>129</v>
+        <v>187</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
@@ -1430,15 +1430,15 @@
         <v>882</v>
       </c>
       <c r="I13" t="s">
-        <v>157</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>142</v>
+        <v>33</v>
       </c>
       <c r="B14" t="n">
-        <v>5598</v>
+        <v>1454</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
@@ -1447,952 +1447,952 @@
         <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="F14" t="s">
-        <v>207</v>
+        <v>130</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
       </c>
       <c r="H14" t="n">
-        <v>876</v>
+        <v>882</v>
       </c>
       <c r="I14" t="s">
-        <v>0</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>142</v>
       </c>
       <c r="B15" t="n">
-        <v>5347</v>
+        <v>5598</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
       </c>
       <c r="D15" t="n">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>345</v>
+        <v>292</v>
       </c>
       <c r="F15" t="s">
-        <v>96</v>
+        <v>206</v>
       </c>
       <c r="G15" t="n">
-        <v>97</v>
+        <v>1</v>
       </c>
       <c r="H15" t="n">
-        <v>1035</v>
+        <v>876</v>
       </c>
       <c r="I15" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>213</v>
+        <v>60</v>
       </c>
       <c r="B16" t="n">
-        <v>5563</v>
+        <v>5347</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="D16" t="n">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="E16" t="n">
-        <v>279</v>
+        <v>345</v>
       </c>
       <c r="F16" t="s">
-        <v>199</v>
+        <v>97</v>
       </c>
       <c r="G16" t="n">
-        <v>16</v>
+        <v>97</v>
       </c>
       <c r="H16" t="n">
-        <v>837</v>
+        <v>1035</v>
       </c>
       <c r="I16" t="s">
-        <v>110</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>212</v>
       </c>
       <c r="B17" t="n">
-        <v>1025</v>
+        <v>5563</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E17" t="n">
-        <v>330</v>
+        <v>279</v>
       </c>
       <c r="F17" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="G17" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="H17" t="n">
-        <v>990</v>
+        <v>837</v>
       </c>
       <c r="I17" t="s">
-        <v>186</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>133</v>
+        <v>42</v>
       </c>
       <c r="B18" t="n">
-        <v>5747</v>
+        <v>1025</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
       </c>
       <c r="D18" t="n">
-        <v>411</v>
+        <v>1</v>
       </c>
       <c r="E18" t="n">
-        <v>689</v>
+        <v>330</v>
       </c>
       <c r="F18" t="s">
-        <v>217</v>
+        <v>188</v>
       </c>
       <c r="G18" t="n">
-        <v>1231</v>
+        <v>1</v>
       </c>
       <c r="H18" t="n">
-        <v>2067</v>
+        <v>990</v>
       </c>
       <c r="I18" t="s">
-        <v>160</v>
+        <v>185</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>94</v>
+        <v>134</v>
       </c>
       <c r="B19" t="n">
-        <v>8569</v>
+        <v>5747</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
       </c>
       <c r="D19" t="n">
-        <v>37</v>
+        <v>411</v>
       </c>
       <c r="E19" t="n">
-        <v>382</v>
+        <v>689</v>
       </c>
       <c r="F19" t="s">
-        <v>48</v>
+        <v>216</v>
       </c>
       <c r="G19" t="n">
-        <v>109</v>
+        <v>1231</v>
       </c>
       <c r="H19" t="n">
-        <v>1146</v>
+        <v>2067</v>
       </c>
       <c r="I19" t="s">
-        <v>51</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="B20" t="n">
-        <v>5292</v>
+        <v>8569</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="D20" t="n">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E20" t="n">
-        <v>313</v>
+        <v>382</v>
       </c>
       <c r="F20" t="s">
-        <v>168</v>
+        <v>48</v>
       </c>
       <c r="G20" t="n">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="H20" t="n">
-        <v>939</v>
+        <v>1146</v>
       </c>
       <c r="I20" t="s">
-        <v>205</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B21" t="n">
-        <v>7272</v>
+        <v>5292</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="D21" t="n">
-        <v>519</v>
+        <v>29</v>
       </c>
       <c r="E21" t="n">
-        <v>808</v>
+        <v>313</v>
       </c>
       <c r="F21" t="s">
-        <v>21</v>
+        <v>166</v>
       </c>
       <c r="G21" t="n">
-        <v>1555</v>
+        <v>85</v>
       </c>
       <c r="H21" t="n">
-        <v>2424</v>
+        <v>939</v>
       </c>
       <c r="I21" t="s">
-        <v>40</v>
+        <v>204</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>209</v>
+        <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>8428</v>
+        <v>7272</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
       </c>
       <c r="D22" t="n">
-        <v>19</v>
+        <v>519</v>
       </c>
       <c r="E22" t="n">
-        <v>289</v>
+        <v>808</v>
       </c>
       <c r="F22" t="s">
-        <v>161</v>
+        <v>21</v>
       </c>
       <c r="G22" t="n">
-        <v>55</v>
+        <v>1555</v>
       </c>
       <c r="H22" t="n">
-        <v>867</v>
+        <v>2424</v>
       </c>
       <c r="I22" t="s">
-        <v>202</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>3</v>
+        <v>208</v>
       </c>
       <c r="B23" t="n">
-        <v>83903</v>
+        <v>8428</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
       </c>
       <c r="D23" t="n">
-        <v>465</v>
+        <v>19</v>
       </c>
       <c r="E23" t="n">
-        <v>798</v>
+        <v>289</v>
       </c>
       <c r="F23" t="s">
-        <v>126</v>
+        <v>160</v>
       </c>
       <c r="G23" t="n">
-        <v>1393</v>
+        <v>55</v>
       </c>
       <c r="H23" t="n">
-        <v>2394</v>
+        <v>867</v>
       </c>
       <c r="I23" t="s">
-        <v>47</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>214</v>
+        <v>3</v>
       </c>
       <c r="B24" t="n">
-        <v>1198</v>
+        <v>83903</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
       </c>
       <c r="D24" t="n">
+        <v>465</v>
+      </c>
+      <c r="E24" t="n">
+        <v>798</v>
+      </c>
+      <c r="F24" t="s">
         <v>127</v>
       </c>
-      <c r="E24" t="n">
-        <v>484</v>
-      </c>
-      <c r="F24" t="s">
-        <v>141</v>
-      </c>
       <c r="G24" t="n">
-        <v>379</v>
+        <v>1393</v>
       </c>
       <c r="H24" t="n">
-        <v>1452</v>
+        <v>2394</v>
       </c>
       <c r="I24" t="s">
-        <v>111</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>213</v>
       </c>
       <c r="B25" t="n">
-        <v>1613</v>
+        <v>1198</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
       </c>
       <c r="D25" t="n">
-        <v>9</v>
+        <v>127</v>
       </c>
       <c r="E25" t="n">
-        <v>289</v>
+        <v>484</v>
       </c>
       <c r="F25" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="G25" t="n">
-        <v>25</v>
+        <v>379</v>
       </c>
       <c r="H25" t="n">
-        <v>867</v>
+        <v>1452</v>
       </c>
       <c r="I25" t="s">
-        <v>9</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="B26" t="n">
-        <v>7867</v>
+        <v>1613</v>
       </c>
       <c r="C26" t="s">
         <v>2</v>
       </c>
       <c r="D26" t="n">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="E26" t="n">
-        <v>349</v>
+        <v>289</v>
       </c>
       <c r="F26" t="s">
-        <v>208</v>
+        <v>167</v>
       </c>
       <c r="G26" t="n">
-        <v>97</v>
+        <v>25</v>
       </c>
       <c r="H26" t="n">
-        <v>1047</v>
+        <v>867</v>
       </c>
       <c r="I26" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>161</v>
       </c>
       <c r="B27" t="n">
-        <v>9748</v>
+        <v>7867</v>
       </c>
       <c r="C27" t="s">
         <v>2</v>
       </c>
       <c r="D27" t="n">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="E27" t="n">
-        <v>320</v>
+        <v>349</v>
       </c>
       <c r="F27" t="s">
-        <v>116</v>
+        <v>207</v>
       </c>
       <c r="G27" t="n">
+        <v>97</v>
+      </c>
+      <c r="H27" t="n">
+        <v>1047</v>
+      </c>
+      <c r="I27" t="s">
         <v>55</v>
-      </c>
-      <c r="H27" t="n">
-        <v>960</v>
-      </c>
-      <c r="I27" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>139</v>
+        <v>84</v>
       </c>
       <c r="B28" t="n">
-        <v>8445</v>
+        <v>9748</v>
       </c>
       <c r="C28" t="s">
         <v>2</v>
       </c>
       <c r="D28" t="n">
-        <v>146</v>
+        <v>19</v>
       </c>
       <c r="E28" t="n">
-        <v>552</v>
+        <v>320</v>
       </c>
       <c r="F28" t="s">
-        <v>145</v>
+        <v>116</v>
       </c>
       <c r="G28" t="n">
-        <v>436</v>
+        <v>55</v>
       </c>
       <c r="H28" t="n">
-        <v>1656</v>
+        <v>960</v>
       </c>
       <c r="I28" t="s">
-        <v>196</v>
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>101</v>
+        <v>139</v>
       </c>
       <c r="B29" t="n">
-        <v>815</v>
+        <v>8445</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
       </c>
       <c r="D29" t="n">
-        <v>13</v>
+        <v>146</v>
       </c>
       <c r="E29" t="n">
-        <v>302</v>
+        <v>552</v>
       </c>
       <c r="F29" t="s">
-        <v>18</v>
+        <v>145</v>
       </c>
       <c r="G29" t="n">
-        <v>37</v>
+        <v>436</v>
       </c>
       <c r="H29" t="n">
-        <v>906</v>
+        <v>1656</v>
       </c>
       <c r="I29" t="s">
-        <v>38</v>
+        <v>195</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>179</v>
+        <v>102</v>
       </c>
       <c r="B30" t="n">
-        <v>9262</v>
+        <v>815</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
       </c>
       <c r="D30" t="n">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E30" t="n">
-        <v>329</v>
+        <v>302</v>
       </c>
       <c r="F30" t="s">
-        <v>127</v>
+        <v>18</v>
       </c>
       <c r="G30" t="n">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="H30" t="n">
-        <v>987</v>
+        <v>906</v>
       </c>
       <c r="I30" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>99</v>
+        <v>178</v>
       </c>
       <c r="B31" t="n">
-        <v>814</v>
+        <v>9262</v>
       </c>
       <c r="C31" t="s">
         <v>2</v>
       </c>
       <c r="D31" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E31" t="n">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="F31" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G31" t="n">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="H31" t="n">
-        <v>1020</v>
+        <v>987</v>
       </c>
       <c r="I31" t="s">
-        <v>64</v>
+        <v>199</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>174</v>
+        <v>100</v>
       </c>
       <c r="B32" t="n">
-        <v>8814</v>
+        <v>814</v>
       </c>
       <c r="C32" t="s">
         <v>2</v>
       </c>
       <c r="D32" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E32" t="n">
-        <v>265</v>
+        <v>340</v>
       </c>
       <c r="F32" t="s">
-        <v>74</v>
+        <v>131</v>
       </c>
       <c r="G32" t="n">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="H32" t="n">
-        <v>795</v>
+        <v>1020</v>
       </c>
       <c r="I32" t="s">
-        <v>198</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>115</v>
+        <v>172</v>
       </c>
       <c r="B33" t="n">
-        <v>818</v>
+        <v>8814</v>
       </c>
       <c r="C33" t="s">
         <v>2</v>
       </c>
       <c r="D33" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E33" t="n">
-        <v>315</v>
+        <v>265</v>
       </c>
       <c r="F33" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="G33" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="H33" t="n">
-        <v>945</v>
+        <v>795</v>
       </c>
       <c r="I33" t="s">
-        <v>106</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="B34" t="n">
-        <v>56924</v>
+        <v>818</v>
       </c>
       <c r="C34" t="s">
         <v>2</v>
       </c>
       <c r="D34" t="n">
-        <v>383</v>
+        <v>5</v>
       </c>
       <c r="E34" t="n">
-        <v>681</v>
+        <v>315</v>
       </c>
       <c r="F34" t="s">
-        <v>185</v>
+        <v>89</v>
       </c>
       <c r="G34" t="n">
-        <v>1147</v>
+        <v>13</v>
       </c>
       <c r="H34" t="n">
-        <v>2043</v>
+        <v>945</v>
       </c>
       <c r="I34" t="s">
-        <v>177</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="B35" t="n">
-        <v>57144</v>
+        <v>56924</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
       </c>
       <c r="D35" t="n">
-        <v>425</v>
+        <v>383</v>
       </c>
       <c r="E35" t="n">
-        <v>719</v>
+        <v>681</v>
       </c>
       <c r="F35" t="s">
-        <v>84</v>
+        <v>184</v>
       </c>
       <c r="G35" t="n">
-        <v>1273</v>
+        <v>1147</v>
       </c>
       <c r="H35" t="n">
-        <v>2157</v>
+        <v>2043</v>
       </c>
       <c r="I35" t="s">
-        <v>80</v>
+        <v>176</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="B36" t="n">
-        <v>5261</v>
+        <v>57144</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
       </c>
       <c r="D36" t="n">
-        <v>6</v>
+        <v>425</v>
       </c>
       <c r="E36" t="n">
-        <v>293</v>
+        <v>719</v>
       </c>
       <c r="F36" t="s">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="G36" t="n">
-        <v>16</v>
+        <v>1273</v>
       </c>
       <c r="H36" t="n">
-        <v>879</v>
+        <v>2157</v>
       </c>
       <c r="I36" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="B37" t="n">
-        <v>9088</v>
+        <v>5261</v>
       </c>
       <c r="C37" t="s">
         <v>2</v>
       </c>
       <c r="D37" t="n">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="E37" t="n">
-        <v>360</v>
+        <v>293</v>
       </c>
       <c r="F37" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="G37" t="n">
-        <v>217</v>
+        <v>16</v>
       </c>
       <c r="H37" t="n">
-        <v>1080</v>
+        <v>879</v>
       </c>
       <c r="I37" t="s">
-        <v>167</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>109</v>
+        <v>38</v>
       </c>
       <c r="B38" t="n">
-        <v>8576</v>
+        <v>9088</v>
       </c>
       <c r="C38" t="s">
         <v>2</v>
       </c>
       <c r="D38" t="n">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="E38" t="n">
-        <v>294</v>
+        <v>360</v>
       </c>
       <c r="F38" t="s">
-        <v>203</v>
+        <v>36</v>
       </c>
       <c r="G38" t="n">
-        <v>37</v>
+        <v>217</v>
       </c>
       <c r="H38" t="n">
-        <v>882</v>
+        <v>1080</v>
       </c>
       <c r="I38" t="s">
-        <v>66</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>28</v>
+        <v>109</v>
       </c>
       <c r="B39" t="n">
-        <v>92335</v>
+        <v>8576</v>
       </c>
       <c r="C39" t="s">
         <v>2</v>
       </c>
       <c r="D39" t="n">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="E39" t="n">
-        <v>402</v>
+        <v>294</v>
       </c>
       <c r="F39" t="s">
-        <v>171</v>
+        <v>202</v>
       </c>
       <c r="G39" t="n">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="H39" t="n">
-        <v>1206</v>
+        <v>882</v>
       </c>
       <c r="I39" t="s">
-        <v>181</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B40" t="n">
-        <v>7444</v>
+        <v>92335</v>
       </c>
       <c r="C40" t="s">
         <v>2</v>
       </c>
       <c r="D40" t="n">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E40" t="n">
-        <v>335</v>
+        <v>402</v>
       </c>
       <c r="F40" t="s">
-        <v>206</v>
+        <v>169</v>
       </c>
       <c r="G40" t="n">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="H40" t="n">
-        <v>1005</v>
+        <v>1206</v>
       </c>
       <c r="I40" t="s">
-        <v>16</v>
+        <v>180</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="B41" t="n">
-        <v>51231</v>
+        <v>7444</v>
       </c>
       <c r="C41" t="s">
         <v>2</v>
       </c>
       <c r="D41" t="n">
-        <v>146</v>
+        <v>14</v>
       </c>
       <c r="E41" t="n">
-        <v>474</v>
+        <v>335</v>
       </c>
       <c r="F41" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="G41" t="n">
-        <v>436</v>
+        <v>40</v>
       </c>
       <c r="H41" t="n">
-        <v>1422</v>
+        <v>1005</v>
       </c>
       <c r="I41" t="s">
-        <v>150</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>119</v>
+        <v>49</v>
       </c>
       <c r="B42" t="n">
-        <v>2042</v>
+        <v>51231</v>
       </c>
       <c r="C42" t="s">
         <v>2</v>
       </c>
       <c r="D42" t="n">
-        <v>606</v>
+        <v>146</v>
       </c>
       <c r="E42" t="n">
-        <v>947</v>
+        <v>474</v>
       </c>
       <c r="F42" t="s">
-        <v>85</v>
+        <v>220</v>
       </c>
       <c r="G42" t="n">
-        <v>1816</v>
+        <v>436</v>
       </c>
       <c r="H42" t="n">
-        <v>2841</v>
+        <v>1422</v>
       </c>
       <c r="I42" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>119</v>
       </c>
       <c r="B43" t="n">
-        <v>2260</v>
+        <v>2042</v>
       </c>
       <c r="C43" t="s">
         <v>2</v>
       </c>
       <c r="D43" t="n">
-        <v>456</v>
+        <v>606</v>
       </c>
       <c r="E43" t="n">
-        <v>772</v>
+        <v>947</v>
       </c>
       <c r="F43" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="G43" t="n">
-        <v>1366</v>
+        <v>1816</v>
       </c>
       <c r="H43" t="n">
-        <v>2316</v>
+        <v>2841</v>
       </c>
       <c r="I43" t="s">
-        <v>228</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="B44" t="n">
-        <v>8573</v>
+        <v>2260</v>
       </c>
       <c r="C44" t="s">
         <v>2</v>
       </c>
       <c r="D44" t="n">
-        <v>1</v>
+        <v>456</v>
       </c>
       <c r="E44" t="n">
-        <v>340</v>
+        <v>772</v>
       </c>
       <c r="F44" t="s">
-        <v>132</v>
+        <v>53</v>
       </c>
       <c r="G44" t="n">
-        <v>1</v>
+        <v>1366</v>
       </c>
       <c r="H44" t="n">
-        <v>1020</v>
+        <v>2316</v>
       </c>
       <c r="I44" t="s">
-        <v>194</v>
+        <v>228</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>97</v>
+        <v>12</v>
       </c>
       <c r="B45" t="n">
-        <v>3702</v>
+        <v>8573</v>
       </c>
       <c r="C45" t="s">
         <v>2</v>
       </c>
       <c r="D45" t="n">
-        <v>357</v>
+        <v>1</v>
       </c>
       <c r="E45" t="n">
-        <v>620</v>
+        <v>340</v>
       </c>
       <c r="F45" t="s">
-        <v>89</v>
+        <v>133</v>
       </c>
       <c r="G45" t="n">
-        <v>1069</v>
+        <v>1</v>
       </c>
       <c r="H45" t="n">
-        <v>1860</v>
+        <v>1020</v>
       </c>
       <c r="I45" t="s">
-        <v>136</v>
+        <v>193</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>144</v>
+        <v>98</v>
       </c>
       <c r="B46" t="n">
-        <v>6197</v>
+        <v>3702</v>
       </c>
       <c r="C46" t="s">
         <v>2</v>
       </c>
       <c r="D46" t="n">
-        <v>399</v>
+        <v>357</v>
       </c>
       <c r="E46" t="n">
-        <v>740</v>
+        <v>620</v>
       </c>
       <c r="F46" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="G46" t="n">
-        <v>1195</v>
+        <v>1069</v>
       </c>
       <c r="H46" t="n">
-        <v>2220</v>
+        <v>1860</v>
       </c>
       <c r="I46" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>98</v>
+        <v>144</v>
       </c>
       <c r="B47" t="n">
         <v>6197</v>
@@ -2421,60 +2421,60 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>170</v>
+        <v>99</v>
       </c>
       <c r="B48" t="n">
-        <v>4233</v>
+        <v>6197</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
       </c>
       <c r="D48" t="n">
-        <v>1038</v>
+        <v>399</v>
       </c>
       <c r="E48" t="n">
-        <v>1346</v>
+        <v>740</v>
       </c>
       <c r="F48" t="s">
-        <v>180</v>
+        <v>113</v>
       </c>
       <c r="G48" t="n">
-        <v>3112</v>
+        <v>1195</v>
       </c>
       <c r="H48" t="n">
-        <v>4038</v>
+        <v>2220</v>
       </c>
       <c r="I48" t="s">
-        <v>17</v>
+        <v>143</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>76</v>
+        <v>168</v>
       </c>
       <c r="B49" t="n">
-        <v>673</v>
+        <v>4233</v>
       </c>
       <c r="C49" t="s">
         <v>2</v>
       </c>
       <c r="D49" t="n">
-        <v>444</v>
+        <v>1038</v>
       </c>
       <c r="E49" t="n">
-        <v>719</v>
+        <v>1346</v>
       </c>
       <c r="F49" t="s">
-        <v>45</v>
+        <v>179</v>
       </c>
       <c r="G49" t="n">
-        <v>1330</v>
+        <v>3112</v>
       </c>
       <c r="H49" t="n">
-        <v>2157</v>
+        <v>4038</v>
       </c>
       <c r="I49" t="s">
-        <v>149</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2494,7 +2494,7 @@
         <v>352</v>
       </c>
       <c r="F50" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G50" t="n">
         <v>1</v>
@@ -2523,7 +2523,7 @@
         <v>399</v>
       </c>
       <c r="F51" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G51" t="n">
         <v>238</v>
@@ -2532,12 +2532,12 @@
         <v>1197</v>
       </c>
       <c r="I51" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B52" t="n">
         <v>6195</v>
@@ -2552,7 +2552,7 @@
         <v>735</v>
       </c>
       <c r="F52" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G52" t="n">
         <v>1231</v>
@@ -2561,7 +2561,7 @@
         <v>2205</v>
       </c>
       <c r="I52" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -2581,7 +2581,7 @@
         <v>735</v>
       </c>
       <c r="F53" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G53" t="n">
         <v>1231</v>
@@ -2590,479 +2590,479 @@
         <v>2205</v>
       </c>
       <c r="I53" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>39</v>
+        <v>222</v>
       </c>
       <c r="B54" t="n">
-        <v>5599</v>
+        <v>10769</v>
       </c>
       <c r="C54" t="s">
-        <v>219</v>
+        <v>2</v>
       </c>
       <c r="D54" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E54" t="n">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F54" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="G54" t="n">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="H54" t="n">
-        <v>1092</v>
+        <v>1080</v>
       </c>
       <c r="I54" t="s">
-        <v>220</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
       <c r="B55" t="n">
-        <v>4751</v>
+        <v>5599</v>
       </c>
       <c r="C55" t="s">
+        <v>218</v>
+      </c>
+      <c r="D55" t="n">
+        <v>1</v>
+      </c>
+      <c r="E55" t="n">
+        <v>364</v>
+      </c>
+      <c r="F55" t="s">
+        <v>27</v>
+      </c>
+      <c r="G55" t="n">
+        <v>1</v>
+      </c>
+      <c r="H55" t="n">
+        <v>1092</v>
+      </c>
+      <c r="I55" t="s">
         <v>219</v>
-      </c>
-      <c r="D55" t="n">
-        <v>1</v>
-      </c>
-      <c r="E55" t="n">
-        <v>271</v>
-      </c>
-      <c r="F55" t="s">
-        <v>201</v>
-      </c>
-      <c r="G55" t="n">
-        <v>1</v>
-      </c>
-      <c r="H55" t="n">
-        <v>813</v>
-      </c>
-      <c r="I55" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>172</v>
+        <v>122</v>
       </c>
       <c r="B56" t="n">
-        <v>5604</v>
+        <v>4751</v>
       </c>
       <c r="C56" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D56" t="n">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="E56" t="n">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F56" t="s">
-        <v>6</v>
+        <v>200</v>
       </c>
       <c r="G56" t="n">
-        <v>184</v>
+        <v>1</v>
       </c>
       <c r="H56" t="n">
-        <v>819</v>
+        <v>813</v>
       </c>
       <c r="I56" t="s">
-        <v>112</v>
+        <v>163</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>41</v>
+        <v>170</v>
       </c>
       <c r="B57" t="n">
-        <v>5058</v>
+        <v>5604</v>
       </c>
       <c r="C57" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D57" t="n">
-        <v>248</v>
+        <v>62</v>
       </c>
       <c r="E57" t="n">
-        <v>545</v>
+        <v>273</v>
       </c>
       <c r="F57" t="s">
-        <v>137</v>
+        <v>6</v>
       </c>
       <c r="G57" t="n">
-        <v>742</v>
+        <v>184</v>
       </c>
       <c r="H57" t="n">
-        <v>1635</v>
+        <v>819</v>
       </c>
       <c r="I57" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="B58" t="n">
-        <v>1021</v>
+        <v>5058</v>
       </c>
       <c r="C58" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D58" t="n">
-        <v>1</v>
+        <v>248</v>
       </c>
       <c r="E58" t="n">
-        <v>301</v>
+        <v>545</v>
       </c>
       <c r="F58" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="G58" t="n">
-        <v>1</v>
+        <v>742</v>
       </c>
       <c r="H58" t="n">
-        <v>903</v>
+        <v>1635</v>
       </c>
       <c r="I58" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" t="n">
+        <v>1021</v>
+      </c>
+      <c r="C59" t="s">
+        <v>218</v>
+      </c>
+      <c r="D59" t="n">
+        <v>1</v>
+      </c>
+      <c r="E59" t="n">
+        <v>301</v>
+      </c>
+      <c r="F59" t="s">
+        <v>118</v>
+      </c>
+      <c r="G59" t="n">
+        <v>1</v>
+      </c>
+      <c r="H59" t="n">
+        <v>903</v>
+      </c>
+      <c r="I59" t="s">
         <v>73</v>
-      </c>
-      <c r="B59" t="n">
-        <v>5610</v>
-      </c>
-      <c r="C59" t="s">
-        <v>219</v>
-      </c>
-      <c r="D59" t="n">
-        <v>254</v>
-      </c>
-      <c r="E59" t="n">
-        <v>551</v>
-      </c>
-      <c r="F59" t="s">
-        <v>121</v>
-      </c>
-      <c r="G59" t="n">
-        <v>760</v>
-      </c>
-      <c r="H59" t="n">
-        <v>1653</v>
-      </c>
-      <c r="I59" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>92</v>
+        <v>194</v>
       </c>
       <c r="B60" t="n">
-        <v>5608</v>
+        <v>5610</v>
       </c>
       <c r="C60" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D60" t="n">
-        <v>1</v>
+        <v>254</v>
       </c>
       <c r="E60" t="n">
-        <v>334</v>
+        <v>551</v>
       </c>
       <c r="F60" t="s">
-        <v>138</v>
+        <v>171</v>
       </c>
       <c r="G60" t="n">
-        <v>1</v>
+        <v>760</v>
       </c>
       <c r="H60" t="n">
-        <v>1002</v>
+        <v>1653</v>
       </c>
       <c r="I60" t="s">
-        <v>159</v>
+        <v>43</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="B61" t="n">
-        <v>140609</v>
+        <v>5608</v>
       </c>
       <c r="C61" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D61" t="n">
         <v>1</v>
       </c>
       <c r="E61" t="n">
-        <v>302</v>
+        <v>334</v>
       </c>
       <c r="F61" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="G61" t="n">
         <v>1</v>
       </c>
       <c r="H61" t="n">
-        <v>906</v>
+        <v>1002</v>
       </c>
       <c r="I61" t="s">
-        <v>77</v>
+        <v>158</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B62" t="n">
-        <v>659</v>
+        <v>140609</v>
       </c>
       <c r="C62" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D62" t="n">
-        <v>189</v>
+        <v>1</v>
       </c>
       <c r="E62" t="n">
-        <v>517</v>
+        <v>302</v>
       </c>
       <c r="F62" t="s">
-        <v>65</v>
+        <v>126</v>
       </c>
       <c r="G62" t="n">
-        <v>565</v>
+        <v>1</v>
       </c>
       <c r="H62" t="n">
-        <v>1551</v>
+        <v>906</v>
       </c>
       <c r="I62" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B63" t="n">
-        <v>5127</v>
+        <v>659</v>
       </c>
       <c r="C63" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D63" t="n">
-        <v>163</v>
+        <v>189</v>
       </c>
       <c r="E63" t="n">
-        <v>478</v>
+        <v>517</v>
       </c>
       <c r="F63" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="G63" t="n">
-        <v>487</v>
+        <v>565</v>
       </c>
       <c r="H63" t="n">
-        <v>1434</v>
+        <v>1551</v>
       </c>
       <c r="I63" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B64" t="n">
-        <v>5605</v>
+        <v>5127</v>
       </c>
       <c r="C64" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D64" t="n">
-        <v>55</v>
+        <v>163</v>
       </c>
       <c r="E64" t="n">
-        <v>400</v>
+        <v>478</v>
       </c>
       <c r="F64" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G64" t="n">
-        <v>163</v>
+        <v>487</v>
       </c>
       <c r="H64" t="n">
-        <v>1200</v>
+        <v>1434</v>
       </c>
       <c r="I64" t="s">
-        <v>215</v>
+        <v>107</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
       <c r="B65" t="n">
-        <v>1457</v>
+        <v>5605</v>
       </c>
       <c r="C65" t="s">
-        <v>2</v>
+        <v>218</v>
       </c>
       <c r="D65" t="n">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="E65" t="n">
-        <v>335</v>
+        <v>400</v>
       </c>
       <c r="F65" t="s">
-        <v>226</v>
+        <v>31</v>
       </c>
       <c r="G65" t="n">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="H65" t="n">
-        <v>1005</v>
+        <v>1200</v>
       </c>
       <c r="I65" t="s">
-        <v>173</v>
+        <v>214</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>135</v>
+        <v>88</v>
       </c>
       <c r="B66" t="n">
-        <v>11200</v>
+        <v>1457</v>
       </c>
       <c r="C66" t="s">
         <v>2</v>
       </c>
       <c r="D66" t="n">
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E66" t="n">
-        <v>531</v>
+        <v>335</v>
       </c>
       <c r="F66" t="s">
-        <v>197</v>
+        <v>226</v>
       </c>
       <c r="G66" t="n">
-        <v>628</v>
+        <v>1</v>
       </c>
       <c r="H66" t="n">
-        <v>1593</v>
+        <v>1005</v>
       </c>
       <c r="I66" t="s">
-        <v>10</v>
+        <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="B67" t="n">
-        <v>5566</v>
+        <v>11200</v>
       </c>
       <c r="C67" t="s">
         <v>2</v>
       </c>
       <c r="D67" t="n">
-        <v>16</v>
+        <v>210</v>
       </c>
       <c r="E67" t="n">
-        <v>351</v>
+        <v>531</v>
       </c>
       <c r="F67" t="s">
-        <v>79</v>
+        <v>196</v>
       </c>
       <c r="G67" t="n">
-        <v>46</v>
+        <v>628</v>
       </c>
       <c r="H67" t="n">
-        <v>1053</v>
+        <v>1593</v>
       </c>
       <c r="I67" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="B68" t="n">
-        <v>1445</v>
+        <v>5566</v>
       </c>
       <c r="C68" t="s">
         <v>2</v>
       </c>
       <c r="D68" t="n">
-        <v>188</v>
+        <v>16</v>
       </c>
       <c r="E68" t="n">
-        <v>450</v>
+        <v>351</v>
       </c>
       <c r="F68" t="s">
-        <v>154</v>
+        <v>80</v>
       </c>
       <c r="G68" t="n">
-        <v>562</v>
+        <v>46</v>
       </c>
       <c r="H68" t="n">
-        <v>1350</v>
+        <v>1053</v>
       </c>
       <c r="I68" t="s">
-        <v>191</v>
+        <v>22</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="B69" t="n">
-        <v>5600</v>
+        <v>1445</v>
       </c>
       <c r="C69" t="s">
         <v>2</v>
       </c>
       <c r="D69" t="n">
-        <v>1</v>
+        <v>188</v>
       </c>
       <c r="E69" t="n">
-        <v>364</v>
+        <v>450</v>
       </c>
       <c r="F69" t="s">
-        <v>11</v>
+        <v>153</v>
       </c>
       <c r="G69" t="n">
-        <v>1</v>
+        <v>562</v>
       </c>
       <c r="H69" t="n">
-        <v>1092</v>
+        <v>1350</v>
       </c>
       <c r="I69" t="s">
-        <v>72</v>
+        <v>190</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>218</v>
+        <v>57</v>
       </c>
       <c r="B70" t="n">
-        <v>1459</v>
+        <v>5600</v>
       </c>
       <c r="C70" t="s">
         <v>2</v>
@@ -3071,169 +3071,169 @@
         <v>1</v>
       </c>
       <c r="E70" t="n">
-        <v>334</v>
+        <v>364</v>
       </c>
       <c r="F70" t="s">
-        <v>155</v>
+        <v>174</v>
       </c>
       <c r="G70" t="n">
         <v>1</v>
       </c>
       <c r="H70" t="n">
-        <v>1002</v>
+        <v>1092</v>
       </c>
       <c r="I70" t="s">
-        <v>120</v>
+        <v>74</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>175</v>
+        <v>217</v>
       </c>
       <c r="B71" t="n">
-        <v>4140</v>
+        <v>1459</v>
       </c>
       <c r="C71" t="s">
         <v>2</v>
       </c>
       <c r="D71" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E71" t="n">
-        <v>370</v>
+        <v>334</v>
       </c>
       <c r="F71" t="s">
-        <v>204</v>
+        <v>154</v>
       </c>
       <c r="G71" t="n">
-        <v>142</v>
+        <v>1</v>
       </c>
       <c r="H71" t="n">
-        <v>1110</v>
+        <v>1002</v>
       </c>
       <c r="I71" t="s">
-        <v>166</v>
+        <v>120</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>14</v>
+        <v>173</v>
       </c>
       <c r="B72" t="n">
-        <v>2011</v>
+        <v>4140</v>
       </c>
       <c r="C72" t="s">
         <v>2</v>
       </c>
       <c r="D72" t="n">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="E72" t="n">
-        <v>330</v>
+        <v>370</v>
       </c>
       <c r="F72" t="s">
-        <v>184</v>
+        <v>203</v>
       </c>
       <c r="G72" t="n">
-        <v>46</v>
+        <v>142</v>
       </c>
       <c r="H72" t="n">
-        <v>990</v>
+        <v>1110</v>
       </c>
       <c r="I72" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>158</v>
+        <v>15</v>
       </c>
       <c r="B73" t="n">
-        <v>5595</v>
+        <v>2011</v>
       </c>
       <c r="C73" t="s">
         <v>2</v>
       </c>
       <c r="D73" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E73" t="n">
-        <v>379</v>
+        <v>330</v>
       </c>
       <c r="F73" t="s">
-        <v>54</v>
+        <v>183</v>
       </c>
       <c r="G73" t="n">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="H73" t="n">
-        <v>1137</v>
+        <v>990</v>
       </c>
       <c r="I73" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>195</v>
+        <v>157</v>
       </c>
       <c r="B74" t="n">
-        <v>7443</v>
+        <v>5595</v>
       </c>
       <c r="C74" t="s">
         <v>2</v>
       </c>
       <c r="D74" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E74" t="n">
-        <v>364</v>
+        <v>379</v>
       </c>
       <c r="F74" t="s">
-        <v>93</v>
+        <v>54</v>
       </c>
       <c r="G74" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H74" t="n">
-        <v>1092</v>
+        <v>1137</v>
       </c>
       <c r="I74" t="s">
-        <v>90</v>
+        <v>223</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>134</v>
+        <v>75</v>
       </c>
       <c r="B75" t="n">
-        <v>1612</v>
+        <v>7443</v>
       </c>
       <c r="C75" t="s">
-        <v>219</v>
+        <v>2</v>
       </c>
       <c r="D75" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E75" t="n">
-        <v>285</v>
+        <v>364</v>
       </c>
       <c r="F75" t="s">
-        <v>165</v>
+        <v>94</v>
       </c>
       <c r="G75" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H75" t="n">
-        <v>855</v>
+        <v>1092</v>
       </c>
       <c r="I75" t="s">
-        <v>15</v>
+        <v>91</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B76" t="n">
         <v>1956</v>
@@ -3262,7 +3262,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B77" t="n">
         <v>673</v>
@@ -3274,24 +3274,24 @@
         <v>444</v>
       </c>
       <c r="E77" t="n">
-        <v>719</v>
+        <v>712</v>
       </c>
       <c r="F77" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="G77" t="n">
         <v>1330</v>
       </c>
       <c r="H77" t="n">
-        <v>2157</v>
+        <v>2136</v>
       </c>
       <c r="I77" t="s">
-        <v>149</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B78" t="n">
         <v>4233</v>
@@ -3306,7 +3306,7 @@
         <v>1346</v>
       </c>
       <c r="F78" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G78" t="n">
         <v>3112</v>
@@ -3320,7 +3320,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B79" t="n">
         <v>2260</v>
@@ -3364,7 +3364,7 @@
         <v>512</v>
       </c>
       <c r="F80" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G80" t="n">
         <v>685</v>
@@ -3393,7 +3393,7 @@
         <v>360</v>
       </c>
       <c r="F81" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G81" t="n">
         <v>1</v>
@@ -3407,7 +3407,7 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>24</v>
+        <v>123</v>
       </c>
       <c r="B82" t="n">
         <v>5594</v>
@@ -3431,7 +3431,7 @@
         <v>1080</v>
       </c>
       <c r="I82" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -3451,7 +3451,7 @@
         <v>531</v>
       </c>
       <c r="F83" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G83" t="n">
         <v>628</v>
@@ -3460,7 +3460,7 @@
         <v>1593</v>
       </c>
       <c r="I83" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -3509,7 +3509,7 @@
         <v>345</v>
       </c>
       <c r="F85" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G85" t="n">
         <v>97</v>
@@ -3523,7 +3523,7 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B86" t="n">
         <v>5747</v>
@@ -3538,7 +3538,7 @@
         <v>689</v>
       </c>
       <c r="F86" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G86" t="n">
         <v>1231</v>
@@ -3547,7 +3547,7 @@
         <v>2067</v>
       </c>
       <c r="I86" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -3558,7 +3558,7 @@
         <v>5599</v>
       </c>
       <c r="C87" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D87" t="n">
         <v>1</v>
@@ -3576,18 +3576,18 @@
         <v>1092</v>
       </c>
       <c r="I87" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B88" t="n">
         <v>5604</v>
       </c>
       <c r="C88" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D88" t="n">
         <v>62</v>
@@ -3610,7 +3610,7 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B89" t="n">
         <v>6790</v>
@@ -3625,7 +3625,7 @@
         <v>391</v>
       </c>
       <c r="F89" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G89" t="n">
         <v>373</v>
@@ -3634,12 +3634,12 @@
         <v>1173</v>
       </c>
       <c r="I89" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B90" t="n">
         <v>5595</v>
@@ -3697,7 +3697,7 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B92" t="n">
         <v>6197</v>
@@ -3726,7 +3726,7 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B93" t="n">
         <v>3702</v>
@@ -3741,7 +3741,7 @@
         <v>620</v>
       </c>
       <c r="F93" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G93" t="n">
         <v>1069</v>
@@ -3770,7 +3770,7 @@
         <v>351</v>
       </c>
       <c r="F94" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G94" t="n">
         <v>46</v>
@@ -3784,7 +3784,7 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B95" t="n">
         <v>1457</v>
@@ -3808,7 +3808,7 @@
         <v>1005</v>
       </c>
       <c r="I95" t="s">
-        <v>173</v>
+        <v>121</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -3828,7 +3828,7 @@
         <v>330</v>
       </c>
       <c r="F96" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G96" t="n">
         <v>1</v>
@@ -3837,12 +3837,12 @@
         <v>990</v>
       </c>
       <c r="I96" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="97" spans="1:9">
       <c r="A97" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B97" t="n">
         <v>9261</v>
@@ -3857,7 +3857,7 @@
         <v>348</v>
       </c>
       <c r="F97" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G97" t="n">
         <v>73</v>

</xml_diff>

<commit_message>
Updates to PDB construct selection manual exceptions.
</commit_message>
<xml_diff>
--- a/analysis/PDB_construct_selection/PDB_constructs.xlsx
+++ b/analysis/PDB_construct_selection/PDB_constructs.xlsx
@@ -47,649 +47,649 @@
     <t>GTGGAGGACCATTATGAGATGGGGGAGGAGCTGGGCAGCGGCCAGTTTGCGATCGTGCGGAAGTGCCGGCAGAAGGGCACGGGCAAGGAGTACGCAGCCAAGTTCATCAAGAAGCGCCGCCTGTCATCCAGCCGGCGTGGGGTGAGCCGGGAGGAGATCGAGCGGGAGGTGAACATCCTGCGGGAGATCCGGCACCCCAACATCATCACCCTGCACGACATCTTCGAGAACAAGACGGACGTGGTCCTCATCCTGGAGCTGGTCTCTGGCGGGGAGCTCTTTGACTTCCTGGCGGAGAAGGAGTCGCTGACGGAGGACGAGGCCACCCAGTTCCTCAAGCAGATCCTGGACGGCGTTCACTACCTGCACTCTAAGCGCATCGCACACTTTGACCTGAAGCCGGAAAACATCATGCTGCTGGACAAGAACGTGCCCAACCCACGAATCAAGCTCATCGACTTCGGCATCGCGCACAAGATCGAGGCGGGGAACGAGTTCAAGAACATCTTCGGCACCCCGGAGTTTGTGGCCCCAGAGATTGTGAACTATGAGCCGCTGGGCCTGGAGGCGGACATGTGGAGCATCGGTGTCATCACCTATATCCTCCTGAGCGGTGCATCCCCGTTCCTGGGCGAGACCAAGCAGGAGACGCTCACCAACATCTCAGCCGTGAACTACGACTTCGACGAGGAGTACTTCAGCAACACCAGCGAGCTGGCCAAGGACTTCATTCGCCGGCTGCTCGTCAAAGATCCCAAGCGGAGAATGACCATTGCCCAGAGCCTGGAACATTCCTGGATTAAGGCGATCCGGCGGCGGAACGTGCGTGGTGAGGACAGCGGC</t>
   </si>
   <si>
+    <t>AAGCACGACGGGCGGGTGAAGATCGGACACTACGTGCTGGGCGACACGCTGGGCGTCGGCACCTTCGGCAAAGTGAAGATTGGAGAACATCAATTAACAGGCCATAAAGTGGCAGTTAAAATCTTAAATAGACAGAAGATTCGCAGTTTAGATGTTGTTGGAAAAATAAAACGAGAAATTCAAAATCTAAAACTCTTTCGTCATCCTCATATTATCAAACTATACCAGGTGATCAGCACTCCAACAGATTTTTTTATGGTAATGGAATATGTGTCTGGAGGTGAATTATTTGACTACATCTGTAAGCATGGACGGGTTGAAGAGATGGAAGCCAGGCGRCTCTTTCAGCAGATTCTGTCTGCTGTGGATTACTGTCATAGGCATATGGTTGTTCATCGAGACCTGAAACCAGAGAATGTCCTGTTGGATGCACACATGAATGCCAAGATAGCCGATTTCGGATTATCTAATATGATGTCAGATGGTGAATTTCTGAGAACTAGTTGCGGATCTCCAAATTATGCAGCACCTGAAGTCATCTCAGGCAGATTGTATGCAGGTCCTGAAGTTGATATCTGGAGCTGTGGTGTTATCTTGTATGCTCTTCTTTGTGGCACCCTCCCATTTGATGATGAGCATGTACCTACGTTATTTAAGAAGATCCGAGGGGGTGTCTTTTATATCCCAGAATATCTCAATCGTTCTGTCGCCACTCTCCTGATGCATATGCTGCAGGTTGACCCACTGAAACGAGCAACTATCAAAGACATAAGAGAGCATGAATGGTTTAAACAAGATTTGCCCAGTTACTTATTTCCTGAA</t>
+  </si>
+  <si>
+    <t>CSKP_HUMAN_D0_3TAC_A</t>
+  </si>
+  <si>
+    <t>MST4_HUMAN_D0_4FZD_B</t>
+  </si>
+  <si>
+    <t>CGGGACTCGAGTGATGATTGGGAGATTCCTGATGGGCAGATTACAGTGGGACAAAGAATTGGATCTGGATCATTTGGAACAGTCTACAAGGGAAAGTGGCATGGTGATGTGGCAGTGAAAATGTTGAATGTGACAGCACCTACACCTCAGCAGTTACAAGCCTTCAAAAATGAAGTAGGAGTACTCAGGAAAACACGACATGTGAATATCCTACTCTTCATGGGCTATTCCACAAAGCCACAACTGGCTATTGTTACCCAGTGGTGTGAGGGCTCCAGCTTGTATCACCATCTCCATATCATTGAGACCAAATTTGAGATGATCAAgCTTATAGATATTGCACGACAGACTGCACAGGGCATGGATTACTTACACGCCAAGTCAATCATCCACAGAGACCTCAAGAGTAATAATATATTTCTTCATGAAGACCTCACAGTAAAAATAGGTGATTTTGGTCTAGCTACAGTGAAATCTCGATGGAGTGGGTCCCATCAGTTTGAACAGTTGTCTGGgTCCATTTTGTGGATGGCACCAGAAGTCATCAGAATGCAAGATAAAAATCCATACAGCTTTCAGTCAGATGTATATGCATTTGGgATTGTTCTGTATGAATTGATGACTGGACAGTTACCTTATTCAAACATCAACAACAGGGACCAGATAATTTTTATGGTGGGACGAGGATACCTGTCTCCAGATCTCAGTAAGGTACGGAGTAACTGTCCAAAAGCCATGAAGAGATTAATGGCAGAGTGCCTCAAAAAGAAAAGAGATGAGAGACCACTCTTTCCCCAAATTCTCGCC</t>
+  </si>
+  <si>
+    <t>MARK2_HUMAN_D0_3IEC_D</t>
+  </si>
+  <si>
+    <t>CCATTTCCAGAAGGCAAGGTTCTGGATGATATGGAAGGCAATCAGTGGGTACTGGGCAAGAAGATTGGCTCTGGAGGATTTGGATTGATATATTTAGCTTTCCCCACAAATAAACCAGAGAAAGATGCAAGACATGTAGTAAAAGTGGAATATCAAGAAAATGGCCCGTTATTTTCAGAACTTAAATTTTATCAGAGAGTTGCAAAAAAAGACTGTATCAAAAAGTGGATAGAACGCAAACAACTTGATTATTTAGGAATTCCTCTGTTTTATGGATCTGGTCTGACTGAATTCAAGGGAAGAAGTTACAGATTTATGGTAATGGAAAGACTAGGAATAGATTTACAGAAGATCTCAGGCCAGAATGGTACCTTTAAAAAGTCAACTGTCCTGCAATTAGGTATCCGAATGTTGGATGTACTGGAATATATACATGAAAATGAATATGTTCATGGTGATATAAAAGCAGCAAATCTACTTTTGGGTTACAAAAATCCAGACCAGGTTTATCTTGCAGATTATGGACTTTCCTACAGATATTGTCCCAATGGGAACCACAAACAGTATCAGGAAAATCCTAGAAAAGGCCATAATGGGACAATAGAGTTTACCAGCTTGGATGCCCACAAGGGAGTAGCCTTGTCCAGACGAAGTGACGTTGAGATCCTCGGCTACTGCATGCTGCGGTGGTTGTGTGGGAAACTTCCCTGGGAACAGAACCTGAAGGACCCTGTGGCTGTGCAGACTGCTAAAACAAATCTGTTGGACGAGCTCCCCCAGTCAGTGCTTAAATGGGCTCCTTCTGGAAGCAGTTGCTGTGAAATAGCCCAATTTTTGGTATGTGCTCATAGTTTAGCATATGATGAAAAGCCAAACTATCAAGCCCTCAAGAAAATTTTGAACCCTCATGGAATACCTTTAGGACCACTGGACTTTTCCACAAAAGGACAGAGTATAAATGTCCAT</t>
+  </si>
+  <si>
+    <t>GGGGACTCTGATATATCCAGTCCATTACTGCAAAATACTGTCCACATTGACCTCAGTGCTCTAAATCCAGAGCTGGTCCAGGCAGTGCAGCATGTAGTGATTGGGCCCAGTAGCCTGATTGTGCATTTCAATGAAGTCATAGGAAGAGGGCATTTTGGTTGTGTATATCATGGGACTTTGTTGGACAATGATGGCAAGAAAATTCACTGTGCTGTGAAATCCTTGAACAGAATCACTGACATAGGAGAAGTTTCCCAATTTCTGACCGAGGGAATCATCATGAAAGATTTTAGTCATCCCAATGTCCTCTCGCTCCTGGGAATCTGCCTGCGAAGTGAAGGGTCTCCGCTGGTGGTCCTACCATACATGAAACATGGAGATCTTCGAAATTTCATTCGAAATGAGACTCATAATCCAACTGTAAAAGATCTTATTGGCTTTGGTCTTCAAGTAGCCAAAGGCATGAAATATCTTGCAAGCAAAAAGTTTGTCCACAGAGACTTGGCTGCAAGAAACTGTATGCTGGATGAAAAATTCACAGTCAAGGTTGCTGATTTTGGTCTTGCCAGAGACATGTATGATAAAGAATACTATAGTGTACACAACAAAACAGGTGCAAAGCTGCCAGTGAAGTGGATGGCTTTGGAAAGTCTGCAAACTCAAAAGTTTACCACCAAGTCAGATGTGTGGTCCTTTGGCGTGCTCCTCTGGGAGCTGATGACAAGAGGAGCCCCACCTTATCCTGACGTAAACACCTTTGATATAACTGTTTACTTGTTGCAAGGGAGAAGACTCCTACAACCCGAATACTGCCCAGACCCCTTATATGAAGTAATGCTAAAATGCTGGCACCCTAAAGCCGAAATGCGCCCATCCTTTTCTGAACTGGTGTCCCGGATATCAGCGATCTTCTCTACTTTCATTGGG</t>
+  </si>
+  <si>
+    <t>YQLFEELGKGAFSVVRRCVKVLAGQEYAAKIINTKKLSARDHQKLEREARICRLLKHPNIVRLHDSISEEGHHYLIFDLVTGGELFEDIVAREYYSEADASHCIQQILEAVLHCHQMGVVHRDLKPENLLLASKLKGAAVKLADFGLAIEVEGEQQAWFGFAGTPGYLSPEVLRKDPYGKPVDLWACGVILYILLVGYPPFWDEDQHRLYLQIKAGAYDFPSPEWDTVTPEAKDLINKMLTINPSKRITAAEALKHPWISHRSTVASCMHRQETVDCLKKFNARRKLKGA</t>
+  </si>
+  <si>
+    <t>ENFQKVEKIGEGTYGVVYKARNKLTGEVVALKKIRLDTETEGVPSTAIREISLLKELNHPNIVKLLDVIHTENKLYLVFEFLHQDLKKFMDASALTGIPLPLIKSYLFQLLQGLAFCHSHRVLHRDLKPQNLLINTEGAIKLADFGLARAFGVPVRTYTHEVVTLWYRAPEILLGCKYYSTAVDIWSLGCIFAEMVTRRALFPGDSEIDQLFRIFRTLGTPDEVVWPGVTSMPDYKPSFPKWARQDFSKVVPPLDEDGRSLLSQMLHYDPNKRISAKAALAHPFFQDVTKPVPHL</t>
+  </si>
+  <si>
+    <t>TTK_HUMAN_D0_3H9F_A</t>
+  </si>
+  <si>
+    <t>SVKGRIYSILKQIGSGGSSKVFQVLNEKKQIYAIKYVNLEEADNQTLDSYRNEIAYLNKLQQHSDKIIRLYDYEITDQYIYMVMECGNIDLNSWLKKKKSIDPWERKSYWKNMLEAVHTIHQHGIVHSDLKPANFLIVDGMLKLIDFGIANQMQPDTTSVVKDSQVGTVNYMPPEAIKDMSSSRENGKSKSKISPKSDVWSLGCILYYMTYGKTPFQQIINQISKLHAIIDPNHEIEFPDIPEKDLQDVLKCCLKRDPKQRISIPELLAHPYVQIQTHPVNQMAKGTTEE</t>
+  </si>
+  <si>
+    <t>GTGAAAGAATTCTTAGCCAAAGCCAAAGAAGATTTTCTTAAAAAATGGGAAAGTCCCGCTCAGAACACAGCCCACTTGGATCAGTTTGAACGAATCAAGACCCTCGGCACGGGCTCCTTCGGGCGGGTGATGCTGGTGAAACACAAGGAGACCGGGAACCACTATGCCATGAAGATCCTCGACAAACAGAAGGTGGTGAAACTGAAACAGATCGAACACACCCTGAATGAAAAGCGCATCCTGCAAGCTGTCAACTTTCCGTTCCTCGTCAAACTCGAGTTCTCCTTCAAGGACAACTCAAACTTATACATGGTCATGGAGTACGTGCCCGGCGGGGAGATGTTCTCACACCTACGGCGGATCGGAAGGTTCAGTGAGCCCCATGCCCGTTTCTACGCGGCCCAGATCGTCCTGACCTTTGAGTATCTGCACTCGCTGGATCTCATCTACAGGGACCTGAAGCCGGAGAATCTGCTCATTGACCAGCAGGGCTACATTCAGGTGACAGACTTCGGTTTCGCCAAGCGCGTGAAGGGCCGCACTTGGACCTTGTGCGGCACCCCTGAGTACCTGGCCCCTGAGATTATCCTGAGCAAAGGCTACAACAAGGCCGTGGACTGGTGGGCCCTGGGGGTTCTTATCTATGAAATGGCCGCTGGCTACCCGCCCTTCTTCGCAGACCAGCCCATCCAGATCTATGAGAAGATCGTCTCTGGGAAGGTGCGCTTCCCTTCCCACTTCAGCTCTGACTTGAAGGACCTGCTGCGGAACCTCCTGCAGGTAGATCTCACCAAGCGCTTTGGGAACCTCAAGAATGGGGTCAACGATATCAAGAACCACAAGTGGTTTGCCACAACTGACTGGATTGCCATCTACCAGAGGAAGGTGGAAGCTCCCTTCATACCAAAGTTTAAAGGCCCTGGGGATACGAGTAACTTTGACGACTATGAGGAAGAAGAAATCCGGGTCTCCATCAATGAGAAGTGTGGCAAGGAGTTTTCTGAGTTT</t>
+  </si>
+  <si>
+    <t>TCCCCCAACTACGACAAGTGGGAGATGGAACGCACGGACATCACCATGAAGCACAAGCTGGGCGGGGGCCAGTACGGGGAGGTGTACGAGGGCGTGTGGAAGAAATACAGCCTGACGGTGGCCGTGAAGACCTTGAAGGAGGACACCATGGAGGTGGAAGAGTTCTTGAAAGAAGCTGCAGTCATGAAAGAGATCAAACACCCTAACCTGGTGCAGCTCCTTGGGGTCTGCACCCGGGAGCCCCCGTTCTATATCATCACTGAGTTCATGACCTACGGGAACCTCCTGGACTACCTGAGGGAGTGCAACCGGCAGGAGGTGAACGCCGTGGTGCTGCTGTACATGGCCACTCAGATCTCGTCAGCCATGGAGTACCTGGAGAAGAAAAACTTCATCCACAGAGATCTTGCTGCCCGAAACTGCCTGGTAGGGGAGAACCACTTGGTGAAGGTAGCTGATTTTGGCCTGAGCAGGTTGATGACAGGGGACACCTACACAGCCCATGCTGGAGCCAAGTTCCCCATCAAATGGACTGCACCCGAGAGCCTGGCCTACAACAAGTTCTCCATCAAGTCCGACGTCTGGGCATTTGGAGTATTGCTTTGGGAAATTGCTACCTATGGCATGTCCCCTTACCCGGGAATTGACCTGTCCCAGGTGTATGAGCTGCTAGAGAAGGACTACCGCATGGAGCGCCCAGAAGGCTGCCCAGAGAAGGTCTATGAACTCATGCGAGCATGTTGGCAGTGGAATCCCTCTGACCGGCCCTCCTTTGCTGAAATCCACCAAGCCTTTGAAACAATGTTCCAGGAATCCAGTATCTCAGACGAAGTGGAAAAGGAGCTGGGGAAA</t>
+  </si>
+  <si>
+    <t>RDSSDDWEIPDGQITVGQRIGSGSFGTVYKGKWHGDVAVKMLNVTAPTPQQLQAFKNEVGVLRKTRHVNILLFMGYSTKPQLAIVTQWCEGSSLYHHLHIIETKFEMIKLIDIARQTAQGMDYLHAKSIIHRDLKSNNIFLHEDLTVKIGDFGLATVKSRWSGSHQFEQLSGSILWMAPEVIRMQDKNPYSFQSDVYAFGIVLYELMTGQLPYSNINNRDQIIFMVGRGYLSPDLSKVRSNCPKAMKRLMAECLKKKRDERPLFPQILA</t>
+  </si>
+  <si>
+    <t>KS6A1_HUMAN_D1_3RNY_B</t>
+  </si>
+  <si>
+    <t>WALNMKELKLLQTIGKGEFGDVMLGDYRGNKVAVKCIKNDATAQAFLAEASVMTQLRHSNLVQLLGVIVEEKGGLYIVTEYMAKGSLVDYLRSRGRSVLGGDCLLKFSLDVCEAMEYLEGNNFVHRDLAARNVLVSEDNVAKVSDFGLTKEASSTQDTGKLPVKWTAPEALREKKFSTKSDVWSFGILLWEIYSFGRVPYPRIPLKDVVPRVEKGYKMDAPDGCPPAVYEVMKNCWHLDAAMRPSFLQLREQLEHIKTHELHL</t>
+  </si>
+  <si>
+    <t>MSRSKRDNNFYSVEIGDSTFTVLKRYQNLKPIGSGAQGIVCAAYDAILERNVAIKKLSRPFQNQTHAKRAYRELVLMKCVNHKNIIGLLNVFTPQKSLEEFQDVYIVMELMDANLCQVIQMELDHERMSYLLYQMLCGIKHLHSAGIIHRDLKPSNIVVKSDCTLKILDFGLARTAGTSFMMTPYVVTRYYRAPEVILGMGYKENVDLWSVGCIMGEMVCHKILFPGRDYIDQWNKVIEQLGTPCPEFMKKLQPTVRTYVENRPKYAGYSFEKLFPDVLFPADSEHNKLKASQARDLLSKMLVIDASKRISVDEALQHPYINVWYDPSEAEAPPPKIPDKQLDEREHTIEEWKELIYKEVMDLE</t>
+  </si>
+  <si>
+    <t>STRAA_HUMAN_D0_3GNI_B</t>
+  </si>
+  <si>
+    <t>MP2K2_HUMAN_D0_1S9I_A</t>
+  </si>
+  <si>
+    <t>PIM1_HUMAN_D0_4A7C_A</t>
+  </si>
+  <si>
+    <t>EAFLTQKAKVGELKDDDFERISELGAGNGGVVTKVQHRPSGLIMARKLIHLEIKPAIRNQIIRELQVLHECNSPYIVGFYGAFYSDGEISICMEHMDGGSLDQVLKEAKRIPEEILGKVSIAVLRGLAYLREKHQIMHRDVKPSNILVNSRGEIKLCDFGVSGQLIDSMANSFVGTRSYMAPERLQGTHYSVQSDIWSMGLSLVELAVGRYPIPPPDAKELEAIFGRPVVDGEEGEPHSISPRPRPPGRPVSGHGMDSRPAMAIFELLDYIVNEPPPKLPNGVFTPDFQEFVNKCLIKNPAERADLKMLTNHTFIKRSEVEEVDFAGWLCKTLRLNQPGTPTRTAV</t>
+  </si>
+  <si>
+    <t>GGGCCGGAGGATGAGCTGCCCGACTGGGCCGCCGCCAAAGAGTTTTACCAGAAGTACGACCCTAAGGACGTCATCGGCAGAGGAGTGAGCTCTGTGGTCCGCCGTTGTGTTCATCGAGCTACTGGCCACGAGTTTGCGGTGAAGATTATGGAAGTGACAGCTGAGCGGCTGAGTCCTGAGCAGCTGGAGGAGGTGCGGGAAGCCACACGGCGAGAGACACACATCCTTCGCCAGGTCGCCGGCCACCCCCACATCATCACCCTCATCGATTCCTACGAGTCTTCTAGCTTCATGTTCCTGGTGTTTGACCTGATGCGGAAGGGAGAGCTGTTTGACTATCTCACAGAGAAGGTGGCCCTCTCTGAAAAGGAAACCAGGTCCATCATGCGGTCTCTGCTGGAAGCAGTGAGCTTTCTCCATGCCAACAACATTGTGCATCGAGATCTGAAGCCCGAGAATATTCTCCTAGATGACAATATGCAGATCCGACTTTCAGATTTCGGGTTCTCCTGCCACTTGGAACCTGGCGAGAAGCTTCGAGAGTTGTGTGGGACCCCAGGGTATCTAGCGCCAGAGATCCTTAAATGCTCCATGGATGAAACCCACCCAGGCTATGGCAAGGAGGTCGACCTCTGGGCCTGTGGGGTGATCTTGTTCACACTCCTGGCTGGCTCGCCACCCTTCTGGCACCGGCGGCAGATCCTGATGTTACGCATGATCATGGAGGGCCAGTACCAGTTCAGTTCCCCCGAGTGGGATGACCGTTCCAGCACTGTCAAAGACCTGATCTCCAGGCTGCTGCAGGTGGATCCTGAGGCACGCCTGACAGCTGAGCAGGCCCTACAGCACCCCTTCTTTGAGCGT</t>
+  </si>
+  <si>
+    <t>KC1E_HUMAN_D0_4HNI_A</t>
+  </si>
+  <si>
+    <t>VRK2_HUMAN_D0_2V62_B</t>
+  </si>
+  <si>
+    <t>ETYIKLDKLGEGTYATVYKGKSKLTDNLVALKEIRLEHEEGAPCTAIREVSLLKDLKHANIVTLHDIIHTEKSLTLVFEYLDKDLKQYLDDCGNIINMHNVKLFLFQLLRGLAYCHRQKVLHRDLKPQNLLINERGELKLADFGLARAKSIPTKTYSNEVVTLWYRPPDILLGSTDYSTQIDMWGVGCIFYEMATGRPLFPGSTVEEQLHFIFRILGTPTEETWPGILSNEEFKTYNYPKYRAEALLSHAPRLDSDGADLLTKLLQFEGRNRISAEDAMKHPFFLSLGERIHKLPDTTSIFALKEIQLQKEASLRS</t>
+  </si>
+  <si>
+    <t>HQLQPRRVSFRGEASETLQSPGYDPSRPESFFQQSFQRLSRLGHGSYGEVFKVRSKEDGRLYAVKRSMSPFRGPKDRARKLAEVGSHEKVGQHPCCVRLEQAWEEGGILYLQTELCGPSLQQHCEAWGASLPEAQVWGYLRDTLLALAHLHSQGLVHLDVKPANIFLGPRGRCKLGDFGLLVELGTAGAGEVQEGDPRYMAPELLQGSYGTAADVFSLGLTILEVACNMELPHGGEGWQQLRQGYLPPEFTAGLSSELRSVLVMMLEPDPKLRATAEALLALPVLRQP</t>
+  </si>
+  <si>
+    <t>aa_end</t>
+  </si>
+  <si>
+    <t>PMYT1_HUMAN_D0_3P1A_A</t>
+  </si>
+  <si>
+    <t>MK08_HUMAN_D0_2NO3_A</t>
+  </si>
+  <si>
+    <t>TCGGTTAAAGGAAGAATTTATTCCATATTAAAGCAGATAGGAAGTGGAGGTTCAAGCAAGGTATTTCAGGTGTTAAATGAAAAGAAACAGATATATGCTATAAAATATGTGAACTTAGAAGAAGCAGATAACCAAACTCTTGATAGTTACCGGAACGAAATAGCTTATTTGAATAAACTACAACAACACAGTGATAAGATCATCCGACTTTATGATTATGAAATCACGGACCAGTACATCTACATGGTAATGGAGTGTGGAAATATTGATCTTAATAGTTGGCTTAAAAAGAAAAAATCCATTGATCCATGGGAACGCAAGAGTTACTGGAAAAATATGTTAGAGGCAGTTCACACAATCCATCAACATGGCATTGTTCACAGTGATCTTAAACCAGCTAACTTTCTGATAGTTGATGGAATGCTAAAGCTAATTGATTTTGGGATTGCAAACCAAATGCAACCAGATACAACAAGTGTTGTTAAAGATTCTCAGGTTGGCACAGTTAATTATATGCCACCAGAAGCAATCAAAGATATGTCTTCCTCCAGAGAGAATGGGAAATCTAAGTCAAAGATAAGCCCCAAAAGTGATGTTTGGTCCTTAGGATGTATTTTGTACTATATGACTTACGGGAAAACACCATTTCAGCAGATAATTAATCAGATTTCTAAATTACATGCCATAATTGATCCTAATCATGAAATTGAATTTCCCGATATTCCAGAGAAAGATCTTCAAGATGTGTTAAAGTGTTGTTTAAAAAGGGACCCAAAACAGAGGATATCCATTCCTGAGCTCCTGGCTCATCCATATGTTCAAATTCAAACTCATCCAGTTAACCAAATGGCCAAGGGAACCACTGAAGAA</t>
+  </si>
+  <si>
+    <t>PAK1_HUMAN_D0_3Q52_A</t>
+  </si>
+  <si>
     <t>CACCACCATCACCACCATTCGCACTCGGGGCCGGAGATCTCGCGGATTATCGTCGACCCCACGACTGGGAAGCGCTACTGCCGGGGCAAAGTGCTGGGAAAGGGTGGCTTTGCAAAATGTTACGAGATGACAGATTTGACAAATAACAAAGTCTACGCCGCAAAAATTATTCCTCACAGCAGAGTAGCTAAACCTCATCAAAGGGAAAAGATTGACAAAGAAATAGAGCTTCACAGAATTCTTCATCATAAGCATGTAGTGCAGTTTTACCACTACTTCGAGGACAAAGAAAACATTTACATTCTCTTGGAATACTGCAGTAGAAGGTCAATGGCTCATATTTTGAAAGCAAGAAAGGTGTTGACAGAGCCAGAAGTTCGATACTACCTCAGGCAGATTGTGTCTGGACTGAAATACCTTCATGAACAAGAAATCTTGCACAGAGATCTCAAACTAGGGAACTTTTTTATTAATGAAGCCATGGAACTAAAAGTTGGGGACTTCGGTCTGGCAGCCAGGCTAGAACCCTTGGAACACAGAAGGAGAACGATATGTGGTACCCCAAATTATCTCTCTCCTGAAGTCCTCAACAAACAAGGACATGGCTGTGAATCAGACATTTGGGCCCTGGGCTGTGTAATGTATACAATGTTACTAGGGAGGCCCCCATTTGAAACTACAAATCTCAAAGAAACTTATAGGTGCATAAGGGAAGCAAGGTATACAATGCCGTCCTCATTGCTGGCTCCTGCCAAGCACTTAATTGCTAGTATGTTGTCCAAAAACCCAGAGGATCGTCCCAGTTTGGATGACATCATTCGACATGACTTTTTTTTGCAGGGCTTCACTCCGGACAGACTGTCTTCTAGCTGTTGTCATACAGTTCCAGATTTCCACTTATCAAGCCCAGCT</t>
   </si>
   <si>
-    <t>AAGCACGACGGGCGGGTGAAGATCGGACACTACGTGCTGGGCGACACGCTGGGCGTCGGCACCTTCGGCAAAGTGAAGATTGGAGAACATCAATTAACAGGCCATAAAGTGGCAGTTAAAATCTTAAATAGACAGAAGATTCGCAGTTTAGATGTTGTTGGAAAAATAAAACGAGAAATTCAAAATCTAAAACTCTTTCGTCATCCTCATATTATCAAACTATACCAGGTGATCAGCACTCCAACAGATTTTTTTATGGTAATGGAATATGTGTCTGGAGGTGAATTATTTGACTACATCTGTAAGCATGGACGGGTTGAAGAGATGGAAGCCAGGCGRCTCTTTCAGCAGATTCTGTCTGCTGTGGATTACTGTCATAGGCATATGGTTGTTCATCGAGACCTGAAACCAGAGAATGTCCTGTTGGATGCACACATGAATGCCAAGATAGCCGATTTCGGATTATCTAATATGATGTCAGATGGTGAATTTCTGAGAACTAGTTGCGGATCTCCAAATTATGCAGCACCTGAAGTCATCTCAGGCAGATTGTATGCAGGTCCTGAAGTTGATATCTGGAGCTGTGGTGTTATCTTGTATGCTCTTCTTTGTGGCACCCTCCCATTTGATGATGAGCATGTACCTACGTTATTTAAGAAGATCCGAGGGGGTGTCTTTTATATCCCAGAATATCTCAATCGTTCTGTCGCCACTCTCCTGATGCATATGCTGCAGGTTGACCCACTGAAACGAGCAACTATCAAAGACATAAGAGAGCATGAATGGTTTAAACAAGATTTGCCCAGTTACTTATTTCCTGAA</t>
-  </si>
-  <si>
-    <t>CSKP_HUMAN_D0_3TAC_A</t>
-  </si>
-  <si>
-    <t>MST4_HUMAN_D0_4FZD_B</t>
-  </si>
-  <si>
-    <t>CGGGACTCGAGTGATGATTGGGAGATTCCTGATGGGCAGATTACAGTGGGACAAAGAATTGGATCTGGATCATTTGGAACAGTCTACAAGGGAAAGTGGCATGGTGATGTGGCAGTGAAAATGTTGAATGTGACAGCACCTACACCTCAGCAGTTACAAGCCTTCAAAAATGAAGTAGGAGTACTCAGGAAAACACGACATGTGAATATCCTACTCTTCATGGGCTATTCCACAAAGCCACAACTGGCTATTGTTACCCAGTGGTGTGAGGGCTCCAGCTTGTATCACCATCTCCATATCATTGAGACCAAATTTGAGATGATCAAgCTTATAGATATTGCACGACAGACTGCACAGGGCATGGATTACTTACACGCCAAGTCAATCATCCACAGAGACCTCAAGAGTAATAATATATTTCTTCATGAAGACCTCACAGTAAAAATAGGTGATTTTGGTCTAGCTACAGTGAAATCTCGATGGAGTGGGTCCCATCAGTTTGAACAGTTGTCTGGgTCCATTTTGTGGATGGCACCAGAAGTCATCAGAATGCAAGATAAAAATCCATACAGCTTTCAGTCAGATGTATATGCATTTGGgATTGTTCTGTATGAATTGATGACTGGACAGTTACCTTATTCAAACATCAACAACAGGGACCAGATAATTTTTATGGTGGGACGAGGATACCTGTCTCCAGATCTCAGTAAGGTACGGAGTAACTGTCCAAAAGCCATGAAGAGATTAATGGCAGAGTGCCTCAAAAAGAAAAGAGATGAGAGACCACTCTTTCCCCAAATTCTCGCC</t>
-  </si>
-  <si>
-    <t>MARK2_HUMAN_D0_3IEC_D</t>
-  </si>
-  <si>
-    <t>CCATTTCCAGAAGGCAAGGTTCTGGATGATATGGAAGGCAATCAGTGGGTACTGGGCAAGAAGATTGGCTCTGGAGGATTTGGATTGATATATTTAGCTTTCCCCACAAATAAACCAGAGAAAGATGCAAGACATGTAGTAAAAGTGGAATATCAAGAAAATGGCCCGTTATTTTCAGAACTTAAATTTTATCAGAGAGTTGCAAAAAAAGACTGTATCAAAAAGTGGATAGAACGCAAACAACTTGATTATTTAGGAATTCCTCTGTTTTATGGATCTGGTCTGACTGAATTCAAGGGAAGAAGTTACAGATTTATGGTAATGGAAAGACTAGGAATAGATTTACAGAAGATCTCAGGCCAGAATGGTACCTTTAAAAAGTCAACTGTCCTGCAATTAGGTATCCGAATGTTGGATGTACTGGAATATATACATGAAAATGAATATGTTCATGGTGATATAAAAGCAGCAAATCTACTTTTGGGTTACAAAAATCCAGACCAGGTTTATCTTGCAGATTATGGACTTTCCTACAGATATTGTCCCAATGGGAACCACAAACAGTATCAGGAAAATCCTAGAAAAGGCCATAATGGGACAATAGAGTTTACCAGCTTGGATGCCCACAAGGGAGTAGCCTTGTCCAGACGAAGTGACGTTGAGATCCTCGGCTACTGCATGCTGCGGTGGTTGTGTGGGAAACTTCCCTGGGAACAGAACCTGAAGGACCCTGTGGCTGTGCAGACTGCTAAAACAAATCTGTTGGACGAGCTCCCCCAGTCAGTGCTTAAATGGGCTCCTTCTGGAAGCAGTTGCTGTGAAATAGCCCAATTTTTGGTATGTGCTCATAGTTTAGCATATGATGAAAAGCCAAACTATCAAGCCCTCAAGAAAATTTTGAACCCTCATGGAATACCTTTAGGACCACTGGACTTTTCCACAAAAGGACAGAGTATAAATGTCCAT</t>
-  </si>
-  <si>
-    <t>GGGGACTCTGATATATCCAGTCCATTACTGCAAAATACTGTCCACATTGACCTCAGTGCTCTAAATCCAGAGCTGGTCCAGGCAGTGCAGCATGTAGTGATTGGGCCCAGTAGCCTGATTGTGCATTTCAATGAAGTCATAGGAAGAGGGCATTTTGGTTGTGTATATCATGGGACTTTGTTGGACAATGATGGCAAGAAAATTCACTGTGCTGTGAAATCCTTGAACAGAATCACTGACATAGGAGAAGTTTCCCAATTTCTGACCGAGGGAATCATCATGAAAGATTTTAGTCATCCCAATGTCCTCTCGCTCCTGGGAATCTGCCTGCGAAGTGAAGGGTCTCCGCTGGTGGTCCTACCATACATGAAACATGGAGATCTTCGAAATTTCATTCGAAATGAGACTCATAATCCAACTGTAAAAGATCTTATTGGCTTTGGTCTTCAAGTAGCCAAAGGCATGAAATATCTTGCAAGCAAAAAGTTTGTCCACAGAGACTTGGCTGCAAGAAACTGTATGCTGGATGAAAAATTCACAGTCAAGGTTGCTGATTTTGGTCTTGCCAGAGACATGTATGATAAAGAATACTATAGTGTACACAACAAAACAGGTGCAAAGCTGCCAGTGAAGTGGATGGCTTTGGAAAGTCTGCAAACTCAAAAGTTTACCACCAAGTCAGATGTGTGGTCCTTTGGCGTGCTCCTCTGGGAGCTGATGACAAGAGGAGCCCCACCTTATCCTGACGTAAACACCTTTGATATAACTGTTTACTTGTTGCAAGGGAGAAGACTCCTACAACCCGAATACTGCCCAGACCCCTTATATGAAGTAATGCTAAAATGCTGGCACCCTAAAGCCGAAATGCGCCCATCCTTTTCTGAACTGGTGTCCCGGATATCAGCGATCTTCTCTACTTTCATTGGG</t>
-  </si>
-  <si>
-    <t>YQLFEELGKGAFSVVRRCVKVLAGQEYAAKIINTKKLSARDHQKLEREARICRLLKHPNIVRLHDSISEEGHHYLIFDLVTGGELFEDIVAREYYSEADASHCIQQILEAVLHCHQMGVVHRDLKPENLLLASKLKGAAVKLADFGLAIEVEGEQQAWFGFAGTPGYLSPEVLRKDPYGKPVDLWACGVILYILLVGYPPFWDEDQHRLYLQIKAGAYDFPSPEWDTVTPEAKDLINKMLTINPSKRITAAEALKHPWISHRSTVASCMHRQETVDCLKKFNARRKLKGA</t>
-  </si>
-  <si>
-    <t>ENFQKVEKIGEGTYGVVYKARNKLTGEVVALKKIRLDTETEGVPSTAIREISLLKELNHPNIVKLLDVIHTENKLYLVFEFLHQDLKKFMDASALTGIPLPLIKSYLFQLLQGLAFCHSHRVLHRDLKPQNLLINTEGAIKLADFGLARAFGVPVRTYTHEVVTLWYRAPEILLGCKYYSTAVDIWSLGCIFAEMVTRRALFPGDSEIDQLFRIFRTLGTPDEVVWPGVTSMPDYKPSFPKWARQDFSKVVPPLDEDGRSLLSQMLHYDPNKRISAKAALAHPFFQDVTKPVPHL</t>
-  </si>
-  <si>
-    <t>TTK_HUMAN_D0_3H9F_A</t>
-  </si>
-  <si>
-    <t>SVKGRIYSILKQIGSGGSSKVFQVLNEKKQIYAIKYVNLEEADNQTLDSYRNEIAYLNKLQQHSDKIIRLYDYEITDQYIYMVMECGNIDLNSWLKKKKSIDPWERKSYWKNMLEAVHTIHQHGIVHSDLKPANFLIVDGMLKLIDFGIANQMQPDTTSVVKDSQVGTVNYMPPEAIKDMSSSRENGKSKSKISPKSDVWSLGCILYYMTYGKTPFQQIINQISKLHAIIDPNHEIEFPDIPEKDLQDVLKCCLKRDPKQRISIPELLAHPYVQIQTHPVNQMAKGTTEE</t>
-  </si>
-  <si>
-    <t>GTGAAAGAATTCTTAGCCAAAGCCAAAGAAGATTTTCTTAAAAAATGGGAAAGTCCCGCTCAGAACACAGCCCACTTGGATCAGTTTGAACGAATCAAGACCCTCGGCACGGGCTCCTTCGGGCGGGTGATGCTGGTGAAACACAAGGAGACCGGGAACCACTATGCCATGAAGATCCTCGACAAACAGAAGGTGGTGAAACTGAAACAGATCGAACACACCCTGAATGAAAAGCGCATCCTGCAAGCTGTCAACTTTCCGTTCCTCGTCAAACTCGAGTTCTCCTTCAAGGACAACTCAAACTTATACATGGTCATGGAGTACGTGCCCGGCGGGGAGATGTTCTCACACCTACGGCGGATCGGAAGGTTCAGTGAGCCCCATGCCCGTTTCTACGCGGCCCAGATCGTCCTGACCTTTGAGTATCTGCACTCGCTGGATCTCATCTACAGGGACCTGAAGCCGGAGAATCTGCTCATTGACCAGCAGGGCTACATTCAGGTGACAGACTTCGGTTTCGCCAAGCGCGTGAAGGGCCGCACTTGGACCTTGTGCGGCACCCCTGAGTACCTGGCCCCTGAGATTATCCTGAGCAAAGGCTACAACAAGGCCGTGGACTGGTGGGCCCTGGGGGTTCTTATCTATGAAATGGCCGCTGGCTACCCGCCCTTCTTCGCAGACCAGCCCATCCAGATCTATGAGAAGATCGTCTCTGGGAAGGTGCGCTTCCCTTCCCACTTCAGCTCTGACTTGAAGGACCTGCTGCGGAACCTCCTGCAGGTAGATCTCACCAAGCGCTTTGGGAACCTCAAGAATGGGGTCAACGATATCAAGAACCACAAGTGGTTTGCCACAACTGACTGGATTGCCATCTACCAGAGGAAGGTGGAAGCTCCCTTCATACCAAAGTTTAAAGGCCCTGGGGATACGAGTAACTTTGACGACTATGAGGAAGAAGAAATCCGGGTCTCCATCAATGAGAAGTGTGGCAAGGAGTTTTCTGAGTTT</t>
-  </si>
-  <si>
-    <t>TCCCCCAACTACGACAAGTGGGAGATGGAACGCACGGACATCACCATGAAGCACAAGCTGGGCGGGGGCCAGTACGGGGAGGTGTACGAGGGCGTGTGGAAGAAATACAGCCTGACGGTGGCCGTGAAGACCTTGAAGGAGGACACCATGGAGGTGGAAGAGTTCTTGAAAGAAGCTGCAGTCATGAAAGAGATCAAACACCCTAACCTGGTGCAGCTCCTTGGGGTCTGCACCCGGGAGCCCCCGTTCTATATCATCACTGAGTTCATGACCTACGGGAACCTCCTGGACTACCTGAGGGAGTGCAACCGGCAGGAGGTGAACGCCGTGGTGCTGCTGTACATGGCCACTCAGATCTCGTCAGCCATGGAGTACCTGGAGAAGAAAAACTTCATCCACAGAGATCTTGCTGCCCGAAACTGCCTGGTAGGGGAGAACCACTTGGTGAAGGTAGCTGATTTTGGCCTGAGCAGGTTGATGACAGGGGACACCTACACAGCCCATGCTGGAGCCAAGTTCCCCATCAAATGGACTGCACCCGAGAGCCTGGCCTACAACAAGTTCTCCATCAAGTCCGACGTCTGGGCATTTGGAGTATTGCTTTGGGAAATTGCTACCTATGGCATGTCCCCTTACCCGGGAATTGACCTGTCCCAGGTGTATGAGCTGCTAGAGAAGGACTACCGCATGGAGCGCCCAGAAGGCTGCCCAGAGAAGGTCTATGAACTCATGCGAGCATGTTGGCAGTGGAATCCCTCTGACCGGCCCTCCTTTGCTGAAATCCACCAAGCCTTTGAAACAATGTTCCAGGAATCCAGTATCTCAGACGAAGTGGAAAAGGAGCTGGGGAAA</t>
-  </si>
-  <si>
-    <t>RDSSDDWEIPDGQITVGQRIGSGSFGTVYKGKWHGDVAVKMLNVTAPTPQQLQAFKNEVGVLRKTRHVNILLFMGYSTKPQLAIVTQWCEGSSLYHHLHIIETKFEMIKLIDIARQTAQGMDYLHAKSIIHRDLKSNNIFLHEDLTVKIGDFGLATVKSRWSGSHQFEQLSGSILWMAPEVIRMQDKNPYSFQSDVYAFGIVLYELMTGQLPYSNINNRDQIIFMVGRGYLSPDLSKVRSNCPKAMKRLMAECLKKKRDERPLFPQILA</t>
-  </si>
-  <si>
-    <t>KS6A1_HUMAN_D1_3RNY_B</t>
+    <t>GAAACAAAGTATACTGTGGACAAGAGGTTTGGCATGGATTTTAAAGAAATAGAATTAATTGGCTCAGGTGGATTTGGCCAAGTTTTCAAAGCAAAACACAGAATTGACGGAAAGACTTACGTTATTAAACGTGTTAAATATAATAACGAGAAGGCGGAGCGTGAAGTAAAAGCATTGGCAAAACTTGATCATGTAAATATTGTTCACTACAATGGCTGTTGGGATGGATTTGATTATGATCCTGAGACCAGTGATGATTCTCTTGAGAGCAGTGATTATGATCCTGAGAACAGCAAAAATAGTTCAAGGTCAAAGACTAAGTGCCTTTTCATCCAAATGGAATTCTGTGATAAAGGGACCTTGGAACAATGGATTGAAAAAAGAAGAGGCGAGAAACTAGACAAAGTTTTGGCTTTGGAACTCTTTGAACAAATAACAAAAGGGGTGGATTATATACATTCAAAAAAATTAATTCATAGAGATCTTAAGCCAAGTAATATATTCTTAGTAGATACAAAACAAGTAAAGATTGGAGACTTTGGACTTGTAACATCTCTGAAAAATGATGGAAAGCGAACAAGGAGTAAGGGAACTTTGCGATACATGAGCCCAGAACAGATTTCTTCGCAAGACTATGGAAAGGAAGTGGACCTCTACGCTTTGGGGCTAATTCTTGCTGAACTTCTTCATGTATGTGACACTGCTTTTGAAACATCAAAGTTTTTCACAGACCTACGGGATGGCATCATCTCAGATATATTTGATAAAAAAGAAAAAACTCTTCTACAGAAATTACTCTCAAAGAAACCTGAGGATCGACCTAACACATCTGAAATACTAAGGACCTTGACTGTGTGGAAGAAAAGCCCAGAGAAAAATGAACGACACACATGT</t>
+  </si>
+  <si>
+    <t>PAK7_HUMAN_D0_2F57_B</t>
+  </si>
+  <si>
+    <t>expression tag location</t>
+  </si>
+  <si>
+    <t>GAGAACTTCCAAAAGGTGGAAAAGATCGGAGAGGGCACGTACGGAGTTGTGTACAAAGCCAGAAACAAGTTGACGGGAGAGGTGGTGGCGCTTAAGAAAATCCGCCTGGACACTGAGACTGAGGGTGTGCCCAGTACTGCCATCCGAGAGATCTCTCTGCTTAAGGAGCTTAACCATCCTAATATTGTCAAGCTGCTGGATGTCATTCACACAGAAAATAAACTCTACCTGGTTTTTGAATTTCTGCACCAAGATCTCAAGAAATTCATGGATGCCTCTGCTCTCACTGGCATTCCTCTTCCCCTCATCAAGAGCTATCTGTTCCAGCTGCTCCAGGGCCTAGCTTTCTGCCATTCTCATCGGGTCCTCCACCGAGACCTTAAACCTCAGAATCTGCTTATTAACACAGAGGGGGCCATCAAGCTAGCAGACTTTGGACTAGCCAGAGCTTTTGGAGTCCCTGTTCGTACTTACACCCATGAGGTGGTGACCCTGTGGTACCGAGCTCCTGAAATCCTCCTGGGCTGCAAATATTATTCCACAGCTGTGGACATCTGGAGCCTGGGCTGCATCTTTGCTGAGATGGTGACTCGCCGGGCCCTATTCCCTGGAGATTCTGAGATTGACCAGCTCTTCCGGATCTTTCGGACTCTGGGGACCCCAGATGAGGTGGTGTGGCCAGGAGTTACTTCTATGCCTGATTACAAGCCAAGTTTCCCCAAGTGGGCCCGGCAAGATTTTAGTAAAGTTGTACCTCCCCTGGATGAAGATGGACGGAGCTTGTTATCGCAAATGCTGCACTACGACCCTAACAAGCGGATTTCGGCCAAGGCAGCCCTGGCTCACCCTTTCTTCCAGGATGTGACCAAGCCAGTACCCCATCTT</t>
+  </si>
+  <si>
+    <t>GGGGAATGCAGTCAGAAGGGTCCTGTCCCCTTTAGCCATTGCCTTCCCACAGAAAAACTGCAACGCTGTGAGAAGATTGGGGAAGGGGTGTTTGGCGAAGTGTTTCAAACAATTGCTGATCACACACCCGTAGCCATAAAAATCATTGCTATTGAAGGACCAGATTTAGTCAATGGATCCCATCAGAAAACCTTTGAGGAAATCCTGCCAGAGATCATCATCTCCAAAGAGTTGAGCCTCTTATCCGGTGAAGTGTGCAACCGCACAGAAGGCTTTATCGGGCTGAACTCAGTGCACTGTGTCCAGGGATCTTACCCTCCCTTGCTCCTCAAAGCCTGGGATCACTATAATTCAACCAAAGGCTCTGCAAATGACCGGCCTGATTTTTTTAAAGACGACCAGCTCTTCATTGTGCTGGAATTTGAGTTTGGAGGGATTGACTTAGAGCAAATGCGAACCAAGTTGTCTTCCTTGGCTACTGCAAAGAGCATTCTACACCAGCTCACAGCCTCCCTCGCAGTGGCAGAGGCATCACTGCGCTTTGAGCACCGAGACTTACACTGGGGGAACGTGCTCTTAAAGAAAACCAGCCTCAAAAAACTCCACTACACCCTCAATGGGAAGAGCAGCACTATCCCCAGCTGTGGGTTGCAAGTGAGCATCATTGACTACACCCTGTCGCGCTTGGAACGGGATGGGATTGTGGTTTTCTGTGACGTTTCCATGGATGAGGACCTGTTTACCGGTGACGGTGACTACCAGTTTGACATCTACAGGCTCATGAAGAAGGAGAATAACAACCGCTGGGGTGAATATCACCCTTATAGTAATGTGCTCTGGTTACATTACCTGACAGACAAGATGCTGAAACAAATGACCTTCAAGACTAAATGTAACACTCCTGCCATGAAGCAAATTAAGAGAAAAATCCAGGAGTTCCACAGGACAATGCTGAACTTCAGCTCTGCCACTGACTTGCTCTGCCAGCACAGACTGTTTAAG</t>
+  </si>
+  <si>
+    <t>TDSLPGKFEDMYKLTSELLGEGAYAKVQGAVSLQNGKEYAVKIIEKQAGHSRSRVFREVETLYQCQGNKNILELIEFFEDDTRFYLVFEKLQGGSILAHIQKQKHFNEREASRVVRDVAAALDFLHTKDKVSLCHLGGSARAPSGLTAAPTSLGSSDPPTSASQVAGTTGIDHRDLKPENILCESPEKVSPVKICDFDLGSGMKLNNSCTPITTPELTTPCGSAEYMAPEVGEVFTDQATFYDKRCDLWSLGVVLYIMLSGYPPFVGHCGADCGWDRGEVCRVCQNKLFESIQEGKYEFPDKDWAHISSEAKDLISKLLVRDAKQRLSAAQVLQHPWVQGQAPEKG</t>
+  </si>
+  <si>
+    <t>DAPK1_HUMAN_D0_4B4L_A</t>
+  </si>
+  <si>
+    <t>VIDPSELTFVQEIGSGQFGLVHLGYWLNKDKVAIKTIREGAMSEEDFIEEAEVMMKLSHPKLVQLYGVCLEQAPICLVFEFMEHGCLSDYLRTQRGLFAAETLLGMCLDVCEGMAYLEEACVIHRDLAARNCLVGENQVIKVSDFGMTRFVLDDQYTSSTGTKFPVKWASPEVFSFSRYSSKSDVWSFGVLMWEVFSEGKIPYENRSNSEVVEDISTGFRLYKPRLASTHVYQIMNHCWKERPEDRPAFSRLLRQLAEIAESGL</t>
+  </si>
+  <si>
+    <t>ATGAGCCTCATCCGGAAAAAGGGCTTCTACAAGCAGGACGTCAACAAGACCGCCTGGGAGCTGCCCAAGACCTACGTGTCCCCGACGCACGTCGGCAGCGGGGCCTATGGCTCCGTGTGCTCGGCCATCGACAAGCGGTCAGGGGAGAAGGTGGCCATCAAGAAGCTGAGCCGACCCTTTCAGTCCGAGATCTTCGCCAAGCGCGCCTACCGGGAGCTGCTGCTGCTGAAGCACATGCAGCATGAGAACGTCATTGGGCTCCTGGATGTCTTCACCCCAGCCTCCTCCCTGCGCAACTTCTATGACTTCTACCTGGTGATGCCCTTCATGCAGACGGATCTGCAGAAGATCATGGGGATGGAGTTCAGTGAGGAGAAGATCCAGTACCTGGTGTATCAGATGCTCAAAGGCCTTAAGTACATCCACTCTGCTGGGGTCGTGCACAGGGACCTGAAGCCAGGCAACCTGGCTGTGAATGAGGACTGTGAACTGAAGATTCTGGATTTTGGGCTGGCGCGACATGCAGACGCCGAGATGACTGGCTACGTGGTGACCCGCTGGTACCGAGCCCCCGAGGTGATCCTCAGCTGGATGCACTACAACCAGACAGTGGACATCTGGTCTGTGGTCTGTATCATGGCAGAGATGCTGACAGGGAAAACTCTGTTCAAGGGGAAAGATTACCTGGACCAGCTGACCCAGATCCTGAAAGTGACCGGGGTGCCTGGCACGGAGTTTGTGCAGAAGCTGAACGACAAAGCGGCCAAATCCTACATCCAGTCCCTGCCACAGACCCCCAGGAAGGATTTCACTCAGCTGTTCCCACGGGCCAGCCCCCAGGCTGCGGACCTGCTGGAGAAGATGCTGGAGCTAGACGTGGACAAGCGCCTGACGGCCGCGCAGGCCCTCACCCATCCCTTCTTTGAACCCTTCCGGGACCCTGAGGAAGAGACGGAGGCCCAGCAGCCGTTTGATGATTCCTTAGAACACGAGAAACTCACAGTGGATGAATGGAAGCAGCACATCTACAAGGAGATTGTGAACTTCAGCCCCATT</t>
+  </si>
+  <si>
+    <t>ATGAAAGATTATGATGAACTTCTCAAATATTATGAATTACATGAAACTATTGGGACAGGTGGCTTTGCAAAGGTCAAACTTGCCTGCCATATCCTTACTGGAGAGATGGTAGCTATAAAAATCATGGATAAAAACACACTAGGGAGTGATTTGCCCCGGATCAAAACGGAGATTGAGGCCTTGAAGAACCTGAGACATCAGCATATATGTCAACTCTACCATGTGCTAGAGACAGCCAACAAAATATTCATGGTTCTTGAGTACTGCCCTGGAGGAGAGCTGTTTGACTATATAATTTCCCAGGATCGCCTGTCAGAAGAGGAGACCCGGGTTGTCTTCCGTCAGATAGTATCTGCTGTTGCTTATGTGCACAGCCAGGGCTATGCTCACAGGGACCTCAAGCCAGAAAATTTGCTGTTTGATGAATATCATAAATTAAAGCTGATTGACTTTGGTCTCTGTGCAAAACCCAAGGGTAACAAGGATTACCATCTACAGACATGCTGTGGGAGTCTGGCTTATGCAGCACCTGAGTTAATACAAGGCAAATCATATCTTGGATCAGAGGCAGATGTTTGGAGCATGGGCATACTGTTATATGTTCTTATGTGTGGATTTCTACCATTTGATGATGATAATGTAATGGCTTTATACAAGAAGATTATGAGAGGAAAATATGATGTTCCCAAGTGGCTCTCTCCCAGTAGCATTCTGCTTCTTCAACAAATGCTGCAGGTGGACCCAAAGAAACGGATTTCTATGAAAAATCTATTGAACCATCCCTGGATCATGCAAGATTACAACTATCCTGTTGAGTGGCAAAGCAAGAATCCTTTTATTCACCTCGATGATGATTGCGTAACAGAACTTTCTGTACATCACAGAAACAACAGGCAAACAATGGAGGATTTAATTTCACTGTGGCAGTATGATCACCTCACGGCTACCTATCTTCTGCTTCTAGCCAAGAAGGCTCGGGGAAAACCAGTTCGTTTAAGGCTTTCTTCTTTCTCCTGTGGA</t>
+  </si>
+  <si>
+    <t>PAK4_HUMAN_D0_2J0I_A</t>
+  </si>
+  <si>
+    <t>AGVSEYELPEDPRWELPRDRLVLGKPLGEGCFGQVVLAEAIGLDKDKPNRVTKVAVKMLKSDATEKDLSDLISEMEMMKMIGKHKNIINLLGACTQDGPLYVIVEYASKGNLREYLQARRPPGLEYCYNPSHNPEEQLSSKDLVSCAYQVARGMEYLASKKCIHRDLAARNVLVTEDNVMKIADFGLARDIHHIDYYKKTTNGRLPVKWMAPEALFDRIYTHQSDVWSFGVLLWEIFTLGGSPYPGVPVEELFKLLKEGHRMDKPSNCTNELYMMMRDCWHAVPSQRPTFKQLVEDLDRIVALTSNQEYLDLSMPLD</t>
+  </si>
+  <si>
+    <t>GAGCCCAAGAAGTACGCAGTGACCGACGACTACCAGTTGTCCAAGCAGGTGCTGGGCCTGGGTGTGAACGGCAAAGTGCTGGAGTGCTTCCATCGGCGCACTGGACAGAAGTGTGCCCTGAAGCTCCTGTATGACAGCCCCAAGGCCCGGCAGGAGGTAGACCATCACTGGCAGGCTTCTGGCGGCCCCCATATTGTCTGCATCCTGGATGTGTATGAGAACATGCACCATGGCAAGCGCTGTCTCCTCATCATCATGGAATGCATGGAAGGTGGTGAGTTGTTCAGCAGGATTCAGGAGCGTGGCGACCAGGCTTTCACTGAGAGAGAAGCTGCAGAGATAATGCGGGATATTGGCACTGCCATCCAGTTTCTGCACAGCCATAACATTGCCCACCGAGATGTCAAGCCTGAAAACCTACTCTACACATCTAAGGAGAAAGACGCAGTGCTTAAGCTCACCGATTTTGGCTTTGCTAAGGAGACCACCCAAAATGCCCTGCAGACACCCTGCTATACTCCCTATTATGTGGCCCCTGAGGTCCTGGGTCCAGAGAAGTATGACAAGTCATGTGACATGTGGTCCCTGGGTGTCATCATGTACATCCTCCTTTGTGGCTTCCCACCCTTCTACTCCAACACGGGCCAGGCCATCTCCCCGGGGATGAAGAGGAGGATTCGCCTGGGCCAGTACGGCTTCCCCAATCCTGAGTGGTCAGAAGTCTCTGAGGATGCCAAGCAGCTGATCCGCCTCCTGTTGAAGACAGACCCCACAGAGAGGCTGACCATCACTCAGTTCATGAACCACCCCTGGATCAACCAATCGATGGTAGTGCCACAGACCCCACTCCACACGGCCCGAGTGCTGCAGGAGGACAAAGACCACTGGGACGAAGTCAAGGAGGAGATGACCAGTGCCTTGGCCACTATGCGGGTAGACTACGACCAGGTG</t>
+  </si>
+  <si>
+    <t>ATGTCTCAGGAGAGGCCCACGTTCTACCGGCAGGAGCTGAACAAGACAATCTGGGAGGTGCCCGAGCGTTACCAGAACCTGTCTCCAGTGGGCTCTGGCGCCTATGGCTCTGTGTGTGCTGCTTTTGACACAAAAACGGGGTTACGTGTGGCAGTGAAGAAGCTCTCCAGACCATTTCAGTCCATCATTCATGCGAAAAGAACCTACAGAGAACTGCGGTTACTTAAACATATGAAACATGAAAATGTGATTGGTCTGTTGGACGTTTTTACACCTGCAAGGTCTCTGGAGGAATTCAATGATGTGTATCTGGTGACCCATCTCATGGGGGCAGATCTGAACAACATTGTGAAATGTCAGAAGCTTACAGATGACCATGTTCAGTTCCTTATCTACCAAATTCTCCGAGGTCTAAAGTATATACATTCAGCTGACATAATTCACAGGGACCTAAAACCTAGTAATCTAGCTGTGAATGAAGACTGTGAGCTGAAGATTCTGGATTTTGGACTGGCTCGGCACACAGATGATGAAATGACAGGCTACGTGGCCACTAGGTGGTACAGGGCTCCTGAGATCATGCTGAACTGGATGCATTACAACCAGACAGTTGATATTTGGTCAGTGGGATGCATAATGGCCGAGCTGTTGACTGGAAGAACATTGTTTCCTGGTACAGACCATATTGATCAGTTGAAGCTCATTTTAAGACTCGTTGGAACCCCAGGGGCTGAGCTTTTGAAGAAAATCTCCTCAGAGTCTGCAAGAAACTATATTCAGTCTTTGACTCAGATGCCGAAGATGAACTTTGCGAATGTATTTATTGGTGCCAATCCCCTGGCTGTCGACTTGCTGGAGAAGATGCTTGTATTGGACTCAGATAAGAGAATTACAGCGGCCCAAGCCCTTGCACATGCCTACTTTGCTCAGTACCACGATCCTGATGATGAACCAGTGGCCGATCCTTATGATCAGTCCTTTGAAAGCAGGGACCTCCTTATAGATGAGTGGAAAAGCCTGACCTATGATGAAGTCATCAGCTTTGTGCCACCACCCCTTGACCAAGAAGAGATGGAGTCC</t>
+  </si>
+  <si>
+    <t>MK11_HUMAN_D0_3GC8_A</t>
+  </si>
+  <si>
+    <t>VRK3_HUMAN_D0_2JII_A</t>
+  </si>
+  <si>
+    <t>MK14_HUMAN_D0_3K3J_A</t>
+  </si>
+  <si>
+    <t>CDK16_HUMAN_D0_3MTL_A</t>
+  </si>
+  <si>
+    <t>BRAF_HUMAN_D0_4JVG_D</t>
+  </si>
+  <si>
+    <t>NEK7_HUMAN_D0_2WQN_A</t>
+  </si>
+  <si>
+    <t>PAK6_HUMAN_D0_2C30_A</t>
+  </si>
+  <si>
+    <t>FGFR1_HUMAN_D0_3GQL_B</t>
+  </si>
+  <si>
+    <t>TCTTCGGTCACCGCCAGTGCGGCCCCGGGGACCGCGAGCCTCGTCCCGGATTACTGGATCGACGGCTCCAACAGGGATGCGCTGAGCGATTTCTTCGAGGTGGAGTCGGAGCTGGGACGGGGTGCTACATCCATTGTGTACAGATGCAAACAGAAGGGGACCCAGAAGCCTTATGCTCTCAAAGTGTTAAAGAAAACAGTGGACAAAAAAATCGTAAGAACTGAGATAGGAGTTCTTCTTCGCCTCTCACATCCAAACATTATAAAACTTAAAGAGATATTTGAAACCCCTACAGAAATCAGTCTGGTCCTAGAACTCGTCACAGGAGGAGAACTGTTTGATAGGATTGTGGAAAAGGGATATTACAGTGAGCGAGATGCTGCAGATGCCGTTAAACAAATCCTGGAGGCAGTTGCTTATCTACATGAAAATGGGATTGTCCATCGTGATCTCAAACCAGAGAATCTTCTTTATGCAACTCCAGCCCCAGATGCACCACTCAAAATCGCTGATTTTGGACTCTCTAAAATTGTGGAACATCAAGTGCTCATGAAGACAGTATGTGGAACCCCAGGGTACTGCGCACCTGAAATTCTTAGAGGTTGTGCCTATGGACCTGAGGTGGACATGTGGTCTGTAGGAATAATCACCTACATCTTACTTTGTGGATTTGAACCATTCTATGATGAAAGAGGCGATCAGTTCATGTTCAGGAGAATTCTGAATTGTGAATATTACTTTATCTCCCCCTGGTGGGATGAAGTATCTCTAAATGCCAAGGACTTGGTCAGAAAATTAATTGTTTTGGATCCAAAGAAACGGCTGACTACATTTCAAGCTCTCCAGCATCCGTGGGTCACAGGTAAAGCAGCCAATTTTGTACACATGGATACCGCTCAAAAGAAGCTCCAAGAATTCAATGCCCGGCGTAAGCTTAAGGCAGCGGTGAAGGCTGTGGTGGCCTCTTCCCGCCTGGGA</t>
+  </si>
+  <si>
+    <t>MEAAASEPSLDLDNLKLLELIGRGRYGAVYKGSLDERPVAVKVFSFANRQNFINEKNIYRVPLMEHDNIARFIVGDERVTADGRMEYLLVMEYYPNGSLCKYLSLHTSDWVSSCRLAHSVTRGLAYLHTELPRGDHYKPAISHRDLNSRNVLVKNDGTCVISDFGLSMRLTGNRLVRPGEEDNAAISEVGTIRYMAPEVLEGAVNLRDCESALKQVDMYALGLIYWEIFMRCTDLFPGESVPEYQMAFQTEVGNHPTFEDMQVLVSREKQRPKFPEAWKENSLAVRSLKETIEDCWDQDAEARLTAQCAEERMAELMMIWERNKSVSPT</t>
+  </si>
+  <si>
+    <t>GTCATCATTGACAATAAGCGCTACCTCTTCATCCAGAAACTGGGGGAGGGTGGGTTCAGCTATGTGGACCTAGTGGAAGGGTTACATGATGGACACTTCTACGCCCTGAAGCGAATCCTGTGTCACGAGCAGCAGGACCGGGAGGAGGCCCAGCGAGAAGCCGACATGCATCGCCTCTTCAATCACCCCAACATCCTTCGCCTCGTGGCTTACTGTCTGAGGGAACGGGGTGCTAAGCATGAGGCCTGGCTGCTGCTACCATTCTTCAAGAGAGGTACGCTGTGGAATGAGATAGAAAGGCTGAAGGACAAAGGCAACTTCCTGACCGAGGATCAAATCCTTTGGCTGCTGCTGGGGATCTGCAGAGGCCTTGAGGCCATTCATGCCAAGGGTTATGCCCACAGAGACTTGAAGCCCACCAATATATTGCTTGGAGATGAGGGGCAGCCAGTTTTAATGGACTTGGGTTCCATGAATCAAGCATGCATCCATGTGGAGGGCTCCCGCCAGGCTCTGACCCTGCAGGACTGGGCAGCCCAGCGGTGCACCATCTCCTACCGAGCCCCAGAGCTCTTCTCTGTGCAGAGTCACTGTGTCATCGATGAGCGGACTGATGTCTGGTCCCTAGGCTGCGTGCTATATGCCATGATGTTTGGGGAAGGCCCTTATGACATGGTGTTCCAAAAGGGTGACAGTGTGGCCCTTGCTGTGCAGAACCAACTCAGCATCCCACAAAGCCCCAGGCATTCTTCAGCATTGTGGCAGCTCCTGAACTCGATGATGACCGTGGACCCGCATCAGCGTCCTCACATTCCTCTCCTCCTCAGTCAGCTGGAGGCGCTGCAG</t>
+  </si>
+  <si>
+    <t>BMPR2_HUMAN_D0_3G2F_A</t>
+  </si>
+  <si>
+    <t>dna_start</t>
+  </si>
+  <si>
+    <t>PHKG2_HUMAN_D0_2Y7J_D</t>
+  </si>
+  <si>
+    <t>MAPK2_HUMAN_D0_2JBO_A</t>
+  </si>
+  <si>
+    <t>HHHHHHSHSGPEISRIIVDPTTGKRYCRGKVLGKGGFAKCYEMTDLTNNKVYAAKIIPHSRVAKPHQREKIDKEIELHRILHHKHVVQFYHYFEDKENIYILLEYCSRRSMAHILKARKVLTEPEVRYYLRQIVSGLKYLHEQEILHRDLKLGNFFINEAMELKVGDFGLAARLEPLEHRRRTICGTPNYLSPEVLNKQGHGCESDIWALGCVMYTMLLGRPPFETTNLKETYRCIREARYTMPSSLLAPAKHLIASMLSKNPEDRPSLDDIIRHDFFLQGFTPDRLSSSCCHTVPDFHLSSPA</t>
+  </si>
+  <si>
+    <t>ATGGAGAAGGACGGCCTGTGCCGCGCTGACCAGCAGTACGAATGCGTGGCGGAGATCGGGGAGGGCGCCTATGGGAAGGTGTTCAAGGCCCGCGACTTGAAGAACGGAGGCCGTTTCGTGGCGTTGAAGCGCGTGCGGGTGCAGACCGGCGAGGAGGGCATGCCGCTCTCCACCATCCGCGAGGTGGCGGTGCTGAGGCACCTGGAGACCTTCGAGCACCCCAACGTGGTCAGGTTGTTTGATGTGTGCACAGTGTCACGAACAGACAGAGAAACCAAACTAACTTTAGTGTTTGAACATGTCGATCAAGACTTGACCACTTACTTGGATAAAGTTCCAGAGCCTGGAGTGCCCACTGAAACCATAAAGGATATGATGTTTCAGCTTCTCCGAGGTCTGGACTTTCTTCATTCACACCGAGTAGTGCATCGCGATCTAAAACCACAGAACATTCTGGTGACCAGCAGCGGACAAATAAAACTCGCTGACTTCGGCCTTGCCCGCATCTATAGTTTCCAGATGGCTCTAACCTCAGTGGTCGTCACGCTGTGGTACAGAGCACCCGAAGTCTTGCTCCAGTCCAGCTACGCCACCCCCGTGGATCTCTGGAGTGTTGGCTGCATATTTGCAGAAATGTTTCGTAGAAAGCCTCTTTTTCGTGGAAGTTCAGATGTTGATCAACTAGGAAAAATCTTGGACGTGATTGGACTCCCAGGAGAAGAAGACTGGCCTAGAGATGTTGCCCTTCCCAGGCAGGCTTTTCATTCAAAATCTGCCCAACCAATTGAGAAGTTTGTAACAGATATCGATGAACTAGGCAAAGACCTACTTCTGAAGTGTTTGACATTTAACCCAGCCAAAAGAATATCTGCCTACAGTGCCCTGTCTCACCCATACTTCCAG</t>
+  </si>
+  <si>
+    <t>ATGTCGGGCCCTCGCGCCGGCTTCTACCGGCAGGAGCTGAACAAGACCGTGTGGGAGGTGCCGCAGCGGCTGCAGGGGCTGCGCCCGGTGGGCTCCGGCGCCTACGGCTCCGTCTGTTCGGCCTACGACGCCCGGCTGCGCCAGAAGGTGGCGGTGAAGAAGCTGTCGCGCCCCTTCCAGTCGCTGATCCACGCGCGCAGAACGTACCGGGAGCTGCGGCTGCTCAAGCACCTGAAGCACGAGAACGTCATCGGGCTTCTGGACGTCTTCACGCCGGCCACGTCCATCGAGGACTTCAGCGAAGTGTACTTGGTGACCACCCTGATGGGCGCCGACCTGAACAACATCGTCAAGTGCCAGGCGCTGAGCGACGAGCACGTTCAATTCCTGGTTTACCAGCTGCTGCGCGGGCTGAAGTACATCCACTCGGCCGGGATCATCCACCGGGACCTGAAGCCCAGCAACGTGGCTGTGAACGAGGACTGTGAGCTCAGGATCCTGGATTTCGGGCTGGCGCGCCAGGCGGACGAGGAGATGACCGGCTATGTGGCCACGCGCTGGTACCGGGCACCTGAGATCATGCTCAACTGGATGCATTACAACCAAACAGTGGATATCTGGTCCGTGGGCTGCATCATGGCTGAGCTGCTCCAGGGCAAGGCCCTCTTCCCGGGAAGCGACTACATTGACCAGCTGAAGCGCATCATGGAAGTGGTGGGCACACCCAGCCCTGAGGTTCTGGCAAAAATCTCCTCGGAACACGCCCGGACATATATCCAGTCCCTGCCCCCCATGCCCCAGAAGGACCTGAGCAGCATCTTCCGTGGAGCCAACCCCCTGGCCATAGACCTCCTTGGAAGGATGCTGGTGCTGGACAGTGACCAGAGGGTCAGTGCAGCTGAGGCACTGGCCCACGCCTACTTCAGCCAGTACCACGACCCCGAGGATGAGCCAGAGGCCGAGCCATATGATGAGAGCGTTGAGGCCAAGGAGCGCACGCTGGAGGAGTGGAAGGAGCTCACTTACCAGGAAGTCCTCAGCTTCAAGCCCCCAGAGCCACCGAAGCCACCTGGCAGCCTGGAGATTGAGCAG</t>
+  </si>
+  <si>
+    <t>E2AK2_HUMAN_D0_3UIU_A</t>
+  </si>
+  <si>
+    <t>MEKYEKIGKIGEGSYGVVFKCRNRDTGQIVAIKKFLESEDDPVIKKIALREIRMLKQLKHPNLVNLLEVFRRKRRLHLVFEYCDHTVLHELDRYQRGVPEHLVKSITWQTLQAVNFCHKHNCIHRDVKPENILITKHSVIKLCDFGFARLLTGPSDYYTDYVATRWYRSPELLVGDTQYGPPVDVWAIGCVFAELLSGVPLWPGKSDVDQLYLIRKTLGDLIPRHQQVFSTNQYFSGVKIPDPEDMEPLELKFPNISYPALGLL</t>
+  </si>
+  <si>
+    <t>GeneID</t>
+  </si>
+  <si>
+    <t>ATGGATGAGCAATCACAAGGAATGCAAGGGCCACCTGTTCCTCAGTTCCAACCACAGAAGGCCTTACGACCGGATATGGGCTATAATACATTAGCCAACTTTCGAATAGAAAAGAAAATTGGTCGCGGACAATTTAGTGAAGTTTATAGAGCAGCCTGTCTCTTGGATGGAGTACCAGTAGCTTTAAAAAAAGTGCAGATATTTGATTTAATGGATGCCAAAGCACGTGCTGATTGCATCAAAGAAATAGATCTTCTTAAGCAACTCAACCATCCAAATGTAATAAAATATTATGCATCATTCATTGAAGATAATGAACTAAACATAGTTTTGGAACTAGCAGATGCTGGCGACCTATCCAGAATGATCAAGCATTTTAAGAAGCAAAAGAGGCTAATTCCTGAAAGAACTGTTTGGAAGTATTTTGTTCAGCTTTGCAGTGCATTGGAACACATGCATTCTCGAAGAGTCATGCATAGAGATATAAAACCAGCTAATGTGTTCATTACAGCCACTGGGGTGGTAAAACTTGGAGATCTTGGGCTTGGCCGGTTTTTCAGCTCAAAAACCACAGCTGCACATTCTTTAGTTGGTACGCCTTATTACATGTCTCCAGAGAGAATACATGAAAATGGATACAACTTCAAATCTGACATCTGGTCTCTTGGCTGTCTACTATATGAGATGGCTGCATTACAAAGTCCTTTCTATGGTGACAAAATGAATTTATACTCACTGTGTAAGAAGATAGAACAGTGTGACTACCCACCTCTTCCTTCAGATCACTATTCAGAAGAACTCCGACAGTTAGTTAATATGTGCATCAACCCAGATCCAGAGAAGCGACCAGACGTCACCTATGTTTATGACGTAGCAAAGAGGATGCATGCATGCACTGCAAGCAGC</t>
+  </si>
+  <si>
+    <t>DAPK3_HUMAN_D0_2J90_A</t>
+  </si>
+  <si>
+    <t>GAAGACAGTTTGACTAAGCAGCCTGAAGAAGTTTTTGATGTATTAGAGAAGCTTGGAGAAGGGTCTTATGGAAGTGTATTTAAAGCAATACACAAGGAATCCGGTCAAGTTGTCGCAATTAAACAAGTACCTGTTGAATCAGATCTTCAGGAAATAATCAAAGAAATTTCCATAATGCAGCAATGTGACAGCCCATATGTTGTAAAGTACTATGGCAGTTATTTTAAGAATACAGACCTCTGGATTGTTATGGAGTACTGTGGCGCTGGCTCTGTCTCAGACATAATTAGATTACGAAACAAGACATTAATAGAAGATGAAATTGCAACCATTCTTAAATCTACATTGAAAGGACTAGAATATTTGCACTTTATGAGAAAAATACACAGAGATATAAAAGCTGGAAATATTCTCCTCAATACAGAAGGACATGCAAAATTGGCAGATTTTGGAGTGGCTGGTCAGTTAACAGATACAATGGCAAAACGCAATACTGTAATAGGAACTCCATTTTGGATGGCTCCTGAGGTGATTCAAGAAATAGGCTATAACTGTGTGGCCGACATCTGGTCCCTTGGCATTACTTCTATAGAAATGGCTGAAGGAAAACCTCCTTATGCTGATATACATCCAATGAGGGCTATTTTTATGATTCCCACAAATCCACCACCAACATTCAGAAAGCCAGAACTTTGGTCCGATGATTTCACCGATTTTGTTAAAAAGTGTTTGGTGAAGAATCCTGAGCAGAGAGCTACTGCAACACAACTTTTACAGCATCCTTTTATCAAGAATGCCAAACCTGTATCAATATTAAGAGACCTGATCACAGAAGCTATGGAGATCAAAGCTAAAAGACATGAGGAACAGCAACGAGAATTGGAAGAGGAAGAA</t>
+  </si>
+  <si>
+    <t>VKEFLAKAKEDFLKKWESPAQNTAHLDQFERIKTLGTGSFGRVMLVKHKETGNHYAMKILDKQKVVKLKQIEHTLNEKRILQAVNFPFLVKLEFSFKDNSNLYMVMEYVPGGEMFSHLRRIGRFSEPHARFYAAQIVLTFEYLHSLDLIYRDLKPENLLIDQQGYIQVTDFGFAKRVKGRTWTLCGTPEYLAPEIILSKGYNKAVDWWALGVLIYEMAAGYPPFFADQPIQIYEKIVSGKVRFPSHFSSDLKDLLRNLLQVDLTKRFGNLKNGVNDIKNHKWFATTDWIAIYQRKVEAPFIPKFKGPGDTSNFDDYEEEEIRVSINEKCGKEFSEF</t>
+  </si>
+  <si>
+    <t>TCCAGGGTGTCCCATGAACAGTTTCGGGCGGCCCTGCAGCTGGTGGTCAGCCCAGGAGACCCCAGGGAATACTTGGCCAACTTTATCAAAATCGGGGAAGGCTCAACCGGCATCGTATGCATCGCCACCGAGAAACACACAGGGAAACAAGTTGCAGTGAAGAAAATGGACCTCCGGAAGCAACAGAGACGAGAACTGCTTTTCAATGAGGTCGTGATCATGCGGGATTACCACCATGACAATGTGGTTGACATGTACAGCAGCTACCTTGTCGGCGATGAGCTCTGGGTGGTCATGGAGTTTCTAGAAGGTGGTGCCTTGACAGACATTGTGACTCACACCAGAATGAATGAAGAACAGATAGCTACTGTCTGCCTGTCAGTTCTGAGAGCTCTCTCCTACCTTCATAACCAAGGAGTGATTCACAGGGACATAAAAAGTGACTCCATCCTCCTGACAAGCGATGGCCGGATAAAGTTGTCTGATTTTGGTTTCTGTGCTCAAGTTTCCAAAGAGGTGCCGAAGAGGAAATCATTGGTTGGCACTCCCTACTGGATGGCCCCTGAGGTGATTTCTAGGCTACCTTATGGGACAGAGGTGGACATCTGGTCCCTCGGGATCATGGTGATAGAAATGATTGATGGCGAGCCCCCCTACTTCAATGAGCCTCCCCTCCAGGCGATGCGGAGGATCCGGGACAGTTTACCTCCAAGAGTGAAGGACCTACACAAGGTTTCTTCAGTGCTCCGGGGATTCCTAGACTTGATGTTGGTGAGGGAGCCCTCTCAGAGAGCAACAGCCCAGGAACTCCTCGGACATCCATTCTTAAAACTAGCAGGTCCACCGTCTTGCATTGTCCCCCTCATGAGACAATACAGGCATCAC</t>
+  </si>
+  <si>
+    <t>KRQWALEDFEIGRPLGKGKFGNVYLAREKQSKFILALKVLFKAQLEKAGVEHQLRREVEIQSHLRHPNILRLYGYFHDATRVYLILEYAPLGTVYRELQKLSKFDEQRTATYITELANALSYCHSKRVIHRDIKPENLLLGSAGELKIADFGWSVHAPSSRRTTLCGTLDYLPPEMIEGRMHDEKVDLWSLGVLCYEFLVGKPPFEANTYQETYKRISRVEFTFPDFVTEGARDLISRLLKHNPSQRPMLREVLEHPWITANSSKPS</t>
+  </si>
+  <si>
+    <t>SLK_HUMAN_D0_2JFL_A</t>
+  </si>
+  <si>
+    <t>SRVSHEQFRAALQLVVSPGDPREYLANFIKIGEGSTGIVCIATEKHTGKQVAVKKMDLRKQQRRELLFNEVVIMRDYHHDNVVDMYSSYLVGDELWVVMEFLEGGALTDIVTHTRMNEEQIATVCLSVLRALSYLHNQGVIHRDIKSDSILLTSDGRIKLSDFGFCAQVSKEVPKRKSLVGTPYWMAPEVISRLPYGTEVDIWSLGIMVIEMIDGEPPYFNEPPLQAMRRIRDSLPPRVKDLHKVSSVLRGFLDLMLVREPSQRATAQELLGHPFLKLAGPPSCIVPLMRQYRHH</t>
+  </si>
+  <si>
+    <t>TQTVHEFAKELDATNISIDKVVGAGEFGEVCSGRLKLPSKKEISVAIKTLKVGYTEKQRRDFLGEASIMGQFDHPNIIRLEGVVTKSKPVMIVTEYMENGSLDSFLRKHDAQFTVIQLVGMLRGIASGMKYLSDMGYVHRDLAARNILINSNLVCKVSDFGLSRVLEDDPEAAYTTRGGKIPIRWTSPEAIAYRKFTSASDVWSYGIVLWEVMSYGERPYWEMSNQDVIKAVDEGYRLPPPMDCPAALYQLMLDCWQKDRNNRPKFEQIVSILDKLIRNPGSLKIITSAAARPSNLLLDQSNVDITTFRTTGDWLNGVWTAHCKEIFTGVEYSSCDTIAKIS</t>
+  </si>
+  <si>
+    <t>QQFPQFHVKSGLQIKKNAIIDDYKVTSQVLGLGINGKVLQIFNKRTQEKFALKMLQDCPKARREVELHWRASQCPHIVRIVDVYENLYAGRKCLLIVMECLDGGELFSRIQDRGDQAFTEREASEIMKSIGEAIQYLHSINIAHRDVKPENLLYTSKRPNAILKLTDFGFAKETTSHNSLTTPCYTPYYVAPEVLGPEKYDKSCDMWSLGVIMYILLCGYPPFYSNHGLAISPGMKTRIRMGQYEFPNPEWSEVSEEVKMLIRNLLKTEPTQRMTITEFMNHPWIMQSTKVPQTPLHTSRVLKEDKERWEDVKGCLHDKNSDQA</t>
+  </si>
+  <si>
+    <t>CSK21_HUMAN_D0_3AXW_A</t>
+  </si>
+  <si>
+    <t>ATCTRFTDDYQLFEELGKGAFSVVRRCVKKTPTQEYAAKIINTKKLSARDHQKLEREARICRLLKHPNIVRLHDSISEEGFHYLVFDLVTGGELFEDIVAREYYSEADASHCIHQILESVNHIHQHDIVHRDLKPENLLLASKCKGAAVKLADFGLAIEVQGEQQAWFGFAGTPGYLSPEVLRKDPYGKPVDIWACGVILYILLVGYPPFWDEDQHKLYQQIKAGAYDFPSPEWDTVTPEAKNLINQMLTINPAKRITADQALKHPWVCQRSTVASMMHRQETVECLRKFNARRKLKGAILTTMLVSRNFS</t>
+  </si>
+  <si>
+    <t>EDSLTKQPEEVFDVLEKLGEGSYGSVFKAIHKESGQVVAIKQVPVESDLQEIIKEISIMQQCDSPYVVKYYGSYFKNTDLWIVMEYCGAGSVSDIIRLRNKTLIEDEIATILKSTLKGLEYLHFMRKIHRDIKAGNILLNTEGHAKLADFGVAGQLTDTMAKRNTVIGTPFWMAPEVIQEIGYNCVADIWSLGITSIEMAEGKPPYADIHPMRAIFMIPTNPPPTFRKPELWSDDFTDFVKKCLVKNPEQRATATQLLQHPFIKNAKPVSILRDLITEAMEIKAKRHEEQQRELEEEE</t>
+  </si>
+  <si>
+    <t>CGTGTAAAAGCAGCTCAAGCTGGAAGACAGAGCTCTGCAAAGAGACATCTTGCAGAACAATTTGCAGTTGGAGAGATAATAACTGACATGGCAAAAAAGGAATGGAAAGTAGGATTACCCATTGGCCAAGGAGGCTTTGGCTGTATATATCTTGCTGATATGAATTCTTCAGAGTCAGTTGGCAGTGATGCACCTTGTGTTGTAAAAGTGGAACCCAGTGACAATGGACCTCTTTTTACTGAATTAAAGTTCTACCAACGAGCTGCAAAACCAGAGCAAATTCAGAAATGGATTCGTACCCGTAAGCTGAAGTACCTGGGTGTTCCTAAGTATTGGGGGTCTGGTCTACATGACAAAAATGGAAAAAGTTACAGGTTTATGATAATGGATCGCTTTGGGAGTGACCTTCAGAAAATATATGAAGCAAATGCCAAAAGGTTTTCTCGGAAAACTGTCTTGCAGCTAAGCTTAAGAATTCTGGATATTCTGGAATATATTCACGAGCATGAGTATGTGCATGGAGATATCAAGGCCTCAAATCTTCTTCTGAACTACAAGAATCCTGACCAGGTGTACTTGGTAGATTATGGCCTTGCTTATCGGTACTGCCCAGAAGGAGTTCATAAAGAATACAAAGAAGACCCCAAAAGATGTCACGATGGCACTATTGAATTCACGAGCATCGATGCACACAATGGCGTGGCCCCATCAAGACGTGGTGATTTGGAAATACTTGGTTATTGCATGATCCAATGGCTTACTGGCCATCTTCCTTGGGAGGATAATTTGAAAGATCCTAAATATGTTAGAGATTCCAAAATTAGATACAGAGAAAATATTGCAAGTTTGATGGACAAATGTTTTCCTGAGAAAAACAAACCAGGTGAAATTGCCAAATACATGGAAACAGTGAAATTACTAGACTACACTGAAAAACCTCTTTATGAAAATTTACGTGACATTCTTTTGCAAGGACTAAAAGCTATAGGAAGTAAGGATGATGGCAAATTGGACCTCAGTGTTGTGGAGAATGGAGGTTTGAAAGCAAAAACAATAACAAAGAAGCGAAAGAAAGAAATTGAAGAA</t>
+  </si>
+  <si>
+    <t>KS6A1_HUMAN_D0_3RNY_B</t>
+  </si>
+  <si>
+    <t>MP2K6_HUMAN_D0_3VN9_A</t>
+  </si>
+  <si>
+    <t>RVKAAQAGRQSSAKRHLAEQFAVGEIITDMAKKEWKVGLPIGQGGFGCIYLADMNSSESVGSDAPCVVKVEPSDNGPLFTELKFYQRAAKPEQIQKWIRTRKLKYLGVPKYWGSGLHDKNGKSYRFMIMDRFGSDLQKIYEANAKRFSRKTVLQLSLRILDILEYIHEHEYVHGDIKASNLLLNYKNPDQVYLVDYGLAYRYCPEGVHKEYKEDPKRCHDGTIEFTSIDAHNGVAPSRRGDLEILGYCMIQWLTGHLPWEDNLKDPKYVRDSKIRYRENIASLMDKCFPEKNKPGEIAKYMETVKLLDYTEKPLYENLRDILLQGLKAIGSKDDGKLDLSVVENGGLKAKTITKKRKKEIEE</t>
+  </si>
+  <si>
+    <t>MKNK1_HUMAN_D0_2HW6_B</t>
+  </si>
+  <si>
+    <t>MSLIRKKGFYKQDVNKTAWELPKTYVSPTHVGSGAYGSVCSAIDKRSGEKVAIKKLSRPFQSEIFAKRAYRELLLLKHMQHENVIGLLDVFTPASSLRNFYDFYLVMPFMQTDLQKIMGMEFSEEKIQYLVYQMLKGLKYIHSAGVVHRDLKPGNLAVNEDCELKILDFGLARHADAEMTGYVVTRWYRAPEVILSWMHYNQTVDIWSVVCIMAEMLTGKTLFKGKDYLDQLTQILKVTGVPGTEFVQKLNDKAAKSYIQSLPQTPRKDFTQLFPRASPQAADLLEKMLELDVDKRLTAAQALTHPFFEPFRDPEEETEAQQPFDDSLEHEKLTVDEWKQHIYKEIVNFSPI</t>
+  </si>
+  <si>
+    <t>DEQPHIGNYRLLKTIGKGNFAKVKLARHILTGREVAIKIIDKTQLNPTSLQKLFREVRIMKILNHPNIVKLFEVIETEKTLYLIMEYASGGEVFDYLVAHGRMKEKEARSKFRQIVSAVQYCHQKRIVHRDLKAENLLLDADMNIKIADFGFSNEFTVGGKLDTFCGSPPYAAPELFQGKKYDGPEVDVWSLGVILYTLVSGSLPFDGQNLKELRERVLRGKYRIPFYMSTDCENLLKRFLVLNPIKRGTLEQIMKDRWINAGHEEDELKPFVEPELDISDQKRIDIMVGMGYSQEEIQESLSKMKYDEITATYLLLGRKSSE</t>
+  </si>
+  <si>
+    <t>ITK_HUMAN_D0_3QGW_B</t>
+  </si>
+  <si>
+    <t>KS6A3_HUMAN_D1_4JG7_A</t>
+  </si>
+  <si>
+    <t>KCC4_HUMAN_D0_2W4O_A</t>
+  </si>
+  <si>
+    <t>CSK_HUMAN_D0_3D7T_A</t>
+  </si>
+  <si>
+    <t>KCC2A_HUMAN_D0_2VZ6_B</t>
+  </si>
+  <si>
+    <t>ATGTCTGATGAGGAGATCTTGGAGAAATTACGAAGCATAGTGAGTGTGGGCGATCCTAAGAAGAAATATACACGGTTTGAGAAGATTGGACAAGGTGCTTCAGGCACCGTGTACACAGCAATGGATGTGGCCACAGGACAGGAGGTGGCCATTAAGCAGATGAATCTTCAGCAGCAGCCCAAGAAAGAGCTGATTATTAATGAGATCCTGGTCATGAGGGAAAACAAGAACCCAAACATTGTGAATTACTTGGACAGTTACCTCGTGGGAGATGAGCTGTGGGTTGTTATGGAATACTTGGCTGGAGGCTCCTTGACAGATGTGGTGACAGAAACTTGCATGGATGAAGGCCAAATTGCAGCTGTGTGCCGTGAGTGTCTGCAGGCTCTGGAGTTCTTGCATTCGAACCAGGTCATTCACAGAGACATCAAGAGTGACAATATTCTGTTGGGAATGGATGGCTCTGTCAAGCTAACTGACTTTGGATTCTGTGCACAGATAACCCCAGAGCAGAGCAAACGGAGCACCATGGTAGGAACCCCATACTGGATGGCACCAGAGGTTGTGACACGAAAGGCCTATGGGCCCAAGGTTGACATCTGGTCCCTGGGCATCAAGGCCATCGAAATGATTGAAGGGGAGCCTCCATACCTCAATGAAAACCCTCTGAGAGCCTTGTACCTCATTGCCACCAATGGGACCCCAGAACTTCAGAACCCAGAGAAGCTGTCAGCTATCTTCCGGGACTTTCTGAACCGCTGTCTCGAGATGGATGTGGAGAAGAGAGGTTCAGCTAAAGAGCTGCTACAGCATCAATTCCTGAAGATTGCCAAGCCCCTCTCCAGCCTCACTCCACTTATTGCTGCAGCTAAGGAGGCAACAAAGAACAATCAC</t>
+  </si>
+  <si>
+    <t>ATGGAGGCAGCAGCATCCGAACCCTCTCTTGATCTAGATAATCTGAAACTGTTGGAGCTGATTGGCCGAGGTCGATATGGAGCAGTATATAAAGGCTCCTTGGATGAGCGTCCAGTTGCTGTAAAAGTGTTTTCCTTTGCAAACCGTCAGAATTTTATCAACGAAAAGAACATTTACAGAGTGCCTTTGATGGAACATGACAACATTGCCCGCTTTATAGTTGGAGATGAGAGAGTCACTGCAGATGGACGCATGGAATATTTGCTTGTGATGGAGTACTATCCCAATGGATCTTTATGCAAGTATTTAAGTCTCCACACAAGTGACTGGGTAAGCTCTTGCCGTCTTGCTCATTCTGTTACTAGAGGACTGGCTTATCTTCACACAGAATTACCACGAGGAGATCATTATAAACCTGCAATTTCCCATCGAGATTTAAACAGCAGAAATGTCCTAGTGAAAAATGATGGAACCTGTGTTATTAGTGACTTTGGACTGTCCATGAGGCTGACTGGAAATAGACTGGTGCGCCCAGGGGAGGAAGATAATGCAGCCATAAGCGAGGTTGGCACTATCAGATATATGGCACCAGAAGTGCTAGAAGGAGCTGTGAACTTGAGGGACTGTGAATCAGCTTTGAAACAAGTAGACATGTATGCTCTTGGACTAATCTATTGGGAGATATTTATGAGATGTACAGACCTCTTCCCAGGGGAATCCGTACCAGAGTACCAGATGGCTTTTCAGACAGAGGTTGGAAACCATCCCACTTTTGAGGATATGCAGGTTCTCGTGTCTAGGGAAAAACAGAGACCCAAGTTCCCAGAAGCCTGGAAAGAAAATAGCCTGGCAGTGAGGTCACTCAAGGAGACAATCGAAGACTGTTGGGACCAGGATGCAGAGGCTCGGCTTACTGCACAGTGTGCTGAGGAAAGGATGGCTGAACTTATGATGATTTGGGAAAGAAACAAATCTGTGAGCCCAACA</t>
+  </si>
+  <si>
+    <t>GCCACCTGCACACGTTTCACCGACGACTACCAGCTCTTCGAGGAGCTTGGCAAGGGTGCTTTCTCTGTGGTCCGCAGGTGTGTGAAGAAAACCCCCACGCAGGAGTACGCAGCAAAAATCATCAATACCAAGAAATTGTCTGCCCGGGATCACCAGAAACTAGAACGTGAGGCTCGGATATGTCGACTTCTGAAACATCCAAACATCGTGCGCCTCCATGACAGTATTTCTGAAGAAGGGTTTCACTACCTCGTGTTTGACCTTGTTACCGGCGGGGAGCTGTTTGAAGACATTGTGGCCAGAGAGTACTACAGTGAAGCAGATGCCAGCCACTGTATACATCAGATTCTGGAGAGTGTTAACCACATCCACCAGCATGACATCGTCCACAGGGACCTGAAGCCTGAGAACCTGCTGCTGGCGAGTAAATGCAAGGGTGCCGCCGTCAAGCTGGCTGATTTTGGCCTAGCCATCGAAGTACAGGGAGAGCAGCAGGCTTGGTTTGGTTTTGCTGGCACCCCAGGTTACTTGTCCCCTGAGGTCTTGAGGAAAGATCCCTATGGAAAACCTGTGGATATCTGGGCCTGCGGGGTCATCCTGTATATCCTCCTGGTGGGCTATCCTCCCTTCTGGGATGAGGATCAGCACAAGCTGTATCAGCAGATCAAGGCTGGAGCCTATGATTTCCCATCACCAGAATGGGACACGGTAACTCCTGAAGCCAAGAACTTGATCAACCAGATGCTGACCATAAACCCAGCAAAGCGCATCACGGCTGACCAGGCTCTCAAGCACCCGTGGGTCTGTCAACGATCCACGGTGGCATCCATGATGCATCGTCAGGAGACTGTGGAGTGTTTGCGCAAGTTCAATGCCCGGAGAAAACTGAAGGGTGCCATCCTCACGACCATGCTTGTCTCCAGGAACTTCTCA</t>
+  </si>
+  <si>
+    <t>GAGACCTACATTAAGCTGGACAAACTGGGCGAGGGTACCTATGCCACCGTCTACAAAGGCAAAAGCAAGCTCACAGACAACCTTGTGGCACTCAAGGAGATCAGACTGGAACATGAAGAGGGGGCACCCTGCACCGCCATCCGGGAAGTGTCCCTACTCAAGGACCTCAAACACGCCAACATCGTTACGCTACATGACATTATCCACACGGAGAAGTCCCTCACCCTTGTCTTTGAGTACCTGGACAAGGACCTGAAGCAGTACCTGGATGACTGTGGGAACATCATCAACATGCACAACGTGAAACTGTTCCTGTTCCAGCTGCTCCGTGGCCTGGCCTACTGCCACCGGCAGAAGGTGCTACACCGAGACCTCAAGCCCCAGAACCTGCTCATCAACGAGAGGGGAGAGCTCAAGCTGGCTGACTTTGGCCTGGCCCGAGCCAAGTCAATCCCAACAAAGACATACTCCAATGAGGTGGTGACACTGTGGTACCGGCCCCCTGACATCCTGCTTGGGTCCACGGACTACTCCACTCAGATTGACATGTGGGGTGTGGGCTGCATCTTCTATGAGATGGCCACAGGCCGTCCCCTCTTTCCGGGCTCCACGGTGGAGGAACAGCTACACTTCATCTTCCGTATCTTAGGAACCCCAACTGAGGAGACGTGGCCAGGCATCCTGTCCAACGAGGAGTTCAAGACATACAACTACCCCAAGTACCGAGCCGAGGCCCTTTTGAGCCACGCACCCCGACTTGATAGCGACGGGGCCGACCTCCTCACCAAGCTGTTGCAGTTTGAGGGTCGAAATCGGATCTCCGCAGAGGATGCCATGAAACATCCATTCTTCCTCAGTCTGGGGGAGCGGATCCACAAACTTCCTGACACTACTTCCATATTTGCACTAAAGGAGATTCAGCTACAAAAGGAGGCCAGCCTTCGGTCT</t>
+  </si>
+  <si>
+    <t>MK13_HUMAN_D0_4EYJ_A</t>
+  </si>
+  <si>
+    <t>STK16_HUMAN_D0_2BUJ_B</t>
+  </si>
+  <si>
+    <t>ATGGAAAGCGACCTGCACCAGATCATCCACTCCTCACAGCCCCTCACACTGGAACACGTGCGCTACTTCCTGTACCAACTGCTGCGGGGCCTGAAGTACATGCACTCGGCTCAGGTCATCCACCGTGACCTGAAGCCCTCCAACCTATTGGTGAATGAGAACTGTGAGCTCAAGATTGGTGACTTTGGTATGGCTCGTGGCCTGTGCACCTCGCCCGCTGAACATCAGTACTTCATGACTGAGTATGTGGCCACGCGCTGGTACCGTGCGCCCGAGCTCATGCTCTCTTTGCATGAGTATACACAGGCTATTGACCTCTGGTCTGTGGGCTGCATCTTTGGTGAGATGCTGGCCCGGCGCCAGCTCTTCCCAGGCAAAAACTATGTACACCAGCTACAGCTCATCATGATGGTGCTGGGTACCCCATCACCAGCCGTGATTCAGGCTGTGGGGGCTGAGAGGGTGCGGGCCTATATCCAGAGCTTGCCACCACGCCAGCCTGTGCCCTGGGAGACAGTGTACCCAGGTGCCGACCGCCAGGCCCTATCACTGCTGGGTCGCATGCTGCGTTTTGAGCCCAGCGCTCGCATCTCAGCAGCTGCTGCCCTTCGCCACCCTTTCCTGGCCAAGTACCATGATCCTGATGATGAGCCTGACTGTGCCCCGCCCTTTGACTTTGCCTTTGACCGCGAAGCCCTCACTCGGGAGCGCATTAAGGAGGCCATTGTGGCTGAAATTGAGGACTTCCATGCAAGGCGTGAGGGCATCCGCCAACAGATCCGCTTCCAGCCTTCTCTACAGCCTGTGGCTAGTGAGCCTGGCTGTCCAGATGTTGAAATGCCCAGTCCCTGGGCTCCCAGTGGGGACTGTGCCATG</t>
+  </si>
+  <si>
+    <t>CAGAGCAGTAAGCGCAGCAGCCGGAGTGTGGAAGATGACAAGGAGGGTCACCTGGTGTGCCGGATCGGCGATTGGCTCCAAGAGCGATATGAGATTGTGGGGAACCTGGGTGAAGGCACCTTTGGCAAGGTGGTGGAGTGCTTGGACCATGCCAGAGGGAAGTCTCAGGTTGCCCTGAAGATCATCCGCAACGTGGGCAAGTACCGGGAGGCTGCCCGGCTAGAAATCAACGTGCTCAAAAAAATCAAGGAGAAGGACAAAGAAAACAAGTTCCTGTGTGTCTTGATGTCTGACTGGTTCAACTTCCACGGTCACATGTGCATCGCCTTTGAGCTCCTGGGCAAGAACACCTTTGAGTTCCTGAAGGAGAATAACTTCCAGCCTTACCCCCTACCACATGTCCGGCACATGGCCTACCAGCTCTGCCACGCCCTTAGATTTCTGCATGAGAATCAGCTGACCCATACAGACTTGAAACCAGAGAACATCCTGTTTGTGAATTCTGAGTTTGAAACCCTCTACAATGAGCACAAGAGCTGTGAGGAGAAGTCAGTGAAGAACACCAGCATCCGAGTGGCTGACTTTGGCAGTGCCACATTTGACCATGAGCACCACACCACCATTGTGGCCACCCGTCACTATCGCCCGCCTGAGGTGATCCTTGAGCTGGGCTGGGCACAGCCCTGTGACGTCTGGAGCATTGGCTGCATTCTCTTTGAGTACTACCGGGGCTTCACACTCTTCCAGACCCACGAAAACCGAGAGCACCTGGTGATGATGGAGAAGATCCTAGGGCCCATCCCATCACACATGATCCACCGTACCAGGAAGCAGAAATATTTCTACAAAGGGGGCCTAGTTTGGGATGAGAACAGCTCTGACGGCCGGTATGTGAAGGAGAACTGCAAACCTCTGAAGAGTTACATGCTCCAAGACTCCCTGGAGCACGTGCAGCTGTTTGACCTGATGAGGAGGATGTTAGAATTTGACCCTGCCCAGCGCATCACACTGGCCGAGGCCCTGCTGCACCCCTTCTTTGCTGGCCTGACCCCTGAGGAGCGGTCCTTCCACACC</t>
+  </si>
+  <si>
+    <t>GAACTGAAGGATGACGACTTTGAGAAGATCAGTGAGCTGGGGGCTGGCAATGGCGGTGTGGTGTTCAAGGTCTCCCACAAGCCTTCTGGCCTGGTCATGGCCAGAAAGCTAATTCATCTGGAGATCAAACCCGCAATCCGGAACCAGATCATAAGGGAGCTGCAGGTTCTGCATGAGTGCAACTCTCCGTACATCGTGGGCTTCTATGGTGCGTTCTACAGCGATGGCGAGATCAGTATCTGCATGGAGCACATGGATGGAGGTTCTCTGGATCAAGTCCTGAAGAAAGCTGGAAGAATTCCTGAACAAATTTTAGGAAAAGTTAGCATTGCTGTAATAAAAGGCCTGACATATCTGAGGGAGAAGCACAAGATCATGCACAGAGCATACGGAATGGACAGCCGACCTCCCATGGCAATTTTTGAGTTGTTGGATTACATAGTCAACGAGCCTCCTCCAAAACTGCCCAGTGGAGTGTTCAGTCTGGAATTTCAAGATTTTGTGAATAAATGCTTAATAAAAAACCCCGCAGAGAGAGCAGATTTGAAGCAACTCATGGTTCATGCTTTTATCAAGAGATCTGATGCTGAGGAAGTGGATTTTGCAGGTTGGCTCTGCTCCACCATCGGCCTTAAC</t>
+  </si>
+  <si>
+    <t>MQTVGVHSIVQQLHRNSIQFTDGYEVKEDIGVGSYSVCKRCIHKATNMEFAVKIIDKSKRDPTEEIEILLRYGQHPNIITLKDVYDDGKYVYVVTELMKGGELLDKILRQKFFSEREASAVLFTITKTVEYLHAQGVVHRDLKPSNILYVDESGNPESIRICDFGFAKQLRAENGLLMTPCYTANFVAPEVLKRQGYDAACDIWSLGVLLYTMLTGYTPFANGPDDTPEEILARIGSGKFSLSGGYWNSVSDTAKDLVSKMLHVDPHQRLTAALVLRHPWIVHWDQLPQYQLNRQDAPHLVKGAMAATYSALNRNQSPVLEPVGRSTLAQRRGIKKITSTAL</t>
+  </si>
+  <si>
+    <t>KAPCA_HUMAN_D0_4AE9_A</t>
+  </si>
+  <si>
+    <t>KCC2G_HUMAN_D0_2V7O_A</t>
+  </si>
+  <si>
+    <t>KQYEHVKRDLNPEDFWEIIGELGDGAFGKVYKAQNKETSVLAAAKVIDTKSEEELEDYMVEIDILASCDHPNIVKLLDAFYYENNLWILIEFCAGGAVDAVMLELERPLTESQIQVVCKQTLDALNYLHDNKIIHRDLKAGNILFTLDGDIKLADFGVSAKNMRTIQRRDSFIGTPYWMAPEVVMCETSKDRPYDYKADVWSLGITLIEMAEIEPPHHELNPMRVLLKIAKSEPPTLAQPSRWSSNFKDFLKKCLEKNVDARWTTSQLLQHPFVTVDSNKPIRELIAEAKAEVTEEVEDGKE</t>
+  </si>
+  <si>
+    <t>ACCCAAACTGTTCATGAGTTTGCCAAGGAATTGGATGCCACCAACATATCCATTGATAAAGTTGTTGGAGCAGGTGAATTTGGAGAGGTGTGCAGTGGTCGCTTAAAACTTCCTTCAAAAAAAGAGATTTCAGTGGCCATTAAGACCCTGAAAGTTGGCTACACAGAAAAGCAGAGGAGAGACTTCCTGGGAGAAGCAAGCATTATGGGACAGTTTGACCACCCCAATATCATTCGACTGGAAGGAGTTGTTACCAAAAGTAAGCCAGTTATGATTGTCACAGAATACATGGAGAATGGTTCCTTGGATAGTTTCCTACGTAAACACGATGCCCAGTTTACTGTCATTCAGCTAGTGGGGATGCTTCGAGGGATAGCATCTGGCATGAAGTACCTGTCAGACATGGGCTATGTTCACCGAGACCTCGCTGCTCGGAACATCTTGATCAACAGTAACTTGGTGTGTAAGGTTTCTGATTTCGGACTTTCGCGTGTCCTGGAGGATGACCCAGAAGCTGCTTATACAACAAGAGGAGGGAAGATCCCAATCAGGTGGACATCACCAGAAGCTATAGCCTACCGCAAGTTCACGTCAGCCAGCGATGTATGGAGTTATGGGATTGTTCTCTGGGAGGTGATGTCTTATGGAGAGAGACCATACTGGGAGATGTCCAATCAGGATGTAATTAAAGCTGTAGATGAGGGCTATCGACTGCCACCCCCCATGGACTGCCCAGCTGCCTTGTATCAGCTGATGCTGGACTGCTGGCAGAAAGACAGGAACAACAGACCCAAGTTTGAGCAGATTGTTAGTATTCTGGACAAGCTTATCCGGAATCCCGGCAGCCTGAAGATCATCACCAGTGCAGCCGCAAGGCCATCAAACCTTCTTCTGGACCAAAGCAATGTGGATATCACTACCTTCCGCACAACAGGTGACTGGCTTAATGGTGTCTGGACAGCACACTGCAAGGAAATCTTCACGGGTGTGGAGTACAGTTCTTGTGACACAATAGCCAAGATTTCC</t>
+  </si>
+  <si>
+    <t>MEKDGLCRADQQYECVAEIGEGAYGKVFKARDLKNGGRFVALKRVRVQTGEEGMPLSTIREVAVLRHLETFEHPNVVRLFDVCTVSRTDRETKLTLVFEHVDQDLTTYLDKVPEPGVPTETIKDMMFQLLRGLDFLHSHRVVHRDLKPQNILVTSSGQIKLADFGLARIYSFQMALTSVVVTLWYRAPEVLLQSSYATPVDLWSVGCIFAEMFRRKPLFRGSSDVDQLGKILDVIGLPGEEDWPRDVALPRQAFHSKSAQPIEKFVTDIDELGKDLLLKCLTFNPAKRISAYSALSHPYFQ</t>
+  </si>
+  <si>
+    <t>EPHA3_HUMAN_D0_4GK2_A</t>
+  </si>
+  <si>
+    <t>ATGCCCGGCCCGGCCGCGGGCAGCAGGGCCCGGGTCTACGCCGAGGTGAACAGTCTGAGGAGCCGCGAGTACTGGGACTACGAGGCTCACGTCCCGAGCTGGGGTAATCAAGATGATTACCAACTGGTTCGAAAACTTGGTCGGGGAAAATATAGTGAAGTATTTGAGGCCATTAATATCACCAACAATGAGAGAGTGGTTGTAAAAATCCTGAAGCCAGTGAAGAAAAAGAAGATAAAACGAGAGGTTAAGATTCTGGAGAACCTTCGTGGTGGAACAAATATCATTAAGCTGATTGACACTGTAAAGGACCCCGTGTCAAAGACACCAGCTTTGGTATTTGAATATATCAATAATACAGATTTTAAGCAACTCTACCAGATCCTGACAGACTTTGATATCCGGTTTTATATGTATGAACTACTTAAAGCTCTGGATTACTGCCACAGCAAGGGAATCATGCACAGGGATGTGAAACCTCACAATGTCATGATAGATCACCAACAGAAAAAGCTGCGACTGATAGATTGGGGTCTGGCAGAATTCTATCATCCTGCTCAGGAGTACAATGTTCGTGTAGCCTCAAGGTACTTCAAGGGACCAGAGCTCCTCGTGGACTATCAGATGTATGATTATAGCTTGGACATGTGGAGTTTGGGCTGTATGTTAGCAAGCATGATCTTTCGAAGGGAACCATTCTTCCATGGACAGGACAACTATGACCAGCTTGTTCGCATTGCCAAGGTTCTGGGTACAGAAGAACTGTATGGGTATCTGAAGAAGTATCACATAGACCTAGATCCACACTTCAACGATATCCTGGGACAACATTCACGGAAACGCTGGGAAAACTTTATCCATAGTGAGAACAGACACCTTGTCAGCCCTGAGGCCCTAGATCTTCTGGACAAACTTCTGCGATACGACCATCAACAGAGACTGACTGCCAAAGAGGCCATGGAGCACCCATACTTCTACCCTGTGGTGAAGGAGCAGTCCCAG</t>
+  </si>
+  <si>
+    <t>ATGTCGGGACCCGTGCCAAGCAGGGCCAGAGTTTACACAGATGTTAATACACACAGACCTCGAGAATACTGGGATTACGAGTCACATGTGGTGGAATGGGGAAATCAAGATGACTACCAGCTGGTTCGAAAATTAGGCCGAGGTAAATACAGTGAAGTATTTGAAGCCATCAACATCACAAATAATGAAAAAGTTGTTGTTAAAATTCTCAAGCCAGTAAAAAAGAAGAAAATTAAGCGTGAAATAAAGATTTTGGAGAATTTGAGAGGAGGTCCCAACATCATCACACTGGCAGACATTGTAAAAGACCCTGTGTCACGAACCCCCGCCTTGGTTTTTGAACACGTAAACAACACAGACTTCAAGCAATTGTACCAGACGTTAACAGACTATGATATTCGATTTTACATGTATGAGATTCTGAAGGCCCTGGATTATTGTCACAGCATGGGAATTATGCACAGAGATGTCAAGCCCCATAATGTCATGATTGATCATGAGCACAGAAAGCTACGACTAATAGACTGGGGTTTGGCTGAGTTTTATCATCCTGGCCAAGAATATAATGTCCGAGTTGCTTCCCGATACTTCAAAGGTCCTGAGCTACTTGTAGACTATCAGATGTACGATTATAGTTTGGATATGTGGAGTTTGGGTTGTATGCTGGCAAGTATGATCTTTCGGAAGGAGCCATTTTTCCATGGACATGACAATTATGATCAGTTGGTGAGGATAGCCAAGGTTCTGGGGACAGAAGATTTATATGACTATATTGACAAATACAACATTGAATTAGATCCACGTTTCAATGATATCTTGGGCAGACACTCTCGAAAGCGATGGGAACGCTTTGTCCACAGTGAAAATCAGCACCTTGTCAGCCCTGAGGCCTTGGATTTCCTGGACAAACTGCTGCGATATGACCACCAGTCACGGCTTACTGCAAGAGAGGCAATGGAGCACCCCTATTTCTACACTGTTGTGAAGGACCAGGCTCGAATGGGT</t>
+  </si>
+  <si>
+    <t>NEK2_HUMAN_D0_2XKE_A</t>
+  </si>
+  <si>
+    <t>MK01_HUMAN_D0_4FMQ_A</t>
+  </si>
+  <si>
+    <t>ATGGAGCTGAGAGTCGGGAACAGGTACCGGCTGGGCCGGAAGATCGGCAGCGGCTCCTTCGGAGACATCTATCTCGGTACGGACATTGCTGCAGGAGAAGAGGTTGCCATCAAGCTTGAATGTGTCAAAACCAAACACCCTCAGCTCCACATTGAGAGCAAAATCTACAAGATGATGCAGGGAGGAGTGGGCATCCCCACCATCAGATGGTGCGGGGCAGAGGGGGACTACAACGTCATGGTGATGGAGCTGCTGGGGCCAAGCCTGGAGGACCTCTTCAACTTCTGCTCCAGGAAATTCAGCCTCAAAACCGTCCTGCTGCTTGCTGACCAAATGATCAGTCGCATCGAATACATTCATTCAAAGAACTTCATCCACCGGGATGTGAAGCCAGACAACTTCCTCATGGGCCTGGGGAAGAAGGGCAACCTGGTGTACATCATCGACTTCGGGCTGGCCAAGAAGTACCGGGATGCACGCACCCACCAGCACATCCCCTATCGTGAGAACAAGAACCTCACGGGGACGGCGCGGTACGCCTCCATCAACACGCACCTTGGAATTGAACAATCCCGAAGAGATGACTTGGAGTCTCTGGGCTACGTGCTAATGTACTTCAACCTGGGCTCTCTCCCCTGGCAGGGGCTGAAGGCTGCCACCAAGAGACAGAAATACGAAAGGATTAGCGAGAAGAAAATGTCCACCCCCATCGAAGTGTTGTGTAAAGGCTACCCTTCCGAATTTGCCACATACCTGAATTTCTGCCGTTCCTTGCGTTTTGACGACAAGCCTGACTACTCGTACCTGCGGCAGCTTTTCCGGAATCTGTTCCATCGCCAGGGCTTCTCCTATGACTACGTGTTCGACTGGAACATGCTCAAA</t>
+  </si>
+  <si>
+    <t>ATGGCGGCGGCGGCGGCGGCGGGCGCGGGCCCGGAGATGGTCCGCGGGCAGGTGTTCGACGTGGGGCCGCGCTACACCAACCTCTCGTACATCGGCGAGGGCGCCTACGGCATGGTGTGCTCTGCTTATGATAATGTCAACAAAGTTCGAGTAGCTATCAAGAAAATCAGCCCCTTTGAGCACCAGACCTACTGCCAGAGAACCCTGAGGGAGATAAAAATCTTACTGCGCTTCAGACATGAGAACATCATTGGAATCAATGACATTATTCGAGCACCAACCATCGAGCAAATGAAAGATGTATATATAGTACAGGACCTCATGGAAACAGATCTTTACAAGCTCTTGAAGACACAACACCTCAGCAATGACCATATCTGCTATTTTCTCTACCAGATCCTCAGAGGGTTAAAATATATCCATTCAGCTAACGTTCTGCACCGTGACCTCAAGCCTTCCAACCTGCTGCTCAACACCACCTGTGATCTCAAGATCTGTGACTTTGGCCTGGCCCGTGTTGCAGATCCAGACCATGATCACACAGGGTTCCTGACAGAATATGTGGCCACACGTTGGTACAGGGCTCCAGAAATTATGTTGAATTCCAAGGGCTACACCAAGTCCATTGATATTTGGTCTGTAGGCTGCATTCTGGCAGAAATGCTTTCTAACAGGCCCATCTTTCCAGGGAAGCATTATCTTGACCAGCTGAACCACATTTTGGGTATTCTTGGATCCCCATCACAAGAAGACCTGAATTGTATAATAAATTTAAAAGCTAGGAACTATTTGCTTTCTCTTCCACACAAAAATAAGGTGCCATGGAACAGGCTGTTCCCAAATGCTGACTCCAAAGCTCTGGACTTATTGGACAAAATGTTGACATTCAACCCACACAAGAGGATTGAAGTAGAACAGGCTCTGGCCCACCCATATCTGGAGCAGTATTACGACCCGAGTGACGAGCCCATCGCCGAAGCACCATTCAAGTTCGACATGGAATTGGATGACTTGCCTAAGGAAAAGCTCAAAGAACTAATTTTTGAAGAGACTGCTAGATTCCAGCCAGGATACAGATCT</t>
+  </si>
+  <si>
+    <t>MDEQSQGMQGPPVPQFQPQKALRPDMGYNTLANFRIEKKIGRGQFSEVYRAACLLDGVPVALKKVQIFDLMDAKARADCIKEIDLLKQLNHPNVIKYYASFIEDNELNIVLELADAGDLSRMIKHFKKQKRLIPERTVWKYFVQLCSALEHMHSRRVMHRDIKPANVFITATGVVKLGDLGLGRFFSSKTTAAHSLVGTPYYMSPERIHENGYNFKSDIWSLGCLLYEMAALQSPFYGDKMNLYSLCKKIEQCDYPPLPSDHYSEELRQLVNMCINPDPEKRPDVTYVYDVAKRMHACTASS</t>
+  </si>
+  <si>
+    <t>GECSQKGPVPFSHCLPTEKLQRCEKIGEGVFGEVFQTIADHTPVAIKIIAIEGPDLVNGSHQKTFEEILPEIIISKELSLLSGEVCNRTEGFIGLNSVHCVQGSYPPLLLKAWDHYNSTKGSANDRPDFFKDDQLFIVLEFEFGGIDLEQMRTKLSSLATAKSILHQLTASLAVAEASLRFEHRDLHWGNVLLKKTSLKKLHYTLNGKSSTIPSCGLQVSIIDYTLSRLERDGIVVFCDVSMDEDLFTGDGDYQFDIYRLMKKENNNRWGEYHPYSNVLWLHYLTDKMLKQMTFKTKCNTPAMKQIKRKIQEFHRTMLNFSSATDLLCQHRLFK</t>
+  </si>
+  <si>
+    <t>MENFNNFYILTSKELGRGKFAVVRQCISKSTGQEYAAKFLKKRRRGQDCRAEILHEIAVLELAKSCPRVINLHEVYENTSEIILILEYAAGGEIFSLCLPELAEMVSENDVIRLIKQILEGVYYLHQNNIVHLDLKPQNILLSSIYPLGDIKIVDFGMSRKIGHACELREIMGTPEYLAPEILNYDPITTATDMWNIGIIAYMLLTHTSPFVGEDNQETYLNISQVNVDYSEETFSSVSQLATDFIQSLLVKNPEKRPTAEICLSHSWLQQWDFENLFHPEETSSSSQTQDHSVRSSEDKTSKSS</t>
+  </si>
+  <si>
+    <t>GCTGATCCAGAAGAACTGTTCACAAAATTAGAGCGCATTGGGAAAGGCTCATTTGGGGAAGTTTTCAAAGGAATTGATAACCGTACCCAGCAAGTCGTTGCTATTAAAATCATAGACCTTGAGGAAGCCGAAGATGAAATAGAAGACATTCAGCAAGAAATAACTGTCTTGAGTCAATGTGACAGCTCATATGTAACAAAATACTATGGGTCATATTTAAAGGGGTCTAAATTATGGATAATAATGGAATACCTGGGCGGTGGTTCAGCACTGGATCTTCTTCGAGCTGGTCCATTTGATGAGTTCCAGATTGCTACCATGCTAAAGGAAATTTTAAAAGGTCTGGACTATCTGCATTCAGAAAAGAAAATTCACCGAGACATAAAAGCTGCCAATGTCTTGCTCTCAGAACAAGGAGATGTTAAACTTGCTGATTTTGGAGTTGCTGGTCAGCTGACAGATACACAGATTAAAAGAAATACCTTTGTGGGAACTCCATTTTGGATGGCTCCTGAAGTTATTCAACAGTCAGCTTATGACTCAAAAGCTGACATTTGGTCATTGGGAATTACTGCTATTGAACTAGCCAAGGGAGAGCCACCTAACTCCGATATGCATCCAATGAGAGTTCTGTTTCTTATTCCCAAAAACAATCCTCCAACTCTTGTTGGAGACTTTACTAAGTCTTTTAAGGAGTTTATTGATGCTTGCCTGAACAAAGATCCATCATTTCGTCCTACAGCAAAAGAACTTCTGAAACACAAATTCATTGTAAAAAATTCAAAGAAGACTTCTTATCTGACTGAACTGATAGATCGTTTTAAGAGATGGAAGGCAGAA</t>
+  </si>
+  <si>
+    <t>MELRVGNKYRLGRKIGSGSFGDIYLGANIASGEEVAIKLECVKTKHPQLHIESKFYKMMQGGVGIPSIKWCGAEGDYNVMVMELLGPSLEDLFNFCSRKFSLKTVLLLADQMISRIEYIHSKNFIHRDVKPDNFLMGLGKKGNLVYIIDFGLAKKYRDARTHQHIPYRENKNLTGTARYASINTHLGIEQSRRDDLESLGYVLMYFNLGSLPWQGLKAATKRQKYERISEKKMSTPIEVLCKGYPSEFSTYLNFCRSLRFDDKPDYSYLRQLFRNLFHRQGFSYDYVFDWNMLK</t>
+  </si>
+  <si>
+    <t>SSVTASAAPGTASLVPDYWIDGSNRDALSDFFEVESELGRGATSIVYRCKQKGTQKPYALKVLKKTVDKKIVRTEIGVLLRLSHPNIIKLKEIFETPTEISLVLELVTGGELFDRIVEKGYYSERDAADAVKQILEAVAYLHENGIVHRDLKPENLLYATPAPDAPLKIADFGLSKIVEHQVLMKTVCGTPGYCAPEILRGCAYGPEVDMWSVGIITYILLCGFEPFYDERGDQFMFRRILNCEYYFISPWWDEVSLNAKDLVRKLIVLDPKKRLTTFQALQHPWVTGKAANFVHMDTAQKKLQEFNARRKLKAAVKAVVASSRLG</t>
+  </si>
+  <si>
+    <t>dna_end</t>
+  </si>
+  <si>
+    <t>MADDDVLFEDVYELCEVIGKGPFSVVRRCINRETGQQFAVKIVDVAKFTSSPGLSTEDLKREASICHMLKHPHIVELLETYSSDGMLYMVFEFMDGADLCFEIVKRADAGFVYSEAVASHYMRQILEALRYCHDNNIIHRDVKPHCVLLASKENSAPVKLGGFGVAIQLGESGLVAGGRVGTPHFMAPEVVKREPYGKPVDVWGCGVILFILLSGCLPFYGTKERLFEGIIKGKYKMNPRQWSHISESAKDLVRRMLMLDPAERITVYEALNHPWLKERDRYAYKIHLPETVEQLRKFNARRKLKGAVLAAVSSHKFNSFYGDPPEELPDFSEDPTSSGA</t>
+  </si>
+  <si>
+    <t>FAK1_HUMAN_D0_2IJM_B</t>
+  </si>
+  <si>
+    <t>CHK2_HUMAN_D0_2CN5_A</t>
+  </si>
+  <si>
+    <t>GTGATCGACCCCTCAGAGCTCACTTTTGTCCAAGAGATTGGCAGTGGGCAATTTGGGTTGGTGCATCTGGGCTACTGGCTCAACAAGGACAAGGTGGCTATCAAAACCATTCGGGAAGGGGCTATGTCAGAAGAGGACTTCATAGAGGAGGCTGAAGTAATGATGAAACTCTCTCATCCCAAACTGGTGCAGCTGTATGGGGTGTGCCTGGAGCAGGCCCCCATCTGCCTGGTGTTTGAGTTCATGGAGCACGGCTGCCTGTCAGATTATCTACGCACCCAGCGGGGACTTTTTGCTGCAGAGACCCTGCTGGGCATGTGTCTGGATGTGTGTGAGGGCATGGCCTACCTGGAAGAGGCATGTGTCATCCACAGAGACTTGGCTGCCAGAAATTGTTTGGTGGGAGAAAACCAAGTCATCAAGGTGTCTGACTTTGGGATGACAAGGTTCGTTCTGGATGATCAGTACACCAGTTCCACAGGCACCAAATTCCCGGTGAAGTGGGCATCCCCAGAGGTTTTCTCTTTCAGTCGCTATAGCAGCAAGTCCGATGTGTGGTCATTTGGTGTGCTGATGTGGGAAGTTTTCAGTGAAGGCAAAATCCCGTATGAAAACCGAAGCAACTCAGAGGTGGTGGAAGACATCAGTACCGGATTTCGGTTGTACAAGCCCCGGCTGGCCTCCACACACGTCTACCAGATTATGAATCACTGCTGGAAAGAGAGACCAGAAGATCGGCCAGCCTTCTCCAGACTGCTGCGTCAACTGGCTGAAATTGCAGAATCAGGACTT</t>
+  </si>
+  <si>
+    <t>MSDEEILEKLRSIVSVGDPKKKYTRFEKIGQGASGTVYTAMDVATGQEVAIKQMNLQQQPKKELIINEILVMRENKNPNIVNYLDSYLVGDELWVVMEYLAGGSLTDVVTETCMDEGQIAAVCRECLQALEFLHSNQVIHRDIKSDNILLGMDGSVKLTDFGFCAQITPEQSKRSTMVGTPYWMAPEVVTRKAYGPKVDIWSLGIKAIEMIEGEPPYLNENPLRALYLIATNGTPELQNPEKLSAIFRDFLNRCLEMDVEKRGSAKELLQHQFLKIAKPLSSLTPLIAAAKEATKNNH</t>
+  </si>
+  <si>
+    <t>MSQSKGKKRNPGLKIPKEAFEQPQTSSTPPRDLDSKACISIGNQNFEVKADDLEPIMELGRGAYGVVEKMRHVPSGQIMAVKRIRATVNSQEQKRLLMDLDISMRTVDCPFTVTFYGALFREGDVWICMELMDTSLDKFYKQVIDKGQTIPEDILGKIAVSIVKALEHLHSKLSVIHRDVKPSNVLINALGQVKMCDFGISGYLVDSVAKTIDAGCKPYMAPERINPELNQKGYSVKSDIWSLGITMIELAILRFPYDSWGTPFQQLKQVVEEPSPQLPADKFSAEFVDFTSQCLKKNSKERPTYPELMQHPFFTLHESKGTDVASFVKLILGD</t>
+  </si>
+  <si>
+    <t>DYRK2_HUMAN_D0_3KVW_A</t>
+  </si>
+  <si>
+    <t>QSSKRSSRSVEDDKEGHLVCRIGDWLQERYEIVGNLGEGTFGKVVECLDHARGKSQVALKIIRNVGKYREAARLEINVLKKIKEKDKENKFLCVLMSDWFNFHGHMCIAFELLGKNTFEFLKENNFQPYPLPHVRHMAYQLCHALRFLHENQLTHTDLKPENILFVNSEFETLYNEHKSCEEKSVKNTSIRVADFGSATFDHEHHTTIVATRHYRPPEVILELGWAQPCDVWSIGCILFEYYRGFTLFQTHENREHLVMMEKILGPIPSHMIHRTRKQKYFYKGGLVWDENSSDGRYVKENCKPLKSYMLQDSLEHVQLFDLMRRMLEFDPAQRITLAEALLHPFFAGLTPEERSFHT</t>
+  </si>
+  <si>
+    <t>MK07_HUMAN_D0_4IC7_D</t>
+  </si>
+  <si>
+    <t>ATGCAGACAGTTGGTGTACATTCAATTGTTCAGCAGTTACACAGGAACAGTATTCAGTTTACTGATGGATATGAAGTAAAAGAAGATATTGGAGTTGGCTCCTACTCTGTTTGCAAGAGATGTATACATAAAGCTACAAACATGGAGTTTGCAGTGAAGATTATTGATAAAAGCAAGAGAGACCCAACAGAAGAAATTGAAATTCTTCTTCGTTATGGACAGCATCCAAACATTATCACTCTAAAGGATGTATATGATGATGGAAAGTATGTGTATGTAGTAACAGAACTTATGAAAGGAGGTGAATTGCTGGATAAAATTCTTAGACAAAAATTTTTCTCTGAACGAGAGGCCAGTGCTGTCCTGTTCACTATAACTAAAACCGTTGAATATCTTCACGCACAAGGGGTGGTTCATAGAGACTTGAAACCTAGCAACATTCTTTATGTGGATGAATCTGGTAATCCGGAATCTATTCGAATTTGTGATTTTGGCTTTGCAAAACAGCTGAGAGCGGAAAATGGTCTTCTCATGACTCCTTGTTACACTGCAAATTTTGTTGCACCAGAGGTTTTAAAAAGACAAGGCTATGATGCTGCTTGTGATATATGGAGTCTTGGTGTCCTACTCTATACAATGCTTACCGGTTACACTCCATTTGCAAATGGTCCTGATGATACACCAGAGGAAATATTGGCACGAATAGGTAGCGGAAAATTCTCACTCAGTGGTGGTTACTGGAATTCTGTTTCAGACACAGCAAAGGACCTGGTGTCAAAGATGCTTCATGTAGACCCTCATCAGAGACTGACTGCTGCTCTTGTGCTCAGACATCCTTGGATCGTCCACTGGGACCAACTGCCACAATACCAACTAAACAGACAGGATGCACCACATCTAGTAAAGGGTGCCATGGCAGCTACATATTCTGCTTTGAACCGTAATCAGTCACCAGTTTTGGAACCAGTAGGCCGCTCTACTCTTGCTCAGCGGAGAGGTATTAAAAAAATCACCTCAACAGCCCTG</t>
+  </si>
+  <si>
+    <t>KS6A3_HUMAN_D0_4JG7_A</t>
+  </si>
+  <si>
+    <t>MGKVKATPMTPEQAMKQYMQKLTAFEHHEIFSYPEIYFLGLNAKKRQGMTGGPNNGGYDDDQGSYVQVPHDHVAYRYEVLKVIGKGSFGQVVKAYDHKVHQHVALKMVRNEKRFHRQAAEEIRILEHLRKQDKDNTMNVIHMLENFTFRNHICMTFELLSMNLYELIKKNKFQGFSLPLVRKFAHSILQCLDALHKNRIIHCDLKPENILLKQQGRSGIKVIDFGSSCYEHQRVYTYIQSRFYRAPEVILGARYGMPIDMWSLGCILAELLTGYPLLPGEDEGDQLACMIELLGMPSQKLLDASKRAKNFVSSKGYPRYCTVTTLSDGSVVLNGGRSRRGKLRGPPESREWGNALKGCDDPLFLDFLKQCLEWDPAVRMTPGQALRHPWLRRRLPKPPTGEKTSVKR</t>
+  </si>
+  <si>
+    <t>CAGCAGTTCCCGCAGTTCCACGTCAAGTCCGGCCTGCAGATCAAGAAGAACGCCATCATCGATGACTACAAGGTCACCAGCCAGGTCCTGGGGCTGGGCATCAACGGCAAAGTTTTGCAGATCTTCAACAAGAGGACCCAGGAGAAATTCGCCCTCAAAATGCTTCAGGACTGCCCCAAGGCCCGCAGGGAGGTGGAGCTGCACTGGCGGGCCTCCCAGTGCCCGCACATCGTACGGATCGTGGATGTGTACGAGAATCTGTACGCAGGGAGGAAGTGCCTGCTGATTGTCATGGAATGTTTGGACGGTGGAGAACTCTTTAGCCGAATCCAGGATCGAGGAGACCAGGCATTCACAGAAAGAGAAGCATCCGAAATCATGAAGAGCATCGGTGAGGCCATCCAGTATCTGCATTCAATCAACATTGCCCATCGGGATGTCAAGCCTGAGAATCTCTTATACACCTCCAAAAGGCCCAACGCCATCCTGAAACTCACTGACTTTGGCTTTGCCAAGGAAACCACCAGCCACAACTCTTTGACCACTCCTTGTTATACACCGTACTATGTGGCTCCAGAAGTGCTGGGTCCAGAGAAGTATGACAAGTCCTGTGACATGTGGTCCCTGGGTGTCATCATGTACATCCTGCTGTGTGGGTATCCCCCCTTCTACTCCAACCACGGCCTTGCCATCTCTCCGGGCATGAAGACTCGCATCCGAATGGGCCAGTATGAATTTCCCAACCCAGAATGGTCAGAAGTATCAGAGGAAGTGAAGATGCTCATTCGGAATCTGCTGAAAACAGAGCCCACCCAGAGAATGACCATCACCGAGTTTATGAACCACCCTTGGATCATGCAATCAACAAAGGTCCCTCAAACCCCACTGCACACCAGCCGGGTCCTGAAGGAGGACAAGGAGCGGTGGGAGGATGTCAAGGGGTGTCTTCATGACAAGAACAGCGACCAGGCC</t>
+  </si>
+  <si>
+    <t>CDK2_HUMAN_D0_4BCP_A</t>
+  </si>
+  <si>
+    <t>MP2K4_HUMAN_D0_3ALN_C</t>
+  </si>
+  <si>
+    <t>ACCACCTCACTTGAAGCTTTGCCCACAGGGACAGTGCTGACAGACAAGAGTGGGCGACAGTGGAAGCTGAAGTCCTTCCAGACCAGGGACAACCAGGGCATTCTCTATGAAGCTGCACCCACCTCCACCCTCACCTGTGACTCAGGACCACAGAAGCAAAAGTTCTCACTCAAACTGGATGCCAAGGATGGGCGCTTGTTCAATGAGCAGAACTTCTTCCAGCGGGCCGCCAAGCCTCTGCAAGTCAACAAGTGGAAGAAGCTGTACTCGACCCCACTGCTGGCCATCCCTACCTGCATGGGTTTCGGTGTTCACCAGGACAAATACAGGTTCTTGGTGTTACCCAGCCTGGGGAGGAGCCTTCAGTCGGCCCTGGATGTCAGCCCAAAGCATGTGCTGTCAGAGAGGTCTGTGCTGCAGGTGGCCTGCCGGCTGCTGGATGCCCTGGAGTTCCTCCATGAGAATGAGTATGTTCATGGAAATGTGACAGCTGAAAATATCTTTGTGGATCCAGAGGACCAGAGTCAGGTGACTTTGGCAGGCTATGGCTTCGCCTTCCGCTATTGCCCAAGTGGCAAACACGTGGCCTACGTGGAAGGCAGCAGGAGCCCTCACGAGGGGGACCTTGAGTTCATTAGCATGGACCTGCACAAGGGATGCGGGCCCTCCCGCCGCAGCGACCTCCAGAGCCTGGGCTACTGCATGCTGAAGTGGCTCTACGGGTTTCTGCCATGGACAAATTGCCTTCCCAACACTGAGGACATCATGAAGCAAAAACAGAAGTTTGTTGATAAGCCGGGGCCCTTCGTGGGACCCTGCGGTCACTGGATCAGGCCCTCAGAGACCCTGCAGAAGTACCTGAAGGTGGTGATGGCCCTCACGTATGAGGAGAAGCCGCCCTACGCCATGCTGAGGAACAACCTAGAAGCTTTGCTGCAGGATCTGCGTGTGTCTCCATATGACCCCATTGGCCTCCCGATGGTGCCC</t>
+  </si>
+  <si>
+    <t>TCACCACAGCGGGAGCCACAGCGAGTATCCCATGAGCAGTTCCGGGCTGCCCTGCAGCTGGTGGTGGACCCAGGCGACCCCCGCTCCTACCTGGACAACTTCATCAAGATTGGCGAGGGCTCCACGGGCATCGTGTGCATCGCCACCGTGCGCAGCTCGGGCAAGCTGGTGGCCGTCAAGAAGATGGACCTGCGCAAGCAGCAGAGGCGCGAGCTGCTCTTCAACGAGGTGGTAATCATGAGGGACTACCAGCACGAGAATGTGGTGGAGATGTACAACAGCTACCTGGTGGGGGACGAGCTCTGGGTGGTCATGGAGTTCCTGGAAGGAGGCGCCCTCACCGACATCGTCACCCACACCAGGATGAACGAGGAGCAGATCGCGGCCGTGTGCCTTGCAGTGCTGCAGGCCCTGTCGGTGCTCCACGCCCAGGGCGTCATCCACCGGGACATCAAGAGCGACTCGATCCTGCTGACCCATGATGGCAGGGTGAAGCTGTCAGACTTTGGGTTCTGCGCCCAGGTGAGCAAGGAAGTGCCCCGAAGGAAGTCGCTGGTCGGCACGCCCTACTGGATGGCCCCAGAGCTCATCTCCCGCCTTCCCTACGGGCCAGAGGTAGACATCTGGTCGCTGGGGATAATGGTGATTGAGATGGTGGACGGAGAGCCCCCCTACTTCAACGAGCCACCCCTCAAAGCCATGAAGATGATTCGGGACAACCTGCCACCCCGACTGAAGAACCTGCACAAGGTGTCGCCATCCCTGAAGGGCTTCCTGGACCGCCTGCTGGTGCGAGACCCTGCCCAGCGGGCCACGGCAGCCGAGCTGCTGAAGCACCCATTCCTGGCCAAGGCAGGGCCGCCTGCCAGCATCGTGCCCCTCATGCGCCAGAACCGCACCAGA</t>
+  </si>
+  <si>
+    <t>SIESSGKLKISPEQHWDFTAEDLKDLGEIGRGAYGSVNKMVHKPSGQIMAVKRIRSTVDEKEQKQLLMDLDVVMRSSDCPYIVQFYGALFREGDCWICMELMSTSFDKFYKYVYSVLDDVIPEEILGKITLATVKALNHLKENLKIIHRDIKPSNILLDRSGNIKLCDFGISGQLVDSIAKTRDAGCRPYMAPERIDPSASRQGYDVRSDVWSLGITLYELATGRFPYPKWNSVFDQLTQVVKGDPPQLSNSEEREFSPSFINFVNLCLTKDESKRPKYKELLKHPFILMYEERAVEVACYVCKILDQMPATPSSPMYVD</t>
+  </si>
+  <si>
+    <t>TDSFSGRFEDVYQLQEDVLGEGAHARVQTCINLITSQEYAVKIIEKQPGHIRSRVFREVEMLYQCQGHRNVLELIEFFEEEDRFYLVFEKMRGGSILSHIHKRRHFNELEASVVVQDVASALDFLHNKGIAHRDLKPENILCEHPNQVSPVKICDFDLGSGIKLNGDCSPISTPELLTPCGSAEYMAPEVVEAFSEEASIYDKRCDLWSLGVILYILLSGYPPFVGRCGSDCGWDRGEACPACQNMLFESIQEGKYEFPDKDWAHISCAAKDLISKLLVRDAKQRLSAAQVLQHPWVQGCAPENTLPTPMVLQR</t>
+  </si>
+  <si>
+    <t>ST17B_HUMAN_D0_3LM0_A</t>
+  </si>
+  <si>
+    <t>MPGPAAGSRARVYAEVNSLRSREYWDYEAHVPSWGNQDDYQLVRKLGRGKYSEVFEAINITNNERVVVKILKPVKKKKIKREVKILENLRGGTNIIKLIDTVKDPVSKTPALVFEYINNTDFKQLYQILTDFDIRFYMYELLKALDYCHSKGIMHRDVKPHNVMIDHQQKKLRLIDWGLAEFYHPAQEYNVRVASRYFKGPELLVDYQMYDYSLDMWSLGCMLASMIFRREPFFHGQDNYDQLVRIAKVLGTEELYGYLKKYHIDLDPHFNDILGQHSRKRWENFIHSENRHLVSPEALDLLDKLLRYDHQQRLTAKEAMEHPYFYPVVKEQSQ</t>
+  </si>
+  <si>
+    <t>AAGAGGCAGTGGGCTTTGGAAGACTTTGAAATTGGTCGCCCTCTGGGTAAAGGAAAGTTTGGTAATGTTTATTTGGCAAGAGAAAAGCAAAGCAAGTTTATTCTGGCTCTTAAAGTGTTATTTAAAGCTCAGCTGGAGAAAGCCGGAGTGGAGCATCAGCTCAGAAGAGAAGTAGAAATACAGTCCCACCTTCGGCATCCTAATATTCTTAGACTGTATGGTTATTTCCATGATGCTACCAGAGTCTACCTAATTCTGGAATATGCACCACTTGGAACAGTTTATAGAGAACTTCAGAAACTTTCAAAGTTTGATGAGCAGAGAACTGCTACTTATATAACAGAATTGGCAAATGCCCTGTCTTACTGTCATTCGAAGAGAGTTATTCATAGAGACATTAAGCCAGAGAACTTACTTCTTGGATCAGCTGGAGAGCTTAAAATTGCAGATTTTGGGTGGTCAGTACATGCTCCATCTTCCAGGAGGACCACTCTCTGTGGCACCCTGGACTACCTGCCCCCTGAAATGATTGAAGGTCGGATGCATGATGAGAAGGTGGATCTCTGGAGCCTTGGAGTTCTTTGCTATGAATTTTTAGTTGGGAAGCCTCCTTTTGAGGCAAACACATACCAAGAGACCTACAAAAGAATATCACGGGTTGAATTCACATTCCCTGACTTTGTAACAGAGGGAGCCAGGGACCTCATTTCAAGACTGTTGAAGCATAATCCCAGCCAGAGGCCAATGCTCAGAGAAGTACTTGAACACCCCTGGATCACAGCAAATTCATCAAAACCATCA</t>
+  </si>
+  <si>
+    <t>ATGGAGCTACGTGTGGGGAACAAGTACCGCCTGGGACGGAAGATCGGGAGCGGGTCCTTCGGAGATATCTACCTGGGTGCCAACATCGCCTCTGGTGAGGAAGTCGCCATCAAGCTGGAGTGTGTGAAGACAAAGCACCCCCAGCTGCACATCGAGAGCAAGTTCTACAAGATGATGCAGGGTGGCGTGGGGATCCCGTCCATCAAGTGGTGCGGAGCTGAGGGCGACTACAACGTGATGGTCATGGAGCTGCTGGGGCCTAGCCTCGAGGACCTGTTCAACTTCTGTTCCCGCAAATTCAGCCTCAAGACGGTGCTGCTCTTGGCCGACCAGATGATCAGCCGCATCGAGTATATCCACTCCAAGAACTTCATCCACCGGGACGTCAAGCCCGACAACTTCCTCATGGGGCTGGGGAAGAAGGGCAACCTGGTCTACATCATCGACTTCGGCCTGGCCAAGAAGTACCGGGACGCCCGCACCCACCAGCACATTCCCTACCGGGAAAACAAGAACCTGACCGGCACGGCCCGCTACGCTTCCATCAACACGCACCTGGGCATTGAGCAAAGCCGTCGAGATGACCTGGAGAGCCTGGGCTACGTGCTCATGTACTTCAACCTGGGCTCCCTGCCCTGGCAGGGGCTCAAAGCAGCCACCAAGCGCCAGAAGTATGAACGGATCAGCGAGAAGAAGATGTCAACGCCCATCGAGGTCCTCTGCAAAGGCTATCCCTCCGAATTCTCAACATACCTCAACTTCTGCCGCTCCCTGCGGTTTGACGACAAGCCCGACTACTCTTACCTACGTCAGCTCTTCCGCAACCTCTTCCACCGGCAGGGCTTCTCCTATGACTACGTCTTTGACTGGAACATGCTGAAA</t>
+  </si>
+  <si>
+    <t>MK03_HUMAN_D0_2ZOQ_B</t>
+  </si>
+  <si>
+    <t>ATGTCTCAGTCGAAAGGCAAGAAGCGAAACCCTGGCCTTAAAATTCCAAAAGAAGCATTTGAACAACCTCAGACCAGTTCCACACCACCTCGAGATTTAGACTCCAAGGCTTGCATTTCTATTGGAAATCAGAACTTTGAGGTGAAGGCAGATGACCTGGAGCCTATAATGGAACTGGGACGAGGTGCGTACGGGGTGGTGGAGAAGATGCGGCACGTGCCCAGCGGGCAGATCATGGCAGTGAAGCGGATCCGAGCCACAGTAAATAGCCAGGAACAGAAACGGCTACTGATGGATTTGGATATTTCCATGAGGACGGTGGACTGTCCATTCACTGTCACCTTTTATGGCGCACTGTTTCGGGAGGGTGATGTGTGGATCTGCATGGAGCTCATGGATACATCACTAGATAAATTCTACAAACAAGTTATTGATAAAGGCCAGACAATTCCAGAGGACATCTTAGGGAAAATAGCAGTTTCTATTGTAAAAGCATTAGAACATTTACATAGTAAGCTGTCTGTCATTCACAGAGACGTCAAGCCTTCTAATGTACTCATCAATGCTCTCGGTCAAGTGAAGATGTGCGATTTTGGAATCAGTGGCTACTTGGTGGACTCTGTTGCTAAAACAATTGATGCAGGTTGCAAACCATACATGGCCCCTGAAAGAATAAACCCAGAGCTCAACCAGAAGGGATACAGTGTGAAGTCTGACATTTGGAGTCTGGGCATCACGATGATTGAGTTGGCCATCCTTCGATTTCCCTATGATTCATGGGGAACTCCATTTCAGCAGCTCAAACAGGTGGTAGAGGAGCCATCGCCACAACTCCCAGCAGACAAGTTCTCTGCAGAGTTTGTTGACTTTACCTCACAGTGCTTAAAGAAGAATTCCAAAGAACGGCCTACATACCCAGAGCTAATGCAACATCCATTTTTCACCCTACATGAATCCAAAGGAACAGATGTGGCATCTTTTGTAAAACTGATTCTTGGAGAC</t>
+  </si>
+  <si>
+    <t>TCAACCAGGGATTATGAGATTCAAAGAGAAAGAATAGAACTTGGACGATGTATTGGAGAAGGCCAATTTGGAGATGTACATCAAGGCATTTATATGAGTCCAGAGAATCCAGCTTTGGCGGTTGCAATTAAAACATGTAAAAACTGTACTTCGGACAGCGTGAGAGAGAAATTTCTTCAAGAAGCCTTAACAATGCGTCAGTTTGACCATCCTCATATTGTGAAGCTGATTGGAGTCATCACAGAGAATCCTGTCTGGATAATCATGGAGCTGTGCACACTTGGAGAGCTGAGGTCATTTTTGCAAGTAAGGAAATACAGTTTGGATCTAGCATCTTTGATCCTGTATGCCTATCAGCTTAGTACAGCTCTTGCATATCTAGAGAGCAAAAGATTTGTACACAGGGACATTGCTGCTCGGAATGTTCTGGTGTCCTCAAATGATTGTGTAAAATTAGGAGACTTTGGATTATCCCGATATATGGAAGATAGTACTTACTACAAAGCTTCCAAAGGAAAATTGCCTATTAAATGGATGGCTCCAGAGTCAATCAATTTTCGACGTTTTACCTCAGCTAGTGACGTATGGATGTTTGGTGTGTGTATGTGGGAGATACTGATGCATGGTGTGAAGCCTTTTCAAGGAGTGAAGAACAATGATGTAATCGGTCGAATTGAAAATGGGGAAAGATTACCAATGCCTCCAAATTGTCCTCCTACCCTCTACAGCCTTATGACGAAATGCTGGGCCTATGACCCCAGCAGGCGGCCCAGGTTTACTGAACTTAAAGCTCAGCTCAGCACAATCCTGGAGGAAGAGAAGGCTCAGCAAGAAGAG</t>
+  </si>
+  <si>
+    <t>DPEELFTKLEKIGKGSFGEVFKGIDNRTQKVVAIKIIDLEEAEDEIEDIQQEITVLSQCDSPYVTKYYGSYLKDTKLWIIMEYLGGGSALDLLEPGPLDETQIATILREILKGLDYLHSEKKIHRDIKAANVLLSEHGEVKLADFGVAGQLTDTQIKRNTFVGTPFWMAPEVIKQSAYDSKADIWSLGITAIELARGEPPHSELHPMKVLFLIPKNNPPTLEGNYSKPLKEFVEACLNKEPSFRPTAKELLKHKFILRNAKKTSYLTELID</t>
+  </si>
+  <si>
+    <t>MAPK3_HUMAN_D0_3FXW_A</t>
+  </si>
+  <si>
+    <t>AAGCAGTACGAACACGTGAAGAGGGACCTGAACCCCGAAGACTTTTGGGAGATTATAGGAGAACTGGGCGACGGAGCCTTTGGGAAAGTGTACAAGGCCCAGAATAAAGAGACCAGTGTTTTAGCTGCTGCAAAAGTGATTGACACTAAATCTGAAGAAGAACTTGAAGATTACATGGTAGAGATTGACATATTAGCATCTTGTGATCACCCAAATATAGTCAAGCTTCTAGATGCCTTCTATTATGAGAACAATCTTTGGATCCTCATTGAATTTTGTGCAGGTGGAGCAGTAGATGCTGTGATGCTTGAACTTGAGAGACCATTAACTGAGTCCCAAATACAAGTAGTTTGCAAGCAGACTTTAGATGCATTGAACTACTTACATGATAATAAGATCATCCACAGAGATCTGAAGGCTGGCAACATTCTCTTTACCTTAGATGGAGATATCAAATTGGCGGATTTTGGAGTATCAGCTAAAAACATGAGGACAATTCAAAGAAGAGATTCCTTTATTGGTACACCATATTGGATGGCTCCTGAAGTAGTCATGTGTGAAACATCTAAGGACAGACCCTATGACTACAAAGCTGATGTTTGGTCCCTGGGTATCACTTTAATAGAAATGGCTGAGATAGAACCACCTCATCATGAATTAAATCCAATGCGAGTGCTGCTAAAAATAGCAAAATCTGAGCCACCTACATTAGCACAGCCATCCAGATGGTCTTCAAATTTTAAGGACTTTCTAAAGAAATGCTTAGAAAAGAATGTGGATGCCAGGTGGACTACATCTCAGCTGCTGCAGCATCCCTTTGTTACTGTTGATTCCAACAAACCCATCCGAGAATTGATTGCAGAGGCGAAGGCTGAAGTAACAGAAGAAGTTGAAGATGGCAAAGAG</t>
+  </si>
+  <si>
+    <t>ATGCCTTCCCGGGCTGAGGACTATGAAGTGTTGTACACCATTGGCACAGGCTCCTACGGCCGCTGCCAGAAGATCCGGAGGAAGAGTGATGGCAAGATATTAGTTTGGAAAGAACTTGACTATGGCTCCATGACAGAAGCTGAGAAACAGATGCTTGTTTCTGAAGTGAATTTGCTTCGTGAACTGAAACATCCAAACATCGTTCGTTACTATGATCGGATTATTGACCGGACCAATACAACACTGTACATTGTAATGGAATATTGTGAAGGAGGGGATCTGGCTAGTGTAATTACAAAGGGAACCAAGGAAAGGCAATACTTAGATGAAGAGTTTGTTCTTCGAGTGATGACTCAGTTGACTCTGGCCCTGAAGGAATGCCACAGACGAAGTGATGGTGGTCATACCGTATTGCATCGGGATCTGAAACCAGCCAATGTTTTCCTGGATGGCAAGCAAAACGTCAAGCTTGGAGACTTTGGGCTAGCTAGAATATTAAACCATGACACGAGTTTTGCAAAAACATTTGTTGGCACACCTTATTACATGTCTCCTGAACAAATGAATCGCATGTCCTACAATGAGAAATCAGATATCTGGTCATTGGGCTGCTTGCTGTATGAGTTATGTGCATTAATGCCTCCATTTACAGCTTTTAGCCAGAAAGAACTCGCTGGGAAAATCAGAGAAGGCAAATTCAGGCGAATTCCATACCGTTACTCTGATGAATTGAATGAAATTATTACGAGGATGTTAAACTTAAAGGATTACCATCGACCTTCTGTTGAAGAAATTCTTGAGAACCCTTTAATA</t>
+  </si>
+  <si>
+    <t>STK3_HUMAN_D0_4LG4_B</t>
+  </si>
+  <si>
+    <t>CACCAGCTGCAGCCCCGGCGGGTGTCATTCCGGGGCGAGGCCTCAGAGACTCTGCAGAGCCCTGGGTATGACCCAAGCCGGCCAGAGTCCTTCTTCCAGCAGAGCTTCCAGAGGCTCAGCCGCCTGGGCCATGGCTCCTACGGAGAGGTCTTCAAGGTGCGCTCCAAGGAGGACGGCCGGCTCTATGCGGTAAAGCGTTCCATGTCACCATTCCGGGGCCCCAAGGACCGGGCCCGCAAGTTGGCCGAGGTGGGCAGCCACGAGAAGGTGGGGCAGCACCCATGCTGCGTGCGGCTGGAGCAGGCCTGGGAGGAGGGCGGCATCCTGTACCTGCAGACGGAGCTGTGCGGGCCCAGCCTGCAGCAACACTGTGAGGCCTGGGGTGCCAGCCTGCCTGAGGCCCAGGTCTGGGGCTACCTGCGGGACACGCTGCTTGCCCTGGCCCATCTGCACAGCCAGGGCCTGGTGCACCTTGATGTCAAGCCTGCCAACATCTTCCTGGGGCCCCGGGGCCGCTGCAAGCTGGGTGACTTCGGACTGCTGGTGGAGCTGGGTACAGCAGGAGCTGGTGAGGTCCAGGAGGGAGACCCCCGCTACATGGCCCCCGAGCTGCTGCAGGGCTCCTATGGGACAGCAGCGGATGTGTTCAGTCTGGGCCTCACCATCCTGGAAGTGGCATGCAACATGGAGCTGCCCCACGGTGGGGAGGGCTGGCAGCAGCTGCGCCAGGGCTACCTGCCCCCTGAGTTCACTGCCGGTCTGTCTTCCGAGCTGCGTTCTGTCCTTGTCATGATGCTGGAGCCAGACCCCAAGCTGCGGGCCACGGCCGAGGCCCTGCTGGCACTGCCTGTGTTGAGGCAGCCG</t>
+  </si>
+  <si>
+    <t>KEKEPLESQYQVGPLLGSGGFGSVYSGIRVSDNLPVAIKHVEKDRISDWGELPNGTRVPMEVVLLKKVSSGFSGVIRLLDWFERPDSFVLILERPEPVQDLFDFITERGALQEELARSFFWQVLEAVRHCHNCGVLHRDIKDENILIDLNRGELKLIDFGSGALLKDTVYTDFDGTRVYSPPEWIRYHRYHGRSAAVWSLGILLYDMVCGDIPFEHDEEIIGGQVFFRQRVSSECQHLIRWCLALRPSDRPTFEEIQNHPWMQDVLLPQETAEIHLHSLSPGPSK</t>
+  </si>
+  <si>
+    <t>VEDHYEMGEELGSGQFAIVRKCRQKGTGKEYAAKFIKKRRLSSSRRGVSREEIEREVNILREIRHPNIITLHDIFENKTDVVLILELVSGGELFDFLAEKESLTEDEATQFLKQILDGVHYLHSKRIAHFDLKPENIMLLDKNVPNPRIKLIDFGIAHKIEAGNEFKNIFGTPEFVAPEIVNYEPLGLEADMWSIGVITYILLSGASPFLGETKQETLTNISAVNYDFDEEYFSNTSELAKDFIRRLLVKDPKRRMTIAQSLEHSWIKAIRRRNVRGEDSG</t>
   </si>
   <si>
     <t>ACCGACAGCTTCTCGGGCAGGTTTGAAGACGTCTACCAGCTGCAGGAAGATGTGCTGGGGGAGGGCGCTCATGCCCGAGTGCAGACCTGCATCAACCTGATCACCAGCCAGGAGTACGCCGTCAAGATCATTGAGAAGCAGCCAGGCCACATTCGGAGCAGGGTTTTCAGGGAGGTGGAGATGCTGTACCAGTGCCAGGGACACAGGAACGTCCTAGAGCTGATTGAGTTCTTCGAGGAGGAGGACCGCTTCTACCTGGTGTTTGAGAAGATGCGGGGAGGCTCCATCCTGAGCCACATCCACAAGCGCCGGCACTTCAACGAGCTGGAGGCCAGCGTGGTGGTGCAGGACGTGGCCAGCGCCTTGGACTTTCTGCATAACAAAGGCATCGCCCACAGGGACCTAAAGCCGGAAAACATCCTCTGTGAGCACCCCAACCAGGTCTCCCCCGTGAAGATCTGTGACTTCGACCTGGGCAGCGGCATCAAACTCAACGGGGACTGCTCCCCTATCTCCACCCCGGAGCTGCTCACTCCGTGCGGCTCGGCGGAGTACATGGCCCCGGAGGTAGTGGAGGCCTTCAGCGAGGAGGCTAGCATCTACGACAAGCGCTGCGACCTGTGGAGCCTGGGCGTCATCTTGTATATCCTACTCAGCGGCTACCCGCCCTTCGTGGGCCGCTGTGGCAGCGACTGCGGCTGGGACCGCGGCGAGGCCTGCCCTGCCTGCCAGAACATGCTGTTTGAGAGCATCCAGGAGGGCAAGTACGAGTTCCCCGACAAGGACTGGGCCCACATCTCCTGCGCTGCCAAAGACCTCATCTCCAAGCTGCTGGTCCGTGACGCCAAGCAGAGGCTGAGTGCCGCCCAAGTCCTGCAGCACCCCTGGGTTCAGGGGTGCGCCCCGGAGAACACCTTGCCCACTCCCATGGTCCTGCAGAGG</t>
   </si>
   <si>
-    <t>MSRSKRDNNFYSVEIGDSTFTVLKRYQNLKPIGSGAQGIVCAAYDAILERNVAIKKLSRPFQNQTHAKRAYRELVLMKCVNHKNIIGLLNVFTPQKSLEEFQDVYIVMELMDANLCQVIQMELDHERMSYLLYQMLCGIKHLHSAGIIHRDLKPSNIVVKSDCTLKILDFGLARTAGTSFMMTPYVVTRYYRAPEVILGMGYKENVDLWSVGCIMGEMVCHKILFPGRDYIDQWNKVIEQLGTPCPEFMKKLQPTVRTYVENRPKYAGYSFEKLFPDVLFPADSEHNKLKASQARDLLSKMLVIDASKRISVDEALQHPYINVWYDPSEAEAPPPKIPDKQLDEREHTIEEWKELIYKEVMDLE</t>
-  </si>
-  <si>
-    <t>STRAA_HUMAN_D0_3GNI_B</t>
-  </si>
-  <si>
-    <t>MP2K2_HUMAN_D0_1S9I_A</t>
-  </si>
-  <si>
-    <t>PIM1_HUMAN_D0_4A7C_A</t>
-  </si>
-  <si>
-    <t>EAFLTQKAKVGELKDDDFERISELGAGNGGVVTKVQHRPSGLIMARKLIHLEIKPAIRNQIIRELQVLHECNSPYIVGFYGAFYSDGEISICMEHMDGGSLDQVLKEAKRIPEEILGKVSIAVLRGLAYLREKHQIMHRDVKPSNILVNSRGEIKLCDFGVSGQLIDSMANSFVGTRSYMAPERLQGTHYSVQSDIWSMGLSLVELAVGRYPIPPPDAKELEAIFGRPVVDGEEGEPHSISPRPRPPGRPVSGHGMDSRPAMAIFELLDYIVNEPPPKLPNGVFTPDFQEFVNKCLIKNPAERADLKMLTNHTFIKRSEVEEVDFAGWLCKTLRLNQPGTPTRTAV</t>
-  </si>
-  <si>
-    <t>GGGCCGGAGGATGAGCTGCCCGACTGGGCCGCCGCCAAAGAGTTTTACCAGAAGTACGACCCTAAGGACGTCATCGGCAGAGGAGTGAGCTCTGTGGTCCGCCGTTGTGTTCATCGAGCTACTGGCCACGAGTTTGCGGTGAAGATTATGGAAGTGACAGCTGAGCGGCTGAGTCCTGAGCAGCTGGAGGAGGTGCGGGAAGCCACACGGCGAGAGACACACATCCTTCGCCAGGTCGCCGGCCACCCCCACATCATCACCCTCATCGATTCCTACGAGTCTTCTAGCTTCATGTTCCTGGTGTTTGACCTGATGCGGAAGGGAGAGCTGTTTGACTATCTCACAGAGAAGGTGGCCCTCTCTGAAAAGGAAACCAGGTCCATCATGCGGTCTCTGCTGGAAGCAGTGAGCTTTCTCCATGCCAACAACATTGTGCATCGAGATCTGAAGCCCGAGAATATTCTCCTAGATGACAATATGCAGATCCGACTTTCAGATTTCGGGTTCTCCTGCCACTTGGAACCTGGCGAGAAGCTTCGAGAGTTGTGTGGGACCCCAGGGTATCTAGCGCCAGAGATCCTTAAATGCTCCATGGATGAAACCCACCCAGGCTATGGCAAGGAGGTCGACCTCTGGGCCTGTGGGGTGATCTTGTTCACACTCCTGGCTGGCTCGCCACCCTTCTGGCACCGGCGGCAGATCCTGATGTTACGCATGATCATGGAGGGCCAGTACCAGTTCAGTTCCCCCGAGTGGGATGACCGTTCCAGCACTGTCAAAGACCTGATCTCCAGGCTGCTGCAGGTGGATCCTGAGGCACGCCTGACAGCTGAGCAGGCCCTACAGCACCCCTTCTTTGAGCGT</t>
-  </si>
-  <si>
-    <t>KC1E_HUMAN_D0_4HNI_A</t>
-  </si>
-  <si>
-    <t>VRK2_HUMAN_D0_2V62_B</t>
-  </si>
-  <si>
-    <t>ETYIKLDKLGEGTYATVYKGKSKLTDNLVALKEIRLEHEEGAPCTAIREVSLLKDLKHANIVTLHDIIHTEKSLTLVFEYLDKDLKQYLDDCGNIINMHNVKLFLFQLLRGLAYCHRQKVLHRDLKPQNLLINERGELKLADFGLARAKSIPTKTYSNEVVTLWYRPPDILLGSTDYSTQIDMWGVGCIFYEMATGRPLFPGSTVEEQLHFIFRILGTPTEETWPGILSNEEFKTYNYPKYRAEALLSHAPRLDSDGADLLTKLLQFEGRNRISAEDAMKHPFFLSLGERIHKLPDTTSIFALKEIQLQKEASLRS</t>
-  </si>
-  <si>
-    <t>HQLQPRRVSFRGEASETLQSPGYDPSRPESFFQQSFQRLSRLGHGSYGEVFKVRSKEDGRLYAVKRSMSPFRGPKDRARKLAEVGSHEKVGQHPCCVRLEQAWEEGGILYLQTELCGPSLQQHCEAWGASLPEAQVWGYLRDTLLALAHLHSQGLVHLDVKPANIFLGPRGRCKLGDFGLLVELGTAGAGEVQEGDPRYMAPELLQGSYGTAADVFSLGLTILEVACNMELPHGGEGWQQLRQGYLPPEFTAGLSSELRSVLVMMLEPDPKLRATAEALLALPVLRQP</t>
-  </si>
-  <si>
-    <t>aa_end</t>
-  </si>
-  <si>
-    <t>PMYT1_HUMAN_D0_3P1A_A</t>
-  </si>
-  <si>
-    <t>MK08_HUMAN_D0_2NO3_A</t>
-  </si>
-  <si>
-    <t>TCGGTTAAAGGAAGAATTTATTCCATATTAAAGCAGATAGGAAGTGGAGGTTCAAGCAAGGTATTTCAGGTGTTAAATGAAAAGAAACAGATATATGCTATAAAATATGTGAACTTAGAAGAAGCAGATAACCAAACTCTTGATAGTTACCGGAACGAAATAGCTTATTTGAATAAACTACAACAACACAGTGATAAGATCATCCGACTTTATGATTATGAAATCACGGACCAGTACATCTACATGGTAATGGAGTGTGGAAATATTGATCTTAATAGTTGGCTTAAAAAGAAAAAATCCATTGATCCATGGGAACGCAAGAGTTACTGGAAAAATATGTTAGAGGCAGTTCACACAATCCATCAACATGGCATTGTTCACAGTGATCTTAAACCAGCTAACTTTCTGATAGTTGATGGAATGCTAAAGCTAATTGATTTTGGGATTGCAAACCAAATGCAACCAGATACAACAAGTGTTGTTAAAGATTCTCAGGTTGGCACAGTTAATTATATGCCACCAGAAGCAATCAAAGATATGTCTTCCTCCAGAGAGAATGGGAAATCTAAGTCAAAGATAAGCCCCAAAAGTGATGTTTGGTCCTTAGGATGTATTTTGTACTATATGACTTACGGGAAAACACCATTTCAGCAGATAATTAATCAGATTTCTAAATTACATGCCATAATTGATCCTAATCATGAAATTGAATTTCCCGATATTCCAGAGAAAGATCTTCAAGATGTGTTAAAGTGTTGTTTAAAAAGGGACCCAAAACAGAGGATATCCATTCCTGAGCTCCTGGCTCATCCATATGTTCAAATTCAAACTCATCCAGTTAACCAAATGGCCAAGGGAACCACTGAAGAA</t>
-  </si>
-  <si>
-    <t>PAK1_HUMAN_D0_3Q52_A</t>
-  </si>
-  <si>
-    <t>CDK9_HUMAN_D0_4IMY_A</t>
-  </si>
-  <si>
-    <t>GAAACAAAGTATACTGTGGACAAGAGGTTTGGCATGGATTTTAAAGAAATAGAATTAATTGGCTCAGGTGGATTTGGCCAAGTTTTCAAAGCAAAACACAGAATTGACGGAAAGACTTACGTTATTAAACGTGTTAAATATAATAACGAGAAGGCGGAGCGTGAAGTAAAAGCATTGGCAAAACTTGATCATGTAAATATTGTTCACTACAATGGCTGTTGGGATGGATTTGATTATGATCCTGAGACCAGTGATGATTCTCTTGAGAGCAGTGATTATGATCCTGAGAACAGCAAAAATAGTTCAAGGTCAAAGACTAAGTGCCTTTTCATCCAAATGGAATTCTGTGATAAAGGGACCTTGGAACAATGGATTGAAAAAAGAAGAGGCGAGAAACTAGACAAAGTTTTGGCTTTGGAACTCTTTGAACAAATAACAAAAGGGGTGGATTATATACATTCAAAAAAATTAATTCATAGAGATCTTAAGCCAAGTAATATATTCTTAGTAGATACAAAACAAGTAAAGATTGGAGACTTTGGACTTGTAACATCTCTGAAAAATGATGGAAAGCGAACAAGGAGTAAGGGAACTTTGCGATACATGAGCCCAGAACAGATTTCTTCGCAAGACTATGGAAAGGAAGTGGACCTCTACGCTTTGGGGCTAATTCTTGCTGAACTTCTTCATGTATGTGACACTGCTTTTGAAACATCAAAGTTTTTCACAGACCTACGGGATGGCATCATCTCAGATATATTTGATAAAAAAGAAAAAACTCTTCTACAGAAATTACTCTCAAAGAAACCTGAGGATCGACCTAACACATCTGAAATACTAAGGACCTTGACTGTGTGGAAGAAAAGCCCAGAGAAAAATGAACGACACACATGT</t>
-  </si>
-  <si>
-    <t>PAK7_HUMAN_D0_2F57_B</t>
-  </si>
-  <si>
-    <t>expression tag location</t>
-  </si>
-  <si>
-    <t>GAGAACTTCCAAAAGGTGGAAAAGATCGGAGAGGGCACGTACGGAGTTGTGTACAAAGCCAGAAACAAGTTGACGGGAGAGGTGGTGGCGCTTAAGAAAATCCGCCTGGACACTGAGACTGAGGGTGTGCCCAGTACTGCCATCCGAGAGATCTCTCTGCTTAAGGAGCTTAACCATCCTAATATTGTCAAGCTGCTGGATGTCATTCACACAGAAAATAAACTCTACCTGGTTTTTGAATTTCTGCACCAAGATCTCAAGAAATTCATGGATGCCTCTGCTCTCACTGGCATTCCTCTTCCCCTCATCAAGAGCTATCTGTTCCAGCTGCTCCAGGGCCTAGCTTTCTGCCATTCTCATCGGGTCCTCCACCGAGACCTTAAACCTCAGAATCTGCTTATTAACACAGAGGGGGCCATCAAGCTAGCAGACTTTGGACTAGCCAGAGCTTTTGGAGTCCCTGTTCGTACTTACACCCATGAGGTGGTGACCCTGTGGTACCGAGCTCCTGAAATCCTCCTGGGCTGCAAATATTATTCCACAGCTGTGGACATCTGGAGCCTGGGCTGCATCTTTGCTGAGATGGTGACTCGCCGGGCCCTATTCCCTGGAGATTCTGAGATTGACCAGCTCTTCCGGATCTTTCGGACTCTGGGGACCCCAGATGAGGTGGTGTGGCCAGGAGTTACTTCTATGCCTGATTACAAGCCAAGTTTCCCCAAGTGGGCCCGGCAAGATTTTAGTAAAGTTGTACCTCCCCTGGATGAAGATGGACGGAGCTTGTTATCGCAAATGCTGCACTACGACCCTAACAAGCGGATTTCGGCCAAGGCAGCCCTGGCTCACCCTTTCTTCCAGGATGTGACCAAGCCAGTACCCCATCTT</t>
-  </si>
-  <si>
-    <t>GGGGAATGCAGTCAGAAGGGTCCTGTCCCCTTTAGCCATTGCCTTCCCACAGAAAAACTGCAACGCTGTGAGAAGATTGGGGAAGGGGTGTTTGGCGAAGTGTTTCAAACAATTGCTGATCACACACCCGTAGCCATAAAAATCATTGCTATTGAAGGACCAGATTTAGTCAATGGATCCCATCAGAAAACCTTTGAGGAAATCCTGCCAGAGATCATCATCTCCAAAGAGTTGAGCCTCTTATCCGGTGAAGTGTGCAACCGCACAGAAGGCTTTATCGGGCTGAACTCAGTGCACTGTGTCCAGGGATCTTACCCTCCCTTGCTCCTCAAAGCCTGGGATCACTATAATTCAACCAAAGGCTCTGCAAATGACCGGCCTGATTTTTTTAAAGACGACCAGCTCTTCATTGTGCTGGAATTTGAGTTTGGAGGGATTGACTTAGAGCAAATGCGAACCAAGTTGTCTTCCTTGGCTACTGCAAAGAGCATTCTACACCAGCTCACAGCCTCCCTCGCAGTGGCAGAGGCATCACTGCGCTTTGAGCACCGAGACTTACACTGGGGGAACGTGCTCTTAAAGAAAACCAGCCTCAAAAAACTCCACTACACCCTCAATGGGAAGAGCAGCACTATCCCCAGCTGTGGGTTGCAAGTGAGCATCATTGACTACACCCTGTCGCGCTTGGAACGGGATGGGATTGTGGTTTTCTGTGACGTTTCCATGGATGAGGACCTGTTTACCGGTGACGGTGACTACCAGTTTGACATCTACAGGCTCATGAAGAAGGAGAATAACAACCGCTGGGGTGAATATCACCCTTATAGTAATGTGCTCTGGTTACATTACCTGACAGACAAGATGCTGAAACAAATGACCTTCAAGACTAAATGTAACACTCCTGCCATGAAGCAAATTAAGAGAAAAATCCAGGAGTTCCACAGGACAATGCTGAACTTCAGCTCTGCCACTGACTTGCTCTGCCAGCACAGACTGTTTAAG</t>
-  </si>
-  <si>
-    <t>TDSLPGKFEDMYKLTSELLGEGAYAKVQGAVSLQNGKEYAVKIIEKQAGHSRSRVFREVETLYQCQGNKNILELIEFFEDDTRFYLVFEKLQGGSILAHIQKQKHFNEREASRVVRDVAAALDFLHTKDKVSLCHLGGSARAPSGLTAAPTSLGSSDPPTSASQVAGTTGIDHRDLKPENILCESPEKVSPVKICDFDLGSGMKLNNSCTPITTPELTTPCGSAEYMAPEVGEVFTDQATFYDKRCDLWSLGVVLYIMLSGYPPFVGHCGADCGWDRGEVCRVCQNKLFESIQEGKYEFPDKDWAHISSEAKDLISKLLVRDAKQRLSAAQVLQHPWVQGQAPEKG</t>
-  </si>
-  <si>
-    <t>VRK3_HUMAN_D0_2JII_A</t>
-  </si>
-  <si>
-    <t>ATGAGCCTCATCCGGAAAAAGGGCTTCTACAAGCAGGACGTCAACAAGACCGCCTGGGAGCTGCCCAAGACCTACGTGTCCCCGACGCACGTCGGCAGCGGGGCCTATGGCTCCGTGTGCTCGGCCATCGACAAGCGGTCAGGGGAGAAGGTGGCCATCAAGAAGCTGAGCCGACCCTTTCAGTCCGAGATCTTCGCCAAGCGCGCCTACCGGGAGCTGCTGCTGCTGAAGCACATGCAGCATGAGAACGTCATTGGGCTCCTGGATGTCTTCACCCCAGCCTCCTCCCTGCGCAACTTCTATGACTTCTACCTGGTGATGCCCTTCATGCAGACGGATCTGCAGAAGATCATGGGGATGGAGTTCAGTGAGGAGAAGATCCAGTACCTGGTGTATCAGATGCTCAAAGGCCTTAAGTACATCCACTCTGCTGGGGTCGTGCACAGGGACCTGAAGCCAGGCAACCTGGCTGTGAATGAGGACTGTGAACTGAAGATTCTGGATTTTGGGCTGGCGCGACATGCAGACGCCGAGATGACTGGCTACGTGGTGACCCGCTGGTACCGAGCCCCCGAGGTGATCCTCAGCTGGATGCACTACAACCAGACAGTGGACATCTGGTCTGTGGTCTGTATCATGGCAGAGATGCTGACAGGGAAAACTCTGTTCAAGGGGAAAGATTACCTGGACCAGCTGACCCAGATCCTGAAAGTGACCGGGGTGCCTGGCACGGAGTTTGTGCAGAAGCTGAACGACAAAGCGGCCAAATCCTACATCCAGTCCCTGCCACAGACCCCCAGGAAGGATTTCACTCAGCTGTTCCCACGGGCCAGCCCCCAGGCTGCGGACCTGCTGGAGAAGATGCTGGAGCTAGACGTGGACAAGCGCCTGACGGCCGCGCAGGCCCTCACCCATCCCTTCTTTGAACCCTTCCGGGACCCTGAGGAAGAGACGGAGGCCCAGCAGCCGTTTGATGATTCCTTAGAACACGAGAAACTCACAGTGGATGAATGGAAGCAGCACATCTACAAGGAGATTGTGAACTTCAGCCCCATT</t>
+    <t>MET_HUMAN_D0_4EEV_A</t>
+  </si>
+  <si>
+    <t>MSSFLPEGGCYELLTVIGKGFEDLMTVNLARYKPTGEYVTVRRINLEACSNEMVTFLQGELHVSKLFNHPNIVPYRATFIADNELWVVTSFMAYGSAKDLICTHFMDGMNELAIAYILQGVLKALDYIHHMGYVHRSVKASHILISVDGKVYLSGLRSNLSMISHGQRQRVVHDFPKYSVKVLPWLSPEVLQQNLQGYDAKSDIYSVGITACELANGHVPFKDMPATQMLLEKLNGTVPCLLDTSTIPAEELTMSPSRSVANSGLSDSLTTSTPRPSNGDSPSHPYHRTFSPHFHHFVEQCLQRNPDARPSASTLLNHSFFKQIKRRASEVLPELLRPVTPITNFEGSQSQDHSGIFGLVTNLEELEVDDWEF</t>
+  </si>
+  <si>
+    <t>MP2K1_HUMAN_D0_3MBL_A</t>
+  </si>
+  <si>
+    <t>ETKYTVDKRFGMDFKEIELIGSGGFGQVFKAKHRIDGKTYVIKRVKYNNEKAEREVKALAKLDHVNIVHYNGCWDGFDYDPETSDDSLESSDYDPENSKNSSRSKTKCLFIQMEFCDKGTLEQWIEKRRGEKLDKVLALELFEQITKGVDYIHSKKLIHRDLKPSNIFLVDTKQVKIGDFGLVTSLKNDGKRTRSKGTLRYMSPEQISSQDYGKEVDLYALGLILAELLHVCDTAFETSKFFTDLRDGIISDIFDKKEKTLLQKLLSKKPEDRPNTSEILRTLTVWKKSPEKNERHTC</t>
+  </si>
+  <si>
+    <t>CDKL1_HUMAN_D0_4AGU_C</t>
+  </si>
+  <si>
+    <t>MARK3_HUMAN_D0_2QNJ_A</t>
+  </si>
+  <si>
+    <t>MSGPRAGFYRQELNKTVWEVPQRLQGLRPVGSGAYGSVCSAYDARLRQKVAVKKLSRPFQSLIHARRTYRELRLLKHLKHENVIGLLDVFTPATSIEDFSEVYLVTTLMGADLNNIVKCQALSDEHVQFLVYQLLRGLKYIHSAGIIHRDLKPSNVAVNEDCELRILDFGLARQADEEMTGYVATRWYRAPEIMLNWMHYNQTVDIWSVGCIMAELLQGKALFPGSDYIDQLKRIMEVVGTPSPEVLAKISSEHARTYIQSLPPMPQKDLSSIFRGANPLAIDLLGRMLVLDSDQRVSAAEALAHAYFSQYHDPEDEPEAEPYDESVEAKERTLEEWKELTYQEVLSFKPPEPPKPPGSLEIEQ</t>
+  </si>
+  <si>
+    <t>NLVFSDGYVVKETIGVGSYSECKRCVHKATNMEYAVKVIDKSKRDPSEEIEILLRYGQHPNIITLKDVYDDGKHVYLVTELMRGGELLDKILRQKFFSEREASFVLHTIGKTVEYLHSQGVVHRDLKPSNILYVDESGNPECLRICDFGFAKQLRAENGLLMTPCYTANFVAPEVLKRQGYDEGCDIWSLGILLYTMLAGYTPFANGPSDTPEEILTRIGSGKFTLSGGNWNTVSETAKDLVSKMLHVDPHQRLTAKQVLQHPWVTQKDKLPQSQLSHQDLQLVKGAMAATYSALNSSKPTPQLKPIESSILAQRRVRKLPSTTL</t>
+  </si>
+  <si>
+    <t>GGTGTTGTGACACATGAGCAGTTCAAGGCTGCGCTCAGGATGGTGGTGGACCAGGGTGACCCCCGGCTGCTGCTGGACAGCTACGTGAAGATTGGCGAGGGCTCCACCGGCATCGTCTGCTTGGCCCGGGAGAAGCACTCGGGCCGCCAGGTGGCCGTCAAGATGATGGACCTCAGGAAGCAGCAGCGCAGGGAGCTGCTCTTCAACGAGGTGGTGATCATGCGGGACTACCAGCACTTCAACGTGGTGGAGATGTACAAGAGCTACCTGGTGGGCGAGGAGCTGTGGGTGCTCATGGAGTTCCTGCAGGGAGGAGCCCTCACAGACATCGTCTCCCAAGTCAGGCTGAATGAGGAGCAGATTGCCACTGTGTGTGAGGCTGTGCTGCAGGCCCTGGCCTACCTGCATGCTCAGGGTGTCATCCACCGGGACATCAAGAGTGACTCCATCCTGCTGACCCTCGATGGCAGGGTGAAGCTCTCGGACTTCGGATTCTGTGCTCAGATCAGCAAAGACGTCCCTAAGAGGAAGTCCCTGGTGGGAACCCCCTACTGGATGGCTCCTGAAGTGATCTCCAGGTCTTTGTATGCCACTGAGGTGGATATCTGGTCTCTGGGCATCATGGTGATTGAGATGGTAGATGGGGAGCCACCGTACTTCAGTGACTCCCCAGTGCAAGCCATGAAGAGGCTCCGGGACAGCCCCCCACCCAAGCTGAAAAACTCTCACAAGGTCTCCCCAGTGCTGCGAGACTTCCTGGAGCGGATGCTGGTGCGGGACCCCCAAGAGAGAGCCACAGCCCAGGAGCTCCTAGACCACCCCTTCCTGCTGCAGACAGGGCTACCTGAGTGCCTGGTGCCCCTGATCCAGCTCTACCGAAAGCAGACCTCCACCTGC</t>
+  </si>
+  <si>
+    <t>CACATTGGAAACTACCGGCTCCTCAAGACCATTGGCAAGGGTAATTTTGCCAAGGTGAAGTTGGCCCGACACATCCTGACTGGGAAAGAGGTAGCTGTGAAGATCATTGACAAGACTCAACTGAACTCCTCCAGCCTCCAGAAACTATTCCGCGAAGTAAGAATAATGAAGGTTTTGAATCATCCCAACATAGTTAAATTATTTGAAGTGATTGAGACTGAGAAAACGCTCTACCTTGTCATGGAGTACGCTAGTGGCGGAGAGGTATTTGATTACCTAGTGGCTCATGGCAGGATGAAAGAAAAAGAGGCTCGAGCCAAATTCCGCCAGATAGTGTCTGCTGTGCAGTACTGTCACCAGAAGTTTATTGTCCATAGAGACTTAAAGGCAGAAAACCTGCTCTTGGATGCTGATATGAACATCAAGATTGCAGACTTTGGCTTCAGCAATGAATTCACCTTTGGGAACAAGCTGGACACCTTCTGTGGCAGTCCCCCTTATGCTGCCCCAGAACTCTTCCAGGGCAAAAAATATGATGGACCCGAGGTGGATGTGTGGAGCCTAGGAGTTATCCTCTATACACTGGTCAGCGGATCCCTGCCTTTTGATGGACAGAACCTCAAGGAGCTGCGGGAACGGGTACTGAGGGGAAAATACCGTATTCCATTCTACATGTCCACGGACTGTGAAAACCTGCTTAAGAAATTTCTCATTCTTAATCCCAGCAAGAGAGGCACTTTAGAGCAAATCATGAAAGATCGATGGATGAATGTGGGTCACGAAGATGATGAACTAAAGCCTTACGTGGAGCCACTCCCTGACTACAAGGACCCCCGGCGGACAGAGCTGATGGTGTCCATGGGTTATACACGGGAAGAGATCCAGGACTCGCTGGTGGGCCAGAGATACAACGAGGTGATGGCCACCTATCTGCTCCTGGGCTAC</t>
+  </si>
+  <si>
+    <t>MAAAAAQGGGGGEPRRTEGVGPGVPGEVEMVKGQPFDVGPRYTQLQYIGEGAYGMVSSAYDHVRKTRVAIKKISPFEHQTYCQRTLREIQILLRFRHENVIGIRDILRASTLEAMRDVYIVQDLMETDLYKLLKSQQLSNDHICYFLYQILRGLKYIHSANVLHRDLKPSNLLINTTCDLKICDFGLARIADPEHDHTGFLTEYVATRWYRAPEIMLNSKGYTKSIDIWSVGCILAEMLSNRPIFPGKHYLDQLNHILGILGSPSQEDLNCIINMKARNYLQSLPSKTKVAWAKLFPKSDSKALDLLDRMLTFNPNKRITVEEALAHPYLEQYYDPTDEPVAEEPFTFAMELDDLPKERLKELIFQETARFQPGVLEAP</t>
+  </si>
+  <si>
+    <t>GDSDISSPLLQNTVHIDLSALNPELVQAVQHVVIGPSSLIVHFNEVIGRGHFGCVYHGTLLDNDGKKIHCAVKSLNRITDIGEVSQFLTEGIIMKDFSHPNVLSLLGICLRSEGSPLVVLPYMKHGDLRNFIRNETHNPTVKDLIGFGLQVAKGMKYLASKKFVHRDLAARNCMLDEKFTVKVADFGLARDMYDKEYYSVHNKTGAKLPVKWMALESLQTQKFTTKSDVWSFGVLLWELMTRGAPPYPDVNTFDITVYLLQGRRLLQPEYCPDPLYEVMLKCWHPKAEMRPSFSELVSRISAIFSTFIG</t>
+  </si>
+  <si>
+    <t>ATGAGTAGCTTTCTGCCAGAGGGAGGGTGTTACGAGCTGCTCACTGTGATAGGCAAAGGATTTGAGGACCTGATGACTGTGAATCTAGCAAGGTACAAACCAACAGGAGAGTACGTGACTGTACGGAGGATTAACCTAGAAGCTTGTTCCAATGAGATGGTAACATTCTTGCAGGGCGAGCTGCATGTCTCCAAACTCTTCAACCATCCCAATATCGTGCCATATCGAGCCACTTTTATTGCAGACAATGAGCTGTGGGTTGTCACATCATTCATGGCATACGGTTCTGCAAAAGATCTCATCTGTACACACTTCATGGATGGCATGAATGAGCTGGCGATTGCTTACATCCTGCAGGGGGTGCTGAAGGCCCTCGACTACATCCACCACATGGGATATGTACACAGGAGTGTCAAAGCCAGCCACATCCTGATCTCTGTGGATGGGAAGGTCTACCTGTCTGGTTTGCGCAGCAACCTCAGCATGATAAGCCATGGGCAGCGGCAGCGAGTGGTCCACGATTTTCCCAAGTACAGTGTCAAGGTTCTGCCGTGGCTCAGCCCCGAGGTCCTCCAGCAGAATCTCCAGGGTTATGATGCCAAGTCTGACATCTACAGTGTGGGAATCACAGCCTGTGAACTGGCCAACGGCCATGTCCCCTTTAAGGATATGCCTGCCACCCAGATGCTGCTAGAGAAACTGAACGGCACAGTGCCCTGCCTGTTGGATACCAGCACCATCCCCGCTGAGGAGCTGACCATGAGCCCTTCGCGCTCAGTGGCCAACTCTGGCCTGAGTGACAGCCTGACCACCAGCACCCCCCGGCCCTCCAACGGTGACTCGCCCTCCCACCCCTACCACCGAACCTTCTCCCCCCACTTCCACCACTTTGTGGAGCAGTGCCTTCAGCGCAACCCGGATGCCAGGCCCAGTGCCAGCACCCTCCTGAACCACTCTTTCTTCAAGCAGATCAAGCGACGTGCCTCAGAGGTTTTGCCCGAATTGCTTCGTCCTGTCACCCCCATCACCAATTTTGAGGGCAGCCAGTCTCAGGACCACAGTGGAATCTTTGGCCTGGTAACAAACCTGGAAGAGCTGGAGGTGGACGATTGGGAGTTC</t>
+  </si>
+  <si>
+    <t>ADPEELFTKLERIGKGSFGEVFKGIDNRTQQVVAIKIIDLEEAEDEIEDIQQEITVLSQCDSSYVTKYYGSYLKGSKLWIIMEYLGGGSALDLLRAGPFDEFQIATMLKEILKGLDYLHSEKKIHRDIKAANVLLSEQGDVKLADFGVAGQLTDTQIKRNTFVGTPFWMAPEVIQQSAYDSKADIWSLGITAIELAKGEPPNSDMHPMRVLFLIPKNNPPTLVGDFTKSFKEFIDACLNKDPSFRPTAKELLKHKFIVKNSKKTSYLTELIDRFKRWKAE</t>
+  </si>
+  <si>
+    <t>GATGAACAACCTCACATCGGAAACTACAGACTGTTGAAAACAATCGGCAAGGGGAATTTTGCAAAAGTAAAATTGGCAAGACATATCCTTACAGGCAGAGAGGTTGCAATAAAAATAATTGACAAAACTCAGTTGAATCCAACAAGTCTACAAAAGCTCTTCAGAGAAGTAAGAATAATGAAGATTTTAAATCATCCCAATATAGTGAAGTTATTCGAAGTCATTGAAACTGAAAAAACACTCTACCTAATCATGGAATATGCAAGTGGAGGTGAAGTATTTGACTATTTGGTTGCACATGGCAGGATGAAGGAAAAAGAAGCAAGATCTAAATTTAGACAGATTGTGTCTGCAGTTCAATACTGCCATCAGAAACGGATCGTACATCGAGACCTCAAGGCTGAAAATCTATTGTTAGATGCCGATATGAACATTAAAATAGCAGATTTCGGTTTTAGCAATGAATTTACTGTTGGCGGTAAACTCGACACGTTTTGTGGCAGTCCTCCATACGCAGCACCTGAGCTCTTCCAGGGCAAGAAATATGACGGGCCAGAAGTGGATGTGTGGAGTCTGGGGGTCATTTTATACACACTAGTCAGTGGCTCACTTCCCTTTGATGGGCAAAACCTAAAGGAACTGAGAGAGAGAGTATTAAGAGGGAAATACAGAATTCCCTTCTACATGTCTACAGACTGTGAAAACCTTCTCAAACGTTTCCTGGTGCTAAATCCAATTAAACGCGGCACTCTAGAGCAAATCATGAAGGACAGGTGGATCAATGCAGGGCATGAAGAAGATGAACTCAAACCATTTGTTGAACCAGAGCTAGACATCTCAGACCAAAAAAGAATAGATATTATGGTGGGAATGGGATATTCACAAGAAGAAATTCAAGAATCTCTTAGTAAGATGAAATACGATGAAATCACAGCTACATATTTGTTATTGGGGAGAAAATCTTCAGAG</t>
+  </si>
+  <si>
+    <t>HIGNYRLLKTIGKGNFAKVKLARHILTGKEVAVKIIDKTQLNSSSLQKLFREVRIMKVLNHPNIVKLFEVIETEKTLYLVMEYASGGEVFDYLVAHGRMKEKEARAKFRQIVSAVQYCHQKFIVHRDLKAENLLLDADMNIKIADFGFSNEFTFGNKLDTFCGSPPYAAPELFQGKKYDGPEVDVWSLGVILYTLVSGSLPFDGQNLKELRERVLRGKYRIPFYMSTDCENLLKKFLILNPSKRGTLEQIMKDRWMNVGHEDDELKPYVEPLPDYKDPRRTELMVSMGYTREEIQDSLVGQRYNEVMATYLLLGY</t>
+  </si>
+  <si>
+    <t>GVVTHEQFKAALRMVVDQGDPRLLLDSYVKIGEGSTGIVCLAREKHSGRQVAVKMMDLRKQQRRELLFNEVVIMRDYQHFNVVEMYKSYLVGEELWVLMEFLQGGALTDIVSQVRLNEEQIATVCEAVLQALAYLHAQGVIHRDIKSDSILLTLDGRVKLSDFGFCAQISKDVPKRKSLVGTPYWMAPEVISRSLYATEVDIWSLGIMVIEMVDGEPPYFSDSPVQAMKRLRDSPPPKLKNSHKVSPVLRDFLERMLVRDPQERATAQELLDHPFLLQTGLPECLVPLIQLYRKQTSTC</t>
+  </si>
+  <si>
+    <t>MKDYDELLKYYELHETIGTGGFAKVKLACHILTGEMVAIKIMDKNTLGSDLPRIKTEIEALKNLRHQHICQLYHVLETANKIFMVLEYCPGGELFDYIISQDRLSEEETRVVFRQIVSAVAYVHSQGYAHRDLKPENLLFDEYHKLKLIDFGLCAKPKGNKDYHLQTCCGSLAYAAPELIQGKSYLGSEADVWSMGILLYVLMCGFLPFDDDNVMALYKKIMRGKYDVPKWLSPSSILLLQQMLQVDPKKRISMKNLLNHPWIMQDYNYPVEWQSKNPFIHLDDDCVTELSVHHRNNRQTMEDLISLWQYDHLTATYLLLLAKKARGKPVRLRLSSFSCG</t>
+  </si>
+  <si>
+    <t>MSQERPTFYRQELNKTIWEVPERYQNLSPVGSGAYGSVCAAFDTKTGLRVAVKKLSRPFQSIIHAKRTYRELRLLKHMKHENVIGLLDVFTPARSLEEFNDVYLVTHLMGADLNNIVKCQKLTDDHVQFLIYQILRGLKYIHSADIIHRDLKPSNLAVNEDCELKILDFGLARHTDDEMTGYVATRWYRAPEIMLNWMHYNQTVDIWSVGCIMAELLTGRTLFPGTDHIDQLKLILRLVGTPGAELLKKISSESARNYIQSLTQMPKMNFANVFIGANPLAVDLLEKMLVLDSDKRITAAQALAHAYFAQYHDPDDEPVADPYDQSFESRDLLIDEWKSLTYDEVISFVPPPLDQEEMES</t>
+  </si>
+  <si>
+    <t>MELRVGNRYRLGRKIGSGSFGDIYLGTDIAAGEEVAIKLECVKTKHPQLHIESKIYKMMQGGVGIPTIRWCGAEGDYNVMVMELLGPSLEDLFNFCSRKFSLKTVLLLADQMISRIEYIHSKNFIHRDVKPDNFLMGLGKKGNLVYIIDFGLAKKYRDARTHQHIPYRENKNLTGTARYASINTHLGIEQSRRDDLESLGYVLMYFNLGSLPWQGLKAATKRQKYERISEKKMSTPIEVLCKGYPSEFATYLNFCRSLRFDDKPDYSYLRQLFRNLFHRQGFSYDYVFDWNMLK</t>
+  </si>
+  <si>
+    <t>targetID</t>
+  </si>
+  <si>
+    <t>TGGGCCCTGAACATGAAGGAGCTGAAGCTGCTGCAGACCATCGGGAAGGGGGAGTTCGGAGACGTGATGCTGGGCGATTACCGAGGGAACAAAGTCGCCGTCAAGTGCATTAAGAACGACGCCACTGCCCAGGCCTTCCTGGCTGAAGCCTCAGTCATGACGCAACTGCGGCATAGCAACCTGGTGCAGCTCCTGGGCGTGATCGTGGAGGAGAAGGGCGGGCTCTACATCGTCACTGAGTACATGGCCAAGGGGAGCCTTGTGGACTACCTGCGGTCTAGGGGTCGGTCAGTGCTGGGCGGAGACTGTCTCCTCAAGTTCTCGCTAGATGTCTGCGAGGCCATGGAATACCTGGAGGGCAACAATTTCGTGCATCGAGACCTGGCTGCCCGCAATGTGCTGGTGTCTGAGGACAACGTGGCCAAGGTCAGCGACTTTGGTCTCACCAAGGAGGCGTCCAGCACCCAGGACACGGGCAAGCTGCCAGTCAAGTGGACAGCCCCTGAGGCCCTGAGAGAGAAGAAATTCTCCACTAAGTCTGACGTGTGGAGTTTCGGAATCCTTCTCTGGGAAATCTACTCCTTTGGGCGAGTGCCTTATCCAAGAATTCCCCTGAAGGACGTCGTCCCTCGGGTGGAGAAGGGCTACAAGATGGATGCCCCCGACGGCTGCCCGCCCGCAGTCTATGAAGTCATGAAGAACTGCTGGCACCTGGACGCCGCCATGCGGCCCTCCTTCCTACAGCTCCGAGAGCAGCTTGAGCACATCAAAACCCACGAGCTGCACCTG</t>
+  </si>
+  <si>
+    <t>dna_seq</t>
+  </si>
+  <si>
+    <t>AACCTGGTTTTTAGTGACGGCTACGTGGTAAAGGAGACAATTGGTGTGGGCTCCTACTCTGAGTGCAAGCGCTGTGTCCACAAGGCCACCAACATGGAGTATGCTGTCAAGGTCATTGATAAGAGCAAGCGGGATCCTTCAGAAGAGATTGAGATTCTTCTGCGGTATGGCCAGCACCCCAACATCATCACTCTGAAAGATGTGTATGATGATGGCAAACACGTGTACCTGGTGACAGAGCTGATGCGGGGTGGGGAGCTGCTGGACAAGATCCTGCGGCAGAAGTTCTTCTCAGAGCGGGAGGCCAGCTTTGTCCTGCACACCATTGGCAAAACTGTGGAGTATCTGCACTCACAGGGGGTTGTGCACAGGGACCTGAAGCCCAGCAACATCCTGTATGTGGACGAGTCCGGGAATCCCGAGTGCCTGCGCATCTGTGACTTTGGTTTTGCCAAACAGCTGCGGGCTGAGAATGGGCTCCTCATGACACCTTGCTACACAGCCAACTTTGTGGCGCCTGAGGTGCTGAAGCGCCAGGGCTACGATGAAGGCTGCGACATCTGGAGCCTGGGCATTCTGCTGTACACCATGCTGGCAGGATATACTCCATTTGCCAACGGTCCCAGTGACACACCAGAGGAAATCCTAACCCGGATCGGCAGTGGGAAGTTTACCCTCAGTGGGGGAAATTGGAACACAGTTTCAGAGACAGCCAAGGACCTGGTGTCCAAGATGCTACACGTGGATCCCCACCAGCGCCTCACAGCTAAGCAGGTTCTGCAGCATCCATGGGTCACCCAGAAAGACAAGCTTCCCCAAAGCCAGCTGTCCCACCAGGACCTACAGCTTGTGAAGGGAGCCATGGCTGCCACGTACTCCGCACTCAACAGCTCCAAGCCCACCCCCCAGCTGAAGCCCATCGAGTCATCCATCCTGGCCCAGCGGCGAGTGAGGAAGTTGCCATCCACCACCCTG</t>
+  </si>
+  <si>
+    <t>ATGGCCGACGACGACGTGCTGTTCGAGGATGTGTACGAGCTGTGCGAGGTGATCGGAAAGGGTCCCTTCAGTGTTGTACGACGATGTATCAACAGAGAAACTGGGCAACAATTTGCTGTAAAAATTGTTGATGTAGCCAAGTTCACATCAAGTCCAGGGTTAAGTACAGAAGATCTAAAGCGGGAAGCCAGTATCTGTCATATGCTGAAACATCCACACATTGTAGAGTTATTGGAGACATATAGCTCAGATGGAATGCTTTACATGGTTTTCGAATTTATGGATGGAGCAGATCTGTGTTTTGAAATCGTAAAGCGAGCTGACGCTGGTTTTGTGTACAGTGAAGCTGTAGCCAGCCATTATATGAGACAGATACTGGAAGCTCTACGCTACTGCCATGATAATAACATAATTCACAGGGATGTGAAGCCCCACTGTGTTCTCCTTGCCTCAAAAGAAAACTCGGCACCTGTTAAACTTGGAGGCTTTGGGGTAGCTATTCAATTAGGGGAGTCTGGACTTGTAGCTGGAGGACGTGTTGGAACACCTCATTTTATGGCACCAGAAGTGGTCAAAAGAGAGCCTTACGGAAAGCCTGTAGACGTCTGGGGGTGCGGTGTGATCCTTTTTATCCTGCTCAGTGGTTGTTTGCCTTTTTACGGAACCAAGGAAAGATTGTTTGAAGGCATTATTAAAGGAAAATATAAGATGAATCCAAGGCAGTGGAGCCATATCTCTGAAAGTGCCAAAGACCTAGTACGTCGCATGCTGATGCTGGATCCAGCTGAAAGGATCACTGTTTATGAAGCACTGAATCACCCATGGCTTAAGGAGCGGGATCGTTACGCCTACAAGATTCATCTTCCAGAAACAGTAGAGCAGCTGAGGAAATTCAATGCAAGGAGGAAACTAAAGGGTGCAGTACTAGCCGCTGTGTCAAGTCACAAATTCAACTCATTCTATGGGGATCCCCCTGAAGAGTTACCAGATTTCTCCGAAGACCCTACCTCCTCAGGAGCA</t>
+  </si>
+  <si>
+    <t>VRK1_HUMAN_D0_3OP5_D</t>
+  </si>
+  <si>
+    <t>ATGGGGAAGGTGAAAGCCACCCCCATGACACCTGAACAAGCAATGAAGCAATACATGCAAAAACTCACAGCCTTCGAACACCATGAGATTTTCAGCTACCCTGAAATATATTTCTTGGGTCTAAATGCTAAGAAGCGCCAGGGCATGACAGGTGGGCCCAACAATGGTGGCTATGATGATGACCAGGGATCATATGTGCAGGTGCCCCACGATCACGTGGCTTACAGGTATGAGGTCCTCAAGGTCATTGGGAAGGGGAGCTTTGGGCAGGTGGTCAAGGCCTACGATCACAAAGTCCACCAGCACGTGGCCCTAAAGATGGTGCGGAATGAGAAGCGCTTCCACCGGCAAGCAGCGGAGGAGATCCGAATCCTGGAACACCTGCGGAAGCAGGACAAGGATAACACAATGAATGTCATCCATATGCTGGAGAATTTCACCTTCCGCAACCACATCTGCATGACGTTTGAGCTGCTGAGCATGAACCTCTATGAGCTCATCAAGAAGAATAAATTCCAGGGCTTCAGTCTGCCTTTGGTTCGCAAGTTTGCCCACTCGATTCTGCAGTGCTTGGATGCTTTGCACAAAAACAGAATAATTCACTGTGACCTTAAGCCCGAGAACATTTTGTTAAAGCAGCAGGGTAGAAGCGGTATTAAAGTAATTGATTTTGGCTCCAGTTGTTACGAGCATCAGCGTGTCTACACGTACATCCAGTCGCGTTTTTACCGGGCTCCAGAAGTGATCCTTGGGGCCAGGTATGGCATGCCCATTGATATGTGGAGCCTGGGCTGCATTTTAGCAGAGCTCCTGACGGGTTACCCCCTCTTGCCTGGGGAAGATGAAGGGGACCAGCTGGCCTGTATGATTGAACTGTTGGGCATGCCCTCACAGAAACTGCTGGATGCATCCAAACGAGCCAAAAATTTTGTGAGCTCCAAGGGTTATCCCCGTTACTGCACTGTCACGACTCTCTCAGATGGCTCTGTGGTCCTAAACGGAGGCCGTTCCCGGAGGGGGAAACTGAGGGGCCCACCGGAGAGCAGAGAGTGGGGGAACGCGCTGAAGGGGTGTGATGATCCCCTTTTCCTTGACTTCTTAAAACAGTGTTTAGAGTGGGATCCTGCAGTGCGCATGACCCCAGGCCAGGCTTTGCGGCACCCCTGGCTGAGGAGGCGGTTGCCAAAGCCTCCCACCGGGGAGAAAACGTCAGTGAAAAGG</t>
   </si>
   <si>
     <t>ACTGACTCCTTGCCAGGAAAGTTTGAAGATATGTACAAGCTGACCTCTGAATTGCTGGGAGAGGGAGCCTATGCCAAAGTTCAAGGTGCCGTGAGCCTACAGAATGGCAAAGAGTATGCCGTCAAAATCATCGAGAAACAAGCAGGGCACAGTCGGAGTAGGGTGTTTCGAGAGGTGGAGACGCTGTATCAGTGTCAGGGAAACAAGAACATTTTGGAGCTGATTGAGTTCTTTGAAGATGACACAAGGTTTTACTTGGTCTTTGAGAAATTGCAAGGAGGTTCCATCTTAGCCCACATCCAGAAGCAAAAGCACTTCAATGAGCGAGAAGCCAGCCGAGTGGTGCGGGACGTTGCTGCTGCCCTTGACTTCCTGCATACCAAAGACAAAGTCTCTCTCTGTCACCTAGGCGGGAGTGCTAGGGCGCCATCAGGGCTCACTGCAGCCCCAACCTCCCTGGGCTCCAGTGATCCTCCCACCTCAGCCTCCCAAGTAGCTGGGACTACAGGCATTGATCATCGTGATCTGAAACCAGAAAATATATTGTGTGAATCTCCAGAAAAGGTGTCTCCAGTGAAAATCTGTGACTTTGACTTGGGCAGTGGGATGAAACTGAACAACTCCTGTACCCCCATAACCACACCAGAGCTGACCACCCCATGTGGCTCTGCAGAATACATGGCCCCTGAGGTAGGGGAGGTCTTCACGGACCAGGCCACATTCTACGACAAGCGCTGTGACCTGTGGAGCCTGGGCGTGGTCCTCTACATCATGCTGAGTGGCTACCCACCCTTCGTGGGTCACTGCGGGGCCGACTGTGGCTGGGACCGGGGCGAGGTCTGCAGGGTGTGCCAGAACAAGCTGTTTGAAAGCATCCAGGAAGGCAAGTATGAGTTTCCTGACAAGGACTGGGCACACATCTCCAGTGAAGCCAAAGACCTCATCTCCAAGCTCCTGGTGCGAGATGCAAAGCAGAGACTTAGCGCCGCCCAAGTTCTGCAGCACCCATGGGTGCAGGGGCAAGCTCCAGAAAAGGGA</t>
   </si>
   <si>
-    <t>PAK4_HUMAN_D0_2J0I_A</t>
-  </si>
-  <si>
-    <t>AGVSEYELPEDPRWELPRDRLVLGKPLGEGCFGQVVLAEAIGLDKDKPNRVTKVAVKMLKSDATEKDLSDLISEMEMMKMIGKHKNIINLLGACTQDGPLYVIVEYASKGNLREYLQARRPPGLEYCYNPSHNPEEQLSSKDLVSCAYQVARGMEYLASKKCIHRDLAARNVLVTEDNVMKIADFGLARDIHHIDYYKKTTNGRLPVKWMAPEALFDRIYTHQSDVWSFGVLLWEIFTLGGSPYPGVPVEELFKLLKEGHRMDKPSNCTNELYMMMRDCWHAVPSQRPTFKQLVEDLDRIVALTSNQEYLDLSMPLD</t>
-  </si>
-  <si>
-    <t>MAAAAAQGGGGGEPRRTEGVGPGVPGEVEMVKGQPFDVGPRYTQLQYIGEGAYGMVSSAYDHVRKTRVAIKKISPFEHQTYCQRTLREIQILLRFRHENVIGIRDILRASTLEAMRDVYIVQDLMETDLYKLLKSQQLSNDHICYFLYQILRGLKYIHSANVLHRDLKPSNLLINTTCDLKICDFGLARIADPEHDHTGFLTEYVATRWYRAPEIMLNSKGYTKSIDIWSVGCILAEMLSNRPIFPGKHYLDQLNHILGILGSPSQEDLNCIINMKARNYLQSLPSKTKVAWAKLFPKSDSKALDLLDRMLTFNPNKRITVEEALAHPYLEQYYDPTDEPVAEEPFTFAMELDDLPKERLKELIFQETARFQPGVLEAP</t>
-  </si>
-  <si>
-    <t>GAGCCCAAGAAGTACGCAGTGACCGACGACTACCAGTTGTCCAAGCAGGTGCTGGGCCTGGGTGTGAACGGCAAAGTGCTGGAGTGCTTCCATCGGCGCACTGGACAGAAGTGTGCCCTGAAGCTCCTGTATGACAGCCCCAAGGCCCGGCAGGAGGTAGACCATCACTGGCAGGCTTCTGGCGGCCCCCATATTGTCTGCATCCTGGATGTGTATGAGAACATGCACCATGGCAAGCGCTGTCTCCTCATCATCATGGAATGCATGGAAGGTGGTGAGTTGTTCAGCAGGATTCAGGAGCGTGGCGACCAGGCTTTCACTGAGAGAGAAGCTGCAGAGATAATGCGGGATATTGGCACTGCCATCCAGTTTCTGCACAGCCATAACATTGCCCACCGAGATGTCAAGCCTGAAAACCTACTCTACACATCTAAGGAGAAAGACGCAGTGCTTAAGCTCACCGATTTTGGCTTTGCTAAGGAGACCACCCAAAATGCCCTGCAGACACCCTGCTATACTCCCTATTATGTGGCCCCTGAGGTCCTGGGTCCAGAGAAGTATGACAAGTCATGTGACATGTGGTCCCTGGGTGTCATCATGTACATCCTCCTTTGTGGCTTCCCACCCTTCTACTCCAACACGGGCCAGGCCATCTCCCCGGGGATGAAGAGGAGGATTCGCCTGGGCCAGTACGGCTTCCCCAATCCTGAGTGGTCAGAAGTCTCTGAGGATGCCAAGCAGCTGATCCGCCTCCTGTTGAAGACAGACCCCACAGAGAGGCTGACCATCACTCAGTTCATGAACCACCCCTGGATCAACCAATCGATGGTAGTGCCACAGACCCCACTCCACACGGCCCGAGTGCTGCAGGAGGACAAAGACCACTGGGACGAAGTCAAGGAGGAGATGACCAGTGCCTTGGCCACTATGCGGGTAGACTACGACCAGGTG</t>
-  </si>
-  <si>
-    <t>ATGTCTCAGGAGAGGCCCACGTTCTACCGGCAGGAGCTGAACAAGACAATCTGGGAGGTGCCCGAGCGTTACCAGAACCTGTCTCCAGTGGGCTCTGGCGCCTATGGCTCTGTGTGTGCTGCTTTTGACACAAAAACGGGGTTACGTGTGGCAGTGAAGAAGCTCTCCAGACCATTTCAGTCCATCATTCATGCGAAAAGAACCTACAGAGAACTGCGGTTACTTAAACATATGAAACATGAAAATGTGATTGGTCTGTTGGACGTTTTTACACCTGCAAGGTCTCTGGAGGAATTCAATGATGTGTATCTGGTGACCCATCTCATGGGGGCAGATCTGAACAACATTGTGAAATGTCAGAAGCTTACAGATGACCATGTTCAGTTCCTTATCTACCAAATTCTCCGAGGTCTAAAGTATATACATTCAGCTGACATAATTCACAGGGACCTAAAACCTAGTAATCTAGCTGTGAATGAAGACTGTGAGCTGAAGATTCTGGATTTTGGACTGGCTCGGCACACAGATGATGAAATGACAGGCTACGTGGCCACTAGGTGGTACAGGGCTCCTGAGATCATGCTGAACTGGATGCATTACAACCAGACAGTTGATATTTGGTCAGTGGGATGCATAATGGCCGAGCTGTTGACTGGAAGAACATTGTTTCCTGGTACAGACCATATTGATCAGTTGAAGCTCATTTTAAGACTCGTTGGAACCCCAGGGGCTGAGCTTTTGAAGAAAATCTCCTCAGAGTCTGCAAGAAACTATATTCAGTCTTTGACTCAGATGCCGAAGATGAACTTTGCGAATGTATTTATTGGTGCCAATCCCCTGGCTGTCGACTTGCTGGAGAAGATGCTTGTATTGGACTCAGATAAGAGAATTACAGCGGCCCAAGCCCTTGCACATGCCTACTTTGCTCAGTACCACGATCCTGATGATGAACCAGTGGCCGATCCTTATGATCAGTCCTTTGAAAGCAGGGACCTCCTTATAGATGAGTGGAAAAGCCTGACCTATGATGAAGTCATCAGCTTTGTGCCACCACCCCTTGACCAAGAAGAGATGGAGTCC</t>
-  </si>
-  <si>
-    <t>MK11_HUMAN_D0_3GC8_A</t>
-  </si>
-  <si>
-    <t>MK14_HUMAN_D0_3K3J_A</t>
-  </si>
-  <si>
-    <t>CDK16_HUMAN_D0_3MTL_A</t>
-  </si>
-  <si>
-    <t>PLK1_HUMAN_D0_2V5Q_A</t>
-  </si>
-  <si>
-    <t>BRAF_HUMAN_D0_4JVG_D</t>
-  </si>
-  <si>
-    <t>NEK7_HUMAN_D0_2WQN_A</t>
-  </si>
-  <si>
-    <t>PAK6_HUMAN_D0_2C30_A</t>
-  </si>
-  <si>
-    <t>FGFR1_HUMAN_D0_3GQL_B</t>
-  </si>
-  <si>
-    <t>TCTTCGGTCACCGCCAGTGCGGCCCCGGGGACCGCGAGCCTCGTCCCGGATTACTGGATCGACGGCTCCAACAGGGATGCGCTGAGCGATTTCTTCGAGGTGGAGTCGGAGCTGGGACGGGGTGCTACATCCATTGTGTACAGATGCAAACAGAAGGGGACCCAGAAGCCTTATGCTCTCAAAGTGTTAAAGAAAACAGTGGACAAAAAAATCGTAAGAACTGAGATAGGAGTTCTTCTTCGCCTCTCACATCCAAACATTATAAAACTTAAAGAGATATTTGAAACCCCTACAGAAATCAGTCTGGTCCTAGAACTCGTCACAGGAGGAGAACTGTTTGATAGGATTGTGGAAAAGGGATATTACAGTGAGCGAGATGCTGCAGATGCCGTTAAACAAATCCTGGAGGCAGTTGCTTATCTACATGAAAATGGGATTGTCCATCGTGATCTCAAACCAGAGAATCTTCTTTATGCAACTCCAGCCCCAGATGCACCACTCAAAATCGCTGATTTTGGACTCTCTAAAATTGTGGAACATCAAGTGCTCATGAAGACAGTATGTGGAACCCCAGGGTACTGCGCACCTGAAATTCTTAGAGGTTGTGCCTATGGACCTGAGGTGGACATGTGGTCTGTAGGAATAATCACCTACATCTTACTTTGTGGATTTGAACCATTCTATGATGAAAGAGGCGATCAGTTCATGTTCAGGAGAATTCTGAATTGTGAATATTACTTTATCTCCCCCTGGTGGGATGAAGTATCTCTAAATGCCAAGGACTTGGTCAGAAAATTAATTGTTTTGGATCCAAAGAAACGGCTGACTACATTTCAAGCTCTCCAGCATCCGTGGGTCACAGGTAAAGCAGCCAATTTTGTACACATGGATACCGCTCAAAAGAAGCTCCAAGAATTCAATGCCCGGCGTAAGCTTAAGGCAGCGGTGAAGGCTGTGGTGGCCTCTTCCCGCCTGGGA</t>
-  </si>
-  <si>
-    <t>MEAAASEPSLDLDNLKLLELIGRGRYGAVYKGSLDERPVAVKVFSFANRQNFINEKNIYRVPLMEHDNIARFIVGDERVTADGRMEYLLVMEYYPNGSLCKYLSLHTSDWVSSCRLAHSVTRGLAYLHTELPRGDHYKPAISHRDLNSRNVLVKNDGTCVISDFGLSMRLTGNRLVRPGEEDNAAISEVGTIRYMAPEVLEGAVNLRDCESALKQVDMYALGLIYWEIFMRCTDLFPGESVPEYQMAFQTEVGNHPTFEDMQVLVSREKQRPKFPEAWKENSLAVRSLKETIEDCWDQDAEARLTAQCAEERMAELMMIWERNKSVSPT</t>
-  </si>
-  <si>
-    <t>GTCATCATTGACAATAAGCGCTACCTCTTCATCCAGAAACTGGGGGAGGGTGGGTTCAGCTATGTGGACCTAGTGGAAGGGTTACATGATGGACACTTCTACGCCCTGAAGCGAATCCTGTGTCACGAGCAGCAGGACCGGGAGGAGGCCCAGCGAGAAGCCGACATGCATCGCCTCTTCAATCACCCCAACATCCTTCGCCTCGTGGCTTACTGTCTGAGGGAACGGGGTGCTAAGCATGAGGCCTGGCTGCTGCTACCATTCTTCAAGAGAGGTACGCTGTGGAATGAGATAGAAAGGCTGAAGGACAAAGGCAACTTCCTGACCGAGGATCAAATCCTTTGGCTGCTGCTGGGGATCTGCAGAGGCCTTGAGGCCATTCATGCCAAGGGTTATGCCCACAGAGACTTGAAGCCCACCAATATATTGCTTGGAGATGAGGGGCAGCCAGTTTTAATGGACTTGGGTTCCATGAATCAAGCATGCATCCATGTGGAGGGCTCCCGCCAGGCTCTGACCCTGCAGGACTGGGCAGCCCAGCGGTGCACCATCTCCTACCGAGCCCCAGAGCTCTTCTCTGTGCAGAGTCACTGTGTCATCGATGAGCGGACTGATGTCTGGTCCCTAGGCTGCGTGCTATATGCCATGATGTTTGGGGAAGGCCCTTATGACATGGTGTTCCAAAAGGGTGACAGTGTGGCCCTTGCTGTGCAGAACCAACTCAGCATCCCACAAAGCCCCAGGCATTCTTCAGCATTGTGGCAGCTCCTGAACTCGATGATGACCGTGGACCCGCATCAGCGTCCTCACATTCCTCTCCTCCTCAGTCAGCTGGAGGCGCTGCAG</t>
-  </si>
-  <si>
-    <t>BMPR2_HUMAN_D0_3G2F_A</t>
-  </si>
-  <si>
-    <t>dna_start</t>
-  </si>
-  <si>
-    <t>PHKG2_HUMAN_D0_2Y7J_D</t>
-  </si>
-  <si>
-    <t>MAPK2_HUMAN_D0_2JBO_A</t>
-  </si>
-  <si>
-    <t>HHHHHHSHSGPEISRIIVDPTTGKRYCRGKVLGKGGFAKCYEMTDLTNNKVYAAKIIPHSRVAKPHQREKIDKEIELHRILHHKHVVQFYHYFEDKENIYILLEYCSRRSMAHILKARKVLTEPEVRYYLRQIVSGLKYLHEQEILHRDLKLGNFFINEAMELKVGDFGLAARLEPLEHRRRTICGTPNYLSPEVLNKQGHGCESDIWALGCVMYTMLLGRPPFETTNLKETYRCIREARYTMPSSLLAPAKHLIASMLSKNPEDRPSLDDIIRHDFFLQGFTPDRLSSSCCHTVPDFHLSSPA</t>
-  </si>
-  <si>
-    <t>ATGGAGAAGGACGGCCTGTGCCGCGCTGACCAGCAGTACGAATGCGTGGCGGAGATCGGGGAGGGCGCCTATGGGAAGGTGTTCAAGGCCCGCGACTTGAAGAACGGAGGCCGTTTCGTGGCGTTGAAGCGCGTGCGGGTGCAGACCGGCGAGGAGGGCATGCCGCTCTCCACCATCCGCGAGGTGGCGGTGCTGAGGCACCTGGAGACCTTCGAGCACCCCAACGTGGTCAGGTTGTTTGATGTGTGCACAGTGTCACGAACAGACAGAGAAACCAAACTAACTTTAGTGTTTGAACATGTCGATCAAGACTTGACCACTTACTTGGATAAAGTTCCAGAGCCTGGAGTGCCCACTGAAACCATAAAGGATATGATGTTTCAGCTTCTCCGAGGTCTGGACTTTCTTCATTCACACCGAGTAGTGCATCGCGATCTAAAACCACAGAACATTCTGGTGACCAGCAGCGGACAAATAAAACTCGCTGACTTCGGCCTTGCCCGCATCTATAGTTTCCAGATGGCTCTAACCTCAGTGGTCGTCACGCTGTGGTACAGAGCACCCGAAGTCTTGCTCCAGTCCAGCTACGCCACCCCCGTGGATCTCTGGAGTGTTGGCTGCATATTTGCAGAAATGTTTCGTAGAAAGCCTCTTTTTCGTGGAAGTTCAGATGTTGATCAACTAGGAAAAATCTTGGACGTGATTGGACTCCCAGGAGAAGAAGACTGGCCTAGAGATGTTGCCCTTCCCAGGCAGGCTTTTCATTCAAAATCTGCCCAACCAATTGAGAAGTTTGTAACAGATATCGATGAACTAGGCAAAGACCTACTTCTGAAGTGTTTGACATTTAACCCAGCCAAAAGAATATCTGCCTACAGTGCCCTGTCTCACCCATACTTCCAG</t>
-  </si>
-  <si>
-    <t>ATGTCGGGCCCTCGCGCCGGCTTCTACCGGCAGGAGCTGAACAAGACCGTGTGGGAGGTGCCGCAGCGGCTGCAGGGGCTGCGCCCGGTGGGCTCCGGCGCCTACGGCTCCGTCTGTTCGGCCTACGACGCCCGGCTGCGCCAGAAGGTGGCGGTGAAGAAGCTGTCGCGCCCCTTCCAGTCGCTGATCCACGCGCGCAGAACGTACCGGGAGCTGCGGCTGCTCAAGCACCTGAAGCACGAGAACGTCATCGGGCTTCTGGACGTCTTCACGCCGGCCACGTCCATCGAGGACTTCAGCGAAGTGTACTTGGTGACCACCCTGATGGGCGCCGACCTGAACAACATCGTCAAGTGCCAGGCGCTGAGCGACGAGCACGTTCAATTCCTGGTTTACCAGCTGCTGCGCGGGCTGAAGTACATCCACTCGGCCGGGATCATCCACCGGGACCTGAAGCCCAGCAACGTGGCTGTGAACGAGGACTGTGAGCTCAGGATCCTGGATTTCGGGCTGGCGCGCCAGGCGGACGAGGAGATGACCGGCTATGTGGCCACGCGCTGGTACCGGGCACCTGAGATCATGCTCAACTGGATGCATTACAACCAAACAGTGGATATCTGGTCCGTGGGCTGCATCATGGCTGAGCTGCTCCAGGGCAAGGCCCTCTTCCCGGGAAGCGACTACATTGACCAGCTGAAGCGCATCATGGAAGTGGTGGGCACACCCAGCCCTGAGGTTCTGGCAAAAATCTCCTCGGAACACGCCCGGACATATATCCAGTCCCTGCCCCCCATGCCCCAGAAGGACCTGAGCAGCATCTTCCGTGGAGCCAACCCCCTGGCCATAGACCTCCTTGGAAGGATGCTGGTGCTGGACAGTGACCAGAGGGTCAGTGCAGCTGAGGCACTGGCCCACGCCTACTTCAGCCAGTACCACGACCCCGAGGATGAGCCAGAGGCCGAGCCATATGATGAGAGCGTTGAGGCCAAGGAGCGCACGCTGGAGGAGTGGAAGGAGCTCACTTACCAGGAAGTCCTCAGCTTCAAGCCCCCAGAGCCACCGAAGCCACCTGGCAGCCTGGAGATTGAGCAG</t>
-  </si>
-  <si>
-    <t>VRK1_HUMAN_D0_3OP5_D</t>
-  </si>
-  <si>
-    <t>MEKYEKIGKIGEGSYGVVFKCRNRDTGQIVAIKKFLESEDDPVIKKIALREIRMLKQLKHPNLVNLLEVFRRKRRLHLVFEYCDHTVLHELDRYQRGVPEHLVKSITWQTLQAVNFCHKHNCIHRDVKPENILITKHSVIKLCDFGFARLLTGPSDYYTDYVATRWYRSPELLVGDTQYGPPVDVWAIGCVFAELLSGVPLWPGKSDVDQLYLIRKTLGDLIPRHQQVFSTNQYFSGVKIPDPEDMEPLELKFPNISYPALGLL</t>
-  </si>
-  <si>
-    <t>GeneID</t>
-  </si>
-  <si>
-    <t>ATGGATGAGCAATCACAAGGAATGCAAGGGCCACCTGTTCCTCAGTTCCAACCACAGAAGGCCTTACGACCGGATATGGGCTATAATACATTAGCCAACTTTCGAATAGAAAAGAAAATTGGTCGCGGACAATTTAGTGAAGTTTATAGAGCAGCCTGTCTCTTGGATGGAGTACCAGTAGCTTTAAAAAAAGTGCAGATATTTGATTTAATGGATGCCAAAGCACGTGCTGATTGCATCAAAGAAATAGATCTTCTTAAGCAACTCAACCATCCAAATGTAATAAAATATTATGCATCATTCATTGAAGATAATGAACTAAACATAGTTTTGGAACTAGCAGATGCTGGCGACCTATCCAGAATGATCAAGCATTTTAAGAAGCAAAAGAGGCTAATTCCTGAAAGAACTGTTTGGAAGTATTTTGTTCAGCTTTGCAGTGCATTGGAACACATGCATTCTCGAAGAGTCATGCATAGAGATATAAAACCAGCTAATGTGTTCATTACAGCCACTGGGGTGGTAAAACTTGGAGATCTTGGGCTTGGCCGGTTTTTCAGCTCAAAAACCACAGCTGCACATTCTTTAGTTGGTACGCCTTATTACATGTCTCCAGAGAGAATACATGAAAATGGATACAACTTCAAATCTGACATCTGGTCTCTTGGCTGTCTACTATATGAGATGGCTGCATTACAAAGTCCTTTCTATGGTGACAAAATGAATTTATACTCACTGTGTAAGAAGATAGAACAGTGTGACTACCCACCTCTTCCTTCAGATCACTATTCAGAAGAACTCCGACAGTTAGTTAATATGTGCATCAACCCAGATCCAGAGAAGCGACCAGACGTCACCTATGTTTATGACGTAGCAAAGAGGATGCATGCATGCACTGCAAGCAGC</t>
-  </si>
-  <si>
-    <t>DAPK3_HUMAN_D0_2J90_A</t>
-  </si>
-  <si>
-    <t>VKEFLAKAKEDFLKKWESPAQNTAHLDQFERIKTLGTGSFGRVMLVKHKETGNHYAMKILDKQKVVKLKQIEHTLNEKRILQAVNFPFLVKLEFSFKDNSNLYMVMEYVPGGEMFSHLRRIGRFSEPHARFYAAQIVLTFEYLHSLDLIYRDLKPENLLIDQQGYIQVTDFGFAKRVKGRTWTLCGTPEYLAPEIILSKGYNKAVDWWALGVLIYEMAAGYPPFFADQPIQIYEKIVSGKVRFPSHFSSDLKDLLRNLLQVDLTKRFGNLKNGVNDIKNHKWFATTDWIAIYQRKVEAPFIPKFKGPGDTSNFDDYEEEEIRVSINEKCGKEFSEF</t>
-  </si>
-  <si>
-    <t>TCCAGGGTGTCCCATGAACAGTTTCGGGCGGCCCTGCAGCTGGTGGTCAGCCCAGGAGACCCCAGGGAATACTTGGCCAACTTTATCAAAATCGGGGAAGGCTCAACCGGCATCGTATGCATCGCCACCGAGAAACACACAGGGAAACAAGTTGCAGTGAAGAAAATGGACCTCCGGAAGCAACAGAGACGAGAACTGCTTTTCAATGAGGTCGTGATCATGCGGGATTACCACCATGACAATGTGGTTGACATGTACAGCAGCTACCTTGTCGGCGATGAGCTCTGGGTGGTCATGGAGTTTCTAGAAGGTGGTGCCTTGACAGACATTGTGACTCACACCAGAATGAATGAAGAACAGATAGCTACTGTCTGCCTGTCAGTTCTGAGAGCTCTCTCCTACCTTCATAACCAAGGAGTGATTCACAGGGACATAAAAAGTGACTCCATCCTCCTGACAAGCGATGGCCGGATAAAGTTGTCTGATTTTGGTTTCTGTGCTCAAGTTTCCAAAGAGGTGCCGAAGAGGAAATCATTGGTTGGCACTCCCTACTGGATGGCCCCTGAGGTGATTTCTAGGCTACCTTATGGGACAGAGGTGGACATCTGGTCCCTCGGGATCATGGTGATAGAAATGATTGATGGCGAGCCCCCCTACTTCAATGAGCCTCCCCTCCAGGCGATGCGGAGGATCCGGGACAGTTTACCTCCAAGAGTGAAGGACCTACACAAGGTTTCTTCAGTGCTCCGGGGATTCCTAGACTTGATGTTGGTGAGGGAGCCCTCTCAGAGAGCAACAGCCCAGGAACTCCTCGGACATCCATTCTTAAAACTAGCAGGTCCACCGTCTTGCATTGTCCCCCTCATGAGACAATACAGGCATCAC</t>
-  </si>
-  <si>
-    <t>KRQWALEDFEIGRPLGKGKFGNVYLAREKQSKFILALKVLFKAQLEKAGVEHQLRREVEIQSHLRHPNILRLYGYFHDATRVYLILEYAPLGTVYRELQKLSKFDEQRTATYITELANALSYCHSKRVIHRDIKPENLLLGSAGELKIADFGWSVHAPSSRRTTLCGTLDYLPPEMIEGRMHDEKVDLWSLGVLCYEFLVGKPPFEANTYQETYKRISRVEFTFPDFVTEGARDLISRLLKHNPSQRPMLREVLEHPWITANSSKPS</t>
-  </si>
-  <si>
-    <t>EGFR_HUMAN_D0_2RF9_A</t>
-  </si>
-  <si>
-    <t>SLK_HUMAN_D0_2JFL_A</t>
-  </si>
-  <si>
-    <t>SRVSHEQFRAALQLVVSPGDPREYLANFIKIGEGSTGIVCIATEKHTGKQVAVKKMDLRKQQRRELLFNEVVIMRDYHHDNVVDMYSSYLVGDELWVVMEFLEGGALTDIVTHTRMNEEQIATVCLSVLRALSYLHNQGVIHRDIKSDSILLTSDGRIKLSDFGFCAQVSKEVPKRKSLVGTPYWMAPEVISRLPYGTEVDIWSLGIMVIEMIDGEPPYFNEPPLQAMRRIRDSLPPRVKDLHKVSSVLRGFLDLMLVREPSQRATAQELLGHPFLKLAGPPSCIVPLMRQYRHH</t>
-  </si>
-  <si>
-    <t>TQTVHEFAKELDATNISIDKVVGAGEFGEVCSGRLKLPSKKEISVAIKTLKVGYTEKQRRDFLGEASIMGQFDHPNIIRLEGVVTKSKPVMIVTEYMENGSLDSFLRKHDAQFTVIQLVGMLRGIASGMKYLSDMGYVHRDLAARNILINSNLVCKVSDFGLSRVLEDDPEAAYTTRGGKIPIRWTSPEAIAYRKFTSASDVWSYGIVLWEVMSYGERPYWEMSNQDVIKAVDEGYRLPPPMDCPAALYQLMLDCWQKDRNNRPKFEQIVSILDKLIRNPGSLKIITSAAARPSNLLLDQSNVDITTFRTTGDWLNGVWTAHCKEIFTGVEYSSCDTIAKIS</t>
-  </si>
-  <si>
-    <t>QQFPQFHVKSGLQIKKNAIIDDYKVTSQVLGLGINGKVLQIFNKRTQEKFALKMLQDCPKARREVELHWRASQCPHIVRIVDVYENLYAGRKCLLIVMECLDGGELFSRIQDRGDQAFTEREASEIMKSIGEAIQYLHSINIAHRDVKPENLLYTSKRPNAILKLTDFGFAKETTSHNSLTTPCYTPYYVAPEVLGPEKYDKSCDMWSLGVIMYILLCGYPPFYSNHGLAISPGMKTRIRMGQYEFPNPEWSEVSEEVKMLIRNLLKTEPTQRMTITEFMNHPWIMQSTKVPQTPLHTSRVLKEDKERWEDVKGCLHDKNSDQA</t>
-  </si>
-  <si>
-    <t>CSK21_HUMAN_D0_3AXW_A</t>
-  </si>
-  <si>
-    <t>ATCTRFTDDYQLFEELGKGAFSVVRRCVKKTPTQEYAAKIINTKKLSARDHQKLEREARICRLLKHPNIVRLHDSISEEGFHYLVFDLVTGGELFEDIVAREYYSEADASHCIHQILESVNHIHQHDIVHRDLKPENLLLASKCKGAAVKLADFGLAIEVQGEQQAWFGFAGTPGYLSPEVLRKDPYGKPVDIWACGVILYILLVGYPPFWDEDQHKLYQQIKAGAYDFPSPEWDTVTPEAKNLINQMLTINPAKRITADQALKHPWVCQRSTVASMMHRQETVECLRKFNARRKLKGAILTTMLVSRNFS</t>
-  </si>
-  <si>
-    <t>VIDPSELTFVQEIGSGQFGLVHLGYWLNKDKVAIKTIREGAMSEEDFIEEAEVMMKLSHPKLVQLYGVCLEQAPICLVFEFMEHGCLSDYLRTQRGLFAAETLLGMCLDVCEGMAYLEEACVIHRDLAARNCLVGENQVIKVSDFGMTRFVLDDQYTSSTGTKFPVKWASPEVFSFSRYSSKSDVWSFGVLMWEVFSEGKIPYENRSNSEVVEDISTGFRLYKPRLASTHVYQIMNHCWKERPEDRPAFSRLLRQLAEIAESGL</t>
-  </si>
-  <si>
-    <t>CGTGTAAAAGCAGCTCAAGCTGGAAGACAGAGCTCTGCAAAGAGACATCTTGCAGAACAATTTGCAGTTGGAGAGATAATAACTGACATGGCAAAAAAGGAATGGAAAGTAGGATTACCCATTGGCCAAGGAGGCTTTGGCTGTATATATCTTGCTGATATGAATTCTTCAGAGTCAGTTGGCAGTGATGCACCTTGTGTTGTAAAAGTGGAACCCAGTGACAATGGACCTCTTTTTACTGAATTAAAGTTCTACCAACGAGCTGCAAAACCAGAGCAAATTCAGAAATGGATTCGTACCCGTAAGCTGAAGTACCTGGGTGTTCCTAAGTATTGGGGGTCTGGTCTACATGACAAAAATGGAAAAAGTTACAGGTTTATGATAATGGATCGCTTTGGGAGTGACCTTCAGAAAATATATGAAGCAAATGCCAAAAGGTTTTCTCGGAAAACTGTCTTGCAGCTAAGCTTAAGAATTCTGGATATTCTGGAATATATTCACGAGCATGAGTATGTGCATGGAGATATCAAGGCCTCAAATCTTCTTCTGAACTACAAGAATCCTGACCAGGTGTACTTGGTAGATTATGGCCTTGCTTATCGGTACTGCCCAGAAGGAGTTCATAAAGAATACAAAGAAGACCCCAAAAGATGTCACGATGGCACTATTGAATTCACGAGCATCGATGCACACAATGGCGTGGCCCCATCAAGACGTGGTGATTTGGAAATACTTGGTTATTGCATGATCCAATGGCTTACTGGCCATCTTCCTTGGGAGGATAATTTGAAAGATCCTAAATATGTTAGAGATTCCAAAATTAGATACAGAGAAAATATTGCAAGTTTGATGGACAAATGTTTTCCTGAGAAAAACAAACCAGGTGAAATTGCCAAATACATGGAAACAGTGAAATTACTAGACTACACTGAAAAACCTCTTTATGAAAATTTACGTGACATTCTTTTGCAAGGACTAAAAGCTATAGGAAGTAAGGATGATGGCAAATTGGACCTCAGTGTTGTGGAGAATGGAGGTTTGAAAGCAAAAACAATAACAAAGAAGCGAAAGAAAGAAATTGAAGAA</t>
-  </si>
-  <si>
-    <t>KS6A1_HUMAN_D0_3RNY_B</t>
-  </si>
-  <si>
-    <t>MP2K6_HUMAN_D0_3VN9_A</t>
-  </si>
-  <si>
-    <t>RVKAAQAGRQSSAKRHLAEQFAVGEIITDMAKKEWKVGLPIGQGGFGCIYLADMNSSESVGSDAPCVVKVEPSDNGPLFTELKFYQRAAKPEQIQKWIRTRKLKYLGVPKYWGSGLHDKNGKSYRFMIMDRFGSDLQKIYEANAKRFSRKTVLQLSLRILDILEYIHEHEYVHGDIKASNLLLNYKNPDQVYLVDYGLAYRYCPEGVHKEYKEDPKRCHDGTIEFTSIDAHNGVAPSRRGDLEILGYCMIQWLTGHLPWEDNLKDPKYVRDSKIRYRENIASLMDKCFPEKNKPGEIAKYMETVKLLDYTEKPLYENLRDILLQGLKAIGSKDDGKLDLSVVENGGLKAKTITKKRKKEIEE</t>
-  </si>
-  <si>
-    <t>MKNK1_HUMAN_D0_2HW6_B</t>
-  </si>
-  <si>
-    <t>MSLIRKKGFYKQDVNKTAWELPKTYVSPTHVGSGAYGSVCSAIDKRSGEKVAIKKLSRPFQSEIFAKRAYRELLLLKHMQHENVIGLLDVFTPASSLRNFYDFYLVMPFMQTDLQKIMGMEFSEEKIQYLVYQMLKGLKYIHSAGVVHRDLKPGNLAVNEDCELKILDFGLARHADAEMTGYVVTRWYRAPEVILSWMHYNQTVDIWSVVCIMAEMLTGKTLFKGKDYLDQLTQILKVTGVPGTEFVQKLNDKAAKSYIQSLPQTPRKDFTQLFPRASPQAADLLEKMLELDVDKRLTAAQALTHPFFEPFRDPEEETEAQQPFDDSLEHEKLTVDEWKQHIYKEIVNFSPI</t>
-  </si>
-  <si>
-    <t>AAPPAKEIPEVLVDPRSRRRYVRGRFLGKGGFAKCFEISDADTKEVFAGKIVPKSLLLKPHQREKMSMEISIHRSLAHQHVVGFHGFFEDNDFVFVVLELCRRRSLLELHKRRKALTEPEARYYLRQIVLGCQYLHRNRVIHRDLKLGNLFLNEDLEVKIGDFGLATKVEYDGERKKTLCGTPNYIAPEVLSKKGHSFEVDVWSIGCIMYTLLVGKPPFETSCLKETYLRIKKNEYSIPKHINPVAASLIQKMLQTDPTARPTINELLNDEFFTSGYIPARLPITCLTIPPRFSIAPSSLDPSNRKPLTVLNK</t>
-  </si>
-  <si>
-    <t>ITK_HUMAN_D0_3QGW_B</t>
-  </si>
-  <si>
-    <t>KS6A3_HUMAN_D1_4JG7_A</t>
-  </si>
-  <si>
-    <t>KCC4_HUMAN_D0_2W4O_A</t>
-  </si>
-  <si>
-    <t>CSK_HUMAN_D0_3D7T_A</t>
-  </si>
-  <si>
-    <t>KCC2A_HUMAN_D0_2VZ6_B</t>
-  </si>
-  <si>
-    <t>ATGTCTGATGAGGAGATCTTGGAGAAATTACGAAGCATAGTGAGTGTGGGCGATCCTAAGAAGAAATATACACGGTTTGAGAAGATTGGACAAGGTGCTTCAGGCACCGTGTACACAGCAATGGATGTGGCCACAGGACAGGAGGTGGCCATTAAGCAGATGAATCTTCAGCAGCAGCCCAAGAAAGAGCTGATTATTAATGAGATCCTGGTCATGAGGGAAAACAAGAACCCAAACATTGTGAATTACTTGGACAGTTACCTCGTGGGAGATGAGCTGTGGGTTGTTATGGAATACTTGGCTGGAGGCTCCTTGACAGATGTGGTGACAGAAACTTGCATGGATGAAGGCCAAATTGCAGCTGTGTGCCGTGAGTGTCTGCAGGCTCTGGAGTTCTTGCATTCGAACCAGGTCATTCACAGAGACATCAAGAGTGACAATATTCTGTTGGGAATGGATGGCTCTGTCAAGCTAACTGACTTTGGATTCTGTGCACAGATAACCCCAGAGCAGAGCAAACGGAGCACCATGGTAGGAACCCCATACTGGATGGCACCAGAGGTTGTGACACGAAAGGCCTATGGGCCCAAGGTTGACATCTGGTCCCTGGGCATCAAGGCCATCGAAATGATTGAAGGGGAGCCTCCATACCTCAATGAAAACCCTCTGAGAGCCTTGTACCTCATTGCCACCAATGGGACCCCAGAACTTCAGAACCCAGAGAAGCTGTCAGCTATCTTCCGGGACTTTCTGAACCGCTGTCTCGAGATGGATGTGGAGAAGAGAGGTTCAGCTAAAGAGCTGCTACAGCATCAATTCCTGAAGATTGCCAAGCCCCTCTCCAGCCTCACTCCACTTATTGCTGCAGCTAAGGAGGCAACAAAGAACAATCAC</t>
-  </si>
-  <si>
-    <t>ATGGAGGCAGCAGCATCCGAACCCTCTCTTGATCTAGATAATCTGAAACTGTTGGAGCTGATTGGCCGAGGTCGATATGGAGCAGTATATAAAGGCTCCTTGGATGAGCGTCCAGTTGCTGTAAAAGTGTTTTCCTTTGCAAACCGTCAGAATTTTATCAACGAAAAGAACATTTACAGAGTGCCTTTGATGGAACATGACAACATTGCCCGCTTTATAGTTGGAGATGAGAGAGTCACTGCAGATGGACGCATGGAATATTTGCTTGTGATGGAGTACTATCCCAATGGATCTTTATGCAAGTATTTAAGTCTCCACACAAGTGACTGGGTAAGCTCTTGCCGTCTTGCTCATTCTGTTACTAGAGGACTGGCTTATCTTCACACAGAATTACCACGAGGAGATCATTATAAACCTGCAATTTCCCATCGAGATTTAAACAGCAGAAATGTCCTAGTGAAAAATGATGGAACCTGTGTTATTAGTGACTTTGGACTGTCCATGAGGCTGACTGGAAATAGACTGGTGCGCCCAGGGGAGGAAGATAATGCAGCCATAAGCGAGGTTGGCACTATCAGATATATGGCACCAGAAGTGCTAGAAGGAGCTGTGAACTTGAGGGACTGTGAATCAGCTTTGAAACAAGTAGACATGTATGCTCTTGGACTAATCTATTGGGAGATATTTATGAGATGTACAGACCTCTTCCCAGGGGAATCCGTACCAGAGTACCAGATGGCTTTTCAGACAGAGGTTGGAAACCATCCCACTTTTGAGGATATGCAGGTTCTCGTGTCTAGGGAAAAACAGAGACCCAAGTTCCCAGAAGCCTGGAAAGAAAATAGCCTGGCAGTGAGGTCACTCAAGGAGACAATCGAAGACTGTTGGGACCAGGATGCAGAGGCTCGGCTTACTGCACAGTGTGCTGAGGAAAGGATGGCTGAACTTATGATGATTTGGGAAAGAAACAAATCTGTGAGCCCAACA</t>
-  </si>
-  <si>
-    <t>GGAGAAGCTCCCAACCAAGCTCTCTTGAGGATCTTGAAGGAAACTGAATTCAAAAAGATCAAAGTGCTGGGCTCCGGTGCGTTCGGCACGGTGTATAAGGGACTCTGGATCCCAGAAGGTGAGAAAGTTAAAATTCCCGTCGCTATCAAGGAATTAAGAGAAGCAACATCTCCGAAAGCCAACAAGGAAATCCTCGATGAAGCCTACGTGATGGCCAGCGTGGACAACCCCCACGTGTGCCGCCTGCTGGGCATCTGCCTCACCTCCACCGTGCAaCTCATCACGCAGCTCATGCCCTTCGGCTGCCTCCTGGACTATGTCCGGGAACACAAAGACAATATTGGCTCCCAGTACCTGCTCAACTGGTGTGTGCAGATCGCAAAGGGCATGAACTACTTGGAGGACCGTCGCTTGGTGCACCGCGACCTGGCAGCCAGGAACGTACTGGTGAAAACACCGCAGCATGTCAAGATCACAGATTTTGGGCgGGCCAAACTGCTGGGTGCGGAAGAGAAAGAATACCATGCAGAAGGAGGCAAAGTGCCTATCAAGTGGATGGCATTGGAATCAATTTTACACAGAATCTATACCCACCAGAGTGATGTCTGGAGCTACGGGGTGACCGTTTGGGAGTTGATGACCTTTGGATCCAAGCCATATGACGGAATCCCTGCCAGCGAGATCTCCTCCATCCTGGAGAAAGGAGAACGCCTCCCTCAGCCACCCATATGTACCATCGATGTCTACATGATCATGGTCAAGTGCTGGATGATAGACGCAGATAGTCGCCCAAAGTTCCGTGAGTTGATCATCGAATTCTCCAAAATGGCCCGAGACCCCCAGCGCTACCTTGTCATTCAGGGGGATGAAAGAATGCATTTGCCAAGTCCTACAGACTCCAACTTCTACCGTGCCCTGATGGATGAAGAAGACATGGACGACGTGGTGGATGCCGACGAGTACCTCATCCCACAGCAGGGC</t>
-  </si>
-  <si>
-    <t>GCCACCTGCACACGTTTCACCGACGACTACCAGCTCTTCGAGGAGCTTGGCAAGGGTGCTTTCTCTGTGGTCCGCAGGTGTGTGAAGAAAACCCCCACGCAGGAGTACGCAGCAAAAATCATCAATACCAAGAAATTGTCTGCCCGGGATCACCAGAAACTAGAACGTGAGGCTCGGATATGTCGACTTCTGAAACATCCAAACATCGTGCGCCTCCATGACAGTATTTCTGAAGAAGGGTTTCACTACCTCGTGTTTGACCTTGTTACCGGCGGGGAGCTGTTTGAAGACATTGTGGCCAGAGAGTACTACAGTGAAGCAGATGCCAGCCACTGTATACATCAGATTCTGGAGAGTGTTAACCACATCCACCAGCATGACATCGTCCACAGGGACCTGAAGCCTGAGAACCTGCTGCTGGCGAGTAAATGCAAGGGTGCCGCCGTCAAGCTGGCTGATTTTGGCCTAGCCATCGAAGTACAGGGAGAGCAGCAGGCTTGGTTTGGTTTTGCTGGCACCCCAGGTTACTTGTCCCCTGAGGTCTTGAGGAAAGATCCCTATGGAAAACCTGTGGATATCTGGGCCTGCGGGGTCATCCTGTATATCCTCCTGGTGGGCTATCCTCCCTTCTGGGATGAGGATCAGCACAAGCTGTATCAGCAGATCAAGGCTGGAGCCTATGATTTCCCATCACCAGAATGGGACACGGTAACTCCTGAAGCCAAGAACTTGATCAACCAGATGCTGACCATAAACCCAGCAAAGCGCATCACGGCTGACCAGGCTCTCAAGCACCCGTGGGTCTGTCAACGATCCACGGTGGCATCCATGATGCATCGTCAGGAGACTGTGGAGTGTTTGCGCAAGTTCAATGCCCGGAGAAAACTGAAGGGTGCCATCCTCACGACCATGCTTGTCTCCAGGAACTTCTCA</t>
-  </si>
-  <si>
-    <t>GAGACCTACATTAAGCTGGACAAACTGGGCGAGGGTACCTATGCCACCGTCTACAAAGGCAAAAGCAAGCTCACAGACAACCTTGTGGCACTCAAGGAGATCAGACTGGAACATGAAGAGGGGGCACCCTGCACCGCCATCCGGGAAGTGTCCCTACTCAAGGACCTCAAACACGCCAACATCGTTACGCTACATGACATTATCCACACGGAGAAGTCCCTCACCCTTGTCTTTGAGTACCTGGACAAGGACCTGAAGCAGTACCTGGATGACTGTGGGAACATCATCAACATGCACAACGTGAAACTGTTCCTGTTCCAGCTGCTCCGTGGCCTGGCCTACTGCCACCGGCAGAAGGTGCTACACCGAGACCTCAAGCCCCAGAACCTGCTCATCAACGAGAGGGGAGAGCTCAAGCTGGCTGACTTTGGCCTGGCCCGAGCCAAGTCAATCCCAACAAAGACATACTCCAATGAGGTGGTGACACTGTGGTACCGGCCCCCTGACATCCTGCTTGGGTCCACGGACTACTCCACTCAGATTGACATGTGGGGTGTGGGCTGCATCTTCTATGAGATGGCCACAGGCCGTCCCCTCTTTCCGGGCTCCACGGTGGAGGAACAGCTACACTTCATCTTCCGTATCTTAGGAACCCCAACTGAGGAGACGTGGCCAGGCATCCTGTCCAACGAGGAGTTCAAGACATACAACTACCCCAAGTACCGAGCCGAGGCCCTTTTGAGCCACGCACCCCGACTTGATAGCGACGGGGCCGACCTCCTCACCAAGCTGTTGCAGTTTGAGGGTCGAAATCGGATCTCCGCAGAGGATGCCATGAAACATCCATTCTTCCTCAGTCTGGGGGAGCGGATCCACAAACTTCCTGACACTACTTCCATATTTGCACTAAAGGAGATTCAGCTACAAAAGGAGGCCAGCCTTCGGTCT</t>
-  </si>
-  <si>
-    <t>MK13_HUMAN_D0_4EYJ_A</t>
-  </si>
-  <si>
-    <t>STK16_HUMAN_D0_2BUJ_B</t>
-  </si>
-  <si>
-    <t>ATGGAAAGCGACCTGCACCAGATCATCCACTCCTCACAGCCCCTCACACTGGAACACGTGCGCTACTTCCTGTACCAACTGCTGCGGGGCCTGAAGTACATGCACTCGGCTCAGGTCATCCACCGTGACCTGAAGCCCTCCAACCTATTGGTGAATGAGAACTGTGAGCTCAAGATTGGTGACTTTGGTATGGCTCGTGGCCTGTGCACCTCGCCCGCTGAACATCAGTACTTCATGACTGAGTATGTGGCCACGCGCTGGTACCGTGCGCCCGAGCTCATGCTCTCTTTGCATGAGTATACACAGGCTATTGACCTCTGGTCTGTGGGCTGCATCTTTGGTGAGATGCTGGCCCGGCGCCAGCTCTTCCCAGGCAAAAACTATGTACACCAGCTACAGCTCATCATGATGGTGCTGGGTACCCCATCACCAGCCGTGATTCAGGCTGTGGGGGCTGAGAGGGTGCGGGCCTATATCCAGAGCTTGCCACCACGCCAGCCTGTGCCCTGGGAGACAGTGTACCCAGGTGCCGACCGCCAGGCCCTATCACTGCTGGGTCGCATGCTGCGTTTTGAGCCCAGCGCTCGCATCTCAGCAGCTGCTGCCCTTCGCCACCCTTTCCTGGCCAAGTACCATGATCCTGATGATGAGCCTGACTGTGCCCCGCCCTTTGACTTTGCCTTTGACCGCGAAGCCCTCACTCGGGAGCGCATTAAGGAGGCCATTGTGGCTGAAATTGAGGACTTCCATGCAAGGCGTGAGGGCATCCGCCAACAGATCCGCTTCCAGCCTTCTCTACAGCCTGTGGCTAGTGAGCCTGGCTGTCCAGATGTTGAAATGCCCAGTCCCTGGGCTCCCAGTGGGGACTGTGCCATG</t>
-  </si>
-  <si>
-    <t>CAGAGCAGTAAGCGCAGCAGCCGGAGTGTGGAAGATGACAAGGAGGGTCACCTGGTGTGCCGGATCGGCGATTGGCTCCAAGAGCGATATGAGATTGTGGGGAACCTGGGTGAAGGCACCTTTGGCAAGGTGGTGGAGTGCTTGGACCATGCCAGAGGGAAGTCTCAGGTTGCCCTGAAGATCATCCGCAACGTGGGCAAGTACCGGGAGGCTGCCCGGCTAGAAATCAACGTGCTCAAAAAAATCAAGGAGAAGGACAAAGAAAACAAGTTCCTGTGTGTCTTGATGTCTGACTGGTTCAACTTCCACGGTCACATGTGCATCGCCTTTGAGCTCCTGGGCAAGAACACCTTTGAGTTCCTGAAGGAGAATAACTTCCAGCCTTACCCCCTACCACATGTCCGGCACATGGCCTACCAGCTCTGCCACGCCCTTAGATTTCTGCATGAGAATCAGCTGACCCATACAGACTTGAAACCAGAGAACATCCTGTTTGTGAATTCTGAGTTTGAAACCCTCTACAATGAGCACAAGAGCTGTGAGGAGAAGTCAGTGAAGAACACCAGCATCCGAGTGGCTGACTTTGGCAGTGCCACATTTGACCATGAGCACCACACCACCATTGTGGCCACCCGTCACTATCGCCCGCCTGAGGTGATCCTTGAGCTGGGCTGGGCACAGCCCTGTGACGTCTGGAGCATTGGCTGCATTCTCTTTGAGTACTACCGGGGCTTCACACTCTTCCAGACCCACGAAAACCGAGAGCACCTGGTGATGATGGAGAAGATCCTAGGGCCCATCCCATCACACATGATCCACCGTACCAGGAAGCAGAAATATTTCTACAAAGGGGGCCTAGTTTGGGATGAGAACAGCTCTGACGGCCGGTATGTGAAGGAGAACTGCAAACCTCTGAAGAGTTACATGCTCCAAGACTCCCTGGAGCACGTGCAGCTGTTTGACCTGATGAGGAGGATGTTAGAATTTGACCCTGCCCAGCGCATCACACTGGCCGAGGCCCTGCTGCACCCCTTCTTTGCTGGCCTGACCCCTGAGGAGCGGTCCTTCCACACC</t>
-  </si>
-  <si>
-    <t>GAACTGAAGGATGACGACTTTGAGAAGATCAGTGAGCTGGGGGCTGGCAATGGCGGTGTGGTGTTCAAGGTCTCCCACAAGCCTTCTGGCCTGGTCATGGCCAGAAAGCTAATTCATCTGGAGATCAAACCCGCAATCCGGAACCAGATCATAAGGGAGCTGCAGGTTCTGCATGAGTGCAACTCTCCGTACATCGTGGGCTTCTATGGTGCGTTCTACAGCGATGGCGAGATCAGTATCTGCATGGAGCACATGGATGGAGGTTCTCTGGATCAAGTCCTGAAGAAAGCTGGAAGAATTCCTGAACAAATTTTAGGAAAAGTTAGCATTGCTGTAATAAAAGGCCTGACATATCTGAGGGAGAAGCACAAGATCATGCACAGAGCATACGGAATGGACAGCCGACCTCCCATGGCAATTTTTGAGTTGTTGGATTACATAGTCAACGAGCCTCCTCCAAAACTGCCCAGTGGAGTGTTCAGTCTGGAATTTCAAGATTTTGTGAATAAATGCTTAATAAAAAACCCCGCAGAGAGAGCAGATTTGAAGCAACTCATGGTTCATGCTTTTATCAAGAGATCTGATGCTGAGGAAGTGGATTTTGCAGGTTGGCTCTGCTCCACCATCGGCCTTAAC</t>
-  </si>
-  <si>
-    <t>MQTVGVHSIVQQLHRNSIQFTDGYEVKEDIGVGSYSVCKRCIHKATNMEFAVKIIDKSKRDPTEEIEILLRYGQHPNIITLKDVYDDGKYVYVVTELMKGGELLDKILRQKFFSEREASAVLFTITKTVEYLHAQGVVHRDLKPSNILYVDESGNPESIRICDFGFAKQLRAENGLLMTPCYTANFVAPEVLKRQGYDAACDIWSLGVLLYTMLTGYTPFANGPDDTPEEILARIGSGKFSLSGGYWNSVSDTAKDLVSKMLHVDPHQRLTAALVLRHPWIVHWDQLPQYQLNRQDAPHLVKGAMAATYSALNRNQSPVLEPVGRSTLAQRRGIKKITSTAL</t>
-  </si>
-  <si>
-    <t>KAPCA_HUMAN_D0_4AE9_A</t>
-  </si>
-  <si>
-    <t>KCC2G_HUMAN_D0_2V7O_A</t>
-  </si>
-  <si>
-    <t>KQYEHVKRDLNPEDFWEIIGELGDGAFGKVYKAQNKETSVLAAAKVIDTKSEEELEDYMVEIDILASCDHPNIVKLLDAFYYENNLWILIEFCAGGAVDAVMLELERPLTESQIQVVCKQTLDALNYLHDNKIIHRDLKAGNILFTLDGDIKLADFGVSAKNMRTIQRRDSFIGTPYWMAPEVVMCETSKDRPYDYKADVWSLGITLIEMAEIEPPHHELNPMRVLLKIAKSEPPTLAQPSRWSSNFKDFLKKCLEKNVDARWTTSQLLQHPFVTVDSNKPIRELIAEAKAEVTEEVEDGKE</t>
-  </si>
-  <si>
-    <t>ACCCAAACTGTTCATGAGTTTGCCAAGGAATTGGATGCCACCAACATATCCATTGATAAAGTTGTTGGAGCAGGTGAATTTGGAGAGGTGTGCAGTGGTCGCTTAAAACTTCCTTCAAAAAAAGAGATTTCAGTGGCCATTAAGACCCTGAAAGTTGGCTACACAGAAAAGCAGAGGAGAGACTTCCTGGGAGAAGCAAGCATTATGGGACAGTTTGACCACCCCAATATCATTCGACTGGAAGGAGTTGTTACCAAAAGTAAGCCAGTTATGATTGTCACAGAATACATGGAGAATGGTTCCTTGGATAGTTTCCTACGTAAACACGATGCCCAGTTTACTGTCATTCAGCTAGTGGGGATGCTTCGAGGGATAGCATCTGGCATGAAGTACCTGTCAGACATGGGCTATGTTCACCGAGACCTCGCTGCTCGGAACATCTTGATCAACAGTAACTTGGTGTGTAAGGTTTCTGATTTCGGACTTTCGCGTGTCCTGGAGGATGACCCAGAAGCTGCTTATACAACAAGAGGAGGGAAGATCCCAATCAGGTGGACATCACCAGAAGCTATAGCCTACCGCAAGTTCACGTCAGCCAGCGATGTATGGAGTTATGGGATTGTTCTCTGGGAGGTGATGTCTTATGGAGAGAGACCATACTGGGAGATGTCCAATCAGGATGTAATTAAAGCTGTAGATGAGGGCTATCGACTGCCACCCCCCATGGACTGCCCAGCTGCCTTGTATCAGCTGATGCTGGACTGCTGGCAGAAAGACAGGAACAACAGACCCAAGTTTGAGCAGATTGTTAGTATTCTGGACAAGCTTATCCGGAATCCCGGCAGCCTGAAGATCATCACCAGTGCAGCCGCAAGGCCATCAAACCTTCTTCTGGACCAAAGCAATGTGGATATCACTACCTTCCGCACAACAGGTGACTGGCTTAATGGTGTCTGGACAGCACACTGCAAGGAAATCTTCACGGGTGTGGAGTACAGTTCTTGTGACACAATAGCCAAGATTTCC</t>
-  </si>
-  <si>
-    <t>MEKDGLCRADQQYECVAEIGEGAYGKVFKARDLKNGGRFVALKRVRVQTGEEGMPLSTIREVAVLRHLETFEHPNVVRLFDVCTVSRTDRETKLTLVFEHVDQDLTTYLDKVPEPGVPTETIKDMMFQLLRGLDFLHSHRVVHRDLKPQNILVTSSGQIKLADFGLARIYSFQMALTSVVVTLWYRAPEVLLQSSYATPVDLWSVGCIFAEMFRRKPLFRGSSDVDQLGKILDVIGLPGEEDWPRDVALPRQAFHSKSAQPIEKFVTDIDELGKDLLLKCLTFNPAKRISAYSALSHPYFQ</t>
-  </si>
-  <si>
-    <t>EPHA3_HUMAN_D0_4GK2_A</t>
-  </si>
-  <si>
-    <t>ATGCCCGGCCCGGCCGCGGGCAGCAGGGCCCGGGTCTACGCCGAGGTGAACAGTCTGAGGAGCCGCGAGTACTGGGACTACGAGGCTCACGTCCCGAGCTGGGGTAATCAAGATGATTACCAACTGGTTCGAAAACTTGGTCGGGGAAAATATAGTGAAGTATTTGAGGCCATTAATATCACCAACAATGAGAGAGTGGTTGTAAAAATCCTGAAGCCAGTGAAGAAAAAGAAGATAAAACGAGAGGTTAAGATTCTGGAGAACCTTCGTGGTGGAACAAATATCATTAAGCTGATTGACACTGTAAAGGACCCCGTGTCAAAGACACCAGCTTTGGTATTTGAATATATCAATAATACAGATTTTAAGCAACTCTACCAGATCCTGACAGACTTTGATATCCGGTTTTATATGTATGAACTACTTAAAGCTCTGGATTACTGCCACAGCAAGGGAATCATGCACAGGGATGTGAAACCTCACAATGTCATGATAGATCACCAACAGAAAAAGCTGCGACTGATAGATTGGGGTCTGGCAGAATTCTATCATCCTGCTCAGGAGTACAATGTTCGTGTAGCCTCAAGGTACTTCAAGGGACCAGAGCTCCTCGTGGACTATCAGATGTATGATTATAGCTTGGACATGTGGAGTTTGGGCTGTATGTTAGCAAGCATGATCTTTCGAAGGGAACCATTCTTCCATGGACAGGACAACTATGACCAGCTTGTTCGCATTGCCAAGGTTCTGGGTACAGAAGAACTGTATGGGTATCTGAAGAAGTATCACATAGACCTAGATCCACACTTCAACGATATCCTGGGACAACATTCACGGAAACGCTGGGAAAACTTTATCCATAGTGAGAACAGACACCTTGTCAGCCCTGAGGCCCTAGATCTTCTGGACAAACTTCTGCGATACGACCATCAACAGAGACTGACTGCCAAAGAGGCCATGGAGCACCCATACTTCTACCCTGTGGTGAAGGAGCAGTCCCAG</t>
-  </si>
-  <si>
-    <t>ATGTCGGGACCCGTGCCAAGCAGGGCCAGAGTTTACACAGATGTTAATACACACAGACCTCGAGAATACTGGGATTACGAGTCACATGTGGTGGAATGGGGAAATCAAGATGACTACCAGCTGGTTCGAAAATTAGGCCGAGGTAAATACAGTGAAGTATTTGAAGCCATCAACATCACAAATAATGAAAAAGTTGTTGTTAAAATTCTCAAGCCAGTAAAAAAGAAGAAAATTAAGCGTGAAATAAAGATTTTGGAGAATTTGAGAGGAGGTCCCAACATCATCACACTGGCAGACATTGTAAAAGACCCTGTGTCACGAACCCCCGCCTTGGTTTTTGAACACGTAAACAACACAGACTTCAAGCAATTGTACCAGACGTTAACAGACTATGATATTCGATTTTACATGTATGAGATTCTGAAGGCCCTGGATTATTGTCACAGCATGGGAATTATGCACAGAGATGTCAAGCCCCATAATGTCATGATTGATCATGAGCACAGAAAGCTACGACTAATAGACTGGGGTTTGGCTGAGTTTTATCATCCTGGCCAAGAATATAATGTCCGAGTTGCTTCCCGATACTTCAAAGGTCCTGAGCTACTTGTAGACTATCAGATGTACGATTATAGTTTGGATATGTGGAGTTTGGGTTGTATGCTGGCAAGTATGATCTTTCGGAAGGAGCCATTTTTCCATGGACATGACAATTATGATCAGTTGGTGAGGATAGCCAAGGTTCTGGGGACAGAAGATTTATATGACTATATTGACAAATACAACATTGAATTAGATCCACGTTTCAATGATATCTTGGGCAGACACTCTCGAAAGCGATGGGAACGCTTTGTCCACAGTGAAAATCAGCACCTTGTCAGCCCTGAGGCCTTGGATTTCCTGGACAAACTGCTGCGATATGACCACCAGTCACGGCTTACTGCAAGAGAGGCAATGGAGCACCCCTATTTCTACACTGTTGTGAAGGACCAGGCTCGAATGGGT</t>
-  </si>
-  <si>
-    <t>NEK2_HUMAN_D0_2XKE_A</t>
-  </si>
-  <si>
-    <t>MK01_HUMAN_D0_4FMQ_A</t>
-  </si>
-  <si>
-    <t>ATGGAGCTGAGAGTCGGGAACAGGTACCGGCTGGGCCGGAAGATCGGCAGCGGCTCCTTCGGAGACATCTATCTCGGTACGGACATTGCTGCAGGAGAAGAGGTTGCCATCAAGCTTGAATGTGTCAAAACCAAACACCCTCAGCTCCACATTGAGAGCAAAATCTACAAGATGATGCAGGGAGGAGTGGGCATCCCCACCATCAGATGGTGCGGGGCAGAGGGGGACTACAACGTCATGGTGATGGAGCTGCTGGGGCCAAGCCTGGAGGACCTCTTCAACTTCTGCTCCAGGAAATTCAGCCTCAAAACCGTCCTGCTGCTTGCTGACCAAATGATCAGTCGCATCGAATACATTCATTCAAAGAACTTCATCCACCGGGATGTGAAGCCAGACAACTTCCTCATGGGCCTGGGGAAGAAGGGCAACCTGGTGTACATCATCGACTTCGGGCTGGCCAAGAAGTACCGGGATGCACGCACCCACCAGCACATCCCCTATCGTGAGAACAAGAACCTCACGGGGACGGCGCGGTACGCCTCCATCAACACGCACCTTGGAATTGAACAATCCCGAAGAGATGACTTGGAGTCTCTGGGCTACGTGCTAATGTACTTCAACCTGGGCTCTCTCCCCTGGCAGGGGCTGAAGGCTGCCACCAAGAGACAGAAATACGAAAGGATTAGCGAGAAGAAAATGTCCACCCCCATCGAAGTGTTGTGTAAAGGCTACCCTTCCGAATTTGCCACATACCTGAATTTCTGCCGTTCCTTGCGTTTTGACGACAAGCCTGACTACTCGTACCTGCGGCAGCTTTTCCGGAATCTGTTCCATCGCCAGGGCTTCTCCTATGACTACGTGTTCGACTGGAACATGCTCAAA</t>
-  </si>
-  <si>
-    <t>ATGGCGGCGGCGGCGGCGGCGGGCGCGGGCCCGGAGATGGTCCGCGGGCAGGTGTTCGACGTGGGGCCGCGCTACACCAACCTCTCGTACATCGGCGAGGGCGCCTACGGCATGGTGTGCTCTGCTTATGATAATGTCAACAAAGTTCGAGTAGCTATCAAGAAAATCAGCCCCTTTGAGCACCAGACCTACTGCCAGAGAACCCTGAGGGAGATAAAAATCTTACTGCGCTTCAGACATGAGAACATCATTGGAATCAATGACATTATTCGAGCACCAACCATCGAGCAAATGAAAGATGTATATATAGTACAGGACCTCATGGAAACAGATCTTTACAAGCTCTTGAAGACACAACACCTCAGCAATGACCATATCTGCTATTTTCTCTACCAGATCCTCAGAGGGTTAAAATATATCCATTCAGCTAACGTTCTGCACCGTGACCTCAAGCCTTCCAACCTGCTGCTCAACACCACCTGTGATCTCAAGATCTGTGACTTTGGCCTGGCCCGTGTTGCAGATCCAGACCATGATCACACAGGGTTCCTGACAGAATATGTGGCCACACGTTGGTACAGGGCTCCAGAAATTATGTTGAATTCCAAGGGCTACACCAAGTCCATTGATATTTGGTCTGTAGGCTGCATTCTGGCAGAAATGCTTTCTAACAGGCCCATCTTTCCAGGGAAGCATTATCTTGACCAGCTGAACCACATTTTGGGTATTCTTGGATCCCCATCACAAGAAGACCTGAATTGTATAATAAATTTAAAAGCTAGGAACTATTTGCTTTCTCTTCCACACAAAAATAAGGTGCCATGGAACAGGCTGTTCCCAAATGCTGACTCCAAAGCTCTGGACTTATTGGACAAAATGTTGACATTCAACCCACACAAGAGGATTGAAGTAGAACAGGCTCTGGCCCACCCATATCTGGAGCAGTATTACGACCCGAGTGACGAGCCCATCGCCGAAGCACCATTCAAGTTCGACATGGAATTGGATGACTTGCCTAAGGAAAAGCTCAAAGAACTAATTTTTGAAGAGACTGCTAGATTCCAGCCAGGATACAGATCT</t>
-  </si>
-  <si>
-    <t>MDEQSQGMQGPPVPQFQPQKALRPDMGYNTLANFRIEKKIGRGQFSEVYRAACLLDGVPVALKKVQIFDLMDAKARADCIKEIDLLKQLNHPNVIKYYASFIEDNELNIVLELADAGDLSRMIKHFKKQKRLIPERTVWKYFVQLCSALEHMHSRRVMHRDIKPANVFITATGVVKLGDLGLGRFFSSKTTAAHSLVGTPYYMSPERIHENGYNFKSDIWSLGCLLYEMAALQSPFYGDKMNLYSLCKKIEQCDYPPLPSDHYSEELRQLVNMCINPDPEKRPDVTYVYDVAKRMHACTASS</t>
-  </si>
-  <si>
-    <t>GECSQKGPVPFSHCLPTEKLQRCEKIGEGVFGEVFQTIADHTPVAIKIIAIEGPDLVNGSHQKTFEEILPEIIISKELSLLSGEVCNRTEGFIGLNSVHCVQGSYPPLLLKAWDHYNSTKGSANDRPDFFKDDQLFIVLEFEFGGIDLEQMRTKLSSLATAKSILHQLTASLAVAEASLRFEHRDLHWGNVLLKKTSLKKLHYTLNGKSSTIPSCGLQVSIIDYTLSRLERDGIVVFCDVSMDEDLFTGDGDYQFDIYRLMKKENNNRWGEYHPYSNVLWLHYLTDKMLKQMTFKTKCNTPAMKQIKRKIQEFHRTMLNFSSATDLLCQHRLFK</t>
-  </si>
-  <si>
-    <t>MENFNNFYILTSKELGRGKFAVVRQCISKSTGQEYAAKFLKKRRRGQDCRAEILHEIAVLELAKSCPRVINLHEVYENTSEIILILEYAAGGEIFSLCLPELAEMVSENDVIRLIKQILEGVYYLHQNNIVHLDLKPQNILLSSIYPLGDIKIVDFGMSRKIGHACELREIMGTPEYLAPEILNYDPITTATDMWNIGIIAYMLLTHTSPFVGEDNQETYLNISQVNVDYSEETFSSVSQLATDFIQSLLVKNPEKRPTAEICLSHSWLQQWDFENLFHPEETSSSSQTQDHSVRSSEDKTSKSS</t>
-  </si>
-  <si>
-    <t>GCTGATCCAGAAGAACTGTTCACAAAATTAGAGCGCATTGGGAAAGGCTCATTTGGGGAAGTTTTCAAAGGAATTGATAACCGTACCCAGCAAGTCGTTGCTATTAAAATCATAGACCTTGAGGAAGCCGAAGATGAAATAGAAGACATTCAGCAAGAAATAACTGTCTTGAGTCAATGTGACAGCTCATATGTAACAAAATACTATGGGTCATATTTAAAGGGGTCTAAATTATGGATAATAATGGAATACCTGGGCGGTGGTTCAGCACTGGATCTTCTTCGAGCTGGTCCATTTGATGAGTTCCAGATTGCTACCATGCTAAAGGAAATTTTAAAAGGTCTGGACTATCTGCATTCAGAAAAGAAAATTCACCGAGACATAAAAGCTGCCAATGTCTTGCTCTCAGAACAAGGAGATGTTAAACTTGCTGATTTTGGAGTTGCTGGTCAGCTGACAGATACACAGATTAAAAGAAATACCTTTGTGGGAACTCCATTTTGGATGGCTCCTGAAGTTATTCAACAGTCAGCTTATGACTCAAAAGCTGACATTTGGTCATTGGGAATTACTGCTATTGAACTAGCCAAGGGAGAGCCACCTAACTCCGATATGCATCCAATGAGAGTTCTGTTTCTTATTCCCAAAAACAATCCTCCAACTCTTGTTGGAGACTTTACTAAGTCTTTTAAGGAGTTTATTGATGCTTGCCTGAACAAAGATCCATCATTTCGTCCTACAGCAAAAGAACTTCTGAAACACAAATTCATTGTAAAAAATTCAAAGAAGACTTCTTATCTGACTGAACTGATAGATCGTTTTAAGAGATGGAAGGCAGAA</t>
-  </si>
-  <si>
-    <t>MELRVGNKYRLGRKIGSGSFGDIYLGANIASGEEVAIKLECVKTKHPQLHIESKFYKMMQGGVGIPSIKWCGAEGDYNVMVMELLGPSLEDLFNFCSRKFSLKTVLLLADQMISRIEYIHSKNFIHRDVKPDNFLMGLGKKGNLVYIIDFGLAKKYRDARTHQHIPYRENKNLTGTARYASINTHLGIEQSRRDDLESLGYVLMYFNLGSLPWQGLKAATKRQKYERISEKKMSTPIEVLCKGYPSEFSTYLNFCRSLRFDDKPDYSYLRQLFRNLFHRQGFSYDYVFDWNMLK</t>
-  </si>
-  <si>
-    <t>SSVTASAAPGTASLVPDYWIDGSNRDALSDFFEVESELGRGATSIVYRCKQKGTQKPYALKVLKKTVDKKIVRTEIGVLLRLSHPNIIKLKEIFETPTEISLVLELVTGGELFDRIVEKGYYSERDAADAVKQILEAVAYLHENGIVHRDLKPENLLYATPAPDAPLKIADFGLSKIVEHQVLMKTVCGTPGYCAPEILRGCAYGPEVDMWSVGIITYILLCGFEPFYDERGDQFMFRRILNCEYYFISPWWDEVSLNAKDLVRKLIVLDPKKRLTTFQALQHPWVTGKAANFVHMDTAQKKLQEFNARRKLKAAVKAVVASSRLG</t>
-  </si>
-  <si>
-    <t>dna_end</t>
-  </si>
-  <si>
-    <t>MADDDVLFEDVYELCEVIGKGPFSVVRRCINRETGQQFAVKIVDVAKFTSSPGLSTEDLKREASICHMLKHPHIVELLETYSSDGMLYMVFEFMDGADLCFEIVKRADAGFVYSEAVASHYMRQILEALRYCHDNNIIHRDVKPHCVLLASKENSAPVKLGGFGVAIQLGESGLVAGGRVGTPHFMAPEVVKREPYGKPVDVWGCGVILFILLSGCLPFYGTKERLFEGIIKGKYKMNPRQWSHISESAKDLVRRMLMLDPAERITVYEALNHPWLKERDRYAYKIHLPETVEQLRKFNARRKLKGAVLAAVSSHKFNSFYGDPPEELPDFSEDPTSSGA</t>
-  </si>
-  <si>
-    <t>FAK1_HUMAN_D0_2IJM_B</t>
-  </si>
-  <si>
-    <t>CHK2_HUMAN_D0_2CN5_A</t>
-  </si>
-  <si>
-    <t>GTGATCGACCCCTCAGAGCTCACTTTTGTCCAAGAGATTGGCAGTGGGCAATTTGGGTTGGTGCATCTGGGCTACTGGCTCAACAAGGACAAGGTGGCTATCAAAACCATTCGGGAAGGGGCTATGTCAGAAGAGGACTTCATAGAGGAGGCTGAAGTAATGATGAAACTCTCTCATCCCAAACTGGTGCAGCTGTATGGGGTGTGCCTGGAGCAGGCCCCCATCTGCCTGGTGTTTGAGTTCATGGAGCACGGCTGCCTGTCAGATTATCTACGCACCCAGCGGGGACTTTTTGCTGCAGAGACCCTGCTGGGCATGTGTCTGGATGTGTGTGAGGGCATGGCCTACCTGGAAGAGGCATGTGTCATCCACAGAGACTTGGCTGCCAGAAATTGTTTGGTGGGAGAAAACCAAGTCATCAAGGTGTCTGACTTTGGGATGACAAGGTTCGTTCTGGATGATCAGTACACCAGTTCCACAGGCACCAAATTCCCGGTGAAGTGGGCATCCCCAGAGGTTTTCTCTTTCAGTCGCTATAGCAGCAAGTCCGATGTGTGGTCATTTGGTGTGCTGATGTGGGAAGTTTTCAGTGAAGGCAAAATCCCGTATGAAAACCGAAGCAACTCAGAGGTGGTGGAAGACATCAGTACCGGATTTCGGTTGTACAAGCCCCGGCTGGCCTCCACACACGTCTACCAGATTATGAATCACTGCTGGAAAGAGAGACCAGAAGATCGGCCAGCCTTCTCCAGACTGCTGCGTCAACTGGCTGAAATTGCAGAATCAGGACTT</t>
-  </si>
-  <si>
-    <t>MSDEEILEKLRSIVSVGDPKKKYTRFEKIGQGASGTVYTAMDVATGQEVAIKQMNLQQQPKKELIINEILVMRENKNPNIVNYLDSYLVGDELWVVMEYLAGGSLTDVVTETCMDEGQIAAVCRECLQALEFLHSNQVIHRDIKSDNILLGMDGSVKLTDFGFCAQITPEQSKRSTMVGTPYWMAPEVVTRKAYGPKVDIWSLGIKAIEMIEGEPPYLNENPLRALYLIATNGTPELQNPEKLSAIFRDFLNRCLEMDVEKRGSAKELLQHQFLKIAKPLSSLTPLIAAAKEATKNNH</t>
-  </si>
-  <si>
-    <t>MSQSKGKKRNPGLKIPKEAFEQPQTSSTPPRDLDSKACISIGNQNFEVKADDLEPIMELGRGAYGVVEKMRHVPSGQIMAVKRIRATVNSQEQKRLLMDLDISMRTVDCPFTVTFYGALFREGDVWICMELMDTSLDKFYKQVIDKGQTIPEDILGKIAVSIVKALEHLHSKLSVIHRDVKPSNVLINALGQVKMCDFGISGYLVDSVAKTIDAGCKPYMAPERINPELNQKGYSVKSDIWSLGITMIELAILRFPYDSWGTPFQQLKQVVEEPSPQLPADKFSAEFVDFTSQCLKKNSKERPTYPELMQHPFFTLHESKGTDVASFVKLILGD</t>
-  </si>
-  <si>
-    <t>DYRK2_HUMAN_D0_3KVW_A</t>
-  </si>
-  <si>
-    <t>GCGGCTCCACCGGCGAAAGAGATCCCGGAGGTCCTAGTGGACCCACGCAGCCGGCGGCGCTATGTGCGGGGCCGCTTTTTGGGCAAGGGCGGCTTTGCCAAGTGCTTCGAGATCTCGGACGCGGACACCAAGGAGGTGTTCGCGGGCAAGATTGTGCCTAAGTCTCTGCTGCTCAAGCCGCACCAGAGGGAGAAGATGTCCATGGAAATATCCATTCACCGCAGCCTCGCCCACCAGCACGTCGTAGGATTCCACGGCTTTTTCGAGGACAACGACTTCGTGTTCGTGGTGTTGGAGCTCTGCCGCCGGAGGTCTCTCCTGGAGCTGCACAAGAGGAGGAAAGCCCTGACTGAGCCTGAGGCCCGATACTACCTACGGCAAATTGTGCTTGGCTGCCAGTACCTGCACCGAAACCGAGTTATTCATCGAGACCTCAAGCTGGGCAACCTTTTCCTGAATGAAGATCTGGAGGTGAAAATAGGGGATTTTGGACTGGCAACCAAAGTCGAATATGACGGGGAGAGGAAGAAGACCCTGTGTGGGACTCCTAATTACATAGCTCCCGAGGTGCTGAGCAAGAAAGGGCACAGTTTCGAGGTGGATGTGTGGTCCATTGGGTGTATCATGTATACCTTGTTAGTGGGCAAACCACCTTTTGAGACTTCTTGCCTAAAAGAGACCTACCTCCGGATCAAGAAGAATGAATACAGTATTCCCAAGCACATCAACCCCGTGGCCGCCTCCCTCATCCAGAAGATGCTTCAGACAGATCCCACTGCCCGCCCAACCATTAACGAGCTGCTTAATGACGAGTTCTTTACTTCTGGCTATATCCCTGCCCGTCTCCCCATCACCTGCCTGACCATTCCACCAAGGTTTTCGATTGCTCCCAGCAGCCTGGACCCCAGCAACCGGAAGCCCCTCACAGTCCTCAATAAA</t>
-  </si>
-  <si>
-    <t>QSSKRSSRSVEDDKEGHLVCRIGDWLQERYEIVGNLGEGTFGKVVECLDHARGKSQVALKIIRNVGKYREAARLEINVLKKIKEKDKENKFLCVLMSDWFNFHGHMCIAFELLGKNTFEFLKENNFQPYPLPHVRHMAYQLCHALRFLHENQLTHTDLKPENILFVNSEFETLYNEHKSCEEKSVKNTSIRVADFGSATFDHEHHTTIVATRHYRPPEVILELGWAQPCDVWSIGCILFEYYRGFTLFQTHENREHLVMMEKILGPIPSHMIHRTRKQKYFYKGGLVWDENSSDGRYVKENCKPLKSYMLQDSLEHVQLFDLMRRMLEFDPAQRITLAEALLHPFFAGLTPEERSFHT</t>
-  </si>
-  <si>
-    <t>MK07_HUMAN_D0_4IC7_D</t>
-  </si>
-  <si>
-    <t>ATGCAGACAGTTGGTGTACATTCAATTGTTCAGCAGTTACACAGGAACAGTATTCAGTTTACTGATGGATATGAAGTAAAAGAAGATATTGGAGTTGGCTCCTACTCTGTTTGCAAGAGATGTATACATAAAGCTACAAACATGGAGTTTGCAGTGAAGATTATTGATAAAAGCAAGAGAGACCCAACAGAAGAAATTGAAATTCTTCTTCGTTATGGACAGCATCCAAACATTATCACTCTAAAGGATGTATATGATGATGGAAAGTATGTGTATGTAGTAACAGAACTTATGAAAGGAGGTGAATTGCTGGATAAAATTCTTAGACAAAAATTTTTCTCTGAACGAGAGGCCAGTGCTGTCCTGTTCACTATAACTAAAACCGTTGAATATCTTCACGCACAAGGGGTGGTTCATAGAGACTTGAAACCTAGCAACATTCTTTATGTGGATGAATCTGGTAATCCGGAATCTATTCGAATTTGTGATTTTGGCTTTGCAAAACAGCTGAGAGCGGAAAATGGTCTTCTCATGACTCCTTGTTACACTGCAAATTTTGTTGCACCAGAGGTTTTAAAAAGACAAGGCTATGATGCTGCTTGTGATATATGGAGTCTTGGTGTCCTACTCTATACAATGCTTACCGGTTACACTCCATTTGCAAATGGTCCTGATGATACACCAGAGGAAATATTGGCACGAATAGGTAGCGGAAAATTCTCACTCAGTGGTGGTTACTGGAATTCTGTTTCAGACACAGCAAAGGACCTGGTGTCAAAGATGCTTCATGTAGACCCTCATCAGAGACTGACTGCTGCTCTTGTGCTCAGACATCCTTGGATCGTCCACTGGGACCAACTGCCACAATACCAACTAAACAGACAGGATGCACCACATCTAGTAAAGGGTGCCATGGCAGCTACATATTCTGCTTTGAACCGTAATCAGTCACCAGTTTTGGAACCAGTAGGCCGCTCTACTCTTGCTCAGCGGAGAGGTATTAAAAAAATCACCTCAACAGCCCTG</t>
-  </si>
-  <si>
-    <t>KS6A3_HUMAN_D0_4JG7_A</t>
-  </si>
-  <si>
-    <t>MGKVKATPMTPEQAMKQYMQKLTAFEHHEIFSYPEIYFLGLNAKKRQGMTGGPNNGGYDDDQGSYVQVPHDHVAYRYEVLKVIGKGSFGQVVKAYDHKVHQHVALKMVRNEKRFHRQAAEEIRILEHLRKQDKDNTMNVIHMLENFTFRNHICMTFELLSMNLYELIKKNKFQGFSLPLVRKFAHSILQCLDALHKNRIIHCDLKPENILLKQQGRSGIKVIDFGSSCYEHQRVYTYIQSRFYRAPEVILGARYGMPIDMWSLGCILAELLTGYPLLPGEDEGDQLACMIELLGMPSQKLLDASKRAKNFVSSKGYPRYCTVTTLSDGSVVLNGGRSRRGKLRGPPESREWGNALKGCDDPLFLDFLKQCLEWDPAVRMTPGQALRHPWLRRRLPKPPTGEKTSVKR</t>
-  </si>
-  <si>
-    <t>CAGCAGTTCCCGCAGTTCCACGTCAAGTCCGGCCTGCAGATCAAGAAGAACGCCATCATCGATGACTACAAGGTCACCAGCCAGGTCCTGGGGCTGGGCATCAACGGCAAAGTTTTGCAGATCTTCAACAAGAGGACCCAGGAGAAATTCGCCCTCAAAATGCTTCAGGACTGCCCCAAGGCCCGCAGGGAGGTGGAGCTGCACTGGCGGGCCTCCCAGTGCCCGCACATCGTACGGATCGTGGATGTGTACGAGAATCTGTACGCAGGGAGGAAGTGCCTGCTGATTGTCATGGAATGTTTGGACGGTGGAGAACTCTTTAGCCGAATCCAGGATCGAGGAGACCAGGCATTCACAGAAAGAGAAGCATCCGAAATCATGAAGAGCATCGGTGAGGCCATCCAGTATCTGCATTCAATCAACATTGCCCATCGGGATGTCAAGCCTGAGAATCTCTTATACACCTCCAAAAGGCCCAACGCCATCCTGAAACTCACTGACTTTGGCTTTGCCAAGGAAACCACCAGCCACAACTCTTTGACCACTCCTTGTTATACACCGTACTATGTGGCTCCAGAAGTGCTGGGTCCAGAGAAGTATGACAAGTCCTGTGACATGTGGTCCCTGGGTGTCATCATGTACATCCTGCTGTGTGGGTATCCCCCCTTCTACTCCAACCACGGCCTTGCCATCTCTCCGGGCATGAAGACTCGCATCCGAATGGGCCAGTATGAATTTCCCAACCCAGAATGGTCAGAAGTATCAGAGGAAGTGAAGATGCTCATTCGGAATCTGCTGAAAACAGAGCCCACCCAGAGAATGACCATCACCGAGTTTATGAACCACCCTTGGATCATGCAATCAACAAAGGTCCCTCAAACCCCACTGCACACCAGCCGGGTCCTGAAGGAGGACAAGGAGCGGTGGGAGGATGTCAAGGGGTGTCTTCATGACAAGAACAGCGACCAGGCC</t>
-  </si>
-  <si>
-    <t>CDK2_HUMAN_D0_4BCP_A</t>
-  </si>
-  <si>
-    <t>MP2K4_HUMAN_D0_3ALN_C</t>
-  </si>
-  <si>
-    <t>ACCACCTCACTTGAAGCTTTGCCCACAGGGACAGTGCTGACAGACAAGAGTGGGCGACAGTGGAAGCTGAAGTCCTTCCAGACCAGGGACAACCAGGGCATTCTCTATGAAGCTGCACCCACCTCCACCCTCACCTGTGACTCAGGACCACAGAAGCAAAAGTTCTCACTCAAACTGGATGCCAAGGATGGGCGCTTGTTCAATGAGCAGAACTTCTTCCAGCGGGCCGCCAAGCCTCTGCAAGTCAACAAGTGGAAGAAGCTGTACTCGACCCCACTGCTGGCCATCCCTACCTGCATGGGTTTCGGTGTTCACCAGGACAAATACAGGTTCTTGGTGTTACCCAGCCTGGGGAGGAGCCTTCAGTCGGCCCTGGATGTCAGCCCAAAGCATGTGCTGTCAGAGAGGTCTGTGCTGCAGGTGGCCTGCCGGCTGCTGGATGCCCTGGAGTTCCTCCATGAGAATGAGTATGTTCATGGAAATGTGACAGCTGAAAATATCTTTGTGGATCCAGAGGACCAGAGTCAGGTGACTTTGGCAGGCTATGGCTTCGCCTTCCGCTATTGCCCAAGTGGCAAACACGTGGCCTACGTGGAAGGCAGCAGGAGCCCTCACGAGGGGGACCTTGAGTTCATTAGCATGGACCTGCACAAGGGATGCGGGCCCTCCCGCCGCAGCGACCTCCAGAGCCTGGGCTACTGCATGCTGAAGTGGCTCTACGGGTTTCTGCCATGGACAAATTGCCTTCCCAACACTGAGGACATCATGAAGCAAAAACAGAAGTTTGTTGATAAGCCGGGGCCCTTCGTGGGACCCTGCGGTCACTGGATCAGGCCCTCAGAGACCCTGCAGAAGTACCTGAAGGTGGTGATGGCCCTCACGTATGAGGAGAAGCCGCCCTACGCCATGCTGAGGAACAACCTAGAAGCTTTGCTGCAGGATCTGCGTGTGTCTCCATATGACCCCATTGGCCTCCCGATGGTGCCC</t>
-  </si>
-  <si>
-    <t>TCACCACAGCGGGAGCCACAGCGAGTATCCCATGAGCAGTTCCGGGCTGCCCTGCAGCTGGTGGTGGACCCAGGCGACCCCCGCTCCTACCTGGACAACTTCATCAAGATTGGCGAGGGCTCCACGGGCATCGTGTGCATCGCCACCGTGCGCAGCTCGGGCAAGCTGGTGGCCGTCAAGAAGATGGACCTGCGCAAGCAGCAGAGGCGCGAGCTGCTCTTCAACGAGGTGGTAATCATGAGGGACTACCAGCACGAGAATGTGGTGGAGATGTACAACAGCTACCTGGTGGGGGACGAGCTCTGGGTGGTCATGGAGTTCCTGGAAGGAGGCGCCCTCACCGACATCGTCACCCACACCAGGATGAACGAGGAGCAGATCGCGGCCGTGTGCCTTGCAGTGCTGCAGGCCCTGTCGGTGCTCCACGCCCAGGGCGTCATCCACCGGGACATCAAGAGCGACTCGATCCTGCTGACCCATGATGGCAGGGTGAAGCTGTCAGACTTTGGGTTCTGCGCCCAGGTGAGCAAGGAAGTGCCCCGAAGGAAGTCGCTGGTCGGCACGCCCTACTGGATGGCCCCAGAGCTCATCTCCCGCCTTCCCTACGGGCCAGAGGTAGACATCTGGTCGCTGGGGATAATGGTGATTGAGATGGTGGACGGAGAGCCCCCCTACTTCAACGAGCCACCCCTCAAAGCCATGAAGATGATTCGGGACAACCTGCCACCCCGACTGAAGAACCTGCACAAGGTGTCGCCATCCCTGAAGGGCTTCCTGGACCGCCTGCTGGTGCGAGACCCTGCCCAGCGGGCCACGGCAGCCGAGCTGCTGAAGCACCCATTCCTGGCCAAGGCAGGGCCGCCTGCCAGCATCGTGCCCCTCATGCGCCAGAACCGCACCAGA</t>
-  </si>
-  <si>
-    <t>SIESSGKLKISPEQHWDFTAEDLKDLGEIGRGAYGSVNKMVHKPSGQIMAVKRIRSTVDEKEQKQLLMDLDVVMRSSDCPYIVQFYGALFREGDCWICMELMSTSFDKFYKYVYSVLDDVIPEEILGKITLATVKALNHLKENLKIIHRDIKPSNILLDRSGNIKLCDFGISGQLVDSIAKTRDAGCRPYMAPERIDPSASRQGYDVRSDVWSLGITLYELATGRFPYPKWNSVFDQLTQVVKGDPPQLSNSEEREFSPSFINFVNLCLTKDESKRPKYKELLKHPFILMYEERAVEVACYVCKILDQMPATPSSPMYVD</t>
-  </si>
-  <si>
-    <t>TDSFSGRFEDVYQLQEDVLGEGAHARVQTCINLITSQEYAVKIIEKQPGHIRSRVFREVEMLYQCQGHRNVLELIEFFEEEDRFYLVFEKMRGGSILSHIHKRRHFNELEASVVVQDVASALDFLHNKGIAHRDLKPENILCEHPNQVSPVKICDFDLGSGIKLNGDCSPISTPELLTPCGSAEYMAPEVVEAFSEEASIYDKRCDLWSLGVILYILLSGYPPFVGRCGSDCGWDRGEACPACQNMLFESIQEGKYEFPDKDWAHISCAAKDLISKLLVRDAKQRLSAAQVLQHPWVQGCAPENTLPTPMVLQR</t>
-  </si>
-  <si>
-    <t>WALNMKELKLLQTIGKGEFGDVMLGDYRGNKVAVKCIKNDATAQAFLAEASVMTQLRHSNLVQLLGVIVEEKGGLYIVTEYMAKGSLVDYLRSRGRSVLGGDCLLKFSLDVCEAMEYLEGNNFVHRDLAARNVLVSEDNVAKVSDFGLTKEASSTQDTGKLPVKWTAPEALREKKFSTKSDVWSFGILLWEIYSFGRVPYPRIPLKDVVPRVEKGYKMDAPDGCPPAVYEVMKNCWHLDAAMRPSFLQLREQLEHIKTHELHL</t>
-  </si>
-  <si>
-    <t>MPGPAAGSRARVYAEVNSLRSREYWDYEAHVPSWGNQDDYQLVRKLGRGKYSEVFEAINITNNERVVVKILKPVKKKKIKREVKILENLRGGTNIIKLIDTVKDPVSKTPALVFEYINNTDFKQLYQILTDFDIRFYMYELLKALDYCHSKGIMHRDVKPHNVMIDHQQKKLRLIDWGLAEFYHPAQEYNVRVASRYFKGPELLVDYQMYDYSLDMWSLGCMLASMIFRREPFFHGQDNYDQLVRIAKVLGTEELYGYLKKYHIDLDPHFNDILGQHSRKRWENFIHSENRHLVSPEALDLLDKLLRYDHQQRLTAKEAMEHPYFYPVVKEQSQ</t>
-  </si>
-  <si>
-    <t>AAGAGGCAGTGGGCTTTGGAAGACTTTGAAATTGGTCGCCCTCTGGGTAAAGGAAAGTTTGGTAATGTTTATTTGGCAAGAGAAAAGCAAAGCAAGTTTATTCTGGCTCTTAAAGTGTTATTTAAAGCTCAGCTGGAGAAAGCCGGAGTGGAGCATCAGCTCAGAAGAGAAGTAGAAATACAGTCCCACCTTCGGCATCCTAATATTCTTAGACTGTATGGTTATTTCCATGATGCTACCAGAGTCTACCTAATTCTGGAATATGCACCACTTGGAACAGTTTATAGAGAACTTCAGAAACTTTCAAAGTTTGATGAGCAGAGAACTGCTACTTATATAACAGAATTGGCAAATGCCCTGTCTTACTGTCATTCGAAGAGAGTTATTCATAGAGACATTAAGCCAGAGAACTTACTTCTTGGATCAGCTGGAGAGCTTAAAATTGCAGATTTTGGGTGGTCAGTACATGCTCCATCTTCCAGGAGGACCACTCTCTGTGGCACCCTGGACTACCTGCCCCCTGAAATGATTGAAGGTCGGATGCATGATGAGAAGGTGGATCTCTGGAGCCTTGGAGTTCTTTGCTATGAATTTTTAGTTGGGAAGCCTCCTTTTGAGGCAAACACATACCAAGAGACCTACAAAAGAATATCACGGGTTGAATTCACATTCCCTGACTTTGTAACAGAGGGAGCCAGGGACCTCATTTCAAGACTGTTGAAGCATAATCCCAGCCAGAGGCCAATGCTCAGAGAAGTACTTGAACACCCCTGGATCACAGCAAATTCATCAAAACCATCA</t>
-  </si>
-  <si>
-    <t>ATGGAGCTACGTGTGGGGAACAAGTACCGCCTGGGACGGAAGATCGGGAGCGGGTCCTTCGGAGATATCTACCTGGGTGCCAACATCGCCTCTGGTGAGGAAGTCGCCATCAAGCTGGAGTGTGTGAAGACAAAGCACCCCCAGCTGCACATCGAGAGCAAGTTCTACAAGATGATGCAGGGTGGCGTGGGGATCCCGTCCATCAAGTGGTGCGGAGCTGAGGGCGACTACAACGTGATGGTCATGGAGCTGCTGGGGCCTAGCCTCGAGGACCTGTTCAACTTCTGTTCCCGCAAATTCAGCCTCAAGACGGTGCTGCTCTTGGCCGACCAGATGATCAGCCGCATCGAGTATATCCACTCCAAGAACTTCATCCACCGGGACGTCAAGCCCGACAACTTCCTCATGGGGCTGGGGAAGAAGGGCAACCTGGTCTACATCATCGACTTCGGCCTGGCCAAGAAGTACCGGGACGCCCGCACCCACCAGCACATTCCCTACCGGGAAAACAAGAACCTGACCGGCACGGCCCGCTACGCTTCCATCAACACGCACCTGGGCATTGAGCAAAGCCGTCGAGATGACCTGGAGAGCCTGGGCTACGTGCTCATGTACTTCAACCTGGGCTCCCTGCCCTGGCAGGGGCTCAAAGCAGCCACCAAGCGCCAGAAGTATGAACGGATCAGCGAGAAGAAGATGTCAACGCCCATCGAGGTCCTCTGCAAAGGCTATCCCTCCGAATTCTCAACATACCTCAACTTCTGCCGCTCCCTGCGGTTTGACGACAAGCCCGACTACTCTTACCTACGTCAGCTCTTCCGCAACCTCTTCCACCGGCAGGGCTTCTCCTATGACTACGTCTTTGACTGGAACATGCTGAAA</t>
-  </si>
-  <si>
-    <t>MK03_HUMAN_D0_2ZOQ_B</t>
-  </si>
-  <si>
-    <t>ATGTCTCAGTCGAAAGGCAAGAAGCGAAACCCTGGCCTTAAAATTCCAAAAGAAGCATTTGAACAACCTCAGACCAGTTCCACACCACCTCGAGATTTAGACTCCAAGGCTTGCATTTCTATTGGAAATCAGAACTTTGAGGTGAAGGCAGATGACCTGGAGCCTATAATGGAACTGGGACGAGGTGCGTACGGGGTGGTGGAGAAGATGCGGCACGTGCCCAGCGGGCAGATCATGGCAGTGAAGCGGATCCGAGCCACAGTAAATAGCCAGGAACAGAAACGGCTACTGATGGATTTGGATATTTCCATGAGGACGGTGGACTGTCCATTCACTGTCACCTTTTATGGCGCACTGTTTCGGGAGGGTGATGTGTGGATCTGCATGGAGCTCATGGATACATCACTAGATAAATTCTACAAACAAGTTATTGATAAAGGCCAGACAATTCCAGAGGACATCTTAGGGAAAATAGCAGTTTCTATTGTAAAAGCATTAGAACATTTACATAGTAAGCTGTCTGTCATTCACAGAGACGTCAAGCCTTCTAATGTACTCATCAATGCTCTCGGTCAAGTGAAGATGTGCGATTTTGGAATCAGTGGCTACTTGGTGGACTCTGTTGCTAAAACAATTGATGCAGGTTGCAAACCATACATGGCCCCTGAAAGAATAAACCCAGAGCTCAACCAGAAGGGATACAGTGTGAAGTCTGACATTTGGAGTCTGGGCATCACGATGATTGAGTTGGCCATCCTTCGATTTCCCTATGATTCATGGGGAACTCCATTTCAGCAGCTCAAACAGGTGGTAGAGGAGCCATCGCCACAACTCCCAGCAGACAAGTTCTCTGCAGAGTTTGTTGACTTTACCTCACAGTGCTTAAAGAAGAATTCCAAAGAACGGCCTACATACCCAGAGCTAATGCAACATCCATTTTTCACCCTACATGAATCCAAAGGAACAGATGTGGCATCTTTTGTAAAACTGATTCTTGGAGAC</t>
-  </si>
-  <si>
-    <t>TCAACCAGGGATTATGAGATTCAAAGAGAAAGAATAGAACTTGGACGATGTATTGGAGAAGGCCAATTTGGAGATGTACATCAAGGCATTTATATGAGTCCAGAGAATCCAGCTTTGGCGGTTGCAATTAAAACATGTAAAAACTGTACTTCGGACAGCGTGAGAGAGAAATTTCTTCAAGAAGCCTTAACAATGCGTCAGTTTGACCATCCTCATATTGTGAAGCTGATTGGAGTCATCACAGAGAATCCTGTCTGGATAATCATGGAGCTGTGCACACTTGGAGAGCTGAGGTCATTTTTGCAAGTAAGGAAATACAGTTTGGATCTAGCATCTTTGATCCTGTATGCCTATCAGCTTAGTACAGCTCTTGCATATCTAGAGAGCAAAAGATTTGTACACAGGGACATTGCTGCTCGGAATGTTCTGGTGTCCTCAAATGATTGTGTAAAATTAGGAGACTTTGGATTATCCCGATATATGGAAGATAGTACTTACTACAAAGCTTCCAAAGGAAAATTGCCTATTAAATGGATGGCTCCAGAGTCAATCAATTTTCGACGTTTTACCTCAGCTAGTGACGTATGGATGTTTGGTGTGTGTATGTGGGAGATACTGATGCATGGTGTGAAGCCTTTTCAAGGAGTGAAGAACAATGATGTAATCGGTCGAATTGAAAATGGGGAAAGATTACCAATGCCTCCAAATTGTCCTCCTACCCTCTACAGCCTTATGACGAAATGCTGGGCCTATGACCCCAGCAGGCGGCCCAGGTTTACTGAACTTAAAGCTCAGCTCAGCACAATCCTGGAGGAAGAGAAGGCTCAGCAAGAAGAG</t>
-  </si>
-  <si>
-    <t>DPEELFTKLEKIGKGSFGEVFKGIDNRTQKVVAIKIIDLEEAEDEIEDIQQEITVLSQCDSPYVTKYYGSYLKDTKLWIIMEYLGGGSALDLLEPGPLDETQIATILREILKGLDYLHSEKKIHRDIKAANVLLSEHGEVKLADFGVAGQLTDTQIKRNTFVGTPFWMAPEVIKQSAYDSKADIWSLGITAIELARGEPPHSELHPMKVLFLIPKNNPPTLEGNYSKPLKEFVEACLNKEPSFRPTAKELLKHKFILRNAKKTSYLTELID</t>
-  </si>
-  <si>
-    <t>MAPK3_HUMAN_D0_3FXW_A</t>
-  </si>
-  <si>
-    <t>AAGCAGTACGAACACGTGAAGAGGGACCTGAACCCCGAAGACTTTTGGGAGATTATAGGAGAACTGGGCGACGGAGCCTTTGGGAAAGTGTACAAGGCCCAGAATAAAGAGACCAGTGTTTTAGCTGCTGCAAAAGTGATTGACACTAAATCTGAAGAAGAACTTGAAGATTACATGGTAGAGATTGACATATTAGCATCTTGTGATCACCCAAATATAGTCAAGCTTCTAGATGCCTTCTATTATGAGAACAATCTTTGGATCCTCATTGAATTTTGTGCAGGTGGAGCAGTAGATGCTGTGATGCTTGAACTTGAGAGACCATTAACTGAGTCCCAAATACAAGTAGTTTGCAAGCAGACTTTAGATGCATTGAACTACTTACATGATAATAAGATCATCCACAGAGATCTGAAGGCTGGCAACATTCTCTTTACCTTAGATGGAGATATCAAATTGGCGGATTTTGGAGTATCAGCTAAAAACATGAGGACAATTCAAAGAAGAGATTCCTTTATTGGTACACCATATTGGATGGCTCCTGAAGTAGTCATGTGTGAAACATCTAAGGACAGACCCTATGACTACAAAGCTGATGTTTGGTCCCTGGGTATCACTTTAATAGAAATGGCTGAGATAGAACCACCTCATCATGAATTAAATCCAATGCGAGTGCTGCTAAAAATAGCAAAATCTGAGCCACCTACATTAGCACAGCCATCCAGATGGTCTTCAAATTTTAAGGACTTTCTAAAGAAATGCTTAGAAAAGAATGTGGATGCCAGGTGGACTACATCTCAGCTGCTGCAGCATCCCTTTGTTACTGTTGATTCCAACAAACCCATCCGAGAATTGATTGCAGAGGCGAAGGCTGAAGTAACAGAAGAAGTTGAAGATGGCAAAGAG</t>
-  </si>
-  <si>
-    <t>ATGCCTTCCCGGGCTGAGGACTATGAAGTGTTGTACACCATTGGCACAGGCTCCTACGGCCGCTGCCAGAAGATCCGGAGGAAGAGTGATGGCAAGATATTAGTTTGGAAAGAACTTGACTATGGCTCCATGACAGAAGCTGAGAAACAGATGCTTGTTTCTGAAGTGAATTTGCTTCGTGAACTGAAACATCCAAACATCGTTCGTTACTATGATCGGATTATTGACCGGACCAATACAACACTGTACATTGTAATGGAATATTGTGAAGGAGGGGATCTGGCTAGTGTAATTACAAAGGGAACCAAGGAAAGGCAATACTTAGATGAAGAGTTTGTTCTTCGAGTGATGACTCAGTTGACTCTGGCCCTGAAGGAATGCCACAGACGAAGTGATGGTGGTCATACCGTATTGCATCGGGATCTGAAACCAGCCAATGTTTTCCTGGATGGCAAGCAAAACGTCAAGCTTGGAGACTTTGGGCTAGCTAGAATATTAAACCATGACACGAGTTTTGCAAAAACATTTGTTGGCACACCTTATTACATGTCTCCTGAACAAATGAATCGCATGTCCTACAATGAGAAATCAGATATCTGGTCATTGGGCTGCTTGCTGTATGAGTTATGTGCATTAATGCCTCCATTTACAGCTTTTAGCCAGAAAGAACTCGCTGGGAAAATCAGAGAAGGCAAATTCAGGCGAATTCCATACCGTTACTCTGATGAATTGAATGAAATTATTACGAGGATGTTAAACTTAAAGGATTACCATCGACCTTCTGTTGAAGAAATTCTTGAGAACCCTTTAATA</t>
-  </si>
-  <si>
-    <t>GATGAACAACCTCACATCGGAAACTACAGACTGTTGAAAACAATCGGCAAGGGGAATTTTGCAAAAGTAAAATTGGCAAGACATATCCTTACAGGCAGAGAGGTTGCAATAAAAATAATTGACAAAACTCAGTTGAATCCAACAAGTCTACAAAAGCTCTTCAGAGAAGTAAGAATAATGAAGATTTTAAATCATCCCAATATAGTGAAGTTATTCGAAGTCATTGAAACTGAAAAAACACTCTACCTAATCATGGAATATGCAAGTGGAGGTGAAGTATTTGACTATTTGGTTGCACATGGCAGGATGAAGGAAAAAGAAGCAAGATCTAAATTTAGACAGATTGTGTCTGCAGTTCAATACTGCCATCAGAAACGGATCGTACATCGAGACCTCAAGGCTGAAAATCTATTGTTAGATGCCGATATGAACATTAAAATAGCAGATTTCGGTTTTAGCAATGAATTTACTGTTGGCGGTAAACTCGACACGTTTTGTGGCAGTCCTCCATACGCAGCACCTGAGCTCTTCCAGGGCAAGAAATATGACGGGCCAGAAGTGGATGTGTGGAGTCTGGGGGTCATTTTATACACACTAGTCAGTGGCTCACTTCCCTTTGATGGGCAAAACCTAAAGGAACTGAGAGAGAGAGTATTAAGAGGGAAATACAGAATTCCCTTCTACATGTCTACAGACTGTGAAAACCTTCTCAAACGTTTCCTGGTGCTAAATCCAATTAAACGCGGCACTCTAGAGCAAATCATGAAGGACAGGTGGATCAATGCAGGGCATGAAGAAGATGAACTCAAACCATTTGTTGAACCAGAGCTAGACATCTCAGACCAAAAAAGAATAGATATTATGGTGGGAATGGGATATTCACAAGAAGAAATTCAAGAATCTCTTAGTAAGATGAAATACGATGAAATCACAGCTACATATTTGTTATTGGGGAGAAAATCTTCAGAG</t>
-  </si>
-  <si>
-    <t>CACCAGCTGCAGCCCCGGCGGGTGTCATTCCGGGGCGAGGCCTCAGAGACTCTGCAGAGCCCTGGGTATGACCCAAGCCGGCCAGAGTCCTTCTTCCAGCAGAGCTTCCAGAGGCTCAGCCGCCTGGGCCATGGCTCCTACGGAGAGGTCTTCAAGGTGCGCTCCAAGGAGGACGGCCGGCTCTATGCGGTAAAGCGTTCCATGTCACCATTCCGGGGCCCCAAGGACCGGGCCCGCAAGTTGGCCGAGGTGGGCAGCCACGAGAAGGTGGGGCAGCACCCATGCTGCGTGCGGCTGGAGCAGGCCTGGGAGGAGGGCGGCATCCTGTACCTGCAGACGGAGCTGTGCGGGCCCAGCCTGCAGCAACACTGTGAGGCCTGGGGTGCCAGCCTGCCTGAGGCCCAGGTCTGGGGCTACCTGCGGGACACGCTGCTTGCCCTGGCCCATCTGCACAGCCAGGGCCTGGTGCACCTTGATGTCAAGCCTGCCAACATCTTCCTGGGGCCCCGGGGCCGCTGCAAGCTGGGTGACTTCGGACTGCTGGTGGAGCTGGGTACAGCAGGAGCTGGTGAGGTCCAGGAGGGAGACCCCCGCTACATGGCCCCCGAGCTGCTGCAGGGCTCCTATGGGACAGCAGCGGATGTGTTCAGTCTGGGCCTCACCATCCTGGAAGTGGCATGCAACATGGAGCTGCCCCACGGTGGGGAGGGCTGGCAGCAGCTGCGCCAGGGCTACCTGCCCCCTGAGTTCACTGCCGGTCTGTCTTCCGAGCTGCGTTCTGTCCTTGTCATGATGCTGGAGCCAGACCCCAAGCTGCGGGCCACGGCCGAGGCCCTGCTGGCACTGCCTGTGTTGAGGCAGCCG</t>
-  </si>
-  <si>
-    <t>KEKEPLESQYQVGPLLGSGGFGSVYSGIRVSDNLPVAIKHVEKDRISDWGELPNGTRVPMEVVLLKKVSSGFSGVIRLLDWFERPDSFVLILERPEPVQDLFDFITERGALQEELARSFFWQVLEAVRHCHNCGVLHRDIKDENILIDLNRGELKLIDFGSGALLKDTVYTDFDGTRVYSPPEWIRYHRYHGRSAAVWSLGILLYDMVCGDIPFEHDEEIIGGQVFFRQRVSSECQHLIRWCLALRPSDRPTFEEIQNHPWMQDVLLPQETAEIHLHSLSPGPSK</t>
-  </si>
-  <si>
-    <t>VEDHYEMGEELGSGQFAIVRKCRQKGTGKEYAAKFIKKRRLSSSRRGVSREEIEREVNILREIRHPNIITLHDIFENKTDVVLILELVSGGELFDFLAEKESLTEDEATQFLKQILDGVHYLHSKRIAHFDLKPENIMLLDKNVPNPRIKLIDFGIAHKIEAGNEFKNIFGTPEFVAPEIVNYEPLGLEADMWSIGVITYILLSGASPFLGETKQETLTNISAVNYDFDEEYFSNTSELAKDFIRRLLVKDPKRRMTIAQSLEHSWIKAIRRRNVRGEDSG</t>
-  </si>
-  <si>
-    <t>MET_HUMAN_D0_4EEV_A</t>
-  </si>
-  <si>
-    <t>MSSFLPEGGCYELLTVIGKGFEDLMTVNLARYKPTGEYVTVRRINLEACSNEMVTFLQGELHVSKLFNHPNIVPYRATFIADNELWVVTSFMAYGSAKDLICTHFMDGMNELAIAYILQGVLKALDYIHHMGYVHRSVKASHILISVDGKVYLSGLRSNLSMISHGQRQRVVHDFPKYSVKVLPWLSPEVLQQNLQGYDAKSDIYSVGITACELANGHVPFKDMPATQMLLEKLNGTVPCLLDTSTIPAEELTMSPSRSVANSGLSDSLTTSTPRPSNGDSPSHPYHRTFSPHFHHFVEQCLQRNPDARPSASTLLNHSFFKQIKRRASEVLPELLRPVTPITNFEGSQSQDHSGIFGLVTNLEELEVDDWEF</t>
-  </si>
-  <si>
-    <t>MP2K1_HUMAN_D0_3MBL_A</t>
-  </si>
-  <si>
-    <t>ETKYTVDKRFGMDFKEIELIGSGGFGQVFKAKHRIDGKTYVIKRVKYNNEKAEREVKALAKLDHVNIVHYNGCWDGFDYDPETSDDSLESSDYDPENSKNSSRSKTKCLFIQMEFCDKGTLEQWIEKRRGEKLDKVLALELFEQITKGVDYIHSKKLIHRDLKPSNIFLVDTKQVKIGDFGLVTSLKNDGKRTRSKGTLRYMSPEQISSQDYGKEVDLYALGLILAELLHVCDTAFETSKFFTDLRDGIISDIFDKKEKTLLQKLLSKKPEDRPNTSEILRTLTVWKKSPEKNERHTC</t>
-  </si>
-  <si>
-    <t>CDKL1_HUMAN_D0_4AGU_C</t>
-  </si>
-  <si>
-    <t>MARK3_HUMAN_D0_2QNJ_A</t>
-  </si>
-  <si>
-    <t>MSGPRAGFYRQELNKTVWEVPQRLQGLRPVGSGAYGSVCSAYDARLRQKVAVKKLSRPFQSLIHARRTYRELRLLKHLKHENVIGLLDVFTPATSIEDFSEVYLVTTLMGADLNNIVKCQALSDEHVQFLVYQLLRGLKYIHSAGIIHRDLKPSNVAVNEDCELRILDFGLARQADEEMTGYVATRWYRAPEIMLNWMHYNQTVDIWSVGCIMAELLQGKALFPGSDYIDQLKRIMEVVGTPSPEVLAKISSEHARTYIQSLPPMPQKDLSSIFRGANPLAIDLLGRMLVLDSDQRVSAAEALAHAYFSQYHDPEDEPEAEPYDESVEAKERTLEEWKELTYQEVLSFKPPEPPKPPGSLEIEQ</t>
-  </si>
-  <si>
-    <t>NLVFSDGYVVKETIGVGSYSECKRCVHKATNMEYAVKVIDKSKRDPSEEIEILLRYGQHPNIITLKDVYDDGKHVYLVTELMRGGELLDKILRQKFFSEREASFVLHTIGKTVEYLHSQGVVHRDLKPSNILYVDESGNPECLRICDFGFAKQLRAENGLLMTPCYTANFVAPEVLKRQGYDEGCDIWSLGILLYTMLAGYTPFANGPSDTPEEILTRIGSGKFTLSGGNWNTVSETAKDLVSKMLHVDPHQRLTAKQVLQHPWVTQKDKLPQSQLSHQDLQLVKGAMAATYSALNSSKPTPQLKPIESSILAQRRVRKLPSTTL</t>
-  </si>
-  <si>
-    <t>GGTGTTGTGACACATGAGCAGTTCAAGGCTGCGCTCAGGATGGTGGTGGACCAGGGTGACCCCCGGCTGCTGCTGGACAGCTACGTGAAGATTGGCGAGGGCTCCACCGGCATCGTCTGCTTGGCCCGGGAGAAGCACTCGGGCCGCCAGGTGGCCGTCAAGATGATGGACCTCAGGAAGCAGCAGCGCAGGGAGCTGCTCTTCAACGAGGTGGTGATCATGCGGGACTACCAGCACTTCAACGTGGTGGAGATGTACAAGAGCTACCTGGTGGGCGAGGAGCTGTGGGTGCTCATGGAGTTCCTGCAGGGAGGAGCCCTCACAGACATCGTCTCCCAAGTCAGGCTGAATGAGGAGCAGATTGCCACTGTGTGTGAGGCTGTGCTGCAGGCCCTGGCCTACCTGCATGCTCAGGGTGTCATCCACCGGGACATCAAGAGTGACTCCATCCTGCTGACCCTCGATGGCAGGGTGAAGCTCTCGGACTTCGGATTCTGTGCTCAGATCAGCAAAGACGTCCCTAAGAGGAAGTCCCTGGTGGGAACCCCCTACTGGATGGCTCCTGAAGTGATCTCCAGGTCTTTGTATGCCACTGAGGTGGATATCTGGTCTCTGGGCATCATGGTGATTGAGATGGTAGATGGGGAGCCACCGTACTTCAGTGACTCCCCAGTGCAAGCCATGAAGAGGCTCCGGGACAGCCCCCCACCCAAGCTGAAAAACTCTCACAAGGTCTCCCCAGTGCTGCGAGACTTCCTGGAGCGGATGCTGGTGCGGGACCCCCAAGAGAGAGCCACAGCCCAGGAGCTCCTAGACCACCCCTTCCTGCTGCAGACAGGGCTACCTGAGTGCCTGGTGCCCCTGATCCAGCTCTACCGAAAGCAGACCTCCACCTGC</t>
-  </si>
-  <si>
-    <t>CACATTGGAAACTACCGGCTCCTCAAGACCATTGGCAAGGGTAATTTTGCCAAGGTGAAGTTGGCCCGACACATCCTGACTGGGAAAGAGGTAGCTGTGAAGATCATTGACAAGACTCAACTGAACTCCTCCAGCCTCCAGAAACTATTCCGCGAAGTAAGAATAATGAAGGTTTTGAATCATCCCAACATAGTTAAATTATTTGAAGTGATTGAGACTGAGAAAACGCTCTACCTTGTCATGGAGTACGCTAGTGGCGGAGAGGTATTTGATTACCTAGTGGCTCATGGCAGGATGAAAGAAAAAGAGGCTCGAGCCAAATTCCGCCAGATAGTGTCTGCTGTGCAGTACTGTCACCAGAAGTTTATTGTCCATAGAGACTTAAAGGCAGAAAACCTGCTCTTGGATGCTGATATGAACATCAAGATTGCAGACTTTGGCTTCAGCAATGAATTCACCTTTGGGAACAAGCTGGACACCTTCTGTGGCAGTCCCCCTTATGCTGCCCCAGAACTCTTCCAGGGCAAAAAATATGATGGACCCGAGGTGGATGTGTGGAGCCTAGGAGTTATCCTCTATACACTGGTCAGCGGATCCCTGCCTTTTGATGGACAGAACCTCAAGGAGCTGCGGGAACGGGTACTGAGGGGAAAATACCGTATTCCATTCTACATGTCCACGGACTGTGAAAACCTGCTTAAGAAATTTCTCATTCTTAATCCCAGCAAGAGAGGCACTTTAGAGCAAATCATGAAAGATCGATGGATGAATGTGGGTCACGAAGATGATGAACTAAAGCCTTACGTGGAGCCACTCCCTGACTACAAGGACCCCCGGCGGACAGAGCTGATGGTGTCCATGGGTTATACACGGGAAGAGATCCAGGACTCGCTGGTGGGCCAGAGATACAACGAGGTGATGGCCACCTATCTGCTCCTGGGCTAC</t>
-  </si>
-  <si>
-    <t>ST17B_HUMAN_D0_3LM0_A</t>
-  </si>
-  <si>
-    <t>GDSDISSPLLQNTVHIDLSALNPELVQAVQHVVIGPSSLIVHFNEVIGRGHFGCVYHGTLLDNDGKKIHCAVKSLNRITDIGEVSQFLTEGIIMKDFSHPNVLSLLGICLRSEGSPLVVLPYMKHGDLRNFIRNETHNPTVKDLIGFGLQVAKGMKYLASKKFVHRDLAARNCMLDEKFTVKVADFGLARDMYDKEYYSVHNKTGAKLPVKWMALESLQTQKFTTKSDVWSFGVLLWELMTRGAPPYPDVNTFDITVYLLQGRRLLQPEYCPDPLYEVMLKCWHPKAEMRPSFSELVSRISAIFSTFIG</t>
-  </si>
-  <si>
-    <t>ATGAGTAGCTTTCTGCCAGAGGGAGGGTGTTACGAGCTGCTCACTGTGATAGGCAAAGGATTTGAGGACCTGATGACTGTGAATCTAGCAAGGTACAAACCAACAGGAGAGTACGTGACTGTACGGAGGATTAACCTAGAAGCTTGTTCCAATGAGATGGTAACATTCTTGCAGGGCGAGCTGCATGTCTCCAAACTCTTCAACCATCCCAATATCGTGCCATATCGAGCCACTTTTATTGCAGACAATGAGCTGTGGGTTGTCACATCATTCATGGCATACGGTTCTGCAAAAGATCTCATCTGTACACACTTCATGGATGGCATGAATGAGCTGGCGATTGCTTACATCCTGCAGGGGGTGCTGAAGGCCCTCGACTACATCCACCACATGGGATATGTACACAGGAGTGTCAAAGCCAGCCACATCCTGATCTCTGTGGATGGGAAGGTCTACCTGTCTGGTTTGCGCAGCAACCTCAGCATGATAAGCCATGGGCAGCGGCAGCGAGTGGTCCACGATTTTCCCAAGTACAGTGTCAAGGTTCTGCCGTGGCTCAGCCCCGAGGTCCTCCAGCAGAATCTCCAGGGTTATGATGCCAAGTCTGACATCTACAGTGTGGGAATCACAGCCTGTGAACTGGCCAACGGCCATGTCCCCTTTAAGGATATGCCTGCCACCCAGATGCTGCTAGAGAAACTGAACGGCACAGTGCCCTGCCTGTTGGATACCAGCACCATCCCCGCTGAGGAGCTGACCATGAGCCCTTCGCGCTCAGTGGCCAACTCTGGCCTGAGTGACAGCCTGACCACCAGCACCCCCCGGCCCTCCAACGGTGACTCGCCCTCCCACCCCTACCACCGAACCTTCTCCCCCCACTTCCACCACTTTGTGGAGCAGTGCCTTCAGCGCAACCCGGATGCCAGGCCCAGTGCCAGCACCCTCCTGAACCACTCTTTCTTCAAGCAGATCAAGCGACGTGCCTCAGAGGTTTTGCCCGAATTGCTTCGTCCTGTCACCCCCATCACCAATTTTGAGGGCAGCCAGTCTCAGGACCACAGTGGAATCTTTGGCCTGGTAACAAACCTGGAAGAGCTGGAGGTGGACGATTGGGAGTTC</t>
-  </si>
-  <si>
-    <t>ADPEELFTKLERIGKGSFGEVFKGIDNRTQQVVAIKIIDLEEAEDEIEDIQQEITVLSQCDSSYVTKYYGSYLKGSKLWIIMEYLGGGSALDLLRAGPFDEFQIATMLKEILKGLDYLHSEKKIHRDIKAANVLLSEQGDVKLADFGVAGQLTDTQIKRNTFVGTPFWMAPEVIQQSAYDSKADIWSLGITAIELAKGEPPNSDMHPMRVLFLIPKNNPPTLVGDFTKSFKEFIDACLNKDPSFRPTAKELLKHKFIVKNSKKTSYLTELIDRFKRWKAE</t>
+    <t>SVYPKALRDEYIMSKTLGSGACGEVKLAFERKTCKKVAIKIISKRKFAIGSAREADPALNVETEIEILKKLNHPCIIKIKNFFDAEDYYIVLELMEGGELFDKVVGNKRLKEATCKLYFYQMLLAVQYLHENGIIHRDLKPENVLLSSQEEDCLIKITDFGHSKIWGETSLMRTLCGTPTYLAPEVLVSVGTAGYNRAVDCWSLGVILFICLSGYPPFSEHRTQVSLKDQITSGKYNFIPEVWAEVSEKALDLVKKLLVVDPKARFTTEEALRHPWLQDEDMKRKFQDLLSEENESTALPQVLAQPSTSRKRPREGEAEGAE</t>
+  </si>
+  <si>
+    <t>ATGGAGAAGTATGAAAAAATTGGGAAAATTGGAGAAGGATCCTATGGAGTTGTTTTCAAATGTAGAAACAGGGACACGGGTCAGATTGTGGCCATCAAGAAGTTTCTGGAATCAGAAGATGACCCTGTCATAAAGAAAATTGCCCTTCGGGAAATCCGAATGCTCAAGCAACTCAAGCATCCCAACCTTGTTAACCTCCTGGAAGTCTTCAGGAGGAAACGGAGGCTTCACCTGGTGTTTGAATATTGTGACCACACAGTTCTCCATGAGTTGGACAGATACCAAAGAGGGGTACCAGAACATCTCGTGAAGAGCATAACTTGGCAGACACTGCAAGCTGTAAATTTTTGCCATAAACACAATTGCATACATAGAGACGTGAAGCCAGAAAATATCCTCATCACGAAACATTCCGTGATTAAGCTTTGTGACTTTGGATTTGCTCGGCTTTTGACTGGACCGAGTGACTACTATACAGACTACGTGGCTACCAGGTGGTACCGCTCCCCTGAGCTGCTGGTGGGGGACACGCAGTACGGCCCCCCGGTGGATGTTTGGGCAATTGGCTGTGTCTTTGCTGAGCTGCTGTCAGGAGTGCCTCTGTGGCCAGGAAAATCGGATGTGGATCAGCTGTATCTGATTAGGAAGACCTTGGGGGATCTCATTCCTAGGCACCAGCAAGTGTTTAGCACGAATCAGTACTTCAGTGGAGTGAAAATTCCAGACCCTGAAGATATGGAACCACTTGAATTAAAATTCCCAAACATCTCTTATCCTGCCCTGGGGCTCCTA</t>
+  </si>
+  <si>
+    <t>KHDGRVKIGHYVLGDTLGVGTFGKVKIGEHQLTGHKVAVKILNRQKIRSLDVVGKIKREIQNLKLFRHPHIIKLYQVISTPTDFFMVMEYVSGGELFDYICKHGRVEEMEARRLFQQILSAVDYCHRHMVVHRDLKPENVLLDAHMNAKIADFGLSNMMSDGEFLRTSCGSPNYAAPEVISGRLYAGPEVDIWSCGVILYALLCGTLPFDDEHVPTLFKKIRGGVFYIPEYLNRSVATLLMHMLQVDPLKRATIKDIREHEWFKQDLPSYLFPE</t>
+  </si>
+  <si>
+    <t>ATGGAAAACTTTAATAATTTCTATATACTTACATCTAAAGAGCTAGGGAGAGGAAAATTTGCTGTGGTTAGACAATGTATATCAAAATCTACTGGCCAAGAATATGCTGCAAAATTTCTAAAAAAGAGAAGAAGAGGACAGGATTGTCGAGCAGAAATTTTACACGAGATTGCTGTGCTTGAATTGGCAAAGTCTTGTCCCCGTGTTATTAATCTTCATGAGGTCTATGAAAATACAAGTGAAATCATTTTGATATTGGAATATGCTGCAGGTGGAGAAATTTTCAGCCTGTGTTTACCTGAGTTGGCTGAAATGGTTTCTGAAAATGATGTTATCAGACTCATTAAACAAATACTTGAAGGAGTTTATTATCTACATCAGAATAACATTGTACACCTTGATTTAAAGCCACAGAATATATTACTGAGCAGCATATACCCTCTCGGGGACATTAAAATAGTAGATTTTGGAATGTCTCGAAAAATAGGGCATGCGTGTGAACTTCGGGAAATCATGGGAACACCAGAATATTTAGCTCCAGAAATCCTGAACTATGATCCCATTACCACAGCAACAGATATGTGGAATATTGGTATAATAGCATATATGTTGTTAACTCACACATCACCATTTGTGGGAGAAGATAATCAAGAAACATACCTCAATATTTCTCAAGTTAATGTAGATTATTCGGAAGAAACTTTTTCATCAGTTTCACAGCTGGCCACAGACTTTATTCAGAGCCTTTTAGTAAAAAATCCAGAGAAAAGACCAACAGCAGAGATATGCCTTTCTCATTCTTGGCTACAGCAGTGGGACTTTGAAAACTTGTTTCACCCTGAAGAAACTTCCAGTTCCTCTCAAACTCAGGATCATTCTGTAAGGTCCTCTGAAGACAAGACTTCTAAATCCTCC</t>
+  </si>
+  <si>
+    <t>MPSRAEDYEVLYTIGTGSYGRCQKIRRKSDGKILVWKELDYGSMTEAEKQMLVSEVNLLRELKHPNIVRYYDRIIDRTNTTLYIVMEYCEGGDLASVITKGTKERQYLDEEFVLRVMTQLTLALKECHRRSDGGHTVLHRDLKPANVFLDGKQNVKLGDFGLARILNHDTSFAKTFVGTPYYMSPEQMNRMSYNEKSDIWSLGCLLYELCALMPPFTAFSQKELAGKIREGKFRRIPYRYSDELNEIITRMLNLKDYHRPSVEEILENPLI</t>
+  </si>
+  <si>
+    <t>GACCCAGAAGAGCTTTTTACAAAACTAGAGAAAATTGGGAAGGGCTCCTTTGGAGAGGTGTTCAAAGGCATTGACAATCGGACTCAGAAAGTGGTTGCCATAAAGATCATTGATCTGGAAGAAGCTGAAGATGAGATAGAGGACATTCAACAAGAAATCACAGTGCTGAGTCAGTGTGACAGTCCATATGTAACCAAATATTATGGATCCTATCTGAAGGATACAAAATTATGGATAATAATGGAATATCTTGGTGGAGGCTCCGCACTAGATCTATTAGAACCTGGCCCATTAGATGAAACCCAGATCGCTACTATATTAAGAGAAATACTGAAAGGACTCGATTATCTCCATTCGGAGAAGAAAATCCACAGAGACATTAAAGCGGCCAACGTCCTGCTGTCTGAGCATGGCGAGGTGAAGCTGGCGGACTTTGGCGTGGCTGGCCAGCTGACAGACACCCAGATCAAAAGGAACACCTTCGTGGGCACCCCATTCTGGATGGCACCCGAGGTCATCAAACAGTCGGCCTATGACTCGAAGGCAGACATCTGGTCCCTGGGCATAACAGCTATTGAACTTGCAAGAGGGGAACCACCTCATTCCGAGCTGCACCCCATGAAAGTTTTATTCCTCATTCCAAAGAACAACCCACCGACGTTGGAAGGAAACTACAGTAAACCCCTCAAGGAGTTTGTGGAGGCCTGTTTGAATAAGGAGCCGAGCTTTAGACCCACTGCTAAGGAGTTATTGAAGCACAAGTTTATACTACGCAATGCAAAGAAAACTTCCTACTTGACCGAGCTCATCGAC</t>
+  </si>
+  <si>
+    <t>VIIDNKRYLFIQKLGEGGFSYVDLVEGLHDGHFYALKRILCHEQQDREEAQREADMHRLFNHPNILRLVAYCLRERGAKHEAWLLLPFFKRGTLWNEIERLKDKGNFLTEDQILWLLLGICRGLEAIHAKGYAHRDLKPTNILLGDEGQPVLMDLGSMNQACIHVEGSRQALTLQDWAAQRCTISYRAPELFSVQSHCVIDERTDVWSLGCVLYAMMFGEGPYDMVFQKGDSVALAVQNQLSIPQSPRHSSALWQLLNSMMTVDPHQRPHIPLLLSQLEALQ</t>
+  </si>
+  <si>
+    <t>MELK_HUMAN_D0_4IXP_A</t>
+  </si>
+  <si>
+    <t>AAGGAGAAGGAGCCCCTGGAGTCGCAGTACCAGGTGGGCCCGCTACTGGGCAGCGGCGGCTTCGGCTCGGTCTACTCAGGCATCCGCGTCTCCGACAACTTGCCGGTGGCCATCAAACACGTGGAGAAGGACCGGATTTCCGACTGGGGAGAGCTGCCTAATGGCACTCGAGTGCCCATGGAAGTGGTCCTGCTGAAGAAGGTGAGCTCGGGTTTCTCCGGCGTCATTAGGCTCCTGGACTGGTTCGAGAGGCCCGACAGTTTCGTCCTGATCCTGGAGAGGCCCGAGCCGGTGCAAGATCTCTTCGACTTCATCACGGAAAGGGGAGCCCTGCAAGAGGAGCTGGCCCGCAGCTTCTTCTGGCAGGTGCTGGAGGCCGTGCGGCACTGCCACAACTGCGGGGTGCTCCACCGCGACATCAAGGACGAAAACATCCTTATCGACCTCAATCGCGGCGAGCTCAAGCTCATCGACTTCGGGTCGGGGGCGCTGCTCAAGGACACCGTCTACACGGACTTCGATGGGACCCGAGTGTATAGCCCTCCAGAGTGGATCCGCTACCATCGCTACCATGGCAGGTCGGCGGCAGTCTGGTCCCTGGGGATCCTGCTGTATGATATGGTGTGTGGAGATATTCCTTTCGAGCATGACGAAGAGATCATCGGGGGCCAGGTTTTCTTCAGGCAGAGGGTCTCTTCAGAATGTCAGCATCTCATTAGATGGTGCTTGGCCCTGAGACCATCAGATAGGCCAACCTTCGAAGAAATCCAGAACCATCCATGGATGCAAGATGTTCTCCTGCCCCAGGAAACTGCTGAGATCCACCTCCACAGCCTGTCGCCGGGGCCCAGCAAA</t>
+  </si>
+  <si>
+    <t>PFPEGKVLDDMEGNQWVLGKKIGSGGFGLIYLAFPTNKPEKDARHVVKVEYQENGPLFSELKFYQRVAKKDCIKKWIERKQLDYLGIPLFYGSGLTEFKGRSYRFMVMERLGIDLQKISGQNGTFKKSTVLQLGIRMLDVLEYIHENEYVHGDIKAANLLLGYKNPDQVYLADYGLSYRYCPNGNHKQYQENPRKGHNGTIEFTSLDAHKGVALSRRSDVEILGYCMLRWLCGKLPWEQNLKDPVAVQTAKTNLLDELPQSVLKWAPSGSSCCEIAQFLVCAHSLAYDEKPNYQALKKILNPHGIPLGPLDFSTKGQSINVH</t>
+  </si>
+  <si>
+    <t>MESDLHQIIHSSQPLTLEHVRYFLYQLLRGLKYMHSAQVIHRDLKPSNLLVNENCELKIGDFGMARGLCTSPAEHQYFMTEYVATRWYRAPELMLSLHEYTQAIDLWSVGCIFGEMLARRQLFPGKNYVHQLQLIMMVLGTPSPAVIQAVGAERVRAYIQSLPPRQPVPWETVYPGADRQALSLLGRMLRFEPSARISAAAALRHPFLAKYHDPDDEPDCAPPFDFAFDREALTRERIKEAIVAEIEDFHARREGIRQQIRFQPSLQPVASEPGCPDVEMPSPWAPSGDCAM</t>
+  </si>
+  <si>
+    <t>EPKKYAVTDDYQLSKQVLGLGVNGKVLECFHRRTGQKCALKLLYDSPKARQEVDHHWQASGGPHIVCILDVYENMHHGKRCLLIIMECMEGGELFSRIQERGDQAFTEREAAEIMRDIGTAIQFLHSHNIAHRDVKPENLLYTSKEKDAVLKLTDFGFAKETTQNALQTPCYTPYYVAPEVLGPEKYDKSCDMWSLGVIMYILLCGFPPFYSNTGQAISPGMKRRIRLGQYGFPNPEWSEVSEDAKQLIRLLLKTDPTERLTITQFMNHPWINQSMVVPQTPLHTARVLQEDKDHWDEVKEEMTSALATMRVDYDQV</t>
+  </si>
+  <si>
+    <t>STK24_HUMAN_D0_3ZHP_C</t>
+  </si>
+  <si>
+    <t>aa_seq</t>
+  </si>
+  <si>
+    <t>KC1D_HUMAN_D0_4HNF_B</t>
+  </si>
+  <si>
+    <t>AGCATTGAGTCATCAGGAAAACTGAAGATCTCCCCTGAACAACACTGGGATTTCACTGCAGAGGACTTGAAAGACCTTGGAGAAATTGGACGAGGAGCTTATGGTTCTGTCAACAAAATGGTCCACAAACCAAGTGGGCAAATAATGGCAGTTAAAAGAATTCGGTCAACAGTGGATGAAAAAGAACAAAAACAACTTCTTATGGATTTGGATGTAGTAATGCGGAGTAGTGATTGCCCATACATTGTTCAGTTTTATGGTGCACTCTTCAGAGAGGGTGACTGTTGGATCTGTATGGAACTCATGTCTACCTCGTTTGATAAGTTTTACAAATATGTATATAGTGTATTAGATGATGTTATTCCAGAAGAAATTTTAGGCAAAATCACTTTAGCAACTGTGAAAGCACTAAACCACTTAAAAGAAAACTTGAAAATTATTCACAGAGATATCAAACCTTCCAATATTCTTCTGGACAGAAGTGGAAATATTAAGCTCTGTGACTTCGGCATCAGTGGACAGCTTGTGGACTCTATTGCCAAGACAAGAGATGCTGGCTGTAGGCCATACATGGCACCTGAAAGAATAGACCCAAGCGCATCACGACAAGGATATGATGTCCGCTCTGATGTCTGGAGTTTGGGGATCACATTGTATGAGTTGGCCACAGGCCGATTTCCTTATCCAAAGTGGAATAGTGTATTTGATCAACTAACACAAGTCGTGAAAGGAGATCCTCCGCAGCTGAGTAATTCTGAGGAAAGGGAATTCTCCCCGAGTTTCATCAACTTTGTCAACTTGTGCCTTACGAAGGATGAATCCAAAAGGCCAAAGTATAAAGAGCTTCTGAAACATCCCTTTATTTTGATGTATGAAGAACGTGCCGTTGAGGTCGCATGCTATGTTTGTAAAATCCTGGATCAAATGCCAGCTACTCCCAGCTCTCCCATGTATGTCGAT</t>
+  </si>
+  <si>
+    <t>AAPK2_HUMAN_D0_2H6D_A</t>
+  </si>
+  <si>
+    <t>CLK3_HUMAN_D0_2WU7_A</t>
+  </si>
+  <si>
+    <t>ATGACCGTGTTCAGGCAGGAAAACGTGGATGATTACTACGACACCGGCGAGGAACTTGGCAGTGGACAGTTTGCGGTTGTGAAGAAATGCCGTGAGAAAAGCACCGGCCTCCAGTATGCCGCCAAATTCATCAAGAAAAGGAGGACTAAGTCCAGCCGGCGGGGTGTGAGCCGCGAGGACATCGAGCGGGAGGTCAGCATCCTGAAGGAGATCCAGCACCCCAATGTCATCACCCTGCACGAGGTCTATGAGAACAAGACGGACGTCATCCTGATCTTGGAACTCGTTGCAGGTGGCGAGCTGTTTGACTTCTTAGCTGAAAAGGAATCTTTAACTGAAGAGGAAGCAACTGAATTTCTCAAACAAACTCTTAATGGTGTTTACTACCTGCACTCCCTTCAAATCGCCCACTTTGATCTTAAGCCTGAGAACATAATGCTTTTGGATAGAAATGTCCCCAAACCTCGGATCAAGATCATTGACTTTGGGTTGGCCCATAAAATTGACTTTGGAAATGAATTTAAAAACATATTTGGGACTCCAGAGTTTGTCGCTCCTGAGATAGTCAACTATGAACCTCTTGGTCTTGAGGCAGATATGTGGAGTATCGGGGTAATAACCTATATCCTCCTAAGTGGGGCCTCCCCATTTCTTGGAGACACTAAGCAAGAAACGTTAGCAAATGTATCCGCTGTCAACTACGAATTTGAGGATGAATACTTCAGTAATACCAGTGCCCTAGCCAAAGATTTCATAAGAAGACTTCTGGTCAAGGATCCAAAGAAGAGAATGACAATTCAAGATAGTTTGCAGCATCCCTGGATCAAGCCTAAAGATACACAACAGGCACTTAGTAGAAAAGCATCAGCAGTAAACATGGAGAAATTCAAGAAGTTTGCAGCCCGGAAAAAATGGAAACAATCCGTTCGCTTGATATCACTGTGCCAAAGATTATCCAGGTCATTCCTGTCCAGAAGTAACATGAGTGTTGCCAGAAGCGAT</t>
+  </si>
+  <si>
+    <t>GAAGCCTTTCTCACCCAGAAAGCCAAGGTCGGCGAACTCAAAGACGATGACTTCGAAAGGATCTCAGAGCTGGGCGCGGGCAACGGCGGGGTGGTCACCAAAGTCCAGCACAGACCCTCGGGCCTCATCATGGCCAGGAAGCTGATCCACCTTGAGATCAAGCCGGCCATCCGGAACCAGATCATCCGCGAGCTGCAGGTCCTGCACGAATGCAACTCGCCGTACATCGTGGGCTTCTACGGGGCCTTCTACAGTGACGGGGAGATCAGCATTTGCATGGAACACATGGACGGCGGCTCCCTGGACCAGGTGCTGAAAGAGGCCAAGAGGATTCCCGAGGAGATCCTGGGGAAAGTCAGCATCGCGGTTCTCCGGGGCTTGGCGTACCTCCGAGAGAAGCACCAGATCATGCACCGAGATGTGAAGCCCTCCAACATCCTCGTGAACTCTAGAGGGGAGATCAAGCTGTGTGACTTCGGGGTGAGCGGCCAGCTCATAGACTCCATGGCCAACTCCTTCGTGGGCACGCGCTCCTACATGGCTCCGGAGCGGTTGCAGGGCACACATTACTCGGTGCAGTCGGACATCTGGAGCATGGGCCTGTCCCTGGTGGAGCTGGCCGTCGGAAGGTACCCCATCCCCCCGCCCGACGCCAAAGAGCTGGAGGCCATCTTTGGCCGGCCCGTGGTCGACGGGGAAGAAGGAGAGCCTCACAGCATCTCGCCTCGGCCGAGGCCCCCCGGGCGCCCCGTCAGCGGTCACGGGATGGATAGCCGGCCTGCCATGGCCATCTTTGAACTCCTGGACTATATTGTGAACGAGCCACCTCCTAAGCTGCCCAACGGTGTGTTCACCCCCGACTTCCAGGAGTTTGTCAATAAATGCCTCATCAAGAACCCAGCGGAGCGGGCGGACCTGAAGATGCTCACAAACCACACCTTCATCAAGCGGTCCGAGGTGGAAGAAGTGGATTTTGCCGGCTGGTTGTGTAAAACCCTGCGGCTGAACCAGCCCGGCACACCCACGCGCACCGCCGTG</t>
+  </si>
+  <si>
+    <t>MKNK2_HUMAN_D0_2AC3_A</t>
+  </si>
+  <si>
+    <t>STRDYEIQRERIELGRCIGEGQFGDVHQGIYMSPENPALAVAIKTCKNCTSDSVREKFLQEALTMRQFDHPHIVKLIGVITENPVWIIMELCTLGELRSFLQVRKYSLDLASLILYAYQLSTALAYLESKRFVHRDIAARNVLVSSNDCVKLGDFGLSRYMEDSTYYKASKGKLPIKWMAPESINFRRFTSASDVWMFGVCMWEILMHGVKPFQGVKNNDVIGRIENGERLPMPPNCPPTLYSLMTKCWAYDPSRRPRFTELKAQLSTILEEEKAQQEE</t>
+  </si>
+  <si>
+    <t>CSK22_HUMAN_D0_3E3B_X</t>
+  </si>
+  <si>
+    <t>Cterm</t>
+  </si>
+  <si>
+    <t>ATGAGCAGAAGCAAGCGTGACAACAATTTTTATAGTGTAGAGATTGGAGATTCTACATTCACAGTCCTGAAACGATATCAGAATTTAAAACCTATAGGCTCAGGAGCTCAAGGAATAGTATGCGCAGCTTATGATGCCATTCTTGAAAGAAATGTTGCAATCAAGAAGCTAAGCCGACCATTTCAGAATCAGACTCATGCCAAGCGGGCCTACAGAGAGCTAGTTCTTATGAAATGTGTTAATCACAAAAATATAATTGGCCTTTTGAATGTTTTCACACCACAGAAATCCCTAGAAGAATTTCAAGATGTTTACATAGTCATGGAGCTCATGGATGCAAATCTTTGCCAAGTGATTCAGATGGAGCTAGATCATGAAAGAATGTCCTACCTTCTCTATCAGATGCTGTGTGGAATCAAGCACCTTCATTCTGCTGGAATTATTCATCGGGACTTAAAGCCCAGTAATATAGTAGTAAAATCTGATTGCACTTTGAAGATTCTTGACTTCGGTCTGGCCAGGACTGCAGGAACGAGTTTTATGATGACGCCTTATGTAGTGACTCGCTACTACAGAGCACCCGAGGTCATCCTTGGCATGGGCTACAAGGAAAACGTGGATTTATGGTCTGTGGGGTGCATTATGGGAGAAATGGTTTGCCACAAAATCCTCTTTCCAGGAAGGGACTATATTGATCAGTGGAATAAAGTTATTGAACAGCTTGGAACACCATGTCCTGAATTCATGAAGAAACTGCAACCAACAGTAAGGACTTACGTTGAAAACAGACCTAAATATGCTGGATATAGCTTTGAGAAACTCTTCCCTGATGTCCTTTTCCCAGCTGACTCAGAACACAACAAACTTAAAGCCAGTCAGGCAAGGGATTTGTTATCCAAAATGCTGGTAATAGATGCATCTAAAAGGATCTCTGTAGATGAAGCTCTCCAACACCCGTACATCAATGTCTGGTATGATCCTTCTGAAGCAGAAGCTCCACCACCAAAGATCCCTGACAAGCAGTTAGATGAAAGGGAACACACAATAGAAGAGTGGAAAGAATTGATATATAAGGAAGTTATGGACTTGGAG</t>
+  </si>
+  <si>
+    <t>TTSLEALPTGTVLTDKSGRQWKLKSFQTRDNQGILYEAAPTSTLTCDSGPQKQKFSLKLDAKDGRLFNEQNFFQRAAKPLQVNKWKKLYSTPLLAIPTCMGFGVHQDKYRFLVLPSLGRSLQSALDVSPKHVLSERSVLQVACRLLDALEFLHENEYVHGNVTAENIFVDPEDQSQVTLAGYGFAFRYCPSGKHVAYVEGSRSPHEGDLEFISMDLHKGCGPSRRSDLQSLGYCMLKWLYGFLPWTNCLPNTEDIMKQKQKFVDKPGPFVGPCGHWIRPSETLQKYLKVVMALTYEEKPPYAMLRNNLEALLQDLRVSPYDPIGLPMVP</t>
+  </si>
+  <si>
+    <t>SPNYDKWEMERTDITMKHKLGGGQYGEVYEGVWKKYSLTVAVKTLKEDTMEVEEFLKEAAVMKEIKHPNLVQLLGVCTREPPFYIITEFMTYGNLLDYLRECNRQEVNAVVLLYMATQISSAMEYLEKKNFIHRDLAARNCLVGENHLVKVADFGLSRLMTGDTYTAHAGAKFPIKWTAPESLAYNKFSIKSDVWAFGVLLWEIATYGMSPYPGIDLSQVYELLEKDYRMERPEGCPEKVYELMRACWQWNPSDRPSFAEIHQAFETMFQESSISDEVEKELGK</t>
+  </si>
+  <si>
+    <t>PLK2_HUMAN_D0_4I6B_A</t>
+  </si>
+  <si>
+    <t>ATGGCGGCGGCGGCGGCTCAGGGGGGCGGGGGCGGGGAGCCCCGTAGAACCGAGGGGGTCGGCCCGGGGGTCCCGGGGGAGGTGGAGATGGTGAAGGGGCAGCCGTTCGACGTGGGCCCGCGCTACACGCAGTTGCAGTACATCGGCGAGGGCGCGTACGGCATGGTCAGCTCGGCCTATGACCACGTGCGCAAGACTCGCGTGGCCATCAAGAAGATCAGCCCCTTCGAACATCAGACCTACTGCCAGCGCACGCTCCGGGAGATCCAGATCCTGCTGCGCTTCCGCCATGAGAATGTCATCGGCATCCGAGACATTCTGCGGGCGTCCACCCTGGAAGCCATGAGAGATGTCTACATTGTGCAGGACCTGATGGAGACTGACCTGTACAAGTTGCTGAAAAGCCAGCAGCTGAGCAATGACCATATCTGCTACTTCCTCTACCAGATCCTGCGGGGCCTCAAGTACATCCACTCCGCCAACGTGCTCCACCGAGATCTAAAGCCCTCCAACCTGCTCATCAACACCACCTGCGACCTTAAGATTTGTGATTTCGGCCTGGCCCGGATTGCCGATCCTGAGCATGACCACACCGGCTTCCTGACGGAGTATGTGGCTACGCGCTGGTACCGGGCCCCAGAGATCATGCTGAACTCCAAGGGCTATACCAAGTCCATCGACATCTGGTCTGTGGGCTGCATTCTGGCTGAGATGCTCTCTAACCGGCCCATCTTCCCTGGCAAGCACTACCTGGATCAGCTCAACCACATTCTGGGCATCCTGGGCTCCCCATCCCAGGAGGACCTGAATTGTATCATCAACATGAAGGCCCGAAACTACCTACAGTCTCTGCCCTCCAAGACCAAGGTGGCTTGGGCCAAGCTTTTCCCCAAGTCAGACTCCAAAGCCCTTGACCTGCTGGACCGGATGTTAACCTTTAACCCCAATAAACGGATCACAGTGGAGGAAGCGCTGGCTCACCCCTACCTGGAGCAGTACTATGACCCGACGGATGAGCCAGTGGCCGAGGAGCCCTTCACCTTCGCCATGGAGCTGGATGACCTACCTAAGGAGCGGCTGAAGGAGCTCATCTTCCAGGAGACAGCACGCTTCCAGCCCGGAGTGCTGGAGGCCCCC</t>
+  </si>
+  <si>
+    <t>MTVFRQENVDDYYDTGEELGSGQFAVVKKCREKSTGLQYAAKFIKKRRTKSSRRGVSREDIEREVSILKEIQHPNVITLHEVYENKTDVILILELVAGGELFDFLAEKESLTEEEATEFLKQTLNGVYYLHSLQIAHFDLKPENIMLLDRNVPKPRIKIIDFGLAHKIDFGNEFKNIFGTPEFVAPEIVNYEPLGLEADMWSIGVITYILLSGASPFLGDTKQETLANVSAVNYEFEDEYFSNTSALAKDFIRRLLVKDPKKRMTIQDSLQHPWIKPKDTQQALSRKASAVNMEKFKKFAARKKWKQSVRLISLCQRLSRSFLSRSNMSVARSD</t>
   </si>
   <si>
     <t>AURKA_HUMAN_D0_2NP8_A</t>
-  </si>
-  <si>
-    <t>HIGNYRLLKTIGKGNFAKVKLARHILTGKEVAVKIIDKTQLNSSSLQKLFREVRIMKVLNHPNIVKLFEVIETEKTLYLVMEYASGGEVFDYLVAHGRMKEKEARAKFRQIVSAVQYCHQKFIVHRDLKAENLLLDADMNIKIADFGFSNEFTFGNKLDTFCGSPPYAAPELFQGKKYDGPEVDVWSLGVILYTLVSGSLPFDGQNLKELRERVLRGKYRIPFYMSTDCENLLKKFLILNPSKRGTLEQIMKDRWMNVGHEDDELKPYVEPLPDYKDPRRTELMVSMGYTREEIQDSLVGQRYNEVMATYLLLGY</t>
-  </si>
-  <si>
-    <t>GVVTHEQFKAALRMVVDQGDPRLLLDSYVKIGEGSTGIVCLAREKHSGRQVAVKMMDLRKQQRRELLFNEVVIMRDYQHFNVVEMYKSYLVGEELWVLMEFLQGGALTDIVSQVRLNEEQIATVCEAVLQALAYLHAQGVIHRDIKSDSILLTLDGRVKLSDFGFCAQISKDVPKRKSLVGTPYWMAPEVISRSLYATEVDIWSLGIMVIEMVDGEPPYFSDSPVQAMKRLRDSPPPKLKNSHKVSPVLRDFLERMLVRDPQERATAQELLDHPFLLQTGLPECLVPLIQLYRKQTSTC</t>
-  </si>
-  <si>
-    <t>ATGGCAAAGCAGTACGACTCGGTGGAGTGCCCTTTTTGTGATGAAGTTTCCAAATACGAGAAGCTCGCCAAGATCGGCCAAGGCACCTTCGGGGAGGTGTTCAAGGCCAGGCACCGCAAGACCGGCCAGAAGGTGGCTCTGAAGAAGGTGCTGATGGAAAACGAGAAGGAGGGGTTCCCCATTACAGCCTTGCGGGAGATCAAGATCCTTCAGCTTCTAAAACACGAGAATGTGGTCAACTTGATTGAGATTTGTCGAACCAAAGCTTCCCCCTATAACCGCTGCAAGGGTAGTATATACCTGGTGTTCGACTTCTGCGAGCATGACCTTGCTGGGCTGTTGAGCAATGTTTTGGTCAAGTTCACGCTGTCTGAGATCAAGAGGGTGATGCAGATGCTGCTTAACGGCCTCTACTACATCCACAGAAACAAGATCCTGCATAGGGACATGAAGGCTGCTAATGTGCTTATCACTCGTGATGGGGTCCCGAAGCTGGCAGACTTTGGGCTGGCCCGGGCCTTCAGCCTGGCCAAGAACAGCCAGCCCAACCGCTACACCAACCGTGTGGTGACACTCTGGTACCGGCCCCCGGAGCTGTTGCTCGGGGAGCGGGACTACGGCCCCCCCATTGACCTGTGGGGTGCTGGGTGCATCATGGCAGAGATGTGGACCCGCAGCCCCATCATGCAGGGCAACACGGAGCAGCACCAACTCGCCCTCATCAGTCAGCTCTGCGGCTCCATCACCCCTGAGGTGTGGCCAAACGTGGACAACTATGAGCTGTACGAAAAGCTGGAGCTGGTCAAGGGCCAGAAGCGGAAGGTGAAGGACAGGCTGAAGGCCTATGTGCGTGACCCATACGCACTGGACCTCATCGACAAGCTGCTGGTGCTGGACCCTGCCCAGCGCATCGACAGCGATGACGCCCTCAACCACGACTTCTTCTGGTCCGACCCCATGCCCTCCGACCTCAAGGGCATGCTCTCCACC</t>
-  </si>
-  <si>
-    <t>MSQERPTFYRQELNKTIWEVPERYQNLSPVGSGAYGSVCAAFDTKTGLRVAVKKLSRPFQSIIHAKRTYRELRLLKHMKHENVIGLLDVFTPARSLEEFNDVYLVTHLMGADLNNIVKCQKLTDDHVQFLIYQILRGLKYIHSADIIHRDLKPSNLAVNEDCELKILDFGLARHTDDEMTGYVATRWYRAPEIMLNWMHYNQTVDIWSVGCIMAELLTGRTLFPGTDHIDQLKLILRLVGTPGAELLKKISSESARNYIQSLTQMPKMNFANVFIGANPLAVDLLEKMLVLDSDKRITAAQALAHAYFAQYHDPDDEPVADPYDQSFESRDLLIDEWKSLTYDEVISFVPPPLDQEEMES</t>
-  </si>
-  <si>
-    <t>MELRVGNRYRLGRKIGSGSFGDIYLGTDIAAGEEVAIKLECVKTKHPQLHIESKIYKMMQGGVGIPTIRWCGAEGDYNVMVMELLGPSLEDLFNFCSRKFSLKTVLLLADQMISRIEYIHSKNFIHRDVKPDNFLMGLGKKGNLVYIIDFGLAKKYRDARTHQHIPYRENKNLTGTARYASINTHLGIEQSRRDDLESLGYVLMYFNLGSLPWQGLKAATKRQKYERISEKKMSTPIEVLCKGYPSEFATYLNFCRSLRFDDKPDYSYLRQLFRNLFHRQGFSYDYVFDWNMLK</t>
-  </si>
-  <si>
-    <t>MAKQYDSVECPFCDEVSKYEKLAKIGQGTFGEVFKARHRKTGQKVALKKVLMENEKEGFPITALREIKILQLLKHENVVNLIEICRTKASPYNRCKGSIYLVFDFCEHDLAGLLSNVLVKFTLSEIKRVMQMLLNGLYYIHRNKILHRDMKAANVLITRDGVPKLADFGLARAFSLAKNSQPNRYTNRVVTLWYRPPELLLGERDYGPPIDLWGAGCIMAEMWTRSPIMQGNTEQHQLALISQLCGSITPEVWPNVDNYELYEKLELVKGQKRKVKDRLKAYVRDPYALDLIDKLLVLDPAQRIDSDDALNHDFFWSDPMPSDLKGMLST</t>
-  </si>
-  <si>
-    <t>targetID</t>
-  </si>
-  <si>
-    <t>TGGGCCCTGAACATGAAGGAGCTGAAGCTGCTGCAGACCATCGGGAAGGGGGAGTTCGGAGACGTGATGCTGGGCGATTACCGAGGGAACAAAGTCGCCGTCAAGTGCATTAAGAACGACGCCACTGCCCAGGCCTTCCTGGCTGAAGCCTCAGTCATGACGCAACTGCGGCATAGCAACCTGGTGCAGCTCCTGGGCGTGATCGTGGAGGAGAAGGGCGGGCTCTACATCGTCACTGAGTACATGGCCAAGGGGAGCCTTGTGGACTACCTGCGGTCTAGGGGTCGGTCAGTGCTGGGCGGAGACTGTCTCCTCAAGTTCTCGCTAGATGTCTGCGAGGCCATGGAATACCTGGAGGGCAACAATTTCGTGCATCGAGACCTGGCTGCCCGCAATGTGCTGGTGTCTGAGGACAACGTGGCCAAGGTCAGCGACTTTGGTCTCACCAAGGAGGCGTCCAGCACCCAGGACACGGGCAAGCTGCCAGTCAAGTGGACAGCCCCTGAGGCCCTGAGAGAGAAGAAATTCTCCACTAAGTCTGACGTGTGGAGTTTCGGAATCCTTCTCTGGGAAATCTACTCCTTTGGGCGAGTGCCTTATCCAAGAATTCCCCTGAAGGACGTCGTCCCTCGGGTGGAGAAGGGCTACAAGATGGATGCCCCCGACGGCTGCCCGCCCGCAGTCTATGAAGTCATGAAGAACTGCTGGCACCTGGACGCCGCCATGCGGCCCTCCTTCCTACAGCTCCGAGAGCAGCTTGAGCACATCAAAACCCACGAGCTGCACCTG</t>
-  </si>
-  <si>
-    <t>dna_seq</t>
-  </si>
-  <si>
-    <t>AACCTGGTTTTTAGTGACGGCTACGTGGTAAAGGAGACAATTGGTGTGGGCTCCTACTCTGAGTGCAAGCGCTGTGTCCACAAGGCCACCAACATGGAGTATGCTGTCAAGGTCATTGATAAGAGCAAGCGGGATCCTTCAGAAGAGATTGAGATTCTTCTGCGGTATGGCCAGCACCCCAACATCATCACTCTGAAAGATGTGTATGATGATGGCAAACACGTGTACCTGGTGACAGAGCTGATGCGGGGTGGGGAGCTGCTGGACAAGATCCTGCGGCAGAAGTTCTTCTCAGAGCGGGAGGCCAGCTTTGTCCTGCACACCATTGGCAAAACTGTGGAGTATCTGCACTCACAGGGGGTTGTGCACAGGGACCTGAAGCCCAGCAACATCCTGTATGTGGACGAGTCCGGGAATCCCGAGTGCCTGCGCATCTGTGACTTTGGTTTTGCCAAACAGCTGCGGGCTGAGAATGGGCTCCTCATGACACCTTGCTACACAGCCAACTTTGTGGCGCCTGAGGTGCTGAAGCGCCAGGGCTACGATGAAGGCTGCGACATCTGGAGCCTGGGCATTCTGCTGTACACCATGCTGGCAGGATATACTCCATTTGCCAACGGTCCCAGTGACACACCAGAGGAAATCCTAACCCGGATCGGCAGTGGGAAGTTTACCCTCAGTGGGGGAAATTGGAACACAGTTTCAGAGACAGCCAAGGACCTGGTGTCCAAGATGCTACACGTGGATCCCCACCAGCGCCTCACAGCTAAGCAGGTTCTGCAGCATCCATGGGTCACCCAGAAAGACAAGCTTCCCCAAAGCCAGCTGTCCCACCAGGACCTACAGCTTGTGAAGGGAGCCATGGCTGCCACGTACTCCGCACTCAACAGCTCCAAGCCCACCCCCCAGCTGAAGCCCATCGAGTCATCCATCCTGGCCCAGCGGCGAGTGAGGAAGTTGCCATCCACCACCCTG</t>
-  </si>
-  <si>
-    <t>ATGGCCGACGACGACGTGCTGTTCGAGGATGTGTACGAGCTGTGCGAGGTGATCGGAAAGGGTCCCTTCAGTGTTGTACGACGATGTATCAACAGAGAAACTGGGCAACAATTTGCTGTAAAAATTGTTGATGTAGCCAAGTTCACATCAAGTCCAGGGTTAAGTACAGAAGATCTAAAGCGGGAAGCCAGTATCTGTCATATGCTGAAACATCCACACATTGTAGAGTTATTGGAGACATATAGCTCAGATGGAATGCTTTACATGGTTTTCGAATTTATGGATGGAGCAGATCTGTGTTTTGAAATCGTAAAGCGAGCTGACGCTGGTTTTGTGTACAGTGAAGCTGTAGCCAGCCATTATATGAGACAGATACTGGAAGCTCTACGCTACTGCCATGATAATAACATAATTCACAGGGATGTGAAGCCCCACTGTGTTCTCCTTGCCTCAAAAGAAAACTCGGCACCTGTTAAACTTGGAGGCTTTGGGGTAGCTATTCAATTAGGGGAGTCTGGACTTGTAGCTGGAGGACGTGTTGGAACACCTCATTTTATGGCACCAGAAGTGGTCAAAAGAGAGCCTTACGGAAAGCCTGTAGACGTCTGGGGGTGCGGTGTGATCCTTTTTATCCTGCTCAGTGGTTGTTTGCCTTTTTACGGAACCAAGGAAAGATTGTTTGAAGGCATTATTAAAGGAAAATATAAGATGAATCCAAGGCAGTGGAGCCATATCTCTGAAAGTGCCAAAGACCTAGTACGTCGCATGCTGATGCTGGATCCAGCTGAAAGGATCACTGTTTATGAAGCACTGAATCACCCATGGCTTAAGGAGCGGGATCGTTACGCCTACAAGATTCATCTTCCAGAAACAGTAGAGCAGCTGAGGAAATTCAATGCAAGGAGGAAACTAAAGGGTGCAGTACTAGCCGCTGTGTCAAGTCACAAATTCAACTCATTCTATGGGGATCCCCCTGAAGAGTTACCAGATTTCTCCGAAGACCCTACCTCCTCAGGAGCA</t>
-  </si>
-  <si>
-    <t>E2AK2_HUMAN_D0_3UIU_A</t>
-  </si>
-  <si>
-    <t>ATGGGGAAGGTGAAAGCCACCCCCATGACACCTGAACAAGCAATGAAGCAATACATGCAAAAACTCACAGCCTTCGAACACCATGAGATTTTCAGCTACCCTGAAATATATTTCTTGGGTCTAAATGCTAAGAAGCGCCAGGGCATGACAGGTGGGCCCAACAATGGTGGCTATGATGATGACCAGGGATCATATGTGCAGGTGCCCCACGATCACGTGGCTTACAGGTATGAGGTCCTCAAGGTCATTGGGAAGGGGAGCTTTGGGCAGGTGGTCAAGGCCTACGATCACAAAGTCCACCAGCACGTGGCCCTAAAGATGGTGCGGAATGAGAAGCGCTTCCACCGGCAAGCAGCGGAGGAGATCCGAATCCTGGAACACCTGCGGAAGCAGGACAAGGATAACACAATGAATGTCATCCATATGCTGGAGAATTTCACCTTCCGCAACCACATCTGCATGACGTTTGAGCTGCTGAGCATGAACCTCTATGAGCTCATCAAGAAGAATAAATTCCAGGGCTTCAGTCTGCCTTTGGTTCGCAAGTTTGCCCACTCGATTCTGCAGTGCTTGGATGCTTTGCACAAAAACAGAATAATTCACTGTGACCTTAAGCCCGAGAACATTTTGTTAAAGCAGCAGGGTAGAAGCGGTATTAAAGTAATTGATTTTGGCTCCAGTTGTTACGAGCATCAGCGTGTCTACACGTACATCCAGTCGCGTTTTTACCGGGCTCCAGAAGTGATCCTTGGGGCCAGGTATGGCATGCCCATTGATATGTGGAGCCTGGGCTGCATTTTAGCAGAGCTCCTGACGGGTTACCCCCTCTTGCCTGGGGAAGATGAAGGGGACCAGCTGGCCTGTATGATTGAACTGTTGGGCATGCCCTCACAGAAACTGCTGGATGCATCCAAACGAGCCAAAAATTTTGTGAGCTCCAAGGGTTATCCCCGTTACTGCACTGTCACGACTCTCTCAGATGGCTCTGTGGTCCTAAACGGAGGCCGTTCCCGGAGGGGGAAACTGAGGGGCCCACCGGAGAGCAGAGAGTGGGGGAACGCGCTGAAGGGGTGTGATGATCCCCTTTTCCTTGACTTCTTAAAACAGTGTTTAGAGTGGGATCCTGCAGTGCGCATGACCCCAGGCCAGGCTTTGCGGCACCCCTGGCTGAGGAGGCGGTTGCCAAAGCCTCCCACCGGGGAGAAAACGTCAGTGAAAAGG</t>
-  </si>
-  <si>
-    <t>SVYPKALRDEYIMSKTLGSGACGEVKLAFERKTCKKVAIKIISKRKFAIGSAREADPALNVETEIEILKKLNHPCIIKIKNFFDAEDYYIVLELMEGGELFDKVVGNKRLKEATCKLYFYQMLLAVQYLHENGIIHRDLKPENVLLSSQEEDCLIKITDFGHSKIWGETSLMRTLCGTPTYLAPEVLVSVGTAGYNRAVDCWSLGVILFICLSGYPPFSEHRTQVSLKDQITSGKYNFIPEVWAEVSEKALDLVKKLLVVDPKARFTTEEALRHPWLQDEDMKRKFQDLLSEENESTALPQVLAQPSTSRKRPREGEAEGAE</t>
-  </si>
-  <si>
-    <t>ATGGAGAAGTATGAAAAAATTGGGAAAATTGGAGAAGGATCCTATGGAGTTGTTTTCAAATGTAGAAACAGGGACACGGGTCAGATTGTGGCCATCAAGAAGTTTCTGGAATCAGAAGATGACCCTGTCATAAAGAAAATTGCCCTTCGGGAAATCCGAATGCTCAAGCAACTCAAGCATCCCAACCTTGTTAACCTCCTGGAAGTCTTCAGGAGGAAACGGAGGCTTCACCTGGTGTTTGAATATTGTGACCACACAGTTCTCCATGAGTTGGACAGATACCAAAGAGGGGTACCAGAACATCTCGTGAAGAGCATAACTTGGCAGACACTGCAAGCTGTAAATTTTTGCCATAAACACAATTGCATACATAGAGACGTGAAGCCAGAAAATATCCTCATCACGAAACATTCCGTGATTAAGCTTTGTGACTTTGGATTTGCTCGGCTTTTGACTGGACCGAGTGACTACTATACAGACTACGTGGCTACCAGGTGGTACCGCTCCCCTGAGCTGCTGGTGGGGGACACGCAGTACGGCCCCCCGGTGGATGTTTGGGCAATTGGCTGTGTCTTTGCTGAGCTGCTGTCAGGAGTGCCTCTGTGGCCAGGAAAATCGGATGTGGATCAGCTGTATCTGATTAGGAAGACCTTGGGGGATCTCATTCCTAGGCACCAGCAAGTGTTTAGCACGAATCAGTACTTCAGTGGAGTGAAAATTCCAGACCCTGAAGATATGGAACCACTTGAATTAAAATTCCCAAACATCTCTTATCCTGCCCTGGGGCTCCTA</t>
-  </si>
-  <si>
-    <t>KHDGRVKIGHYVLGDTLGVGTFGKVKIGEHQLTGHKVAVKILNRQKIRSLDVVGKIKREIQNLKLFRHPHIIKLYQVISTPTDFFMVMEYVSGGELFDYICKHGRVEEMEARRLFQQILSAVDYCHRHMVVHRDLKPENVLLDAHMNAKIADFGLSNMMSDGEFLRTSCGSPNYAAPEVISGRLYAGPEVDIWSCGVILYALLCGTLPFDDEHVPTLFKKIRGGVFYIPEYLNRSVATLLMHMLQVDPLKRATIKDIREHEWFKQDLPSYLFPE</t>
-  </si>
-  <si>
-    <t>ATGGAAAACTTTAATAATTTCTATATACTTACATCTAAAGAGCTAGGGAGAGGAAAATTTGCTGTGGTTAGACAATGTATATCAAAATCTACTGGCCAAGAATATGCTGCAAAATTTCTAAAAAAGAGAAGAAGAGGACAGGATTGTCGAGCAGAAATTTTACACGAGATTGCTGTGCTTGAATTGGCAAAGTCTTGTCCCCGTGTTATTAATCTTCATGAGGTCTATGAAAATACAAGTGAAATCATTTTGATATTGGAATATGCTGCAGGTGGAGAAATTTTCAGCCTGTGTTTACCTGAGTTGGCTGAAATGGTTTCTGAAAATGATGTTATCAGACTCATTAAACAAATACTTGAAGGAGTTTATTATCTACATCAGAATAACATTGTACACCTTGATTTAAAGCCACAGAATATATTACTGAGCAGCATATACCCTCTCGGGGACATTAAAATAGTAGATTTTGGAATGTCTCGAAAAATAGGGCATGCGTGTGAACTTCGGGAAATCATGGGAACACCAGAATATTTAGCTCCAGAAATCCTGAACTATGATCCCATTACCACAGCAACAGATATGTGGAATATTGGTATAATAGCATATATGTTGTTAACTCACACATCACCATTTGTGGGAGAAGATAATCAAGAAACATACCTCAATATTTCTCAAGTTAATGTAGATTATTCGGAAGAAACTTTTTCATCAGTTTCACAGCTGGCCACAGACTTTATTCAGAGCCTTTTAGTAAAAAATCCAGAGAAAAGACCAACAGCAGAGATATGCCTTTCTCATTCTTGGCTACAGCAGTGGGACTTTGAAAACTTGTTTCACCCTGAAGAAACTTCCAGTTCCTCTCAAACTCAGGATCATTCTGTAAGGTCCTCTGAAGACAAGACTTCTAAATCCTCC</t>
-  </si>
-  <si>
-    <t>MPSRAEDYEVLYTIGTGSYGRCQKIRRKSDGKILVWKELDYGSMTEAEKQMLVSEVNLLRELKHPNIVRYYDRIIDRTNTTLYIVMEYCEGGDLASVITKGTKERQYLDEEFVLRVMTQLTLALKECHRRSDGGHTVLHRDLKPANVFLDGKQNVKLGDFGLARILNHDTSFAKTFVGTPYYMSPEQMNRMSYNEKSDIWSLGCLLYELCALMPPFTAFSQKELAGKIREGKFRRIPYRYSDELNEIITRMLNLKDYHRPSVEEILENPLI</t>
-  </si>
-  <si>
-    <t>GACCCAGAAGAGCTTTTTACAAAACTAGAGAAAATTGGGAAGGGCTCCTTTGGAGAGGTGTTCAAAGGCATTGACAATCGGACTCAGAAAGTGGTTGCCATAAAGATCATTGATCTGGAAGAAGCTGAAGATGAGATAGAGGACATTCAACAAGAAATCACAGTGCTGAGTCAGTGTGACAGTCCATATGTAACCAAATATTATGGATCCTATCTGAAGGATACAAAATTATGGATAATAATGGAATATCTTGGTGGAGGCTCCGCACTAGATCTATTAGAACCTGGCCCATTAGATGAAACCCAGATCGCTACTATATTAAGAGAAATACTGAAAGGACTCGATTATCTCCATTCGGAGAAGAAAATCCACAGAGACATTAAAGCGGCCAACGTCCTGCTGTCTGAGCATGGCGAGGTGAAGCTGGCGGACTTTGGCGTGGCTGGCCAGCTGACAGACACCCAGATCAAAAGGAACACCTTCGTGGGCACCCCATTCTGGATGGCACCCGAGGTCATCAAACAGTCGGCCTATGACTCGAAGGCAGACATCTGGTCCCTGGGCATAACAGCTATTGAACTTGCAAGAGGGGAACCACCTCATTCCGAGCTGCACCCCATGAAAGTTTTATTCCTCATTCCAAAGAACAACCCACCGACGTTGGAAGGAAACTACAGTAAACCCCTCAAGGAGTTTGTGGAGGCCTGTTTGAATAAGGAGCCGAGCTTTAGACCCACTGCTAAGGAGTTATTGAAGCACAAGTTTATACTACGCAATGCAAAGAAAACTTCCTACTTGACCGAGCTCATCGAC</t>
-  </si>
-  <si>
-    <t>VIIDNKRYLFIQKLGEGGFSYVDLVEGLHDGHFYALKRILCHEQQDREEAQREADMHRLFNHPNILRLVAYCLRERGAKHEAWLLLPFFKRGTLWNEIERLKDKGNFLTEDQILWLLLGICRGLEAIHAKGYAHRDLKPTNILLGDEGQPVLMDLGSMNQACIHVEGSRQALTLQDWAAQRCTISYRAPELFSVQSHCVIDERTDVWSLGCVLYAMMFGEGPYDMVFQKGDSVALAVQNQLSIPQSPRHSSALWQLLNSMMTVDPHQRPHIPLLLSQLEALQ</t>
-  </si>
-  <si>
-    <t>DEQPHIGNYRLLKTIGKGNFAKVKLARHILTGREVAIKIIDKTQLNPTSLQKLFREVRIMKILNHPNIVKLFEVIETEKTLYLIMEYASGGEVFDYLVAHGRMKEKEARSKFRQIVSAVQYCHQKRIVHRDLKAENLLLDADMNIKIADFGFSNEFTVGGKLDTFCGSPPYAAPELFQGKKYDGPEVDVWSLGVILYTLVSGSLPFDGQNLKELRERVLRGKYRIPFYMSTDCENLLKRFLVLNPIKRGTLEQIMKDRWINAGHEEDELKPFVEPELDISDQKRIDIMVGMGYSQEEIQESLSKMKYDEITATYLLLGRKSSE</t>
-  </si>
-  <si>
-    <t>AAGGAGAAGGAGCCCCTGGAGTCGCAGTACCAGGTGGGCCCGCTACTGGGCAGCGGCGGCTTCGGCTCGGTCTACTCAGGCATCCGCGTCTCCGACAACTTGCCGGTGGCCATCAAACACGTGGAGAAGGACCGGATTTCCGACTGGGGAGAGCTGCCTAATGGCACTCGAGTGCCCATGGAAGTGGTCCTGCTGAAGAAGGTGAGCTCGGGTTTCTCCGGCGTCATTAGGCTCCTGGACTGGTTCGAGAGGCCCGACAGTTTCGTCCTGATCCTGGAGAGGCCCGAGCCGGTGCAAGATCTCTTCGACTTCATCACGGAAAGGGGAGCCCTGCAAGAGGAGCTGGCCCGCAGCTTCTTCTGGCAGGTGCTGGAGGCCGTGCGGCACTGCCACAACTGCGGGGTGCTCCACCGCGACATCAAGGACGAAAACATCCTTATCGACCTCAATCGCGGCGAGCTCAAGCTCATCGACTTCGGGTCGGGGGCGCTGCTCAAGGACACCGTCTACACGGACTTCGATGGGACCCGAGTGTATAGCCCTCCAGAGTGGATCCGCTACCATCGCTACCATGGCAGGTCGGCGGCAGTCTGGTCCCTGGGGATCCTGCTGTATGATATGGTGTGTGGAGATATTCCTTTCGAGCATGACGAAGAGATCATCGGGGGCCAGGTTTTCTTCAGGCAGAGGGTCTCTTCAGAATGTCAGCATCTCATTAGATGGTGCTTGGCCCTGAGACCATCAGATAGGCCAACCTTCGAAGAAATCCAGAACCATCCATGGATGCAAGATGTTCTCCTGCCCCAGGAAACTGCTGAGATCCACCTCCACAGCCTGTCGCCGGGGCCCAGCAAA</t>
-  </si>
-  <si>
-    <t>PFPEGKVLDDMEGNQWVLGKKIGSGGFGLIYLAFPTNKPEKDARHVVKVEYQENGPLFSELKFYQRVAKKDCIKKWIERKQLDYLGIPLFYGSGLTEFKGRSYRFMVMERLGIDLQKISGQNGTFKKSTVLQLGIRMLDVLEYIHENEYVHGDIKAANLLLGYKNPDQVYLADYGLSYRYCPNGNHKQYQENPRKGHNGTIEFTSLDAHKGVALSRRSDVEILGYCMLRWLCGKLPWEQNLKDPVAVQTAKTNLLDELPQSVLKWAPSGSSCCEIAQFLVCAHSLAYDEKPNYQALKKILNPHGIPLGPLDFSTKGQSINVH</t>
-  </si>
-  <si>
-    <t>MESDLHQIIHSSQPLTLEHVRYFLYQLLRGLKYMHSAQVIHRDLKPSNLLVNENCELKIGDFGMARGLCTSPAEHQYFMTEYVATRWYRAPELMLSLHEYTQAIDLWSVGCIFGEMLARRQLFPGKNYVHQLQLIMMVLGTPSPAVIQAVGAERVRAYIQSLPPRQPVPWETVYPGADRQALSLLGRMLRFEPSARISAAAALRHPFLAKYHDPDDEPDCAPPFDFAFDREALTRERIKEAIVAEIEDFHARREGIRQQIRFQPSLQPVASEPGCPDVEMPSPWAPSGDCAM</t>
-  </si>
-  <si>
-    <t>EPKKYAVTDDYQLSKQVLGLGVNGKVLECFHRRTGQKCALKLLYDSPKARQEVDHHWQASGGPHIVCILDVYENMHHGKRCLLIIMECMEGGELFSRIQERGDQAFTEREAAEIMRDIGTAIQFLHSHNIAHRDVKPENLLYTSKEKDAVLKLTDFGFAKETTQNALQTPCYTPYYVAPEVLGPEKYDKSCDMWSLGVIMYILLCGFPPFYSNTGQAISPGMKRRIRLGQYGFPNPEWSEVSEDAKQLIRLLLKTDPTERLTITQFMNHPWINQSMVVPQTPLHTARVLQEDKDHWDEVKEEMTSALATMRVDYDQV</t>
-  </si>
-  <si>
-    <t>STK24_HUMAN_D0_3ZHP_C</t>
-  </si>
-  <si>
-    <t>aa_seq</t>
-  </si>
-  <si>
-    <t>KC1D_HUMAN_D0_4HNF_B</t>
-  </si>
-  <si>
-    <t>AGCATTGAGTCATCAGGAAAACTGAAGATCTCCCCTGAACAACACTGGGATTTCACTGCAGAGGACTTGAAAGACCTTGGAGAAATTGGACGAGGAGCTTATGGTTCTGTCAACAAAATGGTCCACAAACCAAGTGGGCAAATAATGGCAGTTAAAAGAATTCGGTCAACAGTGGATGAAAAAGAACAAAAACAACTTCTTATGGATTTGGATGTAGTAATGCGGAGTAGTGATTGCCCATACATTGTTCAGTTTTATGGTGCACTCTTCAGAGAGGGTGACTGTTGGATCTGTATGGAACTCATGTCTACCTCGTTTGATAAGTTTTACAAATATGTATATAGTGTATTAGATGATGTTATTCCAGAAGAAATTTTAGGCAAAATCACTTTAGCAACTGTGAAAGCACTAAACCACTTAAAAGAAAACTTGAAAATTATTCACAGAGATATCAAACCTTCCAATATTCTTCTGGACAGAAGTGGAAATATTAAGCTCTGTGACTTCGGCATCAGTGGACAGCTTGTGGACTCTATTGCCAAGACAAGAGATGCTGGCTGTAGGCCATACATGGCACCTGAAAGAATAGACCCAAGCGCATCACGACAAGGATATGATGTCCGCTCTGATGTCTGGAGTTTGGGGATCACATTGTATGAGTTGGCCACAGGCCGATTTCCTTATCCAAAGTGGAATAGTGTATTTGATCAACTAACACAAGTCGTGAAAGGAGATCCTCCGCAGCTGAGTAATTCTGAGGAAAGGGAATTCTCCCCGAGTTTCATCAACTTTGTCAACTTGTGCCTTACGAAGGATGAATCCAAAAGGCCAAAGTATAAAGAGCTTCTGAAACATCCCTTTATTTTGATGTATGAAGAACGTGCCGTTGAGGTCGCATGCTATGTTTGTAAAATCCTGGATCAAATGCCAGCTACTCCCAGCTCTCCCATGTATGTCGAT</t>
-  </si>
-  <si>
-    <t>AAPK2_HUMAN_D0_2H6D_A</t>
-  </si>
-  <si>
-    <t>CLK3_HUMAN_D0_2WU7_A</t>
-  </si>
-  <si>
-    <t>GAAGCCTTTCTCACCCAGAAAGCCAAGGTCGGCGAACTCAAAGACGATGACTTCGAAAGGATCTCAGAGCTGGGCGCGGGCAACGGCGGGGTGGTCACCAAAGTCCAGCACAGACCCTCGGGCCTCATCATGGCCAGGAAGCTGATCCACCTTGAGATCAAGCCGGCCATCCGGAACCAGATCATCCGCGAGCTGCAGGTCCTGCACGAATGCAACTCGCCGTACATCGTGGGCTTCTACGGGGCCTTCTACAGTGACGGGGAGATCAGCATTTGCATGGAACACATGGACGGCGGCTCCCTGGACCAGGTGCTGAAAGAGGCCAAGAGGATTCCCGAGGAGATCCTGGGGAAAGTCAGCATCGCGGTTCTCCGGGGCTTGGCGTACCTCCGAGAGAAGCACCAGATCATGCACCGAGATGTGAAGCCCTCCAACATCCTCGTGAACTCTAGAGGGGAGATCAAGCTGTGTGACTTCGGGGTGAGCGGCCAGCTCATAGACTCCATGGCCAACTCCTTCGTGGGCACGCGCTCCTACATGGCTCCGGAGCGGTTGCAGGGCACACATTACTCGGTGCAGTCGGACATCTGGAGCATGGGCCTGTCCCTGGTGGAGCTGGCCGTCGGAAGGTACCCCATCCCCCCGCCCGACGCCAAAGAGCTGGAGGCCATCTTTGGCCGGCCCGTGGTCGACGGGGAAGAAGGAGAGCCTCACAGCATCTCGCCTCGGCCGAGGCCCCCCGGGCGCCCCGTCAGCGGTCACGGGATGGATAGCCGGCCTGCCATGGCCATCTTTGAACTCCTGGACTATATTGTGAACGAGCCACCTCCTAAGCTGCCCAACGGTGTGTTCACCCCCGACTTCCAGGAGTTTGTCAATAAATGCCTCATCAAGAACCCAGCGGAGCGGGCGGACCTGAAGATGCTCACAAACCACACCTTCATCAAGCGGTCCGAGGTGGAAGAAGTGGATTTTGCCGGCTGGTTGTGTAAAACCCTGCGGCTGAACCAGCCCGGCACACCCACGCGCACCGCCGTG</t>
-  </si>
-  <si>
-    <t>MKNK2_HUMAN_D0_2AC3_A</t>
-  </si>
-  <si>
-    <t>STRDYEIQRERIELGRCIGEGQFGDVHQGIYMSPENPALAVAIKTCKNCTSDSVREKFLQEALTMRQFDHPHIVKLIGVITENPVWIIMELCTLGELRSFLQVRKYSLDLASLILYAYQLSTALAYLESKRFVHRDIAARNVLVSSNDCVKLGDFGLSRYMEDSTYYKASKGKLPIKWMAPESINFRRFTSASDVWMFGVCMWEILMHGVKPFQGVKNNDVIGRIENGERLPMPPNCPPTLYSLMTKCWAYDPSRRPRFTELKAQLSTILEEEKAQQEE</t>
-  </si>
-  <si>
-    <t>CSK22_HUMAN_D0_3E3B_X</t>
-  </si>
-  <si>
-    <t>Cterm</t>
-  </si>
-  <si>
-    <t>ATGAGCAGAAGCAAGCGTGACAACAATTTTTATAGTGTAGAGATTGGAGATTCTACATTCACAGTCCTGAAACGATATCAGAATTTAAAACCTATAGGCTCAGGAGCTCAAGGAATAGTATGCGCAGCTTATGATGCCATTCTTGAAAGAAATGTTGCAATCAAGAAGCTAAGCCGACCATTTCAGAATCAGACTCATGCCAAGCGGGCCTACAGAGAGCTAGTTCTTATGAAATGTGTTAATCACAAAAATATAATTGGCCTTTTGAATGTTTTCACACCACAGAAATCCCTAGAAGAATTTCAAGATGTTTACATAGTCATGGAGCTCATGGATGCAAATCTTTGCCAAGTGATTCAGATGGAGCTAGATCATGAAAGAATGTCCTACCTTCTCTATCAGATGCTGTGTGGAATCAAGCACCTTCATTCTGCTGGAATTATTCATCGGGACTTAAAGCCCAGTAATATAGTAGTAAAATCTGATTGCACTTTGAAGATTCTTGACTTCGGTCTGGCCAGGACTGCAGGAACGAGTTTTATGATGACGCCTTATGTAGTGACTCGCTACTACAGAGCACCCGAGGTCATCCTTGGCATGGGCTACAAGGAAAACGTGGATTTATGGTCTGTGGGGTGCATTATGGGAGAAATGGTTTGCCACAAAATCCTCTTTCCAGGAAGGGACTATATTGATCAGTGGAATAAAGTTATTGAACAGCTTGGAACACCATGTCCTGAATTCATGAAGAAACTGCAACCAACAGTAAGGACTTACGTTGAAAACAGACCTAAATATGCTGGATATAGCTTTGAGAAACTCTTCCCTGATGTCCTTTTCCCAGCTGACTCAGAACACAACAAACTTAAAGCCAGTCAGGCAAGGGATTTGTTATCCAAAATGCTGGTAATAGATGCATCTAAAAGGATCTCTGTAGATGAAGCTCTCCAACACCCGTACATCAATGTCTGGTATGATCCTTCTGAAGCAGAAGCTCCACCACCAAAGATCCCTGACAAGCAGTTAGATGAAAGGGAACACACAATAGAAGAGTGGAAAGAATTGATATATAAGGAAGTTATGGACTTGGAG</t>
-  </si>
-  <si>
-    <t>TTSLEALPTGTVLTDKSGRQWKLKSFQTRDNQGILYEAAPTSTLTCDSGPQKQKFSLKLDAKDGRLFNEQNFFQRAAKPLQVNKWKKLYSTPLLAIPTCMGFGVHQDKYRFLVLPSLGRSLQSALDVSPKHVLSERSVLQVACRLLDALEFLHENEYVHGNVTAENIFVDPEDQSQVTLAGYGFAFRYCPSGKHVAYVEGSRSPHEGDLEFISMDLHKGCGPSRRSDLQSLGYCMLKWLYGFLPWTNCLPNTEDIMKQKQKFVDKPGPFVGPCGHWIRPSETLQKYLKVVMALTYEEKPPYAMLRNNLEALLQDLRVSPYDPIGLPMVP</t>
-  </si>
-  <si>
-    <t>SPNYDKWEMERTDITMKHKLGGGQYGEVYEGVWKKYSLTVAVKTLKEDTMEVEEFLKEAAVMKEIKHPNLVQLLGVCTREPPFYIITEFMTYGNLLDYLRECNRQEVNAVVLLYMATQISSAMEYLEKKNFIHRDLAARNCLVGENHLVKVADFGLSRLMTGDTYTAHAGAKFPIKWTAPESLAYNKFSIKSDVWAFGVLLWEIATYGMSPYPGIDLSQVYELLEKDYRMERPEGCPEKVYELMRACWQWNPSDRPSFAEIHQAFETMFQESSISDEVEKELGK</t>
-  </si>
-  <si>
-    <t>PLK2_HUMAN_D0_4I6B_A</t>
-  </si>
-  <si>
-    <t>ATGGCGGCGGCGGCGGCTCAGGGGGGCGGGGGCGGGGAGCCCCGTAGAACCGAGGGGGTCGGCCCGGGGGTCCCGGGGGAGGTGGAGATGGTGAAGGGGCAGCCGTTCGACGTGGGCCCGCGCTACACGCAGTTGCAGTACATCGGCGAGGGCGCGTACGGCATGGTCAGCTCGGCCTATGACCACGTGCGCAAGACTCGCGTGGCCATCAAGAAGATCAGCCCCTTCGAACATCAGACCTACTGCCAGCGCACGCTCCGGGAGATCCAGATCCTGCTGCGCTTCCGCCATGAGAATGTCATCGGCATCCGAGACATTCTGCGGGCGTCCACCCTGGAAGCCATGAGAGATGTCTACATTGTGCAGGACCTGATGGAGACTGACCTGTACAAGTTGCTGAAAAGCCAGCAGCTGAGCAATGACCATATCTGCTACTTCCTCTACCAGATCCTGCGGGGCCTCAAGTACATCCACTCCGCCAACGTGCTCCACCGAGATCTAAAGCCCTCCAACCTGCTCATCAACACCACCTGCGACCTTAAGATTTGTGATTTCGGCCTGGCCCGGATTGCCGATCCTGAGCATGACCACACCGGCTTCCTGACGGAGTATGTGGCTACGCGCTGGTACCGGGCCCCAGAGATCATGCTGAACTCCAAGGGCTATACCAAGTCCATCGACATCTGGTCTGTGGGCTGCATTCTGGCTGAGATGCTCTCTAACCGGCCCATCTTCCCTGGCAAGCACTACCTGGATCAGCTCAACCACATTCTGGGCATCCTGGGCTCCCCATCCCAGGAGGACCTGAATTGTATCATCAACATGAAGGCCCGAAACTACCTACAGTCTCTGCCCTCCAAGACCAAGGTGGCTTGGGCCAAGCTTTTCCCCAAGTCAGACTCCAAAGCCCTTGACCTGCTGGACCGGATGTTAACCTTTAACCCCAATAAACGGATCACAGTGGAGGAAGCGCTGGCTCACCCCTACCTGGAGCAGTACTATGACCCGACGGATGAGCCAGTGGCCGAGGAGCCCTTCACCTTCGCCATGGAGCTGGATGACCTACCTAAGGAGCGGCTGAAGGAGCTCATCTTCCAGGAGACAGCACGCTTCCAGCCCGGAGTGCTGGAGGCCCCC</t>
-  </si>
-  <si>
-    <t>GEAPNQALLRILKETEFKKIKVLGSGAFGTVYKGLWIPEGEKVKIPVAIKELREATSPKANKEILDEAYVMASVDNPHVCRLLGICLTSTVQLITQLMPFGCLLDYVREHKDNIGSQYLLNWCVQIAKGMNYLEDRRLVHRDLAARNVLVKTPQHVKITDFGRAKLLGAEEKEYHAEGGKVPIKWMALESILHRIYTHQSDVWSYGVTVWELMTFGSKPYDGIPASEISSILEKGERLPQPPICTIDVYMIMVKCWMIDADSRPKFRELIIEFSKMARDPQRYLVIQGDERMHLPSPTDSNFYRALMDEEDMDDVVDADEYLIPQQG</t>
   </si>
   <si>
     <t>aa_start</t>
@@ -1058,94 +1058,94 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
         <v>225</v>
       </c>
       <c r="E1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="B2" t="n">
-        <v>1017</v>
+        <v>1432</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>296</v>
+        <v>360</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>184</v>
       </c>
       <c r="G2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>888</v>
+        <v>1080</v>
       </c>
       <c r="I2" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>144</v>
       </c>
       <c r="B3" t="n">
-        <v>1432</v>
+        <v>1017</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>360</v>
+        <v>296</v>
       </c>
       <c r="F3" t="s">
-        <v>186</v>
+        <v>18</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H3" t="n">
-        <v>1080</v>
+        <v>888</v>
       </c>
       <c r="I3" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>224</v>
       </c>
       <c r="B4" t="n">
         <v>6790</v>
@@ -1169,12 +1169,12 @@
         <v>1173</v>
       </c>
       <c r="I4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B5" t="n">
         <v>5594</v>
@@ -1198,215 +1198,215 @@
         <v>1080</v>
       </c>
       <c r="I5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="B6" t="n">
-        <v>9261</v>
+        <v>1612</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
       <c r="D6" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="F6" t="s">
-        <v>87</v>
+        <v>223</v>
       </c>
       <c r="G6" t="n">
-        <v>73</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>1044</v>
+        <v>1002</v>
       </c>
       <c r="I6" t="s">
-        <v>146</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="B7" t="n">
-        <v>10298</v>
+        <v>9261</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>291</v>
+        <v>25</v>
       </c>
       <c r="E7" t="n">
-        <v>591</v>
+        <v>348</v>
       </c>
       <c r="F7" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="G7" t="n">
-        <v>871</v>
+        <v>73</v>
       </c>
       <c r="H7" t="n">
-        <v>1773</v>
+        <v>1044</v>
       </c>
       <c r="I7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="B8" t="n">
-        <v>25</v>
+        <v>10298</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>229</v>
+        <v>291</v>
       </c>
       <c r="E8" t="n">
-        <v>512</v>
+        <v>591</v>
       </c>
       <c r="F8" t="s">
-        <v>221</v>
+        <v>5</v>
       </c>
       <c r="G8" t="n">
-        <v>685</v>
+        <v>871</v>
       </c>
       <c r="H8" t="n">
-        <v>1536</v>
+        <v>1773</v>
       </c>
       <c r="I8" t="s">
-        <v>23</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>1</v>
       </c>
       <c r="B9" t="n">
-        <v>673</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>444</v>
+        <v>229</v>
       </c>
       <c r="E9" t="n">
-        <v>712</v>
+        <v>512</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>220</v>
       </c>
       <c r="G9" t="n">
-        <v>1330</v>
+        <v>685</v>
       </c>
       <c r="H9" t="n">
-        <v>2136</v>
+        <v>1536</v>
       </c>
       <c r="I9" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="n">
+        <v>673</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>444</v>
+      </c>
+      <c r="E10" t="n">
+        <v>712</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1330</v>
+      </c>
+      <c r="H10" t="n">
+        <v>2136</v>
+      </c>
+      <c r="I10" t="s">
         <v>13</v>
-      </c>
-      <c r="B10" t="n">
-        <v>51765</v>
-      </c>
-      <c r="C10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" t="n">
-        <v>18</v>
-      </c>
-      <c r="E10" t="n">
-        <v>297</v>
-      </c>
-      <c r="F10" t="s">
-        <v>181</v>
-      </c>
-      <c r="G10" t="n">
-        <v>52</v>
-      </c>
-      <c r="H10" t="n">
-        <v>891</v>
-      </c>
-      <c r="I10" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>215</v>
+        <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>2872</v>
+        <v>51765</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
       </c>
       <c r="D11" t="n">
-        <v>72</v>
+        <v>18</v>
       </c>
       <c r="E11" t="n">
-        <v>385</v>
+        <v>297</v>
       </c>
       <c r="F11" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
       <c r="G11" t="n">
-        <v>214</v>
+        <v>52</v>
       </c>
       <c r="H11" t="n">
-        <v>1155</v>
+        <v>891</v>
       </c>
       <c r="I11" t="s">
-        <v>26</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>83</v>
+        <v>214</v>
       </c>
       <c r="B12" t="n">
-        <v>1956</v>
+        <v>2872</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="D12" t="n">
-        <v>696</v>
+        <v>72</v>
       </c>
       <c r="E12" t="n">
-        <v>1022</v>
+        <v>385</v>
       </c>
       <c r="F12" t="s">
-        <v>224</v>
+        <v>149</v>
       </c>
       <c r="G12" t="n">
-        <v>2086</v>
+        <v>214</v>
       </c>
       <c r="H12" t="n">
-        <v>3066</v>
+        <v>1155</v>
       </c>
       <c r="I12" t="s">
-        <v>105</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B13" t="n">
         <v>1453</v>
@@ -1421,7 +1421,7 @@
         <v>294</v>
       </c>
       <c r="F13" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
@@ -1430,12 +1430,12 @@
         <v>882</v>
       </c>
       <c r="I13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" t="n">
         <v>1454</v>
@@ -1450,7 +1450,7 @@
         <v>294</v>
       </c>
       <c r="F14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
@@ -1459,12 +1459,12 @@
         <v>882</v>
       </c>
       <c r="I14" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B15" t="n">
         <v>5598</v>
@@ -1479,7 +1479,7 @@
         <v>292</v>
       </c>
       <c r="F15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G15" t="n">
         <v>1</v>
@@ -1488,41 +1488,41 @@
         <v>876</v>
       </c>
       <c r="I15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>161</v>
       </c>
       <c r="B16" t="n">
-        <v>5347</v>
+        <v>6788</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="D16" t="n">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="E16" t="n">
-        <v>345</v>
+        <v>313</v>
       </c>
       <c r="F16" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="G16" t="n">
-        <v>97</v>
+        <v>46</v>
       </c>
       <c r="H16" t="n">
-        <v>1035</v>
+        <v>939</v>
       </c>
       <c r="I16" t="s">
-        <v>140</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B17" t="n">
         <v>5563</v>
@@ -1537,7 +1537,7 @@
         <v>279</v>
       </c>
       <c r="F17" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G17" t="n">
         <v>16</v>
@@ -1546,360 +1546,360 @@
         <v>837</v>
       </c>
       <c r="I17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>132</v>
       </c>
       <c r="B18" t="n">
-        <v>1025</v>
+        <v>5747</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>411</v>
       </c>
       <c r="E18" t="n">
-        <v>330</v>
+        <v>689</v>
       </c>
       <c r="F18" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="G18" t="n">
-        <v>1</v>
+        <v>1231</v>
       </c>
       <c r="H18" t="n">
-        <v>990</v>
+        <v>2067</v>
       </c>
       <c r="I18" t="s">
-        <v>185</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>134</v>
+        <v>94</v>
       </c>
       <c r="B19" t="n">
-        <v>5747</v>
+        <v>8569</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
       </c>
       <c r="D19" t="n">
-        <v>411</v>
+        <v>37</v>
       </c>
       <c r="E19" t="n">
-        <v>689</v>
+        <v>382</v>
       </c>
       <c r="F19" t="s">
-        <v>216</v>
+        <v>47</v>
       </c>
       <c r="G19" t="n">
-        <v>1231</v>
+        <v>109</v>
       </c>
       <c r="H19" t="n">
-        <v>2067</v>
+        <v>1146</v>
       </c>
       <c r="I19" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>29</v>
       </c>
       <c r="B20" t="n">
-        <v>8569</v>
+        <v>5292</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="D20" t="n">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E20" t="n">
-        <v>382</v>
+        <v>313</v>
       </c>
       <c r="F20" t="s">
-        <v>48</v>
+        <v>163</v>
       </c>
       <c r="G20" t="n">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="H20" t="n">
-        <v>1146</v>
+        <v>939</v>
       </c>
       <c r="I20" t="s">
-        <v>51</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>5292</v>
+        <v>7272</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="D21" t="n">
-        <v>29</v>
+        <v>519</v>
       </c>
       <c r="E21" t="n">
-        <v>313</v>
+        <v>808</v>
       </c>
       <c r="F21" t="s">
-        <v>166</v>
+        <v>20</v>
       </c>
       <c r="G21" t="n">
-        <v>85</v>
+        <v>1555</v>
       </c>
       <c r="H21" t="n">
-        <v>939</v>
+        <v>2424</v>
       </c>
       <c r="I21" t="s">
-        <v>204</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>206</v>
       </c>
       <c r="B22" t="n">
-        <v>7272</v>
+        <v>8428</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
       </c>
       <c r="D22" t="n">
-        <v>519</v>
+        <v>19</v>
       </c>
       <c r="E22" t="n">
-        <v>808</v>
+        <v>289</v>
       </c>
       <c r="F22" t="s">
-        <v>21</v>
+        <v>157</v>
       </c>
       <c r="G22" t="n">
-        <v>1555</v>
+        <v>55</v>
       </c>
       <c r="H22" t="n">
-        <v>2424</v>
+        <v>867</v>
       </c>
       <c r="I22" t="s">
-        <v>40</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>208</v>
+        <v>3</v>
       </c>
       <c r="B23" t="n">
-        <v>8428</v>
+        <v>83903</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
       </c>
       <c r="D23" t="n">
-        <v>19</v>
+        <v>465</v>
       </c>
       <c r="E23" t="n">
-        <v>289</v>
+        <v>798</v>
       </c>
       <c r="F23" t="s">
-        <v>160</v>
+        <v>125</v>
       </c>
       <c r="G23" t="n">
-        <v>55</v>
+        <v>1393</v>
       </c>
       <c r="H23" t="n">
-        <v>867</v>
+        <v>2394</v>
       </c>
       <c r="I23" t="s">
-        <v>201</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>3</v>
+        <v>211</v>
       </c>
       <c r="B24" t="n">
-        <v>83903</v>
+        <v>1198</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
       </c>
       <c r="D24" t="n">
-        <v>465</v>
+        <v>127</v>
       </c>
       <c r="E24" t="n">
-        <v>798</v>
+        <v>484</v>
       </c>
       <c r="F24" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="G24" t="n">
-        <v>1393</v>
+        <v>379</v>
       </c>
       <c r="H24" t="n">
-        <v>2394</v>
+        <v>1452</v>
       </c>
       <c r="I24" t="s">
-        <v>47</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>213</v>
+        <v>78</v>
       </c>
       <c r="B25" t="n">
-        <v>1198</v>
+        <v>1613</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
       </c>
       <c r="D25" t="n">
-        <v>127</v>
+        <v>9</v>
       </c>
       <c r="E25" t="n">
-        <v>484</v>
+        <v>289</v>
       </c>
       <c r="F25" t="s">
-        <v>141</v>
+        <v>164</v>
       </c>
       <c r="G25" t="n">
-        <v>379</v>
+        <v>25</v>
       </c>
       <c r="H25" t="n">
-        <v>1452</v>
+        <v>867</v>
       </c>
       <c r="I25" t="s">
-        <v>111</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>158</v>
       </c>
       <c r="B26" t="n">
-        <v>1613</v>
+        <v>7867</v>
       </c>
       <c r="C26" t="s">
         <v>2</v>
       </c>
       <c r="D26" t="n">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="E26" t="n">
-        <v>289</v>
+        <v>349</v>
       </c>
       <c r="F26" t="s">
-        <v>167</v>
+        <v>205</v>
       </c>
       <c r="G26" t="n">
-        <v>25</v>
+        <v>97</v>
       </c>
       <c r="H26" t="n">
-        <v>867</v>
+        <v>1047</v>
       </c>
       <c r="I26" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>161</v>
+        <v>83</v>
       </c>
       <c r="B27" t="n">
-        <v>7867</v>
+        <v>9748</v>
       </c>
       <c r="C27" t="s">
         <v>2</v>
       </c>
       <c r="D27" t="n">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E27" t="n">
-        <v>349</v>
+        <v>320</v>
       </c>
       <c r="F27" t="s">
-        <v>207</v>
+        <v>114</v>
       </c>
       <c r="G27" t="n">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="H27" t="n">
-        <v>1047</v>
+        <v>960</v>
       </c>
       <c r="I27" t="s">
-        <v>55</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>137</v>
       </c>
       <c r="B28" t="n">
-        <v>9748</v>
+        <v>8445</v>
       </c>
       <c r="C28" t="s">
         <v>2</v>
       </c>
       <c r="D28" t="n">
-        <v>19</v>
+        <v>146</v>
       </c>
       <c r="E28" t="n">
-        <v>320</v>
+        <v>552</v>
       </c>
       <c r="F28" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="G28" t="n">
-        <v>55</v>
+        <v>436</v>
       </c>
       <c r="H28" t="n">
-        <v>960</v>
+        <v>1656</v>
       </c>
       <c r="I28" t="s">
-        <v>162</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>139</v>
+        <v>62</v>
       </c>
       <c r="B29" t="n">
-        <v>8445</v>
+        <v>56924</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
       </c>
       <c r="D29" t="n">
-        <v>146</v>
+        <v>383</v>
       </c>
       <c r="E29" t="n">
-        <v>552</v>
+        <v>681</v>
       </c>
       <c r="F29" t="s">
-        <v>145</v>
+        <v>182</v>
       </c>
       <c r="G29" t="n">
-        <v>436</v>
+        <v>1147</v>
       </c>
       <c r="H29" t="n">
-        <v>1656</v>
+        <v>2043</v>
       </c>
       <c r="I29" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B30" t="n">
         <v>815</v>
@@ -1914,7 +1914,7 @@
         <v>302</v>
       </c>
       <c r="F30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G30" t="n">
         <v>37</v>
@@ -1928,7 +1928,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>178</v>
+        <v>150</v>
       </c>
       <c r="B31" t="n">
         <v>9262</v>
@@ -1943,7 +1943,7 @@
         <v>329</v>
       </c>
       <c r="F31" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G31" t="n">
         <v>73</v>
@@ -1952,12 +1952,12 @@
         <v>987</v>
       </c>
       <c r="I31" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B32" t="n">
         <v>814</v>
@@ -1972,7 +1972,7 @@
         <v>340</v>
       </c>
       <c r="F32" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G32" t="n">
         <v>43</v>
@@ -1981,12 +1981,12 @@
         <v>1020</v>
       </c>
       <c r="I32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B33" t="n">
         <v>8814</v>
@@ -2001,7 +2001,7 @@
         <v>265</v>
       </c>
       <c r="F33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G33" t="n">
         <v>4</v>
@@ -2010,12 +2010,12 @@
         <v>795</v>
       </c>
       <c r="I33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B34" t="n">
         <v>818</v>
@@ -2030,7 +2030,7 @@
         <v>315</v>
       </c>
       <c r="F34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G34" t="n">
         <v>13</v>
@@ -2039,360 +2039,360 @@
         <v>945</v>
       </c>
       <c r="I34" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="B35" t="n">
-        <v>56924</v>
+        <v>57144</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
       </c>
       <c r="D35" t="n">
-        <v>383</v>
+        <v>425</v>
       </c>
       <c r="E35" t="n">
-        <v>681</v>
+        <v>719</v>
       </c>
       <c r="F35" t="s">
-        <v>184</v>
+        <v>84</v>
       </c>
       <c r="G35" t="n">
-        <v>1147</v>
+        <v>1273</v>
       </c>
       <c r="H35" t="n">
-        <v>2043</v>
+        <v>2157</v>
       </c>
       <c r="I35" t="s">
-        <v>176</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="B36" t="n">
-        <v>57144</v>
+        <v>5261</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
       </c>
       <c r="D36" t="n">
-        <v>425</v>
+        <v>6</v>
       </c>
       <c r="E36" t="n">
-        <v>719</v>
+        <v>293</v>
       </c>
       <c r="F36" t="s">
-        <v>85</v>
+        <v>8</v>
       </c>
       <c r="G36" t="n">
-        <v>1273</v>
+        <v>16</v>
       </c>
       <c r="H36" t="n">
-        <v>2157</v>
+        <v>879</v>
       </c>
       <c r="I36" t="s">
-        <v>81</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="B37" t="n">
-        <v>5261</v>
+        <v>9088</v>
       </c>
       <c r="C37" t="s">
         <v>2</v>
       </c>
       <c r="D37" t="n">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E37" t="n">
-        <v>293</v>
+        <v>360</v>
       </c>
       <c r="F37" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="G37" t="n">
-        <v>16</v>
+        <v>217</v>
       </c>
       <c r="H37" t="n">
-        <v>879</v>
+        <v>1080</v>
       </c>
       <c r="I37" t="s">
-        <v>32</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="B38" t="n">
-        <v>9088</v>
+        <v>8576</v>
       </c>
       <c r="C38" t="s">
         <v>2</v>
       </c>
       <c r="D38" t="n">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="E38" t="n">
-        <v>360</v>
+        <v>294</v>
       </c>
       <c r="F38" t="s">
-        <v>36</v>
+        <v>200</v>
       </c>
       <c r="G38" t="n">
-        <v>217</v>
+        <v>37</v>
       </c>
       <c r="H38" t="n">
-        <v>1080</v>
+        <v>882</v>
       </c>
       <c r="I38" t="s">
-        <v>165</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>109</v>
+        <v>27</v>
       </c>
       <c r="B39" t="n">
-        <v>8576</v>
+        <v>92335</v>
       </c>
       <c r="C39" t="s">
         <v>2</v>
       </c>
       <c r="D39" t="n">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="E39" t="n">
-        <v>294</v>
+        <v>402</v>
       </c>
       <c r="F39" t="s">
-        <v>202</v>
+        <v>167</v>
       </c>
       <c r="G39" t="n">
-        <v>37</v>
+        <v>88</v>
       </c>
       <c r="H39" t="n">
-        <v>882</v>
+        <v>1206</v>
       </c>
       <c r="I39" t="s">
-        <v>67</v>
+        <v>178</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B40" t="n">
-        <v>92335</v>
+        <v>7444</v>
       </c>
       <c r="C40" t="s">
         <v>2</v>
       </c>
       <c r="D40" t="n">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="E40" t="n">
-        <v>402</v>
+        <v>335</v>
       </c>
       <c r="F40" t="s">
-        <v>169</v>
+        <v>203</v>
       </c>
       <c r="G40" t="n">
-        <v>88</v>
+        <v>40</v>
       </c>
       <c r="H40" t="n">
-        <v>1206</v>
+        <v>1005</v>
       </c>
       <c r="I40" t="s">
-        <v>180</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="B41" t="n">
-        <v>7444</v>
+        <v>51231</v>
       </c>
       <c r="C41" t="s">
         <v>2</v>
       </c>
       <c r="D41" t="n">
-        <v>14</v>
+        <v>146</v>
       </c>
       <c r="E41" t="n">
-        <v>335</v>
+        <v>474</v>
       </c>
       <c r="F41" t="s">
-        <v>205</v>
+        <v>219</v>
       </c>
       <c r="G41" t="n">
-        <v>40</v>
+        <v>436</v>
       </c>
       <c r="H41" t="n">
-        <v>1005</v>
+        <v>1422</v>
       </c>
       <c r="I41" t="s">
-        <v>16</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>117</v>
       </c>
       <c r="B42" t="n">
-        <v>51231</v>
+        <v>2042</v>
       </c>
       <c r="C42" t="s">
         <v>2</v>
       </c>
       <c r="D42" t="n">
-        <v>146</v>
+        <v>606</v>
       </c>
       <c r="E42" t="n">
-        <v>474</v>
+        <v>947</v>
       </c>
       <c r="F42" t="s">
-        <v>220</v>
+        <v>85</v>
       </c>
       <c r="G42" t="n">
-        <v>436</v>
+        <v>1816</v>
       </c>
       <c r="H42" t="n">
-        <v>1422</v>
+        <v>2841</v>
       </c>
       <c r="I42" t="s">
-        <v>149</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>119</v>
+        <v>63</v>
       </c>
       <c r="B43" t="n">
-        <v>2042</v>
+        <v>2260</v>
       </c>
       <c r="C43" t="s">
         <v>2</v>
       </c>
       <c r="D43" t="n">
-        <v>606</v>
+        <v>456</v>
       </c>
       <c r="E43" t="n">
-        <v>947</v>
+        <v>772</v>
       </c>
       <c r="F43" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="G43" t="n">
-        <v>1816</v>
+        <v>1366</v>
       </c>
       <c r="H43" t="n">
-        <v>2841</v>
+        <v>2316</v>
       </c>
       <c r="I43" t="s">
-        <v>117</v>
+        <v>228</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="B44" t="n">
-        <v>2260</v>
+        <v>8573</v>
       </c>
       <c r="C44" t="s">
         <v>2</v>
       </c>
       <c r="D44" t="n">
-        <v>456</v>
+        <v>1</v>
       </c>
       <c r="E44" t="n">
-        <v>772</v>
+        <v>340</v>
       </c>
       <c r="F44" t="s">
-        <v>53</v>
+        <v>131</v>
       </c>
       <c r="G44" t="n">
-        <v>1366</v>
+        <v>1</v>
       </c>
       <c r="H44" t="n">
-        <v>2316</v>
+        <v>1020</v>
       </c>
       <c r="I44" t="s">
-        <v>228</v>
+        <v>190</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>12</v>
+        <v>97</v>
       </c>
       <c r="B45" t="n">
-        <v>8573</v>
+        <v>3702</v>
       </c>
       <c r="C45" t="s">
         <v>2</v>
       </c>
       <c r="D45" t="n">
-        <v>1</v>
+        <v>357</v>
       </c>
       <c r="E45" t="n">
-        <v>340</v>
+        <v>620</v>
       </c>
       <c r="F45" t="s">
-        <v>133</v>
+        <v>49</v>
       </c>
       <c r="G45" t="n">
-        <v>1</v>
+        <v>1069</v>
       </c>
       <c r="H45" t="n">
-        <v>1020</v>
+        <v>1860</v>
       </c>
       <c r="I45" t="s">
-        <v>193</v>
+        <v>134</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>98</v>
+        <v>141</v>
       </c>
       <c r="B46" t="n">
-        <v>3702</v>
+        <v>6197</v>
       </c>
       <c r="C46" t="s">
         <v>2</v>
       </c>
       <c r="D46" t="n">
-        <v>357</v>
+        <v>399</v>
       </c>
       <c r="E46" t="n">
-        <v>620</v>
+        <v>740</v>
       </c>
       <c r="F46" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="G46" t="n">
-        <v>1069</v>
+        <v>1195</v>
       </c>
       <c r="H46" t="n">
-        <v>1860</v>
+        <v>2220</v>
       </c>
       <c r="I46" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>144</v>
+        <v>98</v>
       </c>
       <c r="B47" t="n">
         <v>6197</v>
@@ -2407,7 +2407,7 @@
         <v>740</v>
       </c>
       <c r="F47" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G47" t="n">
         <v>1195</v>
@@ -2416,128 +2416,128 @@
         <v>2220</v>
       </c>
       <c r="I47" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>99</v>
+        <v>166</v>
       </c>
       <c r="B48" t="n">
-        <v>6197</v>
+        <v>4233</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
       </c>
       <c r="D48" t="n">
-        <v>399</v>
+        <v>1038</v>
       </c>
       <c r="E48" t="n">
-        <v>740</v>
+        <v>1346</v>
       </c>
       <c r="F48" t="s">
-        <v>113</v>
+        <v>177</v>
       </c>
       <c r="G48" t="n">
-        <v>1195</v>
+        <v>3112</v>
       </c>
       <c r="H48" t="n">
-        <v>2220</v>
+        <v>4038</v>
       </c>
       <c r="I48" t="s">
-        <v>143</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>168</v>
+        <v>106</v>
       </c>
       <c r="B49" t="n">
-        <v>4233</v>
+        <v>5603</v>
       </c>
       <c r="C49" t="s">
         <v>2</v>
       </c>
       <c r="D49" t="n">
-        <v>1038</v>
+        <v>1</v>
       </c>
       <c r="E49" t="n">
-        <v>1346</v>
+        <v>352</v>
       </c>
       <c r="F49" t="s">
-        <v>179</v>
+        <v>95</v>
       </c>
       <c r="G49" t="n">
-        <v>3112</v>
+        <v>1</v>
       </c>
       <c r="H49" t="n">
-        <v>4038</v>
+        <v>1056</v>
       </c>
       <c r="I49" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" t="s">
-        <v>108</v>
+        <v>145</v>
       </c>
       <c r="B50" t="n">
-        <v>5603</v>
+        <v>6416</v>
       </c>
       <c r="C50" t="s">
         <v>2</v>
       </c>
       <c r="D50" t="n">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="E50" t="n">
-        <v>352</v>
+        <v>399</v>
       </c>
       <c r="F50" t="s">
-        <v>96</v>
+        <v>148</v>
       </c>
       <c r="G50" t="n">
-        <v>1</v>
+        <v>238</v>
       </c>
       <c r="H50" t="n">
-        <v>1056</v>
+        <v>1197</v>
       </c>
       <c r="I50" t="s">
-        <v>50</v>
+        <v>209</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" t="s">
-        <v>148</v>
+        <v>221</v>
       </c>
       <c r="B51" t="n">
-        <v>6416</v>
+        <v>10769</v>
       </c>
       <c r="C51" t="s">
         <v>2</v>
       </c>
       <c r="D51" t="n">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E51" t="n">
-        <v>399</v>
+        <v>360</v>
       </c>
       <c r="F51" t="s">
-        <v>151</v>
+        <v>71</v>
       </c>
       <c r="G51" t="n">
-        <v>238</v>
+        <v>169</v>
       </c>
       <c r="H51" t="n">
-        <v>1197</v>
+        <v>1080</v>
       </c>
       <c r="I51" t="s">
-        <v>211</v>
+        <v>41</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B52" t="n">
         <v>6195</v>
@@ -2552,7 +2552,7 @@
         <v>735</v>
       </c>
       <c r="F52" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G52" t="n">
         <v>1231</v>
@@ -2561,12 +2561,12 @@
         <v>2205</v>
       </c>
       <c r="I52" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B53" t="n">
         <v>6195</v>
@@ -2581,7 +2581,7 @@
         <v>735</v>
       </c>
       <c r="F53" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G53" t="n">
         <v>1231</v>
@@ -2590,152 +2590,152 @@
         <v>2205</v>
       </c>
       <c r="I53" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>222</v>
+        <v>38</v>
       </c>
       <c r="B54" t="n">
-        <v>10769</v>
+        <v>5599</v>
       </c>
       <c r="C54" t="s">
-        <v>2</v>
+        <v>217</v>
       </c>
       <c r="D54" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E54" t="n">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="F54" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="G54" t="n">
-        <v>169</v>
+        <v>1</v>
       </c>
       <c r="H54" t="n">
-        <v>1080</v>
+        <v>1092</v>
       </c>
       <c r="I54" t="s">
-        <v>10</v>
+        <v>218</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>39</v>
+        <v>120</v>
       </c>
       <c r="B55" t="n">
-        <v>5599</v>
+        <v>4751</v>
       </c>
       <c r="C55" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D55" t="n">
         <v>1</v>
       </c>
       <c r="E55" t="n">
-        <v>364</v>
+        <v>271</v>
       </c>
       <c r="F55" t="s">
-        <v>27</v>
+        <v>198</v>
       </c>
       <c r="G55" t="n">
         <v>1</v>
       </c>
       <c r="H55" t="n">
-        <v>1092</v>
+        <v>813</v>
       </c>
       <c r="I55" t="s">
-        <v>219</v>
+        <v>160</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>122</v>
+        <v>168</v>
       </c>
       <c r="B56" t="n">
-        <v>4751</v>
+        <v>5604</v>
       </c>
       <c r="C56" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D56" t="n">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="E56" t="n">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="F56" t="s">
-        <v>200</v>
+        <v>6</v>
       </c>
       <c r="G56" t="n">
-        <v>1</v>
+        <v>184</v>
       </c>
       <c r="H56" t="n">
-        <v>813</v>
+        <v>819</v>
       </c>
       <c r="I56" t="s">
-        <v>163</v>
+        <v>110</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>170</v>
+        <v>40</v>
       </c>
       <c r="B57" t="n">
-        <v>5604</v>
+        <v>5058</v>
       </c>
       <c r="C57" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D57" t="n">
-        <v>62</v>
+        <v>248</v>
       </c>
       <c r="E57" t="n">
-        <v>273</v>
+        <v>545</v>
       </c>
       <c r="F57" t="s">
-        <v>6</v>
+        <v>135</v>
       </c>
       <c r="G57" t="n">
-        <v>184</v>
+        <v>742</v>
       </c>
       <c r="H57" t="n">
-        <v>819</v>
+        <v>1635</v>
       </c>
       <c r="I57" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="B58" t="n">
-        <v>5058</v>
+        <v>5610</v>
       </c>
       <c r="C58" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D58" t="n">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="E58" t="n">
-        <v>545</v>
+        <v>551</v>
       </c>
       <c r="F58" t="s">
-        <v>137</v>
+        <v>169</v>
       </c>
       <c r="G58" t="n">
-        <v>742</v>
+        <v>760</v>
       </c>
       <c r="H58" t="n">
-        <v>1635</v>
+        <v>1653</v>
       </c>
       <c r="I58" t="s">
-        <v>103</v>
+        <v>42</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -2746,7 +2746,7 @@
         <v>1021</v>
       </c>
       <c r="C59" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D59" t="n">
         <v>1</v>
@@ -2755,7 +2755,7 @@
         <v>301</v>
       </c>
       <c r="F59" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G59" t="n">
         <v>1</v>
@@ -2764,163 +2764,163 @@
         <v>903</v>
       </c>
       <c r="I59" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>194</v>
+        <v>92</v>
       </c>
       <c r="B60" t="n">
-        <v>5610</v>
+        <v>5608</v>
       </c>
       <c r="C60" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D60" t="n">
-        <v>254</v>
+        <v>1</v>
       </c>
       <c r="E60" t="n">
-        <v>551</v>
+        <v>334</v>
       </c>
       <c r="F60" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="G60" t="n">
-        <v>760</v>
+        <v>1</v>
       </c>
       <c r="H60" t="n">
-        <v>1653</v>
+        <v>1002</v>
       </c>
       <c r="I60" t="s">
-        <v>43</v>
+        <v>155</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="B61" t="n">
-        <v>5608</v>
+        <v>140609</v>
       </c>
       <c r="C61" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D61" t="n">
         <v>1</v>
       </c>
       <c r="E61" t="n">
-        <v>334</v>
+        <v>302</v>
       </c>
       <c r="F61" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="G61" t="n">
         <v>1</v>
       </c>
       <c r="H61" t="n">
-        <v>1002</v>
+        <v>906</v>
       </c>
       <c r="I61" t="s">
-        <v>158</v>
+        <v>77</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B62" t="n">
-        <v>140609</v>
+        <v>659</v>
       </c>
       <c r="C62" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D62" t="n">
-        <v>1</v>
+        <v>189</v>
       </c>
       <c r="E62" t="n">
-        <v>302</v>
+        <v>517</v>
       </c>
       <c r="F62" t="s">
-        <v>126</v>
+        <v>65</v>
       </c>
       <c r="G62" t="n">
-        <v>1</v>
+        <v>565</v>
       </c>
       <c r="H62" t="n">
-        <v>906</v>
+        <v>1551</v>
       </c>
       <c r="I62" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B63" t="n">
-        <v>659</v>
+        <v>5127</v>
       </c>
       <c r="C63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D63" t="n">
-        <v>189</v>
+        <v>163</v>
       </c>
       <c r="E63" t="n">
-        <v>517</v>
+        <v>478</v>
       </c>
       <c r="F63" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="G63" t="n">
-        <v>565</v>
+        <v>487</v>
       </c>
       <c r="H63" t="n">
-        <v>1551</v>
+        <v>1434</v>
       </c>
       <c r="I63" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>59</v>
+        <v>201</v>
       </c>
       <c r="B64" t="n">
-        <v>5127</v>
+        <v>9833</v>
       </c>
       <c r="C64" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D64" t="n">
-        <v>163</v>
+        <v>1</v>
       </c>
       <c r="E64" t="n">
-        <v>478</v>
+        <v>340</v>
       </c>
       <c r="F64" t="s">
-        <v>35</v>
+        <v>183</v>
       </c>
       <c r="G64" t="n">
-        <v>487</v>
+        <v>1</v>
       </c>
       <c r="H64" t="n">
-        <v>1434</v>
+        <v>1020</v>
       </c>
       <c r="I64" t="s">
-        <v>107</v>
+        <v>51</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B65" t="n">
         <v>5605</v>
       </c>
       <c r="C65" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D65" t="n">
         <v>55</v>
@@ -2929,7 +2929,7 @@
         <v>400</v>
       </c>
       <c r="F65" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G65" t="n">
         <v>163</v>
@@ -2938,12 +2938,12 @@
         <v>1200</v>
       </c>
       <c r="I65" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B66" t="n">
         <v>1457</v>
@@ -2967,12 +2967,12 @@
         <v>1005</v>
       </c>
       <c r="I66" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B67" t="n">
         <v>11200</v>
@@ -2987,7 +2987,7 @@
         <v>531</v>
       </c>
       <c r="F67" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G67" t="n">
         <v>628</v>
@@ -3001,7 +3001,7 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B68" t="n">
         <v>5566</v>
@@ -3025,12 +3025,12 @@
         <v>1053</v>
       </c>
       <c r="I68" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B69" t="n">
         <v>1445</v>
@@ -3045,7 +3045,7 @@
         <v>450</v>
       </c>
       <c r="F69" t="s">
-        <v>153</v>
+        <v>25</v>
       </c>
       <c r="G69" t="n">
         <v>562</v>
@@ -3054,12 +3054,12 @@
         <v>1350</v>
       </c>
       <c r="I69" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B70" t="n">
         <v>5600</v>
@@ -3074,7 +3074,7 @@
         <v>364</v>
       </c>
       <c r="F70" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G70" t="n">
         <v>1</v>
@@ -3083,12 +3083,12 @@
         <v>1092</v>
       </c>
       <c r="I70" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B71" t="n">
         <v>1459</v>
@@ -3103,7 +3103,7 @@
         <v>334</v>
       </c>
       <c r="F71" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G71" t="n">
         <v>1</v>
@@ -3112,12 +3112,12 @@
         <v>1002</v>
       </c>
       <c r="I71" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B72" t="n">
         <v>4140</v>
@@ -3132,7 +3132,7 @@
         <v>370</v>
       </c>
       <c r="F72" t="s">
-        <v>203</v>
+        <v>96</v>
       </c>
       <c r="G72" t="n">
         <v>142</v>
@@ -3141,12 +3141,12 @@
         <v>1110</v>
       </c>
       <c r="I72" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B73" t="n">
         <v>2011</v>
@@ -3161,7 +3161,7 @@
         <v>330</v>
       </c>
       <c r="F73" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G73" t="n">
         <v>46</v>
@@ -3170,12 +3170,12 @@
         <v>990</v>
       </c>
       <c r="I73" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B74" t="n">
         <v>5595</v>
@@ -3190,7 +3190,7 @@
         <v>379</v>
       </c>
       <c r="F74" t="s">
-        <v>54</v>
+        <v>176</v>
       </c>
       <c r="G74" t="n">
         <v>1</v>
@@ -3199,12 +3199,12 @@
         <v>1137</v>
       </c>
       <c r="I74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>75</v>
+        <v>191</v>
       </c>
       <c r="B75" t="n">
         <v>7443</v>
@@ -3219,7 +3219,7 @@
         <v>364</v>
       </c>
       <c r="F75" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G75" t="n">
         <v>7</v>
@@ -3228,160 +3228,160 @@
         <v>1092</v>
       </c>
       <c r="I75" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="B76" t="n">
-        <v>1956</v>
+        <v>673</v>
       </c>
       <c r="C76" t="s">
         <v>2</v>
       </c>
       <c r="D76" t="n">
-        <v>696</v>
+        <v>444</v>
       </c>
       <c r="E76" t="n">
-        <v>1022</v>
+        <v>712</v>
       </c>
       <c r="F76" t="s">
-        <v>224</v>
+        <v>23</v>
       </c>
       <c r="G76" t="n">
-        <v>2086</v>
+        <v>1330</v>
       </c>
       <c r="H76" t="n">
-        <v>3066</v>
+        <v>2136</v>
       </c>
       <c r="I76" t="s">
-        <v>105</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>61</v>
+        <v>166</v>
       </c>
       <c r="B77" t="n">
-        <v>673</v>
+        <v>4233</v>
       </c>
       <c r="C77" t="s">
         <v>2</v>
       </c>
       <c r="D77" t="n">
-        <v>444</v>
+        <v>1038</v>
       </c>
       <c r="E77" t="n">
-        <v>712</v>
+        <v>1346</v>
       </c>
       <c r="F77" t="s">
-        <v>24</v>
+        <v>177</v>
       </c>
       <c r="G77" t="n">
-        <v>1330</v>
+        <v>3112</v>
       </c>
       <c r="H77" t="n">
-        <v>2136</v>
+        <v>4038</v>
       </c>
       <c r="I77" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>168</v>
+        <v>63</v>
       </c>
       <c r="B78" t="n">
-        <v>4233</v>
+        <v>2260</v>
       </c>
       <c r="C78" t="s">
         <v>2</v>
       </c>
       <c r="D78" t="n">
-        <v>1038</v>
+        <v>456</v>
       </c>
       <c r="E78" t="n">
-        <v>1346</v>
+        <v>772</v>
       </c>
       <c r="F78" t="s">
-        <v>179</v>
+        <v>53</v>
       </c>
       <c r="G78" t="n">
-        <v>3112</v>
+        <v>1366</v>
       </c>
       <c r="H78" t="n">
-        <v>4038</v>
+        <v>2316</v>
       </c>
       <c r="I78" t="s">
-        <v>17</v>
+        <v>228</v>
       </c>
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="B79" t="n">
-        <v>2260</v>
+        <v>25</v>
       </c>
       <c r="C79" t="s">
         <v>2</v>
       </c>
       <c r="D79" t="n">
-        <v>456</v>
+        <v>229</v>
       </c>
       <c r="E79" t="n">
-        <v>772</v>
+        <v>512</v>
       </c>
       <c r="F79" t="s">
-        <v>53</v>
+        <v>220</v>
       </c>
       <c r="G79" t="n">
-        <v>1366</v>
+        <v>685</v>
       </c>
       <c r="H79" t="n">
-        <v>2316</v>
+        <v>1536</v>
       </c>
       <c r="I79" t="s">
-        <v>228</v>
+        <v>22</v>
       </c>
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="B80" t="n">
-        <v>25</v>
+        <v>1432</v>
       </c>
       <c r="C80" t="s">
         <v>2</v>
       </c>
       <c r="D80" t="n">
-        <v>229</v>
+        <v>1</v>
       </c>
       <c r="E80" t="n">
-        <v>512</v>
+        <v>360</v>
       </c>
       <c r="F80" t="s">
-        <v>221</v>
+        <v>184</v>
       </c>
       <c r="G80" t="n">
-        <v>685</v>
+        <v>1</v>
       </c>
       <c r="H80" t="n">
-        <v>1536</v>
+        <v>1080</v>
       </c>
       <c r="I80" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>58</v>
+        <v>121</v>
       </c>
       <c r="B81" t="n">
-        <v>1432</v>
+        <v>5594</v>
       </c>
       <c r="C81" t="s">
         <v>2</v>
@@ -3393,7 +3393,7 @@
         <v>360</v>
       </c>
       <c r="F81" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="G81" t="n">
         <v>1</v>
@@ -3402,471 +3402,471 @@
         <v>1080</v>
       </c>
       <c r="I81" t="s">
-        <v>56</v>
+        <v>123</v>
       </c>
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="B82" t="n">
-        <v>5594</v>
+        <v>11200</v>
       </c>
       <c r="C82" t="s">
         <v>2</v>
       </c>
       <c r="D82" t="n">
-        <v>1</v>
+        <v>210</v>
       </c>
       <c r="E82" t="n">
-        <v>360</v>
+        <v>531</v>
       </c>
       <c r="F82" t="s">
-        <v>227</v>
+        <v>194</v>
       </c>
       <c r="G82" t="n">
-        <v>1</v>
+        <v>628</v>
       </c>
       <c r="H82" t="n">
-        <v>1080</v>
+        <v>1593</v>
       </c>
       <c r="I82" t="s">
-        <v>125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="B83" t="n">
-        <v>11200</v>
+        <v>1017</v>
       </c>
       <c r="C83" t="s">
         <v>2</v>
       </c>
       <c r="D83" t="n">
-        <v>210</v>
+        <v>2</v>
       </c>
       <c r="E83" t="n">
-        <v>531</v>
+        <v>296</v>
       </c>
       <c r="F83" t="s">
-        <v>196</v>
+        <v>18</v>
       </c>
       <c r="G83" t="n">
-        <v>628</v>
+        <v>4</v>
       </c>
       <c r="H83" t="n">
-        <v>1593</v>
+        <v>888</v>
       </c>
       <c r="I83" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="B84" t="n">
-        <v>1017</v>
+        <v>5747</v>
       </c>
       <c r="C84" t="s">
         <v>2</v>
       </c>
       <c r="D84" t="n">
-        <v>2</v>
+        <v>411</v>
       </c>
       <c r="E84" t="n">
-        <v>296</v>
+        <v>689</v>
       </c>
       <c r="F84" t="s">
-        <v>19</v>
+        <v>215</v>
       </c>
       <c r="G84" t="n">
-        <v>4</v>
+        <v>1231</v>
       </c>
       <c r="H84" t="n">
-        <v>888</v>
+        <v>2067</v>
       </c>
       <c r="I84" t="s">
-        <v>46</v>
+        <v>156</v>
       </c>
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="B85" t="n">
-        <v>5347</v>
+        <v>5599</v>
       </c>
       <c r="C85" t="s">
-        <v>2</v>
+        <v>217</v>
       </c>
       <c r="D85" t="n">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="E85" t="n">
-        <v>345</v>
+        <v>364</v>
       </c>
       <c r="F85" t="s">
-        <v>97</v>
+        <v>26</v>
       </c>
       <c r="G85" t="n">
-        <v>97</v>
+        <v>1</v>
       </c>
       <c r="H85" t="n">
-        <v>1035</v>
+        <v>1092</v>
       </c>
       <c r="I85" t="s">
-        <v>140</v>
+        <v>218</v>
       </c>
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="B86" t="n">
-        <v>5747</v>
+        <v>5604</v>
       </c>
       <c r="C86" t="s">
-        <v>2</v>
+        <v>217</v>
       </c>
       <c r="D86" t="n">
-        <v>411</v>
+        <v>62</v>
       </c>
       <c r="E86" t="n">
-        <v>689</v>
+        <v>273</v>
       </c>
       <c r="F86" t="s">
-        <v>216</v>
+        <v>6</v>
       </c>
       <c r="G86" t="n">
-        <v>1231</v>
+        <v>184</v>
       </c>
       <c r="H86" t="n">
-        <v>2067</v>
+        <v>819</v>
       </c>
       <c r="I86" t="s">
-        <v>159</v>
+        <v>110</v>
       </c>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>39</v>
+        <v>224</v>
       </c>
       <c r="B87" t="n">
-        <v>5599</v>
+        <v>6790</v>
       </c>
       <c r="C87" t="s">
-        <v>218</v>
+        <v>2</v>
       </c>
       <c r="D87" t="n">
-        <v>1</v>
+        <v>125</v>
       </c>
       <c r="E87" t="n">
-        <v>364</v>
+        <v>391</v>
       </c>
       <c r="F87" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="G87" t="n">
-        <v>1</v>
+        <v>373</v>
       </c>
       <c r="H87" t="n">
-        <v>1092</v>
+        <v>1173</v>
       </c>
       <c r="I87" t="s">
-        <v>219</v>
+        <v>152</v>
       </c>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="B88" t="n">
-        <v>5604</v>
+        <v>5595</v>
       </c>
       <c r="C88" t="s">
-        <v>218</v>
+        <v>2</v>
       </c>
       <c r="D88" t="n">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="E88" t="n">
-        <v>273</v>
+        <v>379</v>
       </c>
       <c r="F88" t="s">
-        <v>6</v>
+        <v>176</v>
       </c>
       <c r="G88" t="n">
-        <v>184</v>
+        <v>1</v>
       </c>
       <c r="H88" t="n">
-        <v>819</v>
+        <v>1137</v>
       </c>
       <c r="I88" t="s">
-        <v>112</v>
+        <v>222</v>
       </c>
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>182</v>
+        <v>141</v>
       </c>
       <c r="B89" t="n">
-        <v>6790</v>
+        <v>6197</v>
       </c>
       <c r="C89" t="s">
         <v>2</v>
       </c>
       <c r="D89" t="n">
-        <v>125</v>
+        <v>399</v>
       </c>
       <c r="E89" t="n">
-        <v>391</v>
+        <v>740</v>
       </c>
       <c r="F89" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="G89" t="n">
-        <v>373</v>
+        <v>1195</v>
       </c>
       <c r="H89" t="n">
-        <v>1173</v>
+        <v>2220</v>
       </c>
       <c r="I89" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>157</v>
+        <v>98</v>
       </c>
       <c r="B90" t="n">
-        <v>5595</v>
+        <v>6197</v>
       </c>
       <c r="C90" t="s">
         <v>2</v>
       </c>
       <c r="D90" t="n">
-        <v>1</v>
+        <v>399</v>
       </c>
       <c r="E90" t="n">
-        <v>379</v>
+        <v>740</v>
       </c>
       <c r="F90" t="s">
-        <v>54</v>
+        <v>111</v>
       </c>
       <c r="G90" t="n">
-        <v>1</v>
+        <v>1195</v>
       </c>
       <c r="H90" t="n">
-        <v>1137</v>
+        <v>2220</v>
       </c>
       <c r="I90" t="s">
-        <v>223</v>
+        <v>140</v>
       </c>
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>144</v>
+        <v>97</v>
       </c>
       <c r="B91" t="n">
-        <v>6197</v>
+        <v>3702</v>
       </c>
       <c r="C91" t="s">
         <v>2</v>
       </c>
       <c r="D91" t="n">
-        <v>399</v>
+        <v>357</v>
       </c>
       <c r="E91" t="n">
-        <v>740</v>
+        <v>620</v>
       </c>
       <c r="F91" t="s">
-        <v>113</v>
+        <v>49</v>
       </c>
       <c r="G91" t="n">
-        <v>1195</v>
+        <v>1069</v>
       </c>
       <c r="H91" t="n">
-        <v>2220</v>
+        <v>1860</v>
       </c>
       <c r="I91" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="B92" t="n">
-        <v>6197</v>
+        <v>5566</v>
       </c>
       <c r="C92" t="s">
         <v>2</v>
       </c>
       <c r="D92" t="n">
-        <v>399</v>
+        <v>16</v>
       </c>
       <c r="E92" t="n">
-        <v>740</v>
+        <v>351</v>
       </c>
       <c r="F92" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="G92" t="n">
-        <v>1195</v>
+        <v>46</v>
       </c>
       <c r="H92" t="n">
-        <v>2220</v>
+        <v>1053</v>
       </c>
       <c r="I92" t="s">
-        <v>143</v>
+        <v>21</v>
       </c>
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B93" t="n">
-        <v>3702</v>
+        <v>1457</v>
       </c>
       <c r="C93" t="s">
         <v>2</v>
       </c>
       <c r="D93" t="n">
-        <v>357</v>
+        <v>1</v>
       </c>
       <c r="E93" t="n">
-        <v>620</v>
+        <v>335</v>
       </c>
       <c r="F93" t="s">
-        <v>90</v>
+        <v>226</v>
       </c>
       <c r="G93" t="n">
-        <v>1069</v>
+        <v>1</v>
       </c>
       <c r="H93" t="n">
-        <v>1860</v>
+        <v>1005</v>
       </c>
       <c r="I93" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
-        <v>114</v>
+        <v>70</v>
       </c>
       <c r="B94" t="n">
-        <v>5566</v>
+        <v>9261</v>
       </c>
       <c r="C94" t="s">
         <v>2</v>
       </c>
       <c r="D94" t="n">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E94" t="n">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="F94" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="G94" t="n">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="H94" t="n">
-        <v>1053</v>
+        <v>1044</v>
       </c>
       <c r="I94" t="s">
-        <v>22</v>
+        <v>143</v>
       </c>
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>88</v>
+        <v>29</v>
       </c>
       <c r="B95" t="n">
-        <v>1457</v>
+        <v>5292</v>
       </c>
       <c r="C95" t="s">
         <v>2</v>
       </c>
       <c r="D95" t="n">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E95" t="n">
-        <v>335</v>
+        <v>313</v>
       </c>
       <c r="F95" t="s">
-        <v>226</v>
+        <v>163</v>
       </c>
       <c r="G95" t="n">
-        <v>1</v>
+        <v>85</v>
       </c>
       <c r="H95" t="n">
-        <v>1005</v>
+        <v>939</v>
       </c>
       <c r="I95" t="s">
-        <v>121</v>
+        <v>202</v>
       </c>
     </row>
     <row r="96" spans="1:9">
       <c r="A96" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="B96" t="n">
-        <v>1025</v>
+        <v>659</v>
       </c>
       <c r="C96" t="s">
-        <v>2</v>
+        <v>217</v>
       </c>
       <c r="D96" t="n">
-        <v>1</v>
+        <v>189</v>
       </c>
       <c r="E96" t="n">
-        <v>330</v>
+        <v>517</v>
       </c>
       <c r="F96" t="s">
-        <v>188</v>
+        <v>65</v>
       </c>
       <c r="G96" t="n">
-        <v>1</v>
+        <v>565</v>
       </c>
       <c r="H96" t="n">
-        <v>990</v>
+        <v>1551</v>
       </c>
       <c r="I96" t="s">
-        <v>185</v>
+        <v>103</v>
       </c>
     </row>
     <row r="97" spans="1:9">
       <c r="A97" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="B97" t="n">
-        <v>9261</v>
+        <v>5605</v>
       </c>
       <c r="C97" t="s">
-        <v>2</v>
+        <v>217</v>
       </c>
       <c r="D97" t="n">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E97" t="n">
-        <v>348</v>
+        <v>400</v>
       </c>
       <c r="F97" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="G97" t="n">
-        <v>73</v>
+        <v>163</v>
       </c>
       <c r="H97" t="n">
-        <v>1044</v>
+        <v>1200</v>
       </c>
       <c r="I97" t="s">
-        <v>146</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed PDB construct selection script so that it selects PDBs which correspond to the correct target domain.
</commit_message>
<xml_diff>
--- a/analysis/PDB_construct_selection/PDB_constructs.xlsx
+++ b/analysis/PDB_construct_selection/PDB_constructs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="233">
   <si>
     <t>TCAGTTTATCCTAAGGCATTAAGAGATGAATACATCATGTCAAAAACTCTTGGAAGTGGTGCCTGTGGAGAGGTAAAGCTGGCTTTCGAGAGGAAAACATGTAAGAAAGTAGCCATAAAGATCATCAGCAAAAGGAAGTTTGCTATTGGTTCAGCAAGAGAGGCAGACCCAGCTCTCAATGTTGAAACAGAAATAGAAATTTTGAAAAAGCTAAATCATCCTTGCATCATCAAGATTAAAAACTTTTTTGATGCAGAAGATTATTATATTGTTTTGGAATTGATGGAAGGGGGAGAGCTGTTTGACAAAGTGGTGGGGAATAAACGCCTGAAAGAAGCTACCTGCAAGCTCTATTTTTACCAGATGCTCTTGGCTGTGCAGTACCTTCATGAAAACGGTATTATACACCGTGACTTAAAGCCAGAGAATGTTTTACTGTCATCTCAAGAAGAGGACTGTCTTATAAAGATTACTGATTTTGGGCACTCCAAGATTTGGGGAGAGACCTCTCTCATGAGAACCTTATGTGGAACCCCCACCTACTTGGCGCCTGAAGTTCTTGTTTCTGTTGGGACTGCTGGGTATAACCGTGCTGTGGACTGCTGGAGTTTAGGAGTTATTCTTTTTATCTGCCTTAGTGGGTATCCACCTTTCTCTGAGCATAGGACTCAAGTGTCACTGAAGGATCAGATCACCAGTGGAAAATACAACTTCATTCCTGAAGTCTGGGCAGAAGTCTCAGAGAAAGCTCTGGACCTTGTCAAGAAGTTGTTGGTAGTGGATCCAAAGGCACGTTTTACGACAGAAGAAGCCTTAAGACACCCGTGGCTTCAGGATGAAGACATGAAGAGAAAGTTTCAAGATCTTCTGTCTGAGGAAAATGAATCCACAGCTCTACCCCAGGTTCTAGCCCAGCCTTCTACTAGTCGAAAGCGGCCCCGTGAAGGGGAAGCCGAGGGTGCCGAG</t>
   </si>
@@ -47,507 +47,516 @@
     <t>GTGGAGGACCATTATGAGATGGGGGAGGAGCTGGGCAGCGGCCAGTTTGCGATCGTGCGGAAGTGCCGGCAGAAGGGCACGGGCAAGGAGTACGCAGCCAAGTTCATCAAGAAGCGCCGCCTGTCATCCAGCCGGCGTGGGGTGAGCCGGGAGGAGATCGAGCGGGAGGTGAACATCCTGCGGGAGATCCGGCACCCCAACATCATCACCCTGCACGACATCTTCGAGAACAAGACGGACGTGGTCCTCATCCTGGAGCTGGTCTCTGGCGGGGAGCTCTTTGACTTCCTGGCGGAGAAGGAGTCGCTGACGGAGGACGAGGCCACCCAGTTCCTCAAGCAGATCCTGGACGGCGTTCACTACCTGCACTCTAAGCGCATCGCACACTTTGACCTGAAGCCGGAAAACATCATGCTGCTGGACAAGAACGTGCCCAACCCACGAATCAAGCTCATCGACTTCGGCATCGCGCACAAGATCGAGGCGGGGAACGAGTTCAAGAACATCTTCGGCACCCCGGAGTTTGTGGCCCCAGAGATTGTGAACTATGAGCCGCTGGGCCTGGAGGCGGACATGTGGAGCATCGGTGTCATCACCTATATCCTCCTGAGCGGTGCATCCCCGTTCCTGGGCGAGACCAAGCAGGAGACGCTCACCAACATCTCAGCCGTGAACTACGACTTCGACGAGGAGTACTTCAGCAACACCAGCGAGCTGGCCAAGGACTTCATTCGCCGGCTGCTCGTCAAAGATCCCAAGCGGAGAATGACCATTGCCCAGAGCCTGGAACATTCCTGGATTAAGGCGATCCGGCGGCGGAACGTGCGTGGTGAGGACAGCGGC</t>
   </si>
   <si>
+    <t>MSGPRAGFYRQELNKTVWEVPQRLQGLRPVGSGAYGSVCSAYDARLRQKVAVKKLSRPFQSLIHARRTYRELRLLKHLKHENVIGLLDVFTPATSIEDFSEVYLVTTLMGADLNNIVKCQALSDEHVQFLVYQLLRGLKYIHSAGIIHRDLKPSNVAVNEDCELRILDFGLARQADEEMTGYVATRWYRAPEIMLNWMHYNQTVDIWSVGCIMAELLQGKALFPGSDYIDQLKRIMEVVGTPSPEVLAKISSEHARTYIQSLPPMPQKDLSSIFRGANPLAIDLLGRMLVLDSDQRVSAAEALAHAYFSQYHDPEDEPEAEPYDESVEAKERTLEEWKELTYQEVLSFKPPEPPKPPGSLEIEQ</t>
+  </si>
+  <si>
+    <t>CSKP_HUMAN_D0_3TAC_A</t>
+  </si>
+  <si>
+    <t>MST4_HUMAN_D0_4FZD_B</t>
+  </si>
+  <si>
+    <t>CGGGACTCGAGTGATGATTGGGAGATTCCTGATGGGCAGATTACAGTGGGACAAAGAATTGGATCTGGATCATTTGGAACAGTCTACAAGGGAAAGTGGCATGGTGATGTGGCAGTGAAAATGTTGAATGTGACAGCACCTACACCTCAGCAGTTACAAGCCTTCAAAAATGAAGTAGGAGTACTCAGGAAAACACGACATGTGAATATCCTACTCTTCATGGGCTATTCCACAAAGCCACAACTGGCTATTGTTACCCAGTGGTGTGAGGGCTCCAGCTTGTATCACCATCTCCATATCATTGAGACCAAATTTGAGATGATCAAgCTTATAGATATTGCACGACAGACTGCACAGGGCATGGATTACTTACACGCCAAGTCAATCATCCACAGAGACCTCAAGAGTAATAATATATTTCTTCATGAAGACCTCACAGTAAAAATAGGTGATTTTGGTCTAGCTACAGTGAAATCTCGATGGAGTGGGTCCCATCAGTTTGAACAGTTGTCTGGgTCCATTTTGTGGATGGCACCAGAAGTCATCAGAATGCAAGATAAAAATCCATACAGCTTTCAGTCAGATGTATATGCATTTGGgATTGTTCTGTATGAATTGATGACTGGACAGTTACCTTATTCAAACATCAACAACAGGGACCAGATAATTTTTATGGTGGGACGAGGATACCTGTCTCCAGATCTCAGTAAGGTACGGAGTAACTGTCCAAAAGCCATGAAGAGATTAATGGCAGAGTGCCTCAAAAAGAAAAGAGATGAGAGACCACTCTTTCCCCAAATTCTCGCC</t>
+  </si>
+  <si>
+    <t>MARK2_HUMAN_D0_3IEC_D</t>
+  </si>
+  <si>
+    <t>MK10_HUMAN_D0_2B1P_A</t>
+  </si>
+  <si>
+    <t>CCATTTCCAGAAGGCAAGGTTCTGGATGATATGGAAGGCAATCAGTGGGTACTGGGCAAGAAGATTGGCTCTGGAGGATTTGGATTGATATATTTAGCTTTCCCCACAAATAAACCAGAGAAAGATGCAAGACATGTAGTAAAAGTGGAATATCAAGAAAATGGCCCGTTATTTTCAGAACTTAAATTTTATCAGAGAGTTGCAAAAAAAGACTGTATCAAAAAGTGGATAGAACGCAAACAACTTGATTATTTAGGAATTCCTCTGTTTTATGGATCTGGTCTGACTGAATTCAAGGGAAGAAGTTACAGATTTATGGTAATGGAAAGACTAGGAATAGATTTACAGAAGATCTCAGGCCAGAATGGTACCTTTAAAAAGTCAACTGTCCTGCAATTAGGTATCCGAATGTTGGATGTACTGGAATATATACATGAAAATGAATATGTTCATGGTGATATAAAAGCAGCAAATCTACTTTTGGGTTACAAAAATCCAGACCAGGTTTATCTTGCAGATTATGGACTTTCCTACAGATATTGTCCCAATGGGAACCACAAACAGTATCAGGAAAATCCTAGAAAAGGCCATAATGGGACAATAGAGTTTACCAGCTTGGATGCCCACAAGGGAGTAGCCTTGTCCAGACGAAGTGACGTTGAGATCCTCGGCTACTGCATGCTGCGGTGGTTGTGTGGGAAACTTCCCTGGGAACAGAACCTGAAGGACCCTGTGGCTGTGCAGACTGCTAAAACAAATCTGTTGGACGAGCTCCCCCAGTCAGTGCTTAAATGGGCTCCTTCTGGAAGCAGTTGCTGTGAAATAGCCCAATTTTTGGTATGTGCTCATAGTTTAGCATATGATGAAAAGCCAAACTATCAAGCCCTCAAGAAAATTTTGAACCCTCATGGAATACCTTTAGGACCACTGGACTTTTCCACAAAAGGACAGAGTATAAATGTCCAT</t>
+  </si>
+  <si>
+    <t>GGGGACTCTGATATATCCAGTCCATTACTGCAAAATACTGTCCACATTGACCTCAGTGCTCTAAATCCAGAGCTGGTCCAGGCAGTGCAGCATGTAGTGATTGGGCCCAGTAGCCTGATTGTGCATTTCAATGAAGTCATAGGAAGAGGGCATTTTGGTTGTGTATATCATGGGACTTTGTTGGACAATGATGGCAAGAAAATTCACTGTGCTGTGAAATCCTTGAACAGAATCACTGACATAGGAGAAGTTTCCCAATTTCTGACCGAGGGAATCATCATGAAAGATTTTAGTCATCCCAATGTCCTCTCGCTCCTGGGAATCTGCCTGCGAAGTGAAGGGTCTCCGCTGGTGGTCCTACCATACATGAAACATGGAGATCTTCGAAATTTCATTCGAAATGAGACTCATAATCCAACTGTAAAAGATCTTATTGGCTTTGGTCTTCAAGTAGCCAAAGGCATGAAATATCTTGCAAGCAAAAAGTTTGTCCACAGAGACTTGGCTGCAAGAAACTGTATGCTGGATGAAAAATTCACAGTCAAGGTTGCTGATTTTGGTCTTGCCAGAGACATGTATGATAAAGAATACTATAGTGTACACAACAAAACAGGTGCAAAGCTGCCAGTGAAGTGGATGGCTTTGGAAAGTCTGCAAACTCAAAAGTTTACCACCAAGTCAGATGTGTGGTCCTTTGGCGTGCTCCTCTGGGAGCTGATGACAAGAGGAGCCCCACCTTATCCTGACGTAAACACCTTTGATATAACTGTTTACTTGTTGCAAGGGAGAAGACTCCTACAACCCGAATACTGCCCAGACCCCTTATATGAAGTAATGCTAAAATGCTGGCACCCTAAAGCCGAAATGCGCCCATCCTTTTCTGAACTGGTGTCCCGGATATCAGCGATCTTCTCTACTTTCATTGGG</t>
+  </si>
+  <si>
+    <t>YQLFEELGKGAFSVVRRCVKVLAGQEYAAKIINTKKLSARDHQKLEREARICRLLKHPNIVRLHDSISEEGHHYLIFDLVTGGELFEDIVAREYYSEADASHCIQQILEAVLHCHQMGVVHRDLKPENLLLASKLKGAAVKLADFGLAIEVEGEQQAWFGFAGTPGYLSPEVLRKDPYGKPVDLWACGVILYILLVGYPPFWDEDQHRLYLQIKAGAYDFPSPEWDTVTPEAKDLINKMLTINPSKRITAAEALKHPWISHRSTVASCMHRQETVDCLKKFNARRKLKGA</t>
+  </si>
+  <si>
+    <t>ENFQKVEKIGEGTYGVVYKARNKLTGEVVALKKIRLDTETEGVPSTAIREISLLKELNHPNIVKLLDVIHTENKLYLVFEFLHQDLKKFMDASALTGIPLPLIKSYLFQLLQGLAFCHSHRVLHRDLKPQNLLINTEGAIKLADFGLARAFGVPVRTYTHEVVTLWYRAPEILLGCKYYSTAVDIWSLGCIFAEMVTRRALFPGDSEIDQLFRIFRTLGTPDEVVWPGVTSMPDYKPSFPKWARQDFSKVVPPLDEDGRSLLSQMLHYDPNKRISAKAALAHPFFQDVTKPVPHL</t>
+  </si>
+  <si>
+    <t>TTK_HUMAN_D0_3H9F_A</t>
+  </si>
+  <si>
+    <t>SVKGRIYSILKQIGSGGSSKVFQVLNEKKQIYAIKYVNLEEADNQTLDSYRNEIAYLNKLQQHSDKIIRLYDYEITDQYIYMVMECGNIDLNSWLKKKKSIDPWERKSYWKNMLEAVHTIHQHGIVHSDLKPANFLIVDGMLKLIDFGIANQMQPDTTSVVKDSQVGTVNYMPPEAIKDMSSSRENGKSKSKISPKSDVWSLGCILYYMTYGKTPFQQIINQISKLHAIIDPNHEIEFPDIPEKDLQDVLKCCLKRDPKQRISIPELLAHPYVQIQTHPVNQMAKGTTEE</t>
+  </si>
+  <si>
+    <t>GTGAAAGAATTCTTAGCCAAAGCCAAAGAAGATTTTCTTAAAAAATGGGAAAGTCCCGCTCAGAACACAGCCCACTTGGATCAGTTTGAACGAATCAAGACCCTCGGCACGGGCTCCTTCGGGCGGGTGATGCTGGTGAAACACAAGGAGACCGGGAACCACTATGCCATGAAGATCCTCGACAAACAGAAGGTGGTGAAACTGAAACAGATCGAACACACCCTGAATGAAAAGCGCATCCTGCAAGCTGTCAACTTTCCGTTCCTCGTCAAACTCGAGTTCTCCTTCAAGGACAACTCAAACTTATACATGGTCATGGAGTACGTGCCCGGCGGGGAGATGTTCTCACACCTACGGCGGATCGGAAGGTTCAGTGAGCCCCATGCCCGTTTCTACGCGGCCCAGATCGTCCTGACCTTTGAGTATCTGCACTCGCTGGATCTCATCTACAGGGACCTGAAGCCGGAGAATCTGCTCATTGACCAGCAGGGCTACATTCAGGTGACAGACTTCGGTTTCGCCAAGCGCGTGAAGGGCCGCACTTGGACCTTGTGCGGCACCCCTGAGTACCTGGCCCCTGAGATTATCCTGAGCAAAGGCTACAACAAGGCCGTGGACTGGTGGGCCCTGGGGGTTCTTATCTATGAAATGGCCGCTGGCTACCCGCCCTTCTTCGCAGACCAGCCCATCCAGATCTATGAGAAGATCGTCTCTGGGAAGGTGCGCTTCCCTTCCCACTTCAGCTCTGACTTGAAGGACCTGCTGCGGAACCTCCTGCAGGTAGATCTCACCAAGCGCTTTGGGAACCTCAAGAATGGGGTCAACGATATCAAGAACCACAAGTGGTTTGCCACAACTGACTGGATTGCCATCTACCAGAGGAAGGTGGAAGCTCCCTTCATACCAAAGTTTAAAGGCCCTGGGGATACGAGTAACTTTGACGACTATGAGGAAGAAGAAATCCGGGTCTCCATCAATGAGAAGTGTGGCAAGGAGTTTTCTGAGTTT</t>
+  </si>
+  <si>
+    <t>TCCCCCAACTACGACAAGTGGGAGATGGAACGCACGGACATCACCATGAAGCACAAGCTGGGCGGGGGCCAGTACGGGGAGGTGTACGAGGGCGTGTGGAAGAAATACAGCCTGACGGTGGCCGTGAAGACCTTGAAGGAGGACACCATGGAGGTGGAAGAGTTCTTGAAAGAAGCTGCAGTCATGAAAGAGATCAAACACCCTAACCTGGTGCAGCTCCTTGGGGTCTGCACCCGGGAGCCCCCGTTCTATATCATCACTGAGTTCATGACCTACGGGAACCTCCTGGACTACCTGAGGGAGTGCAACCGGCAGGAGGTGAACGCCGTGGTGCTGCTGTACATGGCCACTCAGATCTCGTCAGCCATGGAGTACCTGGAGAAGAAAAACTTCATCCACAGAGATCTTGCTGCCCGAAACTGCCTGGTAGGGGAGAACCACTTGGTGAAGGTAGCTGATTTTGGCCTGAGCAGGTTGATGACAGGGGACACCTACACAGCCCATGCTGGAGCCAAGTTCCCCATCAAATGGACTGCACCCGAGAGCCTGGCCTACAACAAGTTCTCCATCAAGTCCGACGTCTGGGCATTTGGAGTATTGCTTTGGGAAATTGCTACCTATGGCATGTCCCCTTACCCGGGAATTGACCTGTCCCAGGTGTATGAGCTGCTAGAGAAGGACTACCGCATGGAGCGCCCAGAAGGCTGCCCAGAGAAGGTCTATGAACTCATGCGAGCATGTTGGCAGTGGAATCCCTCTGACCGGCCCTCCTTTGCTGAAATCCACCAAGCCTTTGAAACAATGTTCCAGGAATCCAGTATCTCAGACGAAGTGGAAAAGGAGCTGGGGAAA</t>
+  </si>
+  <si>
+    <t>RDSSDDWEIPDGQITVGQRIGSGSFGTVYKGKWHGDVAVKMLNVTAPTPQQLQAFKNEVGVLRKTRHVNILLFMGYSTKPQLAIVTQWCEGSSLYHHLHIIETKFEMIKLIDIARQTAQGMDYLHAKSIIHRDLKSNNIFLHEDLTVKIGDFGLATVKSRWSGSHQFEQLSGSILWMAPEVIRMQDKNPYSFQSDVYAFGIVLYELMTGQLPYSNINNRDQIIFMVGRGYLSPDLSKVRSNCPKAMKRLMAECLKKKRDERPLFPQILA</t>
+  </si>
+  <si>
+    <t>KS6A1_HUMAN_D1_3RNY_B</t>
+  </si>
+  <si>
+    <t>ACCGACAGCTTCTCGGGCAGGTTTGAAGACGTCTACCAGCTGCAGGAAGATGTGCTGGGGGAGGGCGCTCATGCCCGAGTGCAGACCTGCATCAACCTGATCACCAGCCAGGAGTACGCCGTCAAGATCATTGAGAAGCAGCCAGGCCACATTCGGAGCAGGGTTTTCAGGGAGGTGGAGATGCTGTACCAGTGCCAGGGACACAGGAACGTCCTAGAGCTGATTGAGTTCTTCGAGGAGGAGGACCGCTTCTACCTGGTGTTTGAGAAGATGCGGGGAGGCTCCATCCTGAGCCACATCCACAAGCGCCGGCACTTCAACGAGCTGGAGGCCAGCGTGGTGGTGCAGGACGTGGCCAGCGCCTTGGACTTTCTGCATAACAAAGGCATCGCCCACAGGGACCTAAAGCCGGAAAACATCCTCTGTGAGCACCCCAACCAGGTCTCCCCCGTGAAGATCTGTGACTTCGACCTGGGCAGCGGCATCAAACTCAACGGGGACTGCTCCCCTATCTCCACCCCGGAGCTGCTCACTCCGTGCGGCTCGGCGGAGTACATGGCCCCGGAGGTAGTGGAGGCCTTCAGCGAGGAGGCTAGCATCTACGACAAGCGCTGCGACCTGTGGAGCCTGGGCGTCATCTTGTATATCCTACTCAGCGGCTACCCGCCCTTCGTGGGCCGCTGTGGCAGCGACTGCGGCTGGGACCGCGGCGAGGCCTGCCCTGCCTGCCAGAACATGCTGTTTGAGAGCATCCAGGAGGGCAAGTACGAGTTCCCCGACAAGGACTGGGCCCACATCTCCTGCGCTGCCAAAGACCTCATCTCCAAGCTGCTGGTCCGTGACGCCAAGCAGAGGCTGAGTGCCGCCCAAGTCCTGCAGCACCCCTGGGTTCAGGGGTGCGCCCCGGAGAACACCTTGCCCACTCCCATGGTCCTGCAGAGG</t>
+  </si>
+  <si>
+    <t>MSRSKRDNNFYSVEIGDSTFTVLKRYQNLKPIGSGAQGIVCAAYDAILERNVAIKKLSRPFQNQTHAKRAYRELVLMKCVNHKNIIGLLNVFTPQKSLEEFQDVYIVMELMDANLCQVIQMELDHERMSYLLYQMLCGIKHLHSAGIIHRDLKPSNIVVKSDCTLKILDFGLARTAGTSFMMTPYVVTRYYRAPEVILGMGYKENVDLWSVGCIMGEMVCHKILFPGRDYIDQWNKVIEQLGTPCPEFMKKLQPTVRTYVENRPKYAGYSFEKLFPDVLFPADSEHNKLKASQARDLLSKMLVIDASKRISVDEALQHPYINVWYDPSEAEAPPPKIPDKQLDEREHTIEEWKELIYKEVMDLE</t>
+  </si>
+  <si>
+    <t>STRAA_HUMAN_D0_3GNI_B</t>
+  </si>
+  <si>
+    <t>MP2K2_HUMAN_D0_1S9I_A</t>
+  </si>
+  <si>
+    <t>PIM1_HUMAN_D0_4A7C_A</t>
+  </si>
+  <si>
+    <t>NEK7_HUMAN_D0_2WQN_A</t>
+  </si>
+  <si>
+    <t>GGGCCGGAGGATGAGCTGCCCGACTGGGCCGCCGCCAAAGAGTTTTACCAGAAGTACGACCCTAAGGACGTCATCGGCAGAGGAGTGAGCTCTGTGGTCCGCCGTTGTGTTCATCGAGCTACTGGCCACGAGTTTGCGGTGAAGATTATGGAAGTGACAGCTGAGCGGCTGAGTCCTGAGCAGCTGGAGGAGGTGCGGGAAGCCACACGGCGAGAGACACACATCCTTCGCCAGGTCGCCGGCCACCCCCACATCATCACCCTCATCGATTCCTACGAGTCTTCTAGCTTCATGTTCCTGGTGTTTGACCTGATGCGGAAGGGAGAGCTGTTTGACTATCTCACAGAGAAGGTGGCCCTCTCTGAAAAGGAAACCAGGTCCATCATGCGGTCTCTGCTGGAAGCAGTGAGCTTTCTCCATGCCAACAACATTGTGCATCGAGATCTGAAGCCCGAGAATATTCTCCTAGATGACAATATGCAGATCCGACTTTCAGATTTCGGGTTCTCCTGCCACTTGGAACCTGGCGAGAAGCTTCGAGAGTTGTGTGGGACCCCAGGGTATCTAGCGCCAGAGATCCTTAAATGCTCCATGGATGAAACCCACCCAGGCTATGGCAAGGAGGTCGACCTCTGGGCCTGTGGGGTGATCTTGTTCACACTCCTGGCTGGCTCGCCACCCTTCTGGCACCGGCGGCAGATCCTGATGTTACGCATGATCATGGAGGGCCAGTACCAGTTCAGTTCCCCCGAGTGGGATGACCGTTCCAGCACTGTCAAAGACCTGATCTCCAGGCTGCTGCAGGTGGATCCTGAGGCACGCCTGACAGCTGAGCAGGCCCTACAGCACCCCTTCTTTGAGCGT</t>
+  </si>
+  <si>
+    <t>KC1E_HUMAN_D0_4HNI_A</t>
+  </si>
+  <si>
+    <t>VRK2_HUMAN_D0_2V62_B</t>
+  </si>
+  <si>
+    <t>ETYIKLDKLGEGTYATVYKGKSKLTDNLVALKEIRLEHEEGAPCTAIREVSLLKDLKHANIVTLHDIIHTEKSLTLVFEYLDKDLKQYLDDCGNIINMHNVKLFLFQLLRGLAYCHRQKVLHRDLKPQNLLINERGELKLADFGLARAKSIPTKTYSNEVVTLWYRPPDILLGSTDYSTQIDMWGVGCIFYEMATGRPLFPGSTVEEQLHFIFRILGTPTEETWPGILSNEEFKTYNYPKYRAEALLSHAPRLDSDGADLLTKLLQFEGRNRISAEDAMKHPFFLSLGERIHKLPDTTSIFALKEIQLQKEASLRS</t>
+  </si>
+  <si>
+    <t>HQLQPRRVSFRGEASETLQSPGYDPSRPESFFQQSFQRLSRLGHGSYGEVFKVRSKEDGRLYAVKRSMSPFRGPKDRARKLAEVGSHEKVGQHPCCVRLEQAWEEGGILYLQTELCGPSLQQHCEAWGASLPEAQVWGYLRDTLLALAHLHSQGLVHLDVKPANIFLGPRGRCKLGDFGLLVELGTAGAGEVQEGDPRYMAPELLQGSYGTAADVFSLGLTILEVACNMELPHGGEGWQQLRQGYLPPEFTAGLSSELRSVLVMMLEPDPKLRATAEALLALPVLRQP</t>
+  </si>
+  <si>
+    <t>aa_end</t>
+  </si>
+  <si>
+    <t>PMYT1_HUMAN_D0_3P1A_A</t>
+  </si>
+  <si>
+    <t>MK08_HUMAN_D0_2NO3_A</t>
+  </si>
+  <si>
+    <t>TCGGTTAAAGGAAGAATTTATTCCATATTAAAGCAGATAGGAAGTGGAGGTTCAAGCAAGGTATTTCAGGTGTTAAATGAAAAGAAACAGATATATGCTATAAAATATGTGAACTTAGAAGAAGCAGATAACCAAACTCTTGATAGTTACCGGAACGAAATAGCTTATTTGAATAAACTACAACAACACAGTGATAAGATCATCCGACTTTATGATTATGAAATCACGGACCAGTACATCTACATGGTAATGGAGTGTGGAAATATTGATCTTAATAGTTGGCTTAAAAAGAAAAAATCCATTGATCCATGGGAACGCAAGAGTTACTGGAAAAATATGTTAGAGGCAGTTCACACAATCCATCAACATGGCATTGTTCACAGTGATCTTAAACCAGCTAACTTTCTGATAGTTGATGGAATGCTAAAGCTAATTGATTTTGGGATTGCAAACCAAATGCAACCAGATACAACAAGTGTTGTTAAAGATTCTCAGGTTGGCACAGTTAATTATATGCCACCAGAAGCAATCAAAGATATGTCTTCCTCCAGAGAGAATGGGAAATCTAAGTCAAAGATAAGCCCCAAAAGTGATGTTTGGTCCTTAGGATGTATTTTGTACTATATGACTTACGGGAAAACACCATTTCAGCAGATAATTAATCAGATTTCTAAATTACATGCCATAATTGATCCTAATCATGAAATTGAATTTCCCGATATTCCAGAGAAAGATCTTCAAGATGTGTTAAAGTGTTGTTTAAAAAGGGACCCAAAACAGAGGATATCCATTCCTGAGCTCCTGGCTCATCCATATGTTCAAATTCAAACTCATCCAGTTAACCAAATGGCCAAGGGAACCACTGAAGAA</t>
+  </si>
+  <si>
+    <t>PAK1_HUMAN_D0_3Q52_A</t>
+  </si>
+  <si>
+    <t>CACCACCATCACCACCATTCGCACTCGGGGCCGGAGATCTCGCGGATTATCGTCGACCCCACGACTGGGAAGCGCTACTGCCGGGGCAAAGTGCTGGGAAAGGGTGGCTTTGCAAAATGTTACGAGATGACAGATTTGACAAATAACAAAGTCTACGCCGCAAAAATTATTCCTCACAGCAGAGTAGCTAAACCTCATCAAAGGGAAAAGATTGACAAAGAAATAGAGCTTCACAGAATTCTTCATCATAAGCATGTAGTGCAGTTTTACCACTACTTCGAGGACAAAGAAAACATTTACATTCTCTTGGAATACTGCAGTAGAAGGTCAATGGCTCATATTTTGAAAGCAAGAAAGGTGTTGACAGAGCCAGAAGTTCGATACTACCTCAGGCAGATTGTGTCTGGACTGAAATACCTTCATGAACAAGAAATCTTGCACAGAGATCTCAAACTAGGGAACTTTTTTATTAATGAAGCCATGGAACTAAAAGTTGGGGACTTCGGTCTGGCAGCCAGGCTAGAACCCTTGGAACACAGAAGGAGAACGATATGTGGTACCCCAAATTATCTCTCTCCTGAAGTCCTCAACAAACAAGGACATGGCTGTGAATCAGACATTTGGGCCCTGGGCTGTGTAATGTATACAATGTTACTAGGGAGGCCCCCATTTGAAACTACAAATCTCAAAGAAACTTATAGGTGCATAAGGGAAGCAAGGTATACAATGCCGTCCTCATTGCTGGCTCCTGCCAAGCACTTAATTGCTAGTATGTTGTCCAAAAACCCAGAGGATCGTCCCAGTTTGGATGACATCATTCGACATGACTTTTTTTTGCAGGGCTTCACTCCGGACAGACTGTCTTCTAGCTGTTGTCATACAGTTCCAGATTTCCACTTATCAAGCCCAGCT</t>
+  </si>
+  <si>
+    <t>GAAACAAAGTATACTGTGGACAAGAGGTTTGGCATGGATTTTAAAGAAATAGAATTAATTGGCTCAGGTGGATTTGGCCAAGTTTTCAAAGCAAAACACAGAATTGACGGAAAGACTTACGTTATTAAACGTGTTAAATATAATAACGAGAAGGCGGAGCGTGAAGTAAAAGCATTGGCAAAACTTGATCATGTAAATATTGTTCACTACAATGGCTGTTGGGATGGATTTGATTATGATCCTGAGACCAGTGATGATTCTCTTGAGAGCAGTGATTATGATCCTGAGAACAGCAAAAATAGTTCAAGGTCAAAGACTAAGTGCCTTTTCATCCAAATGGAATTCTGTGATAAAGGGACCTTGGAACAATGGATTGAAAAAAGAAGAGGCGAGAAACTAGACAAAGTTTTGGCTTTGGAACTCTTTGAACAAATAACAAAAGGGGTGGATTATATACATTCAAAAAAATTAATTCATAGAGATCTTAAGCCAAGTAATATATTCTTAGTAGATACAAAACAAGTAAAGATTGGAGACTTTGGACTTGTAACATCTCTGAAAAATGATGGAAAGCGAACAAGGAGTAAGGGAACTTTGCGATACATGAGCCCAGAACAGATTTCTTCGCAAGACTATGGAAAGGAAGTGGACCTCTACGCTTTGGGGCTAATTCTTGCTGAACTTCTTCATGTATGTGACACTGCTTTTGAAACATCAAAGTTTTTCACAGACCTACGGGATGGCATCATCTCAGATATATTTGATAAAAAAGAAAAAACTCTTCTACAGAAATTACTCTCAAAGAAACCTGAGGATCGACCTAACACATCTGAAATACTAAGGACCTTGACTGTGTGGAAGAAAAGCCCAGAGAAAAATGAACGACACACATGT</t>
+  </si>
+  <si>
+    <t>PAK7_HUMAN_D0_2F57_B</t>
+  </si>
+  <si>
+    <t>expression tag location</t>
+  </si>
+  <si>
+    <t>GAGAACTTCCAAAAGGTGGAAAAGATCGGAGAGGGCACGTACGGAGTTGTGTACAAAGCCAGAAACAAGTTGACGGGAGAGGTGGTGGCGCTTAAGAAAATCCGCCTGGACACTGAGACTGAGGGTGTGCCCAGTACTGCCATCCGAGAGATCTCTCTGCTTAAGGAGCTTAACCATCCTAATATTGTCAAGCTGCTGGATGTCATTCACACAGAAAATAAACTCTACCTGGTTTTTGAATTTCTGCACCAAGATCTCAAGAAATTCATGGATGCCTCTGCTCTCACTGGCATTCCTCTTCCCCTCATCAAGAGCTATCTGTTCCAGCTGCTCCAGGGCCTAGCTTTCTGCCATTCTCATCGGGTCCTCCACCGAGACCTTAAACCTCAGAATCTGCTTATTAACACAGAGGGGGCCATCAAGCTAGCAGACTTTGGACTAGCCAGAGCTTTTGGAGTCCCTGTTCGTACTTACACCCATGAGGTGGTGACCCTGTGGTACCGAGCTCCTGAAATCCTCCTGGGCTGCAAATATTATTCCACAGCTGTGGACATCTGGAGCCTGGGCTGCATCTTTGCTGAGATGGTGACTCGCCGGGCCCTATTCCCTGGAGATTCTGAGATTGACCAGCTCTTCCGGATCTTTCGGACTCTGGGGACCCCAGATGAGGTGGTGTGGCCAGGAGTTACTTCTATGCCTGATTACAAGCCAAGTTTCCCCAAGTGGGCCCGGCAAGATTTTAGTAAAGTTGTACCTCCCCTGGATGAAGATGGACGGAGCTTGTTATCGCAAATGCTGCACTACGACCCTAACAAGCGGATTTCGGCCAAGGCAGCCCTGGCTCACCCTTTCTTCCAGGATGTGACCAAGCCAGTACCCCATCTT</t>
+  </si>
+  <si>
+    <t>GGGGAATGCAGTCAGAAGGGTCCTGTCCCCTTTAGCCATTGCCTTCCCACAGAAAAACTGCAACGCTGTGAGAAGATTGGGGAAGGGGTGTTTGGCGAAGTGTTTCAAACAATTGCTGATCACACACCCGTAGCCATAAAAATCATTGCTATTGAAGGACCAGATTTAGTCAATGGATCCCATCAGAAAACCTTTGAGGAAATCCTGCCAGAGATCATCATCTCCAAAGAGTTGAGCCTCTTATCCGGTGAAGTGTGCAACCGCACAGAAGGCTTTATCGGGCTGAACTCAGTGCACTGTGTCCAGGGATCTTACCCTCCCTTGCTCCTCAAAGCCTGGGATCACTATAATTCAACCAAAGGCTCTGCAAATGACCGGCCTGATTTTTTTAAAGACGACCAGCTCTTCATTGTGCTGGAATTTGAGTTTGGAGGGATTGACTTAGAGCAAATGCGAACCAAGTTGTCTTCCTTGGCTACTGCAAAGAGCATTCTACACCAGCTCACAGCCTCCCTCGCAGTGGCAGAGGCATCACTGCGCTTTGAGCACCGAGACTTACACTGGGGGAACGTGCTCTTAAAGAAAACCAGCCTCAAAAAACTCCACTACACCCTCAATGGGAAGAGCAGCACTATCCCCAGCTGTGGGTTGCAAGTGAGCATCATTGACTACACCCTGTCGCGCTTGGAACGGGATGGGATTGTGGTTTTCTGTGACGTTTCCATGGATGAGGACCTGTTTACCGGTGACGGTGACTACCAGTTTGACATCTACAGGCTCATGAAGAAGGAGAATAACAACCGCTGGGGTGAATATCACCCTTATAGTAATGTGCTCTGGTTACATTACCTGACAGACAAGATGCTGAAACAAATGACCTTCAAGACTAAATGTAACACTCCTGCCATGAAGCAAATTAAGAGAAAAATCCAGGAGTTCCACAGGACAATGCTGAACTTCAGCTCTGCCACTGACTTGCTCTGCCAGCACAGACTGTTTAAG</t>
+  </si>
+  <si>
+    <t>TDSLPGKFEDMYKLTSELLGEGAYAKVQGAVSLQNGKEYAVKIIEKQAGHSRSRVFREVETLYQCQGNKNILELIEFFEDDTRFYLVFEKLQGGSILAHIQKQKHFNEREASRVVRDVAAALDFLHTKDKVSLCHLGGSARAPSGLTAAPTSLGSSDPPTSASQVAGTTGIDHRDLKPENILCESPEKVSPVKICDFDLGSGMKLNNSCTPITTPELTTPCGSAEYMAPEVGEVFTDQATFYDKRCDLWSLGVVLYIMLSGYPPFVGHCGADCGWDRGEVCRVCQNKLFESIQEGKYEFPDKDWAHISSEAKDLISKLLVRDAKQRLSAAQVLQHPWVQGQAPEKG</t>
+  </si>
+  <si>
+    <t>DAPK1_HUMAN_D0_4B4L_A</t>
+  </si>
+  <si>
+    <t>EDSLTKQPEEVFDVLEKLGEGSYGSVFKAIHKESGQVVAIKQVPVESDLQEIIKEISIMQQCDSPYVVKYYGSYFKNTDLWIVMEYCGAGSVSDIIRLRNKTLIEDEIATILKSTLKGLEYLHFMRKIHRDIKAGNILLNTEGHAKLADFGVAGQLTDTMAKRNTVIGTPFWMAPEVIQEIGYNCVADIWSLGITSIEMAEGKPPYADIHPMRAIFMIPTNPPPTFRKPELWSDDFTDFVKKCLVKNPEQRATATQLLQHPFIKNAKPVSILRDLITEAMEIKAKRHEEQQRELEEEE</t>
+  </si>
+  <si>
+    <t>ATGAGCCTCATCCGGAAAAAGGGCTTCTACAAGCAGGACGTCAACAAGACCGCCTGGGAGCTGCCCAAGACCTACGTGTCCCCGACGCACGTCGGCAGCGGGGCCTATGGCTCCGTGTGCTCGGCCATCGACAAGCGGTCAGGGGAGAAGGTGGCCATCAAGAAGCTGAGCCGACCCTTTCAGTCCGAGATCTTCGCCAAGCGCGCCTACCGGGAGCTGCTGCTGCTGAAGCACATGCAGCATGAGAACGTCATTGGGCTCCTGGATGTCTTCACCCCAGCCTCCTCCCTGCGCAACTTCTATGACTTCTACCTGGTGATGCCCTTCATGCAGACGGATCTGCAGAAGATCATGGGGATGGAGTTCAGTGAGGAGAAGATCCAGTACCTGGTGTATCAGATGCTCAAAGGCCTTAAGTACATCCACTCTGCTGGGGTCGTGCACAGGGACCTGAAGCCAGGCAACCTGGCTGTGAATGAGGACTGTGAACTGAAGATTCTGGATTTTGGGCTGGCGCGACATGCAGACGCCGAGATGACTGGCTACGTGGTGACCCGCTGGTACCGAGCCCCCGAGGTGATCCTCAGCTGGATGCACTACAACCAGACAGTGGACATCTGGTCTGTGGTCTGTATCATGGCAGAGATGCTGACAGGGAAAACTCTGTTCAAGGGGAAAGATTACCTGGACCAGCTGACCCAGATCCTGAAAGTGACCGGGGTGCCTGGCACGGAGTTTGTGCAGAAGCTGAACGACAAAGCGGCCAAATCCTACATCCAGTCCCTGCCACAGACCCCCAGGAAGGATTTCACTCAGCTGTTCCCACGGGCCAGCCCCCAGGCTGCGGACCTGCTGGAGAAGATGCTGGAGCTAGACGTGGACAAGCGCCTGACGGCCGCGCAGGCCCTCACCCATCCCTTCTTTGAACCCTTCCGGGACCCTGAGGAAGAGACGGAGGCCCAGCAGCCGTTTGATGATTCCTTAGAACACGAGAAACTCACAGTGGATGAATGGAAGCAGCACATCTACAAGGAGATTGTGAACTTCAGCCCCATT</t>
+  </si>
+  <si>
+    <t>ATGAAAGATTATGATGAACTTCTCAAATATTATGAATTACATGAAACTATTGGGACAGGTGGCTTTGCAAAGGTCAAACTTGCCTGCCATATCCTTACTGGAGAGATGGTAGCTATAAAAATCATGGATAAAAACACACTAGGGAGTGATTTGCCCCGGATCAAAACGGAGATTGAGGCCTTGAAGAACCTGAGACATCAGCATATATGTCAACTCTACCATGTGCTAGAGACAGCCAACAAAATATTCATGGTTCTTGAGTACTGCCCTGGAGGAGAGCTGTTTGACTATATAATTTCCCAGGATCGCCTGTCAGAAGAGGAGACCCGGGTTGTCTTCCGTCAGATAGTATCTGCTGTTGCTTATGTGCACAGCCAGGGCTATGCTCACAGGGACCTCAAGCCAGAAAATTTGCTGTTTGATGAATATCATAAATTAAAGCTGATTGACTTTGGTCTCTGTGCAAAACCCAAGGGTAACAAGGATTACCATCTACAGACATGCTGTGGGAGTCTGGCTTATGCAGCACCTGAGTTAATACAAGGCAAATCATATCTTGGATCAGAGGCAGATGTTTGGAGCATGGGCATACTGTTATATGTTCTTATGTGTGGATTTCTACCATTTGATGATGATAATGTAATGGCTTTATACAAGAAGATTATGAGAGGAAAATATGATGTTCCCAAGTGGCTCTCTCCCAGTAGCATTCTGCTTCTTCAACAAATGCTGCAGGTGGACCCAAAGAAACGGATTTCTATGAAAAATCTATTGAACCATCCCTGGATCATGCAAGATTACAACTATCCTGTTGAGTGGCAAAGCAAGAATCCTTTTATTCACCTCGATGATGATTGCGTAACAGAACTTTCTGTACATCACAGAAACAACAGGCAAACAATGGAGGATTTAATTTCACTGTGGCAGTATGATCACCTCACGGCTACCTATCTTCTGCTTCTAGCCAAGAAGGCTCGGGGAAAACCAGTTCGTTTAAGGCTTTCTTCTTTCTCCTGTGGA</t>
+  </si>
+  <si>
+    <t>ATGGAGGCAGCAGCATCCGAACCCTCTCTTGATCTAGATAATCTGAAACTGTTGGAGCTGATTGGCCGAGGTCGATATGGAGCAGTATATAAAGGCTCCTTGGATGAGCGTCCAGTTGCTGTAAAAGTGTTTTCCTTTGCAAACCGTCAGAATTTTATCAACGAAAAGAACATTTACAGAGTGCCTTTGATGGAACATGACAACATTGCCCGCTTTATAGTTGGAGATGAGAGAGTCACTGCAGATGGACGCATGGAATATTTGCTTGTGATGGAGTACTATCCCAATGGATCTTTATGCAAGTATTTAAGTCTCCACACAAGTGACTGGGTAAGCTCTTGCCGTCTTGCTCATTCTGTTACTAGAGGACTGGCTTATCTTCACACAGAATTACCACGAGGAGATCATTATAAACCTGCAATTTCCCATCGAGATTTAAACAGCAGAAATGTCCTAGTGAAAAATGATGGAACCTGTGTTATTAGTGACTTTGGACTGTCCATGAGGCTGACTGGAAATAGACTGGTGCGCCCAGGGGAGGAAGATAATGCAGCCATAAGCGAGGTTGGCACTATCAGATATATGGCACCAGAAGTGCTAGAAGGAGCTGTGAACTTGAGGGACTGTGAATCAGCTTTGAAACAAGTAGACATGTATGCTCTTGGACTAATCTATTGGGAGATATTTATGAGATGTACAGACCTCTTCCCAGGGGAATCCGTACCAGAGTACCAGATGGCTTTTCAGACAGAGGTTGGAAACCATCCCACTTTTGAGGATATGCAGGTTCTCGTGTCTAGGGAAAAACAGAGACCCAAGTTCCCAGAAGCCTGGAAAGAAAATAGCCTGGCAGTGAGGTCACTCAAGGAGACAATCGAAGACTGTTGGGACCAGGATGCAGAGGCTCGGCTTACTGCACAGTGTGCTGAGGAAAGGATGGCTGAACTTATGATGATTTGGGAAAGAAACAAATCTGTGAGCCCAACA</t>
+  </si>
+  <si>
+    <t>PAK4_HUMAN_D0_2J0I_A</t>
+  </si>
+  <si>
+    <t>AGVSEYELPEDPRWELPRDRLVLGKPLGEGCFGQVVLAEAIGLDKDKPNRVTKVAVKMLKSDATEKDLSDLISEMEMMKMIGKHKNIINLLGACTQDGPLYVIVEYASKGNLREYLQARRPPGLEYCYNPSHNPEEQLSSKDLVSCAYQVARGMEYLASKKCIHRDLAARNVLVTEDNVMKIADFGLARDIHHIDYYKKTTNGRLPVKWMAPEALFDRIYTHQSDVWSFGVLLWEIFTLGGSPYPGVPVEELFKLLKEGHRMDKPSNCTNELYMMMRDCWHAVPSQRPTFKQLVEDLDRIVALTSNQEYLDLSMPLD</t>
+  </si>
+  <si>
+    <t>MAAAAAQGGGGGEPRRTEGVGPGVPGEVEMVKGQPFDVGPRYTQLQYIGEGAYGMVSSAYDHVRKTRVAIKKISPFEHQTYCQRTLREIQILLRFRHENVIGIRDILRASTLEAMRDVYIVQDLMETDLYKLLKSQQLSNDHICYFLYQILRGLKYIHSANVLHRDLKPSNLLINTTCDLKICDFGLARIADPEHDHTGFLTEYVATRWYRAPEIMLNSKGYTKSIDIWSVGCILAEMLSNRPIFPGKHYLDQLNHILGILGSPSQEDLNCIINMKARNYLQSLPSKTKVAWAKLFPKSDSKALDLLDRMLTFNPNKRITVEEALAHPYLEQYYDPTDEPVAEEPFTFAMELDDLPKERLKELIFQETARFQPGVLEAP</t>
+  </si>
+  <si>
+    <t>GAGCCCAAGAAGTACGCAGTGACCGACGACTACCAGTTGTCCAAGCAGGTGCTGGGCCTGGGTGTGAACGGCAAAGTGCTGGAGTGCTTCCATCGGCGCACTGGACAGAAGTGTGCCCTGAAGCTCCTGTATGACAGCCCCAAGGCCCGGCAGGAGGTAGACCATCACTGGCAGGCTTCTGGCGGCCCCCATATTGTCTGCATCCTGGATGTGTATGAGAACATGCACCATGGCAAGCGCTGTCTCCTCATCATCATGGAATGCATGGAAGGTGGTGAGTTGTTCAGCAGGATTCAGGAGCGTGGCGACCAGGCTTTCACTGAGAGAGAAGCTGCAGAGATAATGCGGGATATTGGCACTGCCATCCAGTTTCTGCACAGCCATAACATTGCCCACCGAGATGTCAAGCCTGAAAACCTACTCTACACATCTAAGGAGAAAGACGCAGTGCTTAAGCTCACCGATTTTGGCTTTGCTAAGGAGACCACCCAAAATGCCCTGCAGACACCCTGCTATACTCCCTATTATGTGGCCCCTGAGGTCCTGGGTCCAGAGAAGTATGACAAGTCATGTGACATGTGGTCCCTGGGTGTCATCATGTACATCCTCCTTTGTGGCTTCCCACCCTTCTACTCCAACACGGGCCAGGCCATCTCCCCGGGGATGAAGAGGAGGATTCGCCTGGGCCAGTACGGCTTCCCCAATCCTGAGTGGTCAGAAGTCTCTGAGGATGCCAAGCAGCTGATCCGCCTCCTGTTGAAGACAGACCCCACAGAGAGGCTGACCATCACTCAGTTCATGAACCACCCCTGGATCAACCAATCGATGGTAGTGCCACAGACCCCACTCCACACGGCCCGAGTGCTGCAGGAGGACAAAGACCACTGGGACGAAGTCAAGGAGGAGATGACCAGTGCCTTGGCCACTATGCGGGTAGACTACGACCAGGTG</t>
+  </si>
+  <si>
+    <t>ATGTCTCAGGAGAGGCCCACGTTCTACCGGCAGGAGCTGAACAAGACAATCTGGGAGGTGCCCGAGCGTTACCAGAACCTGTCTCCAGTGGGCTCTGGCGCCTATGGCTCTGTGTGTGCTGCTTTTGACACAAAAACGGGGTTACGTGTGGCAGTGAAGAAGCTCTCCAGACCATTTCAGTCCATCATTCATGCGAAAAGAACCTACAGAGAACTGCGGTTACTTAAACATATGAAACATGAAAATGTGATTGGTCTGTTGGACGTTTTTACACCTGCAAGGTCTCTGGAGGAATTCAATGATGTGTATCTGGTGACCCATCTCATGGGGGCAGATCTGAACAACATTGTGAAATGTCAGAAGCTTACAGATGACCATGTTCAGTTCCTTATCTACCAAATTCTCCGAGGTCTAAAGTATATACATTCAGCTGACATAATTCACAGGGACCTAAAACCTAGTAATCTAGCTGTGAATGAAGACTGTGAGCTGAAGATTCTGGATTTTGGACTGGCTCGGCACACAGATGATGAAATGACAGGCTACGTGGCCACTAGGTGGTACAGGGCTCCTGAGATCATGCTGAACTGGATGCATTACAACCAGACAGTTGATATTTGGTCAGTGGGATGCATAATGGCCGAGCTGTTGACTGGAAGAACATTGTTTCCTGGTACAGACCATATTGATCAGTTGAAGCTCATTTTAAGACTCGTTGGAACCCCAGGGGCTGAGCTTTTGAAGAAAATCTCCTCAGAGTCTGCAAGAAACTATATTCAGTCTTTGACTCAGATGCCGAAGATGAACTTTGCGAATGTATTTATTGGTGCCAATCCCCTGGCTGTCGACTTGCTGGAGAAGATGCTTGTATTGGACTCAGATAAGAGAATTACAGCGGCCCAAGCCCTTGCACATGCCTACTTTGCTCAGTACCACGATCCTGATGATGAACCAGTGGCCGATCCTTATGATCAGTCCTTTGAAAGCAGGGACCTCCTTATAGATGAGTGGAAAAGCCTGACCTATGATGAAGTCATCAGCTTTGTGCCACCACCCCTTGACCAAGAAGAGATGGAGTCC</t>
+  </si>
+  <si>
+    <t>MK11_HUMAN_D0_3GC8_A</t>
+  </si>
+  <si>
+    <t>VRK3_HUMAN_D0_2JII_A</t>
+  </si>
+  <si>
+    <t>MK14_HUMAN_D0_3K3J_A</t>
+  </si>
+  <si>
+    <t>CDK16_HUMAN_D0_3MTL_A</t>
+  </si>
+  <si>
+    <t>GCTGATCCAGAAGAACTGTTCACAAAATTAGAGCGCATTGGGAAAGGCTCATTTGGGGAAGTTTTCAAAGGAATTGATAACCGTACCCAGCAAGTCGTTGCTATTAAAATCATAGACCTTGAGGAAGCCGAAGATGAAATAGAAGACATTCAGCAAGAAATAACTGTCTTGAGTCAATGTGACAGCTCATATGTAACAAAATACTATGGGTCATATTTAAAGGGGTCTAAATTATGGATAATAATGGAATACCTGGGCGGTGGTTCAGCACTGGATCTTCTTCGAGCTGGTCCATTTGATGAGTTCCAGATTGCTACCATGCTAAAGGAAATTTTAAAAGGTCTGGACTATCTGCATTCAGAAAAGAAAATTCACCGAGACATAAAAGCTGCCAATGTCTTGCTCTCAGAACAAGGAGATGTTAAACTTGCTGATTTTGGAGTTGCTGGTCAGCTGACAGATACACAGATTAAAAGAAATACCTTTGTGGGAACTCCATTTTGGATGGCTCCTGAAGTTATTCAACAGTCAGCTTATGACTCAAAAGCTGACATTTGGTCATTGGGAATTACTGCTATTGAACTAGCCAAGGGAGAGCCACCTAACTCCGATATGCATCCAATGAGAGTTCTGTTTCTTATTCCCAAAAACAATCCTCCAACTCTTGTTGGAGACTTTACTAAGTCTTTTAAGGAGTTTATTGATGCTTGCCTGAACAAAGATCCATCATTTCGTCCTACAGCAAAAGAACTTCTGAAACACAAATTCATTGTAAAAAATTCAAAGAAGACTTCTTATCTGACTGAACTGATAGATCGTTTTAAGAGATGGAAGGCAGAA</t>
+  </si>
+  <si>
+    <t>BRAF_HUMAN_D0_4JVG_D</t>
+  </si>
+  <si>
+    <t>PAK6_HUMAN_D0_2C30_A</t>
+  </si>
+  <si>
+    <t>FGFR1_HUMAN_D0_3GQL_B</t>
+  </si>
+  <si>
+    <t>TCTTCGGTCACCGCCAGTGCGGCCCCGGGGACCGCGAGCCTCGTCCCGGATTACTGGATCGACGGCTCCAACAGGGATGCGCTGAGCGATTTCTTCGAGGTGGAGTCGGAGCTGGGACGGGGTGCTACATCCATTGTGTACAGATGCAAACAGAAGGGGACCCAGAAGCCTTATGCTCTCAAAGTGTTAAAGAAAACAGTGGACAAAAAAATCGTAAGAACTGAGATAGGAGTTCTTCTTCGCCTCTCACATCCAAACATTATAAAACTTAAAGAGATATTTGAAACCCCTACAGAAATCAGTCTGGTCCTAGAACTCGTCACAGGAGGAGAACTGTTTGATAGGATTGTGGAAAAGGGATATTACAGTGAGCGAGATGCTGCAGATGCCGTTAAACAAATCCTGGAGGCAGTTGCTTATCTACATGAAAATGGGATTGTCCATCGTGATCTCAAACCAGAGAATCTTCTTTATGCAACTCCAGCCCCAGATGCACCACTCAAAATCGCTGATTTTGGACTCTCTAAAATTGTGGAACATCAAGTGCTCATGAAGACAGTATGTGGAACCCCAGGGTACTGCGCACCTGAAATTCTTAGAGGTTGTGCCTATGGACCTGAGGTGGACATGTGGTCTGTAGGAATAATCACCTACATCTTACTTTGTGGATTTGAACCATTCTATGATGAAAGAGGCGATCAGTTCATGTTCAGGAGAATTCTGAATTGTGAATATTACTTTATCTCCCCCTGGTGGGATGAAGTATCTCTAAATGCCAAGGACTTGGTCAGAAAATTAATTGTTTTGGATCCAAAGAAACGGCTGACTACATTTCAAGCTCTCCAGCATCCGTGGGTCACAGGTAAAGCAGCCAATTTTGTACACATGGATACCGCTCAAAAGAAGCTCCAAGAATTCAATGCCCGGCGTAAGCTTAAGGCAGCGGTGAAGGCTGTGGTGGCCTCTTCCCGCCTGGGA</t>
+  </si>
+  <si>
+    <t>EAFLTQKAKVGELKDDDFERISELGAGNGGVVTKVQHRPSGLIMARKLIHLEIKPAIRNQIIRELQVLHECNSPYIVGFYGAFYSDGEISICMEHMDGGSLDQVLKEAKRIPEEILGKVSIAVLRGLAYLREKHQIMHRDVKPSNILVNSRGEIKLCDFGVSGQLIDSMANSFVGTRSYMAPERLQGTHYSVQSDIWSMGLSLVELAVGRYPIPPPDAKELEAIFGRPVVDGEEGEPHSISPRPRPPGRPVSGHGMDSRPAMAIFELLDYIVNEPPPKLPNGVFTPDFQEFVNKCLIKNPAERADLKMLTNHTFIKRSEVEEVDFAGWLCKTLRLNQPGTPTRTAV</t>
+  </si>
+  <si>
+    <t>GTCATCATTGACAATAAGCGCTACCTCTTCATCCAGAAACTGGGGGAGGGTGGGTTCAGCTATGTGGACCTAGTGGAAGGGTTACATGATGGACACTTCTACGCCCTGAAGCGAATCCTGTGTCACGAGCAGCAGGACCGGGAGGAGGCCCAGCGAGAAGCCGACATGCATCGCCTCTTCAATCACCCCAACATCCTTCGCCTCGTGGCTTACTGTCTGAGGGAACGGGGTGCTAAGCATGAGGCCTGGCTGCTGCTACCATTCTTCAAGAGAGGTACGCTGTGGAATGAGATAGAAAGGCTGAAGGACAAAGGCAACTTCCTGACCGAGGATCAAATCCTTTGGCTGCTGCTGGGGATCTGCAGAGGCCTTGAGGCCATTCATGCCAAGGGTTATGCCCACAGAGACTTGAAGCCCACCAATATATTGCTTGGAGATGAGGGGCAGCCAGTTTTAATGGACTTGGGTTCCATGAATCAAGCATGCATCCATGTGGAGGGCTCCCGCCAGGCTCTGACCCTGCAGGACTGGGCAGCCCAGCGGTGCACCATCTCCTACCGAGCCCCAGAGCTCTTCTCTGTGCAGAGTCACTGTGTCATCGATGAGCGGACTGATGTCTGGTCCCTAGGCTGCGTGCTATATGCCATGATGTTTGGGGAAGGCCCTTATGACATGGTGTTCCAAAAGGGTGACAGTGTGGCCCTTGCTGTGCAGAACCAACTCAGCATCCCACAAAGCCCCAGGCATTCTTCAGCATTGTGGCAGCTCCTGAACTCGATGATGACCGTGGACCCGCATCAGCGTCCTCACATTCCTCTCCTCCTCAGTCAGCTGGAGGCGCTGCAG</t>
+  </si>
+  <si>
+    <t>BMPR2_HUMAN_D0_3G2F_A</t>
+  </si>
+  <si>
+    <t>CACCAGCTGCAGCCCCGGCGGGTGTCATTCCGGGGCGAGGCCTCAGAGACTCTGCAGAGCCCTGGGTATGACCCAAGCCGGCCAGAGTCCTTCTTCCAGCAGAGCTTCCAGAGGCTCAGCCGCCTGGGCCATGGCTCCTACGGAGAGGTCTTCAAGGTGCGCTCCAAGGAGGACGGCCGGCTCTATGCGGTAAAGCGTTCCATGTCACCATTCCGGGGCCCCAAGGACCGGGCCCGCAAGTTGGCCGAGGTGGGCAGCCACGAGAAGGTGGGGCAGCACCCATGCTGCGTGCGGCTGGAGCAGGCCTGGGAGGAGGGCGGCATCCTGTACCTGCAGACGGAGCTGTGCGGGCCCAGCCTGCAGCAACACTGTGAGGCCTGGGGTGCCAGCCTGCCTGAGGCCCAGGTCTGGGGCTACCTGCGGGACACGCTGCTTGCCCTGGCCCATCTGCACAGCCAGGGCCTGGTGCACCTTGATGTCAAGCCTGCCAACATCTTCCTGGGGCCCCGGGGCCGCTGCAAGCTGGGTGACTTCGGACTGCTGGTGGAGCTGGGTACAGCAGGAGCTGGTGAGGTCCAGGAGGGAGACCCCCGCTACATGGCCCCCGAGCTGCTGCAGGGCTCCTATGGGACAGCAGCGGATGTGTTCAGTCTGGGCCTCACCATCCTGGAAGTGGCATGCAACATGGAGCTGCCCCACGGTGGGGAGGGCTGGCAGCAGCTGCGCCAGGGCTACCTGCCCCCTGAGTTCACTGCCGGTCTGTCTTCCGAGCTGCGTTCTGTCCTTGTCATGATGCTGGAGCCAGACCCCAAGCTGCGGGCCACGGCCGAGGCCCTGCTGGCACTGCCTGTGTTGAGGCAGCCG</t>
+  </si>
+  <si>
+    <t>PHKG2_HUMAN_D0_2Y7J_D</t>
+  </si>
+  <si>
+    <t>MAPK2_HUMAN_D0_2JBO_A</t>
+  </si>
+  <si>
+    <t>HHHHHHSHSGPEISRIIVDPTTGKRYCRGKVLGKGGFAKCYEMTDLTNNKVYAAKIIPHSRVAKPHQREKIDKEIELHRILHHKHVVQFYHYFEDKENIYILLEYCSRRSMAHILKARKVLTEPEVRYYLRQIVSGLKYLHEQEILHRDLKLGNFFINEAMELKVGDFGLAARLEPLEHRRRTICGTPNYLSPEVLNKQGHGCESDIWALGCVMYTMLLGRPPFETTNLKETYRCIREARYTMPSSLLAPAKHLIASMLSKNPEDRPSLDDIIRHDFFLQGFTPDRLSSSCCHTVPDFHLSSPA</t>
+  </si>
+  <si>
+    <t>ATGGAGAAGGACGGCCTGTGCCGCGCTGACCAGCAGTACGAATGCGTGGCGGAGATCGGGGAGGGCGCCTATGGGAAGGTGTTCAAGGCCCGCGACTTGAAGAACGGAGGCCGTTTCGTGGCGTTGAAGCGCGTGCGGGTGCAGACCGGCGAGGAGGGCATGCCGCTCTCCACCATCCGCGAGGTGGCGGTGCTGAGGCACCTGGAGACCTTCGAGCACCCCAACGTGGTCAGGTTGTTTGATGTGTGCACAGTGTCACGAACAGACAGAGAAACCAAACTAACTTTAGTGTTTGAACATGTCGATCAAGACTTGACCACTTACTTGGATAAAGTTCCAGAGCCTGGAGTGCCCACTGAAACCATAAAGGATATGATGTTTCAGCTTCTCCGAGGTCTGGACTTTCTTCATTCACACCGAGTAGTGCATCGCGATCTAAAACCACAGAACATTCTGGTGACCAGCAGCGGACAAATAAAACTCGCTGACTTCGGCCTTGCCCGCATCTATAGTTTCCAGATGGCTCTAACCTCAGTGGTCGTCACGCTGTGGTACAGAGCACCCGAAGTCTTGCTCCAGTCCAGCTACGCCACCCCCGTGGATCTCTGGAGTGTTGGCTGCATATTTGCAGAAATGTTTCGTAGAAAGCCTCTTTTTCGTGGAAGTTCAGATGTTGATCAACTAGGAAAAATCTTGGACGTGATTGGACTCCCAGGAGAAGAAGACTGGCCTAGAGATGTTGCCCTTCCCAGGCAGGCTTTTCATTCAAAATCTGCCCAACCAATTGAGAAGTTTGTAACAGATATCGATGAACTAGGCAAAGACCTACTTCTGAAGTGTTTGACATTTAACCCAGCCAAAAGAATATCTGCCTACAGTGCCCTGTCTCACCCATACTTCCAG</t>
+  </si>
+  <si>
+    <t>MEAAASEPSLDLDNLKLLELIGRGRYGAVYKGSLDERPVAVKVFSFANRQNFINEKNIYRVPLMEHDNIARFIVGDERVTADGRMEYLLVMEYYPNGSLCKYLSLHTSDWVSSCRLAHSVTRGLAYLHTELPRGDHYKPAISHRDLNSRNVLVKNDGTCVISDFGLSMRLTGNRLVRPGEEDNAAISEVGTIRYMAPEVLEGAVNLRDCESALKQVDMYALGLIYWEIFMRCTDLFPGESVPEYQMAFQTEVGNHPTFEDMQVLVSREKQRPKFPEAWKENSLAVRSLKETIEDCWDQDAEARLTAQCAEERMAELMMIWERNKSVSPT</t>
+  </si>
+  <si>
+    <t>ATGTCGGGCCCTCGCGCCGGCTTCTACCGGCAGGAGCTGAACAAGACCGTGTGGGAGGTGCCGCAGCGGCTGCAGGGGCTGCGCCCGGTGGGCTCCGGCGCCTACGGCTCCGTCTGTTCGGCCTACGACGCCCGGCTGCGCCAGAAGGTGGCGGTGAAGAAGCTGTCGCGCCCCTTCCAGTCGCTGATCCACGCGCGCAGAACGTACCGGGAGCTGCGGCTGCTCAAGCACCTGAAGCACGAGAACGTCATCGGGCTTCTGGACGTCTTCACGCCGGCCACGTCCATCGAGGACTTCAGCGAAGTGTACTTGGTGACCACCCTGATGGGCGCCGACCTGAACAACATCGTCAAGTGCCAGGCGCTGAGCGACGAGCACGTTCAATTCCTGGTTTACCAGCTGCTGCGCGGGCTGAAGTACATCCACTCGGCCGGGATCATCCACCGGGACCTGAAGCCCAGCAACGTGGCTGTGAACGAGGACTGTGAGCTCAGGATCCTGGATTTCGGGCTGGCGCGCCAGGCGGACGAGGAGATGACCGGCTATGTGGCCACGCGCTGGTACCGGGCACCTGAGATCATGCTCAACTGGATGCATTACAACCAAACAGTGGATATCTGGTCCGTGGGCTGCATCATGGCTGAGCTGCTCCAGGGCAAGGCCCTCTTCCCGGGAAGCGACTACATTGACCAGCTGAAGCGCATCATGGAAGTGGTGGGCACACCCAGCCCTGAGGTTCTGGCAAAAATCTCCTCGGAACACGCCCGGACATATATCCAGTCCCTGCCCCCCATGCCCCAGAAGGACCTGAGCAGCATCTTCCGTGGAGCCAACCCCCTGGCCATAGACCTCCTTGGAAGGATGCTGGTGCTGGACAGTGACCAGAGGGTCAGTGCAGCTGAGGCACTGGCCCACGCCTACTTCAGCCAGTACCACGACCCCGAGGATGAGCCAGAGGCCGAGCCATATGATGAGAGCGTTGAGGCCAAGGAGCGCACGCTGGAGGAGTGGAAGGAGCTCACTTACCAGGAAGTCCTCAGCTTCAAGCCCCCAGAGCCACCGAAGCCACCTGGCAGCCTGGAGATTGAGCAG</t>
+  </si>
+  <si>
+    <t>E2AK2_HUMAN_D0_3UIU_A</t>
+  </si>
+  <si>
+    <t>MEKYEKIGKIGEGSYGVVFKCRNRDTGQIVAIKKFLESEDDPVIKKIALREIRMLKQLKHPNLVNLLEVFRRKRRLHLVFEYCDHTVLHELDRYQRGVPEHLVKSITWQTLQAVNFCHKHNCIHRDVKPENILITKHSVIKLCDFGFARLLTGPSDYYTDYVATRWYRSPELLVGDTQYGPPVDVWAIGCVFAELLSGVPLWPGKSDVDQLYLIRKTLGDLIPRHQQVFSTNQYFSGVKIPDPEDMEPLELKFPNISYPALGLL</t>
+  </si>
+  <si>
+    <t>GeneID</t>
+  </si>
+  <si>
+    <t>ATGGATGAGCAATCACAAGGAATGCAAGGGCCACCTGTTCCTCAGTTCCAACCACAGAAGGCCTTACGACCGGATATGGGCTATAATACATTAGCCAACTTTCGAATAGAAAAGAAAATTGGTCGCGGACAATTTAGTGAAGTTTATAGAGCAGCCTGTCTCTTGGATGGAGTACCAGTAGCTTTAAAAAAAGTGCAGATATTTGATTTAATGGATGCCAAAGCACGTGCTGATTGCATCAAAGAAATAGATCTTCTTAAGCAACTCAACCATCCAAATGTAATAAAATATTATGCATCATTCATTGAAGATAATGAACTAAACATAGTTTTGGAACTAGCAGATGCTGGCGACCTATCCAGAATGATCAAGCATTTTAAGAAGCAAAAGAGGCTAATTCCTGAAAGAACTGTTTGGAAGTATTTTGTTCAGCTTTGCAGTGCATTGGAACACATGCATTCTCGAAGAGTCATGCATAGAGATATAAAACCAGCTAATGTGTTCATTACAGCCACTGGGGTGGTAAAACTTGGAGATCTTGGGCTTGGCCGGTTTTTCAGCTCAAAAACCACAGCTGCACATTCTTTAGTTGGTACGCCTTATTACATGTCTCCAGAGAGAATACATGAAAATGGATACAACTTCAAATCTGACATCTGGTCTCTTGGCTGTCTACTATATGAGATGGCTGCATTACAAAGTCCTTTCTATGGTGACAAAATGAATTTATACTCACTGTGTAAGAAGATAGAACAGTGTGACTACCCACCTCTTCCTTCAGATCACTATTCAGAAGAACTCCGACAGTTAGTTAATATGTGCATCAACCCAGATCCAGAGAAGCGACCAGACGTCACCTATGTTTATGACGTAGCAAAGAGGATGCATGCATGCACTGCAAGCAGC</t>
+  </si>
+  <si>
+    <t>DAPK3_HUMAN_D0_2J90_A</t>
+  </si>
+  <si>
+    <t>GAAGACAGTTTGACTAAGCAGCCTGAAGAAGTTTTTGATGTATTAGAGAAGCTTGGAGAAGGGTCTTATGGAAGTGTATTTAAAGCAATACACAAGGAATCCGGTCAAGTTGTCGCAATTAAACAAGTACCTGTTGAATCAGATCTTCAGGAAATAATCAAAGAAATTTCCATAATGCAGCAATGTGACAGCCCATATGTTGTAAAGTACTATGGCAGTTATTTTAAGAATACAGACCTCTGGATTGTTATGGAGTACTGTGGCGCTGGCTCTGTCTCAGACATAATTAGATTACGAAACAAGACATTAATAGAAGATGAAATTGCAACCATTCTTAAATCTACATTGAAAGGACTAGAATATTTGCACTTTATGAGAAAAATACACAGAGATATAAAAGCTGGAAATATTCTCCTCAATACAGAAGGACATGCAAAATTGGCAGATTTTGGAGTGGCTGGTCAGTTAACAGATACAATGGCAAAACGCAATACTGTAATAGGAACTCCATTTTGGATGGCTCCTGAGGTGATTCAAGAAATAGGCTATAACTGTGTGGCCGACATCTGGTCCCTTGGCATTACTTCTATAGAAATGGCTGAAGGAAAACCTCCTTATGCTGATATACATCCAATGAGGGCTATTTTTATGATTCCCACAAATCCACCACCAACATTCAGAAAGCCAGAACTTTGGTCCGATGATTTCACCGATTTTGTTAAAAAGTGTTTGGTGAAGAATCCTGAGCAGAGAGCTACTGCAACACAACTTTTACAGCATCCTTTTATCAAGAATGCCAAACCTGTATCAATATTAAGAGACCTGATCACAGAAGCTATGGAGATCAAAGCTAAAAGACATGAGGAACAGCAACGAGAATTGGAAGAGGAAGAA</t>
+  </si>
+  <si>
+    <t>VKEFLAKAKEDFLKKWESPAQNTAHLDQFERIKTLGTGSFGRVMLVKHKETGNHYAMKILDKQKVVKLKQIEHTLNEKRILQAVNFPFLVKLEFSFKDNSNLYMVMEYVPGGEMFSHLRRIGRFSEPHARFYAAQIVLTFEYLHSLDLIYRDLKPENLLIDQQGYIQVTDFGFAKRVKGRTWTLCGTPEYLAPEIILSKGYNKAVDWWALGVLIYEMAAGYPPFFADQPIQIYEKIVSGKVRFPSHFSSDLKDLLRNLLQVDLTKRFGNLKNGVNDIKNHKWFATTDWIAIYQRKVEAPFIPKFKGPGDTSNFDDYEEEEIRVSINEKCGKEFSEF</t>
+  </si>
+  <si>
+    <t>TCCAGGGTGTCCCATGAACAGTTTCGGGCGGCCCTGCAGCTGGTGGTCAGCCCAGGAGACCCCAGGGAATACTTGGCCAACTTTATCAAAATCGGGGAAGGCTCAACCGGCATCGTATGCATCGCCACCGAGAAACACACAGGGAAACAAGTTGCAGTGAAGAAAATGGACCTCCGGAAGCAACAGAGACGAGAACTGCTTTTCAATGAGGTCGTGATCATGCGGGATTACCACCATGACAATGTGGTTGACATGTACAGCAGCTACCTTGTCGGCGATGAGCTCTGGGTGGTCATGGAGTTTCTAGAAGGTGGTGCCTTGACAGACATTGTGACTCACACCAGAATGAATGAAGAACAGATAGCTACTGTCTGCCTGTCAGTTCTGAGAGCTCTCTCCTACCTTCATAACCAAGGAGTGATTCACAGGGACATAAAAAGTGACTCCATCCTCCTGACAAGCGATGGCCGGATAAAGTTGTCTGATTTTGGTTTCTGTGCTCAAGTTTCCAAAGAGGTGCCGAAGAGGAAATCATTGGTTGGCACTCCCTACTGGATGGCCCCTGAGGTGATTTCTAGGCTACCTTATGGGACAGAGGTGGACATCTGGTCCCTCGGGATCATGGTGATAGAAATGATTGATGGCGAGCCCCCCTACTTCAATGAGCCTCCCCTCCAGGCGATGCGGAGGATCCGGGACAGTTTACCTCCAAGAGTGAAGGACCTACACAAGGTTTCTTCAGTGCTCCGGGGATTCCTAGACTTGATGTTGGTGAGGGAGCCCTCTCAGAGAGCAACAGCCCAGGAACTCCTCGGACATCCATTCTTAAAACTAGCAGGTCCACCGTCTTGCATTGTCCCCCTCATGAGACAATACAGGCATCAC</t>
+  </si>
+  <si>
+    <t>KRQWALEDFEIGRPLGKGKFGNVYLAREKQSKFILALKVLFKAQLEKAGVEHQLRREVEIQSHLRHPNILRLYGYFHDATRVYLILEYAPLGTVYRELQKLSKFDEQRTATYITELANALSYCHSKRVIHRDIKPENLLLGSAGELKIADFGWSVHAPSSRRTTLCGTLDYLPPEMIEGRMHDEKVDLWSLGVLCYEFLVGKPPFEANTYQETYKRISRVEFTFPDFVTEGARDLISRLLKHNPSQRPMLREVLEHPWITANSSKPS</t>
+  </si>
+  <si>
+    <t>SLK_HUMAN_D0_2JFL_A</t>
+  </si>
+  <si>
+    <t>SRVSHEQFRAALQLVVSPGDPREYLANFIKIGEGSTGIVCIATEKHTGKQVAVKKMDLRKQQRRELLFNEVVIMRDYHHDNVVDMYSSYLVGDELWVVMEFLEGGALTDIVTHTRMNEEQIATVCLSVLRALSYLHNQGVIHRDIKSDSILLTSDGRIKLSDFGFCAQVSKEVPKRKSLVGTPYWMAPEVISRLPYGTEVDIWSLGIMVIEMIDGEPPYFNEPPLQAMRRIRDSLPPRVKDLHKVSSVLRGFLDLMLVREPSQRATAQELLGHPFLKLAGPPSCIVPLMRQYRHH</t>
+  </si>
+  <si>
+    <t>TQTVHEFAKELDATNISIDKVVGAGEFGEVCSGRLKLPSKKEISVAIKTLKVGYTEKQRRDFLGEASIMGQFDHPNIIRLEGVVTKSKPVMIVTEYMENGSLDSFLRKHDAQFTVIQLVGMLRGIASGMKYLSDMGYVHRDLAARNILINSNLVCKVSDFGLSRVLEDDPEAAYTTRGGKIPIRWTSPEAIAYRKFTSASDVWSYGIVLWEVMSYGERPYWEMSNQDVIKAVDEGYRLPPPMDCPAALYQLMLDCWQKDRNNRPKFEQIVSILDKLIRNPGSLKIITSAAARPSNLLLDQSNVDITTFRTTGDWLNGVWTAHCKEIFTGVEYSSCDTIAKIS</t>
+  </si>
+  <si>
+    <t>QQFPQFHVKSGLQIKKNAIIDDYKVTSQVLGLGINGKVLQIFNKRTQEKFALKMLQDCPKARREVELHWRASQCPHIVRIVDVYENLYAGRKCLLIVMECLDGGELFSRIQDRGDQAFTEREASEIMKSIGEAIQYLHSINIAHRDVKPENLLYTSKRPNAILKLTDFGFAKETTSHNSLTTPCYTPYYVAPEVLGPEKYDKSCDMWSLGVIMYILLCGYPPFYSNHGLAISPGMKTRIRMGQYEFPNPEWSEVSEEVKMLIRNLLKTEPTQRMTITEFMNHPWIMQSTKVPQTPLHTSRVLKEDKERWEDVKGCLHDKNSDQA</t>
+  </si>
+  <si>
+    <t>CSK21_HUMAN_D0_3AXW_A</t>
+  </si>
+  <si>
+    <t>ATCTRFTDDYQLFEELGKGAFSVVRRCVKKTPTQEYAAKIINTKKLSARDHQKLEREARICRLLKHPNIVRLHDSISEEGFHYLVFDLVTGGELFEDIVAREYYSEADASHCIHQILESVNHIHQHDIVHRDLKPENLLLASKCKGAAVKLADFGLAIEVQGEQQAWFGFAGTPGYLSPEVLRKDPYGKPVDIWACGVILYILLVGYPPFWDEDQHKLYQQIKAGAYDFPSPEWDTVTPEAKNLINQMLTINPAKRITADQALKHPWVCQRSTVASMMHRQETVECLRKFNARRKLKGAILTTMLVSRNFS</t>
+  </si>
+  <si>
+    <t>VIDPSELTFVQEIGSGQFGLVHLGYWLNKDKVAIKTIREGAMSEEDFIEEAEVMMKLSHPKLVQLYGVCLEQAPICLVFEFMEHGCLSDYLRTQRGLFAAETLLGMCLDVCEGMAYLEEACVIHRDLAARNCLVGENQVIKVSDFGMTRFVLDDQYTSSTGTKFPVKWASPEVFSFSRYSSKSDVWSFGVLMWEVFSEGKIPYENRSNSEVVEDISTGFRLYKPRLASTHVYQIMNHCWKERPEDRPAFSRLLRQLAEIAESGL</t>
+  </si>
+  <si>
+    <t>CGTGTAAAAGCAGCTCAAGCTGGAAGACAGAGCTCTGCAAAGAGACATCTTGCAGAACAATTTGCAGTTGGAGAGATAATAACTGACATGGCAAAAAAGGAATGGAAAGTAGGATTACCCATTGGCCAAGGAGGCTTTGGCTGTATATATCTTGCTGATATGAATTCTTCAGAGTCAGTTGGCAGTGATGCACCTTGTGTTGTAAAAGTGGAACCCAGTGACAATGGACCTCTTTTTACTGAATTAAAGTTCTACCAACGAGCTGCAAAACCAGAGCAAATTCAGAAATGGATTCGTACCCGTAAGCTGAAGTACCTGGGTGTTCCTAAGTATTGGGGGTCTGGTCTACATGACAAAAATGGAAAAAGTTACAGGTTTATGATAATGGATCGCTTTGGGAGTGACCTTCAGAAAATATATGAAGCAAATGCCAAAAGGTTTTCTCGGAAAACTGTCTTGCAGCTAAGCTTAAGAATTCTGGATATTCTGGAATATATTCACGAGCATGAGTATGTGCATGGAGATATCAAGGCCTCAAATCTTCTTCTGAACTACAAGAATCCTGACCAGGTGTACTTGGTAGATTATGGCCTTGCTTATCGGTACTGCCCAGAAGGAGTTCATAAAGAATACAAAGAAGACCCCAAAAGATGTCACGATGGCACTATTGAATTCACGAGCATCGATGCACACAATGGCGTGGCCCCATCAAGACGTGGTGATTTGGAAATACTTGGTTATTGCATGATCCAATGGCTTACTGGCCATCTTCCTTGGGAGGATAATTTGAAAGATCCTAAATATGTTAGAGATTCCAAAATTAGATACAGAGAAAATATTGCAAGTTTGATGGACAAATGTTTTCCTGAGAAAAACAAACCAGGTGAAATTGCCAAATACATGGAAACAGTGAAATTACTAGACTACACTGAAAAACCTCTTTATGAAAATTTACGTGACATTCTTTTGCAAGGACTAAAAGCTATAGGAAGTAAGGATGATGGCAAATTGGACCTCAGTGTTGTGGAGAATGGAGGTTTGAAAGCAAAAACAATAACAAAGAAGCGAAAGAAAGAAATTGAAGAA</t>
+  </si>
+  <si>
+    <t>MP2K6_HUMAN_D0_3VN9_A</t>
+  </si>
+  <si>
+    <t>RVKAAQAGRQSSAKRHLAEQFAVGEIITDMAKKEWKVGLPIGQGGFGCIYLADMNSSESVGSDAPCVVKVEPSDNGPLFTELKFYQRAAKPEQIQKWIRTRKLKYLGVPKYWGSGLHDKNGKSYRFMIMDRFGSDLQKIYEANAKRFSRKTVLQLSLRILDILEYIHEHEYVHGDIKASNLLLNYKNPDQVYLVDYGLAYRYCPEGVHKEYKEDPKRCHDGTIEFTSIDAHNGVAPSRRGDLEILGYCMIQWLTGHLPWEDNLKDPKYVRDSKIRYRENIASLMDKCFPEKNKPGEIAKYMETVKLLDYTEKPLYENLRDILLQGLKAIGSKDDGKLDLSVVENGGLKAKTITKKRKKEIEE</t>
+  </si>
+  <si>
+    <t>MKNK1_HUMAN_D0_2HW6_B</t>
+  </si>
+  <si>
+    <t>MSLIRKKGFYKQDVNKTAWELPKTYVSPTHVGSGAYGSVCSAIDKRSGEKVAIKKLSRPFQSEIFAKRAYRELLLLKHMQHENVIGLLDVFTPASSLRNFYDFYLVMPFMQTDLQKIMGMEFSEEKIQYLVYQMLKGLKYIHSAGVVHRDLKPGNLAVNEDCELKILDFGLARHADAEMTGYVVTRWYRAPEVILSWMHYNQTVDIWSVVCIMAEMLTGKTLFKGKDYLDQLTQILKVTGVPGTEFVQKLNDKAAKSYIQSLPQTPRKDFTQLFPRASPQAADLLEKMLELDVDKRLTAAQALTHPFFEPFRDPEEETEAQQPFDDSLEHEKLTVDEWKQHIYKEIVNFSPI</t>
+  </si>
+  <si>
+    <t>DEQPHIGNYRLLKTIGKGNFAKVKLARHILTGREVAIKIIDKTQLNPTSLQKLFREVRIMKILNHPNIVKLFEVIETEKTLYLIMEYASGGEVFDYLVAHGRMKEKEARSKFRQIVSAVQYCHQKRIVHRDLKAENLLLDADMNIKIADFGFSNEFTVGGKLDTFCGSPPYAAPELFQGKKYDGPEVDVWSLGVILYTLVSGSLPFDGQNLKELRERVLRGKYRIPFYMSTDCENLLKRFLVLNPIKRGTLEQIMKDRWINAGHEEDELKPFVEPELDISDQKRIDIMVGMGYSQEEIQESLSKMKYDEITATYLLLGRKSSE</t>
+  </si>
+  <si>
+    <t>ITK_HUMAN_D0_3QGW_B</t>
+  </si>
+  <si>
+    <t>KS6A3_HUMAN_D1_4JG7_A</t>
+  </si>
+  <si>
+    <t>KCC4_HUMAN_D0_2W4O_A</t>
+  </si>
+  <si>
+    <t>CSK_HUMAN_D0_3D7T_A</t>
+  </si>
+  <si>
+    <t>KCC2A_HUMAN_D0_2VZ6_B</t>
+  </si>
+  <si>
+    <t>ATGTCTGATGAGGAGATCTTGGAGAAATTACGAAGCATAGTGAGTGTGGGCGATCCTAAGAAGAAATATACACGGTTTGAGAAGATTGGACAAGGTGCTTCAGGCACCGTGTACACAGCAATGGATGTGGCCACAGGACAGGAGGTGGCCATTAAGCAGATGAATCTTCAGCAGCAGCCCAAGAAAGAGCTGATTATTAATGAGATCCTGGTCATGAGGGAAAACAAGAACCCAAACATTGTGAATTACTTGGACAGTTACCTCGTGGGAGATGAGCTGTGGGTTGTTATGGAATACTTGGCTGGAGGCTCCTTGACAGATGTGGTGACAGAAACTTGCATGGATGAAGGCCAAATTGCAGCTGTGTGCCGTGAGTGTCTGCAGGCTCTGGAGTTCTTGCATTCGAACCAGGTCATTCACAGAGACATCAAGAGTGACAATATTCTGTTGGGAATGGATGGCTCTGTCAAGCTAACTGACTTTGGATTCTGTGCACAGATAACCCCAGAGCAGAGCAAACGGAGCACCATGGTAGGAACCCCATACTGGATGGCACCAGAGGTTGTGACACGAAAGGCCTATGGGCCCAAGGTTGACATCTGGTCCCTGGGCATCAAGGCCATCGAAATGATTGAAGGGGAGCCTCCATACCTCAATGAAAACCCTCTGAGAGCCTTGTACCTCATTGCCACCAATGGGACCCCAGAACTTCAGAACCCAGAGAAGCTGTCAGCTATCTTCCGGGACTTTCTGAACCGCTGTCTCGAGATGGATGTGGAGAAGAGAGGTTCAGCTAAAGAGCTGCTACAGCATCAATTCCTGAAGATTGCCAAGCCCCTCTCCAGCCTCACTCCACTTATTGCTGCAGCTAAGGAGGCAACAAAGAACAATCAC</t>
+  </si>
+  <si>
+    <t>AVPFVEDWDLVQTLGEGAYGEVQLAVNRVTEEAVAVKIVDMKRAVDCPENIKKEICINKMLNHENVVKFYGHRREGNIQYLFLEYCSGGELFDRIEPDIGMPEPDAQRFFHQLMAGVVYLHGIGITHRDIKPENLLLDERDNLKISDFGLATVFRYNNRERLLNKMCGTLPYVAPELLKRREFHAEPVDVWSCGIVLTAMLAGELPWDQPSDSCQEYSDWKEKKTYLNPWKKIDSAPLALLHKILVENPSARITIPDIKKDRWYNKPL</t>
+  </si>
+  <si>
+    <t>GCCACCTGCACACGTTTCACCGACGACTACCAGCTCTTCGAGGAGCTTGGCAAGGGTGCTTTCTCTGTGGTCCGCAGGTGTGTGAAGAAAACCCCCACGCAGGAGTACGCAGCAAAAATCATCAATACCAAGAAATTGTCTGCCCGGGATCACCAGAAACTAGAACGTGAGGCTCGGATATGTCGACTTCTGAAACATCCAAACATCGTGCGCCTCCATGACAGTATTTCTGAAGAAGGGTTTCACTACCTCGTGTTTGACCTTGTTACCGGCGGGGAGCTGTTTGAAGACATTGTGGCCAGAGAGTACTACAGTGAAGCAGATGCCAGCCACTGTATACATCAGATTCTGGAGAGTGTTAACCACATCCACCAGCATGACATCGTCCACAGGGACCTGAAGCCTGAGAACCTGCTGCTGGCGAGTAAATGCAAGGGTGCCGCCGTCAAGCTGGCTGATTTTGGCCTAGCCATCGAAGTACAGGGAGAGCAGCAGGCTTGGTTTGGTTTTGCTGGCACCCCAGGTTACTTGTCCCCTGAGGTCTTGAGGAAAGATCCCTATGGAAAACCTGTGGATATCTGGGCCTGCGGGGTCATCCTGTATATCCTCCTGGTGGGCTATCCTCCCTTCTGGGATGAGGATCAGCACAAGCTGTATCAGCAGATCAAGGCTGGAGCCTATGATTTCCCATCACCAGAATGGGACACGGTAACTCCTGAAGCCAAGAACTTGATCAACCAGATGCTGACCATAAACCCAGCAAAGCGCATCACGGCTGACCAGGCTCTCAAGCACCCGTGGGTCTGTCAACGATCCACGGTGGCATCCATGATGCATCGTCAGGAGACTGTGGAGTGTTTGCGCAAGTTCAATGCCCGGAGAAAACTGAAGGGTGCCATCCTCACGACCATGCTTGTCTCCAGGAACTTCTCA</t>
+  </si>
+  <si>
+    <t>GAGACCTACATTAAGCTGGACAAACTGGGCGAGGGTACCTATGCCACCGTCTACAAAGGCAAAAGCAAGCTCACAGACAACCTTGTGGCACTCAAGGAGATCAGACTGGAACATGAAGAGGGGGCACCCTGCACCGCCATCCGGGAAGTGTCCCTACTCAAGGACCTCAAACACGCCAACATCGTTACGCTACATGACATTATCCACACGGAGAAGTCCCTCACCCTTGTCTTTGAGTACCTGGACAAGGACCTGAAGCAGTACCTGGATGACTGTGGGAACATCATCAACATGCACAACGTGAAACTGTTCCTGTTCCAGCTGCTCCGTGGCCTGGCCTACTGCCACCGGCAGAAGGTGCTACACCGAGACCTCAAGCCCCAGAACCTGCTCATCAACGAGAGGGGAGAGCTCAAGCTGGCTGACTTTGGCCTGGCCCGAGCCAAGTCAATCCCAACAAAGACATACTCCAATGAGGTGGTGACACTGTGGTACCGGCCCCCTGACATCCTGCTTGGGTCCACGGACTACTCCACTCAGATTGACATGTGGGGTGTGGGCTGCATCTTCTATGAGATGGCCACAGGCCGTCCCCTCTTTCCGGGCTCCACGGTGGAGGAACAGCTACACTTCATCTTCCGTATCTTAGGAACCCCAACTGAGGAGACGTGGCCAGGCATCCTGTCCAACGAGGAGTTCAAGACATACAACTACCCCAAGTACCGAGCCGAGGCCCTTTTGAGCCACGCACCCCGACTTGATAGCGACGGGGCCGACCTCCTCACCAAGCTGTTGCAGTTTGAGGGTCGAAATCGGATCTCCGCAGAGGATGCCATGAAACATCCATTCTTCCTCAGTCTGGGGGAGCGGATCCACAAACTTCCTGACACTACTTCCATATTTGCACTAAAGGAGATTCAGCTACAAAAGGAGGCCAGCCTTCGGTCT</t>
+  </si>
+  <si>
+    <t>MK13_HUMAN_D0_4EYJ_A</t>
+  </si>
+  <si>
+    <t>STK16_HUMAN_D0_2BUJ_B</t>
+  </si>
+  <si>
     <t>AAGCACGACGGGCGGGTGAAGATCGGACACTACGTGCTGGGCGACACGCTGGGCGTCGGCACCTTCGGCAAAGTGAAGATTGGAGAACATCAATTAACAGGCCATAAAGTGGCAGTTAAAATCTTAAATAGACAGAAGATTCGCAGTTTAGATGTTGTTGGAAAAATAAAACGAGAAATTCAAAATCTAAAACTCTTTCGTCATCCTCATATTATCAAACTATACCAGGTGATCAGCACTCCAACAGATTTTTTTATGGTAATGGAATATGTGTCTGGAGGTGAATTATTTGACTACATCTGTAAGCATGGACGGGTTGAAGAGATGGAAGCCAGGCGRCTCTTTCAGCAGATTCTGTCTGCTGTGGATTACTGTCATAGGCATATGGTTGTTCATCGAGACCTGAAACCAGAGAATGTCCTGTTGGATGCACACATGAATGCCAAGATAGCCGATTTCGGATTATCTAATATGATGTCAGATGGTGAATTTCTGAGAACTAGTTGCGGATCTCCAAATTATGCAGCACCTGAAGTCATCTCAGGCAGATTGTATGCAGGTCCTGAAGTTGATATCTGGAGCTGTGGTGTTATCTTGTATGCTCTTCTTTGTGGCACCCTCCCATTTGATGATGAGCATGTACCTACGTTATTTAAGAAGATCCGAGGGGGTGTCTTTTATATCCCAGAATATCTCAATCGTTCTGTCGCCACTCTCCTGATGCATATGCTGCAGGTTGACCCACTGAAACGAGCAACTATCAAAGACATAAGAGAGCATGAATGGTTTAAACAAGATTTGCCCAGTTACTTATTTCCTGAA</t>
   </si>
   <si>
-    <t>CSKP_HUMAN_D0_3TAC_A</t>
-  </si>
-  <si>
-    <t>MST4_HUMAN_D0_4FZD_B</t>
-  </si>
-  <si>
-    <t>CGGGACTCGAGTGATGATTGGGAGATTCCTGATGGGCAGATTACAGTGGGACAAAGAATTGGATCTGGATCATTTGGAACAGTCTACAAGGGAAAGTGGCATGGTGATGTGGCAGTGAAAATGTTGAATGTGACAGCACCTACACCTCAGCAGTTACAAGCCTTCAAAAATGAAGTAGGAGTACTCAGGAAAACACGACATGTGAATATCCTACTCTTCATGGGCTATTCCACAAAGCCACAACTGGCTATTGTTACCCAGTGGTGTGAGGGCTCCAGCTTGTATCACCATCTCCATATCATTGAGACCAAATTTGAGATGATCAAgCTTATAGATATTGCACGACAGACTGCACAGGGCATGGATTACTTACACGCCAAGTCAATCATCCACAGAGACCTCAAGAGTAATAATATATTTCTTCATGAAGACCTCACAGTAAAAATAGGTGATTTTGGTCTAGCTACAGTGAAATCTCGATGGAGTGGGTCCCATCAGTTTGAACAGTTGTCTGGgTCCATTTTGTGGATGGCACCAGAAGTCATCAGAATGCAAGATAAAAATCCATACAGCTTTCAGTCAGATGTATATGCATTTGGgATTGTTCTGTATGAATTGATGACTGGACAGTTACCTTATTCAAACATCAACAACAGGGACCAGATAATTTTTATGGTGGGACGAGGATACCTGTCTCCAGATCTCAGTAAGGTACGGAGTAACTGTCCAAAAGCCATGAAGAGATTAATGGCAGAGTGCCTCAAAAAGAAAAGAGATGAGAGACCACTCTTTCCCCAAATTCTCGCC</t>
-  </si>
-  <si>
-    <t>MARK2_HUMAN_D0_3IEC_D</t>
-  </si>
-  <si>
-    <t>CCATTTCCAGAAGGCAAGGTTCTGGATGATATGGAAGGCAATCAGTGGGTACTGGGCAAGAAGATTGGCTCTGGAGGATTTGGATTGATATATTTAGCTTTCCCCACAAATAAACCAGAGAAAGATGCAAGACATGTAGTAAAAGTGGAATATCAAGAAAATGGCCCGTTATTTTCAGAACTTAAATTTTATCAGAGAGTTGCAAAAAAAGACTGTATCAAAAAGTGGATAGAACGCAAACAACTTGATTATTTAGGAATTCCTCTGTTTTATGGATCTGGTCTGACTGAATTCAAGGGAAGAAGTTACAGATTTATGGTAATGGAAAGACTAGGAATAGATTTACAGAAGATCTCAGGCCAGAATGGTACCTTTAAAAAGTCAACTGTCCTGCAATTAGGTATCCGAATGTTGGATGTACTGGAATATATACATGAAAATGAATATGTTCATGGTGATATAAAAGCAGCAAATCTACTTTTGGGTTACAAAAATCCAGACCAGGTTTATCTTGCAGATTATGGACTTTCCTACAGATATTGTCCCAATGGGAACCACAAACAGTATCAGGAAAATCCTAGAAAAGGCCATAATGGGACAATAGAGTTTACCAGCTTGGATGCCCACAAGGGAGTAGCCTTGTCCAGACGAAGTGACGTTGAGATCCTCGGCTACTGCATGCTGCGGTGGTTGTGTGGGAAACTTCCCTGGGAACAGAACCTGAAGGACCCTGTGGCTGTGCAGACTGCTAAAACAAATCTGTTGGACGAGCTCCCCCAGTCAGTGCTTAAATGGGCTCCTTCTGGAAGCAGTTGCTGTGAAATAGCCCAATTTTTGGTATGTGCTCATAGTTTAGCATATGATGAAAAGCCAAACTATCAAGCCCTCAAGAAAATTTTGAACCCTCATGGAATACCTTTAGGACCACTGGACTTTTCCACAAAAGGACAGAGTATAAATGTCCAT</t>
-  </si>
-  <si>
-    <t>GGGGACTCTGATATATCCAGTCCATTACTGCAAAATACTGTCCACATTGACCTCAGTGCTCTAAATCCAGAGCTGGTCCAGGCAGTGCAGCATGTAGTGATTGGGCCCAGTAGCCTGATTGTGCATTTCAATGAAGTCATAGGAAGAGGGCATTTTGGTTGTGTATATCATGGGACTTTGTTGGACAATGATGGCAAGAAAATTCACTGTGCTGTGAAATCCTTGAACAGAATCACTGACATAGGAGAAGTTTCCCAATTTCTGACCGAGGGAATCATCATGAAAGATTTTAGTCATCCCAATGTCCTCTCGCTCCTGGGAATCTGCCTGCGAAGTGAAGGGTCTCCGCTGGTGGTCCTACCATACATGAAACATGGAGATCTTCGAAATTTCATTCGAAATGAGACTCATAATCCAACTGTAAAAGATCTTATTGGCTTTGGTCTTCAAGTAGCCAAAGGCATGAAATATCTTGCAAGCAAAAAGTTTGTCCACAGAGACTTGGCTGCAAGAAACTGTATGCTGGATGAAAAATTCACAGTCAAGGTTGCTGATTTTGGTCTTGCCAGAGACATGTATGATAAAGAATACTATAGTGTACACAACAAAACAGGTGCAAAGCTGCCAGTGAAGTGGATGGCTTTGGAAAGTCTGCAAACTCAAAAGTTTACCACCAAGTCAGATGTGTGGTCCTTTGGCGTGCTCCTCTGGGAGCTGATGACAAGAGGAGCCCCACCTTATCCTGACGTAAACACCTTTGATATAACTGTTTACTTGTTGCAAGGGAGAAGACTCCTACAACCCGAATACTGCCCAGACCCCTTATATGAAGTAATGCTAAAATGCTGGCACCCTAAAGCCGAAATGCGCCCATCCTTTTCTGAACTGGTGTCCCGGATATCAGCGATCTTCTCTACTTTCATTGGG</t>
-  </si>
-  <si>
-    <t>YQLFEELGKGAFSVVRRCVKVLAGQEYAAKIINTKKLSARDHQKLEREARICRLLKHPNIVRLHDSISEEGHHYLIFDLVTGGELFEDIVAREYYSEADASHCIQQILEAVLHCHQMGVVHRDLKPENLLLASKLKGAAVKLADFGLAIEVEGEQQAWFGFAGTPGYLSPEVLRKDPYGKPVDLWACGVILYILLVGYPPFWDEDQHRLYLQIKAGAYDFPSPEWDTVTPEAKDLINKMLTINPSKRITAAEALKHPWISHRSTVASCMHRQETVDCLKKFNARRKLKGA</t>
-  </si>
-  <si>
-    <t>ENFQKVEKIGEGTYGVVYKARNKLTGEVVALKKIRLDTETEGVPSTAIREISLLKELNHPNIVKLLDVIHTENKLYLVFEFLHQDLKKFMDASALTGIPLPLIKSYLFQLLQGLAFCHSHRVLHRDLKPQNLLINTEGAIKLADFGLARAFGVPVRTYTHEVVTLWYRAPEILLGCKYYSTAVDIWSLGCIFAEMVTRRALFPGDSEIDQLFRIFRTLGTPDEVVWPGVTSMPDYKPSFPKWARQDFSKVVPPLDEDGRSLLSQMLHYDPNKRISAKAALAHPFFQDVTKPVPHL</t>
-  </si>
-  <si>
-    <t>TTK_HUMAN_D0_3H9F_A</t>
-  </si>
-  <si>
-    <t>SVKGRIYSILKQIGSGGSSKVFQVLNEKKQIYAIKYVNLEEADNQTLDSYRNEIAYLNKLQQHSDKIIRLYDYEITDQYIYMVMECGNIDLNSWLKKKKSIDPWERKSYWKNMLEAVHTIHQHGIVHSDLKPANFLIVDGMLKLIDFGIANQMQPDTTSVVKDSQVGTVNYMPPEAIKDMSSSRENGKSKSKISPKSDVWSLGCILYYMTYGKTPFQQIINQISKLHAIIDPNHEIEFPDIPEKDLQDVLKCCLKRDPKQRISIPELLAHPYVQIQTHPVNQMAKGTTEE</t>
-  </si>
-  <si>
-    <t>GTGAAAGAATTCTTAGCCAAAGCCAAAGAAGATTTTCTTAAAAAATGGGAAAGTCCCGCTCAGAACACAGCCCACTTGGATCAGTTTGAACGAATCAAGACCCTCGGCACGGGCTCCTTCGGGCGGGTGATGCTGGTGAAACACAAGGAGACCGGGAACCACTATGCCATGAAGATCCTCGACAAACAGAAGGTGGTGAAACTGAAACAGATCGAACACACCCTGAATGAAAAGCGCATCCTGCAAGCTGTCAACTTTCCGTTCCTCGTCAAACTCGAGTTCTCCTTCAAGGACAACTCAAACTTATACATGGTCATGGAGTACGTGCCCGGCGGGGAGATGTTCTCACACCTACGGCGGATCGGAAGGTTCAGTGAGCCCCATGCCCGTTTCTACGCGGCCCAGATCGTCCTGACCTTTGAGTATCTGCACTCGCTGGATCTCATCTACAGGGACCTGAAGCCGGAGAATCTGCTCATTGACCAGCAGGGCTACATTCAGGTGACAGACTTCGGTTTCGCCAAGCGCGTGAAGGGCCGCACTTGGACCTTGTGCGGCACCCCTGAGTACCTGGCCCCTGAGATTATCCTGAGCAAAGGCTACAACAAGGCCGTGGACTGGTGGGCCCTGGGGGTTCTTATCTATGAAATGGCCGCTGGCTACCCGCCCTTCTTCGCAGACCAGCCCATCCAGATCTATGAGAAGATCGTCTCTGGGAAGGTGCGCTTCCCTTCCCACTTCAGCTCTGACTTGAAGGACCTGCTGCGGAACCTCCTGCAGGTAGATCTCACCAAGCGCTTTGGGAACCTCAAGAATGGGGTCAACGATATCAAGAACCACAAGTGGTTTGCCACAACTGACTGGATTGCCATCTACCAGAGGAAGGTGGAAGCTCCCTTCATACCAAAGTTTAAAGGCCCTGGGGATACGAGTAACTTTGACGACTATGAGGAAGAAGAAATCCGGGTCTCCATCAATGAGAAGTGTGGCAAGGAGTTTTCTGAGTTT</t>
-  </si>
-  <si>
-    <t>TCCCCCAACTACGACAAGTGGGAGATGGAACGCACGGACATCACCATGAAGCACAAGCTGGGCGGGGGCCAGTACGGGGAGGTGTACGAGGGCGTGTGGAAGAAATACAGCCTGACGGTGGCCGTGAAGACCTTGAAGGAGGACACCATGGAGGTGGAAGAGTTCTTGAAAGAAGCTGCAGTCATGAAAGAGATCAAACACCCTAACCTGGTGCAGCTCCTTGGGGTCTGCACCCGGGAGCCCCCGTTCTATATCATCACTGAGTTCATGACCTACGGGAACCTCCTGGACTACCTGAGGGAGTGCAACCGGCAGGAGGTGAACGCCGTGGTGCTGCTGTACATGGCCACTCAGATCTCGTCAGCCATGGAGTACCTGGAGAAGAAAAACTTCATCCACAGAGATCTTGCTGCCCGAAACTGCCTGGTAGGGGAGAACCACTTGGTGAAGGTAGCTGATTTTGGCCTGAGCAGGTTGATGACAGGGGACACCTACACAGCCCATGCTGGAGCCAAGTTCCCCATCAAATGGACTGCACCCGAGAGCCTGGCCTACAACAAGTTCTCCATCAAGTCCGACGTCTGGGCATTTGGAGTATTGCTTTGGGAAATTGCTACCTATGGCATGTCCCCTTACCCGGGAATTGACCTGTCCCAGGTGTATGAGCTGCTAGAGAAGGACTACCGCATGGAGCGCCCAGAAGGCTGCCCAGAGAAGGTCTATGAACTCATGCGAGCATGTTGGCAGTGGAATCCCTCTGACCGGCCCTCCTTTGCTGAAATCCACCAAGCCTTTGAAACAATGTTCCAGGAATCCAGTATCTCAGACGAAGTGGAAAAGGAGCTGGGGAAA</t>
-  </si>
-  <si>
-    <t>RDSSDDWEIPDGQITVGQRIGSGSFGTVYKGKWHGDVAVKMLNVTAPTPQQLQAFKNEVGVLRKTRHVNILLFMGYSTKPQLAIVTQWCEGSSLYHHLHIIETKFEMIKLIDIARQTAQGMDYLHAKSIIHRDLKSNNIFLHEDLTVKIGDFGLATVKSRWSGSHQFEQLSGSILWMAPEVIRMQDKNPYSFQSDVYAFGIVLYELMTGQLPYSNINNRDQIIFMVGRGYLSPDLSKVRSNCPKAMKRLMAECLKKKRDERPLFPQILA</t>
-  </si>
-  <si>
-    <t>KS6A1_HUMAN_D1_3RNY_B</t>
+    <t>ATGGAAAGCGACCTGCACCAGATCATCCACTCCTCACAGCCCCTCACACTGGAACACGTGCGCTACTTCCTGTACCAACTGCTGCGGGGCCTGAAGTACATGCACTCGGCTCAGGTCATCCACCGTGACCTGAAGCCCTCCAACCTATTGGTGAATGAGAACTGTGAGCTCAAGATTGGTGACTTTGGTATGGCTCGTGGCCTGTGCACCTCGCCCGCTGAACATCAGTACTTCATGACTGAGTATGTGGCCACGCGCTGGTACCGTGCGCCCGAGCTCATGCTCTCTTTGCATGAGTATACACAGGCTATTGACCTCTGGTCTGTGGGCTGCATCTTTGGTGAGATGCTGGCCCGGCGCCAGCTCTTCCCAGGCAAAAACTATGTACACCAGCTACAGCTCATCATGATGGTGCTGGGTACCCCATCACCAGCCGTGATTCAGGCTGTGGGGGCTGAGAGGGTGCGGGCCTATATCCAGAGCTTGCCACCACGCCAGCCTGTGCCCTGGGAGACAGTGTACCCAGGTGCCGACCGCCAGGCCCTATCACTGCTGGGTCGCATGCTGCGTTTTGAGCCCAGCGCTCGCATCTCAGCAGCTGCTGCCCTTCGCCACCCTTTCCTGGCCAAGTACCATGATCCTGATGATGAGCCTGACTGTGCCCCGCCCTTTGACTTTGCCTTTGACCGCGAAGCCCTCACTCGGGAGCGCATTAAGGAGGCCATTGTGGCTGAAATTGAGGACTTCCATGCAAGGCGTGAGGGCATCCGCCAACAGATCCGCTTCCAGCCTTCTCTACAGCCTGTGGCTAGTGAGCCTGGCTGTCCAGATGTTGAAATGCCCAGTCCCTGGGCTCCCAGTGGGGACTGTGCCATG</t>
+  </si>
+  <si>
+    <t>CAGAGCAGTAAGCGCAGCAGCCGGAGTGTGGAAGATGACAAGGAGGGTCACCTGGTGTGCCGGATCGGCGATTGGCTCCAAGAGCGATATGAGATTGTGGGGAACCTGGGTGAAGGCACCTTTGGCAAGGTGGTGGAGTGCTTGGACCATGCCAGAGGGAAGTCTCAGGTTGCCCTGAAGATCATCCGCAACGTGGGCAAGTACCGGGAGGCTGCCCGGCTAGAAATCAACGTGCTCAAAAAAATCAAGGAGAAGGACAAAGAAAACAAGTTCCTGTGTGTCTTGATGTCTGACTGGTTCAACTTCCACGGTCACATGTGCATCGCCTTTGAGCTCCTGGGCAAGAACACCTTTGAGTTCCTGAAGGAGAATAACTTCCAGCCTTACCCCCTACCACATGTCCGGCACATGGCCTACCAGCTCTGCCACGCCCTTAGATTTCTGCATGAGAATCAGCTGACCCATACAGACTTGAAACCAGAGAACATCCTGTTTGTGAATTCTGAGTTTGAAACCCTCTACAATGAGCACAAGAGCTGTGAGGAGAAGTCAGTGAAGAACACCAGCATCCGAGTGGCTGACTTTGGCAGTGCCACATTTGACCATGAGCACCACACCACCATTGTGGCCACCCGTCACTATCGCCCGCCTGAGGTGATCCTTGAGCTGGGCTGGGCACAGCCCTGTGACGTCTGGAGCATTGGCTGCATTCTCTTTGAGTACTACCGGGGCTTCACACTCTTCCAGACCCACGAAAACCGAGAGCACCTGGTGATGATGGAGAAGATCCTAGGGCCCATCCCATCACACATGATCCACCGTACCAGGAAGCAGAAATATTTCTACAAAGGGGGCCTAGTTTGGGATGAGAACAGCTCTGACGGCCGGTATGTGAAGGAGAACTGCAAACCTCTGAAGAGTTACATGCTCCAAGACTCCCTGGAGCACGTGCAGCTGTTTGACCTGATGAGGAGGATGTTAGAATTTGACCCTGCCCAGCGCATCACACTGGCCGAGGCCCTGCTGCACCCCTTCTTTGCTGGCCTGACCCCTGAGGAGCGGTCCTTCCACACC</t>
+  </si>
+  <si>
+    <t>GAACTGAAGGATGACGACTTTGAGAAGATCAGTGAGCTGGGGGCTGGCAATGGCGGTGTGGTGTTCAAGGTCTCCCACAAGCCTTCTGGCCTGGTCATGGCCAGAAAGCTAATTCATCTGGAGATCAAACCCGCAATCCGGAACCAGATCATAAGGGAGCTGCAGGTTCTGCATGAGTGCAACTCTCCGTACATCGTGGGCTTCTATGGTGCGTTCTACAGCGATGGCGAGATCAGTATCTGCATGGAGCACATGGATGGAGGTTCTCTGGATCAAGTCCTGAAGAAAGCTGGAAGAATTCCTGAACAAATTTTAGGAAAAGTTAGCATTGCTGTAATAAAAGGCCTGACATATCTGAGGGAGAAGCACAAGATCATGCACAGAGCATACGGAATGGACAGCCGACCTCCCATGGCAATTTTTGAGTTGTTGGATTACATAGTCAACGAGCCTCCTCCAAAACTGCCCAGTGGAGTGTTCAGTCTGGAATTTCAAGATTTTGTGAATAAATGCTTAATAAAAAACCCCGCAGAGAGAGCAGATTTGAAGCAACTCATGGTTCATGCTTTTATCAAGAGATCTGATGCTGAGGAAGTGGATTTTGCAGGTTGGCTCTGCTCCACCATCGGCCTTAAC</t>
+  </si>
+  <si>
+    <t>MQTVGVHSIVQQLHRNSIQFTDGYEVKEDIGVGSYSVCKRCIHKATNMEFAVKIIDKSKRDPTEEIEILLRYGQHPNIITLKDVYDDGKYVYVVTELMKGGELLDKILRQKFFSEREASAVLFTITKTVEYLHAQGVVHRDLKPSNILYVDESGNPESIRICDFGFAKQLRAENGLLMTPCYTANFVAPEVLKRQGYDAACDIWSLGVLLYTMLTGYTPFANGPDDTPEEILARIGSGKFSLSGGYWNSVSDTAKDLVSKMLHVDPHQRLTAALVLRHPWIVHWDQLPQYQLNRQDAPHLVKGAMAATYSALNRNQSPVLEPVGRSTLAQRRGIKKITSTAL</t>
+  </si>
+  <si>
+    <t>MSSFLPEGGCYELLTVIGKGFEDLMTVNLARYKPTGEYVTVRRINLEACSNEMVTFLQGELHVSKLFNHPNIVPYRATFIADNELWVVTSFMAYGSAKDLICTHFMDGMNELAIAYILQGVLKALDYIHHMGYVHRSVKASHILISVDGKVYLSGLRSNLSMISHGQRQRVVHDFPKYSVKVLPWLSPEVLQQNLQGYDAKSDIYSVGITACELANGHVPFKDMPATQMLLEKLNGTVPCLLDTSTIPAEELTMSPSRSVANSGLSDSLTTSTPRPSNGDSPSHPYHRTFSPHFHHFVEQCLQRNPDARPSASTLLNHSFFKQIKRRASEVLPELLRPVTPITNFEGSQSQDHSGIFGLVTNLEELEVDDWEF</t>
+  </si>
+  <si>
+    <t>KAPCA_HUMAN_D0_4AE9_A</t>
+  </si>
+  <si>
+    <t>KCC2G_HUMAN_D0_2V7O_A</t>
+  </si>
+  <si>
+    <t>KQYEHVKRDLNPEDFWEIIGELGDGAFGKVYKAQNKETSVLAAAKVIDTKSEEELEDYMVEIDILASCDHPNIVKLLDAFYYENNLWILIEFCAGGAVDAVMLELERPLTESQIQVVCKQTLDALNYLHDNKIIHRDLKAGNILFTLDGDIKLADFGVSAKNMRTIQRRDSFIGTPYWMAPEVVMCETSKDRPYDYKADVWSLGITLIEMAEIEPPHHELNPMRVLLKIAKSEPPTLAQPSRWSSNFKDFLKKCLEKNVDARWTTSQLLQHPFVTVDSNKPIRELIAEAKAEVTEEVEDGKE</t>
+  </si>
+  <si>
+    <t>ACCCAAACTGTTCATGAGTTTGCCAAGGAATTGGATGCCACCAACATATCCATTGATAAAGTTGTTGGAGCAGGTGAATTTGGAGAGGTGTGCAGTGGTCGCTTAAAACTTCCTTCAAAAAAAGAGATTTCAGTGGCCATTAAGACCCTGAAAGTTGGCTACACAGAAAAGCAGAGGAGAGACTTCCTGGGAGAAGCAAGCATTATGGGACAGTTTGACCACCCCAATATCATTCGACTGGAAGGAGTTGTTACCAAAAGTAAGCCAGTTATGATTGTCACAGAATACATGGAGAATGGTTCCTTGGATAGTTTCCTACGTAAACACGATGCCCAGTTTACTGTCATTCAGCTAGTGGGGATGCTTCGAGGGATAGCATCTGGCATGAAGTACCTGTCAGACATGGGCTATGTTCACCGAGACCTCGCTGCTCGGAACATCTTGATCAACAGTAACTTGGTGTGTAAGGTTTCTGATTTCGGACTTTCGCGTGTCCTGGAGGATGACCCAGAAGCTGCTTATACAACAAGAGGAGGGAAGATCCCAATCAGGTGGACATCACCAGAAGCTATAGCCTACCGCAAGTTCACGTCAGCCAGCGATGTATGGAGTTATGGGATTGTTCTCTGGGAGGTGATGTCTTATGGAGAGAGACCATACTGGGAGATGTCCAATCAGGATGTAATTAAAGCTGTAGATGAGGGCTATCGACTGCCACCCCCCATGGACTGCCCAGCTGCCTTGTATCAGCTGATGCTGGACTGCTGGCAGAAAGACAGGAACAACAGACCCAAGTTTGAGCAGATTGTTAGTATTCTGGACAAGCTTATCCGGAATCCCGGCAGCCTGAAGATCATCACCAGTGCAGCCGCAAGGCCATCAAACCTTCTTCTGGACCAAAGCAATGTGGATATCACTACCTTCCGCACAACAGGTGACTGGCTTAATGGTGTCTGGACAGCACACTGCAAGGAAATCTTCACGGGTGTGGAGTACAGTTCTTGTGACACAATAGCCAAGATTTCC</t>
+  </si>
+  <si>
+    <t>MEKDGLCRADQQYECVAEIGEGAYGKVFKARDLKNGGRFVALKRVRVQTGEEGMPLSTIREVAVLRHLETFEHPNVVRLFDVCTVSRTDRETKLTLVFEHVDQDLTTYLDKVPEPGVPTETIKDMMFQLLRGLDFLHSHRVVHRDLKPQNILVTSSGQIKLADFGLARIYSFQMALTSVVVTLWYRAPEVLLQSSYATPVDLWSVGCIFAEMFRRKPLFRGSSDVDQLGKILDVIGLPGEEDWPRDVALPRQAFHSKSAQPIEKFVTDIDELGKDLLLKCLTFNPAKRISAYSALSHPYFQ</t>
+  </si>
+  <si>
+    <t>EPHA3_HUMAN_D0_4GK2_A</t>
+  </si>
+  <si>
+    <t>ATGCCCGGCCCGGCCGCGGGCAGCAGGGCCCGGGTCTACGCCGAGGTGAACAGTCTGAGGAGCCGCGAGTACTGGGACTACGAGGCTCACGTCCCGAGCTGGGGTAATCAAGATGATTACCAACTGGTTCGAAAACTTGGTCGGGGAAAATATAGTGAAGTATTTGAGGCCATTAATATCACCAACAATGAGAGAGTGGTTGTAAAAATCCTGAAGCCAGTGAAGAAAAAGAAGATAAAACGAGAGGTTAAGATTCTGGAGAACCTTCGTGGTGGAACAAATATCATTAAGCTGATTGACACTGTAAAGGACCCCGTGTCAAAGACACCAGCTTTGGTATTTGAATATATCAATAATACAGATTTTAAGCAACTCTACCAGATCCTGACAGACTTTGATATCCGGTTTTATATGTATGAACTACTTAAAGCTCTGGATTACTGCCACAGCAAGGGAATCATGCACAGGGATGTGAAACCTCACAATGTCATGATAGATCACCAACAGAAAAAGCTGCGACTGATAGATTGGGGTCTGGCAGAATTCTATCATCCTGCTCAGGAGTACAATGTTCGTGTAGCCTCAAGGTACTTCAAGGGACCAGAGCTCCTCGTGGACTATCAGATGTATGATTATAGCTTGGACATGTGGAGTTTGGGCTGTATGTTAGCAAGCATGATCTTTCGAAGGGAACCATTCTTCCATGGACAGGACAACTATGACCAGCTTGTTCGCATTGCCAAGGTTCTGGGTACAGAAGAACTGTATGGGTATCTGAAGAAGTATCACATAGACCTAGATCCACACTTCAACGATATCCTGGGACAACATTCACGGAAACGCTGGGAAAACTTTATCCATAGTGAGAACAGACACCTTGTCAGCCCTGAGGCCCTAGATCTTCTGGACAAACTTCTGCGATACGACCATCAACAGAGACTGACTGCCAAAGAGGCCATGGAGCACCCATACTTCTACCCTGTGGTGAAGGAGCAGTCCCAG</t>
+  </si>
+  <si>
+    <t>ATGTCGGGACCCGTGCCAAGCAGGGCCAGAGTTTACACAGATGTTAATACACACAGACCTCGAGAATACTGGGATTACGAGTCACATGTGGTGGAATGGGGAAATCAAGATGACTACCAGCTGGTTCGAAAATTAGGCCGAGGTAAATACAGTGAAGTATTTGAAGCCATCAACATCACAAATAATGAAAAAGTTGTTGTTAAAATTCTCAAGCCAGTAAAAAAGAAGAAAATTAAGCGTGAAATAAAGATTTTGGAGAATTTGAGAGGAGGTCCCAACATCATCACACTGGCAGACATTGTAAAAGACCCTGTGTCACGAACCCCCGCCTTGGTTTTTGAACACGTAAACAACACAGACTTCAAGCAATTGTACCAGACGTTAACAGACTATGATATTCGATTTTACATGTATGAGATTCTGAAGGCCCTGGATTATTGTCACAGCATGGGAATTATGCACAGAGATGTCAAGCCCCATAATGTCATGATTGATCATGAGCACAGAAAGCTACGACTAATAGACTGGGGTTTGGCTGAGTTTTATCATCCTGGCCAAGAATATAATGTCCGAGTTGCTTCCCGATACTTCAAAGGTCCTGAGCTACTTGTAGACTATCAGATGTACGATTATAGTTTGGATATGTGGAGTTTGGGTTGTATGCTGGCAAGTATGATCTTTCGGAAGGAGCCATTTTTCCATGGACATGACAATTATGATCAGTTGGTGAGGATAGCCAAGGTTCTGGGGACAGAAGATTTATATGACTATATTGACAAATACAACATTGAATTAGATCCACGTTTCAATGATATCTTGGGCAGACACTCTCGAAAGCGATGGGAACGCTTTGTCCACAGTGAAAATCAGCACCTTGTCAGCCCTGAGGCCTTGGATTTCCTGGACAAACTGCTGCGATATGACCACCAGTCACGGCTTACTGCAAGAGAGGCAATGGAGCACCCCTATTTCTACACTGTTGTGAAGGACCAGGCTCGAATGGGT</t>
+  </si>
+  <si>
+    <t>NEK2_HUMAN_D0_2XKE_A</t>
+  </si>
+  <si>
+    <t>MK01_HUMAN_D0_4FMQ_A</t>
+  </si>
+  <si>
+    <t>ATGGAGCTGAGAGTCGGGAACAGGTACCGGCTGGGCCGGAAGATCGGCAGCGGCTCCTTCGGAGACATCTATCTCGGTACGGACATTGCTGCAGGAGAAGAGGTTGCCATCAAGCTTGAATGTGTCAAAACCAAACACCCTCAGCTCCACATTGAGAGCAAAATCTACAAGATGATGCAGGGAGGAGTGGGCATCCCCACCATCAGATGGTGCGGGGCAGAGGGGGACTACAACGTCATGGTGATGGAGCTGCTGGGGCCAAGCCTGGAGGACCTCTTCAACTTCTGCTCCAGGAAATTCAGCCTCAAAACCGTCCTGCTGCTTGCTGACCAAATGATCAGTCGCATCGAATACATTCATTCAAAGAACTTCATCCACCGGGATGTGAAGCCAGACAACTTCCTCATGGGCCTGGGGAAGAAGGGCAACCTGGTGTACATCATCGACTTCGGGCTGGCCAAGAAGTACCGGGATGCACGCACCCACCAGCACATCCCCTATCGTGAGAACAAGAACCTCACGGGGACGGCGCGGTACGCCTCCATCAACACGCACCTTGGAATTGAACAATCCCGAAGAGATGACTTGGAGTCTCTGGGCTACGTGCTAATGTACTTCAACCTGGGCTCTCTCCCCTGGCAGGGGCTGAAGGCTGCCACCAAGAGACAGAAATACGAAAGGATTAGCGAGAAGAAAATGTCCACCCCCATCGAAGTGTTGTGTAAAGGCTACCCTTCCGAATTTGCCACATACCTGAATTTCTGCCGTTCCTTGCGTTTTGACGACAAGCCTGACTACTCGTACCTGCGGCAGCTTTTCCGGAATCTGTTCCATCGCCAGGGCTTCTCCTATGACTACGTGTTCGACTGGAACATGCTCAAA</t>
+  </si>
+  <si>
+    <t>ATGGCGGCGGCGGCGGCGGCGGGCGCGGGCCCGGAGATGGTCCGCGGGCAGGTGTTCGACGTGGGGCCGCGCTACACCAACCTCTCGTACATCGGCGAGGGCGCCTACGGCATGGTGTGCTCTGCTTATGATAATGTCAACAAAGTTCGAGTAGCTATCAAGAAAATCAGCCCCTTTGAGCACCAGACCTACTGCCAGAGAACCCTGAGGGAGATAAAAATCTTACTGCGCTTCAGACATGAGAACATCATTGGAATCAATGACATTATTCGAGCACCAACCATCGAGCAAATGAAAGATGTATATATAGTACAGGACCTCATGGAAACAGATCTTTACAAGCTCTTGAAGACACAACACCTCAGCAATGACCATATCTGCTATTTTCTCTACCAGATCCTCAGAGGGTTAAAATATATCCATTCAGCTAACGTTCTGCACCGTGACCTCAAGCCTTCCAACCTGCTGCTCAACACCACCTGTGATCTCAAGATCTGTGACTTTGGCCTGGCCCGTGTTGCAGATCCAGACCATGATCACACAGGGTTCCTGACAGAATATGTGGCCACACGTTGGTACAGGGCTCCAGAAATTATGTTGAATTCCAAGGGCTACACCAAGTCCATTGATATTTGGTCTGTAGGCTGCATTCTGGCAGAAATGCTTTCTAACAGGCCCATCTTTCCAGGGAAGCATTATCTTGACCAGCTGAACCACATTTTGGGTATTCTTGGATCCCCATCACAAGAAGACCTGAATTGTATAATAAATTTAAAAGCTAGGAACTATTTGCTTTCTCTTCCACACAAAAATAAGGTGCCATGGAACAGGCTGTTCCCAAATGCTGACTCCAAAGCTCTGGACTTATTGGACAAAATGTTGACATTCAACCCACACAAGAGGATTGAAGTAGAACAGGCTCTGGCCCACCCATATCTGGAGCAGTATTACGACCCGAGTGACGAGCCCATCGCCGAAGCACCATTCAAGTTCGACATGGAATTGGATGACTTGCCTAAGGAAAAGCTCAAAGAACTAATTTTTGAAGAGACTGCTAGATTCCAGCCAGGATACAGATCT</t>
+  </si>
+  <si>
+    <t>MDEQSQGMQGPPVPQFQPQKALRPDMGYNTLANFRIEKKIGRGQFSEVYRAACLLDGVPVALKKVQIFDLMDAKARADCIKEIDLLKQLNHPNVIKYYASFIEDNELNIVLELADAGDLSRMIKHFKKQKRLIPERTVWKYFVQLCSALEHMHSRRVMHRDIKPANVFITATGVVKLGDLGLGRFFSSKTTAAHSLVGTPYYMSPERIHENGYNFKSDIWSLGCLLYEMAALQSPFYGDKMNLYSLCKKIEQCDYPPLPSDHYSEELRQLVNMCINPDPEKRPDVTYVYDVAKRMHACTASS</t>
+  </si>
+  <si>
+    <t>GECSQKGPVPFSHCLPTEKLQRCEKIGEGVFGEVFQTIADHTPVAIKIIAIEGPDLVNGSHQKTFEEILPEIIISKELSLLSGEVCNRTEGFIGLNSVHCVQGSYPPLLLKAWDHYNSTKGSANDRPDFFKDDQLFIVLEFEFGGIDLEQMRTKLSSLATAKSILHQLTASLAVAEASLRFEHRDLHWGNVLLKKTSLKKLHYTLNGKSSTIPSCGLQVSIIDYTLSRLERDGIVVFCDVSMDEDLFTGDGDYQFDIYRLMKKENNNRWGEYHPYSNVLWLHYLTDKMLKQMTFKTKCNTPAMKQIKRKIQEFHRTMLNFSSATDLLCQHRLFK</t>
+  </si>
+  <si>
+    <t>MENFNNFYILTSKELGRGKFAVVRQCISKSTGQEYAAKFLKKRRRGQDCRAEILHEIAVLELAKSCPRVINLHEVYENTSEIILILEYAAGGEIFSLCLPELAEMVSENDVIRLIKQILEGVYYLHQNNIVHLDLKPQNILLSSIYPLGDIKIVDFGMSRKIGHACELREIMGTPEYLAPEILNYDPITTATDMWNIGIIAYMLLTHTSPFVGEDNQETYLNISQVNVDYSEETFSSVSQLATDFIQSLLVKNPEKRPTAEICLSHSWLQQWDFENLFHPEETSSSSQTQDHSVRSSEDKTSKSS</t>
+  </si>
+  <si>
+    <t>CHK1_HUMAN_D0_2E9V_A</t>
+  </si>
+  <si>
+    <t>MELRVGNKYRLGRKIGSGSFGDIYLGANIASGEEVAIKLECVKTKHPQLHIESKFYKMMQGGVGIPSIKWCGAEGDYNVMVMELLGPSLEDLFNFCSRKFSLKTVLLLADQMISRIEYIHSKNFIHRDVKPDNFLMGLGKKGNLVYIIDFGLAKKYRDARTHQHIPYRENKNLTGTARYASINTHLGIEQSRRDDLESLGYVLMYFNLGSLPWQGLKAATKRQKYERISEKKMSTPIEVLCKGYPSEFSTYLNFCRSLRFDDKPDYSYLRQLFRNLFHRQGFSYDYVFDWNMLK</t>
+  </si>
+  <si>
+    <t>SSVTASAAPGTASLVPDYWIDGSNRDALSDFFEVESELGRGATSIVYRCKQKGTQKPYALKVLKKTVDKKIVRTEIGVLLRLSHPNIIKLKEIFETPTEISLVLELVTGGELFDRIVEKGYYSERDAADAVKQILEAVAYLHENGIVHRDLKPENLLYATPAPDAPLKIADFGLSKIVEHQVLMKTVCGTPGYCAPEILRGCAYGPEVDMWSVGIITYILLCGFEPFYDERGDQFMFRRILNCEYYFISPWWDEVSLNAKDLVRKLIVLDPKKRLTTFQALQHPWVTGKAANFVHMDTAQKKLQEFNARRKLKAAVKAVVASSRLG</t>
+  </si>
+  <si>
+    <t>dna_end</t>
+  </si>
+  <si>
+    <t>MADDDVLFEDVYELCEVIGKGPFSVVRRCINRETGQQFAVKIVDVAKFTSSPGLSTEDLKREASICHMLKHPHIVELLETYSSDGMLYMVFEFMDGADLCFEIVKRADAGFVYSEAVASHYMRQILEALRYCHDNNIIHRDVKPHCVLLASKENSAPVKLGGFGVAIQLGESGLVAGGRVGTPHFMAPEVVKREPYGKPVDVWGCGVILFILLSGCLPFYGTKERLFEGIIKGKYKMNPRQWSHISESAKDLVRRMLMLDPAERITVYEALNHPWLKERDRYAYKIHLPETVEQLRKFNARRKLKGAVLAAVSSHKFNSFYGDPPEELPDFSEDPTSSGA</t>
+  </si>
+  <si>
+    <t>FAK1_HUMAN_D0_2IJM_B</t>
+  </si>
+  <si>
+    <t>CHK2_HUMAN_D0_2CN5_A</t>
+  </si>
+  <si>
+    <t>GTGATCGACCCCTCAGAGCTCACTTTTGTCCAAGAGATTGGCAGTGGGCAATTTGGGTTGGTGCATCTGGGCTACTGGCTCAACAAGGACAAGGTGGCTATCAAAACCATTCGGGAAGGGGCTATGTCAGAAGAGGACTTCATAGAGGAGGCTGAAGTAATGATGAAACTCTCTCATCCCAAACTGGTGCAGCTGTATGGGGTGTGCCTGGAGCAGGCCCCCATCTGCCTGGTGTTTGAGTTCATGGAGCACGGCTGCCTGTCAGATTATCTACGCACCCAGCGGGGACTTTTTGCTGCAGAGACCCTGCTGGGCATGTGTCTGGATGTGTGTGAGGGCATGGCCTACCTGGAAGAGGCATGTGTCATCCACAGAGACTTGGCTGCCAGAAATTGTTTGGTGGGAGAAAACCAAGTCATCAAGGTGTCTGACTTTGGGATGACAAGGTTCGTTCTGGATGATCAGTACACCAGTTCCACAGGCACCAAATTCCCGGTGAAGTGGGCATCCCCAGAGGTTTTCTCTTTCAGTCGCTATAGCAGCAAGTCCGATGTGTGGTCATTTGGTGTGCTGATGTGGGAAGTTTTCAGTGAAGGCAAAATCCCGTATGAAAACCGAAGCAACTCAGAGGTGGTGGAAGACATCAGTACCGGATTTCGGTTGTACAAGCCCCGGCTGGCCTCCACACACGTCTACCAGATTATGAATCACTGCTGGAAAGAGAGACCAGAAGATCGGCCAGCCTTCTCCAGACTGCTGCGTCAACTGGCTGAAATTGCAGAATCAGGACTT</t>
+  </si>
+  <si>
+    <t>MSDEEILEKLRSIVSVGDPKKKYTRFEKIGQGASGTVYTAMDVATGQEVAIKQMNLQQQPKKELIINEILVMRENKNPNIVNYLDSYLVGDELWVVMEYLAGGSLTDVVTETCMDEGQIAAVCRECLQALEFLHSNQVIHRDIKSDNILLGMDGSVKLTDFGFCAQITPEQSKRSTMVGTPYWMAPEVVTRKAYGPKVDIWSLGIKAIEMIEGEPPYLNENPLRALYLIATNGTPELQNPEKLSAIFRDFLNRCLEMDVEKRGSAKELLQHQFLKIAKPLSSLTPLIAAAKEATKNNH</t>
+  </si>
+  <si>
+    <t>MSQSKGKKRNPGLKIPKEAFEQPQTSSTPPRDLDSKACISIGNQNFEVKADDLEPIMELGRGAYGVVEKMRHVPSGQIMAVKRIRATVNSQEQKRLLMDLDISMRTVDCPFTVTFYGALFREGDVWICMELMDTSLDKFYKQVIDKGQTIPEDILGKIAVSIVKALEHLHSKLSVIHRDVKPSNVLINALGQVKMCDFGISGYLVDSVAKTIDAGCKPYMAPERINPELNQKGYSVKSDIWSLGITMIELAILRFPYDSWGTPFQQLKQVVEEPSPQLPADKFSAEFVDFTSQCLKKNSKERPTYPELMQHPFFTLHESKGTDVASFVKLILGD</t>
+  </si>
+  <si>
+    <t>DYRK2_HUMAN_D0_3KVW_A</t>
+  </si>
+  <si>
+    <t>QSSKRSSRSVEDDKEGHLVCRIGDWLQERYEIVGNLGEGTFGKVVECLDHARGKSQVALKIIRNVGKYREAARLEINVLKKIKEKDKENKFLCVLMSDWFNFHGHMCIAFELLGKNTFEFLKENNFQPYPLPHVRHMAYQLCHALRFLHENQLTHTDLKPENILFVNSEFETLYNEHKSCEEKSVKNTSIRVADFGSATFDHEHHTTIVATRHYRPPEVILELGWAQPCDVWSIGCILFEYYRGFTLFQTHENREHLVMMEKILGPIPSHMIHRTRKQKYFYKGGLVWDENSSDGRYVKENCKPLKSYMLQDSLEHVQLFDLMRRMLEFDPAQRITLAEALLHPFFAGLTPEERSFHT</t>
+  </si>
+  <si>
+    <t>MK07_HUMAN_D0_4IC7_D</t>
+  </si>
+  <si>
+    <t>ATGCAGACAGTTGGTGTACATTCAATTGTTCAGCAGTTACACAGGAACAGTATTCAGTTTACTGATGGATATGAAGTAAAAGAAGATATTGGAGTTGGCTCCTACTCTGTTTGCAAGAGATGTATACATAAAGCTACAAACATGGAGTTTGCAGTGAAGATTATTGATAAAAGCAAGAGAGACCCAACAGAAGAAATTGAAATTCTTCTTCGTTATGGACAGCATCCAAACATTATCACTCTAAAGGATGTATATGATGATGGAAAGTATGTGTATGTAGTAACAGAACTTATGAAAGGAGGTGAATTGCTGGATAAAATTCTTAGACAAAAATTTTTCTCTGAACGAGAGGCCAGTGCTGTCCTGTTCACTATAACTAAAACCGTTGAATATCTTCACGCACAAGGGGTGGTTCATAGAGACTTGAAACCTAGCAACATTCTTTATGTGGATGAATCTGGTAATCCGGAATCTATTCGAATTTGTGATTTTGGCTTTGCAAAACAGCTGAGAGCGGAAAATGGTCTTCTCATGACTCCTTGTTACACTGCAAATTTTGTTGCACCAGAGGTTTTAAAAAGACAAGGCTATGATGCTGCTTGTGATATATGGAGTCTTGGTGTCCTACTCTATACAATGCTTACCGGTTACACTCCATTTGCAAATGGTCCTGATGATACACCAGAGGAAATATTGGCACGAATAGGTAGCGGAAAATTCTCACTCAGTGGTGGTTACTGGAATTCTGTTTCAGACACAGCAAAGGACCTGGTGTCAAAGATGCTTCATGTAGACCCTCATCAGAGACTGACTGCTGCTCTTGTGCTCAGACATCCTTGGATCGTCCACTGGGACCAACTGCCACAATACCAACTAAACAGACAGGATGCACCACATCTAGTAAAGGGTGCCATGGCAGCTACATATTCTGCTTTGAACCGTAATCAGTCACCAGTTTTGGAACCAGTAGGCCGCTCTACTCTTGCTCAGCGGAGAGGTATTAAAAAAATCACCTCAACAGCCCTG</t>
+  </si>
+  <si>
+    <t>MGKVKATPMTPEQAMKQYMQKLTAFEHHEIFSYPEIYFLGLNAKKRQGMTGGPNNGGYDDDQGSYVQVPHDHVAYRYEVLKVIGKGSFGQVVKAYDHKVHQHVALKMVRNEKRFHRQAAEEIRILEHLRKQDKDNTMNVIHMLENFTFRNHICMTFELLSMNLYELIKKNKFQGFSLPLVRKFAHSILQCLDALHKNRIIHCDLKPENILLKQQGRSGIKVIDFGSSCYEHQRVYTYIQSRFYRAPEVILGARYGMPIDMWSLGCILAELLTGYPLLPGEDEGDQLACMIELLGMPSQKLLDASKRAKNFVSSKGYPRYCTVTTLSDGSVVLNGGRSRRGKLRGPPESREWGNALKGCDDPLFLDFLKQCLEWDPAVRMTPGQALRHPWLRRRLPKPPTGEKTSVKR</t>
+  </si>
+  <si>
+    <t>CAGCAGTTCCCGCAGTTCCACGTCAAGTCCGGCCTGCAGATCAAGAAGAACGCCATCATCGATGACTACAAGGTCACCAGCCAGGTCCTGGGGCTGGGCATCAACGGCAAAGTTTTGCAGATCTTCAACAAGAGGACCCAGGAGAAATTCGCCCTCAAAATGCTTCAGGACTGCCCCAAGGCCCGCAGGGAGGTGGAGCTGCACTGGCGGGCCTCCCAGTGCCCGCACATCGTACGGATCGTGGATGTGTACGAGAATCTGTACGCAGGGAGGAAGTGCCTGCTGATTGTCATGGAATGTTTGGACGGTGGAGAACTCTTTAGCCGAATCCAGGATCGAGGAGACCAGGCATTCACAGAAAGAGAAGCATCCGAAATCATGAAGAGCATCGGTGAGGCCATCCAGTATCTGCATTCAATCAACATTGCCCATCGGGATGTCAAGCCTGAGAATCTCTTATACACCTCCAAAAGGCCCAACGCCATCCTGAAACTCACTGACTTTGGCTTTGCCAAGGAAACCACCAGCCACAACTCTTTGACCACTCCTTGTTATACACCGTACTATGTGGCTCCAGAAGTGCTGGGTCCAGAGAAGTATGACAAGTCCTGTGACATGTGGTCCCTGGGTGTCATCATGTACATCCTGCTGTGTGGGTATCCCCCCTTCTACTCCAACCACGGCCTTGCCATCTCTCCGGGCATGAAGACTCGCATCCGAATGGGCCAGTATGAATTTCCCAACCCAGAATGGTCAGAAGTATCAGAGGAAGTGAAGATGCTCATTCGGAATCTGCTGAAAACAGAGCCCACCCAGAGAATGACCATCACCGAGTTTATGAACCACCCTTGGATCATGCAATCAACAAAGGTCCCTCAAACCCCACTGCACACCAGCCGGGTCCTGAAGGAGGACAAGGAGCGGTGGGAGGATGTCAAGGGGTGTCTTCATGACAAGAACAGCGACCAGGCC</t>
+  </si>
+  <si>
+    <t>CDK2_HUMAN_D0_4BCP_A</t>
+  </si>
+  <si>
+    <t>MP2K4_HUMAN_D0_3ALN_C</t>
+  </si>
+  <si>
+    <t>ACCACCTCACTTGAAGCTTTGCCCACAGGGACAGTGCTGACAGACAAGAGTGGGCGACAGTGGAAGCTGAAGTCCTTCCAGACCAGGGACAACCAGGGCATTCTCTATGAAGCTGCACCCACCTCCACCCTCACCTGTGACTCAGGACCACAGAAGCAAAAGTTCTCACTCAAACTGGATGCCAAGGATGGGCGCTTGTTCAATGAGCAGAACTTCTTCCAGCGGGCCGCCAAGCCTCTGCAAGTCAACAAGTGGAAGAAGCTGTACTCGACCCCACTGCTGGCCATCCCTACCTGCATGGGTTTCGGTGTTCACCAGGACAAATACAGGTTCTTGGTGTTACCCAGCCTGGGGAGGAGCCTTCAGTCGGCCCTGGATGTCAGCCCAAAGCATGTGCTGTCAGAGAGGTCTGTGCTGCAGGTGGCCTGCCGGCTGCTGGATGCCCTGGAGTTCCTCCATGAGAATGAGTATGTTCATGGAAATGTGACAGCTGAAAATATCTTTGTGGATCCAGAGGACCAGAGTCAGGTGACTTTGGCAGGCTATGGCTTCGCCTTCCGCTATTGCCCAAGTGGCAAACACGTGGCCTACGTGGAAGGCAGCAGGAGCCCTCACGAGGGGGACCTTGAGTTCATTAGCATGGACCTGCACAAGGGATGCGGGCCCTCCCGCCGCAGCGACCTCCAGAGCCTGGGCTACTGCATGCTGAAGTGGCTCTACGGGTTTCTGCCATGGACAAATTGCCTTCCCAACACTGAGGACATCATGAAGCAAAAACAGAAGTTTGTTGATAAGCCGGGGCCCTTCGTGGGACCCTGCGGTCACTGGATCAGGCCCTCAGAGACCCTGCAGAAGTACCTGAAGGTGGTGATGGCCCTCACGTATGAGGAGAAGCCGCCCTACGCCATGCTGAGGAACAACCTAGAAGCTTTGCTGCAGGATCTGCGTGTGTCTCCATATGACCCCATTGGCCTCCCGATGGTGCCC</t>
+  </si>
+  <si>
+    <t>TCACCACAGCGGGAGCCACAGCGAGTATCCCATGAGCAGTTCCGGGCTGCCCTGCAGCTGGTGGTGGACCCAGGCGACCCCCGCTCCTACCTGGACAACTTCATCAAGATTGGCGAGGGCTCCACGGGCATCGTGTGCATCGCCACCGTGCGCAGCTCGGGCAAGCTGGTGGCCGTCAAGAAGATGGACCTGCGCAAGCAGCAGAGGCGCGAGCTGCTCTTCAACGAGGTGGTAATCATGAGGGACTACCAGCACGAGAATGTGGTGGAGATGTACAACAGCTACCTGGTGGGGGACGAGCTCTGGGTGGTCATGGAGTTCCTGGAAGGAGGCGCCCTCACCGACATCGTCACCCACACCAGGATGAACGAGGAGCAGATCGCGGCCGTGTGCCTTGCAGTGCTGCAGGCCCTGTCGGTGCTCCACGCCCAGGGCGTCATCCACCGGGACATCAAGAGCGACTCGATCCTGCTGACCCATGATGGCAGGGTGAAGCTGTCAGACTTTGGGTTCTGCGCCCAGGTGAGCAAGGAAGTGCCCCGAAGGAAGTCGCTGGTCGGCACGCCCTACTGGATGGCCCCAGAGCTCATCTCCCGCCTTCCCTACGGGCCAGAGGTAGACATCTGGTCGCTGGGGATAATGGTGATTGAGATGGTGGACGGAGAGCCCCCCTACTTCAACGAGCCACCCCTCAAAGCCATGAAGATGATTCGGGACAACCTGCCACCCCGACTGAAGAACCTGCACAAGGTGTCGCCATCCCTGAAGGGCTTCCTGGACCGCCTGCTGGTGCGAGACCCTGCCCAGCGGGCCACGGCAGCCGAGCTGCTGAAGCACCCATTCCTGGCCAAGGCAGGGCCGCCTGCCAGCATCGTGCCCCTCATGCGCCAGAACCGCACCAGA</t>
+  </si>
+  <si>
+    <t>SIESSGKLKISPEQHWDFTAEDLKDLGEIGRGAYGSVNKMVHKPSGQIMAVKRIRSTVDEKEQKQLLMDLDVVMRSSDCPYIVQFYGALFREGDCWICMELMSTSFDKFYKYVYSVLDDVIPEEILGKITLATVKALNHLKENLKIIHRDIKPSNILLDRSGNIKLCDFGISGQLVDSIAKTRDAGCRPYMAPERIDPSASRQGYDVRSDVWSLGITLYELATGRFPYPKWNSVFDQLTQVVKGDPPQLSNSEEREFSPSFINFVNLCLTKDESKRPKYKELLKHPFILMYEERAVEVACYVCKILDQMPATPSSPMYVD</t>
+  </si>
+  <si>
+    <t>TDSFSGRFEDVYQLQEDVLGEGAHARVQTCINLITSQEYAVKIIEKQPGHIRSRVFREVEMLYQCQGHRNVLELIEFFEEEDRFYLVFEKMRGGSILSHIHKRRHFNELEASVVVQDVASALDFLHNKGIAHRDLKPENILCEHPNQVSPVKICDFDLGSGIKLNGDCSPISTPELLTPCGSAEYMAPEVVEAFSEEASIYDKRCDLWSLGVILYILLSGYPPFVGRCGSDCGWDRGEACPACQNMLFESIQEGKYEFPDKDWAHISCAAKDLISKLLVRDAKQRLSAAQVLQHPWVQGCAPENTLPTPMVLQR</t>
   </si>
   <si>
     <t>WALNMKELKLLQTIGKGEFGDVMLGDYRGNKVAVKCIKNDATAQAFLAEASVMTQLRHSNLVQLLGVIVEEKGGLYIVTEYMAKGSLVDYLRSRGRSVLGGDCLLKFSLDVCEAMEYLEGNNFVHRDLAARNVLVSEDNVAKVSDFGLTKEASSTQDTGKLPVKWTAPEALREKKFSTKSDVWSFGILLWEIYSFGRVPYPRIPLKDVVPRVEKGYKMDAPDGCPPAVYEVMKNCWHLDAAMRPSFLQLREQLEHIKTHELHL</t>
   </si>
   <si>
-    <t>MSRSKRDNNFYSVEIGDSTFTVLKRYQNLKPIGSGAQGIVCAAYDAILERNVAIKKLSRPFQNQTHAKRAYRELVLMKCVNHKNIIGLLNVFTPQKSLEEFQDVYIVMELMDANLCQVIQMELDHERMSYLLYQMLCGIKHLHSAGIIHRDLKPSNIVVKSDCTLKILDFGLARTAGTSFMMTPYVVTRYYRAPEVILGMGYKENVDLWSVGCIMGEMVCHKILFPGRDYIDQWNKVIEQLGTPCPEFMKKLQPTVRTYVENRPKYAGYSFEKLFPDVLFPADSEHNKLKASQARDLLSKMLVIDASKRISVDEALQHPYINVWYDPSEAEAPPPKIPDKQLDEREHTIEEWKELIYKEVMDLE</t>
-  </si>
-  <si>
-    <t>STRAA_HUMAN_D0_3GNI_B</t>
-  </si>
-  <si>
-    <t>MP2K2_HUMAN_D0_1S9I_A</t>
-  </si>
-  <si>
-    <t>PIM1_HUMAN_D0_4A7C_A</t>
-  </si>
-  <si>
-    <t>EAFLTQKAKVGELKDDDFERISELGAGNGGVVTKVQHRPSGLIMARKLIHLEIKPAIRNQIIRELQVLHECNSPYIVGFYGAFYSDGEISICMEHMDGGSLDQVLKEAKRIPEEILGKVSIAVLRGLAYLREKHQIMHRDVKPSNILVNSRGEIKLCDFGVSGQLIDSMANSFVGTRSYMAPERLQGTHYSVQSDIWSMGLSLVELAVGRYPIPPPDAKELEAIFGRPVVDGEEGEPHSISPRPRPPGRPVSGHGMDSRPAMAIFELLDYIVNEPPPKLPNGVFTPDFQEFVNKCLIKNPAERADLKMLTNHTFIKRSEVEEVDFAGWLCKTLRLNQPGTPTRTAV</t>
-  </si>
-  <si>
-    <t>GGGCCGGAGGATGAGCTGCCCGACTGGGCCGCCGCCAAAGAGTTTTACCAGAAGTACGACCCTAAGGACGTCATCGGCAGAGGAGTGAGCTCTGTGGTCCGCCGTTGTGTTCATCGAGCTACTGGCCACGAGTTTGCGGTGAAGATTATGGAAGTGACAGCTGAGCGGCTGAGTCCTGAGCAGCTGGAGGAGGTGCGGGAAGCCACACGGCGAGAGACACACATCCTTCGCCAGGTCGCCGGCCACCCCCACATCATCACCCTCATCGATTCCTACGAGTCTTCTAGCTTCATGTTCCTGGTGTTTGACCTGATGCGGAAGGGAGAGCTGTTTGACTATCTCACAGAGAAGGTGGCCCTCTCTGAAAAGGAAACCAGGTCCATCATGCGGTCTCTGCTGGAAGCAGTGAGCTTTCTCCATGCCAACAACATTGTGCATCGAGATCTGAAGCCCGAGAATATTCTCCTAGATGACAATATGCAGATCCGACTTTCAGATTTCGGGTTCTCCTGCCACTTGGAACCTGGCGAGAAGCTTCGAGAGTTGTGTGGGACCCCAGGGTATCTAGCGCCAGAGATCCTTAAATGCTCCATGGATGAAACCCACCCAGGCTATGGCAAGGAGGTCGACCTCTGGGCCTGTGGGGTGATCTTGTTCACACTCCTGGCTGGCTCGCCACCCTTCTGGCACCGGCGGCAGATCCTGATGTTACGCATGATCATGGAGGGCCAGTACCAGTTCAGTTCCCCCGAGTGGGATGACCGTTCCAGCACTGTCAAAGACCTGATCTCCAGGCTGCTGCAGGTGGATCCTGAGGCACGCCTGACAGCTGAGCAGGCCCTACAGCACCCCTTCTTTGAGCGT</t>
-  </si>
-  <si>
-    <t>KC1E_HUMAN_D0_4HNI_A</t>
-  </si>
-  <si>
-    <t>VRK2_HUMAN_D0_2V62_B</t>
-  </si>
-  <si>
-    <t>ETYIKLDKLGEGTYATVYKGKSKLTDNLVALKEIRLEHEEGAPCTAIREVSLLKDLKHANIVTLHDIIHTEKSLTLVFEYLDKDLKQYLDDCGNIINMHNVKLFLFQLLRGLAYCHRQKVLHRDLKPQNLLINERGELKLADFGLARAKSIPTKTYSNEVVTLWYRPPDILLGSTDYSTQIDMWGVGCIFYEMATGRPLFPGSTVEEQLHFIFRILGTPTEETWPGILSNEEFKTYNYPKYRAEALLSHAPRLDSDGADLLTKLLQFEGRNRISAEDAMKHPFFLSLGERIHKLPDTTSIFALKEIQLQKEASLRS</t>
-  </si>
-  <si>
-    <t>HQLQPRRVSFRGEASETLQSPGYDPSRPESFFQQSFQRLSRLGHGSYGEVFKVRSKEDGRLYAVKRSMSPFRGPKDRARKLAEVGSHEKVGQHPCCVRLEQAWEEGGILYLQTELCGPSLQQHCEAWGASLPEAQVWGYLRDTLLALAHLHSQGLVHLDVKPANIFLGPRGRCKLGDFGLLVELGTAGAGEVQEGDPRYMAPELLQGSYGTAADVFSLGLTILEVACNMELPHGGEGWQQLRQGYLPPEFTAGLSSELRSVLVMMLEPDPKLRATAEALLALPVLRQP</t>
-  </si>
-  <si>
-    <t>aa_end</t>
-  </si>
-  <si>
-    <t>PMYT1_HUMAN_D0_3P1A_A</t>
-  </si>
-  <si>
-    <t>MK08_HUMAN_D0_2NO3_A</t>
-  </si>
-  <si>
-    <t>TCGGTTAAAGGAAGAATTTATTCCATATTAAAGCAGATAGGAAGTGGAGGTTCAAGCAAGGTATTTCAGGTGTTAAATGAAAAGAAACAGATATATGCTATAAAATATGTGAACTTAGAAGAAGCAGATAACCAAACTCTTGATAGTTACCGGAACGAAATAGCTTATTTGAATAAACTACAACAACACAGTGATAAGATCATCCGACTTTATGATTATGAAATCACGGACCAGTACATCTACATGGTAATGGAGTGTGGAAATATTGATCTTAATAGTTGGCTTAAAAAGAAAAAATCCATTGATCCATGGGAACGCAAGAGTTACTGGAAAAATATGTTAGAGGCAGTTCACACAATCCATCAACATGGCATTGTTCACAGTGATCTTAAACCAGCTAACTTTCTGATAGTTGATGGAATGCTAAAGCTAATTGATTTTGGGATTGCAAACCAAATGCAACCAGATACAACAAGTGTTGTTAAAGATTCTCAGGTTGGCACAGTTAATTATATGCCACCAGAAGCAATCAAAGATATGTCTTCCTCCAGAGAGAATGGGAAATCTAAGTCAAAGATAAGCCCCAAAAGTGATGTTTGGTCCTTAGGATGTATTTTGTACTATATGACTTACGGGAAAACACCATTTCAGCAGATAATTAATCAGATTTCTAAATTACATGCCATAATTGATCCTAATCATGAAATTGAATTTCCCGATATTCCAGAGAAAGATCTTCAAGATGTGTTAAAGTGTTGTTTAAAAAGGGACCCAAAACAGAGGATATCCATTCCTGAGCTCCTGGCTCATCCATATGTTCAAATTCAAACTCATCCAGTTAACCAAATGGCCAAGGGAACCACTGAAGAA</t>
-  </si>
-  <si>
-    <t>PAK1_HUMAN_D0_3Q52_A</t>
-  </si>
-  <si>
-    <t>CACCACCATCACCACCATTCGCACTCGGGGCCGGAGATCTCGCGGATTATCGTCGACCCCACGACTGGGAAGCGCTACTGCCGGGGCAAAGTGCTGGGAAAGGGTGGCTTTGCAAAATGTTACGAGATGACAGATTTGACAAATAACAAAGTCTACGCCGCAAAAATTATTCCTCACAGCAGAGTAGCTAAACCTCATCAAAGGGAAAAGATTGACAAAGAAATAGAGCTTCACAGAATTCTTCATCATAAGCATGTAGTGCAGTTTTACCACTACTTCGAGGACAAAGAAAACATTTACATTCTCTTGGAATACTGCAGTAGAAGGTCAATGGCTCATATTTTGAAAGCAAGAAAGGTGTTGACAGAGCCAGAAGTTCGATACTACCTCAGGCAGATTGTGTCTGGACTGAAATACCTTCATGAACAAGAAATCTTGCACAGAGATCTCAAACTAGGGAACTTTTTTATTAATGAAGCCATGGAACTAAAAGTTGGGGACTTCGGTCTGGCAGCCAGGCTAGAACCCTTGGAACACAGAAGGAGAACGATATGTGGTACCCCAAATTATCTCTCTCCTGAAGTCCTCAACAAACAAGGACATGGCTGTGAATCAGACATTTGGGCCCTGGGCTGTGTAATGTATACAATGTTACTAGGGAGGCCCCCATTTGAAACTACAAATCTCAAAGAAACTTATAGGTGCATAAGGGAAGCAAGGTATACAATGCCGTCCTCATTGCTGGCTCCTGCCAAGCACTTAATTGCTAGTATGTTGTCCAAAAACCCAGAGGATCGTCCCAGTTTGGATGACATCATTCGACATGACTTTTTTTTGCAGGGCTTCACTCCGGACAGACTGTCTTCTAGCTGTTGTCATACAGTTCCAGATTTCCACTTATCAAGCCCAGCT</t>
-  </si>
-  <si>
-    <t>GAAACAAAGTATACTGTGGACAAGAGGTTTGGCATGGATTTTAAAGAAATAGAATTAATTGGCTCAGGTGGATTTGGCCAAGTTTTCAAAGCAAAACACAGAATTGACGGAAAGACTTACGTTATTAAACGTGTTAAATATAATAACGAGAAGGCGGAGCGTGAAGTAAAAGCATTGGCAAAACTTGATCATGTAAATATTGTTCACTACAATGGCTGTTGGGATGGATTTGATTATGATCCTGAGACCAGTGATGATTCTCTTGAGAGCAGTGATTATGATCCTGAGAACAGCAAAAATAGTTCAAGGTCAAAGACTAAGTGCCTTTTCATCCAAATGGAATTCTGTGATAAAGGGACCTTGGAACAATGGATTGAAAAAAGAAGAGGCGAGAAACTAGACAAAGTTTTGGCTTTGGAACTCTTTGAACAAATAACAAAAGGGGTGGATTATATACATTCAAAAAAATTAATTCATAGAGATCTTAAGCCAAGTAATATATTCTTAGTAGATACAAAACAAGTAAAGATTGGAGACTTTGGACTTGTAACATCTCTGAAAAATGATGGAAAGCGAACAAGGAGTAAGGGAACTTTGCGATACATGAGCCCAGAACAGATTTCTTCGCAAGACTATGGAAAGGAAGTGGACCTCTACGCTTTGGGGCTAATTCTTGCTGAACTTCTTCATGTATGTGACACTGCTTTTGAAACATCAAAGTTTTTCACAGACCTACGGGATGGCATCATCTCAGATATATTTGATAAAAAAGAAAAAACTCTTCTACAGAAATTACTCTCAAAGAAACCTGAGGATCGACCTAACACATCTGAAATACTAAGGACCTTGACTGTGTGGAAGAAAAGCCCAGAGAAAAATGAACGACACACATGT</t>
-  </si>
-  <si>
-    <t>PAK7_HUMAN_D0_2F57_B</t>
-  </si>
-  <si>
-    <t>expression tag location</t>
-  </si>
-  <si>
-    <t>GAGAACTTCCAAAAGGTGGAAAAGATCGGAGAGGGCACGTACGGAGTTGTGTACAAAGCCAGAAACAAGTTGACGGGAGAGGTGGTGGCGCTTAAGAAAATCCGCCTGGACACTGAGACTGAGGGTGTGCCCAGTACTGCCATCCGAGAGATCTCTCTGCTTAAGGAGCTTAACCATCCTAATATTGTCAAGCTGCTGGATGTCATTCACACAGAAAATAAACTCTACCTGGTTTTTGAATTTCTGCACCAAGATCTCAAGAAATTCATGGATGCCTCTGCTCTCACTGGCATTCCTCTTCCCCTCATCAAGAGCTATCTGTTCCAGCTGCTCCAGGGCCTAGCTTTCTGCCATTCTCATCGGGTCCTCCACCGAGACCTTAAACCTCAGAATCTGCTTATTAACACAGAGGGGGCCATCAAGCTAGCAGACTTTGGACTAGCCAGAGCTTTTGGAGTCCCTGTTCGTACTTACACCCATGAGGTGGTGACCCTGTGGTACCGAGCTCCTGAAATCCTCCTGGGCTGCAAATATTATTCCACAGCTGTGGACATCTGGAGCCTGGGCTGCATCTTTGCTGAGATGGTGACTCGCCGGGCCCTATTCCCTGGAGATTCTGAGATTGACCAGCTCTTCCGGATCTTTCGGACTCTGGGGACCCCAGATGAGGTGGTGTGGCCAGGAGTTACTTCTATGCCTGATTACAAGCCAAGTTTCCCCAAGTGGGCCCGGCAAGATTTTAGTAAAGTTGTACCTCCCCTGGATGAAGATGGACGGAGCTTGTTATCGCAAATGCTGCACTACGACCCTAACAAGCGGATTTCGGCCAAGGCAGCCCTGGCTCACCCTTTCTTCCAGGATGTGACCAAGCCAGTACCCCATCTT</t>
-  </si>
-  <si>
-    <t>GGGGAATGCAGTCAGAAGGGTCCTGTCCCCTTTAGCCATTGCCTTCCCACAGAAAAACTGCAACGCTGTGAGAAGATTGGGGAAGGGGTGTTTGGCGAAGTGTTTCAAACAATTGCTGATCACACACCCGTAGCCATAAAAATCATTGCTATTGAAGGACCAGATTTAGTCAATGGATCCCATCAGAAAACCTTTGAGGAAATCCTGCCAGAGATCATCATCTCCAAAGAGTTGAGCCTCTTATCCGGTGAAGTGTGCAACCGCACAGAAGGCTTTATCGGGCTGAACTCAGTGCACTGTGTCCAGGGATCTTACCCTCCCTTGCTCCTCAAAGCCTGGGATCACTATAATTCAACCAAAGGCTCTGCAAATGACCGGCCTGATTTTTTTAAAGACGACCAGCTCTTCATTGTGCTGGAATTTGAGTTTGGAGGGATTGACTTAGAGCAAATGCGAACCAAGTTGTCTTCCTTGGCTACTGCAAAGAGCATTCTACACCAGCTCACAGCCTCCCTCGCAGTGGCAGAGGCATCACTGCGCTTTGAGCACCGAGACTTACACTGGGGGAACGTGCTCTTAAAGAAAACCAGCCTCAAAAAACTCCACTACACCCTCAATGGGAAGAGCAGCACTATCCCCAGCTGTGGGTTGCAAGTGAGCATCATTGACTACACCCTGTCGCGCTTGGAACGGGATGGGATTGTGGTTTTCTGTGACGTTTCCATGGATGAGGACCTGTTTACCGGTGACGGTGACTACCAGTTTGACATCTACAGGCTCATGAAGAAGGAGAATAACAACCGCTGGGGTGAATATCACCCTTATAGTAATGTGCTCTGGTTACATTACCTGACAGACAAGATGCTGAAACAAATGACCTTCAAGACTAAATGTAACACTCCTGCCATGAAGCAAATTAAGAGAAAAATCCAGGAGTTCCACAGGACAATGCTGAACTTCAGCTCTGCCACTGACTTGCTCTGCCAGCACAGACTGTTTAAG</t>
-  </si>
-  <si>
-    <t>TDSLPGKFEDMYKLTSELLGEGAYAKVQGAVSLQNGKEYAVKIIEKQAGHSRSRVFREVETLYQCQGNKNILELIEFFEDDTRFYLVFEKLQGGSILAHIQKQKHFNEREASRVVRDVAAALDFLHTKDKVSLCHLGGSARAPSGLTAAPTSLGSSDPPTSASQVAGTTGIDHRDLKPENILCESPEKVSPVKICDFDLGSGMKLNNSCTPITTPELTTPCGSAEYMAPEVGEVFTDQATFYDKRCDLWSLGVVLYIMLSGYPPFVGHCGADCGWDRGEVCRVCQNKLFESIQEGKYEFPDKDWAHISSEAKDLISKLLVRDAKQRLSAAQVLQHPWVQGQAPEKG</t>
-  </si>
-  <si>
-    <t>DAPK1_HUMAN_D0_4B4L_A</t>
-  </si>
-  <si>
-    <t>VIDPSELTFVQEIGSGQFGLVHLGYWLNKDKVAIKTIREGAMSEEDFIEEAEVMMKLSHPKLVQLYGVCLEQAPICLVFEFMEHGCLSDYLRTQRGLFAAETLLGMCLDVCEGMAYLEEACVIHRDLAARNCLVGENQVIKVSDFGMTRFVLDDQYTSSTGTKFPVKWASPEVFSFSRYSSKSDVWSFGVLMWEVFSEGKIPYENRSNSEVVEDISTGFRLYKPRLASTHVYQIMNHCWKERPEDRPAFSRLLRQLAEIAESGL</t>
-  </si>
-  <si>
-    <t>ATGAGCCTCATCCGGAAAAAGGGCTTCTACAAGCAGGACGTCAACAAGACCGCCTGGGAGCTGCCCAAGACCTACGTGTCCCCGACGCACGTCGGCAGCGGGGCCTATGGCTCCGTGTGCTCGGCCATCGACAAGCGGTCAGGGGAGAAGGTGGCCATCAAGAAGCTGAGCCGACCCTTTCAGTCCGAGATCTTCGCCAAGCGCGCCTACCGGGAGCTGCTGCTGCTGAAGCACATGCAGCATGAGAACGTCATTGGGCTCCTGGATGTCTTCACCCCAGCCTCCTCCCTGCGCAACTTCTATGACTTCTACCTGGTGATGCCCTTCATGCAGACGGATCTGCAGAAGATCATGGGGATGGAGTTCAGTGAGGAGAAGATCCAGTACCTGGTGTATCAGATGCTCAAAGGCCTTAAGTACATCCACTCTGCTGGGGTCGTGCACAGGGACCTGAAGCCAGGCAACCTGGCTGTGAATGAGGACTGTGAACTGAAGATTCTGGATTTTGGGCTGGCGCGACATGCAGACGCCGAGATGACTGGCTACGTGGTGACCCGCTGGTACCGAGCCCCCGAGGTGATCCTCAGCTGGATGCACTACAACCAGACAGTGGACATCTGGTCTGTGGTCTGTATCATGGCAGAGATGCTGACAGGGAAAACTCTGTTCAAGGGGAAAGATTACCTGGACCAGCTGACCCAGATCCTGAAAGTGACCGGGGTGCCTGGCACGGAGTTTGTGCAGAAGCTGAACGACAAAGCGGCCAAATCCTACATCCAGTCCCTGCCACAGACCCCCAGGAAGGATTTCACTCAGCTGTTCCCACGGGCCAGCCCCCAGGCTGCGGACCTGCTGGAGAAGATGCTGGAGCTAGACGTGGACAAGCGCCTGACGGCCGCGCAGGCCCTCACCCATCCCTTCTTTGAACCCTTCCGGGACCCTGAGGAAGAGACGGAGGCCCAGCAGCCGTTTGATGATTCCTTAGAACACGAGAAACTCACAGTGGATGAATGGAAGCAGCACATCTACAAGGAGATTGTGAACTTCAGCCCCATT</t>
-  </si>
-  <si>
-    <t>ATGAAAGATTATGATGAACTTCTCAAATATTATGAATTACATGAAACTATTGGGACAGGTGGCTTTGCAAAGGTCAAACTTGCCTGCCATATCCTTACTGGAGAGATGGTAGCTATAAAAATCATGGATAAAAACACACTAGGGAGTGATTTGCCCCGGATCAAAACGGAGATTGAGGCCTTGAAGAACCTGAGACATCAGCATATATGTCAACTCTACCATGTGCTAGAGACAGCCAACAAAATATTCATGGTTCTTGAGTACTGCCCTGGAGGAGAGCTGTTTGACTATATAATTTCCCAGGATCGCCTGTCAGAAGAGGAGACCCGGGTTGTCTTCCGTCAGATAGTATCTGCTGTTGCTTATGTGCACAGCCAGGGCTATGCTCACAGGGACCTCAAGCCAGAAAATTTGCTGTTTGATGAATATCATAAATTAAAGCTGATTGACTTTGGTCTCTGTGCAAAACCCAAGGGTAACAAGGATTACCATCTACAGACATGCTGTGGGAGTCTGGCTTATGCAGCACCTGAGTTAATACAAGGCAAATCATATCTTGGATCAGAGGCAGATGTTTGGAGCATGGGCATACTGTTATATGTTCTTATGTGTGGATTTCTACCATTTGATGATGATAATGTAATGGCTTTATACAAGAAGATTATGAGAGGAAAATATGATGTTCCCAAGTGGCTCTCTCCCAGTAGCATTCTGCTTCTTCAACAAATGCTGCAGGTGGACCCAAAGAAACGGATTTCTATGAAAAATCTATTGAACCATCCCTGGATCATGCAAGATTACAACTATCCTGTTGAGTGGCAAAGCAAGAATCCTTTTATTCACCTCGATGATGATTGCGTAACAGAACTTTCTGTACATCACAGAAACAACAGGCAAACAATGGAGGATTTAATTTCACTGTGGCAGTATGATCACCTCACGGCTACCTATCTTCTGCTTCTAGCCAAGAAGGCTCGGGGAAAACCAGTTCGTTTAAGGCTTTCTTCTTTCTCCTGTGGA</t>
-  </si>
-  <si>
-    <t>PAK4_HUMAN_D0_2J0I_A</t>
-  </si>
-  <si>
-    <t>AGVSEYELPEDPRWELPRDRLVLGKPLGEGCFGQVVLAEAIGLDKDKPNRVTKVAVKMLKSDATEKDLSDLISEMEMMKMIGKHKNIINLLGACTQDGPLYVIVEYASKGNLREYLQARRPPGLEYCYNPSHNPEEQLSSKDLVSCAYQVARGMEYLASKKCIHRDLAARNVLVTEDNVMKIADFGLARDIHHIDYYKKTTNGRLPVKWMAPEALFDRIYTHQSDVWSFGVLLWEIFTLGGSPYPGVPVEELFKLLKEGHRMDKPSNCTNELYMMMRDCWHAVPSQRPTFKQLVEDLDRIVALTSNQEYLDLSMPLD</t>
-  </si>
-  <si>
-    <t>GAGCCCAAGAAGTACGCAGTGACCGACGACTACCAGTTGTCCAAGCAGGTGCTGGGCCTGGGTGTGAACGGCAAAGTGCTGGAGTGCTTCCATCGGCGCACTGGACAGAAGTGTGCCCTGAAGCTCCTGTATGACAGCCCCAAGGCCCGGCAGGAGGTAGACCATCACTGGCAGGCTTCTGGCGGCCCCCATATTGTCTGCATCCTGGATGTGTATGAGAACATGCACCATGGCAAGCGCTGTCTCCTCATCATCATGGAATGCATGGAAGGTGGTGAGTTGTTCAGCAGGATTCAGGAGCGTGGCGACCAGGCTTTCACTGAGAGAGAAGCTGCAGAGATAATGCGGGATATTGGCACTGCCATCCAGTTTCTGCACAGCCATAACATTGCCCACCGAGATGTCAAGCCTGAAAACCTACTCTACACATCTAAGGAGAAAGACGCAGTGCTTAAGCTCACCGATTTTGGCTTTGCTAAGGAGACCACCCAAAATGCCCTGCAGACACCCTGCTATACTCCCTATTATGTGGCCCCTGAGGTCCTGGGTCCAGAGAAGTATGACAAGTCATGTGACATGTGGTCCCTGGGTGTCATCATGTACATCCTCCTTTGTGGCTTCCCACCCTTCTACTCCAACACGGGCCAGGCCATCTCCCCGGGGATGAAGAGGAGGATTCGCCTGGGCCAGTACGGCTTCCCCAATCCTGAGTGGTCAGAAGTCTCTGAGGATGCCAAGCAGCTGATCCGCCTCCTGTTGAAGACAGACCCCACAGAGAGGCTGACCATCACTCAGTTCATGAACCACCCCTGGATCAACCAATCGATGGTAGTGCCACAGACCCCACTCCACACGGCCCGAGTGCTGCAGGAGGACAAAGACCACTGGGACGAAGTCAAGGAGGAGATGACCAGTGCCTTGGCCACTATGCGGGTAGACTACGACCAGGTG</t>
-  </si>
-  <si>
-    <t>ATGTCTCAGGAGAGGCCCACGTTCTACCGGCAGGAGCTGAACAAGACAATCTGGGAGGTGCCCGAGCGTTACCAGAACCTGTCTCCAGTGGGCTCTGGCGCCTATGGCTCTGTGTGTGCTGCTTTTGACACAAAAACGGGGTTACGTGTGGCAGTGAAGAAGCTCTCCAGACCATTTCAGTCCATCATTCATGCGAAAAGAACCTACAGAGAACTGCGGTTACTTAAACATATGAAACATGAAAATGTGATTGGTCTGTTGGACGTTTTTACACCTGCAAGGTCTCTGGAGGAATTCAATGATGTGTATCTGGTGACCCATCTCATGGGGGCAGATCTGAACAACATTGTGAAATGTCAGAAGCTTACAGATGACCATGTTCAGTTCCTTATCTACCAAATTCTCCGAGGTCTAAAGTATATACATTCAGCTGACATAATTCACAGGGACCTAAAACCTAGTAATCTAGCTGTGAATGAAGACTGTGAGCTGAAGATTCTGGATTTTGGACTGGCTCGGCACACAGATGATGAAATGACAGGCTACGTGGCCACTAGGTGGTACAGGGCTCCTGAGATCATGCTGAACTGGATGCATTACAACCAGACAGTTGATATTTGGTCAGTGGGATGCATAATGGCCGAGCTGTTGACTGGAAGAACATTGTTTCCTGGTACAGACCATATTGATCAGTTGAAGCTCATTTTAAGACTCGTTGGAACCCCAGGGGCTGAGCTTTTGAAGAAAATCTCCTCAGAGTCTGCAAGAAACTATATTCAGTCTTTGACTCAGATGCCGAAGATGAACTTTGCGAATGTATTTATTGGTGCCAATCCCCTGGCTGTCGACTTGCTGGAGAAGATGCTTGTATTGGACTCAGATAAGAGAATTACAGCGGCCCAAGCCCTTGCACATGCCTACTTTGCTCAGTACCACGATCCTGATGATGAACCAGTGGCCGATCCTTATGATCAGTCCTTTGAAAGCAGGGACCTCCTTATAGATGAGTGGAAAAGCCTGACCTATGATGAAGTCATCAGCTTTGTGCCACCACCCCTTGACCAAGAAGAGATGGAGTCC</t>
-  </si>
-  <si>
-    <t>MK11_HUMAN_D0_3GC8_A</t>
-  </si>
-  <si>
-    <t>VRK3_HUMAN_D0_2JII_A</t>
-  </si>
-  <si>
-    <t>MK14_HUMAN_D0_3K3J_A</t>
-  </si>
-  <si>
-    <t>CDK16_HUMAN_D0_3MTL_A</t>
-  </si>
-  <si>
-    <t>BRAF_HUMAN_D0_4JVG_D</t>
-  </si>
-  <si>
-    <t>NEK7_HUMAN_D0_2WQN_A</t>
-  </si>
-  <si>
-    <t>PAK6_HUMAN_D0_2C30_A</t>
-  </si>
-  <si>
-    <t>FGFR1_HUMAN_D0_3GQL_B</t>
-  </si>
-  <si>
-    <t>TCTTCGGTCACCGCCAGTGCGGCCCCGGGGACCGCGAGCCTCGTCCCGGATTACTGGATCGACGGCTCCAACAGGGATGCGCTGAGCGATTTCTTCGAGGTGGAGTCGGAGCTGGGACGGGGTGCTACATCCATTGTGTACAGATGCAAACAGAAGGGGACCCAGAAGCCTTATGCTCTCAAAGTGTTAAAGAAAACAGTGGACAAAAAAATCGTAAGAACTGAGATAGGAGTTCTTCTTCGCCTCTCACATCCAAACATTATAAAACTTAAAGAGATATTTGAAACCCCTACAGAAATCAGTCTGGTCCTAGAACTCGTCACAGGAGGAGAACTGTTTGATAGGATTGTGGAAAAGGGATATTACAGTGAGCGAGATGCTGCAGATGCCGTTAAACAAATCCTGGAGGCAGTTGCTTATCTACATGAAAATGGGATTGTCCATCGTGATCTCAAACCAGAGAATCTTCTTTATGCAACTCCAGCCCCAGATGCACCACTCAAAATCGCTGATTTTGGACTCTCTAAAATTGTGGAACATCAAGTGCTCATGAAGACAGTATGTGGAACCCCAGGGTACTGCGCACCTGAAATTCTTAGAGGTTGTGCCTATGGACCTGAGGTGGACATGTGGTCTGTAGGAATAATCACCTACATCTTACTTTGTGGATTTGAACCATTCTATGATGAAAGAGGCGATCAGTTCATGTTCAGGAGAATTCTGAATTGTGAATATTACTTTATCTCCCCCTGGTGGGATGAAGTATCTCTAAATGCCAAGGACTTGGTCAGAAAATTAATTGTTTTGGATCCAAAGAAACGGCTGACTACATTTCAAGCTCTCCAGCATCCGTGGGTCACAGGTAAAGCAGCCAATTTTGTACACATGGATACCGCTCAAAAGAAGCTCCAAGAATTCAATGCCCGGCGTAAGCTTAAGGCAGCGGTGAAGGCTGTGGTGGCCTCTTCCCGCCTGGGA</t>
-  </si>
-  <si>
-    <t>MEAAASEPSLDLDNLKLLELIGRGRYGAVYKGSLDERPVAVKVFSFANRQNFINEKNIYRVPLMEHDNIARFIVGDERVTADGRMEYLLVMEYYPNGSLCKYLSLHTSDWVSSCRLAHSVTRGLAYLHTELPRGDHYKPAISHRDLNSRNVLVKNDGTCVISDFGLSMRLTGNRLVRPGEEDNAAISEVGTIRYMAPEVLEGAVNLRDCESALKQVDMYALGLIYWEIFMRCTDLFPGESVPEYQMAFQTEVGNHPTFEDMQVLVSREKQRPKFPEAWKENSLAVRSLKETIEDCWDQDAEARLTAQCAEERMAELMMIWERNKSVSPT</t>
-  </si>
-  <si>
-    <t>GTCATCATTGACAATAAGCGCTACCTCTTCATCCAGAAACTGGGGGAGGGTGGGTTCAGCTATGTGGACCTAGTGGAAGGGTTACATGATGGACACTTCTACGCCCTGAAGCGAATCCTGTGTCACGAGCAGCAGGACCGGGAGGAGGCCCAGCGAGAAGCCGACATGCATCGCCTCTTCAATCACCCCAACATCCTTCGCCTCGTGGCTTACTGTCTGAGGGAACGGGGTGCTAAGCATGAGGCCTGGCTGCTGCTACCATTCTTCAAGAGAGGTACGCTGTGGAATGAGATAGAAAGGCTGAAGGACAAAGGCAACTTCCTGACCGAGGATCAAATCCTTTGGCTGCTGCTGGGGATCTGCAGAGGCCTTGAGGCCATTCATGCCAAGGGTTATGCCCACAGAGACTTGAAGCCCACCAATATATTGCTTGGAGATGAGGGGCAGCCAGTTTTAATGGACTTGGGTTCCATGAATCAAGCATGCATCCATGTGGAGGGCTCCCGCCAGGCTCTGACCCTGCAGGACTGGGCAGCCCAGCGGTGCACCATCTCCTACCGAGCCCCAGAGCTCTTCTCTGTGCAGAGTCACTGTGTCATCGATGAGCGGACTGATGTCTGGTCCCTAGGCTGCGTGCTATATGCCATGATGTTTGGGGAAGGCCCTTATGACATGGTGTTCCAAAAGGGTGACAGTGTGGCCCTTGCTGTGCAGAACCAACTCAGCATCCCACAAAGCCCCAGGCATTCTTCAGCATTGTGGCAGCTCCTGAACTCGATGATGACCGTGGACCCGCATCAGCGTCCTCACATTCCTCTCCTCCTCAGTCAGCTGGAGGCGCTGCAG</t>
-  </si>
-  <si>
-    <t>BMPR2_HUMAN_D0_3G2F_A</t>
+    <t>MPGPAAGSRARVYAEVNSLRSREYWDYEAHVPSWGNQDDYQLVRKLGRGKYSEVFEAINITNNERVVVKILKPVKKKKIKREVKILENLRGGTNIIKLIDTVKDPVSKTPALVFEYINNTDFKQLYQILTDFDIRFYMYELLKALDYCHSKGIMHRDVKPHNVMIDHQQKKLRLIDWGLAEFYHPAQEYNVRVASRYFKGPELLVDYQMYDYSLDMWSLGCMLASMIFRREPFFHGQDNYDQLVRIAKVLGTEELYGYLKKYHIDLDPHFNDILGQHSRKRWENFIHSENRHLVSPEALDLLDKLLRYDHQQRLTAKEAMEHPYFYPVVKEQSQ</t>
+  </si>
+  <si>
+    <t>AAGAGGCAGTGGGCTTTGGAAGACTTTGAAATTGGTCGCCCTCTGGGTAAAGGAAAGTTTGGTAATGTTTATTTGGCAAGAGAAAAGCAAAGCAAGTTTATTCTGGCTCTTAAAGTGTTATTTAAAGCTCAGCTGGAGAAAGCCGGAGTGGAGCATCAGCTCAGAAGAGAAGTAGAAATACAGTCCCACCTTCGGCATCCTAATATTCTTAGACTGTATGGTTATTTCCATGATGCTACCAGAGTCTACCTAATTCTGGAATATGCACCACTTGGAACAGTTTATAGAGAACTTCAGAAACTTTCAAAGTTTGATGAGCAGAGAACTGCTACTTATATAACAGAATTGGCAAATGCCCTGTCTTACTGTCATTCGAAGAGAGTTATTCATAGAGACATTAAGCCAGAGAACTTACTTCTTGGATCAGCTGGAGAGCTTAAAATTGCAGATTTTGGGTGGTCAGTACATGCTCCATCTTCCAGGAGGACCACTCTCTGTGGCACCCTGGACTACCTGCCCCCTGAAATGATTGAAGGTCGGATGCATGATGAGAAGGTGGATCTCTGGAGCCTTGGAGTTCTTTGCTATGAATTTTTAGTTGGGAAGCCTCCTTTTGAGGCAAACACATACCAAGAGACCTACAAAAGAATATCACGGGTTGAATTCACATTCCCTGACTTTGTAACAGAGGGAGCCAGGGACCTCATTTCAAGACTGTTGAAGCATAATCCCAGCCAGAGGCCAATGCTCAGAGAAGTACTTGAACACCCCTGGATCACAGCAAATTCATCAAAACCATCA</t>
+  </si>
+  <si>
+    <t>ATGGAGCTACGTGTGGGGAACAAGTACCGCCTGGGACGGAAGATCGGGAGCGGGTCCTTCGGAGATATCTACCTGGGTGCCAACATCGCCTCTGGTGAGGAAGTCGCCATCAAGCTGGAGTGTGTGAAGACAAAGCACCCCCAGCTGCACATCGAGAGCAAGTTCTACAAGATGATGCAGGGTGGCGTGGGGATCCCGTCCATCAAGTGGTGCGGAGCTGAGGGCGACTACAACGTGATGGTCATGGAGCTGCTGGGGCCTAGCCTCGAGGACCTGTTCAACTTCTGTTCCCGCAAATTCAGCCTCAAGACGGTGCTGCTCTTGGCCGACCAGATGATCAGCCGCATCGAGTATATCCACTCCAAGAACTTCATCCACCGGGACGTCAAGCCCGACAACTTCCTCATGGGGCTGGGGAAGAAGGGCAACCTGGTCTACATCATCGACTTCGGCCTGGCCAAGAAGTACCGGGACGCCCGCACCCACCAGCACATTCCCTACCGGGAAAACAAGAACCTGACCGGCACGGCCCGCTACGCTTCCATCAACACGCACCTGGGCATTGAGCAAAGCCGTCGAGATGACCTGGAGAGCCTGGGCTACGTGCTCATGTACTTCAACCTGGGCTCCCTGCCCTGGCAGGGGCTCAAAGCAGCCACCAAGCGCCAGAAGTATGAACGGATCAGCGAGAAGAAGATGTCAACGCCCATCGAGGTCCTCTGCAAAGGCTATCCCTCCGAATTCTCAACATACCTCAACTTCTGCCGCTCCCTGCGGTTTGACGACAAGCCCGACTACTCTTACCTACGTCAGCTCTTCCGCAACCTCTTCCACCGGCAGGGCTTCTCCTATGACTACGTCTTTGACTGGAACATGCTGAAA</t>
+  </si>
+  <si>
+    <t>MK03_HUMAN_D0_2ZOQ_B</t>
+  </si>
+  <si>
+    <t>ATGTCTCAGTCGAAAGGCAAGAAGCGAAACCCTGGCCTTAAAATTCCAAAAGAAGCATTTGAACAACCTCAGACCAGTTCCACACCACCTCGAGATTTAGACTCCAAGGCTTGCATTTCTATTGGAAATCAGAACTTTGAGGTGAAGGCAGATGACCTGGAGCCTATAATGGAACTGGGACGAGGTGCGTACGGGGTGGTGGAGAAGATGCGGCACGTGCCCAGCGGGCAGATCATGGCAGTGAAGCGGATCCGAGCCACAGTAAATAGCCAGGAACAGAAACGGCTACTGATGGATTTGGATATTTCCATGAGGACGGTGGACTGTCCATTCACTGTCACCTTTTATGGCGCACTGTTTCGGGAGGGTGATGTGTGGATCTGCATGGAGCTCATGGATACATCACTAGATAAATTCTACAAACAAGTTATTGATAAAGGCCAGACAATTCCAGAGGACATCTTAGGGAAAATAGCAGTTTCTATTGTAAAAGCATTAGAACATTTACATAGTAAGCTGTCTGTCATTCACAGAGACGTCAAGCCTTCTAATGTACTCATCAATGCTCTCGGTCAAGTGAAGATGTGCGATTTTGGAATCAGTGGCTACTTGGTGGACTCTGTTGCTAAAACAATTGATGCAGGTTGCAAACCATACATGGCCCCTGAAAGAATAAACCCAGAGCTCAACCAGAAGGGATACAGTGTGAAGTCTGACATTTGGAGTCTGGGCATCACGATGATTGAGTTGGCCATCCTTCGATTTCCCTATGATTCATGGGGAACTCCATTTCAGCAGCTCAAACAGGTGGTAGAGGAGCCATCGCCACAACTCCCAGCAGACAAGTTCTCTGCAGAGTTTGTTGACTTTACCTCACAGTGCTTAAAGAAGAATTCCAAAGAACGGCCTACATACCCAGAGCTAATGCAACATCCATTTTTCACCCTACATGAATCCAAAGGAACAGATGTGGCATCTTTTGTAAAACTGATTCTTGGAGAC</t>
+  </si>
+  <si>
+    <t>TCAACCAGGGATTATGAGATTCAAAGAGAAAGAATAGAACTTGGACGATGTATTGGAGAAGGCCAATTTGGAGATGTACATCAAGGCATTTATATGAGTCCAGAGAATCCAGCTTTGGCGGTTGCAATTAAAACATGTAAAAACTGTACTTCGGACAGCGTGAGAGAGAAATTTCTTCAAGAAGCCTTAACAATGCGTCAGTTTGACCATCCTCATATTGTGAAGCTGATTGGAGTCATCACAGAGAATCCTGTCTGGATAATCATGGAGCTGTGCACACTTGGAGAGCTGAGGTCATTTTTGCAAGTAAGGAAATACAGTTTGGATCTAGCATCTTTGATCCTGTATGCCTATCAGCTTAGTACAGCTCTTGCATATCTAGAGAGCAAAAGATTTGTACACAGGGACATTGCTGCTCGGAATGTTCTGGTGTCCTCAAATGATTGTGTAAAATTAGGAGACTTTGGATTATCCCGATATATGGAAGATAGTACTTACTACAAAGCTTCCAAAGGAAAATTGCCTATTAAATGGATGGCTCCAGAGTCAATCAATTTTCGACGTTTTACCTCAGCTAGTGACGTATGGATGTTTGGTGTGTGTATGTGGGAGATACTGATGCATGGTGTGAAGCCTTTTCAAGGAGTGAAGAACAATGATGTAATCGGTCGAATTGAAAATGGGGAAAGATTACCAATGCCTCCAAATTGTCCTCCTACCCTCTACAGCCTTATGACGAAATGCTGGGCCTATGACCCCAGCAGGCGGCCCAGGTTTACTGAACTTAAAGCTCAGCTCAGCACAATCCTGGAGGAAGAGAAGGCTCAGCAAGAAGAG</t>
+  </si>
+  <si>
+    <t>DPEELFTKLEKIGKGSFGEVFKGIDNRTQKVVAIKIIDLEEAEDEIEDIQQEITVLSQCDSPYVTKYYGSYLKDTKLWIIMEYLGGGSALDLLEPGPLDETQIATILREILKGLDYLHSEKKIHRDIKAANVLLSEHGEVKLADFGVAGQLTDTQIKRNTFVGTPFWMAPEVIKQSAYDSKADIWSLGITAIELARGEPPHSELHPMKVLFLIPKNNPPTLEGNYSKPLKEFVEACLNKEPSFRPTAKELLKHKFILRNAKKTSYLTELID</t>
+  </si>
+  <si>
+    <t>MAPK3_HUMAN_D0_3FXW_A</t>
+  </si>
+  <si>
+    <t>AAGCAGTACGAACACGTGAAGAGGGACCTGAACCCCGAAGACTTTTGGGAGATTATAGGAGAACTGGGCGACGGAGCCTTTGGGAAAGTGTACAAGGCCCAGAATAAAGAGACCAGTGTTTTAGCTGCTGCAAAAGTGATTGACACTAAATCTGAAGAAGAACTTGAAGATTACATGGTAGAGATTGACATATTAGCATCTTGTGATCACCCAAATATAGTCAAGCTTCTAGATGCCTTCTATTATGAGAACAATCTTTGGATCCTCATTGAATTTTGTGCAGGTGGAGCAGTAGATGCTGTGATGCTTGAACTTGAGAGACCATTAACTGAGTCCCAAATACAAGTAGTTTGCAAGCAGACTTTAGATGCATTGAACTACTTACATGATAATAAGATCATCCACAGAGATCTGAAGGCTGGCAACATTCTCTTTACCTTAGATGGAGATATCAAATTGGCGGATTTTGGAGTATCAGCTAAAAACATGAGGACAATTCAAAGAAGAGATTCCTTTATTGGTACACCATATTGGATGGCTCCTGAAGTAGTCATGTGTGAAACATCTAAGGACAGACCCTATGACTACAAAGCTGATGTTTGGTCCCTGGGTATCACTTTAATAGAAATGGCTGAGATAGAACCACCTCATCATGAATTAAATCCAATGCGAGTGCTGCTAAAAATAGCAAAATCTGAGCCACCTACATTAGCACAGCCATCCAGATGGTCTTCAAATTTTAAGGACTTTCTAAAGAAATGCTTAGAAAAGAATGTGGATGCCAGGTGGACTACATCTCAGCTGCTGCAGCATCCCTTTGTTACTGTTGATTCCAACAAACCCATCCGAGAATTGATTGCAGAGGCGAAGGCTGAAGTAACAGAAGAAGTTGAAGATGGCAAAGAG</t>
+  </si>
+  <si>
+    <t>ATGCCTTCCCGGGCTGAGGACTATGAAGTGTTGTACACCATTGGCACAGGCTCCTACGGCCGCTGCCAGAAGATCCGGAGGAAGAGTGATGGCAAGATATTAGTTTGGAAAGAACTTGACTATGGCTCCATGACAGAAGCTGAGAAACAGATGCTTGTTTCTGAAGTGAATTTGCTTCGTGAACTGAAACATCCAAACATCGTTCGTTACTATGATCGGATTATTGACCGGACCAATACAACACTGTACATTGTAATGGAATATTGTGAAGGAGGGGATCTGGCTAGTGTAATTACAAAGGGAACCAAGGAAAGGCAATACTTAGATGAAGAGTTTGTTCTTCGAGTGATGACTCAGTTGACTCTGGCCCTGAAGGAATGCCACAGACGAAGTGATGGTGGTCATACCGTATTGCATCGGGATCTGAAACCAGCCAATGTTTTCCTGGATGGCAAGCAAAACGTCAAGCTTGGAGACTTTGGGCTAGCTAGAATATTAAACCATGACACGAGTTTTGCAAAAACATTTGTTGGCACACCTTATTACATGTCTCCTGAACAAATGAATCGCATGTCCTACAATGAGAAATCAGATATCTGGTCATTGGGCTGCTTGCTGTATGAGTTATGTGCATTAATGCCTCCATTTACAGCTTTTAGCCAGAAAGAACTCGCTGGGAAAATCAGAGAAGGCAAATTCAGGCGAATTCCATACCGTTACTCTGATGAATTGAATGAAATTATTACGAGGATGTTAAACTTAAAGGATTACCATCGACCTTCTGTTGAAGAAATTCTTGAGAACCCTTTAATA</t>
+  </si>
+  <si>
+    <t>STK3_HUMAN_D0_4LG4_B</t>
+  </si>
+  <si>
+    <t>GATGAACAACCTCACATCGGAAACTACAGACTGTTGAAAACAATCGGCAAGGGGAATTTTGCAAAAGTAAAATTGGCAAGACATATCCTTACAGGCAGAGAGGTTGCAATAAAAATAATTGACAAAACTCAGTTGAATCCAACAAGTCTACAAAAGCTCTTCAGAGAAGTAAGAATAATGAAGATTTTAAATCATCCCAATATAGTGAAGTTATTCGAAGTCATTGAAACTGAAAAAACACTCTACCTAATCATGGAATATGCAAGTGGAGGTGAAGTATTTGACTATTTGGTTGCACATGGCAGGATGAAGGAAAAAGAAGCAAGATCTAAATTTAGACAGATTGTGTCTGCAGTTCAATACTGCCATCAGAAACGGATCGTACATCGAGACCTCAAGGCTGAAAATCTATTGTTAGATGCCGATATGAACATTAAAATAGCAGATTTCGGTTTTAGCAATGAATTTACTGTTGGCGGTAAACTCGACACGTTTTGTGGCAGTCCTCCATACGCAGCACCTGAGCTCTTCCAGGGCAAGAAATATGACGGGCCAGAAGTGGATGTGTGGAGTCTGGGGGTCATTTTATACACACTAGTCAGTGGCTCACTTCCCTTTGATGGGCAAAACCTAAAGGAACTGAGAGAGAGAGTATTAAGAGGGAAATACAGAATTCCCTTCTACATGTCTACAGACTGTGAAAACCTTCTCAAACGTTTCCTGGTGCTAAATCCAATTAAACGCGGCACTCTAGAGCAAATCATGAAGGACAGGTGGATCAATGCAGGGCATGAAGAAGATGAACTCAAACCATTTGTTGAACCAGAGCTAGACATCTCAGACCAAAAAAGAATAGATATTATGGTGGGAATGGGATATTCACAAGAAGAAATTCAAGAATCTCTTAGTAAGATGAAATACGATGAAATCACAGCTACATATTTGTTATTGGGGAGAAAATCTTCAGAG</t>
   </si>
   <si>
     <t>dna_start</t>
   </si>
   <si>
-    <t>PHKG2_HUMAN_D0_2Y7J_D</t>
-  </si>
-  <si>
-    <t>MAPK2_HUMAN_D0_2JBO_A</t>
-  </si>
-  <si>
-    <t>HHHHHHSHSGPEISRIIVDPTTGKRYCRGKVLGKGGFAKCYEMTDLTNNKVYAAKIIPHSRVAKPHQREKIDKEIELHRILHHKHVVQFYHYFEDKENIYILLEYCSRRSMAHILKARKVLTEPEVRYYLRQIVSGLKYLHEQEILHRDLKLGNFFINEAMELKVGDFGLAARLEPLEHRRRTICGTPNYLSPEVLNKQGHGCESDIWALGCVMYTMLLGRPPFETTNLKETYRCIREARYTMPSSLLAPAKHLIASMLSKNPEDRPSLDDIIRHDFFLQGFTPDRLSSSCCHTVPDFHLSSPA</t>
-  </si>
-  <si>
-    <t>ATGGAGAAGGACGGCCTGTGCCGCGCTGACCAGCAGTACGAATGCGTGGCGGAGATCGGGGAGGGCGCCTATGGGAAGGTGTTCAAGGCCCGCGACTTGAAGAACGGAGGCCGTTTCGTGGCGTTGAAGCGCGTGCGGGTGCAGACCGGCGAGGAGGGCATGCCGCTCTCCACCATCCGCGAGGTGGCGGTGCTGAGGCACCTGGAGACCTTCGAGCACCCCAACGTGGTCAGGTTGTTTGATGTGTGCACAGTGTCACGAACAGACAGAGAAACCAAACTAACTTTAGTGTTTGAACATGTCGATCAAGACTTGACCACTTACTTGGATAAAGTTCCAGAGCCTGGAGTGCCCACTGAAACCATAAAGGATATGATGTTTCAGCTTCTCCGAGGTCTGGACTTTCTTCATTCACACCGAGTAGTGCATCGCGATCTAAAACCACAGAACATTCTGGTGACCAGCAGCGGACAAATAAAACTCGCTGACTTCGGCCTTGCCCGCATCTATAGTTTCCAGATGGCTCTAACCTCAGTGGTCGTCACGCTGTGGTACAGAGCACCCGAAGTCTTGCTCCAGTCCAGCTACGCCACCCCCGTGGATCTCTGGAGTGTTGGCTGCATATTTGCAGAAATGTTTCGTAGAAAGCCTCTTTTTCGTGGAAGTTCAGATGTTGATCAACTAGGAAAAATCTTGGACGTGATTGGACTCCCAGGAGAAGAAGACTGGCCTAGAGATGTTGCCCTTCCCAGGCAGGCTTTTCATTCAAAATCTGCCCAACCAATTGAGAAGTTTGTAACAGATATCGATGAACTAGGCAAAGACCTACTTCTGAAGTGTTTGACATTTAACCCAGCCAAAAGAATATCTGCCTACAGTGCCCTGTCTCACCCATACTTCCAG</t>
-  </si>
-  <si>
-    <t>ATGTCGGGCCCTCGCGCCGGCTTCTACCGGCAGGAGCTGAACAAGACCGTGTGGGAGGTGCCGCAGCGGCTGCAGGGGCTGCGCCCGGTGGGCTCCGGCGCCTACGGCTCCGTCTGTTCGGCCTACGACGCCCGGCTGCGCCAGAAGGTGGCGGTGAAGAAGCTGTCGCGCCCCTTCCAGTCGCTGATCCACGCGCGCAGAACGTACCGGGAGCTGCGGCTGCTCAAGCACCTGAAGCACGAGAACGTCATCGGGCTTCTGGACGTCTTCACGCCGGCCACGTCCATCGAGGACTTCAGCGAAGTGTACTTGGTGACCACCCTGATGGGCGCCGACCTGAACAACATCGTCAAGTGCCAGGCGCTGAGCGACGAGCACGTTCAATTCCTGGTTTACCAGCTGCTGCGCGGGCTGAAGTACATCCACTCGGCCGGGATCATCCACCGGGACCTGAAGCCCAGCAACGTGGCTGTGAACGAGGACTGTGAGCTCAGGATCCTGGATTTCGGGCTGGCGCGCCAGGCGGACGAGGAGATGACCGGCTATGTGGCCACGCGCTGGTACCGGGCACCTGAGATCATGCTCAACTGGATGCATTACAACCAAACAGTGGATATCTGGTCCGTGGGCTGCATCATGGCTGAGCTGCTCCAGGGCAAGGCCCTCTTCCCGGGAAGCGACTACATTGACCAGCTGAAGCGCATCATGGAAGTGGTGGGCACACCCAGCCCTGAGGTTCTGGCAAAAATCTCCTCGGAACACGCCCGGACATATATCCAGTCCCTGCCCCCCATGCCCCAGAAGGACCTGAGCAGCATCTTCCGTGGAGCCAACCCCCTGGCCATAGACCTCCTTGGAAGGATGCTGGTGCTGGACAGTGACCAGAGGGTCAGTGCAGCTGAGGCACTGGCCCACGCCTACTTCAGCCAGTACCACGACCCCGAGGATGAGCCAGAGGCCGAGCCATATGATGAGAGCGTTGAGGCCAAGGAGCGCACGCTGGAGGAGTGGAAGGAGCTCACTTACCAGGAAGTCCTCAGCTTCAAGCCCCCAGAGCCACCGAAGCCACCTGGCAGCCTGGAGATTGAGCAG</t>
-  </si>
-  <si>
-    <t>E2AK2_HUMAN_D0_3UIU_A</t>
-  </si>
-  <si>
-    <t>MEKYEKIGKIGEGSYGVVFKCRNRDTGQIVAIKKFLESEDDPVIKKIALREIRMLKQLKHPNLVNLLEVFRRKRRLHLVFEYCDHTVLHELDRYQRGVPEHLVKSITWQTLQAVNFCHKHNCIHRDVKPENILITKHSVIKLCDFGFARLLTGPSDYYTDYVATRWYRSPELLVGDTQYGPPVDVWAIGCVFAELLSGVPLWPGKSDVDQLYLIRKTLGDLIPRHQQVFSTNQYFSGVKIPDPEDMEPLELKFPNISYPALGLL</t>
-  </si>
-  <si>
-    <t>GeneID</t>
-  </si>
-  <si>
-    <t>ATGGATGAGCAATCACAAGGAATGCAAGGGCCACCTGTTCCTCAGTTCCAACCACAGAAGGCCTTACGACCGGATATGGGCTATAATACATTAGCCAACTTTCGAATAGAAAAGAAAATTGGTCGCGGACAATTTAGTGAAGTTTATAGAGCAGCCTGTCTCTTGGATGGAGTACCAGTAGCTTTAAAAAAAGTGCAGATATTTGATTTAATGGATGCCAAAGCACGTGCTGATTGCATCAAAGAAATAGATCTTCTTAAGCAACTCAACCATCCAAATGTAATAAAATATTATGCATCATTCATTGAAGATAATGAACTAAACATAGTTTTGGAACTAGCAGATGCTGGCGACCTATCCAGAATGATCAAGCATTTTAAGAAGCAAAAGAGGCTAATTCCTGAAAGAACTGTTTGGAAGTATTTTGTTCAGCTTTGCAGTGCATTGGAACACATGCATTCTCGAAGAGTCATGCATAGAGATATAAAACCAGCTAATGTGTTCATTACAGCCACTGGGGTGGTAAAACTTGGAGATCTTGGGCTTGGCCGGTTTTTCAGCTCAAAAACCACAGCTGCACATTCTTTAGTTGGTACGCCTTATTACATGTCTCCAGAGAGAATACATGAAAATGGATACAACTTCAAATCTGACATCTGGTCTCTTGGCTGTCTACTATATGAGATGGCTGCATTACAAAGTCCTTTCTATGGTGACAAAATGAATTTATACTCACTGTGTAAGAAGATAGAACAGTGTGACTACCCACCTCTTCCTTCAGATCACTATTCAGAAGAACTCCGACAGTTAGTTAATATGTGCATCAACCCAGATCCAGAGAAGCGACCAGACGTCACCTATGTTTATGACGTAGCAAAGAGGATGCATGCATGCACTGCAAGCAGC</t>
-  </si>
-  <si>
-    <t>DAPK3_HUMAN_D0_2J90_A</t>
-  </si>
-  <si>
-    <t>GAAGACAGTTTGACTAAGCAGCCTGAAGAAGTTTTTGATGTATTAGAGAAGCTTGGAGAAGGGTCTTATGGAAGTGTATTTAAAGCAATACACAAGGAATCCGGTCAAGTTGTCGCAATTAAACAAGTACCTGTTGAATCAGATCTTCAGGAAATAATCAAAGAAATTTCCATAATGCAGCAATGTGACAGCCCATATGTTGTAAAGTACTATGGCAGTTATTTTAAGAATACAGACCTCTGGATTGTTATGGAGTACTGTGGCGCTGGCTCTGTCTCAGACATAATTAGATTACGAAACAAGACATTAATAGAAGATGAAATTGCAACCATTCTTAAATCTACATTGAAAGGACTAGAATATTTGCACTTTATGAGAAAAATACACAGAGATATAAAAGCTGGAAATATTCTCCTCAATACAGAAGGACATGCAAAATTGGCAGATTTTGGAGTGGCTGGTCAGTTAACAGATACAATGGCAAAACGCAATACTGTAATAGGAACTCCATTTTGGATGGCTCCTGAGGTGATTCAAGAAATAGGCTATAACTGTGTGGCCGACATCTGGTCCCTTGGCATTACTTCTATAGAAATGGCTGAAGGAAAACCTCCTTATGCTGATATACATCCAATGAGGGCTATTTTTATGATTCCCACAAATCCACCACCAACATTCAGAAAGCCAGAACTTTGGTCCGATGATTTCACCGATTTTGTTAAAAAGTGTTTGGTGAAGAATCCTGAGCAGAGAGCTACTGCAACACAACTTTTACAGCATCCTTTTATCAAGAATGCCAAACCTGTATCAATATTAAGAGACCTGATCACAGAAGCTATGGAGATCAAAGCTAAAAGACATGAGGAACAGCAACGAGAATTGGAAGAGGAAGAA</t>
-  </si>
-  <si>
-    <t>VKEFLAKAKEDFLKKWESPAQNTAHLDQFERIKTLGTGSFGRVMLVKHKETGNHYAMKILDKQKVVKLKQIEHTLNEKRILQAVNFPFLVKLEFSFKDNSNLYMVMEYVPGGEMFSHLRRIGRFSEPHARFYAAQIVLTFEYLHSLDLIYRDLKPENLLIDQQGYIQVTDFGFAKRVKGRTWTLCGTPEYLAPEIILSKGYNKAVDWWALGVLIYEMAAGYPPFFADQPIQIYEKIVSGKVRFPSHFSSDLKDLLRNLLQVDLTKRFGNLKNGVNDIKNHKWFATTDWIAIYQRKVEAPFIPKFKGPGDTSNFDDYEEEEIRVSINEKCGKEFSEF</t>
-  </si>
-  <si>
-    <t>TCCAGGGTGTCCCATGAACAGTTTCGGGCGGCCCTGCAGCTGGTGGTCAGCCCAGGAGACCCCAGGGAATACTTGGCCAACTTTATCAAAATCGGGGAAGGCTCAACCGGCATCGTATGCATCGCCACCGAGAAACACACAGGGAAACAAGTTGCAGTGAAGAAAATGGACCTCCGGAAGCAACAGAGACGAGAACTGCTTTTCAATGAGGTCGTGATCATGCGGGATTACCACCATGACAATGTGGTTGACATGTACAGCAGCTACCTTGTCGGCGATGAGCTCTGGGTGGTCATGGAGTTTCTAGAAGGTGGTGCCTTGACAGACATTGTGACTCACACCAGAATGAATGAAGAACAGATAGCTACTGTCTGCCTGTCAGTTCTGAGAGCTCTCTCCTACCTTCATAACCAAGGAGTGATTCACAGGGACATAAAAAGTGACTCCATCCTCCTGACAAGCGATGGCCGGATAAAGTTGTCTGATTTTGGTTTCTGTGCTCAAGTTTCCAAAGAGGTGCCGAAGAGGAAATCATTGGTTGGCACTCCCTACTGGATGGCCCCTGAGGTGATTTCTAGGCTACCTTATGGGACAGAGGTGGACATCTGGTCCCTCGGGATCATGGTGATAGAAATGATTGATGGCGAGCCCCCCTACTTCAATGAGCCTCCCCTCCAGGCGATGCGGAGGATCCGGGACAGTTTACCTCCAAGAGTGAAGGACCTACACAAGGTTTCTTCAGTGCTCCGGGGATTCCTAGACTTGATGTTGGTGAGGGAGCCCTCTCAGAGAGCAACAGCCCAGGAACTCCTCGGACATCCATTCTTAAAACTAGCAGGTCCACCGTCTTGCATTGTCCCCCTCATGAGACAATACAGGCATCAC</t>
-  </si>
-  <si>
-    <t>KRQWALEDFEIGRPLGKGKFGNVYLAREKQSKFILALKVLFKAQLEKAGVEHQLRREVEIQSHLRHPNILRLYGYFHDATRVYLILEYAPLGTVYRELQKLSKFDEQRTATYITELANALSYCHSKRVIHRDIKPENLLLGSAGELKIADFGWSVHAPSSRRTTLCGTLDYLPPEMIEGRMHDEKVDLWSLGVLCYEFLVGKPPFEANTYQETYKRISRVEFTFPDFVTEGARDLISRLLKHNPSQRPMLREVLEHPWITANSSKPS</t>
-  </si>
-  <si>
-    <t>SLK_HUMAN_D0_2JFL_A</t>
-  </si>
-  <si>
-    <t>SRVSHEQFRAALQLVVSPGDPREYLANFIKIGEGSTGIVCIATEKHTGKQVAVKKMDLRKQQRRELLFNEVVIMRDYHHDNVVDMYSSYLVGDELWVVMEFLEGGALTDIVTHTRMNEEQIATVCLSVLRALSYLHNQGVIHRDIKSDSILLTSDGRIKLSDFGFCAQVSKEVPKRKSLVGTPYWMAPEVISRLPYGTEVDIWSLGIMVIEMIDGEPPYFNEPPLQAMRRIRDSLPPRVKDLHKVSSVLRGFLDLMLVREPSQRATAQELLGHPFLKLAGPPSCIVPLMRQYRHH</t>
-  </si>
-  <si>
-    <t>TQTVHEFAKELDATNISIDKVVGAGEFGEVCSGRLKLPSKKEISVAIKTLKVGYTEKQRRDFLGEASIMGQFDHPNIIRLEGVVTKSKPVMIVTEYMENGSLDSFLRKHDAQFTVIQLVGMLRGIASGMKYLSDMGYVHRDLAARNILINSNLVCKVSDFGLSRVLEDDPEAAYTTRGGKIPIRWTSPEAIAYRKFTSASDVWSYGIVLWEVMSYGERPYWEMSNQDVIKAVDEGYRLPPPMDCPAALYQLMLDCWQKDRNNRPKFEQIVSILDKLIRNPGSLKIITSAAARPSNLLLDQSNVDITTFRTTGDWLNGVWTAHCKEIFTGVEYSSCDTIAKIS</t>
-  </si>
-  <si>
-    <t>QQFPQFHVKSGLQIKKNAIIDDYKVTSQVLGLGINGKVLQIFNKRTQEKFALKMLQDCPKARREVELHWRASQCPHIVRIVDVYENLYAGRKCLLIVMECLDGGELFSRIQDRGDQAFTEREASEIMKSIGEAIQYLHSINIAHRDVKPENLLYTSKRPNAILKLTDFGFAKETTSHNSLTTPCYTPYYVAPEVLGPEKYDKSCDMWSLGVIMYILLCGYPPFYSNHGLAISPGMKTRIRMGQYEFPNPEWSEVSEEVKMLIRNLLKTEPTQRMTITEFMNHPWIMQSTKVPQTPLHTSRVLKEDKERWEDVKGCLHDKNSDQA</t>
-  </si>
-  <si>
-    <t>CSK21_HUMAN_D0_3AXW_A</t>
-  </si>
-  <si>
-    <t>ATCTRFTDDYQLFEELGKGAFSVVRRCVKKTPTQEYAAKIINTKKLSARDHQKLEREARICRLLKHPNIVRLHDSISEEGFHYLVFDLVTGGELFEDIVAREYYSEADASHCIHQILESVNHIHQHDIVHRDLKPENLLLASKCKGAAVKLADFGLAIEVQGEQQAWFGFAGTPGYLSPEVLRKDPYGKPVDIWACGVILYILLVGYPPFWDEDQHKLYQQIKAGAYDFPSPEWDTVTPEAKNLINQMLTINPAKRITADQALKHPWVCQRSTVASMMHRQETVECLRKFNARRKLKGAILTTMLVSRNFS</t>
-  </si>
-  <si>
-    <t>EDSLTKQPEEVFDVLEKLGEGSYGSVFKAIHKESGQVVAIKQVPVESDLQEIIKEISIMQQCDSPYVVKYYGSYFKNTDLWIVMEYCGAGSVSDIIRLRNKTLIEDEIATILKSTLKGLEYLHFMRKIHRDIKAGNILLNTEGHAKLADFGVAGQLTDTMAKRNTVIGTPFWMAPEVIQEIGYNCVADIWSLGITSIEMAEGKPPYADIHPMRAIFMIPTNPPPTFRKPELWSDDFTDFVKKCLVKNPEQRATATQLLQHPFIKNAKPVSILRDLITEAMEIKAKRHEEQQRELEEEE</t>
-  </si>
-  <si>
-    <t>CGTGTAAAAGCAGCTCAAGCTGGAAGACAGAGCTCTGCAAAGAGACATCTTGCAGAACAATTTGCAGTTGGAGAGATAATAACTGACATGGCAAAAAAGGAATGGAAAGTAGGATTACCCATTGGCCAAGGAGGCTTTGGCTGTATATATCTTGCTGATATGAATTCTTCAGAGTCAGTTGGCAGTGATGCACCTTGTGTTGTAAAAGTGGAACCCAGTGACAATGGACCTCTTTTTACTGAATTAAAGTTCTACCAACGAGCTGCAAAACCAGAGCAAATTCAGAAATGGATTCGTACCCGTAAGCTGAAGTACCTGGGTGTTCCTAAGTATTGGGGGTCTGGTCTACATGACAAAAATGGAAAAAGTTACAGGTTTATGATAATGGATCGCTTTGGGAGTGACCTTCAGAAAATATATGAAGCAAATGCCAAAAGGTTTTCTCGGAAAACTGTCTTGCAGCTAAGCTTAAGAATTCTGGATATTCTGGAATATATTCACGAGCATGAGTATGTGCATGGAGATATCAAGGCCTCAAATCTTCTTCTGAACTACAAGAATCCTGACCAGGTGTACTTGGTAGATTATGGCCTTGCTTATCGGTACTGCCCAGAAGGAGTTCATAAAGAATACAAAGAAGACCCCAAAAGATGTCACGATGGCACTATTGAATTCACGAGCATCGATGCACACAATGGCGTGGCCCCATCAAGACGTGGTGATTTGGAAATACTTGGTTATTGCATGATCCAATGGCTTACTGGCCATCTTCCTTGGGAGGATAATTTGAAAGATCCTAAATATGTTAGAGATTCCAAAATTAGATACAGAGAAAATATTGCAAGTTTGATGGACAAATGTTTTCCTGAGAAAAACAAACCAGGTGAAATTGCCAAATACATGGAAACAGTGAAATTACTAGACTACACTGAAAAACCTCTTTATGAAAATTTACGTGACATTCTTTTGCAAGGACTAAAAGCTATAGGAAGTAAGGATGATGGCAAATTGGACCTCAGTGTTGTGGAGAATGGAGGTTTGAAAGCAAAAACAATAACAAAGAAGCGAAAGAAAGAAATTGAAGAA</t>
-  </si>
-  <si>
-    <t>KS6A1_HUMAN_D0_3RNY_B</t>
-  </si>
-  <si>
-    <t>MP2K6_HUMAN_D0_3VN9_A</t>
-  </si>
-  <si>
-    <t>RVKAAQAGRQSSAKRHLAEQFAVGEIITDMAKKEWKVGLPIGQGGFGCIYLADMNSSESVGSDAPCVVKVEPSDNGPLFTELKFYQRAAKPEQIQKWIRTRKLKYLGVPKYWGSGLHDKNGKSYRFMIMDRFGSDLQKIYEANAKRFSRKTVLQLSLRILDILEYIHEHEYVHGDIKASNLLLNYKNPDQVYLVDYGLAYRYCPEGVHKEYKEDPKRCHDGTIEFTSIDAHNGVAPSRRGDLEILGYCMIQWLTGHLPWEDNLKDPKYVRDSKIRYRENIASLMDKCFPEKNKPGEIAKYMETVKLLDYTEKPLYENLRDILLQGLKAIGSKDDGKLDLSVVENGGLKAKTITKKRKKEIEE</t>
-  </si>
-  <si>
-    <t>MKNK1_HUMAN_D0_2HW6_B</t>
-  </si>
-  <si>
-    <t>MSLIRKKGFYKQDVNKTAWELPKTYVSPTHVGSGAYGSVCSAIDKRSGEKVAIKKLSRPFQSEIFAKRAYRELLLLKHMQHENVIGLLDVFTPASSLRNFYDFYLVMPFMQTDLQKIMGMEFSEEKIQYLVYQMLKGLKYIHSAGVVHRDLKPGNLAVNEDCELKILDFGLARHADAEMTGYVVTRWYRAPEVILSWMHYNQTVDIWSVVCIMAEMLTGKTLFKGKDYLDQLTQILKVTGVPGTEFVQKLNDKAAKSYIQSLPQTPRKDFTQLFPRASPQAADLLEKMLELDVDKRLTAAQALTHPFFEPFRDPEEETEAQQPFDDSLEHEKLTVDEWKQHIYKEIVNFSPI</t>
-  </si>
-  <si>
-    <t>DEQPHIGNYRLLKTIGKGNFAKVKLARHILTGREVAIKIIDKTQLNPTSLQKLFREVRIMKILNHPNIVKLFEVIETEKTLYLIMEYASGGEVFDYLVAHGRMKEKEARSKFRQIVSAVQYCHQKRIVHRDLKAENLLLDADMNIKIADFGFSNEFTVGGKLDTFCGSPPYAAPELFQGKKYDGPEVDVWSLGVILYTLVSGSLPFDGQNLKELRERVLRGKYRIPFYMSTDCENLLKRFLVLNPIKRGTLEQIMKDRWINAGHEEDELKPFVEPELDISDQKRIDIMVGMGYSQEEIQESLSKMKYDEITATYLLLGRKSSE</t>
-  </si>
-  <si>
-    <t>ITK_HUMAN_D0_3QGW_B</t>
-  </si>
-  <si>
-    <t>KS6A3_HUMAN_D1_4JG7_A</t>
-  </si>
-  <si>
-    <t>KCC4_HUMAN_D0_2W4O_A</t>
-  </si>
-  <si>
-    <t>CSK_HUMAN_D0_3D7T_A</t>
-  </si>
-  <si>
-    <t>KCC2A_HUMAN_D0_2VZ6_B</t>
-  </si>
-  <si>
-    <t>ATGTCTGATGAGGAGATCTTGGAGAAATTACGAAGCATAGTGAGTGTGGGCGATCCTAAGAAGAAATATACACGGTTTGAGAAGATTGGACAAGGTGCTTCAGGCACCGTGTACACAGCAATGGATGTGGCCACAGGACAGGAGGTGGCCATTAAGCAGATGAATCTTCAGCAGCAGCCCAAGAAAGAGCTGATTATTAATGAGATCCTGGTCATGAGGGAAAACAAGAACCCAAACATTGTGAATTACTTGGACAGTTACCTCGTGGGAGATGAGCTGTGGGTTGTTATGGAATACTTGGCTGGAGGCTCCTTGACAGATGTGGTGACAGAAACTTGCATGGATGAAGGCCAAATTGCAGCTGTGTGCCGTGAGTGTCTGCAGGCTCTGGAGTTCTTGCATTCGAACCAGGTCATTCACAGAGACATCAAGAGTGACAATATTCTGTTGGGAATGGATGGCTCTGTCAAGCTAACTGACTTTGGATTCTGTGCACAGATAACCCCAGAGCAGAGCAAACGGAGCACCATGGTAGGAACCCCATACTGGATGGCACCAGAGGTTGTGACACGAAAGGCCTATGGGCCCAAGGTTGACATCTGGTCCCTGGGCATCAAGGCCATCGAAATGATTGAAGGGGAGCCTCCATACCTCAATGAAAACCCTCTGAGAGCCTTGTACCTCATTGCCACCAATGGGACCCCAGAACTTCAGAACCCAGAGAAGCTGTCAGCTATCTTCCGGGACTTTCTGAACCGCTGTCTCGAGATGGATGTGGAGAAGAGAGGTTCAGCTAAAGAGCTGCTACAGCATCAATTCCTGAAGATTGCCAAGCCCCTCTCCAGCCTCACTCCACTTATTGCTGCAGCTAAGGAGGCAACAAAGAACAATCAC</t>
-  </si>
-  <si>
-    <t>ATGGAGGCAGCAGCATCCGAACCCTCTCTTGATCTAGATAATCTGAAACTGTTGGAGCTGATTGGCCGAGGTCGATATGGAGCAGTATATAAAGGCTCCTTGGATGAGCGTCCAGTTGCTGTAAAAGTGTTTTCCTTTGCAAACCGTCAGAATTTTATCAACGAAAAGAACATTTACAGAGTGCCTTTGATGGAACATGACAACATTGCCCGCTTTATAGTTGGAGATGAGAGAGTCACTGCAGATGGACGCATGGAATATTTGCTTGTGATGGAGTACTATCCCAATGGATCTTTATGCAAGTATTTAAGTCTCCACACAAGTGACTGGGTAAGCTCTTGCCGTCTTGCTCATTCTGTTACTAGAGGACTGGCTTATCTTCACACAGAATTACCACGAGGAGATCATTATAAACCTGCAATTTCCCATCGAGATTTAAACAGCAGAAATGTCCTAGTGAAAAATGATGGAACCTGTGTTATTAGTGACTTTGGACTGTCCATGAGGCTGACTGGAAATAGACTGGTGCGCCCAGGGGAGGAAGATAATGCAGCCATAAGCGAGGTTGGCACTATCAGATATATGGCACCAGAAGTGCTAGAAGGAGCTGTGAACTTGAGGGACTGTGAATCAGCTTTGAAACAAGTAGACATGTATGCTCTTGGACTAATCTATTGGGAGATATTTATGAGATGTACAGACCTCTTCCCAGGGGAATCCGTACCAGAGTACCAGATGGCTTTTCAGACAGAGGTTGGAAACCATCCCACTTTTGAGGATATGCAGGTTCTCGTGTCTAGGGAAAAACAGAGACCCAAGTTCCCAGAAGCCTGGAAAGAAAATAGCCTGGCAGTGAGGTCACTCAAGGAGACAATCGAAGACTGTTGGGACCAGGATGCAGAGGCTCGGCTTACTGCACAGTGTGCTGAGGAAAGGATGGCTGAACTTATGATGATTTGGGAAAGAAACAAATCTGTGAGCCCAACA</t>
-  </si>
-  <si>
-    <t>GCCACCTGCACACGTTTCACCGACGACTACCAGCTCTTCGAGGAGCTTGGCAAGGGTGCTTTCTCTGTGGTCCGCAGGTGTGTGAAGAAAACCCCCACGCAGGAGTACGCAGCAAAAATCATCAATACCAAGAAATTGTCTGCCCGGGATCACCAGAAACTAGAACGTGAGGCTCGGATATGTCGACTTCTGAAACATCCAAACATCGTGCGCCTCCATGACAGTATTTCTGAAGAAGGGTTTCACTACCTCGTGTTTGACCTTGTTACCGGCGGGGAGCTGTTTGAAGACATTGTGGCCAGAGAGTACTACAGTGAAGCAGATGCCAGCCACTGTATACATCAGATTCTGGAGAGTGTTAACCACATCCACCAGCATGACATCGTCCACAGGGACCTGAAGCCTGAGAACCTGCTGCTGGCGAGTAAATGCAAGGGTGCCGCCGTCAAGCTGGCTGATTTTGGCCTAGCCATCGAAGTACAGGGAGAGCAGCAGGCTTGGTTTGGTTTTGCTGGCACCCCAGGTTACTTGTCCCCTGAGGTCTTGAGGAAAGATCCCTATGGAAAACCTGTGGATATCTGGGCCTGCGGGGTCATCCTGTATATCCTCCTGGTGGGCTATCCTCCCTTCTGGGATGAGGATCAGCACAAGCTGTATCAGCAGATCAAGGCTGGAGCCTATGATTTCCCATCACCAGAATGGGACACGGTAACTCCTGAAGCCAAGAACTTGATCAACCAGATGCTGACCATAAACCCAGCAAAGCGCATCACGGCTGACCAGGCTCTCAAGCACCCGTGGGTCTGTCAACGATCCACGGTGGCATCCATGATGCATCGTCAGGAGACTGTGGAGTGTTTGCGCAAGTTCAATGCCCGGAGAAAACTGAAGGGTGCCATCCTCACGACCATGCTTGTCTCCAGGAACTTCTCA</t>
-  </si>
-  <si>
-    <t>GAGACCTACATTAAGCTGGACAAACTGGGCGAGGGTACCTATGCCACCGTCTACAAAGGCAAAAGCAAGCTCACAGACAACCTTGTGGCACTCAAGGAGATCAGACTGGAACATGAAGAGGGGGCACCCTGCACCGCCATCCGGGAAGTGTCCCTACTCAAGGACCTCAAACACGCCAACATCGTTACGCTACATGACATTATCCACACGGAGAAGTCCCTCACCCTTGTCTTTGAGTACCTGGACAAGGACCTGAAGCAGTACCTGGATGACTGTGGGAACATCATCAACATGCACAACGTGAAACTGTTCCTGTTCCAGCTGCTCCGTGGCCTGGCCTACTGCCACCGGCAGAAGGTGCTACACCGAGACCTCAAGCCCCAGAACCTGCTCATCAACGAGAGGGGAGAGCTCAAGCTGGCTGACTTTGGCCTGGCCCGAGCCAAGTCAATCCCAACAAAGACATACTCCAATGAGGTGGTGACACTGTGGTACCGGCCCCCTGACATCCTGCTTGGGTCCACGGACTACTCCACTCAGATTGACATGTGGGGTGTGGGCTGCATCTTCTATGAGATGGCCACAGGCCGTCCCCTCTTTCCGGGCTCCACGGTGGAGGAACAGCTACACTTCATCTTCCGTATCTTAGGAACCCCAACTGAGGAGACGTGGCCAGGCATCCTGTCCAACGAGGAGTTCAAGACATACAACTACCCCAAGTACCGAGCCGAGGCCCTTTTGAGCCACGCACCCCGACTTGATAGCGACGGGGCCGACCTCCTCACCAAGCTGTTGCAGTTTGAGGGTCGAAATCGGATCTCCGCAGAGGATGCCATGAAACATCCATTCTTCCTCAGTCTGGGGGAGCGGATCCACAAACTTCCTGACACTACTTCCATATTTGCACTAAAGGAGATTCAGCTACAAAAGGAGGCCAGCCTTCGGTCT</t>
-  </si>
-  <si>
-    <t>MK13_HUMAN_D0_4EYJ_A</t>
-  </si>
-  <si>
-    <t>STK16_HUMAN_D0_2BUJ_B</t>
-  </si>
-  <si>
-    <t>ATGGAAAGCGACCTGCACCAGATCATCCACTCCTCACAGCCCCTCACACTGGAACACGTGCGCTACTTCCTGTACCAACTGCTGCGGGGCCTGAAGTACATGCACTCGGCTCAGGTCATCCACCGTGACCTGAAGCCCTCCAACCTATTGGTGAATGAGAACTGTGAGCTCAAGATTGGTGACTTTGGTATGGCTCGTGGCCTGTGCACCTCGCCCGCTGAACATCAGTACTTCATGACTGAGTATGTGGCCACGCGCTGGTACCGTGCGCCCGAGCTCATGCTCTCTTTGCATGAGTATACACAGGCTATTGACCTCTGGTCTGTGGGCTGCATCTTTGGTGAGATGCTGGCCCGGCGCCAGCTCTTCCCAGGCAAAAACTATGTACACCAGCTACAGCTCATCATGATGGTGCTGGGTACCCCATCACCAGCCGTGATTCAGGCTGTGGGGGCTGAGAGGGTGCGGGCCTATATCCAGAGCTTGCCACCACGCCAGCCTGTGCCCTGGGAGACAGTGTACCCAGGTGCCGACCGCCAGGCCCTATCACTGCTGGGTCGCATGCTGCGTTTTGAGCCCAGCGCTCGCATCTCAGCAGCTGCTGCCCTTCGCCACCCTTTCCTGGCCAAGTACCATGATCCTGATGATGAGCCTGACTGTGCCCCGCCCTTTGACTTTGCCTTTGACCGCGAAGCCCTCACTCGGGAGCGCATTAAGGAGGCCATTGTGGCTGAAATTGAGGACTTCCATGCAAGGCGTGAGGGCATCCGCCAACAGATCCGCTTCCAGCCTTCTCTACAGCCTGTGGCTAGTGAGCCTGGCTGTCCAGATGTTGAAATGCCCAGTCCCTGGGCTCCCAGTGGGGACTGTGCCATG</t>
-  </si>
-  <si>
-    <t>CAGAGCAGTAAGCGCAGCAGCCGGAGTGTGGAAGATGACAAGGAGGGTCACCTGGTGTGCCGGATCGGCGATTGGCTCCAAGAGCGATATGAGATTGTGGGGAACCTGGGTGAAGGCACCTTTGGCAAGGTGGTGGAGTGCTTGGACCATGCCAGAGGGAAGTCTCAGGTTGCCCTGAAGATCATCCGCAACGTGGGCAAGTACCGGGAGGCTGCCCGGCTAGAAATCAACGTGCTCAAAAAAATCAAGGAGAAGGACAAAGAAAACAAGTTCCTGTGTGTCTTGATGTCTGACTGGTTCAACTTCCACGGTCACATGTGCATCGCCTTTGAGCTCCTGGGCAAGAACACCTTTGAGTTCCTGAAGGAGAATAACTTCCAGCCTTACCCCCTACCACATGTCCGGCACATGGCCTACCAGCTCTGCCACGCCCTTAGATTTCTGCATGAGAATCAGCTGACCCATACAGACTTGAAACCAGAGAACATCCTGTTTGTGAATTCTGAGTTTGAAACCCTCTACAATGAGCACAAGAGCTGTGAGGAGAAGTCAGTGAAGAACACCAGCATCCGAGTGGCTGACTTTGGCAGTGCCACATTTGACCATGAGCACCACACCACCATTGTGGCCACCCGTCACTATCGCCCGCCTGAGGTGATCCTTGAGCTGGGCTGGGCACAGCCCTGTGACGTCTGGAGCATTGGCTGCATTCTCTTTGAGTACTACCGGGGCTTCACACTCTTCCAGACCCACGAAAACCGAGAGCACCTGGTGATGATGGAGAAGATCCTAGGGCCCATCCCATCACACATGATCCACCGTACCAGGAAGCAGAAATATTTCTACAAAGGGGGCCTAGTTTGGGATGAGAACAGCTCTGACGGCCGGTATGTGAAGGAGAACTGCAAACCTCTGAAGAGTTACATGCTCCAAGACTCCCTGGAGCACGTGCAGCTGTTTGACCTGATGAGGAGGATGTTAGAATTTGACCCTGCCCAGCGCATCACACTGGCCGAGGCCCTGCTGCACCCCTTCTTTGCTGGCCTGACCCCTGAGGAGCGGTCCTTCCACACC</t>
-  </si>
-  <si>
-    <t>GAACTGAAGGATGACGACTTTGAGAAGATCAGTGAGCTGGGGGCTGGCAATGGCGGTGTGGTGTTCAAGGTCTCCCACAAGCCTTCTGGCCTGGTCATGGCCAGAAAGCTAATTCATCTGGAGATCAAACCCGCAATCCGGAACCAGATCATAAGGGAGCTGCAGGTTCTGCATGAGTGCAACTCTCCGTACATCGTGGGCTTCTATGGTGCGTTCTACAGCGATGGCGAGATCAGTATCTGCATGGAGCACATGGATGGAGGTTCTCTGGATCAAGTCCTGAAGAAAGCTGGAAGAATTCCTGAACAAATTTTAGGAAAAGTTAGCATTGCTGTAATAAAAGGCCTGACATATCTGAGGGAGAAGCACAAGATCATGCACAGAGCATACGGAATGGACAGCCGACCTCCCATGGCAATTTTTGAGTTGTTGGATTACATAGTCAACGAGCCTCCTCCAAAACTGCCCAGTGGAGTGTTCAGTCTGGAATTTCAAGATTTTGTGAATAAATGCTTAATAAAAAACCCCGCAGAGAGAGCAGATTTGAAGCAACTCATGGTTCATGCTTTTATCAAGAGATCTGATGCTGAGGAAGTGGATTTTGCAGGTTGGCTCTGCTCCACCATCGGCCTTAAC</t>
-  </si>
-  <si>
-    <t>MQTVGVHSIVQQLHRNSIQFTDGYEVKEDIGVGSYSVCKRCIHKATNMEFAVKIIDKSKRDPTEEIEILLRYGQHPNIITLKDVYDDGKYVYVVTELMKGGELLDKILRQKFFSEREASAVLFTITKTVEYLHAQGVVHRDLKPSNILYVDESGNPESIRICDFGFAKQLRAENGLLMTPCYTANFVAPEVLKRQGYDAACDIWSLGVLLYTMLTGYTPFANGPDDTPEEILARIGSGKFSLSGGYWNSVSDTAKDLVSKMLHVDPHQRLTAALVLRHPWIVHWDQLPQYQLNRQDAPHLVKGAMAATYSALNRNQSPVLEPVGRSTLAQRRGIKKITSTAL</t>
-  </si>
-  <si>
-    <t>KAPCA_HUMAN_D0_4AE9_A</t>
-  </si>
-  <si>
-    <t>KCC2G_HUMAN_D0_2V7O_A</t>
-  </si>
-  <si>
-    <t>KQYEHVKRDLNPEDFWEIIGELGDGAFGKVYKAQNKETSVLAAAKVIDTKSEEELEDYMVEIDILASCDHPNIVKLLDAFYYENNLWILIEFCAGGAVDAVMLELERPLTESQIQVVCKQTLDALNYLHDNKIIHRDLKAGNILFTLDGDIKLADFGVSAKNMRTIQRRDSFIGTPYWMAPEVVMCETSKDRPYDYKADVWSLGITLIEMAEIEPPHHELNPMRVLLKIAKSEPPTLAQPSRWSSNFKDFLKKCLEKNVDARWTTSQLLQHPFVTVDSNKPIRELIAEAKAEVTEEVEDGKE</t>
-  </si>
-  <si>
-    <t>ACCCAAACTGTTCATGAGTTTGCCAAGGAATTGGATGCCACCAACATATCCATTGATAAAGTTGTTGGAGCAGGTGAATTTGGAGAGGTGTGCAGTGGTCGCTTAAAACTTCCTTCAAAAAAAGAGATTTCAGTGGCCATTAAGACCCTGAAAGTTGGCTACACAGAAAAGCAGAGGAGAGACTTCCTGGGAGAAGCAAGCATTATGGGACAGTTTGACCACCCCAATATCATTCGACTGGAAGGAGTTGTTACCAAAAGTAAGCCAGTTATGATTGTCACAGAATACATGGAGAATGGTTCCTTGGATAGTTTCCTACGTAAACACGATGCCCAGTTTACTGTCATTCAGCTAGTGGGGATGCTTCGAGGGATAGCATCTGGCATGAAGTACCTGTCAGACATGGGCTATGTTCACCGAGACCTCGCTGCTCGGAACATCTTGATCAACAGTAACTTGGTGTGTAAGGTTTCTGATTTCGGACTTTCGCGTGTCCTGGAGGATGACCCAGAAGCTGCTTATACAACAAGAGGAGGGAAGATCCCAATCAGGTGGACATCACCAGAAGCTATAGCCTACCGCAAGTTCACGTCAGCCAGCGATGTATGGAGTTATGGGATTGTTCTCTGGGAGGTGATGTCTTATGGAGAGAGACCATACTGGGAGATGTCCAATCAGGATGTAATTAAAGCTGTAGATGAGGGCTATCGACTGCCACCCCCCATGGACTGCCCAGCTGCCTTGTATCAGCTGATGCTGGACTGCTGGCAGAAAGACAGGAACAACAGACCCAAGTTTGAGCAGATTGTTAGTATTCTGGACAAGCTTATCCGGAATCCCGGCAGCCTGAAGATCATCACCAGTGCAGCCGCAAGGCCATCAAACCTTCTTCTGGACCAAAGCAATGTGGATATCACTACCTTCCGCACAACAGGTGACTGGCTTAATGGTGTCTGGACAGCACACTGCAAGGAAATCTTCACGGGTGTGGAGTACAGTTCTTGTGACACAATAGCCAAGATTTCC</t>
-  </si>
-  <si>
-    <t>MEKDGLCRADQQYECVAEIGEGAYGKVFKARDLKNGGRFVALKRVRVQTGEEGMPLSTIREVAVLRHLETFEHPNVVRLFDVCTVSRTDRETKLTLVFEHVDQDLTTYLDKVPEPGVPTETIKDMMFQLLRGLDFLHSHRVVHRDLKPQNILVTSSGQIKLADFGLARIYSFQMALTSVVVTLWYRAPEVLLQSSYATPVDLWSVGCIFAEMFRRKPLFRGSSDVDQLGKILDVIGLPGEEDWPRDVALPRQAFHSKSAQPIEKFVTDIDELGKDLLLKCLTFNPAKRISAYSALSHPYFQ</t>
-  </si>
-  <si>
-    <t>EPHA3_HUMAN_D0_4GK2_A</t>
-  </si>
-  <si>
-    <t>ATGCCCGGCCCGGCCGCGGGCAGCAGGGCCCGGGTCTACGCCGAGGTGAACAGTCTGAGGAGCCGCGAGTACTGGGACTACGAGGCTCACGTCCCGAGCTGGGGTAATCAAGATGATTACCAACTGGTTCGAAAACTTGGTCGGGGAAAATATAGTGAAGTATTTGAGGCCATTAATATCACCAACAATGAGAGAGTGGTTGTAAAAATCCTGAAGCCAGTGAAGAAAAAGAAGATAAAACGAGAGGTTAAGATTCTGGAGAACCTTCGTGGTGGAACAAATATCATTAAGCTGATTGACACTGTAAAGGACCCCGTGTCAAAGACACCAGCTTTGGTATTTGAATATATCAATAATACAGATTTTAAGCAACTCTACCAGATCCTGACAGACTTTGATATCCGGTTTTATATGTATGAACTACTTAAAGCTCTGGATTACTGCCACAGCAAGGGAATCATGCACAGGGATGTGAAACCTCACAATGTCATGATAGATCACCAACAGAAAAAGCTGCGACTGATAGATTGGGGTCTGGCAGAATTCTATCATCCTGCTCAGGAGTACAATGTTCGTGTAGCCTCAAGGTACTTCAAGGGACCAGAGCTCCTCGTGGACTATCAGATGTATGATTATAGCTTGGACATGTGGAGTTTGGGCTGTATGTTAGCAAGCATGATCTTTCGAAGGGAACCATTCTTCCATGGACAGGACAACTATGACCAGCTTGTTCGCATTGCCAAGGTTCTGGGTACAGAAGAACTGTATGGGTATCTGAAGAAGTATCACATAGACCTAGATCCACACTTCAACGATATCCTGGGACAACATTCACGGAAACGCTGGGAAAACTTTATCCATAGTGAGAACAGACACCTTGTCAGCCCTGAGGCCCTAGATCTTCTGGACAAACTTCTGCGATACGACCATCAACAGAGACTGACTGCCAAAGAGGCCATGGAGCACCCATACTTCTACCCTGTGGTGAAGGAGCAGTCCCAG</t>
-  </si>
-  <si>
-    <t>ATGTCGGGACCCGTGCCAAGCAGGGCCAGAGTTTACACAGATGTTAATACACACAGACCTCGAGAATACTGGGATTACGAGTCACATGTGGTGGAATGGGGAAATCAAGATGACTACCAGCTGGTTCGAAAATTAGGCCGAGGTAAATACAGTGAAGTATTTGAAGCCATCAACATCACAAATAATGAAAAAGTTGTTGTTAAAATTCTCAAGCCAGTAAAAAAGAAGAAAATTAAGCGTGAAATAAAGATTTTGGAGAATTTGAGAGGAGGTCCCAACATCATCACACTGGCAGACATTGTAAAAGACCCTGTGTCACGAACCCCCGCCTTGGTTTTTGAACACGTAAACAACACAGACTTCAAGCAATTGTACCAGACGTTAACAGACTATGATATTCGATTTTACATGTATGAGATTCTGAAGGCCCTGGATTATTGTCACAGCATGGGAATTATGCACAGAGATGTCAAGCCCCATAATGTCATGATTGATCATGAGCACAGAAAGCTACGACTAATAGACTGGGGTTTGGCTGAGTTTTATCATCCTGGCCAAGAATATAATGTCCGAGTTGCTTCCCGATACTTCAAAGGTCCTGAGCTACTTGTAGACTATCAGATGTACGATTATAGTTTGGATATGTGGAGTTTGGGTTGTATGCTGGCAAGTATGATCTTTCGGAAGGAGCCATTTTTCCATGGACATGACAATTATGATCAGTTGGTGAGGATAGCCAAGGTTCTGGGGACAGAAGATTTATATGACTATATTGACAAATACAACATTGAATTAGATCCACGTTTCAATGATATCTTGGGCAGACACTCTCGAAAGCGATGGGAACGCTTTGTCCACAGTGAAAATCAGCACCTTGTCAGCCCTGAGGCCTTGGATTTCCTGGACAAACTGCTGCGATATGACCACCAGTCACGGCTTACTGCAAGAGAGGCAATGGAGCACCCCTATTTCTACACTGTTGTGAAGGACCAGGCTCGAATGGGT</t>
-  </si>
-  <si>
-    <t>NEK2_HUMAN_D0_2XKE_A</t>
-  </si>
-  <si>
-    <t>MK01_HUMAN_D0_4FMQ_A</t>
-  </si>
-  <si>
-    <t>ATGGAGCTGAGAGTCGGGAACAGGTACCGGCTGGGCCGGAAGATCGGCAGCGGCTCCTTCGGAGACATCTATCTCGGTACGGACATTGCTGCAGGAGAAGAGGTTGCCATCAAGCTTGAATGTGTCAAAACCAAACACCCTCAGCTCCACATTGAGAGCAAAATCTACAAGATGATGCAGGGAGGAGTGGGCATCCCCACCATCAGATGGTGCGGGGCAGAGGGGGACTACAACGTCATGGTGATGGAGCTGCTGGGGCCAAGCCTGGAGGACCTCTTCAACTTCTGCTCCAGGAAATTCAGCCTCAAAACCGTCCTGCTGCTTGCTGACCAAATGATCAGTCGCATCGAATACATTCATTCAAAGAACTTCATCCACCGGGATGTGAAGCCAGACAACTTCCTCATGGGCCTGGGGAAGAAGGGCAACCTGGTGTACATCATCGACTTCGGGCTGGCCAAGAAGTACCGGGATGCACGCACCCACCAGCACATCCCCTATCGTGAGAACAAGAACCTCACGGGGACGGCGCGGTACGCCTCCATCAACACGCACCTTGGAATTGAACAATCCCGAAGAGATGACTTGGAGTCTCTGGGCTACGTGCTAATGTACTTCAACCTGGGCTCTCTCCCCTGGCAGGGGCTGAAGGCTGCCACCAAGAGACAGAAATACGAAAGGATTAGCGAGAAGAAAATGTCCACCCCCATCGAAGTGTTGTGTAAAGGCTACCCTTCCGAATTTGCCACATACCTGAATTTCTGCCGTTCCTTGCGTTTTGACGACAAGCCTGACTACTCGTACCTGCGGCAGCTTTTCCGGAATCTGTTCCATCGCCAGGGCTTCTCCTATGACTACGTGTTCGACTGGAACATGCTCAAA</t>
-  </si>
-  <si>
-    <t>ATGGCGGCGGCGGCGGCGGCGGGCGCGGGCCCGGAGATGGTCCGCGGGCAGGTGTTCGACGTGGGGCCGCGCTACACCAACCTCTCGTACATCGGCGAGGGCGCCTACGGCATGGTGTGCTCTGCTTATGATAATGTCAACAAAGTTCGAGTAGCTATCAAGAAAATCAGCCCCTTTGAGCACCAGACCTACTGCCAGAGAACCCTGAGGGAGATAAAAATCTTACTGCGCTTCAGACATGAGAACATCATTGGAATCAATGACATTATTCGAGCACCAACCATCGAGCAAATGAAAGATGTATATATAGTACAGGACCTCATGGAAACAGATCTTTACAAGCTCTTGAAGACACAACACCTCAGCAATGACCATATCTGCTATTTTCTCTACCAGATCCTCAGAGGGTTAAAATATATCCATTCAGCTAACGTTCTGCACCGTGACCTCAAGCCTTCCAACCTGCTGCTCAACACCACCTGTGATCTCAAGATCTGTGACTTTGGCCTGGCCCGTGTTGCAGATCCAGACCATGATCACACAGGGTTCCTGACAGAATATGTGGCCACACGTTGGTACAGGGCTCCAGAAATTATGTTGAATTCCAAGGGCTACACCAAGTCCATTGATATTTGGTCTGTAGGCTGCATTCTGGCAGAAATGCTTTCTAACAGGCCCATCTTTCCAGGGAAGCATTATCTTGACCAGCTGAACCACATTTTGGGTATTCTTGGATCCCCATCACAAGAAGACCTGAATTGTATAATAAATTTAAAAGCTAGGAACTATTTGCTTTCTCTTCCACACAAAAATAAGGTGCCATGGAACAGGCTGTTCCCAAATGCTGACTCCAAAGCTCTGGACTTATTGGACAAAATGTTGACATTCAACCCACACAAGAGGATTGAAGTAGAACAGGCTCTGGCCCACCCATATCTGGAGCAGTATTACGACCCGAGTGACGAGCCCATCGCCGAAGCACCATTCAAGTTCGACATGGAATTGGATGACTTGCCTAAGGAAAAGCTCAAAGAACTAATTTTTGAAGAGACTGCTAGATTCCAGCCAGGATACAGATCT</t>
-  </si>
-  <si>
-    <t>MDEQSQGMQGPPVPQFQPQKALRPDMGYNTLANFRIEKKIGRGQFSEVYRAACLLDGVPVALKKVQIFDLMDAKARADCIKEIDLLKQLNHPNVIKYYASFIEDNELNIVLELADAGDLSRMIKHFKKQKRLIPERTVWKYFVQLCSALEHMHSRRVMHRDIKPANVFITATGVVKLGDLGLGRFFSSKTTAAHSLVGTPYYMSPERIHENGYNFKSDIWSLGCLLYEMAALQSPFYGDKMNLYSLCKKIEQCDYPPLPSDHYSEELRQLVNMCINPDPEKRPDVTYVYDVAKRMHACTASS</t>
-  </si>
-  <si>
-    <t>GECSQKGPVPFSHCLPTEKLQRCEKIGEGVFGEVFQTIADHTPVAIKIIAIEGPDLVNGSHQKTFEEILPEIIISKELSLLSGEVCNRTEGFIGLNSVHCVQGSYPPLLLKAWDHYNSTKGSANDRPDFFKDDQLFIVLEFEFGGIDLEQMRTKLSSLATAKSILHQLTASLAVAEASLRFEHRDLHWGNVLLKKTSLKKLHYTLNGKSSTIPSCGLQVSIIDYTLSRLERDGIVVFCDVSMDEDLFTGDGDYQFDIYRLMKKENNNRWGEYHPYSNVLWLHYLTDKMLKQMTFKTKCNTPAMKQIKRKIQEFHRTMLNFSSATDLLCQHRLFK</t>
-  </si>
-  <si>
-    <t>MENFNNFYILTSKELGRGKFAVVRQCISKSTGQEYAAKFLKKRRRGQDCRAEILHEIAVLELAKSCPRVINLHEVYENTSEIILILEYAAGGEIFSLCLPELAEMVSENDVIRLIKQILEGVYYLHQNNIVHLDLKPQNILLSSIYPLGDIKIVDFGMSRKIGHACELREIMGTPEYLAPEILNYDPITTATDMWNIGIIAYMLLTHTSPFVGEDNQETYLNISQVNVDYSEETFSSVSQLATDFIQSLLVKNPEKRPTAEICLSHSWLQQWDFENLFHPEETSSSSQTQDHSVRSSEDKTSKSS</t>
-  </si>
-  <si>
-    <t>GCTGATCCAGAAGAACTGTTCACAAAATTAGAGCGCATTGGGAAAGGCTCATTTGGGGAAGTTTTCAAAGGAATTGATAACCGTACCCAGCAAGTCGTTGCTATTAAAATCATAGACCTTGAGGAAGCCGAAGATGAAATAGAAGACATTCAGCAAGAAATAACTGTCTTGAGTCAATGTGACAGCTCATATGTAACAAAATACTATGGGTCATATTTAAAGGGGTCTAAATTATGGATAATAATGGAATACCTGGGCGGTGGTTCAGCACTGGATCTTCTTCGAGCTGGTCCATTTGATGAGTTCCAGATTGCTACCATGCTAAAGGAAATTTTAAAAGGTCTGGACTATCTGCATTCAGAAAAGAAAATTCACCGAGACATAAAAGCTGCCAATGTCTTGCTCTCAGAACAAGGAGATGTTAAACTTGCTGATTTTGGAGTTGCTGGTCAGCTGACAGATACACAGATTAAAAGAAATACCTTTGTGGGAACTCCATTTTGGATGGCTCCTGAAGTTATTCAACAGTCAGCTTATGACTCAAAAGCTGACATTTGGTCATTGGGAATTACTGCTATTGAACTAGCCAAGGGAGAGCCACCTAACTCCGATATGCATCCAATGAGAGTTCTGTTTCTTATTCCCAAAAACAATCCTCCAACTCTTGTTGGAGACTTTACTAAGTCTTTTAAGGAGTTTATTGATGCTTGCCTGAACAAAGATCCATCATTTCGTCCTACAGCAAAAGAACTTCTGAAACACAAATTCATTGTAAAAAATTCAAAGAAGACTTCTTATCTGACTGAACTGATAGATCGTTTTAAGAGATGGAAGGCAGAA</t>
-  </si>
-  <si>
-    <t>MELRVGNKYRLGRKIGSGSFGDIYLGANIASGEEVAIKLECVKTKHPQLHIESKFYKMMQGGVGIPSIKWCGAEGDYNVMVMELLGPSLEDLFNFCSRKFSLKTVLLLADQMISRIEYIHSKNFIHRDVKPDNFLMGLGKKGNLVYIIDFGLAKKYRDARTHQHIPYRENKNLTGTARYASINTHLGIEQSRRDDLESLGYVLMYFNLGSLPWQGLKAATKRQKYERISEKKMSTPIEVLCKGYPSEFSTYLNFCRSLRFDDKPDYSYLRQLFRNLFHRQGFSYDYVFDWNMLK</t>
-  </si>
-  <si>
-    <t>SSVTASAAPGTASLVPDYWIDGSNRDALSDFFEVESELGRGATSIVYRCKQKGTQKPYALKVLKKTVDKKIVRTEIGVLLRLSHPNIIKLKEIFETPTEISLVLELVTGGELFDRIVEKGYYSERDAADAVKQILEAVAYLHENGIVHRDLKPENLLYATPAPDAPLKIADFGLSKIVEHQVLMKTVCGTPGYCAPEILRGCAYGPEVDMWSVGIITYILLCGFEPFYDERGDQFMFRRILNCEYYFISPWWDEVSLNAKDLVRKLIVLDPKKRLTTFQALQHPWVTGKAANFVHMDTAQKKLQEFNARRKLKAAVKAVVASSRLG</t>
-  </si>
-  <si>
-    <t>dna_end</t>
-  </si>
-  <si>
-    <t>MADDDVLFEDVYELCEVIGKGPFSVVRRCINRETGQQFAVKIVDVAKFTSSPGLSTEDLKREASICHMLKHPHIVELLETYSSDGMLYMVFEFMDGADLCFEIVKRADAGFVYSEAVASHYMRQILEALRYCHDNNIIHRDVKPHCVLLASKENSAPVKLGGFGVAIQLGESGLVAGGRVGTPHFMAPEVVKREPYGKPVDVWGCGVILFILLSGCLPFYGTKERLFEGIIKGKYKMNPRQWSHISESAKDLVRRMLMLDPAERITVYEALNHPWLKERDRYAYKIHLPETVEQLRKFNARRKLKGAVLAAVSSHKFNSFYGDPPEELPDFSEDPTSSGA</t>
-  </si>
-  <si>
-    <t>FAK1_HUMAN_D0_2IJM_B</t>
-  </si>
-  <si>
-    <t>CHK2_HUMAN_D0_2CN5_A</t>
-  </si>
-  <si>
-    <t>GTGATCGACCCCTCAGAGCTCACTTTTGTCCAAGAGATTGGCAGTGGGCAATTTGGGTTGGTGCATCTGGGCTACTGGCTCAACAAGGACAAGGTGGCTATCAAAACCATTCGGGAAGGGGCTATGTCAGAAGAGGACTTCATAGAGGAGGCTGAAGTAATGATGAAACTCTCTCATCCCAAACTGGTGCAGCTGTATGGGGTGTGCCTGGAGCAGGCCCCCATCTGCCTGGTGTTTGAGTTCATGGAGCACGGCTGCCTGTCAGATTATCTACGCACCCAGCGGGGACTTTTTGCTGCAGAGACCCTGCTGGGCATGTGTCTGGATGTGTGTGAGGGCATGGCCTACCTGGAAGAGGCATGTGTCATCCACAGAGACTTGGCTGCCAGAAATTGTTTGGTGGGAGAAAACCAAGTCATCAAGGTGTCTGACTTTGGGATGACAAGGTTCGTTCTGGATGATCAGTACACCAGTTCCACAGGCACCAAATTCCCGGTGAAGTGGGCATCCCCAGAGGTTTTCTCTTTCAGTCGCTATAGCAGCAAGTCCGATGTGTGGTCATTTGGTGTGCTGATGTGGGAAGTTTTCAGTGAAGGCAAAATCCCGTATGAAAACCGAAGCAACTCAGAGGTGGTGGAAGACATCAGTACCGGATTTCGGTTGTACAAGCCCCGGCTGGCCTCCACACACGTCTACCAGATTATGAATCACTGCTGGAAAGAGAGACCAGAAGATCGGCCAGCCTTCTCCAGACTGCTGCGTCAACTGGCTGAAATTGCAGAATCAGGACTT</t>
-  </si>
-  <si>
-    <t>MSDEEILEKLRSIVSVGDPKKKYTRFEKIGQGASGTVYTAMDVATGQEVAIKQMNLQQQPKKELIINEILVMRENKNPNIVNYLDSYLVGDELWVVMEYLAGGSLTDVVTETCMDEGQIAAVCRECLQALEFLHSNQVIHRDIKSDNILLGMDGSVKLTDFGFCAQITPEQSKRSTMVGTPYWMAPEVVTRKAYGPKVDIWSLGIKAIEMIEGEPPYLNENPLRALYLIATNGTPELQNPEKLSAIFRDFLNRCLEMDVEKRGSAKELLQHQFLKIAKPLSSLTPLIAAAKEATKNNH</t>
-  </si>
-  <si>
-    <t>MSQSKGKKRNPGLKIPKEAFEQPQTSSTPPRDLDSKACISIGNQNFEVKADDLEPIMELGRGAYGVVEKMRHVPSGQIMAVKRIRATVNSQEQKRLLMDLDISMRTVDCPFTVTFYGALFREGDVWICMELMDTSLDKFYKQVIDKGQTIPEDILGKIAVSIVKALEHLHSKLSVIHRDVKPSNVLINALGQVKMCDFGISGYLVDSVAKTIDAGCKPYMAPERINPELNQKGYSVKSDIWSLGITMIELAILRFPYDSWGTPFQQLKQVVEEPSPQLPADKFSAEFVDFTSQCLKKNSKERPTYPELMQHPFFTLHESKGTDVASFVKLILGD</t>
-  </si>
-  <si>
-    <t>DYRK2_HUMAN_D0_3KVW_A</t>
-  </si>
-  <si>
-    <t>QSSKRSSRSVEDDKEGHLVCRIGDWLQERYEIVGNLGEGTFGKVVECLDHARGKSQVALKIIRNVGKYREAARLEINVLKKIKEKDKENKFLCVLMSDWFNFHGHMCIAFELLGKNTFEFLKENNFQPYPLPHVRHMAYQLCHALRFLHENQLTHTDLKPENILFVNSEFETLYNEHKSCEEKSVKNTSIRVADFGSATFDHEHHTTIVATRHYRPPEVILELGWAQPCDVWSIGCILFEYYRGFTLFQTHENREHLVMMEKILGPIPSHMIHRTRKQKYFYKGGLVWDENSSDGRYVKENCKPLKSYMLQDSLEHVQLFDLMRRMLEFDPAQRITLAEALLHPFFAGLTPEERSFHT</t>
-  </si>
-  <si>
-    <t>MK07_HUMAN_D0_4IC7_D</t>
-  </si>
-  <si>
-    <t>ATGCAGACAGTTGGTGTACATTCAATTGTTCAGCAGTTACACAGGAACAGTATTCAGTTTACTGATGGATATGAAGTAAAAGAAGATATTGGAGTTGGCTCCTACTCTGTTTGCAAGAGATGTATACATAAAGCTACAAACATGGAGTTTGCAGTGAAGATTATTGATAAAAGCAAGAGAGACCCAACAGAAGAAATTGAAATTCTTCTTCGTTATGGACAGCATCCAAACATTATCACTCTAAAGGATGTATATGATGATGGAAAGTATGTGTATGTAGTAACAGAACTTATGAAAGGAGGTGAATTGCTGGATAAAATTCTTAGACAAAAATTTTTCTCTGAACGAGAGGCCAGTGCTGTCCTGTTCACTATAACTAAAACCGTTGAATATCTTCACGCACAAGGGGTGGTTCATAGAGACTTGAAACCTAGCAACATTCTTTATGTGGATGAATCTGGTAATCCGGAATCTATTCGAATTTGTGATTTTGGCTTTGCAAAACAGCTGAGAGCGGAAAATGGTCTTCTCATGACTCCTTGTTACACTGCAAATTTTGTTGCACCAGAGGTTTTAAAAAGACAAGGCTATGATGCTGCTTGTGATATATGGAGTCTTGGTGTCCTACTCTATACAATGCTTACCGGTTACACTCCATTTGCAAATGGTCCTGATGATACACCAGAGGAAATATTGGCACGAATAGGTAGCGGAAAATTCTCACTCAGTGGTGGTTACTGGAATTCTGTTTCAGACACAGCAAAGGACCTGGTGTCAAAGATGCTTCATGTAGACCCTCATCAGAGACTGACTGCTGCTCTTGTGCTCAGACATCCTTGGATCGTCCACTGGGACCAACTGCCACAATACCAACTAAACAGACAGGATGCACCACATCTAGTAAAGGGTGCCATGGCAGCTACATATTCTGCTTTGAACCGTAATCAGTCACCAGTTTTGGAACCAGTAGGCCGCTCTACTCTTGCTCAGCGGAGAGGTATTAAAAAAATCACCTCAACAGCCCTG</t>
-  </si>
-  <si>
-    <t>KS6A3_HUMAN_D0_4JG7_A</t>
-  </si>
-  <si>
-    <t>MGKVKATPMTPEQAMKQYMQKLTAFEHHEIFSYPEIYFLGLNAKKRQGMTGGPNNGGYDDDQGSYVQVPHDHVAYRYEVLKVIGKGSFGQVVKAYDHKVHQHVALKMVRNEKRFHRQAAEEIRILEHLRKQDKDNTMNVIHMLENFTFRNHICMTFELLSMNLYELIKKNKFQGFSLPLVRKFAHSILQCLDALHKNRIIHCDLKPENILLKQQGRSGIKVIDFGSSCYEHQRVYTYIQSRFYRAPEVILGARYGMPIDMWSLGCILAELLTGYPLLPGEDEGDQLACMIELLGMPSQKLLDASKRAKNFVSSKGYPRYCTVTTLSDGSVVLNGGRSRRGKLRGPPESREWGNALKGCDDPLFLDFLKQCLEWDPAVRMTPGQALRHPWLRRRLPKPPTGEKTSVKR</t>
-  </si>
-  <si>
-    <t>CAGCAGTTCCCGCAGTTCCACGTCAAGTCCGGCCTGCAGATCAAGAAGAACGCCATCATCGATGACTACAAGGTCACCAGCCAGGTCCTGGGGCTGGGCATCAACGGCAAAGTTTTGCAGATCTTCAACAAGAGGACCCAGGAGAAATTCGCCCTCAAAATGCTTCAGGACTGCCCCAAGGCCCGCAGGGAGGTGGAGCTGCACTGGCGGGCCTCCCAGTGCCCGCACATCGTACGGATCGTGGATGTGTACGAGAATCTGTACGCAGGGAGGAAGTGCCTGCTGATTGTCATGGAATGTTTGGACGGTGGAGAACTCTTTAGCCGAATCCAGGATCGAGGAGACCAGGCATTCACAGAAAGAGAAGCATCCGAAATCATGAAGAGCATCGGTGAGGCCATCCAGTATCTGCATTCAATCAACATTGCCCATCGGGATGTCAAGCCTGAGAATCTCTTATACACCTCCAAAAGGCCCAACGCCATCCTGAAACTCACTGACTTTGGCTTTGCCAAGGAAACCACCAGCCACAACTCTTTGACCACTCCTTGTTATACACCGTACTATGTGGCTCCAGAAGTGCTGGGTCCAGAGAAGTATGACAAGTCCTGTGACATGTGGTCCCTGGGTGTCATCATGTACATCCTGCTGTGTGGGTATCCCCCCTTCTACTCCAACCACGGCCTTGCCATCTCTCCGGGCATGAAGACTCGCATCCGAATGGGCCAGTATGAATTTCCCAACCCAGAATGGTCAGAAGTATCAGAGGAAGTGAAGATGCTCATTCGGAATCTGCTGAAAACAGAGCCCACCCAGAGAATGACCATCACCGAGTTTATGAACCACCCTTGGATCATGCAATCAACAAAGGTCCCTCAAACCCCACTGCACACCAGCCGGGTCCTGAAGGAGGACAAGGAGCGGTGGGAGGATGTCAAGGGGTGTCTTCATGACAAGAACAGCGACCAGGCC</t>
-  </si>
-  <si>
-    <t>CDK2_HUMAN_D0_4BCP_A</t>
-  </si>
-  <si>
-    <t>MP2K4_HUMAN_D0_3ALN_C</t>
-  </si>
-  <si>
-    <t>ACCACCTCACTTGAAGCTTTGCCCACAGGGACAGTGCTGACAGACAAGAGTGGGCGACAGTGGAAGCTGAAGTCCTTCCAGACCAGGGACAACCAGGGCATTCTCTATGAAGCTGCACCCACCTCCACCCTCACCTGTGACTCAGGACCACAGAAGCAAAAGTTCTCACTCAAACTGGATGCCAAGGATGGGCGCTTGTTCAATGAGCAGAACTTCTTCCAGCGGGCCGCCAAGCCTCTGCAAGTCAACAAGTGGAAGAAGCTGTACTCGACCCCACTGCTGGCCATCCCTACCTGCATGGGTTTCGGTGTTCACCAGGACAAATACAGGTTCTTGGTGTTACCCAGCCTGGGGAGGAGCCTTCAGTCGGCCCTGGATGTCAGCCCAAAGCATGTGCTGTCAGAGAGGTCTGTGCTGCAGGTGGCCTGCCGGCTGCTGGATGCCCTGGAGTTCCTCCATGAGAATGAGTATGTTCATGGAAATGTGACAGCTGAAAATATCTTTGTGGATCCAGAGGACCAGAGTCAGGTGACTTTGGCAGGCTATGGCTTCGCCTTCCGCTATTGCCCAAGTGGCAAACACGTGGCCTACGTGGAAGGCAGCAGGAGCCCTCACGAGGGGGACCTTGAGTTCATTAGCATGGACCTGCACAAGGGATGCGGGCCCTCCCGCCGCAGCGACCTCCAGAGCCTGGGCTACTGCATGCTGAAGTGGCTCTACGGGTTTCTGCCATGGACAAATTGCCTTCCCAACACTGAGGACATCATGAAGCAAAAACAGAAGTTTGTTGATAAGCCGGGGCCCTTCGTGGGACCCTGCGGTCACTGGATCAGGCCCTCAGAGACCCTGCAGAAGTACCTGAAGGTGGTGATGGCCCTCACGTATGAGGAGAAGCCGCCCTACGCCATGCTGAGGAACAACCTAGAAGCTTTGCTGCAGGATCTGCGTGTGTCTCCATATGACCCCATTGGCCTCCCGATGGTGCCC</t>
-  </si>
-  <si>
-    <t>TCACCACAGCGGGAGCCACAGCGAGTATCCCATGAGCAGTTCCGGGCTGCCCTGCAGCTGGTGGTGGACCCAGGCGACCCCCGCTCCTACCTGGACAACTTCATCAAGATTGGCGAGGGCTCCACGGGCATCGTGTGCATCGCCACCGTGCGCAGCTCGGGCAAGCTGGTGGCCGTCAAGAAGATGGACCTGCGCAAGCAGCAGAGGCGCGAGCTGCTCTTCAACGAGGTGGTAATCATGAGGGACTACCAGCACGAGAATGTGGTGGAGATGTACAACAGCTACCTGGTGGGGGACGAGCTCTGGGTGGTCATGGAGTTCCTGGAAGGAGGCGCCCTCACCGACATCGTCACCCACACCAGGATGAACGAGGAGCAGATCGCGGCCGTGTGCCTTGCAGTGCTGCAGGCCCTGTCGGTGCTCCACGCCCAGGGCGTCATCCACCGGGACATCAAGAGCGACTCGATCCTGCTGACCCATGATGGCAGGGTGAAGCTGTCAGACTTTGGGTTCTGCGCCCAGGTGAGCAAGGAAGTGCCCCGAAGGAAGTCGCTGGTCGGCACGCCCTACTGGATGGCCCCAGAGCTCATCTCCCGCCTTCCCTACGGGCCAGAGGTAGACATCTGGTCGCTGGGGATAATGGTGATTGAGATGGTGGACGGAGAGCCCCCCTACTTCAACGAGCCACCCCTCAAAGCCATGAAGATGATTCGGGACAACCTGCCACCCCGACTGAAGAACCTGCACAAGGTGTCGCCATCCCTGAAGGGCTTCCTGGACCGCCTGCTGGTGCGAGACCCTGCCCAGCGGGCCACGGCAGCCGAGCTGCTGAAGCACCCATTCCTGGCCAAGGCAGGGCCGCCTGCCAGCATCGTGCCCCTCATGCGCCAGAACCGCACCAGA</t>
-  </si>
-  <si>
-    <t>SIESSGKLKISPEQHWDFTAEDLKDLGEIGRGAYGSVNKMVHKPSGQIMAVKRIRSTVDEKEQKQLLMDLDVVMRSSDCPYIVQFYGALFREGDCWICMELMSTSFDKFYKYVYSVLDDVIPEEILGKITLATVKALNHLKENLKIIHRDIKPSNILLDRSGNIKLCDFGISGQLVDSIAKTRDAGCRPYMAPERIDPSASRQGYDVRSDVWSLGITLYELATGRFPYPKWNSVFDQLTQVVKGDPPQLSNSEEREFSPSFINFVNLCLTKDESKRPKYKELLKHPFILMYEERAVEVACYVCKILDQMPATPSSPMYVD</t>
-  </si>
-  <si>
-    <t>TDSFSGRFEDVYQLQEDVLGEGAHARVQTCINLITSQEYAVKIIEKQPGHIRSRVFREVEMLYQCQGHRNVLELIEFFEEEDRFYLVFEKMRGGSILSHIHKRRHFNELEASVVVQDVASALDFLHNKGIAHRDLKPENILCEHPNQVSPVKICDFDLGSGIKLNGDCSPISTPELLTPCGSAEYMAPEVVEAFSEEASIYDKRCDLWSLGVILYILLSGYPPFVGRCGSDCGWDRGEACPACQNMLFESIQEGKYEFPDKDWAHISCAAKDLISKLLVRDAKQRLSAAQVLQHPWVQGCAPENTLPTPMVLQR</t>
+    <t>KEKEPLESQYQVGPLLGSGGFGSVYSGIRVSDNLPVAIKHVEKDRISDWGELPNGTRVPMEVVLLKKVSSGFSGVIRLLDWFERPDSFVLILERPEPVQDLFDFITERGALQEELARSFFWQVLEAVRHCHNCGVLHRDIKDENILIDLNRGELKLIDFGSGALLKDTVYTDFDGTRVYSPPEWIRYHRYHGRSAAVWSLGILLYDMVCGDIPFEHDEEIIGGQVFFRQRVSSECQHLIRWCLALRPSDRPTFEEIQNHPWMQDVLLPQETAEIHLHSLSPGPSK</t>
+  </si>
+  <si>
+    <t>VEDHYEMGEELGSGQFAIVRKCRQKGTGKEYAAKFIKKRRLSSSRRGVSREEIEREVNILREIRHPNIITLHDIFENKTDVVLILELVSGGELFDFLAEKESLTEDEATQFLKQILDGVHYLHSKRIAHFDLKPENIMLLDKNVPNPRIKLIDFGIAHKIEAGNEFKNIFGTPEFVAPEIVNYEPLGLEADMWSIGVITYILLSGASPFLGETKQETLTNISAVNYDFDEEYFSNTSELAKDFIRRLLVKDPKRRMTIAQSLEHSWIKAIRRRNVRGEDSG</t>
+  </si>
+  <si>
+    <t>MET_HUMAN_D0_4EEV_A</t>
+  </si>
+  <si>
+    <t>AACCAGTTCTACAGTGTGGAAGTGGGAGACTCAACCTTCACAGTTCTCAAGCGCTACCAGAATCTAAAGCCTATTGGCTCTGGGGCTCAGGGCATAGTTTGTGCCGCGTATGATGCTGTCCTTGACAGAAATGTGGCCATTAAGAAGCTCAGCAGACCCTTTCAGAACCAAACACATGCCAAGAGAGCGTACCGGGAGCTGGTCCTCATGAAGTGTGTGAACCATAAAAACATTATTAGTTTATTAAATGTCTTCACACCCCAGAAAACGCTGGAGGAGTTCCAAGATGTTTACTTAGTAATGGAACTGATGGATGCCAACTTATGTCAAGTGATTCAGATGGAATTAGACCATGAGCGAATGTCTTACCTGCTGTACCAAATGTTGTGTGGCATTAAGCACCTCCATTCTGCTGGAATTATTCACAGGGATTTAAAACCAAGTAACATTGTAGTCAAGTCTGATTGCACATTGAAAATCCTGGACTTTGGACTGGCCAGGACAGCAGGCACAAGCTTCATGATGACTCCATATGTGGTGACACGTTATTACAGAGCCCCTGAGGTCATCCTGGGGATGGGCTACAAGGAGAACGTGGATATATGGTCTGTGGGATGCATTATGGGAGAAATGGTTCGCCACAAAATCCTCTTTCCAGGAAGGGACTATATTGACCAGTGGAATAAGGTAATTGAACAACTAGGAACACCATGTCCAGAATTCATGAAGAAATTGCAACCCACAGTAAGAAACTATGTGGAGAATCGGCCCAAGTATGCGGGACTCACCTTCCCCAAACTCTTCCCAGATTCCCTCTTCCCAGCGGACTCCGAGCACAATAAACTCAAAGCCAGCCAAGCCAGGGACTTGTTGTCAAAGATGCTAGTGATTGACCCAGCAAAAAGAATATCAGTGGACGACGCCTTACAGCATCCCTACATCAACGTCTGGTATGACCCAGCCGAAGTGGAGGCGCCTCCACCTCAGATATATGACAAGCAGTTGGATGAAAGAGAACACACAATTGAAGAATGGAAAGAACTTATCTACAAGGAAGTAATGAAT</t>
+  </si>
+  <si>
+    <t>MP2K1_HUMAN_D0_3MBL_A</t>
+  </si>
+  <si>
+    <t>ETKYTVDKRFGMDFKEIELIGSGGFGQVFKAKHRIDGKTYVIKRVKYNNEKAEREVKALAKLDHVNIVHYNGCWDGFDYDPETSDDSLESSDYDPENSKNSSRSKTKCLFIQMEFCDKGTLEQWIEKRRGEKLDKVLALELFEQITKGVDYIHSKKLIHRDLKPSNIFLVDTKQVKIGDFGLVTSLKNDGKRTRSKGTLRYMSPEQISSQDYGKEVDLYALGLILAELLHVCDTAFETSKFFTDLRDGIISDIFDKKEKTLLQKLLSKKPEDRPNTSEILRTLTVWKKSPEKNERHTC</t>
+  </si>
+  <si>
+    <t>CDKL1_HUMAN_D0_4AGU_C</t>
+  </si>
+  <si>
+    <t>MARK3_HUMAN_D0_2QNJ_A</t>
+  </si>
+  <si>
+    <t>NLVFSDGYVVKETIGVGSYSECKRCVHKATNMEYAVKVIDKSKRDPSEEIEILLRYGQHPNIITLKDVYDDGKHVYLVTELMRGGELLDKILRQKFFSEREASFVLHTIGKTVEYLHSQGVVHRDLKPSNILYVDESGNPECLRICDFGFAKQLRAENGLLMTPCYTANFVAPEVLKRQGYDEGCDIWSLGILLYTMLAGYTPFANGPSDTPEEILTRIGSGKFTLSGGNWNTVSETAKDLVSKMLHVDPHQRLTAKQVLQHPWVTQKDKLPQSQLSHQDLQLVKGAMAATYSALNSSKPTPQLKPIESSILAQRRVRKLPSTTL</t>
+  </si>
+  <si>
+    <t>GGTGTTGTGACACATGAGCAGTTCAAGGCTGCGCTCAGGATGGTGGTGGACCAGGGTGACCCCCGGCTGCTGCTGGACAGCTACGTGAAGATTGGCGAGGGCTCCACCGGCATCGTCTGCTTGGCCCGGGAGAAGCACTCGGGCCGCCAGGTGGCCGTCAAGATGATGGACCTCAGGAAGCAGCAGCGCAGGGAGCTGCTCTTCAACGAGGTGGTGATCATGCGGGACTACCAGCACTTCAACGTGGTGGAGATGTACAAGAGCTACCTGGTGGGCGAGGAGCTGTGGGTGCTCATGGAGTTCCTGCAGGGAGGAGCCCTCACAGACATCGTCTCCCAAGTCAGGCTGAATGAGGAGCAGATTGCCACTGTGTGTGAGGCTGTGCTGCAGGCCCTGGCCTACCTGCATGCTCAGGGTGTCATCCACCGGGACATCAAGAGTGACTCCATCCTGCTGACCCTCGATGGCAGGGTGAAGCTCTCGGACTTCGGATTCTGTGCTCAGATCAGCAAAGACGTCCCTAAGAGGAAGTCCCTGGTGGGAACCCCCTACTGGATGGCTCCTGAAGTGATCTCCAGGTCTTTGTATGCCACTGAGGTGGATATCTGGTCTCTGGGCATCATGGTGATTGAGATGGTAGATGGGGAGCCACCGTACTTCAGTGACTCCCCAGTGCAAGCCATGAAGAGGCTCCGGGACAGCCCCCCACCCAAGCTGAAAAACTCTCACAAGGTCTCCCCAGTGCTGCGAGACTTCCTGGAGCGGATGCTGGTGCGGGACCCCCAAGAGAGAGCCACAGCCCAGGAGCTCCTAGACCACCCCTTCCTGCTGCAGACAGGGCTACCTGAGTGCCTGGTGCCCCTGATCCAGCTCTACCGAAAGCAGACCTCCACCTGC</t>
+  </si>
+  <si>
+    <t>CACATTGGAAACTACCGGCTCCTCAAGACCATTGGCAAGGGTAATTTTGCCAAGGTGAAGTTGGCCCGACACATCCTGACTGGGAAAGAGGTAGCTGTGAAGATCATTGACAAGACTCAACTGAACTCCTCCAGCCTCCAGAAACTATTCCGCGAAGTAAGAATAATGAAGGTTTTGAATCATCCCAACATAGTTAAATTATTTGAAGTGATTGAGACTGAGAAAACGCTCTACCTTGTCATGGAGTACGCTAGTGGCGGAGAGGTATTTGATTACCTAGTGGCTCATGGCAGGATGAAAGAAAAAGAGGCTCGAGCCAAATTCCGCCAGATAGTGTCTGCTGTGCAGTACTGTCACCAGAAGTTTATTGTCCATAGAGACTTAAAGGCAGAAAACCTGCTCTTGGATGCTGATATGAACATCAAGATTGCAGACTTTGGCTTCAGCAATGAATTCACCTTTGGGAACAAGCTGGACACCTTCTGTGGCAGTCCCCCTTATGCTGCCCCAGAACTCTTCCAGGGCAAAAAATATGATGGACCCGAGGTGGATGTGTGGAGCCTAGGAGTTATCCTCTATACACTGGTCAGCGGATCCCTGCCTTTTGATGGACAGAACCTCAAGGAGCTGCGGGAACGGGTACTGAGGGGAAAATACCGTATTCCATTCTACATGTCCACGGACTGTGAAAACCTGCTTAAGAAATTTCTCATTCTTAATCCCAGCAAGAGAGGCACTTTAGAGCAAATCATGAAAGATCGATGGATGAATGTGGGTCACGAAGATGATGAACTAAAGCCTTACGTGGAGCCACTCCCTGACTACAAGGACCCCCGGCGGACAGAGCTGATGGTGTCCATGGGTTATACACGGGAAGAGATCCAGGACTCGCTGGTGGGCCAGAGATACAACGAGGTGATGGCCACCTATCTGCTCCTGGGCTAC</t>
   </si>
   <si>
     <t>ST17B_HUMAN_D0_3LM0_A</t>
   </si>
   <si>
-    <t>MPGPAAGSRARVYAEVNSLRSREYWDYEAHVPSWGNQDDYQLVRKLGRGKYSEVFEAINITNNERVVVKILKPVKKKKIKREVKILENLRGGTNIIKLIDTVKDPVSKTPALVFEYINNTDFKQLYQILTDFDIRFYMYELLKALDYCHSKGIMHRDVKPHNVMIDHQQKKLRLIDWGLAEFYHPAQEYNVRVASRYFKGPELLVDYQMYDYSLDMWSLGCMLASMIFRREPFFHGQDNYDQLVRIAKVLGTEELYGYLKKYHIDLDPHFNDILGQHSRKRWENFIHSENRHLVSPEALDLLDKLLRYDHQQRLTAKEAMEHPYFYPVVKEQSQ</t>
-  </si>
-  <si>
-    <t>AAGAGGCAGTGGGCTTTGGAAGACTTTGAAATTGGTCGCCCTCTGGGTAAAGGAAAGTTTGGTAATGTTTATTTGGCAAGAGAAAAGCAAAGCAAGTTTATTCTGGCTCTTAAAGTGTTATTTAAAGCTCAGCTGGAGAAAGCCGGAGTGGAGCATCAGCTCAGAAGAGAAGTAGAAATACAGTCCCACCTTCGGCATCCTAATATTCTTAGACTGTATGGTTATTTCCATGATGCTACCAGAGTCTACCTAATTCTGGAATATGCACCACTTGGAACAGTTTATAGAGAACTTCAGAAACTTTCAAAGTTTGATGAGCAGAGAACTGCTACTTATATAACAGAATTGGCAAATGCCCTGTCTTACTGTCATTCGAAGAGAGTTATTCATAGAGACATTAAGCCAGAGAACTTACTTCTTGGATCAGCTGGAGAGCTTAAAATTGCAGATTTTGGGTGGTCAGTACATGCTCCATCTTCCAGGAGGACCACTCTCTGTGGCACCCTGGACTACCTGCCCCCTGAAATGATTGAAGGTCGGATGCATGATGAGAAGGTGGATCTCTGGAGCCTTGGAGTTCTTTGCTATGAATTTTTAGTTGGGAAGCCTCCTTTTGAGGCAAACACATACCAAGAGACCTACAAAAGAATATCACGGGTTGAATTCACATTCCCTGACTTTGTAACAGAGGGAGCCAGGGACCTCATTTCAAGACTGTTGAAGCATAATCCCAGCCAGAGGCCAATGCTCAGAGAAGTACTTGAACACCCCTGGATCACAGCAAATTCATCAAAACCATCA</t>
-  </si>
-  <si>
-    <t>ATGGAGCTACGTGTGGGGAACAAGTACCGCCTGGGACGGAAGATCGGGAGCGGGTCCTTCGGAGATATCTACCTGGGTGCCAACATCGCCTCTGGTGAGGAAGTCGCCATCAAGCTGGAGTGTGTGAAGACAAAGCACCCCCAGCTGCACATCGAGAGCAAGTTCTACAAGATGATGCAGGGTGGCGTGGGGATCCCGTCCATCAAGTGGTGCGGAGCTGAGGGCGACTACAACGTGATGGTCATGGAGCTGCTGGGGCCTAGCCTCGAGGACCTGTTCAACTTCTGTTCCCGCAAATTCAGCCTCAAGACGGTGCTGCTCTTGGCCGACCAGATGATCAGCCGCATCGAGTATATCCACTCCAAGAACTTCATCCACCGGGACGTCAAGCCCGACAACTTCCTCATGGGGCTGGGGAAGAAGGGCAACCTGGTCTACATCATCGACTTCGGCCTGGCCAAGAAGTACCGGGACGCCCGCACCCACCAGCACATTCCCTACCGGGAAAACAAGAACCTGACCGGCACGGCCCGCTACGCTTCCATCAACACGCACCTGGGCATTGAGCAAAGCCGTCGAGATGACCTGGAGAGCCTGGGCTACGTGCTCATGTACTTCAACCTGGGCTCCCTGCCCTGGCAGGGGCTCAAAGCAGCCACCAAGCGCCAGAAGTATGAACGGATCAGCGAGAAGAAGATGTCAACGCCCATCGAGGTCCTCTGCAAAGGCTATCCCTCCGAATTCTCAACATACCTCAACTTCTGCCGCTCCCTGCGGTTTGACGACAAGCCCGACTACTCTTACCTACGTCAGCTCTTCCGCAACCTCTTCCACCGGCAGGGCTTCTCCTATGACTACGTCTTTGACTGGAACATGCTGAAA</t>
-  </si>
-  <si>
-    <t>MK03_HUMAN_D0_2ZOQ_B</t>
-  </si>
-  <si>
-    <t>ATGTCTCAGTCGAAAGGCAAGAAGCGAAACCCTGGCCTTAAAATTCCAAAAGAAGCATTTGAACAACCTCAGACCAGTTCCACACCACCTCGAGATTTAGACTCCAAGGCTTGCATTTCTATTGGAAATCAGAACTTTGAGGTGAAGGCAGATGACCTGGAGCCTATAATGGAACTGGGACGAGGTGCGTACGGGGTGGTGGAGAAGATGCGGCACGTGCCCAGCGGGCAGATCATGGCAGTGAAGCGGATCCGAGCCACAGTAAATAGCCAGGAACAGAAACGGCTACTGATGGATTTGGATATTTCCATGAGGACGGTGGACTGTCCATTCACTGTCACCTTTTATGGCGCACTGTTTCGGGAGGGTGATGTGTGGATCTGCATGGAGCTCATGGATACATCACTAGATAAATTCTACAAACAAGTTATTGATAAAGGCCAGACAATTCCAGAGGACATCTTAGGGAAAATAGCAGTTTCTATTGTAAAAGCATTAGAACATTTACATAGTAAGCTGTCTGTCATTCACAGAGACGTCAAGCCTTCTAATGTACTCATCAATGCTCTCGGTCAAGTGAAGATGTGCGATTTTGGAATCAGTGGCTACTTGGTGGACTCTGTTGCTAAAACAATTGATGCAGGTTGCAAACCATACATGGCCCCTGAAAGAATAAACCCAGAGCTCAACCAGAAGGGATACAGTGTGAAGTCTGACATTTGGAGTCTGGGCATCACGATGATTGAGTTGGCCATCCTTCGATTTCCCTATGATTCATGGGGAACTCCATTTCAGCAGCTCAAACAGGTGGTAGAGGAGCCATCGCCACAACTCCCAGCAGACAAGTTCTCTGCAGAGTTTGTTGACTTTACCTCACAGTGCTTAAAGAAGAATTCCAAAGAACGGCCTACATACCCAGAGCTAATGCAACATCCATTTTTCACCCTACATGAATCCAAAGGAACAGATGTGGCATCTTTTGTAAAACTGATTCTTGGAGAC</t>
-  </si>
-  <si>
-    <t>TCAACCAGGGATTATGAGATTCAAAGAGAAAGAATAGAACTTGGACGATGTATTGGAGAAGGCCAATTTGGAGATGTACATCAAGGCATTTATATGAGTCCAGAGAATCCAGCTTTGGCGGTTGCAATTAAAACATGTAAAAACTGTACTTCGGACAGCGTGAGAGAGAAATTTCTTCAAGAAGCCTTAACAATGCGTCAGTTTGACCATCCTCATATTGTGAAGCTGATTGGAGTCATCACAGAGAATCCTGTCTGGATAATCATGGAGCTGTGCACACTTGGAGAGCTGAGGTCATTTTTGCAAGTAAGGAAATACAGTTTGGATCTAGCATCTTTGATCCTGTATGCCTATCAGCTTAGTACAGCTCTTGCATATCTAGAGAGCAAAAGATTTGTACACAGGGACATTGCTGCTCGGAATGTTCTGGTGTCCTCAAATGATTGTGTAAAATTAGGAGACTTTGGATTATCCCGATATATGGAAGATAGTACTTACTACAAAGCTTCCAAAGGAAAATTGCCTATTAAATGGATGGCTCCAGAGTCAATCAATTTTCGACGTTTTACCTCAGCTAGTGACGTATGGATGTTTGGTGTGTGTATGTGGGAGATACTGATGCATGGTGTGAAGCCTTTTCAAGGAGTGAAGAACAATGATGTAATCGGTCGAATTGAAAATGGGGAAAGATTACCAATGCCTCCAAATTGTCCTCCTACCCTCTACAGCCTTATGACGAAATGCTGGGCCTATGACCCCAGCAGGCGGCCCAGGTTTACTGAACTTAAAGCTCAGCTCAGCACAATCCTGGAGGAAGAGAAGGCTCAGCAAGAAGAG</t>
-  </si>
-  <si>
-    <t>DPEELFTKLEKIGKGSFGEVFKGIDNRTQKVVAIKIIDLEEAEDEIEDIQQEITVLSQCDSPYVTKYYGSYLKDTKLWIIMEYLGGGSALDLLEPGPLDETQIATILREILKGLDYLHSEKKIHRDIKAANVLLSEHGEVKLADFGVAGQLTDTQIKRNTFVGTPFWMAPEVIKQSAYDSKADIWSLGITAIELARGEPPHSELHPMKVLFLIPKNNPPTLEGNYSKPLKEFVEACLNKEPSFRPTAKELLKHKFILRNAKKTSYLTELID</t>
-  </si>
-  <si>
-    <t>MAPK3_HUMAN_D0_3FXW_A</t>
-  </si>
-  <si>
-    <t>AAGCAGTACGAACACGTGAAGAGGGACCTGAACCCCGAAGACTTTTGGGAGATTATAGGAGAACTGGGCGACGGAGCCTTTGGGAAAGTGTACAAGGCCCAGAATAAAGAGACCAGTGTTTTAGCTGCTGCAAAAGTGATTGACACTAAATCTGAAGAAGAACTTGAAGATTACATGGTAGAGATTGACATATTAGCATCTTGTGATCACCCAAATATAGTCAAGCTTCTAGATGCCTTCTATTATGAGAACAATCTTTGGATCCTCATTGAATTTTGTGCAGGTGGAGCAGTAGATGCTGTGATGCTTGAACTTGAGAGACCATTAACTGAGTCCCAAATACAAGTAGTTTGCAAGCAGACTTTAGATGCATTGAACTACTTACATGATAATAAGATCATCCACAGAGATCTGAAGGCTGGCAACATTCTCTTTACCTTAGATGGAGATATCAAATTGGCGGATTTTGGAGTATCAGCTAAAAACATGAGGACAATTCAAAGAAGAGATTCCTTTATTGGTACACCATATTGGATGGCTCCTGAAGTAGTCATGTGTGAAACATCTAAGGACAGACCCTATGACTACAAAGCTGATGTTTGGTCCCTGGGTATCACTTTAATAGAAATGGCTGAGATAGAACCACCTCATCATGAATTAAATCCAATGCGAGTGCTGCTAAAAATAGCAAAATCTGAGCCACCTACATTAGCACAGCCATCCAGATGGTCTTCAAATTTTAAGGACTTTCTAAAGAAATGCTTAGAAAAGAATGTGGATGCCAGGTGGACTACATCTCAGCTGCTGCAGCATCCCTTTGTTACTGTTGATTCCAACAAACCCATCCGAGAATTGATTGCAGAGGCGAAGGCTGAAGTAACAGAAGAAGTTGAAGATGGCAAAGAG</t>
-  </si>
-  <si>
-    <t>ATGCCTTCCCGGGCTGAGGACTATGAAGTGTTGTACACCATTGGCACAGGCTCCTACGGCCGCTGCCAGAAGATCCGGAGGAAGAGTGATGGCAAGATATTAGTTTGGAAAGAACTTGACTATGGCTCCATGACAGAAGCTGAGAAACAGATGCTTGTTTCTGAAGTGAATTTGCTTCGTGAACTGAAACATCCAAACATCGTTCGTTACTATGATCGGATTATTGACCGGACCAATACAACACTGTACATTGTAATGGAATATTGTGAAGGAGGGGATCTGGCTAGTGTAATTACAAAGGGAACCAAGGAAAGGCAATACTTAGATGAAGAGTTTGTTCTTCGAGTGATGACTCAGTTGACTCTGGCCCTGAAGGAATGCCACAGACGAAGTGATGGTGGTCATACCGTATTGCATCGGGATCTGAAACCAGCCAATGTTTTCCTGGATGGCAAGCAAAACGTCAAGCTTGGAGACTTTGGGCTAGCTAGAATATTAAACCATGACACGAGTTTTGCAAAAACATTTGTTGGCACACCTTATTACATGTCTCCTGAACAAATGAATCGCATGTCCTACAATGAGAAATCAGATATCTGGTCATTGGGCTGCTTGCTGTATGAGTTATGTGCATTAATGCCTCCATTTACAGCTTTTAGCCAGAAAGAACTCGCTGGGAAAATCAGAGAAGGCAAATTCAGGCGAATTCCATACCGTTACTCTGATGAATTGAATGAAATTATTACGAGGATGTTAAACTTAAAGGATTACCATCGACCTTCTGTTGAAGAAATTCTTGAGAACCCTTTAATA</t>
-  </si>
-  <si>
-    <t>STK3_HUMAN_D0_4LG4_B</t>
-  </si>
-  <si>
-    <t>CACCAGCTGCAGCCCCGGCGGGTGTCATTCCGGGGCGAGGCCTCAGAGACTCTGCAGAGCCCTGGGTATGACCCAAGCCGGCCAGAGTCCTTCTTCCAGCAGAGCTTCCAGAGGCTCAGCCGCCTGGGCCATGGCTCCTACGGAGAGGTCTTCAAGGTGCGCTCCAAGGAGGACGGCCGGCTCTATGCGGTAAAGCGTTCCATGTCACCATTCCGGGGCCCCAAGGACCGGGCCCGCAAGTTGGCCGAGGTGGGCAGCCACGAGAAGGTGGGGCAGCACCCATGCTGCGTGCGGCTGGAGCAGGCCTGGGAGGAGGGCGGCATCCTGTACCTGCAGACGGAGCTGTGCGGGCCCAGCCTGCAGCAACACTGTGAGGCCTGGGGTGCCAGCCTGCCTGAGGCCCAGGTCTGGGGCTACCTGCGGGACACGCTGCTTGCCCTGGCCCATCTGCACAGCCAGGGCCTGGTGCACCTTGATGTCAAGCCTGCCAACATCTTCCTGGGGCCCCGGGGCCGCTGCAAGCTGGGTGACTTCGGACTGCTGGTGGAGCTGGGTACAGCAGGAGCTGGTGAGGTCCAGGAGGGAGACCCCCGCTACATGGCCCCCGAGCTGCTGCAGGGCTCCTATGGGACAGCAGCGGATGTGTTCAGTCTGGGCCTCACCATCCTGGAAGTGGCATGCAACATGGAGCTGCCCCACGGTGGGGAGGGCTGGCAGCAGCTGCGCCAGGGCTACCTGCCCCCTGAGTTCACTGCCGGTCTGTCTTCCGAGCTGCGTTCTGTCCTTGTCATGATGCTGGAGCCAGACCCCAAGCTGCGGGCCACGGCCGAGGCCCTGCTGGCACTGCCTGTGTTGAGGCAGCCG</t>
-  </si>
-  <si>
-    <t>KEKEPLESQYQVGPLLGSGGFGSVYSGIRVSDNLPVAIKHVEKDRISDWGELPNGTRVPMEVVLLKKVSSGFSGVIRLLDWFERPDSFVLILERPEPVQDLFDFITERGALQEELARSFFWQVLEAVRHCHNCGVLHRDIKDENILIDLNRGELKLIDFGSGALLKDTVYTDFDGTRVYSPPEWIRYHRYHGRSAAVWSLGILLYDMVCGDIPFEHDEEIIGGQVFFRQRVSSECQHLIRWCLALRPSDRPTFEEIQNHPWMQDVLLPQETAEIHLHSLSPGPSK</t>
-  </si>
-  <si>
-    <t>VEDHYEMGEELGSGQFAIVRKCRQKGTGKEYAAKFIKKRRLSSSRRGVSREEIEREVNILREIRHPNIITLHDIFENKTDVVLILELVSGGELFDFLAEKESLTEDEATQFLKQILDGVHYLHSKRIAHFDLKPENIMLLDKNVPNPRIKLIDFGIAHKIEAGNEFKNIFGTPEFVAPEIVNYEPLGLEADMWSIGVITYILLSGASPFLGETKQETLTNISAVNYDFDEEYFSNTSELAKDFIRRLLVKDPKRRMTIAQSLEHSWIKAIRRRNVRGEDSG</t>
-  </si>
-  <si>
-    <t>ACCGACAGCTTCTCGGGCAGGTTTGAAGACGTCTACCAGCTGCAGGAAGATGTGCTGGGGGAGGGCGCTCATGCCCGAGTGCAGACCTGCATCAACCTGATCACCAGCCAGGAGTACGCCGTCAAGATCATTGAGAAGCAGCCAGGCCACATTCGGAGCAGGGTTTTCAGGGAGGTGGAGATGCTGTACCAGTGCCAGGGACACAGGAACGTCCTAGAGCTGATTGAGTTCTTCGAGGAGGAGGACCGCTTCTACCTGGTGTTTGAGAAGATGCGGGGAGGCTCCATCCTGAGCCACATCCACAAGCGCCGGCACTTCAACGAGCTGGAGGCCAGCGTGGTGGTGCAGGACGTGGCCAGCGCCTTGGACTTTCTGCATAACAAAGGCATCGCCCACAGGGACCTAAAGCCGGAAAACATCCTCTGTGAGCACCCCAACCAGGTCTCCCCCGTGAAGATCTGTGACTTCGACCTGGGCAGCGGCATCAAACTCAACGGGGACTGCTCCCCTATCTCCACCCCGGAGCTGCTCACTCCGTGCGGCTCGGCGGAGTACATGGCCCCGGAGGTAGTGGAGGCCTTCAGCGAGGAGGCTAGCATCTACGACAAGCGCTGCGACCTGTGGAGCCTGGGCGTCATCTTGTATATCCTACTCAGCGGCTACCCGCCCTTCGTGGGCCGCTGTGGCAGCGACTGCGGCTGGGACCGCGGCGAGGCCTGCCCTGCCTGCCAGAACATGCTGTTTGAGAGCATCCAGGAGGGCAAGTACGAGTTCCCCGACAAGGACTGGGCCCACATCTCCTGCGCTGCCAAAGACCTCATCTCCAAGCTGCTGGTCCGTGACGCCAAGCAGAGGCTGAGTGCCGCCCAAGTCCTGCAGCACCCCTGGGTTCAGGGGTGCGCCCCGGAGAACACCTTGCCCACTCCCATGGTCCTGCAGAGG</t>
-  </si>
-  <si>
-    <t>MET_HUMAN_D0_4EEV_A</t>
-  </si>
-  <si>
-    <t>MSSFLPEGGCYELLTVIGKGFEDLMTVNLARYKPTGEYVTVRRINLEACSNEMVTFLQGELHVSKLFNHPNIVPYRATFIADNELWVVTSFMAYGSAKDLICTHFMDGMNELAIAYILQGVLKALDYIHHMGYVHRSVKASHILISVDGKVYLSGLRSNLSMISHGQRQRVVHDFPKYSVKVLPWLSPEVLQQNLQGYDAKSDIYSVGITACELANGHVPFKDMPATQMLLEKLNGTVPCLLDTSTIPAEELTMSPSRSVANSGLSDSLTTSTPRPSNGDSPSHPYHRTFSPHFHHFVEQCLQRNPDARPSASTLLNHSFFKQIKRRASEVLPELLRPVTPITNFEGSQSQDHSGIFGLVTNLEELEVDDWEF</t>
-  </si>
-  <si>
-    <t>MP2K1_HUMAN_D0_3MBL_A</t>
-  </si>
-  <si>
-    <t>ETKYTVDKRFGMDFKEIELIGSGGFGQVFKAKHRIDGKTYVIKRVKYNNEKAEREVKALAKLDHVNIVHYNGCWDGFDYDPETSDDSLESSDYDPENSKNSSRSKTKCLFIQMEFCDKGTLEQWIEKRRGEKLDKVLALELFEQITKGVDYIHSKKLIHRDLKPSNIFLVDTKQVKIGDFGLVTSLKNDGKRTRSKGTLRYMSPEQISSQDYGKEVDLYALGLILAELLHVCDTAFETSKFFTDLRDGIISDIFDKKEKTLLQKLLSKKPEDRPNTSEILRTLTVWKKSPEKNERHTC</t>
-  </si>
-  <si>
-    <t>CDKL1_HUMAN_D0_4AGU_C</t>
-  </si>
-  <si>
-    <t>MARK3_HUMAN_D0_2QNJ_A</t>
-  </si>
-  <si>
-    <t>MSGPRAGFYRQELNKTVWEVPQRLQGLRPVGSGAYGSVCSAYDARLRQKVAVKKLSRPFQSLIHARRTYRELRLLKHLKHENVIGLLDVFTPATSIEDFSEVYLVTTLMGADLNNIVKCQALSDEHVQFLVYQLLRGLKYIHSAGIIHRDLKPSNVAVNEDCELRILDFGLARQADEEMTGYVATRWYRAPEIMLNWMHYNQTVDIWSVGCIMAELLQGKALFPGSDYIDQLKRIMEVVGTPSPEVLAKISSEHARTYIQSLPPMPQKDLSSIFRGANPLAIDLLGRMLVLDSDQRVSAAEALAHAYFSQYHDPEDEPEAEPYDESVEAKERTLEEWKELTYQEVLSFKPPEPPKPPGSLEIEQ</t>
-  </si>
-  <si>
-    <t>NLVFSDGYVVKETIGVGSYSECKRCVHKATNMEYAVKVIDKSKRDPSEEIEILLRYGQHPNIITLKDVYDDGKHVYLVTELMRGGELLDKILRQKFFSEREASFVLHTIGKTVEYLHSQGVVHRDLKPSNILYVDESGNPECLRICDFGFAKQLRAENGLLMTPCYTANFVAPEVLKRQGYDEGCDIWSLGILLYTMLAGYTPFANGPSDTPEEILTRIGSGKFTLSGGNWNTVSETAKDLVSKMLHVDPHQRLTAKQVLQHPWVTQKDKLPQSQLSHQDLQLVKGAMAATYSALNSSKPTPQLKPIESSILAQRRVRKLPSTTL</t>
-  </si>
-  <si>
-    <t>GGTGTTGTGACACATGAGCAGTTCAAGGCTGCGCTCAGGATGGTGGTGGACCAGGGTGACCCCCGGCTGCTGCTGGACAGCTACGTGAAGATTGGCGAGGGCTCCACCGGCATCGTCTGCTTGGCCCGGGAGAAGCACTCGGGCCGCCAGGTGGCCGTCAAGATGATGGACCTCAGGAAGCAGCAGCGCAGGGAGCTGCTCTTCAACGAGGTGGTGATCATGCGGGACTACCAGCACTTCAACGTGGTGGAGATGTACAAGAGCTACCTGGTGGGCGAGGAGCTGTGGGTGCTCATGGAGTTCCTGCAGGGAGGAGCCCTCACAGACATCGTCTCCCAAGTCAGGCTGAATGAGGAGCAGATTGCCACTGTGTGTGAGGCTGTGCTGCAGGCCCTGGCCTACCTGCATGCTCAGGGTGTCATCCACCGGGACATCAAGAGTGACTCCATCCTGCTGACCCTCGATGGCAGGGTGAAGCTCTCGGACTTCGGATTCTGTGCTCAGATCAGCAAAGACGTCCCTAAGAGGAAGTCCCTGGTGGGAACCCCCTACTGGATGGCTCCTGAAGTGATCTCCAGGTCTTTGTATGCCACTGAGGTGGATATCTGGTCTCTGGGCATCATGGTGATTGAGATGGTAGATGGGGAGCCACCGTACTTCAGTGACTCCCCAGTGCAAGCCATGAAGAGGCTCCGGGACAGCCCCCCACCCAAGCTGAAAAACTCTCACAAGGTCTCCCCAGTGCTGCGAGACTTCCTGGAGCGGATGCTGGTGCGGGACCCCCAAGAGAGAGCCACAGCCCAGGAGCTCCTAGACCACCCCTTCCTGCTGCAGACAGGGCTACCTGAGTGCCTGGTGCCCCTGATCCAGCTCTACCGAAAGCAGACCTCCACCTGC</t>
-  </si>
-  <si>
-    <t>CACATTGGAAACTACCGGCTCCTCAAGACCATTGGCAAGGGTAATTTTGCCAAGGTGAAGTTGGCCCGACACATCCTGACTGGGAAAGAGGTAGCTGTGAAGATCATTGACAAGACTCAACTGAACTCCTCCAGCCTCCAGAAACTATTCCGCGAAGTAAGAATAATGAAGGTTTTGAATCATCCCAACATAGTTAAATTATTTGAAGTGATTGAGACTGAGAAAACGCTCTACCTTGTCATGGAGTACGCTAGTGGCGGAGAGGTATTTGATTACCTAGTGGCTCATGGCAGGATGAAAGAAAAAGAGGCTCGAGCCAAATTCCGCCAGATAGTGTCTGCTGTGCAGTACTGTCACCAGAAGTTTATTGTCCATAGAGACTTAAAGGCAGAAAACCTGCTCTTGGATGCTGATATGAACATCAAGATTGCAGACTTTGGCTTCAGCAATGAATTCACCTTTGGGAACAAGCTGGACACCTTCTGTGGCAGTCCCCCTTATGCTGCCCCAGAACTCTTCCAGGGCAAAAAATATGATGGACCCGAGGTGGATGTGTGGAGCCTAGGAGTTATCCTCTATACACTGGTCAGCGGATCCCTGCCTTTTGATGGACAGAACCTCAAGGAGCTGCGGGAACGGGTACTGAGGGGAAAATACCGTATTCCATTCTACATGTCCACGGACTGTGAAAACCTGCTTAAGAAATTTCTCATTCTTAATCCCAGCAAGAGAGGCACTTTAGAGCAAATCATGAAAGATCGATGGATGAATGTGGGTCACGAAGATGATGAACTAAAGCCTTACGTGGAGCCACTCCCTGACTACAAGGACCCCCGGCGGACAGAGCTGATGGTGTCCATGGGTTATACACGGGAAGAGATCCAGGACTCGCTGGTGGGCCAGAGATACAACGAGGTGATGGCCACCTATCTGCTCCTGGGCTAC</t>
-  </si>
-  <si>
-    <t>MAAAAAQGGGGGEPRRTEGVGPGVPGEVEMVKGQPFDVGPRYTQLQYIGEGAYGMVSSAYDHVRKTRVAIKKISPFEHQTYCQRTLREIQILLRFRHENVIGIRDILRASTLEAMRDVYIVQDLMETDLYKLLKSQQLSNDHICYFLYQILRGLKYIHSANVLHRDLKPSNLLINTTCDLKICDFGLARIADPEHDHTGFLTEYVATRWYRAPEIMLNSKGYTKSIDIWSVGCILAEMLSNRPIFPGKHYLDQLNHILGILGSPSQEDLNCIINMKARNYLQSLPSKTKVAWAKLFPKSDSKALDLLDRMLTFNPNKRITVEEALAHPYLEQYYDPTDEPVAEEPFTFAMELDDLPKERLKELIFQETARFQPGVLEAP</t>
-  </si>
-  <si>
     <t>GDSDISSPLLQNTVHIDLSALNPELVQAVQHVVIGPSSLIVHFNEVIGRGHFGCVYHGTLLDNDGKKIHCAVKSLNRITDIGEVSQFLTEGIIMKDFSHPNVLSLLGICLRSEGSPLVVLPYMKHGDLRNFIRNETHNPTVKDLIGFGLQVAKGMKYLASKKFVHRDLAARNCMLDEKFTVKVADFGLARDMYDKEYYSVHNKTGAKLPVKWMALESLQTQKFTTKSDVWSFGVLLWELMTRGAPPYPDVNTFDITVYLLQGRRLLQPEYCPDPLYEVMLKCWHPKAEMRPSFSELVSRISAIFSTFIG</t>
   </si>
   <si>
@@ -557,7 +566,7 @@
     <t>ADPEELFTKLERIGKGSFGEVFKGIDNRTQQVVAIKIIDLEEAEDEIEDIQQEITVLSQCDSSYVTKYYGSYLKGSKLWIIMEYLGGGSALDLLRAGPFDEFQIATMLKEILKGLDYLHSEKKIHRDIKAANVLLSEQGDVKLADFGVAGQLTDTQIKRNTFVGTPFWMAPEVIQQSAYDSKADIWSLGITAIELAKGEPPNSDMHPMRVLFLIPKNNPPTLVGDFTKSFKEFIDACLNKDPSFRPTAKELLKHKFIVKNSKKTSYLTELIDRFKRWKAE</t>
   </si>
   <si>
-    <t>GATGAACAACCTCACATCGGAAACTACAGACTGTTGAAAACAATCGGCAAGGGGAATTTTGCAAAAGTAAAATTGGCAAGACATATCCTTACAGGCAGAGAGGTTGCAATAAAAATAATTGACAAAACTCAGTTGAATCCAACAAGTCTACAAAAGCTCTTCAGAGAAGTAAGAATAATGAAGATTTTAAATCATCCCAATATAGTGAAGTTATTCGAAGTCATTGAAACTGAAAAAACACTCTACCTAATCATGGAATATGCAAGTGGAGGTGAAGTATTTGACTATTTGGTTGCACATGGCAGGATGAAGGAAAAAGAAGCAAGATCTAAATTTAGACAGATTGTGTCTGCAGTTCAATACTGCCATCAGAAACGGATCGTACATCGAGACCTCAAGGCTGAAAATCTATTGTTAGATGCCGATATGAACATTAAAATAGCAGATTTCGGTTTTAGCAATGAATTTACTGTTGGCGGTAAACTCGACACGTTTTGTGGCAGTCCTCCATACGCAGCACCTGAGCTCTTCCAGGGCAAGAAATATGACGGGCCAGAAGTGGATGTGTGGAGTCTGGGGGTCATTTTATACACACTAGTCAGTGGCTCACTTCCCTTTGATGGGCAAAACCTAAAGGAACTGAGAGAGAGAGTATTAAGAGGGAAATACAGAATTCCCTTCTACATGTCTACAGACTGTGAAAACCTTCTCAAACGTTTCCTGGTGCTAAATCCAATTAAACGCGGCACTCTAGAGCAAATCATGAAGGACAGGTGGATCAATGCAGGGCATGAAGAAGATGAACTCAAACCATTTGTTGAACCAGAGCTAGACATCTCAGACCAAAAAAGAATAGATATTATGGTGGGAATGGGATATTCACAAGAAGAAATTCAAGAATCTCTTAGTAAGATGAAATACGATGAAATCACAGCTACATATTTGTTATTGGGGAGAAAATCTTCAGAG</t>
+    <t>AURKA_HUMAN_D0_2NP8_A</t>
   </si>
   <si>
     <t>HIGNYRLLKTIGKGNFAKVKLARHILTGKEVAVKIIDKTQLNSSSLQKLFREVRIMKVLNHPNIVKLFEVIETEKTLYLVMEYASGGEVFDYLVAHGRMKEKEARAKFRQIVSAVQYCHQKFIVHRDLKAENLLLDADMNIKIADFGFSNEFTFGNKLDTFCGSPPYAAPELFQGKKYDGPEVDVWSLGVILYTLVSGSLPFDGQNLKELRERVLRGKYRIPFYMSTDCENLLKKFLILNPSKRGTLEQIMKDRWMNVGHEDDELKPYVEPLPDYKDPRRTELMVSMGYTREEIQDSLVGQRYNEVMATYLLLGY</t>
@@ -566,6 +575,9 @@
     <t>GVVTHEQFKAALRMVVDQGDPRLLLDSYVKIGEGSTGIVCLAREKHSGRQVAVKMMDLRKQQRRELLFNEVVIMRDYQHFNVVEMYKSYLVGEELWVLMEFLQGGALTDIVSQVRLNEEQIATVCEAVLQALAYLHAQGVIHRDIKSDSILLTLDGRVKLSDFGFCAQISKDVPKRKSLVGTPYWMAPEVISRSLYATEVDIWSLGIMVIEMVDGEPPYFSDSPVQAMKRLRDSPPPKLKNSHKVSPVLRDFLERMLVRDPQERATAQELLDHPFLLQTGLPECLVPLIQLYRKQTSTC</t>
   </si>
   <si>
+    <t>NQFYSVEVGDSTFTVLKRYQNLKPIGSGAQGIVCAAYDAVLDRNVAIKKLSRPFQNQTHAKRAYRELVLMKCVNHKNIISLLNVFTPQKTLEEFQDVYLVMELMDANLCQVIQMELDHERMSYLLYQMLCGIKHLHSAGIIHRDLKPSNIVVKSDCTLKILDFGLARTAGTSFMMTPYVVTRYYRAPEVILGMGYKENVDIWSVGCIMGEMVRHKILFPGRDYIDQWNKVIEQLGTPCPEFMKKLQPTVRNYVENRPKYAGLTFPKLFPDSLFPADSEHNKLKASQARDLLSKMLVIDPAKRISVDDALQHPYINVWYDPAEVEAPPPQIYDKQLDEREHTIEEWKELIYKEVMN</t>
+  </si>
+  <si>
     <t>MKDYDELLKYYELHETIGTGGFAKVKLACHILTGEMVAIKIMDKNTLGSDLPRIKTEIEALKNLRHQHICQLYHVLETANKIFMVLEYCPGGELFDYIISQDRLSEEETRVVFRQIVSAVAYVHSQGYAHRDLKPENLLFDEYHKLKLIDFGLCAKPKGNKDYHLQTCCGSLAYAAPELIQGKSYLGSEADVWSMGILLYVLMCGFLPFDDDNVMALYKKIMRGKYDVPKWLSPSSILLLQQMLQVDPKKRISMKNLLNHPWIMQDYNYPVEWQSKNPFIHLDDDCVTELSVHHRNNRQTMEDLISLWQYDHLTATYLLLLAKKARGKPVRLRLSSFSCG</t>
   </si>
   <si>
@@ -689,10 +701,10 @@
     <t>MTVFRQENVDDYYDTGEELGSGQFAVVKKCREKSTGLQYAAKFIKKRRTKSSRRGVSREDIEREVSILKEIQHPNVITLHEVYENKTDVILILELVAGGELFDFLAEKESLTEEEATEFLKQTLNGVYYLHSLQIAHFDLKPENIMLLDRNVPKPRIKIIDFGLAHKIDFGNEFKNIFGTPEFVAPEIVNYEPLGLEADMWSIGVITYILLSGASPFLGDTKQETLANVSAVNYEFEDEYFSNTSALAKDFIRRLLVKDPKKRMTIQDSLQHPWIKPKDTQQALSRKASAVNMEKFKKFAARKKWKQSVRLISLCQRLSRSFLSRSNMSVARSD</t>
   </si>
   <si>
-    <t>AURKA_HUMAN_D0_2NP8_A</t>
-  </si>
-  <si>
     <t>aa_start</t>
+  </si>
+  <si>
+    <t>GCAGTGCCCTTTGTGGAAGACTGGGACTTGGTGCAAACCCTGGGAGAAGGTGCCTATGGAGAAGTTCAACTTGCTGTGAATAGAGTAACTGAAGAAGCAGTCGCAGTGAAGATTGTAGATATGAAGCGTGCCGTAGACTGTCCAGAAAATATTAAGAAAGAGATCTGTATCAATAAAATGCTAAATCATGAAAATGTAGTAAAATTCTATGGTCACAGGAGAGAAGGCAATATCCAATATTTATTTCTGGAGTACTGTAGTGGAGGAGAGCTTTTTGACAGAATAGAGCCAGACATAGGCATGCCTGAACCAGATGCTCAGAGATTCTTCCATCAACTCATGGCAGGGGTGGTTTATCTGCATGGTATTGGAATAACTCACAGGGATATTAAACCAGAAAATCTTCTGTTGGATGAAAGGGATAACCTCAAAATCTCAGACTTTGGCTTGGCAACAGTATTTCGGTATAATAATCGTGAGCGTTTGTTGAACAAGATGTGTGGTACTTTACCATATGTTGCTCCAGAACTTCTGAAGAGAAGAGAATTTCATGCAGAACCAGTTGATGTTTGGTCCTGTGGAATAGTACTTACTGCAATGCTCGCTGGAGAATTGCCATGGGACCAACCCAGTGACAGCTGTCAGGAGTATTCTGACTGGAAAGAAAAAAAAACATACCTCAACCCTTGGAAAAAAATCGATTCTGCTCCTCTAGCTCTGCTGCATAAAATCTTAGTTGAGAATCCATCAGCAAGAATTACCATTCCAGACATCAAAAAAGATAGATGGTACAACAAACCCCTC</t>
   </si>
   <si>
     <t>MSGPVPSRARVYTDVNTHRPREYWDYESHVVEWGNQDDYQLVRKLGRGKYSEVFEAINITNNEKVVVKILKPVKKKKIKREIKILENLRGGPNIITLADIVKDPVSRTPALVFEHVNNTDFKQLYQTLTDYDIRFYMYEILKALDYCHSMGIMHRDVKPHNVMIDHEHRKLRLIDWGLAEFYHPGQEYNVRVASRYFKGPELLVDYQMYDYSLDMWSLGCMLASMIFRKEPFFHGHDNYDQLVRIAKVLGTEDLYDYIDKYNIELDPRFNDILGRHSRKRWERFVHSENQHLVSPEALDFLDKLLRYDHQSRLTAREAMEHPYFYTVVKDQARMG</t>
@@ -1058,36 +1070,36 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="G1" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="H1" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="I1" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B2" t="n">
         <v>1432</v>
@@ -1102,7 +1114,7 @@
         <v>360</v>
       </c>
       <c r="F2" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
@@ -1111,12 +1123,12 @@
         <v>1080</v>
       </c>
       <c r="I2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B3" t="n">
         <v>1017</v>
@@ -1131,7 +1143,7 @@
         <v>296</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G3" t="n">
         <v>4</v>
@@ -1140,12 +1152,12 @@
         <v>888</v>
       </c>
       <c r="I3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>224</v>
+        <v>183</v>
       </c>
       <c r="B4" t="n">
         <v>6790</v>
@@ -1160,7 +1172,7 @@
         <v>391</v>
       </c>
       <c r="F4" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G4" t="n">
         <v>373</v>
@@ -1169,12 +1181,12 @@
         <v>1173</v>
       </c>
       <c r="I4" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B5" t="n">
         <v>5594</v>
@@ -1189,7 +1201,7 @@
         <v>360</v>
       </c>
       <c r="F5" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="G5" t="n">
         <v>1</v>
@@ -1198,12 +1210,12 @@
         <v>1080</v>
       </c>
       <c r="I5" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B6" t="n">
         <v>1612</v>
@@ -1218,7 +1230,7 @@
         <v>334</v>
       </c>
       <c r="F6" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="G6" t="n">
         <v>1</v>
@@ -1227,12 +1239,12 @@
         <v>1002</v>
       </c>
       <c r="I6" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B7" t="n">
         <v>9261</v>
@@ -1247,7 +1259,7 @@
         <v>348</v>
       </c>
       <c r="F7" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="G7" t="n">
         <v>73</v>
@@ -1256,12 +1268,12 @@
         <v>1044</v>
       </c>
       <c r="I7" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B8" t="n">
         <v>10298</v>
@@ -1285,7 +1297,7 @@
         <v>1773</v>
       </c>
       <c r="I8" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1305,7 +1317,7 @@
         <v>512</v>
       </c>
       <c r="F9" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="G9" t="n">
         <v>685</v>
@@ -1314,12 +1326,12 @@
         <v>1536</v>
       </c>
       <c r="I9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B10" t="n">
         <v>673</v>
@@ -1334,7 +1346,7 @@
         <v>712</v>
       </c>
       <c r="F10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G10" t="n">
         <v>1330</v>
@@ -1363,7 +1375,7 @@
         <v>297</v>
       </c>
       <c r="F11" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="G11" t="n">
         <v>52</v>
@@ -1372,12 +1384,12 @@
         <v>891</v>
       </c>
       <c r="I11" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B12" t="n">
         <v>2872</v>
@@ -1392,7 +1404,7 @@
         <v>385</v>
       </c>
       <c r="F12" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="G12" t="n">
         <v>214</v>
@@ -1401,12 +1413,12 @@
         <v>1155</v>
       </c>
       <c r="I12" t="s">
-        <v>165</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B13" t="n">
         <v>1453</v>
@@ -1421,7 +1433,7 @@
         <v>294</v>
       </c>
       <c r="F13" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
@@ -1430,12 +1442,12 @@
         <v>882</v>
       </c>
       <c r="I13" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" t="n">
         <v>1454</v>
@@ -1450,7 +1462,7 @@
         <v>294</v>
       </c>
       <c r="F14" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
@@ -1459,12 +1471,12 @@
         <v>882</v>
       </c>
       <c r="I14" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B15" t="n">
         <v>5598</v>
@@ -1479,7 +1491,7 @@
         <v>292</v>
       </c>
       <c r="F15" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="G15" t="n">
         <v>1</v>
@@ -1488,12 +1500,12 @@
         <v>876</v>
       </c>
       <c r="I15" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B16" t="n">
         <v>6788</v>
@@ -1508,7 +1520,7 @@
         <v>313</v>
       </c>
       <c r="F16" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="G16" t="n">
         <v>46</v>
@@ -1517,12 +1529,12 @@
         <v>939</v>
       </c>
       <c r="I16" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B17" t="n">
         <v>5563</v>
@@ -1537,7 +1549,7 @@
         <v>279</v>
       </c>
       <c r="F17" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="G17" t="n">
         <v>16</v>
@@ -1546,12 +1558,12 @@
         <v>837</v>
       </c>
       <c r="I17" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="B18" t="n">
         <v>5747</v>
@@ -1566,7 +1578,7 @@
         <v>689</v>
       </c>
       <c r="F18" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="G18" t="n">
         <v>1231</v>
@@ -1575,12 +1587,12 @@
         <v>2067</v>
       </c>
       <c r="I18" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B19" t="n">
         <v>8569</v>
@@ -1595,7 +1607,7 @@
         <v>382</v>
       </c>
       <c r="F19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G19" t="n">
         <v>109</v>
@@ -1604,12 +1616,12 @@
         <v>1146</v>
       </c>
       <c r="I19" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B20" t="n">
         <v>5292</v>
@@ -1624,7 +1636,7 @@
         <v>313</v>
       </c>
       <c r="F20" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="G20" t="n">
         <v>85</v>
@@ -1633,12 +1645,12 @@
         <v>939</v>
       </c>
       <c r="I20" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" t="n">
         <v>7272</v>
@@ -1653,7 +1665,7 @@
         <v>808</v>
       </c>
       <c r="F21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G21" t="n">
         <v>1555</v>
@@ -1662,12 +1674,12 @@
         <v>2424</v>
       </c>
       <c r="I21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B22" t="n">
         <v>8428</v>
@@ -1682,7 +1694,7 @@
         <v>289</v>
       </c>
       <c r="F22" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="G22" t="n">
         <v>55</v>
@@ -1691,7 +1703,7 @@
         <v>867</v>
       </c>
       <c r="I22" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1711,7 +1723,7 @@
         <v>798</v>
       </c>
       <c r="F23" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="G23" t="n">
         <v>1393</v>
@@ -1720,12 +1732,12 @@
         <v>2394</v>
       </c>
       <c r="I23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B24" t="n">
         <v>1198</v>
@@ -1740,7 +1752,7 @@
         <v>484</v>
       </c>
       <c r="F24" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="G24" t="n">
         <v>379</v>
@@ -1749,12 +1761,12 @@
         <v>1452</v>
       </c>
       <c r="I24" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B25" t="n">
         <v>1613</v>
@@ -1769,7 +1781,7 @@
         <v>289</v>
       </c>
       <c r="F25" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="G25" t="n">
         <v>25</v>
@@ -1783,7 +1795,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B26" t="n">
         <v>7867</v>
@@ -1798,7 +1810,7 @@
         <v>349</v>
       </c>
       <c r="F26" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="G26" t="n">
         <v>97</v>
@@ -1807,12 +1819,12 @@
         <v>1047</v>
       </c>
       <c r="I26" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B27" t="n">
         <v>9748</v>
@@ -1827,7 +1839,7 @@
         <v>320</v>
       </c>
       <c r="F27" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="G27" t="n">
         <v>55</v>
@@ -1836,12 +1848,12 @@
         <v>960</v>
       </c>
       <c r="I27" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B28" t="n">
         <v>8445</v>
@@ -1856,7 +1868,7 @@
         <v>552</v>
       </c>
       <c r="F28" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="G28" t="n">
         <v>436</v>
@@ -1865,12 +1877,12 @@
         <v>1656</v>
       </c>
       <c r="I28" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B29" t="n">
         <v>56924</v>
@@ -1885,7 +1897,7 @@
         <v>681</v>
       </c>
       <c r="F29" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="G29" t="n">
         <v>1147</v>
@@ -1894,12 +1906,12 @@
         <v>2043</v>
       </c>
       <c r="I29" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B30" t="n">
         <v>815</v>
@@ -1914,7 +1926,7 @@
         <v>302</v>
       </c>
       <c r="F30" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G30" t="n">
         <v>37</v>
@@ -1928,7 +1940,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>150</v>
+        <v>179</v>
       </c>
       <c r="B31" t="n">
         <v>9262</v>
@@ -1943,7 +1955,7 @@
         <v>329</v>
       </c>
       <c r="F31" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="G31" t="n">
         <v>73</v>
@@ -1952,12 +1964,12 @@
         <v>987</v>
       </c>
       <c r="I31" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B32" t="n">
         <v>814</v>
@@ -1972,7 +1984,7 @@
         <v>340</v>
       </c>
       <c r="F32" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="G32" t="n">
         <v>43</v>
@@ -1981,12 +1993,12 @@
         <v>1020</v>
       </c>
       <c r="I32" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B33" t="n">
         <v>8814</v>
@@ -2001,7 +2013,7 @@
         <v>265</v>
       </c>
       <c r="F33" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G33" t="n">
         <v>4</v>
@@ -2010,12 +2022,12 @@
         <v>795</v>
       </c>
       <c r="I33" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B34" t="n">
         <v>818</v>
@@ -2030,7 +2042,7 @@
         <v>315</v>
       </c>
       <c r="F34" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="G34" t="n">
         <v>13</v>
@@ -2039,12 +2051,12 @@
         <v>945</v>
       </c>
       <c r="I34" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B35" t="n">
         <v>57144</v>
@@ -2059,7 +2071,7 @@
         <v>719</v>
       </c>
       <c r="F35" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="G35" t="n">
         <v>1273</v>
@@ -2068,12 +2080,12 @@
         <v>2157</v>
       </c>
       <c r="I35" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B36" t="n">
         <v>5261</v>
@@ -2097,12 +2109,12 @@
         <v>879</v>
       </c>
       <c r="I36" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B37" t="n">
         <v>9088</v>
@@ -2117,7 +2129,7 @@
         <v>360</v>
       </c>
       <c r="F37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G37" t="n">
         <v>217</v>
@@ -2126,12 +2138,12 @@
         <v>1080</v>
       </c>
       <c r="I37" t="s">
-        <v>162</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B38" t="n">
         <v>8576</v>
@@ -2146,7 +2158,7 @@
         <v>294</v>
       </c>
       <c r="F38" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="G38" t="n">
         <v>37</v>
@@ -2155,12 +2167,12 @@
         <v>882</v>
       </c>
       <c r="I38" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B39" t="n">
         <v>92335</v>
@@ -2175,7 +2187,7 @@
         <v>402</v>
       </c>
       <c r="F39" t="s">
-        <v>167</v>
+        <v>116</v>
       </c>
       <c r="G39" t="n">
         <v>88</v>
@@ -2184,12 +2196,12 @@
         <v>1206</v>
       </c>
       <c r="I39" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B40" t="n">
         <v>7444</v>
@@ -2204,7 +2216,7 @@
         <v>335</v>
       </c>
       <c r="F40" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="G40" t="n">
         <v>40</v>
@@ -2213,12 +2225,12 @@
         <v>1005</v>
       </c>
       <c r="I40" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B41" t="n">
         <v>51231</v>
@@ -2233,7 +2245,7 @@
         <v>474</v>
       </c>
       <c r="F41" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="G41" t="n">
         <v>436</v>
@@ -2242,12 +2254,12 @@
         <v>1422</v>
       </c>
       <c r="I41" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B42" t="n">
         <v>2042</v>
@@ -2262,7 +2274,7 @@
         <v>947</v>
       </c>
       <c r="F42" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="G42" t="n">
         <v>1816</v>
@@ -2271,12 +2283,12 @@
         <v>2841</v>
       </c>
       <c r="I42" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B43" t="n">
         <v>2260</v>
@@ -2291,7 +2303,7 @@
         <v>772</v>
       </c>
       <c r="F43" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G43" t="n">
         <v>1366</v>
@@ -2300,7 +2312,7 @@
         <v>2316</v>
       </c>
       <c r="I43" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -2320,7 +2332,7 @@
         <v>340</v>
       </c>
       <c r="F44" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="G44" t="n">
         <v>1</v>
@@ -2329,12 +2341,12 @@
         <v>1020</v>
       </c>
       <c r="I44" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B45" t="n">
         <v>3702</v>
@@ -2349,7 +2361,7 @@
         <v>620</v>
       </c>
       <c r="F45" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="G45" t="n">
         <v>1069</v>
@@ -2358,12 +2370,12 @@
         <v>1860</v>
       </c>
       <c r="I45" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>141</v>
+        <v>101</v>
       </c>
       <c r="B46" t="n">
         <v>6197</v>
@@ -2378,7 +2390,7 @@
         <v>740</v>
       </c>
       <c r="F46" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G46" t="n">
         <v>1195</v>
@@ -2387,853 +2399,847 @@
         <v>2220</v>
       </c>
       <c r="I46" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>98</v>
+        <v>170</v>
       </c>
       <c r="B47" t="n">
-        <v>6197</v>
+        <v>4233</v>
       </c>
       <c r="C47" t="s">
         <v>2</v>
       </c>
       <c r="D47" t="n">
-        <v>399</v>
+        <v>1038</v>
       </c>
       <c r="E47" t="n">
-        <v>740</v>
+        <v>1346</v>
       </c>
       <c r="F47" t="s">
-        <v>111</v>
+        <v>180</v>
       </c>
       <c r="G47" t="n">
-        <v>1195</v>
+        <v>3112</v>
       </c>
       <c r="H47" t="n">
-        <v>2220</v>
+        <v>4038</v>
       </c>
       <c r="I47" t="s">
-        <v>140</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>166</v>
+        <v>109</v>
       </c>
       <c r="B48" t="n">
-        <v>4233</v>
+        <v>5603</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
       </c>
       <c r="D48" t="n">
-        <v>1038</v>
+        <v>1</v>
       </c>
       <c r="E48" t="n">
-        <v>1346</v>
+        <v>352</v>
       </c>
       <c r="F48" t="s">
-        <v>177</v>
+        <v>98</v>
       </c>
       <c r="G48" t="n">
-        <v>3112</v>
+        <v>1</v>
       </c>
       <c r="H48" t="n">
-        <v>4038</v>
+        <v>1056</v>
       </c>
       <c r="I48" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="B49" t="n">
-        <v>5603</v>
+        <v>6416</v>
       </c>
       <c r="C49" t="s">
         <v>2</v>
       </c>
       <c r="D49" t="n">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="E49" t="n">
-        <v>352</v>
+        <v>399</v>
       </c>
       <c r="F49" t="s">
-        <v>95</v>
+        <v>152</v>
       </c>
       <c r="G49" t="n">
-        <v>1</v>
+        <v>238</v>
       </c>
       <c r="H49" t="n">
-        <v>1056</v>
+        <v>1197</v>
       </c>
       <c r="I49" t="s">
-        <v>50</v>
+        <v>213</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" t="s">
-        <v>145</v>
+        <v>225</v>
       </c>
       <c r="B50" t="n">
-        <v>6416</v>
+        <v>10769</v>
       </c>
       <c r="C50" t="s">
         <v>2</v>
       </c>
       <c r="D50" t="n">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E50" t="n">
-        <v>399</v>
+        <v>360</v>
       </c>
       <c r="F50" t="s">
-        <v>148</v>
+        <v>74</v>
       </c>
       <c r="G50" t="n">
-        <v>238</v>
+        <v>169</v>
       </c>
       <c r="H50" t="n">
-        <v>1197</v>
+        <v>1080</v>
       </c>
       <c r="I50" t="s">
-        <v>209</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" t="s">
-        <v>221</v>
+        <v>25</v>
       </c>
       <c r="B51" t="n">
-        <v>10769</v>
+        <v>6195</v>
       </c>
       <c r="C51" t="s">
         <v>2</v>
       </c>
       <c r="D51" t="n">
-        <v>57</v>
+        <v>411</v>
       </c>
       <c r="E51" t="n">
-        <v>360</v>
+        <v>735</v>
       </c>
       <c r="F51" t="s">
-        <v>71</v>
+        <v>176</v>
       </c>
       <c r="G51" t="n">
-        <v>169</v>
+        <v>1231</v>
       </c>
       <c r="H51" t="n">
-        <v>1080</v>
+        <v>2205</v>
       </c>
       <c r="I51" t="s">
-        <v>41</v>
+        <v>193</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
-        <v>91</v>
+        <v>39</v>
       </c>
       <c r="B52" t="n">
-        <v>6195</v>
+        <v>5599</v>
       </c>
       <c r="C52" t="s">
-        <v>2</v>
+        <v>221</v>
       </c>
       <c r="D52" t="n">
-        <v>411</v>
+        <v>1</v>
       </c>
       <c r="E52" t="n">
-        <v>735</v>
+        <v>364</v>
       </c>
       <c r="F52" t="s">
-        <v>173</v>
+        <v>27</v>
       </c>
       <c r="G52" t="n">
-        <v>1231</v>
+        <v>1</v>
       </c>
       <c r="H52" t="n">
-        <v>2205</v>
+        <v>1092</v>
       </c>
       <c r="I52" t="s">
-        <v>189</v>
+        <v>222</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" t="s">
-        <v>24</v>
+        <v>125</v>
       </c>
       <c r="B53" t="n">
-        <v>6195</v>
+        <v>4751</v>
       </c>
       <c r="C53" t="s">
-        <v>2</v>
+        <v>221</v>
       </c>
       <c r="D53" t="n">
-        <v>411</v>
+        <v>1</v>
       </c>
       <c r="E53" t="n">
-        <v>735</v>
+        <v>271</v>
       </c>
       <c r="F53" t="s">
-        <v>173</v>
+        <v>202</v>
       </c>
       <c r="G53" t="n">
-        <v>1231</v>
+        <v>1</v>
       </c>
       <c r="H53" t="n">
-        <v>2205</v>
+        <v>813</v>
       </c>
       <c r="I53" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>38</v>
+        <v>172</v>
       </c>
       <c r="B54" t="n">
-        <v>5599</v>
+        <v>5604</v>
       </c>
       <c r="C54" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D54" t="n">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="E54" t="n">
-        <v>364</v>
+        <v>273</v>
       </c>
       <c r="F54" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="G54" t="n">
-        <v>1</v>
+        <v>184</v>
       </c>
       <c r="H54" t="n">
-        <v>1092</v>
+        <v>819</v>
       </c>
       <c r="I54" t="s">
-        <v>218</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>120</v>
+        <v>41</v>
       </c>
       <c r="B55" t="n">
-        <v>4751</v>
+        <v>5058</v>
       </c>
       <c r="C55" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D55" t="n">
-        <v>1</v>
+        <v>248</v>
       </c>
       <c r="E55" t="n">
-        <v>271</v>
+        <v>545</v>
       </c>
       <c r="F55" t="s">
-        <v>198</v>
+        <v>140</v>
       </c>
       <c r="G55" t="n">
-        <v>1</v>
+        <v>742</v>
       </c>
       <c r="H55" t="n">
-        <v>813</v>
+        <v>1635</v>
       </c>
       <c r="I55" t="s">
-        <v>160</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>168</v>
+        <v>78</v>
       </c>
       <c r="B56" t="n">
-        <v>5604</v>
+        <v>5610</v>
       </c>
       <c r="C56" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D56" t="n">
-        <v>62</v>
+        <v>254</v>
       </c>
       <c r="E56" t="n">
-        <v>273</v>
+        <v>551</v>
       </c>
       <c r="F56" t="s">
-        <v>6</v>
+        <v>173</v>
       </c>
       <c r="G56" t="n">
-        <v>184</v>
+        <v>760</v>
       </c>
       <c r="H56" t="n">
-        <v>819</v>
+        <v>1653</v>
       </c>
       <c r="I56" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="B57" t="n">
-        <v>5058</v>
+        <v>1021</v>
       </c>
       <c r="C57" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D57" t="n">
-        <v>248</v>
+        <v>1</v>
       </c>
       <c r="E57" t="n">
-        <v>545</v>
+        <v>301</v>
       </c>
       <c r="F57" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="G57" t="n">
-        <v>742</v>
+        <v>1</v>
       </c>
       <c r="H57" t="n">
-        <v>1635</v>
+        <v>903</v>
       </c>
       <c r="I57" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="B58" t="n">
-        <v>5610</v>
+        <v>5608</v>
       </c>
       <c r="C58" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D58" t="n">
-        <v>254</v>
+        <v>1</v>
       </c>
       <c r="E58" t="n">
-        <v>551</v>
+        <v>334</v>
       </c>
       <c r="F58" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="G58" t="n">
-        <v>760</v>
+        <v>1</v>
       </c>
       <c r="H58" t="n">
-        <v>1653</v>
+        <v>1002</v>
       </c>
       <c r="I58" t="s">
-        <v>42</v>
+        <v>159</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B59" t="n">
-        <v>1021</v>
+        <v>140609</v>
       </c>
       <c r="C59" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D59" t="n">
         <v>1</v>
       </c>
       <c r="E59" t="n">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="F59" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="G59" t="n">
         <v>1</v>
       </c>
       <c r="H59" t="n">
-        <v>903</v>
+        <v>906</v>
       </c>
       <c r="I59" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="B60" t="n">
-        <v>5608</v>
+        <v>659</v>
       </c>
       <c r="C60" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D60" t="n">
-        <v>1</v>
+        <v>189</v>
       </c>
       <c r="E60" t="n">
-        <v>334</v>
+        <v>517</v>
       </c>
       <c r="F60" t="s">
-        <v>136</v>
+        <v>76</v>
       </c>
       <c r="G60" t="n">
-        <v>1</v>
+        <v>565</v>
       </c>
       <c r="H60" t="n">
-        <v>1002</v>
+        <v>1551</v>
       </c>
       <c r="I60" t="s">
-        <v>155</v>
+        <v>53</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B61" t="n">
-        <v>140609</v>
+        <v>5127</v>
       </c>
       <c r="C61" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D61" t="n">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="E61" t="n">
-        <v>302</v>
+        <v>478</v>
       </c>
       <c r="F61" t="s">
-        <v>124</v>
+        <v>35</v>
       </c>
       <c r="G61" t="n">
-        <v>1</v>
+        <v>487</v>
       </c>
       <c r="H61" t="n">
-        <v>906</v>
+        <v>1434</v>
       </c>
       <c r="I61" t="s">
-        <v>77</v>
+        <v>108</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>67</v>
+        <v>205</v>
       </c>
       <c r="B62" t="n">
-        <v>659</v>
+        <v>9833</v>
       </c>
       <c r="C62" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D62" t="n">
-        <v>189</v>
+        <v>1</v>
       </c>
       <c r="E62" t="n">
-        <v>517</v>
+        <v>340</v>
       </c>
       <c r="F62" t="s">
-        <v>65</v>
+        <v>187</v>
       </c>
       <c r="G62" t="n">
-        <v>565</v>
+        <v>1</v>
       </c>
       <c r="H62" t="n">
-        <v>1551</v>
+        <v>1020</v>
       </c>
       <c r="I62" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="B63" t="n">
-        <v>5127</v>
+        <v>5605</v>
       </c>
       <c r="C63" t="s">
+        <v>221</v>
+      </c>
+      <c r="D63" t="n">
+        <v>55</v>
+      </c>
+      <c r="E63" t="n">
+        <v>400</v>
+      </c>
+      <c r="F63" t="s">
+        <v>68</v>
+      </c>
+      <c r="G63" t="n">
+        <v>163</v>
+      </c>
+      <c r="H63" t="n">
+        <v>1200</v>
+      </c>
+      <c r="I63" t="s">
         <v>217</v>
-      </c>
-      <c r="D63" t="n">
-        <v>163</v>
-      </c>
-      <c r="E63" t="n">
-        <v>478</v>
-      </c>
-      <c r="F63" t="s">
-        <v>34</v>
-      </c>
-      <c r="G63" t="n">
-        <v>487</v>
-      </c>
-      <c r="H63" t="n">
-        <v>1434</v>
-      </c>
-      <c r="I63" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>201</v>
+        <v>91</v>
       </c>
       <c r="B64" t="n">
-        <v>9833</v>
+        <v>1457</v>
       </c>
       <c r="C64" t="s">
-        <v>217</v>
+        <v>2</v>
       </c>
       <c r="D64" t="n">
         <v>1</v>
       </c>
       <c r="E64" t="n">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F64" t="s">
-        <v>183</v>
+        <v>230</v>
       </c>
       <c r="G64" t="n">
         <v>1</v>
       </c>
       <c r="H64" t="n">
-        <v>1020</v>
+        <v>1005</v>
       </c>
       <c r="I64" t="s">
-        <v>51</v>
+        <v>124</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>28</v>
+        <v>138</v>
       </c>
       <c r="B65" t="n">
-        <v>5605</v>
+        <v>11200</v>
       </c>
       <c r="C65" t="s">
-        <v>217</v>
+        <v>2</v>
       </c>
       <c r="D65" t="n">
-        <v>55</v>
+        <v>210</v>
       </c>
       <c r="E65" t="n">
-        <v>400</v>
+        <v>531</v>
       </c>
       <c r="F65" t="s">
-        <v>30</v>
+        <v>198</v>
       </c>
       <c r="G65" t="n">
-        <v>163</v>
+        <v>628</v>
       </c>
       <c r="H65" t="n">
-        <v>1200</v>
+        <v>1593</v>
       </c>
       <c r="I65" t="s">
-        <v>213</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>87</v>
+        <v>117</v>
       </c>
       <c r="B66" t="n">
-        <v>1457</v>
+        <v>5566</v>
       </c>
       <c r="C66" t="s">
         <v>2</v>
       </c>
       <c r="D66" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E66" t="n">
-        <v>335</v>
+        <v>351</v>
       </c>
       <c r="F66" t="s">
-        <v>226</v>
+        <v>84</v>
       </c>
       <c r="G66" t="n">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="H66" t="n">
-        <v>1005</v>
+        <v>1053</v>
       </c>
       <c r="I66" t="s">
-        <v>119</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>133</v>
+        <v>103</v>
       </c>
       <c r="B67" t="n">
-        <v>11200</v>
+        <v>1445</v>
       </c>
       <c r="C67" t="s">
         <v>2</v>
       </c>
       <c r="D67" t="n">
-        <v>210</v>
+        <v>188</v>
       </c>
       <c r="E67" t="n">
-        <v>531</v>
+        <v>450</v>
       </c>
       <c r="F67" t="s">
-        <v>194</v>
+        <v>154</v>
       </c>
       <c r="G67" t="n">
-        <v>628</v>
+        <v>562</v>
       </c>
       <c r="H67" t="n">
-        <v>1593</v>
+        <v>1350</v>
       </c>
       <c r="I67" t="s">
-        <v>0</v>
+        <v>191</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>112</v>
+        <v>59</v>
       </c>
       <c r="B68" t="n">
-        <v>5566</v>
+        <v>5600</v>
       </c>
       <c r="C68" t="s">
         <v>2</v>
       </c>
       <c r="D68" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E68" t="n">
-        <v>351</v>
+        <v>364</v>
       </c>
       <c r="F68" t="s">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="G68" t="n">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="H68" t="n">
-        <v>1053</v>
+        <v>1092</v>
       </c>
       <c r="I68" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>100</v>
+        <v>220</v>
       </c>
       <c r="B69" t="n">
-        <v>1445</v>
+        <v>1459</v>
       </c>
       <c r="C69" t="s">
         <v>2</v>
       </c>
       <c r="D69" t="n">
-        <v>188</v>
+        <v>1</v>
       </c>
       <c r="E69" t="n">
-        <v>450</v>
+        <v>334</v>
       </c>
       <c r="F69" t="s">
-        <v>25</v>
+        <v>155</v>
       </c>
       <c r="G69" t="n">
-        <v>562</v>
+        <v>1</v>
       </c>
       <c r="H69" t="n">
-        <v>1350</v>
+        <v>1002</v>
       </c>
       <c r="I69" t="s">
-        <v>187</v>
+        <v>123</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
       <c r="B70" t="n">
-        <v>5600</v>
+        <v>4140</v>
       </c>
       <c r="C70" t="s">
         <v>2</v>
       </c>
       <c r="D70" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E70" t="n">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="F70" t="s">
-        <v>172</v>
+        <v>99</v>
       </c>
       <c r="G70" t="n">
-        <v>1</v>
+        <v>142</v>
       </c>
       <c r="H70" t="n">
-        <v>1092</v>
+        <v>1110</v>
       </c>
       <c r="I70" t="s">
-        <v>73</v>
+        <v>166</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>216</v>
+        <v>14</v>
       </c>
       <c r="B71" t="n">
-        <v>1459</v>
+        <v>2011</v>
       </c>
       <c r="C71" t="s">
         <v>2</v>
       </c>
       <c r="D71" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E71" t="n">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="F71" t="s">
-        <v>151</v>
+        <v>184</v>
       </c>
       <c r="G71" t="n">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="H71" t="n">
-        <v>1002</v>
+        <v>990</v>
       </c>
       <c r="I71" t="s">
-        <v>118</v>
+        <v>178</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="B72" t="n">
-        <v>4140</v>
+        <v>5595</v>
       </c>
       <c r="C72" t="s">
         <v>2</v>
       </c>
       <c r="D72" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E72" t="n">
-        <v>370</v>
+        <v>379</v>
       </c>
       <c r="F72" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="G72" t="n">
-        <v>142</v>
+        <v>1</v>
       </c>
       <c r="H72" t="n">
-        <v>1110</v>
+        <v>1137</v>
       </c>
       <c r="I72" t="s">
-        <v>180</v>
+        <v>226</v>
       </c>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>14</v>
+        <v>195</v>
       </c>
       <c r="B73" t="n">
-        <v>2011</v>
+        <v>7443</v>
       </c>
       <c r="C73" t="s">
         <v>2</v>
       </c>
       <c r="D73" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E73" t="n">
-        <v>330</v>
+        <v>364</v>
       </c>
       <c r="F73" t="s">
-        <v>181</v>
+        <v>96</v>
       </c>
       <c r="G73" t="n">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="H73" t="n">
-        <v>990</v>
+        <v>1092</v>
       </c>
       <c r="I73" t="s">
-        <v>175</v>
+        <v>94</v>
       </c>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>154</v>
+        <v>15</v>
       </c>
       <c r="B74" t="n">
-        <v>5595</v>
-      </c>
-      <c r="C74" t="s">
-        <v>2</v>
+        <v>5602</v>
       </c>
       <c r="D74" t="n">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="E74" t="n">
-        <v>379</v>
+        <v>400</v>
       </c>
       <c r="F74" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="G74" t="n">
-        <v>1</v>
+        <v>136</v>
       </c>
       <c r="H74" t="n">
-        <v>1137</v>
+        <v>1200</v>
       </c>
       <c r="I74" t="s">
-        <v>222</v>
+        <v>171</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>191</v>
+        <v>132</v>
       </c>
       <c r="B75" t="n">
-        <v>7443</v>
-      </c>
-      <c r="C75" t="s">
-        <v>2</v>
+        <v>1111</v>
       </c>
       <c r="D75" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E75" t="n">
-        <v>364</v>
+        <v>269</v>
       </c>
       <c r="F75" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="G75" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H75" t="n">
-        <v>1092</v>
+        <v>807</v>
       </c>
       <c r="I75" t="s">
-        <v>90</v>
+        <v>229</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B76" t="n">
         <v>673</v>
@@ -3248,7 +3254,7 @@
         <v>712</v>
       </c>
       <c r="F76" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G76" t="n">
         <v>1330</v>
@@ -3262,7 +3268,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B77" t="n">
         <v>4233</v>
@@ -3277,7 +3283,7 @@
         <v>1346</v>
       </c>
       <c r="F77" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="G77" t="n">
         <v>3112</v>
@@ -3286,12 +3292,12 @@
         <v>4038</v>
       </c>
       <c r="I77" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B78" t="n">
         <v>2260</v>
@@ -3306,7 +3312,7 @@
         <v>772</v>
       </c>
       <c r="F78" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G78" t="n">
         <v>1366</v>
@@ -3315,7 +3321,7 @@
         <v>2316</v>
       </c>
       <c r="I78" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -3335,7 +3341,7 @@
         <v>512</v>
       </c>
       <c r="F79" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="G79" t="n">
         <v>685</v>
@@ -3344,12 +3350,12 @@
         <v>1536</v>
       </c>
       <c r="I79" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B80" t="n">
         <v>1432</v>
@@ -3364,7 +3370,7 @@
         <v>360</v>
       </c>
       <c r="F80" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="G80" t="n">
         <v>1</v>
@@ -3373,12 +3379,12 @@
         <v>1080</v>
       </c>
       <c r="I80" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B81" t="n">
         <v>5594</v>
@@ -3393,7 +3399,7 @@
         <v>360</v>
       </c>
       <c r="F81" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="G81" t="n">
         <v>1</v>
@@ -3402,12 +3408,12 @@
         <v>1080</v>
       </c>
       <c r="I81" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="B82" t="n">
         <v>11200</v>
@@ -3422,7 +3428,7 @@
         <v>531</v>
       </c>
       <c r="F82" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="G82" t="n">
         <v>628</v>
@@ -3436,7 +3442,7 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B83" t="n">
         <v>1017</v>
@@ -3451,7 +3457,7 @@
         <v>296</v>
       </c>
       <c r="F83" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G83" t="n">
         <v>4</v>
@@ -3460,12 +3466,12 @@
         <v>888</v>
       </c>
       <c r="I83" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="B84" t="n">
         <v>5747</v>
@@ -3480,7 +3486,7 @@
         <v>689</v>
       </c>
       <c r="F84" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="G84" t="n">
         <v>1231</v>
@@ -3489,18 +3495,18 @@
         <v>2067</v>
       </c>
       <c r="I84" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B85" t="n">
         <v>5599</v>
       </c>
       <c r="C85" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D85" t="n">
         <v>1</v>
@@ -3509,7 +3515,7 @@
         <v>364</v>
       </c>
       <c r="F85" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G85" t="n">
         <v>1</v>
@@ -3518,355 +3524,349 @@
         <v>1092</v>
       </c>
       <c r="I85" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>168</v>
+        <v>132</v>
       </c>
       <c r="B86" t="n">
-        <v>5604</v>
-      </c>
-      <c r="C86" t="s">
-        <v>217</v>
+        <v>1111</v>
       </c>
       <c r="D86" t="n">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="E86" t="n">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="F86" t="s">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="G86" t="n">
-        <v>184</v>
+        <v>4</v>
       </c>
       <c r="H86" t="n">
-        <v>819</v>
+        <v>807</v>
       </c>
       <c r="I86" t="s">
-        <v>110</v>
+        <v>229</v>
       </c>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>224</v>
+        <v>172</v>
       </c>
       <c r="B87" t="n">
-        <v>6790</v>
+        <v>5604</v>
       </c>
       <c r="C87" t="s">
-        <v>2</v>
+        <v>221</v>
       </c>
       <c r="D87" t="n">
-        <v>125</v>
+        <v>62</v>
       </c>
       <c r="E87" t="n">
-        <v>391</v>
+        <v>273</v>
       </c>
       <c r="F87" t="s">
-        <v>82</v>
+        <v>6</v>
       </c>
       <c r="G87" t="n">
-        <v>373</v>
+        <v>184</v>
       </c>
       <c r="H87" t="n">
-        <v>1173</v>
+        <v>819</v>
       </c>
       <c r="I87" t="s">
-        <v>152</v>
+        <v>114</v>
       </c>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>154</v>
+        <v>15</v>
       </c>
       <c r="B88" t="n">
-        <v>5595</v>
-      </c>
-      <c r="C88" t="s">
-        <v>2</v>
+        <v>5602</v>
       </c>
       <c r="D88" t="n">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="E88" t="n">
-        <v>379</v>
+        <v>400</v>
       </c>
       <c r="F88" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="G88" t="n">
-        <v>1</v>
+        <v>136</v>
       </c>
       <c r="H88" t="n">
-        <v>1137</v>
+        <v>1200</v>
       </c>
       <c r="I88" t="s">
-        <v>222</v>
+        <v>171</v>
       </c>
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>141</v>
+        <v>183</v>
       </c>
       <c r="B89" t="n">
-        <v>6197</v>
+        <v>6790</v>
       </c>
       <c r="C89" t="s">
         <v>2</v>
       </c>
       <c r="D89" t="n">
-        <v>399</v>
+        <v>125</v>
       </c>
       <c r="E89" t="n">
-        <v>740</v>
+        <v>391</v>
       </c>
       <c r="F89" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="G89" t="n">
-        <v>1195</v>
+        <v>373</v>
       </c>
       <c r="H89" t="n">
-        <v>2220</v>
+        <v>1173</v>
       </c>
       <c r="I89" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>98</v>
+        <v>158</v>
       </c>
       <c r="B90" t="n">
-        <v>6197</v>
+        <v>5595</v>
       </c>
       <c r="C90" t="s">
         <v>2</v>
       </c>
       <c r="D90" t="n">
-        <v>399</v>
+        <v>1</v>
       </c>
       <c r="E90" t="n">
-        <v>740</v>
+        <v>379</v>
       </c>
       <c r="F90" t="s">
-        <v>111</v>
+        <v>56</v>
       </c>
       <c r="G90" t="n">
-        <v>1195</v>
+        <v>1</v>
       </c>
       <c r="H90" t="n">
-        <v>2220</v>
+        <v>1137</v>
       </c>
       <c r="I90" t="s">
-        <v>140</v>
+        <v>226</v>
       </c>
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B91" t="n">
-        <v>3702</v>
+        <v>6197</v>
       </c>
       <c r="C91" t="s">
         <v>2</v>
       </c>
       <c r="D91" t="n">
-        <v>357</v>
+        <v>399</v>
       </c>
       <c r="E91" t="n">
-        <v>620</v>
+        <v>740</v>
       </c>
       <c r="F91" t="s">
-        <v>49</v>
+        <v>115</v>
       </c>
       <c r="G91" t="n">
-        <v>1069</v>
+        <v>1195</v>
       </c>
       <c r="H91" t="n">
-        <v>1860</v>
+        <v>2220</v>
       </c>
       <c r="I91" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B92" t="n">
-        <v>5566</v>
+        <v>3702</v>
       </c>
       <c r="C92" t="s">
         <v>2</v>
       </c>
       <c r="D92" t="n">
-        <v>16</v>
+        <v>357</v>
       </c>
       <c r="E92" t="n">
-        <v>351</v>
+        <v>620</v>
       </c>
       <c r="F92" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="G92" t="n">
-        <v>46</v>
+        <v>1069</v>
       </c>
       <c r="H92" t="n">
-        <v>1053</v>
+        <v>1860</v>
       </c>
       <c r="I92" t="s">
-        <v>21</v>
+        <v>139</v>
       </c>
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>87</v>
+        <v>117</v>
       </c>
       <c r="B93" t="n">
-        <v>1457</v>
+        <v>5566</v>
       </c>
       <c r="C93" t="s">
         <v>2</v>
       </c>
       <c r="D93" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E93" t="n">
-        <v>335</v>
+        <v>351</v>
       </c>
       <c r="F93" t="s">
-        <v>226</v>
+        <v>84</v>
       </c>
       <c r="G93" t="n">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="H93" t="n">
-        <v>1005</v>
+        <v>1053</v>
       </c>
       <c r="I93" t="s">
-        <v>119</v>
+        <v>22</v>
       </c>
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="B94" t="n">
-        <v>9261</v>
+        <v>1457</v>
       </c>
       <c r="C94" t="s">
         <v>2</v>
       </c>
       <c r="D94" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E94" t="n">
-        <v>348</v>
+        <v>335</v>
       </c>
       <c r="F94" t="s">
-        <v>86</v>
+        <v>230</v>
       </c>
       <c r="G94" t="n">
-        <v>73</v>
+        <v>1</v>
       </c>
       <c r="H94" t="n">
-        <v>1044</v>
+        <v>1005</v>
       </c>
       <c r="I94" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="B95" t="n">
-        <v>5292</v>
+        <v>9261</v>
       </c>
       <c r="C95" t="s">
         <v>2</v>
       </c>
       <c r="D95" t="n">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E95" t="n">
-        <v>313</v>
+        <v>348</v>
       </c>
       <c r="F95" t="s">
-        <v>163</v>
+        <v>90</v>
       </c>
       <c r="G95" t="n">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="H95" t="n">
-        <v>939</v>
+        <v>1044</v>
       </c>
       <c r="I95" t="s">
-        <v>202</v>
+        <v>147</v>
       </c>
     </row>
     <row r="96" spans="1:9">
       <c r="A96" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="B96" t="n">
-        <v>659</v>
+        <v>5292</v>
       </c>
       <c r="C96" t="s">
-        <v>217</v>
+        <v>2</v>
       </c>
       <c r="D96" t="n">
-        <v>189</v>
+        <v>29</v>
       </c>
       <c r="E96" t="n">
-        <v>517</v>
+        <v>313</v>
       </c>
       <c r="F96" t="s">
-        <v>65</v>
+        <v>168</v>
       </c>
       <c r="G96" t="n">
-        <v>565</v>
+        <v>85</v>
       </c>
       <c r="H96" t="n">
-        <v>1551</v>
+        <v>939</v>
       </c>
       <c r="I96" t="s">
-        <v>103</v>
+        <v>206</v>
       </c>
     </row>
     <row r="97" spans="1:9">
       <c r="A97" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="B97" t="n">
-        <v>5605</v>
+        <v>659</v>
       </c>
       <c r="C97" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D97" t="n">
-        <v>55</v>
+        <v>189</v>
       </c>
       <c r="E97" t="n">
-        <v>400</v>
+        <v>517</v>
       </c>
       <c r="F97" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="G97" t="n">
-        <v>163</v>
+        <v>565</v>
       </c>
       <c r="H97" t="n">
-        <v>1200</v>
+        <v>1551</v>
       </c>
       <c r="I97" t="s">
-        <v>213</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to PDB construct selection script.
</commit_message>
<xml_diff>
--- a/analysis/PDB_construct_selection/PDB_constructs.xlsx
+++ b/analysis/PDB_construct_selection/PDB_constructs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="218">
   <si>
     <t>TCAGTTTATCCTAAGGCATTAAGAGATGAATACATCATGTCAAAAACTCTTGGAAGTGGTGCCTGTGGAGAGGTAAAGCTGGCTTTCGAGAGGAAAACATGTAAGAAAGTAGCCATAAAGATCATCAGCAAAAGGAAGTTTGCTATTGGTTCAGCAAGAGAGGCAGACCCAGCTCTCAATGTTGAAACAGAAATAGAAATTTTGAAAAAGCTAAATCATCCTTGCATCATCAAGATTAAAAACTTTTTTGATGCAGAAGATTATTATATTGTTTTGGAATTGATGGAAGGGGGAGAGCTGTTTGACAAAGTGGTGGGGAATAAACGCCTGAAAGAAGCTACCTGCAAGCTCTATTTTTACCAGATGCTCTTGGCTGTGCAGTACCTTCATGAAAACGGTATTATACACCGTGACTTAAAGCCAGAGAATGTTTTACTGTCATCTCAAGAAGAGGACTGTCTTATAAAGATTACTGATTTTGGGCACTCCAAGATTTGGGGAGAGACCTCTCTCATGAGAACCTTATGTGGAACCCCCACCTACTTGGCGCCTGAAGTTCTTGTTTCTGTTGGGACTGCTGGGTATAACCGTGCTGTGGACTGCTGGAGTTTAGGAGTTATTCTTTTTATCTGCCTTAGTGGGTATCCACCTTTCTCTGAGCATAGGACTCAAGTGTCACTGAAGGATCAGATCACCAGTGGAAAATACAACTTCATTCCTGAAGTCTGGGCAGAAGTCTCAGAGAAAGCTCTGGACCTTGTCAAGAAGTTGTTGGTAGTGGATCCAAAGGCACGTTTTACGACAGAAGAAGCCTTAAGACACCCGTGGCTTCAGGATGAAGACATGAAGAGAAAGTTTCAAGATCTTCTGTCTGAGGAAAATGAATCCACAGCTCTACCCCAGGTTCTAGCCCAGCCTTCTACTAGTCGAAAGCGGCCCCGTGAAGGGGAAGCCGAGGGTGCCGAG</t>
   </si>
@@ -35,7 +35,7 @@
     <t>SPQREPQRVSHEQFRAALQLVVDPGDPRSYLDNFIKIGEGSTGIVCIATVRSSGKLVAVKKMDLRKQQRRELLFNEVVIMRDYQHENVVEMYNSYLVGDELWVVMEFLEGGALTDIVTHTRMNEEQIAAVCLAVLQALSVLHAQGVIHRDIKSDSILLTHDGRVKLSDFGFCAQVSKEVPRRKSLVGTPYWMAPELISRLPYGPEVDIWSLGIMVIEMVDGEPPYFNEPPLKAMKMIRDNLPPRLKNLHKVSPSLKGFLDRLLVRDPAQRATAAELLKHPFLAKAGPPASIVPLMRQNRTR</t>
   </si>
   <si>
-    <t>ELKDDDFEKISELGAGNGGVVFKVSHKPSGLVMARKLIHLEIKPAIRNQIIRELQVLHECNSPYIVGFYGAFYSDGEISICMEHMDGGSLDQVLKKAGRIPEQILGKVSIAVIKGLTYLREKHKIMHRAYGMDSRPPMAIFELLDYIVNEPPPKLPSGVFSLEFQDFVNKCLIKNPAERADLKQLMVHAFIKRSDAEEVDFAGWLCSTIGLN</t>
+    <t>EAFLTQKAKVGELKDDDFERISELGAGNGGVVTKVQHRPSGLIMARKLIHLEIKPAIRNQIIRELQVLHECNSPYIVGFYGAFYSDGEISICMEHMDGGSLDQVLKEAKRIPEEILGKVSIAVLRGLAYLREKHQIMHRDVKPSNILVNSRGEIKLCDFGVSGQLIDSMANSFVGTRSYMAPERLQGTHYSVQSDIWSMGLSLVELAVGRYPIPPPDAKELEAIFGRPVVDGEEGEPHSISPRPRPPGRPVSGHGMDSRPAMAIFELLDYIVNEPPPKLPNGVFTPDFQEFVNKCLIKNPAERADLKMLTNHTFIKRSEVEEVDFAGWLCKTLRLNQPGTPTRTAV</t>
   </si>
   <si>
     <t>TACCAGCTCTTCGAGGAATTGGGCAAGGGAGCCTTCTCGGTGGTGCGAAGGTGTGTGAAGGTGCTGGCTGGCCAGGAGTATGCTGCCAAGATCATCAACACAAAGAAGCTGTCAGCCAGAGACCATCAGAAGCTGGAGCGTGAAGCCCGCATCTGCCGCCTGCTGAAGCACCCCAACATCGTCCGACTACATGACAGCATCTCAGAGGAGGGACACCACTACCTGATCTTCGACCTGGTCACTGGTGGGGAACTGTTTGAAGATATCGTGGCCCGGGAGTATTACAGTGAGGCGGATGCCAGTCACTGTATCCAGCAGATCCTGGAGGCTGTGCTGCACTGCCACCAGATGGGGGTGGTGCACCGGGACCTGAAGCCTGAGAATCTGTTGCTGGCCTCCAAGCTCAAGGGTGCCGCAGTGAAGCTGGCAGACTTTGGCCTGGCCATAGAGGTGGAGGGGGAGCAGCAGGCATGGTTTGGGTTTGCAGGGACTCCTGGATATCTCTCCCCAGAAGTGCTGCGGAAGGACCCGTACGGGAAGCCTGTGGACCTGTGGGCTTGTGGGGTCATCCTGTACATCCTGCTGGTTGGGTACCCCCCGTTCTGGGATGAGGACCAGCACCGCCTGTACCTGCAGATCAAAGCCGGCGCCTATGATTTCCCATCGCCGGAATGGGACACTGTCACCCCGGAAGCCAAGGATCTGATCAATAAGATGCTGACCATTAACCCATCCAAACGCATCACAGCTGCCGAAGCCCTTAAGCACCCCTGGATCTCGCACCGCTCCACCGTGGCATCCTGCATGCACAGACAGGAGACCGTGGACTGCCTGAAGAAGTTCAATGCCAGGAGGAAACTGAAGGGAGCC</t>
@@ -62,9 +62,6 @@
     <t>MARK2_HUMAN_D0_3IEC_D</t>
   </si>
   <si>
-    <t>MK10_HUMAN_D0_2B1P_A</t>
-  </si>
-  <si>
     <t>CCATTTCCAGAAGGCAAGGTTCTGGATGATATGGAAGGCAATCAGTGGGTACTGGGCAAGAAGATTGGCTCTGGAGGATTTGGATTGATATATTTAGCTTTCCCCACAAATAAACCAGAGAAAGATGCAAGACATGTAGTAAAAGTGGAATATCAAGAAAATGGCCCGTTATTTTCAGAACTTAAATTTTATCAGAGAGTTGCAAAAAAAGACTGTATCAAAAAGTGGATAGAACGCAAACAACTTGATTATTTAGGAATTCCTCTGTTTTATGGATCTGGTCTGACTGAATTCAAGGGAAGAAGTTACAGATTTATGGTAATGGAAAGACTAGGAATAGATTTACAGAAGATCTCAGGCCAGAATGGTACCTTTAAAAAGTCAACTGTCCTGCAATTAGGTATCCGAATGTTGGATGTACTGGAATATATACATGAAAATGAATATGTTCATGGTGATATAAAAGCAGCAAATCTACTTTTGGGTTACAAAAATCCAGACCAGGTTTATCTTGCAGATTATGGACTTTCCTACAGATATTGTCCCAATGGGAACCACAAACAGTATCAGGAAAATCCTAGAAAAGGCCATAATGGGACAATAGAGTTTACCAGCTTGGATGCCCACAAGGGAGTAGCCTTGTCCAGACGAAGTGACGTTGAGATCCTCGGCTACTGCATGCTGCGGTGGTTGTGTGGGAAACTTCCCTGGGAACAGAACCTGAAGGACCCTGTGGCTGTGCAGACTGCTAAAACAAATCTGTTGGACGAGCTCCCCCAGTCAGTGCTTAAATGGGCTCCTTCTGGAAGCAGTTGCTGTGAAATAGCCCAATTTTTGGTATGTGCTCATAGTTTAGCATATGATGAAAAGCCAAACTATCAAGCCCTCAAGAAAATTTTGAACCCTCATGGAATACCTTTAGGACCACTGGACTTTTCCACAAAAGGACAGAGTATAAATGTCCAT</t>
   </si>
   <si>
@@ -83,7 +80,7 @@
     <t>SVKGRIYSILKQIGSGGSSKVFQVLNEKKQIYAIKYVNLEEADNQTLDSYRNEIAYLNKLQQHSDKIIRLYDYEITDQYIYMVMECGNIDLNSWLKKKKSIDPWERKSYWKNMLEAVHTIHQHGIVHSDLKPANFLIVDGMLKLIDFGIANQMQPDTTSVVKDSQVGTVNYMPPEAIKDMSSSRENGKSKSKISPKSDVWSLGCILYYMTYGKTPFQQIINQISKLHAIIDPNHEIEFPDIPEKDLQDVLKCCLKRDPKQRISIPELLAHPYVQIQTHPVNQMAKGTTEE</t>
   </si>
   <si>
-    <t>GTGAAAGAATTCTTAGCCAAAGCCAAAGAAGATTTTCTTAAAAAATGGGAAAGTCCCGCTCAGAACACAGCCCACTTGGATCAGTTTGAACGAATCAAGACCCTCGGCACGGGCTCCTTCGGGCGGGTGATGCTGGTGAAACACAAGGAGACCGGGAACCACTATGCCATGAAGATCCTCGACAAACAGAAGGTGGTGAAACTGAAACAGATCGAACACACCCTGAATGAAAAGCGCATCCTGCAAGCTGTCAACTTTCCGTTCCTCGTCAAACTCGAGTTCTCCTTCAAGGACAACTCAAACTTATACATGGTCATGGAGTACGTGCCCGGCGGGGAGATGTTCTCACACCTACGGCGGATCGGAAGGTTCAGTGAGCCCCATGCCCGTTTCTACGCGGCCCAGATCGTCCTGACCTTTGAGTATCTGCACTCGCTGGATCTCATCTACAGGGACCTGAAGCCGGAGAATCTGCTCATTGACCAGCAGGGCTACATTCAGGTGACAGACTTCGGTTTCGCCAAGCGCGTGAAGGGCCGCACTTGGACCTTGTGCGGCACCCCTGAGTACCTGGCCCCTGAGATTATCCTGAGCAAAGGCTACAACAAGGCCGTGGACTGGTGGGCCCTGGGGGTTCTTATCTATGAAATGGCCGCTGGCTACCCGCCCTTCTTCGCAGACCAGCCCATCCAGATCTATGAGAAGATCGTCTCTGGGAAGGTGCGCTTCCCTTCCCACTTCAGCTCTGACTTGAAGGACCTGCTGCGGAACCTCCTGCAGGTAGATCTCACCAAGCGCTTTGGGAACCTCAAGAATGGGGTCAACGATATCAAGAACCACAAGTGGTTTGCCACAACTGACTGGATTGCCATCTACCAGAGGAAGGTGGAAGCTCCCTTCATACCAAAGTTTAAAGGCCCTGGGGATACGAGTAACTTTGACGACTATGAGGAAGAAGAAATCCGGGTCTCCATCAATGAGAAGTGTGGCAAGGAGTTTTCTGAGTTT</t>
+    <t>ATGTCTCAGGAGAGGCCCACGTTCTACCGGCAGGAGCTGAACAAGACAATCTGGGAGGTGCCCGAGCGTTACCAGAACCTGTCTCCAGTGGGCTCTGGCGCCTATGGCTCTGTGTGTGCTGCTTTTGACACAAAAACGGGGTTACGTGTGGCAGTGAAGAAGCTCTCCAGACCATTTCAGTCCATCATTCATGCGAAAAGAACCTACAGAGAACTGCGGTTACTTAAACATATGAAACATGAAAATGTGATTGGTCTGTTGGACGTTTTTACACCTGCAAGGTCTCTGGAGGAATTCAATGATGTGTATCTGGTGACCCATCTCATGGGGGCAGATCTGAACAACATTGTGAAATGTCAGAAGCTTACAGATGACCATGTTCAGTTCCTTATCTACCAAATTCTCCGAGGTCTAAAGTATATACATTCAGCTGACATAATTCACAGGGACCTAAAACCTAGTAATCTAGCTGTGAATGAAGACTGTGAGCTGAAGATTCTGGATTTTGGACTGGCTCGGCACACAGATGATGAAATGACAGGCTACGTGGCCACTAGGTGGTACAGGGCTCCTGAGATCATGCTGAACTGGATGCATTACAACCAGACAGTTGATATTTGGTCAGTGGGATGCATAATGGCCGAGCTGTTGACTGGAAGAACATTGTTTCCTGGTACAGACCATATTGATCAGTTGAAGCTCATTTTAAGACTCGTTGGAACCCCAGGGGCTGAGCTTTTGAAGAAAATCTCCTCAGAGTCTGCAAGAAACTATATTCAGTCTTTGACTCAGATGCCGAAGATGAACTTTGCGAATGTATTTATTGGTGCCAATCCCCTGGCTGTCGACTTGCTGGAGAAGATGCTTGTATTGGACTCAGATAAGAGAATTACAGCGGCCCAAGCCCTTGCACATGCCTACTTTGCTCAGTACCACGATCCTGATGATGAACCAGTGGCCGATCCTTATGATCAGTCCTTTGAAAGCAGGGACCTCCTTATAGATGAGTGGAAAAGCCTGACCTATGATGAAGTCATCAGCTTTGTGCCACCACCCCTTGACCAAGAAGAGATGGAGTCC</t>
   </si>
   <si>
     <t>TCCCCCAACTACGACAAGTGGGAGATGGAACGCACGGACATCACCATGAAGCACAAGCTGGGCGGGGGCCAGTACGGGGAGGTGTACGAGGGCGTGTGGAAGAAATACAGCCTGACGGTGGCCGTGAAGACCTTGAAGGAGGACACCATGGAGGTGGAAGAGTTCTTGAAAGAAGCTGCAGTCATGAAAGAGATCAAACACCCTAACCTGGTGCAGCTCCTTGGGGTCTGCACCCGGGAGCCCCCGTTCTATATCATCACTGAGTTCATGACCTACGGGAACCTCCTGGACTACCTGAGGGAGTGCAACCGGCAGGAGGTGAACGCCGTGGTGCTGCTGTACATGGCCACTCAGATCTCGTCAGCCATGGAGTACCTGGAGAAGAAAAACTTCATCCACAGAGATCTTGCTGCCCGAAACTGCCTGGTAGGGGAGAACCACTTGGTGAAGGTAGCTGATTTTGGCCTGAGCAGGTTGATGACAGGGGACACCTACACAGCCCATGCTGGAGCCAAGTTCCCCATCAAATGGACTGCACCCGAGAGCCTGGCCTACAACAAGTTCTCCATCAAGTCCGACGTCTGGGCATTTGGAGTATTGCTTTGGGAAATTGCTACCTATGGCATGTCCCCTTACCCGGGAATTGACCTGTCCCAGGTGTATGAGCTGCTAGAGAAGGACTACCGCATGGAGCGCCCAGAAGGCTGCCCAGAGAAGGTCTATGAACTCATGCGAGCATGTTGGCAGTGGAATCCCTCTGACCGGCCCTCCTTTGCTGAAATCCACCAAGCCTTTGAAACAATGTTCCAGGAATCCAGTATCTCAGACGAAGTGGAAAAGGAGCTGGGGAAA</t>
@@ -95,588 +92,552 @@
     <t>KS6A1_HUMAN_D1_3RNY_B</t>
   </si>
   <si>
+    <t>WALNMKELKLLQTIGKGEFGDVMLGDYRGNKVAVKCIKNDATAQAFLAEASVMTQLRHSNLVQLLGVIVEEKGGLYIVTEYMAKGSLVDYLRSRGRSVLGGDCLLKFSLDVCEAMEYLEGNNFVHRDLAARNVLVSEDNVAKVSDFGLTKEASSTQDTGKLPVKWTAPEALREKKFSTKSDVWSFGILLWEIYSFGRVPYPRIPLKDVVPRVEKGYKMDAPDGCPPAVYEVMKNCWHLDAAMRPSFLQLREQLEHIKTHELHL</t>
+  </si>
+  <si>
+    <t>MSRSKRDNNFYSVEIGDSTFTVLKRYQNLKPIGSGAQGIVCAAYDAILERNVAIKKLSRPFQNQTHAKRAYRELVLMKCVNHKNIIGLLNVFTPQKSLEEFQDVYIVMELMDANLCQVIQMELDHERMSYLLYQMLCGIKHLHSAGIIHRDLKPSNIVVKSDCTLKILDFGLARTAGTSFMMTPYVVTRYYRAPEVILGMGYKENVDLWSVGCIMGEMVCHKILFPGRDYIDQWNKVIEQLGTPCPEFMKKLQPTVRTYVENRPKYAGYSFEKLFPDVLFPADSEHNKLKASQARDLLSKMLVIDASKRISVDEALQHPYINVWYDPSEAEAPPPKIPDKQLDEREHTIEEWKELIYKEVMDLE</t>
+  </si>
+  <si>
+    <t>STRAA_HUMAN_D0_3GNI_B</t>
+  </si>
+  <si>
+    <t>MP2K2_HUMAN_D0_1S9I_A</t>
+  </si>
+  <si>
+    <t>PIM1_HUMAN_D0_4A7C_A</t>
+  </si>
+  <si>
+    <t>ATGCCCGGCCCGGCCGCGGGCAGCAGGGCCCGGGTCTACGCCGAGGTGAACAGTCTGAGGAGCCGCGAGTACTGGGACTACGAGGCTCACGTCCCGAGCTGGGGTAATCAAGATGATTACCAACTGGTTCGAAAACTTGGTCGGGGAAAATATAGTGAAGTATTTGAGGCCATTAATATCACCAACAATGAGAGAGTGGTTGTAAAAATCCTGAAGCCAGTGAAGAAAAAGAAGATAAAACGAGAGGTTAAGATTCTGGAGAACCTTCGTGGTGGAACAAATATCATTAAGCTGATTGACACTGTAAAGGACCCCGTGTCAAAGACACCAGCTTTGGTATTTGAATATATCAATAATACAGATTTTAAGCAACTCTACCAGATCCTGACAGACTTTGATATCCGGTTTTATATGTATGAACTACTTAAAGCTCTGGATTACTGCCACAGCAAGGGAATCATGCACAGGGATGTGAAACCTCACAATGTCATGATAGATCACCAACAGAAAAAGCTGCGACTGATAGATTGGGGTCTGGCAGAATTCTATCATCCTGCTCAGGAGTACAATGTTCGTGTAGCCTCAAGGTACTTCAAGGGACCAGAGCTCCTCGTGGACTATCAGATGTATGATTATAGCTTGGACATGTGGAGTTTGGGCTGTATGTTAGCAAGCATGATCTTTCGAAGGGAACCATTCTTCCATGGACAGGACAACTATGACCAGCTTGTTCGCATTGCCAAGGTTCTGGGTACAGAAGAACTGTATGGGTATCTGAAGAAGTATCACATAGACCTAGATCCACACTTCAACGATATCCTGGGACAACATTCACGGAAACGCTGGGAAAACTTTATCCATAGTGAGAACAGACACCTTGTCAGCCCTGAGGCCCTAGATCTTCTGGACAAACTTCTGCGATACGACCATCAACAGAGACTGACTGCCAAAGAGGCCATGGAGCACCCATACTTCTACCCTGTGGTGAAGGAGCAGTCCCAG</t>
+  </si>
+  <si>
+    <t>GGGCCGGAGGATGAGCTGCCCGACTGGGCCGCCGCCAAAGAGTTTTACCAGAAGTACGACCCTAAGGACGTCATCGGCAGAGGAGTGAGCTCTGTGGTCCGCCGTTGTGTTCATCGAGCTACTGGCCACGAGTTTGCGGTGAAGATTATGGAAGTGACAGCTGAGCGGCTGAGTCCTGAGCAGCTGGAGGAGGTGCGGGAAGCCACACGGCGAGAGACACACATCCTTCGCCAGGTCGCCGGCCACCCCCACATCATCACCCTCATCGATTCCTACGAGTCTTCTAGCTTCATGTTCCTGGTGTTTGACCTGATGCGGAAGGGAGAGCTGTTTGACTATCTCACAGAGAAGGTGGCCCTCTCTGAAAAGGAAACCAGGTCCATCATGCGGTCTCTGCTGGAAGCAGTGAGCTTTCTCCATGCCAACAACATTGTGCATCGAGATCTGAAGCCCGAGAATATTCTCCTAGATGACAATATGCAGATCCGACTTTCAGATTTCGGGTTCTCCTGCCACTTGGAACCTGGCGAGAAGCTTCGAGAGTTGTGTGGGACCCCAGGGTATCTAGCGCCAGAGATCCTTAAATGCTCCATGGATGAAACCCACCCAGGCTATGGCAAGGAGGTCGACCTCTGGGCCTGTGGGGTGATCTTGTTCACACTCCTGGCTGGCTCGCCACCCTTCTGGCACCGGCGGCAGATCCTGATGTTACGCATGATCATGGAGGGCCAGTACCAGTTCAGTTCCCCCGAGTGGGATGACCGTTCCAGCACTGTCAAAGACCTGATCTCCAGGCTGCTGCAGGTGGATCCTGAGGCACGCCTGACAGCTGAGCAGGCCCTACAGCACCCCTTCTTTGAGCGT</t>
+  </si>
+  <si>
+    <t>KC1E_HUMAN_D0_4HNI_A</t>
+  </si>
+  <si>
+    <t>VRK2_HUMAN_D0_2V62_B</t>
+  </si>
+  <si>
+    <t>ETYIKLDKLGEGTYATVYKGKSKLTDNLVALKEIRLEHEEGAPCTAIREVSLLKDLKHANIVTLHDIIHTEKSLTLVFEYLDKDLKQYLDDCGNIINMHNVKLFLFQLLRGLAYCHRQKVLHRDLKPQNLLINERGELKLADFGLARAKSIPTKTYSNEVVTLWYRPPDILLGSTDYSTQIDMWGVGCIFYEMATGRPLFPGSTVEEQLHFIFRILGTPTEETWPGILSNEEFKTYNYPKYRAEALLSHAPRLDSDGADLLTKLLQFEGRNRISAEDAMKHPFFLSLGERIHKLPDTTSIFALKEIQLQKEASLRS</t>
+  </si>
+  <si>
+    <t>HQLQPRRVSFRGEASETLQSPGYDPSRPESFFQQSFQRLSRLGHGSYGEVFKVRSKEDGRLYAVKRSMSPFRGPKDRARKLAEVGSHEKVGQHPCCVRLEQAWEEGGILYLQTELCGPSLQQHCEAWGASLPEAQVWGYLRDTLLALAHLHSQGLVHLDVKPANIFLGPRGRCKLGDFGLLVELGTAGAGEVQEGDPRYMAPELLQGSYGTAADVFSLGLTILEVACNMELPHGGEGWQQLRQGYLPPEFTAGLSSELRSVLVMMLEPDPKLRATAEALLALPVLRQP</t>
+  </si>
+  <si>
+    <t>aa_end</t>
+  </si>
+  <si>
+    <t>PMYT1_HUMAN_D0_3P1A_A</t>
+  </si>
+  <si>
+    <t>MK08_HUMAN_D0_2NO3_A</t>
+  </si>
+  <si>
+    <t>TCGGTTAAAGGAAGAATTTATTCCATATTAAAGCAGATAGGAAGTGGAGGTTCAAGCAAGGTATTTCAGGTGTTAAATGAAAAGAAACAGATATATGCTATAAAATATGTGAACTTAGAAGAAGCAGATAACCAAACTCTTGATAGTTACCGGAACGAAATAGCTTATTTGAATAAACTACAACAACACAGTGATAAGATCATCCGACTTTATGATTATGAAATCACGGACCAGTACATCTACATGGTAATGGAGTGTGGAAATATTGATCTTAATAGTTGGCTTAAAAAGAAAAAATCCATTGATCCATGGGAACGCAAGAGTTACTGGAAAAATATGTTAGAGGCAGTTCACACAATCCATCAACATGGCATTGTTCACAGTGATCTTAAACCAGCTAACTTTCTGATAGTTGATGGAATGCTAAAGCTAATTGATTTTGGGATTGCAAACCAAATGCAACCAGATACAACAAGTGTTGTTAAAGATTCTCAGGTTGGCACAGTTAATTATATGCCACCAGAAGCAATCAAAGATATGTCTTCCTCCAGAGAGAATGGGAAATCTAAGTCAAAGATAAGCCCCAAAAGTGATGTTTGGTCCTTAGGATGTATTTTGTACTATATGACTTACGGGAAAACACCATTTCAGCAGATAATTAATCAGATTTCTAAATTACATGCCATAATTGATCCTAATCATGAAATTGAATTTCCCGATATTCCAGAGAAAGATCTTCAAGATGTGTTAAAGTGTTGTTTAAAAAGGGACCCAAAACAGAGGATATCCATTCCTGAGCTCCTGGCTCATCCATATGTTCAAATTCAAACTCATCCAGTTAACCAAATGGCCAAGGGAACCACTGAAGAA</t>
+  </si>
+  <si>
+    <t>PAK1_HUMAN_D0_3Q52_A</t>
+  </si>
+  <si>
+    <t>CACCACCATCACCACCATTCGCACTCGGGGCCGGAGATCTCGCGGATTATCGTCGACCCCACGACTGGGAAGCGCTACTGCCGGGGCAAAGTGCTGGGAAAGGGTGGCTTTGCAAAATGTTACGAGATGACAGATTTGACAAATAACAAAGTCTACGCCGCAAAAATTATTCCTCACAGCAGAGTAGCTAAACCTCATCAAAGGGAAAAGATTGACAAAGAAATAGAGCTTCACAGAATTCTTCATCATAAGCATGTAGTGCAGTTTTACCACTACTTCGAGGACAAAGAAAACATTTACATTCTCTTGGAATACTGCAGTAGAAGGTCAATGGCTCATATTTTGAAAGCAAGAAAGGTGTTGACAGAGCCAGAAGTTCGATACTACCTCAGGCAGATTGTGTCTGGACTGAAATACCTTCATGAACAAGAAATCTTGCACAGAGATCTCAAACTAGGGAACTTTTTTATTAATGAAGCCATGGAACTAAAAGTTGGGGACTTCGGTCTGGCAGCCAGGCTAGAACCCTTGGAACACAGAAGGAGAACGATATGTGGTACCCCAAATTATCTCTCTCCTGAAGTCCTCAACAAACAAGGACATGGCTGTGAATCAGACATTTGGGCCCTGGGCTGTGTAATGTATACAATGTTACTAGGGAGGCCCCCATTTGAAACTACAAATCTCAAAGAAACTTATAGGTGCATAAGGGAAGCAAGGTATACAATGCCGTCCTCATTGCTGGCTCCTGCCAAGCACTTAATTGCTAGTATGTTGTCCAAAAACCCAGAGGATCGTCCCAGTTTGGATGACATCATTCGACATGACTTTTTTTTGCAGGGCTTCACTCCGGACAGACTGTCTTCTAGCTGTTGTCATACAGTTCCAGATTTCCACTTATCAAGCCCAGCT</t>
+  </si>
+  <si>
+    <t>GAAACAAAGTATACTGTGGACAAGAGGTTTGGCATGGATTTTAAAGAAATAGAATTAATTGGCTCAGGTGGATTTGGCCAAGTTTTCAAAGCAAAACACAGAATTGACGGAAAGACTTACGTTATTAAACGTGTTAAATATAATAACGAGAAGGCGGAGCGTGAAGTAAAAGCATTGGCAAAACTTGATCATGTAAATATTGTTCACTACAATGGCTGTTGGGATGGATTTGATTATGATCCTGAGACCAGTGATGATTCTCTTGAGAGCAGTGATTATGATCCTGAGAACAGCAAAAATAGTTCAAGGTCAAAGACTAAGTGCCTTTTCATCCAAATGGAATTCTGTGATAAAGGGACCTTGGAACAATGGATTGAAAAAAGAAGAGGCGAGAAACTAGACAAAGTTTTGGCTTTGGAACTCTTTGAACAAATAACAAAAGGGGTGGATTATATACATTCAAAAAAATTAATTCATAGAGATCTTAAGCCAAGTAATATATTCTTAGTAGATACAAAACAAGTAAAGATTGGAGACTTTGGACTTGTAACATCTCTGAAAAATGATGGAAAGCGAACAAGGAGTAAGGGAACTTTGCGATACATGAGCCCAGAACAGATTTCTTCGCAAGACTATGGAAAGGAAGTGGACCTCTACGCTTTGGGGCTAATTCTTGCTGAACTTCTTCATGTATGTGACACTGCTTTTGAAACATCAAAGTTTTTCACAGACCTACGGGATGGCATCATCTCAGATATATTTGATAAAAAAGAAAAAACTCTTCTACAGAAATTACTCTCAAAGAAACCTGAGGATCGACCTAACACATCTGAAATACTAAGGACCTTGACTGTGTGGAAGAAAAGCCCAGAGAAAAATGAACGACACACATGT</t>
+  </si>
+  <si>
+    <t>PAK7_HUMAN_D0_2F57_B</t>
+  </si>
+  <si>
+    <t>expression tag location</t>
+  </si>
+  <si>
+    <t>GAGAACTTCCAAAAGGTGGAAAAGATCGGAGAGGGCACGTACGGAGTTGTGTACAAAGCCAGAAACAAGTTGACGGGAGAGGTGGTGGCGCTTAAGAAAATCCGCCTGGACACTGAGACTGAGGGTGTGCCCAGTACTGCCATCCGAGAGATCTCTCTGCTTAAGGAGCTTAACCATCCTAATATTGTCAAGCTGCTGGATGTCATTCACACAGAAAATAAACTCTACCTGGTTTTTGAATTTCTGCACCAAGATCTCAAGAAATTCATGGATGCCTCTGCTCTCACTGGCATTCCTCTTCCCCTCATCAAGAGCTATCTGTTCCAGCTGCTCCAGGGCCTAGCTTTCTGCCATTCTCATCGGGTCCTCCACCGAGACCTTAAACCTCAGAATCTGCTTATTAACACAGAGGGGGCCATCAAGCTAGCAGACTTTGGACTAGCCAGAGCTTTTGGAGTCCCTGTTCGTACTTACACCCATGAGGTGGTGACCCTGTGGTACCGAGCTCCTGAAATCCTCCTGGGCTGCAAATATTATTCCACAGCTGTGGACATCTGGAGCCTGGGCTGCATCTTTGCTGAGATGGTGACTCGCCGGGCCCTATTCCCTGGAGATTCTGAGATTGACCAGCTCTTCCGGATCTTTCGGACTCTGGGGACCCCAGATGAGGTGGTGTGGCCAGGAGTTACTTCTATGCCTGATTACAAGCCAAGTTTCCCCAAGTGGGCCCGGCAAGATTTTAGTAAAGTTGTACCTCCCCTGGATGAAGATGGACGGAGCTTGTTATCGCAAATGCTGCACTACGACCCTAACAAGCGGATTTCGGCCAAGGCAGCCCTGGCTCACCCTTTCTTCCAGGATGTGACCAAGCCAGTACCCCATCTT</t>
+  </si>
+  <si>
+    <t>GGGGAATGCAGTCAGAAGGGTCCTGTCCCCTTTAGCCATTGCCTTCCCACAGAAAAACTGCAACGCTGTGAGAAGATTGGGGAAGGGGTGTTTGGCGAAGTGTTTCAAACAATTGCTGATCACACACCCGTAGCCATAAAAATCATTGCTATTGAAGGACCAGATTTAGTCAATGGATCCCATCAGAAAACCTTTGAGGAAATCCTGCCAGAGATCATCATCTCCAAAGAGTTGAGCCTCTTATCCGGTGAAGTGTGCAACCGCACAGAAGGCTTTATCGGGCTGAACTCAGTGCACTGTGTCCAGGGATCTTACCCTCCCTTGCTCCTCAAAGCCTGGGATCACTATAATTCAACCAAAGGCTCTGCAAATGACCGGCCTGATTTTTTTAAAGACGACCAGCTCTTCATTGTGCTGGAATTTGAGTTTGGAGGGATTGACTTAGAGCAAATGCGAACCAAGTTGTCTTCCTTGGCTACTGCAAAGAGCATTCTACACCAGCTCACAGCCTCCCTCGCAGTGGCAGAGGCATCACTGCGCTTTGAGCACCGAGACTTACACTGGGGGAACGTGCTCTTAAAGAAAACCAGCCTCAAAAAACTCCACTACACCCTCAATGGGAAGAGCAGCACTATCCCCAGCTGTGGGTTGCAAGTGAGCATCATTGACTACACCCTGTCGCGCTTGGAACGGGATGGGATTGTGGTTTTCTGTGACGTTTCCATGGATGAGGACCTGTTTACCGGTGACGGTGACTACCAGTTTGACATCTACAGGCTCATGAAGAAGGAGAATAACAACCGCTGGGGTGAATATCACCCTTATAGTAATGTGCTCTGGTTACATTACCTGACAGACAAGATGCTGAAACAAATGACCTTCAAGACTAAATGTAACACTCCTGCCATGAAGCAAATTAAGAGAAAAATCCAGGAGTTCCACAGGACAATGCTGAACTTCAGCTCTGCCACTGACTTGCTCTGCCAGCACAGACTGTTTAAG</t>
+  </si>
+  <si>
+    <t>TDSLPGKFEDMYKLTSELLGEGAYAKVQGAVSLQNGKEYAVKIIEKQAGHSRSRVFREVETLYQCQGNKNILELIEFFEDDTRFYLVFEKLQGGSILAHIQKQKHFNEREASRVVRDVAAALDFLHTKDKVSLCHLGGSARAPSGLTAAPTSLGSSDPPTSASQVAGTTGIDHRDLKPENILCESPEKVSPVKICDFDLGSGMKLNNSCTPITTPELTTPCGSAEYMAPEVGEVFTDQATFYDKRCDLWSLGVVLYIMLSGYPPFVGHCGADCGWDRGEVCRVCQNKLFESIQEGKYEFPDKDWAHISSEAKDLISKLLVRDAKQRLSAAQVLQHPWVQGQAPEKG</t>
+  </si>
+  <si>
+    <t>DAPK1_HUMAN_D0_4B4L_A</t>
+  </si>
+  <si>
+    <t>EDSLTKQPEEVFDVLEKLGEGSYGSVFKAIHKESGQVVAIKQVPVESDLQEIIKEISIMQQCDSPYVVKYYGSYFKNTDLWIVMEYCGAGSVSDIIRLRNKTLIEDEIATILKSTLKGLEYLHFMRKIHRDIKAGNILLNTEGHAKLADFGVAGQLTDTMAKRNTVIGTPFWMAPEVIQEIGYNCVADIWSLGITSIEMAEGKPPYADIHPMRAIFMIPTNPPPTFRKPELWSDDFTDFVKKCLVKNPEQRATATQLLQHPFIKNAKPVSILRDLITEAMEIKAKRHEEQQRELEEEE</t>
+  </si>
+  <si>
+    <t>ATGAGCCTCATCCGGAAAAAGGGCTTCTACAAGCAGGACGTCAACAAGACCGCCTGGGAGCTGCCCAAGACCTACGTGTCCCCGACGCACGTCGGCAGCGGGGCCTATGGCTCCGTGTGCTCGGCCATCGACAAGCGGTCAGGGGAGAAGGTGGCCATCAAGAAGCTGAGCCGACCCTTTCAGTCCGAGATCTTCGCCAAGCGCGCCTACCGGGAGCTGCTGCTGCTGAAGCACATGCAGCATGAGAACGTCATTGGGCTCCTGGATGTCTTCACCCCAGCCTCCTCCCTGCGCAACTTCTATGACTTCTACCTGGTGATGCCCTTCATGCAGACGGATCTGCAGAAGATCATGGGGATGGAGTTCAGTGAGGAGAAGATCCAGTACCTGGTGTATCAGATGCTCAAAGGCCTTAAGTACATCCACTCTGCTGGGGTCGTGCACAGGGACCTGAAGCCAGGCAACCTGGCTGTGAATGAGGACTGTGAACTGAAGATTCTGGATTTTGGGCTGGCGCGACATGCAGACGCCGAGATGACTGGCTACGTGGTGACCCGCTGGTACCGAGCCCCCGAGGTGATCCTCAGCTGGATGCACTACAACCAGACAGTGGACATCTGGTCTGTGGTCTGTATCATGGCAGAGATGCTGACAGGGAAAACTCTGTTCAAGGGGAAAGATTACCTGGACCAGCTGACCCAGATCCTGAAAGTGACCGGGGTGCCTGGCACGGAGTTTGTGCAGAAGCTGAACGACAAAGCGGCCAAATCCTACATCCAGTCCCTGCCACAGACCCCCAGGAAGGATTTCACTCAGCTGTTCCCACGGGCCAGCCCCCAGGCTGCGGACCTGCTGGAGAAGATGCTGGAGCTAGACGTGGACAAGCGCCTGACGGCCGCGCAGGCCCTCACCCATCCCTTCTTTGAACCCTTCCGGGACCCTGAGGAAGAGACGGAGGCCCAGCAGCCGTTTGATGATTCCTTAGAACACGAGAAACTCACAGTGGATGAATGGAAGCAGCACATCTACAAGGAGATTGTGAACTTCAGCCCCATT</t>
+  </si>
+  <si>
+    <t>ATGAAAGATTATGATGAACTTCTCAAATATTATGAATTACATGAAACTATTGGGACAGGTGGCTTTGCAAAGGTCAAACTTGCCTGCCATATCCTTACTGGAGAGATGGTAGCTATAAAAATCATGGATAAAAACACACTAGGGAGTGATTTGCCCCGGATCAAAACGGAGATTGAGGCCTTGAAGAACCTGAGACATCAGCATATATGTCAACTCTACCATGTGCTAGAGACAGCCAACAAAATATTCATGGTTCTTGAGTACTGCCCTGGAGGAGAGCTGTTTGACTATATAATTTCCCAGGATCGCCTGTCAGAAGAGGAGACCCGGGTTGTCTTCCGTCAGATAGTATCTGCTGTTGCTTATGTGCACAGCCAGGGCTATGCTCACAGGGACCTCAAGCCAGAAAATTTGCTGTTTGATGAATATCATAAATTAAAGCTGATTGACTTTGGTCTCTGTGCAAAACCCAAGGGTAACAAGGATTACCATCTACAGACATGCTGTGGGAGTCTGGCTTATGCAGCACCTGAGTTAATACAAGGCAAATCATATCTTGGATCAGAGGCAGATGTTTGGAGCATGGGCATACTGTTATATGTTCTTATGTGTGGATTTCTACCATTTGATGATGATAATGTAATGGCTTTATACAAGAAGATTATGAGAGGAAAATATGATGTTCCCAAGTGGCTCTCTCCCAGTAGCATTCTGCTTCTTCAACAAATGCTGCAGGTGGACCCAAAGAAACGGATTTCTATGAAAAATCTATTGAACCATCCCTGGATCATGCAAGATTACAACTATCCTGTTGAGTGGCAAAGCAAGAATCCTTTTATTCACCTCGATGATGATTGCGTAACAGAACTTTCTGTACATCACAGAAACAACAGGCAAACAATGGAGGATTTAATTTCACTGTGGCAGTATGATCACCTCACGGCTACCTATCTTCTGCTTCTAGCCAAGAAGGCTCGGGGAAAACCAGTTCGTTTAAGGCTTTCTTCTTTCTCCTGTGGA</t>
+  </si>
+  <si>
+    <t>PAK4_HUMAN_D0_2J0I_A</t>
+  </si>
+  <si>
+    <t>AGVSEYELPEDPRWELPRDRLVLGKPLGEGCFGQVVLAEAIGLDKDKPNRVTKVAVKMLKSDATEKDLSDLISEMEMMKMIGKHKNIINLLGACTQDGPLYVIVEYASKGNLREYLQARRPPGLEYCYNPSHNPEEQLSSKDLVSCAYQVARGMEYLASKKCIHRDLAARNVLVTEDNVMKIADFGLARDIHHIDYYKKTTNGRLPVKWMAPEALFDRIYTHQSDVWSFGVLLWEIFTLGGSPYPGVPVEELFKLLKEGHRMDKPSNCTNELYMMMRDCWHAVPSQRPTFKQLVEDLDRIVALTSNQEYLDLSMPLD</t>
+  </si>
+  <si>
+    <t>ATGGCGGCGGCGGCGGCGGCGGGCGCGGGCCCGGAGATGGTCCGCGGGCAGGTGTTCGACGTGGGGCCGCGCTACACCAACCTCTCGTACATCGGCGAGGGCGCCTACGGCATGGTGTGCTCTGCTTATGATAATGTCAACAAAGTTCGAGTAGCTATCAAGAAAATCAGCCCCTTTGAGCACCAGACCTACTGCCAGAGAACCCTGAGGGAGATAAAAATCTTACTGCGCTTCAGACATGAGAACATCATTGGAATCAATGACATTATTCGAGCACCAACCATCGAGCAAATGAAAGATGTATATATAGTACAGGACCTCATGGAAACAGATCTTTACAAGCTCTTGAAGACACAACACCTCAGCAATGACCATATCTGCTATTTTCTCTACCAGATCCTCAGAGGGTTAAAATATATCCATTCAGCTAACGTTCTGCACCGTGACCTCAAGCCTTCCAACCTGCTGCTCAACACCACCTGTGATCTCAAGATCTGTGACTTTGGCCTGGCCCGTGTTGCAGATCCAGACCATGATCACACAGGGTTCCTGACAGAATATGTGGCCACACGTTGGTACAGGGCTCCAGAAATTATGTTGAATTCCAAGGGCTACACCAAGTCCATTGATATTTGGTCTGTAGGCTGCATTCTGGCAGAAATGCTTTCTAACAGGCCCATCTTTCCAGGGAAGCATTATCTTGACCAGCTGAACCACATTTTGGGTATTCTTGGATCCCCATCACAAGAAGACCTGAATTGTATAATAAATTTAAAAGCTAGGAACTATTTGCTTTCTCTTCCACACAAAAATAAGGTGCCATGGAACAGGCTGTTCCCAAATGCTGACTCCAAAGCTCTGGACTTATTGGACAAAATGTTGACATTCAACCCACACAAGAGGATTGAAGTAGAACAGGCTCTGGCCCACCCATATCTGGAGCAGTATTACGACCCGAGTGACGAGCCCATCGCCGAAGCACCATTCAAGTTCGACATGGAATTGGATGACTTGCCTAAGGAAAAGCTCAAAGAACTAATTTTTGAAGAGACTGCTAGATTCCAGCCAGGATACAGATCT</t>
+  </si>
+  <si>
+    <t>GAGCCCAAGAAGTACGCAGTGACCGACGACTACCAGTTGTCCAAGCAGGTGCTGGGCCTGGGTGTGAACGGCAAAGTGCTGGAGTGCTTCCATCGGCGCACTGGACAGAAGTGTGCCCTGAAGCTCCTGTATGACAGCCCCAAGGCCCGGCAGGAGGTAGACCATCACTGGCAGGCTTCTGGCGGCCCCCATATTGTCTGCATCCTGGATGTGTATGAGAACATGCACCATGGCAAGCGCTGTCTCCTCATCATCATGGAATGCATGGAAGGTGGTGAGTTGTTCAGCAGGATTCAGGAGCGTGGCGACCAGGCTTTCACTGAGAGAGAAGCTGCAGAGATAATGCGGGATATTGGCACTGCCATCCAGTTTCTGCACAGCCATAACATTGCCCACCGAGATGTCAAGCCTGAAAACCTACTCTACACATCTAAGGAGAAAGACGCAGTGCTTAAGCTCACCGATTTTGGCTTTGCTAAGGAGACCACCCAAAATGCCCTGCAGACACCCTGCTATACTCCCTATTATGTGGCCCCTGAGGTCCTGGGTCCAGAGAAGTATGACAAGTCATGTGACATGTGGTCCCTGGGTGTCATCATGTACATCCTCCTTTGTGGCTTCCCACCCTTCTACTCCAACACGGGCCAGGCCATCTCCCCGGGGATGAAGAGGAGGATTCGCCTGGGCCAGTACGGCTTCCCCAATCCTGAGTGGTCAGAAGTCTCTGAGGATGCCAAGCAGCTGATCCGCCTCCTGTTGAAGACAGACCCCACAGAGAGGCTGACCATCACTCAGTTCATGAACCACCCCTGGATCAACCAATCGATGGTAGTGCCACAGACCCCACTCCACACGGCCCGAGTGCTGCAGGAGGACAAAGACCACTGGGACGAAGTCAAGGAGGAGATGACCAGTGCCTTGGCCACTATGCGGGTAGACTACGACCAGGTG</t>
+  </si>
+  <si>
+    <t>MK11_HUMAN_D0_3GC8_A</t>
+  </si>
+  <si>
+    <t>MK14_HUMAN_D0_3K3J_A</t>
+  </si>
+  <si>
+    <t>CDK16_HUMAN_D0_3MTL_A</t>
+  </si>
+  <si>
+    <t>STRDYEIQRERIELGRCIGEGQFGDVHQGIYMSPENPALAVAIKTCKNCTSDSVREKFLQEALTMRQFDHPHIVKLIGVITENPVWIIMELCTLGELRSFLQVRKYSLDLASLILYAYQLSTALAYLESKRFVHRDIAARNVLVSSNDCVKLGDFGLSRYMEDSTYYKASKGKLPIKWMAPESINFRRFTSASDVWMFGVCMWEILMHGVKPFQGVKNNDVIGRIENGERLPMPPNCPPTLYSLMTKCWAYDPSRRPRFTELKAQLSTILEEEKAQQEE</t>
+  </si>
+  <si>
+    <t>PAK6_HUMAN_D0_2C30_A</t>
+  </si>
+  <si>
+    <t>FGFR1_HUMAN_D0_3GQL_B</t>
+  </si>
+  <si>
+    <t>TCTTCGGTCACCGCCAGTGCGGCCCCGGGGACCGCGAGCCTCGTCCCGGATTACTGGATCGACGGCTCCAACAGGGATGCGCTGAGCGATTTCTTCGAGGTGGAGTCGGAGCTGGGACGGGGTGCTACATCCATTGTGTACAGATGCAAACAGAAGGGGACCCAGAAGCCTTATGCTCTCAAAGTGTTAAAGAAAACAGTGGACAAAAAAATCGTAAGAACTGAGATAGGAGTTCTTCTTCGCCTCTCACATCCAAACATTATAAAACTTAAAGAGATATTTGAAACCCCTACAGAAATCAGTCTGGTCCTAGAACTCGTCACAGGAGGAGAACTGTTTGATAGGATTGTGGAAAAGGGATATTACAGTGAGCGAGATGCTGCAGATGCCGTTAAACAAATCCTGGAGGCAGTTGCTTATCTACATGAAAATGGGATTGTCCATCGTGATCTCAAACCAGAGAATCTTCTTTATGCAACTCCAGCCCCAGATGCACCACTCAAAATCGCTGATTTTGGACTCTCTAAAATTGTGGAACATCAAGTGCTCATGAAGACAGTATGTGGAACCCCAGGGTACTGCGCACCTGAAATTCTTAGAGGTTGTGCCTATGGACCTGAGGTGGACATGTGGTCTGTAGGAATAATCACCTACATCTTACTTTGTGGATTTGAACCATTCTATGATGAAAGAGGCGATCAGTTCATGTTCAGGAGAATTCTGAATTGTGAATATTACTTTATCTCCCCCTGGTGGGATGAAGTATCTCTAAATGCCAAGGACTTGGTCAGAAAATTAATTGTTTTGGATCCAAAGAAACGGCTGACTACATTTCAAGCTCTCCAGCATCCGTGGGTCACAGGTAAAGCAGCCAATTTTGTACACATGGATACCGCTCAAAAGAAGCTCCAAGAATTCAATGCCCGGCGTAAGCTTAAGGCAGCGGTGAAGGCTGTGGTGGCCTCTTCCCGCCTGGGA</t>
+  </si>
+  <si>
+    <t>GTCATCATTGACAATAAGCGCTACCTCTTCATCCAGAAACTGGGGGAGGGTGGGTTCAGCTATGTGGACCTAGTGGAAGGGTTACATGATGGACACTTCTACGCCCTGAAGCGAATCCTGTGTCACGAGCAGCAGGACCGGGAGGAGGCCCAGCGAGAAGCCGACATGCATCGCCTCTTCAATCACCCCAACATCCTTCGCCTCGTGGCTTACTGTCTGAGGGAACGGGGTGCTAAGCATGAGGCCTGGCTGCTGCTACCATTCTTCAAGAGAGGTACGCTGTGGAATGAGATAGAAAGGCTGAAGGACAAAGGCAACTTCCTGACCGAGGATCAAATCCTTTGGCTGCTGCTGGGGATCTGCAGAGGCCTTGAGGCCATTCATGCCAAGGGTTATGCCCACAGAGACTTGAAGCCCACCAATATATTGCTTGGAGATGAGGGGCAGCCAGTTTTAATGGACTTGGGTTCCATGAATCAAGCATGCATCCATGTGGAGGGCTCCCGCCAGGCTCTGACCCTGCAGGACTGGGCAGCCCAGCGGTGCACCATCTCCTACCGAGCCCCAGAGCTCTTCTCTGTGCAGAGTCACTGTGTCATCGATGAGCGGACTGATGTCTGGTCCCTAGGCTGCGTGCTATATGCCATGATGTTTGGGGAAGGCCCTTATGACATGGTGTTCCAAAAGGGTGACAGTGTGGCCCTTGCTGTGCAGAACCAACTCAGCATCCCACAAAGCCCCAGGCATTCTTCAGCATTGTGGCAGCTCCTGAACTCGATGATGACCGTGGACCCGCATCAGCGTCCTCACATTCCTCTCCTCCTCAGTCAGCTGGAGGCGCTGCAG</t>
+  </si>
+  <si>
+    <t>BMPR2_HUMAN_D0_3G2F_A</t>
+  </si>
+  <si>
+    <t>CACCAGCTGCAGCCCCGGCGGGTGTCATTCCGGGGCGAGGCCTCAGAGACTCTGCAGAGCCCTGGGTATGACCCAAGCCGGCCAGAGTCCTTCTTCCAGCAGAGCTTCCAGAGGCTCAGCCGCCTGGGCCATGGCTCCTACGGAGAGGTCTTCAAGGTGCGCTCCAAGGAGGACGGCCGGCTCTATGCGGTAAAGCGTTCCATGTCACCATTCCGGGGCCCCAAGGACCGGGCCCGCAAGTTGGCCGAGGTGGGCAGCCACGAGAAGGTGGGGCAGCACCCATGCTGCGTGCGGCTGGAGCAGGCCTGGGAGGAGGGCGGCATCCTGTACCTGCAGACGGAGCTGTGCGGGCCCAGCCTGCAGCAACACTGTGAGGCCTGGGGTGCCAGCCTGCCTGAGGCCCAGGTCTGGGGCTACCTGCGGGACACGCTGCTTGCCCTGGCCCATCTGCACAGCCAGGGCCTGGTGCACCTTGATGTCAAGCCTGCCAACATCTTCCTGGGGCCCCGGGGCCGCTGCAAGCTGGGTGACTTCGGACTGCTGGTGGAGCTGGGTACAGCAGGAGCTGGTGAGGTCCAGGAGGGAGACCCCCGCTACATGGCCCCCGAGCTGCTGCAGGGCTCCTATGGGACAGCAGCGGATGTGTTCAGTCTGGGCCTCACCATCCTGGAAGTGGCATGCAACATGGAGCTGCCCCACGGTGGGGAGGGCTGGCAGCAGCTGCGCCAGGGCTACCTGCCCCCTGAGTTCACTGCCGGTCTGTCTTCCGAGCTGCGTTCTGTCCTTGTCATGATGCTGGAGCCAGACCCCAAGCTGCGGGCCACGGCCGAGGCCCTGCTGGCACTGCCTGTGTTGAGGCAGCCG</t>
+  </si>
+  <si>
+    <t>PHKG2_HUMAN_D0_2Y7J_D</t>
+  </si>
+  <si>
+    <t>MAPK2_HUMAN_D0_2JBO_A</t>
+  </si>
+  <si>
+    <t>HHHHHHSHSGPEISRIIVDPTTGKRYCRGKVLGKGGFAKCYEMTDLTNNKVYAAKIIPHSRVAKPHQREKIDKEIELHRILHHKHVVQFYHYFEDKENIYILLEYCSRRSMAHILKARKVLTEPEVRYYLRQIVSGLKYLHEQEILHRDLKLGNFFINEAMELKVGDFGLAARLEPLEHRRRTICGTPNYLSPEVLNKQGHGCESDIWALGCVMYTMLLGRPPFETTNLKETYRCIREARYTMPSSLLAPAKHLIASMLSKNPEDRPSLDDIIRHDFFLQGFTPDRLSSSCCHTVPDFHLSSPA</t>
+  </si>
+  <si>
+    <t>ATGGAGAAGGACGGCCTGTGCCGCGCTGACCAGCAGTACGAATGCGTGGCGGAGATCGGGGAGGGCGCCTATGGGAAGGTGTTCAAGGCCCGCGACTTGAAGAACGGAGGCCGTTTCGTGGCGTTGAAGCGCGTGCGGGTGCAGACCGGCGAGGAGGGCATGCCGCTCTCCACCATCCGCGAGGTGGCGGTGCTGAGGCACCTGGAGACCTTCGAGCACCCCAACGTGGTCAGGTTGTTTGATGTGTGCACAGTGTCACGAACAGACAGAGAAACCAAACTAACTTTAGTGTTTGAACATGTCGATCAAGACTTGACCACTTACTTGGATAAAGTTCCAGAGCCTGGAGTGCCCACTGAAACCATAAAGGATATGATGTTTCAGCTTCTCCGAGGTCTGGACTTTCTTCATTCACACCGAGTAGTGCATCGCGATCTAAAACCACAGAACATTCTGGTGACCAGCAGCGGACAAATAAAACTCGCTGACTTCGGCCTTGCCCGCATCTATAGTTTCCAGATGGCTCTAACCTCAGTGGTCGTCACGCTGTGGTACAGAGCACCCGAAGTCTTGCTCCAGTCCAGCTACGCCACCCCCGTGGATCTCTGGAGTGTTGGCTGCATATTTGCAGAAATGTTTCGTAGAAAGCCTCTTTTTCGTGGAAGTTCAGATGTTGATCAACTAGGAAAAATCTTGGACGTGATTGGACTCCCAGGAGAAGAAGACTGGCCTAGAGATGTTGCCCTTCCCAGGCAGGCTTTTCATTCAAAATCTGCCCAACCAATTGAGAAGTTTGTAACAGATATCGATGAACTAGGCAAAGACCTACTTCTGAAGTGTTTGACATTTAACCCAGCCAAAAGAATATCTGCCTACAGTGCCCTGTCTCACCCATACTTCCAG</t>
+  </si>
+  <si>
+    <t>ATGTCGGGCCCTCGCGCCGGCTTCTACCGGCAGGAGCTGAACAAGACCGTGTGGGAGGTGCCGCAGCGGCTGCAGGGGCTGCGCCCGGTGGGCTCCGGCGCCTACGGCTCCGTCTGTTCGGCCTACGACGCCCGGCTGCGCCAGAAGGTGGCGGTGAAGAAGCTGTCGCGCCCCTTCCAGTCGCTGATCCACGCGCGCAGAACGTACCGGGAGCTGCGGCTGCTCAAGCACCTGAAGCACGAGAACGTCATCGGGCTTCTGGACGTCTTCACGCCGGCCACGTCCATCGAGGACTTCAGCGAAGTGTACTTGGTGACCACCCTGATGGGCGCCGACCTGAACAACATCGTCAAGTGCCAGGCGCTGAGCGACGAGCACGTTCAATTCCTGGTTTACCAGCTGCTGCGCGGGCTGAAGTACATCCACTCGGCCGGGATCATCCACCGGGACCTGAAGCCCAGCAACGTGGCTGTGAACGAGGACTGTGAGCTCAGGATCCTGGATTTCGGGCTGGCGCGCCAGGCGGACGAGGAGATGACCGGCTATGTGGCCACGCGCTGGTACCGGGCACCTGAGATCATGCTCAACTGGATGCATTACAACCAAACAGTGGATATCTGGTCCGTGGGCTGCATCATGGCTGAGCTGCTCCAGGGCAAGGCCCTCTTCCCGGGAAGCGACTACATTGACCAGCTGAAGCGCATCATGGAAGTGGTGGGCACACCCAGCCCTGAGGTTCTGGCAAAAATCTCCTCGGAACACGCCCGGACATATATCCAGTCCCTGCCCCCCATGCCCCAGAAGGACCTGAGCAGCATCTTCCGTGGAGCCAACCCCCTGGCCATAGACCTCCTTGGAAGGATGCTGGTGCTGGACAGTGACCAGAGGGTCAGTGCAGCTGAGGCACTGGCCCACGCCTACTTCAGCCAGTACCACGACCCCGAGGATGAGCCAGAGGCCGAGCCATATGATGAGAGCGTTGAGGCCAAGGAGCGCACGCTGGAGGAGTGGAAGGAGCTCACTTACCAGGAAGTCCTCAGCTTCAAGCCCCCAGAGCCACCGAAGCCACCTGGCAGCCTGGAGATTGAGCAG</t>
+  </si>
+  <si>
+    <t>E2AK2_HUMAN_D0_3UIU_A</t>
+  </si>
+  <si>
+    <t>MEKYEKIGKIGEGSYGVVFKCRNRDTGQIVAIKKFLESEDDPVIKKIALREIRMLKQLKHPNLVNLLEVFRRKRRLHLVFEYCDHTVLHELDRYQRGVPEHLVKSITWQTLQAVNFCHKHNCIHRDVKPENILITKHSVIKLCDFGFARLLTGPSDYYTDYVATRWYRSPELLVGDTQYGPPVDVWAIGCVFAELLSGVPLWPGKSDVDQLYLIRKTLGDLIPRHQQVFSTNQYFSGVKIPDPEDMEPLELKFPNISYPALGLL</t>
+  </si>
+  <si>
+    <t>GeneID</t>
+  </si>
+  <si>
+    <t>ATGGATGAGCAATCACAAGGAATGCAAGGGCCACCTGTTCCTCAGTTCCAACCACAGAAGGCCTTACGACCGGATATGGGCTATAATACATTAGCCAACTTTCGAATAGAAAAGAAAATTGGTCGCGGACAATTTAGTGAAGTTTATAGAGCAGCCTGTCTCTTGGATGGAGTACCAGTAGCTTTAAAAAAAGTGCAGATATTTGATTTAATGGATGCCAAAGCACGTGCTGATTGCATCAAAGAAATAGATCTTCTTAAGCAACTCAACCATCCAAATGTAATAAAATATTATGCATCATTCATTGAAGATAATGAACTAAACATAGTTTTGGAACTAGCAGATGCTGGCGACCTATCCAGAATGATCAAGCATTTTAAGAAGCAAAAGAGGCTAATTCCTGAAAGAACTGTTTGGAAGTATTTTGTTCAGCTTTGCAGTGCATTGGAACACATGCATTCTCGAAGAGTCATGCATAGAGATATAAAACCAGCTAATGTGTTCATTACAGCCACTGGGGTGGTAAAACTTGGAGATCTTGGGCTTGGCCGGTTTTTCAGCTCAAAAACCACAGCTGCACATTCTTTAGTTGGTACGCCTTATTACATGTCTCCAGAGAGAATACATGAAAATGGATACAACTTCAAATCTGACATCTGGTCTCTTGGCTGTCTACTATATGAGATGGCTGCATTACAAAGTCCTTTCTATGGTGACAAAATGAATTTATACTCACTGTGTAAGAAGATAGAACAGTGTGACTACCCACCTCTTCCTTCAGATCACTATTCAGAAGAACTCCGACAGTTAGTTAATATGTGCATCAACCCAGATCCAGAGAAGCGACCAGACGTCACCTATGTTTATGACGTAGCAAAGAGGATGCATGCATGCACTGCAAGCAGC</t>
+  </si>
+  <si>
+    <t>DAPK3_HUMAN_D0_2J90_A</t>
+  </si>
+  <si>
+    <t>GAAGACAGTTTGACTAAGCAGCCTGAAGAAGTTTTTGATGTATTAGAGAAGCTTGGAGAAGGGTCTTATGGAAGTGTATTTAAAGCAATACACAAGGAATCCGGTCAAGTTGTCGCAATTAAACAAGTACCTGTTGAATCAGATCTTCAGGAAATAATCAAAGAAATTTCCATAATGCAGCAATGTGACAGCCCATATGTTGTAAAGTACTATGGCAGTTATTTTAAGAATACAGACCTCTGGATTGTTATGGAGTACTGTGGCGCTGGCTCTGTCTCAGACATAATTAGATTACGAAACAAGACATTAATAGAAGATGAAATTGCAACCATTCTTAAATCTACATTGAAAGGACTAGAATATTTGCACTTTATGAGAAAAATACACAGAGATATAAAAGCTGGAAATATTCTCCTCAATACAGAAGGACATGCAAAATTGGCAGATTTTGGAGTGGCTGGTCAGTTAACAGATACAATGGCAAAACGCAATACTGTAATAGGAACTCCATTTTGGATGGCTCCTGAGGTGATTCAAGAAATAGGCTATAACTGTGTGGCCGACATCTGGTCCCTTGGCATTACTTCTATAGAAATGGCTGAAGGAAAACCTCCTTATGCTGATATACATCCAATGAGGGCTATTTTTATGATTCCCACAAATCCACCACCAACATTCAGAAAGCCAGAACTTTGGTCCGATGATTTCACCGATTTTGTTAAAAAGTGTTTGGTGAAGAATCCTGAGCAGAGAGCTACTGCAACACAACTTTTACAGCATCCTTTTATCAAGAATGCCAAACCTGTATCAATATTAAGAGACCTGATCACAGAAGCTATGGAGATCAAAGCTAAAAGACATGAGGAACAGCAACGAGAATTGGAAGAGGAAGAA</t>
+  </si>
+  <si>
+    <t>MSGPVPSRARVYTDVNTHRPREYWDYESHVVEWGNQDDYQLVRKLGRGKYSEVFEAINITNNEKVVVKILKPVKKKKIKREIKILENLRGGPNIITLADIVKDPVSRTPALVFEHVNNTDFKQLYQTLTDYDIRFYMYEILKALDYCHSMGIMHRDVKPHNVMIDHEHRKLRLIDWGLAEFYHPGQEYNVRVASRYFKGPELLVDYQMYDYSLDMWSLGCMLASMIFRKEPFFHGHDNYDQLVRIAKVLGTEDLYDYIDKYNIELDPRFNDILGRHSRKRWERFVHSENQHLVSPEALDFLDKLLRYDHQSRLTAREAMEHPYFYTVVKDQARMG</t>
+  </si>
+  <si>
+    <t>TCCAGGGTGTCCCATGAACAGTTTCGGGCGGCCCTGCAGCTGGTGGTCAGCCCAGGAGACCCCAGGGAATACTTGGCCAACTTTATCAAAATCGGGGAAGGCTCAACCGGCATCGTATGCATCGCCACCGAGAAACACACAGGGAAACAAGTTGCAGTGAAGAAAATGGACCTCCGGAAGCAACAGAGACGAGAACTGCTTTTCAATGAGGTCGTGATCATGCGGGATTACCACCATGACAATGTGGTTGACATGTACAGCAGCTACCTTGTCGGCGATGAGCTCTGGGTGGTCATGGAGTTTCTAGAAGGTGGTGCCTTGACAGACATTGTGACTCACACCAGAATGAATGAAGAACAGATAGCTACTGTCTGCCTGTCAGTTCTGAGAGCTCTCTCCTACCTTCATAACCAAGGAGTGATTCACAGGGACATAAAAAGTGACTCCATCCTCCTGACAAGCGATGGCCGGATAAAGTTGTCTGATTTTGGTTTCTGTGCTCAAGTTTCCAAAGAGGTGCCGAAGAGGAAATCATTGGTTGGCACTCCCTACTGGATGGCCCCTGAGGTGATTTCTAGGCTACCTTATGGGACAGAGGTGGACATCTGGTCCCTCGGGATCATGGTGATAGAAATGATTGATGGCGAGCCCCCCTACTTCAATGAGCCTCCCCTCCAGGCGATGCGGAGGATCCGGGACAGTTTACCTCCAAGAGTGAAGGACCTACACAAGGTTTCTTCAGTGCTCCGGGGATTCCTAGACTTGATGTTGGTGAGGGAGCCCTCTCAGAGAGCAACAGCCCAGGAACTCCTCGGACATCCATTCTTAAAACTAGCAGGTCCACCGTCTTGCATTGTCCCCCTCATGAGACAATACAGGCATCAC</t>
+  </si>
+  <si>
+    <t>KRQWALEDFEIGRPLGKGKFGNVYLAREKQSKFILALKVLFKAQLEKAGVEHQLRREVEIQSHLRHPNILRLYGYFHDATRVYLILEYAPLGTVYRELQKLSKFDEQRTATYITELANALSYCHSKRVIHRDIKPENLLLGSAGELKIADFGWSVHAPSSRRTTLCGTLDYLPPEMIEGRMHDEKVDLWSLGVLCYEFLVGKPPFEANTYQETYKRISRVEFTFPDFVTEGARDLISRLLKHNPSQRPMLREVLEHPWITANSSKPS</t>
+  </si>
+  <si>
+    <t>SLK_HUMAN_D0_2JFL_A</t>
+  </si>
+  <si>
+    <t>SRVSHEQFRAALQLVVSPGDPREYLANFIKIGEGSTGIVCIATEKHTGKQVAVKKMDLRKQQRRELLFNEVVIMRDYHHDNVVDMYSSYLVGDELWVVMEFLEGGALTDIVTHTRMNEEQIATVCLSVLRALSYLHNQGVIHRDIKSDSILLTSDGRIKLSDFGFCAQVSKEVPKRKSLVGTPYWMAPEVISRLPYGTEVDIWSLGIMVIEMIDGEPPYFNEPPLQAMRRIRDSLPPRVKDLHKVSSVLRGFLDLMLVREPSQRATAQELLGHPFLKLAGPPSCIVPLMRQYRHH</t>
+  </si>
+  <si>
+    <t>TQTVHEFAKELDATNISIDKVVGAGEFGEVCSGRLKLPSKKEISVAIKTLKVGYTEKQRRDFLGEASIMGQFDHPNIIRLEGVVTKSKPVMIVTEYMENGSLDSFLRKHDAQFTVIQLVGMLRGIASGMKYLSDMGYVHRDLAARNILINSNLVCKVSDFGLSRVLEDDPEAAYTTRGGKIPIRWTSPEAIAYRKFTSASDVWSYGIVLWEVMSYGERPYWEMSNQDVIKAVDEGYRLPPPMDCPAALYQLMLDCWQKDRNNRPKFEQIVSILDKLIRNPGSLKIITSAAARPSNLLLDQSNVDITTFRTTGDWLNGVWTAHCKEIFTGVEYSSCDTIAKIS</t>
+  </si>
+  <si>
+    <t>QQFPQFHVKSGLQIKKNAIIDDYKVTSQVLGLGINGKVLQIFNKRTQEKFALKMLQDCPKARREVELHWRASQCPHIVRIVDVYENLYAGRKCLLIVMECLDGGELFSRIQDRGDQAFTEREASEIMKSIGEAIQYLHSINIAHRDVKPENLLYTSKRPNAILKLTDFGFAKETTSHNSLTTPCYTPYYVAPEVLGPEKYDKSCDMWSLGVIMYILLCGYPPFYSNHGLAISPGMKTRIRMGQYEFPNPEWSEVSEEVKMLIRNLLKTEPTQRMTITEFMNHPWIMQSTKVPQTPLHTSRVLKEDKERWEDVKGCLHDKNSDQA</t>
+  </si>
+  <si>
+    <t>CSK21_HUMAN_D0_3AXW_A</t>
+  </si>
+  <si>
+    <t>ATCTRFTDDYQLFEELGKGAFSVVRRCVKKTPTQEYAAKIINTKKLSARDHQKLEREARICRLLKHPNIVRLHDSISEEGFHYLVFDLVTGGELFEDIVAREYYSEADASHCIHQILESVNHIHQHDIVHRDLKPENLLLASKCKGAAVKLADFGLAIEVQGEQQAWFGFAGTPGYLSPEVLRKDPYGKPVDIWACGVILYILLVGYPPFWDEDQHKLYQQIKAGAYDFPSPEWDTVTPEAKNLINQMLTINPAKRITADQALKHPWVCQRSTVASMMHRQETVECLRKFNARRKLKGAILTTMLVSRNFS</t>
+  </si>
+  <si>
+    <t>VRK3_HUMAN_D0_2JII_A</t>
+  </si>
+  <si>
+    <t>CGTGTAAAAGCAGCTCAAGCTGGAAGACAGAGCTCTGCAAAGAGACATCTTGCAGAACAATTTGCAGTTGGAGAGATAATAACTGACATGGCAAAAAAGGAATGGAAAGTAGGATTACCCATTGGCCAAGGAGGCTTTGGCTGTATATATCTTGCTGATATGAATTCTTCAGAGTCAGTTGGCAGTGATGCACCTTGTGTTGTAAAAGTGGAACCCAGTGACAATGGACCTCTTTTTACTGAATTAAAGTTCTACCAACGAGCTGCAAAACCAGAGCAAATTCAGAAATGGATTCGTACCCGTAAGCTGAAGTACCTGGGTGTTCCTAAGTATTGGGGGTCTGGTCTACATGACAAAAATGGAAAAAGTTACAGGTTTATGATAATGGATCGCTTTGGGAGTGACCTTCAGAAAATATATGAAGCAAATGCCAAAAGGTTTTCTCGGAAAACTGTCTTGCAGCTAAGCTTAAGAATTCTGGATATTCTGGAATATATTCACGAGCATGAGTATGTGCATGGAGATATCAAGGCCTCAAATCTTCTTCTGAACTACAAGAATCCTGACCAGGTGTACTTGGTAGATTATGGCCTTGCTTATCGGTACTGCCCAGAAGGAGTTCATAAAGAATACAAAGAAGACCCCAAAAGATGTCACGATGGCACTATTGAATTCACGAGCATCGATGCACACAATGGCGTGGCCCCATCAAGACGTGGTGATTTGGAAATACTTGGTTATTGCATGATCCAATGGCTTACTGGCCATCTTCCTTGGGAGGATAATTTGAAAGATCCTAAATATGTTAGAGATTCCAAAATTAGATACAGAGAAAATATTGCAAGTTTGATGGACAAATGTTTTCCTGAGAAAAACAAACCAGGTGAAATTGCCAAATACATGGAAACAGTGAAATTACTAGACTACACTGAAAAACCTCTTTATGAAAATTTACGTGACATTCTTTTGCAAGGACTAAAAGCTATAGGAAGTAAGGATGATGGCAAATTGGACCTCAGTGTTGTGGAGAATGGAGGTTTGAAAGCAAAAACAATAACAAAGAAGCGAAAGAAAGAAATTGAAGAA</t>
+  </si>
+  <si>
+    <t>MP2K6_HUMAN_D0_3VN9_A</t>
+  </si>
+  <si>
+    <t>RVKAAQAGRQSSAKRHLAEQFAVGEIITDMAKKEWKVGLPIGQGGFGCIYLADMNSSESVGSDAPCVVKVEPSDNGPLFTELKFYQRAAKPEQIQKWIRTRKLKYLGVPKYWGSGLHDKNGKSYRFMIMDRFGSDLQKIYEANAKRFSRKTVLQLSLRILDILEYIHEHEYVHGDIKASNLLLNYKNPDQVYLVDYGLAYRYCPEGVHKEYKEDPKRCHDGTIEFTSIDAHNGVAPSRRGDLEILGYCMIQWLTGHLPWEDNLKDPKYVRDSKIRYRENIASLMDKCFPEKNKPGEIAKYMETVKLLDYTEKPLYENLRDILLQGLKAIGSKDDGKLDLSVVENGGLKAKTITKKRKKEIEE</t>
+  </si>
+  <si>
+    <t>MKNK1_HUMAN_D0_2HW6_B</t>
+  </si>
+  <si>
+    <t>ATGGAGGCAGCAGCATCCGAACCCTCTCTTGATCTAGATAATCTGAAACTGTTGGAGCTGATTGGCCGAGGTCGATATGGAGCAGTATATAAAGGCTCCTTGGATGAGCGTCCAGTTGCTGTAAAAGTGTTTTCCTTTGCAAACCGTCAGAATTTTATCAACGAAAAGAACATTTACAGAGTGCCTTTGATGGAACATGACAACATTGCCCGCTTTATAGTTGGAGATGAGAGAGTCACTGCAGATGGACGCATGGAATATTTGCTTGTGATGGAGTACTATCCCAATGGATCTTTATGCAAGTATTTAAGTCTCCACACAAGTGACTGGGTAAGCTCTTGCCGTCTTGCTCATTCTGTTACTAGAGGACTGGCTTATCTTCACACAGAATTACCACGAGGAGATCATTATAAACCTGCAATTTCCCATCGAGATTTAAACAGCAGAAATGTCCTAGTGAAAAATGATGGAACCTGTGTTATTAGTGACTTTGGACTGTCCATGAGGCTGACTGGAAATAGACTGGTGCGCCCAGGGGAGGAAGATAATGCAGCCATAAGCGAGGTTGGCACTATCAGATATATGGCACCAGAAGTGCTAGAAGGAGCTGTGAACTTGAGGGACTGTGAATCAGCTTTGAAACAAGTAGACATGTATGCTCTTGGACTAATCTATTGGGAGATATTTATGAGATGTACAGACCTCTTCCCAGGGGAATCCGTACCAGAGTACCAGATGGCTTTTCAGACAGAGGTTGGAAACCATCCCACTTTTGAGGATATGCAGGTTCTCGTGTCTAGGGAAAAACAGAGACCCAAGTTCCCAGAAGCCTGGAAAGAAAATAGCCTGGCAGTGAGGTCACTCAAGGAGACAATCGAAGACTGTTGGGACCAGGATGCAGAGGCTCGGCTTACTGCACAGTGTGCTGAGGAAAGGATGGCTGAACTTATGATGATTTGGGAAAGAAACAAATCTGTGAGCCCAACA</t>
+  </si>
+  <si>
+    <t>DEQPHIGNYRLLKTIGKGNFAKVKLARHILTGREVAIKIIDKTQLNPTSLQKLFREVRIMKILNHPNIVKLFEVIETEKTLYLIMEYASGGEVFDYLVAHGRMKEKEARSKFRQIVSAVQYCHQKRIVHRDLKAENLLLDADMNIKIADFGFSNEFTVGGKLDTFCGSPPYAAPELFQGKKYDGPEVDVWSLGVILYTLVSGSLPFDGQNLKELRERVLRGKYRIPFYMSTDCENLLKRFLVLNPIKRGTLEQIMKDRWINAGHEEDELKPFVEPELDISDQKRIDIMVGMGYSQEEIQESLSKMKYDEITATYLLLGRKSSE</t>
+  </si>
+  <si>
+    <t>KS6A3_HUMAN_D1_4JG7_A</t>
+  </si>
+  <si>
+    <t>KCC4_HUMAN_D0_2W4O_A</t>
+  </si>
+  <si>
+    <t>CSK_HUMAN_D0_3D7T_A</t>
+  </si>
+  <si>
+    <t>KCC2A_HUMAN_D0_2VZ6_B</t>
+  </si>
+  <si>
+    <t>ATGTCTGATGAGGAGATCTTGGAGAAATTACGAAGCATAGTGAGTGTGGGCGATCCTAAGAAGAAATATACACGGTTTGAGAAGATTGGACAAGGTGCTTCAGGCACCGTGTACACAGCAATGGATGTGGCCACAGGACAGGAGGTGGCCATTAAGCAGATGAATCTTCAGCAGCAGCCCAAGAAAGAGCTGATTATTAATGAGATCCTGGTCATGAGGGAAAACAAGAACCCAAACATTGTGAATTACTTGGACAGTTACCTCGTGGGAGATGAGCTGTGGGTTGTTATGGAATACTTGGCTGGAGGCTCCTTGACAGATGTGGTGACAGAAACTTGCATGGATGAAGGCCAAATTGCAGCTGTGTGCCGTGAGTGTCTGCAGGCTCTGGAGTTCTTGCATTCGAACCAGGTCATTCACAGAGACATCAAGAGTGACAATATTCTGTTGGGAATGGATGGCTCTGTCAAGCTAACTGACTTTGGATTCTGTGCACAGATAACCCCAGAGCAGAGCAAACGGAGCACCATGGTAGGAACCCCATACTGGATGGCACCAGAGGTTGTGACACGAAAGGCCTATGGGCCCAAGGTTGACATCTGGTCCCTGGGCATCAAGGCCATCGAAATGATTGAAGGGGAGCCTCCATACCTCAATGAAAACCCTCTGAGAGCCTTGTACCTCATTGCCACCAATGGGACCCCAGAACTTCAGAACCCAGAGAAGCTGTCAGCTATCTTCCGGGACTTTCTGAACCGCTGTCTCGAGATGGATGTGGAGAAGAGAGGTTCAGCTAAAGAGCTGCTACAGCATCAATTCCTGAAGATTGCCAAGCCCCTCTCCAGCCTCACTCCACTTATTGCTGCAGCTAAGGAGGCAACAAAGAACAATCAC</t>
+  </si>
+  <si>
+    <t>MSLIRKKGFYKQDVNKTAWELPKTYVSPTHVGSGAYGSVCSAIDKRSGEKVAIKKLSRPFQSEIFAKRAYRELLLLKHMQHENVIGLLDVFTPASSLRNFYDFYLVMPFMQTDLQKIMGMEFSEEKIQYLVYQMLKGLKYIHSAGVVHRDLKPGNLAVNEDCELKILDFGLARHADAEMTGYVVTRWYRAPEVILSWMHYNQTVDIWSVVCIMAEMLTGKTLFKGKDYLDQLTQILKVTGVPGTEFVQKLNDKAAKSYIQSLPQTPRKDFTQLFPRASPQAADLLEKMLELDVDKRLTAAQALTHPFFEPFRDPEEETEAQQPFDDSLEHEKLTVDEWKQHIYKEIVNFSPI</t>
+  </si>
+  <si>
+    <t>GCCACCTGCACACGTTTCACCGACGACTACCAGCTCTTCGAGGAGCTTGGCAAGGGTGCTTTCTCTGTGGTCCGCAGGTGTGTGAAGAAAACCCCCACGCAGGAGTACGCAGCAAAAATCATCAATACCAAGAAATTGTCTGCCCGGGATCACCAGAAACTAGAACGTGAGGCTCGGATATGTCGACTTCTGAAACATCCAAACATCGTGCGCCTCCATGACAGTATTTCTGAAGAAGGGTTTCACTACCTCGTGTTTGACCTTGTTACCGGCGGGGAGCTGTTTGAAGACATTGTGGCCAGAGAGTACTACAGTGAAGCAGATGCCAGCCACTGTATACATCAGATTCTGGAGAGTGTTAACCACATCCACCAGCATGACATCGTCCACAGGGACCTGAAGCCTGAGAACCTGCTGCTGGCGAGTAAATGCAAGGGTGCCGCCGTCAAGCTGGCTGATTTTGGCCTAGCCATCGAAGTACAGGGAGAGCAGCAGGCTTGGTTTGGTTTTGCTGGCACCCCAGGTTACTTGTCCCCTGAGGTCTTGAGGAAAGATCCCTATGGAAAACCTGTGGATATCTGGGCCTGCGGGGTCATCCTGTATATCCTCCTGGTGGGCTATCCTCCCTTCTGGGATGAGGATCAGCACAAGCTGTATCAGCAGATCAAGGCTGGAGCCTATGATTTCCCATCACCAGAATGGGACACGGTAACTCCTGAAGCCAAGAACTTGATCAACCAGATGCTGACCATAAACCCAGCAAAGCGCATCACGGCTGACCAGGCTCTCAAGCACCCGTGGGTCTGTCAACGATCCACGGTGGCATCCATGATGCATCGTCAGGAGACTGTGGAGTGTTTGCGCAAGTTCAATGCCCGGAGAAAACTGAAGGGTGCCATCCTCACGACCATGCTTGTCTCCAGGAACTTCTCA</t>
+  </si>
+  <si>
+    <t>GAGACCTACATTAAGCTGGACAAACTGGGCGAGGGTACCTATGCCACCGTCTACAAAGGCAAAAGCAAGCTCACAGACAACCTTGTGGCACTCAAGGAGATCAGACTGGAACATGAAGAGGGGGCACCCTGCACCGCCATCCGGGAAGTGTCCCTACTCAAGGACCTCAAACACGCCAACATCGTTACGCTACATGACATTATCCACACGGAGAAGTCCCTCACCCTTGTCTTTGAGTACCTGGACAAGGACCTGAAGCAGTACCTGGATGACTGTGGGAACATCATCAACATGCACAACGTGAAACTGTTCCTGTTCCAGCTGCTCCGTGGCCTGGCCTACTGCCACCGGCAGAAGGTGCTACACCGAGACCTCAAGCCCCAGAACCTGCTCATCAACGAGAGGGGAGAGCTCAAGCTGGCTGACTTTGGCCTGGCCCGAGCCAAGTCAATCCCAACAAAGACATACTCCAATGAGGTGGTGACACTGTGGTACCGGCCCCCTGACATCCTGCTTGGGTCCACGGACTACTCCACTCAGATTGACATGTGGGGTGTGGGCTGCATCTTCTATGAGATGGCCACAGGCCGTCCCCTCTTTCCGGGCTCCACGGTGGAGGAACAGCTACACTTCATCTTCCGTATCTTAGGAACCCCAACTGAGGAGACGTGGCCAGGCATCCTGTCCAACGAGGAGTTCAAGACATACAACTACCCCAAGTACCGAGCCGAGGCCCTTTTGAGCCACGCACCCCGACTTGATAGCGACGGGGCCGACCTCCTCACCAAGCTGTTGCAGTTTGAGGGTCGAAATCGGATCTCCGCAGAGGATGCCATGAAACATCCATTCTTCCTCAGTCTGGGGGAGCGGATCCACAAACTTCCTGACACTACTTCCATATTTGCACTAAAGGAGATTCAGCTACAAAAGGAGGCCAGCCTTCGGTCT</t>
+  </si>
+  <si>
+    <t>MK13_HUMAN_D0_4EYJ_A</t>
+  </si>
+  <si>
+    <t>STK16_HUMAN_D0_2BUJ_B</t>
+  </si>
+  <si>
+    <t>ATGGAAAGCGACCTGCACCAGATCATCCACTCCTCACAGCCCCTCACACTGGAACACGTGCGCTACTTCCTGTACCAACTGCTGCGGGGCCTGAAGTACATGCACTCGGCTCAGGTCATCCACCGTGACCTGAAGCCCTCCAACCTATTGGTGAATGAGAACTGTGAGCTCAAGATTGGTGACTTTGGTATGGCTCGTGGCCTGTGCACCTCGCCCGCTGAACATCAGTACTTCATGACTGAGTATGTGGCCACGCGCTGGTACCGTGCGCCCGAGCTCATGCTCTCTTTGCATGAGTATACACAGGCTATTGACCTCTGGTCTGTGGGCTGCATCTTTGGTGAGATGCTGGCCCGGCGCCAGCTCTTCCCAGGCAAAAACTATGTACACCAGCTACAGCTCATCATGATGGTGCTGGGTACCCCATCACCAGCCGTGATTCAGGCTGTGGGGGCTGAGAGGGTGCGGGCCTATATCCAGAGCTTGCCACCACGCCAGCCTGTGCCCTGGGAGACAGTGTACCCAGGTGCCGACCGCCAGGCCCTATCACTGCTGGGTCGCATGCTGCGTTTTGAGCCCAGCGCTCGCATCTCAGCAGCTGCTGCCCTTCGCCACCCTTTCCTGGCCAAGTACCATGATCCTGATGATGAGCCTGACTGTGCCCCGCCCTTTGACTTTGCCTTTGACCGCGAAGCCCTCACTCGGGAGCGCATTAAGGAGGCCATTGTGGCTGAAATTGAGGACTTCCATGCAAGGCGTGAGGGCATCCGCCAACAGATCCGCTTCCAGCCTTCTCTACAGCCTGTGGCTAGTGAGCCTGGCTGTCCAGATGTTGAAATGCCCAGTCCCTGGGCTCCCAGTGGGGACTGTGCCATG</t>
+  </si>
+  <si>
+    <t>CAGAGCAGTAAGCGCAGCAGCCGGAGTGTGGAAGATGACAAGGAGGGTCACCTGGTGTGCCGGATCGGCGATTGGCTCCAAGAGCGATATGAGATTGTGGGGAACCTGGGTGAAGGCACCTTTGGCAAGGTGGTGGAGTGCTTGGACCATGCCAGAGGGAAGTCTCAGGTTGCCCTGAAGATCATCCGCAACGTGGGCAAGTACCGGGAGGCTGCCCGGCTAGAAATCAACGTGCTCAAAAAAATCAAGGAGAAGGACAAAGAAAACAAGTTCCTGTGTGTCTTGATGTCTGACTGGTTCAACTTCCACGGTCACATGTGCATCGCCTTTGAGCTCCTGGGCAAGAACACCTTTGAGTTCCTGAAGGAGAATAACTTCCAGCCTTACCCCCTACCACATGTCCGGCACATGGCCTACCAGCTCTGCCACGCCCTTAGATTTCTGCATGAGAATCAGCTGACCCATACAGACTTGAAACCAGAGAACATCCTGTTTGTGAATTCTGAGTTTGAAACCCTCTACAATGAGCACAAGAGCTGTGAGGAGAAGTCAGTGAAGAACACCAGCATCCGAGTGGCTGACTTTGGCAGTGCCACATTTGACCATGAGCACCACACCACCATTGTGGCCACCCGTCACTATCGCCCGCCTGAGGTGATCCTTGAGCTGGGCTGGGCACAGCCCTGTGACGTCTGGAGCATTGGCTGCATTCTCTTTGAGTACTACCGGGGCTTCACACTCTTCCAGACCCACGAAAACCGAGAGCACCTGGTGATGATGGAGAAGATCCTAGGGCCCATCCCATCACACATGATCCACCGTACCAGGAAGCAGAAATATTTCTACAAAGGGGGCCTAGTTTGGGATGAGAACAGCTCTGACGGCCGGTATGTGAAGGAGAACTGCAAACCTCTGAAGAGTTACATGCTCCAAGACTCCCTGGAGCACGTGCAGCTGTTTGACCTGATGAGGAGGATGTTAGAATTTGACCCTGCCCAGCGCATCACACTGGCCGAGGCCCTGCTGCACCCCTTCTTTGCTGGCCTGACCCCTGAGGAGCGGTCCTTCCACACC</t>
+  </si>
+  <si>
+    <t>AAGCACGACGGGCGGGTGAAGATCGGACACTACGTGCTGGGCGACACGCTGGGCGTCGGCACCTTCGGCAAAGTGAAGATTGGAGAACATCAATTAACAGGCCATAAAGTGGCAGTTAAAATCTTAAATAGACAGAAGATTCGCAGTTTAGATGTTGTTGGAAAAATAAAACGAGAAATTCAAAATCTAAAACTCTTTCGTCATCCTCATATTATCAAACTATACCAGGTGATCAGCACTCCAACAGATTTTTTTATGGTAATGGAATATGTGTCTGGAGGTGAATTATTTGACTACATCTGTAAGCATGGACGGGTTGAAGAGATGGAAGCCAGGCGRCTCTTTCAGCAGATTCTGTCTGCTGTGGATTACTGTCATAGGCATATGGTTGTTCATCGAGACCTGAAACCAGAGAATGTCCTGTTGGATGCACACATGAATGCCAAGATAGCCGATTTCGGATTATCTAATATGATGTCAGATGGTGAATTTCTGAGAACTAGTTGCGGATCTCCAAATTATGCAGCACCTGAAGTCATCTCAGGCAGATTGTATGCAGGTCCTGAAGTTGATATCTGGAGCTGTGGTGTTATCTTGTATGCTCTTCTTTGTGGCACCCTCCCATTTGATGATGAGCATGTACCTACGTTATTTAAGAAGATCCGAGGGGGTGTCTTTTATATCCCAGAATATCTCAATCGTTCTGTCGCCACTCTCCTGATGCATATGCTGCAGGTTGACCCACTGAAACGAGCAACTATCAAAGACATAAGAGAGCATGAATGGTTTAAACAAGATTTGCCCAGTTACTTATTTCCTGAA</t>
+  </si>
+  <si>
+    <t>MQTVGVHSIVQQLHRNSIQFTDGYEVKEDIGVGSYSVCKRCIHKATNMEFAVKIIDKSKRDPTEEIEILLRYGQHPNIITLKDVYDDGKYVYVVTELMKGGELLDKILRQKFFSEREASAVLFTITKTVEYLHAQGVVHRDLKPSNILYVDESGNPESIRICDFGFAKQLRAENGLLMTPCYTANFVAPEVLKRQGYDAACDIWSLGVLLYTMLTGYTPFANGPDDTPEEILARIGSGKFSLSGGYWNSVSDTAKDLVSKMLHVDPHQRLTAALVLRHPWIVHWDQLPQYQLNRQDAPHLVKGAMAATYSALNRNQSPVLEPVGRSTLAQRRGIKKITSTAL</t>
+  </si>
+  <si>
+    <t>KCC2G_HUMAN_D0_2V7O_A</t>
+  </si>
+  <si>
+    <t>KQYEHVKRDLNPEDFWEIIGELGDGAFGKVYKAQNKETSVLAAAKVIDTKSEEELEDYMVEIDILASCDHPNIVKLLDAFYYENNLWILIEFCAGGAVDAVMLELERPLTESQIQVVCKQTLDALNYLHDNKIIHRDLKAGNILFTLDGDIKLADFGVSAKNMRTIQRRDSFIGTPYWMAPEVVMCETSKDRPYDYKADVWSLGITLIEMAEIEPPHHELNPMRVLLKIAKSEPPTLAQPSRWSSNFKDFLKKCLEKNVDARWTTSQLLQHPFVTVDSNKPIRELIAEAKAEVTEEVEDGKE</t>
+  </si>
+  <si>
+    <t>ACCCAAACTGTTCATGAGTTTGCCAAGGAATTGGATGCCACCAACATATCCATTGATAAAGTTGTTGGAGCAGGTGAATTTGGAGAGGTGTGCAGTGGTCGCTTAAAACTTCCTTCAAAAAAAGAGATTTCAGTGGCCATTAAGACCCTGAAAGTTGGCTACACAGAAAAGCAGAGGAGAGACTTCCTGGGAGAAGCAAGCATTATGGGACAGTTTGACCACCCCAATATCATTCGACTGGAAGGAGTTGTTACCAAAAGTAAGCCAGTTATGATTGTCACAGAATACATGGAGAATGGTTCCTTGGATAGTTTCCTACGTAAACACGATGCCCAGTTTACTGTCATTCAGCTAGTGGGGATGCTTCGAGGGATAGCATCTGGCATGAAGTACCTGTCAGACATGGGCTATGTTCACCGAGACCTCGCTGCTCGGAACATCTTGATCAACAGTAACTTGGTGTGTAAGGTTTCTGATTTCGGACTTTCGCGTGTCCTGGAGGATGACCCAGAAGCTGCTTATACAACAAGAGGAGGGAAGATCCCAATCAGGTGGACATCACCAGAAGCTATAGCCTACCGCAAGTTCACGTCAGCCAGCGATGTATGGAGTTATGGGATTGTTCTCTGGGAGGTGATGTCTTATGGAGAGAGACCATACTGGGAGATGTCCAATCAGGATGTAATTAAAGCTGTAGATGAGGGCTATCGACTGCCACCCCCCATGGACTGCCCAGCTGCCTTGTATCAGCTGATGCTGGACTGCTGGCAGAAAGACAGGAACAACAGACCCAAGTTTGAGCAGATTGTTAGTATTCTGGACAAGCTTATCCGGAATCCCGGCAGCCTGAAGATCATCACCAGTGCAGCCGCAAGGCCATCAAACCTTCTTCTGGACCAAAGCAATGTGGATATCACTACCTTCCGCACAACAGGTGACTGGCTTAATGGTGTCTGGACAGCACACTGCAAGGAAATCTTCACGGGTGTGGAGTACAGTTCTTGTGACACAATAGCCAAGATTTCC</t>
+  </si>
+  <si>
+    <t>MEKDGLCRADQQYECVAEIGEGAYGKVFKARDLKNGGRFVALKRVRVQTGEEGMPLSTIREVAVLRHLETFEHPNVVRLFDVCTVSRTDRETKLTLVFEHVDQDLTTYLDKVPEPGVPTETIKDMMFQLLRGLDFLHSHRVVHRDLKPQNILVTSSGQIKLADFGLARIYSFQMALTSVVVTLWYRAPEVLLQSSYATPVDLWSVGCIFAEMFRRKPLFRGSSDVDQLGKILDVIGLPGEEDWPRDVALPRQAFHSKSAQPIEKFVTDIDELGKDLLLKCLTFNPAKRISAYSALSHPYFQ</t>
+  </si>
+  <si>
+    <t>EPHA3_HUMAN_D0_4GK2_A</t>
+  </si>
+  <si>
+    <t>MEAAASEPSLDLDNLKLLELIGRGRYGAVYKGSLDERPVAVKVFSFANRQNFINEKNIYRVPLMEHDNIARFIVGDERVTADGRMEYLLVMEYYPNGSLCKYLSLHTSDWVSSCRLAHSVTRGLAYLHTELPRGDHYKPAISHRDLNSRNVLVKNDGTCVISDFGLSMRLTGNRLVRPGEEDNAAISEVGTIRYMAPEVLEGAVNLRDCESALKQVDMYALGLIYWEIFMRCTDLFPGESVPEYQMAFQTEVGNHPTFEDMQVLVSREKQRPKFPEAWKENSLAVRSLKETIEDCWDQDAEARLTAQCAEERMAELMMIWERNKSVSPT</t>
+  </si>
+  <si>
+    <t>ATGTCGGGACCCGTGCCAAGCAGGGCCAGAGTTTACACAGATGTTAATACACACAGACCTCGAGAATACTGGGATTACGAGTCACATGTGGTGGAATGGGGAAATCAAGATGACTACCAGCTGGTTCGAAAATTAGGCCGAGGTAAATACAGTGAAGTATTTGAAGCCATCAACATCACAAATAATGAAAAAGTTGTTGTTAAAATTCTCAAGCCAGTAAAAAAGAAGAAAATTAAGCGTGAAATAAAGATTTTGGAGAATTTGAGAGGAGGTCCCAACATCATCACACTGGCAGACATTGTAAAAGACCCTGTGTCACGAACCCCCGCCTTGGTTTTTGAACACGTAAACAACACAGACTTCAAGCAATTGTACCAGACGTTAACAGACTATGATATTCGATTTTACATGTATGAGATTCTGAAGGCCCTGGATTATTGTCACAGCATGGGAATTATGCACAGAGATGTCAAGCCCCATAATGTCATGATTGATCATGAGCACAGAAAGCTACGACTAATAGACTGGGGTTTGGCTGAGTTTTATCATCCTGGCCAAGAATATAATGTCCGAGTTGCTTCCCGATACTTCAAAGGTCCTGAGCTACTTGTAGACTATCAGATGTACGATTATAGTTTGGATATGTGGAGTTTGGGTTGTATGCTGGCAAGTATGATCTTTCGGAAGGAGCCATTTTTCCATGGACATGACAATTATGATCAGTTGGTGAGGATAGCCAAGGTTCTGGGGACAGAAGATTTATATGACTATATTGACAAATACAACATTGAATTAGATCCACGTTTCAATGATATCTTGGGCAGACACTCTCGAAAGCGATGGGAACGCTTTGTCCACAGTGAAAATCAGCACCTTGTCAGCCCTGAGGCCTTGGATTTCCTGGACAAACTGCTGCGATATGACCACCAGTCACGGCTTACTGCAAGAGAGGCAATGGAGCACCCCTATTTCTACACTGTTGTGAAGGACCAGGCTCGAATGGGT</t>
+  </si>
+  <si>
+    <t>NEK2_HUMAN_D0_2XKE_A</t>
+  </si>
+  <si>
+    <t>MK01_HUMAN_D0_4FMQ_A</t>
+  </si>
+  <si>
+    <t>ATGGAGCTGAGAGTCGGGAACAGGTACCGGCTGGGCCGGAAGATCGGCAGCGGCTCCTTCGGAGACATCTATCTCGGTACGGACATTGCTGCAGGAGAAGAGGTTGCCATCAAGCTTGAATGTGTCAAAACCAAACACCCTCAGCTCCACATTGAGAGCAAAATCTACAAGATGATGCAGGGAGGAGTGGGCATCCCCACCATCAGATGGTGCGGGGCAGAGGGGGACTACAACGTCATGGTGATGGAGCTGCTGGGGCCAAGCCTGGAGGACCTCTTCAACTTCTGCTCCAGGAAATTCAGCCTCAAAACCGTCCTGCTGCTTGCTGACCAAATGATCAGTCGCATCGAATACATTCATTCAAAGAACTTCATCCACCGGGATGTGAAGCCAGACAACTTCCTCATGGGCCTGGGGAAGAAGGGCAACCTGGTGTACATCATCGACTTCGGGCTGGCCAAGAAGTACCGGGATGCACGCACCCACCAGCACATCCCCTATCGTGAGAACAAGAACCTCACGGGGACGGCGCGGTACGCCTCCATCAACACGCACCTTGGAATTGAACAATCCCGAAGAGATGACTTGGAGTCTCTGGGCTACGTGCTAATGTACTTCAACCTGGGCTCTCTCCCCTGGCAGGGGCTGAAGGCTGCCACCAAGAGACAGAAATACGAAAGGATTAGCGAGAAGAAAATGTCCACCCCCATCGAAGTGTTGTGTAAAGGCTACCCTTCCGAATTTGCCACATACCTGAATTTCTGCCGTTCCTTGCGTTTTGACGACAAGCCTGACTACTCGTACCTGCGGCAGCTTTTCCGGAATCTGTTCCATCGCCAGGGCTTCTCCTATGACTACGTGTTCGACTGGAACATGCTCAAA</t>
+  </si>
+  <si>
+    <t>BRAF_HUMAN_D0_4JVG_D</t>
+  </si>
+  <si>
+    <t>MSDEEILEKLRSIVSVGDPKKKYTRFEKIGQGASGTVYTAMDVATGQEVAIKQMNLQQQPKKELIINEILVMRENKNPNIVNYLDSYLVGDELWVVMEYLAGGSLTDVVTETCMDEGQIAAVCRECLQALEFLHSNQVIHRDIKSDNILLGMDGSVKLTDFGFCAQITPEQSKRSTMVGTPYWMAPEVVTRKAYGPKVDIWSLGIKAIEMIEGEPPYLNENPLRALYLIATNGTPELQNPEKLSAIFRDFLNRCLEMDVEKRGSAKELLQHQFLKIAKPLSSLTPLIAAAKEATKNNH</t>
+  </si>
+  <si>
+    <t>GECSQKGPVPFSHCLPTEKLQRCEKIGEGVFGEVFQTIADHTPVAIKIIAIEGPDLVNGSHQKTFEEILPEIIISKELSLLSGEVCNRTEGFIGLNSVHCVQGSYPPLLLKAWDHYNSTKGSANDRPDFFKDDQLFIVLEFEFGGIDLEQMRTKLSSLATAKSILHQLTASLAVAEASLRFEHRDLHWGNVLLKKTSLKKLHYTLNGKSSTIPSCGLQVSIIDYTLSRLERDGIVVFCDVSMDEDLFTGDGDYQFDIYRLMKKENNNRWGEYHPYSNVLWLHYLTDKMLKQMTFKTKCNTPAMKQIKRKIQEFHRTMLNFSSATDLLCQHRLFK</t>
+  </si>
+  <si>
+    <t>MENFNNFYILTSKELGRGKFAVVRQCISKSTGQEYAAKFLKKRRRGQDCRAEILHEIAVLELAKSCPRVINLHEVYENTSEIILILEYAAGGEIFSLCLPELAEMVSENDVIRLIKQILEGVYYLHQNNIVHLDLKPQNILLSSIYPLGDIKIVDFGMSRKIGHACELREIMGTPEYLAPEILNYDPITTATDMWNIGIIAYMLLTHTSPFVGEDNQETYLNISQVNVDYSEETFSSVSQLATDFIQSLLVKNPEKRPTAEICLSHSWLQQWDFENLFHPEETSSSSQTQDHSVRSSEDKTSKSS</t>
+  </si>
+  <si>
+    <t>GCTGATCCAGAAGAACTGTTCACAAAATTAGAGCGCATTGGGAAAGGCTCATTTGGGGAAGTTTTCAAAGGAATTGATAACCGTACCCAGCAAGTCGTTGCTATTAAAATCATAGACCTTGAGGAAGCCGAAGATGAAATAGAAGACATTCAGCAAGAAATAACTGTCTTGAGTCAATGTGACAGCTCATATGTAACAAAATACTATGGGTCATATTTAAAGGGGTCTAAATTATGGATAATAATGGAATACCTGGGCGGTGGTTCAGCACTGGATCTTCTTCGAGCTGGTCCATTTGATGAGTTCCAGATTGCTACCATGCTAAAGGAAATTTTAAAAGGTCTGGACTATCTGCATTCAGAAAAGAAAATTCACCGAGACATAAAAGCTGCCAATGTCTTGCTCTCAGAACAAGGAGATGTTAAACTTGCTGATTTTGGAGTTGCTGGTCAGCTGACAGATACACAGATTAAAAGAAATACCTTTGTGGGAACTCCATTTTGGATGGCTCCTGAAGTTATTCAACAGTCAGCTTATGACTCAAAAGCTGACATTTGGTCATTGGGAATTACTGCTATTGAACTAGCCAAGGGAGAGCCACCTAACTCCGATATGCATCCAATGAGAGTTCTGTTTCTTATTCCCAAAAACAATCCTCCAACTCTTGTTGGAGACTTTACTAAGTCTTTTAAGGAGTTTATTGATGCTTGCCTGAACAAAGATCCATCATTTCGTCCTACAGCAAAAGAACTTCTGAAACACAAATTCATTGTAAAAAATTCAAAGAAGACTTCTTATCTGACTGAACTGATAGATCGTTTTAAGAGATGGAAGGCAGAA</t>
+  </si>
+  <si>
+    <t>MELRVGNKYRLGRKIGSGSFGDIYLGANIASGEEVAIKLECVKTKHPQLHIESKFYKMMQGGVGIPSIKWCGAEGDYNVMVMELLGPSLEDLFNFCSRKFSLKTVLLLADQMISRIEYIHSKNFIHRDVKPDNFLMGLGKKGNLVYIIDFGLAKKYRDARTHQHIPYRENKNLTGTARYASINTHLGIEQSRRDDLESLGYVLMYFNLGSLPWQGLKAATKRQKYERISEKKMSTPIEVLCKGYPSEFSTYLNFCRSLRFDDKPDYSYLRQLFRNLFHRQGFSYDYVFDWNMLK</t>
+  </si>
+  <si>
+    <t>dna_end</t>
+  </si>
+  <si>
+    <t>MADDDVLFEDVYELCEVIGKGPFSVVRRCINRETGQQFAVKIVDVAKFTSSPGLSTEDLKREASICHMLKHPHIVELLETYSSDGMLYMVFEFMDGADLCFEIVKRADAGFVYSEAVASHYMRQILEALRYCHDNNIIHRDVKPHCVLLASKENSAPVKLGGFGVAIQLGESGLVAGGRVGTPHFMAPEVVKREPYGKPVDVWGCGVILFILLSGCLPFYGTKERLFEGIIKGKYKMNPRQWSHISESAKDLVRRMLMLDPAERITVYEALNHPWLKERDRYAYKIHLPETVEQLRKFNARRKLKGAVLAAVSSHKFNSFYGDPPEELPDFSEDPTSSGA</t>
+  </si>
+  <si>
+    <t>FAK1_HUMAN_D0_2IJM_B</t>
+  </si>
+  <si>
+    <t>CHK2_HUMAN_D0_2CN5_A</t>
+  </si>
+  <si>
+    <t>SSVTASAAPGTASLVPDYWIDGSNRDALSDFFEVESELGRGATSIVYRCKQKGTQKPYALKVLKKTVDKKIVRTEIGVLLRLSHPNIIKLKEIFETPTEISLVLELVTGGELFDRIVEKGYYSERDAADAVKQILEAVAYLHENGIVHRDLKPENLLYATPAPDAPLKIADFGLSKIVEHQVLMKTVCGTPGYCAPEILRGCAYGPEVDMWSVGIITYILLCGFEPFYDERGDQFMFRRILNCEYYFISPWWDEVSLNAKDLVRKLIVLDPKKRLTTFQALQHPWVTGKAANFVHMDTAQKKLQEFNARRKLKAAVKAVVASSRLG</t>
+  </si>
+  <si>
+    <t>MDEQSQGMQGPPVPQFQPQKALRPDMGYNTLANFRIEKKIGRGQFSEVYRAACLLDGVPVALKKVQIFDLMDAKARADCIKEIDLLKQLNHPNVIKYYASFIEDNELNIVLELADAGDLSRMIKHFKKQKRLIPERTVWKYFVQLCSALEHMHSRRVMHRDIKPANVFITATGVVKLGDLGLGRFFSSKTTAAHSLVGTPYYMSPERIHENGYNFKSDIWSLGCLLYEMAALQSPFYGDKMNLYSLCKKIEQCDYPPLPSDHYSEELRQLVNMCINPDPEKRPDVTYVYDVAKRMHACTASS</t>
+  </si>
+  <si>
+    <t>MSQSKGKKRNPGLKIPKEAFEQPQTSSTPPRDLDSKACISIGNQNFEVKADDLEPIMELGRGAYGVVEKMRHVPSGQIMAVKRIRATVNSQEQKRLLMDLDISMRTVDCPFTVTFYGALFREGDVWICMELMDTSLDKFYKQVIDKGQTIPEDILGKIAVSIVKALEHLHSKLSVIHRDVKPSNVLINALGQVKMCDFGISGYLVDSVAKTIDAGCKPYMAPERINPELNQKGYSVKSDIWSLGITMIELAILRFPYDSWGTPFQQLKQVVEEPSPQLPADKFSAEFVDFTSQCLKKNSKERPTYPELMQHPFFTLHESKGTDVASFVKLILGD</t>
+  </si>
+  <si>
+    <t>DYRK2_HUMAN_D0_3KVW_A</t>
+  </si>
+  <si>
+    <t>QSSKRSSRSVEDDKEGHLVCRIGDWLQERYEIVGNLGEGTFGKVVECLDHARGKSQVALKIIRNVGKYREAARLEINVLKKIKEKDKENKFLCVLMSDWFNFHGHMCIAFELLGKNTFEFLKENNFQPYPLPHVRHMAYQLCHALRFLHENQLTHTDLKPENILFVNSEFETLYNEHKSCEEKSVKNTSIRVADFGSATFDHEHHTTIVATRHYRPPEVILELGWAQPCDVWSIGCILFEYYRGFTLFQTHENREHLVMMEKILGPIPSHMIHRTRKQKYFYKGGLVWDENSSDGRYVKENCKPLKSYMLQDSLEHVQLFDLMRRMLEFDPAQRITLAEALLHPFFAGLTPEERSFHT</t>
+  </si>
+  <si>
+    <t>MK07_HUMAN_D0_4IC7_D</t>
+  </si>
+  <si>
+    <t>ATGCAGACAGTTGGTGTACATTCAATTGTTCAGCAGTTACACAGGAACAGTATTCAGTTTACTGATGGATATGAAGTAAAAGAAGATATTGGAGTTGGCTCCTACTCTGTTTGCAAGAGATGTATACATAAAGCTACAAACATGGAGTTTGCAGTGAAGATTATTGATAAAAGCAAGAGAGACCCAACAGAAGAAATTGAAATTCTTCTTCGTTATGGACAGCATCCAAACATTATCACTCTAAAGGATGTATATGATGATGGAAAGTATGTGTATGTAGTAACAGAACTTATGAAAGGAGGTGAATTGCTGGATAAAATTCTTAGACAAAAATTTTTCTCTGAACGAGAGGCCAGTGCTGTCCTGTTCACTATAACTAAAACCGTTGAATATCTTCACGCACAAGGGGTGGTTCATAGAGACTTGAAACCTAGCAACATTCTTTATGTGGATGAATCTGGTAATCCGGAATCTATTCGAATTTGTGATTTTGGCTTTGCAAAACAGCTGAGAGCGGAAAATGGTCTTCTCATGACTCCTTGTTACACTGCAAATTTTGTTGCACCAGAGGTTTTAAAAAGACAAGGCTATGATGCTGCTTGTGATATATGGAGTCTTGGTGTCCTACTCTATACAATGCTTACCGGTTACACTCCATTTGCAAATGGTCCTGATGATACACCAGAGGAAATATTGGCACGAATAGGTAGCGGAAAATTCTCACTCAGTGGTGGTTACTGGAATTCTGTTTCAGACACAGCAAAGGACCTGGTGTCAAAGATGCTTCATGTAGACCCTCATCAGAGACTGACTGCTGCTCTTGTGCTCAGACATCCTTGGATCGTCCACTGGGACCAACTGCCACAATACCAACTAAACAGACAGGATGCACCACATCTAGTAAAGGGTGCCATGGCAGCTACATATTCTGCTTTGAACCGTAATCAGTCACCAGTTTTGGAACCAGTAGGCCGCTCTACTCTTGCTCAGCGGAGAGGTATTAAAAAAATCACCTCAACAGCCCTG</t>
+  </si>
+  <si>
+    <t>CACATTGGAAACTACCGGCTCCTCAAGACCATTGGCAAGGGTAATTTTGCCAAGGTGAAGTTGGCCCGACACATCCTGACTGGGAAAGAGGTAGCTGTGAAGATCATTGACAAGACTCAACTGAACTCCTCCAGCCTCCAGAAACTATTCCGCGAAGTAAGAATAATGAAGGTTTTGAATCATCCCAACATAGTTAAATTATTTGAAGTGATTGAGACTGAGAAAACGCTCTACCTTGTCATGGAGTACGCTAGTGGCGGAGAGGTATTTGATTACCTAGTGGCTCATGGCAGGATGAAAGAAAAAGAGGCTCGAGCCAAATTCCGCCAGATAGTGTCTGCTGTGCAGTACTGTCACCAGAAGTTTATTGTCCATAGAGACTTAAAGGCAGAAAACCTGCTCTTGGATGCTGATATGAACATCAAGATTGCAGACTTTGGCTTCAGCAATGAATTCACCTTTGGGAACAAGCTGGACACCTTCTGTGGCAGTCCCCCTTATGCTGCCCCAGAACTCTTCCAGGGCAAAAAATATGATGGACCCGAGGTGGATGTGTGGAGCCTAGGAGTTATCCTCTATACACTGGTCAGCGGATCCCTGCCTTTTGATGGACAGAACCTCAAGGAGCTGCGGGAACGGGTACTGAGGGGAAAATACCGTATTCCATTCTACATGTCCACGGACTGTGAAAACCTGCTTAAGAAATTTCTCATTCTTAATCCCAGCAAGAGAGGCACTTTAGAGCAAATCATGAAAGATCGATGGATGAATGTGGGTCACGAAGATGATGAACTAAAGCCTTACGTGGAGCCACTCCCTGACTACAAGGACCCCCGGCGGACAGAGCTGATGGTGTCCATGGGTTATACACGGGAAGAGATCCAGGACTCGCTGGTGGGCCAGAGATACAACGAGGTGATGGCCACCTATCTGCTCCTGGGCTAC</t>
+  </si>
+  <si>
+    <t>CAGCAGTTCCCGCAGTTCCACGTCAAGTCCGGCCTGCAGATCAAGAAGAACGCCATCATCGATGACTACAAGGTCACCAGCCAGGTCCTGGGGCTGGGCATCAACGGCAAAGTTTTGCAGATCTTCAACAAGAGGACCCAGGAGAAATTCGCCCTCAAAATGCTTCAGGACTGCCCCAAGGCCCGCAGGGAGGTGGAGCTGCACTGGCGGGCCTCCCAGTGCCCGCACATCGTACGGATCGTGGATGTGTACGAGAATCTGTACGCAGGGAGGAAGTGCCTGCTGATTGTCATGGAATGTTTGGACGGTGGAGAACTCTTTAGCCGAATCCAGGATCGAGGAGACCAGGCATTCACAGAAAGAGAAGCATCCGAAATCATGAAGAGCATCGGTGAGGCCATCCAGTATCTGCATTCAATCAACATTGCCCATCGGGATGTCAAGCCTGAGAATCTCTTATACACCTCCAAAAGGCCCAACGCCATCCTGAAACTCACTGACTTTGGCTTTGCCAAGGAAACCACCAGCCACAACTCTTTGACCACTCCTTGTTATACACCGTACTATGTGGCTCCAGAAGTGCTGGGTCCAGAGAAGTATGACAAGTCCTGTGACATGTGGTCCCTGGGTGTCATCATGTACATCCTGCTGTGTGGGTATCCCCCCTTCTACTCCAACCACGGCCTTGCCATCTCTCCGGGCATGAAGACTCGCATCCGAATGGGCCAGTATGAATTTCCCAACCCAGAATGGTCAGAAGTATCAGAGGAAGTGAAGATGCTCATTCGGAATCTGCTGAAAACAGAGCCCACCCAGAGAATGACCATCACCGAGTTTATGAACCACCCTTGGATCATGCAATCAACAAAGGTCCCTCAAACCCCACTGCACACCAGCCGGGTCCTGAAGGAGGACAAGGAGCGGTGGGAGGATGTCAAGGGGTGTCTTCATGACAAGAACAGCGACCAGGCC</t>
+  </si>
+  <si>
+    <t>CDK2_HUMAN_D0_4BCP_A</t>
+  </si>
+  <si>
+    <t>MP2K4_HUMAN_D0_3ALN_C</t>
+  </si>
+  <si>
+    <t>ACCACCTCACTTGAAGCTTTGCCCACAGGGACAGTGCTGACAGACAAGAGTGGGCGACAGTGGAAGCTGAAGTCCTTCCAGACCAGGGACAACCAGGGCATTCTCTATGAAGCTGCACCCACCTCCACCCTCACCTGTGACTCAGGACCACAGAAGCAAAAGTTCTCACTCAAACTGGATGCCAAGGATGGGCGCTTGTTCAATGAGCAGAACTTCTTCCAGCGGGCCGCCAAGCCTCTGCAAGTCAACAAGTGGAAGAAGCTGTACTCGACCCCACTGCTGGCCATCCCTACCTGCATGGGTTTCGGTGTTCACCAGGACAAATACAGGTTCTTGGTGTTACCCAGCCTGGGGAGGAGCCTTCAGTCGGCCCTGGATGTCAGCCCAAAGCATGTGCTGTCAGAGAGGTCTGTGCTGCAGGTGGCCTGCCGGCTGCTGGATGCCCTGGAGTTCCTCCATGAGAATGAGTATGTTCATGGAAATGTGACAGCTGAAAATATCTTTGTGGATCCAGAGGACCAGAGTCAGGTGACTTTGGCAGGCTATGGCTTCGCCTTCCGCTATTGCCCAAGTGGCAAACACGTGGCCTACGTGGAAGGCAGCAGGAGCCCTCACGAGGGGGACCTTGAGTTCATTAGCATGGACCTGCACAAGGGATGCGGGCCCTCCCGCCGCAGCGACCTCCAGAGCCTGGGCTACTGCATGCTGAAGTGGCTCTACGGGTTTCTGCCATGGACAAATTGCCTTCCCAACACTGAGGACATCATGAAGCAAAAACAGAAGTTTGTTGATAAGCCGGGGCCCTTCGTGGGACCCTGCGGTCACTGGATCAGGCCCTCAGAGACCCTGCAGAAGTACCTGAAGGTGGTGATGGCCCTCACGTATGAGGAGAAGCCGCCCTACGCCATGCTGAGGAACAACCTAGAAGCTTTGCTGCAGGATCTGCGTGTGTCTCCATATGACCCCATTGGCCTCCCGATGGTGCCC</t>
+  </si>
+  <si>
+    <t>TCACCACAGCGGGAGCCACAGCGAGTATCCCATGAGCAGTTCCGGGCTGCCCTGCAGCTGGTGGTGGACCCAGGCGACCCCCGCTCCTACCTGGACAACTTCATCAAGATTGGCGAGGGCTCCACGGGCATCGTGTGCATCGCCACCGTGCGCAGCTCGGGCAAGCTGGTGGCCGTCAAGAAGATGGACCTGCGCAAGCAGCAGAGGCGCGAGCTGCTCTTCAACGAGGTGGTAATCATGAGGGACTACCAGCACGAGAATGTGGTGGAGATGTACAACAGCTACCTGGTGGGGGACGAGCTCTGGGTGGTCATGGAGTTCCTGGAAGGAGGCGCCCTCACCGACATCGTCACCCACACCAGGATGAACGAGGAGCAGATCGCGGCCGTGTGCCTTGCAGTGCTGCAGGCCCTGTCGGTGCTCCACGCCCAGGGCGTCATCCACCGGGACATCAAGAGCGACTCGATCCTGCTGACCCATGATGGCAGGGTGAAGCTGTCAGACTTTGGGTTCTGCGCCCAGGTGAGCAAGGAAGTGCCCCGAAGGAAGTCGCTGGTCGGCACGCCCTACTGGATGGCCCCAGAGCTCATCTCCCGCCTTCCCTACGGGCCAGAGGTAGACATCTGGTCGCTGGGGATAATGGTGATTGAGATGGTGGACGGAGAGCCCCCCTACTTCAACGAGCCACCCCTCAAAGCCATGAAGATGATTCGGGACAACCTGCCACCCCGACTGAAGAACCTGCACAAGGTGTCGCCATCCCTGAAGGGCTTCCTGGACCGCCTGCTGGTGCGAGACCCTGCCCAGCGGGCCACGGCAGCCGAGCTGCTGAAGCACCCATTCCTGGCCAAGGCAGGGCCGCCTGCCAGCATCGTGCCCCTCATGCGCCAGAACCGCACCAGA</t>
+  </si>
+  <si>
+    <t>SIESSGKLKISPEQHWDFTAEDLKDLGEIGRGAYGSVNKMVHKPSGQIMAVKRIRSTVDEKEQKQLLMDLDVVMRSSDCPYIVQFYGALFREGDCWICMELMSTSFDKFYKYVYSVLDDVIPEEILGKITLATVKALNHLKENLKIIHRDIKPSNILLDRSGNIKLCDFGISGQLVDSIAKTRDAGCRPYMAPERIDPSASRQGYDVRSDVWSLGITLYELATGRFPYPKWNSVFDQLTQVVKGDPPQLSNSEEREFSPSFINFVNLCLTKDESKRPKYKELLKHPFILMYEERAVEVACYVCKILDQMPATPSSPMYVD</t>
+  </si>
+  <si>
+    <t>TDSFSGRFEDVYQLQEDVLGEGAHARVQTCINLITSQEYAVKIIEKQPGHIRSRVFREVEMLYQCQGHRNVLELIEFFEEEDRFYLVFEKMRGGSILSHIHKRRHFNELEASVVVQDVASALDFLHNKGIAHRDLKPENILCEHPNQVSPVKICDFDLGSGIKLNGDCSPISTPELLTPCGSAEYMAPEVVEAFSEEASIYDKRCDLWSLGVILYILLSGYPPFVGRCGSDCGWDRGEACPACQNMLFESIQEGKYEFPDKDWAHISCAAKDLISKLLVRDAKQRLSAAQVLQHPWVQGCAPENTLPTPMVLQR</t>
+  </si>
+  <si>
+    <t>ST17B_HUMAN_D0_3LM0_A</t>
+  </si>
+  <si>
+    <t>MPGPAAGSRARVYAEVNSLRSREYWDYEAHVPSWGNQDDYQLVRKLGRGKYSEVFEAINITNNERVVVKILKPVKKKKIKREVKILENLRGGTNIIKLIDTVKDPVSKTPALVFEYINNTDFKQLYQILTDFDIRFYMYELLKALDYCHSKGIMHRDVKPHNVMIDHQQKKLRLIDWGLAEFYHPAQEYNVRVASRYFKGPELLVDYQMYDYSLDMWSLGCMLASMIFRREPFFHGQDNYDQLVRIAKVLGTEELYGYLKKYHIDLDPHFNDILGQHSRKRWENFIHSENRHLVSPEALDLLDKLLRYDHQQRLTAKEAMEHPYFYPVVKEQSQ</t>
+  </si>
+  <si>
+    <t>AAGAGGCAGTGGGCTTTGGAAGACTTTGAAATTGGTCGCCCTCTGGGTAAAGGAAAGTTTGGTAATGTTTATTTGGCAAGAGAAAAGCAAAGCAAGTTTATTCTGGCTCTTAAAGTGTTATTTAAAGCTCAGCTGGAGAAAGCCGGAGTGGAGCATCAGCTCAGAAGAGAAGTAGAAATACAGTCCCACCTTCGGCATCCTAATATTCTTAGACTGTATGGTTATTTCCATGATGCTACCAGAGTCTACCTAATTCTGGAATATGCACCACTTGGAACAGTTTATAGAGAACTTCAGAAACTTTCAAAGTTTGATGAGCAGAGAACTGCTACTTATATAACAGAATTGGCAAATGCCCTGTCTTACTGTCATTCGAAGAGAGTTATTCATAGAGACATTAAGCCAGAGAACTTACTTCTTGGATCAGCTGGAGAGCTTAAAATTGCAGATTTTGGGTGGTCAGTACATGCTCCATCTTCCAGGAGGACCACTCTCTGTGGCACCCTGGACTACCTGCCCCCTGAAATGATTGAAGGTCGGATGCATGATGAGAAGGTGGATCTCTGGAGCCTTGGAGTTCTTTGCTATGAATTTTTAGTTGGGAAGCCTCCTTTTGAGGCAAACACATACCAAGAGACCTACAAAAGAATATCACGGGTTGAATTCACATTCCCTGACTTTGTAACAGAGGGAGCCAGGGACCTCATTTCAAGACTGTTGAAGCATAATCCCAGCCAGAGGCCAATGCTCAGAGAAGTACTTGAACACCCCTGGATCACAGCAAATTCATCAAAACCATCA</t>
+  </si>
+  <si>
+    <t>ATGGAGCTACGTGTGGGGAACAAGTACCGCCTGGGACGGAAGATCGGGAGCGGGTCCTTCGGAGATATCTACCTGGGTGCCAACATCGCCTCTGGTGAGGAAGTCGCCATCAAGCTGGAGTGTGTGAAGACAAAGCACCCCCAGCTGCACATCGAGAGCAAGTTCTACAAGATGATGCAGGGTGGCGTGGGGATCCCGTCCATCAAGTGGTGCGGAGCTGAGGGCGACTACAACGTGATGGTCATGGAGCTGCTGGGGCCTAGCCTCGAGGACCTGTTCAACTTCTGTTCCCGCAAATTCAGCCTCAAGACGGTGCTGCTCTTGGCCGACCAGATGATCAGCCGCATCGAGTATATCCACTCCAAGAACTTCATCCACCGGGACGTCAAGCCCGACAACTTCCTCATGGGGCTGGGGAAGAAGGGCAACCTGGTCTACATCATCGACTTCGGCCTGGCCAAGAAGTACCGGGACGCCCGCACCCACCAGCACATTCCCTACCGGGAAAACAAGAACCTGACCGGCACGGCCCGCTACGCTTCCATCAACACGCACCTGGGCATTGAGCAAAGCCGTCGAGATGACCTGGAGAGCCTGGGCTACGTGCTCATGTACTTCAACCTGGGCTCCCTGCCCTGGCAGGGGCTCAAAGCAGCCACCAAGCGCCAGAAGTATGAACGGATCAGCGAGAAGAAGATGTCAACGCCCATCGAGGTCCTCTGCAAAGGCTATCCCTCCGAATTCTCAACATACCTCAACTTCTGCCGCTCCCTGCGGTTTGACGACAAGCCCGACTACTCTTACCTACGTCAGCTCTTCCGCAACCTCTTCCACCGGCAGGGCTTCTCCTATGACTACGTCTTTGACTGGAACATGCTGAAA</t>
+  </si>
+  <si>
+    <t>MK03_HUMAN_D0_2ZOQ_B</t>
+  </si>
+  <si>
+    <t>ATGTCTCAGTCGAAAGGCAAGAAGCGAAACCCTGGCCTTAAAATTCCAAAAGAAGCATTTGAACAACCTCAGACCAGTTCCACACCACCTCGAGATTTAGACTCCAAGGCTTGCATTTCTATTGGAAATCAGAACTTTGAGGTGAAGGCAGATGACCTGGAGCCTATAATGGAACTGGGACGAGGTGCGTACGGGGTGGTGGAGAAGATGCGGCACGTGCCCAGCGGGCAGATCATGGCAGTGAAGCGGATCCGAGCCACAGTAAATAGCCAGGAACAGAAACGGCTACTGATGGATTTGGATATTTCCATGAGGACGGTGGACTGTCCATTCACTGTCACCTTTTATGGCGCACTGTTTCGGGAGGGTGATGTGTGGATCTGCATGGAGCTCATGGATACATCACTAGATAAATTCTACAAACAAGTTATTGATAAAGGCCAGACAATTCCAGAGGACATCTTAGGGAAAATAGCAGTTTCTATTGTAAAAGCATTAGAACATTTACATAGTAAGCTGTCTGTCATTCACAGAGACGTCAAGCCTTCTAATGTACTCATCAATGCTCTCGGTCAAGTGAAGATGTGCGATTTTGGAATCAGTGGCTACTTGGTGGACTCTGTTGCTAAAACAATTGATGCAGGTTGCAAACCATACATGGCCCCTGAAAGAATAAACCCAGAGCTCAACCAGAAGGGATACAGTGTGAAGTCTGACATTTGGAGTCTGGGCATCACGATGATTGAGTTGGCCATCCTTCGATTTCCCTATGATTCATGGGGAACTCCATTTCAGCAGCTCAAACAGGTGGTAGAGGAGCCATCGCCACAACTCCCAGCAGACAAGTTCTCTGCAGAGTTTGTTGACTTTACCTCACAGTGCTTAAAGAAGAATTCCAAAGAACGGCCTACATACCCAGAGCTAATGCAACATCCATTTTTCACCCTACATGAATCCAAAGGAACAGATGTGGCATCTTTTGTAAAACTGATTCTTGGAGAC</t>
+  </si>
+  <si>
+    <t>TCAACCAGGGATTATGAGATTCAAAGAGAAAGAATAGAACTTGGACGATGTATTGGAGAAGGCCAATTTGGAGATGTACATCAAGGCATTTATATGAGTCCAGAGAATCCAGCTTTGGCGGTTGCAATTAAAACATGTAAAAACTGTACTTCGGACAGCGTGAGAGAGAAATTTCTTCAAGAAGCCTTAACAATGCGTCAGTTTGACCATCCTCATATTGTGAAGCTGATTGGAGTCATCACAGAGAATCCTGTCTGGATAATCATGGAGCTGTGCACACTTGGAGAGCTGAGGTCATTTTTGCAAGTAAGGAAATACAGTTTGGATCTAGCATCTTTGATCCTGTATGCCTATCAGCTTAGTACAGCTCTTGCATATCTAGAGAGCAAAAGATTTGTACACAGGGACATTGCTGCTCGGAATGTTCTGGTGTCCTCAAATGATTGTGTAAAATTAGGAGACTTTGGATTATCCCGATATATGGAAGATAGTACTTACTACAAAGCTTCCAAAGGAAAATTGCCTATTAAATGGATGGCTCCAGAGTCAATCAATTTTCGACGTTTTACCTCAGCTAGTGACGTATGGATGTTTGGTGTGTGTATGTGGGAGATACTGATGCATGGTGTGAAGCCTTTTCAAGGAGTGAAGAACAATGATGTAATCGGTCGAATTGAAAATGGGGAAAGATTACCAATGCCTCCAAATTGTCCTCCTACCCTCTACAGCCTTATGACGAAATGCTGGGCCTATGACCCCAGCAGGCGGCCCAGGTTTACTGAACTTAAAGCTCAGCTCAGCACAATCCTGGAGGAAGAGAAGGCTCAGCAAGAAGAG</t>
+  </si>
+  <si>
+    <t>DPEELFTKLEKIGKGSFGEVFKGIDNRTQKVVAIKIIDLEEAEDEIEDIQQEITVLSQCDSPYVTKYYGSYLKDTKLWIIMEYLGGGSALDLLEPGPLDETQIATILREILKGLDYLHSEKKIHRDIKAANVLLSEHGEVKLADFGVAGQLTDTQIKRNTFVGTPFWMAPEVIKQSAYDSKADIWSLGITAIELARGEPPHSELHPMKVLFLIPKNNPPTLEGNYSKPLKEFVEACLNKEPSFRPTAKELLKHKFILRNAKKTSYLTELID</t>
+  </si>
+  <si>
+    <t>MAPK3_HUMAN_D0_3FXW_A</t>
+  </si>
+  <si>
+    <t>AAGCAGTACGAACACGTGAAGAGGGACCTGAACCCCGAAGACTTTTGGGAGATTATAGGAGAACTGGGCGACGGAGCCTTTGGGAAAGTGTACAAGGCCCAGAATAAAGAGACCAGTGTTTTAGCTGCTGCAAAAGTGATTGACACTAAATCTGAAGAAGAACTTGAAGATTACATGGTAGAGATTGACATATTAGCATCTTGTGATCACCCAAATATAGTCAAGCTTCTAGATGCCTTCTATTATGAGAACAATCTTTGGATCCTCATTGAATTTTGTGCAGGTGGAGCAGTAGATGCTGTGATGCTTGAACTTGAGAGACCATTAACTGAGTCCCAAATACAAGTAGTTTGCAAGCAGACTTTAGATGCATTGAACTACTTACATGATAATAAGATCATCCACAGAGATCTGAAGGCTGGCAACATTCTCTTTACCTTAGATGGAGATATCAAATTGGCGGATTTTGGAGTATCAGCTAAAAACATGAGGACAATTCAAAGAAGAGATTCCTTTATTGGTACACCATATTGGATGGCTCCTGAAGTAGTCATGTGTGAAACATCTAAGGACAGACCCTATGACTACAAAGCTGATGTTTGGTCCCTGGGTATCACTTTAATAGAAATGGCTGAGATAGAACCACCTCATCATGAATTAAATCCAATGCGAGTGCTGCTAAAAATAGCAAAATCTGAGCCACCTACATTAGCACAGCCATCCAGATGGTCTTCAAATTTTAAGGACTTTCTAAAGAAATGCTTAGAAAAGAATGTGGATGCCAGGTGGACTACATCTCAGCTGCTGCAGCATCCCTTTGTTACTGTTGATTCCAACAAACCCATCCGAGAATTGATTGCAGAGGCGAAGGCTGAAGTAACAGAAGAAGTTGAAGATGGCAAAGAG</t>
+  </si>
+  <si>
+    <t>ATGCCTTCCCGGGCTGAGGACTATGAAGTGTTGTACACCATTGGCACAGGCTCCTACGGCCGCTGCCAGAAGATCCGGAGGAAGAGTGATGGCAAGATATTAGTTTGGAAAGAACTTGACTATGGCTCCATGACAGAAGCTGAGAAACAGATGCTTGTTTCTGAAGTGAATTTGCTTCGTGAACTGAAACATCCAAACATCGTTCGTTACTATGATCGGATTATTGACCGGACCAATACAACACTGTACATTGTAATGGAATATTGTGAAGGAGGGGATCTGGCTAGTGTAATTACAAAGGGAACCAAGGAAAGGCAATACTTAGATGAAGAGTTTGTTCTTCGAGTGATGACTCAGTTGACTCTGGCCCTGAAGGAATGCCACAGACGAAGTGATGGTGGTCATACCGTATTGCATCGGGATCTGAAACCAGCCAATGTTTTCCTGGATGGCAAGCAAAACGTCAAGCTTGGAGACTTTGGGCTAGCTAGAATATTAAACCATGACACGAGTTTTGCAAAAACATTTGTTGGCACACCTTATTACATGTCTCCTGAACAAATGAATCGCATGTCCTACAATGAGAAATCAGATATCTGGTCATTGGGCTGCTTGCTGTATGAGTTATGTGCATTAATGCCTCCATTTACAGCTTTTAGCCAGAAAGAACTCGCTGGGAAAATCAGAGAAGGCAAATTCAGGCGAATTCCATACCGTTACTCTGATGAATTGAATGAAATTATTACGAGGATGTTAAACTTAAAGGATTACCATCGACCTTCTGTTGAAGAAATTCTTGAGAACCCTTTAATA</t>
+  </si>
+  <si>
+    <t>STK3_HUMAN_D0_4LG4_B</t>
+  </si>
+  <si>
+    <t>GATGAACAACCTCACATCGGAAACTACAGACTGTTGAAAACAATCGGCAAGGGGAATTTTGCAAAAGTAAAATTGGCAAGACATATCCTTACAGGCAGAGAGGTTGCAATAAAAATAATTGACAAAACTCAGTTGAATCCAACAAGTCTACAAAAGCTCTTCAGAGAAGTAAGAATAATGAAGATTTTAAATCATCCCAATATAGTGAAGTTATTCGAAGTCATTGAAACTGAAAAAACACTCTACCTAATCATGGAATATGCAAGTGGAGGTGAAGTATTTGACTATTTGGTTGCACATGGCAGGATGAAGGAAAAAGAAGCAAGATCTAAATTTAGACAGATTGTGTCTGCAGTTCAATACTGCCATCAGAAACGGATCGTACATCGAGACCTCAAGGCTGAAAATCTATTGTTAGATGCCGATATGAACATTAAAATAGCAGATTTCGGTTTTAGCAATGAATTTACTGTTGGCGGTAAACTCGACACGTTTTGTGGCAGTCCTCCATACGCAGCACCTGAGCTCTTCCAGGGCAAGAAATATGACGGGCCAGAAGTGGATGTGTGGAGTCTGGGGGTCATTTTATACACACTAGTCAGTGGCTCACTTCCCTTTGATGGGCAAAACCTAAAGGAACTGAGAGAGAGAGTATTAAGAGGGAAATACAGAATTCCCTTCTACATGTCTACAGACTGTGAAAACCTTCTCAAACGTTTCCTGGTGCTAAATCCAATTAAACGCGGCACTCTAGAGCAAATCATGAAGGACAGGTGGATCAATGCAGGGCATGAAGAAGATGAACTCAAACCATTTGTTGAACCAGAGCTAGACATCTCAGACCAAAAAAGAATAGATATTATGGTGGGAATGGGATATTCACAAGAAGAAATTCAAGAATCTCTTAGTAAGATGAAATACGATGAAATCACAGCTACATATTTGTTATTGGGGAGAAAATCTTCAGAG</t>
+  </si>
+  <si>
+    <t>dna_start</t>
+  </si>
+  <si>
+    <t>KEKEPLESQYQVGPLLGSGGFGSVYSGIRVSDNLPVAIKHVEKDRISDWGELPNGTRVPMEVVLLKKVSSGFSGVIRLLDWFERPDSFVLILERPEPVQDLFDFITERGALQEELARSFFWQVLEAVRHCHNCGVLHRDIKDENILIDLNRGELKLIDFGSGALLKDTVYTDFDGTRVYSPPEWIRYHRYHGRSAAVWSLGILLYDMVCGDIPFEHDEEIIGGQVFFRQRVSSECQHLIRWCLALRPSDRPTFEEIQNHPWMQDVLLPQETAEIHLHSLSPGPSK</t>
+  </si>
+  <si>
+    <t>VEDHYEMGEELGSGQFAIVRKCRQKGTGKEYAAKFIKKRRLSSSRRGVSREEIEREVNILREIRHPNIITLHDIFENKTDVVLILELVSGGELFDFLAEKESLTEDEATQFLKQILDGVHYLHSKRIAHFDLKPENIMLLDKNVPNPRIKLIDFGIAHKIEAGNEFKNIFGTPEFVAPEIVNYEPLGLEADMWSIGVITYILLSGASPFLGETKQETLTNISAVNYDFDEEYFSNTSELAKDFIRRLLVKDPKRRMTIAQSLEHSWIKAIRRRNVRGEDSG</t>
+  </si>
+  <si>
     <t>ACCGACAGCTTCTCGGGCAGGTTTGAAGACGTCTACCAGCTGCAGGAAGATGTGCTGGGGGAGGGCGCTCATGCCCGAGTGCAGACCTGCATCAACCTGATCACCAGCCAGGAGTACGCCGTCAAGATCATTGAGAAGCAGCCAGGCCACATTCGGAGCAGGGTTTTCAGGGAGGTGGAGATGCTGTACCAGTGCCAGGGACACAGGAACGTCCTAGAGCTGATTGAGTTCTTCGAGGAGGAGGACCGCTTCTACCTGGTGTTTGAGAAGATGCGGGGAGGCTCCATCCTGAGCCACATCCACAAGCGCCGGCACTTCAACGAGCTGGAGGCCAGCGTGGTGGTGCAGGACGTGGCCAGCGCCTTGGACTTTCTGCATAACAAAGGCATCGCCCACAGGGACCTAAAGCCGGAAAACATCCTCTGTGAGCACCCCAACCAGGTCTCCCCCGTGAAGATCTGTGACTTCGACCTGGGCAGCGGCATCAAACTCAACGGGGACTGCTCCCCTATCTCCACCCCGGAGCTGCTCACTCCGTGCGGCTCGGCGGAGTACATGGCCCCGGAGGTAGTGGAGGCCTTCAGCGAGGAGGCTAGCATCTACGACAAGCGCTGCGACCTGTGGAGCCTGGGCGTCATCTTGTATATCCTACTCAGCGGCTACCCGCCCTTCGTGGGCCGCTGTGGCAGCGACTGCGGCTGGGACCGCGGCGAGGCCTGCCCTGCCTGCCAGAACATGCTGTTTGAGAGCATCCAGGAGGGCAAGTACGAGTTCCCCGACAAGGACTGGGCCCACATCTCCTGCGCTGCCAAAGACCTCATCTCCAAGCTGCTGGTCCGTGACGCCAAGCAGAGGCTGAGTGCCGCCCAAGTCCTGCAGCACCCCTGGGTTCAGGGGTGCGCCCCGGAGAACACCTTGCCCACTCCCATGGTCCTGCAGAGG</t>
   </si>
   <si>
-    <t>MSRSKRDNNFYSVEIGDSTFTVLKRYQNLKPIGSGAQGIVCAAYDAILERNVAIKKLSRPFQNQTHAKRAYRELVLMKCVNHKNIIGLLNVFTPQKSLEEFQDVYIVMELMDANLCQVIQMELDHERMSYLLYQMLCGIKHLHSAGIIHRDLKPSNIVVKSDCTLKILDFGLARTAGTSFMMTPYVVTRYYRAPEVILGMGYKENVDLWSVGCIMGEMVCHKILFPGRDYIDQWNKVIEQLGTPCPEFMKKLQPTVRTYVENRPKYAGYSFEKLFPDVLFPADSEHNKLKASQARDLLSKMLVIDASKRISVDEALQHPYINVWYDPSEAEAPPPKIPDKQLDEREHTIEEWKELIYKEVMDLE</t>
-  </si>
-  <si>
-    <t>STRAA_HUMAN_D0_3GNI_B</t>
-  </si>
-  <si>
-    <t>MP2K2_HUMAN_D0_1S9I_A</t>
-  </si>
-  <si>
-    <t>PIM1_HUMAN_D0_4A7C_A</t>
+    <t>MET_HUMAN_D0_4EEV_A</t>
+  </si>
+  <si>
+    <t>MSSFLPEGGCYELLTVIGKGFEDLMTVNLARYKPTGEYVTVRRINLEACSNEMVTFLQGELHVSKLFNHPNIVPYRATFIADNELWVVTSFMAYGSAKDLICTHFMDGMNELAIAYILQGVLKALDYIHHMGYVHRSVKASHILISVDGKVYLSGLRSNLSMISHGQRQRVVHDFPKYSVKVLPWLSPEVLQQNLQGYDAKSDIYSVGITACELANGHVPFKDMPATQMLLEKLNGTVPCLLDTSTIPAEELTMSPSRSVANSGLSDSLTTSTPRPSNGDSPSHPYHRTFSPHFHHFVEQCLQRNPDARPSASTLLNHSFFKQIKRRASEVLPELLRPVTPITNFEGSQSQDHSGIFGLVTNLEELEVDDWEF</t>
+  </si>
+  <si>
+    <t>ETKYTVDKRFGMDFKEIELIGSGGFGQVFKAKHRIDGKTYVIKRVKYNNEKAEREVKALAKLDHVNIVHYNGCWDGFDYDPETSDDSLESSDYDPENSKNSSRSKTKCLFIQMEFCDKGTLEQWIEKRRGEKLDKVLALELFEQITKGVDYIHSKKLIHRDLKPSNIFLVDTKQVKIGDFGLVTSLKNDGKRTRSKGTLRYMSPEQISSQDYGKEVDLYALGLILAELLHVCDTAFETSKFFTDLRDGIISDIFDKKEKTLLQKLLSKKPEDRPNTSEILRTLTVWKKSPEKNERHTC</t>
+  </si>
+  <si>
+    <t>CDKL1_HUMAN_D0_4AGU_C</t>
+  </si>
+  <si>
+    <t>MARK3_HUMAN_D0_2QNJ_A</t>
+  </si>
+  <si>
+    <t>NLVFSDGYVVKETIGVGSYSECKRCVHKATNMEYAVKVIDKSKRDPSEEIEILLRYGQHPNIITLKDVYDDGKHVYLVTELMRGGELLDKILRQKFFSEREASFVLHTIGKTVEYLHSQGVVHRDLKPSNILYVDESGNPECLRICDFGFAKQLRAENGLLMTPCYTANFVAPEVLKRQGYDEGCDIWSLGILLYTMLAGYTPFANGPSDTPEEILTRIGSGKFTLSGGNWNTVSETAKDLVSKMLHVDPHQRLTAKQVLQHPWVTQKDKLPQSQLSHQDLQLVKGAMAATYSALNSSKPTPQLKPIESSILAQRRVRKLPSTTL</t>
+  </si>
+  <si>
+    <t>GGTGTTGTGACACATGAGCAGTTCAAGGCTGCGCTCAGGATGGTGGTGGACCAGGGTGACCCCCGGCTGCTGCTGGACAGCTACGTGAAGATTGGCGAGGGCTCCACCGGCATCGTCTGCTTGGCCCGGGAGAAGCACTCGGGCCGCCAGGTGGCCGTCAAGATGATGGACCTCAGGAAGCAGCAGCGCAGGGAGCTGCTCTTCAACGAGGTGGTGATCATGCGGGACTACCAGCACTTCAACGTGGTGGAGATGTACAAGAGCTACCTGGTGGGCGAGGAGCTGTGGGTGCTCATGGAGTTCCTGCAGGGAGGAGCCCTCACAGACATCGTCTCCCAAGTCAGGCTGAATGAGGAGCAGATTGCCACTGTGTGTGAGGCTGTGCTGCAGGCCCTGGCCTACCTGCATGCTCAGGGTGTCATCCACCGGGACATCAAGAGTGACTCCATCCTGCTGACCCTCGATGGCAGGGTGAAGCTCTCGGACTTCGGATTCTGTGCTCAGATCAGCAAAGACGTCCCTAAGAGGAAGTCCCTGGTGGGAACCCCCTACTGGATGGCTCCTGAAGTGATCTCCAGGTCTTTGTATGCCACTGAGGTGGATATCTGGTCTCTGGGCATCATGGTGATTGAGATGGTAGATGGGGAGCCACCGTACTTCAGTGACTCCCCAGTGCAAGCCATGAAGAGGCTCCGGGACAGCCCCCCACCCAAGCTGAAAAACTCTCACAAGGTCTCCCCAGTGCTGCGAGACTTCCTGGAGCGGATGCTGGTGCGGGACCCCCAAGAGAGAGCCACAGCCCAGGAGCTCCTAGACCACCCCTTCCTGCTGCAGACAGGGCTACCTGAGTGCCTGGTGCCCCTGATCCAGCTCTACCGAAAGCAGACCTCCACCTGC</t>
+  </si>
+  <si>
+    <t>MGKVKATPMTPEQAMKQYMQKLTAFEHHEIFSYPEIYFLGLNAKKRQGMTGGPNNGGYDDDQGSYVQVPHDHVAYRYEVLKVIGKGSFGQVVKAYDHKVHQHVALKMVRNEKRFHRQAAEEIRILEHLRKQDKDNTMNVIHMLENFTFRNHICMTFELLSMNLYELIKKNKFQGFSLPLVRKFAHSILQCLDALHKNRIIHCDLKPENILLKQQGRSGIKVIDFGSSCYEHQRVYTYIQSRFYRAPEVILGARYGMPIDMWSLGCILAELLTGYPLLPGEDEGDQLACMIELLGMPSQKLLDASKRAKNFVSSKGYPRYCTVTTLSDGSVVLNGGRSRRGKLRGPPESREWGNALKGCDDPLFLDFLKQCLEWDPAVRMTPGQALRHPWLRRRLPKPPTGEKTSVKR</t>
+  </si>
+  <si>
+    <t>MAAAAAQGGGGGEPRRTEGVGPGVPGEVEMVKGQPFDVGPRYTQLQYIGEGAYGMVSSAYDHVRKTRVAIKKISPFEHQTYCQRTLREIQILLRFRHENVIGIRDILRASTLEAMRDVYIVQDLMETDLYKLLKSQQLSNDHICYFLYQILRGLKYIHSANVLHRDLKPSNLLINTTCDLKICDFGLARIADPEHDHTGFLTEYVATRWYRAPEIMLNSKGYTKSIDIWSVGCILAEMLSNRPIFPGKHYLDQLNHILGILGSPSQEDLNCIINMKARNYLQSLPSKTKVAWAKLFPKSDSKALDLLDRMLTFNPNKRITVEEALAHPYLEQYYDPTDEPVAEEPFTFAMELDDLPKERLKELIFQETARFQPGVLEAP</t>
+  </si>
+  <si>
+    <t>GDSDISSPLLQNTVHIDLSALNPELVQAVQHVVIGPSSLIVHFNEVIGRGHFGCVYHGTLLDNDGKKIHCAVKSLNRITDIGEVSQFLTEGIIMKDFSHPNVLSLLGICLRSEGSPLVVLPYMKHGDLRNFIRNETHNPTVKDLIGFGLQVAKGMKYLASKKFVHRDLAARNCMLDEKFTVKVADFGLARDMYDKEYYSVHNKTGAKLPVKWMALESLQTQKFTTKSDVWSFGVLLWELMTRGAPPYPDVNTFDITVYLLQGRRLLQPEYCPDPLYEVMLKCWHPKAEMRPSFSELVSRISAIFSTFIG</t>
+  </si>
+  <si>
+    <t>ATGAGTAGCTTTCTGCCAGAGGGAGGGTGTTACGAGCTGCTCACTGTGATAGGCAAAGGATTTGAGGACCTGATGACTGTGAATCTAGCAAGGTACAAACCAACAGGAGAGTACGTGACTGTACGGAGGATTAACCTAGAAGCTTGTTCCAATGAGATGGTAACATTCTTGCAGGGCGAGCTGCATGTCTCCAAACTCTTCAACCATCCCAATATCGTGCCATATCGAGCCACTTTTATTGCAGACAATGAGCTGTGGGTTGTCACATCATTCATGGCATACGGTTCTGCAAAAGATCTCATCTGTACACACTTCATGGATGGCATGAATGAGCTGGCGATTGCTTACATCCTGCAGGGGGTGCTGAAGGCCCTCGACTACATCCACCACATGGGATATGTACACAGGAGTGTCAAAGCCAGCCACATCCTGATCTCTGTGGATGGGAAGGTCTACCTGTCTGGTTTGCGCAGCAACCTCAGCATGATAAGCCATGGGCAGCGGCAGCGAGTGGTCCACGATTTTCCCAAGTACAGTGTCAAGGTTCTGCCGTGGCTCAGCCCCGAGGTCCTCCAGCAGAATCTCCAGGGTTATGATGCCAAGTCTGACATCTACAGTGTGGGAATCACAGCCTGTGAACTGGCCAACGGCCATGTCCCCTTTAAGGATATGCCTGCCACCCAGATGCTGCTAGAGAAACTGAACGGCACAGTGCCCTGCCTGTTGGATACCAGCACCATCCCCGCTGAGGAGCTGACCATGAGCCCTTCGCGCTCAGTGGCCAACTCTGGCCTGAGTGACAGCCTGACCACCAGCACCCCCCGGCCCTCCAACGGTGACTCGCCCTCCCACCCCTACCACCGAACCTTCTCCCCCCACTTCCACCACTTTGTGGAGCAGTGCCTTCAGCGCAACCCGGATGCCAGGCCCAGTGCCAGCACCCTCCTGAACCACTCTTTCTTCAAGCAGATCAAGCGACGTGCCTCAGAGGTTTTGCCCGAATTGCTTCGTCCTGTCACCCCCATCACCAATTTTGAGGGCAGCCAGTCTCAGGACCACAGTGGAATCTTTGGCCTGGTAACAAACCTGGAAGAGCTGGAGGTGGACGATTGGGAGTTC</t>
+  </si>
+  <si>
+    <t>ADPEELFTKLERIGKGSFGEVFKGIDNRTQQVVAIKIIDLEEAEDEIEDIQQEITVLSQCDSSYVTKYYGSYLKGSKLWIIMEYLGGGSALDLLRAGPFDEFQIATMLKEILKGLDYLHSEKKIHRDIKAANVLLSEQGDVKLADFGVAGQLTDTQIKRNTFVGTPFWMAPEVIQQSAYDSKADIWSLGITAIELAKGEPPNSDMHPMRVLFLIPKNNPPTLVGDFTKSFKEFIDACLNKDPSFRPTAKELLKHKFIVKNSKKTSYLTELIDRFKRWKAE</t>
+  </si>
+  <si>
+    <t>AURKA_HUMAN_D0_2NP8_A</t>
+  </si>
+  <si>
+    <t>HIGNYRLLKTIGKGNFAKVKLARHILTGKEVAVKIIDKTQLNSSSLQKLFREVRIMKVLNHPNIVKLFEVIETEKTLYLVMEYASGGEVFDYLVAHGRMKEKEARAKFRQIVSAVQYCHQKFIVHRDLKAENLLLDADMNIKIADFGFSNEFTFGNKLDTFCGSPPYAAPELFQGKKYDGPEVDVWSLGVILYTLVSGSLPFDGQNLKELRERVLRGKYRIPFYMSTDCENLLKKFLILNPSKRGTLEQIMKDRWMNVGHEDDELKPYVEPLPDYKDPRRTELMVSMGYTREEIQDSLVGQRYNEVMATYLLLGY</t>
+  </si>
+  <si>
+    <t>GVVTHEQFKAALRMVVDQGDPRLLLDSYVKIGEGSTGIVCLAREKHSGRQVAVKMMDLRKQQRRELLFNEVVIMRDYQHFNVVEMYKSYLVGEELWVLMEFLQGGALTDIVSQVRLNEEQIATVCEAVLQALAYLHAQGVIHRDIKSDSILLTLDGRVKLSDFGFCAQISKDVPKRKSLVGTPYWMAPEVISRSLYATEVDIWSLGIMVIEMVDGEPPYFSDSPVQAMKRLRDSPPPKLKNSHKVSPVLRDFLERMLVRDPQERATAQELLDHPFLLQTGLPECLVPLIQLYRKQTSTC</t>
+  </si>
+  <si>
+    <t>MKDYDELLKYYELHETIGTGGFAKVKLACHILTGEMVAIKIMDKNTLGSDLPRIKTEIEALKNLRHQHICQLYHVLETANKIFMVLEYCPGGELFDYIISQDRLSEEETRVVFRQIVSAVAYVHSQGYAHRDLKPENLLFDEYHKLKLIDFGLCAKPKGNKDYHLQTCCGSLAYAAPELIQGKSYLGSEADVWSMGILLYVLMCGFLPFDDDNVMALYKKIMRGKYDVPKWLSPSSILLLQQMLQVDPKKRISMKNLLNHPWIMQDYNYPVEWQSKNPFIHLDDDCVTELSVHHRNNRQTMEDLISLWQYDHLTATYLLLLAKKARGKPVRLRLSSFSCG</t>
+  </si>
+  <si>
+    <t>MSQERPTFYRQELNKTIWEVPERYQNLSPVGSGAYGSVCAAFDTKTGLRVAVKKLSRPFQSIIHAKRTYRELRLLKHMKHENVIGLLDVFTPARSLEEFNDVYLVTHLMGADLNNIVKCQKLTDDHVQFLIYQILRGLKYIHSADIIHRDLKPSNLAVNEDCELKILDFGLARHTDDEMTGYVATRWYRAPEIMLNWMHYNQTVDIWSVGCIMAELLTGRTLFPGTDHIDQLKLILRLVGTPGAELLKKISSESARNYIQSLTQMPKMNFANVFIGANPLAVDLLEKMLVLDSDKRITAAQALAHAYFAQYHDPDDEPVADPYDQSFESRDLLIDEWKSLTYDEVISFVPPPLDQEEMES</t>
+  </si>
+  <si>
+    <t>MELRVGNRYRLGRKIGSGSFGDIYLGTDIAAGEEVAIKLECVKTKHPQLHIESKIYKMMQGGVGIPTIRWCGAEGDYNVMVMELLGPSLEDLFNFCSRKFSLKTVLLLADQMISRIEYIHSKNFIHRDVKPDNFLMGLGKKGNLVYIIDFGLAKKYRDARTHQHIPYRENKNLTGTARYASINTHLGIEQSRRDDLESLGYVLMYFNLGSLPWQGLKAATKRQKYERISEKKMSTPIEVLCKGYPSEFATYLNFCRSLRFDDKPDYSYLRQLFRNLFHRQGFSYDYVFDWNMLK</t>
+  </si>
+  <si>
+    <t>targetID</t>
+  </si>
+  <si>
+    <t>TGGGCCCTGAACATGAAGGAGCTGAAGCTGCTGCAGACCATCGGGAAGGGGGAGTTCGGAGACGTGATGCTGGGCGATTACCGAGGGAACAAAGTCGCCGTCAAGTGCATTAAGAACGACGCCACTGCCCAGGCCTTCCTGGCTGAAGCCTCAGTCATGACGCAACTGCGGCATAGCAACCTGGTGCAGCTCCTGGGCGTGATCGTGGAGGAGAAGGGCGGGCTCTACATCGTCACTGAGTACATGGCCAAGGGGAGCCTTGTGGACTACCTGCGGTCTAGGGGTCGGTCAGTGCTGGGCGGAGACTGTCTCCTCAAGTTCTCGCTAGATGTCTGCGAGGCCATGGAATACCTGGAGGGCAACAATTTCGTGCATCGAGACCTGGCTGCCCGCAATGTGCTGGTGTCTGAGGACAACGTGGCCAAGGTCAGCGACTTTGGTCTCACCAAGGAGGCGTCCAGCACCCAGGACACGGGCAAGCTGCCAGTCAAGTGGACAGCCCCTGAGGCCCTGAGAGAGAAGAAATTCTCCACTAAGTCTGACGTGTGGAGTTTCGGAATCCTTCTCTGGGAAATCTACTCCTTTGGGCGAGTGCCTTATCCAAGAATTCCCCTGAAGGACGTCGTCCCTCGGGTGGAGAAGGGCTACAAGATGGATGCCCCCGACGGCTGCCCGCCCGCAGTCTATGAAGTCATGAAGAACTGCTGGCACCTGGACGCCGCCATGCGGCCCTCCTTCCTACAGCTCCGAGAGCAGCTTGAGCACATCAAAACCCACGAGCTGCACCTG</t>
+  </si>
+  <si>
+    <t>dna_seq</t>
+  </si>
+  <si>
+    <t>AACCTGGTTTTTAGTGACGGCTACGTGGTAAAGGAGACAATTGGTGTGGGCTCCTACTCTGAGTGCAAGCGCTGTGTCCACAAGGCCACCAACATGGAGTATGCTGTCAAGGTCATTGATAAGAGCAAGCGGGATCCTTCAGAAGAGATTGAGATTCTTCTGCGGTATGGCCAGCACCCCAACATCATCACTCTGAAAGATGTGTATGATGATGGCAAACACGTGTACCTGGTGACAGAGCTGATGCGGGGTGGGGAGCTGCTGGACAAGATCCTGCGGCAGAAGTTCTTCTCAGAGCGGGAGGCCAGCTTTGTCCTGCACACCATTGGCAAAACTGTGGAGTATCTGCACTCACAGGGGGTTGTGCACAGGGACCTGAAGCCCAGCAACATCCTGTATGTGGACGAGTCCGGGAATCCCGAGTGCCTGCGCATCTGTGACTTTGGTTTTGCCAAACAGCTGCGGGCTGAGAATGGGCTCCTCATGACACCTTGCTACACAGCCAACTTTGTGGCGCCTGAGGTGCTGAAGCGCCAGGGCTACGATGAAGGCTGCGACATCTGGAGCCTGGGCATTCTGCTGTACACCATGCTGGCAGGATATACTCCATTTGCCAACGGTCCCAGTGACACACCAGAGGAAATCCTAACCCGGATCGGCAGTGGGAAGTTTACCCTCAGTGGGGGAAATTGGAACACAGTTTCAGAGACAGCCAAGGACCTGGTGTCCAAGATGCTACACGTGGATCCCCACCAGCGCCTCACAGCTAAGCAGGTTCTGCAGCATCCATGGGTCACCCAGAAAGACAAGCTTCCCCAAAGCCAGCTGTCCCACCAGGACCTACAGCTTGTGAAGGGAGCCATGGCTGCCACGTACTCCGCACTCAACAGCTCCAAGCCCACCCCCCAGCTGAAGCCCATCGAGTCATCCATCCTGGCCCAGCGGCGAGTGAGGAAGTTGCCATCCACCACCCTG</t>
+  </si>
+  <si>
+    <t>ATGGCCGACGACGACGTGCTGTTCGAGGATGTGTACGAGCTGTGCGAGGTGATCGGAAAGGGTCCCTTCAGTGTTGTACGACGATGTATCAACAGAGAAACTGGGCAACAATTTGCTGTAAAAATTGTTGATGTAGCCAAGTTCACATCAAGTCCAGGGTTAAGTACAGAAGATCTAAAGCGGGAAGCCAGTATCTGTCATATGCTGAAACATCCACACATTGTAGAGTTATTGGAGACATATAGCTCAGATGGAATGCTTTACATGGTTTTCGAATTTATGGATGGAGCAGATCTGTGTTTTGAAATCGTAAAGCGAGCTGACGCTGGTTTTGTGTACAGTGAAGCTGTAGCCAGCCATTATATGAGACAGATACTGGAAGCTCTACGCTACTGCCATGATAATAACATAATTCACAGGGATGTGAAGCCCCACTGTGTTCTCCTTGCCTCAAAAGAAAACTCGGCACCTGTTAAACTTGGAGGCTTTGGGGTAGCTATTCAATTAGGGGAGTCTGGACTTGTAGCTGGAGGACGTGTTGGAACACCTCATTTTATGGCACCAGAAGTGGTCAAAAGAGAGCCTTACGGAAAGCCTGTAGACGTCTGGGGGTGCGGTGTGATCCTTTTTATCCTGCTCAGTGGTTGTTTGCCTTTTTACGGAACCAAGGAAAGATTGTTTGAAGGCATTATTAAAGGAAAATATAAGATGAATCCAAGGCAGTGGAGCCATATCTCTGAAAGTGCCAAAGACCTAGTACGTCGCATGCTGATGCTGGATCCAGCTGAAAGGATCACTGTTTATGAAGCACTGAATCACCCATGGCTTAAGGAGCGGGATCGTTACGCCTACAAGATTCATCTTCCAGAAACAGTAGAGCAGCTGAGGAAATTCAATGCAAGGAGGAAACTAAAGGGTGCAGTACTAGCCGCTGTGTCAAGTCACAAATTCAACTCATTCTATGGGGATCCCCCTGAAGAGTTACCAGATTTCTCCGAAGACCCTACCTCCTCAGGAGCA</t>
+  </si>
+  <si>
+    <t>VRK1_HUMAN_D0_3OP5_D</t>
+  </si>
+  <si>
+    <t>ATGGGGAAGGTGAAAGCCACCCCCATGACACCTGAACAAGCAATGAAGCAATACATGCAAAAACTCACAGCCTTCGAACACCATGAGATTTTCAGCTACCCTGAAATATATTTCTTGGGTCTAAATGCTAAGAAGCGCCAGGGCATGACAGGTGGGCCCAACAATGGTGGCTATGATGATGACCAGGGATCATATGTGCAGGTGCCCCACGATCACGTGGCTTACAGGTATGAGGTCCTCAAGGTCATTGGGAAGGGGAGCTTTGGGCAGGTGGTCAAGGCCTACGATCACAAAGTCCACCAGCACGTGGCCCTAAAGATGGTGCGGAATGAGAAGCGCTTCCACCGGCAAGCAGCGGAGGAGATCCGAATCCTGGAACACCTGCGGAAGCAGGACAAGGATAACACAATGAATGTCATCCATATGCTGGAGAATTTCACCTTCCGCAACCACATCTGCATGACGTTTGAGCTGCTGAGCATGAACCTCTATGAGCTCATCAAGAAGAATAAATTCCAGGGCTTCAGTCTGCCTTTGGTTCGCAAGTTTGCCCACTCGATTCTGCAGTGCTTGGATGCTTTGCACAAAAACAGAATAATTCACTGTGACCTTAAGCCCGAGAACATTTTGTTAAAGCAGCAGGGTAGAAGCGGTATTAAAGTAATTGATTTTGGCTCCAGTTGTTACGAGCATCAGCGTGTCTACACGTACATCCAGTCGCGTTTTTACCGGGCTCCAGAAGTGATCCTTGGGGCCAGGTATGGCATGCCCATTGATATGTGGAGCCTGGGCTGCATTTTAGCAGAGCTCCTGACGGGTTACCCCCTCTTGCCTGGGGAAGATGAAGGGGACCAGCTGGCCTGTATGATTGAACTGTTGGGCATGCCCTCACAGAAACTGCTGGATGCATCCAAACGAGCCAAAAATTTTGTGAGCTCCAAGGGTTATCCCCGTTACTGCACTGTCACGACTCTCTCAGATGGCTCTGTGGTCCTAAACGGAGGCCGTTCCCGGAGGGGGAAACTGAGGGGCCCACCGGAGAGCAGAGAGTGGGGGAACGCGCTGAAGGGGTGTGATGATCCCCTTTTCCTTGACTTCTTAAAACAGTGTTTAGAGTGGGATCCTGCAGTGCGCATGACCCCAGGCCAGGCTTTGCGGCACCCCTGGCTGAGGAGGCGGTTGCCAAAGCCTCCCACCGGGGAGAAAACGTCAGTGAAAAGG</t>
+  </si>
+  <si>
+    <t>ACTGACTCCTTGCCAGGAAAGTTTGAAGATATGTACAAGCTGACCTCTGAATTGCTGGGAGAGGGAGCCTATGCCAAAGTTCAAGGTGCCGTGAGCCTACAGAATGGCAAAGAGTATGCCGTCAAAATCATCGAGAAACAAGCAGGGCACAGTCGGAGTAGGGTGTTTCGAGAGGTGGAGACGCTGTATCAGTGTCAGGGAAACAAGAACATTTTGGAGCTGATTGAGTTCTTTGAAGATGACACAAGGTTTTACTTGGTCTTTGAGAAATTGCAAGGAGGTTCCATCTTAGCCCACATCCAGAAGCAAAAGCACTTCAATGAGCGAGAAGCCAGCCGAGTGGTGCGGGACGTTGCTGCTGCCCTTGACTTCCTGCATACCAAAGACAAAGTCTCTCTCTGTCACCTAGGCGGGAGTGCTAGGGCGCCATCAGGGCTCACTGCAGCCCCAACCTCCCTGGGCTCCAGTGATCCTCCCACCTCAGCCTCCCAAGTAGCTGGGACTACAGGCATTGATCATCGTGATCTGAAACCAGAAAATATATTGTGTGAATCTCCAGAAAAGGTGTCTCCAGTGAAAATCTGTGACTTTGACTTGGGCAGTGGGATGAAACTGAACAACTCCTGTACCCCCATAACCACACCAGAGCTGACCACCCCATGTGGCTCTGCAGAATACATGGCCCCTGAGGTAGGGGAGGTCTTCACGGACCAGGCCACATTCTACGACAAGCGCTGTGACCTGTGGAGCCTGGGCGTGGTCCTCTACATCATGCTGAGTGGCTACCCACCCTTCGTGGGTCACTGCGGGGCCGACTGTGGCTGGGACCGGGGCGAGGTCTGCAGGGTGTGCCAGAACAAGCTGTTTGAAAGCATCCAGGAAGGCAAGTATGAGTTTCCTGACAAGGACTGGGCACACATCTCCAGTGAAGCCAAAGACCTCATCTCCAAGCTCCTGGTGCGAGATGCAAAGCAGAGACTTAGCGCCGCCCAAGTTCTGCAGCACCCATGGGTGCAGGGGCAAGCTCCAGAAAAGGGA</t>
+  </si>
+  <si>
+    <t>SVYPKALRDEYIMSKTLGSGACGEVKLAFERKTCKKVAIKIISKRKFAIGSAREADPALNVETEIEILKKLNHPCIIKIKNFFDAEDYYIVLELMEGGELFDKVVGNKRLKEATCKLYFYQMLLAVQYLHENGIIHRDLKPENVLLSSQEEDCLIKITDFGHSKIWGETSLMRTLCGTPTYLAPEVLVSVGTAGYNRAVDCWSLGVILFICLSGYPPFSEHRTQVSLKDQITSGKYNFIPEVWAEVSEKALDLVKKLLVVDPKARFTTEEALRHPWLQDEDMKRKFQDLLSEENESTALPQVLAQPSTSRKRPREGEAEGAE</t>
+  </si>
+  <si>
+    <t>ATGGAGAAGTATGAAAAAATTGGGAAAATTGGAGAAGGATCCTATGGAGTTGTTTTCAAATGTAGAAACAGGGACACGGGTCAGATTGTGGCCATCAAGAAGTTTCTGGAATCAGAAGATGACCCTGTCATAAAGAAAATTGCCCTTCGGGAAATCCGAATGCTCAAGCAACTCAAGCATCCCAACCTTGTTAACCTCCTGGAAGTCTTCAGGAGGAAACGGAGGCTTCACCTGGTGTTTGAATATTGTGACCACACAGTTCTCCATGAGTTGGACAGATACCAAAGAGGGGTACCAGAACATCTCGTGAAGAGCATAACTTGGCAGACACTGCAAGCTGTAAATTTTTGCCATAAACACAATTGCATACATAGAGACGTGAAGCCAGAAAATATCCTCATCACGAAACATTCCGTGATTAAGCTTTGTGACTTTGGATTTGCTCGGCTTTTGACTGGACCGAGTGACTACTATACAGACTACGTGGCTACCAGGTGGTACCGCTCCCCTGAGCTGCTGGTGGGGGACACGCAGTACGGCCCCCCGGTGGATGTTTGGGCAATTGGCTGTGTCTTTGCTGAGCTGCTGTCAGGAGTGCCTCTGTGGCCAGGAAAATCGGATGTGGATCAGCTGTATCTGATTAGGAAGACCTTGGGGGATCTCATTCCTAGGCACCAGCAAGTGTTTAGCACGAATCAGTACTTCAGTGGAGTGAAAATTCCAGACCCTGAAGATATGGAACCACTTGAATTAAAATTCCCAAACATCTCTTATCCTGCCCTGGGGCTCCTA</t>
+  </si>
+  <si>
+    <t>KHDGRVKIGHYVLGDTLGVGTFGKVKIGEHQLTGHKVAVKILNRQKIRSLDVVGKIKREIQNLKLFRHPHIIKLYQVISTPTDFFMVMEYVSGGELFDYICKHGRVEEMEARRLFQQILSAVDYCHRHMVVHRDLKPENVLLDAHMNAKIADFGLSNMMSDGEFLRTSCGSPNYAAPEVISGRLYAGPEVDIWSCGVILYALLCGTLPFDDEHVPTLFKKIRGGVFYIPEYLNRSVATLLMHMLQVDPLKRATIKDIREHEWFKQDLPSYLFPE</t>
+  </si>
+  <si>
+    <t>ATGGAAAACTTTAATAATTTCTATATACTTACATCTAAAGAGCTAGGGAGAGGAAAATTTGCTGTGGTTAGACAATGTATATCAAAATCTACTGGCCAAGAATATGCTGCAAAATTTCTAAAAAAGAGAAGAAGAGGACAGGATTGTCGAGCAGAAATTTTACACGAGATTGCTGTGCTTGAATTGGCAAAGTCTTGTCCCCGTGTTATTAATCTTCATGAGGTCTATGAAAATACAAGTGAAATCATTTTGATATTGGAATATGCTGCAGGTGGAGAAATTTTCAGCCTGTGTTTACCTGAGTTGGCTGAAATGGTTTCTGAAAATGATGTTATCAGACTCATTAAACAAATACTTGAAGGAGTTTATTATCTACATCAGAATAACATTGTACACCTTGATTTAAAGCCACAGAATATATTACTGAGCAGCATATACCCTCTCGGGGACATTAAAATAGTAGATTTTGGAATGTCTCGAAAAATAGGGCATGCGTGTGAACTTCGGGAAATCATGGGAACACCAGAATATTTAGCTCCAGAAATCCTGAACTATGATCCCATTACCACAGCAACAGATATGTGGAATATTGGTATAATAGCATATATGTTGTTAACTCACACATCACCATTTGTGGGAGAAGATAATCAAGAAACATACCTCAATATTTCTCAAGTTAATGTAGATTATTCGGAAGAAACTTTTTCATCAGTTTCACAGCTGGCCACAGACTTTATTCAGAGCCTTTTAGTAAAAAATCCAGAGAAAAGACCAACAGCAGAGATATGCCTTTCTCATTCTTGGCTACAGCAGTGGGACTTTGAAAACTTGTTTCACCCTGAAGAAACTTCCAGTTCCTCTCAAACTCAGGATCATTCTGTAAGGTCCTCTGAAGACAAGACTTCTAAATCCTCC</t>
+  </si>
+  <si>
+    <t>MPSRAEDYEVLYTIGTGSYGRCQKIRRKSDGKILVWKELDYGSMTEAEKQMLVSEVNLLRELKHPNIVRYYDRIIDRTNTTLYIVMEYCEGGDLASVITKGTKERQYLDEEFVLRVMTQLTLALKECHRRSDGGHTVLHRDLKPANVFLDGKQNVKLGDFGLARILNHDTSFAKTFVGTPYYMSPEQMNRMSYNEKSDIWSLGCLLYELCALMPPFTAFSQKELAGKIREGKFRRIPYRYSDELNEIITRMLNLKDYHRPSVEEILENPLI</t>
+  </si>
+  <si>
+    <t>GACCCAGAAGAGCTTTTTACAAAACTAGAGAAAATTGGGAAGGGCTCCTTTGGAGAGGTGTTCAAAGGCATTGACAATCGGACTCAGAAAGTGGTTGCCATAAAGATCATTGATCTGGAAGAAGCTGAAGATGAGATAGAGGACATTCAACAAGAAATCACAGTGCTGAGTCAGTGTGACAGTCCATATGTAACCAAATATTATGGATCCTATCTGAAGGATACAAAATTATGGATAATAATGGAATATCTTGGTGGAGGCTCCGCACTAGATCTATTAGAACCTGGCCCATTAGATGAAACCCAGATCGCTACTATATTAAGAGAAATACTGAAAGGACTCGATTATCTCCATTCGGAGAAGAAAATCCACAGAGACATTAAAGCGGCCAACGTCCTGCTGTCTGAGCATGGCGAGGTGAAGCTGGCGGACTTTGGCGTGGCTGGCCAGCTGACAGACACCCAGATCAAAAGGAACACCTTCGTGGGCACCCCATTCTGGATGGCACCCGAGGTCATCAAACAGTCGGCCTATGACTCGAAGGCAGACATCTGGTCCCTGGGCATAACAGCTATTGAACTTGCAAGAGGGGAACCACCTCATTCCGAGCTGCACCCCATGAAAGTTTTATTCCTCATTCCAAAGAACAACCCACCGACGTTGGAAGGAAACTACAGTAAACCCCTCAAGGAGTTTGTGGAGGCCTGTTTGAATAAGGAGCCGAGCTTTAGACCCACTGCTAAGGAGTTATTGAAGCACAAGTTTATACTACGCAATGCAAAGAAAACTTCCTACTTGACCGAGCTCATCGAC</t>
+  </si>
+  <si>
+    <t>VIIDNKRYLFIQKLGEGGFSYVDLVEGLHDGHFYALKRILCHEQQDREEAQREADMHRLFNHPNILRLVAYCLRERGAKHEAWLLLPFFKRGTLWNEIERLKDKGNFLTEDQILWLLLGICRGLEAIHAKGYAHRDLKPTNILLGDEGQPVLMDLGSMNQACIHVEGSRQALTLQDWAAQRCTISYRAPELFSVQSHCVIDERTDVWSLGCVLYAMMFGEGPYDMVFQKGDSVALAVQNQLSIPQSPRHSSALWQLLNSMMTVDPHQRPHIPLLLSQLEALQ</t>
+  </si>
+  <si>
+    <t>MELK_HUMAN_D0_4IXP_A</t>
+  </si>
+  <si>
+    <t>AAGGAGAAGGAGCCCCTGGAGTCGCAGTACCAGGTGGGCCCGCTACTGGGCAGCGGCGGCTTCGGCTCGGTCTACTCAGGCATCCGCGTCTCCGACAACTTGCCGGTGGCCATCAAACACGTGGAGAAGGACCGGATTTCCGACTGGGGAGAGCTGCCTAATGGCACTCGAGTGCCCATGGAAGTGGTCCTGCTGAAGAAGGTGAGCTCGGGTTTCTCCGGCGTCATTAGGCTCCTGGACTGGTTCGAGAGGCCCGACAGTTTCGTCCTGATCCTGGAGAGGCCCGAGCCGGTGCAAGATCTCTTCGACTTCATCACGGAAAGGGGAGCCCTGCAAGAGGAGCTGGCCCGCAGCTTCTTCTGGCAGGTGCTGGAGGCCGTGCGGCACTGCCACAACTGCGGGGTGCTCCACCGCGACATCAAGGACGAAAACATCCTTATCGACCTCAATCGCGGCGAGCTCAAGCTCATCGACTTCGGGTCGGGGGCGCTGCTCAAGGACACCGTCTACACGGACTTCGATGGGACCCGAGTGTATAGCCCTCCAGAGTGGATCCGCTACCATCGCTACCATGGCAGGTCGGCGGCAGTCTGGTCCCTGGGGATCCTGCTGTATGATATGGTGTGTGGAGATATTCCTTTCGAGCATGACGAAGAGATCATCGGGGGCCAGGTTTTCTTCAGGCAGAGGGTCTCTTCAGAATGTCAGCATCTCATTAGATGGTGCTTGGCCCTGAGACCATCAGATAGGCCAACCTTCGAAGAAATCCAGAACCATCCATGGATGCAAGATGTTCTCCTGCCCCAGGAAACTGCTGAGATCCACCTCCACAGCCTGTCGCCGGGGCCCAGCAAA</t>
+  </si>
+  <si>
+    <t>PFPEGKVLDDMEGNQWVLGKKIGSGGFGLIYLAFPTNKPEKDARHVVKVEYQENGPLFSELKFYQRVAKKDCIKKWIERKQLDYLGIPLFYGSGLTEFKGRSYRFMVMERLGIDLQKISGQNGTFKKSTVLQLGIRMLDVLEYIHENEYVHGDIKAANLLLGYKNPDQVYLADYGLSYRYCPNGNHKQYQENPRKGHNGTIEFTSLDAHKGVALSRRSDVEILGYCMLRWLCGKLPWEQNLKDPVAVQTAKTNLLDELPQSVLKWAPSGSSCCEIAQFLVCAHSLAYDEKPNYQALKKILNPHGIPLGPLDFSTKGQSINVH</t>
+  </si>
+  <si>
+    <t>MESDLHQIIHSSQPLTLEHVRYFLYQLLRGLKYMHSAQVIHRDLKPSNLLVNENCELKIGDFGMARGLCTSPAEHQYFMTEYVATRWYRAPELMLSLHEYTQAIDLWSVGCIFGEMLARRQLFPGKNYVHQLQLIMMVLGTPSPAVIQAVGAERVRAYIQSLPPRQPVPWETVYPGADRQALSLLGRMLRFEPSARISAAAALRHPFLAKYHDPDDEPDCAPPFDFAFDREALTRERIKEAIVAEIEDFHARREGIRQQIRFQPSLQPVASEPGCPDVEMPSPWAPSGDCAM</t>
+  </si>
+  <si>
+    <t>EPKKYAVTDDYQLSKQVLGLGVNGKVLECFHRRTGQKCALKLLYDSPKARQEVDHHWQASGGPHIVCILDVYENMHHGKRCLLIIMECMEGGELFSRIQERGDQAFTEREAAEIMRDIGTAIQFLHSHNIAHRDVKPENLLYTSKEKDAVLKLTDFGFAKETTQNALQTPCYTPYYVAPEVLGPEKYDKSCDMWSLGVIMYILLCGFPPFYSNTGQAISPGMKRRIRLGQYGFPNPEWSEVSEDAKQLIRLLLKTDPTERLTITQFMNHPWINQSMVVPQTPLHTARVLQEDKDHWDEVKEEMTSALATMRVDYDQV</t>
+  </si>
+  <si>
+    <t>STK24_HUMAN_D0_3ZHP_C</t>
+  </si>
+  <si>
+    <t>aa_seq</t>
+  </si>
+  <si>
+    <t>KC1D_HUMAN_D0_4HNF_B</t>
+  </si>
+  <si>
+    <t>AGCATTGAGTCATCAGGAAAACTGAAGATCTCCCCTGAACAACACTGGGATTTCACTGCAGAGGACTTGAAAGACCTTGGAGAAATTGGACGAGGAGCTTATGGTTCTGTCAACAAAATGGTCCACAAACCAAGTGGGCAAATAATGGCAGTTAAAAGAATTCGGTCAACAGTGGATGAAAAAGAACAAAAACAACTTCTTATGGATTTGGATGTAGTAATGCGGAGTAGTGATTGCCCATACATTGTTCAGTTTTATGGTGCACTCTTCAGAGAGGGTGACTGTTGGATCTGTATGGAACTCATGTCTACCTCGTTTGATAAGTTTTACAAATATGTATATAGTGTATTAGATGATGTTATTCCAGAAGAAATTTTAGGCAAAATCACTTTAGCAACTGTGAAAGCACTAAACCACTTAAAAGAAAACTTGAAAATTATTCACAGAGATATCAAACCTTCCAATATTCTTCTGGACAGAAGTGGAAATATTAAGCTCTGTGACTTCGGCATCAGTGGACAGCTTGTGGACTCTATTGCCAAGACAAGAGATGCTGGCTGTAGGCCATACATGGCACCTGAAAGAATAGACCCAAGCGCATCACGACAAGGATATGATGTCCGCTCTGATGTCTGGAGTTTGGGGATCACATTGTATGAGTTGGCCACAGGCCGATTTCCTTATCCAAAGTGGAATAGTGTATTTGATCAACTAACACAAGTCGTGAAAGGAGATCCTCCGCAGCTGAGTAATTCTGAGGAAAGGGAATTCTCCCCGAGTTTCATCAACTTTGTCAACTTGTGCCTTACGAAGGATGAATCCAAAAGGCCAAAGTATAAAGAGCTTCTGAAACATCCCTTTATTTTGATGTATGAAGAACGTGCCGTTGAGGTCGCATGCTATGTTTGTAAAATCCTGGATCAAATGCCAGCTACTCCCAGCTCTCCCATGTATGTCGAT</t>
+  </si>
+  <si>
+    <t>AAPK2_HUMAN_D0_2H6D_A</t>
+  </si>
+  <si>
+    <t>CLK3_HUMAN_D0_2WU7_A</t>
+  </si>
+  <si>
+    <t>ATGACCGTGTTCAGGCAGGAAAACGTGGATGATTACTACGACACCGGCGAGGAACTTGGCAGTGGACAGTTTGCGGTTGTGAAGAAATGCCGTGAGAAAAGCACCGGCCTCCAGTATGCCGCCAAATTCATCAAGAAAAGGAGGACTAAGTCCAGCCGGCGGGGTGTGAGCCGCGAGGACATCGAGCGGGAGGTCAGCATCCTGAAGGAGATCCAGCACCCCAATGTCATCACCCTGCACGAGGTCTATGAGAACAAGACGGACGTCATCCTGATCTTGGAACTCGTTGCAGGTGGCGAGCTGTTTGACTTCTTAGCTGAAAAGGAATCTTTAACTGAAGAGGAAGCAACTGAATTTCTCAAACAAACTCTTAATGGTGTTTACTACCTGCACTCCCTTCAAATCGCCCACTTTGATCTTAAGCCTGAGAACATAATGCTTTTGGATAGAAATGTCCCCAAACCTCGGATCAAGATCATTGACTTTGGGTTGGCCCATAAAATTGACTTTGGAAATGAATTTAAAAACATATTTGGGACTCCAGAGTTTGTCGCTCCTGAGATAGTCAACTATGAACCTCTTGGTCTTGAGGCAGATATGTGGAGTATCGGGGTAATAACCTATATCCTCCTAAGTGGGGCCTCCCCATTTCTTGGAGACACTAAGCAAGAAACGTTAGCAAATGTATCCGCTGTCAACTACGAATTTGAGGATGAATACTTCAGTAATACCAGTGCCCTAGCCAAAGATTTCATAAGAAGACTTCTGGTCAAGGATCCAAAGAAGAGAATGACAATTCAAGATAGTTTGCAGCATCCCTGGATCAAGCCTAAAGATACACAACAGGCACTTAGTAGAAAAGCATCAGCAGTAAACATGGAGAAATTCAAGAAGTTTGCAGCCCGGAAAAAATGGAAACAATCCGTTCGCTTGATATCACTGTGCCAAAGATTATCCAGGTCATTCCTGTCCAGAAGTAACATGAGTGTTGCCAGAAGCGAT</t>
+  </si>
+  <si>
+    <t>GAAGCCTTTCTCACCCAGAAAGCCAAGGTCGGCGAACTCAAAGACGATGACTTCGAAAGGATCTCAGAGCTGGGCGCGGGCAACGGCGGGGTGGTCACCAAAGTCCAGCACAGACCCTCGGGCCTCATCATGGCCAGGAAGCTGATCCACCTTGAGATCAAGCCGGCCATCCGGAACCAGATCATCCGCGAGCTGCAGGTCCTGCACGAATGCAACTCGCCGTACATCGTGGGCTTCTACGGGGCCTTCTACAGTGACGGGGAGATCAGCATTTGCATGGAACACATGGACGGCGGCTCCCTGGACCAGGTGCTGAAAGAGGCCAAGAGGATTCCCGAGGAGATCCTGGGGAAAGTCAGCATCGCGGTTCTCCGGGGCTTGGCGTACCTCCGAGAGAAGCACCAGATCATGCACCGAGATGTGAAGCCCTCCAACATCCTCGTGAACTCTAGAGGGGAGATCAAGCTGTGTGACTTCGGGGTGAGCGGCCAGCTCATAGACTCCATGGCCAACTCCTTCGTGGGCACGCGCTCCTACATGGCTCCGGAGCGGTTGCAGGGCACACATTACTCGGTGCAGTCGGACATCTGGAGCATGGGCCTGTCCCTGGTGGAGCTGGCCGTCGGAAGGTACCCCATCCCCCCGCCCGACGCCAAAGAGCTGGAGGCCATCTTTGGCCGGCCCGTGGTCGACGGGGAAGAAGGAGAGCCTCACAGCATCTCGCCTCGGCCGAGGCCCCCCGGGCGCCCCGTCAGCGGTCACGGGATGGATAGCCGGCCTGCCATGGCCATCTTTGAACTCCTGGACTATATTGTGAACGAGCCACCTCCTAAGCTGCCCAACGGTGTGTTCACCCCCGACTTCCAGGAGTTTGTCAATAAATGCCTCATCAAGAACCCAGCGGAGCGGGCGGACCTGAAGATGCTCACAAACCACACCTTCATCAAGCGGTCCGAGGTGGAAGAAGTGGATTTTGCCGGCTGGTTGTGTAAAACCCTGCGGCTGAACCAGCCCGGCACACCCACGCGCACCGCCGTG</t>
+  </si>
+  <si>
+    <t>MKNK2_HUMAN_D0_2AC3_A</t>
   </si>
   <si>
     <t>NEK7_HUMAN_D0_2WQN_A</t>
   </si>
   <si>
-    <t>GGGCCGGAGGATGAGCTGCCCGACTGGGCCGCCGCCAAAGAGTTTTACCAGAAGTACGACCCTAAGGACGTCATCGGCAGAGGAGTGAGCTCTGTGGTCCGCCGTTGTGTTCATCGAGCTACTGGCCACGAGTTTGCGGTGAAGATTATGGAAGTGACAGCTGAGCGGCTGAGTCCTGAGCAGCTGGAGGAGGTGCGGGAAGCCACACGGCGAGAGACACACATCCTTCGCCAGGTCGCCGGCCACCCCCACATCATCACCCTCATCGATTCCTACGAGTCTTCTAGCTTCATGTTCCTGGTGTTTGACCTGATGCGGAAGGGAGAGCTGTTTGACTATCTCACAGAGAAGGTGGCCCTCTCTGAAAAGGAAACCAGGTCCATCATGCGGTCTCTGCTGGAAGCAGTGAGCTTTCTCCATGCCAACAACATTGTGCATCGAGATCTGAAGCCCGAGAATATTCTCCTAGATGACAATATGCAGATCCGACTTTCAGATTTCGGGTTCTCCTGCCACTTGGAACCTGGCGAGAAGCTTCGAGAGTTGTGTGGGACCCCAGGGTATCTAGCGCCAGAGATCCTTAAATGCTCCATGGATGAAACCCACCCAGGCTATGGCAAGGAGGTCGACCTCTGGGCCTGTGGGGTGATCTTGTTCACACTCCTGGCTGGCTCGCCACCCTTCTGGCACCGGCGGCAGATCCTGATGTTACGCATGATCATGGAGGGCCAGTACCAGTTCAGTTCCCCCGAGTGGGATGACCGTTCCAGCACTGTCAAAGACCTGATCTCCAGGCTGCTGCAGGTGGATCCTGAGGCACGCCTGACAGCTGAGCAGGCCCTACAGCACCCCTTCTTTGAGCGT</t>
-  </si>
-  <si>
-    <t>KC1E_HUMAN_D0_4HNI_A</t>
-  </si>
-  <si>
-    <t>VRK2_HUMAN_D0_2V62_B</t>
-  </si>
-  <si>
-    <t>ETYIKLDKLGEGTYATVYKGKSKLTDNLVALKEIRLEHEEGAPCTAIREVSLLKDLKHANIVTLHDIIHTEKSLTLVFEYLDKDLKQYLDDCGNIINMHNVKLFLFQLLRGLAYCHRQKVLHRDLKPQNLLINERGELKLADFGLARAKSIPTKTYSNEVVTLWYRPPDILLGSTDYSTQIDMWGVGCIFYEMATGRPLFPGSTVEEQLHFIFRILGTPTEETWPGILSNEEFKTYNYPKYRAEALLSHAPRLDSDGADLLTKLLQFEGRNRISAEDAMKHPFFLSLGERIHKLPDTTSIFALKEIQLQKEASLRS</t>
-  </si>
-  <si>
-    <t>HQLQPRRVSFRGEASETLQSPGYDPSRPESFFQQSFQRLSRLGHGSYGEVFKVRSKEDGRLYAVKRSMSPFRGPKDRARKLAEVGSHEKVGQHPCCVRLEQAWEEGGILYLQTELCGPSLQQHCEAWGASLPEAQVWGYLRDTLLALAHLHSQGLVHLDVKPANIFLGPRGRCKLGDFGLLVELGTAGAGEVQEGDPRYMAPELLQGSYGTAADVFSLGLTILEVACNMELPHGGEGWQQLRQGYLPPEFTAGLSSELRSVLVMMLEPDPKLRATAEALLALPVLRQP</t>
-  </si>
-  <si>
-    <t>aa_end</t>
-  </si>
-  <si>
-    <t>PMYT1_HUMAN_D0_3P1A_A</t>
-  </si>
-  <si>
-    <t>MK08_HUMAN_D0_2NO3_A</t>
-  </si>
-  <si>
-    <t>TCGGTTAAAGGAAGAATTTATTCCATATTAAAGCAGATAGGAAGTGGAGGTTCAAGCAAGGTATTTCAGGTGTTAAATGAAAAGAAACAGATATATGCTATAAAATATGTGAACTTAGAAGAAGCAGATAACCAAACTCTTGATAGTTACCGGAACGAAATAGCTTATTTGAATAAACTACAACAACACAGTGATAAGATCATCCGACTTTATGATTATGAAATCACGGACCAGTACATCTACATGGTAATGGAGTGTGGAAATATTGATCTTAATAGTTGGCTTAAAAAGAAAAAATCCATTGATCCATGGGAACGCAAGAGTTACTGGAAAAATATGTTAGAGGCAGTTCACACAATCCATCAACATGGCATTGTTCACAGTGATCTTAAACCAGCTAACTTTCTGATAGTTGATGGAATGCTAAAGCTAATTGATTTTGGGATTGCAAACCAAATGCAACCAGATACAACAAGTGTTGTTAAAGATTCTCAGGTTGGCACAGTTAATTATATGCCACCAGAAGCAATCAAAGATATGTCTTCCTCCAGAGAGAATGGGAAATCTAAGTCAAAGATAAGCCCCAAAAGTGATGTTTGGTCCTTAGGATGTATTTTGTACTATATGACTTACGGGAAAACACCATTTCAGCAGATAATTAATCAGATTTCTAAATTACATGCCATAATTGATCCTAATCATGAAATTGAATTTCCCGATATTCCAGAGAAAGATCTTCAAGATGTGTTAAAGTGTTGTTTAAAAAGGGACCCAAAACAGAGGATATCCATTCCTGAGCTCCTGGCTCATCCATATGTTCAAATTCAAACTCATCCAGTTAACCAAATGGCCAAGGGAACCACTGAAGAA</t>
-  </si>
-  <si>
-    <t>PAK1_HUMAN_D0_3Q52_A</t>
-  </si>
-  <si>
-    <t>CACCACCATCACCACCATTCGCACTCGGGGCCGGAGATCTCGCGGATTATCGTCGACCCCACGACTGGGAAGCGCTACTGCCGGGGCAAAGTGCTGGGAAAGGGTGGCTTTGCAAAATGTTACGAGATGACAGATTTGACAAATAACAAAGTCTACGCCGCAAAAATTATTCCTCACAGCAGAGTAGCTAAACCTCATCAAAGGGAAAAGATTGACAAAGAAATAGAGCTTCACAGAATTCTTCATCATAAGCATGTAGTGCAGTTTTACCACTACTTCGAGGACAAAGAAAACATTTACATTCTCTTGGAATACTGCAGTAGAAGGTCAATGGCTCATATTTTGAAAGCAAGAAAGGTGTTGACAGAGCCAGAAGTTCGATACTACCTCAGGCAGATTGTGTCTGGACTGAAATACCTTCATGAACAAGAAATCTTGCACAGAGATCTCAAACTAGGGAACTTTTTTATTAATGAAGCCATGGAACTAAAAGTTGGGGACTTCGGTCTGGCAGCCAGGCTAGAACCCTTGGAACACAGAAGGAGAACGATATGTGGTACCCCAAATTATCTCTCTCCTGAAGTCCTCAACAAACAAGGACATGGCTGTGAATCAGACATTTGGGCCCTGGGCTGTGTAATGTATACAATGTTACTAGGGAGGCCCCCATTTGAAACTACAAATCTCAAAGAAACTTATAGGTGCATAAGGGAAGCAAGGTATACAATGCCGTCCTCATTGCTGGCTCCTGCCAAGCACTTAATTGCTAGTATGTTGTCCAAAAACCCAGAGGATCGTCCCAGTTTGGATGACATCATTCGACATGACTTTTTTTTGCAGGGCTTCACTCCGGACAGACTGTCTTCTAGCTGTTGTCATACAGTTCCAGATTTCCACTTATCAAGCCCAGCT</t>
-  </si>
-  <si>
-    <t>GAAACAAAGTATACTGTGGACAAGAGGTTTGGCATGGATTTTAAAGAAATAGAATTAATTGGCTCAGGTGGATTTGGCCAAGTTTTCAAAGCAAAACACAGAATTGACGGAAAGACTTACGTTATTAAACGTGTTAAATATAATAACGAGAAGGCGGAGCGTGAAGTAAAAGCATTGGCAAAACTTGATCATGTAAATATTGTTCACTACAATGGCTGTTGGGATGGATTTGATTATGATCCTGAGACCAGTGATGATTCTCTTGAGAGCAGTGATTATGATCCTGAGAACAGCAAAAATAGTTCAAGGTCAAAGACTAAGTGCCTTTTCATCCAAATGGAATTCTGTGATAAAGGGACCTTGGAACAATGGATTGAAAAAAGAAGAGGCGAGAAACTAGACAAAGTTTTGGCTTTGGAACTCTTTGAACAAATAACAAAAGGGGTGGATTATATACATTCAAAAAAATTAATTCATAGAGATCTTAAGCCAAGTAATATATTCTTAGTAGATACAAAACAAGTAAAGATTGGAGACTTTGGACTTGTAACATCTCTGAAAAATGATGGAAAGCGAACAAGGAGTAAGGGAACTTTGCGATACATGAGCCCAGAACAGATTTCTTCGCAAGACTATGGAAAGGAAGTGGACCTCTACGCTTTGGGGCTAATTCTTGCTGAACTTCTTCATGTATGTGACACTGCTTTTGAAACATCAAAGTTTTTCACAGACCTACGGGATGGCATCATCTCAGATATATTTGATAAAAAAGAAAAAACTCTTCTACAGAAATTACTCTCAAAGAAACCTGAGGATCGACCTAACACATCTGAAATACTAAGGACCTTGACTGTGTGGAAGAAAAGCCCAGAGAAAAATGAACGACACACATGT</t>
-  </si>
-  <si>
-    <t>PAK7_HUMAN_D0_2F57_B</t>
-  </si>
-  <si>
-    <t>expression tag location</t>
-  </si>
-  <si>
-    <t>GAGAACTTCCAAAAGGTGGAAAAGATCGGAGAGGGCACGTACGGAGTTGTGTACAAAGCCAGAAACAAGTTGACGGGAGAGGTGGTGGCGCTTAAGAAAATCCGCCTGGACACTGAGACTGAGGGTGTGCCCAGTACTGCCATCCGAGAGATCTCTCTGCTTAAGGAGCTTAACCATCCTAATATTGTCAAGCTGCTGGATGTCATTCACACAGAAAATAAACTCTACCTGGTTTTTGAATTTCTGCACCAAGATCTCAAGAAATTCATGGATGCCTCTGCTCTCACTGGCATTCCTCTTCCCCTCATCAAGAGCTATCTGTTCCAGCTGCTCCAGGGCCTAGCTTTCTGCCATTCTCATCGGGTCCTCCACCGAGACCTTAAACCTCAGAATCTGCTTATTAACACAGAGGGGGCCATCAAGCTAGCAGACTTTGGACTAGCCAGAGCTTTTGGAGTCCCTGTTCGTACTTACACCCATGAGGTGGTGACCCTGTGGTACCGAGCTCCTGAAATCCTCCTGGGCTGCAAATATTATTCCACAGCTGTGGACATCTGGAGCCTGGGCTGCATCTTTGCTGAGATGGTGACTCGCCGGGCCCTATTCCCTGGAGATTCTGAGATTGACCAGCTCTTCCGGATCTTTCGGACTCTGGGGACCCCAGATGAGGTGGTGTGGCCAGGAGTTACTTCTATGCCTGATTACAAGCCAAGTTTCCCCAAGTGGGCCCGGCAAGATTTTAGTAAAGTTGTACCTCCCCTGGATGAAGATGGACGGAGCTTGTTATCGCAAATGCTGCACTACGACCCTAACAAGCGGATTTCGGCCAAGGCAGCCCTGGCTCACCCTTTCTTCCAGGATGTGACCAAGCCAGTACCCCATCTT</t>
-  </si>
-  <si>
-    <t>GGGGAATGCAGTCAGAAGGGTCCTGTCCCCTTTAGCCATTGCCTTCCCACAGAAAAACTGCAACGCTGTGAGAAGATTGGGGAAGGGGTGTTTGGCGAAGTGTTTCAAACAATTGCTGATCACACACCCGTAGCCATAAAAATCATTGCTATTGAAGGACCAGATTTAGTCAATGGATCCCATCAGAAAACCTTTGAGGAAATCCTGCCAGAGATCATCATCTCCAAAGAGTTGAGCCTCTTATCCGGTGAAGTGTGCAACCGCACAGAAGGCTTTATCGGGCTGAACTCAGTGCACTGTGTCCAGGGATCTTACCCTCCCTTGCTCCTCAAAGCCTGGGATCACTATAATTCAACCAAAGGCTCTGCAAATGACCGGCCTGATTTTTTTAAAGACGACCAGCTCTTCATTGTGCTGGAATTTGAGTTTGGAGGGATTGACTTAGAGCAAATGCGAACCAAGTTGTCTTCCTTGGCTACTGCAAAGAGCATTCTACACCAGCTCACAGCCTCCCTCGCAGTGGCAGAGGCATCACTGCGCTTTGAGCACCGAGACTTACACTGGGGGAACGTGCTCTTAAAGAAAACCAGCCTCAAAAAACTCCACTACACCCTCAATGGGAAGAGCAGCACTATCCCCAGCTGTGGGTTGCAAGTGAGCATCATTGACTACACCCTGTCGCGCTTGGAACGGGATGGGATTGTGGTTTTCTGTGACGTTTCCATGGATGAGGACCTGTTTACCGGTGACGGTGACTACCAGTTTGACATCTACAGGCTCATGAAGAAGGAGAATAACAACCGCTGGGGTGAATATCACCCTTATAGTAATGTGCTCTGGTTACATTACCTGACAGACAAGATGCTGAAACAAATGACCTTCAAGACTAAATGTAACACTCCTGCCATGAAGCAAATTAAGAGAAAAATCCAGGAGTTCCACAGGACAATGCTGAACTTCAGCTCTGCCACTGACTTGCTCTGCCAGCACAGACTGTTTAAG</t>
-  </si>
-  <si>
-    <t>TDSLPGKFEDMYKLTSELLGEGAYAKVQGAVSLQNGKEYAVKIIEKQAGHSRSRVFREVETLYQCQGNKNILELIEFFEDDTRFYLVFEKLQGGSILAHIQKQKHFNEREASRVVRDVAAALDFLHTKDKVSLCHLGGSARAPSGLTAAPTSLGSSDPPTSASQVAGTTGIDHRDLKPENILCESPEKVSPVKICDFDLGSGMKLNNSCTPITTPELTTPCGSAEYMAPEVGEVFTDQATFYDKRCDLWSLGVVLYIMLSGYPPFVGHCGADCGWDRGEVCRVCQNKLFESIQEGKYEFPDKDWAHISSEAKDLISKLLVRDAKQRLSAAQVLQHPWVQGQAPEKG</t>
-  </si>
-  <si>
-    <t>DAPK1_HUMAN_D0_4B4L_A</t>
-  </si>
-  <si>
-    <t>EDSLTKQPEEVFDVLEKLGEGSYGSVFKAIHKESGQVVAIKQVPVESDLQEIIKEISIMQQCDSPYVVKYYGSYFKNTDLWIVMEYCGAGSVSDIIRLRNKTLIEDEIATILKSTLKGLEYLHFMRKIHRDIKAGNILLNTEGHAKLADFGVAGQLTDTMAKRNTVIGTPFWMAPEVIQEIGYNCVADIWSLGITSIEMAEGKPPYADIHPMRAIFMIPTNPPPTFRKPELWSDDFTDFVKKCLVKNPEQRATATQLLQHPFIKNAKPVSILRDLITEAMEIKAKRHEEQQRELEEEE</t>
-  </si>
-  <si>
-    <t>ATGAGCCTCATCCGGAAAAAGGGCTTCTACAAGCAGGACGTCAACAAGACCGCCTGGGAGCTGCCCAAGACCTACGTGTCCCCGACGCACGTCGGCAGCGGGGCCTATGGCTCCGTGTGCTCGGCCATCGACAAGCGGTCAGGGGAGAAGGTGGCCATCAAGAAGCTGAGCCGACCCTTTCAGTCCGAGATCTTCGCCAAGCGCGCCTACCGGGAGCTGCTGCTGCTGAAGCACATGCAGCATGAGAACGTCATTGGGCTCCTGGATGTCTTCACCCCAGCCTCCTCCCTGCGCAACTTCTATGACTTCTACCTGGTGATGCCCTTCATGCAGACGGATCTGCAGAAGATCATGGGGATGGAGTTCAGTGAGGAGAAGATCCAGTACCTGGTGTATCAGATGCTCAAAGGCCTTAAGTACATCCACTCTGCTGGGGTCGTGCACAGGGACCTGAAGCCAGGCAACCTGGCTGTGAATGAGGACTGTGAACTGAAGATTCTGGATTTTGGGCTGGCGCGACATGCAGACGCCGAGATGACTGGCTACGTGGTGACCCGCTGGTACCGAGCCCCCGAGGTGATCCTCAGCTGGATGCACTACAACCAGACAGTGGACATCTGGTCTGTGGTCTGTATCATGGCAGAGATGCTGACAGGGAAAACTCTGTTCAAGGGGAAAGATTACCTGGACCAGCTGACCCAGATCCTGAAAGTGACCGGGGTGCCTGGCACGGAGTTTGTGCAGAAGCTGAACGACAAAGCGGCCAAATCCTACATCCAGTCCCTGCCACAGACCCCCAGGAAGGATTTCACTCAGCTGTTCCCACGGGCCAGCCCCCAGGCTGCGGACCTGCTGGAGAAGATGCTGGAGCTAGACGTGGACAAGCGCCTGACGGCCGCGCAGGCCCTCACCCATCCCTTCTTTGAACCCTTCCGGGACCCTGAGGAAGAGACGGAGGCCCAGCAGCCGTTTGATGATTCCTTAGAACACGAGAAACTCACAGTGGATGAATGGAAGCAGCACATCTACAAGGAGATTGTGAACTTCAGCCCCATT</t>
-  </si>
-  <si>
-    <t>ATGAAAGATTATGATGAACTTCTCAAATATTATGAATTACATGAAACTATTGGGACAGGTGGCTTTGCAAAGGTCAAACTTGCCTGCCATATCCTTACTGGAGAGATGGTAGCTATAAAAATCATGGATAAAAACACACTAGGGAGTGATTTGCCCCGGATCAAAACGGAGATTGAGGCCTTGAAGAACCTGAGACATCAGCATATATGTCAACTCTACCATGTGCTAGAGACAGCCAACAAAATATTCATGGTTCTTGAGTACTGCCCTGGAGGAGAGCTGTTTGACTATATAATTTCCCAGGATCGCCTGTCAGAAGAGGAGACCCGGGTTGTCTTCCGTCAGATAGTATCTGCTGTTGCTTATGTGCACAGCCAGGGCTATGCTCACAGGGACCTCAAGCCAGAAAATTTGCTGTTTGATGAATATCATAAATTAAAGCTGATTGACTTTGGTCTCTGTGCAAAACCCAAGGGTAACAAGGATTACCATCTACAGACATGCTGTGGGAGTCTGGCTTATGCAGCACCTGAGTTAATACAAGGCAAATCATATCTTGGATCAGAGGCAGATGTTTGGAGCATGGGCATACTGTTATATGTTCTTATGTGTGGATTTCTACCATTTGATGATGATAATGTAATGGCTTTATACAAGAAGATTATGAGAGGAAAATATGATGTTCCCAAGTGGCTCTCTCCCAGTAGCATTCTGCTTCTTCAACAAATGCTGCAGGTGGACCCAAAGAAACGGATTTCTATGAAAAATCTATTGAACCATCCCTGGATCATGCAAGATTACAACTATCCTGTTGAGTGGCAAAGCAAGAATCCTTTTATTCACCTCGATGATGATTGCGTAACAGAACTTTCTGTACATCACAGAAACAACAGGCAAACAATGGAGGATTTAATTTCACTGTGGCAGTATGATCACCTCACGGCTACCTATCTTCTGCTTCTAGCCAAGAAGGCTCGGGGAAAACCAGTTCGTTTAAGGCTTTCTTCTTTCTCCTGTGGA</t>
-  </si>
-  <si>
-    <t>ATGGAGGCAGCAGCATCCGAACCCTCTCTTGATCTAGATAATCTGAAACTGTTGGAGCTGATTGGCCGAGGTCGATATGGAGCAGTATATAAAGGCTCCTTGGATGAGCGTCCAGTTGCTGTAAAAGTGTTTTCCTTTGCAAACCGTCAGAATTTTATCAACGAAAAGAACATTTACAGAGTGCCTTTGATGGAACATGACAACATTGCCCGCTTTATAGTTGGAGATGAGAGAGTCACTGCAGATGGACGCATGGAATATTTGCTTGTGATGGAGTACTATCCCAATGGATCTTTATGCAAGTATTTAAGTCTCCACACAAGTGACTGGGTAAGCTCTTGCCGTCTTGCTCATTCTGTTACTAGAGGACTGGCTTATCTTCACACAGAATTACCACGAGGAGATCATTATAAACCTGCAATTTCCCATCGAGATTTAAACAGCAGAAATGTCCTAGTGAAAAATGATGGAACCTGTGTTATTAGTGACTTTGGACTGTCCATGAGGCTGACTGGAAATAGACTGGTGCGCCCAGGGGAGGAAGATAATGCAGCCATAAGCGAGGTTGGCACTATCAGATATATGGCACCAGAAGTGCTAGAAGGAGCTGTGAACTTGAGGGACTGTGAATCAGCTTTGAAACAAGTAGACATGTATGCTCTTGGACTAATCTATTGGGAGATATTTATGAGATGTACAGACCTCTTCCCAGGGGAATCCGTACCAGAGTACCAGATGGCTTTTCAGACAGAGGTTGGAAACCATCCCACTTTTGAGGATATGCAGGTTCTCGTGTCTAGGGAAAAACAGAGACCCAAGTTCCCAGAAGCCTGGAAAGAAAATAGCCTGGCAGTGAGGTCACTCAAGGAGACAATCGAAGACTGTTGGGACCAGGATGCAGAGGCTCGGCTTACTGCACAGTGTGCTGAGGAAAGGATGGCTGAACTTATGATGATTTGGGAAAGAAACAAATCTGTGAGCCCAACA</t>
-  </si>
-  <si>
-    <t>PAK4_HUMAN_D0_2J0I_A</t>
-  </si>
-  <si>
-    <t>AGVSEYELPEDPRWELPRDRLVLGKPLGEGCFGQVVLAEAIGLDKDKPNRVTKVAVKMLKSDATEKDLSDLISEMEMMKMIGKHKNIINLLGACTQDGPLYVIVEYASKGNLREYLQARRPPGLEYCYNPSHNPEEQLSSKDLVSCAYQVARGMEYLASKKCIHRDLAARNVLVTEDNVMKIADFGLARDIHHIDYYKKTTNGRLPVKWMAPEALFDRIYTHQSDVWSFGVLLWEIFTLGGSPYPGVPVEELFKLLKEGHRMDKPSNCTNELYMMMRDCWHAVPSQRPTFKQLVEDLDRIVALTSNQEYLDLSMPLD</t>
-  </si>
-  <si>
-    <t>MAAAAAQGGGGGEPRRTEGVGPGVPGEVEMVKGQPFDVGPRYTQLQYIGEGAYGMVSSAYDHVRKTRVAIKKISPFEHQTYCQRTLREIQILLRFRHENVIGIRDILRASTLEAMRDVYIVQDLMETDLYKLLKSQQLSNDHICYFLYQILRGLKYIHSANVLHRDLKPSNLLINTTCDLKICDFGLARIADPEHDHTGFLTEYVATRWYRAPEIMLNSKGYTKSIDIWSVGCILAEMLSNRPIFPGKHYLDQLNHILGILGSPSQEDLNCIINMKARNYLQSLPSKTKVAWAKLFPKSDSKALDLLDRMLTFNPNKRITVEEALAHPYLEQYYDPTDEPVAEEPFTFAMELDDLPKERLKELIFQETARFQPGVLEAP</t>
-  </si>
-  <si>
-    <t>GAGCCCAAGAAGTACGCAGTGACCGACGACTACCAGTTGTCCAAGCAGGTGCTGGGCCTGGGTGTGAACGGCAAAGTGCTGGAGTGCTTCCATCGGCGCACTGGACAGAAGTGTGCCCTGAAGCTCCTGTATGACAGCCCCAAGGCCCGGCAGGAGGTAGACCATCACTGGCAGGCTTCTGGCGGCCCCCATATTGTCTGCATCCTGGATGTGTATGAGAACATGCACCATGGCAAGCGCTGTCTCCTCATCATCATGGAATGCATGGAAGGTGGTGAGTTGTTCAGCAGGATTCAGGAGCGTGGCGACCAGGCTTTCACTGAGAGAGAAGCTGCAGAGATAATGCGGGATATTGGCACTGCCATCCAGTTTCTGCACAGCCATAACATTGCCCACCGAGATGTCAAGCCTGAAAACCTACTCTACACATCTAAGGAGAAAGACGCAGTGCTTAAGCTCACCGATTTTGGCTTTGCTAAGGAGACCACCCAAAATGCCCTGCAGACACCCTGCTATACTCCCTATTATGTGGCCCCTGAGGTCCTGGGTCCAGAGAAGTATGACAAGTCATGTGACATGTGGTCCCTGGGTGTCATCATGTACATCCTCCTTTGTGGCTTCCCACCCTTCTACTCCAACACGGGCCAGGCCATCTCCCCGGGGATGAAGAGGAGGATTCGCCTGGGCCAGTACGGCTTCCCCAATCCTGAGTGGTCAGAAGTCTCTGAGGATGCCAAGCAGCTGATCCGCCTCCTGTTGAAGACAGACCCCACAGAGAGGCTGACCATCACTCAGTTCATGAACCACCCCTGGATCAACCAATCGATGGTAGTGCCACAGACCCCACTCCACACGGCCCGAGTGCTGCAGGAGGACAAAGACCACTGGGACGAAGTCAAGGAGGAGATGACCAGTGCCTTGGCCACTATGCGGGTAGACTACGACCAGGTG</t>
-  </si>
-  <si>
-    <t>ATGTCTCAGGAGAGGCCCACGTTCTACCGGCAGGAGCTGAACAAGACAATCTGGGAGGTGCCCGAGCGTTACCAGAACCTGTCTCCAGTGGGCTCTGGCGCCTATGGCTCTGTGTGTGCTGCTTTTGACACAAAAACGGGGTTACGTGTGGCAGTGAAGAAGCTCTCCAGACCATTTCAGTCCATCATTCATGCGAAAAGAACCTACAGAGAACTGCGGTTACTTAAACATATGAAACATGAAAATGTGATTGGTCTGTTGGACGTTTTTACACCTGCAAGGTCTCTGGAGGAATTCAATGATGTGTATCTGGTGACCCATCTCATGGGGGCAGATCTGAACAACATTGTGAAATGTCAGAAGCTTACAGATGACCATGTTCAGTTCCTTATCTACCAAATTCTCCGAGGTCTAAAGTATATACATTCAGCTGACATAATTCACAGGGACCTAAAACCTAGTAATCTAGCTGTGAATGAAGACTGTGAGCTGAAGATTCTGGATTTTGGACTGGCTCGGCACACAGATGATGAAATGACAGGCTACGTGGCCACTAGGTGGTACAGGGCTCCTGAGATCATGCTGAACTGGATGCATTACAACCAGACAGTTGATATTTGGTCAGTGGGATGCATAATGGCCGAGCTGTTGACTGGAAGAACATTGTTTCCTGGTACAGACCATATTGATCAGTTGAAGCTCATTTTAAGACTCGTTGGAACCCCAGGGGCTGAGCTTTTGAAGAAAATCTCCTCAGAGTCTGCAAGAAACTATATTCAGTCTTTGACTCAGATGCCGAAGATGAACTTTGCGAATGTATTTATTGGTGCCAATCCCCTGGCTGTCGACTTGCTGGAGAAGATGCTTGTATTGGACTCAGATAAGAGAATTACAGCGGCCCAAGCCCTTGCACATGCCTACTTTGCTCAGTACCACGATCCTGATGATGAACCAGTGGCCGATCCTTATGATCAGTCCTTTGAAAGCAGGGACCTCCTTATAGATGAGTGGAAAAGCCTGACCTATGATGAAGTCATCAGCTTTGTGCCACCACCCCTTGACCAAGAAGAGATGGAGTCC</t>
-  </si>
-  <si>
-    <t>MK11_HUMAN_D0_3GC8_A</t>
-  </si>
-  <si>
-    <t>VRK3_HUMAN_D0_2JII_A</t>
-  </si>
-  <si>
-    <t>MK14_HUMAN_D0_3K3J_A</t>
-  </si>
-  <si>
-    <t>CDK16_HUMAN_D0_3MTL_A</t>
-  </si>
-  <si>
-    <t>GCTGATCCAGAAGAACTGTTCACAAAATTAGAGCGCATTGGGAAAGGCTCATTTGGGGAAGTTTTCAAAGGAATTGATAACCGTACCCAGCAAGTCGTTGCTATTAAAATCATAGACCTTGAGGAAGCCGAAGATGAAATAGAAGACATTCAGCAAGAAATAACTGTCTTGAGTCAATGTGACAGCTCATATGTAACAAAATACTATGGGTCATATTTAAAGGGGTCTAAATTATGGATAATAATGGAATACCTGGGCGGTGGTTCAGCACTGGATCTTCTTCGAGCTGGTCCATTTGATGAGTTCCAGATTGCTACCATGCTAAAGGAAATTTTAAAAGGTCTGGACTATCTGCATTCAGAAAAGAAAATTCACCGAGACATAAAAGCTGCCAATGTCTTGCTCTCAGAACAAGGAGATGTTAAACTTGCTGATTTTGGAGTTGCTGGTCAGCTGACAGATACACAGATTAAAAGAAATACCTTTGTGGGAACTCCATTTTGGATGGCTCCTGAAGTTATTCAACAGTCAGCTTATGACTCAAAAGCTGACATTTGGTCATTGGGAATTACTGCTATTGAACTAGCCAAGGGAGAGCCACCTAACTCCGATATGCATCCAATGAGAGTTCTGTTTCTTATTCCCAAAAACAATCCTCCAACTCTTGTTGGAGACTTTACTAAGTCTTTTAAGGAGTTTATTGATGCTTGCCTGAACAAAGATCCATCATTTCGTCCTACAGCAAAAGAACTTCTGAAACACAAATTCATTGTAAAAAATTCAAAGAAGACTTCTTATCTGACTGAACTGATAGATCGTTTTAAGAGATGGAAGGCAGAA</t>
-  </si>
-  <si>
-    <t>BRAF_HUMAN_D0_4JVG_D</t>
-  </si>
-  <si>
-    <t>PAK6_HUMAN_D0_2C30_A</t>
-  </si>
-  <si>
-    <t>FGFR1_HUMAN_D0_3GQL_B</t>
-  </si>
-  <si>
-    <t>TCTTCGGTCACCGCCAGTGCGGCCCCGGGGACCGCGAGCCTCGTCCCGGATTACTGGATCGACGGCTCCAACAGGGATGCGCTGAGCGATTTCTTCGAGGTGGAGTCGGAGCTGGGACGGGGTGCTACATCCATTGTGTACAGATGCAAACAGAAGGGGACCCAGAAGCCTTATGCTCTCAAAGTGTTAAAGAAAACAGTGGACAAAAAAATCGTAAGAACTGAGATAGGAGTTCTTCTTCGCCTCTCACATCCAAACATTATAAAACTTAAAGAGATATTTGAAACCCCTACAGAAATCAGTCTGGTCCTAGAACTCGTCACAGGAGGAGAACTGTTTGATAGGATTGTGGAAAAGGGATATTACAGTGAGCGAGATGCTGCAGATGCCGTTAAACAAATCCTGGAGGCAGTTGCTTATCTACATGAAAATGGGATTGTCCATCGTGATCTCAAACCAGAGAATCTTCTTTATGCAACTCCAGCCCCAGATGCACCACTCAAAATCGCTGATTTTGGACTCTCTAAAATTGTGGAACATCAAGTGCTCATGAAGACAGTATGTGGAACCCCAGGGTACTGCGCACCTGAAATTCTTAGAGGTTGTGCCTATGGACCTGAGGTGGACATGTGGTCTGTAGGAATAATCACCTACATCTTACTTTGTGGATTTGAACCATTCTATGATGAAAGAGGCGATCAGTTCATGTTCAGGAGAATTCTGAATTGTGAATATTACTTTATCTCCCCCTGGTGGGATGAAGTATCTCTAAATGCCAAGGACTTGGTCAGAAAATTAATTGTTTTGGATCCAAAGAAACGGCTGACTACATTTCAAGCTCTCCAGCATCCGTGGGTCACAGGTAAAGCAGCCAATTTTGTACACATGGATACCGCTCAAAAGAAGCTCCAAGAATTCAATGCCCGGCGTAAGCTTAAGGCAGCGGTGAAGGCTGTGGTGGCCTCTTCCCGCCTGGGA</t>
-  </si>
-  <si>
-    <t>EAFLTQKAKVGELKDDDFERISELGAGNGGVVTKVQHRPSGLIMARKLIHLEIKPAIRNQIIRELQVLHECNSPYIVGFYGAFYSDGEISICMEHMDGGSLDQVLKEAKRIPEEILGKVSIAVLRGLAYLREKHQIMHRDVKPSNILVNSRGEIKLCDFGVSGQLIDSMANSFVGTRSYMAPERLQGTHYSVQSDIWSMGLSLVELAVGRYPIPPPDAKELEAIFGRPVVDGEEGEPHSISPRPRPPGRPVSGHGMDSRPAMAIFELLDYIVNEPPPKLPNGVFTPDFQEFVNKCLIKNPAERADLKMLTNHTFIKRSEVEEVDFAGWLCKTLRLNQPGTPTRTAV</t>
-  </si>
-  <si>
-    <t>GTCATCATTGACAATAAGCGCTACCTCTTCATCCAGAAACTGGGGGAGGGTGGGTTCAGCTATGTGGACCTAGTGGAAGGGTTACATGATGGACACTTCTACGCCCTGAAGCGAATCCTGTGTCACGAGCAGCAGGACCGGGAGGAGGCCCAGCGAGAAGCCGACATGCATCGCCTCTTCAATCACCCCAACATCCTTCGCCTCGTGGCTTACTGTCTGAGGGAACGGGGTGCTAAGCATGAGGCCTGGCTGCTGCTACCATTCTTCAAGAGAGGTACGCTGTGGAATGAGATAGAAAGGCTGAAGGACAAAGGCAACTTCCTGACCGAGGATCAAATCCTTTGGCTGCTGCTGGGGATCTGCAGAGGCCTTGAGGCCATTCATGCCAAGGGTTATGCCCACAGAGACTTGAAGCCCACCAATATATTGCTTGGAGATGAGGGGCAGCCAGTTTTAATGGACTTGGGTTCCATGAATCAAGCATGCATCCATGTGGAGGGCTCCCGCCAGGCTCTGACCCTGCAGGACTGGGCAGCCCAGCGGTGCACCATCTCCTACCGAGCCCCAGAGCTCTTCTCTGTGCAGAGTCACTGTGTCATCGATGAGCGGACTGATGTCTGGTCCCTAGGCTGCGTGCTATATGCCATGATGTTTGGGGAAGGCCCTTATGACATGGTGTTCCAAAAGGGTGACAGTGTGGCCCTTGCTGTGCAGAACCAACTCAGCATCCCACAAAGCCCCAGGCATTCTTCAGCATTGTGGCAGCTCCTGAACTCGATGATGACCGTGGACCCGCATCAGCGTCCTCACATTCCTCTCCTCCTCAGTCAGCTGGAGGCGCTGCAG</t>
-  </si>
-  <si>
-    <t>BMPR2_HUMAN_D0_3G2F_A</t>
-  </si>
-  <si>
-    <t>CACCAGCTGCAGCCCCGGCGGGTGTCATTCCGGGGCGAGGCCTCAGAGACTCTGCAGAGCCCTGGGTATGACCCAAGCCGGCCAGAGTCCTTCTTCCAGCAGAGCTTCCAGAGGCTCAGCCGCCTGGGCCATGGCTCCTACGGAGAGGTCTTCAAGGTGCGCTCCAAGGAGGACGGCCGGCTCTATGCGGTAAAGCGTTCCATGTCACCATTCCGGGGCCCCAAGGACCGGGCCCGCAAGTTGGCCGAGGTGGGCAGCCACGAGAAGGTGGGGCAGCACCCATGCTGCGTGCGGCTGGAGCAGGCCTGGGAGGAGGGCGGCATCCTGTACCTGCAGACGGAGCTGTGCGGGCCCAGCCTGCAGCAACACTGTGAGGCCTGGGGTGCCAGCCTGCCTGAGGCCCAGGTCTGGGGCTACCTGCGGGACACGCTGCTTGCCCTGGCCCATCTGCACAGCCAGGGCCTGGTGCACCTTGATGTCAAGCCTGCCAACATCTTCCTGGGGCCCCGGGGCCGCTGCAAGCTGGGTGACTTCGGACTGCTGGTGGAGCTGGGTACAGCAGGAGCTGGTGAGGTCCAGGAGGGAGACCCCCGCTACATGGCCCCCGAGCTGCTGCAGGGCTCCTATGGGACAGCAGCGGATGTGTTCAGTCTGGGCCTCACCATCCTGGAAGTGGCATGCAACATGGAGCTGCCCCACGGTGGGGAGGGCTGGCAGCAGCTGCGCCAGGGCTACCTGCCCCCTGAGTTCACTGCCGGTCTGTCTTCCGAGCTGCGTTCTGTCCTTGTCATGATGCTGGAGCCAGACCCCAAGCTGCGGGCCACGGCCGAGGCCCTGCTGGCACTGCCTGTGTTGAGGCAGCCG</t>
-  </si>
-  <si>
-    <t>PHKG2_HUMAN_D0_2Y7J_D</t>
-  </si>
-  <si>
-    <t>MAPK2_HUMAN_D0_2JBO_A</t>
-  </si>
-  <si>
-    <t>HHHHHHSHSGPEISRIIVDPTTGKRYCRGKVLGKGGFAKCYEMTDLTNNKVYAAKIIPHSRVAKPHQREKIDKEIELHRILHHKHVVQFYHYFEDKENIYILLEYCSRRSMAHILKARKVLTEPEVRYYLRQIVSGLKYLHEQEILHRDLKLGNFFINEAMELKVGDFGLAARLEPLEHRRRTICGTPNYLSPEVLNKQGHGCESDIWALGCVMYTMLLGRPPFETTNLKETYRCIREARYTMPSSLLAPAKHLIASMLSKNPEDRPSLDDIIRHDFFLQGFTPDRLSSSCCHTVPDFHLSSPA</t>
-  </si>
-  <si>
-    <t>ATGGAGAAGGACGGCCTGTGCCGCGCTGACCAGCAGTACGAATGCGTGGCGGAGATCGGGGAGGGCGCCTATGGGAAGGTGTTCAAGGCCCGCGACTTGAAGAACGGAGGCCGTTTCGTGGCGTTGAAGCGCGTGCGGGTGCAGACCGGCGAGGAGGGCATGCCGCTCTCCACCATCCGCGAGGTGGCGGTGCTGAGGCACCTGGAGACCTTCGAGCACCCCAACGTGGTCAGGTTGTTTGATGTGTGCACAGTGTCACGAACAGACAGAGAAACCAAACTAACTTTAGTGTTTGAACATGTCGATCAAGACTTGACCACTTACTTGGATAAAGTTCCAGAGCCTGGAGTGCCCACTGAAACCATAAAGGATATGATGTTTCAGCTTCTCCGAGGTCTGGACTTTCTTCATTCACACCGAGTAGTGCATCGCGATCTAAAACCACAGAACATTCTGGTGACCAGCAGCGGACAAATAAAACTCGCTGACTTCGGCCTTGCCCGCATCTATAGTTTCCAGATGGCTCTAACCTCAGTGGTCGTCACGCTGTGGTACAGAGCACCCGAAGTCTTGCTCCAGTCCAGCTACGCCACCCCCGTGGATCTCTGGAGTGTTGGCTGCATATTTGCAGAAATGTTTCGTAGAAAGCCTCTTTTTCGTGGAAGTTCAGATGTTGATCAACTAGGAAAAATCTTGGACGTGATTGGACTCCCAGGAGAAGAAGACTGGCCTAGAGATGTTGCCCTTCCCAGGCAGGCTTTTCATTCAAAATCTGCCCAACCAATTGAGAAGTTTGTAACAGATATCGATGAACTAGGCAAAGACCTACTTCTGAAGTGTTTGACATTTAACCCAGCCAAAAGAATATCTGCCTACAGTGCCCTGTCTCACCCATACTTCCAG</t>
-  </si>
-  <si>
-    <t>MEAAASEPSLDLDNLKLLELIGRGRYGAVYKGSLDERPVAVKVFSFANRQNFINEKNIYRVPLMEHDNIARFIVGDERVTADGRMEYLLVMEYYPNGSLCKYLSLHTSDWVSSCRLAHSVTRGLAYLHTELPRGDHYKPAISHRDLNSRNVLVKNDGTCVISDFGLSMRLTGNRLVRPGEEDNAAISEVGTIRYMAPEVLEGAVNLRDCESALKQVDMYALGLIYWEIFMRCTDLFPGESVPEYQMAFQTEVGNHPTFEDMQVLVSREKQRPKFPEAWKENSLAVRSLKETIEDCWDQDAEARLTAQCAEERMAELMMIWERNKSVSPT</t>
-  </si>
-  <si>
-    <t>ATGTCGGGCCCTCGCGCCGGCTTCTACCGGCAGGAGCTGAACAAGACCGTGTGGGAGGTGCCGCAGCGGCTGCAGGGGCTGCGCCCGGTGGGCTCCGGCGCCTACGGCTCCGTCTGTTCGGCCTACGACGCCCGGCTGCGCCAGAAGGTGGCGGTGAAGAAGCTGTCGCGCCCCTTCCAGTCGCTGATCCACGCGCGCAGAACGTACCGGGAGCTGCGGCTGCTCAAGCACCTGAAGCACGAGAACGTCATCGGGCTTCTGGACGTCTTCACGCCGGCCACGTCCATCGAGGACTTCAGCGAAGTGTACTTGGTGACCACCCTGATGGGCGCCGACCTGAACAACATCGTCAAGTGCCAGGCGCTGAGCGACGAGCACGTTCAATTCCTGGTTTACCAGCTGCTGCGCGGGCTGAAGTACATCCACTCGGCCGGGATCATCCACCGGGACCTGAAGCCCAGCAACGTGGCTGTGAACGAGGACTGTGAGCTCAGGATCCTGGATTTCGGGCTGGCGCGCCAGGCGGACGAGGAGATGACCGGCTATGTGGCCACGCGCTGGTACCGGGCACCTGAGATCATGCTCAACTGGATGCATTACAACCAAACAGTGGATATCTGGTCCGTGGGCTGCATCATGGCTGAGCTGCTCCAGGGCAAGGCCCTCTTCCCGGGAAGCGACTACATTGACCAGCTGAAGCGCATCATGGAAGTGGTGGGCACACCCAGCCCTGAGGTTCTGGCAAAAATCTCCTCGGAACACGCCCGGACATATATCCAGTCCCTGCCCCCCATGCCCCAGAAGGACCTGAGCAGCATCTTCCGTGGAGCCAACCCCCTGGCCATAGACCTCCTTGGAAGGATGCTGGTGCTGGACAGTGACCAGAGGGTCAGTGCAGCTGAGGCACTGGCCCACGCCTACTTCAGCCAGTACCACGACCCCGAGGATGAGCCAGAGGCCGAGCCATATGATGAGAGCGTTGAGGCCAAGGAGCGCACGCTGGAGGAGTGGAAGGAGCTCACTTACCAGGAAGTCCTCAGCTTCAAGCCCCCAGAGCCACCGAAGCCACCTGGCAGCCTGGAGATTGAGCAG</t>
-  </si>
-  <si>
-    <t>E2AK2_HUMAN_D0_3UIU_A</t>
-  </si>
-  <si>
-    <t>MEKYEKIGKIGEGSYGVVFKCRNRDTGQIVAIKKFLESEDDPVIKKIALREIRMLKQLKHPNLVNLLEVFRRKRRLHLVFEYCDHTVLHELDRYQRGVPEHLVKSITWQTLQAVNFCHKHNCIHRDVKPENILITKHSVIKLCDFGFARLLTGPSDYYTDYVATRWYRSPELLVGDTQYGPPVDVWAIGCVFAELLSGVPLWPGKSDVDQLYLIRKTLGDLIPRHQQVFSTNQYFSGVKIPDPEDMEPLELKFPNISYPALGLL</t>
-  </si>
-  <si>
-    <t>GeneID</t>
-  </si>
-  <si>
-    <t>ATGGATGAGCAATCACAAGGAATGCAAGGGCCACCTGTTCCTCAGTTCCAACCACAGAAGGCCTTACGACCGGATATGGGCTATAATACATTAGCCAACTTTCGAATAGAAAAGAAAATTGGTCGCGGACAATTTAGTGAAGTTTATAGAGCAGCCTGTCTCTTGGATGGAGTACCAGTAGCTTTAAAAAAAGTGCAGATATTTGATTTAATGGATGCCAAAGCACGTGCTGATTGCATCAAAGAAATAGATCTTCTTAAGCAACTCAACCATCCAAATGTAATAAAATATTATGCATCATTCATTGAAGATAATGAACTAAACATAGTTTTGGAACTAGCAGATGCTGGCGACCTATCCAGAATGATCAAGCATTTTAAGAAGCAAAAGAGGCTAATTCCTGAAAGAACTGTTTGGAAGTATTTTGTTCAGCTTTGCAGTGCATTGGAACACATGCATTCTCGAAGAGTCATGCATAGAGATATAAAACCAGCTAATGTGTTCATTACAGCCACTGGGGTGGTAAAACTTGGAGATCTTGGGCTTGGCCGGTTTTTCAGCTCAAAAACCACAGCTGCACATTCTTTAGTTGGTACGCCTTATTACATGTCTCCAGAGAGAATACATGAAAATGGATACAACTTCAAATCTGACATCTGGTCTCTTGGCTGTCTACTATATGAGATGGCTGCATTACAAAGTCCTTTCTATGGTGACAAAATGAATTTATACTCACTGTGTAAGAAGATAGAACAGTGTGACTACCCACCTCTTCCTTCAGATCACTATTCAGAAGAACTCCGACAGTTAGTTAATATGTGCATCAACCCAGATCCAGAGAAGCGACCAGACGTCACCTATGTTTATGACGTAGCAAAGAGGATGCATGCATGCACTGCAAGCAGC</t>
-  </si>
-  <si>
-    <t>DAPK3_HUMAN_D0_2J90_A</t>
-  </si>
-  <si>
-    <t>GAAGACAGTTTGACTAAGCAGCCTGAAGAAGTTTTTGATGTATTAGAGAAGCTTGGAGAAGGGTCTTATGGAAGTGTATTTAAAGCAATACACAAGGAATCCGGTCAAGTTGTCGCAATTAAACAAGTACCTGTTGAATCAGATCTTCAGGAAATAATCAAAGAAATTTCCATAATGCAGCAATGTGACAGCCCATATGTTGTAAAGTACTATGGCAGTTATTTTAAGAATACAGACCTCTGGATTGTTATGGAGTACTGTGGCGCTGGCTCTGTCTCAGACATAATTAGATTACGAAACAAGACATTAATAGAAGATGAAATTGCAACCATTCTTAAATCTACATTGAAAGGACTAGAATATTTGCACTTTATGAGAAAAATACACAGAGATATAAAAGCTGGAAATATTCTCCTCAATACAGAAGGACATGCAAAATTGGCAGATTTTGGAGTGGCTGGTCAGTTAACAGATACAATGGCAAAACGCAATACTGTAATAGGAACTCCATTTTGGATGGCTCCTGAGGTGATTCAAGAAATAGGCTATAACTGTGTGGCCGACATCTGGTCCCTTGGCATTACTTCTATAGAAATGGCTGAAGGAAAACCTCCTTATGCTGATATACATCCAATGAGGGCTATTTTTATGATTCCCACAAATCCACCACCAACATTCAGAAAGCCAGAACTTTGGTCCGATGATTTCACCGATTTTGTTAAAAAGTGTTTGGTGAAGAATCCTGAGCAGAGAGCTACTGCAACACAACTTTTACAGCATCCTTTTATCAAGAATGCCAAACCTGTATCAATATTAAGAGACCTGATCACAGAAGCTATGGAGATCAAAGCTAAAAGACATGAGGAACAGCAACGAGAATTGGAAGAGGAAGAA</t>
-  </si>
-  <si>
-    <t>VKEFLAKAKEDFLKKWESPAQNTAHLDQFERIKTLGTGSFGRVMLVKHKETGNHYAMKILDKQKVVKLKQIEHTLNEKRILQAVNFPFLVKLEFSFKDNSNLYMVMEYVPGGEMFSHLRRIGRFSEPHARFYAAQIVLTFEYLHSLDLIYRDLKPENLLIDQQGYIQVTDFGFAKRVKGRTWTLCGTPEYLAPEIILSKGYNKAVDWWALGVLIYEMAAGYPPFFADQPIQIYEKIVSGKVRFPSHFSSDLKDLLRNLLQVDLTKRFGNLKNGVNDIKNHKWFATTDWIAIYQRKVEAPFIPKFKGPGDTSNFDDYEEEEIRVSINEKCGKEFSEF</t>
-  </si>
-  <si>
-    <t>TCCAGGGTGTCCCATGAACAGTTTCGGGCGGCCCTGCAGCTGGTGGTCAGCCCAGGAGACCCCAGGGAATACTTGGCCAACTTTATCAAAATCGGGGAAGGCTCAACCGGCATCGTATGCATCGCCACCGAGAAACACACAGGGAAACAAGTTGCAGTGAAGAAAATGGACCTCCGGAAGCAACAGAGACGAGAACTGCTTTTCAATGAGGTCGTGATCATGCGGGATTACCACCATGACAATGTGGTTGACATGTACAGCAGCTACCTTGTCGGCGATGAGCTCTGGGTGGTCATGGAGTTTCTAGAAGGTGGTGCCTTGACAGACATTGTGACTCACACCAGAATGAATGAAGAACAGATAGCTACTGTCTGCCTGTCAGTTCTGAGAGCTCTCTCCTACCTTCATAACCAAGGAGTGATTCACAGGGACATAAAAAGTGACTCCATCCTCCTGACAAGCGATGGCCGGATAAAGTTGTCTGATTTTGGTTTCTGTGCTCAAGTTTCCAAAGAGGTGCCGAAGAGGAAATCATTGGTTGGCACTCCCTACTGGATGGCCCCTGAGGTGATTTCTAGGCTACCTTATGGGACAGAGGTGGACATCTGGTCCCTCGGGATCATGGTGATAGAAATGATTGATGGCGAGCCCCCCTACTTCAATGAGCCTCCCCTCCAGGCGATGCGGAGGATCCGGGACAGTTTACCTCCAAGAGTGAAGGACCTACACAAGGTTTCTTCAGTGCTCCGGGGATTCCTAGACTTGATGTTGGTGAGGGAGCCCTCTCAGAGAGCAACAGCCCAGGAACTCCTCGGACATCCATTCTTAAAACTAGCAGGTCCACCGTCTTGCATTGTCCCCCTCATGAGACAATACAGGCATCAC</t>
-  </si>
-  <si>
-    <t>KRQWALEDFEIGRPLGKGKFGNVYLAREKQSKFILALKVLFKAQLEKAGVEHQLRREVEIQSHLRHPNILRLYGYFHDATRVYLILEYAPLGTVYRELQKLSKFDEQRTATYITELANALSYCHSKRVIHRDIKPENLLLGSAGELKIADFGWSVHAPSSRRTTLCGTLDYLPPEMIEGRMHDEKVDLWSLGVLCYEFLVGKPPFEANTYQETYKRISRVEFTFPDFVTEGARDLISRLLKHNPSQRPMLREVLEHPWITANSSKPS</t>
-  </si>
-  <si>
-    <t>SLK_HUMAN_D0_2JFL_A</t>
-  </si>
-  <si>
-    <t>SRVSHEQFRAALQLVVSPGDPREYLANFIKIGEGSTGIVCIATEKHTGKQVAVKKMDLRKQQRRELLFNEVVIMRDYHHDNVVDMYSSYLVGDELWVVMEFLEGGALTDIVTHTRMNEEQIATVCLSVLRALSYLHNQGVIHRDIKSDSILLTSDGRIKLSDFGFCAQVSKEVPKRKSLVGTPYWMAPEVISRLPYGTEVDIWSLGIMVIEMIDGEPPYFNEPPLQAMRRIRDSLPPRVKDLHKVSSVLRGFLDLMLVREPSQRATAQELLGHPFLKLAGPPSCIVPLMRQYRHH</t>
-  </si>
-  <si>
-    <t>TQTVHEFAKELDATNISIDKVVGAGEFGEVCSGRLKLPSKKEISVAIKTLKVGYTEKQRRDFLGEASIMGQFDHPNIIRLEGVVTKSKPVMIVTEYMENGSLDSFLRKHDAQFTVIQLVGMLRGIASGMKYLSDMGYVHRDLAARNILINSNLVCKVSDFGLSRVLEDDPEAAYTTRGGKIPIRWTSPEAIAYRKFTSASDVWSYGIVLWEVMSYGERPYWEMSNQDVIKAVDEGYRLPPPMDCPAALYQLMLDCWQKDRNNRPKFEQIVSILDKLIRNPGSLKIITSAAARPSNLLLDQSNVDITTFRTTGDWLNGVWTAHCKEIFTGVEYSSCDTIAKIS</t>
-  </si>
-  <si>
-    <t>QQFPQFHVKSGLQIKKNAIIDDYKVTSQVLGLGINGKVLQIFNKRTQEKFALKMLQDCPKARREVELHWRASQCPHIVRIVDVYENLYAGRKCLLIVMECLDGGELFSRIQDRGDQAFTEREASEIMKSIGEAIQYLHSINIAHRDVKPENLLYTSKRPNAILKLTDFGFAKETTSHNSLTTPCYTPYYVAPEVLGPEKYDKSCDMWSLGVIMYILLCGYPPFYSNHGLAISPGMKTRIRMGQYEFPNPEWSEVSEEVKMLIRNLLKTEPTQRMTITEFMNHPWIMQSTKVPQTPLHTSRVLKEDKERWEDVKGCLHDKNSDQA</t>
-  </si>
-  <si>
-    <t>CSK21_HUMAN_D0_3AXW_A</t>
-  </si>
-  <si>
-    <t>ATCTRFTDDYQLFEELGKGAFSVVRRCVKKTPTQEYAAKIINTKKLSARDHQKLEREARICRLLKHPNIVRLHDSISEEGFHYLVFDLVTGGELFEDIVAREYYSEADASHCIHQILESVNHIHQHDIVHRDLKPENLLLASKCKGAAVKLADFGLAIEVQGEQQAWFGFAGTPGYLSPEVLRKDPYGKPVDIWACGVILYILLVGYPPFWDEDQHKLYQQIKAGAYDFPSPEWDTVTPEAKNLINQMLTINPAKRITADQALKHPWVCQRSTVASMMHRQETVECLRKFNARRKLKGAILTTMLVSRNFS</t>
-  </si>
-  <si>
-    <t>VIDPSELTFVQEIGSGQFGLVHLGYWLNKDKVAIKTIREGAMSEEDFIEEAEVMMKLSHPKLVQLYGVCLEQAPICLVFEFMEHGCLSDYLRTQRGLFAAETLLGMCLDVCEGMAYLEEACVIHRDLAARNCLVGENQVIKVSDFGMTRFVLDDQYTSSTGTKFPVKWASPEVFSFSRYSSKSDVWSFGVLMWEVFSEGKIPYENRSNSEVVEDISTGFRLYKPRLASTHVYQIMNHCWKERPEDRPAFSRLLRQLAEIAESGL</t>
-  </si>
-  <si>
-    <t>CGTGTAAAAGCAGCTCAAGCTGGAAGACAGAGCTCTGCAAAGAGACATCTTGCAGAACAATTTGCAGTTGGAGAGATAATAACTGACATGGCAAAAAAGGAATGGAAAGTAGGATTACCCATTGGCCAAGGAGGCTTTGGCTGTATATATCTTGCTGATATGAATTCTTCAGAGTCAGTTGGCAGTGATGCACCTTGTGTTGTAAAAGTGGAACCCAGTGACAATGGACCTCTTTTTACTGAATTAAAGTTCTACCAACGAGCTGCAAAACCAGAGCAAATTCAGAAATGGATTCGTACCCGTAAGCTGAAGTACCTGGGTGTTCCTAAGTATTGGGGGTCTGGTCTACATGACAAAAATGGAAAAAGTTACAGGTTTATGATAATGGATCGCTTTGGGAGTGACCTTCAGAAAATATATGAAGCAAATGCCAAAAGGTTTTCTCGGAAAACTGTCTTGCAGCTAAGCTTAAGAATTCTGGATATTCTGGAATATATTCACGAGCATGAGTATGTGCATGGAGATATCAAGGCCTCAAATCTTCTTCTGAACTACAAGAATCCTGACCAGGTGTACTTGGTAGATTATGGCCTTGCTTATCGGTACTGCCCAGAAGGAGTTCATAAAGAATACAAAGAAGACCCCAAAAGATGTCACGATGGCACTATTGAATTCACGAGCATCGATGCACACAATGGCGTGGCCCCATCAAGACGTGGTGATTTGGAAATACTTGGTTATTGCATGATCCAATGGCTTACTGGCCATCTTCCTTGGGAGGATAATTTGAAAGATCCTAAATATGTTAGAGATTCCAAAATTAGATACAGAGAAAATATTGCAAGTTTGATGGACAAATGTTTTCCTGAGAAAAACAAACCAGGTGAAATTGCCAAATACATGGAAACAGTGAAATTACTAGACTACACTGAAAAACCTCTTTATGAAAATTTACGTGACATTCTTTTGCAAGGACTAAAAGCTATAGGAAGTAAGGATGATGGCAAATTGGACCTCAGTGTTGTGGAGAATGGAGGTTTGAAAGCAAAAACAATAACAAAGAAGCGAAAGAAAGAAATTGAAGAA</t>
-  </si>
-  <si>
-    <t>MP2K6_HUMAN_D0_3VN9_A</t>
-  </si>
-  <si>
-    <t>RVKAAQAGRQSSAKRHLAEQFAVGEIITDMAKKEWKVGLPIGQGGFGCIYLADMNSSESVGSDAPCVVKVEPSDNGPLFTELKFYQRAAKPEQIQKWIRTRKLKYLGVPKYWGSGLHDKNGKSYRFMIMDRFGSDLQKIYEANAKRFSRKTVLQLSLRILDILEYIHEHEYVHGDIKASNLLLNYKNPDQVYLVDYGLAYRYCPEGVHKEYKEDPKRCHDGTIEFTSIDAHNGVAPSRRGDLEILGYCMIQWLTGHLPWEDNLKDPKYVRDSKIRYRENIASLMDKCFPEKNKPGEIAKYMETVKLLDYTEKPLYENLRDILLQGLKAIGSKDDGKLDLSVVENGGLKAKTITKKRKKEIEE</t>
-  </si>
-  <si>
-    <t>MKNK1_HUMAN_D0_2HW6_B</t>
-  </si>
-  <si>
-    <t>MSLIRKKGFYKQDVNKTAWELPKTYVSPTHVGSGAYGSVCSAIDKRSGEKVAIKKLSRPFQSEIFAKRAYRELLLLKHMQHENVIGLLDVFTPASSLRNFYDFYLVMPFMQTDLQKIMGMEFSEEKIQYLVYQMLKGLKYIHSAGVVHRDLKPGNLAVNEDCELKILDFGLARHADAEMTGYVVTRWYRAPEVILSWMHYNQTVDIWSVVCIMAEMLTGKTLFKGKDYLDQLTQILKVTGVPGTEFVQKLNDKAAKSYIQSLPQTPRKDFTQLFPRASPQAADLLEKMLELDVDKRLTAAQALTHPFFEPFRDPEEETEAQQPFDDSLEHEKLTVDEWKQHIYKEIVNFSPI</t>
-  </si>
-  <si>
-    <t>DEQPHIGNYRLLKTIGKGNFAKVKLARHILTGREVAIKIIDKTQLNPTSLQKLFREVRIMKILNHPNIVKLFEVIETEKTLYLIMEYASGGEVFDYLVAHGRMKEKEARSKFRQIVSAVQYCHQKRIVHRDLKAENLLLDADMNIKIADFGFSNEFTVGGKLDTFCGSPPYAAPELFQGKKYDGPEVDVWSLGVILYTLVSGSLPFDGQNLKELRERVLRGKYRIPFYMSTDCENLLKRFLVLNPIKRGTLEQIMKDRWINAGHEEDELKPFVEPELDISDQKRIDIMVGMGYSQEEIQESLSKMKYDEITATYLLLGRKSSE</t>
-  </si>
-  <si>
-    <t>ITK_HUMAN_D0_3QGW_B</t>
-  </si>
-  <si>
-    <t>KS6A3_HUMAN_D1_4JG7_A</t>
-  </si>
-  <si>
-    <t>KCC4_HUMAN_D0_2W4O_A</t>
-  </si>
-  <si>
-    <t>CSK_HUMAN_D0_3D7T_A</t>
-  </si>
-  <si>
-    <t>KCC2A_HUMAN_D0_2VZ6_B</t>
-  </si>
-  <si>
-    <t>ATGTCTGATGAGGAGATCTTGGAGAAATTACGAAGCATAGTGAGTGTGGGCGATCCTAAGAAGAAATATACACGGTTTGAGAAGATTGGACAAGGTGCTTCAGGCACCGTGTACACAGCAATGGATGTGGCCACAGGACAGGAGGTGGCCATTAAGCAGATGAATCTTCAGCAGCAGCCCAAGAAAGAGCTGATTATTAATGAGATCCTGGTCATGAGGGAAAACAAGAACCCAAACATTGTGAATTACTTGGACAGTTACCTCGTGGGAGATGAGCTGTGGGTTGTTATGGAATACTTGGCTGGAGGCTCCTTGACAGATGTGGTGACAGAAACTTGCATGGATGAAGGCCAAATTGCAGCTGTGTGCCGTGAGTGTCTGCAGGCTCTGGAGTTCTTGCATTCGAACCAGGTCATTCACAGAGACATCAAGAGTGACAATATTCTGTTGGGAATGGATGGCTCTGTCAAGCTAACTGACTTTGGATTCTGTGCACAGATAACCCCAGAGCAGAGCAAACGGAGCACCATGGTAGGAACCCCATACTGGATGGCACCAGAGGTTGTGACACGAAAGGCCTATGGGCCCAAGGTTGACATCTGGTCCCTGGGCATCAAGGCCATCGAAATGATTGAAGGGGAGCCTCCATACCTCAATGAAAACCCTCTGAGAGCCTTGTACCTCATTGCCACCAATGGGACCCCAGAACTTCAGAACCCAGAGAAGCTGTCAGCTATCTTCCGGGACTTTCTGAACCGCTGTCTCGAGATGGATGTGGAGAAGAGAGGTTCAGCTAAAGAGCTGCTACAGCATCAATTCCTGAAGATTGCCAAGCCCCTCTCCAGCCTCACTCCACTTATTGCTGCAGCTAAGGAGGCAACAAAGAACAATCAC</t>
-  </si>
-  <si>
-    <t>AVPFVEDWDLVQTLGEGAYGEVQLAVNRVTEEAVAVKIVDMKRAVDCPENIKKEICINKMLNHENVVKFYGHRREGNIQYLFLEYCSGGELFDRIEPDIGMPEPDAQRFFHQLMAGVVYLHGIGITHRDIKPENLLLDERDNLKISDFGLATVFRYNNRERLLNKMCGTLPYVAPELLKRREFHAEPVDVWSCGIVLTAMLAGELPWDQPSDSCQEYSDWKEKKTYLNPWKKIDSAPLALLHKILVENPSARITIPDIKKDRWYNKPL</t>
-  </si>
-  <si>
-    <t>GCCACCTGCACACGTTTCACCGACGACTACCAGCTCTTCGAGGAGCTTGGCAAGGGTGCTTTCTCTGTGGTCCGCAGGTGTGTGAAGAAAACCCCCACGCAGGAGTACGCAGCAAAAATCATCAATACCAAGAAATTGTCTGCCCGGGATCACCAGAAACTAGAACGTGAGGCTCGGATATGTCGACTTCTGAAACATCCAAACATCGTGCGCCTCCATGACAGTATTTCTGAAGAAGGGTTTCACTACCTCGTGTTTGACCTTGTTACCGGCGGGGAGCTGTTTGAAGACATTGTGGCCAGAGAGTACTACAGTGAAGCAGATGCCAGCCACTGTATACATCAGATTCTGGAGAGTGTTAACCACATCCACCAGCATGACATCGTCCACAGGGACCTGAAGCCTGAGAACCTGCTGCTGGCGAGTAAATGCAAGGGTGCCGCCGTCAAGCTGGCTGATTTTGGCCTAGCCATCGAAGTACAGGGAGAGCAGCAGGCTTGGTTTGGTTTTGCTGGCACCCCAGGTTACTTGTCCCCTGAGGTCTTGAGGAAAGATCCCTATGGAAAACCTGTGGATATCTGGGCCTGCGGGGTCATCCTGTATATCCTCCTGGTGGGCTATCCTCCCTTCTGGGATGAGGATCAGCACAAGCTGTATCAGCAGATCAAGGCTGGAGCCTATGATTTCCCATCACCAGAATGGGACACGGTAACTCCTGAAGCCAAGAACTTGATCAACCAGATGCTGACCATAAACCCAGCAAAGCGCATCACGGCTGACCAGGCTCTCAAGCACCCGTGGGTCTGTCAACGATCCACGGTGGCATCCATGATGCATCGTCAGGAGACTGTGGAGTGTTTGCGCAAGTTCAATGCCCGGAGAAAACTGAAGGGTGCCATCCTCACGACCATGCTTGTCTCCAGGAACTTCTCA</t>
-  </si>
-  <si>
-    <t>GAGACCTACATTAAGCTGGACAAACTGGGCGAGGGTACCTATGCCACCGTCTACAAAGGCAAAAGCAAGCTCACAGACAACCTTGTGGCACTCAAGGAGATCAGACTGGAACATGAAGAGGGGGCACCCTGCACCGCCATCCGGGAAGTGTCCCTACTCAAGGACCTCAAACACGCCAACATCGTTACGCTACATGACATTATCCACACGGAGAAGTCCCTCACCCTTGTCTTTGAGTACCTGGACAAGGACCTGAAGCAGTACCTGGATGACTGTGGGAACATCATCAACATGCACAACGTGAAACTGTTCCTGTTCCAGCTGCTCCGTGGCCTGGCCTACTGCCACCGGCAGAAGGTGCTACACCGAGACCTCAAGCCCCAGAACCTGCTCATCAACGAGAGGGGAGAGCTCAAGCTGGCTGACTTTGGCCTGGCCCGAGCCAAGTCAATCCCAACAAAGACATACTCCAATGAGGTGGTGACACTGTGGTACCGGCCCCCTGACATCCTGCTTGGGTCCACGGACTACTCCACTCAGATTGACATGTGGGGTGTGGGCTGCATCTTCTATGAGATGGCCACAGGCCGTCCCCTCTTTCCGGGCTCCACGGTGGAGGAACAGCTACACTTCATCTTCCGTATCTTAGGAACCCCAACTGAGGAGACGTGGCCAGGCATCCTGTCCAACGAGGAGTTCAAGACATACAACTACCCCAAGTACCGAGCCGAGGCCCTTTTGAGCCACGCACCCCGACTTGATAGCGACGGGGCCGACCTCCTCACCAAGCTGTTGCAGTTTGAGGGTCGAAATCGGATCTCCGCAGAGGATGCCATGAAACATCCATTCTTCCTCAGTCTGGGGGAGCGGATCCACAAACTTCCTGACACTACTTCCATATTTGCACTAAAGGAGATTCAGCTACAAAAGGAGGCCAGCCTTCGGTCT</t>
-  </si>
-  <si>
-    <t>MK13_HUMAN_D0_4EYJ_A</t>
-  </si>
-  <si>
-    <t>STK16_HUMAN_D0_2BUJ_B</t>
-  </si>
-  <si>
-    <t>AAGCACGACGGGCGGGTGAAGATCGGACACTACGTGCTGGGCGACACGCTGGGCGTCGGCACCTTCGGCAAAGTGAAGATTGGAGAACATCAATTAACAGGCCATAAAGTGGCAGTTAAAATCTTAAATAGACAGAAGATTCGCAGTTTAGATGTTGTTGGAAAAATAAAACGAGAAATTCAAAATCTAAAACTCTTTCGTCATCCTCATATTATCAAACTATACCAGGTGATCAGCACTCCAACAGATTTTTTTATGGTAATGGAATATGTGTCTGGAGGTGAATTATTTGACTACATCTGTAAGCATGGACGGGTTGAAGAGATGGAAGCCAGGCGRCTCTTTCAGCAGATTCTGTCTGCTGTGGATTACTGTCATAGGCATATGGTTGTTCATCGAGACCTGAAACCAGAGAATGTCCTGTTGGATGCACACATGAATGCCAAGATAGCCGATTTCGGATTATCTAATATGATGTCAGATGGTGAATTTCTGAGAACTAGTTGCGGATCTCCAAATTATGCAGCACCTGAAGTCATCTCAGGCAGATTGTATGCAGGTCCTGAAGTTGATATCTGGAGCTGTGGTGTTATCTTGTATGCTCTTCTTTGTGGCACCCTCCCATTTGATGATGAGCATGTACCTACGTTATTTAAGAAGATCCGAGGGGGTGTCTTTTATATCCCAGAATATCTCAATCGTTCTGTCGCCACTCTCCTGATGCATATGCTGCAGGTTGACCCACTGAAACGAGCAACTATCAAAGACATAAGAGAGCATGAATGGTTTAAACAAGATTTGCCCAGTTACTTATTTCCTGAA</t>
-  </si>
-  <si>
-    <t>ATGGAAAGCGACCTGCACCAGATCATCCACTCCTCACAGCCCCTCACACTGGAACACGTGCGCTACTTCCTGTACCAACTGCTGCGGGGCCTGAAGTACATGCACTCGGCTCAGGTCATCCACCGTGACCTGAAGCCCTCCAACCTATTGGTGAATGAGAACTGTGAGCTCAAGATTGGTGACTTTGGTATGGCTCGTGGCCTGTGCACCTCGCCCGCTGAACATCAGTACTTCATGACTGAGTATGTGGCCACGCGCTGGTACCGTGCGCCCGAGCTCATGCTCTCTTTGCATGAGTATACACAGGCTATTGACCTCTGGTCTGTGGGCTGCATCTTTGGTGAGATGCTGGCCCGGCGCCAGCTCTTCCCAGGCAAAAACTATGTACACCAGCTACAGCTCATCATGATGGTGCTGGGTACCCCATCACCAGCCGTGATTCAGGCTGTGGGGGCTGAGAGGGTGCGGGCCTATATCCAGAGCTTGCCACCACGCCAGCCTGTGCCCTGGGAGACAGTGTACCCAGGTGCCGACCGCCAGGCCCTATCACTGCTGGGTCGCATGCTGCGTTTTGAGCCCAGCGCTCGCATCTCAGCAGCTGCTGCCCTTCGCCACCCTTTCCTGGCCAAGTACCATGATCCTGATGATGAGCCTGACTGTGCCCCGCCCTTTGACTTTGCCTTTGACCGCGAAGCCCTCACTCGGGAGCGCATTAAGGAGGCCATTGTGGCTGAAATTGAGGACTTCCATGCAAGGCGTGAGGGCATCCGCCAACAGATCCGCTTCCAGCCTTCTCTACAGCCTGTGGCTAGTGAGCCTGGCTGTCCAGATGTTGAAATGCCCAGTCCCTGGGCTCCCAGTGGGGACTGTGCCATG</t>
-  </si>
-  <si>
-    <t>CAGAGCAGTAAGCGCAGCAGCCGGAGTGTGGAAGATGACAAGGAGGGTCACCTGGTGTGCCGGATCGGCGATTGGCTCCAAGAGCGATATGAGATTGTGGGGAACCTGGGTGAAGGCACCTTTGGCAAGGTGGTGGAGTGCTTGGACCATGCCAGAGGGAAGTCTCAGGTTGCCCTGAAGATCATCCGCAACGTGGGCAAGTACCGGGAGGCTGCCCGGCTAGAAATCAACGTGCTCAAAAAAATCAAGGAGAAGGACAAAGAAAACAAGTTCCTGTGTGTCTTGATGTCTGACTGGTTCAACTTCCACGGTCACATGTGCATCGCCTTTGAGCTCCTGGGCAAGAACACCTTTGAGTTCCTGAAGGAGAATAACTTCCAGCCTTACCCCCTACCACATGTCCGGCACATGGCCTACCAGCTCTGCCACGCCCTTAGATTTCTGCATGAGAATCAGCTGACCCATACAGACTTGAAACCAGAGAACATCCTGTTTGTGAATTCTGAGTTTGAAACCCTCTACAATGAGCACAAGAGCTGTGAGGAGAAGTCAGTGAAGAACACCAGCATCCGAGTGGCTGACTTTGGCAGTGCCACATTTGACCATGAGCACCACACCACCATTGTGGCCACCCGTCACTATCGCCCGCCTGAGGTGATCCTTGAGCTGGGCTGGGCACAGCCCTGTGACGTCTGGAGCATTGGCTGCATTCTCTTTGAGTACTACCGGGGCTTCACACTCTTCCAGACCCACGAAAACCGAGAGCACCTGGTGATGATGGAGAAGATCCTAGGGCCCATCCCATCACACATGATCCACCGTACCAGGAAGCAGAAATATTTCTACAAAGGGGGCCTAGTTTGGGATGAGAACAGCTCTGACGGCCGGTATGTGAAGGAGAACTGCAAACCTCTGAAGAGTTACATGCTCCAAGACTCCCTGGAGCACGTGCAGCTGTTTGACCTGATGAGGAGGATGTTAGAATTTGACCCTGCCCAGCGCATCACACTGGCCGAGGCCCTGCTGCACCCCTTCTTTGCTGGCCTGACCCCTGAGGAGCGGTCCTTCCACACC</t>
-  </si>
-  <si>
-    <t>GAACTGAAGGATGACGACTTTGAGAAGATCAGTGAGCTGGGGGCTGGCAATGGCGGTGTGGTGTTCAAGGTCTCCCACAAGCCTTCTGGCCTGGTCATGGCCAGAAAGCTAATTCATCTGGAGATCAAACCCGCAATCCGGAACCAGATCATAAGGGAGCTGCAGGTTCTGCATGAGTGCAACTCTCCGTACATCGTGGGCTTCTATGGTGCGTTCTACAGCGATGGCGAGATCAGTATCTGCATGGAGCACATGGATGGAGGTTCTCTGGATCAAGTCCTGAAGAAAGCTGGAAGAATTCCTGAACAAATTTTAGGAAAAGTTAGCATTGCTGTAATAAAAGGCCTGACATATCTGAGGGAGAAGCACAAGATCATGCACAGAGCATACGGAATGGACAGCCGACCTCCCATGGCAATTTTTGAGTTGTTGGATTACATAGTCAACGAGCCTCCTCCAAAACTGCCCAGTGGAGTGTTCAGTCTGGAATTTCAAGATTTTGTGAATAAATGCTTAATAAAAAACCCCGCAGAGAGAGCAGATTTGAAGCAACTCATGGTTCATGCTTTTATCAAGAGATCTGATGCTGAGGAAGTGGATTTTGCAGGTTGGCTCTGCTCCACCATCGGCCTTAAC</t>
-  </si>
-  <si>
-    <t>MQTVGVHSIVQQLHRNSIQFTDGYEVKEDIGVGSYSVCKRCIHKATNMEFAVKIIDKSKRDPTEEIEILLRYGQHPNIITLKDVYDDGKYVYVVTELMKGGELLDKILRQKFFSEREASAVLFTITKTVEYLHAQGVVHRDLKPSNILYVDESGNPESIRICDFGFAKQLRAENGLLMTPCYTANFVAPEVLKRQGYDAACDIWSLGVLLYTMLTGYTPFANGPDDTPEEILARIGSGKFSLSGGYWNSVSDTAKDLVSKMLHVDPHQRLTAALVLRHPWIVHWDQLPQYQLNRQDAPHLVKGAMAATYSALNRNQSPVLEPVGRSTLAQRRGIKKITSTAL</t>
-  </si>
-  <si>
-    <t>MSSFLPEGGCYELLTVIGKGFEDLMTVNLARYKPTGEYVTVRRINLEACSNEMVTFLQGELHVSKLFNHPNIVPYRATFIADNELWVVTSFMAYGSAKDLICTHFMDGMNELAIAYILQGVLKALDYIHHMGYVHRSVKASHILISVDGKVYLSGLRSNLSMISHGQRQRVVHDFPKYSVKVLPWLSPEVLQQNLQGYDAKSDIYSVGITACELANGHVPFKDMPATQMLLEKLNGTVPCLLDTSTIPAEELTMSPSRSVANSGLSDSLTTSTPRPSNGDSPSHPYHRTFSPHFHHFVEQCLQRNPDARPSASTLLNHSFFKQIKRRASEVLPELLRPVTPITNFEGSQSQDHSGIFGLVTNLEELEVDDWEF</t>
-  </si>
-  <si>
-    <t>KAPCA_HUMAN_D0_4AE9_A</t>
-  </si>
-  <si>
-    <t>KCC2G_HUMAN_D0_2V7O_A</t>
-  </si>
-  <si>
-    <t>KQYEHVKRDLNPEDFWEIIGELGDGAFGKVYKAQNKETSVLAAAKVIDTKSEEELEDYMVEIDILASCDHPNIVKLLDAFYYENNLWILIEFCAGGAVDAVMLELERPLTESQIQVVCKQTLDALNYLHDNKIIHRDLKAGNILFTLDGDIKLADFGVSAKNMRTIQRRDSFIGTPYWMAPEVVMCETSKDRPYDYKADVWSLGITLIEMAEIEPPHHELNPMRVLLKIAKSEPPTLAQPSRWSSNFKDFLKKCLEKNVDARWTTSQLLQHPFVTVDSNKPIRELIAEAKAEVTEEVEDGKE</t>
-  </si>
-  <si>
-    <t>ACCCAAACTGTTCATGAGTTTGCCAAGGAATTGGATGCCACCAACATATCCATTGATAAAGTTGTTGGAGCAGGTGAATTTGGAGAGGTGTGCAGTGGTCGCTTAAAACTTCCTTCAAAAAAAGAGATTTCAGTGGCCATTAAGACCCTGAAAGTTGGCTACACAGAAAAGCAGAGGAGAGACTTCCTGGGAGAAGCAAGCATTATGGGACAGTTTGACCACCCCAATATCATTCGACTGGAAGGAGTTGTTACCAAAAGTAAGCCAGTTATGATTGTCACAGAATACATGGAGAATGGTTCCTTGGATAGTTTCCTACGTAAACACGATGCCCAGTTTACTGTCATTCAGCTAGTGGGGATGCTTCGAGGGATAGCATCTGGCATGAAGTACCTGTCAGACATGGGCTATGTTCACCGAGACCTCGCTGCTCGGAACATCTTGATCAACAGTAACTTGGTGTGTAAGGTTTCTGATTTCGGACTTTCGCGTGTCCTGGAGGATGACCCAGAAGCTGCTTATACAACAAGAGGAGGGAAGATCCCAATCAGGTGGACATCACCAGAAGCTATAGCCTACCGCAAGTTCACGTCAGCCAGCGATGTATGGAGTTATGGGATTGTTCTCTGGGAGGTGATGTCTTATGGAGAGAGACCATACTGGGAGATGTCCAATCAGGATGTAATTAAAGCTGTAGATGAGGGCTATCGACTGCCACCCCCCATGGACTGCCCAGCTGCCTTGTATCAGCTGATGCTGGACTGCTGGCAGAAAGACAGGAACAACAGACCCAAGTTTGAGCAGATTGTTAGTATTCTGGACAAGCTTATCCGGAATCCCGGCAGCCTGAAGATCATCACCAGTGCAGCCGCAAGGCCATCAAACCTTCTTCTGGACCAAAGCAATGTGGATATCACTACCTTCCGCACAACAGGTGACTGGCTTAATGGTGTCTGGACAGCACACTGCAAGGAAATCTTCACGGGTGTGGAGTACAGTTCTTGTGACACAATAGCCAAGATTTCC</t>
-  </si>
-  <si>
-    <t>MEKDGLCRADQQYECVAEIGEGAYGKVFKARDLKNGGRFVALKRVRVQTGEEGMPLSTIREVAVLRHLETFEHPNVVRLFDVCTVSRTDRETKLTLVFEHVDQDLTTYLDKVPEPGVPTETIKDMMFQLLRGLDFLHSHRVVHRDLKPQNILVTSSGQIKLADFGLARIYSFQMALTSVVVTLWYRAPEVLLQSSYATPVDLWSVGCIFAEMFRRKPLFRGSSDVDQLGKILDVIGLPGEEDWPRDVALPRQAFHSKSAQPIEKFVTDIDELGKDLLLKCLTFNPAKRISAYSALSHPYFQ</t>
-  </si>
-  <si>
-    <t>EPHA3_HUMAN_D0_4GK2_A</t>
-  </si>
-  <si>
-    <t>ATGCCCGGCCCGGCCGCGGGCAGCAGGGCCCGGGTCTACGCCGAGGTGAACAGTCTGAGGAGCCGCGAGTACTGGGACTACGAGGCTCACGTCCCGAGCTGGGGTAATCAAGATGATTACCAACTGGTTCGAAAACTTGGTCGGGGAAAATATAGTGAAGTATTTGAGGCCATTAATATCACCAACAATGAGAGAGTGGTTGTAAAAATCCTGAAGCCAGTGAAGAAAAAGAAGATAAAACGAGAGGTTAAGATTCTGGAGAACCTTCGTGGTGGAACAAATATCATTAAGCTGATTGACACTGTAAAGGACCCCGTGTCAAAGACACCAGCTTTGGTATTTGAATATATCAATAATACAGATTTTAAGCAACTCTACCAGATCCTGACAGACTTTGATATCCGGTTTTATATGTATGAACTACTTAAAGCTCTGGATTACTGCCACAGCAAGGGAATCATGCACAGGGATGTGAAACCTCACAATGTCATGATAGATCACCAACAGAAAAAGCTGCGACTGATAGATTGGGGTCTGGCAGAATTCTATCATCCTGCTCAGGAGTACAATGTTCGTGTAGCCTCAAGGTACTTCAAGGGACCAGAGCTCCTCGTGGACTATCAGATGTATGATTATAGCTTGGACATGTGGAGTTTGGGCTGTATGTTAGCAAGCATGATCTTTCGAAGGGAACCATTCTTCCATGGACAGGACAACTATGACCAGCTTGTTCGCATTGCCAAGGTTCTGGGTACAGAAGAACTGTATGGGTATCTGAAGAAGTATCACATAGACCTAGATCCACACTTCAACGATATCCTGGGACAACATTCACGGAAACGCTGGGAAAACTTTATCCATAGTGAGAACAGACACCTTGTCAGCCCTGAGGCCCTAGATCTTCTGGACAAACTTCTGCGATACGACCATCAACAGAGACTGACTGCCAAAGAGGCCATGGAGCACCCATACTTCTACCCTGTGGTGAAGGAGCAGTCCCAG</t>
-  </si>
-  <si>
-    <t>ATGTCGGGACCCGTGCCAAGCAGGGCCAGAGTTTACACAGATGTTAATACACACAGACCTCGAGAATACTGGGATTACGAGTCACATGTGGTGGAATGGGGAAATCAAGATGACTACCAGCTGGTTCGAAAATTAGGCCGAGGTAAATACAGTGAAGTATTTGAAGCCATCAACATCACAAATAATGAAAAAGTTGTTGTTAAAATTCTCAAGCCAGTAAAAAAGAAGAAAATTAAGCGTGAAATAAAGATTTTGGAGAATTTGAGAGGAGGTCCCAACATCATCACACTGGCAGACATTGTAAAAGACCCTGTGTCACGAACCCCCGCCTTGGTTTTTGAACACGTAAACAACACAGACTTCAAGCAATTGTACCAGACGTTAACAGACTATGATATTCGATTTTACATGTATGAGATTCTGAAGGCCCTGGATTATTGTCACAGCATGGGAATTATGCACAGAGATGTCAAGCCCCATAATGTCATGATTGATCATGAGCACAGAAAGCTACGACTAATAGACTGGGGTTTGGCTGAGTTTTATCATCCTGGCCAAGAATATAATGTCCGAGTTGCTTCCCGATACTTCAAAGGTCCTGAGCTACTTGTAGACTATCAGATGTACGATTATAGTTTGGATATGTGGAGTTTGGGTTGTATGCTGGCAAGTATGATCTTTCGGAAGGAGCCATTTTTCCATGGACATGACAATTATGATCAGTTGGTGAGGATAGCCAAGGTTCTGGGGACAGAAGATTTATATGACTATATTGACAAATACAACATTGAATTAGATCCACGTTTCAATGATATCTTGGGCAGACACTCTCGAAAGCGATGGGAACGCTTTGTCCACAGTGAAAATCAGCACCTTGTCAGCCCTGAGGCCTTGGATTTCCTGGACAAACTGCTGCGATATGACCACCAGTCACGGCTTACTGCAAGAGAGGCAATGGAGCACCCCTATTTCTACACTGTTGTGAAGGACCAGGCTCGAATGGGT</t>
-  </si>
-  <si>
-    <t>NEK2_HUMAN_D0_2XKE_A</t>
-  </si>
-  <si>
-    <t>MK01_HUMAN_D0_4FMQ_A</t>
-  </si>
-  <si>
-    <t>ATGGAGCTGAGAGTCGGGAACAGGTACCGGCTGGGCCGGAAGATCGGCAGCGGCTCCTTCGGAGACATCTATCTCGGTACGGACATTGCTGCAGGAGAAGAGGTTGCCATCAAGCTTGAATGTGTCAAAACCAAACACCCTCAGCTCCACATTGAGAGCAAAATCTACAAGATGATGCAGGGAGGAGTGGGCATCCCCACCATCAGATGGTGCGGGGCAGAGGGGGACTACAACGTCATGGTGATGGAGCTGCTGGGGCCAAGCCTGGAGGACCTCTTCAACTTCTGCTCCAGGAAATTCAGCCTCAAAACCGTCCTGCTGCTTGCTGACCAAATGATCAGTCGCATCGAATACATTCATTCAAAGAACTTCATCCACCGGGATGTGAAGCCAGACAACTTCCTCATGGGCCTGGGGAAGAAGGGCAACCTGGTGTACATCATCGACTTCGGGCTGGCCAAGAAGTACCGGGATGCACGCACCCACCAGCACATCCCCTATCGTGAGAACAAGAACCTCACGGGGACGGCGCGGTACGCCTCCATCAACACGCACCTTGGAATTGAACAATCCCGAAGAGATGACTTGGAGTCTCTGGGCTACGTGCTAATGTACTTCAACCTGGGCTCTCTCCCCTGGCAGGGGCTGAAGGCTGCCACCAAGAGACAGAAATACGAAAGGATTAGCGAGAAGAAAATGTCCACCCCCATCGAAGTGTTGTGTAAAGGCTACCCTTCCGAATTTGCCACATACCTGAATTTCTGCCGTTCCTTGCGTTTTGACGACAAGCCTGACTACTCGTACCTGCGGCAGCTTTTCCGGAATCTGTTCCATCGCCAGGGCTTCTCCTATGACTACGTGTTCGACTGGAACATGCTCAAA</t>
-  </si>
-  <si>
-    <t>ATGGCGGCGGCGGCGGCGGCGGGCGCGGGCCCGGAGATGGTCCGCGGGCAGGTGTTCGACGTGGGGCCGCGCTACACCAACCTCTCGTACATCGGCGAGGGCGCCTACGGCATGGTGTGCTCTGCTTATGATAATGTCAACAAAGTTCGAGTAGCTATCAAGAAAATCAGCCCCTTTGAGCACCAGACCTACTGCCAGAGAACCCTGAGGGAGATAAAAATCTTACTGCGCTTCAGACATGAGAACATCATTGGAATCAATGACATTATTCGAGCACCAACCATCGAGCAAATGAAAGATGTATATATAGTACAGGACCTCATGGAAACAGATCTTTACAAGCTCTTGAAGACACAACACCTCAGCAATGACCATATCTGCTATTTTCTCTACCAGATCCTCAGAGGGTTAAAATATATCCATTCAGCTAACGTTCTGCACCGTGACCTCAAGCCTTCCAACCTGCTGCTCAACACCACCTGTGATCTCAAGATCTGTGACTTTGGCCTGGCCCGTGTTGCAGATCCAGACCATGATCACACAGGGTTCCTGACAGAATATGTGGCCACACGTTGGTACAGGGCTCCAGAAATTATGTTGAATTCCAAGGGCTACACCAAGTCCATTGATATTTGGTCTGTAGGCTGCATTCTGGCAGAAATGCTTTCTAACAGGCCCATCTTTCCAGGGAAGCATTATCTTGACCAGCTGAACCACATTTTGGGTATTCTTGGATCCCCATCACAAGAAGACCTGAATTGTATAATAAATTTAAAAGCTAGGAACTATTTGCTTTCTCTTCCACACAAAAATAAGGTGCCATGGAACAGGCTGTTCCCAAATGCTGACTCCAAAGCTCTGGACTTATTGGACAAAATGTTGACATTCAACCCACACAAGAGGATTGAAGTAGAACAGGCTCTGGCCCACCCATATCTGGAGCAGTATTACGACCCGAGTGACGAGCCCATCGCCGAAGCACCATTCAAGTTCGACATGGAATTGGATGACTTGCCTAAGGAAAAGCTCAAAGAACTAATTTTTGAAGAGACTGCTAGATTCCAGCCAGGATACAGATCT</t>
-  </si>
-  <si>
-    <t>MDEQSQGMQGPPVPQFQPQKALRPDMGYNTLANFRIEKKIGRGQFSEVYRAACLLDGVPVALKKVQIFDLMDAKARADCIKEIDLLKQLNHPNVIKYYASFIEDNELNIVLELADAGDLSRMIKHFKKQKRLIPERTVWKYFVQLCSALEHMHSRRVMHRDIKPANVFITATGVVKLGDLGLGRFFSSKTTAAHSLVGTPYYMSPERIHENGYNFKSDIWSLGCLLYEMAALQSPFYGDKMNLYSLCKKIEQCDYPPLPSDHYSEELRQLVNMCINPDPEKRPDVTYVYDVAKRMHACTASS</t>
-  </si>
-  <si>
-    <t>GECSQKGPVPFSHCLPTEKLQRCEKIGEGVFGEVFQTIADHTPVAIKIIAIEGPDLVNGSHQKTFEEILPEIIISKELSLLSGEVCNRTEGFIGLNSVHCVQGSYPPLLLKAWDHYNSTKGSANDRPDFFKDDQLFIVLEFEFGGIDLEQMRTKLSSLATAKSILHQLTASLAVAEASLRFEHRDLHWGNVLLKKTSLKKLHYTLNGKSSTIPSCGLQVSIIDYTLSRLERDGIVVFCDVSMDEDLFTGDGDYQFDIYRLMKKENNNRWGEYHPYSNVLWLHYLTDKMLKQMTFKTKCNTPAMKQIKRKIQEFHRTMLNFSSATDLLCQHRLFK</t>
-  </si>
-  <si>
-    <t>MENFNNFYILTSKELGRGKFAVVRQCISKSTGQEYAAKFLKKRRRGQDCRAEILHEIAVLELAKSCPRVINLHEVYENTSEIILILEYAAGGEIFSLCLPELAEMVSENDVIRLIKQILEGVYYLHQNNIVHLDLKPQNILLSSIYPLGDIKIVDFGMSRKIGHACELREIMGTPEYLAPEILNYDPITTATDMWNIGIIAYMLLTHTSPFVGEDNQETYLNISQVNVDYSEETFSSVSQLATDFIQSLLVKNPEKRPTAEICLSHSWLQQWDFENLFHPEETSSSSQTQDHSVRSSEDKTSKSS</t>
-  </si>
-  <si>
-    <t>CHK1_HUMAN_D0_2E9V_A</t>
-  </si>
-  <si>
-    <t>MELRVGNKYRLGRKIGSGSFGDIYLGANIASGEEVAIKLECVKTKHPQLHIESKFYKMMQGGVGIPSIKWCGAEGDYNVMVMELLGPSLEDLFNFCSRKFSLKTVLLLADQMISRIEYIHSKNFIHRDVKPDNFLMGLGKKGNLVYIIDFGLAKKYRDARTHQHIPYRENKNLTGTARYASINTHLGIEQSRRDDLESLGYVLMYFNLGSLPWQGLKAATKRQKYERISEKKMSTPIEVLCKGYPSEFSTYLNFCRSLRFDDKPDYSYLRQLFRNLFHRQGFSYDYVFDWNMLK</t>
-  </si>
-  <si>
-    <t>SSVTASAAPGTASLVPDYWIDGSNRDALSDFFEVESELGRGATSIVYRCKQKGTQKPYALKVLKKTVDKKIVRTEIGVLLRLSHPNIIKLKEIFETPTEISLVLELVTGGELFDRIVEKGYYSERDAADAVKQILEAVAYLHENGIVHRDLKPENLLYATPAPDAPLKIADFGLSKIVEHQVLMKTVCGTPGYCAPEILRGCAYGPEVDMWSVGIITYILLCGFEPFYDERGDQFMFRRILNCEYYFISPWWDEVSLNAKDLVRKLIVLDPKKRLTTFQALQHPWVTGKAANFVHMDTAQKKLQEFNARRKLKAAVKAVVASSRLG</t>
-  </si>
-  <si>
-    <t>dna_end</t>
-  </si>
-  <si>
-    <t>MADDDVLFEDVYELCEVIGKGPFSVVRRCINRETGQQFAVKIVDVAKFTSSPGLSTEDLKREASICHMLKHPHIVELLETYSSDGMLYMVFEFMDGADLCFEIVKRADAGFVYSEAVASHYMRQILEALRYCHDNNIIHRDVKPHCVLLASKENSAPVKLGGFGVAIQLGESGLVAGGRVGTPHFMAPEVVKREPYGKPVDVWGCGVILFILLSGCLPFYGTKERLFEGIIKGKYKMNPRQWSHISESAKDLVRRMLMLDPAERITVYEALNHPWLKERDRYAYKIHLPETVEQLRKFNARRKLKGAVLAAVSSHKFNSFYGDPPEELPDFSEDPTSSGA</t>
-  </si>
-  <si>
-    <t>FAK1_HUMAN_D0_2IJM_B</t>
-  </si>
-  <si>
-    <t>CHK2_HUMAN_D0_2CN5_A</t>
-  </si>
-  <si>
-    <t>GTGATCGACCCCTCAGAGCTCACTTTTGTCCAAGAGATTGGCAGTGGGCAATTTGGGTTGGTGCATCTGGGCTACTGGCTCAACAAGGACAAGGTGGCTATCAAAACCATTCGGGAAGGGGCTATGTCAGAAGAGGACTTCATAGAGGAGGCTGAAGTAATGATGAAACTCTCTCATCCCAAACTGGTGCAGCTGTATGGGGTGTGCCTGGAGCAGGCCCCCATCTGCCTGGTGTTTGAGTTCATGGAGCACGGCTGCCTGTCAGATTATCTACGCACCCAGCGGGGACTTTTTGCTGCAGAGACCCTGCTGGGCATGTGTCTGGATGTGTGTGAGGGCATGGCCTACCTGGAAGAGGCATGTGTCATCCACAGAGACTTGGCTGCCAGAAATTGTTTGGTGGGAGAAAACCAAGTCATCAAGGTGTCTGACTTTGGGATGACAAGGTTCGTTCTGGATGATCAGTACACCAGTTCCACAGGCACCAAATTCCCGGTGAAGTGGGCATCCCCAGAGGTTTTCTCTTTCAGTCGCTATAGCAGCAAGTCCGATGTGTGGTCATTTGGTGTGCTGATGTGGGAAGTTTTCAGTGAAGGCAAAATCCCGTATGAAAACCGAAGCAACTCAGAGGTGGTGGAAGACATCAGTACCGGATTTCGGTTGTACAAGCCCCGGCTGGCCTCCACACACGTCTACCAGATTATGAATCACTGCTGGAAAGAGAGACCAGAAGATCGGCCAGCCTTCTCCAGACTGCTGCGTCAACTGGCTGAAATTGCAGAATCAGGACTT</t>
-  </si>
-  <si>
-    <t>MSDEEILEKLRSIVSVGDPKKKYTRFEKIGQGASGTVYTAMDVATGQEVAIKQMNLQQQPKKELIINEILVMRENKNPNIVNYLDSYLVGDELWVVMEYLAGGSLTDVVTETCMDEGQIAAVCRECLQALEFLHSNQVIHRDIKSDNILLGMDGSVKLTDFGFCAQITPEQSKRSTMVGTPYWMAPEVVTRKAYGPKVDIWSLGIKAIEMIEGEPPYLNENPLRALYLIATNGTPELQNPEKLSAIFRDFLNRCLEMDVEKRGSAKELLQHQFLKIAKPLSSLTPLIAAAKEATKNNH</t>
-  </si>
-  <si>
-    <t>MSQSKGKKRNPGLKIPKEAFEQPQTSSTPPRDLDSKACISIGNQNFEVKADDLEPIMELGRGAYGVVEKMRHVPSGQIMAVKRIRATVNSQEQKRLLMDLDISMRTVDCPFTVTFYGALFREGDVWICMELMDTSLDKFYKQVIDKGQTIPEDILGKIAVSIVKALEHLHSKLSVIHRDVKPSNVLINALGQVKMCDFGISGYLVDSVAKTIDAGCKPYMAPERINPELNQKGYSVKSDIWSLGITMIELAILRFPYDSWGTPFQQLKQVVEEPSPQLPADKFSAEFVDFTSQCLKKNSKERPTYPELMQHPFFTLHESKGTDVASFVKLILGD</t>
-  </si>
-  <si>
-    <t>DYRK2_HUMAN_D0_3KVW_A</t>
-  </si>
-  <si>
-    <t>QSSKRSSRSVEDDKEGHLVCRIGDWLQERYEIVGNLGEGTFGKVVECLDHARGKSQVALKIIRNVGKYREAARLEINVLKKIKEKDKENKFLCVLMSDWFNFHGHMCIAFELLGKNTFEFLKENNFQPYPLPHVRHMAYQLCHALRFLHENQLTHTDLKPENILFVNSEFETLYNEHKSCEEKSVKNTSIRVADFGSATFDHEHHTTIVATRHYRPPEVILELGWAQPCDVWSIGCILFEYYRGFTLFQTHENREHLVMMEKILGPIPSHMIHRTRKQKYFYKGGLVWDENSSDGRYVKENCKPLKSYMLQDSLEHVQLFDLMRRMLEFDPAQRITLAEALLHPFFAGLTPEERSFHT</t>
-  </si>
-  <si>
-    <t>MK07_HUMAN_D0_4IC7_D</t>
-  </si>
-  <si>
-    <t>ATGCAGACAGTTGGTGTACATTCAATTGTTCAGCAGTTACACAGGAACAGTATTCAGTTTACTGATGGATATGAAGTAAAAGAAGATATTGGAGTTGGCTCCTACTCTGTTTGCAAGAGATGTATACATAAAGCTACAAACATGGAGTTTGCAGTGAAGATTATTGATAAAAGCAAGAGAGACCCAACAGAAGAAATTGAAATTCTTCTTCGTTATGGACAGCATCCAAACATTATCACTCTAAAGGATGTATATGATGATGGAAAGTATGTGTATGTAGTAACAGAACTTATGAAAGGAGGTGAATTGCTGGATAAAATTCTTAGACAAAAATTTTTCTCTGAACGAGAGGCCAGTGCTGTCCTGTTCACTATAACTAAAACCGTTGAATATCTTCACGCACAAGGGGTGGTTCATAGAGACTTGAAACCTAGCAACATTCTTTATGTGGATGAATCTGGTAATCCGGAATCTATTCGAATTTGTGATTTTGGCTTTGCAAAACAGCTGAGAGCGGAAAATGGTCTTCTCATGACTCCTTGTTACACTGCAAATTTTGTTGCACCAGAGGTTTTAAAAAGACAAGGCTATGATGCTGCTTGTGATATATGGAGTCTTGGTGTCCTACTCTATACAATGCTTACCGGTTACACTCCATTTGCAAATGGTCCTGATGATACACCAGAGGAAATATTGGCACGAATAGGTAGCGGAAAATTCTCACTCAGTGGTGGTTACTGGAATTCTGTTTCAGACACAGCAAAGGACCTGGTGTCAAAGATGCTTCATGTAGACCCTCATCAGAGACTGACTGCTGCTCTTGTGCTCAGACATCCTTGGATCGTCCACTGGGACCAACTGCCACAATACCAACTAAACAGACAGGATGCACCACATCTAGTAAAGGGTGCCATGGCAGCTACATATTCTGCTTTGAACCGTAATCAGTCACCAGTTTTGGAACCAGTAGGCCGCTCTACTCTTGCTCAGCGGAGAGGTATTAAAAAAATCACCTCAACAGCCCTG</t>
-  </si>
-  <si>
-    <t>MGKVKATPMTPEQAMKQYMQKLTAFEHHEIFSYPEIYFLGLNAKKRQGMTGGPNNGGYDDDQGSYVQVPHDHVAYRYEVLKVIGKGSFGQVVKAYDHKVHQHVALKMVRNEKRFHRQAAEEIRILEHLRKQDKDNTMNVIHMLENFTFRNHICMTFELLSMNLYELIKKNKFQGFSLPLVRKFAHSILQCLDALHKNRIIHCDLKPENILLKQQGRSGIKVIDFGSSCYEHQRVYTYIQSRFYRAPEVILGARYGMPIDMWSLGCILAELLTGYPLLPGEDEGDQLACMIELLGMPSQKLLDASKRAKNFVSSKGYPRYCTVTTLSDGSVVLNGGRSRRGKLRGPPESREWGNALKGCDDPLFLDFLKQCLEWDPAVRMTPGQALRHPWLRRRLPKPPTGEKTSVKR</t>
-  </si>
-  <si>
-    <t>CAGCAGTTCCCGCAGTTCCACGTCAAGTCCGGCCTGCAGATCAAGAAGAACGCCATCATCGATGACTACAAGGTCACCAGCCAGGTCCTGGGGCTGGGCATCAACGGCAAAGTTTTGCAGATCTTCAACAAGAGGACCCAGGAGAAATTCGCCCTCAAAATGCTTCAGGACTGCCCCAAGGCCCGCAGGGAGGTGGAGCTGCACTGGCGGGCCTCCCAGTGCCCGCACATCGTACGGATCGTGGATGTGTACGAGAATCTGTACGCAGGGAGGAAGTGCCTGCTGATTGTCATGGAATGTTTGGACGGTGGAGAACTCTTTAGCCGAATCCAGGATCGAGGAGACCAGGCATTCACAGAAAGAGAAGCATCCGAAATCATGAAGAGCATCGGTGAGGCCATCCAGTATCTGCATTCAATCAACATTGCCCATCGGGATGTCAAGCCTGAGAATCTCTTATACACCTCCAAAAGGCCCAACGCCATCCTGAAACTCACTGACTTTGGCTTTGCCAAGGAAACCACCAGCCACAACTCTTTGACCACTCCTTGTTATACACCGTACTATGTGGCTCCAGAAGTGCTGGGTCCAGAGAAGTATGACAAGTCCTGTGACATGTGGTCCCTGGGTGTCATCATGTACATCCTGCTGTGTGGGTATCCCCCCTTCTACTCCAACCACGGCCTTGCCATCTCTCCGGGCATGAAGACTCGCATCCGAATGGGCCAGTATGAATTTCCCAACCCAGAATGGTCAGAAGTATCAGAGGAAGTGAAGATGCTCATTCGGAATCTGCTGAAAACAGAGCCCACCCAGAGAATGACCATCACCGAGTTTATGAACCACCCTTGGATCATGCAATCAACAAAGGTCCCTCAAACCCCACTGCACACCAGCCGGGTCCTGAAGGAGGACAAGGAGCGGTGGGAGGATGTCAAGGGGTGTCTTCATGACAAGAACAGCGACCAGGCC</t>
-  </si>
-  <si>
-    <t>CDK2_HUMAN_D0_4BCP_A</t>
-  </si>
-  <si>
-    <t>MP2K4_HUMAN_D0_3ALN_C</t>
-  </si>
-  <si>
-    <t>ACCACCTCACTTGAAGCTTTGCCCACAGGGACAGTGCTGACAGACAAGAGTGGGCGACAGTGGAAGCTGAAGTCCTTCCAGACCAGGGACAACCAGGGCATTCTCTATGAAGCTGCACCCACCTCCACCCTCACCTGTGACTCAGGACCACAGAAGCAAAAGTTCTCACTCAAACTGGATGCCAAGGATGGGCGCTTGTTCAATGAGCAGAACTTCTTCCAGCGGGCCGCCAAGCCTCTGCAAGTCAACAAGTGGAAGAAGCTGTACTCGACCCCACTGCTGGCCATCCCTACCTGCATGGGTTTCGGTGTTCACCAGGACAAATACAGGTTCTTGGTGTTACCCAGCCTGGGGAGGAGCCTTCAGTCGGCCCTGGATGTCAGCCCAAAGCATGTGCTGTCAGAGAGGTCTGTGCTGCAGGTGGCCTGCCGGCTGCTGGATGCCCTGGAGTTCCTCCATGAGAATGAGTATGTTCATGGAAATGTGACAGCTGAAAATATCTTTGTGGATCCAGAGGACCAGAGTCAGGTGACTTTGGCAGGCTATGGCTTCGCCTTCCGCTATTGCCCAAGTGGCAAACACGTGGCCTACGTGGAAGGCAGCAGGAGCCCTCACGAGGGGGACCTTGAGTTCATTAGCATGGACCTGCACAAGGGATGCGGGCCCTCCCGCCGCAGCGACCTCCAGAGCCTGGGCTACTGCATGCTGAAGTGGCTCTACGGGTTTCTGCCATGGACAAATTGCCTTCCCAACACTGAGGACATCATGAAGCAAAAACAGAAGTTTGTTGATAAGCCGGGGCCCTTCGTGGGACCCTGCGGTCACTGGATCAGGCCCTCAGAGACCCTGCAGAAGTACCTGAAGGTGGTGATGGCCCTCACGTATGAGGAGAAGCCGCCCTACGCCATGCTGAGGAACAACCTAGAAGCTTTGCTGCAGGATCTGCGTGTGTCTCCATATGACCCCATTGGCCTCCCGATGGTGCCC</t>
-  </si>
-  <si>
-    <t>TCACCACAGCGGGAGCCACAGCGAGTATCCCATGAGCAGTTCCGGGCTGCCCTGCAGCTGGTGGTGGACCCAGGCGACCCCCGCTCCTACCTGGACAACTTCATCAAGATTGGCGAGGGCTCCACGGGCATCGTGTGCATCGCCACCGTGCGCAGCTCGGGCAAGCTGGTGGCCGTCAAGAAGATGGACCTGCGCAAGCAGCAGAGGCGCGAGCTGCTCTTCAACGAGGTGGTAATCATGAGGGACTACCAGCACGAGAATGTGGTGGAGATGTACAACAGCTACCTGGTGGGGGACGAGCTCTGGGTGGTCATGGAGTTCCTGGAAGGAGGCGCCCTCACCGACATCGTCACCCACACCAGGATGAACGAGGAGCAGATCGCGGCCGTGTGCCTTGCAGTGCTGCAGGCCCTGTCGGTGCTCCACGCCCAGGGCGTCATCCACCGGGACATCAAGAGCGACTCGATCCTGCTGACCCATGATGGCAGGGTGAAGCTGTCAGACTTTGGGTTCTGCGCCCAGGTGAGCAAGGAAGTGCCCCGAAGGAAGTCGCTGGTCGGCACGCCCTACTGGATGGCCCCAGAGCTCATCTCCCGCCTTCCCTACGGGCCAGAGGTAGACATCTGGTCGCTGGGGATAATGGTGATTGAGATGGTGGACGGAGAGCCCCCCTACTTCAACGAGCCACCCCTCAAAGCCATGAAGATGATTCGGGACAACCTGCCACCCCGACTGAAGAACCTGCACAAGGTGTCGCCATCCCTGAAGGGCTTCCTGGACCGCCTGCTGGTGCGAGACCCTGCCCAGCGGGCCACGGCAGCCGAGCTGCTGAAGCACCCATTCCTGGCCAAGGCAGGGCCGCCTGCCAGCATCGTGCCCCTCATGCGCCAGAACCGCACCAGA</t>
-  </si>
-  <si>
-    <t>SIESSGKLKISPEQHWDFTAEDLKDLGEIGRGAYGSVNKMVHKPSGQIMAVKRIRSTVDEKEQKQLLMDLDVVMRSSDCPYIVQFYGALFREGDCWICMELMSTSFDKFYKYVYSVLDDVIPEEILGKITLATVKALNHLKENLKIIHRDIKPSNILLDRSGNIKLCDFGISGQLVDSIAKTRDAGCRPYMAPERIDPSASRQGYDVRSDVWSLGITLYELATGRFPYPKWNSVFDQLTQVVKGDPPQLSNSEEREFSPSFINFVNLCLTKDESKRPKYKELLKHPFILMYEERAVEVACYVCKILDQMPATPSSPMYVD</t>
-  </si>
-  <si>
-    <t>TDSFSGRFEDVYQLQEDVLGEGAHARVQTCINLITSQEYAVKIIEKQPGHIRSRVFREVEMLYQCQGHRNVLELIEFFEEEDRFYLVFEKMRGGSILSHIHKRRHFNELEASVVVQDVASALDFLHNKGIAHRDLKPENILCEHPNQVSPVKICDFDLGSGIKLNGDCSPISTPELLTPCGSAEYMAPEVVEAFSEEASIYDKRCDLWSLGVILYILLSGYPPFVGRCGSDCGWDRGEACPACQNMLFESIQEGKYEFPDKDWAHISCAAKDLISKLLVRDAKQRLSAAQVLQHPWVQGCAPENTLPTPMVLQR</t>
-  </si>
-  <si>
-    <t>WALNMKELKLLQTIGKGEFGDVMLGDYRGNKVAVKCIKNDATAQAFLAEASVMTQLRHSNLVQLLGVIVEEKGGLYIVTEYMAKGSLVDYLRSRGRSVLGGDCLLKFSLDVCEAMEYLEGNNFVHRDLAARNVLVSEDNVAKVSDFGLTKEASSTQDTGKLPVKWTAPEALREKKFSTKSDVWSFGILLWEIYSFGRVPYPRIPLKDVVPRVEKGYKMDAPDGCPPAVYEVMKNCWHLDAAMRPSFLQLREQLEHIKTHELHL</t>
-  </si>
-  <si>
-    <t>MPGPAAGSRARVYAEVNSLRSREYWDYEAHVPSWGNQDDYQLVRKLGRGKYSEVFEAINITNNERVVVKILKPVKKKKIKREVKILENLRGGTNIIKLIDTVKDPVSKTPALVFEYINNTDFKQLYQILTDFDIRFYMYELLKALDYCHSKGIMHRDVKPHNVMIDHQQKKLRLIDWGLAEFYHPAQEYNVRVASRYFKGPELLVDYQMYDYSLDMWSLGCMLASMIFRREPFFHGQDNYDQLVRIAKVLGTEELYGYLKKYHIDLDPHFNDILGQHSRKRWENFIHSENRHLVSPEALDLLDKLLRYDHQQRLTAKEAMEHPYFYPVVKEQSQ</t>
-  </si>
-  <si>
-    <t>AAGAGGCAGTGGGCTTTGGAAGACTTTGAAATTGGTCGCCCTCTGGGTAAAGGAAAGTTTGGTAATGTTTATTTGGCAAGAGAAAAGCAAAGCAAGTTTATTCTGGCTCTTAAAGTGTTATTTAAAGCTCAGCTGGAGAAAGCCGGAGTGGAGCATCAGCTCAGAAGAGAAGTAGAAATACAGTCCCACCTTCGGCATCCTAATATTCTTAGACTGTATGGTTATTTCCATGATGCTACCAGAGTCTACCTAATTCTGGAATATGCACCACTTGGAACAGTTTATAGAGAACTTCAGAAACTTTCAAAGTTTGATGAGCAGAGAACTGCTACTTATATAACAGAATTGGCAAATGCCCTGTCTTACTGTCATTCGAAGAGAGTTATTCATAGAGACATTAAGCCAGAGAACTTACTTCTTGGATCAGCTGGAGAGCTTAAAATTGCAGATTTTGGGTGGTCAGTACATGCTCCATCTTCCAGGAGGACCACTCTCTGTGGCACCCTGGACTACCTGCCCCCTGAAATGATTGAAGGTCGGATGCATGATGAGAAGGTGGATCTCTGGAGCCTTGGAGTTCTTTGCTATGAATTTTTAGTTGGGAAGCCTCCTTTTGAGGCAAACACATACCAAGAGACCTACAAAAGAATATCACGGGTTGAATTCACATTCCCTGACTTTGTAACAGAGGGAGCCAGGGACCTCATTTCAAGACTGTTGAAGCATAATCCCAGCCAGAGGCCAATGCTCAGAGAAGTACTTGAACACCCCTGGATCACAGCAAATTCATCAAAACCATCA</t>
-  </si>
-  <si>
-    <t>ATGGAGCTACGTGTGGGGAACAAGTACCGCCTGGGACGGAAGATCGGGAGCGGGTCCTTCGGAGATATCTACCTGGGTGCCAACATCGCCTCTGGTGAGGAAGTCGCCATCAAGCTGGAGTGTGTGAAGACAAAGCACCCCCAGCTGCACATCGAGAGCAAGTTCTACAAGATGATGCAGGGTGGCGTGGGGATCCCGTCCATCAAGTGGTGCGGAGCTGAGGGCGACTACAACGTGATGGTCATGGAGCTGCTGGGGCCTAGCCTCGAGGACCTGTTCAACTTCTGTTCCCGCAAATTCAGCCTCAAGACGGTGCTGCTCTTGGCCGACCAGATGATCAGCCGCATCGAGTATATCCACTCCAAGAACTTCATCCACCGGGACGTCAAGCCCGACAACTTCCTCATGGGGCTGGGGAAGAAGGGCAACCTGGTCTACATCATCGACTTCGGCCTGGCCAAGAAGTACCGGGACGCCCGCACCCACCAGCACATTCCCTACCGGGAAAACAAGAACCTGACCGGCACGGCCCGCTACGCTTCCATCAACACGCACCTGGGCATTGAGCAAAGCCGTCGAGATGACCTGGAGAGCCTGGGCTACGTGCTCATGTACTTCAACCTGGGCTCCCTGCCCTGGCAGGGGCTCAAAGCAGCCACCAAGCGCCAGAAGTATGAACGGATCAGCGAGAAGAAGATGTCAACGCCCATCGAGGTCCTCTGCAAAGGCTATCCCTCCGAATTCTCAACATACCTCAACTTCTGCCGCTCCCTGCGGTTTGACGACAAGCCCGACTACTCTTACCTACGTCAGCTCTTCCGCAACCTCTTCCACCGGCAGGGCTTCTCCTATGACTACGTCTTTGACTGGAACATGCTGAAA</t>
-  </si>
-  <si>
-    <t>MK03_HUMAN_D0_2ZOQ_B</t>
-  </si>
-  <si>
-    <t>ATGTCTCAGTCGAAAGGCAAGAAGCGAAACCCTGGCCTTAAAATTCCAAAAGAAGCATTTGAACAACCTCAGACCAGTTCCACACCACCTCGAGATTTAGACTCCAAGGCTTGCATTTCTATTGGAAATCAGAACTTTGAGGTGAAGGCAGATGACCTGGAGCCTATAATGGAACTGGGACGAGGTGCGTACGGGGTGGTGGAGAAGATGCGGCACGTGCCCAGCGGGCAGATCATGGCAGTGAAGCGGATCCGAGCCACAGTAAATAGCCAGGAACAGAAACGGCTACTGATGGATTTGGATATTTCCATGAGGACGGTGGACTGTCCATTCACTGTCACCTTTTATGGCGCACTGTTTCGGGAGGGTGATGTGTGGATCTGCATGGAGCTCATGGATACATCACTAGATAAATTCTACAAACAAGTTATTGATAAAGGCCAGACAATTCCAGAGGACATCTTAGGGAAAATAGCAGTTTCTATTGTAAAAGCATTAGAACATTTACATAGTAAGCTGTCTGTCATTCACAGAGACGTCAAGCCTTCTAATGTACTCATCAATGCTCTCGGTCAAGTGAAGATGTGCGATTTTGGAATCAGTGGCTACTTGGTGGACTCTGTTGCTAAAACAATTGATGCAGGTTGCAAACCATACATGGCCCCTGAAAGAATAAACCCAGAGCTCAACCAGAAGGGATACAGTGTGAAGTCTGACATTTGGAGTCTGGGCATCACGATGATTGAGTTGGCCATCCTTCGATTTCCCTATGATTCATGGGGAACTCCATTTCAGCAGCTCAAACAGGTGGTAGAGGAGCCATCGCCACAACTCCCAGCAGACAAGTTCTCTGCAGAGTTTGTTGACTTTACCTCACAGTGCTTAAAGAAGAATTCCAAAGAACGGCCTACATACCCAGAGCTAATGCAACATCCATTTTTCACCCTACATGAATCCAAAGGAACAGATGTGGCATCTTTTGTAAAACTGATTCTTGGAGAC</t>
-  </si>
-  <si>
-    <t>TCAACCAGGGATTATGAGATTCAAAGAGAAAGAATAGAACTTGGACGATGTATTGGAGAAGGCCAATTTGGAGATGTACATCAAGGCATTTATATGAGTCCAGAGAATCCAGCTTTGGCGGTTGCAATTAAAACATGTAAAAACTGTACTTCGGACAGCGTGAGAGAGAAATTTCTTCAAGAAGCCTTAACAATGCGTCAGTTTGACCATCCTCATATTGTGAAGCTGATTGGAGTCATCACAGAGAATCCTGTCTGGATAATCATGGAGCTGTGCACACTTGGAGAGCTGAGGTCATTTTTGCAAGTAAGGAAATACAGTTTGGATCTAGCATCTTTGATCCTGTATGCCTATCAGCTTAGTACAGCTCTTGCATATCTAGAGAGCAAAAGATTTGTACACAGGGACATTGCTGCTCGGAATGTTCTGGTGTCCTCAAATGATTGTGTAAAATTAGGAGACTTTGGATTATCCCGATATATGGAAGATAGTACTTACTACAAAGCTTCCAAAGGAAAATTGCCTATTAAATGGATGGCTCCAGAGTCAATCAATTTTCGACGTTTTACCTCAGCTAGTGACGTATGGATGTTTGGTGTGTGTATGTGGGAGATACTGATGCATGGTGTGAAGCCTTTTCAAGGAGTGAAGAACAATGATGTAATCGGTCGAATTGAAAATGGGGAAAGATTACCAATGCCTCCAAATTGTCCTCCTACCCTCTACAGCCTTATGACGAAATGCTGGGCCTATGACCCCAGCAGGCGGCCCAGGTTTACTGAACTTAAAGCTCAGCTCAGCACAATCCTGGAGGAAGAGAAGGCTCAGCAAGAAGAG</t>
-  </si>
-  <si>
-    <t>DPEELFTKLEKIGKGSFGEVFKGIDNRTQKVVAIKIIDLEEAEDEIEDIQQEITVLSQCDSPYVTKYYGSYLKDTKLWIIMEYLGGGSALDLLEPGPLDETQIATILREILKGLDYLHSEKKIHRDIKAANVLLSEHGEVKLADFGVAGQLTDTQIKRNTFVGTPFWMAPEVIKQSAYDSKADIWSLGITAIELARGEPPHSELHPMKVLFLIPKNNPPTLEGNYSKPLKEFVEACLNKEPSFRPTAKELLKHKFILRNAKKTSYLTELID</t>
-  </si>
-  <si>
-    <t>MAPK3_HUMAN_D0_3FXW_A</t>
-  </si>
-  <si>
-    <t>AAGCAGTACGAACACGTGAAGAGGGACCTGAACCCCGAAGACTTTTGGGAGATTATAGGAGAACTGGGCGACGGAGCCTTTGGGAAAGTGTACAAGGCCCAGAATAAAGAGACCAGTGTTTTAGCTGCTGCAAAAGTGATTGACACTAAATCTGAAGAAGAACTTGAAGATTACATGGTAGAGATTGACATATTAGCATCTTGTGATCACCCAAATATAGTCAAGCTTCTAGATGCCTTCTATTATGAGAACAATCTTTGGATCCTCATTGAATTTTGTGCAGGTGGAGCAGTAGATGCTGTGATGCTTGAACTTGAGAGACCATTAACTGAGTCCCAAATACAAGTAGTTTGCAAGCAGACTTTAGATGCATTGAACTACTTACATGATAATAAGATCATCCACAGAGATCTGAAGGCTGGCAACATTCTCTTTACCTTAGATGGAGATATCAAATTGGCGGATTTTGGAGTATCAGCTAAAAACATGAGGACAATTCAAAGAAGAGATTCCTTTATTGGTACACCATATTGGATGGCTCCTGAAGTAGTCATGTGTGAAACATCTAAGGACAGACCCTATGACTACAAAGCTGATGTTTGGTCCCTGGGTATCACTTTAATAGAAATGGCTGAGATAGAACCACCTCATCATGAATTAAATCCAATGCGAGTGCTGCTAAAAATAGCAAAATCTGAGCCACCTACATTAGCACAGCCATCCAGATGGTCTTCAAATTTTAAGGACTTTCTAAAGAAATGCTTAGAAAAGAATGTGGATGCCAGGTGGACTACATCTCAGCTGCTGCAGCATCCCTTTGTTACTGTTGATTCCAACAAACCCATCCGAGAATTGATTGCAGAGGCGAAGGCTGAAGTAACAGAAGAAGTTGAAGATGGCAAAGAG</t>
-  </si>
-  <si>
-    <t>ATGCCTTCCCGGGCTGAGGACTATGAAGTGTTGTACACCATTGGCACAGGCTCCTACGGCCGCTGCCAGAAGATCCGGAGGAAGAGTGATGGCAAGATATTAGTTTGGAAAGAACTTGACTATGGCTCCATGACAGAAGCTGAGAAACAGATGCTTGTTTCTGAAGTGAATTTGCTTCGTGAACTGAAACATCCAAACATCGTTCGTTACTATGATCGGATTATTGACCGGACCAATACAACACTGTACATTGTAATGGAATATTGTGAAGGAGGGGATCTGGCTAGTGTAATTACAAAGGGAACCAAGGAAAGGCAATACTTAGATGAAGAGTTTGTTCTTCGAGTGATGACTCAGTTGACTCTGGCCCTGAAGGAATGCCACAGACGAAGTGATGGTGGTCATACCGTATTGCATCGGGATCTGAAACCAGCCAATGTTTTCCTGGATGGCAAGCAAAACGTCAAGCTTGGAGACTTTGGGCTAGCTAGAATATTAAACCATGACACGAGTTTTGCAAAAACATTTGTTGGCACACCTTATTACATGTCTCCTGAACAAATGAATCGCATGTCCTACAATGAGAAATCAGATATCTGGTCATTGGGCTGCTTGCTGTATGAGTTATGTGCATTAATGCCTCCATTTACAGCTTTTAGCCAGAAAGAACTCGCTGGGAAAATCAGAGAAGGCAAATTCAGGCGAATTCCATACCGTTACTCTGATGAATTGAATGAAATTATTACGAGGATGTTAAACTTAAAGGATTACCATCGACCTTCTGTTGAAGAAATTCTTGAGAACCCTTTAATA</t>
-  </si>
-  <si>
-    <t>STK3_HUMAN_D0_4LG4_B</t>
-  </si>
-  <si>
-    <t>GATGAACAACCTCACATCGGAAACTACAGACTGTTGAAAACAATCGGCAAGGGGAATTTTGCAAAAGTAAAATTGGCAAGACATATCCTTACAGGCAGAGAGGTTGCAATAAAAATAATTGACAAAACTCAGTTGAATCCAACAAGTCTACAAAAGCTCTTCAGAGAAGTAAGAATAATGAAGATTTTAAATCATCCCAATATAGTGAAGTTATTCGAAGTCATTGAAACTGAAAAAACACTCTACCTAATCATGGAATATGCAAGTGGAGGTGAAGTATTTGACTATTTGGTTGCACATGGCAGGATGAAGGAAAAAGAAGCAAGATCTAAATTTAGACAGATTGTGTCTGCAGTTCAATACTGCCATCAGAAACGGATCGTACATCGAGACCTCAAGGCTGAAAATCTATTGTTAGATGCCGATATGAACATTAAAATAGCAGATTTCGGTTTTAGCAATGAATTTACTGTTGGCGGTAAACTCGACACGTTTTGTGGCAGTCCTCCATACGCAGCACCTGAGCTCTTCCAGGGCAAGAAATATGACGGGCCAGAAGTGGATGTGTGGAGTCTGGGGGTCATTTTATACACACTAGTCAGTGGCTCACTTCCCTTTGATGGGCAAAACCTAAAGGAACTGAGAGAGAGAGTATTAAGAGGGAAATACAGAATTCCCTTCTACATGTCTACAGACTGTGAAAACCTTCTCAAACGTTTCCTGGTGCTAAATCCAATTAAACGCGGCACTCTAGAGCAAATCATGAAGGACAGGTGGATCAATGCAGGGCATGAAGAAGATGAACTCAAACCATTTGTTGAACCAGAGCTAGACATCTCAGACCAAAAAAGAATAGATATTATGGTGGGAATGGGATATTCACAAGAAGAAATTCAAGAATCTCTTAGTAAGATGAAATACGATGAAATCACAGCTACATATTTGTTATTGGGGAGAAAATCTTCAGAG</t>
-  </si>
-  <si>
-    <t>dna_start</t>
-  </si>
-  <si>
-    <t>KEKEPLESQYQVGPLLGSGGFGSVYSGIRVSDNLPVAIKHVEKDRISDWGELPNGTRVPMEVVLLKKVSSGFSGVIRLLDWFERPDSFVLILERPEPVQDLFDFITERGALQEELARSFFWQVLEAVRHCHNCGVLHRDIKDENILIDLNRGELKLIDFGSGALLKDTVYTDFDGTRVYSPPEWIRYHRYHGRSAAVWSLGILLYDMVCGDIPFEHDEEIIGGQVFFRQRVSSECQHLIRWCLALRPSDRPTFEEIQNHPWMQDVLLPQETAEIHLHSLSPGPSK</t>
-  </si>
-  <si>
-    <t>VEDHYEMGEELGSGQFAIVRKCRQKGTGKEYAAKFIKKRRLSSSRRGVSREEIEREVNILREIRHPNIITLHDIFENKTDVVLILELVSGGELFDFLAEKESLTEDEATQFLKQILDGVHYLHSKRIAHFDLKPENIMLLDKNVPNPRIKLIDFGIAHKIEAGNEFKNIFGTPEFVAPEIVNYEPLGLEADMWSIGVITYILLSGASPFLGETKQETLTNISAVNYDFDEEYFSNTSELAKDFIRRLLVKDPKRRMTIAQSLEHSWIKAIRRRNVRGEDSG</t>
-  </si>
-  <si>
-    <t>MET_HUMAN_D0_4EEV_A</t>
-  </si>
-  <si>
-    <t>AACCAGTTCTACAGTGTGGAAGTGGGAGACTCAACCTTCACAGTTCTCAAGCGCTACCAGAATCTAAAGCCTATTGGCTCTGGGGCTCAGGGCATAGTTTGTGCCGCGTATGATGCTGTCCTTGACAGAAATGTGGCCATTAAGAAGCTCAGCAGACCCTTTCAGAACCAAACACATGCCAAGAGAGCGTACCGGGAGCTGGTCCTCATGAAGTGTGTGAACCATAAAAACATTATTAGTTTATTAAATGTCTTCACACCCCAGAAAACGCTGGAGGAGTTCCAAGATGTTTACTTAGTAATGGAACTGATGGATGCCAACTTATGTCAAGTGATTCAGATGGAATTAGACCATGAGCGAATGTCTTACCTGCTGTACCAAATGTTGTGTGGCATTAAGCACCTCCATTCTGCTGGAATTATTCACAGGGATTTAAAACCAAGTAACATTGTAGTCAAGTCTGATTGCACATTGAAAATCCTGGACTTTGGACTGGCCAGGACAGCAGGCACAAGCTTCATGATGACTCCATATGTGGTGACACGTTATTACAGAGCCCCTGAGGTCATCCTGGGGATGGGCTACAAGGAGAACGTGGATATATGGTCTGTGGGATGCATTATGGGAGAAATGGTTCGCCACAAAATCCTCTTTCCAGGAAGGGACTATATTGACCAGTGGAATAAGGTAATTGAACAACTAGGAACACCATGTCCAGAATTCATGAAGAAATTGCAACCCACAGTAAGAAACTATGTGGAGAATCGGCCCAAGTATGCGGGACTCACCTTCCCCAAACTCTTCCCAGATTCCCTCTTCCCAGCGGACTCCGAGCACAATAAACTCAAAGCCAGCCAAGCCAGGGACTTGTTGTCAAAGATGCTAGTGATTGACCCAGCAAAAAGAATATCAGTGGACGACGCCTTACAGCATCCCTACATCAACGTCTGGTATGACCCAGCCGAAGTGGAGGCGCCTCCACCTCAGATATATGACAAGCAGTTGGATGAAAGAGAACACACAATTGAAGAATGGAAAGAACTTATCTACAAGGAAGTAATGAAT</t>
-  </si>
-  <si>
-    <t>MP2K1_HUMAN_D0_3MBL_A</t>
-  </si>
-  <si>
-    <t>ETKYTVDKRFGMDFKEIELIGSGGFGQVFKAKHRIDGKTYVIKRVKYNNEKAEREVKALAKLDHVNIVHYNGCWDGFDYDPETSDDSLESSDYDPENSKNSSRSKTKCLFIQMEFCDKGTLEQWIEKRRGEKLDKVLALELFEQITKGVDYIHSKKLIHRDLKPSNIFLVDTKQVKIGDFGLVTSLKNDGKRTRSKGTLRYMSPEQISSQDYGKEVDLYALGLILAELLHVCDTAFETSKFFTDLRDGIISDIFDKKEKTLLQKLLSKKPEDRPNTSEILRTLTVWKKSPEKNERHTC</t>
-  </si>
-  <si>
-    <t>CDKL1_HUMAN_D0_4AGU_C</t>
-  </si>
-  <si>
-    <t>MARK3_HUMAN_D0_2QNJ_A</t>
-  </si>
-  <si>
-    <t>NLVFSDGYVVKETIGVGSYSECKRCVHKATNMEYAVKVIDKSKRDPSEEIEILLRYGQHPNIITLKDVYDDGKHVYLVTELMRGGELLDKILRQKFFSEREASFVLHTIGKTVEYLHSQGVVHRDLKPSNILYVDESGNPECLRICDFGFAKQLRAENGLLMTPCYTANFVAPEVLKRQGYDEGCDIWSLGILLYTMLAGYTPFANGPSDTPEEILTRIGSGKFTLSGGNWNTVSETAKDLVSKMLHVDPHQRLTAKQVLQHPWVTQKDKLPQSQLSHQDLQLVKGAMAATYSALNSSKPTPQLKPIESSILAQRRVRKLPSTTL</t>
-  </si>
-  <si>
-    <t>GGTGTTGTGACACATGAGCAGTTCAAGGCTGCGCTCAGGATGGTGGTGGACCAGGGTGACCCCCGGCTGCTGCTGGACAGCTACGTGAAGATTGGCGAGGGCTCCACCGGCATCGTCTGCTTGGCCCGGGAGAAGCACTCGGGCCGCCAGGTGGCCGTCAAGATGATGGACCTCAGGAAGCAGCAGCGCAGGGAGCTGCTCTTCAACGAGGTGGTGATCATGCGGGACTACCAGCACTTCAACGTGGTGGAGATGTACAAGAGCTACCTGGTGGGCGAGGAGCTGTGGGTGCTCATGGAGTTCCTGCAGGGAGGAGCCCTCACAGACATCGTCTCCCAAGTCAGGCTGAATGAGGAGCAGATTGCCACTGTGTGTGAGGCTGTGCTGCAGGCCCTGGCCTACCTGCATGCTCAGGGTGTCATCCACCGGGACATCAAGAGTGACTCCATCCTGCTGACCCTCGATGGCAGGGTGAAGCTCTCGGACTTCGGATTCTGTGCTCAGATCAGCAAAGACGTCCCTAAGAGGAAGTCCCTGGTGGGAACCCCCTACTGGATGGCTCCTGAAGTGATCTCCAGGTCTTTGTATGCCACTGAGGTGGATATCTGGTCTCTGGGCATCATGGTGATTGAGATGGTAGATGGGGAGCCACCGTACTTCAGTGACTCCCCAGTGCAAGCCATGAAGAGGCTCCGGGACAGCCCCCCACCCAAGCTGAAAAACTCTCACAAGGTCTCCCCAGTGCTGCGAGACTTCCTGGAGCGGATGCTGGTGCGGGACCCCCAAGAGAGAGCCACAGCCCAGGAGCTCCTAGACCACCCCTTCCTGCTGCAGACAGGGCTACCTGAGTGCCTGGTGCCCCTGATCCAGCTCTACCGAAAGCAGACCTCCACCTGC</t>
-  </si>
-  <si>
-    <t>CACATTGGAAACTACCGGCTCCTCAAGACCATTGGCAAGGGTAATTTTGCCAAGGTGAAGTTGGCCCGACACATCCTGACTGGGAAAGAGGTAGCTGTGAAGATCATTGACAAGACTCAACTGAACTCCTCCAGCCTCCAGAAACTATTCCGCGAAGTAAGAATAATGAAGGTTTTGAATCATCCCAACATAGTTAAATTATTTGAAGTGATTGAGACTGAGAAAACGCTCTACCTTGTCATGGAGTACGCTAGTGGCGGAGAGGTATTTGATTACCTAGTGGCTCATGGCAGGATGAAAGAAAAAGAGGCTCGAGCCAAATTCCGCCAGATAGTGTCTGCTGTGCAGTACTGTCACCAGAAGTTTATTGTCCATAGAGACTTAAAGGCAGAAAACCTGCTCTTGGATGCTGATATGAACATCAAGATTGCAGACTTTGGCTTCAGCAATGAATTCACCTTTGGGAACAAGCTGGACACCTTCTGTGGCAGTCCCCCTTATGCTGCCCCAGAACTCTTCCAGGGCAAAAAATATGATGGACCCGAGGTGGATGTGTGGAGCCTAGGAGTTATCCTCTATACACTGGTCAGCGGATCCCTGCCTTTTGATGGACAGAACCTCAAGGAGCTGCGGGAACGGGTACTGAGGGGAAAATACCGTATTCCATTCTACATGTCCACGGACTGTGAAAACCTGCTTAAGAAATTTCTCATTCTTAATCCCAGCAAGAGAGGCACTTTAGAGCAAATCATGAAAGATCGATGGATGAATGTGGGTCACGAAGATGATGAACTAAAGCCTTACGTGGAGCCACTCCCTGACTACAAGGACCCCCGGCGGACAGAGCTGATGGTGTCCATGGGTTATACACGGGAAGAGATCCAGGACTCGCTGGTGGGCCAGAGATACAACGAGGTGATGGCCACCTATCTGCTCCTGGGCTAC</t>
-  </si>
-  <si>
-    <t>ST17B_HUMAN_D0_3LM0_A</t>
-  </si>
-  <si>
-    <t>GDSDISSPLLQNTVHIDLSALNPELVQAVQHVVIGPSSLIVHFNEVIGRGHFGCVYHGTLLDNDGKKIHCAVKSLNRITDIGEVSQFLTEGIIMKDFSHPNVLSLLGICLRSEGSPLVVLPYMKHGDLRNFIRNETHNPTVKDLIGFGLQVAKGMKYLASKKFVHRDLAARNCMLDEKFTVKVADFGLARDMYDKEYYSVHNKTGAKLPVKWMALESLQTQKFTTKSDVWSFGVLLWELMTRGAPPYPDVNTFDITVYLLQGRRLLQPEYCPDPLYEVMLKCWHPKAEMRPSFSELVSRISAIFSTFIG</t>
-  </si>
-  <si>
-    <t>ATGAGTAGCTTTCTGCCAGAGGGAGGGTGTTACGAGCTGCTCACTGTGATAGGCAAAGGATTTGAGGACCTGATGACTGTGAATCTAGCAAGGTACAAACCAACAGGAGAGTACGTGACTGTACGGAGGATTAACCTAGAAGCTTGTTCCAATGAGATGGTAACATTCTTGCAGGGCGAGCTGCATGTCTCCAAACTCTTCAACCATCCCAATATCGTGCCATATCGAGCCACTTTTATTGCAGACAATGAGCTGTGGGTTGTCACATCATTCATGGCATACGGTTCTGCAAAAGATCTCATCTGTACACACTTCATGGATGGCATGAATGAGCTGGCGATTGCTTACATCCTGCAGGGGGTGCTGAAGGCCCTCGACTACATCCACCACATGGGATATGTACACAGGAGTGTCAAAGCCAGCCACATCCTGATCTCTGTGGATGGGAAGGTCTACCTGTCTGGTTTGCGCAGCAACCTCAGCATGATAAGCCATGGGCAGCGGCAGCGAGTGGTCCACGATTTTCCCAAGTACAGTGTCAAGGTTCTGCCGTGGCTCAGCCCCGAGGTCCTCCAGCAGAATCTCCAGGGTTATGATGCCAAGTCTGACATCTACAGTGTGGGAATCACAGCCTGTGAACTGGCCAACGGCCATGTCCCCTTTAAGGATATGCCTGCCACCCAGATGCTGCTAGAGAAACTGAACGGCACAGTGCCCTGCCTGTTGGATACCAGCACCATCCCCGCTGAGGAGCTGACCATGAGCCCTTCGCGCTCAGTGGCCAACTCTGGCCTGAGTGACAGCCTGACCACCAGCACCCCCCGGCCCTCCAACGGTGACTCGCCCTCCCACCCCTACCACCGAACCTTCTCCCCCCACTTCCACCACTTTGTGGAGCAGTGCCTTCAGCGCAACCCGGATGCCAGGCCCAGTGCCAGCACCCTCCTGAACCACTCTTTCTTCAAGCAGATCAAGCGACGTGCCTCAGAGGTTTTGCCCGAATTGCTTCGTCCTGTCACCCCCATCACCAATTTTGAGGGCAGCCAGTCTCAGGACCACAGTGGAATCTTTGGCCTGGTAACAAACCTGGAAGAGCTGGAGGTGGACGATTGGGAGTTC</t>
-  </si>
-  <si>
-    <t>ADPEELFTKLERIGKGSFGEVFKGIDNRTQQVVAIKIIDLEEAEDEIEDIQQEITVLSQCDSSYVTKYYGSYLKGSKLWIIMEYLGGGSALDLLRAGPFDEFQIATMLKEILKGLDYLHSEKKIHRDIKAANVLLSEQGDVKLADFGVAGQLTDTQIKRNTFVGTPFWMAPEVIQQSAYDSKADIWSLGITAIELAKGEPPNSDMHPMRVLFLIPKNNPPTLVGDFTKSFKEFIDACLNKDPSFRPTAKELLKHKFIVKNSKKTSYLTELIDRFKRWKAE</t>
-  </si>
-  <si>
-    <t>AURKA_HUMAN_D0_2NP8_A</t>
-  </si>
-  <si>
-    <t>HIGNYRLLKTIGKGNFAKVKLARHILTGKEVAVKIIDKTQLNSSSLQKLFREVRIMKVLNHPNIVKLFEVIETEKTLYLVMEYASGGEVFDYLVAHGRMKEKEARAKFRQIVSAVQYCHQKFIVHRDLKAENLLLDADMNIKIADFGFSNEFTFGNKLDTFCGSPPYAAPELFQGKKYDGPEVDVWSLGVILYTLVSGSLPFDGQNLKELRERVLRGKYRIPFYMSTDCENLLKKFLILNPSKRGTLEQIMKDRWMNVGHEDDELKPYVEPLPDYKDPRRTELMVSMGYTREEIQDSLVGQRYNEVMATYLLLGY</t>
-  </si>
-  <si>
-    <t>GVVTHEQFKAALRMVVDQGDPRLLLDSYVKIGEGSTGIVCLAREKHSGRQVAVKMMDLRKQQRRELLFNEVVIMRDYQHFNVVEMYKSYLVGEELWVLMEFLQGGALTDIVSQVRLNEEQIATVCEAVLQALAYLHAQGVIHRDIKSDSILLTLDGRVKLSDFGFCAQISKDVPKRKSLVGTPYWMAPEVISRSLYATEVDIWSLGIMVIEMVDGEPPYFSDSPVQAMKRLRDSPPPKLKNSHKVSPVLRDFLERMLVRDPQERATAQELLDHPFLLQTGLPECLVPLIQLYRKQTSTC</t>
-  </si>
-  <si>
-    <t>NQFYSVEVGDSTFTVLKRYQNLKPIGSGAQGIVCAAYDAVLDRNVAIKKLSRPFQNQTHAKRAYRELVLMKCVNHKNIISLLNVFTPQKTLEEFQDVYLVMELMDANLCQVIQMELDHERMSYLLYQMLCGIKHLHSAGIIHRDLKPSNIVVKSDCTLKILDFGLARTAGTSFMMTPYVVTRYYRAPEVILGMGYKENVDIWSVGCIMGEMVRHKILFPGRDYIDQWNKVIEQLGTPCPEFMKKLQPTVRNYVENRPKYAGLTFPKLFPDSLFPADSEHNKLKASQARDLLSKMLVIDPAKRISVDDALQHPYINVWYDPAEVEAPPPQIYDKQLDEREHTIEEWKELIYKEVMN</t>
-  </si>
-  <si>
-    <t>MKDYDELLKYYELHETIGTGGFAKVKLACHILTGEMVAIKIMDKNTLGSDLPRIKTEIEALKNLRHQHICQLYHVLETANKIFMVLEYCPGGELFDYIISQDRLSEEETRVVFRQIVSAVAYVHSQGYAHRDLKPENLLFDEYHKLKLIDFGLCAKPKGNKDYHLQTCCGSLAYAAPELIQGKSYLGSEADVWSMGILLYVLMCGFLPFDDDNVMALYKKIMRGKYDVPKWLSPSSILLLQQMLQVDPKKRISMKNLLNHPWIMQDYNYPVEWQSKNPFIHLDDDCVTELSVHHRNNRQTMEDLISLWQYDHLTATYLLLLAKKARGKPVRLRLSSFSCG</t>
-  </si>
-  <si>
-    <t>MSQERPTFYRQELNKTIWEVPERYQNLSPVGSGAYGSVCAAFDTKTGLRVAVKKLSRPFQSIIHAKRTYRELRLLKHMKHENVIGLLDVFTPARSLEEFNDVYLVTHLMGADLNNIVKCQKLTDDHVQFLIYQILRGLKYIHSADIIHRDLKPSNLAVNEDCELKILDFGLARHTDDEMTGYVATRWYRAPEIMLNWMHYNQTVDIWSVGCIMAELLTGRTLFPGTDHIDQLKLILRLVGTPGAELLKKISSESARNYIQSLTQMPKMNFANVFIGANPLAVDLLEKMLVLDSDKRITAAQALAHAYFAQYHDPDDEPVADPYDQSFESRDLLIDEWKSLTYDEVISFVPPPLDQEEMES</t>
-  </si>
-  <si>
-    <t>MELRVGNRYRLGRKIGSGSFGDIYLGTDIAAGEEVAIKLECVKTKHPQLHIESKIYKMMQGGVGIPTIRWCGAEGDYNVMVMELLGPSLEDLFNFCSRKFSLKTVLLLADQMISRIEYIHSKNFIHRDVKPDNFLMGLGKKGNLVYIIDFGLAKKYRDARTHQHIPYRENKNLTGTARYASINTHLGIEQSRRDDLESLGYVLMYFNLGSLPWQGLKAATKRQKYERISEKKMSTPIEVLCKGYPSEFATYLNFCRSLRFDDKPDYSYLRQLFRNLFHRQGFSYDYVFDWNMLK</t>
-  </si>
-  <si>
-    <t>targetID</t>
-  </si>
-  <si>
-    <t>TGGGCCCTGAACATGAAGGAGCTGAAGCTGCTGCAGACCATCGGGAAGGGGGAGTTCGGAGACGTGATGCTGGGCGATTACCGAGGGAACAAAGTCGCCGTCAAGTGCATTAAGAACGACGCCACTGCCCAGGCCTTCCTGGCTGAAGCCTCAGTCATGACGCAACTGCGGCATAGCAACCTGGTGCAGCTCCTGGGCGTGATCGTGGAGGAGAAGGGCGGGCTCTACATCGTCACTGAGTACATGGCCAAGGGGAGCCTTGTGGACTACCTGCGGTCTAGGGGTCGGTCAGTGCTGGGCGGAGACTGTCTCCTCAAGTTCTCGCTAGATGTCTGCGAGGCCATGGAATACCTGGAGGGCAACAATTTCGTGCATCGAGACCTGGCTGCCCGCAATGTGCTGGTGTCTGAGGACAACGTGGCCAAGGTCAGCGACTTTGGTCTCACCAAGGAGGCGTCCAGCACCCAGGACACGGGCAAGCTGCCAGTCAAGTGGACAGCCCCTGAGGCCCTGAGAGAGAAGAAATTCTCCACTAAGTCTGACGTGTGGAGTTTCGGAATCCTTCTCTGGGAAATCTACTCCTTTGGGCGAGTGCCTTATCCAAGAATTCCCCTGAAGGACGTCGTCCCTCGGGTGGAGAAGGGCTACAAGATGGATGCCCCCGACGGCTGCCCGCCCGCAGTCTATGAAGTCATGAAGAACTGCTGGCACCTGGACGCCGCCATGCGGCCCTCCTTCCTACAGCTCCGAGAGCAGCTTGAGCACATCAAAACCCACGAGCTGCACCTG</t>
-  </si>
-  <si>
-    <t>dna_seq</t>
-  </si>
-  <si>
-    <t>AACCTGGTTTTTAGTGACGGCTACGTGGTAAAGGAGACAATTGGTGTGGGCTCCTACTCTGAGTGCAAGCGCTGTGTCCACAAGGCCACCAACATGGAGTATGCTGTCAAGGTCATTGATAAGAGCAAGCGGGATCCTTCAGAAGAGATTGAGATTCTTCTGCGGTATGGCCAGCACCCCAACATCATCACTCTGAAAGATGTGTATGATGATGGCAAACACGTGTACCTGGTGACAGAGCTGATGCGGGGTGGGGAGCTGCTGGACAAGATCCTGCGGCAGAAGTTCTTCTCAGAGCGGGAGGCCAGCTTTGTCCTGCACACCATTGGCAAAACTGTGGAGTATCTGCACTCACAGGGGGTTGTGCACAGGGACCTGAAGCCCAGCAACATCCTGTATGTGGACGAGTCCGGGAATCCCGAGTGCCTGCGCATCTGTGACTTTGGTTTTGCCAAACAGCTGCGGGCTGAGAATGGGCTCCTCATGACACCTTGCTACACAGCCAACTTTGTGGCGCCTGAGGTGCTGAAGCGCCAGGGCTACGATGAAGGCTGCGACATCTGGAGCCTGGGCATTCTGCTGTACACCATGCTGGCAGGATATACTCCATTTGCCAACGGTCCCAGTGACACACCAGAGGAAATCCTAACCCGGATCGGCAGTGGGAAGTTTACCCTCAGTGGGGGAAATTGGAACACAGTTTCAGAGACAGCCAAGGACCTGGTGTCCAAGATGCTACACGTGGATCCCCACCAGCGCCTCACAGCTAAGCAGGTTCTGCAGCATCCATGGGTCACCCAGAAAGACAAGCTTCCCCAAAGCCAGCTGTCCCACCAGGACCTACAGCTTGTGAAGGGAGCCATGGCTGCCACGTACTCCGCACTCAACAGCTCCAAGCCCACCCCCCAGCTGAAGCCCATCGAGTCATCCATCCTGGCCCAGCGGCGAGTGAGGAAGTTGCCATCCACCACCCTG</t>
-  </si>
-  <si>
-    <t>ATGGCCGACGACGACGTGCTGTTCGAGGATGTGTACGAGCTGTGCGAGGTGATCGGAAAGGGTCCCTTCAGTGTTGTACGACGATGTATCAACAGAGAAACTGGGCAACAATTTGCTGTAAAAATTGTTGATGTAGCCAAGTTCACATCAAGTCCAGGGTTAAGTACAGAAGATCTAAAGCGGGAAGCCAGTATCTGTCATATGCTGAAACATCCACACATTGTAGAGTTATTGGAGACATATAGCTCAGATGGAATGCTTTACATGGTTTTCGAATTTATGGATGGAGCAGATCTGTGTTTTGAAATCGTAAAGCGAGCTGACGCTGGTTTTGTGTACAGTGAAGCTGTAGCCAGCCATTATATGAGACAGATACTGGAAGCTCTACGCTACTGCCATGATAATAACATAATTCACAGGGATGTGAAGCCCCACTGTGTTCTCCTTGCCTCAAAAGAAAACTCGGCACCTGTTAAACTTGGAGGCTTTGGGGTAGCTATTCAATTAGGGGAGTCTGGACTTGTAGCTGGAGGACGTGTTGGAACACCTCATTTTATGGCACCAGAAGTGGTCAAAAGAGAGCCTTACGGAAAGCCTGTAGACGTCTGGGGGTGCGGTGTGATCCTTTTTATCCTGCTCAGTGGTTGTTTGCCTTTTTACGGAACCAAGGAAAGATTGTTTGAAGGCATTATTAAAGGAAAATATAAGATGAATCCAAGGCAGTGGAGCCATATCTCTGAAAGTGCCAAAGACCTAGTACGTCGCATGCTGATGCTGGATCCAGCTGAAAGGATCACTGTTTATGAAGCACTGAATCACCCATGGCTTAAGGAGCGGGATCGTTACGCCTACAAGATTCATCTTCCAGAAACAGTAGAGCAGCTGAGGAAATTCAATGCAAGGAGGAAACTAAAGGGTGCAGTACTAGCCGCTGTGTCAAGTCACAAATTCAACTCATTCTATGGGGATCCCCCTGAAGAGTTACCAGATTTCTCCGAAGACCCTACCTCCTCAGGAGCA</t>
-  </si>
-  <si>
-    <t>VRK1_HUMAN_D0_3OP5_D</t>
-  </si>
-  <si>
-    <t>ATGGGGAAGGTGAAAGCCACCCCCATGACACCTGAACAAGCAATGAAGCAATACATGCAAAAACTCACAGCCTTCGAACACCATGAGATTTTCAGCTACCCTGAAATATATTTCTTGGGTCTAAATGCTAAGAAGCGCCAGGGCATGACAGGTGGGCCCAACAATGGTGGCTATGATGATGACCAGGGATCATATGTGCAGGTGCCCCACGATCACGTGGCTTACAGGTATGAGGTCCTCAAGGTCATTGGGAAGGGGAGCTTTGGGCAGGTGGTCAAGGCCTACGATCACAAAGTCCACCAGCACGTGGCCCTAAAGATGGTGCGGAATGAGAAGCGCTTCCACCGGCAAGCAGCGGAGGAGATCCGAATCCTGGAACACCTGCGGAAGCAGGACAAGGATAACACAATGAATGTCATCCATATGCTGGAGAATTTCACCTTCCGCAACCACATCTGCATGACGTTTGAGCTGCTGAGCATGAACCTCTATGAGCTCATCAAGAAGAATAAATTCCAGGGCTTCAGTCTGCCTTTGGTTCGCAAGTTTGCCCACTCGATTCTGCAGTGCTTGGATGCTTTGCACAAAAACAGAATAATTCACTGTGACCTTAAGCCCGAGAACATTTTGTTAAAGCAGCAGGGTAGAAGCGGTATTAAAGTAATTGATTTTGGCTCCAGTTGTTACGAGCATCAGCGTGTCTACACGTACATCCAGTCGCGTTTTTACCGGGCTCCAGAAGTGATCCTTGGGGCCAGGTATGGCATGCCCATTGATATGTGGAGCCTGGGCTGCATTTTAGCAGAGCTCCTGACGGGTTACCCCCTCTTGCCTGGGGAAGATGAAGGGGACCAGCTGGCCTGTATGATTGAACTGTTGGGCATGCCCTCACAGAAACTGCTGGATGCATCCAAACGAGCCAAAAATTTTGTGAGCTCCAAGGGTTATCCCCGTTACTGCACTGTCACGACTCTCTCAGATGGCTCTGTGGTCCTAAACGGAGGCCGTTCCCGGAGGGGGAAACTGAGGGGCCCACCGGAGAGCAGAGAGTGGGGGAACGCGCTGAAGGGGTGTGATGATCCCCTTTTCCTTGACTTCTTAAAACAGTGTTTAGAGTGGGATCCTGCAGTGCGCATGACCCCAGGCCAGGCTTTGCGGCACCCCTGGCTGAGGAGGCGGTTGCCAAAGCCTCCCACCGGGGAGAAAACGTCAGTGAAAAGG</t>
-  </si>
-  <si>
-    <t>ACTGACTCCTTGCCAGGAAAGTTTGAAGATATGTACAAGCTGACCTCTGAATTGCTGGGAGAGGGAGCCTATGCCAAAGTTCAAGGTGCCGTGAGCCTACAGAATGGCAAAGAGTATGCCGTCAAAATCATCGAGAAACAAGCAGGGCACAGTCGGAGTAGGGTGTTTCGAGAGGTGGAGACGCTGTATCAGTGTCAGGGAAACAAGAACATTTTGGAGCTGATTGAGTTCTTTGAAGATGACACAAGGTTTTACTTGGTCTTTGAGAAATTGCAAGGAGGTTCCATCTTAGCCCACATCCAGAAGCAAAAGCACTTCAATGAGCGAGAAGCCAGCCGAGTGGTGCGGGACGTTGCTGCTGCCCTTGACTTCCTGCATACCAAAGACAAAGTCTCTCTCTGTCACCTAGGCGGGAGTGCTAGGGCGCCATCAGGGCTCACTGCAGCCCCAACCTCCCTGGGCTCCAGTGATCCTCCCACCTCAGCCTCCCAAGTAGCTGGGACTACAGGCATTGATCATCGTGATCTGAAACCAGAAAATATATTGTGTGAATCTCCAGAAAAGGTGTCTCCAGTGAAAATCTGTGACTTTGACTTGGGCAGTGGGATGAAACTGAACAACTCCTGTACCCCCATAACCACACCAGAGCTGACCACCCCATGTGGCTCTGCAGAATACATGGCCCCTGAGGTAGGGGAGGTCTTCACGGACCAGGCCACATTCTACGACAAGCGCTGTGACCTGTGGAGCCTGGGCGTGGTCCTCTACATCATGCTGAGTGGCTACCCACCCTTCGTGGGTCACTGCGGGGCCGACTGTGGCTGGGACCGGGGCGAGGTCTGCAGGGTGTGCCAGAACAAGCTGTTTGAAAGCATCCAGGAAGGCAAGTATGAGTTTCCTGACAAGGACTGGGCACACATCTCCAGTGAAGCCAAAGACCTCATCTCCAAGCTCCTGGTGCGAGATGCAAAGCAGAGACTTAGCGCCGCCCAAGTTCTGCAGCACCCATGGGTGCAGGGGCAAGCTCCAGAAAAGGGA</t>
-  </si>
-  <si>
-    <t>SVYPKALRDEYIMSKTLGSGACGEVKLAFERKTCKKVAIKIISKRKFAIGSAREADPALNVETEIEILKKLNHPCIIKIKNFFDAEDYYIVLELMEGGELFDKVVGNKRLKEATCKLYFYQMLLAVQYLHENGIIHRDLKPENVLLSSQEEDCLIKITDFGHSKIWGETSLMRTLCGTPTYLAPEVLVSVGTAGYNRAVDCWSLGVILFICLSGYPPFSEHRTQVSLKDQITSGKYNFIPEVWAEVSEKALDLVKKLLVVDPKARFTTEEALRHPWLQDEDMKRKFQDLLSEENESTALPQVLAQPSTSRKRPREGEAEGAE</t>
-  </si>
-  <si>
-    <t>ATGGAGAAGTATGAAAAAATTGGGAAAATTGGAGAAGGATCCTATGGAGTTGTTTTCAAATGTAGAAACAGGGACACGGGTCAGATTGTGGCCATCAAGAAGTTTCTGGAATCAGAAGATGACCCTGTCATAAAGAAAATTGCCCTTCGGGAAATCCGAATGCTCAAGCAACTCAAGCATCCCAACCTTGTTAACCTCCTGGAAGTCTTCAGGAGGAAACGGAGGCTTCACCTGGTGTTTGAATATTGTGACCACACAGTTCTCCATGAGTTGGACAGATACCAAAGAGGGGTACCAGAACATCTCGTGAAGAGCATAACTTGGCAGACACTGCAAGCTGTAAATTTTTGCCATAAACACAATTGCATACATAGAGACGTGAAGCCAGAAAATATCCTCATCACGAAACATTCCGTGATTAAGCTTTGTGACTTTGGATTTGCTCGGCTTTTGACTGGACCGAGTGACTACTATACAGACTACGTGGCTACCAGGTGGTACCGCTCCCCTGAGCTGCTGGTGGGGGACACGCAGTACGGCCCCCCGGTGGATGTTTGGGCAATTGGCTGTGTCTTTGCTGAGCTGCTGTCAGGAGTGCCTCTGTGGCCAGGAAAATCGGATGTGGATCAGCTGTATCTGATTAGGAAGACCTTGGGGGATCTCATTCCTAGGCACCAGCAAGTGTTTAGCACGAATCAGTACTTCAGTGGAGTGAAAATTCCAGACCCTGAAGATATGGAACCACTTGAATTAAAATTCCCAAACATCTCTTATCCTGCCCTGGGGCTCCTA</t>
-  </si>
-  <si>
-    <t>KHDGRVKIGHYVLGDTLGVGTFGKVKIGEHQLTGHKVAVKILNRQKIRSLDVVGKIKREIQNLKLFRHPHIIKLYQVISTPTDFFMVMEYVSGGELFDYICKHGRVEEMEARRLFQQILSAVDYCHRHMVVHRDLKPENVLLDAHMNAKIADFGLSNMMSDGEFLRTSCGSPNYAAPEVISGRLYAGPEVDIWSCGVILYALLCGTLPFDDEHVPTLFKKIRGGVFYIPEYLNRSVATLLMHMLQVDPLKRATIKDIREHEWFKQDLPSYLFPE</t>
-  </si>
-  <si>
-    <t>ATGGAAAACTTTAATAATTTCTATATACTTACATCTAAAGAGCTAGGGAGAGGAAAATTTGCTGTGGTTAGACAATGTATATCAAAATCTACTGGCCAAGAATATGCTGCAAAATTTCTAAAAAAGAGAAGAAGAGGACAGGATTGTCGAGCAGAAATTTTACACGAGATTGCTGTGCTTGAATTGGCAAAGTCTTGTCCCCGTGTTATTAATCTTCATGAGGTCTATGAAAATACAAGTGAAATCATTTTGATATTGGAATATGCTGCAGGTGGAGAAATTTTCAGCCTGTGTTTACCTGAGTTGGCTGAAATGGTTTCTGAAAATGATGTTATCAGACTCATTAAACAAATACTTGAAGGAGTTTATTATCTACATCAGAATAACATTGTACACCTTGATTTAAAGCCACAGAATATATTACTGAGCAGCATATACCCTCTCGGGGACATTAAAATAGTAGATTTTGGAATGTCTCGAAAAATAGGGCATGCGTGTGAACTTCGGGAAATCATGGGAACACCAGAATATTTAGCTCCAGAAATCCTGAACTATGATCCCATTACCACAGCAACAGATATGTGGAATATTGGTATAATAGCATATATGTTGTTAACTCACACATCACCATTTGTGGGAGAAGATAATCAAGAAACATACCTCAATATTTCTCAAGTTAATGTAGATTATTCGGAAGAAACTTTTTCATCAGTTTCACAGCTGGCCACAGACTTTATTCAGAGCCTTTTAGTAAAAAATCCAGAGAAAAGACCAACAGCAGAGATATGCCTTTCTCATTCTTGGCTACAGCAGTGGGACTTTGAAAACTTGTTTCACCCTGAAGAAACTTCCAGTTCCTCTCAAACTCAGGATCATTCTGTAAGGTCCTCTGAAGACAAGACTTCTAAATCCTCC</t>
-  </si>
-  <si>
-    <t>MPSRAEDYEVLYTIGTGSYGRCQKIRRKSDGKILVWKELDYGSMTEAEKQMLVSEVNLLRELKHPNIVRYYDRIIDRTNTTLYIVMEYCEGGDLASVITKGTKERQYLDEEFVLRVMTQLTLALKECHRRSDGGHTVLHRDLKPANVFLDGKQNVKLGDFGLARILNHDTSFAKTFVGTPYYMSPEQMNRMSYNEKSDIWSLGCLLYELCALMPPFTAFSQKELAGKIREGKFRRIPYRYSDELNEIITRMLNLKDYHRPSVEEILENPLI</t>
-  </si>
-  <si>
-    <t>GACCCAGAAGAGCTTTTTACAAAACTAGAGAAAATTGGGAAGGGCTCCTTTGGAGAGGTGTTCAAAGGCATTGACAATCGGACTCAGAAAGTGGTTGCCATAAAGATCATTGATCTGGAAGAAGCTGAAGATGAGATAGAGGACATTCAACAAGAAATCACAGTGCTGAGTCAGTGTGACAGTCCATATGTAACCAAATATTATGGATCCTATCTGAAGGATACAAAATTATGGATAATAATGGAATATCTTGGTGGAGGCTCCGCACTAGATCTATTAGAACCTGGCCCATTAGATGAAACCCAGATCGCTACTATATTAAGAGAAATACTGAAAGGACTCGATTATCTCCATTCGGAGAAGAAAATCCACAGAGACATTAAAGCGGCCAACGTCCTGCTGTCTGAGCATGGCGAGGTGAAGCTGGCGGACTTTGGCGTGGCTGGCCAGCTGACAGACACCCAGATCAAAAGGAACACCTTCGTGGGCACCCCATTCTGGATGGCACCCGAGGTCATCAAACAGTCGGCCTATGACTCGAAGGCAGACATCTGGTCCCTGGGCATAACAGCTATTGAACTTGCAAGAGGGGAACCACCTCATTCCGAGCTGCACCCCATGAAAGTTTTATTCCTCATTCCAAAGAACAACCCACCGACGTTGGAAGGAAACTACAGTAAACCCCTCAAGGAGTTTGTGGAGGCCTGTTTGAATAAGGAGCCGAGCTTTAGACCCACTGCTAAGGAGTTATTGAAGCACAAGTTTATACTACGCAATGCAAAGAAAACTTCCTACTTGACCGAGCTCATCGAC</t>
-  </si>
-  <si>
-    <t>VIIDNKRYLFIQKLGEGGFSYVDLVEGLHDGHFYALKRILCHEQQDREEAQREADMHRLFNHPNILRLVAYCLRERGAKHEAWLLLPFFKRGTLWNEIERLKDKGNFLTEDQILWLLLGICRGLEAIHAKGYAHRDLKPTNILLGDEGQPVLMDLGSMNQACIHVEGSRQALTLQDWAAQRCTISYRAPELFSVQSHCVIDERTDVWSLGCVLYAMMFGEGPYDMVFQKGDSVALAVQNQLSIPQSPRHSSALWQLLNSMMTVDPHQRPHIPLLLSQLEALQ</t>
-  </si>
-  <si>
-    <t>MELK_HUMAN_D0_4IXP_A</t>
-  </si>
-  <si>
-    <t>AAGGAGAAGGAGCCCCTGGAGTCGCAGTACCAGGTGGGCCCGCTACTGGGCAGCGGCGGCTTCGGCTCGGTCTACTCAGGCATCCGCGTCTCCGACAACTTGCCGGTGGCCATCAAACACGTGGAGAAGGACCGGATTTCCGACTGGGGAGAGCTGCCTAATGGCACTCGAGTGCCCATGGAAGTGGTCCTGCTGAAGAAGGTGAGCTCGGGTTTCTCCGGCGTCATTAGGCTCCTGGACTGGTTCGAGAGGCCCGACAGTTTCGTCCTGATCCTGGAGAGGCCCGAGCCGGTGCAAGATCTCTTCGACTTCATCACGGAAAGGGGAGCCCTGCAAGAGGAGCTGGCCCGCAGCTTCTTCTGGCAGGTGCTGGAGGCCGTGCGGCACTGCCACAACTGCGGGGTGCTCCACCGCGACATCAAGGACGAAAACATCCTTATCGACCTCAATCGCGGCGAGCTCAAGCTCATCGACTTCGGGTCGGGGGCGCTGCTCAAGGACACCGTCTACACGGACTTCGATGGGACCCGAGTGTATAGCCCTCCAGAGTGGATCCGCTACCATCGCTACCATGGCAGGTCGGCGGCAGTCTGGTCCCTGGGGATCCTGCTGTATGATATGGTGTGTGGAGATATTCCTTTCGAGCATGACGAAGAGATCATCGGGGGCCAGGTTTTCTTCAGGCAGAGGGTCTCTTCAGAATGTCAGCATCTCATTAGATGGTGCTTGGCCCTGAGACCATCAGATAGGCCAACCTTCGAAGAAATCCAGAACCATCCATGGATGCAAGATGTTCTCCTGCCCCAGGAAACTGCTGAGATCCACCTCCACAGCCTGTCGCCGGGGCCCAGCAAA</t>
-  </si>
-  <si>
-    <t>PFPEGKVLDDMEGNQWVLGKKIGSGGFGLIYLAFPTNKPEKDARHVVKVEYQENGPLFSELKFYQRVAKKDCIKKWIERKQLDYLGIPLFYGSGLTEFKGRSYRFMVMERLGIDLQKISGQNGTFKKSTVLQLGIRMLDVLEYIHENEYVHGDIKAANLLLGYKNPDQVYLADYGLSYRYCPNGNHKQYQENPRKGHNGTIEFTSLDAHKGVALSRRSDVEILGYCMLRWLCGKLPWEQNLKDPVAVQTAKTNLLDELPQSVLKWAPSGSSCCEIAQFLVCAHSLAYDEKPNYQALKKILNPHGIPLGPLDFSTKGQSINVH</t>
-  </si>
-  <si>
-    <t>MESDLHQIIHSSQPLTLEHVRYFLYQLLRGLKYMHSAQVIHRDLKPSNLLVNENCELKIGDFGMARGLCTSPAEHQYFMTEYVATRWYRAPELMLSLHEYTQAIDLWSVGCIFGEMLARRQLFPGKNYVHQLQLIMMVLGTPSPAVIQAVGAERVRAYIQSLPPRQPVPWETVYPGADRQALSLLGRMLRFEPSARISAAAALRHPFLAKYHDPDDEPDCAPPFDFAFDREALTRERIKEAIVAEIEDFHARREGIRQQIRFQPSLQPVASEPGCPDVEMPSPWAPSGDCAM</t>
-  </si>
-  <si>
-    <t>EPKKYAVTDDYQLSKQVLGLGVNGKVLECFHRRTGQKCALKLLYDSPKARQEVDHHWQASGGPHIVCILDVYENMHHGKRCLLIIMECMEGGELFSRIQERGDQAFTEREAAEIMRDIGTAIQFLHSHNIAHRDVKPENLLYTSKEKDAVLKLTDFGFAKETTQNALQTPCYTPYYVAPEVLGPEKYDKSCDMWSLGVIMYILLCGFPPFYSNTGQAISPGMKRRIRLGQYGFPNPEWSEVSEDAKQLIRLLLKTDPTERLTITQFMNHPWINQSMVVPQTPLHTARVLQEDKDHWDEVKEEMTSALATMRVDYDQV</t>
-  </si>
-  <si>
-    <t>STK24_HUMAN_D0_3ZHP_C</t>
-  </si>
-  <si>
-    <t>aa_seq</t>
-  </si>
-  <si>
-    <t>KC1D_HUMAN_D0_4HNF_B</t>
-  </si>
-  <si>
-    <t>AGCATTGAGTCATCAGGAAAACTGAAGATCTCCCCTGAACAACACTGGGATTTCACTGCAGAGGACTTGAAAGACCTTGGAGAAATTGGACGAGGAGCTTATGGTTCTGTCAACAAAATGGTCCACAAACCAAGTGGGCAAATAATGGCAGTTAAAAGAATTCGGTCAACAGTGGATGAAAAAGAACAAAAACAACTTCTTATGGATTTGGATGTAGTAATGCGGAGTAGTGATTGCCCATACATTGTTCAGTTTTATGGTGCACTCTTCAGAGAGGGTGACTGTTGGATCTGTATGGAACTCATGTCTACCTCGTTTGATAAGTTTTACAAATATGTATATAGTGTATTAGATGATGTTATTCCAGAAGAAATTTTAGGCAAAATCACTTTAGCAACTGTGAAAGCACTAAACCACTTAAAAGAAAACTTGAAAATTATTCACAGAGATATCAAACCTTCCAATATTCTTCTGGACAGAAGTGGAAATATTAAGCTCTGTGACTTCGGCATCAGTGGACAGCTTGTGGACTCTATTGCCAAGACAAGAGATGCTGGCTGTAGGCCATACATGGCACCTGAAAGAATAGACCCAAGCGCATCACGACAAGGATATGATGTCCGCTCTGATGTCTGGAGTTTGGGGATCACATTGTATGAGTTGGCCACAGGCCGATTTCCTTATCCAAAGTGGAATAGTGTATTTGATCAACTAACACAAGTCGTGAAAGGAGATCCTCCGCAGCTGAGTAATTCTGAGGAAAGGGAATTCTCCCCGAGTTTCATCAACTTTGTCAACTTGTGCCTTACGAAGGATGAATCCAAAAGGCCAAAGTATAAAGAGCTTCTGAAACATCCCTTTATTTTGATGTATGAAGAACGTGCCGTTGAGGTCGCATGCTATGTTTGTAAAATCCTGGATCAAATGCCAGCTACTCCCAGCTCTCCCATGTATGTCGAT</t>
-  </si>
-  <si>
-    <t>AAPK2_HUMAN_D0_2H6D_A</t>
-  </si>
-  <si>
-    <t>CLK3_HUMAN_D0_2WU7_A</t>
-  </si>
-  <si>
-    <t>ATGACCGTGTTCAGGCAGGAAAACGTGGATGATTACTACGACACCGGCGAGGAACTTGGCAGTGGACAGTTTGCGGTTGTGAAGAAATGCCGTGAGAAAAGCACCGGCCTCCAGTATGCCGCCAAATTCATCAAGAAAAGGAGGACTAAGTCCAGCCGGCGGGGTGTGAGCCGCGAGGACATCGAGCGGGAGGTCAGCATCCTGAAGGAGATCCAGCACCCCAATGTCATCACCCTGCACGAGGTCTATGAGAACAAGACGGACGTCATCCTGATCTTGGAACTCGTTGCAGGTGGCGAGCTGTTTGACTTCTTAGCTGAAAAGGAATCTTTAACTGAAGAGGAAGCAACTGAATTTCTCAAACAAACTCTTAATGGTGTTTACTACCTGCACTCCCTTCAAATCGCCCACTTTGATCTTAAGCCTGAGAACATAATGCTTTTGGATAGAAATGTCCCCAAACCTCGGATCAAGATCATTGACTTTGGGTTGGCCCATAAAATTGACTTTGGAAATGAATTTAAAAACATATTTGGGACTCCAGAGTTTGTCGCTCCTGAGATAGTCAACTATGAACCTCTTGGTCTTGAGGCAGATATGTGGAGTATCGGGGTAATAACCTATATCCTCCTAAGTGGGGCCTCCCCATTTCTTGGAGACACTAAGCAAGAAACGTTAGCAAATGTATCCGCTGTCAACTACGAATTTGAGGATGAATACTTCAGTAATACCAGTGCCCTAGCCAAAGATTTCATAAGAAGACTTCTGGTCAAGGATCCAAAGAAGAGAATGACAATTCAAGATAGTTTGCAGCATCCCTGGATCAAGCCTAAAGATACACAACAGGCACTTAGTAGAAAAGCATCAGCAGTAAACATGGAGAAATTCAAGAAGTTTGCAGCCCGGAAAAAATGGAAACAATCCGTTCGCTTGATATCACTGTGCCAAAGATTATCCAGGTCATTCCTGTCCAGAAGTAACATGAGTGTTGCCAGAAGCGAT</t>
-  </si>
-  <si>
-    <t>GAAGCCTTTCTCACCCAGAAAGCCAAGGTCGGCGAACTCAAAGACGATGACTTCGAAAGGATCTCAGAGCTGGGCGCGGGCAACGGCGGGGTGGTCACCAAAGTCCAGCACAGACCCTCGGGCCTCATCATGGCCAGGAAGCTGATCCACCTTGAGATCAAGCCGGCCATCCGGAACCAGATCATCCGCGAGCTGCAGGTCCTGCACGAATGCAACTCGCCGTACATCGTGGGCTTCTACGGGGCCTTCTACAGTGACGGGGAGATCAGCATTTGCATGGAACACATGGACGGCGGCTCCCTGGACCAGGTGCTGAAAGAGGCCAAGAGGATTCCCGAGGAGATCCTGGGGAAAGTCAGCATCGCGGTTCTCCGGGGCTTGGCGTACCTCCGAGAGAAGCACCAGATCATGCACCGAGATGTGAAGCCCTCCAACATCCTCGTGAACTCTAGAGGGGAGATCAAGCTGTGTGACTTCGGGGTGAGCGGCCAGCTCATAGACTCCATGGCCAACTCCTTCGTGGGCACGCGCTCCTACATGGCTCCGGAGCGGTTGCAGGGCACACATTACTCGGTGCAGTCGGACATCTGGAGCATGGGCCTGTCCCTGGTGGAGCTGGCCGTCGGAAGGTACCCCATCCCCCCGCCCGACGCCAAAGAGCTGGAGGCCATCTTTGGCCGGCCCGTGGTCGACGGGGAAGAAGGAGAGCCTCACAGCATCTCGCCTCGGCCGAGGCCCCCCGGGCGCCCCGTCAGCGGTCACGGGATGGATAGCCGGCCTGCCATGGCCATCTTTGAACTCCTGGACTATATTGTGAACGAGCCACCTCCTAAGCTGCCCAACGGTGTGTTCACCCCCGACTTCCAGGAGTTTGTCAATAAATGCCTCATCAAGAACCCAGCGGAGCGGGCGGACCTGAAGATGCTCACAAACCACACCTTCATCAAGCGGTCCGAGGTGGAAGAAGTGGATTTTGCCGGCTGGTTGTGTAAAACCCTGCGGCTGAACCAGCCCGGCACACCCACGCGCACCGCCGTG</t>
-  </si>
-  <si>
-    <t>MKNK2_HUMAN_D0_2AC3_A</t>
-  </si>
-  <si>
-    <t>STRDYEIQRERIELGRCIGEGQFGDVHQGIYMSPENPALAVAIKTCKNCTSDSVREKFLQEALTMRQFDHPHIVKLIGVITENPVWIIMELCTLGELRSFLQVRKYSLDLASLILYAYQLSTALAYLESKRFVHRDIAARNVLVSSNDCVKLGDFGLSRYMEDSTYYKASKGKLPIKWMAPESINFRRFTSASDVWMFGVCMWEILMHGVKPFQGVKNNDVIGRIENGERLPMPPNCPPTLYSLMTKCWAYDPSRRPRFTELKAQLSTILEEEKAQQEE</t>
-  </si>
-  <si>
     <t>CSK22_HUMAN_D0_3E3B_X</t>
   </si>
   <si>
@@ -702,12 +663,6 @@
   </si>
   <si>
     <t>aa_start</t>
-  </si>
-  <si>
-    <t>GCAGTGCCCTTTGTGGAAGACTGGGACTTGGTGCAAACCCTGGGAGAAGGTGCCTATGGAGAAGTTCAACTTGCTGTGAATAGAGTAACTGAAGAAGCAGTCGCAGTGAAGATTGTAGATATGAAGCGTGCCGTAGACTGTCCAGAAAATATTAAGAAAGAGATCTGTATCAATAAAATGCTAAATCATGAAAATGTAGTAAAATTCTATGGTCACAGGAGAGAAGGCAATATCCAATATTTATTTCTGGAGTACTGTAGTGGAGGAGAGCTTTTTGACAGAATAGAGCCAGACATAGGCATGCCTGAACCAGATGCTCAGAGATTCTTCCATCAACTCATGGCAGGGGTGGTTTATCTGCATGGTATTGGAATAACTCACAGGGATATTAAACCAGAAAATCTTCTGTTGGATGAAAGGGATAACCTCAAAATCTCAGACTTTGGCTTGGCAACAGTATTTCGGTATAATAATCGTGAGCGTTTGTTGAACAAGATGTGTGGTACTTTACCATATGTTGCTCCAGAACTTCTGAAGAGAAGAGAATTTCATGCAGAACCAGTTGATGTTTGGTCCTGTGGAATAGTACTTACTGCAATGCTCGCTGGAGAATTGCCATGGGACCAACCCAGTGACAGCTGTCAGGAGTATTCTGACTGGAAAGAAAAAAAAACATACCTCAACCCTTGGAAAAAAATCGATTCTGCTCCTCTAGCTCTGCTGCATAAAATCTTAGTTGAGAATCCATCAGCAAGAATTACCATTCCAGACATCAAAAAAGATAGATGGTACAACAAACCCCTC</t>
-  </si>
-  <si>
-    <t>MSGPVPSRARVYTDVNTHRPREYWDYESHVVEWGNQDDYQLVRKLGRGKYSEVFEAINITNNEKVVVKILKPVKKKKIKREIKILENLRGGPNIITLADIVKDPVSRTPALVFEHVNNTDFKQLYQTLTDYDIRFYMYEILKALDYCHSMGIMHRDVKPHNVMIDHEHRKLRLIDWGLAEFYHPGQEYNVRVASRYFKGPELLVDYQMYDYSLDMWSLGCMLASMIFRKEPFFHGHDNYDQLVRIAKVLGTEDLYDYIDKYNIELDPRFNDILGRHSRKRWERFVHSENQHLVSPEALDFLDKLLRYDHQSRLTAREAMEHPYFYTVVKDQARMG</t>
   </si>
   <si>
     <t>MAAAAAAGAGPEMVRGQVFDVGPRYTNLSYIGEGAYGMVCSAYDNVNKVRVAIKKISPFEHQTYCQRTLREIKILLRFRHENIIGINDIIRAPTIEQMKDVYIVQDLMETDLYKLLKTQHLSNDHICYFLYQILRGLKYIHSANVLHRDLKPSNLLLNTTCDLKICDFGLARVADPDHDHTGFLTEYVATRWYRAPEIMLNSKGYTKSIDIWSVGCILAEMLSNRPIFPGKHYLDQLNHILGILGSPSQEDLNCIINLKARNYLLSLPHKNKVPWNRLFPNADSKALDLLDKMLTFNPHKRIEVEQALAHPYLEQYYDPSDEPIAEAPFKFDMELDDLPKEKLKELIFEETARFQPGYRS</t>
@@ -1070,36 +1025,36 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="B1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="E1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="G1" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="H1" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="I1" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B2" t="n">
         <v>1432</v>
@@ -1114,7 +1069,7 @@
         <v>360</v>
       </c>
       <c r="F2" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
@@ -1123,12 +1078,12 @@
         <v>1080</v>
       </c>
       <c r="I2" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="B3" t="n">
         <v>1017</v>
@@ -1143,7 +1098,7 @@
         <v>296</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G3" t="n">
         <v>4</v>
@@ -1152,12 +1107,12 @@
         <v>888</v>
       </c>
       <c r="I3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="B4" t="n">
         <v>6790</v>
@@ -1172,7 +1127,7 @@
         <v>391</v>
       </c>
       <c r="F4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G4" t="n">
         <v>373</v>
@@ -1181,12 +1136,12 @@
         <v>1173</v>
       </c>
       <c r="I4" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B5" t="n">
         <v>5594</v>
@@ -1201,7 +1156,7 @@
         <v>360</v>
       </c>
       <c r="F5" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="G5" t="n">
         <v>1</v>
@@ -1210,12 +1165,12 @@
         <v>1080</v>
       </c>
       <c r="I5" t="s">
-        <v>128</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" t="n">
         <v>1612</v>
@@ -1230,7 +1185,7 @@
         <v>334</v>
       </c>
       <c r="F6" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="G6" t="n">
         <v>1</v>
@@ -1239,12 +1194,12 @@
         <v>1002</v>
       </c>
       <c r="I6" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B7" t="n">
         <v>9261</v>
@@ -1259,7 +1214,7 @@
         <v>348</v>
       </c>
       <c r="F7" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G7" t="n">
         <v>73</v>
@@ -1268,12 +1223,12 @@
         <v>1044</v>
       </c>
       <c r="I7" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B8" t="n">
         <v>10298</v>
@@ -1297,7 +1252,7 @@
         <v>1773</v>
       </c>
       <c r="I8" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1317,7 +1272,7 @@
         <v>512</v>
       </c>
       <c r="F9" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="G9" t="n">
         <v>685</v>
@@ -1326,12 +1281,12 @@
         <v>1536</v>
       </c>
       <c r="I9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>117</v>
       </c>
       <c r="B10" t="n">
         <v>673</v>
@@ -1346,7 +1301,7 @@
         <v>712</v>
       </c>
       <c r="F10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G10" t="n">
         <v>1330</v>
@@ -1375,7 +1330,7 @@
         <v>297</v>
       </c>
       <c r="F11" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="G11" t="n">
         <v>52</v>
@@ -1384,12 +1339,12 @@
         <v>891</v>
       </c>
       <c r="I11" t="s">
-        <v>63</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="B12" t="n">
         <v>2872</v>
@@ -1404,7 +1359,7 @@
         <v>385</v>
       </c>
       <c r="F12" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="G12" t="n">
         <v>214</v>
@@ -1413,12 +1368,12 @@
         <v>1155</v>
       </c>
       <c r="I12" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="B13" t="n">
         <v>1453</v>
@@ -1433,7 +1388,7 @@
         <v>294</v>
       </c>
       <c r="F13" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
@@ -1442,12 +1397,12 @@
         <v>882</v>
       </c>
       <c r="I13" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" t="n">
         <v>1454</v>
@@ -1462,7 +1417,7 @@
         <v>294</v>
       </c>
       <c r="F14" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
@@ -1471,12 +1426,12 @@
         <v>882</v>
       </c>
       <c r="I14" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="B15" t="n">
         <v>5598</v>
@@ -1491,7 +1446,7 @@
         <v>292</v>
       </c>
       <c r="F15" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="G15" t="n">
         <v>1</v>
@@ -1500,12 +1455,12 @@
         <v>876</v>
       </c>
       <c r="I15" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="B16" t="n">
         <v>6788</v>
@@ -1520,7 +1475,7 @@
         <v>313</v>
       </c>
       <c r="F16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G16" t="n">
         <v>46</v>
@@ -1529,12 +1484,12 @@
         <v>939</v>
       </c>
       <c r="I16" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="B17" t="n">
         <v>5563</v>
@@ -1549,7 +1504,7 @@
         <v>279</v>
       </c>
       <c r="F17" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="G17" t="n">
         <v>16</v>
@@ -1558,12 +1513,12 @@
         <v>837</v>
       </c>
       <c r="I17" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="B18" t="n">
         <v>5747</v>
@@ -1578,7 +1533,7 @@
         <v>689</v>
       </c>
       <c r="F18" t="s">
-        <v>219</v>
+        <v>59</v>
       </c>
       <c r="G18" t="n">
         <v>1231</v>
@@ -1587,12 +1542,12 @@
         <v>2067</v>
       </c>
       <c r="I18" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B19" t="n">
         <v>8569</v>
@@ -1607,7 +1562,7 @@
         <v>382</v>
       </c>
       <c r="F19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G19" t="n">
         <v>109</v>
@@ -1616,12 +1571,12 @@
         <v>1146</v>
       </c>
       <c r="I19" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" t="n">
         <v>5292</v>
@@ -1636,7 +1591,7 @@
         <v>313</v>
       </c>
       <c r="F20" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="G20" t="n">
         <v>85</v>
@@ -1645,12 +1600,12 @@
         <v>939</v>
       </c>
       <c r="I20" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" t="n">
         <v>7272</v>
@@ -1665,7 +1620,7 @@
         <v>808</v>
       </c>
       <c r="F21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G21" t="n">
         <v>1555</v>
@@ -1674,12 +1629,12 @@
         <v>2424</v>
       </c>
       <c r="I21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="B22" t="n">
         <v>8428</v>
@@ -1694,7 +1649,7 @@
         <v>289</v>
       </c>
       <c r="F22" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="G22" t="n">
         <v>55</v>
@@ -1703,7 +1658,7 @@
         <v>867</v>
       </c>
       <c r="I22" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1723,7 +1678,7 @@
         <v>798</v>
       </c>
       <c r="F23" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="G23" t="n">
         <v>1393</v>
@@ -1732,12 +1687,12 @@
         <v>2394</v>
       </c>
       <c r="I23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="B24" t="n">
         <v>1198</v>
@@ -1752,7 +1707,7 @@
         <v>484</v>
       </c>
       <c r="F24" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="G24" t="n">
         <v>379</v>
@@ -1761,12 +1716,12 @@
         <v>1452</v>
       </c>
       <c r="I24" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B25" t="n">
         <v>1613</v>
@@ -1781,7 +1736,7 @@
         <v>289</v>
       </c>
       <c r="F25" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="G25" t="n">
         <v>25</v>
@@ -1795,7 +1750,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="B26" t="n">
         <v>7867</v>
@@ -1810,7 +1765,7 @@
         <v>349</v>
       </c>
       <c r="F26" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="G26" t="n">
         <v>97</v>
@@ -1819,12 +1774,12 @@
         <v>1047</v>
       </c>
       <c r="I26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B27" t="n">
         <v>9748</v>
@@ -1839,7 +1794,7 @@
         <v>320</v>
       </c>
       <c r="F27" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="G27" t="n">
         <v>55</v>
@@ -1848,12 +1803,12 @@
         <v>960</v>
       </c>
       <c r="I27" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B28" t="n">
         <v>8445</v>
@@ -1868,7 +1823,7 @@
         <v>552</v>
       </c>
       <c r="F28" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="G28" t="n">
         <v>436</v>
@@ -1877,12 +1832,12 @@
         <v>1656</v>
       </c>
       <c r="I28" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B29" t="n">
         <v>56924</v>
@@ -1897,7 +1852,7 @@
         <v>681</v>
       </c>
       <c r="F29" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="G29" t="n">
         <v>1147</v>
@@ -1906,12 +1861,12 @@
         <v>2043</v>
       </c>
       <c r="I29" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B30" t="n">
         <v>815</v>
@@ -1926,7 +1881,7 @@
         <v>302</v>
       </c>
       <c r="F30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G30" t="n">
         <v>37</v>
@@ -1940,7 +1895,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>179</v>
+        <v>142</v>
       </c>
       <c r="B31" t="n">
         <v>9262</v>
@@ -1955,7 +1910,7 @@
         <v>329</v>
       </c>
       <c r="F31" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="G31" t="n">
         <v>73</v>
@@ -1964,12 +1919,12 @@
         <v>987</v>
       </c>
       <c r="I31" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B32" t="n">
         <v>814</v>
@@ -1984,7 +1939,7 @@
         <v>340</v>
       </c>
       <c r="F32" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="G32" t="n">
         <v>43</v>
@@ -1993,12 +1948,12 @@
         <v>1020</v>
       </c>
       <c r="I32" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="B33" t="n">
         <v>8814</v>
@@ -2013,7 +1968,7 @@
         <v>265</v>
       </c>
       <c r="F33" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G33" t="n">
         <v>4</v>
@@ -2022,12 +1977,12 @@
         <v>795</v>
       </c>
       <c r="I33" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B34" t="n">
         <v>818</v>
@@ -2042,7 +1997,7 @@
         <v>315</v>
       </c>
       <c r="F34" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G34" t="n">
         <v>13</v>
@@ -2051,12 +2006,12 @@
         <v>945</v>
       </c>
       <c r="I34" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B35" t="n">
         <v>57144</v>
@@ -2071,7 +2026,7 @@
         <v>719</v>
       </c>
       <c r="F35" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G35" t="n">
         <v>1273</v>
@@ -2080,12 +2035,12 @@
         <v>2157</v>
       </c>
       <c r="I35" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B36" t="n">
         <v>5261</v>
@@ -2109,12 +2064,12 @@
         <v>879</v>
       </c>
       <c r="I36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" t="n">
         <v>9088</v>
@@ -2129,7 +2084,7 @@
         <v>360</v>
       </c>
       <c r="F37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G37" t="n">
         <v>217</v>
@@ -2138,12 +2093,12 @@
         <v>1080</v>
       </c>
       <c r="I37" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B38" t="n">
         <v>8576</v>
@@ -2158,7 +2113,7 @@
         <v>294</v>
       </c>
       <c r="F38" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="G38" t="n">
         <v>37</v>
@@ -2167,12 +2122,12 @@
         <v>882</v>
       </c>
       <c r="I38" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B39" t="n">
         <v>92335</v>
@@ -2187,7 +2142,7 @@
         <v>402</v>
       </c>
       <c r="F39" t="s">
-        <v>116</v>
+        <v>160</v>
       </c>
       <c r="G39" t="n">
         <v>88</v>
@@ -2196,12 +2151,12 @@
         <v>1206</v>
       </c>
       <c r="I39" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B40" t="n">
         <v>7444</v>
@@ -2216,7 +2171,7 @@
         <v>335</v>
       </c>
       <c r="F40" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="G40" t="n">
         <v>40</v>
@@ -2225,12 +2180,12 @@
         <v>1005</v>
       </c>
       <c r="I40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="B41" t="n">
         <v>51231</v>
@@ -2245,7 +2200,7 @@
         <v>474</v>
       </c>
       <c r="F41" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="G41" t="n">
         <v>436</v>
@@ -2254,12 +2209,12 @@
         <v>1422</v>
       </c>
       <c r="I41" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B42" t="n">
         <v>2042</v>
@@ -2274,7 +2229,7 @@
         <v>947</v>
       </c>
       <c r="F42" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G42" t="n">
         <v>1816</v>
@@ -2283,12 +2238,12 @@
         <v>2841</v>
       </c>
       <c r="I42" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B43" t="n">
         <v>2260</v>
@@ -2303,7 +2258,7 @@
         <v>772</v>
       </c>
       <c r="F43" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G43" t="n">
         <v>1366</v>
@@ -2312,7 +2267,7 @@
         <v>2316</v>
       </c>
       <c r="I43" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -2332,7 +2287,7 @@
         <v>340</v>
       </c>
       <c r="F44" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="G44" t="n">
         <v>1</v>
@@ -2341,711 +2296,711 @@
         <v>1020</v>
       </c>
       <c r="I44" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B45" t="n">
-        <v>3702</v>
+        <v>6197</v>
       </c>
       <c r="C45" t="s">
         <v>2</v>
       </c>
       <c r="D45" t="n">
-        <v>357</v>
+        <v>399</v>
       </c>
       <c r="E45" t="n">
-        <v>620</v>
+        <v>740</v>
       </c>
       <c r="F45" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="G45" t="n">
-        <v>1069</v>
+        <v>1195</v>
       </c>
       <c r="H45" t="n">
-        <v>1860</v>
+        <v>2220</v>
       </c>
       <c r="I45" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>101</v>
+        <v>159</v>
       </c>
       <c r="B46" t="n">
-        <v>6197</v>
+        <v>4233</v>
       </c>
       <c r="C46" t="s">
         <v>2</v>
       </c>
       <c r="D46" t="n">
-        <v>399</v>
+        <v>1038</v>
       </c>
       <c r="E46" t="n">
-        <v>740</v>
+        <v>1346</v>
       </c>
       <c r="F46" t="s">
-        <v>115</v>
+        <v>168</v>
       </c>
       <c r="G46" t="n">
-        <v>1195</v>
+        <v>3112</v>
       </c>
       <c r="H46" t="n">
-        <v>2220</v>
+        <v>4038</v>
       </c>
       <c r="I46" t="s">
-        <v>145</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>170</v>
+        <v>101</v>
       </c>
       <c r="B47" t="n">
-        <v>4233</v>
+        <v>5603</v>
       </c>
       <c r="C47" t="s">
         <v>2</v>
       </c>
       <c r="D47" t="n">
-        <v>1038</v>
+        <v>1</v>
       </c>
       <c r="E47" t="n">
-        <v>1346</v>
+        <v>352</v>
       </c>
       <c r="F47" t="s">
-        <v>180</v>
+        <v>98</v>
       </c>
       <c r="G47" t="n">
-        <v>3112</v>
+        <v>1</v>
       </c>
       <c r="H47" t="n">
-        <v>4038</v>
+        <v>1056</v>
       </c>
       <c r="I47" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>109</v>
+        <v>137</v>
       </c>
       <c r="B48" t="n">
-        <v>5603</v>
+        <v>6416</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
       </c>
       <c r="D48" t="n">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="E48" t="n">
-        <v>352</v>
+        <v>399</v>
       </c>
       <c r="F48" t="s">
-        <v>98</v>
+        <v>140</v>
       </c>
       <c r="G48" t="n">
-        <v>1</v>
+        <v>238</v>
       </c>
       <c r="H48" t="n">
-        <v>1056</v>
+        <v>1197</v>
       </c>
       <c r="I48" t="s">
-        <v>51</v>
+        <v>200</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>149</v>
+        <v>212</v>
       </c>
       <c r="B49" t="n">
-        <v>6416</v>
+        <v>10769</v>
       </c>
       <c r="C49" t="s">
         <v>2</v>
       </c>
       <c r="D49" t="n">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E49" t="n">
-        <v>399</v>
+        <v>360</v>
       </c>
       <c r="F49" t="s">
-        <v>152</v>
+        <v>68</v>
       </c>
       <c r="G49" t="n">
-        <v>238</v>
+        <v>169</v>
       </c>
       <c r="H49" t="n">
-        <v>1197</v>
+        <v>1080</v>
       </c>
       <c r="I49" t="s">
-        <v>213</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" t="s">
-        <v>225</v>
+        <v>24</v>
       </c>
       <c r="B50" t="n">
-        <v>10769</v>
+        <v>6195</v>
       </c>
       <c r="C50" t="s">
         <v>2</v>
       </c>
       <c r="D50" t="n">
-        <v>57</v>
+        <v>411</v>
       </c>
       <c r="E50" t="n">
-        <v>360</v>
+        <v>735</v>
       </c>
       <c r="F50" t="s">
-        <v>74</v>
+        <v>164</v>
       </c>
       <c r="G50" t="n">
-        <v>169</v>
+        <v>1231</v>
       </c>
       <c r="H50" t="n">
-        <v>1080</v>
+        <v>2205</v>
       </c>
       <c r="I50" t="s">
-        <v>42</v>
+        <v>180</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B51" t="n">
-        <v>6195</v>
+        <v>5599</v>
       </c>
       <c r="C51" t="s">
-        <v>2</v>
+        <v>208</v>
       </c>
       <c r="D51" t="n">
-        <v>411</v>
+        <v>1</v>
       </c>
       <c r="E51" t="n">
-        <v>735</v>
+        <v>364</v>
       </c>
       <c r="F51" t="s">
-        <v>176</v>
+        <v>26</v>
       </c>
       <c r="G51" t="n">
-        <v>1231</v>
+        <v>1</v>
       </c>
       <c r="H51" t="n">
-        <v>2205</v>
+        <v>1092</v>
       </c>
       <c r="I51" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
-        <v>39</v>
+        <v>114</v>
       </c>
       <c r="B52" t="n">
-        <v>5599</v>
+        <v>4751</v>
       </c>
       <c r="C52" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="D52" t="n">
         <v>1</v>
       </c>
       <c r="E52" t="n">
-        <v>364</v>
+        <v>271</v>
       </c>
       <c r="F52" t="s">
-        <v>27</v>
+        <v>189</v>
       </c>
       <c r="G52" t="n">
         <v>1</v>
       </c>
       <c r="H52" t="n">
-        <v>1092</v>
+        <v>813</v>
       </c>
       <c r="I52" t="s">
-        <v>222</v>
+        <v>152</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" t="s">
-        <v>125</v>
+        <v>40</v>
       </c>
       <c r="B53" t="n">
-        <v>4751</v>
+        <v>5058</v>
       </c>
       <c r="C53" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="D53" t="n">
-        <v>1</v>
+        <v>248</v>
       </c>
       <c r="E53" t="n">
-        <v>271</v>
+        <v>545</v>
       </c>
       <c r="F53" t="s">
-        <v>202</v>
+        <v>118</v>
       </c>
       <c r="G53" t="n">
-        <v>1</v>
+        <v>742</v>
       </c>
       <c r="H53" t="n">
-        <v>813</v>
+        <v>1635</v>
       </c>
       <c r="I53" t="s">
-        <v>164</v>
+        <v>97</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>172</v>
+        <v>71</v>
       </c>
       <c r="B54" t="n">
-        <v>5604</v>
+        <v>5610</v>
       </c>
       <c r="C54" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="D54" t="n">
-        <v>62</v>
+        <v>254</v>
       </c>
       <c r="E54" t="n">
-        <v>273</v>
+        <v>551</v>
       </c>
       <c r="F54" t="s">
-        <v>6</v>
+        <v>161</v>
       </c>
       <c r="G54" t="n">
-        <v>184</v>
+        <v>760</v>
       </c>
       <c r="H54" t="n">
-        <v>819</v>
+        <v>1653</v>
       </c>
       <c r="I54" t="s">
-        <v>114</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="B55" t="n">
-        <v>5058</v>
+        <v>1021</v>
       </c>
       <c r="C55" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="D55" t="n">
-        <v>248</v>
+        <v>1</v>
       </c>
       <c r="E55" t="n">
-        <v>545</v>
+        <v>301</v>
       </c>
       <c r="F55" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="G55" t="n">
-        <v>742</v>
+        <v>1</v>
       </c>
       <c r="H55" t="n">
-        <v>1635</v>
+        <v>903</v>
       </c>
       <c r="I55" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B56" t="n">
-        <v>5610</v>
+        <v>5608</v>
       </c>
       <c r="C56" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="D56" t="n">
-        <v>254</v>
+        <v>1</v>
       </c>
       <c r="E56" t="n">
-        <v>551</v>
+        <v>334</v>
       </c>
       <c r="F56" t="s">
-        <v>173</v>
+        <v>129</v>
       </c>
       <c r="G56" t="n">
-        <v>760</v>
+        <v>1</v>
       </c>
       <c r="H56" t="n">
-        <v>1653</v>
+        <v>1002</v>
       </c>
       <c r="I56" t="s">
-        <v>43</v>
+        <v>147</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>4</v>
+        <v>206</v>
       </c>
       <c r="B57" t="n">
-        <v>1021</v>
+        <v>140609</v>
       </c>
       <c r="C57" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="D57" t="n">
         <v>1</v>
       </c>
       <c r="E57" t="n">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="F57" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="G57" t="n">
         <v>1</v>
       </c>
       <c r="H57" t="n">
-        <v>903</v>
+        <v>906</v>
       </c>
       <c r="I57" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="B58" t="n">
-        <v>5608</v>
+        <v>659</v>
       </c>
       <c r="C58" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="D58" t="n">
-        <v>1</v>
+        <v>189</v>
       </c>
       <c r="E58" t="n">
-        <v>334</v>
+        <v>517</v>
       </c>
       <c r="F58" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G58" t="n">
-        <v>1</v>
+        <v>565</v>
       </c>
       <c r="H58" t="n">
-        <v>1002</v>
+        <v>1551</v>
       </c>
       <c r="I58" t="s">
-        <v>159</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>140609</v>
+        <v>5127</v>
       </c>
       <c r="C59" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="D59" t="n">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="E59" t="n">
-        <v>302</v>
+        <v>478</v>
       </c>
       <c r="F59" t="s">
-        <v>129</v>
+        <v>34</v>
       </c>
       <c r="G59" t="n">
-        <v>1</v>
+        <v>487</v>
       </c>
       <c r="H59" t="n">
-        <v>906</v>
+        <v>1434</v>
       </c>
       <c r="I59" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>70</v>
+        <v>192</v>
       </c>
       <c r="B60" t="n">
-        <v>659</v>
+        <v>9833</v>
       </c>
       <c r="C60" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="D60" t="n">
-        <v>189</v>
+        <v>1</v>
       </c>
       <c r="E60" t="n">
-        <v>517</v>
+        <v>340</v>
       </c>
       <c r="F60" t="s">
-        <v>76</v>
+        <v>174</v>
       </c>
       <c r="G60" t="n">
-        <v>565</v>
+        <v>1</v>
       </c>
       <c r="H60" t="n">
-        <v>1551</v>
+        <v>1020</v>
       </c>
       <c r="I60" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="B61" t="n">
-        <v>5127</v>
+        <v>5605</v>
       </c>
       <c r="C61" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="D61" t="n">
+        <v>55</v>
+      </c>
+      <c r="E61" t="n">
+        <v>400</v>
+      </c>
+      <c r="F61" t="s">
+        <v>6</v>
+      </c>
+      <c r="G61" t="n">
         <v>163</v>
       </c>
-      <c r="E61" t="n">
-        <v>478</v>
-      </c>
-      <c r="F61" t="s">
-        <v>35</v>
-      </c>
-      <c r="G61" t="n">
-        <v>487</v>
-      </c>
       <c r="H61" t="n">
-        <v>1434</v>
+        <v>1200</v>
       </c>
       <c r="I61" t="s">
-        <v>108</v>
+        <v>204</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>205</v>
+        <v>84</v>
       </c>
       <c r="B62" t="n">
-        <v>9833</v>
+        <v>1457</v>
       </c>
       <c r="C62" t="s">
-        <v>221</v>
+        <v>2</v>
       </c>
       <c r="D62" t="n">
         <v>1</v>
       </c>
       <c r="E62" t="n">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F62" t="s">
-        <v>187</v>
+        <v>77</v>
       </c>
       <c r="G62" t="n">
         <v>1</v>
       </c>
       <c r="H62" t="n">
-        <v>1020</v>
+        <v>1005</v>
       </c>
       <c r="I62" t="s">
-        <v>52</v>
+        <v>113</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>29</v>
+        <v>126</v>
       </c>
       <c r="B63" t="n">
-        <v>5605</v>
+        <v>11200</v>
       </c>
       <c r="C63" t="s">
-        <v>221</v>
+        <v>2</v>
       </c>
       <c r="D63" t="n">
-        <v>55</v>
+        <v>210</v>
       </c>
       <c r="E63" t="n">
-        <v>400</v>
+        <v>531</v>
       </c>
       <c r="F63" t="s">
-        <v>68</v>
+        <v>185</v>
       </c>
       <c r="G63" t="n">
-        <v>163</v>
+        <v>628</v>
       </c>
       <c r="H63" t="n">
-        <v>1200</v>
+        <v>1593</v>
       </c>
       <c r="I63" t="s">
-        <v>217</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B64" t="n">
-        <v>1457</v>
+        <v>1445</v>
       </c>
       <c r="C64" t="s">
         <v>2</v>
       </c>
       <c r="D64" t="n">
-        <v>1</v>
+        <v>188</v>
       </c>
       <c r="E64" t="n">
-        <v>335</v>
+        <v>450</v>
       </c>
       <c r="F64" t="s">
-        <v>230</v>
+        <v>25</v>
       </c>
       <c r="G64" t="n">
-        <v>1</v>
+        <v>562</v>
       </c>
       <c r="H64" t="n">
-        <v>1005</v>
+        <v>1350</v>
       </c>
       <c r="I64" t="s">
-        <v>124</v>
+        <v>178</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>138</v>
+        <v>56</v>
       </c>
       <c r="B65" t="n">
-        <v>11200</v>
+        <v>5600</v>
       </c>
       <c r="C65" t="s">
         <v>2</v>
       </c>
       <c r="D65" t="n">
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E65" t="n">
-        <v>531</v>
+        <v>364</v>
       </c>
       <c r="F65" t="s">
-        <v>198</v>
+        <v>10</v>
       </c>
       <c r="G65" t="n">
-        <v>628</v>
+        <v>1</v>
       </c>
       <c r="H65" t="n">
-        <v>1593</v>
+        <v>1092</v>
       </c>
       <c r="I65" t="s">
-        <v>0</v>
+        <v>70</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>117</v>
+        <v>207</v>
       </c>
       <c r="B66" t="n">
-        <v>5566</v>
+        <v>1459</v>
       </c>
       <c r="C66" t="s">
         <v>2</v>
       </c>
       <c r="D66" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E66" t="n">
-        <v>351</v>
+        <v>334</v>
       </c>
       <c r="F66" t="s">
-        <v>84</v>
+        <v>143</v>
       </c>
       <c r="G66" t="n">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="H66" t="n">
-        <v>1053</v>
+        <v>1002</v>
       </c>
       <c r="I66" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>103</v>
+        <v>163</v>
       </c>
       <c r="B67" t="n">
-        <v>1445</v>
+        <v>4140</v>
       </c>
       <c r="C67" t="s">
         <v>2</v>
       </c>
       <c r="D67" t="n">
-        <v>188</v>
+        <v>48</v>
       </c>
       <c r="E67" t="n">
-        <v>450</v>
+        <v>370</v>
       </c>
       <c r="F67" t="s">
+        <v>92</v>
+      </c>
+      <c r="G67" t="n">
+        <v>142</v>
+      </c>
+      <c r="H67" t="n">
+        <v>1110</v>
+      </c>
+      <c r="I67" t="s">
         <v>154</v>
-      </c>
-      <c r="G67" t="n">
-        <v>562</v>
-      </c>
-      <c r="H67" t="n">
-        <v>1350</v>
-      </c>
-      <c r="I67" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="B68" t="n">
-        <v>5600</v>
+        <v>2011</v>
       </c>
       <c r="C68" t="s">
         <v>2</v>
       </c>
       <c r="D68" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E68" t="n">
-        <v>364</v>
+        <v>330</v>
       </c>
       <c r="F68" t="s">
-        <v>10</v>
+        <v>172</v>
       </c>
       <c r="G68" t="n">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="H68" t="n">
-        <v>1092</v>
+        <v>990</v>
       </c>
       <c r="I68" t="s">
-        <v>77</v>
+        <v>134</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>220</v>
+        <v>146</v>
       </c>
       <c r="B69" t="n">
-        <v>1459</v>
+        <v>5595</v>
       </c>
       <c r="C69" t="s">
         <v>2</v>
@@ -3054,819 +3009,831 @@
         <v>1</v>
       </c>
       <c r="E69" t="n">
-        <v>334</v>
+        <v>379</v>
       </c>
       <c r="F69" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="G69" t="n">
         <v>1</v>
       </c>
       <c r="H69" t="n">
-        <v>1002</v>
+        <v>1137</v>
       </c>
       <c r="I69" t="s">
-        <v>123</v>
+        <v>213</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="B70" t="n">
-        <v>4140</v>
+        <v>7443</v>
       </c>
       <c r="C70" t="s">
         <v>2</v>
       </c>
       <c r="D70" t="n">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="E70" t="n">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="F70" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="G70" t="n">
-        <v>142</v>
+        <v>7</v>
       </c>
       <c r="H70" t="n">
-        <v>1110</v>
+        <v>1092</v>
       </c>
       <c r="I70" t="s">
-        <v>166</v>
+        <v>87</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>14</v>
+        <v>117</v>
       </c>
       <c r="B71" t="n">
-        <v>2011</v>
+        <v>673</v>
       </c>
       <c r="C71" t="s">
         <v>2</v>
       </c>
       <c r="D71" t="n">
-        <v>16</v>
+        <v>444</v>
       </c>
       <c r="E71" t="n">
-        <v>330</v>
+        <v>712</v>
       </c>
       <c r="F71" t="s">
-        <v>184</v>
+        <v>23</v>
       </c>
       <c r="G71" t="n">
-        <v>46</v>
+        <v>1330</v>
       </c>
       <c r="H71" t="n">
-        <v>990</v>
+        <v>2136</v>
       </c>
       <c r="I71" t="s">
-        <v>178</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B72" t="n">
-        <v>5595</v>
+        <v>4233</v>
       </c>
       <c r="C72" t="s">
         <v>2</v>
       </c>
       <c r="D72" t="n">
-        <v>1</v>
+        <v>1038</v>
       </c>
       <c r="E72" t="n">
-        <v>379</v>
+        <v>1346</v>
       </c>
       <c r="F72" t="s">
-        <v>56</v>
+        <v>168</v>
       </c>
       <c r="G72" t="n">
-        <v>1</v>
+        <v>3112</v>
       </c>
       <c r="H72" t="n">
-        <v>1137</v>
+        <v>4038</v>
       </c>
       <c r="I72" t="s">
-        <v>226</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>195</v>
+        <v>61</v>
       </c>
       <c r="B73" t="n">
-        <v>7443</v>
+        <v>2260</v>
       </c>
       <c r="C73" t="s">
         <v>2</v>
       </c>
       <c r="D73" t="n">
-        <v>3</v>
+        <v>456</v>
       </c>
       <c r="E73" t="n">
-        <v>364</v>
+        <v>772</v>
       </c>
       <c r="F73" t="s">
-        <v>96</v>
+        <v>53</v>
       </c>
       <c r="G73" t="n">
-        <v>7</v>
+        <v>1366</v>
       </c>
       <c r="H73" t="n">
-        <v>1092</v>
+        <v>2316</v>
       </c>
       <c r="I73" t="s">
-        <v>94</v>
+        <v>217</v>
       </c>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B74" t="n">
-        <v>5602</v>
+        <v>25</v>
+      </c>
+      <c r="C74" t="s">
+        <v>2</v>
       </c>
       <c r="D74" t="n">
-        <v>46</v>
+        <v>229</v>
       </c>
       <c r="E74" t="n">
-        <v>400</v>
+        <v>512</v>
       </c>
       <c r="F74" t="s">
-        <v>186</v>
+        <v>211</v>
       </c>
       <c r="G74" t="n">
-        <v>136</v>
+        <v>685</v>
       </c>
       <c r="H74" t="n">
-        <v>1200</v>
+        <v>1536</v>
       </c>
       <c r="I74" t="s">
-        <v>171</v>
+        <v>22</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>132</v>
+        <v>57</v>
       </c>
       <c r="B75" t="n">
-        <v>1111</v>
+        <v>1432</v>
+      </c>
+      <c r="C75" t="s">
+        <v>2</v>
       </c>
       <c r="D75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E75" t="n">
-        <v>269</v>
+        <v>360</v>
       </c>
       <c r="F75" t="s">
-        <v>106</v>
+        <v>175</v>
       </c>
       <c r="G75" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H75" t="n">
-        <v>807</v>
+        <v>1080</v>
       </c>
       <c r="I75" t="s">
-        <v>229</v>
+        <v>21</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>64</v>
+        <v>115</v>
       </c>
       <c r="B76" t="n">
-        <v>673</v>
+        <v>5594</v>
       </c>
       <c r="C76" t="s">
         <v>2</v>
       </c>
       <c r="D76" t="n">
-        <v>444</v>
+        <v>1</v>
       </c>
       <c r="E76" t="n">
-        <v>712</v>
+        <v>360</v>
       </c>
       <c r="F76" t="s">
-        <v>24</v>
+        <v>216</v>
       </c>
       <c r="G76" t="n">
-        <v>1330</v>
+        <v>1</v>
       </c>
       <c r="H76" t="n">
-        <v>2136</v>
+        <v>1080</v>
       </c>
       <c r="I76" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="B77" t="n">
-        <v>4233</v>
+        <v>11200</v>
       </c>
       <c r="C77" t="s">
         <v>2</v>
       </c>
       <c r="D77" t="n">
-        <v>1038</v>
+        <v>210</v>
       </c>
       <c r="E77" t="n">
-        <v>1346</v>
+        <v>531</v>
       </c>
       <c r="F77" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="G77" t="n">
-        <v>3112</v>
+        <v>628</v>
       </c>
       <c r="H77" t="n">
-        <v>4038</v>
+        <v>1593</v>
       </c>
       <c r="I77" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>66</v>
+        <v>136</v>
       </c>
       <c r="B78" t="n">
-        <v>2260</v>
+        <v>1017</v>
       </c>
       <c r="C78" t="s">
         <v>2</v>
       </c>
       <c r="D78" t="n">
-        <v>456</v>
+        <v>2</v>
       </c>
       <c r="E78" t="n">
-        <v>772</v>
+        <v>296</v>
       </c>
       <c r="F78" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="G78" t="n">
-        <v>1366</v>
+        <v>4</v>
       </c>
       <c r="H78" t="n">
-        <v>2316</v>
+        <v>888</v>
       </c>
       <c r="I78" t="s">
-        <v>232</v>
+        <v>45</v>
       </c>
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>1</v>
+        <v>125</v>
       </c>
       <c r="B79" t="n">
-        <v>25</v>
+        <v>5747</v>
       </c>
       <c r="C79" t="s">
         <v>2</v>
       </c>
       <c r="D79" t="n">
-        <v>229</v>
+        <v>411</v>
       </c>
       <c r="E79" t="n">
-        <v>512</v>
+        <v>689</v>
       </c>
       <c r="F79" t="s">
-        <v>224</v>
+        <v>59</v>
       </c>
       <c r="G79" t="n">
-        <v>685</v>
+        <v>1231</v>
       </c>
       <c r="H79" t="n">
-        <v>1536</v>
+        <v>2067</v>
       </c>
       <c r="I79" t="s">
-        <v>23</v>
+        <v>148</v>
       </c>
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="B80" t="n">
-        <v>1432</v>
+        <v>5599</v>
       </c>
       <c r="C80" t="s">
-        <v>2</v>
+        <v>208</v>
       </c>
       <c r="D80" t="n">
         <v>1</v>
       </c>
       <c r="E80" t="n">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="F80" t="s">
-        <v>188</v>
+        <v>26</v>
       </c>
       <c r="G80" t="n">
         <v>1</v>
       </c>
       <c r="H80" t="n">
-        <v>1080</v>
+        <v>1092</v>
       </c>
       <c r="I80" t="s">
-        <v>58</v>
+        <v>209</v>
       </c>
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>126</v>
+        <v>171</v>
       </c>
       <c r="B81" t="n">
-        <v>5594</v>
+        <v>6790</v>
       </c>
       <c r="C81" t="s">
         <v>2</v>
       </c>
       <c r="D81" t="n">
-        <v>1</v>
+        <v>125</v>
       </c>
       <c r="E81" t="n">
-        <v>360</v>
+        <v>391</v>
       </c>
       <c r="F81" t="s">
-        <v>231</v>
+        <v>79</v>
       </c>
       <c r="G81" t="n">
-        <v>1</v>
+        <v>373</v>
       </c>
       <c r="H81" t="n">
-        <v>1080</v>
+        <v>1173</v>
       </c>
       <c r="I81" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B82" t="n">
-        <v>11200</v>
+        <v>5595</v>
       </c>
       <c r="C82" t="s">
         <v>2</v>
       </c>
       <c r="D82" t="n">
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="E82" t="n">
-        <v>531</v>
+        <v>379</v>
       </c>
       <c r="F82" t="s">
-        <v>198</v>
+        <v>167</v>
       </c>
       <c r="G82" t="n">
-        <v>628</v>
+        <v>1</v>
       </c>
       <c r="H82" t="n">
-        <v>1593</v>
+        <v>1137</v>
       </c>
       <c r="I82" t="s">
-        <v>0</v>
+        <v>213</v>
       </c>
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>148</v>
+        <v>93</v>
       </c>
       <c r="B83" t="n">
-        <v>1017</v>
+        <v>6197</v>
       </c>
       <c r="C83" t="s">
         <v>2</v>
       </c>
       <c r="D83" t="n">
-        <v>2</v>
+        <v>399</v>
       </c>
       <c r="E83" t="n">
-        <v>296</v>
+        <v>740</v>
       </c>
       <c r="F83" t="s">
-        <v>19</v>
+        <v>106</v>
       </c>
       <c r="G83" t="n">
-        <v>4</v>
+        <v>1195</v>
       </c>
       <c r="H83" t="n">
-        <v>888</v>
+        <v>2220</v>
       </c>
       <c r="I83" t="s">
-        <v>46</v>
+        <v>133</v>
       </c>
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>137</v>
+        <v>84</v>
       </c>
       <c r="B84" t="n">
-        <v>5747</v>
+        <v>1457</v>
       </c>
       <c r="C84" t="s">
         <v>2</v>
       </c>
       <c r="D84" t="n">
-        <v>411</v>
+        <v>1</v>
       </c>
       <c r="E84" t="n">
-        <v>689</v>
+        <v>335</v>
       </c>
       <c r="F84" t="s">
-        <v>219</v>
+        <v>77</v>
       </c>
       <c r="G84" t="n">
-        <v>1231</v>
+        <v>1</v>
       </c>
       <c r="H84" t="n">
-        <v>2067</v>
+        <v>1005</v>
       </c>
       <c r="I84" t="s">
-        <v>160</v>
+        <v>113</v>
       </c>
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="B85" t="n">
-        <v>5599</v>
+        <v>9261</v>
       </c>
       <c r="C85" t="s">
-        <v>221</v>
+        <v>2</v>
       </c>
       <c r="D85" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E85" t="n">
-        <v>364</v>
+        <v>348</v>
       </c>
       <c r="F85" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="G85" t="n">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="H85" t="n">
-        <v>1092</v>
+        <v>1044</v>
       </c>
       <c r="I85" t="s">
-        <v>222</v>
+        <v>135</v>
       </c>
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="B86" t="n">
-        <v>1111</v>
+        <v>5292</v>
+      </c>
+      <c r="C86" t="s">
+        <v>2</v>
       </c>
       <c r="D86" t="n">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="E86" t="n">
-        <v>269</v>
+        <v>313</v>
       </c>
       <c r="F86" t="s">
-        <v>106</v>
+        <v>156</v>
       </c>
       <c r="G86" t="n">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="H86" t="n">
-        <v>807</v>
+        <v>939</v>
       </c>
       <c r="I86" t="s">
-        <v>229</v>
+        <v>193</v>
       </c>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>172</v>
+        <v>64</v>
       </c>
       <c r="B87" t="n">
-        <v>5604</v>
+        <v>659</v>
       </c>
       <c r="C87" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="D87" t="n">
-        <v>62</v>
+        <v>189</v>
       </c>
       <c r="E87" t="n">
-        <v>273</v>
+        <v>517</v>
       </c>
       <c r="F87" t="s">
-        <v>6</v>
+        <v>112</v>
       </c>
       <c r="G87" t="n">
-        <v>184</v>
+        <v>565</v>
       </c>
       <c r="H87" t="n">
-        <v>819</v>
+        <v>1551</v>
       </c>
       <c r="I87" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B88" t="n">
-        <v>5602</v>
+        <v>5605</v>
+      </c>
+      <c r="C88" t="s">
+        <v>208</v>
       </c>
       <c r="D88" t="n">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E88" t="n">
         <v>400</v>
       </c>
       <c r="F88" t="s">
-        <v>186</v>
+        <v>6</v>
       </c>
       <c r="G88" t="n">
-        <v>136</v>
+        <v>163</v>
       </c>
       <c r="H88" t="n">
         <v>1200</v>
       </c>
       <c r="I88" t="s">
-        <v>171</v>
+        <v>204</v>
       </c>
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="B89" t="n">
-        <v>6790</v>
+        <v>1453</v>
       </c>
       <c r="C89" t="s">
         <v>2</v>
       </c>
       <c r="D89" t="n">
-        <v>125</v>
+        <v>1</v>
       </c>
       <c r="E89" t="n">
-        <v>391</v>
+        <v>294</v>
       </c>
       <c r="F89" t="s">
-        <v>86</v>
+        <v>176</v>
       </c>
       <c r="G89" t="n">
-        <v>373</v>
+        <v>1</v>
       </c>
       <c r="H89" t="n">
-        <v>1173</v>
+        <v>882</v>
       </c>
       <c r="I89" t="s">
-        <v>156</v>
+        <v>116</v>
       </c>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>158</v>
+        <v>111</v>
       </c>
       <c r="B90" t="n">
-        <v>5595</v>
+        <v>2042</v>
       </c>
       <c r="C90" t="s">
         <v>2</v>
       </c>
       <c r="D90" t="n">
-        <v>1</v>
+        <v>606</v>
       </c>
       <c r="E90" t="n">
-        <v>379</v>
+        <v>947</v>
       </c>
       <c r="F90" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="G90" t="n">
-        <v>1</v>
+        <v>1816</v>
       </c>
       <c r="H90" t="n">
-        <v>1137</v>
+        <v>2841</v>
       </c>
       <c r="I90" t="s">
-        <v>226</v>
+        <v>109</v>
       </c>
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>101</v>
+        <v>11</v>
       </c>
       <c r="B91" t="n">
-        <v>6197</v>
+        <v>8573</v>
       </c>
       <c r="C91" t="s">
         <v>2</v>
       </c>
       <c r="D91" t="n">
-        <v>399</v>
+        <v>1</v>
       </c>
       <c r="E91" t="n">
-        <v>740</v>
+        <v>340</v>
       </c>
       <c r="F91" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="G91" t="n">
-        <v>1195</v>
+        <v>1</v>
       </c>
       <c r="H91" t="n">
-        <v>2220</v>
+        <v>1020</v>
       </c>
       <c r="I91" t="s">
-        <v>145</v>
+        <v>181</v>
       </c>
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="B92" t="n">
-        <v>3702</v>
+        <v>5610</v>
       </c>
       <c r="C92" t="s">
-        <v>2</v>
+        <v>208</v>
       </c>
       <c r="D92" t="n">
-        <v>357</v>
+        <v>254</v>
       </c>
       <c r="E92" t="n">
-        <v>620</v>
+        <v>551</v>
       </c>
       <c r="F92" t="s">
-        <v>93</v>
+        <v>161</v>
       </c>
       <c r="G92" t="n">
-        <v>1069</v>
+        <v>760</v>
       </c>
       <c r="H92" t="n">
-        <v>1860</v>
+        <v>1653</v>
       </c>
       <c r="I92" t="s">
-        <v>139</v>
+        <v>42</v>
       </c>
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>117</v>
+        <v>24</v>
       </c>
       <c r="B93" t="n">
-        <v>5566</v>
+        <v>6195</v>
       </c>
       <c r="C93" t="s">
         <v>2</v>
       </c>
       <c r="D93" t="n">
-        <v>16</v>
+        <v>411</v>
       </c>
       <c r="E93" t="n">
-        <v>351</v>
+        <v>735</v>
       </c>
       <c r="F93" t="s">
-        <v>84</v>
+        <v>164</v>
       </c>
       <c r="G93" t="n">
-        <v>46</v>
+        <v>1231</v>
       </c>
       <c r="H93" t="n">
-        <v>1053</v>
+        <v>2205</v>
       </c>
       <c r="I93" t="s">
-        <v>22</v>
+        <v>180</v>
       </c>
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="B94" t="n">
-        <v>1457</v>
+        <v>5261</v>
       </c>
       <c r="C94" t="s">
         <v>2</v>
       </c>
       <c r="D94" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E94" t="n">
-        <v>335</v>
+        <v>293</v>
       </c>
       <c r="F94" t="s">
-        <v>230</v>
+        <v>8</v>
       </c>
       <c r="G94" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="H94" t="n">
-        <v>1005</v>
+        <v>879</v>
       </c>
       <c r="I94" t="s">
-        <v>124</v>
+        <v>31</v>
       </c>
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>73</v>
+        <v>192</v>
       </c>
       <c r="B95" t="n">
-        <v>9261</v>
+        <v>9833</v>
       </c>
       <c r="C95" t="s">
-        <v>2</v>
+        <v>208</v>
       </c>
       <c r="D95" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E95" t="n">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="F95" t="s">
-        <v>90</v>
+        <v>174</v>
       </c>
       <c r="G95" t="n">
-        <v>73</v>
+        <v>1</v>
       </c>
       <c r="H95" t="n">
-        <v>1044</v>
+        <v>1020</v>
       </c>
       <c r="I95" t="s">
-        <v>147</v>
+        <v>51</v>
       </c>
     </row>
     <row r="96" spans="1:9">
       <c r="A96" t="s">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="B96" t="n">
-        <v>5292</v>
+        <v>1445</v>
       </c>
       <c r="C96" t="s">
         <v>2</v>
       </c>
       <c r="D96" t="n">
-        <v>29</v>
+        <v>188</v>
       </c>
       <c r="E96" t="n">
-        <v>313</v>
+        <v>450</v>
       </c>
       <c r="F96" t="s">
-        <v>168</v>
+        <v>25</v>
       </c>
       <c r="G96" t="n">
-        <v>85</v>
+        <v>562</v>
       </c>
       <c r="H96" t="n">
-        <v>939</v>
+        <v>1350</v>
       </c>
       <c r="I96" t="s">
-        <v>206</v>
+        <v>178</v>
       </c>
     </row>
     <row r="97" spans="1:9">
       <c r="A97" t="s">
-        <v>70</v>
+        <v>207</v>
       </c>
       <c r="B97" t="n">
-        <v>659</v>
+        <v>1459</v>
       </c>
       <c r="C97" t="s">
-        <v>221</v>
+        <v>2</v>
       </c>
       <c r="D97" t="n">
-        <v>189</v>
+        <v>1</v>
       </c>
       <c r="E97" t="n">
-        <v>517</v>
+        <v>334</v>
       </c>
       <c r="F97" t="s">
-        <v>76</v>
+        <v>143</v>
       </c>
       <c r="G97" t="n">
-        <v>565</v>
+        <v>1</v>
       </c>
       <c r="H97" t="n">
-        <v>1551</v>
+        <v>1002</v>
       </c>
       <c r="I97" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>